<commit_message>
Updating the dashboard and summary screen.
</commit_message>
<xml_diff>
--- a/app/data/MCCD-localisation.xlsx
+++ b/app/data/MCCD-localisation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/JALAT/GIT/medical-certificate-of-cause-of-death/app/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F6A8115-DB07-A241-B2E4-2400B1BC4192}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8124006-537B-CF48-94E6-6FFE4A96BC9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="14100" firstSheet="3" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="14100" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Using this document" sheetId="8" r:id="rId1"/>
@@ -68,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1952" uniqueCount="1360">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1956" uniqueCount="1363">
   <si>
     <r>
       <rPr>
@@ -5646,9 +5646,6 @@
     <t>globalWriteInWelsh</t>
   </si>
   <si>
-    <t>011</t>
-  </si>
-  <si>
     <t>globalEnglish</t>
   </si>
   <si>
@@ -5677,6 +5674,18 @@
   </si>
   <si>
     <t>apConfirmationPageWhatHappensNextContent</t>
+  </si>
+  <si>
+    <t>Attending practitioner's information</t>
+  </si>
+  <si>
+    <t>pmMCCDTasklistAttendingPractitionersInformation</t>
+  </si>
+  <si>
+    <t>Mynychu gwybodaeth ymarferydd</t>
+  </si>
+  <si>
+    <t>012</t>
   </si>
 </sst>
 </file>
@@ -6460,12 +6469,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -6567,6 +6570,12 @@
     </xf>
     <xf numFmtId="0" fontId="15" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -6947,538 +6956,538 @@
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A1" s="123" t="s">
+      <c r="A1" s="121" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="123"/>
-      <c r="C1" s="123"/>
-      <c r="D1" s="123"/>
-      <c r="E1" s="123"/>
-      <c r="F1" s="123"/>
-      <c r="G1" s="123"/>
-      <c r="H1" s="123"/>
-      <c r="I1" s="123"/>
-      <c r="J1" s="123"/>
-      <c r="K1" s="123"/>
-      <c r="L1" s="123"/>
+      <c r="B1" s="121"/>
+      <c r="C1" s="121"/>
+      <c r="D1" s="121"/>
+      <c r="E1" s="121"/>
+      <c r="F1" s="121"/>
+      <c r="G1" s="121"/>
+      <c r="H1" s="121"/>
+      <c r="I1" s="121"/>
+      <c r="J1" s="121"/>
+      <c r="K1" s="121"/>
+      <c r="L1" s="121"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A2" s="123"/>
-      <c r="B2" s="123"/>
-      <c r="C2" s="123"/>
-      <c r="D2" s="123"/>
-      <c r="E2" s="123"/>
-      <c r="F2" s="123"/>
-      <c r="G2" s="123"/>
-      <c r="H2" s="123"/>
-      <c r="I2" s="123"/>
-      <c r="J2" s="123"/>
-      <c r="K2" s="123"/>
-      <c r="L2" s="123"/>
+      <c r="A2" s="121"/>
+      <c r="B2" s="121"/>
+      <c r="C2" s="121"/>
+      <c r="D2" s="121"/>
+      <c r="E2" s="121"/>
+      <c r="F2" s="121"/>
+      <c r="G2" s="121"/>
+      <c r="H2" s="121"/>
+      <c r="I2" s="121"/>
+      <c r="J2" s="121"/>
+      <c r="K2" s="121"/>
+      <c r="L2" s="121"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A3" s="123"/>
-      <c r="B3" s="123"/>
-      <c r="C3" s="123"/>
-      <c r="D3" s="123"/>
-      <c r="E3" s="123"/>
-      <c r="F3" s="123"/>
-      <c r="G3" s="123"/>
-      <c r="H3" s="123"/>
-      <c r="I3" s="123"/>
-      <c r="J3" s="123"/>
-      <c r="K3" s="123"/>
-      <c r="L3" s="123"/>
+      <c r="A3" s="121"/>
+      <c r="B3" s="121"/>
+      <c r="C3" s="121"/>
+      <c r="D3" s="121"/>
+      <c r="E3" s="121"/>
+      <c r="F3" s="121"/>
+      <c r="G3" s="121"/>
+      <c r="H3" s="121"/>
+      <c r="I3" s="121"/>
+      <c r="J3" s="121"/>
+      <c r="K3" s="121"/>
+      <c r="L3" s="121"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A4" s="123"/>
-      <c r="B4" s="123"/>
-      <c r="C4" s="123"/>
-      <c r="D4" s="123"/>
-      <c r="E4" s="123"/>
-      <c r="F4" s="123"/>
-      <c r="G4" s="123"/>
-      <c r="H4" s="123"/>
-      <c r="I4" s="123"/>
-      <c r="J4" s="123"/>
-      <c r="K4" s="123"/>
-      <c r="L4" s="123"/>
+      <c r="A4" s="121"/>
+      <c r="B4" s="121"/>
+      <c r="C4" s="121"/>
+      <c r="D4" s="121"/>
+      <c r="E4" s="121"/>
+      <c r="F4" s="121"/>
+      <c r="G4" s="121"/>
+      <c r="H4" s="121"/>
+      <c r="I4" s="121"/>
+      <c r="J4" s="121"/>
+      <c r="K4" s="121"/>
+      <c r="L4" s="121"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A5" s="123"/>
-      <c r="B5" s="123"/>
-      <c r="C5" s="123"/>
-      <c r="D5" s="123"/>
-      <c r="E5" s="123"/>
-      <c r="F5" s="123"/>
-      <c r="G5" s="123"/>
-      <c r="H5" s="123"/>
-      <c r="I5" s="123"/>
-      <c r="J5" s="123"/>
-      <c r="K5" s="123"/>
-      <c r="L5" s="123"/>
+      <c r="A5" s="121"/>
+      <c r="B5" s="121"/>
+      <c r="C5" s="121"/>
+      <c r="D5" s="121"/>
+      <c r="E5" s="121"/>
+      <c r="F5" s="121"/>
+      <c r="G5" s="121"/>
+      <c r="H5" s="121"/>
+      <c r="I5" s="121"/>
+      <c r="J5" s="121"/>
+      <c r="K5" s="121"/>
+      <c r="L5" s="121"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A6" s="123"/>
-      <c r="B6" s="123"/>
-      <c r="C6" s="123"/>
-      <c r="D6" s="123"/>
-      <c r="E6" s="123"/>
-      <c r="F6" s="123"/>
-      <c r="G6" s="123"/>
-      <c r="H6" s="123"/>
-      <c r="I6" s="123"/>
-      <c r="J6" s="123"/>
-      <c r="K6" s="123"/>
-      <c r="L6" s="123"/>
+      <c r="A6" s="121"/>
+      <c r="B6" s="121"/>
+      <c r="C6" s="121"/>
+      <c r="D6" s="121"/>
+      <c r="E6" s="121"/>
+      <c r="F6" s="121"/>
+      <c r="G6" s="121"/>
+      <c r="H6" s="121"/>
+      <c r="I6" s="121"/>
+      <c r="J6" s="121"/>
+      <c r="K6" s="121"/>
+      <c r="L6" s="121"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A7" s="123"/>
-      <c r="B7" s="123"/>
-      <c r="C7" s="123"/>
-      <c r="D7" s="123"/>
-      <c r="E7" s="123"/>
-      <c r="F7" s="123"/>
-      <c r="G7" s="123"/>
-      <c r="H7" s="123"/>
-      <c r="I7" s="123"/>
-      <c r="J7" s="123"/>
-      <c r="K7" s="123"/>
-      <c r="L7" s="123"/>
+      <c r="A7" s="121"/>
+      <c r="B7" s="121"/>
+      <c r="C7" s="121"/>
+      <c r="D7" s="121"/>
+      <c r="E7" s="121"/>
+      <c r="F7" s="121"/>
+      <c r="G7" s="121"/>
+      <c r="H7" s="121"/>
+      <c r="I7" s="121"/>
+      <c r="J7" s="121"/>
+      <c r="K7" s="121"/>
+      <c r="L7" s="121"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A8" s="123"/>
-      <c r="B8" s="123"/>
-      <c r="C8" s="123"/>
-      <c r="D8" s="123"/>
-      <c r="E8" s="123"/>
-      <c r="F8" s="123"/>
-      <c r="G8" s="123"/>
-      <c r="H8" s="123"/>
-      <c r="I8" s="123"/>
-      <c r="J8" s="123"/>
-      <c r="K8" s="123"/>
-      <c r="L8" s="123"/>
+      <c r="A8" s="121"/>
+      <c r="B8" s="121"/>
+      <c r="C8" s="121"/>
+      <c r="D8" s="121"/>
+      <c r="E8" s="121"/>
+      <c r="F8" s="121"/>
+      <c r="G8" s="121"/>
+      <c r="H8" s="121"/>
+      <c r="I8" s="121"/>
+      <c r="J8" s="121"/>
+      <c r="K8" s="121"/>
+      <c r="L8" s="121"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A9" s="123"/>
-      <c r="B9" s="123"/>
-      <c r="C9" s="123"/>
-      <c r="D9" s="123"/>
-      <c r="E9" s="123"/>
-      <c r="F9" s="123"/>
-      <c r="G9" s="123"/>
-      <c r="H9" s="123"/>
-      <c r="I9" s="123"/>
-      <c r="J9" s="123"/>
-      <c r="K9" s="123"/>
-      <c r="L9" s="123"/>
+      <c r="A9" s="121"/>
+      <c r="B9" s="121"/>
+      <c r="C9" s="121"/>
+      <c r="D9" s="121"/>
+      <c r="E9" s="121"/>
+      <c r="F9" s="121"/>
+      <c r="G9" s="121"/>
+      <c r="H9" s="121"/>
+      <c r="I9" s="121"/>
+      <c r="J9" s="121"/>
+      <c r="K9" s="121"/>
+      <c r="L9" s="121"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A10" s="123"/>
-      <c r="B10" s="123"/>
-      <c r="C10" s="123"/>
-      <c r="D10" s="123"/>
-      <c r="E10" s="123"/>
-      <c r="F10" s="123"/>
-      <c r="G10" s="123"/>
-      <c r="H10" s="123"/>
-      <c r="I10" s="123"/>
-      <c r="J10" s="123"/>
-      <c r="K10" s="123"/>
-      <c r="L10" s="123"/>
+      <c r="A10" s="121"/>
+      <c r="B10" s="121"/>
+      <c r="C10" s="121"/>
+      <c r="D10" s="121"/>
+      <c r="E10" s="121"/>
+      <c r="F10" s="121"/>
+      <c r="G10" s="121"/>
+      <c r="H10" s="121"/>
+      <c r="I10" s="121"/>
+      <c r="J10" s="121"/>
+      <c r="K10" s="121"/>
+      <c r="L10" s="121"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A11" s="123"/>
-      <c r="B11" s="123"/>
-      <c r="C11" s="123"/>
-      <c r="D11" s="123"/>
-      <c r="E11" s="123"/>
-      <c r="F11" s="123"/>
-      <c r="G11" s="123"/>
-      <c r="H11" s="123"/>
-      <c r="I11" s="123"/>
-      <c r="J11" s="123"/>
-      <c r="K11" s="123"/>
-      <c r="L11" s="123"/>
+      <c r="A11" s="121"/>
+      <c r="B11" s="121"/>
+      <c r="C11" s="121"/>
+      <c r="D11" s="121"/>
+      <c r="E11" s="121"/>
+      <c r="F11" s="121"/>
+      <c r="G11" s="121"/>
+      <c r="H11" s="121"/>
+      <c r="I11" s="121"/>
+      <c r="J11" s="121"/>
+      <c r="K11" s="121"/>
+      <c r="L11" s="121"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A12" s="123"/>
-      <c r="B12" s="123"/>
-      <c r="C12" s="123"/>
-      <c r="D12" s="123"/>
-      <c r="E12" s="123"/>
-      <c r="F12" s="123"/>
-      <c r="G12" s="123"/>
-      <c r="H12" s="123"/>
-      <c r="I12" s="123"/>
-      <c r="J12" s="123"/>
-      <c r="K12" s="123"/>
-      <c r="L12" s="123"/>
+      <c r="A12" s="121"/>
+      <c r="B12" s="121"/>
+      <c r="C12" s="121"/>
+      <c r="D12" s="121"/>
+      <c r="E12" s="121"/>
+      <c r="F12" s="121"/>
+      <c r="G12" s="121"/>
+      <c r="H12" s="121"/>
+      <c r="I12" s="121"/>
+      <c r="J12" s="121"/>
+      <c r="K12" s="121"/>
+      <c r="L12" s="121"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A13" s="123"/>
-      <c r="B13" s="123"/>
-      <c r="C13" s="123"/>
-      <c r="D13" s="123"/>
-      <c r="E13" s="123"/>
-      <c r="F13" s="123"/>
-      <c r="G13" s="123"/>
-      <c r="H13" s="123"/>
-      <c r="I13" s="123"/>
-      <c r="J13" s="123"/>
-      <c r="K13" s="123"/>
-      <c r="L13" s="123"/>
+      <c r="A13" s="121"/>
+      <c r="B13" s="121"/>
+      <c r="C13" s="121"/>
+      <c r="D13" s="121"/>
+      <c r="E13" s="121"/>
+      <c r="F13" s="121"/>
+      <c r="G13" s="121"/>
+      <c r="H13" s="121"/>
+      <c r="I13" s="121"/>
+      <c r="J13" s="121"/>
+      <c r="K13" s="121"/>
+      <c r="L13" s="121"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A14" s="123"/>
-      <c r="B14" s="123"/>
-      <c r="C14" s="123"/>
-      <c r="D14" s="123"/>
-      <c r="E14" s="123"/>
-      <c r="F14" s="123"/>
-      <c r="G14" s="123"/>
-      <c r="H14" s="123"/>
-      <c r="I14" s="123"/>
-      <c r="J14" s="123"/>
-      <c r="K14" s="123"/>
-      <c r="L14" s="123"/>
+      <c r="A14" s="121"/>
+      <c r="B14" s="121"/>
+      <c r="C14" s="121"/>
+      <c r="D14" s="121"/>
+      <c r="E14" s="121"/>
+      <c r="F14" s="121"/>
+      <c r="G14" s="121"/>
+      <c r="H14" s="121"/>
+      <c r="I14" s="121"/>
+      <c r="J14" s="121"/>
+      <c r="K14" s="121"/>
+      <c r="L14" s="121"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A15" s="123"/>
-      <c r="B15" s="123"/>
-      <c r="C15" s="123"/>
-      <c r="D15" s="123"/>
-      <c r="E15" s="123"/>
-      <c r="F15" s="123"/>
-      <c r="G15" s="123"/>
-      <c r="H15" s="123"/>
-      <c r="I15" s="123"/>
-      <c r="J15" s="123"/>
-      <c r="K15" s="123"/>
-      <c r="L15" s="123"/>
+      <c r="A15" s="121"/>
+      <c r="B15" s="121"/>
+      <c r="C15" s="121"/>
+      <c r="D15" s="121"/>
+      <c r="E15" s="121"/>
+      <c r="F15" s="121"/>
+      <c r="G15" s="121"/>
+      <c r="H15" s="121"/>
+      <c r="I15" s="121"/>
+      <c r="J15" s="121"/>
+      <c r="K15" s="121"/>
+      <c r="L15" s="121"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A16" s="123"/>
-      <c r="B16" s="123"/>
-      <c r="C16" s="123"/>
-      <c r="D16" s="123"/>
-      <c r="E16" s="123"/>
-      <c r="F16" s="123"/>
-      <c r="G16" s="123"/>
-      <c r="H16" s="123"/>
-      <c r="I16" s="123"/>
-      <c r="J16" s="123"/>
-      <c r="K16" s="123"/>
-      <c r="L16" s="123"/>
+      <c r="A16" s="121"/>
+      <c r="B16" s="121"/>
+      <c r="C16" s="121"/>
+      <c r="D16" s="121"/>
+      <c r="E16" s="121"/>
+      <c r="F16" s="121"/>
+      <c r="G16" s="121"/>
+      <c r="H16" s="121"/>
+      <c r="I16" s="121"/>
+      <c r="J16" s="121"/>
+      <c r="K16" s="121"/>
+      <c r="L16" s="121"/>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A17" s="123"/>
-      <c r="B17" s="123"/>
-      <c r="C17" s="123"/>
-      <c r="D17" s="123"/>
-      <c r="E17" s="123"/>
-      <c r="F17" s="123"/>
-      <c r="G17" s="123"/>
-      <c r="H17" s="123"/>
-      <c r="I17" s="123"/>
-      <c r="J17" s="123"/>
-      <c r="K17" s="123"/>
-      <c r="L17" s="123"/>
+      <c r="A17" s="121"/>
+      <c r="B17" s="121"/>
+      <c r="C17" s="121"/>
+      <c r="D17" s="121"/>
+      <c r="E17" s="121"/>
+      <c r="F17" s="121"/>
+      <c r="G17" s="121"/>
+      <c r="H17" s="121"/>
+      <c r="I17" s="121"/>
+      <c r="J17" s="121"/>
+      <c r="K17" s="121"/>
+      <c r="L17" s="121"/>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A18" s="123"/>
-      <c r="B18" s="123"/>
-      <c r="C18" s="123"/>
-      <c r="D18" s="123"/>
-      <c r="E18" s="123"/>
-      <c r="F18" s="123"/>
-      <c r="G18" s="123"/>
-      <c r="H18" s="123"/>
-      <c r="I18" s="123"/>
-      <c r="J18" s="123"/>
-      <c r="K18" s="123"/>
-      <c r="L18" s="123"/>
+      <c r="A18" s="121"/>
+      <c r="B18" s="121"/>
+      <c r="C18" s="121"/>
+      <c r="D18" s="121"/>
+      <c r="E18" s="121"/>
+      <c r="F18" s="121"/>
+      <c r="G18" s="121"/>
+      <c r="H18" s="121"/>
+      <c r="I18" s="121"/>
+      <c r="J18" s="121"/>
+      <c r="K18" s="121"/>
+      <c r="L18" s="121"/>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A19" s="123"/>
-      <c r="B19" s="123"/>
-      <c r="C19" s="123"/>
-      <c r="D19" s="123"/>
-      <c r="E19" s="123"/>
-      <c r="F19" s="123"/>
-      <c r="G19" s="123"/>
-      <c r="H19" s="123"/>
-      <c r="I19" s="123"/>
-      <c r="J19" s="123"/>
-      <c r="K19" s="123"/>
-      <c r="L19" s="123"/>
+      <c r="A19" s="121"/>
+      <c r="B19" s="121"/>
+      <c r="C19" s="121"/>
+      <c r="D19" s="121"/>
+      <c r="E19" s="121"/>
+      <c r="F19" s="121"/>
+      <c r="G19" s="121"/>
+      <c r="H19" s="121"/>
+      <c r="I19" s="121"/>
+      <c r="J19" s="121"/>
+      <c r="K19" s="121"/>
+      <c r="L19" s="121"/>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A20" s="123"/>
-      <c r="B20" s="123"/>
-      <c r="C20" s="123"/>
-      <c r="D20" s="123"/>
-      <c r="E20" s="123"/>
-      <c r="F20" s="123"/>
-      <c r="G20" s="123"/>
-      <c r="H20" s="123"/>
-      <c r="I20" s="123"/>
-      <c r="J20" s="123"/>
-      <c r="K20" s="123"/>
-      <c r="L20" s="123"/>
+      <c r="A20" s="121"/>
+      <c r="B20" s="121"/>
+      <c r="C20" s="121"/>
+      <c r="D20" s="121"/>
+      <c r="E20" s="121"/>
+      <c r="F20" s="121"/>
+      <c r="G20" s="121"/>
+      <c r="H20" s="121"/>
+      <c r="I20" s="121"/>
+      <c r="J20" s="121"/>
+      <c r="K20" s="121"/>
+      <c r="L20" s="121"/>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A21" s="123"/>
-      <c r="B21" s="123"/>
-      <c r="C21" s="123"/>
-      <c r="D21" s="123"/>
-      <c r="E21" s="123"/>
-      <c r="F21" s="123"/>
-      <c r="G21" s="123"/>
-      <c r="H21" s="123"/>
-      <c r="I21" s="123"/>
-      <c r="J21" s="123"/>
-      <c r="K21" s="123"/>
-      <c r="L21" s="123"/>
+      <c r="A21" s="121"/>
+      <c r="B21" s="121"/>
+      <c r="C21" s="121"/>
+      <c r="D21" s="121"/>
+      <c r="E21" s="121"/>
+      <c r="F21" s="121"/>
+      <c r="G21" s="121"/>
+      <c r="H21" s="121"/>
+      <c r="I21" s="121"/>
+      <c r="J21" s="121"/>
+      <c r="K21" s="121"/>
+      <c r="L21" s="121"/>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A22" s="123"/>
-      <c r="B22" s="123"/>
-      <c r="C22" s="123"/>
-      <c r="D22" s="123"/>
-      <c r="E22" s="123"/>
-      <c r="F22" s="123"/>
-      <c r="G22" s="123"/>
-      <c r="H22" s="123"/>
-      <c r="I22" s="123"/>
-      <c r="J22" s="123"/>
-      <c r="K22" s="123"/>
-      <c r="L22" s="123"/>
+      <c r="A22" s="121"/>
+      <c r="B22" s="121"/>
+      <c r="C22" s="121"/>
+      <c r="D22" s="121"/>
+      <c r="E22" s="121"/>
+      <c r="F22" s="121"/>
+      <c r="G22" s="121"/>
+      <c r="H22" s="121"/>
+      <c r="I22" s="121"/>
+      <c r="J22" s="121"/>
+      <c r="K22" s="121"/>
+      <c r="L22" s="121"/>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A23" s="123"/>
-      <c r="B23" s="123"/>
-      <c r="C23" s="123"/>
-      <c r="D23" s="123"/>
-      <c r="E23" s="123"/>
-      <c r="F23" s="123"/>
-      <c r="G23" s="123"/>
-      <c r="H23" s="123"/>
-      <c r="I23" s="123"/>
-      <c r="J23" s="123"/>
-      <c r="K23" s="123"/>
-      <c r="L23" s="123"/>
+      <c r="A23" s="121"/>
+      <c r="B23" s="121"/>
+      <c r="C23" s="121"/>
+      <c r="D23" s="121"/>
+      <c r="E23" s="121"/>
+      <c r="F23" s="121"/>
+      <c r="G23" s="121"/>
+      <c r="H23" s="121"/>
+      <c r="I23" s="121"/>
+      <c r="J23" s="121"/>
+      <c r="K23" s="121"/>
+      <c r="L23" s="121"/>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A24" s="123"/>
-      <c r="B24" s="123"/>
-      <c r="C24" s="123"/>
-      <c r="D24" s="123"/>
-      <c r="E24" s="123"/>
-      <c r="F24" s="123"/>
-      <c r="G24" s="123"/>
-      <c r="H24" s="123"/>
-      <c r="I24" s="123"/>
-      <c r="J24" s="123"/>
-      <c r="K24" s="123"/>
-      <c r="L24" s="123"/>
+      <c r="A24" s="121"/>
+      <c r="B24" s="121"/>
+      <c r="C24" s="121"/>
+      <c r="D24" s="121"/>
+      <c r="E24" s="121"/>
+      <c r="F24" s="121"/>
+      <c r="G24" s="121"/>
+      <c r="H24" s="121"/>
+      <c r="I24" s="121"/>
+      <c r="J24" s="121"/>
+      <c r="K24" s="121"/>
+      <c r="L24" s="121"/>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A25" s="123"/>
-      <c r="B25" s="123"/>
-      <c r="C25" s="123"/>
-      <c r="D25" s="123"/>
-      <c r="E25" s="123"/>
-      <c r="F25" s="123"/>
-      <c r="G25" s="123"/>
-      <c r="H25" s="123"/>
-      <c r="I25" s="123"/>
-      <c r="J25" s="123"/>
-      <c r="K25" s="123"/>
-      <c r="L25" s="123"/>
+      <c r="A25" s="121"/>
+      <c r="B25" s="121"/>
+      <c r="C25" s="121"/>
+      <c r="D25" s="121"/>
+      <c r="E25" s="121"/>
+      <c r="F25" s="121"/>
+      <c r="G25" s="121"/>
+      <c r="H25" s="121"/>
+      <c r="I25" s="121"/>
+      <c r="J25" s="121"/>
+      <c r="K25" s="121"/>
+      <c r="L25" s="121"/>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A26" s="123"/>
-      <c r="B26" s="123"/>
-      <c r="C26" s="123"/>
-      <c r="D26" s="123"/>
-      <c r="E26" s="123"/>
-      <c r="F26" s="123"/>
-      <c r="G26" s="123"/>
-      <c r="H26" s="123"/>
-      <c r="I26" s="123"/>
-      <c r="J26" s="123"/>
-      <c r="K26" s="123"/>
-      <c r="L26" s="123"/>
+      <c r="A26" s="121"/>
+      <c r="B26" s="121"/>
+      <c r="C26" s="121"/>
+      <c r="D26" s="121"/>
+      <c r="E26" s="121"/>
+      <c r="F26" s="121"/>
+      <c r="G26" s="121"/>
+      <c r="H26" s="121"/>
+      <c r="I26" s="121"/>
+      <c r="J26" s="121"/>
+      <c r="K26" s="121"/>
+      <c r="L26" s="121"/>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A27" s="123"/>
-      <c r="B27" s="123"/>
-      <c r="C27" s="123"/>
-      <c r="D27" s="123"/>
-      <c r="E27" s="123"/>
-      <c r="F27" s="123"/>
-      <c r="G27" s="123"/>
-      <c r="H27" s="123"/>
-      <c r="I27" s="123"/>
-      <c r="J27" s="123"/>
-      <c r="K27" s="123"/>
-      <c r="L27" s="123"/>
+      <c r="A27" s="121"/>
+      <c r="B27" s="121"/>
+      <c r="C27" s="121"/>
+      <c r="D27" s="121"/>
+      <c r="E27" s="121"/>
+      <c r="F27" s="121"/>
+      <c r="G27" s="121"/>
+      <c r="H27" s="121"/>
+      <c r="I27" s="121"/>
+      <c r="J27" s="121"/>
+      <c r="K27" s="121"/>
+      <c r="L27" s="121"/>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A28" s="123"/>
-      <c r="B28" s="123"/>
-      <c r="C28" s="123"/>
-      <c r="D28" s="123"/>
-      <c r="E28" s="123"/>
-      <c r="F28" s="123"/>
-      <c r="G28" s="123"/>
-      <c r="H28" s="123"/>
-      <c r="I28" s="123"/>
-      <c r="J28" s="123"/>
-      <c r="K28" s="123"/>
-      <c r="L28" s="123"/>
+      <c r="A28" s="121"/>
+      <c r="B28" s="121"/>
+      <c r="C28" s="121"/>
+      <c r="D28" s="121"/>
+      <c r="E28" s="121"/>
+      <c r="F28" s="121"/>
+      <c r="G28" s="121"/>
+      <c r="H28" s="121"/>
+      <c r="I28" s="121"/>
+      <c r="J28" s="121"/>
+      <c r="K28" s="121"/>
+      <c r="L28" s="121"/>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A29" s="123"/>
-      <c r="B29" s="123"/>
-      <c r="C29" s="123"/>
-      <c r="D29" s="123"/>
-      <c r="E29" s="123"/>
-      <c r="F29" s="123"/>
-      <c r="G29" s="123"/>
-      <c r="H29" s="123"/>
-      <c r="I29" s="123"/>
-      <c r="J29" s="123"/>
-      <c r="K29" s="123"/>
-      <c r="L29" s="123"/>
+      <c r="A29" s="121"/>
+      <c r="B29" s="121"/>
+      <c r="C29" s="121"/>
+      <c r="D29" s="121"/>
+      <c r="E29" s="121"/>
+      <c r="F29" s="121"/>
+      <c r="G29" s="121"/>
+      <c r="H29" s="121"/>
+      <c r="I29" s="121"/>
+      <c r="J29" s="121"/>
+      <c r="K29" s="121"/>
+      <c r="L29" s="121"/>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A30" s="123"/>
-      <c r="B30" s="123"/>
-      <c r="C30" s="123"/>
-      <c r="D30" s="123"/>
-      <c r="E30" s="123"/>
-      <c r="F30" s="123"/>
-      <c r="G30" s="123"/>
-      <c r="H30" s="123"/>
-      <c r="I30" s="123"/>
-      <c r="J30" s="123"/>
-      <c r="K30" s="123"/>
-      <c r="L30" s="123"/>
+      <c r="A30" s="121"/>
+      <c r="B30" s="121"/>
+      <c r="C30" s="121"/>
+      <c r="D30" s="121"/>
+      <c r="E30" s="121"/>
+      <c r="F30" s="121"/>
+      <c r="G30" s="121"/>
+      <c r="H30" s="121"/>
+      <c r="I30" s="121"/>
+      <c r="J30" s="121"/>
+      <c r="K30" s="121"/>
+      <c r="L30" s="121"/>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A31" s="123"/>
-      <c r="B31" s="123"/>
-      <c r="C31" s="123"/>
-      <c r="D31" s="123"/>
-      <c r="E31" s="123"/>
-      <c r="F31" s="123"/>
-      <c r="G31" s="123"/>
-      <c r="H31" s="123"/>
-      <c r="I31" s="123"/>
-      <c r="J31" s="123"/>
-      <c r="K31" s="123"/>
-      <c r="L31" s="123"/>
+      <c r="A31" s="121"/>
+      <c r="B31" s="121"/>
+      <c r="C31" s="121"/>
+      <c r="D31" s="121"/>
+      <c r="E31" s="121"/>
+      <c r="F31" s="121"/>
+      <c r="G31" s="121"/>
+      <c r="H31" s="121"/>
+      <c r="I31" s="121"/>
+      <c r="J31" s="121"/>
+      <c r="K31" s="121"/>
+      <c r="L31" s="121"/>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A32" s="123"/>
-      <c r="B32" s="123"/>
-      <c r="C32" s="123"/>
-      <c r="D32" s="123"/>
-      <c r="E32" s="123"/>
-      <c r="F32" s="123"/>
-      <c r="G32" s="123"/>
-      <c r="H32" s="123"/>
-      <c r="I32" s="123"/>
-      <c r="J32" s="123"/>
-      <c r="K32" s="123"/>
-      <c r="L32" s="123"/>
+      <c r="A32" s="121"/>
+      <c r="B32" s="121"/>
+      <c r="C32" s="121"/>
+      <c r="D32" s="121"/>
+      <c r="E32" s="121"/>
+      <c r="F32" s="121"/>
+      <c r="G32" s="121"/>
+      <c r="H32" s="121"/>
+      <c r="I32" s="121"/>
+      <c r="J32" s="121"/>
+      <c r="K32" s="121"/>
+      <c r="L32" s="121"/>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A33" s="123"/>
-      <c r="B33" s="123"/>
-      <c r="C33" s="123"/>
-      <c r="D33" s="123"/>
-      <c r="E33" s="123"/>
-      <c r="F33" s="123"/>
-      <c r="G33" s="123"/>
-      <c r="H33" s="123"/>
-      <c r="I33" s="123"/>
-      <c r="J33" s="123"/>
-      <c r="K33" s="123"/>
-      <c r="L33" s="123"/>
+      <c r="A33" s="121"/>
+      <c r="B33" s="121"/>
+      <c r="C33" s="121"/>
+      <c r="D33" s="121"/>
+      <c r="E33" s="121"/>
+      <c r="F33" s="121"/>
+      <c r="G33" s="121"/>
+      <c r="H33" s="121"/>
+      <c r="I33" s="121"/>
+      <c r="J33" s="121"/>
+      <c r="K33" s="121"/>
+      <c r="L33" s="121"/>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A34" s="123"/>
-      <c r="B34" s="123"/>
-      <c r="C34" s="123"/>
-      <c r="D34" s="123"/>
-      <c r="E34" s="123"/>
-      <c r="F34" s="123"/>
-      <c r="G34" s="123"/>
-      <c r="H34" s="123"/>
-      <c r="I34" s="123"/>
-      <c r="J34" s="123"/>
-      <c r="K34" s="123"/>
-      <c r="L34" s="123"/>
+      <c r="A34" s="121"/>
+      <c r="B34" s="121"/>
+      <c r="C34" s="121"/>
+      <c r="D34" s="121"/>
+      <c r="E34" s="121"/>
+      <c r="F34" s="121"/>
+      <c r="G34" s="121"/>
+      <c r="H34" s="121"/>
+      <c r="I34" s="121"/>
+      <c r="J34" s="121"/>
+      <c r="K34" s="121"/>
+      <c r="L34" s="121"/>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A35" s="123"/>
-      <c r="B35" s="123"/>
-      <c r="C35" s="123"/>
-      <c r="D35" s="123"/>
-      <c r="E35" s="123"/>
-      <c r="F35" s="123"/>
-      <c r="G35" s="123"/>
-      <c r="H35" s="123"/>
-      <c r="I35" s="123"/>
-      <c r="J35" s="123"/>
-      <c r="K35" s="123"/>
-      <c r="L35" s="123"/>
+      <c r="A35" s="121"/>
+      <c r="B35" s="121"/>
+      <c r="C35" s="121"/>
+      <c r="D35" s="121"/>
+      <c r="E35" s="121"/>
+      <c r="F35" s="121"/>
+      <c r="G35" s="121"/>
+      <c r="H35" s="121"/>
+      <c r="I35" s="121"/>
+      <c r="J35" s="121"/>
+      <c r="K35" s="121"/>
+      <c r="L35" s="121"/>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A36" s="123"/>
-      <c r="B36" s="123"/>
-      <c r="C36" s="123"/>
-      <c r="D36" s="123"/>
-      <c r="E36" s="123"/>
-      <c r="F36" s="123"/>
-      <c r="G36" s="123"/>
-      <c r="H36" s="123"/>
-      <c r="I36" s="123"/>
-      <c r="J36" s="123"/>
-      <c r="K36" s="123"/>
-      <c r="L36" s="123"/>
+      <c r="A36" s="121"/>
+      <c r="B36" s="121"/>
+      <c r="C36" s="121"/>
+      <c r="D36" s="121"/>
+      <c r="E36" s="121"/>
+      <c r="F36" s="121"/>
+      <c r="G36" s="121"/>
+      <c r="H36" s="121"/>
+      <c r="I36" s="121"/>
+      <c r="J36" s="121"/>
+      <c r="K36" s="121"/>
+      <c r="L36" s="121"/>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A37" s="123"/>
-      <c r="B37" s="123"/>
-      <c r="C37" s="123"/>
-      <c r="D37" s="123"/>
-      <c r="E37" s="123"/>
-      <c r="F37" s="123"/>
-      <c r="G37" s="123"/>
-      <c r="H37" s="123"/>
-      <c r="I37" s="123"/>
-      <c r="J37" s="123"/>
-      <c r="K37" s="123"/>
-      <c r="L37" s="123"/>
+      <c r="A37" s="121"/>
+      <c r="B37" s="121"/>
+      <c r="C37" s="121"/>
+      <c r="D37" s="121"/>
+      <c r="E37" s="121"/>
+      <c r="F37" s="121"/>
+      <c r="G37" s="121"/>
+      <c r="H37" s="121"/>
+      <c r="I37" s="121"/>
+      <c r="J37" s="121"/>
+      <c r="K37" s="121"/>
+      <c r="L37" s="121"/>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A38" s="123"/>
-      <c r="B38" s="123"/>
-      <c r="C38" s="123"/>
-      <c r="D38" s="123"/>
-      <c r="E38" s="123"/>
-      <c r="F38" s="123"/>
-      <c r="G38" s="123"/>
-      <c r="H38" s="123"/>
-      <c r="I38" s="123"/>
-      <c r="J38" s="123"/>
-      <c r="K38" s="123"/>
-      <c r="L38" s="123"/>
+      <c r="A38" s="121"/>
+      <c r="B38" s="121"/>
+      <c r="C38" s="121"/>
+      <c r="D38" s="121"/>
+      <c r="E38" s="121"/>
+      <c r="F38" s="121"/>
+      <c r="G38" s="121"/>
+      <c r="H38" s="121"/>
+      <c r="I38" s="121"/>
+      <c r="J38" s="121"/>
+      <c r="K38" s="121"/>
+      <c r="L38" s="121"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -7493,7 +7502,7 @@
   <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
@@ -7736,8 +7745,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{124C2F8F-96ED-4E65-B816-FFFEB93DC889}">
   <dimension ref="A1:F23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
@@ -7773,14 +7782,14 @@
       </c>
     </row>
     <row r="2" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="155" t="s">
+      <c r="A2" s="153" t="s">
         <v>1191</v>
       </c>
-      <c r="B2" s="156"/>
-      <c r="C2" s="156"/>
-      <c r="D2" s="156"/>
-      <c r="E2" s="156"/>
-      <c r="F2" s="156"/>
+      <c r="B2" s="154"/>
+      <c r="C2" s="154"/>
+      <c r="D2" s="154"/>
+      <c r="E2" s="154"/>
+      <c r="F2" s="154"/>
     </row>
     <row r="3" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
@@ -8000,21 +8009,21 @@
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A18" s="155" t="s">
+      <c r="A18" s="153" t="s">
         <v>1240</v>
       </c>
-      <c r="B18" s="156"/>
-      <c r="C18" s="156"/>
-      <c r="D18" s="156"/>
-      <c r="E18" s="156"/>
-      <c r="F18" s="156"/>
+      <c r="B18" s="154"/>
+      <c r="C18" s="154"/>
+      <c r="D18" s="154"/>
+      <c r="E18" s="154"/>
+      <c r="F18" s="154"/>
     </row>
     <row r="19" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A19" s="5" t="s">
         <v>188</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>1356</v>
+        <v>1355</v>
       </c>
       <c r="C19" s="6" t="s">
         <v>1241</v>
@@ -8031,7 +8040,7 @@
         <v>202</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>1357</v>
+        <v>1356</v>
       </c>
       <c r="C20" s="77" t="s">
         <v>1243</v>
@@ -8045,7 +8054,7 @@
         <v>196</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>1358</v>
+        <v>1357</v>
       </c>
       <c r="C21" s="6" t="s">
         <v>1199</v>
@@ -8059,7 +8068,7 @@
         <v>202</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>1359</v>
+        <v>1358</v>
       </c>
       <c r="C22" s="6" t="s">
         <v>1245</v>
@@ -8087,9 +8096,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F65"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A46" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D60" sqref="D60"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -8127,14 +8136,14 @@
       <c r="B2" s="120" t="s">
         <v>1293</v>
       </c>
-      <c r="C2" s="121" t="s">
-        <v>1349</v>
+      <c r="C2" s="155" t="s">
+        <v>1362</v>
       </c>
       <c r="D2" s="120" t="s">
         <v>1294</v>
       </c>
-      <c r="E2" s="122" t="s">
-        <v>1349</v>
+      <c r="E2" s="156" t="s">
+        <v>1362</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="53.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -9119,24 +9128,24 @@
     </row>
     <row r="64" spans="2:5" ht="16" x14ac:dyDescent="0.2">
       <c r="B64" s="1" t="s">
-        <v>1350</v>
+        <v>1349</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>1352</v>
+        <v>1351</v>
       </c>
       <c r="E64" s="40" t="s">
-        <v>1354</v>
+        <v>1353</v>
       </c>
     </row>
     <row r="65" spans="2:5" ht="16" x14ac:dyDescent="0.2">
       <c r="B65" s="1" t="s">
-        <v>1351</v>
+        <v>1350</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>1353</v>
+        <v>1352</v>
       </c>
       <c r="E65" s="40" t="s">
-        <v>1355</v>
+        <v>1354</v>
       </c>
     </row>
   </sheetData>
@@ -9388,7 +9397,7 @@
   <dimension ref="A1:F30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
@@ -9887,7 +9896,7 @@
   <dimension ref="A1:F330"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
@@ -9923,13 +9932,13 @@
       </c>
     </row>
     <row r="2" spans="1:6" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="127" t="s">
+      <c r="A2" s="125" t="s">
         <v>313</v>
       </c>
-      <c r="B2" s="128"/>
-      <c r="C2" s="128"/>
-      <c r="D2" s="128"/>
-      <c r="E2" s="129"/>
+      <c r="B2" s="126"/>
+      <c r="C2" s="126"/>
+      <c r="D2" s="126"/>
+      <c r="E2" s="127"/>
       <c r="F2" s="33"/>
     </row>
     <row r="3" spans="1:6" ht="48" x14ac:dyDescent="0.2">
@@ -10057,13 +10066,13 @@
       <c r="F9" s="88"/>
     </row>
     <row r="10" spans="1:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="130" t="s">
+      <c r="A10" s="128" t="s">
         <v>342</v>
       </c>
-      <c r="B10" s="131"/>
-      <c r="C10" s="131"/>
-      <c r="D10" s="131"/>
-      <c r="E10" s="132"/>
+      <c r="B10" s="129"/>
+      <c r="C10" s="129"/>
+      <c r="D10" s="129"/>
+      <c r="E10" s="130"/>
       <c r="F10" s="88"/>
     </row>
     <row r="11" spans="1:6" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -10119,13 +10128,13 @@
       <c r="F13" s="88"/>
     </row>
     <row r="14" spans="1:6" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="124" t="s">
+      <c r="A14" s="122" t="s">
         <v>347</v>
       </c>
-      <c r="B14" s="125"/>
-      <c r="C14" s="125"/>
-      <c r="D14" s="125"/>
-      <c r="E14" s="126"/>
+      <c r="B14" s="123"/>
+      <c r="C14" s="123"/>
+      <c r="D14" s="123"/>
+      <c r="E14" s="124"/>
       <c r="F14" s="88"/>
     </row>
     <row r="15" spans="1:6" ht="48" x14ac:dyDescent="0.2">
@@ -10269,13 +10278,13 @@
       <c r="F23" s="88"/>
     </row>
     <row r="24" spans="1:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="124" t="s">
+      <c r="A24" s="122" t="s">
         <v>371</v>
       </c>
-      <c r="B24" s="125"/>
-      <c r="C24" s="125"/>
-      <c r="D24" s="125"/>
-      <c r="E24" s="126"/>
+      <c r="B24" s="123"/>
+      <c r="C24" s="123"/>
+      <c r="D24" s="123"/>
+      <c r="E24" s="124"/>
       <c r="F24" s="88"/>
     </row>
     <row r="25" spans="1:6" ht="32" x14ac:dyDescent="0.2">
@@ -10547,13 +10556,13 @@
       <c r="F42" s="88"/>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A43" s="124" t="s">
+      <c r="A43" s="122" t="s">
         <v>416</v>
       </c>
-      <c r="B43" s="125"/>
-      <c r="C43" s="125"/>
-      <c r="D43" s="125"/>
-      <c r="E43" s="126"/>
+      <c r="B43" s="123"/>
+      <c r="C43" s="123"/>
+      <c r="D43" s="123"/>
+      <c r="E43" s="124"/>
       <c r="F43" s="88"/>
     </row>
     <row r="44" spans="1:6" ht="32" x14ac:dyDescent="0.2">
@@ -10755,13 +10764,13 @@
       <c r="F56" s="88"/>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A57" s="124" t="s">
+      <c r="A57" s="122" t="s">
         <v>448</v>
       </c>
-      <c r="B57" s="125"/>
-      <c r="C57" s="125"/>
-      <c r="D57" s="125"/>
-      <c r="E57" s="126"/>
+      <c r="B57" s="123"/>
+      <c r="C57" s="123"/>
+      <c r="D57" s="123"/>
+      <c r="E57" s="124"/>
       <c r="F57" s="88"/>
     </row>
     <row r="58" spans="1:6" ht="64" x14ac:dyDescent="0.2">
@@ -10819,13 +10828,13 @@
       <c r="F60" s="88"/>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A61" s="124" t="s">
+      <c r="A61" s="122" t="s">
         <v>463</v>
       </c>
-      <c r="B61" s="125"/>
-      <c r="C61" s="125"/>
-      <c r="D61" s="125"/>
-      <c r="E61" s="126"/>
+      <c r="B61" s="123"/>
+      <c r="C61" s="123"/>
+      <c r="D61" s="123"/>
+      <c r="E61" s="124"/>
       <c r="F61" s="88"/>
     </row>
     <row r="62" spans="1:6" ht="48" x14ac:dyDescent="0.2">
@@ -10875,13 +10884,13 @@
       <c r="F64" s="88"/>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A65" s="124" t="s">
+      <c r="A65" s="122" t="s">
         <v>468</v>
       </c>
-      <c r="B65" s="125"/>
-      <c r="C65" s="125"/>
-      <c r="D65" s="125"/>
-      <c r="E65" s="126"/>
+      <c r="B65" s="123"/>
+      <c r="C65" s="123"/>
+      <c r="D65" s="123"/>
+      <c r="E65" s="124"/>
       <c r="F65" s="88"/>
     </row>
     <row r="66" spans="1:6" ht="32" x14ac:dyDescent="0.2">
@@ -11099,13 +11108,13 @@
       <c r="F79" s="88"/>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A80" s="124" t="s">
+      <c r="A80" s="122" t="s">
         <v>489</v>
       </c>
-      <c r="B80" s="125"/>
-      <c r="C80" s="125"/>
-      <c r="D80" s="125"/>
-      <c r="E80" s="126"/>
+      <c r="B80" s="123"/>
+      <c r="C80" s="123"/>
+      <c r="D80" s="123"/>
+      <c r="E80" s="124"/>
       <c r="F80" s="88"/>
     </row>
     <row r="81" spans="1:6" ht="62.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -11255,13 +11264,13 @@
       <c r="F89" s="88"/>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A90" s="124" t="s">
+      <c r="A90" s="122" t="s">
         <v>514</v>
       </c>
-      <c r="B90" s="125"/>
-      <c r="C90" s="125"/>
-      <c r="D90" s="125"/>
-      <c r="E90" s="126"/>
+      <c r="B90" s="123"/>
+      <c r="C90" s="123"/>
+      <c r="D90" s="123"/>
+      <c r="E90" s="124"/>
       <c r="F90" s="88"/>
     </row>
     <row r="91" spans="1:6" ht="48" x14ac:dyDescent="0.2">
@@ -11723,13 +11732,13 @@
       <c r="F120" s="88"/>
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A121" s="124" t="s">
+      <c r="A121" s="122" t="s">
         <v>596</v>
       </c>
-      <c r="B121" s="125"/>
-      <c r="C121" s="125"/>
-      <c r="D121" s="125"/>
-      <c r="E121" s="126"/>
+      <c r="B121" s="123"/>
+      <c r="C121" s="123"/>
+      <c r="D121" s="123"/>
+      <c r="E121" s="124"/>
       <c r="F121" s="88"/>
     </row>
     <row r="122" spans="1:6" ht="32" x14ac:dyDescent="0.2">
@@ -11917,13 +11926,13 @@
       <c r="F134" s="88"/>
     </row>
     <row r="135" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A135" s="124" t="s">
+      <c r="A135" s="122" t="s">
         <v>618</v>
       </c>
-      <c r="B135" s="125"/>
-      <c r="C135" s="125"/>
-      <c r="D135" s="125"/>
-      <c r="E135" s="126"/>
+      <c r="B135" s="123"/>
+      <c r="C135" s="123"/>
+      <c r="D135" s="123"/>
+      <c r="E135" s="124"/>
       <c r="F135" s="88"/>
     </row>
     <row r="136" spans="1:6" ht="64" x14ac:dyDescent="0.2">
@@ -12051,13 +12060,13 @@
       <c r="F143" s="88"/>
     </row>
     <row r="144" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A144" s="124" t="s">
+      <c r="A144" s="122" t="s">
         <v>639</v>
       </c>
-      <c r="B144" s="125"/>
-      <c r="C144" s="125"/>
-      <c r="D144" s="125"/>
-      <c r="E144" s="126"/>
+      <c r="B144" s="123"/>
+      <c r="C144" s="123"/>
+      <c r="D144" s="123"/>
+      <c r="E144" s="124"/>
       <c r="F144" s="88"/>
     </row>
     <row r="145" spans="1:6" ht="48" x14ac:dyDescent="0.2">
@@ -12185,13 +12194,13 @@
       <c r="F152" s="88"/>
     </row>
     <row r="153" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A153" s="124" t="s">
+      <c r="A153" s="122" t="s">
         <v>661</v>
       </c>
-      <c r="B153" s="125"/>
-      <c r="C153" s="125"/>
-      <c r="D153" s="125"/>
-      <c r="E153" s="126"/>
+      <c r="B153" s="123"/>
+      <c r="C153" s="123"/>
+      <c r="D153" s="123"/>
+      <c r="E153" s="124"/>
       <c r="F153" s="88"/>
     </row>
     <row r="154" spans="1:6" ht="48" x14ac:dyDescent="0.2">
@@ -12309,13 +12318,13 @@
       <c r="F160" s="88"/>
     </row>
     <row r="161" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A161" s="124" t="s">
+      <c r="A161" s="122" t="s">
         <v>677</v>
       </c>
-      <c r="B161" s="125"/>
-      <c r="C161" s="125"/>
-      <c r="D161" s="125"/>
-      <c r="E161" s="126"/>
+      <c r="B161" s="123"/>
+      <c r="C161" s="123"/>
+      <c r="D161" s="123"/>
+      <c r="E161" s="124"/>
       <c r="F161" s="88"/>
     </row>
     <row r="162" spans="1:6" ht="32" x14ac:dyDescent="0.2">
@@ -12489,13 +12498,13 @@
       <c r="F172" s="88"/>
     </row>
     <row r="173" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A173" s="124" t="s">
+      <c r="A173" s="122" t="s">
         <v>697</v>
       </c>
-      <c r="B173" s="125"/>
-      <c r="C173" s="125"/>
-      <c r="D173" s="125"/>
-      <c r="E173" s="126"/>
+      <c r="B173" s="123"/>
+      <c r="C173" s="123"/>
+      <c r="D173" s="123"/>
+      <c r="E173" s="124"/>
       <c r="F173" s="88"/>
     </row>
     <row r="174" spans="1:6" ht="32" x14ac:dyDescent="0.2">
@@ -12547,13 +12556,13 @@
       <c r="F176" s="88"/>
     </row>
     <row r="177" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A177" s="124" t="s">
+      <c r="A177" s="122" t="s">
         <v>706</v>
       </c>
-      <c r="B177" s="125"/>
-      <c r="C177" s="125"/>
-      <c r="D177" s="125"/>
-      <c r="E177" s="126"/>
+      <c r="B177" s="123"/>
+      <c r="C177" s="123"/>
+      <c r="D177" s="123"/>
+      <c r="E177" s="124"/>
       <c r="F177" s="88"/>
     </row>
     <row r="178" spans="1:6" ht="64" x14ac:dyDescent="0.2">
@@ -12639,13 +12648,13 @@
       <c r="F182" s="88"/>
     </row>
     <row r="183" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A183" s="124" t="s">
+      <c r="A183" s="122" t="s">
         <v>724</v>
       </c>
-      <c r="B183" s="125"/>
-      <c r="C183" s="125"/>
-      <c r="D183" s="125"/>
-      <c r="E183" s="126"/>
+      <c r="B183" s="123"/>
+      <c r="C183" s="123"/>
+      <c r="D183" s="123"/>
+      <c r="E183" s="124"/>
       <c r="F183" s="88"/>
     </row>
     <row r="184" spans="1:6" ht="32" x14ac:dyDescent="0.2">
@@ -12785,13 +12794,13 @@
       <c r="F192" s="88"/>
     </row>
     <row r="193" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A193" s="124" t="s">
+      <c r="A193" s="122" t="s">
         <v>737</v>
       </c>
-      <c r="B193" s="125"/>
-      <c r="C193" s="125"/>
-      <c r="D193" s="125"/>
-      <c r="E193" s="126"/>
+      <c r="B193" s="123"/>
+      <c r="C193" s="123"/>
+      <c r="D193" s="123"/>
+      <c r="E193" s="124"/>
       <c r="F193" s="88"/>
     </row>
     <row r="194" spans="1:6" ht="48" x14ac:dyDescent="0.2">
@@ -12877,13 +12886,13 @@
       <c r="F198" s="88"/>
     </row>
     <row r="199" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A199" s="124" t="s">
+      <c r="A199" s="122" t="s">
         <v>747</v>
       </c>
-      <c r="B199" s="125"/>
-      <c r="C199" s="125"/>
-      <c r="D199" s="125"/>
-      <c r="E199" s="126"/>
+      <c r="B199" s="123"/>
+      <c r="C199" s="123"/>
+      <c r="D199" s="123"/>
+      <c r="E199" s="124"/>
       <c r="F199" s="88"/>
     </row>
     <row r="200" spans="1:6" ht="32" x14ac:dyDescent="0.2">
@@ -13041,13 +13050,13 @@
       <c r="F209" s="88"/>
     </row>
     <row r="210" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A210" s="124" t="s">
+      <c r="A210" s="122" t="s">
         <v>761</v>
       </c>
-      <c r="B210" s="125"/>
-      <c r="C210" s="125"/>
-      <c r="D210" s="125"/>
-      <c r="E210" s="126"/>
+      <c r="B210" s="123"/>
+      <c r="C210" s="123"/>
+      <c r="D210" s="123"/>
+      <c r="E210" s="124"/>
       <c r="F210" s="88"/>
     </row>
     <row r="211" spans="1:6" ht="48" x14ac:dyDescent="0.2">
@@ -14042,6 +14051,18 @@
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="A210:E210"/>
+    <mergeCell ref="A173:E173"/>
+    <mergeCell ref="A177:E177"/>
+    <mergeCell ref="A183:E183"/>
+    <mergeCell ref="A193:E193"/>
+    <mergeCell ref="A199:E199"/>
+    <mergeCell ref="A57:E57"/>
+    <mergeCell ref="A2:E2"/>
+    <mergeCell ref="A10:E10"/>
+    <mergeCell ref="A14:E14"/>
+    <mergeCell ref="A24:E24"/>
+    <mergeCell ref="A43:E43"/>
     <mergeCell ref="A161:E161"/>
     <mergeCell ref="A153:E153"/>
     <mergeCell ref="A61:E61"/>
@@ -14051,18 +14072,6 @@
     <mergeCell ref="A135:E135"/>
     <mergeCell ref="A144:E144"/>
     <mergeCell ref="A90:E90"/>
-    <mergeCell ref="A57:E57"/>
-    <mergeCell ref="A2:E2"/>
-    <mergeCell ref="A10:E10"/>
-    <mergeCell ref="A14:E14"/>
-    <mergeCell ref="A24:E24"/>
-    <mergeCell ref="A43:E43"/>
-    <mergeCell ref="A210:E210"/>
-    <mergeCell ref="A173:E173"/>
-    <mergeCell ref="A177:E177"/>
-    <mergeCell ref="A183:E183"/>
-    <mergeCell ref="A193:E193"/>
-    <mergeCell ref="A199:E199"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -14070,11 +14079,11 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E7FE5E2-8B99-45DF-8804-30523FDA4B3A}">
-  <dimension ref="A1:F53"/>
+  <dimension ref="A1:F54"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A43" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F48" sqref="F48"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E8" sqref="A8:E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -14109,13 +14118,13 @@
       </c>
     </row>
     <row r="2" spans="1:6" s="24" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="136" t="s">
+      <c r="A2" s="134" t="s">
         <v>812</v>
       </c>
-      <c r="B2" s="137"/>
-      <c r="C2" s="137"/>
-      <c r="D2" s="137"/>
-      <c r="E2" s="138"/>
+      <c r="B2" s="135"/>
+      <c r="C2" s="135"/>
+      <c r="D2" s="135"/>
+      <c r="E2" s="136"/>
     </row>
     <row r="3" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="19" t="s">
@@ -14189,32 +14198,32 @@
       </c>
     </row>
     <row r="8" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A8" s="18" t="s">
+      <c r="A8" s="19" t="s">
+        <v>816</v>
+      </c>
+      <c r="B8" s="19" t="s">
+        <v>1360</v>
+      </c>
+      <c r="C8" s="21" t="s">
+        <v>1359</v>
+      </c>
+      <c r="E8" s="46" t="s">
+        <v>1361</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A9" s="18" t="s">
         <v>648</v>
       </c>
-      <c r="B8" s="28" t="s">
+      <c r="B9" s="28" t="s">
         <v>825</v>
       </c>
-      <c r="C8" s="27" t="s">
+      <c r="C9" s="27" t="s">
         <v>826</v>
       </c>
-      <c r="D8" s="18"/>
-      <c r="E8" s="46" t="s">
+      <c r="D9" s="18"/>
+      <c r="E9" s="46" t="s">
         <v>827</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A9" s="19" t="s">
-        <v>828</v>
-      </c>
-      <c r="B9" s="19" t="s">
-        <v>829</v>
-      </c>
-      <c r="C9" s="21" t="s">
-        <v>150</v>
-      </c>
-      <c r="E9" s="46" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="16" x14ac:dyDescent="0.2">
@@ -14222,56 +14231,53 @@
         <v>828</v>
       </c>
       <c r="B10" s="19" t="s">
+        <v>829</v>
+      </c>
+      <c r="C10" s="21" t="s">
+        <v>150</v>
+      </c>
+      <c r="E10" s="46" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A11" s="19" t="s">
+        <v>828</v>
+      </c>
+      <c r="B11" s="19" t="s">
         <v>830</v>
       </c>
-      <c r="C10" s="21" t="s">
+      <c r="C11" s="21" t="s">
         <v>138</v>
       </c>
-      <c r="E10" s="46" t="s">
+      <c r="E11" s="46" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="11" spans="1:6" s="24" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="136" t="s">
+    <row r="12" spans="1:6" s="24" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="134" t="s">
         <v>831</v>
       </c>
-      <c r="B11" s="137"/>
-      <c r="C11" s="137"/>
-      <c r="D11" s="137"/>
-      <c r="E11" s="138"/>
-    </row>
-    <row r="12" spans="1:6" ht="48" x14ac:dyDescent="0.2">
-      <c r="A12" s="19" t="s">
+      <c r="B12" s="135"/>
+      <c r="C12" s="135"/>
+      <c r="D12" s="135"/>
+      <c r="E12" s="136"/>
+    </row>
+    <row r="13" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+      <c r="A13" s="19" t="s">
         <v>188</v>
       </c>
-      <c r="B12" s="19" t="s">
+      <c r="B13" s="19" t="s">
         <v>832</v>
       </c>
-      <c r="C12" s="21" t="s">
+      <c r="C13" s="21" t="s">
         <v>833</v>
       </c>
-      <c r="D12" s="5" t="s">
+      <c r="D13" s="5" t="s">
         <v>834</v>
       </c>
-      <c r="E12" s="46" t="s">
+      <c r="E13" s="46" t="s">
         <v>835</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="32" x14ac:dyDescent="0.2">
-      <c r="A13" s="19" t="s">
-        <v>82</v>
-      </c>
-      <c r="B13" s="19" t="s">
-        <v>836</v>
-      </c>
-      <c r="C13" s="21" t="s">
-        <v>837</v>
-      </c>
-      <c r="D13" s="19" t="s">
-        <v>838</v>
-      </c>
-      <c r="E13" s="46" t="s">
-        <v>839</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="32" x14ac:dyDescent="0.2">
@@ -14279,467 +14285,467 @@
         <v>82</v>
       </c>
       <c r="B14" s="19" t="s">
-        <v>840</v>
+        <v>836</v>
       </c>
       <c r="C14" s="21" t="s">
-        <v>841</v>
+        <v>837</v>
       </c>
       <c r="D14" s="19" t="s">
         <v>838</v>
       </c>
       <c r="E14" s="46" t="s">
-        <v>842</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+        <v>839</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A15" s="19" t="s">
         <v>82</v>
       </c>
       <c r="B15" s="19" t="s">
-        <v>843</v>
+        <v>840</v>
       </c>
       <c r="C15" s="21" t="s">
-        <v>844</v>
+        <v>841</v>
       </c>
       <c r="D15" s="19" t="s">
         <v>838</v>
       </c>
       <c r="E15" s="46" t="s">
-        <v>845</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+        <v>842</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" s="19" t="s">
         <v>82</v>
       </c>
       <c r="B16" s="19" t="s">
-        <v>846</v>
+        <v>843</v>
       </c>
       <c r="C16" s="21" t="s">
-        <v>1295</v>
+        <v>844</v>
       </c>
       <c r="D16" s="19" t="s">
         <v>838</v>
       </c>
       <c r="E16" s="46" t="s">
+        <v>845</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+      <c r="A17" s="19" t="s">
+        <v>82</v>
+      </c>
+      <c r="B17" s="19" t="s">
+        <v>846</v>
+      </c>
+      <c r="C17" s="21" t="s">
+        <v>1295</v>
+      </c>
+      <c r="D17" s="19" t="s">
+        <v>838</v>
+      </c>
+      <c r="E17" s="46" t="s">
         <v>1296</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" ht="80" x14ac:dyDescent="0.2">
-      <c r="A17" s="18" t="s">
-        <v>352</v>
-      </c>
-      <c r="B17" s="28" t="s">
-        <v>847</v>
-      </c>
-      <c r="C17" s="27"/>
-      <c r="D17" s="18" t="s">
-        <v>848</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="80" x14ac:dyDescent="0.2">
       <c r="A18" s="18" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
       <c r="B18" s="28" t="s">
-        <v>849</v>
+        <v>847</v>
       </c>
       <c r="C18" s="27"/>
       <c r="D18" s="18" t="s">
+        <v>848</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="80" x14ac:dyDescent="0.2">
+      <c r="A19" s="18" t="s">
+        <v>355</v>
+      </c>
+      <c r="B19" s="28" t="s">
+        <v>849</v>
+      </c>
+      <c r="C19" s="27"/>
+      <c r="D19" s="18" t="s">
         <v>850</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="145" t="s">
+    <row r="20" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="143" t="s">
         <v>851</v>
       </c>
-      <c r="B19" s="146"/>
-      <c r="C19" s="146"/>
-      <c r="D19" s="146"/>
-      <c r="E19" s="147"/>
-    </row>
-    <row r="20" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A20" s="5" t="s">
+      <c r="B20" s="144"/>
+      <c r="C20" s="144"/>
+      <c r="D20" s="144"/>
+      <c r="E20" s="145"/>
+    </row>
+    <row r="21" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A21" s="5" t="s">
         <v>852</v>
       </c>
-      <c r="B20" s="5" t="s">
+      <c r="B21" s="5" t="s">
         <v>1297</v>
       </c>
-      <c r="C20" s="6" t="s">
+      <c r="C21" s="6" t="s">
         <v>853</v>
-      </c>
-      <c r="D20" s="82"/>
-      <c r="E20" s="83" t="s">
-        <v>854</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A21" s="82" t="s">
-        <v>855</v>
-      </c>
-      <c r="B21" s="5" t="s">
-        <v>1298</v>
-      </c>
-      <c r="C21" s="84" t="s">
-        <v>856</v>
       </c>
       <c r="D21" s="82"/>
       <c r="E21" s="83" t="s">
-        <v>857</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" ht="64" x14ac:dyDescent="0.2">
+        <v>854</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A22" s="82" t="s">
-        <v>858</v>
+        <v>855</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>1299</v>
+        <v>1298</v>
       </c>
       <c r="C22" s="84" t="s">
-        <v>859</v>
+        <v>856</v>
       </c>
       <c r="D22" s="82"/>
       <c r="E22" s="83" t="s">
+        <v>857</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="64" x14ac:dyDescent="0.2">
+      <c r="A23" s="82" t="s">
+        <v>858</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>1299</v>
+      </c>
+      <c r="C23" s="84" t="s">
+        <v>859</v>
+      </c>
+      <c r="D23" s="82"/>
+      <c r="E23" s="83" t="s">
         <v>860</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A23" s="142" t="s">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A24" s="140" t="s">
         <v>861</v>
       </c>
-      <c r="B23" s="143"/>
-      <c r="C23" s="143"/>
-      <c r="D23" s="143"/>
-      <c r="E23" s="144"/>
-    </row>
-    <row r="24" spans="1:6" ht="32" x14ac:dyDescent="0.2">
-      <c r="A24" s="18" t="s">
+      <c r="B24" s="141"/>
+      <c r="C24" s="141"/>
+      <c r="D24" s="141"/>
+      <c r="E24" s="142"/>
+    </row>
+    <row r="25" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+      <c r="A25" s="18" t="s">
         <v>188</v>
       </c>
-      <c r="B24" s="28" t="s">
+      <c r="B25" s="28" t="s">
         <v>862</v>
       </c>
-      <c r="C24" s="27" t="s">
+      <c r="C25" s="27" t="s">
         <v>863</v>
       </c>
-      <c r="D24" s="18"/>
-      <c r="E24" s="46" t="s">
+      <c r="D25" s="18"/>
+      <c r="E25" s="46" t="s">
         <v>864</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A25" s="133" t="s">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A26" s="131" t="s">
         <v>865</v>
       </c>
-      <c r="B25" s="134"/>
-      <c r="C25" s="134"/>
-      <c r="D25" s="134"/>
-      <c r="E25" s="135"/>
-    </row>
-    <row r="26" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A26" s="18" t="s">
+      <c r="B26" s="132"/>
+      <c r="C26" s="132"/>
+      <c r="D26" s="132"/>
+      <c r="E26" s="133"/>
+    </row>
+    <row r="27" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A27" s="18" t="s">
         <v>188</v>
       </c>
-      <c r="B26" s="28" t="s">
+      <c r="B27" s="28" t="s">
         <v>866</v>
       </c>
-      <c r="C26" s="27" t="s">
+      <c r="C27" s="27" t="s">
         <v>867</v>
       </c>
-      <c r="D26" s="18"/>
-      <c r="E26" s="46" t="s">
+      <c r="D27" s="18"/>
+      <c r="E27" s="46" t="s">
         <v>868</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A27" s="133" t="s">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A28" s="131" t="s">
         <v>869</v>
       </c>
-      <c r="B27" s="134"/>
-      <c r="C27" s="134"/>
-      <c r="D27" s="134"/>
-      <c r="E27" s="135"/>
-    </row>
-    <row r="28" spans="1:6" ht="48" x14ac:dyDescent="0.2">
-      <c r="A28" s="19" t="s">
-        <v>188</v>
-      </c>
-      <c r="B28" s="19" t="s">
-        <v>870</v>
-      </c>
-      <c r="C28" s="21" t="s">
-        <v>1312</v>
-      </c>
-      <c r="D28" s="5" t="s">
-        <v>871</v>
-      </c>
-      <c r="E28" s="46" t="s">
-        <v>872</v>
-      </c>
-      <c r="F28" s="72" t="s">
-        <v>1314</v>
-      </c>
+      <c r="B28" s="132"/>
+      <c r="C28" s="132"/>
+      <c r="D28" s="132"/>
+      <c r="E28" s="133"/>
     </row>
     <row r="29" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A29" s="19" t="s">
+        <v>188</v>
+      </c>
+      <c r="B29" s="19" t="s">
+        <v>870</v>
+      </c>
+      <c r="C29" s="21" t="s">
+        <v>1312</v>
+      </c>
+      <c r="D29" s="5" t="s">
+        <v>871</v>
+      </c>
+      <c r="E29" s="46" t="s">
+        <v>872</v>
+      </c>
+      <c r="F29" s="72" t="s">
+        <v>1314</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+      <c r="A30" s="19" t="s">
         <v>855</v>
       </c>
-      <c r="B29" s="19" t="s">
+      <c r="B30" s="19" t="s">
         <v>873</v>
       </c>
-      <c r="C29" s="21" t="s">
+      <c r="C30" s="21" t="s">
         <v>874</v>
       </c>
-      <c r="D29" s="19" t="s">
+      <c r="D30" s="19" t="s">
         <v>875</v>
       </c>
-      <c r="E29" s="46" t="s">
+      <c r="E30" s="46" t="s">
         <v>876</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="335" x14ac:dyDescent="0.2">
-      <c r="A30" s="19" t="s">
+    <row r="31" spans="1:6" ht="335" x14ac:dyDescent="0.2">
+      <c r="A31" s="19" t="s">
         <v>877</v>
       </c>
-      <c r="B30" s="19" t="s">
+      <c r="B31" s="19" t="s">
         <v>878</v>
       </c>
-      <c r="C30" s="21" t="s">
+      <c r="C31" s="21" t="s">
         <v>1311</v>
       </c>
-      <c r="E30" s="46" t="s">
+      <c r="E31" s="46" t="s">
         <v>1313</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="96" x14ac:dyDescent="0.2">
-      <c r="A31" s="19" t="s">
+    <row r="32" spans="1:6" ht="96" x14ac:dyDescent="0.2">
+      <c r="A32" s="19" t="s">
         <v>202</v>
       </c>
-      <c r="B31" s="19" t="s">
+      <c r="B32" s="19" t="s">
         <v>879</v>
       </c>
-      <c r="C31" s="21" t="s">
+      <c r="C32" s="21" t="s">
         <v>880</v>
       </c>
-      <c r="E31" s="46" t="s">
+      <c r="E32" s="46" t="s">
         <v>881</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="48" x14ac:dyDescent="0.2">
-      <c r="A32" s="19" t="s">
+    <row r="33" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+      <c r="A33" s="19" t="s">
         <v>35</v>
       </c>
-      <c r="B32" s="19" t="s">
+      <c r="B33" s="19" t="s">
         <v>882</v>
       </c>
-      <c r="C32" s="21" t="s">
+      <c r="C33" s="21" t="s">
         <v>883</v>
       </c>
-      <c r="D32" s="26" t="s">
+      <c r="D33" s="26" t="s">
         <v>884</v>
       </c>
-      <c r="E32" s="46" t="s">
+      <c r="E33" s="46" t="s">
         <v>885</v>
       </c>
     </row>
-    <row r="33" spans="1:6" ht="96" x14ac:dyDescent="0.2">
-      <c r="A33" s="18" t="s">
-        <v>352</v>
-      </c>
-      <c r="B33" s="28" t="s">
-        <v>886</v>
-      </c>
-      <c r="C33" s="27"/>
-      <c r="D33" s="18" t="s">
-        <v>887</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" ht="80" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:6" ht="96" x14ac:dyDescent="0.2">
       <c r="A34" s="18" t="s">
         <v>352</v>
       </c>
       <c r="B34" s="28" t="s">
-        <v>888</v>
+        <v>886</v>
       </c>
       <c r="C34" s="27"/>
       <c r="D34" s="18" t="s">
-        <v>889</v>
+        <v>887</v>
       </c>
     </row>
     <row r="35" spans="1:6" ht="80" x14ac:dyDescent="0.2">
       <c r="A35" s="18" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
       <c r="B35" s="28" t="s">
-        <v>890</v>
+        <v>888</v>
       </c>
       <c r="C35" s="27"/>
       <c r="D35" s="18" t="s">
+        <v>889</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" ht="80" x14ac:dyDescent="0.2">
+      <c r="A36" s="18" t="s">
+        <v>355</v>
+      </c>
+      <c r="B36" s="28" t="s">
+        <v>890</v>
+      </c>
+      <c r="C36" s="27"/>
+      <c r="D36" s="18" t="s">
         <v>891</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A36" s="133" t="s">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A37" s="131" t="s">
         <v>892</v>
       </c>
-      <c r="B36" s="134"/>
-      <c r="C36" s="134"/>
-      <c r="D36" s="134"/>
-      <c r="E36" s="135"/>
-    </row>
-    <row r="37" spans="1:6" ht="48" x14ac:dyDescent="0.2">
-      <c r="A37" s="19" t="s">
+      <c r="B37" s="132"/>
+      <c r="C37" s="132"/>
+      <c r="D37" s="132"/>
+      <c r="E37" s="133"/>
+    </row>
+    <row r="38" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+      <c r="A38" s="19" t="s">
         <v>188</v>
       </c>
-      <c r="B37" s="19" t="s">
+      <c r="B38" s="19" t="s">
         <v>893</v>
       </c>
-      <c r="C37" s="21" t="s">
+      <c r="C38" s="21" t="s">
         <v>894</v>
       </c>
-      <c r="D37" s="5" t="s">
+      <c r="D38" s="5" t="s">
         <v>895</v>
       </c>
-      <c r="E37" s="46" t="s">
+      <c r="E38" s="46" t="s">
         <v>896</v>
       </c>
     </row>
-    <row r="38" spans="1:6" ht="64" x14ac:dyDescent="0.2">
-      <c r="A38" s="18" t="s">
+    <row r="39" spans="1:6" ht="64" x14ac:dyDescent="0.2">
+      <c r="A39" s="18" t="s">
         <v>352</v>
       </c>
-      <c r="B38" s="28" t="s">
+      <c r="B39" s="28" t="s">
         <v>897</v>
-      </c>
-      <c r="C38" s="27"/>
-      <c r="D38" s="18" t="s">
-        <v>898</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" ht="80" x14ac:dyDescent="0.2">
-      <c r="A39" s="18" t="s">
-        <v>355</v>
-      </c>
-      <c r="B39" s="28" t="s">
-        <v>899</v>
       </c>
       <c r="C39" s="27"/>
       <c r="D39" s="18" t="s">
+        <v>898</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" ht="80" x14ac:dyDescent="0.2">
+      <c r="A40" s="18" t="s">
+        <v>355</v>
+      </c>
+      <c r="B40" s="28" t="s">
+        <v>899</v>
+      </c>
+      <c r="C40" s="27"/>
+      <c r="D40" s="18" t="s">
         <v>891</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A40" s="139" t="s">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A41" s="137" t="s">
         <v>900</v>
       </c>
-      <c r="B40" s="140"/>
-      <c r="C40" s="140"/>
-      <c r="D40" s="140"/>
-      <c r="E40" s="141"/>
-    </row>
-    <row r="41" spans="1:6" ht="96" x14ac:dyDescent="0.2">
-      <c r="A41" s="85" t="s">
+      <c r="B41" s="138"/>
+      <c r="C41" s="138"/>
+      <c r="D41" s="138"/>
+      <c r="E41" s="139"/>
+    </row>
+    <row r="42" spans="1:6" ht="96" x14ac:dyDescent="0.2">
+      <c r="A42" s="85" t="s">
         <v>188</v>
       </c>
-      <c r="B41" s="85" t="s">
+      <c r="B42" s="85" t="s">
         <v>901</v>
       </c>
-      <c r="C41" s="21" t="s">
+      <c r="C42" s="21" t="s">
         <v>763</v>
       </c>
-      <c r="D41" s="85" t="s">
+      <c r="D42" s="85" t="s">
         <v>902</v>
       </c>
-      <c r="E41" s="46" t="s">
+      <c r="E42" s="46" t="s">
         <v>765</v>
       </c>
-      <c r="F41" s="73" t="s">
+      <c r="F42" s="73" t="s">
         <v>903</v>
       </c>
     </row>
-    <row r="42" spans="1:6" ht="80" x14ac:dyDescent="0.2">
-      <c r="A42" s="85" t="s">
+    <row r="43" spans="1:6" ht="80" x14ac:dyDescent="0.2">
+      <c r="A43" s="85" t="s">
         <v>314</v>
       </c>
-      <c r="B42" s="85" t="s">
+      <c r="B43" s="85" t="s">
         <v>904</v>
       </c>
-      <c r="C42" s="21" t="s">
+      <c r="C43" s="21" t="s">
         <v>823</v>
       </c>
-      <c r="D42" s="85" t="s">
+      <c r="D43" s="85" t="s">
         <v>905</v>
       </c>
-      <c r="E42" s="46" t="s">
+      <c r="E43" s="46" t="s">
         <v>824</v>
       </c>
     </row>
-    <row r="43" spans="1:6" ht="64" x14ac:dyDescent="0.2">
-      <c r="A43" s="85" t="s">
+    <row r="44" spans="1:6" ht="64" x14ac:dyDescent="0.2">
+      <c r="A44" s="85" t="s">
         <v>202</v>
       </c>
-      <c r="B43" s="85" t="s">
+      <c r="B44" s="85" t="s">
         <v>906</v>
       </c>
-      <c r="C43" s="62" t="s">
+      <c r="C44" s="62" t="s">
         <v>907</v>
       </c>
-      <c r="D43" s="85" t="s">
+      <c r="D44" s="85" t="s">
         <v>908</v>
       </c>
-      <c r="E43" s="46" t="s">
+      <c r="E44" s="46" t="s">
         <v>909</v>
       </c>
     </row>
-    <row r="44" spans="1:6" ht="48" x14ac:dyDescent="0.2">
-      <c r="A44" s="85" t="s">
-        <v>328</v>
-      </c>
-      <c r="B44" s="85" t="s">
-        <v>910</v>
-      </c>
-      <c r="C44" s="21" t="s">
-        <v>911</v>
-      </c>
-      <c r="D44" s="90" t="s">
-        <v>912</v>
-      </c>
-      <c r="E44" s="46" t="s">
-        <v>911</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" ht="64" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A45" s="85" t="s">
         <v>328</v>
       </c>
       <c r="B45" s="85" t="s">
-        <v>913</v>
+        <v>910</v>
       </c>
       <c r="C45" s="21" t="s">
-        <v>914</v>
+        <v>911</v>
       </c>
       <c r="D45" s="90" t="s">
-        <v>915</v>
+        <v>912</v>
       </c>
       <c r="E45" s="46" t="s">
-        <v>916</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+        <v>911</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" ht="64" x14ac:dyDescent="0.2">
       <c r="A46" s="85" t="s">
         <v>328</v>
       </c>
       <c r="B46" s="85" t="s">
-        <v>917</v>
+        <v>913</v>
       </c>
       <c r="C46" s="21" t="s">
-        <v>918</v>
+        <v>914</v>
       </c>
       <c r="D46" s="90" t="s">
-        <v>919</v>
+        <v>915</v>
       </c>
       <c r="E46" s="46" t="s">
-        <v>920</v>
+        <v>916</v>
       </c>
     </row>
     <row r="47" spans="1:6" ht="48" x14ac:dyDescent="0.2">
@@ -14747,62 +14753,62 @@
         <v>328</v>
       </c>
       <c r="B47" s="85" t="s">
-        <v>921</v>
+        <v>917</v>
       </c>
       <c r="C47" s="21" t="s">
-        <v>922</v>
+        <v>918</v>
       </c>
       <c r="D47" s="90" t="s">
-        <v>923</v>
+        <v>919</v>
       </c>
       <c r="E47" s="46" t="s">
-        <v>924</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+        <v>920</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A48" s="85" t="s">
         <v>328</v>
       </c>
       <c r="B48" s="85" t="s">
+        <v>921</v>
+      </c>
+      <c r="C48" s="21" t="s">
+        <v>922</v>
+      </c>
+      <c r="D48" s="90" t="s">
+        <v>923</v>
+      </c>
+      <c r="E48" s="46" t="s">
+        <v>924</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A49" s="85" t="s">
+        <v>328</v>
+      </c>
+      <c r="B49" s="85" t="s">
         <v>1315</v>
       </c>
-      <c r="C48" s="21" t="s">
+      <c r="C49" s="21" t="s">
         <v>1316</v>
       </c>
-      <c r="D48" s="90"/>
-      <c r="E48" s="46" t="s">
+      <c r="D49" s="90"/>
+      <c r="E49" s="46" t="s">
         <v>1317</v>
       </c>
     </row>
-    <row r="49" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A49" s="19" t="s">
+    <row r="50" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A50" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="B49" s="19" t="s">
+      <c r="B50" s="19" t="s">
         <v>925</v>
       </c>
-      <c r="C49" s="21" t="s">
+      <c r="C50" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="E49" s="46" t="s">
+      <c r="E50" s="46" t="s">
         <v>34</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" ht="48" x14ac:dyDescent="0.2">
-      <c r="A50" s="19" t="s">
-        <v>926</v>
-      </c>
-      <c r="B50" s="19" t="s">
-        <v>927</v>
-      </c>
-      <c r="C50" s="21" t="s">
-        <v>928</v>
-      </c>
-      <c r="D50" s="19" t="s">
-        <v>929</v>
-      </c>
-      <c r="F50" s="72" t="s">
-        <v>811</v>
       </c>
     </row>
     <row r="51" spans="1:6" ht="48" x14ac:dyDescent="0.2">
@@ -14810,10 +14816,10 @@
         <v>926</v>
       </c>
       <c r="B51" s="19" t="s">
-        <v>930</v>
+        <v>927</v>
       </c>
       <c r="C51" s="21" t="s">
-        <v>931</v>
+        <v>928</v>
       </c>
       <c r="D51" s="19" t="s">
         <v>929</v>
@@ -14823,17 +14829,17 @@
       </c>
     </row>
     <row r="52" spans="1:6" ht="48" x14ac:dyDescent="0.2">
-      <c r="A52" s="85" t="s">
-        <v>328</v>
-      </c>
-      <c r="B52" s="85" t="s">
-        <v>932</v>
+      <c r="A52" s="19" t="s">
+        <v>926</v>
+      </c>
+      <c r="B52" s="19" t="s">
+        <v>930</v>
       </c>
       <c r="C52" s="21" t="s">
-        <v>933</v>
-      </c>
-      <c r="D52" s="90" t="s">
-        <v>934</v>
+        <v>931</v>
+      </c>
+      <c r="D52" s="19" t="s">
+        <v>929</v>
       </c>
       <c r="F52" s="72" t="s">
         <v>811</v>
@@ -14844,28 +14850,45 @@
         <v>328</v>
       </c>
       <c r="B53" s="85" t="s">
-        <v>935</v>
+        <v>932</v>
       </c>
       <c r="C53" s="21" t="s">
-        <v>936</v>
+        <v>933</v>
       </c>
       <c r="D53" s="90" t="s">
-        <v>937</v>
+        <v>934</v>
       </c>
       <c r="F53" s="72" t="s">
         <v>811</v>
       </c>
     </row>
+    <row r="54" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+      <c r="A54" s="85" t="s">
+        <v>328</v>
+      </c>
+      <c r="B54" s="85" t="s">
+        <v>935</v>
+      </c>
+      <c r="C54" s="21" t="s">
+        <v>936</v>
+      </c>
+      <c r="D54" s="90" t="s">
+        <v>937</v>
+      </c>
+      <c r="F54" s="72" t="s">
+        <v>811</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="8">
-    <mergeCell ref="A27:E27"/>
-    <mergeCell ref="A36:E36"/>
-    <mergeCell ref="A11:E11"/>
-    <mergeCell ref="A40:E40"/>
+    <mergeCell ref="A28:E28"/>
+    <mergeCell ref="A37:E37"/>
+    <mergeCell ref="A12:E12"/>
+    <mergeCell ref="A41:E41"/>
     <mergeCell ref="A2:E2"/>
-    <mergeCell ref="A23:E23"/>
-    <mergeCell ref="A25:E25"/>
-    <mergeCell ref="A19:E19"/>
+    <mergeCell ref="A24:E24"/>
+    <mergeCell ref="A26:E26"/>
+    <mergeCell ref="A20:E20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -14876,7 +14899,7 @@
   <dimension ref="A1:F73"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A78" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A59" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D78" sqref="D78"/>
     </sheetView>
   </sheetViews>
@@ -15327,13 +15350,13 @@
       </c>
     </row>
     <row r="28" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="148" t="s">
+      <c r="A28" s="146" t="s">
         <v>1019</v>
       </c>
-      <c r="B28" s="149"/>
-      <c r="C28" s="149"/>
-      <c r="D28" s="149"/>
-      <c r="E28" s="150"/>
+      <c r="B28" s="147"/>
+      <c r="C28" s="147"/>
+      <c r="D28" s="147"/>
+      <c r="E28" s="148"/>
     </row>
     <row r="29" spans="1:5" ht="48" x14ac:dyDescent="0.2">
       <c r="A29" s="103" t="s">
@@ -15396,13 +15419,13 @@
       <c r="E32" s="109"/>
     </row>
     <row r="33" spans="1:6" s="13" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="151" t="s">
+      <c r="A33" s="149" t="s">
         <v>1031</v>
       </c>
-      <c r="B33" s="152"/>
-      <c r="C33" s="153"/>
-      <c r="D33" s="152"/>
-      <c r="E33" s="154"/>
+      <c r="B33" s="150"/>
+      <c r="C33" s="151"/>
+      <c r="D33" s="150"/>
+      <c r="E33" s="152"/>
     </row>
     <row r="34" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A34" s="107" t="s">
@@ -15605,13 +15628,13 @@
       <c r="F45" s="98"/>
     </row>
     <row r="46" spans="1:6" s="13" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="148" t="s">
+      <c r="A46" s="146" t="s">
         <v>1061</v>
       </c>
-      <c r="B46" s="149"/>
-      <c r="C46" s="149"/>
-      <c r="D46" s="149"/>
-      <c r="E46" s="150"/>
+      <c r="B46" s="147"/>
+      <c r="C46" s="147"/>
+      <c r="D46" s="147"/>
+      <c r="E46" s="148"/>
     </row>
     <row r="47" spans="1:6" s="30" customFormat="1" ht="64" x14ac:dyDescent="0.2">
       <c r="A47" s="107" t="s">
@@ -16239,6 +16262,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <Readyforteam_x003f_ xmlns="565e1b1d-057e-4d85-b896-01a5881d8a45">false</Readyforteam_x003f_>
@@ -16277,15 +16309,6 @@
     <TaxCatchAll xmlns="2799d30d-6731-4efe-ac9b-c4895a8828d9" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -16566,6 +16589,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8D7CE8C7-18DC-484F-8376-ED09F13D44C8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{017ACE96-8143-486E-8436-7787F6B96F4A}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -16574,14 +16605,6 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
     <ds:schemaRef ds:uri="bf601f31-63a1-4825-9216-91d773c5ef9c"/>
     <ds:schemaRef ds:uri="2799d30d-6731-4efe-ac9b-c4895a8828d9"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8D7CE8C7-18DC-484F-8376-ED09F13D44C8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Adding in ME and MEO flows to the dashboard test.
</commit_message>
<xml_diff>
--- a/app/data/MCCD-localisation.xlsx
+++ b/app/data/MCCD-localisation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/JALAT/GIT/medical-certificate-of-cause-of-death/app/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8124006-537B-CF48-94E6-6FFE4A96BC9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F534358F-FEBC-7D4A-852B-13CBCE85ECFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="14100" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -68,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1956" uniqueCount="1363">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1959" uniqueCount="1366">
   <si>
     <r>
       <rPr>
@@ -5686,6 +5686,15 @@
   </si>
   <si>
     <t>012</t>
+  </si>
+  <si>
+    <t>globalBackToDashboard</t>
+  </si>
+  <si>
+    <t>Back to dashboard</t>
+  </si>
+  <si>
+    <t>Yn ôl i dashboard</t>
   </si>
 </sst>
 </file>
@@ -6469,6 +6478,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -6570,12 +6585,6 @@
     </xf>
     <xf numFmtId="0" fontId="15" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -6956,538 +6965,538 @@
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A1" s="121" t="s">
+      <c r="A1" s="123" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="121"/>
-      <c r="C1" s="121"/>
-      <c r="D1" s="121"/>
-      <c r="E1" s="121"/>
-      <c r="F1" s="121"/>
-      <c r="G1" s="121"/>
-      <c r="H1" s="121"/>
-      <c r="I1" s="121"/>
-      <c r="J1" s="121"/>
-      <c r="K1" s="121"/>
-      <c r="L1" s="121"/>
+      <c r="B1" s="123"/>
+      <c r="C1" s="123"/>
+      <c r="D1" s="123"/>
+      <c r="E1" s="123"/>
+      <c r="F1" s="123"/>
+      <c r="G1" s="123"/>
+      <c r="H1" s="123"/>
+      <c r="I1" s="123"/>
+      <c r="J1" s="123"/>
+      <c r="K1" s="123"/>
+      <c r="L1" s="123"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A2" s="121"/>
-      <c r="B2" s="121"/>
-      <c r="C2" s="121"/>
-      <c r="D2" s="121"/>
-      <c r="E2" s="121"/>
-      <c r="F2" s="121"/>
-      <c r="G2" s="121"/>
-      <c r="H2" s="121"/>
-      <c r="I2" s="121"/>
-      <c r="J2" s="121"/>
-      <c r="K2" s="121"/>
-      <c r="L2" s="121"/>
+      <c r="A2" s="123"/>
+      <c r="B2" s="123"/>
+      <c r="C2" s="123"/>
+      <c r="D2" s="123"/>
+      <c r="E2" s="123"/>
+      <c r="F2" s="123"/>
+      <c r="G2" s="123"/>
+      <c r="H2" s="123"/>
+      <c r="I2" s="123"/>
+      <c r="J2" s="123"/>
+      <c r="K2" s="123"/>
+      <c r="L2" s="123"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A3" s="121"/>
-      <c r="B3" s="121"/>
-      <c r="C3" s="121"/>
-      <c r="D3" s="121"/>
-      <c r="E3" s="121"/>
-      <c r="F3" s="121"/>
-      <c r="G3" s="121"/>
-      <c r="H3" s="121"/>
-      <c r="I3" s="121"/>
-      <c r="J3" s="121"/>
-      <c r="K3" s="121"/>
-      <c r="L3" s="121"/>
+      <c r="A3" s="123"/>
+      <c r="B3" s="123"/>
+      <c r="C3" s="123"/>
+      <c r="D3" s="123"/>
+      <c r="E3" s="123"/>
+      <c r="F3" s="123"/>
+      <c r="G3" s="123"/>
+      <c r="H3" s="123"/>
+      <c r="I3" s="123"/>
+      <c r="J3" s="123"/>
+      <c r="K3" s="123"/>
+      <c r="L3" s="123"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A4" s="121"/>
-      <c r="B4" s="121"/>
-      <c r="C4" s="121"/>
-      <c r="D4" s="121"/>
-      <c r="E4" s="121"/>
-      <c r="F4" s="121"/>
-      <c r="G4" s="121"/>
-      <c r="H4" s="121"/>
-      <c r="I4" s="121"/>
-      <c r="J4" s="121"/>
-      <c r="K4" s="121"/>
-      <c r="L4" s="121"/>
+      <c r="A4" s="123"/>
+      <c r="B4" s="123"/>
+      <c r="C4" s="123"/>
+      <c r="D4" s="123"/>
+      <c r="E4" s="123"/>
+      <c r="F4" s="123"/>
+      <c r="G4" s="123"/>
+      <c r="H4" s="123"/>
+      <c r="I4" s="123"/>
+      <c r="J4" s="123"/>
+      <c r="K4" s="123"/>
+      <c r="L4" s="123"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A5" s="121"/>
-      <c r="B5" s="121"/>
-      <c r="C5" s="121"/>
-      <c r="D5" s="121"/>
-      <c r="E5" s="121"/>
-      <c r="F5" s="121"/>
-      <c r="G5" s="121"/>
-      <c r="H5" s="121"/>
-      <c r="I5" s="121"/>
-      <c r="J5" s="121"/>
-      <c r="K5" s="121"/>
-      <c r="L5" s="121"/>
+      <c r="A5" s="123"/>
+      <c r="B5" s="123"/>
+      <c r="C5" s="123"/>
+      <c r="D5" s="123"/>
+      <c r="E5" s="123"/>
+      <c r="F5" s="123"/>
+      <c r="G5" s="123"/>
+      <c r="H5" s="123"/>
+      <c r="I5" s="123"/>
+      <c r="J5" s="123"/>
+      <c r="K5" s="123"/>
+      <c r="L5" s="123"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A6" s="121"/>
-      <c r="B6" s="121"/>
-      <c r="C6" s="121"/>
-      <c r="D6" s="121"/>
-      <c r="E6" s="121"/>
-      <c r="F6" s="121"/>
-      <c r="G6" s="121"/>
-      <c r="H6" s="121"/>
-      <c r="I6" s="121"/>
-      <c r="J6" s="121"/>
-      <c r="K6" s="121"/>
-      <c r="L6" s="121"/>
+      <c r="A6" s="123"/>
+      <c r="B6" s="123"/>
+      <c r="C6" s="123"/>
+      <c r="D6" s="123"/>
+      <c r="E6" s="123"/>
+      <c r="F6" s="123"/>
+      <c r="G6" s="123"/>
+      <c r="H6" s="123"/>
+      <c r="I6" s="123"/>
+      <c r="J6" s="123"/>
+      <c r="K6" s="123"/>
+      <c r="L6" s="123"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A7" s="121"/>
-      <c r="B7" s="121"/>
-      <c r="C7" s="121"/>
-      <c r="D7" s="121"/>
-      <c r="E7" s="121"/>
-      <c r="F7" s="121"/>
-      <c r="G7" s="121"/>
-      <c r="H7" s="121"/>
-      <c r="I7" s="121"/>
-      <c r="J7" s="121"/>
-      <c r="K7" s="121"/>
-      <c r="L7" s="121"/>
+      <c r="A7" s="123"/>
+      <c r="B7" s="123"/>
+      <c r="C7" s="123"/>
+      <c r="D7" s="123"/>
+      <c r="E7" s="123"/>
+      <c r="F7" s="123"/>
+      <c r="G7" s="123"/>
+      <c r="H7" s="123"/>
+      <c r="I7" s="123"/>
+      <c r="J7" s="123"/>
+      <c r="K7" s="123"/>
+      <c r="L7" s="123"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A8" s="121"/>
-      <c r="B8" s="121"/>
-      <c r="C8" s="121"/>
-      <c r="D8" s="121"/>
-      <c r="E8" s="121"/>
-      <c r="F8" s="121"/>
-      <c r="G8" s="121"/>
-      <c r="H8" s="121"/>
-      <c r="I8" s="121"/>
-      <c r="J8" s="121"/>
-      <c r="K8" s="121"/>
-      <c r="L8" s="121"/>
+      <c r="A8" s="123"/>
+      <c r="B8" s="123"/>
+      <c r="C8" s="123"/>
+      <c r="D8" s="123"/>
+      <c r="E8" s="123"/>
+      <c r="F8" s="123"/>
+      <c r="G8" s="123"/>
+      <c r="H8" s="123"/>
+      <c r="I8" s="123"/>
+      <c r="J8" s="123"/>
+      <c r="K8" s="123"/>
+      <c r="L8" s="123"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A9" s="121"/>
-      <c r="B9" s="121"/>
-      <c r="C9" s="121"/>
-      <c r="D9" s="121"/>
-      <c r="E9" s="121"/>
-      <c r="F9" s="121"/>
-      <c r="G9" s="121"/>
-      <c r="H9" s="121"/>
-      <c r="I9" s="121"/>
-      <c r="J9" s="121"/>
-      <c r="K9" s="121"/>
-      <c r="L9" s="121"/>
+      <c r="A9" s="123"/>
+      <c r="B9" s="123"/>
+      <c r="C9" s="123"/>
+      <c r="D9" s="123"/>
+      <c r="E9" s="123"/>
+      <c r="F9" s="123"/>
+      <c r="G9" s="123"/>
+      <c r="H9" s="123"/>
+      <c r="I9" s="123"/>
+      <c r="J9" s="123"/>
+      <c r="K9" s="123"/>
+      <c r="L9" s="123"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A10" s="121"/>
-      <c r="B10" s="121"/>
-      <c r="C10" s="121"/>
-      <c r="D10" s="121"/>
-      <c r="E10" s="121"/>
-      <c r="F10" s="121"/>
-      <c r="G10" s="121"/>
-      <c r="H10" s="121"/>
-      <c r="I10" s="121"/>
-      <c r="J10" s="121"/>
-      <c r="K10" s="121"/>
-      <c r="L10" s="121"/>
+      <c r="A10" s="123"/>
+      <c r="B10" s="123"/>
+      <c r="C10" s="123"/>
+      <c r="D10" s="123"/>
+      <c r="E10" s="123"/>
+      <c r="F10" s="123"/>
+      <c r="G10" s="123"/>
+      <c r="H10" s="123"/>
+      <c r="I10" s="123"/>
+      <c r="J10" s="123"/>
+      <c r="K10" s="123"/>
+      <c r="L10" s="123"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A11" s="121"/>
-      <c r="B11" s="121"/>
-      <c r="C11" s="121"/>
-      <c r="D11" s="121"/>
-      <c r="E11" s="121"/>
-      <c r="F11" s="121"/>
-      <c r="G11" s="121"/>
-      <c r="H11" s="121"/>
-      <c r="I11" s="121"/>
-      <c r="J11" s="121"/>
-      <c r="K11" s="121"/>
-      <c r="L11" s="121"/>
+      <c r="A11" s="123"/>
+      <c r="B11" s="123"/>
+      <c r="C11" s="123"/>
+      <c r="D11" s="123"/>
+      <c r="E11" s="123"/>
+      <c r="F11" s="123"/>
+      <c r="G11" s="123"/>
+      <c r="H11" s="123"/>
+      <c r="I11" s="123"/>
+      <c r="J11" s="123"/>
+      <c r="K11" s="123"/>
+      <c r="L11" s="123"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A12" s="121"/>
-      <c r="B12" s="121"/>
-      <c r="C12" s="121"/>
-      <c r="D12" s="121"/>
-      <c r="E12" s="121"/>
-      <c r="F12" s="121"/>
-      <c r="G12" s="121"/>
-      <c r="H12" s="121"/>
-      <c r="I12" s="121"/>
-      <c r="J12" s="121"/>
-      <c r="K12" s="121"/>
-      <c r="L12" s="121"/>
+      <c r="A12" s="123"/>
+      <c r="B12" s="123"/>
+      <c r="C12" s="123"/>
+      <c r="D12" s="123"/>
+      <c r="E12" s="123"/>
+      <c r="F12" s="123"/>
+      <c r="G12" s="123"/>
+      <c r="H12" s="123"/>
+      <c r="I12" s="123"/>
+      <c r="J12" s="123"/>
+      <c r="K12" s="123"/>
+      <c r="L12" s="123"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A13" s="121"/>
-      <c r="B13" s="121"/>
-      <c r="C13" s="121"/>
-      <c r="D13" s="121"/>
-      <c r="E13" s="121"/>
-      <c r="F13" s="121"/>
-      <c r="G13" s="121"/>
-      <c r="H13" s="121"/>
-      <c r="I13" s="121"/>
-      <c r="J13" s="121"/>
-      <c r="K13" s="121"/>
-      <c r="L13" s="121"/>
+      <c r="A13" s="123"/>
+      <c r="B13" s="123"/>
+      <c r="C13" s="123"/>
+      <c r="D13" s="123"/>
+      <c r="E13" s="123"/>
+      <c r="F13" s="123"/>
+      <c r="G13" s="123"/>
+      <c r="H13" s="123"/>
+      <c r="I13" s="123"/>
+      <c r="J13" s="123"/>
+      <c r="K13" s="123"/>
+      <c r="L13" s="123"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A14" s="121"/>
-      <c r="B14" s="121"/>
-      <c r="C14" s="121"/>
-      <c r="D14" s="121"/>
-      <c r="E14" s="121"/>
-      <c r="F14" s="121"/>
-      <c r="G14" s="121"/>
-      <c r="H14" s="121"/>
-      <c r="I14" s="121"/>
-      <c r="J14" s="121"/>
-      <c r="K14" s="121"/>
-      <c r="L14" s="121"/>
+      <c r="A14" s="123"/>
+      <c r="B14" s="123"/>
+      <c r="C14" s="123"/>
+      <c r="D14" s="123"/>
+      <c r="E14" s="123"/>
+      <c r="F14" s="123"/>
+      <c r="G14" s="123"/>
+      <c r="H14" s="123"/>
+      <c r="I14" s="123"/>
+      <c r="J14" s="123"/>
+      <c r="K14" s="123"/>
+      <c r="L14" s="123"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A15" s="121"/>
-      <c r="B15" s="121"/>
-      <c r="C15" s="121"/>
-      <c r="D15" s="121"/>
-      <c r="E15" s="121"/>
-      <c r="F15" s="121"/>
-      <c r="G15" s="121"/>
-      <c r="H15" s="121"/>
-      <c r="I15" s="121"/>
-      <c r="J15" s="121"/>
-      <c r="K15" s="121"/>
-      <c r="L15" s="121"/>
+      <c r="A15" s="123"/>
+      <c r="B15" s="123"/>
+      <c r="C15" s="123"/>
+      <c r="D15" s="123"/>
+      <c r="E15" s="123"/>
+      <c r="F15" s="123"/>
+      <c r="G15" s="123"/>
+      <c r="H15" s="123"/>
+      <c r="I15" s="123"/>
+      <c r="J15" s="123"/>
+      <c r="K15" s="123"/>
+      <c r="L15" s="123"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A16" s="121"/>
-      <c r="B16" s="121"/>
-      <c r="C16" s="121"/>
-      <c r="D16" s="121"/>
-      <c r="E16" s="121"/>
-      <c r="F16" s="121"/>
-      <c r="G16" s="121"/>
-      <c r="H16" s="121"/>
-      <c r="I16" s="121"/>
-      <c r="J16" s="121"/>
-      <c r="K16" s="121"/>
-      <c r="L16" s="121"/>
+      <c r="A16" s="123"/>
+      <c r="B16" s="123"/>
+      <c r="C16" s="123"/>
+      <c r="D16" s="123"/>
+      <c r="E16" s="123"/>
+      <c r="F16" s="123"/>
+      <c r="G16" s="123"/>
+      <c r="H16" s="123"/>
+      <c r="I16" s="123"/>
+      <c r="J16" s="123"/>
+      <c r="K16" s="123"/>
+      <c r="L16" s="123"/>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A17" s="121"/>
-      <c r="B17" s="121"/>
-      <c r="C17" s="121"/>
-      <c r="D17" s="121"/>
-      <c r="E17" s="121"/>
-      <c r="F17" s="121"/>
-      <c r="G17" s="121"/>
-      <c r="H17" s="121"/>
-      <c r="I17" s="121"/>
-      <c r="J17" s="121"/>
-      <c r="K17" s="121"/>
-      <c r="L17" s="121"/>
+      <c r="A17" s="123"/>
+      <c r="B17" s="123"/>
+      <c r="C17" s="123"/>
+      <c r="D17" s="123"/>
+      <c r="E17" s="123"/>
+      <c r="F17" s="123"/>
+      <c r="G17" s="123"/>
+      <c r="H17" s="123"/>
+      <c r="I17" s="123"/>
+      <c r="J17" s="123"/>
+      <c r="K17" s="123"/>
+      <c r="L17" s="123"/>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A18" s="121"/>
-      <c r="B18" s="121"/>
-      <c r="C18" s="121"/>
-      <c r="D18" s="121"/>
-      <c r="E18" s="121"/>
-      <c r="F18" s="121"/>
-      <c r="G18" s="121"/>
-      <c r="H18" s="121"/>
-      <c r="I18" s="121"/>
-      <c r="J18" s="121"/>
-      <c r="K18" s="121"/>
-      <c r="L18" s="121"/>
+      <c r="A18" s="123"/>
+      <c r="B18" s="123"/>
+      <c r="C18" s="123"/>
+      <c r="D18" s="123"/>
+      <c r="E18" s="123"/>
+      <c r="F18" s="123"/>
+      <c r="G18" s="123"/>
+      <c r="H18" s="123"/>
+      <c r="I18" s="123"/>
+      <c r="J18" s="123"/>
+      <c r="K18" s="123"/>
+      <c r="L18" s="123"/>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A19" s="121"/>
-      <c r="B19" s="121"/>
-      <c r="C19" s="121"/>
-      <c r="D19" s="121"/>
-      <c r="E19" s="121"/>
-      <c r="F19" s="121"/>
-      <c r="G19" s="121"/>
-      <c r="H19" s="121"/>
-      <c r="I19" s="121"/>
-      <c r="J19" s="121"/>
-      <c r="K19" s="121"/>
-      <c r="L19" s="121"/>
+      <c r="A19" s="123"/>
+      <c r="B19" s="123"/>
+      <c r="C19" s="123"/>
+      <c r="D19" s="123"/>
+      <c r="E19" s="123"/>
+      <c r="F19" s="123"/>
+      <c r="G19" s="123"/>
+      <c r="H19" s="123"/>
+      <c r="I19" s="123"/>
+      <c r="J19" s="123"/>
+      <c r="K19" s="123"/>
+      <c r="L19" s="123"/>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A20" s="121"/>
-      <c r="B20" s="121"/>
-      <c r="C20" s="121"/>
-      <c r="D20" s="121"/>
-      <c r="E20" s="121"/>
-      <c r="F20" s="121"/>
-      <c r="G20" s="121"/>
-      <c r="H20" s="121"/>
-      <c r="I20" s="121"/>
-      <c r="J20" s="121"/>
-      <c r="K20" s="121"/>
-      <c r="L20" s="121"/>
+      <c r="A20" s="123"/>
+      <c r="B20" s="123"/>
+      <c r="C20" s="123"/>
+      <c r="D20" s="123"/>
+      <c r="E20" s="123"/>
+      <c r="F20" s="123"/>
+      <c r="G20" s="123"/>
+      <c r="H20" s="123"/>
+      <c r="I20" s="123"/>
+      <c r="J20" s="123"/>
+      <c r="K20" s="123"/>
+      <c r="L20" s="123"/>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A21" s="121"/>
-      <c r="B21" s="121"/>
-      <c r="C21" s="121"/>
-      <c r="D21" s="121"/>
-      <c r="E21" s="121"/>
-      <c r="F21" s="121"/>
-      <c r="G21" s="121"/>
-      <c r="H21" s="121"/>
-      <c r="I21" s="121"/>
-      <c r="J21" s="121"/>
-      <c r="K21" s="121"/>
-      <c r="L21" s="121"/>
+      <c r="A21" s="123"/>
+      <c r="B21" s="123"/>
+      <c r="C21" s="123"/>
+      <c r="D21" s="123"/>
+      <c r="E21" s="123"/>
+      <c r="F21" s="123"/>
+      <c r="G21" s="123"/>
+      <c r="H21" s="123"/>
+      <c r="I21" s="123"/>
+      <c r="J21" s="123"/>
+      <c r="K21" s="123"/>
+      <c r="L21" s="123"/>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A22" s="121"/>
-      <c r="B22" s="121"/>
-      <c r="C22" s="121"/>
-      <c r="D22" s="121"/>
-      <c r="E22" s="121"/>
-      <c r="F22" s="121"/>
-      <c r="G22" s="121"/>
-      <c r="H22" s="121"/>
-      <c r="I22" s="121"/>
-      <c r="J22" s="121"/>
-      <c r="K22" s="121"/>
-      <c r="L22" s="121"/>
+      <c r="A22" s="123"/>
+      <c r="B22" s="123"/>
+      <c r="C22" s="123"/>
+      <c r="D22" s="123"/>
+      <c r="E22" s="123"/>
+      <c r="F22" s="123"/>
+      <c r="G22" s="123"/>
+      <c r="H22" s="123"/>
+      <c r="I22" s="123"/>
+      <c r="J22" s="123"/>
+      <c r="K22" s="123"/>
+      <c r="L22" s="123"/>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A23" s="121"/>
-      <c r="B23" s="121"/>
-      <c r="C23" s="121"/>
-      <c r="D23" s="121"/>
-      <c r="E23" s="121"/>
-      <c r="F23" s="121"/>
-      <c r="G23" s="121"/>
-      <c r="H23" s="121"/>
-      <c r="I23" s="121"/>
-      <c r="J23" s="121"/>
-      <c r="K23" s="121"/>
-      <c r="L23" s="121"/>
+      <c r="A23" s="123"/>
+      <c r="B23" s="123"/>
+      <c r="C23" s="123"/>
+      <c r="D23" s="123"/>
+      <c r="E23" s="123"/>
+      <c r="F23" s="123"/>
+      <c r="G23" s="123"/>
+      <c r="H23" s="123"/>
+      <c r="I23" s="123"/>
+      <c r="J23" s="123"/>
+      <c r="K23" s="123"/>
+      <c r="L23" s="123"/>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A24" s="121"/>
-      <c r="B24" s="121"/>
-      <c r="C24" s="121"/>
-      <c r="D24" s="121"/>
-      <c r="E24" s="121"/>
-      <c r="F24" s="121"/>
-      <c r="G24" s="121"/>
-      <c r="H24" s="121"/>
-      <c r="I24" s="121"/>
-      <c r="J24" s="121"/>
-      <c r="K24" s="121"/>
-      <c r="L24" s="121"/>
+      <c r="A24" s="123"/>
+      <c r="B24" s="123"/>
+      <c r="C24" s="123"/>
+      <c r="D24" s="123"/>
+      <c r="E24" s="123"/>
+      <c r="F24" s="123"/>
+      <c r="G24" s="123"/>
+      <c r="H24" s="123"/>
+      <c r="I24" s="123"/>
+      <c r="J24" s="123"/>
+      <c r="K24" s="123"/>
+      <c r="L24" s="123"/>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A25" s="121"/>
-      <c r="B25" s="121"/>
-      <c r="C25" s="121"/>
-      <c r="D25" s="121"/>
-      <c r="E25" s="121"/>
-      <c r="F25" s="121"/>
-      <c r="G25" s="121"/>
-      <c r="H25" s="121"/>
-      <c r="I25" s="121"/>
-      <c r="J25" s="121"/>
-      <c r="K25" s="121"/>
-      <c r="L25" s="121"/>
+      <c r="A25" s="123"/>
+      <c r="B25" s="123"/>
+      <c r="C25" s="123"/>
+      <c r="D25" s="123"/>
+      <c r="E25" s="123"/>
+      <c r="F25" s="123"/>
+      <c r="G25" s="123"/>
+      <c r="H25" s="123"/>
+      <c r="I25" s="123"/>
+      <c r="J25" s="123"/>
+      <c r="K25" s="123"/>
+      <c r="L25" s="123"/>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A26" s="121"/>
-      <c r="B26" s="121"/>
-      <c r="C26" s="121"/>
-      <c r="D26" s="121"/>
-      <c r="E26" s="121"/>
-      <c r="F26" s="121"/>
-      <c r="G26" s="121"/>
-      <c r="H26" s="121"/>
-      <c r="I26" s="121"/>
-      <c r="J26" s="121"/>
-      <c r="K26" s="121"/>
-      <c r="L26" s="121"/>
+      <c r="A26" s="123"/>
+      <c r="B26" s="123"/>
+      <c r="C26" s="123"/>
+      <c r="D26" s="123"/>
+      <c r="E26" s="123"/>
+      <c r="F26" s="123"/>
+      <c r="G26" s="123"/>
+      <c r="H26" s="123"/>
+      <c r="I26" s="123"/>
+      <c r="J26" s="123"/>
+      <c r="K26" s="123"/>
+      <c r="L26" s="123"/>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A27" s="121"/>
-      <c r="B27" s="121"/>
-      <c r="C27" s="121"/>
-      <c r="D27" s="121"/>
-      <c r="E27" s="121"/>
-      <c r="F27" s="121"/>
-      <c r="G27" s="121"/>
-      <c r="H27" s="121"/>
-      <c r="I27" s="121"/>
-      <c r="J27" s="121"/>
-      <c r="K27" s="121"/>
-      <c r="L27" s="121"/>
+      <c r="A27" s="123"/>
+      <c r="B27" s="123"/>
+      <c r="C27" s="123"/>
+      <c r="D27" s="123"/>
+      <c r="E27" s="123"/>
+      <c r="F27" s="123"/>
+      <c r="G27" s="123"/>
+      <c r="H27" s="123"/>
+      <c r="I27" s="123"/>
+      <c r="J27" s="123"/>
+      <c r="K27" s="123"/>
+      <c r="L27" s="123"/>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A28" s="121"/>
-      <c r="B28" s="121"/>
-      <c r="C28" s="121"/>
-      <c r="D28" s="121"/>
-      <c r="E28" s="121"/>
-      <c r="F28" s="121"/>
-      <c r="G28" s="121"/>
-      <c r="H28" s="121"/>
-      <c r="I28" s="121"/>
-      <c r="J28" s="121"/>
-      <c r="K28" s="121"/>
-      <c r="L28" s="121"/>
+      <c r="A28" s="123"/>
+      <c r="B28" s="123"/>
+      <c r="C28" s="123"/>
+      <c r="D28" s="123"/>
+      <c r="E28" s="123"/>
+      <c r="F28" s="123"/>
+      <c r="G28" s="123"/>
+      <c r="H28" s="123"/>
+      <c r="I28" s="123"/>
+      <c r="J28" s="123"/>
+      <c r="K28" s="123"/>
+      <c r="L28" s="123"/>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A29" s="121"/>
-      <c r="B29" s="121"/>
-      <c r="C29" s="121"/>
-      <c r="D29" s="121"/>
-      <c r="E29" s="121"/>
-      <c r="F29" s="121"/>
-      <c r="G29" s="121"/>
-      <c r="H29" s="121"/>
-      <c r="I29" s="121"/>
-      <c r="J29" s="121"/>
-      <c r="K29" s="121"/>
-      <c r="L29" s="121"/>
+      <c r="A29" s="123"/>
+      <c r="B29" s="123"/>
+      <c r="C29" s="123"/>
+      <c r="D29" s="123"/>
+      <c r="E29" s="123"/>
+      <c r="F29" s="123"/>
+      <c r="G29" s="123"/>
+      <c r="H29" s="123"/>
+      <c r="I29" s="123"/>
+      <c r="J29" s="123"/>
+      <c r="K29" s="123"/>
+      <c r="L29" s="123"/>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A30" s="121"/>
-      <c r="B30" s="121"/>
-      <c r="C30" s="121"/>
-      <c r="D30" s="121"/>
-      <c r="E30" s="121"/>
-      <c r="F30" s="121"/>
-      <c r="G30" s="121"/>
-      <c r="H30" s="121"/>
-      <c r="I30" s="121"/>
-      <c r="J30" s="121"/>
-      <c r="K30" s="121"/>
-      <c r="L30" s="121"/>
+      <c r="A30" s="123"/>
+      <c r="B30" s="123"/>
+      <c r="C30" s="123"/>
+      <c r="D30" s="123"/>
+      <c r="E30" s="123"/>
+      <c r="F30" s="123"/>
+      <c r="G30" s="123"/>
+      <c r="H30" s="123"/>
+      <c r="I30" s="123"/>
+      <c r="J30" s="123"/>
+      <c r="K30" s="123"/>
+      <c r="L30" s="123"/>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A31" s="121"/>
-      <c r="B31" s="121"/>
-      <c r="C31" s="121"/>
-      <c r="D31" s="121"/>
-      <c r="E31" s="121"/>
-      <c r="F31" s="121"/>
-      <c r="G31" s="121"/>
-      <c r="H31" s="121"/>
-      <c r="I31" s="121"/>
-      <c r="J31" s="121"/>
-      <c r="K31" s="121"/>
-      <c r="L31" s="121"/>
+      <c r="A31" s="123"/>
+      <c r="B31" s="123"/>
+      <c r="C31" s="123"/>
+      <c r="D31" s="123"/>
+      <c r="E31" s="123"/>
+      <c r="F31" s="123"/>
+      <c r="G31" s="123"/>
+      <c r="H31" s="123"/>
+      <c r="I31" s="123"/>
+      <c r="J31" s="123"/>
+      <c r="K31" s="123"/>
+      <c r="L31" s="123"/>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A32" s="121"/>
-      <c r="B32" s="121"/>
-      <c r="C32" s="121"/>
-      <c r="D32" s="121"/>
-      <c r="E32" s="121"/>
-      <c r="F32" s="121"/>
-      <c r="G32" s="121"/>
-      <c r="H32" s="121"/>
-      <c r="I32" s="121"/>
-      <c r="J32" s="121"/>
-      <c r="K32" s="121"/>
-      <c r="L32" s="121"/>
+      <c r="A32" s="123"/>
+      <c r="B32" s="123"/>
+      <c r="C32" s="123"/>
+      <c r="D32" s="123"/>
+      <c r="E32" s="123"/>
+      <c r="F32" s="123"/>
+      <c r="G32" s="123"/>
+      <c r="H32" s="123"/>
+      <c r="I32" s="123"/>
+      <c r="J32" s="123"/>
+      <c r="K32" s="123"/>
+      <c r="L32" s="123"/>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A33" s="121"/>
-      <c r="B33" s="121"/>
-      <c r="C33" s="121"/>
-      <c r="D33" s="121"/>
-      <c r="E33" s="121"/>
-      <c r="F33" s="121"/>
-      <c r="G33" s="121"/>
-      <c r="H33" s="121"/>
-      <c r="I33" s="121"/>
-      <c r="J33" s="121"/>
-      <c r="K33" s="121"/>
-      <c r="L33" s="121"/>
+      <c r="A33" s="123"/>
+      <c r="B33" s="123"/>
+      <c r="C33" s="123"/>
+      <c r="D33" s="123"/>
+      <c r="E33" s="123"/>
+      <c r="F33" s="123"/>
+      <c r="G33" s="123"/>
+      <c r="H33" s="123"/>
+      <c r="I33" s="123"/>
+      <c r="J33" s="123"/>
+      <c r="K33" s="123"/>
+      <c r="L33" s="123"/>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A34" s="121"/>
-      <c r="B34" s="121"/>
-      <c r="C34" s="121"/>
-      <c r="D34" s="121"/>
-      <c r="E34" s="121"/>
-      <c r="F34" s="121"/>
-      <c r="G34" s="121"/>
-      <c r="H34" s="121"/>
-      <c r="I34" s="121"/>
-      <c r="J34" s="121"/>
-      <c r="K34" s="121"/>
-      <c r="L34" s="121"/>
+      <c r="A34" s="123"/>
+      <c r="B34" s="123"/>
+      <c r="C34" s="123"/>
+      <c r="D34" s="123"/>
+      <c r="E34" s="123"/>
+      <c r="F34" s="123"/>
+      <c r="G34" s="123"/>
+      <c r="H34" s="123"/>
+      <c r="I34" s="123"/>
+      <c r="J34" s="123"/>
+      <c r="K34" s="123"/>
+      <c r="L34" s="123"/>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A35" s="121"/>
-      <c r="B35" s="121"/>
-      <c r="C35" s="121"/>
-      <c r="D35" s="121"/>
-      <c r="E35" s="121"/>
-      <c r="F35" s="121"/>
-      <c r="G35" s="121"/>
-      <c r="H35" s="121"/>
-      <c r="I35" s="121"/>
-      <c r="J35" s="121"/>
-      <c r="K35" s="121"/>
-      <c r="L35" s="121"/>
+      <c r="A35" s="123"/>
+      <c r="B35" s="123"/>
+      <c r="C35" s="123"/>
+      <c r="D35" s="123"/>
+      <c r="E35" s="123"/>
+      <c r="F35" s="123"/>
+      <c r="G35" s="123"/>
+      <c r="H35" s="123"/>
+      <c r="I35" s="123"/>
+      <c r="J35" s="123"/>
+      <c r="K35" s="123"/>
+      <c r="L35" s="123"/>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A36" s="121"/>
-      <c r="B36" s="121"/>
-      <c r="C36" s="121"/>
-      <c r="D36" s="121"/>
-      <c r="E36" s="121"/>
-      <c r="F36" s="121"/>
-      <c r="G36" s="121"/>
-      <c r="H36" s="121"/>
-      <c r="I36" s="121"/>
-      <c r="J36" s="121"/>
-      <c r="K36" s="121"/>
-      <c r="L36" s="121"/>
+      <c r="A36" s="123"/>
+      <c r="B36" s="123"/>
+      <c r="C36" s="123"/>
+      <c r="D36" s="123"/>
+      <c r="E36" s="123"/>
+      <c r="F36" s="123"/>
+      <c r="G36" s="123"/>
+      <c r="H36" s="123"/>
+      <c r="I36" s="123"/>
+      <c r="J36" s="123"/>
+      <c r="K36" s="123"/>
+      <c r="L36" s="123"/>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A37" s="121"/>
-      <c r="B37" s="121"/>
-      <c r="C37" s="121"/>
-      <c r="D37" s="121"/>
-      <c r="E37" s="121"/>
-      <c r="F37" s="121"/>
-      <c r="G37" s="121"/>
-      <c r="H37" s="121"/>
-      <c r="I37" s="121"/>
-      <c r="J37" s="121"/>
-      <c r="K37" s="121"/>
-      <c r="L37" s="121"/>
+      <c r="A37" s="123"/>
+      <c r="B37" s="123"/>
+      <c r="C37" s="123"/>
+      <c r="D37" s="123"/>
+      <c r="E37" s="123"/>
+      <c r="F37" s="123"/>
+      <c r="G37" s="123"/>
+      <c r="H37" s="123"/>
+      <c r="I37" s="123"/>
+      <c r="J37" s="123"/>
+      <c r="K37" s="123"/>
+      <c r="L37" s="123"/>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A38" s="121"/>
-      <c r="B38" s="121"/>
-      <c r="C38" s="121"/>
-      <c r="D38" s="121"/>
-      <c r="E38" s="121"/>
-      <c r="F38" s="121"/>
-      <c r="G38" s="121"/>
-      <c r="H38" s="121"/>
-      <c r="I38" s="121"/>
-      <c r="J38" s="121"/>
-      <c r="K38" s="121"/>
-      <c r="L38" s="121"/>
+      <c r="A38" s="123"/>
+      <c r="B38" s="123"/>
+      <c r="C38" s="123"/>
+      <c r="D38" s="123"/>
+      <c r="E38" s="123"/>
+      <c r="F38" s="123"/>
+      <c r="G38" s="123"/>
+      <c r="H38" s="123"/>
+      <c r="I38" s="123"/>
+      <c r="J38" s="123"/>
+      <c r="K38" s="123"/>
+      <c r="L38" s="123"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -7782,14 +7791,14 @@
       </c>
     </row>
     <row r="2" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="153" t="s">
+      <c r="A2" s="155" t="s">
         <v>1191</v>
       </c>
-      <c r="B2" s="154"/>
-      <c r="C2" s="154"/>
-      <c r="D2" s="154"/>
-      <c r="E2" s="154"/>
-      <c r="F2" s="154"/>
+      <c r="B2" s="156"/>
+      <c r="C2" s="156"/>
+      <c r="D2" s="156"/>
+      <c r="E2" s="156"/>
+      <c r="F2" s="156"/>
     </row>
     <row r="3" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
@@ -8009,14 +8018,14 @@
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A18" s="153" t="s">
+      <c r="A18" s="155" t="s">
         <v>1240</v>
       </c>
-      <c r="B18" s="154"/>
-      <c r="C18" s="154"/>
-      <c r="D18" s="154"/>
-      <c r="E18" s="154"/>
-      <c r="F18" s="154"/>
+      <c r="B18" s="156"/>
+      <c r="C18" s="156"/>
+      <c r="D18" s="156"/>
+      <c r="E18" s="156"/>
+      <c r="F18" s="156"/>
     </row>
     <row r="19" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A19" s="5" t="s">
@@ -8094,11 +8103,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F65"/>
+  <dimension ref="A1:F66"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G3" sqref="G3"/>
+      <pane ySplit="1" topLeftCell="A51" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A66" sqref="A66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -8136,13 +8145,13 @@
       <c r="B2" s="120" t="s">
         <v>1293</v>
       </c>
-      <c r="C2" s="155" t="s">
+      <c r="C2" s="121" t="s">
         <v>1362</v>
       </c>
       <c r="D2" s="120" t="s">
         <v>1294</v>
       </c>
-      <c r="E2" s="156" t="s">
+      <c r="E2" s="122" t="s">
         <v>1362</v>
       </c>
     </row>
@@ -9146,6 +9155,17 @@
       </c>
       <c r="E65" s="40" t="s">
         <v>1354</v>
+      </c>
+    </row>
+    <row r="66" spans="2:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="B66" s="1" t="s">
+        <v>1363</v>
+      </c>
+      <c r="C66" s="2" t="s">
+        <v>1364</v>
+      </c>
+      <c r="E66" s="40" t="s">
+        <v>1365</v>
       </c>
     </row>
   </sheetData>
@@ -9932,13 +9952,13 @@
       </c>
     </row>
     <row r="2" spans="1:6" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="125" t="s">
+      <c r="A2" s="127" t="s">
         <v>313</v>
       </c>
-      <c r="B2" s="126"/>
-      <c r="C2" s="126"/>
-      <c r="D2" s="126"/>
-      <c r="E2" s="127"/>
+      <c r="B2" s="128"/>
+      <c r="C2" s="128"/>
+      <c r="D2" s="128"/>
+      <c r="E2" s="129"/>
       <c r="F2" s="33"/>
     </row>
     <row r="3" spans="1:6" ht="48" x14ac:dyDescent="0.2">
@@ -10066,13 +10086,13 @@
       <c r="F9" s="88"/>
     </row>
     <row r="10" spans="1:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="128" t="s">
+      <c r="A10" s="130" t="s">
         <v>342</v>
       </c>
-      <c r="B10" s="129"/>
-      <c r="C10" s="129"/>
-      <c r="D10" s="129"/>
-      <c r="E10" s="130"/>
+      <c r="B10" s="131"/>
+      <c r="C10" s="131"/>
+      <c r="D10" s="131"/>
+      <c r="E10" s="132"/>
       <c r="F10" s="88"/>
     </row>
     <row r="11" spans="1:6" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -10128,13 +10148,13 @@
       <c r="F13" s="88"/>
     </row>
     <row r="14" spans="1:6" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="122" t="s">
+      <c r="A14" s="124" t="s">
         <v>347</v>
       </c>
-      <c r="B14" s="123"/>
-      <c r="C14" s="123"/>
-      <c r="D14" s="123"/>
-      <c r="E14" s="124"/>
+      <c r="B14" s="125"/>
+      <c r="C14" s="125"/>
+      <c r="D14" s="125"/>
+      <c r="E14" s="126"/>
       <c r="F14" s="88"/>
     </row>
     <row r="15" spans="1:6" ht="48" x14ac:dyDescent="0.2">
@@ -10278,13 +10298,13 @@
       <c r="F23" s="88"/>
     </row>
     <row r="24" spans="1:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="122" t="s">
+      <c r="A24" s="124" t="s">
         <v>371</v>
       </c>
-      <c r="B24" s="123"/>
-      <c r="C24" s="123"/>
-      <c r="D24" s="123"/>
-      <c r="E24" s="124"/>
+      <c r="B24" s="125"/>
+      <c r="C24" s="125"/>
+      <c r="D24" s="125"/>
+      <c r="E24" s="126"/>
       <c r="F24" s="88"/>
     </row>
     <row r="25" spans="1:6" ht="32" x14ac:dyDescent="0.2">
@@ -10556,13 +10576,13 @@
       <c r="F42" s="88"/>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A43" s="122" t="s">
+      <c r="A43" s="124" t="s">
         <v>416</v>
       </c>
-      <c r="B43" s="123"/>
-      <c r="C43" s="123"/>
-      <c r="D43" s="123"/>
-      <c r="E43" s="124"/>
+      <c r="B43" s="125"/>
+      <c r="C43" s="125"/>
+      <c r="D43" s="125"/>
+      <c r="E43" s="126"/>
       <c r="F43" s="88"/>
     </row>
     <row r="44" spans="1:6" ht="32" x14ac:dyDescent="0.2">
@@ -10764,13 +10784,13 @@
       <c r="F56" s="88"/>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A57" s="122" t="s">
+      <c r="A57" s="124" t="s">
         <v>448</v>
       </c>
-      <c r="B57" s="123"/>
-      <c r="C57" s="123"/>
-      <c r="D57" s="123"/>
-      <c r="E57" s="124"/>
+      <c r="B57" s="125"/>
+      <c r="C57" s="125"/>
+      <c r="D57" s="125"/>
+      <c r="E57" s="126"/>
       <c r="F57" s="88"/>
     </row>
     <row r="58" spans="1:6" ht="64" x14ac:dyDescent="0.2">
@@ -10828,13 +10848,13 @@
       <c r="F60" s="88"/>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A61" s="122" t="s">
+      <c r="A61" s="124" t="s">
         <v>463</v>
       </c>
-      <c r="B61" s="123"/>
-      <c r="C61" s="123"/>
-      <c r="D61" s="123"/>
-      <c r="E61" s="124"/>
+      <c r="B61" s="125"/>
+      <c r="C61" s="125"/>
+      <c r="D61" s="125"/>
+      <c r="E61" s="126"/>
       <c r="F61" s="88"/>
     </row>
     <row r="62" spans="1:6" ht="48" x14ac:dyDescent="0.2">
@@ -10884,13 +10904,13 @@
       <c r="F64" s="88"/>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A65" s="122" t="s">
+      <c r="A65" s="124" t="s">
         <v>468</v>
       </c>
-      <c r="B65" s="123"/>
-      <c r="C65" s="123"/>
-      <c r="D65" s="123"/>
-      <c r="E65" s="124"/>
+      <c r="B65" s="125"/>
+      <c r="C65" s="125"/>
+      <c r="D65" s="125"/>
+      <c r="E65" s="126"/>
       <c r="F65" s="88"/>
     </row>
     <row r="66" spans="1:6" ht="32" x14ac:dyDescent="0.2">
@@ -11108,13 +11128,13 @@
       <c r="F79" s="88"/>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A80" s="122" t="s">
+      <c r="A80" s="124" t="s">
         <v>489</v>
       </c>
-      <c r="B80" s="123"/>
-      <c r="C80" s="123"/>
-      <c r="D80" s="123"/>
-      <c r="E80" s="124"/>
+      <c r="B80" s="125"/>
+      <c r="C80" s="125"/>
+      <c r="D80" s="125"/>
+      <c r="E80" s="126"/>
       <c r="F80" s="88"/>
     </row>
     <row r="81" spans="1:6" ht="62.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -11264,13 +11284,13 @@
       <c r="F89" s="88"/>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A90" s="122" t="s">
+      <c r="A90" s="124" t="s">
         <v>514</v>
       </c>
-      <c r="B90" s="123"/>
-      <c r="C90" s="123"/>
-      <c r="D90" s="123"/>
-      <c r="E90" s="124"/>
+      <c r="B90" s="125"/>
+      <c r="C90" s="125"/>
+      <c r="D90" s="125"/>
+      <c r="E90" s="126"/>
       <c r="F90" s="88"/>
     </row>
     <row r="91" spans="1:6" ht="48" x14ac:dyDescent="0.2">
@@ -11732,13 +11752,13 @@
       <c r="F120" s="88"/>
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A121" s="122" t="s">
+      <c r="A121" s="124" t="s">
         <v>596</v>
       </c>
-      <c r="B121" s="123"/>
-      <c r="C121" s="123"/>
-      <c r="D121" s="123"/>
-      <c r="E121" s="124"/>
+      <c r="B121" s="125"/>
+      <c r="C121" s="125"/>
+      <c r="D121" s="125"/>
+      <c r="E121" s="126"/>
       <c r="F121" s="88"/>
     </row>
     <row r="122" spans="1:6" ht="32" x14ac:dyDescent="0.2">
@@ -11926,13 +11946,13 @@
       <c r="F134" s="88"/>
     </row>
     <row r="135" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A135" s="122" t="s">
+      <c r="A135" s="124" t="s">
         <v>618</v>
       </c>
-      <c r="B135" s="123"/>
-      <c r="C135" s="123"/>
-      <c r="D135" s="123"/>
-      <c r="E135" s="124"/>
+      <c r="B135" s="125"/>
+      <c r="C135" s="125"/>
+      <c r="D135" s="125"/>
+      <c r="E135" s="126"/>
       <c r="F135" s="88"/>
     </row>
     <row r="136" spans="1:6" ht="64" x14ac:dyDescent="0.2">
@@ -12060,13 +12080,13 @@
       <c r="F143" s="88"/>
     </row>
     <row r="144" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A144" s="122" t="s">
+      <c r="A144" s="124" t="s">
         <v>639</v>
       </c>
-      <c r="B144" s="123"/>
-      <c r="C144" s="123"/>
-      <c r="D144" s="123"/>
-      <c r="E144" s="124"/>
+      <c r="B144" s="125"/>
+      <c r="C144" s="125"/>
+      <c r="D144" s="125"/>
+      <c r="E144" s="126"/>
       <c r="F144" s="88"/>
     </row>
     <row r="145" spans="1:6" ht="48" x14ac:dyDescent="0.2">
@@ -12194,13 +12214,13 @@
       <c r="F152" s="88"/>
     </row>
     <row r="153" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A153" s="122" t="s">
+      <c r="A153" s="124" t="s">
         <v>661</v>
       </c>
-      <c r="B153" s="123"/>
-      <c r="C153" s="123"/>
-      <c r="D153" s="123"/>
-      <c r="E153" s="124"/>
+      <c r="B153" s="125"/>
+      <c r="C153" s="125"/>
+      <c r="D153" s="125"/>
+      <c r="E153" s="126"/>
       <c r="F153" s="88"/>
     </row>
     <row r="154" spans="1:6" ht="48" x14ac:dyDescent="0.2">
@@ -12318,13 +12338,13 @@
       <c r="F160" s="88"/>
     </row>
     <row r="161" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A161" s="122" t="s">
+      <c r="A161" s="124" t="s">
         <v>677</v>
       </c>
-      <c r="B161" s="123"/>
-      <c r="C161" s="123"/>
-      <c r="D161" s="123"/>
-      <c r="E161" s="124"/>
+      <c r="B161" s="125"/>
+      <c r="C161" s="125"/>
+      <c r="D161" s="125"/>
+      <c r="E161" s="126"/>
       <c r="F161" s="88"/>
     </row>
     <row r="162" spans="1:6" ht="32" x14ac:dyDescent="0.2">
@@ -12498,13 +12518,13 @@
       <c r="F172" s="88"/>
     </row>
     <row r="173" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A173" s="122" t="s">
+      <c r="A173" s="124" t="s">
         <v>697</v>
       </c>
-      <c r="B173" s="123"/>
-      <c r="C173" s="123"/>
-      <c r="D173" s="123"/>
-      <c r="E173" s="124"/>
+      <c r="B173" s="125"/>
+      <c r="C173" s="125"/>
+      <c r="D173" s="125"/>
+      <c r="E173" s="126"/>
       <c r="F173" s="88"/>
     </row>
     <row r="174" spans="1:6" ht="32" x14ac:dyDescent="0.2">
@@ -12556,13 +12576,13 @@
       <c r="F176" s="88"/>
     </row>
     <row r="177" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A177" s="122" t="s">
+      <c r="A177" s="124" t="s">
         <v>706</v>
       </c>
-      <c r="B177" s="123"/>
-      <c r="C177" s="123"/>
-      <c r="D177" s="123"/>
-      <c r="E177" s="124"/>
+      <c r="B177" s="125"/>
+      <c r="C177" s="125"/>
+      <c r="D177" s="125"/>
+      <c r="E177" s="126"/>
       <c r="F177" s="88"/>
     </row>
     <row r="178" spans="1:6" ht="64" x14ac:dyDescent="0.2">
@@ -12648,13 +12668,13 @@
       <c r="F182" s="88"/>
     </row>
     <row r="183" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A183" s="122" t="s">
+      <c r="A183" s="124" t="s">
         <v>724</v>
       </c>
-      <c r="B183" s="123"/>
-      <c r="C183" s="123"/>
-      <c r="D183" s="123"/>
-      <c r="E183" s="124"/>
+      <c r="B183" s="125"/>
+      <c r="C183" s="125"/>
+      <c r="D183" s="125"/>
+      <c r="E183" s="126"/>
       <c r="F183" s="88"/>
     </row>
     <row r="184" spans="1:6" ht="32" x14ac:dyDescent="0.2">
@@ -12794,13 +12814,13 @@
       <c r="F192" s="88"/>
     </row>
     <row r="193" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A193" s="122" t="s">
+      <c r="A193" s="124" t="s">
         <v>737</v>
       </c>
-      <c r="B193" s="123"/>
-      <c r="C193" s="123"/>
-      <c r="D193" s="123"/>
-      <c r="E193" s="124"/>
+      <c r="B193" s="125"/>
+      <c r="C193" s="125"/>
+      <c r="D193" s="125"/>
+      <c r="E193" s="126"/>
       <c r="F193" s="88"/>
     </row>
     <row r="194" spans="1:6" ht="48" x14ac:dyDescent="0.2">
@@ -12886,13 +12906,13 @@
       <c r="F198" s="88"/>
     </row>
     <row r="199" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A199" s="122" t="s">
+      <c r="A199" s="124" t="s">
         <v>747</v>
       </c>
-      <c r="B199" s="123"/>
-      <c r="C199" s="123"/>
-      <c r="D199" s="123"/>
-      <c r="E199" s="124"/>
+      <c r="B199" s="125"/>
+      <c r="C199" s="125"/>
+      <c r="D199" s="125"/>
+      <c r="E199" s="126"/>
       <c r="F199" s="88"/>
     </row>
     <row r="200" spans="1:6" ht="32" x14ac:dyDescent="0.2">
@@ -13050,13 +13070,13 @@
       <c r="F209" s="88"/>
     </row>
     <row r="210" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A210" s="122" t="s">
+      <c r="A210" s="124" t="s">
         <v>761</v>
       </c>
-      <c r="B210" s="123"/>
-      <c r="C210" s="123"/>
-      <c r="D210" s="123"/>
-      <c r="E210" s="124"/>
+      <c r="B210" s="125"/>
+      <c r="C210" s="125"/>
+      <c r="D210" s="125"/>
+      <c r="E210" s="126"/>
       <c r="F210" s="88"/>
     </row>
     <row r="211" spans="1:6" ht="48" x14ac:dyDescent="0.2">
@@ -14051,18 +14071,6 @@
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="A210:E210"/>
-    <mergeCell ref="A173:E173"/>
-    <mergeCell ref="A177:E177"/>
-    <mergeCell ref="A183:E183"/>
-    <mergeCell ref="A193:E193"/>
-    <mergeCell ref="A199:E199"/>
-    <mergeCell ref="A57:E57"/>
-    <mergeCell ref="A2:E2"/>
-    <mergeCell ref="A10:E10"/>
-    <mergeCell ref="A14:E14"/>
-    <mergeCell ref="A24:E24"/>
-    <mergeCell ref="A43:E43"/>
     <mergeCell ref="A161:E161"/>
     <mergeCell ref="A153:E153"/>
     <mergeCell ref="A61:E61"/>
@@ -14072,6 +14080,18 @@
     <mergeCell ref="A135:E135"/>
     <mergeCell ref="A144:E144"/>
     <mergeCell ref="A90:E90"/>
+    <mergeCell ref="A57:E57"/>
+    <mergeCell ref="A2:E2"/>
+    <mergeCell ref="A10:E10"/>
+    <mergeCell ref="A14:E14"/>
+    <mergeCell ref="A24:E24"/>
+    <mergeCell ref="A43:E43"/>
+    <mergeCell ref="A210:E210"/>
+    <mergeCell ref="A173:E173"/>
+    <mergeCell ref="A177:E177"/>
+    <mergeCell ref="A183:E183"/>
+    <mergeCell ref="A193:E193"/>
+    <mergeCell ref="A199:E199"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -14118,13 +14138,13 @@
       </c>
     </row>
     <row r="2" spans="1:6" s="24" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="134" t="s">
+      <c r="A2" s="136" t="s">
         <v>812</v>
       </c>
-      <c r="B2" s="135"/>
-      <c r="C2" s="135"/>
-      <c r="D2" s="135"/>
-      <c r="E2" s="136"/>
+      <c r="B2" s="137"/>
+      <c r="C2" s="137"/>
+      <c r="D2" s="137"/>
+      <c r="E2" s="138"/>
     </row>
     <row r="3" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="19" t="s">
@@ -14255,13 +14275,13 @@
       </c>
     </row>
     <row r="12" spans="1:6" s="24" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="134" t="s">
+      <c r="A12" s="136" t="s">
         <v>831</v>
       </c>
-      <c r="B12" s="135"/>
-      <c r="C12" s="135"/>
-      <c r="D12" s="135"/>
-      <c r="E12" s="136"/>
+      <c r="B12" s="137"/>
+      <c r="C12" s="137"/>
+      <c r="D12" s="137"/>
+      <c r="E12" s="138"/>
     </row>
     <row r="13" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A13" s="19" t="s">
@@ -14373,13 +14393,13 @@
       </c>
     </row>
     <row r="20" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="143" t="s">
+      <c r="A20" s="145" t="s">
         <v>851</v>
       </c>
-      <c r="B20" s="144"/>
-      <c r="C20" s="144"/>
-      <c r="D20" s="144"/>
-      <c r="E20" s="145"/>
+      <c r="B20" s="146"/>
+      <c r="C20" s="146"/>
+      <c r="D20" s="146"/>
+      <c r="E20" s="147"/>
     </row>
     <row r="21" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A21" s="5" t="s">
@@ -14427,13 +14447,13 @@
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A24" s="140" t="s">
+      <c r="A24" s="142" t="s">
         <v>861</v>
       </c>
-      <c r="B24" s="141"/>
-      <c r="C24" s="141"/>
-      <c r="D24" s="141"/>
-      <c r="E24" s="142"/>
+      <c r="B24" s="143"/>
+      <c r="C24" s="143"/>
+      <c r="D24" s="143"/>
+      <c r="E24" s="144"/>
     </row>
     <row r="25" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A25" s="18" t="s">
@@ -14451,13 +14471,13 @@
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A26" s="131" t="s">
+      <c r="A26" s="133" t="s">
         <v>865</v>
       </c>
-      <c r="B26" s="132"/>
-      <c r="C26" s="132"/>
-      <c r="D26" s="132"/>
-      <c r="E26" s="133"/>
+      <c r="B26" s="134"/>
+      <c r="C26" s="134"/>
+      <c r="D26" s="134"/>
+      <c r="E26" s="135"/>
     </row>
     <row r="27" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A27" s="18" t="s">
@@ -14475,13 +14495,13 @@
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A28" s="131" t="s">
+      <c r="A28" s="133" t="s">
         <v>869</v>
       </c>
-      <c r="B28" s="132"/>
-      <c r="C28" s="132"/>
-      <c r="D28" s="132"/>
-      <c r="E28" s="133"/>
+      <c r="B28" s="134"/>
+      <c r="C28" s="134"/>
+      <c r="D28" s="134"/>
+      <c r="E28" s="135"/>
     </row>
     <row r="29" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A29" s="19" t="s">
@@ -14602,13 +14622,13 @@
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A37" s="131" t="s">
+      <c r="A37" s="133" t="s">
         <v>892</v>
       </c>
-      <c r="B37" s="132"/>
-      <c r="C37" s="132"/>
-      <c r="D37" s="132"/>
-      <c r="E37" s="133"/>
+      <c r="B37" s="134"/>
+      <c r="C37" s="134"/>
+      <c r="D37" s="134"/>
+      <c r="E37" s="135"/>
     </row>
     <row r="38" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A38" s="19" t="s">
@@ -14652,13 +14672,13 @@
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A41" s="137" t="s">
+      <c r="A41" s="139" t="s">
         <v>900</v>
       </c>
-      <c r="B41" s="138"/>
-      <c r="C41" s="138"/>
-      <c r="D41" s="138"/>
-      <c r="E41" s="139"/>
+      <c r="B41" s="140"/>
+      <c r="C41" s="140"/>
+      <c r="D41" s="140"/>
+      <c r="E41" s="141"/>
     </row>
     <row r="42" spans="1:6" ht="96" x14ac:dyDescent="0.2">
       <c r="A42" s="85" t="s">
@@ -15350,13 +15370,13 @@
       </c>
     </row>
     <row r="28" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="146" t="s">
+      <c r="A28" s="148" t="s">
         <v>1019</v>
       </c>
-      <c r="B28" s="147"/>
-      <c r="C28" s="147"/>
-      <c r="D28" s="147"/>
-      <c r="E28" s="148"/>
+      <c r="B28" s="149"/>
+      <c r="C28" s="149"/>
+      <c r="D28" s="149"/>
+      <c r="E28" s="150"/>
     </row>
     <row r="29" spans="1:5" ht="48" x14ac:dyDescent="0.2">
       <c r="A29" s="103" t="s">
@@ -15419,13 +15439,13 @@
       <c r="E32" s="109"/>
     </row>
     <row r="33" spans="1:6" s="13" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="149" t="s">
+      <c r="A33" s="151" t="s">
         <v>1031</v>
       </c>
-      <c r="B33" s="150"/>
-      <c r="C33" s="151"/>
-      <c r="D33" s="150"/>
-      <c r="E33" s="152"/>
+      <c r="B33" s="152"/>
+      <c r="C33" s="153"/>
+      <c r="D33" s="152"/>
+      <c r="E33" s="154"/>
     </row>
     <row r="34" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A34" s="107" t="s">
@@ -15628,13 +15648,13 @@
       <c r="F45" s="98"/>
     </row>
     <row r="46" spans="1:6" s="13" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="146" t="s">
+      <c r="A46" s="148" t="s">
         <v>1061</v>
       </c>
-      <c r="B46" s="147"/>
-      <c r="C46" s="147"/>
-      <c r="D46" s="147"/>
-      <c r="E46" s="148"/>
+      <c r="B46" s="149"/>
+      <c r="C46" s="149"/>
+      <c r="D46" s="149"/>
+      <c r="E46" s="150"/>
     </row>
     <row r="47" spans="1:6" s="30" customFormat="1" ht="64" x14ac:dyDescent="0.2">
       <c r="A47" s="107" t="s">
@@ -16262,15 +16282,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <Readyforteam_x003f_ xmlns="565e1b1d-057e-4d85-b896-01a5881d8a45">false</Readyforteam_x003f_>
@@ -16309,6 +16320,15 @@
     <TaxCatchAll xmlns="2799d30d-6731-4efe-ac9b-c4895a8828d9" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -16589,14 +16609,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8D7CE8C7-18DC-484F-8376-ED09F13D44C8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{017ACE96-8143-486E-8436-7787F6B96F4A}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -16605,6 +16617,14 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
     <ds:schemaRef ds:uri="bf601f31-63a1-4825-9216-91d773c5ef9c"/>
     <ds:schemaRef ds:uri="2799d30d-6731-4efe-ac9b-c4895a8828d9"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8D7CE8C7-18DC-484F-8376-ED09F13D44C8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
[MCCDB-636] Prototype Change - AP - Has a post-mortem been held (v10-1, v11, v11bi)
</commit_message>
<xml_diff>
--- a/app/data/MCCD-localisation.xlsx
+++ b/app/data/MCCD-localisation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/JALAT/GIT/medical-certificate-of-cause-of-death/app/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89F2767B-2DC0-D54F-898D-1CEE9B3322F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB276E68-948D-1F48-A916-DDB231A499F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="14220" firstSheet="3" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="14220" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Using this document" sheetId="8" r:id="rId1"/>
@@ -4228,12 +4228,6 @@
     <t>pmInputLabelReportedToCoroner</t>
   </si>
   <si>
-    <t>This death was reported to the coroner who decided not to investigate</t>
-  </si>
-  <si>
-    <t>Cafodd y farwolaeth hon ei hadrodd i'r crwner a benderfynodd beidio ag ymchwilio</t>
-  </si>
-  <si>
     <t>pmValidationSummaryEmpty</t>
   </si>
   <si>
@@ -5749,13 +5743,19 @@
     <t>Neu rhowch god post ysbyty</t>
   </si>
   <si>
-    <t>008</t>
-  </si>
-  <si>
     <t>This certificate will now be sent to the medical examiner office for review and scrutiny.&lt;br /&gt;&lt;br /&gt;A summary of this certificate can be accessed from your dashboard.</t>
   </si>
   <si>
     <t>You will be contacted by the medical examiner office if, following review and scrutiny of the cause of death the medical examiner requests that you amend this MCCD. You must then sign back in to edit the information on this certificate.&lt;br /&gt;&lt;br /&gt;You will be notified by email when the approved certificate is sent to the local register office.</t>
+  </si>
+  <si>
+    <t>This death was reported to the coroner whose duty to investigate under s1 CJA2009 was not engaged</t>
+  </si>
+  <si>
+    <t>Hysbyswyd y crwner am y farwolaeth hon ac nid oedd ei ddyletswydd i ymchwilio o dan adran 1 o Ddeddf Crwneriaid a Chyfiawnder 2009 yn gymwys</t>
+  </si>
+  <si>
+    <t>009</t>
   </si>
 </sst>
 </file>
@@ -6225,7 +6225,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="191">
+  <cellXfs count="193">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -6690,6 +6690,24 @@
     <xf numFmtId="0" fontId="13" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -6699,24 +6717,6 @@
     <xf numFmtId="0" fontId="6" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
@@ -6788,6 +6788,12 @@
     </xf>
     <xf numFmtId="0" fontId="13" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -7758,33 +7764,33 @@
         <v>243</v>
       </c>
       <c r="B2" s="95" t="s">
+        <v>1278</v>
+      </c>
+      <c r="C2" s="96" t="s">
+        <v>1279</v>
+      </c>
+      <c r="D2" s="95" t="s">
         <v>1280</v>
       </c>
-      <c r="C2" s="96" t="s">
+      <c r="E2" s="87" t="s">
         <v>1281</v>
-      </c>
-      <c r="D2" s="95" t="s">
-        <v>1282</v>
-      </c>
-      <c r="E2" s="87" t="s">
-        <v>1283</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="80" x14ac:dyDescent="0.2">
       <c r="A3" s="97" t="s">
+        <v>1282</v>
+      </c>
+      <c r="B3" s="98" t="s">
+        <v>1283</v>
+      </c>
+      <c r="C3" s="99" t="s">
         <v>1284</v>
       </c>
-      <c r="B3" s="98" t="s">
+      <c r="D3" s="98" t="s">
         <v>1285</v>
       </c>
-      <c r="C3" s="99" t="s">
+      <c r="E3" s="92" t="s">
         <v>1286</v>
-      </c>
-      <c r="D3" s="98" t="s">
-        <v>1287</v>
-      </c>
-      <c r="E3" s="92" t="s">
-        <v>1288</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="16" x14ac:dyDescent="0.2">
@@ -7792,16 +7798,16 @@
         <v>771</v>
       </c>
       <c r="B4" s="98" t="s">
-        <v>1289</v>
+        <v>1287</v>
       </c>
       <c r="C4" s="99" t="s">
-        <v>1290</v>
+        <v>1288</v>
       </c>
       <c r="D4" s="98" t="s">
         <v>414</v>
       </c>
       <c r="E4" s="92" t="s">
-        <v>1291</v>
+        <v>1289</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="60.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -7809,13 +7815,13 @@
         <v>421</v>
       </c>
       <c r="B5" s="108" t="s">
-        <v>1292</v>
+        <v>1290</v>
       </c>
       <c r="C5" s="109" t="s">
         <v>414</v>
       </c>
       <c r="D5" s="110" t="s">
-        <v>1293</v>
+        <v>1291</v>
       </c>
       <c r="E5" s="92" t="s">
         <v>414</v>
@@ -7826,13 +7832,13 @@
         <v>424</v>
       </c>
       <c r="B6" s="108" t="s">
-        <v>1294</v>
+        <v>1292</v>
       </c>
       <c r="C6" s="109" t="s">
         <v>414</v>
       </c>
       <c r="D6" s="110" t="s">
-        <v>1295</v>
+        <v>1293</v>
       </c>
       <c r="E6" s="92" t="s">
         <v>414</v>
@@ -7860,33 +7866,33 @@
         <v>243</v>
       </c>
       <c r="B8" s="98" t="s">
+        <v>1294</v>
+      </c>
+      <c r="C8" s="99" t="s">
+        <v>1295</v>
+      </c>
+      <c r="D8" s="98" t="s">
         <v>1296</v>
       </c>
-      <c r="C8" s="99" t="s">
+      <c r="E8" s="92" t="s">
         <v>1297</v>
-      </c>
-      <c r="D8" s="98" t="s">
-        <v>1298</v>
-      </c>
-      <c r="E8" s="92" t="s">
-        <v>1299</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="64" x14ac:dyDescent="0.2">
       <c r="A9" s="97" t="s">
-        <v>1284</v>
+        <v>1282</v>
       </c>
       <c r="B9" s="98" t="s">
+        <v>1298</v>
+      </c>
+      <c r="C9" s="99" t="s">
+        <v>1299</v>
+      </c>
+      <c r="D9" s="98" t="s">
         <v>1300</v>
       </c>
-      <c r="C9" s="99" t="s">
+      <c r="E9" s="92" t="s">
         <v>1301</v>
-      </c>
-      <c r="D9" s="98" t="s">
-        <v>1302</v>
-      </c>
-      <c r="E9" s="92" t="s">
-        <v>1303</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="16" x14ac:dyDescent="0.2">
@@ -7894,10 +7900,10 @@
         <v>771</v>
       </c>
       <c r="B10" s="98" t="s">
-        <v>1304</v>
+        <v>1302</v>
       </c>
       <c r="C10" s="99" t="s">
-        <v>1305</v>
+        <v>1303</v>
       </c>
       <c r="D10" s="98" t="s">
         <v>414</v>
@@ -7911,13 +7917,13 @@
         <v>421</v>
       </c>
       <c r="B11" s="108" t="s">
-        <v>1306</v>
+        <v>1304</v>
       </c>
       <c r="C11" s="109" t="s">
         <v>414</v>
       </c>
       <c r="D11" s="110" t="s">
-        <v>1293</v>
+        <v>1291</v>
       </c>
       <c r="E11" s="92" t="s">
         <v>414</v>
@@ -7928,13 +7934,13 @@
         <v>424</v>
       </c>
       <c r="B12" s="108" t="s">
-        <v>1307</v>
+        <v>1305</v>
       </c>
       <c r="C12" s="109" t="s">
         <v>414</v>
       </c>
       <c r="D12" s="110" t="s">
-        <v>1295</v>
+        <v>1293</v>
       </c>
       <c r="E12" s="92" t="s">
         <v>414</v>
@@ -7962,13 +7968,13 @@
         <v>243</v>
       </c>
       <c r="B14" s="98" t="s">
+        <v>1306</v>
+      </c>
+      <c r="C14" s="99" t="s">
+        <v>1307</v>
+      </c>
+      <c r="D14" s="98" t="s">
         <v>1308</v>
-      </c>
-      <c r="C14" s="99" t="s">
-        <v>1309</v>
-      </c>
-      <c r="D14" s="98" t="s">
-        <v>1310</v>
       </c>
       <c r="E14" s="92" t="s">
         <v>414</v>
@@ -7976,19 +7982,19 @@
     </row>
     <row r="15" spans="1:6" ht="96" x14ac:dyDescent="0.2">
       <c r="A15" s="97" t="s">
-        <v>1284</v>
+        <v>1282</v>
       </c>
       <c r="B15" s="98" t="s">
+        <v>1309</v>
+      </c>
+      <c r="C15" s="99" t="s">
+        <v>1310</v>
+      </c>
+      <c r="D15" s="98" t="s">
         <v>1311</v>
       </c>
-      <c r="C15" s="99" t="s">
+      <c r="E15" s="92" t="s">
         <v>1312</v>
-      </c>
-      <c r="D15" s="98" t="s">
-        <v>1313</v>
-      </c>
-      <c r="E15" s="92" t="s">
-        <v>1314</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="48" x14ac:dyDescent="0.2">
@@ -7996,13 +8002,13 @@
         <v>421</v>
       </c>
       <c r="B16" s="108" t="s">
-        <v>1315</v>
+        <v>1313</v>
       </c>
       <c r="C16" s="109" t="s">
         <v>414</v>
       </c>
       <c r="D16" s="110" t="s">
-        <v>1293</v>
+        <v>1291</v>
       </c>
       <c r="E16" s="92" t="s">
         <v>414</v>
@@ -8013,13 +8019,13 @@
         <v>424</v>
       </c>
       <c r="B17" s="108" t="s">
-        <v>1316</v>
+        <v>1314</v>
       </c>
       <c r="C17" s="109" t="s">
         <v>414</v>
       </c>
       <c r="D17" s="110" t="s">
-        <v>1295</v>
+        <v>1293</v>
       </c>
       <c r="E17" s="92" t="s">
         <v>414</v>
@@ -8030,16 +8036,16 @@
         <v>14</v>
       </c>
       <c r="B18" s="98" t="s">
-        <v>1317</v>
+        <v>1315</v>
       </c>
       <c r="C18" s="99" t="s">
-        <v>1318</v>
+        <v>1316</v>
       </c>
       <c r="D18" s="98" t="s">
         <v>414</v>
       </c>
       <c r="E18" s="92" t="s">
-        <v>1319</v>
+        <v>1317</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -8064,13 +8070,13 @@
         <v>243</v>
       </c>
       <c r="B20" s="98" t="s">
-        <v>1320</v>
+        <v>1318</v>
       </c>
       <c r="C20" s="99" t="s">
-        <v>1321</v>
+        <v>1319</v>
       </c>
       <c r="D20" s="98" t="s">
-        <v>1282</v>
+        <v>1280</v>
       </c>
       <c r="E20" s="92" t="s">
         <v>414</v>
@@ -8078,16 +8084,16 @@
     </row>
     <row r="21" spans="1:5" ht="48" x14ac:dyDescent="0.2">
       <c r="A21" s="97" t="s">
-        <v>1284</v>
+        <v>1282</v>
       </c>
       <c r="B21" s="98" t="s">
+        <v>1320</v>
+      </c>
+      <c r="C21" s="99" t="s">
+        <v>1321</v>
+      </c>
+      <c r="D21" s="98" t="s">
         <v>1322</v>
-      </c>
-      <c r="C21" s="99" t="s">
-        <v>1323</v>
-      </c>
-      <c r="D21" s="98" t="s">
-        <v>1324</v>
       </c>
       <c r="E21" s="92" t="s">
         <v>414</v>
@@ -8098,10 +8104,10 @@
         <v>771</v>
       </c>
       <c r="B22" s="98" t="s">
-        <v>1325</v>
+        <v>1323</v>
       </c>
       <c r="C22" s="99" t="s">
-        <v>1326</v>
+        <v>1324</v>
       </c>
       <c r="D22" s="98" t="s">
         <v>414</v>
@@ -8115,13 +8121,13 @@
         <v>421</v>
       </c>
       <c r="B23" s="108" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="C23" s="109" t="s">
         <v>414</v>
       </c>
       <c r="D23" s="110" t="s">
-        <v>1293</v>
+        <v>1291</v>
       </c>
       <c r="E23" s="92" t="s">
         <v>414</v>
@@ -8132,13 +8138,13 @@
         <v>424</v>
       </c>
       <c r="B24" s="108" t="s">
-        <v>1328</v>
+        <v>1326</v>
       </c>
       <c r="C24" s="109" t="s">
         <v>414</v>
       </c>
       <c r="D24" s="110" t="s">
-        <v>1295</v>
+        <v>1293</v>
       </c>
       <c r="E24" s="92" t="s">
         <v>414</v>
@@ -8153,9 +8159,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{124C2F8F-96ED-4E65-B816-FFFEB93DC889}">
   <dimension ref="A1:F23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C20" sqref="C20:C22"/>
+      <selection pane="bottomLeft" activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -8191,7 +8197,7 @@
     </row>
     <row r="2" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="189" t="s">
-        <v>1329</v>
+        <v>1327</v>
       </c>
       <c r="B2" s="190"/>
       <c r="C2" s="190"/>
@@ -8204,16 +8210,16 @@
         <v>243</v>
       </c>
       <c r="B3" s="5" t="s">
+        <v>1328</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>1329</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>1260</v>
+      </c>
+      <c r="E3" s="37" t="s">
         <v>1330</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>1331</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>1262</v>
-      </c>
-      <c r="E3" s="37" t="s">
-        <v>1332</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="32" x14ac:dyDescent="0.2">
@@ -8221,13 +8227,13 @@
         <v>261</v>
       </c>
       <c r="B4" s="5" t="s">
+        <v>1331</v>
+      </c>
+      <c r="C4" s="59" t="s">
+        <v>1332</v>
+      </c>
+      <c r="E4" s="37" t="s">
         <v>1333</v>
-      </c>
-      <c r="C4" s="59" t="s">
-        <v>1334</v>
-      </c>
-      <c r="E4" s="37" t="s">
-        <v>1335</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="16" x14ac:dyDescent="0.2">
@@ -8235,13 +8241,13 @@
         <v>254</v>
       </c>
       <c r="B5" s="5" t="s">
+        <v>1334</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>1335</v>
+      </c>
+      <c r="E5" s="37" t="s">
         <v>1336</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>1337</v>
-      </c>
-      <c r="E5" s="37" t="s">
-        <v>1338</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="80" x14ac:dyDescent="0.2">
@@ -8249,13 +8255,13 @@
         <v>261</v>
       </c>
       <c r="B6" s="5" t="s">
+        <v>1337</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>1338</v>
+      </c>
+      <c r="E6" s="37" t="s">
         <v>1339</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>1340</v>
-      </c>
-      <c r="E6" s="37" t="s">
-        <v>1341</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="32" x14ac:dyDescent="0.2">
@@ -8263,127 +8269,127 @@
         <v>254</v>
       </c>
       <c r="B7" s="5" t="s">
+        <v>1340</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>1341</v>
+      </c>
+      <c r="E7" s="37" t="s">
         <v>1342</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>1343</v>
-      </c>
-      <c r="E7" s="37" t="s">
-        <v>1344</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
+        <v>1343</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>1344</v>
+      </c>
+      <c r="C8" s="6" t="s">
         <v>1345</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="E8" s="37" t="s">
         <v>1346</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>1347</v>
-      </c>
-      <c r="E8" s="37" t="s">
-        <v>1348</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
+        <v>1347</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>1348</v>
+      </c>
+      <c r="C9" s="6" t="s">
         <v>1349</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="E9" s="37" t="s">
         <v>1350</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>1351</v>
-      </c>
-      <c r="E9" s="37" t="s">
-        <v>1352</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
-        <v>1349</v>
+        <v>1347</v>
       </c>
       <c r="B10" s="5" t="s">
+        <v>1351</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>1352</v>
+      </c>
+      <c r="E10" s="37" t="s">
         <v>1353</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>1354</v>
-      </c>
-      <c r="E10" s="37" t="s">
-        <v>1355</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
-        <v>1349</v>
+        <v>1347</v>
       </c>
       <c r="B11" s="5" t="s">
+        <v>1354</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>1355</v>
+      </c>
+      <c r="E11" s="37" t="s">
         <v>1356</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>1357</v>
-      </c>
-      <c r="E11" s="37" t="s">
-        <v>1358</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="5" t="s">
-        <v>1349</v>
+        <v>1347</v>
       </c>
       <c r="B12" s="5" t="s">
+        <v>1357</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>1358</v>
+      </c>
+      <c r="E12" s="37" t="s">
         <v>1359</v>
-      </c>
-      <c r="C12" s="6" t="s">
-        <v>1360</v>
-      </c>
-      <c r="E12" s="37" t="s">
-        <v>1361</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="s">
-        <v>1349</v>
+        <v>1347</v>
       </c>
       <c r="B13" s="5" t="s">
+        <v>1360</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>1361</v>
+      </c>
+      <c r="E13" s="37" t="s">
         <v>1362</v>
-      </c>
-      <c r="C13" s="6" t="s">
-        <v>1363</v>
-      </c>
-      <c r="E13" s="37" t="s">
-        <v>1364</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A14" s="5" t="s">
-        <v>1345</v>
+        <v>1343</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>1365</v>
+        <v>1363</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>1366</v>
+        <v>1364</v>
       </c>
       <c r="D14" s="1"/>
       <c r="E14" s="37" t="s">
-        <v>1367</v>
+        <v>1365</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A15" s="5" t="s">
-        <v>974</v>
+        <v>972</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>1368</v>
+        <v>1366</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>1369</v>
+        <v>1367</v>
       </c>
       <c r="D15" s="1"/>
       <c r="E15" s="37" t="s">
-        <v>1370</v>
+        <v>1368</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="16" x14ac:dyDescent="0.2">
@@ -8391,34 +8397,34 @@
         <v>14</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>1371</v>
+        <v>1369</v>
       </c>
       <c r="C16" s="75" t="s">
-        <v>1372</v>
+        <v>1370</v>
       </c>
       <c r="D16" s="18"/>
       <c r="E16" s="37" t="s">
-        <v>1373</v>
+        <v>1371</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A17" s="5" t="s">
+        <v>1372</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>1373</v>
+      </c>
+      <c r="C17" s="76" t="s">
         <v>1374</v>
-      </c>
-      <c r="B17" s="7" t="s">
-        <v>1375</v>
-      </c>
-      <c r="C17" s="76" t="s">
-        <v>1376</v>
       </c>
       <c r="D17" s="18"/>
       <c r="E17" s="37" t="s">
-        <v>1377</v>
+        <v>1375</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="189" t="s">
-        <v>1378</v>
+        <v>1376</v>
       </c>
       <c r="B18" s="190"/>
       <c r="C18" s="190"/>
@@ -8431,16 +8437,16 @@
         <v>243</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>1381</v>
+        <v>1379</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>1379</v>
+        <v>1377</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>1262</v>
+        <v>1260</v>
       </c>
       <c r="E19" s="37" t="s">
-        <v>1380</v>
+        <v>1378</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="64" x14ac:dyDescent="0.2">
@@ -8448,10 +8454,10 @@
         <v>261</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>1382</v>
+        <v>1380</v>
       </c>
       <c r="C20" s="59" t="s">
-        <v>1394</v>
+        <v>1391</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="16" x14ac:dyDescent="0.2">
@@ -8459,13 +8465,13 @@
         <v>254</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>1383</v>
+        <v>1381</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>1337</v>
+        <v>1335</v>
       </c>
       <c r="E21" s="37" t="s">
-        <v>1338</v>
+        <v>1336</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="128" x14ac:dyDescent="0.2">
@@ -8473,10 +8479,10 @@
         <v>261</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>1384</v>
+        <v>1382</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>1395</v>
+        <v>1392</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
@@ -8498,9 +8504,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F66"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F3" sqref="F3"/>
+      <selection pane="bottomLeft" activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -8540,13 +8546,13 @@
         <v>7</v>
       </c>
       <c r="C2" s="103" t="s">
-        <v>1393</v>
+        <v>1395</v>
       </c>
       <c r="D2" s="101" t="s">
         <v>8</v>
       </c>
       <c r="E2" s="102" t="s">
-        <v>1393</v>
+        <v>1395</v>
       </c>
       <c r="F2" s="101"/>
     </row>
@@ -10408,13 +10414,13 @@
       </c>
     </row>
     <row r="2" spans="1:6" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="161" t="s">
+      <c r="A2" s="158" t="s">
         <v>374</v>
       </c>
-      <c r="B2" s="162"/>
-      <c r="C2" s="162"/>
-      <c r="D2" s="162"/>
-      <c r="E2" s="163"/>
+      <c r="B2" s="159"/>
+      <c r="C2" s="159"/>
+      <c r="D2" s="159"/>
+      <c r="E2" s="160"/>
       <c r="F2" s="33"/>
     </row>
     <row r="3" spans="1:6" ht="48" x14ac:dyDescent="0.2">
@@ -10542,13 +10548,13 @@
       <c r="F9" s="122"/>
     </row>
     <row r="10" spans="1:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="164" t="s">
+      <c r="A10" s="161" t="s">
         <v>403</v>
       </c>
-      <c r="B10" s="165"/>
-      <c r="C10" s="165"/>
-      <c r="D10" s="165"/>
-      <c r="E10" s="166"/>
+      <c r="B10" s="162"/>
+      <c r="C10" s="162"/>
+      <c r="D10" s="162"/>
+      <c r="E10" s="163"/>
       <c r="F10" s="122"/>
     </row>
     <row r="11" spans="1:6" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -12487,7 +12493,7 @@
         <v>723</v>
       </c>
       <c r="C139" s="116" t="s">
-        <v>1386</v>
+        <v>1384</v>
       </c>
       <c r="D139" s="125" t="s">
         <v>724</v>
@@ -12577,7 +12583,7 @@
         <v>738</v>
       </c>
       <c r="C145" s="59" t="s">
-        <v>1385</v>
+        <v>1383</v>
       </c>
       <c r="D145" s="119" t="s">
         <v>739</v>
@@ -12608,14 +12614,14 @@
         <v>37</v>
       </c>
       <c r="B147" s="119" t="s">
+        <v>1385</v>
+      </c>
+      <c r="C147" s="59" t="s">
         <v>1387</v>
-      </c>
-      <c r="C147" s="59" t="s">
-        <v>1389</v>
       </c>
       <c r="D147" s="119"/>
       <c r="E147" s="123" t="s">
-        <v>1391</v>
+        <v>1389</v>
       </c>
       <c r="F147" s="122"/>
     </row>
@@ -12624,14 +12630,14 @@
         <v>37</v>
       </c>
       <c r="B148" s="119" t="s">
+        <v>1386</v>
+      </c>
+      <c r="C148" s="59" t="s">
         <v>1388</v>
-      </c>
-      <c r="C148" s="59" t="s">
-        <v>1390</v>
       </c>
       <c r="D148" s="119"/>
       <c r="E148" s="123" t="s">
-        <v>1392</v>
+        <v>1390</v>
       </c>
       <c r="F148" s="122"/>
     </row>
@@ -12850,13 +12856,13 @@
       <c r="F162" s="122"/>
     </row>
     <row r="163" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A163" s="158" t="s">
+      <c r="A163" s="164" t="s">
         <v>778</v>
       </c>
-      <c r="B163" s="159"/>
-      <c r="C163" s="159"/>
-      <c r="D163" s="159"/>
-      <c r="E163" s="160"/>
+      <c r="B163" s="165"/>
+      <c r="C163" s="165"/>
+      <c r="D163" s="165"/>
+      <c r="E163" s="166"/>
       <c r="F163" s="132" t="s">
         <v>779</v>
       </c>
@@ -14725,18 +14731,6 @@
     </row>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="A221:E221"/>
-    <mergeCell ref="A184:E184"/>
-    <mergeCell ref="A188:E188"/>
-    <mergeCell ref="A194:E194"/>
-    <mergeCell ref="A204:E204"/>
-    <mergeCell ref="A210:E210"/>
-    <mergeCell ref="A57:E57"/>
-    <mergeCell ref="A2:E2"/>
-    <mergeCell ref="A10:E10"/>
-    <mergeCell ref="A14:E14"/>
-    <mergeCell ref="A24:E24"/>
-    <mergeCell ref="A43:E43"/>
     <mergeCell ref="A172:E172"/>
     <mergeCell ref="A155:E155"/>
     <mergeCell ref="A61:E61"/>
@@ -14747,6 +14741,18 @@
     <mergeCell ref="A144:E144"/>
     <mergeCell ref="A90:E90"/>
     <mergeCell ref="A163:E163"/>
+    <mergeCell ref="A57:E57"/>
+    <mergeCell ref="A2:E2"/>
+    <mergeCell ref="A10:E10"/>
+    <mergeCell ref="A14:E14"/>
+    <mergeCell ref="A24:E24"/>
+    <mergeCell ref="A43:E43"/>
+    <mergeCell ref="A221:E221"/>
+    <mergeCell ref="A184:E184"/>
+    <mergeCell ref="A188:E188"/>
+    <mergeCell ref="A194:E194"/>
+    <mergeCell ref="A204:E204"/>
+    <mergeCell ref="A210:E210"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -14757,8 +14763,8 @@
   <dimension ref="A1:F54"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B8" sqref="B8"/>
+      <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -15009,21 +15015,21 @@
         <v>961</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A17" s="94" t="s">
         <v>84</v>
       </c>
       <c r="B17" s="95" t="s">
         <v>962</v>
       </c>
-      <c r="C17" s="96" t="s">
-        <v>963</v>
+      <c r="C17" s="191" t="s">
+        <v>1393</v>
       </c>
       <c r="D17" s="95" t="s">
         <v>954</v>
       </c>
-      <c r="E17" s="87" t="s">
-        <v>964</v>
+      <c r="E17" s="192" t="s">
+        <v>1394</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="80" x14ac:dyDescent="0.2">
@@ -15031,11 +15037,11 @@
         <v>421</v>
       </c>
       <c r="B18" s="28" t="s">
-        <v>965</v>
+        <v>963</v>
       </c>
       <c r="C18" s="27"/>
       <c r="D18" s="18" t="s">
-        <v>966</v>
+        <v>964</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="80" x14ac:dyDescent="0.2">
@@ -15043,16 +15049,16 @@
         <v>424</v>
       </c>
       <c r="B19" s="28" t="s">
-        <v>967</v>
+        <v>965</v>
       </c>
       <c r="C19" s="27"/>
       <c r="D19" s="18" t="s">
-        <v>968</v>
+        <v>966</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="179" t="s">
-        <v>969</v>
+        <v>967</v>
       </c>
       <c r="B20" s="180"/>
       <c r="C20" s="180"/>
@@ -15061,52 +15067,52 @@
     </row>
     <row r="21" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A21" s="5" t="s">
+        <v>968</v>
+      </c>
+      <c r="B21" s="94" t="s">
+        <v>969</v>
+      </c>
+      <c r="C21" s="6" t="s">
         <v>970</v>
-      </c>
-      <c r="B21" s="94" t="s">
-        <v>971</v>
-      </c>
-      <c r="C21" s="6" t="s">
-        <v>972</v>
       </c>
       <c r="D21" s="81"/>
       <c r="E21" s="82" t="s">
-        <v>973</v>
+        <v>971</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A22" s="81" t="s">
+        <v>972</v>
+      </c>
+      <c r="B22" s="97" t="s">
+        <v>973</v>
+      </c>
+      <c r="C22" s="83" t="s">
         <v>974</v>
-      </c>
-      <c r="B22" s="97" t="s">
-        <v>975</v>
-      </c>
-      <c r="C22" s="83" t="s">
-        <v>976</v>
       </c>
       <c r="D22" s="81"/>
       <c r="E22" s="82" t="s">
-        <v>977</v>
+        <v>975</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="64" x14ac:dyDescent="0.2">
       <c r="A23" s="81" t="s">
+        <v>976</v>
+      </c>
+      <c r="B23" s="97" t="s">
+        <v>977</v>
+      </c>
+      <c r="C23" s="83" t="s">
         <v>978</v>
-      </c>
-      <c r="B23" s="97" t="s">
-        <v>979</v>
-      </c>
-      <c r="C23" s="83" t="s">
-        <v>980</v>
       </c>
       <c r="D23" s="81"/>
       <c r="E23" s="82" t="s">
-        <v>981</v>
+        <v>979</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" s="176" t="s">
-        <v>982</v>
+        <v>980</v>
       </c>
       <c r="B24" s="177"/>
       <c r="C24" s="177"/>
@@ -15118,19 +15124,19 @@
         <v>243</v>
       </c>
       <c r="B25" s="28" t="s">
-        <v>983</v>
+        <v>981</v>
       </c>
       <c r="C25" s="27" t="s">
-        <v>984</v>
+        <v>982</v>
       </c>
       <c r="D25" s="18"/>
       <c r="E25" s="46" t="s">
-        <v>985</v>
+        <v>983</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" s="167" t="s">
-        <v>986</v>
+        <v>984</v>
       </c>
       <c r="B26" s="168"/>
       <c r="C26" s="168"/>
@@ -15142,19 +15148,19 @@
         <v>243</v>
       </c>
       <c r="B27" s="28" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
       <c r="C27" s="27" t="s">
-        <v>988</v>
+        <v>986</v>
       </c>
       <c r="D27" s="18"/>
       <c r="E27" s="46" t="s">
-        <v>989</v>
+        <v>987</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" s="167" t="s">
-        <v>990</v>
+        <v>988</v>
       </c>
       <c r="B28" s="168"/>
       <c r="C28" s="168"/>
@@ -15166,53 +15172,53 @@
         <v>243</v>
       </c>
       <c r="B29" s="95" t="s">
+        <v>989</v>
+      </c>
+      <c r="C29" s="96" t="s">
+        <v>990</v>
+      </c>
+      <c r="D29" s="95" t="s">
         <v>991</v>
       </c>
-      <c r="C29" s="96" t="s">
+      <c r="E29" s="87" t="s">
         <v>992</v>
       </c>
-      <c r="D29" s="95" t="s">
+      <c r="F29" s="72" t="s">
         <v>993</v>
-      </c>
-      <c r="E29" s="87" t="s">
-        <v>994</v>
-      </c>
-      <c r="F29" s="72" t="s">
-        <v>995</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A30" s="97" t="s">
-        <v>974</v>
+        <v>972</v>
       </c>
       <c r="B30" s="98" t="s">
+        <v>994</v>
+      </c>
+      <c r="C30" s="99" t="s">
+        <v>995</v>
+      </c>
+      <c r="D30" s="98" t="s">
         <v>996</v>
       </c>
-      <c r="C30" s="99" t="s">
+      <c r="E30" s="92" t="s">
         <v>997</v>
-      </c>
-      <c r="D30" s="98" t="s">
-        <v>998</v>
-      </c>
-      <c r="E30" s="92" t="s">
-        <v>999</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="335" x14ac:dyDescent="0.2">
       <c r="A31" s="97" t="s">
+        <v>998</v>
+      </c>
+      <c r="B31" s="98" t="s">
+        <v>999</v>
+      </c>
+      <c r="C31" s="99" t="s">
         <v>1000</v>
-      </c>
-      <c r="B31" s="98" t="s">
-        <v>1001</v>
-      </c>
-      <c r="C31" s="99" t="s">
-        <v>1002</v>
       </c>
       <c r="D31" s="98" t="s">
         <v>414</v>
       </c>
       <c r="E31" s="92" t="s">
-        <v>1003</v>
+        <v>1001</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="96" x14ac:dyDescent="0.2">
@@ -15220,13 +15226,13 @@
         <v>261</v>
       </c>
       <c r="B32" s="19" t="s">
+        <v>1002</v>
+      </c>
+      <c r="C32" s="21" t="s">
+        <v>1003</v>
+      </c>
+      <c r="E32" s="46" t="s">
         <v>1004</v>
-      </c>
-      <c r="C32" s="21" t="s">
-        <v>1005</v>
-      </c>
-      <c r="E32" s="46" t="s">
-        <v>1006</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="48" x14ac:dyDescent="0.2">
@@ -15234,16 +15240,16 @@
         <v>37</v>
       </c>
       <c r="B33" s="19" t="s">
+        <v>1005</v>
+      </c>
+      <c r="C33" s="21" t="s">
+        <v>1006</v>
+      </c>
+      <c r="D33" s="26" t="s">
         <v>1007</v>
       </c>
-      <c r="C33" s="21" t="s">
+      <c r="E33" s="46" t="s">
         <v>1008</v>
-      </c>
-      <c r="D33" s="26" t="s">
-        <v>1009</v>
-      </c>
-      <c r="E33" s="46" t="s">
-        <v>1010</v>
       </c>
     </row>
     <row r="34" spans="1:6" ht="96" x14ac:dyDescent="0.2">
@@ -15251,11 +15257,11 @@
         <v>421</v>
       </c>
       <c r="B34" s="28" t="s">
-        <v>1011</v>
+        <v>1009</v>
       </c>
       <c r="C34" s="27"/>
       <c r="D34" s="18" t="s">
-        <v>1012</v>
+        <v>1010</v>
       </c>
     </row>
     <row r="35" spans="1:6" ht="80" x14ac:dyDescent="0.2">
@@ -15263,11 +15269,11 @@
         <v>421</v>
       </c>
       <c r="B35" s="28" t="s">
-        <v>1013</v>
+        <v>1011</v>
       </c>
       <c r="C35" s="27"/>
       <c r="D35" s="18" t="s">
-        <v>1014</v>
+        <v>1012</v>
       </c>
     </row>
     <row r="36" spans="1:6" ht="80" x14ac:dyDescent="0.2">
@@ -15275,16 +15281,16 @@
         <v>424</v>
       </c>
       <c r="B36" s="28" t="s">
-        <v>1015</v>
+        <v>1013</v>
       </c>
       <c r="C36" s="27"/>
       <c r="D36" s="18" t="s">
-        <v>1016</v>
+        <v>1014</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" s="167" t="s">
-        <v>1017</v>
+        <v>1015</v>
       </c>
       <c r="B37" s="168"/>
       <c r="C37" s="168"/>
@@ -15296,16 +15302,16 @@
         <v>243</v>
       </c>
       <c r="B38" s="19" t="s">
+        <v>1016</v>
+      </c>
+      <c r="C38" s="21" t="s">
+        <v>1017</v>
+      </c>
+      <c r="D38" s="5" t="s">
         <v>1018</v>
       </c>
-      <c r="C38" s="21" t="s">
+      <c r="E38" s="46" t="s">
         <v>1019</v>
-      </c>
-      <c r="D38" s="5" t="s">
-        <v>1020</v>
-      </c>
-      <c r="E38" s="46" t="s">
-        <v>1021</v>
       </c>
     </row>
     <row r="39" spans="1:6" ht="64" x14ac:dyDescent="0.2">
@@ -15313,11 +15319,11 @@
         <v>421</v>
       </c>
       <c r="B39" s="28" t="s">
-        <v>1022</v>
+        <v>1020</v>
       </c>
       <c r="C39" s="27"/>
       <c r="D39" s="18" t="s">
-        <v>1023</v>
+        <v>1021</v>
       </c>
     </row>
     <row r="40" spans="1:6" ht="80" x14ac:dyDescent="0.2">
@@ -15325,16 +15331,16 @@
         <v>424</v>
       </c>
       <c r="B40" s="28" t="s">
-        <v>1024</v>
+        <v>1022</v>
       </c>
       <c r="C40" s="27"/>
       <c r="D40" s="18" t="s">
-        <v>1016</v>
+        <v>1014</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" s="173" t="s">
-        <v>1025</v>
+        <v>1023</v>
       </c>
       <c r="B41" s="174"/>
       <c r="C41" s="174"/>
@@ -15346,19 +15352,19 @@
         <v>243</v>
       </c>
       <c r="B42" s="119" t="s">
-        <v>1026</v>
+        <v>1024</v>
       </c>
       <c r="C42" s="21" t="s">
         <v>876</v>
       </c>
       <c r="D42" s="119" t="s">
-        <v>1027</v>
+        <v>1025</v>
       </c>
       <c r="E42" s="46" t="s">
         <v>878</v>
       </c>
       <c r="F42" s="73" t="s">
-        <v>1028</v>
+        <v>1026</v>
       </c>
     </row>
     <row r="43" spans="1:6" ht="80" x14ac:dyDescent="0.2">
@@ -15366,13 +15372,13 @@
         <v>375</v>
       </c>
       <c r="B43" s="119" t="s">
-        <v>1029</v>
+        <v>1027</v>
       </c>
       <c r="C43" s="21" t="s">
         <v>936</v>
       </c>
       <c r="D43" s="119" t="s">
-        <v>1030</v>
+        <v>1028</v>
       </c>
       <c r="E43" s="46" t="s">
         <v>937</v>
@@ -15383,16 +15389,16 @@
         <v>261</v>
       </c>
       <c r="B44" s="119" t="s">
+        <v>1029</v>
+      </c>
+      <c r="C44" s="62" t="s">
+        <v>1030</v>
+      </c>
+      <c r="D44" s="119" t="s">
         <v>1031</v>
       </c>
-      <c r="C44" s="62" t="s">
+      <c r="E44" s="46" t="s">
         <v>1032</v>
-      </c>
-      <c r="D44" s="119" t="s">
-        <v>1033</v>
-      </c>
-      <c r="E44" s="46" t="s">
-        <v>1034</v>
       </c>
     </row>
     <row r="45" spans="1:6" ht="48" x14ac:dyDescent="0.2">
@@ -15400,16 +15406,16 @@
         <v>389</v>
       </c>
       <c r="B45" s="119" t="s">
+        <v>1033</v>
+      </c>
+      <c r="C45" s="21" t="s">
+        <v>1034</v>
+      </c>
+      <c r="D45" s="124" t="s">
         <v>1035</v>
       </c>
-      <c r="C45" s="21" t="s">
-        <v>1036</v>
-      </c>
-      <c r="D45" s="124" t="s">
-        <v>1037</v>
-      </c>
       <c r="E45" s="46" t="s">
-        <v>1036</v>
+        <v>1034</v>
       </c>
     </row>
     <row r="46" spans="1:6" ht="64" x14ac:dyDescent="0.2">
@@ -15417,16 +15423,16 @@
         <v>389</v>
       </c>
       <c r="B46" s="119" t="s">
+        <v>1036</v>
+      </c>
+      <c r="C46" s="21" t="s">
+        <v>1037</v>
+      </c>
+      <c r="D46" s="124" t="s">
         <v>1038</v>
       </c>
-      <c r="C46" s="21" t="s">
+      <c r="E46" s="46" t="s">
         <v>1039</v>
-      </c>
-      <c r="D46" s="124" t="s">
-        <v>1040</v>
-      </c>
-      <c r="E46" s="46" t="s">
-        <v>1041</v>
       </c>
     </row>
     <row r="47" spans="1:6" ht="48" x14ac:dyDescent="0.2">
@@ -15434,16 +15440,16 @@
         <v>389</v>
       </c>
       <c r="B47" s="119" t="s">
+        <v>1040</v>
+      </c>
+      <c r="C47" s="21" t="s">
+        <v>1041</v>
+      </c>
+      <c r="D47" s="124" t="s">
         <v>1042</v>
       </c>
-      <c r="C47" s="21" t="s">
+      <c r="E47" s="46" t="s">
         <v>1043</v>
-      </c>
-      <c r="D47" s="124" t="s">
-        <v>1044</v>
-      </c>
-      <c r="E47" s="46" t="s">
-        <v>1045</v>
       </c>
     </row>
     <row r="48" spans="1:6" ht="48" x14ac:dyDescent="0.2">
@@ -15451,16 +15457,16 @@
         <v>389</v>
       </c>
       <c r="B48" s="119" t="s">
+        <v>1044</v>
+      </c>
+      <c r="C48" s="21" t="s">
+        <v>1045</v>
+      </c>
+      <c r="D48" s="124" t="s">
         <v>1046</v>
       </c>
-      <c r="C48" s="21" t="s">
+      <c r="E48" s="46" t="s">
         <v>1047</v>
-      </c>
-      <c r="D48" s="124" t="s">
-        <v>1048</v>
-      </c>
-      <c r="E48" s="46" t="s">
-        <v>1049</v>
       </c>
     </row>
     <row r="49" spans="1:6" ht="16" x14ac:dyDescent="0.2">
@@ -15468,16 +15474,16 @@
         <v>389</v>
       </c>
       <c r="B49" s="95" t="s">
-        <v>1050</v>
+        <v>1048</v>
       </c>
       <c r="C49" s="96" t="s">
-        <v>1051</v>
+        <v>1049</v>
       </c>
       <c r="D49" s="104" t="s">
         <v>414</v>
       </c>
       <c r="E49" s="87" t="s">
-        <v>1052</v>
+        <v>1050</v>
       </c>
     </row>
     <row r="50" spans="1:6" ht="16" x14ac:dyDescent="0.2">
@@ -15485,7 +15491,7 @@
         <v>32</v>
       </c>
       <c r="B50" s="19" t="s">
-        <v>1053</v>
+        <v>1051</v>
       </c>
       <c r="C50" s="21" t="s">
         <v>34</v>
@@ -15496,16 +15502,16 @@
     </row>
     <row r="51" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A51" s="19" t="s">
+        <v>1052</v>
+      </c>
+      <c r="B51" s="19" t="s">
+        <v>1053</v>
+      </c>
+      <c r="C51" s="21" t="s">
         <v>1054</v>
       </c>
-      <c r="B51" s="19" t="s">
+      <c r="D51" s="19" t="s">
         <v>1055</v>
-      </c>
-      <c r="C51" s="21" t="s">
-        <v>1056</v>
-      </c>
-      <c r="D51" s="19" t="s">
-        <v>1057</v>
       </c>
       <c r="F51" s="72" t="s">
         <v>924</v>
@@ -15513,16 +15519,16 @@
     </row>
     <row r="52" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A52" s="19" t="s">
-        <v>1054</v>
+        <v>1052</v>
       </c>
       <c r="B52" s="19" t="s">
-        <v>1058</v>
+        <v>1056</v>
       </c>
       <c r="C52" s="21" t="s">
-        <v>1059</v>
+        <v>1057</v>
       </c>
       <c r="D52" s="19" t="s">
-        <v>1057</v>
+        <v>1055</v>
       </c>
       <c r="F52" s="72" t="s">
         <v>924</v>
@@ -15533,13 +15539,13 @@
         <v>389</v>
       </c>
       <c r="B53" s="119" t="s">
+        <v>1058</v>
+      </c>
+      <c r="C53" s="21" t="s">
+        <v>1059</v>
+      </c>
+      <c r="D53" s="124" t="s">
         <v>1060</v>
-      </c>
-      <c r="C53" s="21" t="s">
-        <v>1061</v>
-      </c>
-      <c r="D53" s="124" t="s">
-        <v>1062</v>
       </c>
       <c r="F53" s="72" t="s">
         <v>924</v>
@@ -15550,13 +15556,13 @@
         <v>389</v>
       </c>
       <c r="B54" s="119" t="s">
+        <v>1061</v>
+      </c>
+      <c r="C54" s="21" t="s">
+        <v>1062</v>
+      </c>
+      <c r="D54" s="124" t="s">
         <v>1063</v>
-      </c>
-      <c r="C54" s="21" t="s">
-        <v>1064</v>
-      </c>
-      <c r="D54" s="124" t="s">
-        <v>1065</v>
       </c>
       <c r="F54" s="72" t="s">
         <v>924</v>
@@ -15622,52 +15628,52 @@
         <v>243</v>
       </c>
       <c r="B2" s="139" t="s">
-        <v>1066</v>
+        <v>1064</v>
       </c>
       <c r="C2" s="140" t="s">
-        <v>1067</v>
+        <v>1065</v>
       </c>
       <c r="D2" s="139" t="s">
         <v>246</v>
       </c>
       <c r="E2" s="141" t="s">
-        <v>1068</v>
+        <v>1066</v>
       </c>
       <c r="F2" s="138"/>
     </row>
     <row r="3" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A3" s="139" t="s">
-        <v>974</v>
+        <v>972</v>
       </c>
       <c r="B3" s="139" t="s">
+        <v>1067</v>
+      </c>
+      <c r="C3" s="140" t="s">
+        <v>1068</v>
+      </c>
+      <c r="D3" s="139" t="s">
         <v>1069</v>
       </c>
-      <c r="C3" s="140" t="s">
+      <c r="E3" s="141" t="s">
         <v>1070</v>
-      </c>
-      <c r="D3" s="139" t="s">
-        <v>1071</v>
-      </c>
-      <c r="E3" s="141" t="s">
-        <v>1072</v>
       </c>
       <c r="F3" s="138"/>
     </row>
     <row r="4" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A4" s="139" t="s">
+        <v>1071</v>
+      </c>
+      <c r="B4" s="139" t="s">
+        <v>1072</v>
+      </c>
+      <c r="C4" s="140" t="s">
         <v>1073</v>
       </c>
-      <c r="B4" s="139" t="s">
+      <c r="D4" s="139" t="s">
         <v>1074</v>
       </c>
-      <c r="C4" s="140" t="s">
+      <c r="E4" s="141" t="s">
         <v>1075</v>
-      </c>
-      <c r="D4" s="139" t="s">
-        <v>1076</v>
-      </c>
-      <c r="E4" s="141" t="s">
-        <v>1077</v>
       </c>
       <c r="F4" s="138"/>
     </row>
@@ -15676,11 +15682,11 @@
         <v>421</v>
       </c>
       <c r="B5" s="142" t="s">
-        <v>1078</v>
+        <v>1076</v>
       </c>
       <c r="C5" s="27"/>
       <c r="D5" s="139" t="s">
-        <v>1079</v>
+        <v>1077</v>
       </c>
       <c r="E5" s="141"/>
       <c r="F5" s="138"/>
@@ -15690,84 +15696,84 @@
         <v>424</v>
       </c>
       <c r="B6" s="142" t="s">
-        <v>1080</v>
+        <v>1078</v>
       </c>
       <c r="C6" s="27"/>
       <c r="D6" s="139" t="s">
-        <v>1081</v>
+        <v>1079</v>
       </c>
       <c r="E6" s="141"/>
       <c r="F6" s="138"/>
     </row>
     <row r="7" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A7" s="139" t="s">
-        <v>1073</v>
+        <v>1071</v>
       </c>
       <c r="B7" s="139" t="s">
+        <v>1080</v>
+      </c>
+      <c r="C7" s="140" t="s">
+        <v>1081</v>
+      </c>
+      <c r="D7" s="139" t="s">
         <v>1082</v>
       </c>
-      <c r="C7" s="140" t="s">
+      <c r="E7" s="141" t="s">
         <v>1083</v>
-      </c>
-      <c r="D7" s="139" t="s">
-        <v>1084</v>
-      </c>
-      <c r="E7" s="141" t="s">
-        <v>1085</v>
       </c>
       <c r="F7" s="138"/>
     </row>
     <row r="8" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A8" s="139" t="s">
-        <v>1073</v>
+        <v>1071</v>
       </c>
       <c r="B8" s="139" t="s">
+        <v>1084</v>
+      </c>
+      <c r="C8" s="140" t="s">
+        <v>1085</v>
+      </c>
+      <c r="D8" s="139" t="s">
         <v>1086</v>
       </c>
-      <c r="C8" s="140" t="s">
+      <c r="E8" s="141" t="s">
         <v>1087</v>
-      </c>
-      <c r="D8" s="139" t="s">
-        <v>1088</v>
-      </c>
-      <c r="E8" s="141" t="s">
-        <v>1089</v>
       </c>
       <c r="F8" s="138"/>
     </row>
     <row r="9" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A9" s="139" t="s">
-        <v>1073</v>
+        <v>1071</v>
       </c>
       <c r="B9" s="139" t="s">
+        <v>1088</v>
+      </c>
+      <c r="C9" s="140" t="s">
+        <v>1089</v>
+      </c>
+      <c r="D9" s="139" t="s">
         <v>1090</v>
       </c>
-      <c r="C9" s="140" t="s">
+      <c r="E9" s="141" t="s">
         <v>1091</v>
-      </c>
-      <c r="D9" s="139" t="s">
-        <v>1092</v>
-      </c>
-      <c r="E9" s="141" t="s">
-        <v>1093</v>
       </c>
       <c r="F9" s="138"/>
     </row>
     <row r="10" spans="1:6" ht="64" x14ac:dyDescent="0.2">
       <c r="A10" s="139" t="s">
-        <v>1073</v>
+        <v>1071</v>
       </c>
       <c r="B10" s="139" t="s">
+        <v>1092</v>
+      </c>
+      <c r="C10" s="140" t="s">
+        <v>1093</v>
+      </c>
+      <c r="D10" s="139" t="s">
         <v>1094</v>
       </c>
-      <c r="C10" s="140" t="s">
+      <c r="E10" s="141" t="s">
         <v>1095</v>
-      </c>
-      <c r="D10" s="139" t="s">
-        <v>1096</v>
-      </c>
-      <c r="E10" s="141" t="s">
-        <v>1097</v>
       </c>
       <c r="F10" s="138"/>
     </row>
@@ -15776,32 +15782,32 @@
         <v>254</v>
       </c>
       <c r="B11" s="139" t="s">
+        <v>1096</v>
+      </c>
+      <c r="C11" s="140" t="s">
+        <v>1097</v>
+      </c>
+      <c r="D11" s="139" t="s">
         <v>1098</v>
-      </c>
-      <c r="C11" s="140" t="s">
-        <v>1099</v>
-      </c>
-      <c r="D11" s="139" t="s">
-        <v>1100</v>
       </c>
       <c r="E11" s="141"/>
       <c r="F11" s="138"/>
     </row>
     <row r="12" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A12" s="139" t="s">
-        <v>1073</v>
+        <v>1071</v>
       </c>
       <c r="B12" s="139" t="s">
+        <v>1099</v>
+      </c>
+      <c r="C12" s="140" t="s">
+        <v>1100</v>
+      </c>
+      <c r="D12" s="139" t="s">
         <v>1101</v>
       </c>
-      <c r="C12" s="140" t="s">
+      <c r="E12" s="141" t="s">
         <v>1102</v>
-      </c>
-      <c r="D12" s="139" t="s">
-        <v>1103</v>
-      </c>
-      <c r="E12" s="141" t="s">
-        <v>1104</v>
       </c>
       <c r="F12" s="138"/>
     </row>
@@ -15810,11 +15816,11 @@
         <v>421</v>
       </c>
       <c r="B13" s="28" t="s">
-        <v>1105</v>
+        <v>1103</v>
       </c>
       <c r="C13" s="141"/>
       <c r="D13" s="139" t="s">
-        <v>1106</v>
+        <v>1104</v>
       </c>
       <c r="E13" s="141"/>
       <c r="F13" s="138"/>
@@ -15824,83 +15830,83 @@
         <v>424</v>
       </c>
       <c r="B14" s="28" t="s">
-        <v>1107</v>
+        <v>1105</v>
       </c>
       <c r="C14" s="141"/>
       <c r="D14" s="139" t="s">
-        <v>1081</v>
+        <v>1079</v>
       </c>
       <c r="E14" s="141"/>
       <c r="F14" s="138"/>
     </row>
     <row r="15" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A15" s="139" t="s">
-        <v>1073</v>
+        <v>1071</v>
       </c>
       <c r="B15" s="139" t="s">
+        <v>1106</v>
+      </c>
+      <c r="C15" s="140" t="s">
+        <v>1107</v>
+      </c>
+      <c r="D15" s="139" t="s">
         <v>1108</v>
       </c>
-      <c r="C15" s="140" t="s">
+      <c r="E15" s="141" t="s">
         <v>1109</v>
-      </c>
-      <c r="D15" s="139" t="s">
-        <v>1110</v>
-      </c>
-      <c r="E15" s="141" t="s">
-        <v>1111</v>
       </c>
       <c r="F15" s="138"/>
     </row>
     <row r="16" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A16" s="139" t="s">
-        <v>1073</v>
+        <v>1071</v>
       </c>
       <c r="B16" s="139" t="s">
+        <v>1110</v>
+      </c>
+      <c r="C16" s="140" t="s">
+        <v>1111</v>
+      </c>
+      <c r="D16" s="139" t="s">
         <v>1112</v>
       </c>
-      <c r="C16" s="140" t="s">
+      <c r="E16" s="141" t="s">
         <v>1113</v>
-      </c>
-      <c r="D16" s="139" t="s">
-        <v>1114</v>
-      </c>
-      <c r="E16" s="141" t="s">
-        <v>1115</v>
       </c>
       <c r="F16" s="138"/>
     </row>
     <row r="17" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A17" s="139" t="s">
-        <v>1073</v>
+        <v>1071</v>
       </c>
       <c r="B17" s="139" t="s">
+        <v>1114</v>
+      </c>
+      <c r="C17" s="140" t="s">
+        <v>1115</v>
+      </c>
+      <c r="D17" s="139" t="s">
         <v>1116</v>
       </c>
-      <c r="C17" s="140" t="s">
+      <c r="E17" s="141" t="s">
         <v>1117</v>
-      </c>
-      <c r="D17" s="139" t="s">
-        <v>1118</v>
-      </c>
-      <c r="E17" s="141" t="s">
-        <v>1119</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="144" x14ac:dyDescent="0.2">
       <c r="A18" s="139" t="s">
-        <v>1073</v>
+        <v>1071</v>
       </c>
       <c r="B18" s="139" t="s">
+        <v>1118</v>
+      </c>
+      <c r="C18" s="140" t="s">
+        <v>1119</v>
+      </c>
+      <c r="D18" s="29" t="s">
         <v>1120</v>
       </c>
-      <c r="C18" s="140" t="s">
+      <c r="E18" s="141" t="s">
         <v>1121</v>
-      </c>
-      <c r="D18" s="29" t="s">
-        <v>1122</v>
-      </c>
-      <c r="E18" s="141" t="s">
-        <v>1123</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="80" x14ac:dyDescent="0.2">
@@ -15908,11 +15914,11 @@
         <v>421</v>
       </c>
       <c r="B19" s="28" t="s">
-        <v>1124</v>
+        <v>1122</v>
       </c>
       <c r="C19" s="27"/>
       <c r="D19" s="18" t="s">
-        <v>1125</v>
+        <v>1123</v>
       </c>
       <c r="E19" s="141"/>
     </row>
@@ -15921,11 +15927,11 @@
         <v>424</v>
       </c>
       <c r="B20" s="28" t="s">
-        <v>1126</v>
+        <v>1124</v>
       </c>
       <c r="C20" s="27"/>
       <c r="D20" s="18" t="s">
-        <v>1081</v>
+        <v>1079</v>
       </c>
       <c r="E20" s="141"/>
     </row>
@@ -15934,29 +15940,29 @@
         <v>424</v>
       </c>
       <c r="B21" s="28" t="s">
-        <v>1127</v>
+        <v>1125</v>
       </c>
       <c r="C21" s="27"/>
       <c r="D21" s="18" t="s">
-        <v>1128</v>
+        <v>1126</v>
       </c>
       <c r="E21" s="141"/>
     </row>
     <row r="22" spans="1:5" ht="112" x14ac:dyDescent="0.2">
       <c r="A22" s="139" t="s">
+        <v>1127</v>
+      </c>
+      <c r="B22" s="139" t="s">
+        <v>1128</v>
+      </c>
+      <c r="C22" s="140" t="s">
         <v>1129</v>
       </c>
-      <c r="B22" s="139" t="s">
+      <c r="D22" s="139" t="s">
         <v>1130</v>
       </c>
-      <c r="C22" s="140" t="s">
+      <c r="E22" s="141" t="s">
         <v>1131</v>
-      </c>
-      <c r="D22" s="139" t="s">
-        <v>1132</v>
-      </c>
-      <c r="E22" s="141" t="s">
-        <v>1133</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="48" x14ac:dyDescent="0.2">
@@ -15964,11 +15970,11 @@
         <v>421</v>
       </c>
       <c r="B23" s="28" t="s">
-        <v>1134</v>
+        <v>1132</v>
       </c>
       <c r="C23" s="27"/>
       <c r="D23" s="139" t="s">
-        <v>1135</v>
+        <v>1133</v>
       </c>
       <c r="E23" s="141"/>
     </row>
@@ -15977,11 +15983,11 @@
         <v>424</v>
       </c>
       <c r="B24" s="28" t="s">
-        <v>1136</v>
+        <v>1134</v>
       </c>
       <c r="C24" s="27"/>
       <c r="D24" s="139" t="s">
-        <v>1137</v>
+        <v>1135</v>
       </c>
       <c r="E24" s="141"/>
     </row>
@@ -15990,11 +15996,11 @@
         <v>424</v>
       </c>
       <c r="B25" s="28" t="s">
-        <v>1138</v>
+        <v>1136</v>
       </c>
       <c r="C25" s="27"/>
       <c r="D25" s="29" t="s">
-        <v>1139</v>
+        <v>1137</v>
       </c>
       <c r="E25" s="141"/>
     </row>
@@ -16003,38 +16009,38 @@
         <v>254</v>
       </c>
       <c r="B26" s="139" t="s">
+        <v>1138</v>
+      </c>
+      <c r="C26" s="140" t="s">
+        <v>1139</v>
+      </c>
+      <c r="D26" s="139" t="s">
+        <v>1098</v>
+      </c>
+      <c r="E26" s="141" t="s">
         <v>1140</v>
-      </c>
-      <c r="C26" s="140" t="s">
-        <v>1141</v>
-      </c>
-      <c r="D26" s="139" t="s">
-        <v>1100</v>
-      </c>
-      <c r="E26" s="141" t="s">
-        <v>1142</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A27" s="139" t="s">
-        <v>1073</v>
+        <v>1071</v>
       </c>
       <c r="B27" s="139" t="s">
+        <v>1141</v>
+      </c>
+      <c r="C27" s="140" t="s">
+        <v>1142</v>
+      </c>
+      <c r="D27" s="139" t="s">
         <v>1143</v>
       </c>
-      <c r="C27" s="140" t="s">
+      <c r="E27" s="141" t="s">
         <v>1144</v>
-      </c>
-      <c r="D27" s="139" t="s">
-        <v>1145</v>
-      </c>
-      <c r="E27" s="141" t="s">
-        <v>1146</v>
       </c>
     </row>
     <row r="28" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A28" s="182" t="s">
-        <v>1147</v>
+        <v>1145</v>
       </c>
       <c r="B28" s="183"/>
       <c r="C28" s="183"/>
@@ -16046,33 +16052,33 @@
         <v>243</v>
       </c>
       <c r="B29" s="144" t="s">
+        <v>1146</v>
+      </c>
+      <c r="C29" s="145" t="s">
+        <v>1147</v>
+      </c>
+      <c r="D29" s="5" t="s">
         <v>1148</v>
       </c>
-      <c r="C29" s="145" t="s">
+      <c r="E29" s="146" t="s">
         <v>1149</v>
-      </c>
-      <c r="D29" s="5" t="s">
-        <v>1150</v>
-      </c>
-      <c r="E29" s="146" t="s">
-        <v>1151</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="64" x14ac:dyDescent="0.2">
       <c r="A30" s="147" t="s">
+        <v>1150</v>
+      </c>
+      <c r="B30" s="147" t="s">
+        <v>1151</v>
+      </c>
+      <c r="C30" s="148" t="s">
         <v>1152</v>
       </c>
-      <c r="B30" s="147" t="s">
+      <c r="D30" s="147" t="s">
         <v>1153</v>
       </c>
-      <c r="C30" s="148" t="s">
+      <c r="E30" s="149" t="s">
         <v>1154</v>
-      </c>
-      <c r="D30" s="147" t="s">
-        <v>1155</v>
-      </c>
-      <c r="E30" s="149" t="s">
-        <v>1156</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="48" x14ac:dyDescent="0.2">
@@ -16080,11 +16086,11 @@
         <v>421</v>
       </c>
       <c r="B31" s="28" t="s">
-        <v>1157</v>
+        <v>1155</v>
       </c>
       <c r="C31" s="27"/>
       <c r="D31" s="18" t="s">
-        <v>1023</v>
+        <v>1021</v>
       </c>
       <c r="E31" s="149"/>
     </row>
@@ -16093,17 +16099,17 @@
         <v>424</v>
       </c>
       <c r="B32" s="28" t="s">
-        <v>1158</v>
+        <v>1156</v>
       </c>
       <c r="C32" s="27"/>
       <c r="D32" s="18" t="s">
-        <v>1016</v>
+        <v>1014</v>
       </c>
       <c r="E32" s="149"/>
     </row>
     <row r="33" spans="1:6" s="13" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A33" s="185" t="s">
-        <v>1159</v>
+        <v>1157</v>
       </c>
       <c r="B33" s="186"/>
       <c r="C33" s="187"/>
@@ -16115,121 +16121,121 @@
         <v>243</v>
       </c>
       <c r="B34" s="150" t="s">
+        <v>1158</v>
+      </c>
+      <c r="C34" s="148" t="s">
+        <v>1159</v>
+      </c>
+      <c r="D34" s="50" t="s">
         <v>1160</v>
       </c>
-      <c r="C34" s="148" t="s">
+      <c r="E34" s="149" t="s">
         <v>1161</v>
-      </c>
-      <c r="D34" s="50" t="s">
-        <v>1162</v>
-      </c>
-      <c r="E34" s="149" t="s">
-        <v>1163</v>
       </c>
       <c r="F34" s="138"/>
     </row>
     <row r="35" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A35" s="147" t="s">
-        <v>1073</v>
+        <v>1071</v>
       </c>
       <c r="B35" s="151" t="s">
+        <v>1162</v>
+      </c>
+      <c r="C35" s="148" t="s">
+        <v>1163</v>
+      </c>
+      <c r="D35" s="152" t="s">
         <v>1164</v>
       </c>
-      <c r="C35" s="148" t="s">
+      <c r="E35" s="149" t="s">
         <v>1165</v>
-      </c>
-      <c r="D35" s="152" t="s">
-        <v>1166</v>
-      </c>
-      <c r="E35" s="149" t="s">
-        <v>1167</v>
       </c>
       <c r="F35" s="138"/>
     </row>
     <row r="36" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A36" s="147" t="s">
-        <v>1073</v>
+        <v>1071</v>
       </c>
       <c r="B36" s="151" t="s">
+        <v>1166</v>
+      </c>
+      <c r="C36" s="148" t="s">
+        <v>1167</v>
+      </c>
+      <c r="D36" s="152" t="s">
+        <v>1164</v>
+      </c>
+      <c r="E36" s="149" t="s">
         <v>1168</v>
-      </c>
-      <c r="C36" s="148" t="s">
-        <v>1169</v>
-      </c>
-      <c r="D36" s="152" t="s">
-        <v>1166</v>
-      </c>
-      <c r="E36" s="149" t="s">
-        <v>1170</v>
       </c>
       <c r="F36" s="138"/>
     </row>
     <row r="37" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A37" s="147" t="s">
-        <v>1073</v>
+        <v>1071</v>
       </c>
       <c r="B37" s="151" t="s">
+        <v>1169</v>
+      </c>
+      <c r="C37" s="49" t="s">
+        <v>1170</v>
+      </c>
+      <c r="D37" s="152" t="s">
+        <v>1164</v>
+      </c>
+      <c r="E37" s="149" t="s">
         <v>1171</v>
-      </c>
-      <c r="C37" s="49" t="s">
-        <v>1172</v>
-      </c>
-      <c r="D37" s="152" t="s">
-        <v>1166</v>
-      </c>
-      <c r="E37" s="149" t="s">
-        <v>1173</v>
       </c>
       <c r="F37" s="138"/>
     </row>
     <row r="38" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A38" s="147" t="s">
-        <v>1073</v>
+        <v>1071</v>
       </c>
       <c r="B38" s="151" t="s">
+        <v>1172</v>
+      </c>
+      <c r="C38" s="49" t="s">
+        <v>1173</v>
+      </c>
+      <c r="D38" s="152" t="s">
+        <v>1164</v>
+      </c>
+      <c r="E38" s="149" t="s">
         <v>1174</v>
-      </c>
-      <c r="C38" s="49" t="s">
-        <v>1175</v>
-      </c>
-      <c r="D38" s="152" t="s">
-        <v>1166</v>
-      </c>
-      <c r="E38" s="149" t="s">
-        <v>1176</v>
       </c>
       <c r="F38" s="138"/>
     </row>
     <row r="39" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A39" s="147" t="s">
-        <v>1073</v>
+        <v>1071</v>
       </c>
       <c r="B39" s="151" t="s">
+        <v>1175</v>
+      </c>
+      <c r="C39" s="49" t="s">
+        <v>1176</v>
+      </c>
+      <c r="D39" s="152" t="s">
+        <v>1164</v>
+      </c>
+      <c r="E39" s="149" t="s">
         <v>1177</v>
-      </c>
-      <c r="C39" s="49" t="s">
-        <v>1178</v>
-      </c>
-      <c r="D39" s="152" t="s">
-        <v>1166</v>
-      </c>
-      <c r="E39" s="149" t="s">
-        <v>1179</v>
       </c>
       <c r="F39" s="138"/>
     </row>
     <row r="40" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A40" s="147" t="s">
-        <v>1073</v>
+        <v>1071</v>
       </c>
       <c r="B40" s="151" t="s">
-        <v>1180</v>
+        <v>1178</v>
       </c>
       <c r="C40" s="49" t="s">
         <v>93</v>
       </c>
       <c r="D40" s="152" t="s">
-        <v>1166</v>
+        <v>1164</v>
       </c>
       <c r="E40" s="149" t="s">
         <v>95</v>
@@ -16241,11 +16247,11 @@
         <v>421</v>
       </c>
       <c r="B41" s="28" t="s">
-        <v>1181</v>
+        <v>1179</v>
       </c>
       <c r="C41" s="51"/>
       <c r="D41" s="18" t="s">
-        <v>1023</v>
+        <v>1021</v>
       </c>
       <c r="E41" s="149"/>
       <c r="F41" s="138"/>
@@ -16255,11 +16261,11 @@
         <v>424</v>
       </c>
       <c r="B42" s="28" t="s">
-        <v>1182</v>
+        <v>1180</v>
       </c>
       <c r="C42" s="27"/>
       <c r="D42" s="18" t="s">
-        <v>1016</v>
+        <v>1014</v>
       </c>
       <c r="E42" s="149"/>
       <c r="F42" s="138"/>
@@ -16269,16 +16275,16 @@
         <v>243</v>
       </c>
       <c r="B43" s="139" t="s">
+        <v>1181</v>
+      </c>
+      <c r="C43" s="62" t="s">
+        <v>1182</v>
+      </c>
+      <c r="D43" s="5" t="s">
         <v>1183</v>
       </c>
-      <c r="C43" s="62" t="s">
+      <c r="E43" s="149" t="s">
         <v>1184</v>
-      </c>
-      <c r="D43" s="5" t="s">
-        <v>1185</v>
-      </c>
-      <c r="E43" s="149" t="s">
-        <v>1186</v>
       </c>
       <c r="F43" s="138"/>
     </row>
@@ -16287,11 +16293,11 @@
         <v>421</v>
       </c>
       <c r="B44" s="28" t="s">
-        <v>1187</v>
+        <v>1185</v>
       </c>
       <c r="C44" s="27"/>
       <c r="D44" s="18" t="s">
-        <v>1023</v>
+        <v>1021</v>
       </c>
       <c r="E44" s="149"/>
       <c r="F44" s="138"/>
@@ -16301,18 +16307,18 @@
         <v>424</v>
       </c>
       <c r="B45" s="28" t="s">
-        <v>1188</v>
+        <v>1186</v>
       </c>
       <c r="C45" s="27"/>
       <c r="D45" s="18" t="s">
-        <v>1016</v>
+        <v>1014</v>
       </c>
       <c r="E45" s="149"/>
       <c r="F45" s="138"/>
     </row>
     <row r="46" spans="1:6" s="13" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="182" t="s">
-        <v>1189</v>
+        <v>1187</v>
       </c>
       <c r="B46" s="183"/>
       <c r="C46" s="183"/>
@@ -16324,33 +16330,33 @@
         <v>243</v>
       </c>
       <c r="B47" s="147" t="s">
+        <v>1188</v>
+      </c>
+      <c r="C47" s="62" t="s">
+        <v>1189</v>
+      </c>
+      <c r="D47" s="119" t="s">
         <v>1190</v>
-      </c>
-      <c r="C47" s="62" t="s">
-        <v>1191</v>
-      </c>
-      <c r="D47" s="119" t="s">
-        <v>1192</v>
       </c>
       <c r="E47" s="63" t="s">
         <v>878</v>
       </c>
       <c r="F47" s="38" t="s">
-        <v>1193</v>
+        <v>1191</v>
       </c>
     </row>
     <row r="48" spans="1:6" s="30" customFormat="1" ht="64" x14ac:dyDescent="0.2">
       <c r="A48" s="147" t="s">
+        <v>1192</v>
+      </c>
+      <c r="B48" s="147" t="s">
+        <v>1193</v>
+      </c>
+      <c r="C48" s="62" t="s">
         <v>1194</v>
       </c>
-      <c r="B48" s="147" t="s">
+      <c r="D48" s="119" t="s">
         <v>1195</v>
-      </c>
-      <c r="C48" s="62" t="s">
-        <v>1196</v>
-      </c>
-      <c r="D48" s="119" t="s">
-        <v>1197</v>
       </c>
       <c r="E48" s="63" t="s">
         <v>943</v>
@@ -16358,19 +16364,19 @@
     </row>
     <row r="49" spans="1:6" s="30" customFormat="1" ht="64" x14ac:dyDescent="0.2">
       <c r="A49" s="147" t="s">
-        <v>1152</v>
+        <v>1150</v>
       </c>
       <c r="B49" s="147" t="s">
-        <v>1198</v>
+        <v>1196</v>
       </c>
       <c r="C49" s="62" t="s">
-        <v>1199</v>
+        <v>1197</v>
       </c>
       <c r="D49" s="119" t="s">
-        <v>1033</v>
+        <v>1031</v>
       </c>
       <c r="E49" s="63" t="s">
-        <v>1034</v>
+        <v>1032</v>
       </c>
     </row>
     <row r="50" spans="1:6" s="30" customFormat="1" ht="48" x14ac:dyDescent="0.2">
@@ -16378,19 +16384,19 @@
         <v>389</v>
       </c>
       <c r="B50" s="139" t="s">
+        <v>1198</v>
+      </c>
+      <c r="C50" s="148" t="s">
+        <v>1199</v>
+      </c>
+      <c r="D50" s="124" t="s">
         <v>1200</v>
       </c>
-      <c r="C50" s="148" t="s">
+      <c r="E50" s="63" t="s">
+        <v>1075</v>
+      </c>
+      <c r="F50" s="74" t="s">
         <v>1201</v>
-      </c>
-      <c r="D50" s="124" t="s">
-        <v>1202</v>
-      </c>
-      <c r="E50" s="63" t="s">
-        <v>1077</v>
-      </c>
-      <c r="F50" s="74" t="s">
-        <v>1203</v>
       </c>
     </row>
     <row r="51" spans="1:6" s="30" customFormat="1" ht="48" x14ac:dyDescent="0.2">
@@ -16398,16 +16404,16 @@
         <v>389</v>
       </c>
       <c r="B51" s="139" t="s">
+        <v>1202</v>
+      </c>
+      <c r="C51" s="148" t="s">
+        <v>1203</v>
+      </c>
+      <c r="D51" s="124" t="s">
         <v>1204</v>
       </c>
-      <c r="C51" s="148" t="s">
+      <c r="E51" s="63" t="s">
         <v>1205</v>
-      </c>
-      <c r="D51" s="124" t="s">
-        <v>1206</v>
-      </c>
-      <c r="E51" s="63" t="s">
-        <v>1207</v>
       </c>
     </row>
     <row r="52" spans="1:6" s="30" customFormat="1" ht="64" x14ac:dyDescent="0.2">
@@ -16415,16 +16421,16 @@
         <v>389</v>
       </c>
       <c r="B52" s="139" t="s">
+        <v>1206</v>
+      </c>
+      <c r="C52" s="148" t="s">
+        <v>1207</v>
+      </c>
+      <c r="D52" s="124" t="s">
         <v>1208</v>
       </c>
-      <c r="C52" s="148" t="s">
+      <c r="E52" s="63" t="s">
         <v>1209</v>
-      </c>
-      <c r="D52" s="124" t="s">
-        <v>1210</v>
-      </c>
-      <c r="E52" s="63" t="s">
-        <v>1211</v>
       </c>
     </row>
     <row r="53" spans="1:6" s="30" customFormat="1" ht="64" x14ac:dyDescent="0.2">
@@ -16432,16 +16438,16 @@
         <v>389</v>
       </c>
       <c r="B53" s="139" t="s">
+        <v>1210</v>
+      </c>
+      <c r="C53" s="148" t="s">
+        <v>1211</v>
+      </c>
+      <c r="D53" s="124" t="s">
         <v>1212</v>
       </c>
-      <c r="C53" s="148" t="s">
+      <c r="E53" s="63" t="s">
         <v>1213</v>
-      </c>
-      <c r="D53" s="124" t="s">
-        <v>1214</v>
-      </c>
-      <c r="E53" s="63" t="s">
-        <v>1215</v>
       </c>
     </row>
     <row r="54" spans="1:6" s="30" customFormat="1" ht="48" x14ac:dyDescent="0.2">
@@ -16449,16 +16455,16 @@
         <v>389</v>
       </c>
       <c r="B54" s="139" t="s">
+        <v>1214</v>
+      </c>
+      <c r="C54" s="148" t="s">
+        <v>1215</v>
+      </c>
+      <c r="D54" s="124" t="s">
         <v>1216</v>
       </c>
-      <c r="C54" s="148" t="s">
+      <c r="E54" s="63" t="s">
         <v>1217</v>
-      </c>
-      <c r="D54" s="124" t="s">
-        <v>1218</v>
-      </c>
-      <c r="E54" s="63" t="s">
-        <v>1219</v>
       </c>
     </row>
     <row r="55" spans="1:6" s="30" customFormat="1" ht="32" x14ac:dyDescent="0.2">
@@ -16466,19 +16472,19 @@
         <v>389</v>
       </c>
       <c r="B55" s="139" t="s">
+        <v>1218</v>
+      </c>
+      <c r="C55" s="148" t="s">
+        <v>1219</v>
+      </c>
+      <c r="D55" s="124" t="s">
         <v>1220</v>
       </c>
-      <c r="C55" s="148" t="s">
+      <c r="E55" s="63" t="s">
+        <v>1102</v>
+      </c>
+      <c r="F55" s="74" t="s">
         <v>1221</v>
-      </c>
-      <c r="D55" s="124" t="s">
-        <v>1222</v>
-      </c>
-      <c r="E55" s="63" t="s">
-        <v>1104</v>
-      </c>
-      <c r="F55" s="74" t="s">
-        <v>1223</v>
       </c>
     </row>
     <row r="56" spans="1:6" s="30" customFormat="1" ht="48" x14ac:dyDescent="0.2">
@@ -16486,19 +16492,19 @@
         <v>389</v>
       </c>
       <c r="B56" s="139" t="s">
+        <v>1222</v>
+      </c>
+      <c r="C56" s="148" t="s">
+        <v>1223</v>
+      </c>
+      <c r="D56" s="124" t="s">
         <v>1224</v>
       </c>
-      <c r="C56" s="148" t="s">
+      <c r="E56" s="63" t="s">
         <v>1225</v>
       </c>
-      <c r="D56" s="124" t="s">
+      <c r="F56" s="74" t="s">
         <v>1226</v>
-      </c>
-      <c r="E56" s="63" t="s">
-        <v>1227</v>
-      </c>
-      <c r="F56" s="74" t="s">
-        <v>1228</v>
       </c>
     </row>
     <row r="57" spans="1:6" s="30" customFormat="1" ht="48" x14ac:dyDescent="0.2">
@@ -16506,19 +16512,19 @@
         <v>389</v>
       </c>
       <c r="B57" s="139" t="s">
+        <v>1227</v>
+      </c>
+      <c r="C57" s="148" t="s">
+        <v>1228</v>
+      </c>
+      <c r="D57" s="124" t="s">
         <v>1229</v>
       </c>
-      <c r="C57" s="148" t="s">
+      <c r="E57" s="63" t="s">
         <v>1230</v>
       </c>
-      <c r="D57" s="124" t="s">
+      <c r="F57" s="74" t="s">
         <v>1231</v>
-      </c>
-      <c r="E57" s="63" t="s">
-        <v>1232</v>
-      </c>
-      <c r="F57" s="74" t="s">
-        <v>1233</v>
       </c>
     </row>
     <row r="58" spans="1:6" s="30" customFormat="1" ht="32" x14ac:dyDescent="0.2">
@@ -16526,19 +16532,19 @@
         <v>389</v>
       </c>
       <c r="B58" s="139" t="s">
+        <v>1232</v>
+      </c>
+      <c r="C58" s="148" t="s">
+        <v>1233</v>
+      </c>
+      <c r="D58" s="124" t="s">
         <v>1234</v>
       </c>
-      <c r="C58" s="148" t="s">
+      <c r="E58" s="63" t="s">
         <v>1235</v>
       </c>
-      <c r="D58" s="124" t="s">
+      <c r="F58" s="74" t="s">
         <v>1236</v>
-      </c>
-      <c r="E58" s="63" t="s">
-        <v>1237</v>
-      </c>
-      <c r="F58" s="74" t="s">
-        <v>1238</v>
       </c>
     </row>
     <row r="59" spans="1:6" s="30" customFormat="1" ht="48" x14ac:dyDescent="0.2">
@@ -16546,16 +16552,16 @@
         <v>389</v>
       </c>
       <c r="B59" s="139" t="s">
+        <v>1237</v>
+      </c>
+      <c r="C59" s="148" t="s">
+        <v>1238</v>
+      </c>
+      <c r="D59" s="124" t="s">
         <v>1239</v>
       </c>
-      <c r="C59" s="148" t="s">
+      <c r="E59" s="63" t="s">
         <v>1240</v>
-      </c>
-      <c r="D59" s="124" t="s">
-        <v>1241</v>
-      </c>
-      <c r="E59" s="63" t="s">
-        <v>1242</v>
       </c>
     </row>
     <row r="60" spans="1:6" s="30" customFormat="1" ht="48" x14ac:dyDescent="0.2">
@@ -16563,16 +16569,16 @@
         <v>389</v>
       </c>
       <c r="B60" s="139" t="s">
+        <v>1241</v>
+      </c>
+      <c r="C60" s="148" t="s">
+        <v>1242</v>
+      </c>
+      <c r="D60" s="124" t="s">
         <v>1243</v>
       </c>
-      <c r="C60" s="148" t="s">
+      <c r="E60" s="63" t="s">
         <v>1244</v>
-      </c>
-      <c r="D60" s="124" t="s">
-        <v>1245</v>
-      </c>
-      <c r="E60" s="63" t="s">
-        <v>1246</v>
       </c>
     </row>
     <row r="61" spans="1:6" s="30" customFormat="1" ht="48" x14ac:dyDescent="0.2">
@@ -16580,16 +16586,16 @@
         <v>389</v>
       </c>
       <c r="B61" s="18" t="s">
+        <v>1245</v>
+      </c>
+      <c r="C61" s="148" t="s">
+        <v>1246</v>
+      </c>
+      <c r="D61" s="124" t="s">
         <v>1247</v>
       </c>
-      <c r="C61" s="148" t="s">
+      <c r="E61" s="63" t="s">
         <v>1248</v>
-      </c>
-      <c r="D61" s="124" t="s">
-        <v>1249</v>
-      </c>
-      <c r="E61" s="63" t="s">
-        <v>1250</v>
       </c>
     </row>
     <row r="62" spans="1:6" s="30" customFormat="1" ht="48" x14ac:dyDescent="0.2">
@@ -16597,16 +16603,16 @@
         <v>389</v>
       </c>
       <c r="B62" s="139" t="s">
+        <v>1249</v>
+      </c>
+      <c r="C62" s="148" t="s">
+        <v>1250</v>
+      </c>
+      <c r="D62" s="124" t="s">
         <v>1251</v>
       </c>
-      <c r="C62" s="148" t="s">
+      <c r="E62" s="80" t="s">
         <v>1252</v>
-      </c>
-      <c r="D62" s="124" t="s">
-        <v>1253</v>
-      </c>
-      <c r="E62" s="80" t="s">
-        <v>1254</v>
       </c>
     </row>
     <row r="63" spans="1:6" ht="16" x14ac:dyDescent="0.2">
@@ -16614,14 +16620,14 @@
         <v>745</v>
       </c>
       <c r="B63" s="147" t="s">
-        <v>1255</v>
+        <v>1253</v>
       </c>
       <c r="C63" s="148" t="s">
-        <v>1256</v>
+        <v>1254</v>
       </c>
       <c r="D63" s="151"/>
       <c r="E63" s="79" t="s">
-        <v>1257</v>
+        <v>1255</v>
       </c>
       <c r="F63" s="138"/>
     </row>
@@ -16630,14 +16636,14 @@
         <v>745</v>
       </c>
       <c r="B64" s="147" t="s">
-        <v>1258</v>
+        <v>1256</v>
       </c>
       <c r="C64" s="148" t="s">
-        <v>1178</v>
+        <v>1176</v>
       </c>
       <c r="D64" s="151"/>
       <c r="E64" s="79" t="s">
-        <v>1179</v>
+        <v>1177</v>
       </c>
       <c r="F64" s="138"/>
     </row>
@@ -16646,14 +16652,14 @@
         <v>745</v>
       </c>
       <c r="B65" s="139" t="s">
-        <v>1259</v>
+        <v>1257</v>
       </c>
       <c r="C65" s="148" t="s">
-        <v>1165</v>
+        <v>1163</v>
       </c>
       <c r="D65" s="151"/>
       <c r="E65" s="79" t="s">
-        <v>1167</v>
+        <v>1165</v>
       </c>
       <c r="F65" s="138"/>
     </row>
@@ -16768,16 +16774,16 @@
         <v>243</v>
       </c>
       <c r="B2" s="5" t="s">
+        <v>1258</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>1259</v>
+      </c>
+      <c r="D2" s="5" t="s">
         <v>1260</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="F2" s="68" t="s">
         <v>1261</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>1262</v>
-      </c>
-      <c r="F2" s="68" t="s">
-        <v>1263</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="32" x14ac:dyDescent="0.2">
@@ -16785,13 +16791,13 @@
         <v>254</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>1264</v>
+        <v>1262</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>930</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>1265</v>
+        <v>1263</v>
       </c>
       <c r="E3" s="37" t="s">
         <v>931</v>
@@ -16802,13 +16808,13 @@
         <v>32</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>1266</v>
+        <v>1264</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>881</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>1267</v>
+        <v>1265</v>
       </c>
       <c r="E4" s="37" t="s">
         <v>883</v>
@@ -16816,36 +16822,36 @@
     </row>
     <row r="5" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
-        <v>1268</v>
+        <v>1266</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>1269</v>
+        <v>1267</v>
       </c>
       <c r="C5" s="6" t="s">
         <v>152</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>1270</v>
+        <v>1268</v>
       </c>
       <c r="F5" s="68" t="s">
-        <v>1263</v>
+        <v>1261</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
-        <v>1268</v>
+        <v>1266</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>1271</v>
+        <v>1269</v>
       </c>
       <c r="C6" s="6" t="s">
         <v>140</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>1270</v>
+        <v>1268</v>
       </c>
       <c r="F6" s="68" t="s">
-        <v>1263</v>
+        <v>1261</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="32" x14ac:dyDescent="0.2">
@@ -16853,13 +16859,13 @@
         <v>254</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>1272</v>
+        <v>1270</v>
       </c>
       <c r="C7" s="6" t="s">
         <v>933</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>1265</v>
+        <v>1263</v>
       </c>
       <c r="E7" s="37" t="s">
         <v>934</v>
@@ -16870,7 +16876,7 @@
         <v>32</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>1273</v>
+        <v>1271</v>
       </c>
       <c r="C8" s="6" t="s">
         <v>936</v>
@@ -16882,10 +16888,10 @@
     </row>
     <row r="9" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
-        <v>1268</v>
+        <v>1266</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>1274</v>
+        <v>1272</v>
       </c>
       <c r="C9" s="6" t="s">
         <v>942</v>
@@ -16897,22 +16903,22 @@
     </row>
     <row r="10" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="C10" s="27" t="s">
+        <v>1273</v>
+      </c>
+      <c r="D10" s="18" t="s">
+        <v>1274</v>
+      </c>
+      <c r="E10" s="37" t="s">
         <v>1275</v>
-      </c>
-      <c r="D10" s="18" t="s">
-        <v>1276</v>
-      </c>
-      <c r="E10" s="37" t="s">
-        <v>1277</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="C11" s="75" t="s">
-        <v>1278</v>
+        <v>1276</v>
       </c>
       <c r="D11" s="18"/>
       <c r="E11" s="37" t="s">
-        <v>1279</v>
+        <v>1277</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
@@ -16945,15 +16951,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <Readyforteam_x003f_ xmlns="565e1b1d-057e-4d85-b896-01a5881d8a45">false</Readyforteam_x003f_>
@@ -16992,6 +16989,15 @@
     <TaxCatchAll xmlns="2799d30d-6731-4efe-ac9b-c4895a8828d9" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -17272,14 +17278,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8D7CE8C7-18DC-484F-8376-ED09F13D44C8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{017ACE96-8143-486E-8436-7787F6B96F4A}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -17288,6 +17286,14 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
     <ds:schemaRef ds:uri="bf601f31-63a1-4825-9216-91d773c5ef9c"/>
     <ds:schemaRef ds:uri="2799d30d-6731-4efe-ac9b-c4895a8828d9"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8D7CE8C7-18DC-484F-8376-ED09F13D44C8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Updating the v11bi address screens with select boxes.
</commit_message>
<xml_diff>
--- a/app/data/MCCD-localisation.xlsx
+++ b/app/data/MCCD-localisation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/JALAT/GIT/medical-certificate-of-cause-of-death/app/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB276E68-948D-1F48-A916-DDB231A499F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88B99C47-98E5-7D45-872F-FE02B3190973}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="14220" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -68,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2078" uniqueCount="1396">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2084" uniqueCount="1400">
   <si>
     <r>
       <rPr>
@@ -5755,7 +5755,19 @@
     <t>Hysbyswyd y crwner am y farwolaeth hon ac nid oedd ei ddyletswydd i ymchwilio o dan adran 1 o Ddeddf Crwneriaid a Chyfiawnder 2009 yn gymwys</t>
   </si>
   <si>
-    <t>009</t>
+    <t>globalSelectDifferentAddress</t>
+  </si>
+  <si>
+    <t>Select a different address</t>
+  </si>
+  <si>
+    <t>globalEnterAddressManually</t>
+  </si>
+  <si>
+    <t>Dewiswch gyfeiriad gwahanol</t>
+  </si>
+  <si>
+    <t>010</t>
   </si>
 </sst>
 </file>
@@ -6678,6 +6690,12 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -6690,6 +6708,15 @@
     <xf numFmtId="0" fontId="13" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -6708,15 +6735,6 @@
     <xf numFmtId="0" fontId="13" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
@@ -6788,12 +6806,6 @@
     </xf>
     <xf numFmtId="0" fontId="13" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -7178,538 +7190,538 @@
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A1" s="154" t="s">
+      <c r="A1" s="156" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="154"/>
-      <c r="C1" s="154"/>
-      <c r="D1" s="154"/>
-      <c r="E1" s="154"/>
-      <c r="F1" s="154"/>
-      <c r="G1" s="154"/>
-      <c r="H1" s="154"/>
-      <c r="I1" s="154"/>
-      <c r="J1" s="154"/>
-      <c r="K1" s="154"/>
-      <c r="L1" s="154"/>
+      <c r="B1" s="156"/>
+      <c r="C1" s="156"/>
+      <c r="D1" s="156"/>
+      <c r="E1" s="156"/>
+      <c r="F1" s="156"/>
+      <c r="G1" s="156"/>
+      <c r="H1" s="156"/>
+      <c r="I1" s="156"/>
+      <c r="J1" s="156"/>
+      <c r="K1" s="156"/>
+      <c r="L1" s="156"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A2" s="154"/>
-      <c r="B2" s="154"/>
-      <c r="C2" s="154"/>
-      <c r="D2" s="154"/>
-      <c r="E2" s="154"/>
-      <c r="F2" s="154"/>
-      <c r="G2" s="154"/>
-      <c r="H2" s="154"/>
-      <c r="I2" s="154"/>
-      <c r="J2" s="154"/>
-      <c r="K2" s="154"/>
-      <c r="L2" s="154"/>
+      <c r="A2" s="156"/>
+      <c r="B2" s="156"/>
+      <c r="C2" s="156"/>
+      <c r="D2" s="156"/>
+      <c r="E2" s="156"/>
+      <c r="F2" s="156"/>
+      <c r="G2" s="156"/>
+      <c r="H2" s="156"/>
+      <c r="I2" s="156"/>
+      <c r="J2" s="156"/>
+      <c r="K2" s="156"/>
+      <c r="L2" s="156"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A3" s="154"/>
-      <c r="B3" s="154"/>
-      <c r="C3" s="154"/>
-      <c r="D3" s="154"/>
-      <c r="E3" s="154"/>
-      <c r="F3" s="154"/>
-      <c r="G3" s="154"/>
-      <c r="H3" s="154"/>
-      <c r="I3" s="154"/>
-      <c r="J3" s="154"/>
-      <c r="K3" s="154"/>
-      <c r="L3" s="154"/>
+      <c r="A3" s="156"/>
+      <c r="B3" s="156"/>
+      <c r="C3" s="156"/>
+      <c r="D3" s="156"/>
+      <c r="E3" s="156"/>
+      <c r="F3" s="156"/>
+      <c r="G3" s="156"/>
+      <c r="H3" s="156"/>
+      <c r="I3" s="156"/>
+      <c r="J3" s="156"/>
+      <c r="K3" s="156"/>
+      <c r="L3" s="156"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A4" s="154"/>
-      <c r="B4" s="154"/>
-      <c r="C4" s="154"/>
-      <c r="D4" s="154"/>
-      <c r="E4" s="154"/>
-      <c r="F4" s="154"/>
-      <c r="G4" s="154"/>
-      <c r="H4" s="154"/>
-      <c r="I4" s="154"/>
-      <c r="J4" s="154"/>
-      <c r="K4" s="154"/>
-      <c r="L4" s="154"/>
+      <c r="A4" s="156"/>
+      <c r="B4" s="156"/>
+      <c r="C4" s="156"/>
+      <c r="D4" s="156"/>
+      <c r="E4" s="156"/>
+      <c r="F4" s="156"/>
+      <c r="G4" s="156"/>
+      <c r="H4" s="156"/>
+      <c r="I4" s="156"/>
+      <c r="J4" s="156"/>
+      <c r="K4" s="156"/>
+      <c r="L4" s="156"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A5" s="154"/>
-      <c r="B5" s="154"/>
-      <c r="C5" s="154"/>
-      <c r="D5" s="154"/>
-      <c r="E5" s="154"/>
-      <c r="F5" s="154"/>
-      <c r="G5" s="154"/>
-      <c r="H5" s="154"/>
-      <c r="I5" s="154"/>
-      <c r="J5" s="154"/>
-      <c r="K5" s="154"/>
-      <c r="L5" s="154"/>
+      <c r="A5" s="156"/>
+      <c r="B5" s="156"/>
+      <c r="C5" s="156"/>
+      <c r="D5" s="156"/>
+      <c r="E5" s="156"/>
+      <c r="F5" s="156"/>
+      <c r="G5" s="156"/>
+      <c r="H5" s="156"/>
+      <c r="I5" s="156"/>
+      <c r="J5" s="156"/>
+      <c r="K5" s="156"/>
+      <c r="L5" s="156"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A6" s="154"/>
-      <c r="B6" s="154"/>
-      <c r="C6" s="154"/>
-      <c r="D6" s="154"/>
-      <c r="E6" s="154"/>
-      <c r="F6" s="154"/>
-      <c r="G6" s="154"/>
-      <c r="H6" s="154"/>
-      <c r="I6" s="154"/>
-      <c r="J6" s="154"/>
-      <c r="K6" s="154"/>
-      <c r="L6" s="154"/>
+      <c r="A6" s="156"/>
+      <c r="B6" s="156"/>
+      <c r="C6" s="156"/>
+      <c r="D6" s="156"/>
+      <c r="E6" s="156"/>
+      <c r="F6" s="156"/>
+      <c r="G6" s="156"/>
+      <c r="H6" s="156"/>
+      <c r="I6" s="156"/>
+      <c r="J6" s="156"/>
+      <c r="K6" s="156"/>
+      <c r="L6" s="156"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A7" s="154"/>
-      <c r="B7" s="154"/>
-      <c r="C7" s="154"/>
-      <c r="D7" s="154"/>
-      <c r="E7" s="154"/>
-      <c r="F7" s="154"/>
-      <c r="G7" s="154"/>
-      <c r="H7" s="154"/>
-      <c r="I7" s="154"/>
-      <c r="J7" s="154"/>
-      <c r="K7" s="154"/>
-      <c r="L7" s="154"/>
+      <c r="A7" s="156"/>
+      <c r="B7" s="156"/>
+      <c r="C7" s="156"/>
+      <c r="D7" s="156"/>
+      <c r="E7" s="156"/>
+      <c r="F7" s="156"/>
+      <c r="G7" s="156"/>
+      <c r="H7" s="156"/>
+      <c r="I7" s="156"/>
+      <c r="J7" s="156"/>
+      <c r="K7" s="156"/>
+      <c r="L7" s="156"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A8" s="154"/>
-      <c r="B8" s="154"/>
-      <c r="C8" s="154"/>
-      <c r="D8" s="154"/>
-      <c r="E8" s="154"/>
-      <c r="F8" s="154"/>
-      <c r="G8" s="154"/>
-      <c r="H8" s="154"/>
-      <c r="I8" s="154"/>
-      <c r="J8" s="154"/>
-      <c r="K8" s="154"/>
-      <c r="L8" s="154"/>
+      <c r="A8" s="156"/>
+      <c r="B8" s="156"/>
+      <c r="C8" s="156"/>
+      <c r="D8" s="156"/>
+      <c r="E8" s="156"/>
+      <c r="F8" s="156"/>
+      <c r="G8" s="156"/>
+      <c r="H8" s="156"/>
+      <c r="I8" s="156"/>
+      <c r="J8" s="156"/>
+      <c r="K8" s="156"/>
+      <c r="L8" s="156"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A9" s="154"/>
-      <c r="B9" s="154"/>
-      <c r="C9" s="154"/>
-      <c r="D9" s="154"/>
-      <c r="E9" s="154"/>
-      <c r="F9" s="154"/>
-      <c r="G9" s="154"/>
-      <c r="H9" s="154"/>
-      <c r="I9" s="154"/>
-      <c r="J9" s="154"/>
-      <c r="K9" s="154"/>
-      <c r="L9" s="154"/>
+      <c r="A9" s="156"/>
+      <c r="B9" s="156"/>
+      <c r="C9" s="156"/>
+      <c r="D9" s="156"/>
+      <c r="E9" s="156"/>
+      <c r="F9" s="156"/>
+      <c r="G9" s="156"/>
+      <c r="H9" s="156"/>
+      <c r="I9" s="156"/>
+      <c r="J9" s="156"/>
+      <c r="K9" s="156"/>
+      <c r="L9" s="156"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A10" s="154"/>
-      <c r="B10" s="154"/>
-      <c r="C10" s="154"/>
-      <c r="D10" s="154"/>
-      <c r="E10" s="154"/>
-      <c r="F10" s="154"/>
-      <c r="G10" s="154"/>
-      <c r="H10" s="154"/>
-      <c r="I10" s="154"/>
-      <c r="J10" s="154"/>
-      <c r="K10" s="154"/>
-      <c r="L10" s="154"/>
+      <c r="A10" s="156"/>
+      <c r="B10" s="156"/>
+      <c r="C10" s="156"/>
+      <c r="D10" s="156"/>
+      <c r="E10" s="156"/>
+      <c r="F10" s="156"/>
+      <c r="G10" s="156"/>
+      <c r="H10" s="156"/>
+      <c r="I10" s="156"/>
+      <c r="J10" s="156"/>
+      <c r="K10" s="156"/>
+      <c r="L10" s="156"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A11" s="154"/>
-      <c r="B11" s="154"/>
-      <c r="C11" s="154"/>
-      <c r="D11" s="154"/>
-      <c r="E11" s="154"/>
-      <c r="F11" s="154"/>
-      <c r="G11" s="154"/>
-      <c r="H11" s="154"/>
-      <c r="I11" s="154"/>
-      <c r="J11" s="154"/>
-      <c r="K11" s="154"/>
-      <c r="L11" s="154"/>
+      <c r="A11" s="156"/>
+      <c r="B11" s="156"/>
+      <c r="C11" s="156"/>
+      <c r="D11" s="156"/>
+      <c r="E11" s="156"/>
+      <c r="F11" s="156"/>
+      <c r="G11" s="156"/>
+      <c r="H11" s="156"/>
+      <c r="I11" s="156"/>
+      <c r="J11" s="156"/>
+      <c r="K11" s="156"/>
+      <c r="L11" s="156"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A12" s="154"/>
-      <c r="B12" s="154"/>
-      <c r="C12" s="154"/>
-      <c r="D12" s="154"/>
-      <c r="E12" s="154"/>
-      <c r="F12" s="154"/>
-      <c r="G12" s="154"/>
-      <c r="H12" s="154"/>
-      <c r="I12" s="154"/>
-      <c r="J12" s="154"/>
-      <c r="K12" s="154"/>
-      <c r="L12" s="154"/>
+      <c r="A12" s="156"/>
+      <c r="B12" s="156"/>
+      <c r="C12" s="156"/>
+      <c r="D12" s="156"/>
+      <c r="E12" s="156"/>
+      <c r="F12" s="156"/>
+      <c r="G12" s="156"/>
+      <c r="H12" s="156"/>
+      <c r="I12" s="156"/>
+      <c r="J12" s="156"/>
+      <c r="K12" s="156"/>
+      <c r="L12" s="156"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A13" s="154"/>
-      <c r="B13" s="154"/>
-      <c r="C13" s="154"/>
-      <c r="D13" s="154"/>
-      <c r="E13" s="154"/>
-      <c r="F13" s="154"/>
-      <c r="G13" s="154"/>
-      <c r="H13" s="154"/>
-      <c r="I13" s="154"/>
-      <c r="J13" s="154"/>
-      <c r="K13" s="154"/>
-      <c r="L13" s="154"/>
+      <c r="A13" s="156"/>
+      <c r="B13" s="156"/>
+      <c r="C13" s="156"/>
+      <c r="D13" s="156"/>
+      <c r="E13" s="156"/>
+      <c r="F13" s="156"/>
+      <c r="G13" s="156"/>
+      <c r="H13" s="156"/>
+      <c r="I13" s="156"/>
+      <c r="J13" s="156"/>
+      <c r="K13" s="156"/>
+      <c r="L13" s="156"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A14" s="154"/>
-      <c r="B14" s="154"/>
-      <c r="C14" s="154"/>
-      <c r="D14" s="154"/>
-      <c r="E14" s="154"/>
-      <c r="F14" s="154"/>
-      <c r="G14" s="154"/>
-      <c r="H14" s="154"/>
-      <c r="I14" s="154"/>
-      <c r="J14" s="154"/>
-      <c r="K14" s="154"/>
-      <c r="L14" s="154"/>
+      <c r="A14" s="156"/>
+      <c r="B14" s="156"/>
+      <c r="C14" s="156"/>
+      <c r="D14" s="156"/>
+      <c r="E14" s="156"/>
+      <c r="F14" s="156"/>
+      <c r="G14" s="156"/>
+      <c r="H14" s="156"/>
+      <c r="I14" s="156"/>
+      <c r="J14" s="156"/>
+      <c r="K14" s="156"/>
+      <c r="L14" s="156"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A15" s="154"/>
-      <c r="B15" s="154"/>
-      <c r="C15" s="154"/>
-      <c r="D15" s="154"/>
-      <c r="E15" s="154"/>
-      <c r="F15" s="154"/>
-      <c r="G15" s="154"/>
-      <c r="H15" s="154"/>
-      <c r="I15" s="154"/>
-      <c r="J15" s="154"/>
-      <c r="K15" s="154"/>
-      <c r="L15" s="154"/>
+      <c r="A15" s="156"/>
+      <c r="B15" s="156"/>
+      <c r="C15" s="156"/>
+      <c r="D15" s="156"/>
+      <c r="E15" s="156"/>
+      <c r="F15" s="156"/>
+      <c r="G15" s="156"/>
+      <c r="H15" s="156"/>
+      <c r="I15" s="156"/>
+      <c r="J15" s="156"/>
+      <c r="K15" s="156"/>
+      <c r="L15" s="156"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A16" s="154"/>
-      <c r="B16" s="154"/>
-      <c r="C16" s="154"/>
-      <c r="D16" s="154"/>
-      <c r="E16" s="154"/>
-      <c r="F16" s="154"/>
-      <c r="G16" s="154"/>
-      <c r="H16" s="154"/>
-      <c r="I16" s="154"/>
-      <c r="J16" s="154"/>
-      <c r="K16" s="154"/>
-      <c r="L16" s="154"/>
+      <c r="A16" s="156"/>
+      <c r="B16" s="156"/>
+      <c r="C16" s="156"/>
+      <c r="D16" s="156"/>
+      <c r="E16" s="156"/>
+      <c r="F16" s="156"/>
+      <c r="G16" s="156"/>
+      <c r="H16" s="156"/>
+      <c r="I16" s="156"/>
+      <c r="J16" s="156"/>
+      <c r="K16" s="156"/>
+      <c r="L16" s="156"/>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A17" s="154"/>
-      <c r="B17" s="154"/>
-      <c r="C17" s="154"/>
-      <c r="D17" s="154"/>
-      <c r="E17" s="154"/>
-      <c r="F17" s="154"/>
-      <c r="G17" s="154"/>
-      <c r="H17" s="154"/>
-      <c r="I17" s="154"/>
-      <c r="J17" s="154"/>
-      <c r="K17" s="154"/>
-      <c r="L17" s="154"/>
+      <c r="A17" s="156"/>
+      <c r="B17" s="156"/>
+      <c r="C17" s="156"/>
+      <c r="D17" s="156"/>
+      <c r="E17" s="156"/>
+      <c r="F17" s="156"/>
+      <c r="G17" s="156"/>
+      <c r="H17" s="156"/>
+      <c r="I17" s="156"/>
+      <c r="J17" s="156"/>
+      <c r="K17" s="156"/>
+      <c r="L17" s="156"/>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A18" s="154"/>
-      <c r="B18" s="154"/>
-      <c r="C18" s="154"/>
-      <c r="D18" s="154"/>
-      <c r="E18" s="154"/>
-      <c r="F18" s="154"/>
-      <c r="G18" s="154"/>
-      <c r="H18" s="154"/>
-      <c r="I18" s="154"/>
-      <c r="J18" s="154"/>
-      <c r="K18" s="154"/>
-      <c r="L18" s="154"/>
+      <c r="A18" s="156"/>
+      <c r="B18" s="156"/>
+      <c r="C18" s="156"/>
+      <c r="D18" s="156"/>
+      <c r="E18" s="156"/>
+      <c r="F18" s="156"/>
+      <c r="G18" s="156"/>
+      <c r="H18" s="156"/>
+      <c r="I18" s="156"/>
+      <c r="J18" s="156"/>
+      <c r="K18" s="156"/>
+      <c r="L18" s="156"/>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A19" s="154"/>
-      <c r="B19" s="154"/>
-      <c r="C19" s="154"/>
-      <c r="D19" s="154"/>
-      <c r="E19" s="154"/>
-      <c r="F19" s="154"/>
-      <c r="G19" s="154"/>
-      <c r="H19" s="154"/>
-      <c r="I19" s="154"/>
-      <c r="J19" s="154"/>
-      <c r="K19" s="154"/>
-      <c r="L19" s="154"/>
+      <c r="A19" s="156"/>
+      <c r="B19" s="156"/>
+      <c r="C19" s="156"/>
+      <c r="D19" s="156"/>
+      <c r="E19" s="156"/>
+      <c r="F19" s="156"/>
+      <c r="G19" s="156"/>
+      <c r="H19" s="156"/>
+      <c r="I19" s="156"/>
+      <c r="J19" s="156"/>
+      <c r="K19" s="156"/>
+      <c r="L19" s="156"/>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A20" s="154"/>
-      <c r="B20" s="154"/>
-      <c r="C20" s="154"/>
-      <c r="D20" s="154"/>
-      <c r="E20" s="154"/>
-      <c r="F20" s="154"/>
-      <c r="G20" s="154"/>
-      <c r="H20" s="154"/>
-      <c r="I20" s="154"/>
-      <c r="J20" s="154"/>
-      <c r="K20" s="154"/>
-      <c r="L20" s="154"/>
+      <c r="A20" s="156"/>
+      <c r="B20" s="156"/>
+      <c r="C20" s="156"/>
+      <c r="D20" s="156"/>
+      <c r="E20" s="156"/>
+      <c r="F20" s="156"/>
+      <c r="G20" s="156"/>
+      <c r="H20" s="156"/>
+      <c r="I20" s="156"/>
+      <c r="J20" s="156"/>
+      <c r="K20" s="156"/>
+      <c r="L20" s="156"/>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A21" s="154"/>
-      <c r="B21" s="154"/>
-      <c r="C21" s="154"/>
-      <c r="D21" s="154"/>
-      <c r="E21" s="154"/>
-      <c r="F21" s="154"/>
-      <c r="G21" s="154"/>
-      <c r="H21" s="154"/>
-      <c r="I21" s="154"/>
-      <c r="J21" s="154"/>
-      <c r="K21" s="154"/>
-      <c r="L21" s="154"/>
+      <c r="A21" s="156"/>
+      <c r="B21" s="156"/>
+      <c r="C21" s="156"/>
+      <c r="D21" s="156"/>
+      <c r="E21" s="156"/>
+      <c r="F21" s="156"/>
+      <c r="G21" s="156"/>
+      <c r="H21" s="156"/>
+      <c r="I21" s="156"/>
+      <c r="J21" s="156"/>
+      <c r="K21" s="156"/>
+      <c r="L21" s="156"/>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A22" s="154"/>
-      <c r="B22" s="154"/>
-      <c r="C22" s="154"/>
-      <c r="D22" s="154"/>
-      <c r="E22" s="154"/>
-      <c r="F22" s="154"/>
-      <c r="G22" s="154"/>
-      <c r="H22" s="154"/>
-      <c r="I22" s="154"/>
-      <c r="J22" s="154"/>
-      <c r="K22" s="154"/>
-      <c r="L22" s="154"/>
+      <c r="A22" s="156"/>
+      <c r="B22" s="156"/>
+      <c r="C22" s="156"/>
+      <c r="D22" s="156"/>
+      <c r="E22" s="156"/>
+      <c r="F22" s="156"/>
+      <c r="G22" s="156"/>
+      <c r="H22" s="156"/>
+      <c r="I22" s="156"/>
+      <c r="J22" s="156"/>
+      <c r="K22" s="156"/>
+      <c r="L22" s="156"/>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A23" s="154"/>
-      <c r="B23" s="154"/>
-      <c r="C23" s="154"/>
-      <c r="D23" s="154"/>
-      <c r="E23" s="154"/>
-      <c r="F23" s="154"/>
-      <c r="G23" s="154"/>
-      <c r="H23" s="154"/>
-      <c r="I23" s="154"/>
-      <c r="J23" s="154"/>
-      <c r="K23" s="154"/>
-      <c r="L23" s="154"/>
+      <c r="A23" s="156"/>
+      <c r="B23" s="156"/>
+      <c r="C23" s="156"/>
+      <c r="D23" s="156"/>
+      <c r="E23" s="156"/>
+      <c r="F23" s="156"/>
+      <c r="G23" s="156"/>
+      <c r="H23" s="156"/>
+      <c r="I23" s="156"/>
+      <c r="J23" s="156"/>
+      <c r="K23" s="156"/>
+      <c r="L23" s="156"/>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A24" s="154"/>
-      <c r="B24" s="154"/>
-      <c r="C24" s="154"/>
-      <c r="D24" s="154"/>
-      <c r="E24" s="154"/>
-      <c r="F24" s="154"/>
-      <c r="G24" s="154"/>
-      <c r="H24" s="154"/>
-      <c r="I24" s="154"/>
-      <c r="J24" s="154"/>
-      <c r="K24" s="154"/>
-      <c r="L24" s="154"/>
+      <c r="A24" s="156"/>
+      <c r="B24" s="156"/>
+      <c r="C24" s="156"/>
+      <c r="D24" s="156"/>
+      <c r="E24" s="156"/>
+      <c r="F24" s="156"/>
+      <c r="G24" s="156"/>
+      <c r="H24" s="156"/>
+      <c r="I24" s="156"/>
+      <c r="J24" s="156"/>
+      <c r="K24" s="156"/>
+      <c r="L24" s="156"/>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A25" s="154"/>
-      <c r="B25" s="154"/>
-      <c r="C25" s="154"/>
-      <c r="D25" s="154"/>
-      <c r="E25" s="154"/>
-      <c r="F25" s="154"/>
-      <c r="G25" s="154"/>
-      <c r="H25" s="154"/>
-      <c r="I25" s="154"/>
-      <c r="J25" s="154"/>
-      <c r="K25" s="154"/>
-      <c r="L25" s="154"/>
+      <c r="A25" s="156"/>
+      <c r="B25" s="156"/>
+      <c r="C25" s="156"/>
+      <c r="D25" s="156"/>
+      <c r="E25" s="156"/>
+      <c r="F25" s="156"/>
+      <c r="G25" s="156"/>
+      <c r="H25" s="156"/>
+      <c r="I25" s="156"/>
+      <c r="J25" s="156"/>
+      <c r="K25" s="156"/>
+      <c r="L25" s="156"/>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A26" s="154"/>
-      <c r="B26" s="154"/>
-      <c r="C26" s="154"/>
-      <c r="D26" s="154"/>
-      <c r="E26" s="154"/>
-      <c r="F26" s="154"/>
-      <c r="G26" s="154"/>
-      <c r="H26" s="154"/>
-      <c r="I26" s="154"/>
-      <c r="J26" s="154"/>
-      <c r="K26" s="154"/>
-      <c r="L26" s="154"/>
+      <c r="A26" s="156"/>
+      <c r="B26" s="156"/>
+      <c r="C26" s="156"/>
+      <c r="D26" s="156"/>
+      <c r="E26" s="156"/>
+      <c r="F26" s="156"/>
+      <c r="G26" s="156"/>
+      <c r="H26" s="156"/>
+      <c r="I26" s="156"/>
+      <c r="J26" s="156"/>
+      <c r="K26" s="156"/>
+      <c r="L26" s="156"/>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A27" s="154"/>
-      <c r="B27" s="154"/>
-      <c r="C27" s="154"/>
-      <c r="D27" s="154"/>
-      <c r="E27" s="154"/>
-      <c r="F27" s="154"/>
-      <c r="G27" s="154"/>
-      <c r="H27" s="154"/>
-      <c r="I27" s="154"/>
-      <c r="J27" s="154"/>
-      <c r="K27" s="154"/>
-      <c r="L27" s="154"/>
+      <c r="A27" s="156"/>
+      <c r="B27" s="156"/>
+      <c r="C27" s="156"/>
+      <c r="D27" s="156"/>
+      <c r="E27" s="156"/>
+      <c r="F27" s="156"/>
+      <c r="G27" s="156"/>
+      <c r="H27" s="156"/>
+      <c r="I27" s="156"/>
+      <c r="J27" s="156"/>
+      <c r="K27" s="156"/>
+      <c r="L27" s="156"/>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A28" s="154"/>
-      <c r="B28" s="154"/>
-      <c r="C28" s="154"/>
-      <c r="D28" s="154"/>
-      <c r="E28" s="154"/>
-      <c r="F28" s="154"/>
-      <c r="G28" s="154"/>
-      <c r="H28" s="154"/>
-      <c r="I28" s="154"/>
-      <c r="J28" s="154"/>
-      <c r="K28" s="154"/>
-      <c r="L28" s="154"/>
+      <c r="A28" s="156"/>
+      <c r="B28" s="156"/>
+      <c r="C28" s="156"/>
+      <c r="D28" s="156"/>
+      <c r="E28" s="156"/>
+      <c r="F28" s="156"/>
+      <c r="G28" s="156"/>
+      <c r="H28" s="156"/>
+      <c r="I28" s="156"/>
+      <c r="J28" s="156"/>
+      <c r="K28" s="156"/>
+      <c r="L28" s="156"/>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A29" s="154"/>
-      <c r="B29" s="154"/>
-      <c r="C29" s="154"/>
-      <c r="D29" s="154"/>
-      <c r="E29" s="154"/>
-      <c r="F29" s="154"/>
-      <c r="G29" s="154"/>
-      <c r="H29" s="154"/>
-      <c r="I29" s="154"/>
-      <c r="J29" s="154"/>
-      <c r="K29" s="154"/>
-      <c r="L29" s="154"/>
+      <c r="A29" s="156"/>
+      <c r="B29" s="156"/>
+      <c r="C29" s="156"/>
+      <c r="D29" s="156"/>
+      <c r="E29" s="156"/>
+      <c r="F29" s="156"/>
+      <c r="G29" s="156"/>
+      <c r="H29" s="156"/>
+      <c r="I29" s="156"/>
+      <c r="J29" s="156"/>
+      <c r="K29" s="156"/>
+      <c r="L29" s="156"/>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A30" s="154"/>
-      <c r="B30" s="154"/>
-      <c r="C30" s="154"/>
-      <c r="D30" s="154"/>
-      <c r="E30" s="154"/>
-      <c r="F30" s="154"/>
-      <c r="G30" s="154"/>
-      <c r="H30" s="154"/>
-      <c r="I30" s="154"/>
-      <c r="J30" s="154"/>
-      <c r="K30" s="154"/>
-      <c r="L30" s="154"/>
+      <c r="A30" s="156"/>
+      <c r="B30" s="156"/>
+      <c r="C30" s="156"/>
+      <c r="D30" s="156"/>
+      <c r="E30" s="156"/>
+      <c r="F30" s="156"/>
+      <c r="G30" s="156"/>
+      <c r="H30" s="156"/>
+      <c r="I30" s="156"/>
+      <c r="J30" s="156"/>
+      <c r="K30" s="156"/>
+      <c r="L30" s="156"/>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A31" s="154"/>
-      <c r="B31" s="154"/>
-      <c r="C31" s="154"/>
-      <c r="D31" s="154"/>
-      <c r="E31" s="154"/>
-      <c r="F31" s="154"/>
-      <c r="G31" s="154"/>
-      <c r="H31" s="154"/>
-      <c r="I31" s="154"/>
-      <c r="J31" s="154"/>
-      <c r="K31" s="154"/>
-      <c r="L31" s="154"/>
+      <c r="A31" s="156"/>
+      <c r="B31" s="156"/>
+      <c r="C31" s="156"/>
+      <c r="D31" s="156"/>
+      <c r="E31" s="156"/>
+      <c r="F31" s="156"/>
+      <c r="G31" s="156"/>
+      <c r="H31" s="156"/>
+      <c r="I31" s="156"/>
+      <c r="J31" s="156"/>
+      <c r="K31" s="156"/>
+      <c r="L31" s="156"/>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A32" s="154"/>
-      <c r="B32" s="154"/>
-      <c r="C32" s="154"/>
-      <c r="D32" s="154"/>
-      <c r="E32" s="154"/>
-      <c r="F32" s="154"/>
-      <c r="G32" s="154"/>
-      <c r="H32" s="154"/>
-      <c r="I32" s="154"/>
-      <c r="J32" s="154"/>
-      <c r="K32" s="154"/>
-      <c r="L32" s="154"/>
+      <c r="A32" s="156"/>
+      <c r="B32" s="156"/>
+      <c r="C32" s="156"/>
+      <c r="D32" s="156"/>
+      <c r="E32" s="156"/>
+      <c r="F32" s="156"/>
+      <c r="G32" s="156"/>
+      <c r="H32" s="156"/>
+      <c r="I32" s="156"/>
+      <c r="J32" s="156"/>
+      <c r="K32" s="156"/>
+      <c r="L32" s="156"/>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A33" s="154"/>
-      <c r="B33" s="154"/>
-      <c r="C33" s="154"/>
-      <c r="D33" s="154"/>
-      <c r="E33" s="154"/>
-      <c r="F33" s="154"/>
-      <c r="G33" s="154"/>
-      <c r="H33" s="154"/>
-      <c r="I33" s="154"/>
-      <c r="J33" s="154"/>
-      <c r="K33" s="154"/>
-      <c r="L33" s="154"/>
+      <c r="A33" s="156"/>
+      <c r="B33" s="156"/>
+      <c r="C33" s="156"/>
+      <c r="D33" s="156"/>
+      <c r="E33" s="156"/>
+      <c r="F33" s="156"/>
+      <c r="G33" s="156"/>
+      <c r="H33" s="156"/>
+      <c r="I33" s="156"/>
+      <c r="J33" s="156"/>
+      <c r="K33" s="156"/>
+      <c r="L33" s="156"/>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A34" s="154"/>
-      <c r="B34" s="154"/>
-      <c r="C34" s="154"/>
-      <c r="D34" s="154"/>
-      <c r="E34" s="154"/>
-      <c r="F34" s="154"/>
-      <c r="G34" s="154"/>
-      <c r="H34" s="154"/>
-      <c r="I34" s="154"/>
-      <c r="J34" s="154"/>
-      <c r="K34" s="154"/>
-      <c r="L34" s="154"/>
+      <c r="A34" s="156"/>
+      <c r="B34" s="156"/>
+      <c r="C34" s="156"/>
+      <c r="D34" s="156"/>
+      <c r="E34" s="156"/>
+      <c r="F34" s="156"/>
+      <c r="G34" s="156"/>
+      <c r="H34" s="156"/>
+      <c r="I34" s="156"/>
+      <c r="J34" s="156"/>
+      <c r="K34" s="156"/>
+      <c r="L34" s="156"/>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A35" s="154"/>
-      <c r="B35" s="154"/>
-      <c r="C35" s="154"/>
-      <c r="D35" s="154"/>
-      <c r="E35" s="154"/>
-      <c r="F35" s="154"/>
-      <c r="G35" s="154"/>
-      <c r="H35" s="154"/>
-      <c r="I35" s="154"/>
-      <c r="J35" s="154"/>
-      <c r="K35" s="154"/>
-      <c r="L35" s="154"/>
+      <c r="A35" s="156"/>
+      <c r="B35" s="156"/>
+      <c r="C35" s="156"/>
+      <c r="D35" s="156"/>
+      <c r="E35" s="156"/>
+      <c r="F35" s="156"/>
+      <c r="G35" s="156"/>
+      <c r="H35" s="156"/>
+      <c r="I35" s="156"/>
+      <c r="J35" s="156"/>
+      <c r="K35" s="156"/>
+      <c r="L35" s="156"/>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A36" s="154"/>
-      <c r="B36" s="154"/>
-      <c r="C36" s="154"/>
-      <c r="D36" s="154"/>
-      <c r="E36" s="154"/>
-      <c r="F36" s="154"/>
-      <c r="G36" s="154"/>
-      <c r="H36" s="154"/>
-      <c r="I36" s="154"/>
-      <c r="J36" s="154"/>
-      <c r="K36" s="154"/>
-      <c r="L36" s="154"/>
+      <c r="A36" s="156"/>
+      <c r="B36" s="156"/>
+      <c r="C36" s="156"/>
+      <c r="D36" s="156"/>
+      <c r="E36" s="156"/>
+      <c r="F36" s="156"/>
+      <c r="G36" s="156"/>
+      <c r="H36" s="156"/>
+      <c r="I36" s="156"/>
+      <c r="J36" s="156"/>
+      <c r="K36" s="156"/>
+      <c r="L36" s="156"/>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A37" s="154"/>
-      <c r="B37" s="154"/>
-      <c r="C37" s="154"/>
-      <c r="D37" s="154"/>
-      <c r="E37" s="154"/>
-      <c r="F37" s="154"/>
-      <c r="G37" s="154"/>
-      <c r="H37" s="154"/>
-      <c r="I37" s="154"/>
-      <c r="J37" s="154"/>
-      <c r="K37" s="154"/>
-      <c r="L37" s="154"/>
+      <c r="A37" s="156"/>
+      <c r="B37" s="156"/>
+      <c r="C37" s="156"/>
+      <c r="D37" s="156"/>
+      <c r="E37" s="156"/>
+      <c r="F37" s="156"/>
+      <c r="G37" s="156"/>
+      <c r="H37" s="156"/>
+      <c r="I37" s="156"/>
+      <c r="J37" s="156"/>
+      <c r="K37" s="156"/>
+      <c r="L37" s="156"/>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A38" s="154"/>
-      <c r="B38" s="154"/>
-      <c r="C38" s="154"/>
-      <c r="D38" s="154"/>
-      <c r="E38" s="154"/>
-      <c r="F38" s="154"/>
-      <c r="G38" s="154"/>
-      <c r="H38" s="154"/>
-      <c r="I38" s="154"/>
-      <c r="J38" s="154"/>
-      <c r="K38" s="154"/>
-      <c r="L38" s="154"/>
+      <c r="A38" s="156"/>
+      <c r="B38" s="156"/>
+      <c r="C38" s="156"/>
+      <c r="D38" s="156"/>
+      <c r="E38" s="156"/>
+      <c r="F38" s="156"/>
+      <c r="G38" s="156"/>
+      <c r="H38" s="156"/>
+      <c r="I38" s="156"/>
+      <c r="J38" s="156"/>
+      <c r="K38" s="156"/>
+      <c r="L38" s="156"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -8196,14 +8208,14 @@
       </c>
     </row>
     <row r="2" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="189" t="s">
+      <c r="A2" s="191" t="s">
         <v>1327</v>
       </c>
-      <c r="B2" s="190"/>
-      <c r="C2" s="190"/>
-      <c r="D2" s="190"/>
-      <c r="E2" s="190"/>
-      <c r="F2" s="190"/>
+      <c r="B2" s="192"/>
+      <c r="C2" s="192"/>
+      <c r="D2" s="192"/>
+      <c r="E2" s="192"/>
+      <c r="F2" s="192"/>
     </row>
     <row r="3" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
@@ -8423,14 +8435,14 @@
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A18" s="189" t="s">
+      <c r="A18" s="191" t="s">
         <v>1376</v>
       </c>
-      <c r="B18" s="190"/>
-      <c r="C18" s="190"/>
-      <c r="D18" s="190"/>
-      <c r="E18" s="190"/>
-      <c r="F18" s="190"/>
+      <c r="B18" s="192"/>
+      <c r="C18" s="192"/>
+      <c r="D18" s="192"/>
+      <c r="E18" s="192"/>
+      <c r="F18" s="192"/>
     </row>
     <row r="19" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A19" s="5" t="s">
@@ -8502,11 +8514,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F66"/>
+  <dimension ref="A1:F68"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F4" sqref="F4"/>
+      <selection pane="bottomLeft" activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -8546,13 +8558,13 @@
         <v>7</v>
       </c>
       <c r="C2" s="103" t="s">
-        <v>1395</v>
+        <v>1399</v>
       </c>
       <c r="D2" s="101" t="s">
         <v>8</v>
       </c>
       <c r="E2" s="102" t="s">
-        <v>1395</v>
+        <v>1399</v>
       </c>
       <c r="F2" s="101"/>
     </row>
@@ -9619,6 +9631,28 @@
       <c r="D66" s="88"/>
       <c r="E66" s="106" t="s">
         <v>242</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="B67" s="1" t="s">
+        <v>1395</v>
+      </c>
+      <c r="C67" s="2" t="s">
+        <v>1396</v>
+      </c>
+      <c r="E67" s="40" t="s">
+        <v>1398</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="B68" s="1" t="s">
+        <v>1397</v>
+      </c>
+      <c r="C68" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="E68" s="40" t="s">
+        <v>78</v>
       </c>
     </row>
   </sheetData>
@@ -10414,13 +10448,13 @@
       </c>
     </row>
     <row r="2" spans="1:6" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="158" t="s">
+      <c r="A2" s="163" t="s">
         <v>374</v>
       </c>
-      <c r="B2" s="159"/>
-      <c r="C2" s="159"/>
-      <c r="D2" s="159"/>
-      <c r="E2" s="160"/>
+      <c r="B2" s="164"/>
+      <c r="C2" s="164"/>
+      <c r="D2" s="164"/>
+      <c r="E2" s="165"/>
       <c r="F2" s="33"/>
     </row>
     <row r="3" spans="1:6" ht="48" x14ac:dyDescent="0.2">
@@ -10548,13 +10582,13 @@
       <c r="F9" s="122"/>
     </row>
     <row r="10" spans="1:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="161" t="s">
+      <c r="A10" s="166" t="s">
         <v>403</v>
       </c>
-      <c r="B10" s="162"/>
-      <c r="C10" s="162"/>
-      <c r="D10" s="162"/>
-      <c r="E10" s="163"/>
+      <c r="B10" s="167"/>
+      <c r="C10" s="167"/>
+      <c r="D10" s="167"/>
+      <c r="E10" s="168"/>
       <c r="F10" s="122"/>
     </row>
     <row r="11" spans="1:6" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -10612,13 +10646,13 @@
       <c r="F13" s="88"/>
     </row>
     <row r="14" spans="1:6" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="155" t="s">
+      <c r="A14" s="157" t="s">
         <v>416</v>
       </c>
-      <c r="B14" s="156"/>
-      <c r="C14" s="156"/>
-      <c r="D14" s="156"/>
-      <c r="E14" s="157"/>
+      <c r="B14" s="158"/>
+      <c r="C14" s="158"/>
+      <c r="D14" s="158"/>
+      <c r="E14" s="159"/>
       <c r="F14" s="122"/>
     </row>
     <row r="15" spans="1:6" ht="48" x14ac:dyDescent="0.2">
@@ -10762,13 +10796,13 @@
       <c r="F23" s="122"/>
     </row>
     <row r="24" spans="1:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="155" t="s">
+      <c r="A24" s="157" t="s">
         <v>446</v>
       </c>
-      <c r="B24" s="156"/>
-      <c r="C24" s="156"/>
-      <c r="D24" s="156"/>
-      <c r="E24" s="157"/>
+      <c r="B24" s="158"/>
+      <c r="C24" s="158"/>
+      <c r="D24" s="158"/>
+      <c r="E24" s="159"/>
       <c r="F24" s="122"/>
     </row>
     <row r="25" spans="1:6" ht="32" x14ac:dyDescent="0.2">
@@ -11040,13 +11074,13 @@
       <c r="F42" s="122"/>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A43" s="155" t="s">
+      <c r="A43" s="157" t="s">
         <v>490</v>
       </c>
-      <c r="B43" s="156"/>
-      <c r="C43" s="156"/>
-      <c r="D43" s="156"/>
-      <c r="E43" s="157"/>
+      <c r="B43" s="158"/>
+      <c r="C43" s="158"/>
+      <c r="D43" s="158"/>
+      <c r="E43" s="159"/>
       <c r="F43" s="122"/>
     </row>
     <row r="44" spans="1:6" ht="32" x14ac:dyDescent="0.2">
@@ -11248,13 +11282,13 @@
       <c r="F56" s="122"/>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A57" s="155" t="s">
+      <c r="A57" s="157" t="s">
         <v>521</v>
       </c>
-      <c r="B57" s="156"/>
-      <c r="C57" s="156"/>
-      <c r="D57" s="156"/>
-      <c r="E57" s="157"/>
+      <c r="B57" s="158"/>
+      <c r="C57" s="158"/>
+      <c r="D57" s="158"/>
+      <c r="E57" s="159"/>
       <c r="F57" s="122"/>
     </row>
     <row r="58" spans="1:6" ht="64" x14ac:dyDescent="0.2">
@@ -11312,13 +11346,13 @@
       <c r="F60" s="122"/>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A61" s="155" t="s">
+      <c r="A61" s="157" t="s">
         <v>536</v>
       </c>
-      <c r="B61" s="156"/>
-      <c r="C61" s="156"/>
-      <c r="D61" s="156"/>
-      <c r="E61" s="157"/>
+      <c r="B61" s="158"/>
+      <c r="C61" s="158"/>
+      <c r="D61" s="158"/>
+      <c r="E61" s="159"/>
       <c r="F61" s="122"/>
     </row>
     <row r="62" spans="1:6" ht="48" x14ac:dyDescent="0.2">
@@ -11368,13 +11402,13 @@
       <c r="F64" s="122"/>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A65" s="155" t="s">
+      <c r="A65" s="157" t="s">
         <v>541</v>
       </c>
-      <c r="B65" s="156"/>
-      <c r="C65" s="156"/>
-      <c r="D65" s="156"/>
-      <c r="E65" s="157"/>
+      <c r="B65" s="158"/>
+      <c r="C65" s="158"/>
+      <c r="D65" s="158"/>
+      <c r="E65" s="159"/>
       <c r="F65" s="122"/>
     </row>
     <row r="66" spans="1:6" ht="32" x14ac:dyDescent="0.2">
@@ -11606,13 +11640,13 @@
       <c r="F79" s="122"/>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A80" s="155" t="s">
+      <c r="A80" s="157" t="s">
         <v>580</v>
       </c>
-      <c r="B80" s="156"/>
-      <c r="C80" s="156"/>
-      <c r="D80" s="156"/>
-      <c r="E80" s="157"/>
+      <c r="B80" s="158"/>
+      <c r="C80" s="158"/>
+      <c r="D80" s="158"/>
+      <c r="E80" s="159"/>
       <c r="F80" s="122"/>
     </row>
     <row r="81" spans="1:6" ht="62.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -11764,13 +11798,13 @@
       <c r="F89" s="122"/>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A90" s="155" t="s">
+      <c r="A90" s="157" t="s">
         <v>607</v>
       </c>
-      <c r="B90" s="156"/>
-      <c r="C90" s="156"/>
-      <c r="D90" s="156"/>
-      <c r="E90" s="157"/>
+      <c r="B90" s="158"/>
+      <c r="C90" s="158"/>
+      <c r="D90" s="158"/>
+      <c r="E90" s="159"/>
       <c r="F90" s="122"/>
     </row>
     <row r="91" spans="1:6" ht="48" x14ac:dyDescent="0.2">
@@ -12236,13 +12270,13 @@
       <c r="F120" s="122"/>
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A121" s="155" t="s">
+      <c r="A121" s="157" t="s">
         <v>694</v>
       </c>
-      <c r="B121" s="156"/>
-      <c r="C121" s="156"/>
-      <c r="D121" s="156"/>
-      <c r="E121" s="157"/>
+      <c r="B121" s="158"/>
+      <c r="C121" s="158"/>
+      <c r="D121" s="158"/>
+      <c r="E121" s="159"/>
       <c r="F121" s="122"/>
     </row>
     <row r="122" spans="1:6" ht="32" x14ac:dyDescent="0.2">
@@ -12430,13 +12464,13 @@
       <c r="F134" s="122"/>
     </row>
     <row r="135" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A135" s="155" t="s">
+      <c r="A135" s="157" t="s">
         <v>716</v>
       </c>
-      <c r="B135" s="156"/>
-      <c r="C135" s="156"/>
-      <c r="D135" s="156"/>
-      <c r="E135" s="157"/>
+      <c r="B135" s="158"/>
+      <c r="C135" s="158"/>
+      <c r="D135" s="158"/>
+      <c r="E135" s="159"/>
       <c r="F135" s="122"/>
     </row>
     <row r="136" spans="1:6" ht="64" x14ac:dyDescent="0.2">
@@ -12566,13 +12600,13 @@
       <c r="F143" s="122"/>
     </row>
     <row r="144" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A144" s="155" t="s">
+      <c r="A144" s="157" t="s">
         <v>737</v>
       </c>
-      <c r="B144" s="156"/>
-      <c r="C144" s="156"/>
-      <c r="D144" s="156"/>
-      <c r="E144" s="157"/>
+      <c r="B144" s="158"/>
+      <c r="C144" s="158"/>
+      <c r="D144" s="158"/>
+      <c r="E144" s="159"/>
       <c r="F144" s="122"/>
     </row>
     <row r="145" spans="1:6" ht="32" x14ac:dyDescent="0.2">
@@ -12732,13 +12766,13 @@
       <c r="F154" s="122"/>
     </row>
     <row r="155" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A155" s="155" t="s">
+      <c r="A155" s="157" t="s">
         <v>758</v>
       </c>
-      <c r="B155" s="156"/>
-      <c r="C155" s="156"/>
-      <c r="D155" s="156"/>
-      <c r="E155" s="157"/>
+      <c r="B155" s="158"/>
+      <c r="C155" s="158"/>
+      <c r="D155" s="158"/>
+      <c r="E155" s="159"/>
       <c r="F155" s="122"/>
     </row>
     <row r="156" spans="1:6" ht="48" x14ac:dyDescent="0.2">
@@ -12856,13 +12890,13 @@
       <c r="F162" s="122"/>
     </row>
     <row r="163" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A163" s="164" t="s">
+      <c r="A163" s="160" t="s">
         <v>778</v>
       </c>
-      <c r="B163" s="165"/>
-      <c r="C163" s="165"/>
-      <c r="D163" s="165"/>
-      <c r="E163" s="166"/>
+      <c r="B163" s="161"/>
+      <c r="C163" s="161"/>
+      <c r="D163" s="161"/>
+      <c r="E163" s="162"/>
       <c r="F163" s="132" t="s">
         <v>779</v>
       </c>
@@ -12988,13 +13022,13 @@
       </c>
     </row>
     <row r="172" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A172" s="155" t="s">
+      <c r="A172" s="157" t="s">
         <v>790</v>
       </c>
-      <c r="B172" s="156"/>
-      <c r="C172" s="156"/>
-      <c r="D172" s="156"/>
-      <c r="E172" s="157"/>
+      <c r="B172" s="158"/>
+      <c r="C172" s="158"/>
+      <c r="D172" s="158"/>
+      <c r="E172" s="159"/>
       <c r="F172" s="122"/>
     </row>
     <row r="173" spans="1:6" ht="32" x14ac:dyDescent="0.2">
@@ -13180,13 +13214,13 @@
       <c r="F183" s="122"/>
     </row>
     <row r="184" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A184" s="155" t="s">
+      <c r="A184" s="157" t="s">
         <v>811</v>
       </c>
-      <c r="B184" s="156"/>
-      <c r="C184" s="156"/>
-      <c r="D184" s="156"/>
-      <c r="E184" s="157"/>
+      <c r="B184" s="158"/>
+      <c r="C184" s="158"/>
+      <c r="D184" s="158"/>
+      <c r="E184" s="159"/>
       <c r="F184" s="122"/>
     </row>
     <row r="185" spans="1:6" ht="32" x14ac:dyDescent="0.2">
@@ -13236,13 +13270,13 @@
       <c r="F187" s="122"/>
     </row>
     <row r="188" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A188" s="155" t="s">
+      <c r="A188" s="157" t="s">
         <v>819</v>
       </c>
-      <c r="B188" s="156"/>
-      <c r="C188" s="156"/>
-      <c r="D188" s="156"/>
-      <c r="E188" s="157"/>
+      <c r="B188" s="158"/>
+      <c r="C188" s="158"/>
+      <c r="D188" s="158"/>
+      <c r="E188" s="159"/>
       <c r="F188" s="122"/>
     </row>
     <row r="189" spans="1:6" ht="64" x14ac:dyDescent="0.2">
@@ -13328,13 +13362,13 @@
       <c r="F193" s="122"/>
     </row>
     <row r="194" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A194" s="155" t="s">
+      <c r="A194" s="157" t="s">
         <v>836</v>
       </c>
-      <c r="B194" s="156"/>
-      <c r="C194" s="156"/>
-      <c r="D194" s="156"/>
-      <c r="E194" s="157"/>
+      <c r="B194" s="158"/>
+      <c r="C194" s="158"/>
+      <c r="D194" s="158"/>
+      <c r="E194" s="159"/>
       <c r="F194" s="122"/>
     </row>
     <row r="195" spans="1:6" ht="32" x14ac:dyDescent="0.2">
@@ -13474,13 +13508,13 @@
       <c r="F203" s="122"/>
     </row>
     <row r="204" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A204" s="155" t="s">
+      <c r="A204" s="157" t="s">
         <v>850</v>
       </c>
-      <c r="B204" s="156"/>
-      <c r="C204" s="156"/>
-      <c r="D204" s="156"/>
-      <c r="E204" s="157"/>
+      <c r="B204" s="158"/>
+      <c r="C204" s="158"/>
+      <c r="D204" s="158"/>
+      <c r="E204" s="159"/>
       <c r="F204" s="122"/>
     </row>
     <row r="205" spans="1:6" ht="48" x14ac:dyDescent="0.2">
@@ -13566,13 +13600,13 @@
       <c r="F209" s="122"/>
     </row>
     <row r="210" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A210" s="155" t="s">
+      <c r="A210" s="157" t="s">
         <v>860</v>
       </c>
-      <c r="B210" s="156"/>
-      <c r="C210" s="156"/>
-      <c r="D210" s="156"/>
-      <c r="E210" s="157"/>
+      <c r="B210" s="158"/>
+      <c r="C210" s="158"/>
+      <c r="D210" s="158"/>
+      <c r="E210" s="159"/>
       <c r="F210" s="122"/>
     </row>
     <row r="211" spans="1:6" ht="32" x14ac:dyDescent="0.2">
@@ -13730,13 +13764,13 @@
       <c r="F220" s="122"/>
     </row>
     <row r="221" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A221" s="155" t="s">
+      <c r="A221" s="157" t="s">
         <v>874</v>
       </c>
-      <c r="B221" s="156"/>
-      <c r="C221" s="156"/>
-      <c r="D221" s="156"/>
-      <c r="E221" s="157"/>
+      <c r="B221" s="158"/>
+      <c r="C221" s="158"/>
+      <c r="D221" s="158"/>
+      <c r="E221" s="159"/>
       <c r="F221" s="122"/>
     </row>
     <row r="222" spans="1:6" ht="48" x14ac:dyDescent="0.2">
@@ -14731,6 +14765,18 @@
     </row>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="A221:E221"/>
+    <mergeCell ref="A184:E184"/>
+    <mergeCell ref="A188:E188"/>
+    <mergeCell ref="A194:E194"/>
+    <mergeCell ref="A204:E204"/>
+    <mergeCell ref="A210:E210"/>
+    <mergeCell ref="A57:E57"/>
+    <mergeCell ref="A2:E2"/>
+    <mergeCell ref="A10:E10"/>
+    <mergeCell ref="A14:E14"/>
+    <mergeCell ref="A24:E24"/>
+    <mergeCell ref="A43:E43"/>
     <mergeCell ref="A172:E172"/>
     <mergeCell ref="A155:E155"/>
     <mergeCell ref="A61:E61"/>
@@ -14741,18 +14787,6 @@
     <mergeCell ref="A144:E144"/>
     <mergeCell ref="A90:E90"/>
     <mergeCell ref="A163:E163"/>
-    <mergeCell ref="A57:E57"/>
-    <mergeCell ref="A2:E2"/>
-    <mergeCell ref="A10:E10"/>
-    <mergeCell ref="A14:E14"/>
-    <mergeCell ref="A24:E24"/>
-    <mergeCell ref="A43:E43"/>
-    <mergeCell ref="A221:E221"/>
-    <mergeCell ref="A184:E184"/>
-    <mergeCell ref="A188:E188"/>
-    <mergeCell ref="A194:E194"/>
-    <mergeCell ref="A204:E204"/>
-    <mergeCell ref="A210:E210"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -14799,13 +14833,13 @@
       </c>
     </row>
     <row r="2" spans="1:6" s="24" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="170" t="s">
+      <c r="A2" s="172" t="s">
         <v>925</v>
       </c>
-      <c r="B2" s="171"/>
-      <c r="C2" s="171"/>
-      <c r="D2" s="171"/>
-      <c r="E2" s="172"/>
+      <c r="B2" s="173"/>
+      <c r="C2" s="173"/>
+      <c r="D2" s="173"/>
+      <c r="E2" s="174"/>
     </row>
     <row r="3" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="19" t="s">
@@ -14939,13 +14973,13 @@
       </c>
     </row>
     <row r="12" spans="1:6" s="24" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="170" t="s">
+      <c r="A12" s="172" t="s">
         <v>947</v>
       </c>
-      <c r="B12" s="171"/>
-      <c r="C12" s="171"/>
-      <c r="D12" s="171"/>
-      <c r="E12" s="172"/>
+      <c r="B12" s="173"/>
+      <c r="C12" s="173"/>
+      <c r="D12" s="173"/>
+      <c r="E12" s="174"/>
     </row>
     <row r="13" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A13" s="19" t="s">
@@ -15022,13 +15056,13 @@
       <c r="B17" s="95" t="s">
         <v>962</v>
       </c>
-      <c r="C17" s="191" t="s">
+      <c r="C17" s="154" t="s">
         <v>1393</v>
       </c>
       <c r="D17" s="95" t="s">
         <v>954</v>
       </c>
-      <c r="E17" s="192" t="s">
+      <c r="E17" s="155" t="s">
         <v>1394</v>
       </c>
     </row>
@@ -15057,13 +15091,13 @@
       </c>
     </row>
     <row r="20" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="179" t="s">
+      <c r="A20" s="181" t="s">
         <v>967</v>
       </c>
-      <c r="B20" s="180"/>
-      <c r="C20" s="180"/>
-      <c r="D20" s="180"/>
-      <c r="E20" s="181"/>
+      <c r="B20" s="182"/>
+      <c r="C20" s="182"/>
+      <c r="D20" s="182"/>
+      <c r="E20" s="183"/>
     </row>
     <row r="21" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A21" s="5" t="s">
@@ -15111,13 +15145,13 @@
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A24" s="176" t="s">
+      <c r="A24" s="178" t="s">
         <v>980</v>
       </c>
-      <c r="B24" s="177"/>
-      <c r="C24" s="177"/>
-      <c r="D24" s="177"/>
-      <c r="E24" s="178"/>
+      <c r="B24" s="179"/>
+      <c r="C24" s="179"/>
+      <c r="D24" s="179"/>
+      <c r="E24" s="180"/>
     </row>
     <row r="25" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A25" s="18" t="s">
@@ -15135,13 +15169,13 @@
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A26" s="167" t="s">
+      <c r="A26" s="169" t="s">
         <v>984</v>
       </c>
-      <c r="B26" s="168"/>
-      <c r="C26" s="168"/>
-      <c r="D26" s="168"/>
-      <c r="E26" s="169"/>
+      <c r="B26" s="170"/>
+      <c r="C26" s="170"/>
+      <c r="D26" s="170"/>
+      <c r="E26" s="171"/>
     </row>
     <row r="27" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A27" s="18" t="s">
@@ -15159,13 +15193,13 @@
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A28" s="167" t="s">
+      <c r="A28" s="169" t="s">
         <v>988</v>
       </c>
-      <c r="B28" s="168"/>
-      <c r="C28" s="168"/>
-      <c r="D28" s="168"/>
-      <c r="E28" s="169"/>
+      <c r="B28" s="170"/>
+      <c r="C28" s="170"/>
+      <c r="D28" s="170"/>
+      <c r="E28" s="171"/>
     </row>
     <row r="29" spans="1:6" ht="112" x14ac:dyDescent="0.2">
       <c r="A29" s="94" t="s">
@@ -15289,13 +15323,13 @@
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A37" s="167" t="s">
+      <c r="A37" s="169" t="s">
         <v>1015</v>
       </c>
-      <c r="B37" s="168"/>
-      <c r="C37" s="168"/>
-      <c r="D37" s="168"/>
-      <c r="E37" s="169"/>
+      <c r="B37" s="170"/>
+      <c r="C37" s="170"/>
+      <c r="D37" s="170"/>
+      <c r="E37" s="171"/>
     </row>
     <row r="38" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A38" s="19" t="s">
@@ -15339,13 +15373,13 @@
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A41" s="173" t="s">
+      <c r="A41" s="175" t="s">
         <v>1023</v>
       </c>
-      <c r="B41" s="174"/>
-      <c r="C41" s="174"/>
-      <c r="D41" s="174"/>
-      <c r="E41" s="175"/>
+      <c r="B41" s="176"/>
+      <c r="C41" s="176"/>
+      <c r="D41" s="176"/>
+      <c r="E41" s="177"/>
     </row>
     <row r="42" spans="1:6" ht="96" x14ac:dyDescent="0.2">
       <c r="A42" s="119" t="s">
@@ -16039,13 +16073,13 @@
       </c>
     </row>
     <row r="28" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="182" t="s">
+      <c r="A28" s="184" t="s">
         <v>1145</v>
       </c>
-      <c r="B28" s="183"/>
-      <c r="C28" s="183"/>
-      <c r="D28" s="183"/>
-      <c r="E28" s="184"/>
+      <c r="B28" s="185"/>
+      <c r="C28" s="185"/>
+      <c r="D28" s="185"/>
+      <c r="E28" s="186"/>
     </row>
     <row r="29" spans="1:5" ht="48" x14ac:dyDescent="0.2">
       <c r="A29" s="143" t="s">
@@ -16108,13 +16142,13 @@
       <c r="E32" s="149"/>
     </row>
     <row r="33" spans="1:6" s="13" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="185" t="s">
+      <c r="A33" s="187" t="s">
         <v>1157</v>
       </c>
-      <c r="B33" s="186"/>
-      <c r="C33" s="187"/>
-      <c r="D33" s="186"/>
-      <c r="E33" s="188"/>
+      <c r="B33" s="188"/>
+      <c r="C33" s="189"/>
+      <c r="D33" s="188"/>
+      <c r="E33" s="190"/>
     </row>
     <row r="34" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A34" s="147" t="s">
@@ -16317,13 +16351,13 @@
       <c r="F45" s="138"/>
     </row>
     <row r="46" spans="1:6" s="13" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="182" t="s">
+      <c r="A46" s="184" t="s">
         <v>1187</v>
       </c>
-      <c r="B46" s="183"/>
-      <c r="C46" s="183"/>
-      <c r="D46" s="183"/>
-      <c r="E46" s="184"/>
+      <c r="B46" s="185"/>
+      <c r="C46" s="185"/>
+      <c r="D46" s="185"/>
+      <c r="E46" s="186"/>
     </row>
     <row r="47" spans="1:6" s="30" customFormat="1" ht="64" x14ac:dyDescent="0.2">
       <c r="A47" s="147" t="s">
@@ -16951,6 +16985,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <Readyforteam_x003f_ xmlns="565e1b1d-057e-4d85-b896-01a5881d8a45">false</Readyforteam_x003f_>
@@ -16989,15 +17032,6 @@
     <TaxCatchAll xmlns="2799d30d-6731-4efe-ac9b-c4895a8828d9" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -17278,6 +17312,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8D7CE8C7-18DC-484F-8376-ED09F13D44C8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{017ACE96-8143-486E-8436-7787F6B96F4A}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -17286,14 +17328,6 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
     <ds:schemaRef ds:uri="bf601f31-63a1-4825-9216-91d773c5ef9c"/>
     <ds:schemaRef ds:uri="2799d30d-6731-4efe-ac9b-c4895a8828d9"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8D7CE8C7-18DC-484F-8376-ED09F13D44C8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
exact-address and location-death-hospital harmonising with v11
</commit_message>
<xml_diff>
--- a/app/data/MCCD-localisation.xlsx
+++ b/app/data/MCCD-localisation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/JALAT/GIT/medical-certificate-of-cause-of-death/app/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA2F62DB-7B51-3148-9304-189BED334D61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7BDF17E-F5E6-534B-A2AE-42A18653E0F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="14220" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -68,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2092" uniqueCount="1406">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2097" uniqueCount="1409">
   <si>
     <r>
       <rPr>
@@ -3807,15 +3807,6 @@
     <t>dpdOtherLocationPostcodeLink</t>
   </si>
   <si>
-    <t>dpdOtherLocationsFindAddress</t>
-  </si>
-  <si>
-    <t>dpdOtherLocationsLink</t>
-  </si>
-  <si>
-    <t>Or find the address using hospital name or postcode (new content)</t>
-  </si>
-  <si>
     <t>dpdOtherLocationPostcodeSearchValidationSummaryEmpty</t>
   </si>
   <si>
@@ -5753,9 +5744,6 @@
     <t>Er enghraifft, in Castle Park, Bingley near the fountain</t>
   </si>
   <si>
-    <t>012</t>
-  </si>
-  <si>
     <t>dpdPlaceOfBirthHintWelsh</t>
   </si>
   <si>
@@ -5766,6 +5754,27 @@
   </si>
   <si>
     <t>Er enghraifft, Royal Victoria Infirmary, Newcastle</t>
+  </si>
+  <si>
+    <t>Find the address using hospital name or postcode</t>
+  </si>
+  <si>
+    <t>Dewch o hyd i'r cyfeiriad gan ddefnyddio enw ysbyty neu côd post</t>
+  </si>
+  <si>
+    <t>Find the address using postcode</t>
+  </si>
+  <si>
+    <t>dpdOtherLocationHospitalPostcodeLink</t>
+  </si>
+  <si>
+    <t>dpdOtherLocationFindAddress</t>
+  </si>
+  <si>
+    <t>Dod o hyd i'r cyfeiriad gan ddefnyddio côd post</t>
+  </si>
+  <si>
+    <t>014</t>
   </si>
 </sst>
 </file>
@@ -6709,6 +6718,15 @@
     <xf numFmtId="0" fontId="13" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -6725,15 +6743,6 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -7777,33 +7786,33 @@
         <v>243</v>
       </c>
       <c r="B2" s="93" t="s">
+        <v>1268</v>
+      </c>
+      <c r="C2" s="94" t="s">
+        <v>1269</v>
+      </c>
+      <c r="D2" s="93" t="s">
+        <v>1270</v>
+      </c>
+      <c r="E2" s="86" t="s">
         <v>1271</v>
-      </c>
-      <c r="C2" s="94" t="s">
-        <v>1272</v>
-      </c>
-      <c r="D2" s="93" t="s">
-        <v>1273</v>
-      </c>
-      <c r="E2" s="86" t="s">
-        <v>1274</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="80" x14ac:dyDescent="0.2">
       <c r="A3" s="95" t="s">
+        <v>1272</v>
+      </c>
+      <c r="B3" s="96" t="s">
+        <v>1273</v>
+      </c>
+      <c r="C3" s="97" t="s">
+        <v>1274</v>
+      </c>
+      <c r="D3" s="96" t="s">
         <v>1275</v>
       </c>
-      <c r="B3" s="96" t="s">
+      <c r="E3" s="90" t="s">
         <v>1276</v>
-      </c>
-      <c r="C3" s="97" t="s">
-        <v>1277</v>
-      </c>
-      <c r="D3" s="96" t="s">
-        <v>1278</v>
-      </c>
-      <c r="E3" s="90" t="s">
-        <v>1279</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="16" x14ac:dyDescent="0.2">
@@ -7811,16 +7820,16 @@
         <v>766</v>
       </c>
       <c r="B4" s="96" t="s">
-        <v>1280</v>
+        <v>1277</v>
       </c>
       <c r="C4" s="97" t="s">
-        <v>1281</v>
+        <v>1278</v>
       </c>
       <c r="D4" s="96" t="s">
         <v>411</v>
       </c>
       <c r="E4" s="90" t="s">
-        <v>1282</v>
+        <v>1279</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="60.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -7828,13 +7837,13 @@
         <v>417</v>
       </c>
       <c r="B5" s="106" t="s">
-        <v>1283</v>
+        <v>1280</v>
       </c>
       <c r="C5" s="107" t="s">
         <v>411</v>
       </c>
       <c r="D5" s="108" t="s">
-        <v>1284</v>
+        <v>1281</v>
       </c>
       <c r="E5" s="90" t="s">
         <v>411</v>
@@ -7845,13 +7854,13 @@
         <v>420</v>
       </c>
       <c r="B6" s="106" t="s">
-        <v>1285</v>
+        <v>1282</v>
       </c>
       <c r="C6" s="107" t="s">
         <v>411</v>
       </c>
       <c r="D6" s="108" t="s">
-        <v>1286</v>
+        <v>1283</v>
       </c>
       <c r="E6" s="90" t="s">
         <v>411</v>
@@ -7879,33 +7888,33 @@
         <v>243</v>
       </c>
       <c r="B8" s="96" t="s">
+        <v>1284</v>
+      </c>
+      <c r="C8" s="97" t="s">
+        <v>1285</v>
+      </c>
+      <c r="D8" s="96" t="s">
+        <v>1286</v>
+      </c>
+      <c r="E8" s="90" t="s">
         <v>1287</v>
-      </c>
-      <c r="C8" s="97" t="s">
-        <v>1288</v>
-      </c>
-      <c r="D8" s="96" t="s">
-        <v>1289</v>
-      </c>
-      <c r="E8" s="90" t="s">
-        <v>1290</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="64" x14ac:dyDescent="0.2">
       <c r="A9" s="95" t="s">
-        <v>1275</v>
+        <v>1272</v>
       </c>
       <c r="B9" s="96" t="s">
+        <v>1288</v>
+      </c>
+      <c r="C9" s="97" t="s">
+        <v>1289</v>
+      </c>
+      <c r="D9" s="96" t="s">
+        <v>1290</v>
+      </c>
+      <c r="E9" s="90" t="s">
         <v>1291</v>
-      </c>
-      <c r="C9" s="97" t="s">
-        <v>1292</v>
-      </c>
-      <c r="D9" s="96" t="s">
-        <v>1293</v>
-      </c>
-      <c r="E9" s="90" t="s">
-        <v>1294</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="16" x14ac:dyDescent="0.2">
@@ -7913,10 +7922,10 @@
         <v>766</v>
       </c>
       <c r="B10" s="96" t="s">
-        <v>1295</v>
+        <v>1292</v>
       </c>
       <c r="C10" s="97" t="s">
-        <v>1296</v>
+        <v>1293</v>
       </c>
       <c r="D10" s="96" t="s">
         <v>411</v>
@@ -7930,13 +7939,13 @@
         <v>417</v>
       </c>
       <c r="B11" s="106" t="s">
-        <v>1297</v>
+        <v>1294</v>
       </c>
       <c r="C11" s="107" t="s">
         <v>411</v>
       </c>
       <c r="D11" s="108" t="s">
-        <v>1284</v>
+        <v>1281</v>
       </c>
       <c r="E11" s="90" t="s">
         <v>411</v>
@@ -7947,13 +7956,13 @@
         <v>420</v>
       </c>
       <c r="B12" s="106" t="s">
-        <v>1298</v>
+        <v>1295</v>
       </c>
       <c r="C12" s="107" t="s">
         <v>411</v>
       </c>
       <c r="D12" s="108" t="s">
-        <v>1286</v>
+        <v>1283</v>
       </c>
       <c r="E12" s="90" t="s">
         <v>411</v>
@@ -7981,13 +7990,13 @@
         <v>243</v>
       </c>
       <c r="B14" s="96" t="s">
-        <v>1299</v>
+        <v>1296</v>
       </c>
       <c r="C14" s="97" t="s">
-        <v>1300</v>
+        <v>1297</v>
       </c>
       <c r="D14" s="96" t="s">
-        <v>1301</v>
+        <v>1298</v>
       </c>
       <c r="E14" s="90" t="s">
         <v>411</v>
@@ -7995,19 +8004,19 @@
     </row>
     <row r="15" spans="1:6" ht="96" x14ac:dyDescent="0.2">
       <c r="A15" s="95" t="s">
-        <v>1275</v>
+        <v>1272</v>
       </c>
       <c r="B15" s="96" t="s">
+        <v>1299</v>
+      </c>
+      <c r="C15" s="97" t="s">
+        <v>1300</v>
+      </c>
+      <c r="D15" s="96" t="s">
+        <v>1301</v>
+      </c>
+      <c r="E15" s="90" t="s">
         <v>1302</v>
-      </c>
-      <c r="C15" s="97" t="s">
-        <v>1303</v>
-      </c>
-      <c r="D15" s="96" t="s">
-        <v>1304</v>
-      </c>
-      <c r="E15" s="90" t="s">
-        <v>1305</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="48" x14ac:dyDescent="0.2">
@@ -8015,13 +8024,13 @@
         <v>417</v>
       </c>
       <c r="B16" s="106" t="s">
-        <v>1306</v>
+        <v>1303</v>
       </c>
       <c r="C16" s="107" t="s">
         <v>411</v>
       </c>
       <c r="D16" s="108" t="s">
-        <v>1284</v>
+        <v>1281</v>
       </c>
       <c r="E16" s="90" t="s">
         <v>411</v>
@@ -8032,13 +8041,13 @@
         <v>420</v>
       </c>
       <c r="B17" s="106" t="s">
-        <v>1307</v>
+        <v>1304</v>
       </c>
       <c r="C17" s="107" t="s">
         <v>411</v>
       </c>
       <c r="D17" s="108" t="s">
-        <v>1286</v>
+        <v>1283</v>
       </c>
       <c r="E17" s="90" t="s">
         <v>411</v>
@@ -8049,16 +8058,16 @@
         <v>14</v>
       </c>
       <c r="B18" s="96" t="s">
-        <v>1308</v>
+        <v>1305</v>
       </c>
       <c r="C18" s="97" t="s">
-        <v>1309</v>
+        <v>1306</v>
       </c>
       <c r="D18" s="96" t="s">
         <v>411</v>
       </c>
       <c r="E18" s="90" t="s">
-        <v>1310</v>
+        <v>1307</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -8083,13 +8092,13 @@
         <v>243</v>
       </c>
       <c r="B20" s="96" t="s">
-        <v>1311</v>
+        <v>1308</v>
       </c>
       <c r="C20" s="97" t="s">
-        <v>1312</v>
+        <v>1309</v>
       </c>
       <c r="D20" s="96" t="s">
-        <v>1273</v>
+        <v>1270</v>
       </c>
       <c r="E20" s="90" t="s">
         <v>411</v>
@@ -8097,16 +8106,16 @@
     </row>
     <row r="21" spans="1:5" ht="48" x14ac:dyDescent="0.2">
       <c r="A21" s="95" t="s">
-        <v>1275</v>
+        <v>1272</v>
       </c>
       <c r="B21" s="96" t="s">
-        <v>1313</v>
+        <v>1310</v>
       </c>
       <c r="C21" s="97" t="s">
-        <v>1314</v>
+        <v>1311</v>
       </c>
       <c r="D21" s="96" t="s">
-        <v>1315</v>
+        <v>1312</v>
       </c>
       <c r="E21" s="90" t="s">
         <v>411</v>
@@ -8117,10 +8126,10 @@
         <v>766</v>
       </c>
       <c r="B22" s="96" t="s">
-        <v>1316</v>
+        <v>1313</v>
       </c>
       <c r="C22" s="97" t="s">
-        <v>1317</v>
+        <v>1314</v>
       </c>
       <c r="D22" s="96" t="s">
         <v>411</v>
@@ -8134,13 +8143,13 @@
         <v>417</v>
       </c>
       <c r="B23" s="106" t="s">
-        <v>1318</v>
+        <v>1315</v>
       </c>
       <c r="C23" s="107" t="s">
         <v>411</v>
       </c>
       <c r="D23" s="108" t="s">
-        <v>1284</v>
+        <v>1281</v>
       </c>
       <c r="E23" s="90" t="s">
         <v>411</v>
@@ -8151,13 +8160,13 @@
         <v>420</v>
       </c>
       <c r="B24" s="106" t="s">
-        <v>1319</v>
+        <v>1316</v>
       </c>
       <c r="C24" s="107" t="s">
         <v>411</v>
       </c>
       <c r="D24" s="108" t="s">
-        <v>1286</v>
+        <v>1283</v>
       </c>
       <c r="E24" s="90" t="s">
         <v>411</v>
@@ -8210,7 +8219,7 @@
     </row>
     <row r="2" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="192" t="s">
-        <v>1320</v>
+        <v>1317</v>
       </c>
       <c r="B2" s="193"/>
       <c r="C2" s="193"/>
@@ -8223,16 +8232,16 @@
         <v>243</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>1321</v>
+        <v>1318</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>1322</v>
+        <v>1319</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>1253</v>
+        <v>1250</v>
       </c>
       <c r="E3" s="37" t="s">
-        <v>1323</v>
+        <v>1320</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="32" x14ac:dyDescent="0.2">
@@ -8240,13 +8249,13 @@
         <v>261</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>1324</v>
+        <v>1321</v>
       </c>
       <c r="C4" s="59" t="s">
-        <v>1325</v>
+        <v>1322</v>
       </c>
       <c r="E4" s="37" t="s">
-        <v>1326</v>
+        <v>1323</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="16" x14ac:dyDescent="0.2">
@@ -8254,13 +8263,13 @@
         <v>254</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>1327</v>
+        <v>1324</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>1328</v>
+        <v>1325</v>
       </c>
       <c r="E5" s="37" t="s">
-        <v>1329</v>
+        <v>1326</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="80" x14ac:dyDescent="0.2">
@@ -8268,13 +8277,13 @@
         <v>261</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>1330</v>
+        <v>1327</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>1331</v>
+        <v>1328</v>
       </c>
       <c r="E6" s="37" t="s">
-        <v>1332</v>
+        <v>1329</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="32" x14ac:dyDescent="0.2">
@@ -8282,127 +8291,127 @@
         <v>254</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>1333</v>
+        <v>1330</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>1334</v>
+        <v>1331</v>
       </c>
       <c r="E7" s="37" t="s">
-        <v>1335</v>
+        <v>1332</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
+        <v>1333</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>1334</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>1335</v>
+      </c>
+      <c r="E8" s="37" t="s">
         <v>1336</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>1337</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>1338</v>
-      </c>
-      <c r="E8" s="37" t="s">
-        <v>1339</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
+        <v>1337</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>1338</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>1339</v>
+      </c>
+      <c r="E9" s="37" t="s">
         <v>1340</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>1341</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>1342</v>
-      </c>
-      <c r="E9" s="37" t="s">
-        <v>1343</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
-        <v>1340</v>
+        <v>1337</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>1344</v>
+        <v>1341</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>1345</v>
+        <v>1342</v>
       </c>
       <c r="E10" s="37" t="s">
-        <v>1346</v>
+        <v>1343</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
-        <v>1340</v>
+        <v>1337</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>1347</v>
+        <v>1344</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>1348</v>
+        <v>1345</v>
       </c>
       <c r="E11" s="37" t="s">
-        <v>1349</v>
+        <v>1346</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="5" t="s">
-        <v>1340</v>
+        <v>1337</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>1350</v>
+        <v>1347</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>1351</v>
+        <v>1348</v>
       </c>
       <c r="E12" s="37" t="s">
-        <v>1352</v>
+        <v>1349</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="s">
-        <v>1340</v>
+        <v>1337</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>1353</v>
+        <v>1350</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>1354</v>
+        <v>1351</v>
       </c>
       <c r="E13" s="37" t="s">
-        <v>1355</v>
+        <v>1352</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A14" s="5" t="s">
-        <v>1336</v>
+        <v>1333</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>1356</v>
+        <v>1353</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>1357</v>
+        <v>1354</v>
       </c>
       <c r="D14" s="1"/>
       <c r="E14" s="37" t="s">
-        <v>1358</v>
+        <v>1355</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A15" s="5" t="s">
-        <v>965</v>
+        <v>962</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>1359</v>
+        <v>1356</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>1360</v>
+        <v>1357</v>
       </c>
       <c r="D15" s="1"/>
       <c r="E15" s="37" t="s">
-        <v>1361</v>
+        <v>1358</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="16" x14ac:dyDescent="0.2">
@@ -8410,34 +8419,34 @@
         <v>14</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>1362</v>
+        <v>1359</v>
       </c>
       <c r="C16" s="75" t="s">
-        <v>1363</v>
+        <v>1360</v>
       </c>
       <c r="D16" s="18"/>
       <c r="E16" s="37" t="s">
-        <v>1364</v>
+        <v>1361</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A17" s="5" t="s">
-        <v>1365</v>
+        <v>1362</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>1366</v>
+        <v>1363</v>
       </c>
       <c r="C17" s="76" t="s">
-        <v>1367</v>
+        <v>1364</v>
       </c>
       <c r="D17" s="18"/>
       <c r="E17" s="37" t="s">
-        <v>1368</v>
+        <v>1365</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="192" t="s">
-        <v>1369</v>
+        <v>1366</v>
       </c>
       <c r="B18" s="193"/>
       <c r="C18" s="193"/>
@@ -8450,16 +8459,16 @@
         <v>243</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>1372</v>
+        <v>1369</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>1370</v>
+        <v>1367</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>1253</v>
+        <v>1250</v>
       </c>
       <c r="E19" s="37" t="s">
-        <v>1371</v>
+        <v>1368</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="64" x14ac:dyDescent="0.2">
@@ -8467,10 +8476,10 @@
         <v>261</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>1373</v>
+        <v>1370</v>
       </c>
       <c r="C20" s="59" t="s">
-        <v>1384</v>
+        <v>1381</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="16" x14ac:dyDescent="0.2">
@@ -8478,13 +8487,13 @@
         <v>254</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>1374</v>
+        <v>1371</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>1328</v>
+        <v>1325</v>
       </c>
       <c r="E21" s="37" t="s">
-        <v>1329</v>
+        <v>1326</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="128" x14ac:dyDescent="0.2">
@@ -8492,10 +8501,10 @@
         <v>261</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>1375</v>
+        <v>1372</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>1385</v>
+        <v>1382</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
@@ -8519,7 +8528,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F6" sqref="F6"/>
+      <selection pane="bottomLeft" activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -8559,13 +8568,13 @@
         <v>7</v>
       </c>
       <c r="C2" s="101" t="s">
-        <v>1401</v>
+        <v>1408</v>
       </c>
       <c r="D2" s="99" t="s">
         <v>8</v>
       </c>
       <c r="E2" s="100" t="s">
-        <v>1401</v>
+        <v>1408</v>
       </c>
       <c r="F2" s="99"/>
     </row>
@@ -9636,18 +9645,18 @@
     </row>
     <row r="67" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="B67" s="1" t="s">
+        <v>1385</v>
+      </c>
+      <c r="C67" s="2" t="s">
+        <v>1386</v>
+      </c>
+      <c r="E67" s="40" t="s">
         <v>1388</v>
-      </c>
-      <c r="C67" s="2" t="s">
-        <v>1389</v>
-      </c>
-      <c r="E67" s="40" t="s">
-        <v>1391</v>
       </c>
     </row>
     <row r="68" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="B68" s="1" t="s">
-        <v>1390</v>
+        <v>1387</v>
       </c>
       <c r="C68" s="2" t="s">
         <v>76</v>
@@ -10410,11 +10419,11 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B63483B8-55BE-4CA0-9111-55E5C0AEF6CB}">
-  <dimension ref="A1:F343"/>
+  <dimension ref="A1:F344"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A55" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F61" sqref="F61"/>
+      <pane ySplit="1" topLeftCell="A194" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E203" sqref="E203"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -10449,13 +10458,13 @@
       </c>
     </row>
     <row r="2" spans="1:6" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="161" t="s">
+      <c r="A2" s="164" t="s">
         <v>374</v>
       </c>
-      <c r="B2" s="162"/>
-      <c r="C2" s="162"/>
-      <c r="D2" s="162"/>
-      <c r="E2" s="163"/>
+      <c r="B2" s="165"/>
+      <c r="C2" s="165"/>
+      <c r="D2" s="165"/>
+      <c r="E2" s="166"/>
       <c r="F2" s="33"/>
     </row>
     <row r="3" spans="1:6" ht="48" x14ac:dyDescent="0.2">
@@ -10583,13 +10592,13 @@
       <c r="F9" s="120"/>
     </row>
     <row r="10" spans="1:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="164" t="s">
+      <c r="A10" s="167" t="s">
         <v>403</v>
       </c>
-      <c r="B10" s="165"/>
-      <c r="C10" s="165"/>
-      <c r="D10" s="165"/>
-      <c r="E10" s="166"/>
+      <c r="B10" s="168"/>
+      <c r="C10" s="168"/>
+      <c r="D10" s="168"/>
+      <c r="E10" s="169"/>
       <c r="F10" s="120"/>
     </row>
     <row r="11" spans="1:6" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -10618,13 +10627,13 @@
         <v>408</v>
       </c>
       <c r="C12" s="154" t="s">
-        <v>1392</v>
+        <v>1389</v>
       </c>
       <c r="D12" s="85" t="s">
         <v>409</v>
       </c>
       <c r="E12" s="153" t="s">
-        <v>1393</v>
+        <v>1390</v>
       </c>
       <c r="F12" s="87"/>
     </row>
@@ -10636,13 +10645,13 @@
         <v>410</v>
       </c>
       <c r="C13" s="155" t="s">
-        <v>1394</v>
+        <v>1391</v>
       </c>
       <c r="D13" s="89" t="s">
         <v>411</v>
       </c>
       <c r="E13" s="156" t="s">
-        <v>1395</v>
+        <v>1392</v>
       </c>
       <c r="F13" s="87"/>
     </row>
@@ -11342,7 +11351,7 @@
         <v>530</v>
       </c>
       <c r="E60" s="121" t="s">
-        <v>1405</v>
+        <v>1401</v>
       </c>
       <c r="F60" s="120"/>
     </row>
@@ -11351,14 +11360,14 @@
         <v>527</v>
       </c>
       <c r="B61" s="117" t="s">
-        <v>1402</v>
+        <v>1398</v>
       </c>
       <c r="C61" s="118" t="s">
-        <v>1404</v>
+        <v>1400</v>
       </c>
       <c r="D61" s="117"/>
       <c r="E61" s="121" t="s">
-        <v>1403</v>
+        <v>1399</v>
       </c>
       <c r="F61" s="120"/>
     </row>
@@ -12544,7 +12553,7 @@
         <v>718</v>
       </c>
       <c r="C140" s="114" t="s">
-        <v>1377</v>
+        <v>1374</v>
       </c>
       <c r="D140" s="123" t="s">
         <v>719</v>
@@ -12634,7 +12643,7 @@
         <v>733</v>
       </c>
       <c r="C146" s="59" t="s">
-        <v>1376</v>
+        <v>1373</v>
       </c>
       <c r="D146" s="117" t="s">
         <v>734</v>
@@ -12665,14 +12674,14 @@
         <v>37</v>
       </c>
       <c r="B148" s="117" t="s">
-        <v>1378</v>
+        <v>1375</v>
       </c>
       <c r="C148" s="59" t="s">
-        <v>1380</v>
+        <v>1377</v>
       </c>
       <c r="D148" s="117"/>
       <c r="E148" s="121" t="s">
-        <v>1382</v>
+        <v>1379</v>
       </c>
       <c r="F148" s="120"/>
     </row>
@@ -12681,14 +12690,14 @@
         <v>37</v>
       </c>
       <c r="B149" s="117" t="s">
-        <v>1379</v>
+        <v>1376</v>
       </c>
       <c r="C149" s="59" t="s">
-        <v>1381</v>
+        <v>1378</v>
       </c>
       <c r="D149" s="117"/>
       <c r="E149" s="121" t="s">
-        <v>1383</v>
+        <v>1380</v>
       </c>
       <c r="F149" s="120"/>
     </row>
@@ -12907,13 +12916,13 @@
       <c r="F163" s="120"/>
     </row>
     <row r="164" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A164" s="167" t="s">
+      <c r="A164" s="161" t="s">
         <v>773</v>
       </c>
-      <c r="B164" s="168"/>
-      <c r="C164" s="168"/>
-      <c r="D164" s="168"/>
-      <c r="E164" s="169"/>
+      <c r="B164" s="162"/>
+      <c r="C164" s="162"/>
+      <c r="D164" s="162"/>
+      <c r="E164" s="163"/>
       <c r="F164" s="130" t="s">
         <v>774</v>
       </c>
@@ -13340,13 +13349,13 @@
         <v>823</v>
       </c>
       <c r="C192" s="59" t="s">
-        <v>1396</v>
+        <v>1393</v>
       </c>
       <c r="D192" s="117" t="s">
         <v>824</v>
       </c>
       <c r="E192" s="121" t="s">
-        <v>1400</v>
+        <v>1397</v>
       </c>
       <c r="F192" s="120"/>
     </row>
@@ -13355,14 +13364,14 @@
         <v>491</v>
       </c>
       <c r="B193" s="117" t="s">
-        <v>1397</v>
+        <v>1394</v>
       </c>
       <c r="C193" s="59" t="s">
-        <v>1398</v>
+        <v>1395</v>
       </c>
       <c r="D193" s="117"/>
       <c r="E193" s="121" t="s">
-        <v>1399</v>
+        <v>1396</v>
       </c>
       <c r="F193" s="120"/>
     </row>
@@ -13456,223 +13465,225 @@
     </row>
     <row r="200" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A200" s="117" t="s">
-        <v>742</v>
+        <v>740</v>
       </c>
       <c r="B200" s="117" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
       <c r="C200" s="118" t="s">
-        <v>43</v>
+        <v>1404</v>
       </c>
       <c r="D200" s="117"/>
       <c r="E200" s="121" t="s">
+        <v>1407</v>
+      </c>
+      <c r="F200" s="120"/>
+    </row>
+    <row r="201" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A201" s="117" t="s">
+        <v>742</v>
+      </c>
+      <c r="B201" s="117" t="s">
+        <v>1406</v>
+      </c>
+      <c r="C201" s="118" t="s">
+        <v>43</v>
+      </c>
+      <c r="D201" s="117"/>
+      <c r="E201" s="121" t="s">
         <v>45</v>
       </c>
-      <c r="F200" s="120"/>
-    </row>
-    <row r="201" spans="1:6" ht="32" x14ac:dyDescent="0.2">
-      <c r="A201" s="117" t="s">
+      <c r="F201" s="120"/>
+    </row>
+    <row r="202" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+      <c r="A202" s="117" t="s">
         <v>32</v>
       </c>
-      <c r="B201" s="117" t="s">
-        <v>837</v>
-      </c>
-      <c r="C201" s="135" t="s">
-        <v>838</v>
-      </c>
-      <c r="D201" s="117"/>
-      <c r="E201" s="121"/>
-      <c r="F201" s="120"/>
-    </row>
-    <row r="202" spans="1:6" ht="48" x14ac:dyDescent="0.2">
-      <c r="A202" s="117" t="s">
+      <c r="B202" s="117" t="s">
+        <v>1405</v>
+      </c>
+      <c r="C202" s="135" t="s">
+        <v>1402</v>
+      </c>
+      <c r="D202" s="117"/>
+      <c r="E202" s="121" t="s">
+        <v>1403</v>
+      </c>
+      <c r="F202" s="120"/>
+    </row>
+    <row r="203" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+      <c r="A203" s="117" t="s">
         <v>417</v>
       </c>
-      <c r="B202" s="117" t="s">
-        <v>839</v>
-      </c>
-      <c r="C202" s="121"/>
-      <c r="D202" s="20" t="s">
-        <v>745</v>
-      </c>
-      <c r="E202" s="121"/>
-      <c r="F202" s="120"/>
-    </row>
-    <row r="203" spans="1:6" ht="64" x14ac:dyDescent="0.2">
-      <c r="A203" s="117" t="s">
-        <v>420</v>
-      </c>
       <c r="B203" s="117" t="s">
-        <v>840</v>
+        <v>836</v>
       </c>
       <c r="C203" s="121"/>
       <c r="D203" s="20" t="s">
-        <v>747</v>
+        <v>745</v>
       </c>
       <c r="E203" s="121"/>
       <c r="F203" s="120"/>
     </row>
-    <row r="204" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+    <row r="204" spans="1:6" ht="64" x14ac:dyDescent="0.2">
       <c r="A204" s="117" t="s">
-        <v>417</v>
+        <v>420</v>
       </c>
       <c r="B204" s="117" t="s">
-        <v>841</v>
+        <v>837</v>
       </c>
       <c r="C204" s="121"/>
       <c r="D204" s="20" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="E204" s="121"/>
       <c r="F204" s="120"/>
     </row>
-    <row r="205" spans="1:6" ht="64" x14ac:dyDescent="0.2">
+    <row r="205" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A205" s="117" t="s">
-        <v>420</v>
+        <v>417</v>
       </c>
       <c r="B205" s="117" t="s">
-        <v>842</v>
+        <v>838</v>
       </c>
       <c r="C205" s="121"/>
       <c r="D205" s="20" t="s">
-        <v>752</v>
+        <v>749</v>
       </c>
       <c r="E205" s="121"/>
       <c r="F205" s="120"/>
     </row>
-    <row r="206" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A206" s="158" t="s">
+    <row r="206" spans="1:6" ht="64" x14ac:dyDescent="0.2">
+      <c r="A206" s="117" t="s">
+        <v>420</v>
+      </c>
+      <c r="B206" s="117" t="s">
+        <v>839</v>
+      </c>
+      <c r="C206" s="121"/>
+      <c r="D206" s="20" t="s">
+        <v>752</v>
+      </c>
+      <c r="E206" s="121"/>
+      <c r="F206" s="120"/>
+    </row>
+    <row r="207" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A207" s="158" t="s">
+        <v>840</v>
+      </c>
+      <c r="B207" s="159"/>
+      <c r="C207" s="159"/>
+      <c r="D207" s="159"/>
+      <c r="E207" s="160"/>
+      <c r="F207" s="120"/>
+    </row>
+    <row r="208" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+      <c r="A208" s="117" t="s">
+        <v>243</v>
+      </c>
+      <c r="B208" s="117" t="s">
+        <v>841</v>
+      </c>
+      <c r="C208" s="118" t="s">
+        <v>842</v>
+      </c>
+      <c r="D208" s="117" t="s">
         <v>843</v>
       </c>
-      <c r="B206" s="159"/>
-      <c r="C206" s="159"/>
-      <c r="D206" s="159"/>
-      <c r="E206" s="160"/>
-      <c r="F206" s="120"/>
-    </row>
-    <row r="207" spans="1:6" ht="48" x14ac:dyDescent="0.2">
-      <c r="A207" s="117" t="s">
-        <v>243</v>
-      </c>
-      <c r="B207" s="117" t="s">
+      <c r="E208" s="121" t="s">
+        <v>54</v>
+      </c>
+      <c r="F208" s="120"/>
+    </row>
+    <row r="209" spans="1:6" ht="64" x14ac:dyDescent="0.2">
+      <c r="A209" s="117" t="s">
+        <v>261</v>
+      </c>
+      <c r="B209" s="117" t="s">
         <v>844</v>
       </c>
-      <c r="C207" s="118" t="s">
+      <c r="C209" s="118" t="s">
+        <v>759</v>
+      </c>
+      <c r="D209" s="126" t="s">
         <v>845</v>
       </c>
-      <c r="D207" s="117" t="s">
-        <v>846</v>
-      </c>
-      <c r="E207" s="121" t="s">
-        <v>54</v>
-      </c>
-      <c r="F207" s="120"/>
-    </row>
-    <row r="208" spans="1:6" ht="64" x14ac:dyDescent="0.2">
-      <c r="A208" s="117" t="s">
-        <v>261</v>
-      </c>
-      <c r="B208" s="117" t="s">
-        <v>847</v>
-      </c>
-      <c r="C208" s="118" t="s">
-        <v>759</v>
-      </c>
-      <c r="D208" s="126" t="s">
-        <v>848</v>
-      </c>
-      <c r="E208" s="121" t="s">
+      <c r="E209" s="121" t="s">
         <v>761</v>
-      </c>
-      <c r="F208" s="120"/>
-    </row>
-    <row r="209" spans="1:6" ht="48" x14ac:dyDescent="0.2">
-      <c r="A209" s="117" t="s">
-        <v>32</v>
-      </c>
-      <c r="B209" s="117" t="s">
-        <v>849</v>
-      </c>
-      <c r="C209" s="118" t="s">
-        <v>763</v>
-      </c>
-      <c r="D209" s="126" t="s">
-        <v>850</v>
-      </c>
-      <c r="E209" s="121" t="s">
-        <v>765</v>
       </c>
       <c r="F209" s="120"/>
     </row>
     <row r="210" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A210" s="117" t="s">
+        <v>32</v>
+      </c>
+      <c r="B210" s="117" t="s">
+        <v>846</v>
+      </c>
+      <c r="C210" s="118" t="s">
+        <v>763</v>
+      </c>
+      <c r="D210" s="126" t="s">
+        <v>847</v>
+      </c>
+      <c r="E210" s="121" t="s">
+        <v>765</v>
+      </c>
+      <c r="F210" s="120"/>
+    </row>
+    <row r="211" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+      <c r="A211" s="117" t="s">
         <v>417</v>
       </c>
-      <c r="B210" s="117" t="s">
-        <v>851</v>
-      </c>
-      <c r="C210" s="129"/>
-      <c r="D210" s="20" t="s">
+      <c r="B211" s="117" t="s">
+        <v>848</v>
+      </c>
+      <c r="C211" s="129"/>
+      <c r="D211" s="20" t="s">
         <v>770</v>
-      </c>
-      <c r="E210" s="121"/>
-      <c r="F210" s="120"/>
-    </row>
-    <row r="211" spans="1:6" ht="64" x14ac:dyDescent="0.2">
-      <c r="A211" s="117" t="s">
-        <v>420</v>
-      </c>
-      <c r="B211" s="117" t="s">
-        <v>852</v>
-      </c>
-      <c r="C211" s="121"/>
-      <c r="D211" s="20" t="s">
-        <v>772</v>
       </c>
       <c r="E211" s="121"/>
       <c r="F211" s="120"/>
     </row>
-    <row r="212" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A212" s="158" t="s">
+    <row r="212" spans="1:6" ht="64" x14ac:dyDescent="0.2">
+      <c r="A212" s="117" t="s">
+        <v>420</v>
+      </c>
+      <c r="B212" s="117" t="s">
+        <v>849</v>
+      </c>
+      <c r="C212" s="121"/>
+      <c r="D212" s="20" t="s">
+        <v>772</v>
+      </c>
+      <c r="E212" s="121"/>
+      <c r="F212" s="120"/>
+    </row>
+    <row r="213" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A213" s="158" t="s">
+        <v>850</v>
+      </c>
+      <c r="B213" s="159"/>
+      <c r="C213" s="159"/>
+      <c r="D213" s="159"/>
+      <c r="E213" s="160"/>
+      <c r="F213" s="120"/>
+    </row>
+    <row r="214" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+      <c r="A214" s="117" t="s">
+        <v>243</v>
+      </c>
+      <c r="B214" s="117" t="s">
+        <v>851</v>
+      </c>
+      <c r="C214" s="118" t="s">
+        <v>852</v>
+      </c>
+      <c r="D214" s="117" t="s">
         <v>853</v>
       </c>
-      <c r="B212" s="159"/>
-      <c r="C212" s="159"/>
-      <c r="D212" s="159"/>
-      <c r="E212" s="160"/>
-      <c r="F212" s="120"/>
-    </row>
-    <row r="213" spans="1:6" ht="32" x14ac:dyDescent="0.2">
-      <c r="A213" s="117" t="s">
-        <v>243</v>
-      </c>
-      <c r="B213" s="117" t="s">
+      <c r="E214" s="121" t="s">
         <v>854</v>
-      </c>
-      <c r="C213" s="118" t="s">
-        <v>855</v>
-      </c>
-      <c r="D213" s="117" t="s">
-        <v>856</v>
-      </c>
-      <c r="E213" s="121" t="s">
-        <v>857</v>
-      </c>
-      <c r="F213" s="120"/>
-    </row>
-    <row r="214" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A214" s="117" t="s">
-        <v>423</v>
-      </c>
-      <c r="B214" s="117" t="s">
-        <v>858</v>
-      </c>
-      <c r="C214" s="118" t="s">
-        <v>56</v>
-      </c>
-      <c r="D214" s="117"/>
-      <c r="E214" s="121" t="s">
-        <v>58</v>
       </c>
       <c r="F214" s="120"/>
     </row>
@@ -13681,14 +13692,14 @@
         <v>423</v>
       </c>
       <c r="B215" s="117" t="s">
-        <v>859</v>
+        <v>855</v>
       </c>
       <c r="C215" s="118" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="D215" s="117"/>
       <c r="E215" s="121" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="F215" s="120"/>
     </row>
@@ -13697,14 +13708,14 @@
         <v>423</v>
       </c>
       <c r="B216" s="117" t="s">
-        <v>860</v>
+        <v>856</v>
       </c>
       <c r="C216" s="118" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="D216" s="117"/>
       <c r="E216" s="121" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="F216" s="120"/>
     </row>
@@ -13713,14 +13724,14 @@
         <v>423</v>
       </c>
       <c r="B217" s="117" t="s">
-        <v>861</v>
+        <v>857</v>
       </c>
       <c r="C217" s="118" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="D217" s="117"/>
       <c r="E217" s="121" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="F217" s="120"/>
     </row>
@@ -13729,154 +13740,152 @@
         <v>423</v>
       </c>
       <c r="B218" s="117" t="s">
-        <v>862</v>
+        <v>858</v>
       </c>
       <c r="C218" s="118" t="s">
-        <v>39</v>
+        <v>68</v>
       </c>
       <c r="D218" s="117"/>
       <c r="E218" s="121" t="s">
+        <v>70</v>
+      </c>
+      <c r="F218" s="120"/>
+    </row>
+    <row r="219" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A219" s="117" t="s">
+        <v>423</v>
+      </c>
+      <c r="B219" s="117" t="s">
+        <v>859</v>
+      </c>
+      <c r="C219" s="118" t="s">
+        <v>39</v>
+      </c>
+      <c r="D219" s="117"/>
+      <c r="E219" s="121" t="s">
         <v>41</v>
       </c>
-      <c r="F218" s="120"/>
-    </row>
-    <row r="219" spans="1:6" ht="64" x14ac:dyDescent="0.2">
-      <c r="A219" s="117" t="s">
-        <v>417</v>
-      </c>
-      <c r="B219" s="117" t="s">
-        <v>863</v>
-      </c>
-      <c r="C219" s="121"/>
-      <c r="D219" s="20" t="s">
-        <v>799</v>
-      </c>
-      <c r="E219" s="121"/>
       <c r="F219" s="120"/>
     </row>
     <row r="220" spans="1:6" ht="64" x14ac:dyDescent="0.2">
       <c r="A220" s="117" t="s">
-        <v>420</v>
+        <v>417</v>
       </c>
       <c r="B220" s="117" t="s">
-        <v>864</v>
+        <v>860</v>
       </c>
       <c r="C220" s="121"/>
       <c r="D220" s="20" t="s">
-        <v>801</v>
+        <v>799</v>
       </c>
       <c r="E220" s="121"/>
       <c r="F220" s="120"/>
     </row>
-    <row r="221" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+    <row r="221" spans="1:6" ht="64" x14ac:dyDescent="0.2">
       <c r="A221" s="117" t="s">
-        <v>417</v>
+        <v>420</v>
       </c>
       <c r="B221" s="117" t="s">
-        <v>865</v>
+        <v>861</v>
       </c>
       <c r="C221" s="121"/>
       <c r="D221" s="20" t="s">
-        <v>803</v>
+        <v>801</v>
       </c>
       <c r="E221" s="121"/>
       <c r="F221" s="120"/>
     </row>
-    <row r="222" spans="1:6" ht="64" x14ac:dyDescent="0.2">
+    <row r="222" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A222" s="117" t="s">
-        <v>420</v>
+        <v>417</v>
       </c>
       <c r="B222" s="117" t="s">
-        <v>866</v>
+        <v>862</v>
       </c>
       <c r="C222" s="121"/>
       <c r="D222" s="20" t="s">
-        <v>805</v>
+        <v>803</v>
       </c>
       <c r="E222" s="121"/>
       <c r="F222" s="120"/>
     </row>
-    <row r="223" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A223" s="158" t="s">
-        <v>867</v>
-      </c>
-      <c r="B223" s="159"/>
-      <c r="C223" s="159"/>
-      <c r="D223" s="159"/>
-      <c r="E223" s="160"/>
+    <row r="223" spans="1:6" ht="64" x14ac:dyDescent="0.2">
+      <c r="A223" s="117" t="s">
+        <v>420</v>
+      </c>
+      <c r="B223" s="117" t="s">
+        <v>863</v>
+      </c>
+      <c r="C223" s="121"/>
+      <c r="D223" s="20" t="s">
+        <v>805</v>
+      </c>
+      <c r="E223" s="121"/>
       <c r="F223" s="120"/>
     </row>
-    <row r="224" spans="1:6" ht="48" x14ac:dyDescent="0.2">
-      <c r="A224" s="117" t="s">
-        <v>243</v>
-      </c>
-      <c r="B224" s="117" t="s">
-        <v>868</v>
-      </c>
-      <c r="C224" s="118" t="s">
-        <v>869</v>
-      </c>
-      <c r="D224" s="117" t="s">
-        <v>870</v>
-      </c>
-      <c r="E224" s="121" t="s">
-        <v>871</v>
-      </c>
-      <c r="F224" s="38" t="s">
-        <v>872</v>
-      </c>
+    <row r="224" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A224" s="158" t="s">
+        <v>864</v>
+      </c>
+      <c r="B224" s="159"/>
+      <c r="C224" s="159"/>
+      <c r="D224" s="159"/>
+      <c r="E224" s="160"/>
+      <c r="F224" s="120"/>
     </row>
     <row r="225" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A225" s="117" t="s">
+        <v>243</v>
+      </c>
+      <c r="B225" s="117" t="s">
+        <v>865</v>
+      </c>
+      <c r="C225" s="118" t="s">
+        <v>866</v>
+      </c>
+      <c r="D225" s="117" t="s">
+        <v>867</v>
+      </c>
+      <c r="E225" s="121" t="s">
+        <v>868</v>
+      </c>
+      <c r="F225" s="38" t="s">
+        <v>869</v>
+      </c>
+    </row>
+    <row r="226" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+      <c r="A226" s="117" t="s">
         <v>375</v>
       </c>
-      <c r="B225" s="117" t="s">
+      <c r="B226" s="117" t="s">
+        <v>870</v>
+      </c>
+      <c r="C226" s="118" t="s">
+        <v>871</v>
+      </c>
+      <c r="D226" s="117" t="s">
+        <v>872</v>
+      </c>
+      <c r="E226" s="121" t="s">
         <v>873</v>
       </c>
-      <c r="C225" s="118" t="s">
+      <c r="F226" s="120"/>
+    </row>
+    <row r="227" spans="1:6" ht="64" x14ac:dyDescent="0.2">
+      <c r="A227" s="117" t="s">
+        <v>261</v>
+      </c>
+      <c r="B227" s="117" t="s">
         <v>874</v>
       </c>
-      <c r="D225" s="117" t="s">
+      <c r="C227" s="59" t="s">
         <v>875</v>
       </c>
-      <c r="E225" s="121" t="s">
+      <c r="D227" s="117" t="s">
         <v>876</v>
       </c>
-      <c r="F225" s="120"/>
-    </row>
-    <row r="226" spans="1:6" ht="64" x14ac:dyDescent="0.2">
-      <c r="A226" s="117" t="s">
-        <v>261</v>
-      </c>
-      <c r="B226" s="117" t="s">
+      <c r="E227" s="121" t="s">
         <v>877</v>
-      </c>
-      <c r="C226" s="59" t="s">
-        <v>878</v>
-      </c>
-      <c r="D226" s="117" t="s">
-        <v>879</v>
-      </c>
-      <c r="E226" s="121" t="s">
-        <v>880</v>
-      </c>
-      <c r="F226" s="120"/>
-    </row>
-    <row r="227" spans="1:6" ht="32" x14ac:dyDescent="0.2">
-      <c r="A227" s="117" t="s">
-        <v>389</v>
-      </c>
-      <c r="B227" s="117" t="s">
-        <v>881</v>
-      </c>
-      <c r="C227" s="118" t="s">
-        <v>882</v>
-      </c>
-      <c r="D227" s="122" t="s">
-        <v>883</v>
-      </c>
-      <c r="E227" s="121" t="s">
-        <v>884</v>
       </c>
       <c r="F227" s="120"/>
     </row>
@@ -13885,16 +13894,16 @@
         <v>389</v>
       </c>
       <c r="B228" s="117" t="s">
-        <v>885</v>
+        <v>878</v>
       </c>
       <c r="C228" s="118" t="s">
-        <v>391</v>
+        <v>879</v>
       </c>
       <c r="D228" s="122" t="s">
-        <v>886</v>
+        <v>880</v>
       </c>
       <c r="E228" s="121" t="s">
-        <v>393</v>
+        <v>881</v>
       </c>
       <c r="F228" s="120"/>
     </row>
@@ -13903,163 +13912,174 @@
         <v>389</v>
       </c>
       <c r="B229" s="117" t="s">
-        <v>887</v>
+        <v>882</v>
       </c>
       <c r="C229" s="118" t="s">
-        <v>888</v>
+        <v>391</v>
       </c>
       <c r="D229" s="122" t="s">
-        <v>889</v>
+        <v>883</v>
       </c>
       <c r="E229" s="121" t="s">
-        <v>890</v>
+        <v>393</v>
       </c>
       <c r="F229" s="120"/>
     </row>
-    <row r="230" spans="1:6" ht="64" x14ac:dyDescent="0.2">
+    <row r="230" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A230" s="117" t="s">
         <v>389</v>
       </c>
       <c r="B230" s="117" t="s">
-        <v>891</v>
+        <v>884</v>
       </c>
       <c r="C230" s="118" t="s">
-        <v>892</v>
+        <v>885</v>
       </c>
       <c r="D230" s="122" t="s">
-        <v>893</v>
+        <v>886</v>
       </c>
       <c r="E230" s="121" t="s">
-        <v>894</v>
+        <v>887</v>
       </c>
       <c r="F230" s="120"/>
     </row>
-    <row r="231" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+    <row r="231" spans="1:6" ht="64" x14ac:dyDescent="0.2">
       <c r="A231" s="117" t="s">
         <v>389</v>
       </c>
       <c r="B231" s="117" t="s">
-        <v>895</v>
+        <v>888</v>
       </c>
       <c r="C231" s="118" t="s">
-        <v>896</v>
+        <v>889</v>
       </c>
       <c r="D231" s="122" t="s">
-        <v>897</v>
+        <v>890</v>
       </c>
       <c r="E231" s="121" t="s">
-        <v>898</v>
+        <v>891</v>
       </c>
       <c r="F231" s="120"/>
     </row>
     <row r="232" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A232" s="117" t="s">
+        <v>389</v>
+      </c>
+      <c r="B232" s="117" t="s">
+        <v>892</v>
+      </c>
+      <c r="C232" s="118" t="s">
+        <v>893</v>
+      </c>
+      <c r="D232" s="122" t="s">
+        <v>894</v>
+      </c>
+      <c r="E232" s="121" t="s">
+        <v>895</v>
+      </c>
+      <c r="F232" s="120"/>
+    </row>
+    <row r="233" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+      <c r="A233" s="117" t="s">
         <v>498</v>
       </c>
-      <c r="B232" s="117" t="s">
-        <v>899</v>
-      </c>
-      <c r="C232" s="118" t="s">
-        <v>900</v>
-      </c>
-      <c r="D232" s="122" t="s">
+      <c r="B233" s="117" t="s">
+        <v>896</v>
+      </c>
+      <c r="C233" s="118" t="s">
         <v>897</v>
       </c>
-      <c r="E232" s="121" t="s">
-        <v>901</v>
-      </c>
-      <c r="F232" s="120"/>
-    </row>
-    <row r="233" spans="1:6" ht="48" x14ac:dyDescent="0.2">
-      <c r="A233" s="117" t="s">
-        <v>389</v>
-      </c>
-      <c r="B233" s="117" t="s">
-        <v>902</v>
-      </c>
-      <c r="C233" s="118" t="s">
-        <v>903</v>
-      </c>
       <c r="D233" s="122" t="s">
-        <v>904</v>
+        <v>894</v>
       </c>
       <c r="E233" s="121" t="s">
-        <v>905</v>
+        <v>898</v>
       </c>
       <c r="F233" s="120"/>
     </row>
-    <row r="234" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+    <row r="234" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A234" s="117" t="s">
         <v>389</v>
       </c>
       <c r="B234" s="117" t="s">
-        <v>906</v>
+        <v>899</v>
       </c>
       <c r="C234" s="118" t="s">
-        <v>323</v>
+        <v>900</v>
       </c>
       <c r="D234" s="122" t="s">
-        <v>907</v>
+        <v>901</v>
       </c>
       <c r="E234" s="121" t="s">
-        <v>325</v>
+        <v>902</v>
       </c>
       <c r="F234" s="120"/>
     </row>
-    <row r="235" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+    <row r="235" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A235" s="117" t="s">
         <v>389</v>
       </c>
       <c r="B235" s="117" t="s">
-        <v>908</v>
+        <v>903</v>
       </c>
       <c r="C235" s="118" t="s">
-        <v>909</v>
+        <v>323</v>
       </c>
       <c r="D235" s="122" t="s">
-        <v>910</v>
+        <v>904</v>
       </c>
       <c r="E235" s="121" t="s">
-        <v>911</v>
+        <v>325</v>
       </c>
       <c r="F235" s="120"/>
     </row>
-    <row r="236" spans="1:6" ht="96" x14ac:dyDescent="0.2">
+    <row r="236" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A236" s="117" t="s">
         <v>389</v>
       </c>
       <c r="B236" s="117" t="s">
+        <v>905</v>
+      </c>
+      <c r="C236" s="118" t="s">
+        <v>906</v>
+      </c>
+      <c r="D236" s="122" t="s">
+        <v>907</v>
+      </c>
+      <c r="E236" s="121" t="s">
+        <v>908</v>
+      </c>
+      <c r="F236" s="120"/>
+    </row>
+    <row r="237" spans="1:6" ht="96" x14ac:dyDescent="0.2">
+      <c r="A237" s="117" t="s">
+        <v>389</v>
+      </c>
+      <c r="B237" s="117" t="s">
+        <v>909</v>
+      </c>
+      <c r="C237" s="118" t="s">
+        <v>910</v>
+      </c>
+      <c r="D237" s="122" t="s">
+        <v>911</v>
+      </c>
+      <c r="E237" s="121" t="s">
         <v>912</v>
       </c>
-      <c r="C236" s="118" t="s">
-        <v>913</v>
-      </c>
-      <c r="D236" s="122" t="s">
-        <v>914</v>
-      </c>
-      <c r="E236" s="121" t="s">
-        <v>915</v>
-      </c>
-      <c r="F236" s="120"/>
-    </row>
-    <row r="237" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A237" s="5"/>
-      <c r="B237" s="5"/>
-      <c r="C237" s="6" t="s">
-        <v>916</v>
-      </c>
-      <c r="D237" s="5"/>
-      <c r="E237" s="37"/>
-      <c r="F237" s="68" t="s">
-        <v>917</v>
-      </c>
-    </row>
-    <row r="238" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F237" s="120"/>
+    </row>
+    <row r="238" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A238" s="5"/>
       <c r="B238" s="5"/>
-      <c r="C238" s="6"/>
+      <c r="C238" s="6" t="s">
+        <v>913</v>
+      </c>
       <c r="D238" s="5"/>
       <c r="E238" s="37"/>
+      <c r="F238" s="68" t="s">
+        <v>914</v>
+      </c>
     </row>
     <row r="239" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A239" s="5"/>
@@ -14796,8 +14816,27 @@
       <c r="D343" s="5"/>
       <c r="E343" s="37"/>
     </row>
+    <row r="344" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A344" s="5"/>
+      <c r="B344" s="5"/>
+      <c r="C344" s="6"/>
+      <c r="D344" s="5"/>
+      <c r="E344" s="37"/>
+    </row>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="A224:E224"/>
+    <mergeCell ref="A185:E185"/>
+    <mergeCell ref="A189:E189"/>
+    <mergeCell ref="A196:E196"/>
+    <mergeCell ref="A207:E207"/>
+    <mergeCell ref="A213:E213"/>
+    <mergeCell ref="A57:E57"/>
+    <mergeCell ref="A2:E2"/>
+    <mergeCell ref="A10:E10"/>
+    <mergeCell ref="A14:E14"/>
+    <mergeCell ref="A24:E24"/>
+    <mergeCell ref="A43:E43"/>
     <mergeCell ref="A173:E173"/>
     <mergeCell ref="A156:E156"/>
     <mergeCell ref="A62:E62"/>
@@ -14808,18 +14847,6 @@
     <mergeCell ref="A145:E145"/>
     <mergeCell ref="A91:E91"/>
     <mergeCell ref="A164:E164"/>
-    <mergeCell ref="A57:E57"/>
-    <mergeCell ref="A2:E2"/>
-    <mergeCell ref="A10:E10"/>
-    <mergeCell ref="A14:E14"/>
-    <mergeCell ref="A24:E24"/>
-    <mergeCell ref="A43:E43"/>
-    <mergeCell ref="A223:E223"/>
-    <mergeCell ref="A185:E185"/>
-    <mergeCell ref="A189:E189"/>
-    <mergeCell ref="A196:E196"/>
-    <mergeCell ref="A206:E206"/>
-    <mergeCell ref="A212:E212"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -14830,7 +14857,7 @@
   <dimension ref="A1:F54"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A43" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
@@ -14867,7 +14894,7 @@
     </row>
     <row r="2" spans="1:6" s="24" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="173" t="s">
-        <v>918</v>
+        <v>915</v>
       </c>
       <c r="B2" s="174"/>
       <c r="C2" s="174"/>
@@ -14879,28 +14906,28 @@
         <v>243</v>
       </c>
       <c r="B3" s="19" t="s">
-        <v>919</v>
+        <v>916</v>
       </c>
       <c r="C3" s="21" t="s">
-        <v>920</v>
+        <v>917</v>
       </c>
       <c r="D3" s="5"/>
       <c r="E3" s="46" t="s">
-        <v>921</v>
+        <v>918</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="19" t="s">
-        <v>922</v>
+        <v>919</v>
       </c>
       <c r="B4" s="19" t="s">
-        <v>919</v>
+        <v>916</v>
       </c>
       <c r="C4" s="21" t="s">
-        <v>923</v>
+        <v>920</v>
       </c>
       <c r="E4" s="46" t="s">
-        <v>924</v>
+        <v>921</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="16" x14ac:dyDescent="0.2">
@@ -14908,27 +14935,27 @@
         <v>740</v>
       </c>
       <c r="B5" s="19" t="s">
-        <v>925</v>
+        <v>922</v>
       </c>
       <c r="C5" s="21" t="s">
-        <v>874</v>
+        <v>871</v>
       </c>
       <c r="E5" s="46" t="s">
-        <v>876</v>
+        <v>873</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="19" t="s">
-        <v>922</v>
+        <v>919</v>
       </c>
       <c r="B6" s="19" t="s">
-        <v>919</v>
+        <v>916</v>
       </c>
       <c r="C6" s="21" t="s">
-        <v>926</v>
+        <v>923</v>
       </c>
       <c r="E6" s="46" t="s">
-        <v>927</v>
+        <v>924</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="16" x14ac:dyDescent="0.2">
@@ -14936,30 +14963,30 @@
         <v>740</v>
       </c>
       <c r="B7" s="19" t="s">
-        <v>928</v>
+        <v>925</v>
       </c>
       <c r="C7" s="21" t="s">
-        <v>929</v>
+        <v>926</v>
       </c>
       <c r="E7" s="46" t="s">
-        <v>930</v>
+        <v>927</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="92" t="s">
-        <v>922</v>
+        <v>919</v>
       </c>
       <c r="B8" s="93" t="s">
-        <v>931</v>
+        <v>928</v>
       </c>
       <c r="C8" s="94" t="s">
-        <v>932</v>
+        <v>929</v>
       </c>
       <c r="D8" s="93" t="s">
         <v>411</v>
       </c>
       <c r="E8" s="86" t="s">
-        <v>933</v>
+        <v>930</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="16" x14ac:dyDescent="0.2">
@@ -14967,22 +14994,22 @@
         <v>740</v>
       </c>
       <c r="B9" s="28" t="s">
-        <v>934</v>
+        <v>931</v>
       </c>
       <c r="C9" s="27" t="s">
-        <v>935</v>
+        <v>932</v>
       </c>
       <c r="D9" s="18"/>
       <c r="E9" s="46" t="s">
-        <v>936</v>
+        <v>933</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="19" t="s">
-        <v>937</v>
+        <v>934</v>
       </c>
       <c r="B10" s="19" t="s">
-        <v>938</v>
+        <v>935</v>
       </c>
       <c r="C10" s="21" t="s">
         <v>152</v>
@@ -14993,10 +15020,10 @@
     </row>
     <row r="11" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="19" t="s">
-        <v>937</v>
+        <v>934</v>
       </c>
       <c r="B11" s="19" t="s">
-        <v>939</v>
+        <v>936</v>
       </c>
       <c r="C11" s="21" t="s">
         <v>140</v>
@@ -15007,7 +15034,7 @@
     </row>
     <row r="12" spans="1:6" s="24" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="173" t="s">
-        <v>940</v>
+        <v>937</v>
       </c>
       <c r="B12" s="174"/>
       <c r="C12" s="174"/>
@@ -15019,16 +15046,16 @@
         <v>243</v>
       </c>
       <c r="B13" s="19" t="s">
+        <v>938</v>
+      </c>
+      <c r="C13" s="21" t="s">
+        <v>939</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>940</v>
+      </c>
+      <c r="E13" s="46" t="s">
         <v>941</v>
-      </c>
-      <c r="C13" s="21" t="s">
-        <v>942</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>943</v>
-      </c>
-      <c r="E13" s="46" t="s">
-        <v>944</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="32" x14ac:dyDescent="0.2">
@@ -15036,16 +15063,16 @@
         <v>84</v>
       </c>
       <c r="B14" s="19" t="s">
+        <v>942</v>
+      </c>
+      <c r="C14" s="21" t="s">
+        <v>943</v>
+      </c>
+      <c r="D14" s="19" t="s">
+        <v>944</v>
+      </c>
+      <c r="E14" s="46" t="s">
         <v>945</v>
-      </c>
-      <c r="C14" s="21" t="s">
-        <v>946</v>
-      </c>
-      <c r="D14" s="19" t="s">
-        <v>947</v>
-      </c>
-      <c r="E14" s="46" t="s">
-        <v>948</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="32" x14ac:dyDescent="0.2">
@@ -15053,16 +15080,16 @@
         <v>84</v>
       </c>
       <c r="B15" s="19" t="s">
-        <v>949</v>
+        <v>946</v>
       </c>
       <c r="C15" s="21" t="s">
-        <v>950</v>
+        <v>947</v>
       </c>
       <c r="D15" s="19" t="s">
-        <v>947</v>
+        <v>944</v>
       </c>
       <c r="E15" s="46" t="s">
-        <v>951</v>
+        <v>948</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="16" x14ac:dyDescent="0.2">
@@ -15070,16 +15097,16 @@
         <v>84</v>
       </c>
       <c r="B16" s="19" t="s">
-        <v>952</v>
+        <v>949</v>
       </c>
       <c r="C16" s="21" t="s">
-        <v>953</v>
+        <v>950</v>
       </c>
       <c r="D16" s="19" t="s">
-        <v>947</v>
+        <v>944</v>
       </c>
       <c r="E16" s="46" t="s">
-        <v>954</v>
+        <v>951</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="48" x14ac:dyDescent="0.2">
@@ -15087,16 +15114,16 @@
         <v>84</v>
       </c>
       <c r="B17" s="93" t="s">
-        <v>955</v>
+        <v>952</v>
       </c>
       <c r="C17" s="152" t="s">
-        <v>1386</v>
+        <v>1383</v>
       </c>
       <c r="D17" s="93" t="s">
-        <v>947</v>
+        <v>944</v>
       </c>
       <c r="E17" s="153" t="s">
-        <v>1387</v>
+        <v>1384</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="80" x14ac:dyDescent="0.2">
@@ -15104,11 +15131,11 @@
         <v>417</v>
       </c>
       <c r="B18" s="28" t="s">
-        <v>956</v>
+        <v>953</v>
       </c>
       <c r="C18" s="27"/>
       <c r="D18" s="18" t="s">
-        <v>957</v>
+        <v>954</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="80" x14ac:dyDescent="0.2">
@@ -15116,16 +15143,16 @@
         <v>420</v>
       </c>
       <c r="B19" s="28" t="s">
-        <v>958</v>
+        <v>955</v>
       </c>
       <c r="C19" s="27"/>
       <c r="D19" s="18" t="s">
-        <v>959</v>
+        <v>956</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="182" t="s">
-        <v>960</v>
+        <v>957</v>
       </c>
       <c r="B20" s="183"/>
       <c r="C20" s="183"/>
@@ -15134,52 +15161,52 @@
     </row>
     <row r="21" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A21" s="5" t="s">
-        <v>961</v>
+        <v>958</v>
       </c>
       <c r="B21" s="92" t="s">
-        <v>962</v>
+        <v>959</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>963</v>
+        <v>960</v>
       </c>
       <c r="D21" s="81"/>
       <c r="E21" s="82" t="s">
-        <v>964</v>
+        <v>961</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A22" s="81" t="s">
-        <v>965</v>
+        <v>962</v>
       </c>
       <c r="B22" s="95" t="s">
-        <v>966</v>
+        <v>963</v>
       </c>
       <c r="C22" s="83" t="s">
-        <v>967</v>
+        <v>964</v>
       </c>
       <c r="D22" s="81"/>
       <c r="E22" s="82" t="s">
-        <v>968</v>
+        <v>965</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="64" x14ac:dyDescent="0.2">
       <c r="A23" s="81" t="s">
-        <v>969</v>
+        <v>966</v>
       </c>
       <c r="B23" s="95" t="s">
-        <v>970</v>
+        <v>967</v>
       </c>
       <c r="C23" s="83" t="s">
-        <v>971</v>
+        <v>968</v>
       </c>
       <c r="D23" s="81"/>
       <c r="E23" s="82" t="s">
-        <v>972</v>
+        <v>969</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" s="179" t="s">
-        <v>973</v>
+        <v>970</v>
       </c>
       <c r="B24" s="180"/>
       <c r="C24" s="180"/>
@@ -15191,19 +15218,19 @@
         <v>243</v>
       </c>
       <c r="B25" s="28" t="s">
-        <v>974</v>
+        <v>971</v>
       </c>
       <c r="C25" s="27" t="s">
-        <v>975</v>
+        <v>972</v>
       </c>
       <c r="D25" s="18"/>
       <c r="E25" s="46" t="s">
-        <v>976</v>
+        <v>973</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" s="170" t="s">
-        <v>977</v>
+        <v>974</v>
       </c>
       <c r="B26" s="171"/>
       <c r="C26" s="171"/>
@@ -15215,19 +15242,19 @@
         <v>243</v>
       </c>
       <c r="B27" s="28" t="s">
-        <v>978</v>
+        <v>975</v>
       </c>
       <c r="C27" s="27" t="s">
-        <v>979</v>
+        <v>976</v>
       </c>
       <c r="D27" s="18"/>
       <c r="E27" s="46" t="s">
-        <v>980</v>
+        <v>977</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" s="170" t="s">
-        <v>981</v>
+        <v>978</v>
       </c>
       <c r="B28" s="171"/>
       <c r="C28" s="171"/>
@@ -15239,53 +15266,53 @@
         <v>243</v>
       </c>
       <c r="B29" s="93" t="s">
+        <v>979</v>
+      </c>
+      <c r="C29" s="94" t="s">
+        <v>980</v>
+      </c>
+      <c r="D29" s="93" t="s">
+        <v>981</v>
+      </c>
+      <c r="E29" s="86" t="s">
         <v>982</v>
       </c>
-      <c r="C29" s="94" t="s">
+      <c r="F29" s="72" t="s">
         <v>983</v>
-      </c>
-      <c r="D29" s="93" t="s">
-        <v>984</v>
-      </c>
-      <c r="E29" s="86" t="s">
-        <v>985</v>
-      </c>
-      <c r="F29" s="72" t="s">
-        <v>986</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A30" s="95" t="s">
-        <v>965</v>
+        <v>962</v>
       </c>
       <c r="B30" s="96" t="s">
+        <v>984</v>
+      </c>
+      <c r="C30" s="97" t="s">
+        <v>985</v>
+      </c>
+      <c r="D30" s="96" t="s">
+        <v>986</v>
+      </c>
+      <c r="E30" s="90" t="s">
         <v>987</v>
-      </c>
-      <c r="C30" s="97" t="s">
-        <v>988</v>
-      </c>
-      <c r="D30" s="96" t="s">
-        <v>989</v>
-      </c>
-      <c r="E30" s="90" t="s">
-        <v>990</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="335" x14ac:dyDescent="0.2">
       <c r="A31" s="95" t="s">
-        <v>991</v>
+        <v>988</v>
       </c>
       <c r="B31" s="96" t="s">
-        <v>992</v>
+        <v>989</v>
       </c>
       <c r="C31" s="97" t="s">
-        <v>993</v>
+        <v>990</v>
       </c>
       <c r="D31" s="96" t="s">
         <v>411</v>
       </c>
       <c r="E31" s="90" t="s">
-        <v>994</v>
+        <v>991</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="96" x14ac:dyDescent="0.2">
@@ -15293,13 +15320,13 @@
         <v>261</v>
       </c>
       <c r="B32" s="19" t="s">
-        <v>995</v>
+        <v>992</v>
       </c>
       <c r="C32" s="21" t="s">
-        <v>996</v>
+        <v>993</v>
       </c>
       <c r="E32" s="46" t="s">
-        <v>997</v>
+        <v>994</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="48" x14ac:dyDescent="0.2">
@@ -15307,16 +15334,16 @@
         <v>37</v>
       </c>
       <c r="B33" s="19" t="s">
+        <v>995</v>
+      </c>
+      <c r="C33" s="21" t="s">
+        <v>996</v>
+      </c>
+      <c r="D33" s="26" t="s">
+        <v>997</v>
+      </c>
+      <c r="E33" s="46" t="s">
         <v>998</v>
-      </c>
-      <c r="C33" s="21" t="s">
-        <v>999</v>
-      </c>
-      <c r="D33" s="26" t="s">
-        <v>1000</v>
-      </c>
-      <c r="E33" s="46" t="s">
-        <v>1001</v>
       </c>
     </row>
     <row r="34" spans="1:6" ht="96" x14ac:dyDescent="0.2">
@@ -15324,11 +15351,11 @@
         <v>417</v>
       </c>
       <c r="B34" s="28" t="s">
-        <v>1002</v>
+        <v>999</v>
       </c>
       <c r="C34" s="27"/>
       <c r="D34" s="18" t="s">
-        <v>1003</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="35" spans="1:6" ht="80" x14ac:dyDescent="0.2">
@@ -15336,11 +15363,11 @@
         <v>417</v>
       </c>
       <c r="B35" s="28" t="s">
-        <v>1004</v>
+        <v>1001</v>
       </c>
       <c r="C35" s="27"/>
       <c r="D35" s="18" t="s">
-        <v>1005</v>
+        <v>1002</v>
       </c>
     </row>
     <row r="36" spans="1:6" ht="80" x14ac:dyDescent="0.2">
@@ -15348,16 +15375,16 @@
         <v>420</v>
       </c>
       <c r="B36" s="28" t="s">
-        <v>1006</v>
+        <v>1003</v>
       </c>
       <c r="C36" s="27"/>
       <c r="D36" s="18" t="s">
-        <v>1007</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" s="170" t="s">
-        <v>1008</v>
+        <v>1005</v>
       </c>
       <c r="B37" s="171"/>
       <c r="C37" s="171"/>
@@ -15369,16 +15396,16 @@
         <v>243</v>
       </c>
       <c r="B38" s="19" t="s">
+        <v>1006</v>
+      </c>
+      <c r="C38" s="21" t="s">
+        <v>1007</v>
+      </c>
+      <c r="D38" s="5" t="s">
+        <v>1008</v>
+      </c>
+      <c r="E38" s="46" t="s">
         <v>1009</v>
-      </c>
-      <c r="C38" s="21" t="s">
-        <v>1010</v>
-      </c>
-      <c r="D38" s="5" t="s">
-        <v>1011</v>
-      </c>
-      <c r="E38" s="46" t="s">
-        <v>1012</v>
       </c>
     </row>
     <row r="39" spans="1:6" ht="64" x14ac:dyDescent="0.2">
@@ -15386,11 +15413,11 @@
         <v>417</v>
       </c>
       <c r="B39" s="28" t="s">
-        <v>1013</v>
+        <v>1010</v>
       </c>
       <c r="C39" s="27"/>
       <c r="D39" s="18" t="s">
-        <v>1014</v>
+        <v>1011</v>
       </c>
     </row>
     <row r="40" spans="1:6" ht="80" x14ac:dyDescent="0.2">
@@ -15398,16 +15425,16 @@
         <v>420</v>
       </c>
       <c r="B40" s="28" t="s">
-        <v>1015</v>
+        <v>1012</v>
       </c>
       <c r="C40" s="27"/>
       <c r="D40" s="18" t="s">
-        <v>1007</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" s="176" t="s">
-        <v>1016</v>
+        <v>1013</v>
       </c>
       <c r="B41" s="177"/>
       <c r="C41" s="177"/>
@@ -15419,19 +15446,19 @@
         <v>243</v>
       </c>
       <c r="B42" s="117" t="s">
-        <v>1017</v>
+        <v>1014</v>
       </c>
       <c r="C42" s="21" t="s">
-        <v>869</v>
+        <v>866</v>
       </c>
       <c r="D42" s="117" t="s">
-        <v>1018</v>
+        <v>1015</v>
       </c>
       <c r="E42" s="46" t="s">
-        <v>871</v>
+        <v>868</v>
       </c>
       <c r="F42" s="73" t="s">
-        <v>1019</v>
+        <v>1016</v>
       </c>
     </row>
     <row r="43" spans="1:6" ht="80" x14ac:dyDescent="0.2">
@@ -15439,16 +15466,16 @@
         <v>375</v>
       </c>
       <c r="B43" s="117" t="s">
-        <v>1020</v>
+        <v>1017</v>
       </c>
       <c r="C43" s="21" t="s">
-        <v>929</v>
+        <v>926</v>
       </c>
       <c r="D43" s="117" t="s">
-        <v>1021</v>
+        <v>1018</v>
       </c>
       <c r="E43" s="46" t="s">
-        <v>930</v>
+        <v>927</v>
       </c>
     </row>
     <row r="44" spans="1:6" ht="64" x14ac:dyDescent="0.2">
@@ -15456,16 +15483,16 @@
         <v>261</v>
       </c>
       <c r="B44" s="117" t="s">
+        <v>1019</v>
+      </c>
+      <c r="C44" s="62" t="s">
+        <v>1020</v>
+      </c>
+      <c r="D44" s="117" t="s">
+        <v>1021</v>
+      </c>
+      <c r="E44" s="46" t="s">
         <v>1022</v>
-      </c>
-      <c r="C44" s="62" t="s">
-        <v>1023</v>
-      </c>
-      <c r="D44" s="117" t="s">
-        <v>1024</v>
-      </c>
-      <c r="E44" s="46" t="s">
-        <v>1025</v>
       </c>
     </row>
     <row r="45" spans="1:6" ht="48" x14ac:dyDescent="0.2">
@@ -15473,16 +15500,16 @@
         <v>389</v>
       </c>
       <c r="B45" s="117" t="s">
-        <v>1026</v>
+        <v>1023</v>
       </c>
       <c r="C45" s="21" t="s">
-        <v>1027</v>
+        <v>1024</v>
       </c>
       <c r="D45" s="122" t="s">
-        <v>1028</v>
+        <v>1025</v>
       </c>
       <c r="E45" s="46" t="s">
-        <v>1027</v>
+        <v>1024</v>
       </c>
     </row>
     <row r="46" spans="1:6" ht="64" x14ac:dyDescent="0.2">
@@ -15490,16 +15517,16 @@
         <v>389</v>
       </c>
       <c r="B46" s="117" t="s">
+        <v>1026</v>
+      </c>
+      <c r="C46" s="21" t="s">
+        <v>1027</v>
+      </c>
+      <c r="D46" s="122" t="s">
+        <v>1028</v>
+      </c>
+      <c r="E46" s="46" t="s">
         <v>1029</v>
-      </c>
-      <c r="C46" s="21" t="s">
-        <v>1030</v>
-      </c>
-      <c r="D46" s="122" t="s">
-        <v>1031</v>
-      </c>
-      <c r="E46" s="46" t="s">
-        <v>1032</v>
       </c>
     </row>
     <row r="47" spans="1:6" ht="48" x14ac:dyDescent="0.2">
@@ -15507,16 +15534,16 @@
         <v>389</v>
       </c>
       <c r="B47" s="117" t="s">
+        <v>1030</v>
+      </c>
+      <c r="C47" s="21" t="s">
+        <v>1031</v>
+      </c>
+      <c r="D47" s="122" t="s">
+        <v>1032</v>
+      </c>
+      <c r="E47" s="46" t="s">
         <v>1033</v>
-      </c>
-      <c r="C47" s="21" t="s">
-        <v>1034</v>
-      </c>
-      <c r="D47" s="122" t="s">
-        <v>1035</v>
-      </c>
-      <c r="E47" s="46" t="s">
-        <v>1036</v>
       </c>
     </row>
     <row r="48" spans="1:6" ht="48" x14ac:dyDescent="0.2">
@@ -15524,16 +15551,16 @@
         <v>389</v>
       </c>
       <c r="B48" s="117" t="s">
+        <v>1034</v>
+      </c>
+      <c r="C48" s="21" t="s">
+        <v>1035</v>
+      </c>
+      <c r="D48" s="122" t="s">
+        <v>1036</v>
+      </c>
+      <c r="E48" s="46" t="s">
         <v>1037</v>
-      </c>
-      <c r="C48" s="21" t="s">
-        <v>1038</v>
-      </c>
-      <c r="D48" s="122" t="s">
-        <v>1039</v>
-      </c>
-      <c r="E48" s="46" t="s">
-        <v>1040</v>
       </c>
     </row>
     <row r="49" spans="1:6" ht="16" x14ac:dyDescent="0.2">
@@ -15541,16 +15568,16 @@
         <v>389</v>
       </c>
       <c r="B49" s="93" t="s">
-        <v>1041</v>
+        <v>1038</v>
       </c>
       <c r="C49" s="94" t="s">
-        <v>1042</v>
+        <v>1039</v>
       </c>
       <c r="D49" s="102" t="s">
         <v>411</v>
       </c>
       <c r="E49" s="86" t="s">
-        <v>1043</v>
+        <v>1040</v>
       </c>
     </row>
     <row r="50" spans="1:6" ht="16" x14ac:dyDescent="0.2">
@@ -15558,7 +15585,7 @@
         <v>32</v>
       </c>
       <c r="B50" s="19" t="s">
-        <v>1044</v>
+        <v>1041</v>
       </c>
       <c r="C50" s="21" t="s">
         <v>34</v>
@@ -15569,36 +15596,36 @@
     </row>
     <row r="51" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A51" s="19" t="s">
+        <v>1042</v>
+      </c>
+      <c r="B51" s="19" t="s">
+        <v>1043</v>
+      </c>
+      <c r="C51" s="21" t="s">
+        <v>1044</v>
+      </c>
+      <c r="D51" s="19" t="s">
         <v>1045</v>
       </c>
-      <c r="B51" s="19" t="s">
-        <v>1046</v>
-      </c>
-      <c r="C51" s="21" t="s">
-        <v>1047</v>
-      </c>
-      <c r="D51" s="19" t="s">
-        <v>1048</v>
-      </c>
       <c r="F51" s="72" t="s">
-        <v>917</v>
+        <v>914</v>
       </c>
     </row>
     <row r="52" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A52" s="19" t="s">
+        <v>1042</v>
+      </c>
+      <c r="B52" s="19" t="s">
+        <v>1046</v>
+      </c>
+      <c r="C52" s="21" t="s">
+        <v>1047</v>
+      </c>
+      <c r="D52" s="19" t="s">
         <v>1045</v>
       </c>
-      <c r="B52" s="19" t="s">
-        <v>1049</v>
-      </c>
-      <c r="C52" s="21" t="s">
-        <v>1050</v>
-      </c>
-      <c r="D52" s="19" t="s">
-        <v>1048</v>
-      </c>
       <c r="F52" s="72" t="s">
-        <v>917</v>
+        <v>914</v>
       </c>
     </row>
     <row r="53" spans="1:6" ht="48" x14ac:dyDescent="0.2">
@@ -15606,16 +15633,16 @@
         <v>389</v>
       </c>
       <c r="B53" s="117" t="s">
-        <v>1051</v>
+        <v>1048</v>
       </c>
       <c r="C53" s="21" t="s">
-        <v>1052</v>
+        <v>1049</v>
       </c>
       <c r="D53" s="122" t="s">
-        <v>1053</v>
+        <v>1050</v>
       </c>
       <c r="F53" s="72" t="s">
-        <v>917</v>
+        <v>914</v>
       </c>
     </row>
     <row r="54" spans="1:6" ht="48" x14ac:dyDescent="0.2">
@@ -15623,16 +15650,16 @@
         <v>389</v>
       </c>
       <c r="B54" s="117" t="s">
-        <v>1054</v>
+        <v>1051</v>
       </c>
       <c r="C54" s="21" t="s">
-        <v>1055</v>
+        <v>1052</v>
       </c>
       <c r="D54" s="122" t="s">
-        <v>1056</v>
+        <v>1053</v>
       </c>
       <c r="F54" s="72" t="s">
-        <v>917</v>
+        <v>914</v>
       </c>
     </row>
   </sheetData>
@@ -15695,52 +15722,52 @@
         <v>243</v>
       </c>
       <c r="B2" s="137" t="s">
-        <v>1057</v>
+        <v>1054</v>
       </c>
       <c r="C2" s="138" t="s">
-        <v>1058</v>
+        <v>1055</v>
       </c>
       <c r="D2" s="137" t="s">
         <v>246</v>
       </c>
       <c r="E2" s="139" t="s">
-        <v>1059</v>
+        <v>1056</v>
       </c>
       <c r="F2" s="136"/>
     </row>
     <row r="3" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A3" s="137" t="s">
-        <v>965</v>
+        <v>962</v>
       </c>
       <c r="B3" s="137" t="s">
+        <v>1057</v>
+      </c>
+      <c r="C3" s="138" t="s">
+        <v>1058</v>
+      </c>
+      <c r="D3" s="137" t="s">
+        <v>1059</v>
+      </c>
+      <c r="E3" s="139" t="s">
         <v>1060</v>
-      </c>
-      <c r="C3" s="138" t="s">
-        <v>1061</v>
-      </c>
-      <c r="D3" s="137" t="s">
-        <v>1062</v>
-      </c>
-      <c r="E3" s="139" t="s">
-        <v>1063</v>
       </c>
       <c r="F3" s="136"/>
     </row>
     <row r="4" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A4" s="137" t="s">
+        <v>1061</v>
+      </c>
+      <c r="B4" s="137" t="s">
+        <v>1062</v>
+      </c>
+      <c r="C4" s="138" t="s">
+        <v>1063</v>
+      </c>
+      <c r="D4" s="137" t="s">
         <v>1064</v>
       </c>
-      <c r="B4" s="137" t="s">
+      <c r="E4" s="139" t="s">
         <v>1065</v>
-      </c>
-      <c r="C4" s="138" t="s">
-        <v>1066</v>
-      </c>
-      <c r="D4" s="137" t="s">
-        <v>1067</v>
-      </c>
-      <c r="E4" s="139" t="s">
-        <v>1068</v>
       </c>
       <c r="F4" s="136"/>
     </row>
@@ -15749,11 +15776,11 @@
         <v>417</v>
       </c>
       <c r="B5" s="140" t="s">
-        <v>1069</v>
+        <v>1066</v>
       </c>
       <c r="C5" s="27"/>
       <c r="D5" s="137" t="s">
-        <v>1070</v>
+        <v>1067</v>
       </c>
       <c r="E5" s="139"/>
       <c r="F5" s="136"/>
@@ -15763,84 +15790,84 @@
         <v>420</v>
       </c>
       <c r="B6" s="140" t="s">
-        <v>1071</v>
+        <v>1068</v>
       </c>
       <c r="C6" s="27"/>
       <c r="D6" s="137" t="s">
-        <v>1072</v>
+        <v>1069</v>
       </c>
       <c r="E6" s="139"/>
       <c r="F6" s="136"/>
     </row>
     <row r="7" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A7" s="137" t="s">
-        <v>1064</v>
+        <v>1061</v>
       </c>
       <c r="B7" s="137" t="s">
+        <v>1070</v>
+      </c>
+      <c r="C7" s="138" t="s">
+        <v>1071</v>
+      </c>
+      <c r="D7" s="137" t="s">
+        <v>1072</v>
+      </c>
+      <c r="E7" s="139" t="s">
         <v>1073</v>
-      </c>
-      <c r="C7" s="138" t="s">
-        <v>1074</v>
-      </c>
-      <c r="D7" s="137" t="s">
-        <v>1075</v>
-      </c>
-      <c r="E7" s="139" t="s">
-        <v>1076</v>
       </c>
       <c r="F7" s="136"/>
     </row>
     <row r="8" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A8" s="137" t="s">
-        <v>1064</v>
+        <v>1061</v>
       </c>
       <c r="B8" s="137" t="s">
+        <v>1074</v>
+      </c>
+      <c r="C8" s="138" t="s">
+        <v>1075</v>
+      </c>
+      <c r="D8" s="137" t="s">
+        <v>1076</v>
+      </c>
+      <c r="E8" s="139" t="s">
         <v>1077</v>
-      </c>
-      <c r="C8" s="138" t="s">
-        <v>1078</v>
-      </c>
-      <c r="D8" s="137" t="s">
-        <v>1079</v>
-      </c>
-      <c r="E8" s="139" t="s">
-        <v>1080</v>
       </c>
       <c r="F8" s="136"/>
     </row>
     <row r="9" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A9" s="137" t="s">
-        <v>1064</v>
+        <v>1061</v>
       </c>
       <c r="B9" s="137" t="s">
+        <v>1078</v>
+      </c>
+      <c r="C9" s="138" t="s">
+        <v>1079</v>
+      </c>
+      <c r="D9" s="137" t="s">
+        <v>1080</v>
+      </c>
+      <c r="E9" s="139" t="s">
         <v>1081</v>
-      </c>
-      <c r="C9" s="138" t="s">
-        <v>1082</v>
-      </c>
-      <c r="D9" s="137" t="s">
-        <v>1083</v>
-      </c>
-      <c r="E9" s="139" t="s">
-        <v>1084</v>
       </c>
       <c r="F9" s="136"/>
     </row>
     <row r="10" spans="1:6" ht="64" x14ac:dyDescent="0.2">
       <c r="A10" s="137" t="s">
-        <v>1064</v>
+        <v>1061</v>
       </c>
       <c r="B10" s="137" t="s">
+        <v>1082</v>
+      </c>
+      <c r="C10" s="138" t="s">
+        <v>1083</v>
+      </c>
+      <c r="D10" s="137" t="s">
+        <v>1084</v>
+      </c>
+      <c r="E10" s="139" t="s">
         <v>1085</v>
-      </c>
-      <c r="C10" s="138" t="s">
-        <v>1086</v>
-      </c>
-      <c r="D10" s="137" t="s">
-        <v>1087</v>
-      </c>
-      <c r="E10" s="139" t="s">
-        <v>1088</v>
       </c>
       <c r="F10" s="136"/>
     </row>
@@ -15849,32 +15876,32 @@
         <v>254</v>
       </c>
       <c r="B11" s="137" t="s">
-        <v>1089</v>
+        <v>1086</v>
       </c>
       <c r="C11" s="138" t="s">
-        <v>1090</v>
+        <v>1087</v>
       </c>
       <c r="D11" s="137" t="s">
-        <v>1091</v>
+        <v>1088</v>
       </c>
       <c r="E11" s="139"/>
       <c r="F11" s="136"/>
     </row>
     <row r="12" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A12" s="137" t="s">
-        <v>1064</v>
+        <v>1061</v>
       </c>
       <c r="B12" s="137" t="s">
+        <v>1089</v>
+      </c>
+      <c r="C12" s="138" t="s">
+        <v>1090</v>
+      </c>
+      <c r="D12" s="137" t="s">
+        <v>1091</v>
+      </c>
+      <c r="E12" s="139" t="s">
         <v>1092</v>
-      </c>
-      <c r="C12" s="138" t="s">
-        <v>1093</v>
-      </c>
-      <c r="D12" s="137" t="s">
-        <v>1094</v>
-      </c>
-      <c r="E12" s="139" t="s">
-        <v>1095</v>
       </c>
       <c r="F12" s="136"/>
     </row>
@@ -15883,11 +15910,11 @@
         <v>417</v>
       </c>
       <c r="B13" s="28" t="s">
-        <v>1096</v>
+        <v>1093</v>
       </c>
       <c r="C13" s="139"/>
       <c r="D13" s="137" t="s">
-        <v>1097</v>
+        <v>1094</v>
       </c>
       <c r="E13" s="139"/>
       <c r="F13" s="136"/>
@@ -15897,83 +15924,83 @@
         <v>420</v>
       </c>
       <c r="B14" s="28" t="s">
-        <v>1098</v>
+        <v>1095</v>
       </c>
       <c r="C14" s="139"/>
       <c r="D14" s="137" t="s">
-        <v>1072</v>
+        <v>1069</v>
       </c>
       <c r="E14" s="139"/>
       <c r="F14" s="136"/>
     </row>
     <row r="15" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A15" s="137" t="s">
-        <v>1064</v>
+        <v>1061</v>
       </c>
       <c r="B15" s="137" t="s">
+        <v>1096</v>
+      </c>
+      <c r="C15" s="138" t="s">
+        <v>1097</v>
+      </c>
+      <c r="D15" s="137" t="s">
+        <v>1098</v>
+      </c>
+      <c r="E15" s="139" t="s">
         <v>1099</v>
-      </c>
-      <c r="C15" s="138" t="s">
-        <v>1100</v>
-      </c>
-      <c r="D15" s="137" t="s">
-        <v>1101</v>
-      </c>
-      <c r="E15" s="139" t="s">
-        <v>1102</v>
       </c>
       <c r="F15" s="136"/>
     </row>
     <row r="16" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A16" s="137" t="s">
-        <v>1064</v>
+        <v>1061</v>
       </c>
       <c r="B16" s="137" t="s">
+        <v>1100</v>
+      </c>
+      <c r="C16" s="138" t="s">
+        <v>1101</v>
+      </c>
+      <c r="D16" s="137" t="s">
+        <v>1102</v>
+      </c>
+      <c r="E16" s="139" t="s">
         <v>1103</v>
-      </c>
-      <c r="C16" s="138" t="s">
-        <v>1104</v>
-      </c>
-      <c r="D16" s="137" t="s">
-        <v>1105</v>
-      </c>
-      <c r="E16" s="139" t="s">
-        <v>1106</v>
       </c>
       <c r="F16" s="136"/>
     </row>
     <row r="17" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A17" s="137" t="s">
-        <v>1064</v>
+        <v>1061</v>
       </c>
       <c r="B17" s="137" t="s">
+        <v>1104</v>
+      </c>
+      <c r="C17" s="138" t="s">
+        <v>1105</v>
+      </c>
+      <c r="D17" s="137" t="s">
+        <v>1106</v>
+      </c>
+      <c r="E17" s="139" t="s">
         <v>1107</v>
-      </c>
-      <c r="C17" s="138" t="s">
-        <v>1108</v>
-      </c>
-      <c r="D17" s="137" t="s">
-        <v>1109</v>
-      </c>
-      <c r="E17" s="139" t="s">
-        <v>1110</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="144" x14ac:dyDescent="0.2">
       <c r="A18" s="137" t="s">
-        <v>1064</v>
+        <v>1061</v>
       </c>
       <c r="B18" s="137" t="s">
+        <v>1108</v>
+      </c>
+      <c r="C18" s="138" t="s">
+        <v>1109</v>
+      </c>
+      <c r="D18" s="29" t="s">
+        <v>1110</v>
+      </c>
+      <c r="E18" s="139" t="s">
         <v>1111</v>
-      </c>
-      <c r="C18" s="138" t="s">
-        <v>1112</v>
-      </c>
-      <c r="D18" s="29" t="s">
-        <v>1113</v>
-      </c>
-      <c r="E18" s="139" t="s">
-        <v>1114</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="80" x14ac:dyDescent="0.2">
@@ -15981,11 +16008,11 @@
         <v>417</v>
       </c>
       <c r="B19" s="28" t="s">
-        <v>1115</v>
+        <v>1112</v>
       </c>
       <c r="C19" s="27"/>
       <c r="D19" s="18" t="s">
-        <v>1116</v>
+        <v>1113</v>
       </c>
       <c r="E19" s="139"/>
     </row>
@@ -15994,11 +16021,11 @@
         <v>420</v>
       </c>
       <c r="B20" s="28" t="s">
-        <v>1117</v>
+        <v>1114</v>
       </c>
       <c r="C20" s="27"/>
       <c r="D20" s="18" t="s">
-        <v>1072</v>
+        <v>1069</v>
       </c>
       <c r="E20" s="139"/>
     </row>
@@ -16007,29 +16034,29 @@
         <v>420</v>
       </c>
       <c r="B21" s="28" t="s">
-        <v>1118</v>
+        <v>1115</v>
       </c>
       <c r="C21" s="27"/>
       <c r="D21" s="18" t="s">
-        <v>1119</v>
+        <v>1116</v>
       </c>
       <c r="E21" s="139"/>
     </row>
     <row r="22" spans="1:5" ht="112" x14ac:dyDescent="0.2">
       <c r="A22" s="137" t="s">
+        <v>1117</v>
+      </c>
+      <c r="B22" s="137" t="s">
+        <v>1118</v>
+      </c>
+      <c r="C22" s="138" t="s">
+        <v>1119</v>
+      </c>
+      <c r="D22" s="137" t="s">
         <v>1120</v>
       </c>
-      <c r="B22" s="137" t="s">
+      <c r="E22" s="139" t="s">
         <v>1121</v>
-      </c>
-      <c r="C22" s="138" t="s">
-        <v>1122</v>
-      </c>
-      <c r="D22" s="137" t="s">
-        <v>1123</v>
-      </c>
-      <c r="E22" s="139" t="s">
-        <v>1124</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="48" x14ac:dyDescent="0.2">
@@ -16037,11 +16064,11 @@
         <v>417</v>
       </c>
       <c r="B23" s="28" t="s">
-        <v>1125</v>
+        <v>1122</v>
       </c>
       <c r="C23" s="27"/>
       <c r="D23" s="137" t="s">
-        <v>1126</v>
+        <v>1123</v>
       </c>
       <c r="E23" s="139"/>
     </row>
@@ -16050,11 +16077,11 @@
         <v>420</v>
       </c>
       <c r="B24" s="28" t="s">
-        <v>1127</v>
+        <v>1124</v>
       </c>
       <c r="C24" s="27"/>
       <c r="D24" s="137" t="s">
-        <v>1128</v>
+        <v>1125</v>
       </c>
       <c r="E24" s="139"/>
     </row>
@@ -16063,11 +16090,11 @@
         <v>420</v>
       </c>
       <c r="B25" s="28" t="s">
-        <v>1129</v>
+        <v>1126</v>
       </c>
       <c r="C25" s="27"/>
       <c r="D25" s="29" t="s">
-        <v>1130</v>
+        <v>1127</v>
       </c>
       <c r="E25" s="139"/>
     </row>
@@ -16076,38 +16103,38 @@
         <v>254</v>
       </c>
       <c r="B26" s="137" t="s">
-        <v>1131</v>
+        <v>1128</v>
       </c>
       <c r="C26" s="138" t="s">
-        <v>1132</v>
+        <v>1129</v>
       </c>
       <c r="D26" s="137" t="s">
-        <v>1091</v>
+        <v>1088</v>
       </c>
       <c r="E26" s="139" t="s">
-        <v>1133</v>
+        <v>1130</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A27" s="137" t="s">
-        <v>1064</v>
+        <v>1061</v>
       </c>
       <c r="B27" s="137" t="s">
+        <v>1131</v>
+      </c>
+      <c r="C27" s="138" t="s">
+        <v>1132</v>
+      </c>
+      <c r="D27" s="137" t="s">
+        <v>1133</v>
+      </c>
+      <c r="E27" s="139" t="s">
         <v>1134</v>
-      </c>
-      <c r="C27" s="138" t="s">
-        <v>1135</v>
-      </c>
-      <c r="D27" s="137" t="s">
-        <v>1136</v>
-      </c>
-      <c r="E27" s="139" t="s">
-        <v>1137</v>
       </c>
     </row>
     <row r="28" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A28" s="185" t="s">
-        <v>1138</v>
+        <v>1135</v>
       </c>
       <c r="B28" s="186"/>
       <c r="C28" s="186"/>
@@ -16119,33 +16146,33 @@
         <v>243</v>
       </c>
       <c r="B29" s="142" t="s">
+        <v>1136</v>
+      </c>
+      <c r="C29" s="143" t="s">
+        <v>1137</v>
+      </c>
+      <c r="D29" s="5" t="s">
+        <v>1138</v>
+      </c>
+      <c r="E29" s="144" t="s">
         <v>1139</v>
-      </c>
-      <c r="C29" s="143" t="s">
-        <v>1140</v>
-      </c>
-      <c r="D29" s="5" t="s">
-        <v>1141</v>
-      </c>
-      <c r="E29" s="144" t="s">
-        <v>1142</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="64" x14ac:dyDescent="0.2">
       <c r="A30" s="145" t="s">
+        <v>1140</v>
+      </c>
+      <c r="B30" s="145" t="s">
+        <v>1141</v>
+      </c>
+      <c r="C30" s="146" t="s">
+        <v>1142</v>
+      </c>
+      <c r="D30" s="145" t="s">
         <v>1143</v>
       </c>
-      <c r="B30" s="145" t="s">
+      <c r="E30" s="147" t="s">
         <v>1144</v>
-      </c>
-      <c r="C30" s="146" t="s">
-        <v>1145</v>
-      </c>
-      <c r="D30" s="145" t="s">
-        <v>1146</v>
-      </c>
-      <c r="E30" s="147" t="s">
-        <v>1147</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="48" x14ac:dyDescent="0.2">
@@ -16153,11 +16180,11 @@
         <v>417</v>
       </c>
       <c r="B31" s="28" t="s">
-        <v>1148</v>
+        <v>1145</v>
       </c>
       <c r="C31" s="27"/>
       <c r="D31" s="18" t="s">
-        <v>1014</v>
+        <v>1011</v>
       </c>
       <c r="E31" s="147"/>
     </row>
@@ -16166,17 +16193,17 @@
         <v>420</v>
       </c>
       <c r="B32" s="28" t="s">
-        <v>1149</v>
+        <v>1146</v>
       </c>
       <c r="C32" s="27"/>
       <c r="D32" s="18" t="s">
-        <v>1007</v>
+        <v>1004</v>
       </c>
       <c r="E32" s="147"/>
     </row>
     <row r="33" spans="1:6" s="13" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A33" s="188" t="s">
-        <v>1150</v>
+        <v>1147</v>
       </c>
       <c r="B33" s="189"/>
       <c r="C33" s="190"/>
@@ -16188,121 +16215,121 @@
         <v>243</v>
       </c>
       <c r="B34" s="148" t="s">
+        <v>1148</v>
+      </c>
+      <c r="C34" s="146" t="s">
+        <v>1149</v>
+      </c>
+      <c r="D34" s="50" t="s">
+        <v>1150</v>
+      </c>
+      <c r="E34" s="147" t="s">
         <v>1151</v>
-      </c>
-      <c r="C34" s="146" t="s">
-        <v>1152</v>
-      </c>
-      <c r="D34" s="50" t="s">
-        <v>1153</v>
-      </c>
-      <c r="E34" s="147" t="s">
-        <v>1154</v>
       </c>
       <c r="F34" s="136"/>
     </row>
     <row r="35" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A35" s="145" t="s">
-        <v>1064</v>
+        <v>1061</v>
       </c>
       <c r="B35" s="149" t="s">
+        <v>1152</v>
+      </c>
+      <c r="C35" s="146" t="s">
+        <v>1153</v>
+      </c>
+      <c r="D35" s="150" t="s">
+        <v>1154</v>
+      </c>
+      <c r="E35" s="147" t="s">
         <v>1155</v>
-      </c>
-      <c r="C35" s="146" t="s">
-        <v>1156</v>
-      </c>
-      <c r="D35" s="150" t="s">
-        <v>1157</v>
-      </c>
-      <c r="E35" s="147" t="s">
-        <v>1158</v>
       </c>
       <c r="F35" s="136"/>
     </row>
     <row r="36" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A36" s="145" t="s">
-        <v>1064</v>
+        <v>1061</v>
       </c>
       <c r="B36" s="149" t="s">
-        <v>1159</v>
+        <v>1156</v>
       </c>
       <c r="C36" s="146" t="s">
-        <v>1160</v>
+        <v>1157</v>
       </c>
       <c r="D36" s="150" t="s">
-        <v>1157</v>
+        <v>1154</v>
       </c>
       <c r="E36" s="147" t="s">
-        <v>1161</v>
+        <v>1158</v>
       </c>
       <c r="F36" s="136"/>
     </row>
     <row r="37" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A37" s="145" t="s">
-        <v>1064</v>
+        <v>1061</v>
       </c>
       <c r="B37" s="149" t="s">
-        <v>1162</v>
+        <v>1159</v>
       </c>
       <c r="C37" s="49" t="s">
-        <v>1163</v>
+        <v>1160</v>
       </c>
       <c r="D37" s="150" t="s">
-        <v>1157</v>
+        <v>1154</v>
       </c>
       <c r="E37" s="147" t="s">
-        <v>1164</v>
+        <v>1161</v>
       </c>
       <c r="F37" s="136"/>
     </row>
     <row r="38" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A38" s="145" t="s">
-        <v>1064</v>
+        <v>1061</v>
       </c>
       <c r="B38" s="149" t="s">
-        <v>1165</v>
+        <v>1162</v>
       </c>
       <c r="C38" s="49" t="s">
-        <v>1166</v>
+        <v>1163</v>
       </c>
       <c r="D38" s="150" t="s">
-        <v>1157</v>
+        <v>1154</v>
       </c>
       <c r="E38" s="147" t="s">
-        <v>1167</v>
+        <v>1164</v>
       </c>
       <c r="F38" s="136"/>
     </row>
     <row r="39" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A39" s="145" t="s">
-        <v>1064</v>
+        <v>1061</v>
       </c>
       <c r="B39" s="149" t="s">
-        <v>1168</v>
+        <v>1165</v>
       </c>
       <c r="C39" s="49" t="s">
-        <v>1169</v>
+        <v>1166</v>
       </c>
       <c r="D39" s="150" t="s">
-        <v>1157</v>
+        <v>1154</v>
       </c>
       <c r="E39" s="147" t="s">
-        <v>1170</v>
+        <v>1167</v>
       </c>
       <c r="F39" s="136"/>
     </row>
     <row r="40" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A40" s="145" t="s">
-        <v>1064</v>
+        <v>1061</v>
       </c>
       <c r="B40" s="149" t="s">
-        <v>1171</v>
+        <v>1168</v>
       </c>
       <c r="C40" s="49" t="s">
         <v>93</v>
       </c>
       <c r="D40" s="150" t="s">
-        <v>1157</v>
+        <v>1154</v>
       </c>
       <c r="E40" s="147" t="s">
         <v>95</v>
@@ -16314,11 +16341,11 @@
         <v>417</v>
       </c>
       <c r="B41" s="28" t="s">
-        <v>1172</v>
+        <v>1169</v>
       </c>
       <c r="C41" s="51"/>
       <c r="D41" s="18" t="s">
-        <v>1014</v>
+        <v>1011</v>
       </c>
       <c r="E41" s="147"/>
       <c r="F41" s="136"/>
@@ -16328,11 +16355,11 @@
         <v>420</v>
       </c>
       <c r="B42" s="28" t="s">
-        <v>1173</v>
+        <v>1170</v>
       </c>
       <c r="C42" s="27"/>
       <c r="D42" s="18" t="s">
-        <v>1007</v>
+        <v>1004</v>
       </c>
       <c r="E42" s="147"/>
       <c r="F42" s="136"/>
@@ -16342,16 +16369,16 @@
         <v>243</v>
       </c>
       <c r="B43" s="137" t="s">
+        <v>1171</v>
+      </c>
+      <c r="C43" s="62" t="s">
+        <v>1172</v>
+      </c>
+      <c r="D43" s="5" t="s">
+        <v>1173</v>
+      </c>
+      <c r="E43" s="147" t="s">
         <v>1174</v>
-      </c>
-      <c r="C43" s="62" t="s">
-        <v>1175</v>
-      </c>
-      <c r="D43" s="5" t="s">
-        <v>1176</v>
-      </c>
-      <c r="E43" s="147" t="s">
-        <v>1177</v>
       </c>
       <c r="F43" s="136"/>
     </row>
@@ -16360,11 +16387,11 @@
         <v>417</v>
       </c>
       <c r="B44" s="28" t="s">
-        <v>1178</v>
+        <v>1175</v>
       </c>
       <c r="C44" s="27"/>
       <c r="D44" s="18" t="s">
-        <v>1014</v>
+        <v>1011</v>
       </c>
       <c r="E44" s="147"/>
       <c r="F44" s="136"/>
@@ -16374,18 +16401,18 @@
         <v>420</v>
       </c>
       <c r="B45" s="28" t="s">
-        <v>1179</v>
+        <v>1176</v>
       </c>
       <c r="C45" s="27"/>
       <c r="D45" s="18" t="s">
-        <v>1007</v>
+        <v>1004</v>
       </c>
       <c r="E45" s="147"/>
       <c r="F45" s="136"/>
     </row>
     <row r="46" spans="1:6" s="13" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="185" t="s">
-        <v>1180</v>
+        <v>1177</v>
       </c>
       <c r="B46" s="186"/>
       <c r="C46" s="186"/>
@@ -16397,53 +16424,53 @@
         <v>243</v>
       </c>
       <c r="B47" s="145" t="s">
+        <v>1178</v>
+      </c>
+      <c r="C47" s="62" t="s">
+        <v>1179</v>
+      </c>
+      <c r="D47" s="117" t="s">
+        <v>1180</v>
+      </c>
+      <c r="E47" s="63" t="s">
+        <v>868</v>
+      </c>
+      <c r="F47" s="38" t="s">
         <v>1181</v>
-      </c>
-      <c r="C47" s="62" t="s">
-        <v>1182</v>
-      </c>
-      <c r="D47" s="117" t="s">
-        <v>1183</v>
-      </c>
-      <c r="E47" s="63" t="s">
-        <v>871</v>
-      </c>
-      <c r="F47" s="38" t="s">
-        <v>1184</v>
       </c>
     </row>
     <row r="48" spans="1:6" s="30" customFormat="1" ht="64" x14ac:dyDescent="0.2">
       <c r="A48" s="145" t="s">
+        <v>1182</v>
+      </c>
+      <c r="B48" s="145" t="s">
+        <v>1183</v>
+      </c>
+      <c r="C48" s="62" t="s">
+        <v>1184</v>
+      </c>
+      <c r="D48" s="117" t="s">
         <v>1185</v>
       </c>
-      <c r="B48" s="145" t="s">
-        <v>1186</v>
-      </c>
-      <c r="C48" s="62" t="s">
-        <v>1187</v>
-      </c>
-      <c r="D48" s="117" t="s">
-        <v>1188</v>
-      </c>
       <c r="E48" s="63" t="s">
-        <v>936</v>
+        <v>933</v>
       </c>
     </row>
     <row r="49" spans="1:6" s="30" customFormat="1" ht="64" x14ac:dyDescent="0.2">
       <c r="A49" s="145" t="s">
-        <v>1143</v>
+        <v>1140</v>
       </c>
       <c r="B49" s="145" t="s">
-        <v>1189</v>
+        <v>1186</v>
       </c>
       <c r="C49" s="62" t="s">
-        <v>1190</v>
+        <v>1187</v>
       </c>
       <c r="D49" s="117" t="s">
-        <v>1024</v>
+        <v>1021</v>
       </c>
       <c r="E49" s="63" t="s">
-        <v>1025</v>
+        <v>1022</v>
       </c>
     </row>
     <row r="50" spans="1:6" s="30" customFormat="1" ht="48" x14ac:dyDescent="0.2">
@@ -16451,19 +16478,19 @@
         <v>389</v>
       </c>
       <c r="B50" s="137" t="s">
+        <v>1188</v>
+      </c>
+      <c r="C50" s="146" t="s">
+        <v>1189</v>
+      </c>
+      <c r="D50" s="122" t="s">
+        <v>1190</v>
+      </c>
+      <c r="E50" s="63" t="s">
+        <v>1065</v>
+      </c>
+      <c r="F50" s="74" t="s">
         <v>1191</v>
-      </c>
-      <c r="C50" s="146" t="s">
-        <v>1192</v>
-      </c>
-      <c r="D50" s="122" t="s">
-        <v>1193</v>
-      </c>
-      <c r="E50" s="63" t="s">
-        <v>1068</v>
-      </c>
-      <c r="F50" s="74" t="s">
-        <v>1194</v>
       </c>
     </row>
     <row r="51" spans="1:6" s="30" customFormat="1" ht="48" x14ac:dyDescent="0.2">
@@ -16471,16 +16498,16 @@
         <v>389</v>
       </c>
       <c r="B51" s="137" t="s">
+        <v>1192</v>
+      </c>
+      <c r="C51" s="146" t="s">
+        <v>1193</v>
+      </c>
+      <c r="D51" s="122" t="s">
+        <v>1194</v>
+      </c>
+      <c r="E51" s="63" t="s">
         <v>1195</v>
-      </c>
-      <c r="C51" s="146" t="s">
-        <v>1196</v>
-      </c>
-      <c r="D51" s="122" t="s">
-        <v>1197</v>
-      </c>
-      <c r="E51" s="63" t="s">
-        <v>1198</v>
       </c>
     </row>
     <row r="52" spans="1:6" s="30" customFormat="1" ht="64" x14ac:dyDescent="0.2">
@@ -16488,16 +16515,16 @@
         <v>389</v>
       </c>
       <c r="B52" s="137" t="s">
+        <v>1196</v>
+      </c>
+      <c r="C52" s="146" t="s">
+        <v>1197</v>
+      </c>
+      <c r="D52" s="122" t="s">
+        <v>1198</v>
+      </c>
+      <c r="E52" s="63" t="s">
         <v>1199</v>
-      </c>
-      <c r="C52" s="146" t="s">
-        <v>1200</v>
-      </c>
-      <c r="D52" s="122" t="s">
-        <v>1201</v>
-      </c>
-      <c r="E52" s="63" t="s">
-        <v>1202</v>
       </c>
     </row>
     <row r="53" spans="1:6" s="30" customFormat="1" ht="64" x14ac:dyDescent="0.2">
@@ -16505,16 +16532,16 @@
         <v>389</v>
       </c>
       <c r="B53" s="137" t="s">
+        <v>1200</v>
+      </c>
+      <c r="C53" s="146" t="s">
+        <v>1201</v>
+      </c>
+      <c r="D53" s="122" t="s">
+        <v>1202</v>
+      </c>
+      <c r="E53" s="63" t="s">
         <v>1203</v>
-      </c>
-      <c r="C53" s="146" t="s">
-        <v>1204</v>
-      </c>
-      <c r="D53" s="122" t="s">
-        <v>1205</v>
-      </c>
-      <c r="E53" s="63" t="s">
-        <v>1206</v>
       </c>
     </row>
     <row r="54" spans="1:6" s="30" customFormat="1" ht="48" x14ac:dyDescent="0.2">
@@ -16522,16 +16549,16 @@
         <v>389</v>
       </c>
       <c r="B54" s="137" t="s">
+        <v>1204</v>
+      </c>
+      <c r="C54" s="146" t="s">
+        <v>1205</v>
+      </c>
+      <c r="D54" s="122" t="s">
+        <v>1206</v>
+      </c>
+      <c r="E54" s="63" t="s">
         <v>1207</v>
-      </c>
-      <c r="C54" s="146" t="s">
-        <v>1208</v>
-      </c>
-      <c r="D54" s="122" t="s">
-        <v>1209</v>
-      </c>
-      <c r="E54" s="63" t="s">
-        <v>1210</v>
       </c>
     </row>
     <row r="55" spans="1:6" s="30" customFormat="1" ht="32" x14ac:dyDescent="0.2">
@@ -16539,19 +16566,19 @@
         <v>389</v>
       </c>
       <c r="B55" s="137" t="s">
+        <v>1208</v>
+      </c>
+      <c r="C55" s="146" t="s">
+        <v>1209</v>
+      </c>
+      <c r="D55" s="122" t="s">
+        <v>1210</v>
+      </c>
+      <c r="E55" s="63" t="s">
+        <v>1092</v>
+      </c>
+      <c r="F55" s="74" t="s">
         <v>1211</v>
-      </c>
-      <c r="C55" s="146" t="s">
-        <v>1212</v>
-      </c>
-      <c r="D55" s="122" t="s">
-        <v>1213</v>
-      </c>
-      <c r="E55" s="63" t="s">
-        <v>1095</v>
-      </c>
-      <c r="F55" s="74" t="s">
-        <v>1214</v>
       </c>
     </row>
     <row r="56" spans="1:6" s="30" customFormat="1" ht="48" x14ac:dyDescent="0.2">
@@ -16559,19 +16586,19 @@
         <v>389</v>
       </c>
       <c r="B56" s="137" t="s">
+        <v>1212</v>
+      </c>
+      <c r="C56" s="146" t="s">
+        <v>1213</v>
+      </c>
+      <c r="D56" s="122" t="s">
+        <v>1214</v>
+      </c>
+      <c r="E56" s="63" t="s">
         <v>1215</v>
       </c>
-      <c r="C56" s="146" t="s">
+      <c r="F56" s="74" t="s">
         <v>1216</v>
-      </c>
-      <c r="D56" s="122" t="s">
-        <v>1217</v>
-      </c>
-      <c r="E56" s="63" t="s">
-        <v>1218</v>
-      </c>
-      <c r="F56" s="74" t="s">
-        <v>1219</v>
       </c>
     </row>
     <row r="57" spans="1:6" s="30" customFormat="1" ht="48" x14ac:dyDescent="0.2">
@@ -16579,19 +16606,19 @@
         <v>389</v>
       </c>
       <c r="B57" s="137" t="s">
+        <v>1217</v>
+      </c>
+      <c r="C57" s="146" t="s">
+        <v>1218</v>
+      </c>
+      <c r="D57" s="122" t="s">
+        <v>1219</v>
+      </c>
+      <c r="E57" s="63" t="s">
         <v>1220</v>
       </c>
-      <c r="C57" s="146" t="s">
+      <c r="F57" s="74" t="s">
         <v>1221</v>
-      </c>
-      <c r="D57" s="122" t="s">
-        <v>1222</v>
-      </c>
-      <c r="E57" s="63" t="s">
-        <v>1223</v>
-      </c>
-      <c r="F57" s="74" t="s">
-        <v>1224</v>
       </c>
     </row>
     <row r="58" spans="1:6" s="30" customFormat="1" ht="32" x14ac:dyDescent="0.2">
@@ -16599,19 +16626,19 @@
         <v>389</v>
       </c>
       <c r="B58" s="137" t="s">
+        <v>1222</v>
+      </c>
+      <c r="C58" s="146" t="s">
+        <v>1223</v>
+      </c>
+      <c r="D58" s="122" t="s">
+        <v>1224</v>
+      </c>
+      <c r="E58" s="63" t="s">
         <v>1225</v>
       </c>
-      <c r="C58" s="146" t="s">
+      <c r="F58" s="74" t="s">
         <v>1226</v>
-      </c>
-      <c r="D58" s="122" t="s">
-        <v>1227</v>
-      </c>
-      <c r="E58" s="63" t="s">
-        <v>1228</v>
-      </c>
-      <c r="F58" s="74" t="s">
-        <v>1229</v>
       </c>
     </row>
     <row r="59" spans="1:6" s="30" customFormat="1" ht="48" x14ac:dyDescent="0.2">
@@ -16619,16 +16646,16 @@
         <v>389</v>
       </c>
       <c r="B59" s="137" t="s">
+        <v>1227</v>
+      </c>
+      <c r="C59" s="146" t="s">
+        <v>1228</v>
+      </c>
+      <c r="D59" s="122" t="s">
+        <v>1229</v>
+      </c>
+      <c r="E59" s="63" t="s">
         <v>1230</v>
-      </c>
-      <c r="C59" s="146" t="s">
-        <v>1231</v>
-      </c>
-      <c r="D59" s="122" t="s">
-        <v>1232</v>
-      </c>
-      <c r="E59" s="63" t="s">
-        <v>1233</v>
       </c>
     </row>
     <row r="60" spans="1:6" s="30" customFormat="1" ht="48" x14ac:dyDescent="0.2">
@@ -16636,16 +16663,16 @@
         <v>389</v>
       </c>
       <c r="B60" s="137" t="s">
+        <v>1231</v>
+      </c>
+      <c r="C60" s="146" t="s">
+        <v>1232</v>
+      </c>
+      <c r="D60" s="122" t="s">
+        <v>1233</v>
+      </c>
+      <c r="E60" s="63" t="s">
         <v>1234</v>
-      </c>
-      <c r="C60" s="146" t="s">
-        <v>1235</v>
-      </c>
-      <c r="D60" s="122" t="s">
-        <v>1236</v>
-      </c>
-      <c r="E60" s="63" t="s">
-        <v>1237</v>
       </c>
     </row>
     <row r="61" spans="1:6" s="30" customFormat="1" ht="48" x14ac:dyDescent="0.2">
@@ -16653,16 +16680,16 @@
         <v>389</v>
       </c>
       <c r="B61" s="18" t="s">
+        <v>1235</v>
+      </c>
+      <c r="C61" s="146" t="s">
+        <v>1236</v>
+      </c>
+      <c r="D61" s="122" t="s">
+        <v>1237</v>
+      </c>
+      <c r="E61" s="63" t="s">
         <v>1238</v>
-      </c>
-      <c r="C61" s="146" t="s">
-        <v>1239</v>
-      </c>
-      <c r="D61" s="122" t="s">
-        <v>1240</v>
-      </c>
-      <c r="E61" s="63" t="s">
-        <v>1241</v>
       </c>
     </row>
     <row r="62" spans="1:6" s="30" customFormat="1" ht="48" x14ac:dyDescent="0.2">
@@ -16670,16 +16697,16 @@
         <v>389</v>
       </c>
       <c r="B62" s="137" t="s">
+        <v>1239</v>
+      </c>
+      <c r="C62" s="146" t="s">
+        <v>1240</v>
+      </c>
+      <c r="D62" s="122" t="s">
+        <v>1241</v>
+      </c>
+      <c r="E62" s="80" t="s">
         <v>1242</v>
-      </c>
-      <c r="C62" s="146" t="s">
-        <v>1243</v>
-      </c>
-      <c r="D62" s="122" t="s">
-        <v>1244</v>
-      </c>
-      <c r="E62" s="80" t="s">
-        <v>1245</v>
       </c>
     </row>
     <row r="63" spans="1:6" ht="16" x14ac:dyDescent="0.2">
@@ -16687,14 +16714,14 @@
         <v>740</v>
       </c>
       <c r="B63" s="145" t="s">
-        <v>1246</v>
+        <v>1243</v>
       </c>
       <c r="C63" s="146" t="s">
-        <v>1247</v>
+        <v>1244</v>
       </c>
       <c r="D63" s="149"/>
       <c r="E63" s="79" t="s">
-        <v>1248</v>
+        <v>1245</v>
       </c>
       <c r="F63" s="136"/>
     </row>
@@ -16703,14 +16730,14 @@
         <v>740</v>
       </c>
       <c r="B64" s="145" t="s">
-        <v>1249</v>
+        <v>1246</v>
       </c>
       <c r="C64" s="146" t="s">
-        <v>1169</v>
+        <v>1166</v>
       </c>
       <c r="D64" s="149"/>
       <c r="E64" s="79" t="s">
-        <v>1170</v>
+        <v>1167</v>
       </c>
       <c r="F64" s="136"/>
     </row>
@@ -16719,14 +16746,14 @@
         <v>740</v>
       </c>
       <c r="B65" s="137" t="s">
-        <v>1250</v>
+        <v>1247</v>
       </c>
       <c r="C65" s="146" t="s">
-        <v>1156</v>
+        <v>1153</v>
       </c>
       <c r="D65" s="149"/>
       <c r="E65" s="79" t="s">
-        <v>1158</v>
+        <v>1155</v>
       </c>
       <c r="F65" s="136"/>
     </row>
@@ -16841,16 +16868,16 @@
         <v>243</v>
       </c>
       <c r="B2" s="5" t="s">
+        <v>1248</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>1249</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>1250</v>
+      </c>
+      <c r="F2" s="68" t="s">
         <v>1251</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>1252</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>1253</v>
-      </c>
-      <c r="F2" s="68" t="s">
-        <v>1254</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="32" x14ac:dyDescent="0.2">
@@ -16858,16 +16885,16 @@
         <v>254</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>1255</v>
+        <v>1252</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>923</v>
+        <v>920</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>1256</v>
+        <v>1253</v>
       </c>
       <c r="E3" s="37" t="s">
-        <v>924</v>
+        <v>921</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="16" x14ac:dyDescent="0.2">
@@ -16875,50 +16902,50 @@
         <v>32</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>1257</v>
+        <v>1254</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>874</v>
+        <v>871</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>1258</v>
+        <v>1255</v>
       </c>
       <c r="E4" s="37" t="s">
-        <v>876</v>
+        <v>873</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
-        <v>1259</v>
+        <v>1256</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>1260</v>
+        <v>1257</v>
       </c>
       <c r="C5" s="6" t="s">
         <v>152</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>1261</v>
+        <v>1258</v>
       </c>
       <c r="F5" s="68" t="s">
-        <v>1254</v>
+        <v>1251</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
+        <v>1256</v>
+      </c>
+      <c r="B6" s="5" t="s">
         <v>1259</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>1262</v>
       </c>
       <c r="C6" s="6" t="s">
         <v>140</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>1261</v>
+        <v>1258</v>
       </c>
       <c r="F6" s="68" t="s">
-        <v>1254</v>
+        <v>1251</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="32" x14ac:dyDescent="0.2">
@@ -16926,16 +16953,16 @@
         <v>254</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>1263</v>
+        <v>1260</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>926</v>
+        <v>923</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>1256</v>
+        <v>1253</v>
       </c>
       <c r="E7" s="37" t="s">
-        <v>927</v>
+        <v>924</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="16" x14ac:dyDescent="0.2">
@@ -16943,49 +16970,49 @@
         <v>32</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>1264</v>
+        <v>1261</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>929</v>
+        <v>926</v>
       </c>
       <c r="D8" s="1"/>
       <c r="E8" s="37" t="s">
-        <v>930</v>
+        <v>927</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
-        <v>1259</v>
+        <v>1256</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>1265</v>
+        <v>1262</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>935</v>
+        <v>932</v>
       </c>
       <c r="D9" s="1"/>
       <c r="E9" s="37" t="s">
-        <v>936</v>
+        <v>933</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="C10" s="27" t="s">
-        <v>1266</v>
+        <v>1263</v>
       </c>
       <c r="D10" s="18" t="s">
-        <v>1267</v>
+        <v>1264</v>
       </c>
       <c r="E10" s="37" t="s">
-        <v>1268</v>
+        <v>1265</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="C11" s="75" t="s">
-        <v>1269</v>
+        <v>1266</v>
       </c>
       <c r="D11" s="18"/>
       <c r="E11" s="37" t="s">
-        <v>1270</v>
+        <v>1267</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
@@ -17018,6 +17045,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <Readyforteam_x003f_ xmlns="565e1b1d-057e-4d85-b896-01a5881d8a45">false</Readyforteam_x003f_>
@@ -17056,15 +17092,6 @@
     <TaxCatchAll xmlns="2799d30d-6731-4efe-ac9b-c4895a8828d9" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -17345,6 +17372,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8D7CE8C7-18DC-484F-8376-ED09F13D44C8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{017ACE96-8143-486E-8436-7787F6B96F4A}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -17353,14 +17388,6 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
     <ds:schemaRef ds:uri="bf601f31-63a1-4825-9216-91d773c5ef9c"/>
     <ds:schemaRef ds:uri="2799d30d-6731-4efe-ac9b-c4895a8828d9"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8D7CE8C7-18DC-484F-8376-ED09F13D44C8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Bilingualling the qualifications and contact page in v11bi.
</commit_message>
<xml_diff>
--- a/app/data/MCCD-localisation.xlsx
+++ b/app/data/MCCD-localisation.xlsx
@@ -8,22 +8,23 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/JALAT/GIT/medical-certificate-of-cause-of-death/app/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F817A5AC-338C-8647-B0AE-F971B8C4BB58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE29E7A7-4D61-6E48-94C7-2A75ABA09A60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="14220" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="14220" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Using this document" sheetId="8" r:id="rId1"/>
     <sheet name="Global" sheetId="1" r:id="rId2"/>
     <sheet name="Start page" sheetId="7" r:id="rId3"/>
     <sheet name="CIS2 pages" sheetId="9" r:id="rId4"/>
-    <sheet name="Dashboard" sheetId="2" r:id="rId5"/>
-    <sheet name="Deceased persons details" sheetId="3" r:id="rId6"/>
-    <sheet name="Actions after death" sheetId="4" r:id="rId7"/>
-    <sheet name="Cause of death" sheetId="5" r:id="rId8"/>
-    <sheet name="MCCD Tasklist" sheetId="10" r:id="rId9"/>
-    <sheet name="Declaration and submission" sheetId="6" r:id="rId10"/>
-    <sheet name="Confirmation page" sheetId="11" r:id="rId11"/>
+    <sheet name="Onboarding" sheetId="12" r:id="rId5"/>
+    <sheet name="Dashboard" sheetId="2" r:id="rId6"/>
+    <sheet name="Deceased persons details" sheetId="3" r:id="rId7"/>
+    <sheet name="Actions after death" sheetId="4" r:id="rId8"/>
+    <sheet name="Cause of death" sheetId="5" r:id="rId9"/>
+    <sheet name="MCCD Tasklist" sheetId="10" r:id="rId10"/>
+    <sheet name="Declaration and submission" sheetId="6" r:id="rId11"/>
+    <sheet name="Confirmation page" sheetId="11" r:id="rId12"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -68,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2101" uniqueCount="1412">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2124" uniqueCount="1425">
   <si>
     <r>
       <rPr>
@@ -5751,9 +5752,6 @@
     <t>Dod o hyd i'r cyfeiriad gan ddefnyddio côd post</t>
   </si>
   <si>
-    <t>014</t>
-  </si>
-  <si>
     <t>For example, 21 8 2021 or 8 2021 if day of month is not known</t>
   </si>
   <si>
@@ -5764,13 +5762,55 @@
   </si>
   <si>
     <t>dpdDoBHintNeoNatal</t>
+  </si>
+  <si>
+    <t>qualificationPageTitle</t>
+  </si>
+  <si>
+    <t>What is your primary qualification?</t>
+  </si>
+  <si>
+    <t>qualificationPageHint</t>
+  </si>
+  <si>
+    <t>As registered by the GMC, for example MB ChB</t>
+  </si>
+  <si>
+    <t>Contact method</t>
+  </si>
+  <si>
+    <t>contactPageTitle</t>
+  </si>
+  <si>
+    <t>contactPageHint</t>
+  </si>
+  <si>
+    <t>How do you want the medical examiner office to contact you?</t>
+  </si>
+  <si>
+    <t>Following a review of this MCCD, a medical examiner officer or medical examiner may ask you to make an amendment.&lt;br /&gt;&lt;br /&gt;Enter an email address or phone number as your preferred method of contact.</t>
+  </si>
+  <si>
+    <t>Beth yw eich prif gymhwysiad?</t>
+  </si>
+  <si>
+    <t>Fel y cofrestrwyd gan y GMC, er enghraifft MB ChB</t>
+  </si>
+  <si>
+    <t>Sut ydych chi am i'r Swyddfa Arholwr Meddygol gysylltu â chi?</t>
+  </si>
+  <si>
+    <t>Yn dilyn adolygiad o'r MCCD hwn, gall swyddog arholwr meddygol neu arholwr meddygol ofyn i chi wneud diwygiad.&lt;br / &gt;&lt;br /&gt;Rhowch gyfeiriad e-bost neu rif ffôn fel eich dull cyswllt dewisol.</t>
+  </si>
+  <si>
+    <t>015</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="27" x14ac:knownFonts="1">
+  <fonts count="28" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -5966,6 +6006,12 @@
       <color rgb="FF595959"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="16">
@@ -6707,6 +6753,15 @@
     <xf numFmtId="0" fontId="13" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -6723,15 +6778,6 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -7731,6 +7777,227 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{609E324E-AF17-46CE-B967-049626EE1948}">
+  <dimension ref="A1:F17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F10" sqref="F10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="18.1640625" style="5" customWidth="1"/>
+    <col min="2" max="2" width="61" style="5" customWidth="1"/>
+    <col min="3" max="3" width="37" style="6" customWidth="1"/>
+    <col min="4" max="4" width="36" style="5" customWidth="1"/>
+    <col min="5" max="5" width="30.83203125" style="37" customWidth="1"/>
+    <col min="6" max="6" width="26.83203125" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.1640625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A1" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="47" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="136" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+      <c r="A2" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>1247</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>1248</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>1249</v>
+      </c>
+      <c r="F2" s="68" t="s">
+        <v>1250</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+      <c r="A3" s="5" t="s">
+        <v>254</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>1251</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>919</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>1252</v>
+      </c>
+      <c r="E3" s="37" t="s">
+        <v>920</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A4" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>1253</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>870</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>1254</v>
+      </c>
+      <c r="E4" s="37" t="s">
+        <v>872</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+      <c r="A5" s="5" t="s">
+        <v>1255</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>1256</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>152</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>1257</v>
+      </c>
+      <c r="F5" s="68" t="s">
+        <v>1250</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+      <c r="A6" s="5" t="s">
+        <v>1255</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>1258</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>140</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>1257</v>
+      </c>
+      <c r="F6" s="68" t="s">
+        <v>1250</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+      <c r="A7" s="5" t="s">
+        <v>254</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>1259</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>922</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>1252</v>
+      </c>
+      <c r="E7" s="37" t="s">
+        <v>923</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A8" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>1260</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>925</v>
+      </c>
+      <c r="D8" s="1"/>
+      <c r="E8" s="37" t="s">
+        <v>926</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A9" s="5" t="s">
+        <v>1255</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>1261</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>931</v>
+      </c>
+      <c r="D9" s="1"/>
+      <c r="E9" s="37" t="s">
+        <v>932</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+      <c r="C10" s="27" t="s">
+        <v>1262</v>
+      </c>
+      <c r="D10" s="18" t="s">
+        <v>1263</v>
+      </c>
+      <c r="E10" s="37" t="s">
+        <v>1264</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+      <c r="C11" s="75" t="s">
+        <v>1265</v>
+      </c>
+      <c r="D11" s="18"/>
+      <c r="E11" s="37" t="s">
+        <v>1266</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" s="18"/>
+      <c r="B12" s="28"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="18"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" s="18"/>
+      <c r="B13" s="28"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="18"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16" s="18"/>
+      <c r="B16" s="28"/>
+      <c r="C16" s="75"/>
+      <c r="D16" s="18"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" s="18"/>
+      <c r="B17" s="28"/>
+      <c r="C17" s="75"/>
+      <c r="D17" s="18"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E52C375-4A34-4943-A40B-CD02CAD0761B}">
   <dimension ref="A1:F24"/>
   <sheetViews>
@@ -8166,7 +8433,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{124C2F8F-96ED-4E65-B816-FFFEB93DC889}">
   <dimension ref="A1:F23"/>
   <sheetViews>
@@ -8515,9 +8782,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F68"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F3" sqref="F3"/>
+      <selection pane="bottomLeft" activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -8557,13 +8824,13 @@
         <v>7</v>
       </c>
       <c r="C2" s="101" t="s">
-        <v>1407</v>
+        <v>1424</v>
       </c>
       <c r="D2" s="99" t="s">
         <v>8</v>
       </c>
       <c r="E2" s="100" t="s">
-        <v>1407</v>
+        <v>1424</v>
       </c>
       <c r="F2" s="99"/>
     </row>
@@ -9905,12 +10172,275 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF7846F4-4C68-474D-A4ED-20A97546E87B}">
+  <dimension ref="A1:F27"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="16.5" customWidth="1"/>
+    <col min="2" max="2" width="29" customWidth="1"/>
+    <col min="3" max="3" width="33.5" customWidth="1"/>
+    <col min="5" max="5" width="60.6640625" customWidth="1"/>
+    <col min="6" max="6" width="21.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="39" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A2" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>1411</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>1412</v>
+      </c>
+      <c r="D2" s="5"/>
+      <c r="E2" s="43" t="s">
+        <v>1420</v>
+      </c>
+      <c r="F2" s="1"/>
+    </row>
+    <row r="3" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+      <c r="A3" s="5" t="s">
+        <v>491</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>1413</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>1414</v>
+      </c>
+      <c r="D3" s="5"/>
+      <c r="E3" s="43" t="s">
+        <v>1421</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" s="158" t="s">
+        <v>1415</v>
+      </c>
+      <c r="B4" s="159"/>
+      <c r="C4" s="159"/>
+      <c r="D4" s="159"/>
+      <c r="E4" s="160"/>
+    </row>
+    <row r="5" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+      <c r="A5" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>1416</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>1418</v>
+      </c>
+      <c r="D5" s="5"/>
+      <c r="E5" s="43" t="s">
+        <v>1422</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="96" x14ac:dyDescent="0.2">
+      <c r="A6" s="5" t="s">
+        <v>491</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>1417</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>1419</v>
+      </c>
+      <c r="D6" s="5"/>
+      <c r="E6" s="43" t="s">
+        <v>1423</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" s="5"/>
+      <c r="B7" s="5"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="43"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" s="5"/>
+      <c r="B8" s="5"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="43"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" s="5"/>
+      <c r="B9" s="5"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="43"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" s="5"/>
+      <c r="B10" s="5"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="43"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" s="5"/>
+      <c r="B11" s="5"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="43"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" s="5"/>
+      <c r="B12" s="5"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="43"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" s="5"/>
+      <c r="B13" s="5"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="43"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14" s="5"/>
+      <c r="B14" s="5"/>
+      <c r="C14" s="6"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="43"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15" s="5"/>
+      <c r="B15" s="5"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="43"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16" s="5"/>
+      <c r="B16" s="5"/>
+      <c r="C16" s="6"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="43"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17" s="5"/>
+      <c r="B17" s="5"/>
+      <c r="C17" s="6"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="43"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18" s="5"/>
+      <c r="B18" s="5"/>
+      <c r="C18" s="6"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="43"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19" s="5"/>
+      <c r="B19" s="5"/>
+      <c r="C19" s="6"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="43"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20" s="5"/>
+      <c r="B20" s="5"/>
+      <c r="C20" s="6"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="43"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21" s="5"/>
+      <c r="B21" s="5"/>
+      <c r="C21" s="6"/>
+      <c r="D21" s="5"/>
+      <c r="E21" s="43"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22" s="5"/>
+      <c r="B22" s="5"/>
+      <c r="C22" s="6"/>
+      <c r="D22" s="5"/>
+      <c r="E22" s="43"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A23" s="5"/>
+      <c r="B23" s="5"/>
+      <c r="C23" s="6"/>
+      <c r="D23" s="5"/>
+      <c r="E23" s="43"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A24" s="5"/>
+      <c r="B24" s="5"/>
+      <c r="C24" s="6"/>
+      <c r="D24" s="5"/>
+      <c r="E24" s="43"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A25" s="5"/>
+      <c r="B25" s="5"/>
+      <c r="C25" s="6"/>
+      <c r="D25" s="5"/>
+      <c r="E25" s="43"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A26" s="5"/>
+      <c r="B26" s="5"/>
+      <c r="C26" s="6"/>
+      <c r="D26" s="5"/>
+      <c r="E26" s="43"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A27" s="5"/>
+      <c r="B27" s="5"/>
+      <c r="C27" s="6"/>
+      <c r="D27" s="5"/>
+      <c r="E27" s="43"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A4:E4"/>
+  </mergeCells>
+  <phoneticPr fontId="27" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{344327F7-D7B0-4B8B-A26A-307F32EA23BD}">
   <dimension ref="A1:F30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H4" sqref="H4"/>
+      <selection pane="bottomLeft" activeCell="F2" sqref="A1:F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -10406,13 +10936,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B63483B8-55BE-4CA0-9111-55E5C0AEF6CB}">
   <dimension ref="A1:F345"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B47" sqref="B47"/>
+      <selection pane="bottomLeft" activeCell="A43" sqref="A43:E43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -10447,13 +10977,13 @@
       </c>
     </row>
     <row r="2" spans="1:6" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="161" t="s">
+      <c r="A2" s="164" t="s">
         <v>374</v>
       </c>
-      <c r="B2" s="162"/>
-      <c r="C2" s="162"/>
-      <c r="D2" s="162"/>
-      <c r="E2" s="163"/>
+      <c r="B2" s="165"/>
+      <c r="C2" s="165"/>
+      <c r="D2" s="165"/>
+      <c r="E2" s="166"/>
       <c r="F2" s="33"/>
     </row>
     <row r="3" spans="1:6" ht="48" x14ac:dyDescent="0.2">
@@ -10581,13 +11111,13 @@
       <c r="F9" s="120"/>
     </row>
     <row r="10" spans="1:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="164" t="s">
+      <c r="A10" s="167" t="s">
         <v>403</v>
       </c>
-      <c r="B10" s="165"/>
-      <c r="C10" s="165"/>
-      <c r="D10" s="165"/>
-      <c r="E10" s="166"/>
+      <c r="B10" s="168"/>
+      <c r="C10" s="168"/>
+      <c r="D10" s="168"/>
+      <c r="E10" s="169"/>
       <c r="F10" s="120"/>
     </row>
     <row r="11" spans="1:6" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -11108,7 +11638,7 @@
         <v>492</v>
       </c>
       <c r="C45" s="59" t="s">
-        <v>1408</v>
+        <v>1407</v>
       </c>
       <c r="D45" s="117"/>
       <c r="E45" s="121" t="s">
@@ -11121,14 +11651,14 @@
         <v>491</v>
       </c>
       <c r="B46" s="117" t="s">
-        <v>1411</v>
+        <v>1410</v>
       </c>
       <c r="C46" s="59" t="s">
-        <v>1409</v>
+        <v>1408</v>
       </c>
       <c r="D46" s="117"/>
       <c r="E46" s="121" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="F46" s="120"/>
     </row>
@@ -12921,13 +13451,13 @@
       <c r="F164" s="120"/>
     </row>
     <row r="165" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A165" s="167" t="s">
+      <c r="A165" s="161" t="s">
         <v>772</v>
       </c>
-      <c r="B165" s="168"/>
-      <c r="C165" s="168"/>
-      <c r="D165" s="168"/>
-      <c r="E165" s="169"/>
+      <c r="B165" s="162"/>
+      <c r="C165" s="162"/>
+      <c r="D165" s="162"/>
+      <c r="E165" s="163"/>
       <c r="F165" s="130" t="s">
         <v>773</v>
       </c>
@@ -14830,6 +15360,18 @@
     </row>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="A225:E225"/>
+    <mergeCell ref="A186:E186"/>
+    <mergeCell ref="A190:E190"/>
+    <mergeCell ref="A197:E197"/>
+    <mergeCell ref="A208:E208"/>
+    <mergeCell ref="A214:E214"/>
+    <mergeCell ref="A58:E58"/>
+    <mergeCell ref="A2:E2"/>
+    <mergeCell ref="A10:E10"/>
+    <mergeCell ref="A14:E14"/>
+    <mergeCell ref="A24:E24"/>
+    <mergeCell ref="A43:E43"/>
     <mergeCell ref="A174:E174"/>
     <mergeCell ref="A157:E157"/>
     <mergeCell ref="A63:E63"/>
@@ -14840,24 +15382,12 @@
     <mergeCell ref="A146:E146"/>
     <mergeCell ref="A92:E92"/>
     <mergeCell ref="A165:E165"/>
-    <mergeCell ref="A58:E58"/>
-    <mergeCell ref="A2:E2"/>
-    <mergeCell ref="A10:E10"/>
-    <mergeCell ref="A14:E14"/>
-    <mergeCell ref="A24:E24"/>
-    <mergeCell ref="A43:E43"/>
-    <mergeCell ref="A225:E225"/>
-    <mergeCell ref="A186:E186"/>
-    <mergeCell ref="A190:E190"/>
-    <mergeCell ref="A197:E197"/>
-    <mergeCell ref="A208:E208"/>
-    <mergeCell ref="A214:E214"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E7FE5E2-8B99-45DF-8804-30523FDA4B3A}">
   <dimension ref="A1:F54"/>
   <sheetViews>
@@ -15682,7 +16212,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6CA2FE89-1BCA-4888-9BB6-D7A7737E07E4}">
   <dimension ref="A1:F73"/>
   <sheetViews>
@@ -16828,228 +17358,16 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{609E324E-AF17-46CE-B967-049626EE1948}">
-  <dimension ref="A1:F17"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F10" sqref="F10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="18.1640625" style="5" customWidth="1"/>
-    <col min="2" max="2" width="61" style="5" customWidth="1"/>
-    <col min="3" max="3" width="37" style="6" customWidth="1"/>
-    <col min="4" max="4" width="36" style="5" customWidth="1"/>
-    <col min="5" max="5" width="30.83203125" style="37" customWidth="1"/>
-    <col min="6" max="6" width="26.83203125" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.1640625" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A1" s="14" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" s="15" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="E1" s="47" t="s">
-        <v>5</v>
-      </c>
-      <c r="F1" s="136" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="32" x14ac:dyDescent="0.2">
-      <c r="A2" s="5" t="s">
-        <v>243</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>1247</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>1248</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>1249</v>
-      </c>
-      <c r="F2" s="68" t="s">
-        <v>1250</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="32" x14ac:dyDescent="0.2">
-      <c r="A3" s="5" t="s">
-        <v>254</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>1251</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>919</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>1252</v>
-      </c>
-      <c r="E3" s="37" t="s">
-        <v>920</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A4" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>1253</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>870</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>1254</v>
-      </c>
-      <c r="E4" s="37" t="s">
-        <v>872</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="32" x14ac:dyDescent="0.2">
-      <c r="A5" s="5" t="s">
-        <v>1255</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>1256</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>152</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>1257</v>
-      </c>
-      <c r="F5" s="68" t="s">
-        <v>1250</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="32" x14ac:dyDescent="0.2">
-      <c r="A6" s="5" t="s">
-        <v>1255</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>1258</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>140</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>1257</v>
-      </c>
-      <c r="F6" s="68" t="s">
-        <v>1250</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="32" x14ac:dyDescent="0.2">
-      <c r="A7" s="5" t="s">
-        <v>254</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>1259</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>922</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>1252</v>
-      </c>
-      <c r="E7" s="37" t="s">
-        <v>923</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A8" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>1260</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>925</v>
-      </c>
-      <c r="D8" s="1"/>
-      <c r="E8" s="37" t="s">
-        <v>926</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A9" s="5" t="s">
-        <v>1255</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>1261</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>931</v>
-      </c>
-      <c r="D9" s="1"/>
-      <c r="E9" s="37" t="s">
-        <v>932</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="48" x14ac:dyDescent="0.2">
-      <c r="C10" s="27" t="s">
-        <v>1262</v>
-      </c>
-      <c r="D10" s="18" t="s">
-        <v>1263</v>
-      </c>
-      <c r="E10" s="37" t="s">
-        <v>1264</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="32" x14ac:dyDescent="0.2">
-      <c r="C11" s="75" t="s">
-        <v>1265</v>
-      </c>
-      <c r="D11" s="18"/>
-      <c r="E11" s="37" t="s">
-        <v>1266</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A12" s="18"/>
-      <c r="B12" s="28"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="18"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A13" s="18"/>
-      <c r="B13" s="28"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="18"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A16" s="18"/>
-      <c r="B16" s="28"/>
-      <c r="C16" s="75"/>
-      <c r="D16" s="18"/>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" s="18"/>
-      <c r="B17" s="28"/>
-      <c r="C17" s="75"/>
-      <c r="D17" s="18"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <Readyforteam_x003f_ xmlns="565e1b1d-057e-4d85-b896-01a5881d8a45">false</Readyforteam_x003f_>
@@ -17088,15 +17406,6 @@
     <TaxCatchAll xmlns="2799d30d-6731-4efe-ac9b-c4895a8828d9" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -17377,6 +17686,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8D7CE8C7-18DC-484F-8376-ED09F13D44C8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{017ACE96-8143-486E-8436-7787F6B96F4A}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -17385,14 +17702,6 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
     <ds:schemaRef ds:uri="bf601f31-63a1-4825-9216-91d773c5ef9c"/>
     <ds:schemaRef ds:uri="2799d30d-6731-4efe-ac9b-c4895a8828d9"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8D7CE8C7-18DC-484F-8376-ED09F13D44C8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
[MCCDB-631] Prototype Change - Check your answers (ME MCCD)
</commit_message>
<xml_diff>
--- a/app/data/MCCD-localisation.xlsx
+++ b/app/data/MCCD-localisation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/JALAT/GIT/medical-certificate-of-cause-of-death/app/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D5C8C7A-8A17-E14E-94AC-CB28724ACA10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A3CB76E-8E81-CE4B-9EEF-46C05EF45A4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="14220" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -69,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2132" uniqueCount="1428">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2133" uniqueCount="1427">
   <si>
     <r>
       <rPr>
@@ -3854,9 +3854,6 @@
     <t>Provides further context to AP or ME about what they need to do when before continuing</t>
   </si>
   <si>
-    <t>Gwiriwch fod yr holl fanylion yn gywir cyn i chi gyflwyno'r Dystysgrif Feddygol hon o achos marwolaeth i'w harchwilio gan archwiliwr meddygol</t>
-  </si>
-  <si>
     <t>dpdCheckAnswersNHSNumber</t>
   </si>
   <si>
@@ -4326,9 +4323,6 @@
   </si>
   <si>
     <t>Provides further context to AP or ME about what they need to do before continuing</t>
-  </si>
-  <si>
-    <t>Gwiriwch fod yr holl fanylion yn gywir cyn i chi gyflwyno'r Dystysgrif Feddygol hon o achos marwolaeth i'w harchwilio gan archwiliwr meddygol.</t>
   </si>
   <si>
     <t>aadCheckAnswersPostMortem</t>
@@ -5617,12 +5611,6 @@
     <t>You have not created any certificates</t>
   </si>
   <si>
-    <t>Check that all the details are correct before you submit this Medical certificate of cause of death for scrutiny by a medical examiner</t>
-  </si>
-  <si>
-    <t>Check that all the details are correct before you submit this Medical certificate of cause of death for scrutiny by a medical examiner.</t>
-  </si>
-  <si>
     <t>Did the deceased’s pregnancy contribute to their death?</t>
   </si>
   <si>
@@ -5662,7 +5650,16 @@
     <t>&lt;p class="govuk-body"&gt;Mae'r dangosfwrdd hwn yn eich galluogi i greu Tystysgrif Feddygol achos marwolaeth (MCCD) newydd a rheoli MCCDs presennol.&lt;/p&gt;&lt;p class="govuk-body"&gt;Bydd y dangosfwrdd hwn yn rhestru MCCDs sydd:&lt;/p&gt;&lt;ul class="govuk-list govuk-list--bullet"&gt;&lt;li&gt;rydych wedi cyflwyno i archwiliwr meddygol i'w gymeradwyo&lt;/li&gt;&lt;li&gt;mae archwiliwr meddygol wedi gwrthod a rhaid i chi nawr ddiwygio&lt;/li&gt;&lt;li&gt;bod archwiliwr meddygol wedi cymeradwyo a bydd yn cael ei anfon ymlaen i swyddfa’r cofrestrydd gan swyddog archwiliwr meddygol&lt;/li&gt;&lt;/ul&gt;&lt;p class="govuk-body"&gt;Bydd MCCDs wedi'u cwblhau yn cael eu dileu ar ôl tri mis.&lt;/p&gt;</t>
   </si>
   <si>
-    <t>018</t>
+    <t>Check that all the details are correct before continuing.</t>
+  </si>
+  <si>
+    <t>Gwiriwch fod yr holl fanylion yn gywir cyn parhau.</t>
+  </si>
+  <si>
+    <t>019</t>
+  </si>
+  <si>
+    <t>Tystysgrif feddygol achos gwasanaeth marwolaeth</t>
   </si>
 </sst>
 </file>
@@ -6615,6 +6612,15 @@
     <xf numFmtId="0" fontId="13" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -6631,15 +6637,6 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -7683,16 +7680,16 @@
         <v>243</v>
       </c>
       <c r="B2" s="5" t="s">
+        <v>1232</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>1233</v>
+      </c>
+      <c r="D2" s="5" t="s">
         <v>1234</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="F2" s="68" t="s">
         <v>1235</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>1236</v>
-      </c>
-      <c r="F2" s="68" t="s">
-        <v>1237</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="32" x14ac:dyDescent="0.2">
@@ -7700,16 +7697,16 @@
         <v>254</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>1238</v>
+        <v>1236</v>
       </c>
       <c r="C3" s="6" t="s">
+        <v>910</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>1237</v>
+      </c>
+      <c r="E3" s="37" t="s">
         <v>911</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>1239</v>
-      </c>
-      <c r="E3" s="37" t="s">
-        <v>912</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="16" x14ac:dyDescent="0.2">
@@ -7717,13 +7714,13 @@
         <v>32</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>1240</v>
+        <v>1238</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>863</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>1241</v>
+        <v>1239</v>
       </c>
       <c r="E4" s="37" t="s">
         <v>865</v>
@@ -7731,36 +7728,36 @@
     </row>
     <row r="5" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
-        <v>1242</v>
+        <v>1240</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>1243</v>
+        <v>1241</v>
       </c>
       <c r="C5" s="6" t="s">
         <v>152</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>1244</v>
+        <v>1242</v>
       </c>
       <c r="F5" s="68" t="s">
-        <v>1237</v>
+        <v>1235</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
-        <v>1242</v>
+        <v>1240</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>1245</v>
+        <v>1243</v>
       </c>
       <c r="C6" s="6" t="s">
         <v>140</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>1244</v>
+        <v>1242</v>
       </c>
       <c r="F6" s="68" t="s">
-        <v>1237</v>
+        <v>1235</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="32" x14ac:dyDescent="0.2">
@@ -7768,16 +7765,16 @@
         <v>254</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>1246</v>
+        <v>1244</v>
       </c>
       <c r="C7" s="6" t="s">
+        <v>913</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>1237</v>
+      </c>
+      <c r="E7" s="37" t="s">
         <v>914</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>1239</v>
-      </c>
-      <c r="E7" s="37" t="s">
-        <v>915</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="16" x14ac:dyDescent="0.2">
@@ -7785,49 +7782,49 @@
         <v>32</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>1247</v>
+        <v>1245</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>917</v>
+        <v>916</v>
       </c>
       <c r="D8" s="1"/>
       <c r="E8" s="37" t="s">
-        <v>918</v>
+        <v>917</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
-        <v>1242</v>
+        <v>1240</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>1248</v>
+        <v>1246</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="D9" s="1"/>
       <c r="E9" s="37" t="s">
-        <v>924</v>
+        <v>923</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="C10" s="27" t="s">
+        <v>1247</v>
+      </c>
+      <c r="D10" s="18" t="s">
+        <v>1248</v>
+      </c>
+      <c r="E10" s="37" t="s">
         <v>1249</v>
-      </c>
-      <c r="D10" s="18" t="s">
-        <v>1250</v>
-      </c>
-      <c r="E10" s="37" t="s">
-        <v>1251</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="C11" s="74" t="s">
-        <v>1252</v>
+        <v>1250</v>
       </c>
       <c r="D11" s="18"/>
       <c r="E11" s="37" t="s">
-        <v>1253</v>
+        <v>1251</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
@@ -7904,33 +7901,33 @@
         <v>243</v>
       </c>
       <c r="B2" s="92" t="s">
+        <v>1252</v>
+      </c>
+      <c r="C2" s="93" t="s">
+        <v>1253</v>
+      </c>
+      <c r="D2" s="92" t="s">
         <v>1254</v>
       </c>
-      <c r="C2" s="93" t="s">
+      <c r="E2" s="85" t="s">
         <v>1255</v>
-      </c>
-      <c r="D2" s="92" t="s">
-        <v>1256</v>
-      </c>
-      <c r="E2" s="85" t="s">
-        <v>1257</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="80" x14ac:dyDescent="0.2">
       <c r="A3" s="94" t="s">
+        <v>1256</v>
+      </c>
+      <c r="B3" s="95" t="s">
+        <v>1257</v>
+      </c>
+      <c r="C3" s="96" t="s">
         <v>1258</v>
       </c>
-      <c r="B3" s="95" t="s">
+      <c r="D3" s="95" t="s">
         <v>1259</v>
       </c>
-      <c r="C3" s="96" t="s">
+      <c r="E3" s="89" t="s">
         <v>1260</v>
-      </c>
-      <c r="D3" s="95" t="s">
-        <v>1261</v>
-      </c>
-      <c r="E3" s="89" t="s">
-        <v>1262</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="16" x14ac:dyDescent="0.2">
@@ -7938,16 +7935,16 @@
         <v>758</v>
       </c>
       <c r="B4" s="95" t="s">
-        <v>1263</v>
+        <v>1261</v>
       </c>
       <c r="C4" s="96" t="s">
-        <v>1264</v>
+        <v>1262</v>
       </c>
       <c r="D4" s="95" t="s">
         <v>404</v>
       </c>
       <c r="E4" s="89" t="s">
-        <v>1265</v>
+        <v>1263</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="60.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -7955,13 +7952,13 @@
         <v>410</v>
       </c>
       <c r="B5" s="105" t="s">
-        <v>1266</v>
+        <v>1264</v>
       </c>
       <c r="C5" s="106" t="s">
         <v>404</v>
       </c>
       <c r="D5" s="107" t="s">
-        <v>1267</v>
+        <v>1265</v>
       </c>
       <c r="E5" s="89" t="s">
         <v>404</v>
@@ -7972,13 +7969,13 @@
         <v>413</v>
       </c>
       <c r="B6" s="105" t="s">
-        <v>1268</v>
+        <v>1266</v>
       </c>
       <c r="C6" s="106" t="s">
         <v>404</v>
       </c>
       <c r="D6" s="107" t="s">
-        <v>1269</v>
+        <v>1267</v>
       </c>
       <c r="E6" s="89" t="s">
         <v>404</v>
@@ -8006,33 +8003,33 @@
         <v>243</v>
       </c>
       <c r="B8" s="95" t="s">
+        <v>1268</v>
+      </c>
+      <c r="C8" s="96" t="s">
+        <v>1269</v>
+      </c>
+      <c r="D8" s="95" t="s">
         <v>1270</v>
       </c>
-      <c r="C8" s="96" t="s">
+      <c r="E8" s="89" t="s">
         <v>1271</v>
-      </c>
-      <c r="D8" s="95" t="s">
-        <v>1272</v>
-      </c>
-      <c r="E8" s="89" t="s">
-        <v>1273</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="64" x14ac:dyDescent="0.2">
       <c r="A9" s="94" t="s">
-        <v>1258</v>
+        <v>1256</v>
       </c>
       <c r="B9" s="95" t="s">
+        <v>1272</v>
+      </c>
+      <c r="C9" s="96" t="s">
+        <v>1273</v>
+      </c>
+      <c r="D9" s="95" t="s">
         <v>1274</v>
       </c>
-      <c r="C9" s="96" t="s">
+      <c r="E9" s="89" t="s">
         <v>1275</v>
-      </c>
-      <c r="D9" s="95" t="s">
-        <v>1276</v>
-      </c>
-      <c r="E9" s="89" t="s">
-        <v>1277</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="16" x14ac:dyDescent="0.2">
@@ -8040,10 +8037,10 @@
         <v>758</v>
       </c>
       <c r="B10" s="95" t="s">
-        <v>1278</v>
+        <v>1276</v>
       </c>
       <c r="C10" s="96" t="s">
-        <v>1279</v>
+        <v>1277</v>
       </c>
       <c r="D10" s="95" t="s">
         <v>404</v>
@@ -8057,13 +8054,13 @@
         <v>410</v>
       </c>
       <c r="B11" s="105" t="s">
-        <v>1280</v>
+        <v>1278</v>
       </c>
       <c r="C11" s="106" t="s">
         <v>404</v>
       </c>
       <c r="D11" s="107" t="s">
-        <v>1267</v>
+        <v>1265</v>
       </c>
       <c r="E11" s="89" t="s">
         <v>404</v>
@@ -8074,13 +8071,13 @@
         <v>413</v>
       </c>
       <c r="B12" s="105" t="s">
-        <v>1281</v>
+        <v>1279</v>
       </c>
       <c r="C12" s="106" t="s">
         <v>404</v>
       </c>
       <c r="D12" s="107" t="s">
-        <v>1269</v>
+        <v>1267</v>
       </c>
       <c r="E12" s="89" t="s">
         <v>404</v>
@@ -8108,13 +8105,13 @@
         <v>243</v>
       </c>
       <c r="B14" s="95" t="s">
+        <v>1280</v>
+      </c>
+      <c r="C14" s="96" t="s">
+        <v>1281</v>
+      </c>
+      <c r="D14" s="95" t="s">
         <v>1282</v>
-      </c>
-      <c r="C14" s="96" t="s">
-        <v>1283</v>
-      </c>
-      <c r="D14" s="95" t="s">
-        <v>1284</v>
       </c>
       <c r="E14" s="89" t="s">
         <v>404</v>
@@ -8122,19 +8119,19 @@
     </row>
     <row r="15" spans="1:6" ht="96" x14ac:dyDescent="0.2">
       <c r="A15" s="94" t="s">
-        <v>1258</v>
+        <v>1256</v>
       </c>
       <c r="B15" s="95" t="s">
+        <v>1283</v>
+      </c>
+      <c r="C15" s="96" t="s">
+        <v>1284</v>
+      </c>
+      <c r="D15" s="95" t="s">
         <v>1285</v>
       </c>
-      <c r="C15" s="96" t="s">
+      <c r="E15" s="89" t="s">
         <v>1286</v>
-      </c>
-      <c r="D15" s="95" t="s">
-        <v>1287</v>
-      </c>
-      <c r="E15" s="89" t="s">
-        <v>1288</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="48" x14ac:dyDescent="0.2">
@@ -8142,13 +8139,13 @@
         <v>410</v>
       </c>
       <c r="B16" s="105" t="s">
-        <v>1289</v>
+        <v>1287</v>
       </c>
       <c r="C16" s="106" t="s">
         <v>404</v>
       </c>
       <c r="D16" s="107" t="s">
-        <v>1267</v>
+        <v>1265</v>
       </c>
       <c r="E16" s="89" t="s">
         <v>404</v>
@@ -8159,13 +8156,13 @@
         <v>413</v>
       </c>
       <c r="B17" s="105" t="s">
-        <v>1290</v>
+        <v>1288</v>
       </c>
       <c r="C17" s="106" t="s">
         <v>404</v>
       </c>
       <c r="D17" s="107" t="s">
-        <v>1269</v>
+        <v>1267</v>
       </c>
       <c r="E17" s="89" t="s">
         <v>404</v>
@@ -8176,16 +8173,16 @@
         <v>14</v>
       </c>
       <c r="B18" s="95" t="s">
-        <v>1291</v>
+        <v>1289</v>
       </c>
       <c r="C18" s="96" t="s">
-        <v>1292</v>
+        <v>1290</v>
       </c>
       <c r="D18" s="95" t="s">
         <v>404</v>
       </c>
       <c r="E18" s="89" t="s">
-        <v>1293</v>
+        <v>1291</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -8210,13 +8207,13 @@
         <v>243</v>
       </c>
       <c r="B20" s="95" t="s">
-        <v>1294</v>
+        <v>1292</v>
       </c>
       <c r="C20" s="96" t="s">
-        <v>1295</v>
+        <v>1293</v>
       </c>
       <c r="D20" s="95" t="s">
-        <v>1256</v>
+        <v>1254</v>
       </c>
       <c r="E20" s="89" t="s">
         <v>404</v>
@@ -8224,16 +8221,16 @@
     </row>
     <row r="21" spans="1:5" ht="48" x14ac:dyDescent="0.2">
       <c r="A21" s="94" t="s">
-        <v>1258</v>
+        <v>1256</v>
       </c>
       <c r="B21" s="95" t="s">
+        <v>1294</v>
+      </c>
+      <c r="C21" s="96" t="s">
+        <v>1295</v>
+      </c>
+      <c r="D21" s="95" t="s">
         <v>1296</v>
-      </c>
-      <c r="C21" s="96" t="s">
-        <v>1297</v>
-      </c>
-      <c r="D21" s="95" t="s">
-        <v>1298</v>
       </c>
       <c r="E21" s="89" t="s">
         <v>404</v>
@@ -8244,10 +8241,10 @@
         <v>758</v>
       </c>
       <c r="B22" s="95" t="s">
-        <v>1299</v>
+        <v>1297</v>
       </c>
       <c r="C22" s="96" t="s">
-        <v>1300</v>
+        <v>1298</v>
       </c>
       <c r="D22" s="95" t="s">
         <v>404</v>
@@ -8261,13 +8258,13 @@
         <v>410</v>
       </c>
       <c r="B23" s="105" t="s">
-        <v>1301</v>
+        <v>1299</v>
       </c>
       <c r="C23" s="106" t="s">
         <v>404</v>
       </c>
       <c r="D23" s="107" t="s">
-        <v>1267</v>
+        <v>1265</v>
       </c>
       <c r="E23" s="89" t="s">
         <v>404</v>
@@ -8278,13 +8275,13 @@
         <v>413</v>
       </c>
       <c r="B24" s="105" t="s">
-        <v>1302</v>
+        <v>1300</v>
       </c>
       <c r="C24" s="106" t="s">
         <v>404</v>
       </c>
       <c r="D24" s="107" t="s">
-        <v>1269</v>
+        <v>1267</v>
       </c>
       <c r="E24" s="89" t="s">
         <v>404</v>
@@ -8337,7 +8334,7 @@
     </row>
     <row r="2" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="193" t="s">
-        <v>1303</v>
+        <v>1301</v>
       </c>
       <c r="B2" s="194"/>
       <c r="C2" s="194"/>
@@ -8350,16 +8347,16 @@
         <v>243</v>
       </c>
       <c r="B3" s="5" t="s">
+        <v>1302</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>1303</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>1234</v>
+      </c>
+      <c r="E3" s="37" t="s">
         <v>1304</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>1305</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>1236</v>
-      </c>
-      <c r="E3" s="37" t="s">
-        <v>1306</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="32" x14ac:dyDescent="0.2">
@@ -8367,13 +8364,13 @@
         <v>261</v>
       </c>
       <c r="B4" s="5" t="s">
+        <v>1305</v>
+      </c>
+      <c r="C4" s="59" t="s">
+        <v>1306</v>
+      </c>
+      <c r="E4" s="37" t="s">
         <v>1307</v>
-      </c>
-      <c r="C4" s="59" t="s">
-        <v>1308</v>
-      </c>
-      <c r="E4" s="37" t="s">
-        <v>1309</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="16" x14ac:dyDescent="0.2">
@@ -8381,13 +8378,13 @@
         <v>254</v>
       </c>
       <c r="B5" s="5" t="s">
+        <v>1308</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>1309</v>
+      </c>
+      <c r="E5" s="37" t="s">
         <v>1310</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>1311</v>
-      </c>
-      <c r="E5" s="37" t="s">
-        <v>1312</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="80" x14ac:dyDescent="0.2">
@@ -8395,13 +8392,13 @@
         <v>261</v>
       </c>
       <c r="B6" s="5" t="s">
+        <v>1311</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>1312</v>
+      </c>
+      <c r="E6" s="37" t="s">
         <v>1313</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>1314</v>
-      </c>
-      <c r="E6" s="37" t="s">
-        <v>1315</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="32" x14ac:dyDescent="0.2">
@@ -8409,127 +8406,127 @@
         <v>254</v>
       </c>
       <c r="B7" s="5" t="s">
+        <v>1314</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>1315</v>
+      </c>
+      <c r="E7" s="37" t="s">
         <v>1316</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>1317</v>
-      </c>
-      <c r="E7" s="37" t="s">
-        <v>1318</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
+        <v>1317</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>1318</v>
+      </c>
+      <c r="C8" s="6" t="s">
         <v>1319</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="E8" s="37" t="s">
         <v>1320</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>1321</v>
-      </c>
-      <c r="E8" s="37" t="s">
-        <v>1322</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
+        <v>1321</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>1322</v>
+      </c>
+      <c r="C9" s="6" t="s">
         <v>1323</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="E9" s="37" t="s">
         <v>1324</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>1325</v>
-      </c>
-      <c r="E9" s="37" t="s">
-        <v>1326</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
-        <v>1323</v>
+        <v>1321</v>
       </c>
       <c r="B10" s="5" t="s">
+        <v>1325</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>1326</v>
+      </c>
+      <c r="E10" s="37" t="s">
         <v>1327</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>1328</v>
-      </c>
-      <c r="E10" s="37" t="s">
-        <v>1329</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
-        <v>1323</v>
+        <v>1321</v>
       </c>
       <c r="B11" s="5" t="s">
+        <v>1328</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>1329</v>
+      </c>
+      <c r="E11" s="37" t="s">
         <v>1330</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>1331</v>
-      </c>
-      <c r="E11" s="37" t="s">
-        <v>1332</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="5" t="s">
-        <v>1323</v>
+        <v>1321</v>
       </c>
       <c r="B12" s="5" t="s">
+        <v>1331</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>1332</v>
+      </c>
+      <c r="E12" s="37" t="s">
         <v>1333</v>
-      </c>
-      <c r="C12" s="6" t="s">
-        <v>1334</v>
-      </c>
-      <c r="E12" s="37" t="s">
-        <v>1335</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="s">
-        <v>1323</v>
+        <v>1321</v>
       </c>
       <c r="B13" s="5" t="s">
+        <v>1334</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>1335</v>
+      </c>
+      <c r="E13" s="37" t="s">
         <v>1336</v>
-      </c>
-      <c r="C13" s="6" t="s">
-        <v>1337</v>
-      </c>
-      <c r="E13" s="37" t="s">
-        <v>1338</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A14" s="5" t="s">
-        <v>1319</v>
+        <v>1317</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>1339</v>
+        <v>1337</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>1340</v>
+        <v>1338</v>
       </c>
       <c r="D14" s="1"/>
       <c r="E14" s="37" t="s">
-        <v>1341</v>
+        <v>1339</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A15" s="5" t="s">
-        <v>953</v>
+        <v>952</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>1342</v>
+        <v>1340</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>1343</v>
+        <v>1341</v>
       </c>
       <c r="D15" s="1"/>
       <c r="E15" s="37" t="s">
-        <v>1344</v>
+        <v>1342</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="16" x14ac:dyDescent="0.2">
@@ -8537,34 +8534,34 @@
         <v>14</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>1345</v>
+        <v>1343</v>
       </c>
       <c r="C16" s="74" t="s">
-        <v>1346</v>
+        <v>1344</v>
       </c>
       <c r="D16" s="18"/>
       <c r="E16" s="37" t="s">
-        <v>1347</v>
+        <v>1345</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A17" s="5" t="s">
+        <v>1346</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>1347</v>
+      </c>
+      <c r="C17" s="75" t="s">
         <v>1348</v>
-      </c>
-      <c r="B17" s="7" t="s">
-        <v>1349</v>
-      </c>
-      <c r="C17" s="75" t="s">
-        <v>1350</v>
       </c>
       <c r="D17" s="18"/>
       <c r="E17" s="37" t="s">
-        <v>1351</v>
+        <v>1349</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="193" t="s">
-        <v>1352</v>
+        <v>1350</v>
       </c>
       <c r="B18" s="194"/>
       <c r="C18" s="194"/>
@@ -8577,16 +8574,16 @@
         <v>243</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>1355</v>
+        <v>1353</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>1353</v>
+        <v>1351</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>1236</v>
+        <v>1234</v>
       </c>
       <c r="E19" s="37" t="s">
-        <v>1354</v>
+        <v>1352</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="64" x14ac:dyDescent="0.2">
@@ -8594,10 +8591,10 @@
         <v>261</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>1356</v>
+        <v>1354</v>
       </c>
       <c r="C20" s="59" t="s">
-        <v>1367</v>
+        <v>1365</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="16" x14ac:dyDescent="0.2">
@@ -8605,13 +8602,13 @@
         <v>254</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>1357</v>
+        <v>1355</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>1311</v>
+        <v>1309</v>
       </c>
       <c r="E21" s="37" t="s">
-        <v>1312</v>
+        <v>1310</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="128" x14ac:dyDescent="0.2">
@@ -8619,10 +8616,10 @@
         <v>261</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>1358</v>
+        <v>1356</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>1368</v>
+        <v>1366</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
@@ -8646,7 +8643,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G4" sqref="G4"/>
+      <selection pane="bottomLeft" activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -8686,13 +8683,13 @@
         <v>7</v>
       </c>
       <c r="C2" s="100" t="s">
-        <v>1427</v>
+        <v>1425</v>
       </c>
       <c r="D2" s="98" t="s">
         <v>8</v>
       </c>
       <c r="E2" s="99" t="s">
-        <v>1427</v>
+        <v>1425</v>
       </c>
       <c r="F2" s="98"/>
     </row>
@@ -8709,7 +8706,9 @@
       <c r="D3" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="37"/>
+      <c r="E3" s="37" t="s">
+        <v>1426</v>
+      </c>
       <c r="F3" s="5" t="s">
         <v>13</v>
       </c>
@@ -9763,18 +9762,18 @@
     </row>
     <row r="67" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="B67" s="1" t="s">
-        <v>1371</v>
+        <v>1369</v>
       </c>
       <c r="C67" s="2" t="s">
+        <v>1370</v>
+      </c>
+      <c r="E67" s="40" t="s">
         <v>1372</v>
-      </c>
-      <c r="E67" s="40" t="s">
-        <v>1374</v>
       </c>
     </row>
     <row r="68" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="B68" s="1" t="s">
-        <v>1373</v>
+        <v>1371</v>
       </c>
       <c r="C68" s="2" t="s">
         <v>76</v>
@@ -10075,14 +10074,14 @@
         <v>243</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>1398</v>
+        <v>1396</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>1399</v>
+        <v>1397</v>
       </c>
       <c r="D2" s="5"/>
       <c r="E2" s="43" t="s">
-        <v>1407</v>
+        <v>1405</v>
       </c>
       <c r="F2" s="1"/>
     </row>
@@ -10091,19 +10090,19 @@
         <v>484</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>1400</v>
+        <v>1398</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>1401</v>
+        <v>1399</v>
       </c>
       <c r="D3" s="5"/>
       <c r="E3" s="43" t="s">
-        <v>1408</v>
+        <v>1406</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="159" t="s">
-        <v>1402</v>
+        <v>1400</v>
       </c>
       <c r="B4" s="160"/>
       <c r="C4" s="160"/>
@@ -10115,14 +10114,14 @@
         <v>243</v>
       </c>
       <c r="B5" s="5" t="s">
+        <v>1401</v>
+      </c>
+      <c r="C5" s="6" t="s">
         <v>1403</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>1405</v>
       </c>
       <c r="D5" s="5"/>
       <c r="E5" s="43" t="s">
-        <v>1409</v>
+        <v>1407</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="96" x14ac:dyDescent="0.2">
@@ -10130,14 +10129,14 @@
         <v>484</v>
       </c>
       <c r="B6" s="5" t="s">
+        <v>1402</v>
+      </c>
+      <c r="C6" s="6" t="s">
         <v>1404</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>1406</v>
       </c>
       <c r="D6" s="5"/>
       <c r="E6" s="43" t="s">
-        <v>1410</v>
+        <v>1408</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
@@ -10358,7 +10357,7 @@
         <v>243</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>1415</v>
+        <v>1411</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>276</v>
@@ -10382,7 +10381,7 @@
         <v>246</v>
       </c>
       <c r="E4" s="43" t="s">
-        <v>1416</v>
+        <v>1412</v>
       </c>
       <c r="F4" s="68" t="s">
         <v>280</v>
@@ -10396,13 +10395,13 @@
         <v>281</v>
       </c>
       <c r="C5" s="52" t="s">
-        <v>1421</v>
+        <v>1417</v>
       </c>
       <c r="D5" s="66" t="s">
         <v>282</v>
       </c>
       <c r="E5" s="156" t="s">
-        <v>1426</v>
+        <v>1422</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>283</v>
@@ -10416,13 +10415,13 @@
         <v>284</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>1422</v>
+        <v>1418</v>
       </c>
       <c r="D6" s="67" t="s">
         <v>285</v>
       </c>
       <c r="E6" s="157" t="s">
-        <v>1423</v>
+        <v>1419</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="160" x14ac:dyDescent="0.2">
@@ -10433,13 +10432,13 @@
         <v>286</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>1424</v>
+        <v>1420</v>
       </c>
       <c r="D7" s="67" t="s">
         <v>287</v>
       </c>
       <c r="E7" s="157" t="s">
-        <v>1425</v>
+        <v>1421</v>
       </c>
       <c r="F7" s="68" t="s">
         <v>288</v>
@@ -10641,7 +10640,7 @@
         <v>336</v>
       </c>
       <c r="C19" s="64" t="s">
-        <v>1411</v>
+        <v>1409</v>
       </c>
       <c r="D19" s="7" t="s">
         <v>337</v>
@@ -10775,17 +10774,17 @@
     </row>
     <row r="27" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A27" s="5" t="s">
-        <v>1419</v>
+        <v>1415</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>1420</v>
+        <v>1416</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>1417</v>
+        <v>1413</v>
       </c>
       <c r="D27" s="5"/>
       <c r="E27" s="37" t="s">
-        <v>1418</v>
+        <v>1414</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
@@ -10826,8 +10825,8 @@
   <dimension ref="A1:F345"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A212" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C228" sqref="C228"/>
+      <pane ySplit="1" topLeftCell="A223" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F228" sqref="F228"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -10862,13 +10861,13 @@
       </c>
     </row>
     <row r="2" spans="1:6" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="162" t="s">
+      <c r="A2" s="165" t="s">
         <v>367</v>
       </c>
-      <c r="B2" s="163"/>
-      <c r="C2" s="163"/>
-      <c r="D2" s="163"/>
-      <c r="E2" s="164"/>
+      <c r="B2" s="166"/>
+      <c r="C2" s="166"/>
+      <c r="D2" s="166"/>
+      <c r="E2" s="167"/>
       <c r="F2" s="33"/>
     </row>
     <row r="3" spans="1:6" ht="48" x14ac:dyDescent="0.2">
@@ -10996,13 +10995,13 @@
       <c r="F9" s="119"/>
     </row>
     <row r="10" spans="1:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="165" t="s">
+      <c r="A10" s="168" t="s">
         <v>396</v>
       </c>
-      <c r="B10" s="166"/>
-      <c r="C10" s="166"/>
-      <c r="D10" s="166"/>
-      <c r="E10" s="167"/>
+      <c r="B10" s="169"/>
+      <c r="C10" s="169"/>
+      <c r="D10" s="169"/>
+      <c r="E10" s="170"/>
       <c r="F10" s="119"/>
     </row>
     <row r="11" spans="1:6" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -11031,13 +11030,13 @@
         <v>401</v>
       </c>
       <c r="C12" s="153" t="s">
-        <v>1375</v>
+        <v>1373</v>
       </c>
       <c r="D12" s="84" t="s">
         <v>402</v>
       </c>
       <c r="E12" s="152" t="s">
-        <v>1376</v>
+        <v>1374</v>
       </c>
       <c r="F12" s="86"/>
     </row>
@@ -11049,13 +11048,13 @@
         <v>403</v>
       </c>
       <c r="C13" s="154" t="s">
-        <v>1377</v>
+        <v>1375</v>
       </c>
       <c r="D13" s="88" t="s">
         <v>404</v>
       </c>
       <c r="E13" s="155" t="s">
-        <v>1378</v>
+        <v>1376</v>
       </c>
       <c r="F13" s="86"/>
     </row>
@@ -11523,7 +11522,7 @@
         <v>485</v>
       </c>
       <c r="C45" s="59" t="s">
-        <v>1394</v>
+        <v>1392</v>
       </c>
       <c r="D45" s="116"/>
       <c r="E45" s="120" t="s">
@@ -11536,14 +11535,14 @@
         <v>484</v>
       </c>
       <c r="B46" s="116" t="s">
-        <v>1397</v>
+        <v>1395</v>
       </c>
       <c r="C46" s="59" t="s">
-        <v>1395</v>
+        <v>1393</v>
       </c>
       <c r="D46" s="116"/>
       <c r="E46" s="120" t="s">
-        <v>1396</v>
+        <v>1394</v>
       </c>
       <c r="F46" s="119"/>
     </row>
@@ -11771,7 +11770,7 @@
         <v>522</v>
       </c>
       <c r="E61" s="120" t="s">
-        <v>1387</v>
+        <v>1385</v>
       </c>
       <c r="F61" s="119"/>
     </row>
@@ -11780,14 +11779,14 @@
         <v>519</v>
       </c>
       <c r="B62" s="116" t="s">
+        <v>1382</v>
+      </c>
+      <c r="C62" s="117" t="s">
         <v>1384</v>
-      </c>
-      <c r="C62" s="117" t="s">
-        <v>1386</v>
       </c>
       <c r="D62" s="116"/>
       <c r="E62" s="120" t="s">
-        <v>1385</v>
+        <v>1383</v>
       </c>
       <c r="F62" s="119"/>
     </row>
@@ -12973,7 +12972,7 @@
         <v>710</v>
       </c>
       <c r="C141" s="113" t="s">
-        <v>1360</v>
+        <v>1358</v>
       </c>
       <c r="D141" s="122" t="s">
         <v>711</v>
@@ -13063,7 +13062,7 @@
         <v>725</v>
       </c>
       <c r="C147" s="59" t="s">
-        <v>1359</v>
+        <v>1357</v>
       </c>
       <c r="D147" s="116" t="s">
         <v>726</v>
@@ -13094,14 +13093,14 @@
         <v>37</v>
       </c>
       <c r="B149" s="116" t="s">
+        <v>1359</v>
+      </c>
+      <c r="C149" s="59" t="s">
         <v>1361</v>
-      </c>
-      <c r="C149" s="59" t="s">
-        <v>1363</v>
       </c>
       <c r="D149" s="116"/>
       <c r="E149" s="120" t="s">
-        <v>1365</v>
+        <v>1363</v>
       </c>
       <c r="F149" s="119"/>
     </row>
@@ -13110,14 +13109,14 @@
         <v>37</v>
       </c>
       <c r="B150" s="116" t="s">
+        <v>1360</v>
+      </c>
+      <c r="C150" s="59" t="s">
         <v>1362</v>
-      </c>
-      <c r="C150" s="59" t="s">
-        <v>1364</v>
       </c>
       <c r="D150" s="116"/>
       <c r="E150" s="120" t="s">
-        <v>1366</v>
+        <v>1364</v>
       </c>
       <c r="F150" s="119"/>
     </row>
@@ -13336,13 +13335,13 @@
       <c r="F164" s="119"/>
     </row>
     <row r="165" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A165" s="168" t="s">
+      <c r="A165" s="162" t="s">
         <v>765</v>
       </c>
-      <c r="B165" s="169"/>
-      <c r="C165" s="169"/>
-      <c r="D165" s="169"/>
-      <c r="E165" s="170"/>
+      <c r="B165" s="163"/>
+      <c r="C165" s="163"/>
+      <c r="D165" s="163"/>
+      <c r="E165" s="164"/>
       <c r="F165" s="129" t="s">
         <v>766</v>
       </c>
@@ -13769,13 +13768,13 @@
         <v>815</v>
       </c>
       <c r="C193" s="59" t="s">
-        <v>1379</v>
+        <v>1377</v>
       </c>
       <c r="D193" s="116" t="s">
         <v>816</v>
       </c>
       <c r="E193" s="120" t="s">
-        <v>1383</v>
+        <v>1381</v>
       </c>
       <c r="F193" s="119"/>
     </row>
@@ -13784,14 +13783,14 @@
         <v>484</v>
       </c>
       <c r="B194" s="116" t="s">
-        <v>1380</v>
+        <v>1378</v>
       </c>
       <c r="C194" s="59" t="s">
-        <v>1381</v>
+        <v>1379</v>
       </c>
       <c r="D194" s="116"/>
       <c r="E194" s="120" t="s">
-        <v>1382</v>
+        <v>1380</v>
       </c>
       <c r="F194" s="119"/>
     </row>
@@ -13891,11 +13890,11 @@
         <v>827</v>
       </c>
       <c r="C201" s="117" t="s">
-        <v>1390</v>
+        <v>1388</v>
       </c>
       <c r="D201" s="116"/>
       <c r="E201" s="120" t="s">
-        <v>1393</v>
+        <v>1391</v>
       </c>
       <c r="F201" s="119"/>
     </row>
@@ -13904,7 +13903,7 @@
         <v>734</v>
       </c>
       <c r="B202" s="116" t="s">
-        <v>1392</v>
+        <v>1390</v>
       </c>
       <c r="C202" s="117" t="s">
         <v>43</v>
@@ -13920,14 +13919,14 @@
         <v>32</v>
       </c>
       <c r="B203" s="116" t="s">
-        <v>1391</v>
+        <v>1389</v>
       </c>
       <c r="C203" s="134" t="s">
-        <v>1388</v>
+        <v>1386</v>
       </c>
       <c r="D203" s="116"/>
       <c r="E203" s="120" t="s">
-        <v>1389</v>
+        <v>1387</v>
       </c>
       <c r="F203" s="119"/>
     </row>
@@ -14291,7 +14290,7 @@
       </c>
       <c r="F227" s="119"/>
     </row>
-    <row r="228" spans="1:6" ht="64" x14ac:dyDescent="0.2">
+    <row r="228" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A228" s="116" t="s">
         <v>261</v>
       </c>
@@ -14299,13 +14298,13 @@
         <v>866</v>
       </c>
       <c r="C228" s="59" t="s">
-        <v>1412</v>
+        <v>1423</v>
       </c>
       <c r="D228" s="116" t="s">
         <v>867</v>
       </c>
       <c r="E228" s="120" t="s">
-        <v>868</v>
+        <v>1424</v>
       </c>
       <c r="F228" s="119"/>
     </row>
@@ -14314,16 +14313,16 @@
         <v>382</v>
       </c>
       <c r="B229" s="116" t="s">
+        <v>868</v>
+      </c>
+      <c r="C229" s="117" t="s">
         <v>869</v>
       </c>
-      <c r="C229" s="117" t="s">
+      <c r="D229" s="121" t="s">
         <v>870</v>
       </c>
-      <c r="D229" s="121" t="s">
+      <c r="E229" s="120" t="s">
         <v>871</v>
-      </c>
-      <c r="E229" s="120" t="s">
-        <v>872</v>
       </c>
       <c r="F229" s="119"/>
     </row>
@@ -14332,13 +14331,13 @@
         <v>382</v>
       </c>
       <c r="B230" s="116" t="s">
-        <v>873</v>
+        <v>872</v>
       </c>
       <c r="C230" s="117" t="s">
         <v>384</v>
       </c>
       <c r="D230" s="121" t="s">
-        <v>874</v>
+        <v>873</v>
       </c>
       <c r="E230" s="120" t="s">
         <v>386</v>
@@ -14350,16 +14349,16 @@
         <v>382</v>
       </c>
       <c r="B231" s="116" t="s">
+        <v>874</v>
+      </c>
+      <c r="C231" s="117" t="s">
         <v>875</v>
       </c>
-      <c r="C231" s="117" t="s">
+      <c r="D231" s="121" t="s">
         <v>876</v>
       </c>
-      <c r="D231" s="121" t="s">
+      <c r="E231" s="120" t="s">
         <v>877</v>
-      </c>
-      <c r="E231" s="120" t="s">
-        <v>878</v>
       </c>
       <c r="F231" s="119"/>
     </row>
@@ -14368,16 +14367,16 @@
         <v>382</v>
       </c>
       <c r="B232" s="116" t="s">
+        <v>878</v>
+      </c>
+      <c r="C232" s="117" t="s">
         <v>879</v>
       </c>
-      <c r="C232" s="117" t="s">
+      <c r="D232" s="121" t="s">
         <v>880</v>
       </c>
-      <c r="D232" s="121" t="s">
+      <c r="E232" s="120" t="s">
         <v>881</v>
-      </c>
-      <c r="E232" s="120" t="s">
-        <v>882</v>
       </c>
       <c r="F232" s="119"/>
     </row>
@@ -14386,16 +14385,16 @@
         <v>382</v>
       </c>
       <c r="B233" s="116" t="s">
+        <v>882</v>
+      </c>
+      <c r="C233" s="117" t="s">
         <v>883</v>
       </c>
-      <c r="C233" s="117" t="s">
+      <c r="D233" s="121" t="s">
         <v>884</v>
       </c>
-      <c r="D233" s="121" t="s">
+      <c r="E233" s="120" t="s">
         <v>885</v>
-      </c>
-      <c r="E233" s="120" t="s">
-        <v>886</v>
       </c>
       <c r="F233" s="119"/>
     </row>
@@ -14404,16 +14403,16 @@
         <v>490</v>
       </c>
       <c r="B234" s="116" t="s">
+        <v>886</v>
+      </c>
+      <c r="C234" s="117" t="s">
         <v>887</v>
       </c>
-      <c r="C234" s="117" t="s">
+      <c r="D234" s="121" t="s">
+        <v>884</v>
+      </c>
+      <c r="E234" s="120" t="s">
         <v>888</v>
-      </c>
-      <c r="D234" s="121" t="s">
-        <v>885</v>
-      </c>
-      <c r="E234" s="120" t="s">
-        <v>889</v>
       </c>
       <c r="F234" s="119"/>
     </row>
@@ -14422,16 +14421,16 @@
         <v>382</v>
       </c>
       <c r="B235" s="116" t="s">
+        <v>889</v>
+      </c>
+      <c r="C235" s="117" t="s">
         <v>890</v>
       </c>
-      <c r="C235" s="117" t="s">
+      <c r="D235" s="121" t="s">
         <v>891</v>
       </c>
-      <c r="D235" s="121" t="s">
+      <c r="E235" s="120" t="s">
         <v>892</v>
-      </c>
-      <c r="E235" s="120" t="s">
-        <v>893</v>
       </c>
       <c r="F235" s="119"/>
     </row>
@@ -14440,13 +14439,13 @@
         <v>382</v>
       </c>
       <c r="B236" s="116" t="s">
-        <v>894</v>
+        <v>893</v>
       </c>
       <c r="C236" s="117" t="s">
         <v>317</v>
       </c>
       <c r="D236" s="121" t="s">
-        <v>895</v>
+        <v>894</v>
       </c>
       <c r="E236" s="120" t="s">
         <v>319</v>
@@ -14458,16 +14457,16 @@
         <v>382</v>
       </c>
       <c r="B237" s="116" t="s">
+        <v>895</v>
+      </c>
+      <c r="C237" s="117" t="s">
         <v>896</v>
       </c>
-      <c r="C237" s="117" t="s">
+      <c r="D237" s="121" t="s">
         <v>897</v>
       </c>
-      <c r="D237" s="121" t="s">
+      <c r="E237" s="120" t="s">
         <v>898</v>
-      </c>
-      <c r="E237" s="120" t="s">
-        <v>899</v>
       </c>
       <c r="F237" s="119"/>
     </row>
@@ -14476,16 +14475,16 @@
         <v>382</v>
       </c>
       <c r="B238" s="116" t="s">
+        <v>899</v>
+      </c>
+      <c r="C238" s="117" t="s">
         <v>900</v>
       </c>
-      <c r="C238" s="117" t="s">
+      <c r="D238" s="121" t="s">
         <v>901</v>
       </c>
-      <c r="D238" s="121" t="s">
+      <c r="E238" s="120" t="s">
         <v>902</v>
-      </c>
-      <c r="E238" s="120" t="s">
-        <v>903</v>
       </c>
       <c r="F238" s="119"/>
     </row>
@@ -14493,12 +14492,12 @@
       <c r="A239" s="5"/>
       <c r="B239" s="5"/>
       <c r="C239" s="6" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
       <c r="D239" s="5"/>
       <c r="E239" s="37"/>
       <c r="F239" s="68" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
     </row>
     <row r="240" spans="1:6" x14ac:dyDescent="0.2">
@@ -15245,6 +15244,18 @@
     </row>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="A225:E225"/>
+    <mergeCell ref="A186:E186"/>
+    <mergeCell ref="A190:E190"/>
+    <mergeCell ref="A197:E197"/>
+    <mergeCell ref="A208:E208"/>
+    <mergeCell ref="A214:E214"/>
+    <mergeCell ref="A58:E58"/>
+    <mergeCell ref="A2:E2"/>
+    <mergeCell ref="A10:E10"/>
+    <mergeCell ref="A14:E14"/>
+    <mergeCell ref="A24:E24"/>
+    <mergeCell ref="A43:E43"/>
     <mergeCell ref="A174:E174"/>
     <mergeCell ref="A157:E157"/>
     <mergeCell ref="A63:E63"/>
@@ -15255,18 +15266,6 @@
     <mergeCell ref="A146:E146"/>
     <mergeCell ref="A92:E92"/>
     <mergeCell ref="A165:E165"/>
-    <mergeCell ref="A58:E58"/>
-    <mergeCell ref="A2:E2"/>
-    <mergeCell ref="A10:E10"/>
-    <mergeCell ref="A14:E14"/>
-    <mergeCell ref="A24:E24"/>
-    <mergeCell ref="A43:E43"/>
-    <mergeCell ref="A225:E225"/>
-    <mergeCell ref="A186:E186"/>
-    <mergeCell ref="A190:E190"/>
-    <mergeCell ref="A197:E197"/>
-    <mergeCell ref="A208:E208"/>
-    <mergeCell ref="A214:E214"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -15277,8 +15276,8 @@
   <dimension ref="A1:F54"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C45" sqref="C45"/>
+      <pane ySplit="1" topLeftCell="A39" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D44" sqref="D44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -15314,7 +15313,7 @@
     </row>
     <row r="2" spans="1:6" s="24" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="174" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
       <c r="B2" s="175"/>
       <c r="C2" s="175"/>
@@ -15326,28 +15325,28 @@
         <v>243</v>
       </c>
       <c r="B3" s="19" t="s">
+        <v>906</v>
+      </c>
+      <c r="C3" s="21" t="s">
         <v>907</v>
-      </c>
-      <c r="C3" s="21" t="s">
-        <v>908</v>
       </c>
       <c r="D3" s="5"/>
       <c r="E3" s="46" t="s">
-        <v>909</v>
+        <v>908</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="19" t="s">
+        <v>909</v>
+      </c>
+      <c r="B4" s="19" t="s">
+        <v>906</v>
+      </c>
+      <c r="C4" s="21" t="s">
         <v>910</v>
       </c>
-      <c r="B4" s="19" t="s">
-        <v>907</v>
-      </c>
-      <c r="C4" s="21" t="s">
+      <c r="E4" s="46" t="s">
         <v>911</v>
-      </c>
-      <c r="E4" s="46" t="s">
-        <v>912</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="16" x14ac:dyDescent="0.2">
@@ -15355,7 +15354,7 @@
         <v>732</v>
       </c>
       <c r="B5" s="19" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
       <c r="C5" s="21" t="s">
         <v>863</v>
@@ -15366,16 +15365,16 @@
     </row>
     <row r="6" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="19" t="s">
-        <v>910</v>
+        <v>909</v>
       </c>
       <c r="B6" s="19" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
       <c r="C6" s="21" t="s">
+        <v>913</v>
+      </c>
+      <c r="E6" s="46" t="s">
         <v>914</v>
-      </c>
-      <c r="E6" s="46" t="s">
-        <v>915</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="16" x14ac:dyDescent="0.2">
@@ -15383,30 +15382,30 @@
         <v>732</v>
       </c>
       <c r="B7" s="19" t="s">
+        <v>915</v>
+      </c>
+      <c r="C7" s="21" t="s">
         <v>916</v>
       </c>
-      <c r="C7" s="21" t="s">
+      <c r="E7" s="46" t="s">
         <v>917</v>
-      </c>
-      <c r="E7" s="46" t="s">
-        <v>918</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="91" t="s">
-        <v>910</v>
+        <v>909</v>
       </c>
       <c r="B8" s="92" t="s">
+        <v>918</v>
+      </c>
+      <c r="C8" s="93" t="s">
         <v>919</v>
-      </c>
-      <c r="C8" s="93" t="s">
-        <v>920</v>
       </c>
       <c r="D8" s="92" t="s">
         <v>404</v>
       </c>
       <c r="E8" s="85" t="s">
-        <v>921</v>
+        <v>920</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="16" x14ac:dyDescent="0.2">
@@ -15414,22 +15413,22 @@
         <v>732</v>
       </c>
       <c r="B9" s="28" t="s">
+        <v>921</v>
+      </c>
+      <c r="C9" s="27" t="s">
         <v>922</v>
-      </c>
-      <c r="C9" s="27" t="s">
-        <v>923</v>
       </c>
       <c r="D9" s="18"/>
       <c r="E9" s="46" t="s">
-        <v>924</v>
+        <v>923</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="19" t="s">
+        <v>924</v>
+      </c>
+      <c r="B10" s="19" t="s">
         <v>925</v>
-      </c>
-      <c r="B10" s="19" t="s">
-        <v>926</v>
       </c>
       <c r="C10" s="21" t="s">
         <v>152</v>
@@ -15440,10 +15439,10 @@
     </row>
     <row r="11" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="19" t="s">
-        <v>925</v>
+        <v>924</v>
       </c>
       <c r="B11" s="19" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="C11" s="21" t="s">
         <v>140</v>
@@ -15454,7 +15453,7 @@
     </row>
     <row r="12" spans="1:6" s="24" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="174" t="s">
-        <v>928</v>
+        <v>927</v>
       </c>
       <c r="B12" s="175"/>
       <c r="C12" s="175"/>
@@ -15466,16 +15465,16 @@
         <v>243</v>
       </c>
       <c r="B13" s="19" t="s">
+        <v>928</v>
+      </c>
+      <c r="C13" s="21" t="s">
         <v>929</v>
       </c>
-      <c r="C13" s="21" t="s">
+      <c r="D13" s="5" t="s">
         <v>930</v>
       </c>
-      <c r="D13" s="5" t="s">
+      <c r="E13" s="46" t="s">
         <v>931</v>
-      </c>
-      <c r="E13" s="46" t="s">
-        <v>932</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="32" x14ac:dyDescent="0.2">
@@ -15483,16 +15482,16 @@
         <v>84</v>
       </c>
       <c r="B14" s="19" t="s">
+        <v>932</v>
+      </c>
+      <c r="C14" s="21" t="s">
         <v>933</v>
       </c>
-      <c r="C14" s="21" t="s">
+      <c r="D14" s="19" t="s">
         <v>934</v>
       </c>
-      <c r="D14" s="19" t="s">
+      <c r="E14" s="46" t="s">
         <v>935</v>
-      </c>
-      <c r="E14" s="46" t="s">
-        <v>936</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="32" x14ac:dyDescent="0.2">
@@ -15500,16 +15499,16 @@
         <v>84</v>
       </c>
       <c r="B15" s="19" t="s">
+        <v>936</v>
+      </c>
+      <c r="C15" s="21" t="s">
         <v>937</v>
       </c>
-      <c r="C15" s="21" t="s">
+      <c r="D15" s="19" t="s">
+        <v>934</v>
+      </c>
+      <c r="E15" s="46" t="s">
         <v>938</v>
-      </c>
-      <c r="D15" s="19" t="s">
-        <v>935</v>
-      </c>
-      <c r="E15" s="46" t="s">
-        <v>939</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="16" x14ac:dyDescent="0.2">
@@ -15517,16 +15516,16 @@
         <v>84</v>
       </c>
       <c r="B16" s="19" t="s">
+        <v>939</v>
+      </c>
+      <c r="C16" s="21" t="s">
         <v>940</v>
       </c>
-      <c r="C16" s="21" t="s">
+      <c r="D16" s="19" t="s">
+        <v>934</v>
+      </c>
+      <c r="E16" s="46" t="s">
         <v>941</v>
-      </c>
-      <c r="D16" s="19" t="s">
-        <v>935</v>
-      </c>
-      <c r="E16" s="46" t="s">
-        <v>942</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="48" x14ac:dyDescent="0.2">
@@ -15534,16 +15533,16 @@
         <v>84</v>
       </c>
       <c r="B17" s="92" t="s">
-        <v>943</v>
+        <v>942</v>
       </c>
       <c r="C17" s="151" t="s">
-        <v>1369</v>
+        <v>1367</v>
       </c>
       <c r="D17" s="92" t="s">
-        <v>935</v>
+        <v>934</v>
       </c>
       <c r="E17" s="152" t="s">
-        <v>1370</v>
+        <v>1368</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="80" x14ac:dyDescent="0.2">
@@ -15551,11 +15550,11 @@
         <v>410</v>
       </c>
       <c r="B18" s="28" t="s">
-        <v>944</v>
+        <v>943</v>
       </c>
       <c r="C18" s="27"/>
       <c r="D18" s="18" t="s">
-        <v>945</v>
+        <v>944</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="80" x14ac:dyDescent="0.2">
@@ -15563,16 +15562,16 @@
         <v>413</v>
       </c>
       <c r="B19" s="28" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="C19" s="27"/>
       <c r="D19" s="18" t="s">
-        <v>947</v>
+        <v>946</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="183" t="s">
-        <v>948</v>
+        <v>947</v>
       </c>
       <c r="B20" s="184"/>
       <c r="C20" s="184"/>
@@ -15581,52 +15580,52 @@
     </row>
     <row r="21" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A21" s="5" t="s">
+        <v>948</v>
+      </c>
+      <c r="B21" s="91" t="s">
         <v>949</v>
       </c>
-      <c r="B21" s="91" t="s">
+      <c r="C21" s="6" t="s">
         <v>950</v>
-      </c>
-      <c r="C21" s="6" t="s">
-        <v>951</v>
       </c>
       <c r="D21" s="80"/>
       <c r="E21" s="81" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A22" s="80" t="s">
+        <v>952</v>
+      </c>
+      <c r="B22" s="94" t="s">
         <v>953</v>
       </c>
-      <c r="B22" s="94" t="s">
+      <c r="C22" s="82" t="s">
         <v>954</v>
-      </c>
-      <c r="C22" s="82" t="s">
-        <v>955</v>
       </c>
       <c r="D22" s="80"/>
       <c r="E22" s="81" t="s">
-        <v>956</v>
+        <v>955</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="64" x14ac:dyDescent="0.2">
       <c r="A23" s="80" t="s">
+        <v>956</v>
+      </c>
+      <c r="B23" s="94" t="s">
         <v>957</v>
       </c>
-      <c r="B23" s="94" t="s">
+      <c r="C23" s="82" t="s">
         <v>958</v>
-      </c>
-      <c r="C23" s="82" t="s">
-        <v>959</v>
       </c>
       <c r="D23" s="80"/>
       <c r="E23" s="81" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" s="180" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
       <c r="B24" s="181"/>
       <c r="C24" s="181"/>
@@ -15638,19 +15637,19 @@
         <v>243</v>
       </c>
       <c r="B25" s="28" t="s">
+        <v>961</v>
+      </c>
+      <c r="C25" s="27" t="s">
         <v>962</v>
-      </c>
-      <c r="C25" s="27" t="s">
-        <v>963</v>
       </c>
       <c r="D25" s="18"/>
       <c r="E25" s="46" t="s">
-        <v>964</v>
+        <v>963</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" s="171" t="s">
-        <v>965</v>
+        <v>964</v>
       </c>
       <c r="B26" s="172"/>
       <c r="C26" s="172"/>
@@ -15662,19 +15661,19 @@
         <v>243</v>
       </c>
       <c r="B27" s="28" t="s">
+        <v>965</v>
+      </c>
+      <c r="C27" s="27" t="s">
         <v>966</v>
-      </c>
-      <c r="C27" s="27" t="s">
-        <v>967</v>
       </c>
       <c r="D27" s="18"/>
       <c r="E27" s="46" t="s">
-        <v>968</v>
+        <v>967</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" s="171" t="s">
-        <v>969</v>
+        <v>968</v>
       </c>
       <c r="B28" s="172"/>
       <c r="C28" s="172"/>
@@ -15686,53 +15685,53 @@
         <v>243</v>
       </c>
       <c r="B29" s="92" t="s">
+        <v>969</v>
+      </c>
+      <c r="C29" s="93" t="s">
         <v>970</v>
       </c>
-      <c r="C29" s="93" t="s">
+      <c r="D29" s="92" t="s">
         <v>971</v>
       </c>
-      <c r="D29" s="92" t="s">
+      <c r="E29" s="85" t="s">
         <v>972</v>
       </c>
-      <c r="E29" s="85" t="s">
+      <c r="F29" s="71" t="s">
         <v>973</v>
-      </c>
-      <c r="F29" s="71" t="s">
-        <v>974</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A30" s="94" t="s">
-        <v>953</v>
+        <v>952</v>
       </c>
       <c r="B30" s="95" t="s">
+        <v>974</v>
+      </c>
+      <c r="C30" s="96" t="s">
         <v>975</v>
       </c>
-      <c r="C30" s="96" t="s">
+      <c r="D30" s="95" t="s">
         <v>976</v>
       </c>
-      <c r="D30" s="95" t="s">
+      <c r="E30" s="89" t="s">
         <v>977</v>
-      </c>
-      <c r="E30" s="89" t="s">
-        <v>978</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="335" x14ac:dyDescent="0.2">
       <c r="A31" s="94" t="s">
+        <v>978</v>
+      </c>
+      <c r="B31" s="95" t="s">
         <v>979</v>
       </c>
-      <c r="B31" s="95" t="s">
+      <c r="C31" s="96" t="s">
         <v>980</v>
-      </c>
-      <c r="C31" s="96" t="s">
-        <v>981</v>
       </c>
       <c r="D31" s="95" t="s">
         <v>404</v>
       </c>
       <c r="E31" s="89" t="s">
-        <v>982</v>
+        <v>981</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="96" x14ac:dyDescent="0.2">
@@ -15740,13 +15739,13 @@
         <v>261</v>
       </c>
       <c r="B32" s="19" t="s">
+        <v>982</v>
+      </c>
+      <c r="C32" s="21" t="s">
         <v>983</v>
       </c>
-      <c r="C32" s="21" t="s">
+      <c r="E32" s="46" t="s">
         <v>984</v>
-      </c>
-      <c r="E32" s="46" t="s">
-        <v>985</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="48" x14ac:dyDescent="0.2">
@@ -15754,16 +15753,16 @@
         <v>37</v>
       </c>
       <c r="B33" s="19" t="s">
+        <v>985</v>
+      </c>
+      <c r="C33" s="21" t="s">
         <v>986</v>
       </c>
-      <c r="C33" s="21" t="s">
+      <c r="D33" s="26" t="s">
         <v>987</v>
       </c>
-      <c r="D33" s="26" t="s">
+      <c r="E33" s="46" t="s">
         <v>988</v>
-      </c>
-      <c r="E33" s="46" t="s">
-        <v>989</v>
       </c>
     </row>
     <row r="34" spans="1:6" ht="96" x14ac:dyDescent="0.2">
@@ -15771,11 +15770,11 @@
         <v>410</v>
       </c>
       <c r="B34" s="28" t="s">
-        <v>990</v>
+        <v>989</v>
       </c>
       <c r="C34" s="27"/>
       <c r="D34" s="18" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
     </row>
     <row r="35" spans="1:6" ht="80" x14ac:dyDescent="0.2">
@@ -15783,11 +15782,11 @@
         <v>410</v>
       </c>
       <c r="B35" s="28" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="C35" s="27"/>
       <c r="D35" s="18" t="s">
-        <v>993</v>
+        <v>992</v>
       </c>
     </row>
     <row r="36" spans="1:6" ht="80" x14ac:dyDescent="0.2">
@@ -15795,16 +15794,16 @@
         <v>413</v>
       </c>
       <c r="B36" s="28" t="s">
-        <v>994</v>
+        <v>993</v>
       </c>
       <c r="C36" s="27"/>
       <c r="D36" s="18" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" s="171" t="s">
-        <v>996</v>
+        <v>995</v>
       </c>
       <c r="B37" s="172"/>
       <c r="C37" s="172"/>
@@ -15816,16 +15815,16 @@
         <v>243</v>
       </c>
       <c r="B38" s="19" t="s">
+        <v>996</v>
+      </c>
+      <c r="C38" s="21" t="s">
         <v>997</v>
       </c>
-      <c r="C38" s="21" t="s">
+      <c r="D38" s="5" t="s">
         <v>998</v>
       </c>
-      <c r="D38" s="5" t="s">
+      <c r="E38" s="46" t="s">
         <v>999</v>
-      </c>
-      <c r="E38" s="46" t="s">
-        <v>1000</v>
       </c>
     </row>
     <row r="39" spans="1:6" ht="64" x14ac:dyDescent="0.2">
@@ -15833,11 +15832,11 @@
         <v>410</v>
       </c>
       <c r="B39" s="28" t="s">
-        <v>1001</v>
+        <v>1000</v>
       </c>
       <c r="C39" s="27"/>
       <c r="D39" s="18" t="s">
-        <v>1002</v>
+        <v>1001</v>
       </c>
     </row>
     <row r="40" spans="1:6" ht="80" x14ac:dyDescent="0.2">
@@ -15845,16 +15844,16 @@
         <v>413</v>
       </c>
       <c r="B40" s="28" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
       <c r="C40" s="27"/>
       <c r="D40" s="18" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" s="177" t="s">
-        <v>1004</v>
+        <v>1003</v>
       </c>
       <c r="B41" s="178"/>
       <c r="C41" s="178"/>
@@ -15866,19 +15865,19 @@
         <v>243</v>
       </c>
       <c r="B42" s="116" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
       <c r="C42" s="21" t="s">
         <v>858</v>
       </c>
       <c r="D42" s="116" t="s">
-        <v>1006</v>
+        <v>1005</v>
       </c>
       <c r="E42" s="46" t="s">
         <v>860</v>
       </c>
       <c r="F42" s="72" t="s">
-        <v>1007</v>
+        <v>1006</v>
       </c>
     </row>
     <row r="43" spans="1:6" ht="80" x14ac:dyDescent="0.2">
@@ -15886,16 +15885,16 @@
         <v>368</v>
       </c>
       <c r="B43" s="116" t="s">
+        <v>1007</v>
+      </c>
+      <c r="C43" s="21" t="s">
+        <v>916</v>
+      </c>
+      <c r="D43" s="116" t="s">
         <v>1008</v>
       </c>
-      <c r="C43" s="21" t="s">
+      <c r="E43" s="46" t="s">
         <v>917</v>
-      </c>
-      <c r="D43" s="116" t="s">
-        <v>1009</v>
-      </c>
-      <c r="E43" s="46" t="s">
-        <v>918</v>
       </c>
     </row>
     <row r="44" spans="1:6" ht="48" x14ac:dyDescent="0.2">
@@ -15903,16 +15902,16 @@
         <v>261</v>
       </c>
       <c r="B44" s="116" t="s">
+        <v>1009</v>
+      </c>
+      <c r="C44" s="62" t="s">
+        <v>1423</v>
+      </c>
+      <c r="D44" s="116" t="s">
         <v>1010</v>
       </c>
-      <c r="C44" s="62" t="s">
-        <v>1413</v>
-      </c>
-      <c r="D44" s="116" t="s">
-        <v>1011</v>
-      </c>
       <c r="E44" s="46" t="s">
-        <v>1012</v>
+        <v>1424</v>
       </c>
     </row>
     <row r="45" spans="1:6" ht="48" x14ac:dyDescent="0.2">
@@ -15920,16 +15919,16 @@
         <v>382</v>
       </c>
       <c r="B45" s="116" t="s">
+        <v>1011</v>
+      </c>
+      <c r="C45" s="21" t="s">
+        <v>1012</v>
+      </c>
+      <c r="D45" s="121" t="s">
         <v>1013</v>
       </c>
-      <c r="C45" s="21" t="s">
-        <v>1014</v>
-      </c>
-      <c r="D45" s="121" t="s">
-        <v>1015</v>
-      </c>
       <c r="E45" s="46" t="s">
-        <v>1014</v>
+        <v>1012</v>
       </c>
     </row>
     <row r="46" spans="1:6" ht="64" x14ac:dyDescent="0.2">
@@ -15937,16 +15936,16 @@
         <v>382</v>
       </c>
       <c r="B46" s="116" t="s">
+        <v>1014</v>
+      </c>
+      <c r="C46" s="21" t="s">
+        <v>1015</v>
+      </c>
+      <c r="D46" s="121" t="s">
         <v>1016</v>
       </c>
-      <c r="C46" s="21" t="s">
+      <c r="E46" s="46" t="s">
         <v>1017</v>
-      </c>
-      <c r="D46" s="121" t="s">
-        <v>1018</v>
-      </c>
-      <c r="E46" s="46" t="s">
-        <v>1019</v>
       </c>
     </row>
     <row r="47" spans="1:6" ht="48" x14ac:dyDescent="0.2">
@@ -15954,16 +15953,16 @@
         <v>382</v>
       </c>
       <c r="B47" s="116" t="s">
+        <v>1018</v>
+      </c>
+      <c r="C47" s="21" t="s">
+        <v>1019</v>
+      </c>
+      <c r="D47" s="121" t="s">
         <v>1020</v>
       </c>
-      <c r="C47" s="21" t="s">
+      <c r="E47" s="46" t="s">
         <v>1021</v>
-      </c>
-      <c r="D47" s="121" t="s">
-        <v>1022</v>
-      </c>
-      <c r="E47" s="46" t="s">
-        <v>1023</v>
       </c>
     </row>
     <row r="48" spans="1:6" ht="48" x14ac:dyDescent="0.2">
@@ -15971,16 +15970,16 @@
         <v>382</v>
       </c>
       <c r="B48" s="116" t="s">
+        <v>1022</v>
+      </c>
+      <c r="C48" s="21" t="s">
+        <v>1023</v>
+      </c>
+      <c r="D48" s="121" t="s">
         <v>1024</v>
       </c>
-      <c r="C48" s="21" t="s">
+      <c r="E48" s="46" t="s">
         <v>1025</v>
-      </c>
-      <c r="D48" s="121" t="s">
-        <v>1026</v>
-      </c>
-      <c r="E48" s="46" t="s">
-        <v>1027</v>
       </c>
     </row>
     <row r="49" spans="1:6" ht="16" x14ac:dyDescent="0.2">
@@ -15988,16 +15987,16 @@
         <v>382</v>
       </c>
       <c r="B49" s="92" t="s">
-        <v>1028</v>
+        <v>1026</v>
       </c>
       <c r="C49" s="93" t="s">
-        <v>1029</v>
+        <v>1027</v>
       </c>
       <c r="D49" s="101" t="s">
         <v>404</v>
       </c>
       <c r="E49" s="85" t="s">
-        <v>1030</v>
+        <v>1028</v>
       </c>
     </row>
     <row r="50" spans="1:6" ht="16" x14ac:dyDescent="0.2">
@@ -16005,7 +16004,7 @@
         <v>32</v>
       </c>
       <c r="B50" s="19" t="s">
-        <v>1031</v>
+        <v>1029</v>
       </c>
       <c r="C50" s="21" t="s">
         <v>34</v>
@@ -16016,36 +16015,36 @@
     </row>
     <row r="51" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A51" s="19" t="s">
+        <v>1030</v>
+      </c>
+      <c r="B51" s="19" t="s">
+        <v>1031</v>
+      </c>
+      <c r="C51" s="21" t="s">
         <v>1032</v>
       </c>
-      <c r="B51" s="19" t="s">
+      <c r="D51" s="19" t="s">
         <v>1033</v>
       </c>
-      <c r="C51" s="21" t="s">
-        <v>1034</v>
-      </c>
-      <c r="D51" s="19" t="s">
-        <v>1035</v>
-      </c>
       <c r="F51" s="71" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
     </row>
     <row r="52" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A52" s="19" t="s">
-        <v>1032</v>
+        <v>1030</v>
       </c>
       <c r="B52" s="19" t="s">
-        <v>1036</v>
+        <v>1034</v>
       </c>
       <c r="C52" s="21" t="s">
-        <v>1037</v>
+        <v>1035</v>
       </c>
       <c r="D52" s="19" t="s">
-        <v>1035</v>
+        <v>1033</v>
       </c>
       <c r="F52" s="71" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
     </row>
     <row r="53" spans="1:6" ht="48" x14ac:dyDescent="0.2">
@@ -16053,16 +16052,16 @@
         <v>382</v>
       </c>
       <c r="B53" s="116" t="s">
+        <v>1036</v>
+      </c>
+      <c r="C53" s="21" t="s">
+        <v>1037</v>
+      </c>
+      <c r="D53" s="121" t="s">
         <v>1038</v>
       </c>
-      <c r="C53" s="21" t="s">
-        <v>1039</v>
-      </c>
-      <c r="D53" s="121" t="s">
-        <v>1040</v>
-      </c>
       <c r="F53" s="71" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
     </row>
     <row r="54" spans="1:6" ht="48" x14ac:dyDescent="0.2">
@@ -16070,16 +16069,16 @@
         <v>382</v>
       </c>
       <c r="B54" s="116" t="s">
+        <v>1039</v>
+      </c>
+      <c r="C54" s="21" t="s">
+        <v>1040</v>
+      </c>
+      <c r="D54" s="121" t="s">
         <v>1041</v>
       </c>
-      <c r="C54" s="21" t="s">
-        <v>1042</v>
-      </c>
-      <c r="D54" s="121" t="s">
-        <v>1043</v>
-      </c>
       <c r="F54" s="71" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
     </row>
   </sheetData>
@@ -16102,8 +16101,8 @@
   <dimension ref="A1:F73"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A58" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C48" sqref="C48"/>
+      <pane ySplit="1" topLeftCell="A45" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F49" sqref="F49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -16142,52 +16141,52 @@
         <v>243</v>
       </c>
       <c r="B2" s="136" t="s">
-        <v>1044</v>
+        <v>1042</v>
       </c>
       <c r="C2" s="137" t="s">
-        <v>1045</v>
+        <v>1043</v>
       </c>
       <c r="D2" s="136" t="s">
         <v>246</v>
       </c>
       <c r="E2" s="138" t="s">
-        <v>1046</v>
+        <v>1044</v>
       </c>
       <c r="F2" s="135"/>
     </row>
     <row r="3" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A3" s="136" t="s">
-        <v>953</v>
+        <v>952</v>
       </c>
       <c r="B3" s="136" t="s">
+        <v>1045</v>
+      </c>
+      <c r="C3" s="137" t="s">
+        <v>1046</v>
+      </c>
+      <c r="D3" s="136" t="s">
         <v>1047</v>
       </c>
-      <c r="C3" s="137" t="s">
+      <c r="E3" s="138" t="s">
         <v>1048</v>
-      </c>
-      <c r="D3" s="136" t="s">
-        <v>1049</v>
-      </c>
-      <c r="E3" s="138" t="s">
-        <v>1050</v>
       </c>
       <c r="F3" s="135"/>
     </row>
     <row r="4" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A4" s="136" t="s">
+        <v>1049</v>
+      </c>
+      <c r="B4" s="136" t="s">
+        <v>1050</v>
+      </c>
+      <c r="C4" s="137" t="s">
         <v>1051</v>
       </c>
-      <c r="B4" s="136" t="s">
+      <c r="D4" s="136" t="s">
         <v>1052</v>
       </c>
-      <c r="C4" s="137" t="s">
+      <c r="E4" s="138" t="s">
         <v>1053</v>
-      </c>
-      <c r="D4" s="136" t="s">
-        <v>1054</v>
-      </c>
-      <c r="E4" s="138" t="s">
-        <v>1055</v>
       </c>
       <c r="F4" s="135"/>
     </row>
@@ -16196,11 +16195,11 @@
         <v>410</v>
       </c>
       <c r="B5" s="139" t="s">
-        <v>1056</v>
+        <v>1054</v>
       </c>
       <c r="C5" s="27"/>
       <c r="D5" s="136" t="s">
-        <v>1057</v>
+        <v>1055</v>
       </c>
       <c r="E5" s="138"/>
       <c r="F5" s="135"/>
@@ -16210,84 +16209,84 @@
         <v>413</v>
       </c>
       <c r="B6" s="139" t="s">
-        <v>1058</v>
+        <v>1056</v>
       </c>
       <c r="C6" s="27"/>
       <c r="D6" s="136" t="s">
-        <v>1059</v>
+        <v>1057</v>
       </c>
       <c r="E6" s="138"/>
       <c r="F6" s="135"/>
     </row>
     <row r="7" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A7" s="136" t="s">
-        <v>1051</v>
+        <v>1049</v>
       </c>
       <c r="B7" s="136" t="s">
+        <v>1058</v>
+      </c>
+      <c r="C7" s="137" t="s">
+        <v>1059</v>
+      </c>
+      <c r="D7" s="136" t="s">
         <v>1060</v>
       </c>
-      <c r="C7" s="137" t="s">
+      <c r="E7" s="138" t="s">
         <v>1061</v>
-      </c>
-      <c r="D7" s="136" t="s">
-        <v>1062</v>
-      </c>
-      <c r="E7" s="138" t="s">
-        <v>1063</v>
       </c>
       <c r="F7" s="135"/>
     </row>
     <row r="8" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A8" s="136" t="s">
-        <v>1051</v>
+        <v>1049</v>
       </c>
       <c r="B8" s="136" t="s">
+        <v>1062</v>
+      </c>
+      <c r="C8" s="137" t="s">
+        <v>1063</v>
+      </c>
+      <c r="D8" s="136" t="s">
         <v>1064</v>
       </c>
-      <c r="C8" s="137" t="s">
+      <c r="E8" s="138" t="s">
         <v>1065</v>
-      </c>
-      <c r="D8" s="136" t="s">
-        <v>1066</v>
-      </c>
-      <c r="E8" s="138" t="s">
-        <v>1067</v>
       </c>
       <c r="F8" s="135"/>
     </row>
     <row r="9" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A9" s="136" t="s">
-        <v>1051</v>
+        <v>1049</v>
       </c>
       <c r="B9" s="136" t="s">
+        <v>1066</v>
+      </c>
+      <c r="C9" s="137" t="s">
+        <v>1067</v>
+      </c>
+      <c r="D9" s="136" t="s">
         <v>1068</v>
       </c>
-      <c r="C9" s="137" t="s">
+      <c r="E9" s="138" t="s">
         <v>1069</v>
-      </c>
-      <c r="D9" s="136" t="s">
-        <v>1070</v>
-      </c>
-      <c r="E9" s="138" t="s">
-        <v>1071</v>
       </c>
       <c r="F9" s="135"/>
     </row>
     <row r="10" spans="1:6" ht="64" x14ac:dyDescent="0.2">
       <c r="A10" s="136" t="s">
-        <v>1051</v>
+        <v>1049</v>
       </c>
       <c r="B10" s="136" t="s">
+        <v>1070</v>
+      </c>
+      <c r="C10" s="137" t="s">
+        <v>1071</v>
+      </c>
+      <c r="D10" s="136" t="s">
         <v>1072</v>
       </c>
-      <c r="C10" s="137" t="s">
+      <c r="E10" s="138" t="s">
         <v>1073</v>
-      </c>
-      <c r="D10" s="136" t="s">
-        <v>1074</v>
-      </c>
-      <c r="E10" s="138" t="s">
-        <v>1075</v>
       </c>
       <c r="F10" s="135"/>
     </row>
@@ -16296,32 +16295,32 @@
         <v>254</v>
       </c>
       <c r="B11" s="136" t="s">
+        <v>1074</v>
+      </c>
+      <c r="C11" s="137" t="s">
+        <v>1075</v>
+      </c>
+      <c r="D11" s="136" t="s">
         <v>1076</v>
-      </c>
-      <c r="C11" s="137" t="s">
-        <v>1077</v>
-      </c>
-      <c r="D11" s="136" t="s">
-        <v>1078</v>
       </c>
       <c r="E11" s="138"/>
       <c r="F11" s="135"/>
     </row>
     <row r="12" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A12" s="136" t="s">
-        <v>1051</v>
+        <v>1049</v>
       </c>
       <c r="B12" s="136" t="s">
+        <v>1077</v>
+      </c>
+      <c r="C12" s="137" t="s">
+        <v>1078</v>
+      </c>
+      <c r="D12" s="136" t="s">
         <v>1079</v>
       </c>
-      <c r="C12" s="137" t="s">
+      <c r="E12" s="138" t="s">
         <v>1080</v>
-      </c>
-      <c r="D12" s="136" t="s">
-        <v>1081</v>
-      </c>
-      <c r="E12" s="138" t="s">
-        <v>1082</v>
       </c>
       <c r="F12" s="135"/>
     </row>
@@ -16330,11 +16329,11 @@
         <v>410</v>
       </c>
       <c r="B13" s="28" t="s">
-        <v>1083</v>
+        <v>1081</v>
       </c>
       <c r="C13" s="138"/>
       <c r="D13" s="136" t="s">
-        <v>1084</v>
+        <v>1082</v>
       </c>
       <c r="E13" s="138"/>
       <c r="F13" s="135"/>
@@ -16344,83 +16343,83 @@
         <v>413</v>
       </c>
       <c r="B14" s="28" t="s">
-        <v>1085</v>
+        <v>1083</v>
       </c>
       <c r="C14" s="138"/>
       <c r="D14" s="136" t="s">
-        <v>1059</v>
+        <v>1057</v>
       </c>
       <c r="E14" s="138"/>
       <c r="F14" s="135"/>
     </row>
     <row r="15" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A15" s="136" t="s">
-        <v>1051</v>
+        <v>1049</v>
       </c>
       <c r="B15" s="136" t="s">
+        <v>1084</v>
+      </c>
+      <c r="C15" s="137" t="s">
+        <v>1085</v>
+      </c>
+      <c r="D15" s="136" t="s">
         <v>1086</v>
       </c>
-      <c r="C15" s="137" t="s">
+      <c r="E15" s="138" t="s">
         <v>1087</v>
-      </c>
-      <c r="D15" s="136" t="s">
-        <v>1088</v>
-      </c>
-      <c r="E15" s="138" t="s">
-        <v>1089</v>
       </c>
       <c r="F15" s="135"/>
     </row>
     <row r="16" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A16" s="136" t="s">
-        <v>1051</v>
+        <v>1049</v>
       </c>
       <c r="B16" s="136" t="s">
+        <v>1088</v>
+      </c>
+      <c r="C16" s="137" t="s">
+        <v>1089</v>
+      </c>
+      <c r="D16" s="136" t="s">
         <v>1090</v>
       </c>
-      <c r="C16" s="137" t="s">
+      <c r="E16" s="138" t="s">
         <v>1091</v>
-      </c>
-      <c r="D16" s="136" t="s">
-        <v>1092</v>
-      </c>
-      <c r="E16" s="138" t="s">
-        <v>1093</v>
       </c>
       <c r="F16" s="135"/>
     </row>
     <row r="17" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A17" s="136" t="s">
-        <v>1051</v>
+        <v>1049</v>
       </c>
       <c r="B17" s="136" t="s">
+        <v>1092</v>
+      </c>
+      <c r="C17" s="137" t="s">
+        <v>1093</v>
+      </c>
+      <c r="D17" s="136" t="s">
         <v>1094</v>
       </c>
-      <c r="C17" s="137" t="s">
+      <c r="E17" s="138" t="s">
         <v>1095</v>
-      </c>
-      <c r="D17" s="136" t="s">
-        <v>1096</v>
-      </c>
-      <c r="E17" s="138" t="s">
-        <v>1097</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="144" x14ac:dyDescent="0.2">
       <c r="A18" s="136" t="s">
-        <v>1051</v>
+        <v>1049</v>
       </c>
       <c r="B18" s="136" t="s">
+        <v>1096</v>
+      </c>
+      <c r="C18" s="137" t="s">
+        <v>1097</v>
+      </c>
+      <c r="D18" s="29" t="s">
         <v>1098</v>
       </c>
-      <c r="C18" s="137" t="s">
+      <c r="E18" s="138" t="s">
         <v>1099</v>
-      </c>
-      <c r="D18" s="29" t="s">
-        <v>1100</v>
-      </c>
-      <c r="E18" s="138" t="s">
-        <v>1101</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="80" x14ac:dyDescent="0.2">
@@ -16428,11 +16427,11 @@
         <v>410</v>
       </c>
       <c r="B19" s="28" t="s">
-        <v>1102</v>
+        <v>1100</v>
       </c>
       <c r="C19" s="27"/>
       <c r="D19" s="18" t="s">
-        <v>1103</v>
+        <v>1101</v>
       </c>
       <c r="E19" s="138"/>
     </row>
@@ -16441,11 +16440,11 @@
         <v>413</v>
       </c>
       <c r="B20" s="28" t="s">
-        <v>1104</v>
+        <v>1102</v>
       </c>
       <c r="C20" s="27"/>
       <c r="D20" s="18" t="s">
-        <v>1059</v>
+        <v>1057</v>
       </c>
       <c r="E20" s="138"/>
     </row>
@@ -16454,29 +16453,29 @@
         <v>413</v>
       </c>
       <c r="B21" s="28" t="s">
-        <v>1105</v>
+        <v>1103</v>
       </c>
       <c r="C21" s="27"/>
       <c r="D21" s="18" t="s">
-        <v>1106</v>
+        <v>1104</v>
       </c>
       <c r="E21" s="138"/>
     </row>
     <row r="22" spans="1:5" ht="112" x14ac:dyDescent="0.2">
       <c r="A22" s="136" t="s">
+        <v>1105</v>
+      </c>
+      <c r="B22" s="136" t="s">
+        <v>1106</v>
+      </c>
+      <c r="C22" s="137" t="s">
         <v>1107</v>
       </c>
-      <c r="B22" s="136" t="s">
+      <c r="D22" s="136" t="s">
         <v>1108</v>
       </c>
-      <c r="C22" s="137" t="s">
+      <c r="E22" s="138" t="s">
         <v>1109</v>
-      </c>
-      <c r="D22" s="136" t="s">
-        <v>1110</v>
-      </c>
-      <c r="E22" s="138" t="s">
-        <v>1111</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="48" x14ac:dyDescent="0.2">
@@ -16484,11 +16483,11 @@
         <v>410</v>
       </c>
       <c r="B23" s="28" t="s">
-        <v>1112</v>
+        <v>1110</v>
       </c>
       <c r="C23" s="27"/>
       <c r="D23" s="136" t="s">
-        <v>1113</v>
+        <v>1111</v>
       </c>
       <c r="E23" s="138"/>
     </row>
@@ -16497,11 +16496,11 @@
         <v>413</v>
       </c>
       <c r="B24" s="28" t="s">
-        <v>1114</v>
+        <v>1112</v>
       </c>
       <c r="C24" s="27"/>
       <c r="D24" s="136" t="s">
-        <v>1115</v>
+        <v>1113</v>
       </c>
       <c r="E24" s="138"/>
     </row>
@@ -16510,11 +16509,11 @@
         <v>413</v>
       </c>
       <c r="B25" s="28" t="s">
-        <v>1116</v>
+        <v>1114</v>
       </c>
       <c r="C25" s="27"/>
       <c r="D25" s="29" t="s">
-        <v>1117</v>
+        <v>1115</v>
       </c>
       <c r="E25" s="138"/>
     </row>
@@ -16523,38 +16522,38 @@
         <v>254</v>
       </c>
       <c r="B26" s="136" t="s">
+        <v>1116</v>
+      </c>
+      <c r="C26" s="137" t="s">
+        <v>1117</v>
+      </c>
+      <c r="D26" s="136" t="s">
+        <v>1076</v>
+      </c>
+      <c r="E26" s="138" t="s">
         <v>1118</v>
-      </c>
-      <c r="C26" s="137" t="s">
-        <v>1119</v>
-      </c>
-      <c r="D26" s="136" t="s">
-        <v>1078</v>
-      </c>
-      <c r="E26" s="138" t="s">
-        <v>1120</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A27" s="136" t="s">
-        <v>1051</v>
+        <v>1049</v>
       </c>
       <c r="B27" s="136" t="s">
+        <v>1119</v>
+      </c>
+      <c r="C27" s="137" t="s">
+        <v>1120</v>
+      </c>
+      <c r="D27" s="136" t="s">
         <v>1121</v>
       </c>
-      <c r="C27" s="137" t="s">
+      <c r="E27" s="138" t="s">
         <v>1122</v>
-      </c>
-      <c r="D27" s="136" t="s">
-        <v>1123</v>
-      </c>
-      <c r="E27" s="138" t="s">
-        <v>1124</v>
       </c>
     </row>
     <row r="28" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A28" s="186" t="s">
-        <v>1125</v>
+        <v>1123</v>
       </c>
       <c r="B28" s="187"/>
       <c r="C28" s="187"/>
@@ -16566,33 +16565,33 @@
         <v>243</v>
       </c>
       <c r="B29" s="141" t="s">
+        <v>1124</v>
+      </c>
+      <c r="C29" s="142" t="s">
+        <v>1125</v>
+      </c>
+      <c r="D29" s="5" t="s">
         <v>1126</v>
       </c>
-      <c r="C29" s="142" t="s">
+      <c r="E29" s="143" t="s">
         <v>1127</v>
-      </c>
-      <c r="D29" s="5" t="s">
-        <v>1128</v>
-      </c>
-      <c r="E29" s="143" t="s">
-        <v>1129</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="64" x14ac:dyDescent="0.2">
       <c r="A30" s="144" t="s">
+        <v>1128</v>
+      </c>
+      <c r="B30" s="144" t="s">
+        <v>1129</v>
+      </c>
+      <c r="C30" s="145" t="s">
         <v>1130</v>
       </c>
-      <c r="B30" s="144" t="s">
+      <c r="D30" s="144" t="s">
         <v>1131</v>
       </c>
-      <c r="C30" s="145" t="s">
+      <c r="E30" s="146" t="s">
         <v>1132</v>
-      </c>
-      <c r="D30" s="144" t="s">
-        <v>1133</v>
-      </c>
-      <c r="E30" s="146" t="s">
-        <v>1134</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="48" x14ac:dyDescent="0.2">
@@ -16600,11 +16599,11 @@
         <v>410</v>
       </c>
       <c r="B31" s="28" t="s">
-        <v>1135</v>
+        <v>1133</v>
       </c>
       <c r="C31" s="27"/>
       <c r="D31" s="18" t="s">
-        <v>1002</v>
+        <v>1001</v>
       </c>
       <c r="E31" s="146"/>
     </row>
@@ -16613,17 +16612,17 @@
         <v>413</v>
       </c>
       <c r="B32" s="28" t="s">
-        <v>1136</v>
+        <v>1134</v>
       </c>
       <c r="C32" s="27"/>
       <c r="D32" s="18" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="E32" s="146"/>
     </row>
     <row r="33" spans="1:6" s="13" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A33" s="189" t="s">
-        <v>1137</v>
+        <v>1135</v>
       </c>
       <c r="B33" s="190"/>
       <c r="C33" s="191"/>
@@ -16635,121 +16634,121 @@
         <v>243</v>
       </c>
       <c r="B34" s="147" t="s">
+        <v>1136</v>
+      </c>
+      <c r="C34" s="145" t="s">
+        <v>1137</v>
+      </c>
+      <c r="D34" s="50" t="s">
         <v>1138</v>
       </c>
-      <c r="C34" s="145" t="s">
+      <c r="E34" s="146" t="s">
         <v>1139</v>
-      </c>
-      <c r="D34" s="50" t="s">
-        <v>1140</v>
-      </c>
-      <c r="E34" s="146" t="s">
-        <v>1141</v>
       </c>
       <c r="F34" s="135"/>
     </row>
     <row r="35" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A35" s="144" t="s">
-        <v>1051</v>
+        <v>1049</v>
       </c>
       <c r="B35" s="148" t="s">
+        <v>1140</v>
+      </c>
+      <c r="C35" s="145" t="s">
+        <v>1141</v>
+      </c>
+      <c r="D35" s="149" t="s">
         <v>1142</v>
       </c>
-      <c r="C35" s="145" t="s">
+      <c r="E35" s="146" t="s">
         <v>1143</v>
-      </c>
-      <c r="D35" s="149" t="s">
-        <v>1144</v>
-      </c>
-      <c r="E35" s="146" t="s">
-        <v>1145</v>
       </c>
       <c r="F35" s="135"/>
     </row>
     <row r="36" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A36" s="144" t="s">
-        <v>1051</v>
+        <v>1049</v>
       </c>
       <c r="B36" s="148" t="s">
+        <v>1144</v>
+      </c>
+      <c r="C36" s="145" t="s">
+        <v>1145</v>
+      </c>
+      <c r="D36" s="149" t="s">
+        <v>1142</v>
+      </c>
+      <c r="E36" s="146" t="s">
         <v>1146</v>
-      </c>
-      <c r="C36" s="145" t="s">
-        <v>1147</v>
-      </c>
-      <c r="D36" s="149" t="s">
-        <v>1144</v>
-      </c>
-      <c r="E36" s="146" t="s">
-        <v>1148</v>
       </c>
       <c r="F36" s="135"/>
     </row>
     <row r="37" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A37" s="144" t="s">
-        <v>1051</v>
+        <v>1049</v>
       </c>
       <c r="B37" s="148" t="s">
+        <v>1147</v>
+      </c>
+      <c r="C37" s="49" t="s">
+        <v>1148</v>
+      </c>
+      <c r="D37" s="149" t="s">
+        <v>1142</v>
+      </c>
+      <c r="E37" s="146" t="s">
         <v>1149</v>
-      </c>
-      <c r="C37" s="49" t="s">
-        <v>1150</v>
-      </c>
-      <c r="D37" s="149" t="s">
-        <v>1144</v>
-      </c>
-      <c r="E37" s="146" t="s">
-        <v>1151</v>
       </c>
       <c r="F37" s="135"/>
     </row>
     <row r="38" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A38" s="144" t="s">
-        <v>1051</v>
+        <v>1049</v>
       </c>
       <c r="B38" s="148" t="s">
+        <v>1150</v>
+      </c>
+      <c r="C38" s="49" t="s">
+        <v>1151</v>
+      </c>
+      <c r="D38" s="149" t="s">
+        <v>1142</v>
+      </c>
+      <c r="E38" s="146" t="s">
         <v>1152</v>
-      </c>
-      <c r="C38" s="49" t="s">
-        <v>1153</v>
-      </c>
-      <c r="D38" s="149" t="s">
-        <v>1144</v>
-      </c>
-      <c r="E38" s="146" t="s">
-        <v>1154</v>
       </c>
       <c r="F38" s="135"/>
     </row>
     <row r="39" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A39" s="144" t="s">
-        <v>1051</v>
+        <v>1049</v>
       </c>
       <c r="B39" s="148" t="s">
+        <v>1153</v>
+      </c>
+      <c r="C39" s="49" t="s">
+        <v>1154</v>
+      </c>
+      <c r="D39" s="149" t="s">
+        <v>1142</v>
+      </c>
+      <c r="E39" s="146" t="s">
         <v>1155</v>
-      </c>
-      <c r="C39" s="49" t="s">
-        <v>1156</v>
-      </c>
-      <c r="D39" s="149" t="s">
-        <v>1144</v>
-      </c>
-      <c r="E39" s="146" t="s">
-        <v>1157</v>
       </c>
       <c r="F39" s="135"/>
     </row>
     <row r="40" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A40" s="144" t="s">
-        <v>1051</v>
+        <v>1049</v>
       </c>
       <c r="B40" s="148" t="s">
-        <v>1158</v>
+        <v>1156</v>
       </c>
       <c r="C40" s="49" t="s">
         <v>93</v>
       </c>
       <c r="D40" s="149" t="s">
-        <v>1144</v>
+        <v>1142</v>
       </c>
       <c r="E40" s="146" t="s">
         <v>95</v>
@@ -16761,11 +16760,11 @@
         <v>410</v>
       </c>
       <c r="B41" s="28" t="s">
-        <v>1159</v>
+        <v>1157</v>
       </c>
       <c r="C41" s="51"/>
       <c r="D41" s="18" t="s">
-        <v>1002</v>
+        <v>1001</v>
       </c>
       <c r="E41" s="146"/>
       <c r="F41" s="135"/>
@@ -16775,11 +16774,11 @@
         <v>413</v>
       </c>
       <c r="B42" s="28" t="s">
-        <v>1160</v>
+        <v>1158</v>
       </c>
       <c r="C42" s="27"/>
       <c r="D42" s="18" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="E42" s="146"/>
       <c r="F42" s="135"/>
@@ -16789,16 +16788,16 @@
         <v>243</v>
       </c>
       <c r="B43" s="136" t="s">
+        <v>1159</v>
+      </c>
+      <c r="C43" s="62" t="s">
+        <v>1410</v>
+      </c>
+      <c r="D43" s="5" t="s">
+        <v>1160</v>
+      </c>
+      <c r="E43" s="146" t="s">
         <v>1161</v>
-      </c>
-      <c r="C43" s="62" t="s">
-        <v>1414</v>
-      </c>
-      <c r="D43" s="5" t="s">
-        <v>1162</v>
-      </c>
-      <c r="E43" s="146" t="s">
-        <v>1163</v>
       </c>
       <c r="F43" s="135"/>
     </row>
@@ -16807,11 +16806,11 @@
         <v>410</v>
       </c>
       <c r="B44" s="28" t="s">
-        <v>1164</v>
+        <v>1162</v>
       </c>
       <c r="C44" s="27"/>
       <c r="D44" s="18" t="s">
-        <v>1002</v>
+        <v>1001</v>
       </c>
       <c r="E44" s="146"/>
       <c r="F44" s="135"/>
@@ -16821,18 +16820,18 @@
         <v>413</v>
       </c>
       <c r="B45" s="28" t="s">
-        <v>1165</v>
+        <v>1163</v>
       </c>
       <c r="C45" s="27"/>
       <c r="D45" s="18" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="E45" s="146"/>
       <c r="F45" s="135"/>
     </row>
     <row r="46" spans="1:6" s="13" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="186" t="s">
-        <v>1166</v>
+        <v>1164</v>
       </c>
       <c r="B46" s="187"/>
       <c r="C46" s="187"/>
@@ -16844,53 +16843,53 @@
         <v>243</v>
       </c>
       <c r="B47" s="144" t="s">
-        <v>1167</v>
+        <v>1165</v>
       </c>
       <c r="C47" s="62" t="s">
         <v>858</v>
       </c>
       <c r="D47" s="116" t="s">
-        <v>1168</v>
+        <v>1166</v>
       </c>
       <c r="E47" s="63" t="s">
         <v>860</v>
       </c>
       <c r="F47" s="38" t="s">
-        <v>1169</v>
+        <v>1167</v>
       </c>
     </row>
     <row r="48" spans="1:6" s="30" customFormat="1" ht="64" x14ac:dyDescent="0.2">
       <c r="A48" s="144" t="s">
+        <v>1168</v>
+      </c>
+      <c r="B48" s="144" t="s">
+        <v>1169</v>
+      </c>
+      <c r="C48" s="62" t="s">
+        <v>922</v>
+      </c>
+      <c r="D48" s="116" t="s">
         <v>1170</v>
       </c>
-      <c r="B48" s="144" t="s">
+      <c r="E48" s="63" t="s">
+        <v>923</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" s="30" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+      <c r="A49" s="144" t="s">
+        <v>1128</v>
+      </c>
+      <c r="B49" s="144" t="s">
         <v>1171</v>
       </c>
-      <c r="C48" s="62" t="s">
-        <v>923</v>
-      </c>
-      <c r="D48" s="116" t="s">
-        <v>1172</v>
-      </c>
-      <c r="E48" s="63" t="s">
-        <v>924</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" s="30" customFormat="1" ht="64" x14ac:dyDescent="0.2">
-      <c r="A49" s="144" t="s">
-        <v>1130</v>
-      </c>
-      <c r="B49" s="144" t="s">
-        <v>1173</v>
-      </c>
       <c r="C49" s="62" t="s">
-        <v>1413</v>
+        <v>1423</v>
       </c>
       <c r="D49" s="116" t="s">
-        <v>1011</v>
+        <v>1010</v>
       </c>
       <c r="E49" s="63" t="s">
-        <v>1012</v>
+        <v>1424</v>
       </c>
     </row>
     <row r="50" spans="1:6" s="30" customFormat="1" ht="48" x14ac:dyDescent="0.2">
@@ -16898,19 +16897,19 @@
         <v>382</v>
       </c>
       <c r="B50" s="136" t="s">
+        <v>1172</v>
+      </c>
+      <c r="C50" s="145" t="s">
+        <v>1173</v>
+      </c>
+      <c r="D50" s="121" t="s">
         <v>1174</v>
       </c>
-      <c r="C50" s="145" t="s">
+      <c r="E50" s="63" t="s">
+        <v>1053</v>
+      </c>
+      <c r="F50" s="73" t="s">
         <v>1175</v>
-      </c>
-      <c r="D50" s="121" t="s">
-        <v>1176</v>
-      </c>
-      <c r="E50" s="63" t="s">
-        <v>1055</v>
-      </c>
-      <c r="F50" s="73" t="s">
-        <v>1177</v>
       </c>
     </row>
     <row r="51" spans="1:6" s="30" customFormat="1" ht="48" x14ac:dyDescent="0.2">
@@ -16918,16 +16917,16 @@
         <v>382</v>
       </c>
       <c r="B51" s="136" t="s">
+        <v>1176</v>
+      </c>
+      <c r="C51" s="145" t="s">
+        <v>1177</v>
+      </c>
+      <c r="D51" s="121" t="s">
         <v>1178</v>
       </c>
-      <c r="C51" s="145" t="s">
+      <c r="E51" s="63" t="s">
         <v>1179</v>
-      </c>
-      <c r="D51" s="121" t="s">
-        <v>1180</v>
-      </c>
-      <c r="E51" s="63" t="s">
-        <v>1181</v>
       </c>
     </row>
     <row r="52" spans="1:6" s="30" customFormat="1" ht="64" x14ac:dyDescent="0.2">
@@ -16935,16 +16934,16 @@
         <v>382</v>
       </c>
       <c r="B52" s="136" t="s">
+        <v>1180</v>
+      </c>
+      <c r="C52" s="145" t="s">
+        <v>1181</v>
+      </c>
+      <c r="D52" s="121" t="s">
         <v>1182</v>
       </c>
-      <c r="C52" s="145" t="s">
+      <c r="E52" s="63" t="s">
         <v>1183</v>
-      </c>
-      <c r="D52" s="121" t="s">
-        <v>1184</v>
-      </c>
-      <c r="E52" s="63" t="s">
-        <v>1185</v>
       </c>
     </row>
     <row r="53" spans="1:6" s="30" customFormat="1" ht="64" x14ac:dyDescent="0.2">
@@ -16952,16 +16951,16 @@
         <v>382</v>
       </c>
       <c r="B53" s="136" t="s">
+        <v>1184</v>
+      </c>
+      <c r="C53" s="145" t="s">
+        <v>1185</v>
+      </c>
+      <c r="D53" s="121" t="s">
         <v>1186</v>
       </c>
-      <c r="C53" s="145" t="s">
+      <c r="E53" s="63" t="s">
         <v>1187</v>
-      </c>
-      <c r="D53" s="121" t="s">
-        <v>1188</v>
-      </c>
-      <c r="E53" s="63" t="s">
-        <v>1189</v>
       </c>
     </row>
     <row r="54" spans="1:6" s="30" customFormat="1" ht="48" x14ac:dyDescent="0.2">
@@ -16969,16 +16968,16 @@
         <v>382</v>
       </c>
       <c r="B54" s="136" t="s">
+        <v>1188</v>
+      </c>
+      <c r="C54" s="145" t="s">
+        <v>1189</v>
+      </c>
+      <c r="D54" s="121" t="s">
         <v>1190</v>
       </c>
-      <c r="C54" s="145" t="s">
+      <c r="E54" s="63" t="s">
         <v>1191</v>
-      </c>
-      <c r="D54" s="121" t="s">
-        <v>1192</v>
-      </c>
-      <c r="E54" s="63" t="s">
-        <v>1193</v>
       </c>
     </row>
     <row r="55" spans="1:6" s="30" customFormat="1" ht="32" x14ac:dyDescent="0.2">
@@ -16986,19 +16985,19 @@
         <v>382</v>
       </c>
       <c r="B55" s="136" t="s">
+        <v>1192</v>
+      </c>
+      <c r="C55" s="145" t="s">
+        <v>1193</v>
+      </c>
+      <c r="D55" s="121" t="s">
         <v>1194</v>
       </c>
-      <c r="C55" s="145" t="s">
+      <c r="E55" s="63" t="s">
+        <v>1080</v>
+      </c>
+      <c r="F55" s="73" t="s">
         <v>1195</v>
-      </c>
-      <c r="D55" s="121" t="s">
-        <v>1196</v>
-      </c>
-      <c r="E55" s="63" t="s">
-        <v>1082</v>
-      </c>
-      <c r="F55" s="73" t="s">
-        <v>1197</v>
       </c>
     </row>
     <row r="56" spans="1:6" s="30" customFormat="1" ht="48" x14ac:dyDescent="0.2">
@@ -17006,19 +17005,19 @@
         <v>382</v>
       </c>
       <c r="B56" s="136" t="s">
+        <v>1196</v>
+      </c>
+      <c r="C56" s="145" t="s">
+        <v>1197</v>
+      </c>
+      <c r="D56" s="121" t="s">
         <v>1198</v>
       </c>
-      <c r="C56" s="145" t="s">
+      <c r="E56" s="63" t="s">
         <v>1199</v>
       </c>
-      <c r="D56" s="121" t="s">
+      <c r="F56" s="73" t="s">
         <v>1200</v>
-      </c>
-      <c r="E56" s="63" t="s">
-        <v>1201</v>
-      </c>
-      <c r="F56" s="73" t="s">
-        <v>1202</v>
       </c>
     </row>
     <row r="57" spans="1:6" s="30" customFormat="1" ht="48" x14ac:dyDescent="0.2">
@@ -17026,19 +17025,19 @@
         <v>382</v>
       </c>
       <c r="B57" s="136" t="s">
+        <v>1201</v>
+      </c>
+      <c r="C57" s="145" t="s">
+        <v>1202</v>
+      </c>
+      <c r="D57" s="121" t="s">
         <v>1203</v>
       </c>
-      <c r="C57" s="145" t="s">
+      <c r="E57" s="63" t="s">
         <v>1204</v>
       </c>
-      <c r="D57" s="121" t="s">
+      <c r="F57" s="73" t="s">
         <v>1205</v>
-      </c>
-      <c r="E57" s="63" t="s">
-        <v>1206</v>
-      </c>
-      <c r="F57" s="73" t="s">
-        <v>1207</v>
       </c>
     </row>
     <row r="58" spans="1:6" s="30" customFormat="1" ht="32" x14ac:dyDescent="0.2">
@@ -17046,19 +17045,19 @@
         <v>382</v>
       </c>
       <c r="B58" s="136" t="s">
+        <v>1206</v>
+      </c>
+      <c r="C58" s="145" t="s">
+        <v>1207</v>
+      </c>
+      <c r="D58" s="121" t="s">
         <v>1208</v>
       </c>
-      <c r="C58" s="145" t="s">
+      <c r="E58" s="63" t="s">
         <v>1209</v>
       </c>
-      <c r="D58" s="121" t="s">
+      <c r="F58" s="73" t="s">
         <v>1210</v>
-      </c>
-      <c r="E58" s="63" t="s">
-        <v>1211</v>
-      </c>
-      <c r="F58" s="73" t="s">
-        <v>1212</v>
       </c>
     </row>
     <row r="59" spans="1:6" s="30" customFormat="1" ht="48" x14ac:dyDescent="0.2">
@@ -17066,16 +17065,16 @@
         <v>382</v>
       </c>
       <c r="B59" s="136" t="s">
+        <v>1211</v>
+      </c>
+      <c r="C59" s="145" t="s">
+        <v>1212</v>
+      </c>
+      <c r="D59" s="121" t="s">
         <v>1213</v>
       </c>
-      <c r="C59" s="145" t="s">
+      <c r="E59" s="63" t="s">
         <v>1214</v>
-      </c>
-      <c r="D59" s="121" t="s">
-        <v>1215</v>
-      </c>
-      <c r="E59" s="63" t="s">
-        <v>1216</v>
       </c>
     </row>
     <row r="60" spans="1:6" s="30" customFormat="1" ht="48" x14ac:dyDescent="0.2">
@@ -17083,16 +17082,16 @@
         <v>382</v>
       </c>
       <c r="B60" s="136" t="s">
+        <v>1215</v>
+      </c>
+      <c r="C60" s="145" t="s">
+        <v>1216</v>
+      </c>
+      <c r="D60" s="121" t="s">
         <v>1217</v>
       </c>
-      <c r="C60" s="145" t="s">
+      <c r="E60" s="63" t="s">
         <v>1218</v>
-      </c>
-      <c r="D60" s="121" t="s">
-        <v>1219</v>
-      </c>
-      <c r="E60" s="63" t="s">
-        <v>1220</v>
       </c>
     </row>
     <row r="61" spans="1:6" s="30" customFormat="1" ht="48" x14ac:dyDescent="0.2">
@@ -17100,16 +17099,16 @@
         <v>382</v>
       </c>
       <c r="B61" s="18" t="s">
+        <v>1219</v>
+      </c>
+      <c r="C61" s="145" t="s">
+        <v>1220</v>
+      </c>
+      <c r="D61" s="121" t="s">
         <v>1221</v>
       </c>
-      <c r="C61" s="145" t="s">
+      <c r="E61" s="63" t="s">
         <v>1222</v>
-      </c>
-      <c r="D61" s="121" t="s">
-        <v>1223</v>
-      </c>
-      <c r="E61" s="63" t="s">
-        <v>1224</v>
       </c>
     </row>
     <row r="62" spans="1:6" s="30" customFormat="1" ht="48" x14ac:dyDescent="0.2">
@@ -17117,16 +17116,16 @@
         <v>382</v>
       </c>
       <c r="B62" s="136" t="s">
+        <v>1223</v>
+      </c>
+      <c r="C62" s="145" t="s">
+        <v>1224</v>
+      </c>
+      <c r="D62" s="121" t="s">
         <v>1225</v>
       </c>
-      <c r="C62" s="145" t="s">
+      <c r="E62" s="79" t="s">
         <v>1226</v>
-      </c>
-      <c r="D62" s="121" t="s">
-        <v>1227</v>
-      </c>
-      <c r="E62" s="79" t="s">
-        <v>1228</v>
       </c>
     </row>
     <row r="63" spans="1:6" ht="16" x14ac:dyDescent="0.2">
@@ -17134,14 +17133,14 @@
         <v>732</v>
       </c>
       <c r="B63" s="144" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="C63" s="145" t="s">
-        <v>1230</v>
+        <v>1228</v>
       </c>
       <c r="D63" s="148"/>
       <c r="E63" s="78" t="s">
-        <v>1231</v>
+        <v>1229</v>
       </c>
       <c r="F63" s="135"/>
     </row>
@@ -17150,14 +17149,14 @@
         <v>732</v>
       </c>
       <c r="B64" s="144" t="s">
-        <v>1232</v>
+        <v>1230</v>
       </c>
       <c r="C64" s="145" t="s">
-        <v>1156</v>
+        <v>1154</v>
       </c>
       <c r="D64" s="148"/>
       <c r="E64" s="78" t="s">
-        <v>1157</v>
+        <v>1155</v>
       </c>
       <c r="F64" s="135"/>
     </row>
@@ -17166,14 +17165,14 @@
         <v>732</v>
       </c>
       <c r="B65" s="136" t="s">
-        <v>1233</v>
+        <v>1231</v>
       </c>
       <c r="C65" s="145" t="s">
-        <v>1143</v>
+        <v>1141</v>
       </c>
       <c r="D65" s="148"/>
       <c r="E65" s="78" t="s">
-        <v>1145</v>
+        <v>1143</v>
       </c>
       <c r="F65" s="135"/>
     </row>
@@ -17253,6 +17252,47 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Readyforteam_x003f_ xmlns="565e1b1d-057e-4d85-b896-01a5881d8a45">false</Readyforteam_x003f_>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <SharedWithUsers xmlns="bf601f31-63a1-4825-9216-91d773c5ef9c">
+      <UserInfo>
+        <DisplayName>Erika Osti</DisplayName>
+        <AccountId>534</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Penny Johnson</DisplayName>
+        <AccountId>489</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Ben Childs</DisplayName>
+        <AccountId>643</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Thomas Leeds</DisplayName>
+        <AccountId>459</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Kasmyn Chen</DisplayName>
+        <AccountId>532</AccountId>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="565e1b1d-057e-4d85-b896-01a5881d8a45">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="2799d30d-6731-4efe-ac9b-c4895a8828d9" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010096D84A54A9CD274097F17166F184737D" ma:contentTypeVersion="21" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="2fd95a4cfdf4f2f51219070f5dff16a8">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="565e1b1d-057e-4d85-b896-01a5881d8a45" xmlns:ns3="bf601f31-63a1-4825-9216-91d773c5ef9c" xmlns:ns4="2799d30d-6731-4efe-ac9b-c4895a8828d9" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f7499f6f4dc8ad2a533df04863f63fa7" ns1:_="" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -17529,47 +17569,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Readyforteam_x003f_ xmlns="565e1b1d-057e-4d85-b896-01a5881d8a45">false</Readyforteam_x003f_>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <SharedWithUsers xmlns="bf601f31-63a1-4825-9216-91d773c5ef9c">
-      <UserInfo>
-        <DisplayName>Erika Osti</DisplayName>
-        <AccountId>534</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Penny Johnson</DisplayName>
-        <AccountId>489</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Ben Childs</DisplayName>
-        <AccountId>643</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Thomas Leeds</DisplayName>
-        <AccountId>459</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Kasmyn Chen</DisplayName>
-        <AccountId>532</AccountId>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="565e1b1d-057e-4d85-b896-01a5881d8a45">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="2799d30d-6731-4efe-ac9b-c4895a8828d9" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8D7CE8C7-18DC-484F-8376-ED09F13D44C8}">
   <ds:schemaRefs>
@@ -17579,6 +17578,19 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{017ACE96-8143-486E-8436-7787F6B96F4A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="565e1b1d-057e-4d85-b896-01a5881d8a45"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="bf601f31-63a1-4825-9216-91d773c5ef9c"/>
+    <ds:schemaRef ds:uri="2799d30d-6731-4efe-ac9b-c4895a8828d9"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EAFDB110-4046-4E72-A1EF-1908ABEC3151}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -17597,17 +17609,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{017ACE96-8143-486E-8436-7787F6B96F4A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="565e1b1d-057e-4d85-b896-01a5881d8a45"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="bf601f31-63a1-4825-9216-91d773c5ef9c"/>
-    <ds:schemaRef ds:uri="2799d30d-6731-4efe-ac9b-c4895a8828d9"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
[MCCDB-796] Content amend - The AP confirmation page
</commit_message>
<xml_diff>
--- a/app/data/MCCD-localisation.xlsx
+++ b/app/data/MCCD-localisation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/JALAT/GIT/medical-certificate-of-cause-of-death/app/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A3CB76E-8E81-CE4B-9EEF-46C05EF45A4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20B743BA-F15E-6346-A52E-E8C7756BC73F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="14220" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -69,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2133" uniqueCount="1427">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2135" uniqueCount="1429">
   <si>
     <r>
       <rPr>
@@ -5476,12 +5476,6 @@
     <t>Neu rhowch god post ysbyty</t>
   </si>
   <si>
-    <t>This certificate will now be sent to the medical examiner office for review and scrutiny.&lt;br /&gt;&lt;br /&gt;A summary of this certificate can be accessed from your dashboard.</t>
-  </si>
-  <si>
-    <t>You will be contacted by the medical examiner office if, following review and scrutiny of the cause of death the medical examiner requests that you amend this MCCD. You must then sign back in to edit the information on this certificate.&lt;br /&gt;&lt;br /&gt;You will be notified by email when the approved certificate is sent to the local register office.</t>
-  </si>
-  <si>
     <t>This death was reported to the coroner whose duty to investigate under s1 CJA2009 was not engaged</t>
   </si>
   <si>
@@ -5656,10 +5650,22 @@
     <t>Gwiriwch fod yr holl fanylion yn gywir cyn parhau.</t>
   </si>
   <si>
-    <t>019</t>
-  </si>
-  <si>
     <t>Tystysgrif feddygol achos gwasanaeth marwolaeth</t>
+  </si>
+  <si>
+    <t>This Medical certificate of cause of death (MCCD) will be sent to your medical examiner office for review and scrutiny.&lt;br /&gt;&lt;br /&gt;This certificate will be available to view from your dashboard for 3 months.</t>
+  </si>
+  <si>
+    <t>You will be contacted by the medical examiner office if, following review and scrutiny of the cause of death the medical examiner requests that you amend this MCCD.</t>
+  </si>
+  <si>
+    <t>Bydd y dystysgrif feddygol hon o achos marwolaeth (MCCD) yn cael ei hanfon at eich swyddfa arholwr meddygol i'w hadolygu a'i chraffu. &lt;br / &gt;&lt;br / &gt;Bydd y dystysgrif hon ar gael i'w gweld o'ch dangosfwrdd am 3 mis.</t>
+  </si>
+  <si>
+    <t>Bydd swyddfa'r arholwr meddygol yn cysylltu â chi os bydd yr arholwr meddygol, yn dilyn adolygiad a chraffu ar achos y farwolaeth, yn gofyn i chi ddiwygio'r MCCD hwn.</t>
+  </si>
+  <si>
+    <t>020</t>
   </si>
 </sst>
 </file>
@@ -6612,6 +6618,24 @@
     <xf numFmtId="0" fontId="13" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -6619,24 +6643,6 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -7861,7 +7867,7 @@
   <dimension ref="A1:F24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -8297,8 +8303,8 @@
   <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D21" sqref="D21"/>
+      <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -8586,7 +8592,7 @@
         <v>1352</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="64" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" ht="96" x14ac:dyDescent="0.2">
       <c r="A20" s="5" t="s">
         <v>261</v>
       </c>
@@ -8594,7 +8600,10 @@
         <v>1354</v>
       </c>
       <c r="C20" s="59" t="s">
-        <v>1365</v>
+        <v>1424</v>
+      </c>
+      <c r="E20" s="37" t="s">
+        <v>1426</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="16" x14ac:dyDescent="0.2">
@@ -8611,7 +8620,7 @@
         <v>1310</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="128" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6" ht="80" x14ac:dyDescent="0.2">
       <c r="A22" s="5" t="s">
         <v>261</v>
       </c>
@@ -8619,7 +8628,10 @@
         <v>1356</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>1366</v>
+        <v>1425</v>
+      </c>
+      <c r="E22" s="37" t="s">
+        <v>1427</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
@@ -8643,7 +8655,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F6" sqref="F6"/>
+      <selection pane="bottomLeft" activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -8683,13 +8695,13 @@
         <v>7</v>
       </c>
       <c r="C2" s="100" t="s">
-        <v>1425</v>
+        <v>1428</v>
       </c>
       <c r="D2" s="98" t="s">
         <v>8</v>
       </c>
       <c r="E2" s="99" t="s">
-        <v>1425</v>
+        <v>1428</v>
       </c>
       <c r="F2" s="98"/>
     </row>
@@ -8707,7 +8719,7 @@
         <v>12</v>
       </c>
       <c r="E3" s="37" t="s">
-        <v>1426</v>
+        <v>1423</v>
       </c>
       <c r="F3" s="5" t="s">
         <v>13</v>
@@ -9762,18 +9774,18 @@
     </row>
     <row r="67" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="B67" s="1" t="s">
-        <v>1369</v>
+        <v>1367</v>
       </c>
       <c r="C67" s="2" t="s">
+        <v>1368</v>
+      </c>
+      <c r="E67" s="40" t="s">
         <v>1370</v>
-      </c>
-      <c r="E67" s="40" t="s">
-        <v>1372</v>
       </c>
     </row>
     <row r="68" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="B68" s="1" t="s">
-        <v>1371</v>
+        <v>1369</v>
       </c>
       <c r="C68" s="2" t="s">
         <v>76</v>
@@ -10074,14 +10086,14 @@
         <v>243</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>1396</v>
+        <v>1394</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>1397</v>
+        <v>1395</v>
       </c>
       <c r="D2" s="5"/>
       <c r="E2" s="43" t="s">
-        <v>1405</v>
+        <v>1403</v>
       </c>
       <c r="F2" s="1"/>
     </row>
@@ -10090,19 +10102,19 @@
         <v>484</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>1398</v>
+        <v>1396</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>1399</v>
+        <v>1397</v>
       </c>
       <c r="D3" s="5"/>
       <c r="E3" s="43" t="s">
-        <v>1406</v>
+        <v>1404</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="159" t="s">
-        <v>1400</v>
+        <v>1398</v>
       </c>
       <c r="B4" s="160"/>
       <c r="C4" s="160"/>
@@ -10114,14 +10126,14 @@
         <v>243</v>
       </c>
       <c r="B5" s="5" t="s">
+        <v>1399</v>
+      </c>
+      <c r="C5" s="6" t="s">
         <v>1401</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>1403</v>
       </c>
       <c r="D5" s="5"/>
       <c r="E5" s="43" t="s">
-        <v>1407</v>
+        <v>1405</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="96" x14ac:dyDescent="0.2">
@@ -10129,14 +10141,14 @@
         <v>484</v>
       </c>
       <c r="B6" s="5" t="s">
+        <v>1400</v>
+      </c>
+      <c r="C6" s="6" t="s">
         <v>1402</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>1404</v>
       </c>
       <c r="D6" s="5"/>
       <c r="E6" s="43" t="s">
-        <v>1408</v>
+        <v>1406</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
@@ -10357,7 +10369,7 @@
         <v>243</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>1411</v>
+        <v>1409</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>276</v>
@@ -10381,7 +10393,7 @@
         <v>246</v>
       </c>
       <c r="E4" s="43" t="s">
-        <v>1412</v>
+        <v>1410</v>
       </c>
       <c r="F4" s="68" t="s">
         <v>280</v>
@@ -10395,13 +10407,13 @@
         <v>281</v>
       </c>
       <c r="C5" s="52" t="s">
-        <v>1417</v>
+        <v>1415</v>
       </c>
       <c r="D5" s="66" t="s">
         <v>282</v>
       </c>
       <c r="E5" s="156" t="s">
-        <v>1422</v>
+        <v>1420</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>283</v>
@@ -10415,13 +10427,13 @@
         <v>284</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>1418</v>
+        <v>1416</v>
       </c>
       <c r="D6" s="67" t="s">
         <v>285</v>
       </c>
       <c r="E6" s="157" t="s">
-        <v>1419</v>
+        <v>1417</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="160" x14ac:dyDescent="0.2">
@@ -10432,13 +10444,13 @@
         <v>286</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>1420</v>
+        <v>1418</v>
       </c>
       <c r="D7" s="67" t="s">
         <v>287</v>
       </c>
       <c r="E7" s="157" t="s">
-        <v>1421</v>
+        <v>1419</v>
       </c>
       <c r="F7" s="68" t="s">
         <v>288</v>
@@ -10640,7 +10652,7 @@
         <v>336</v>
       </c>
       <c r="C19" s="64" t="s">
-        <v>1409</v>
+        <v>1407</v>
       </c>
       <c r="D19" s="7" t="s">
         <v>337</v>
@@ -10774,17 +10786,17 @@
     </row>
     <row r="27" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A27" s="5" t="s">
-        <v>1415</v>
+        <v>1413</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>1416</v>
+        <v>1414</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>1413</v>
+        <v>1411</v>
       </c>
       <c r="D27" s="5"/>
       <c r="E27" s="37" t="s">
-        <v>1414</v>
+        <v>1412</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
@@ -10861,13 +10873,13 @@
       </c>
     </row>
     <row r="2" spans="1:6" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="165" t="s">
+      <c r="A2" s="162" t="s">
         <v>367</v>
       </c>
-      <c r="B2" s="166"/>
-      <c r="C2" s="166"/>
-      <c r="D2" s="166"/>
-      <c r="E2" s="167"/>
+      <c r="B2" s="163"/>
+      <c r="C2" s="163"/>
+      <c r="D2" s="163"/>
+      <c r="E2" s="164"/>
       <c r="F2" s="33"/>
     </row>
     <row r="3" spans="1:6" ht="48" x14ac:dyDescent="0.2">
@@ -10995,13 +11007,13 @@
       <c r="F9" s="119"/>
     </row>
     <row r="10" spans="1:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="168" t="s">
+      <c r="A10" s="165" t="s">
         <v>396</v>
       </c>
-      <c r="B10" s="169"/>
-      <c r="C10" s="169"/>
-      <c r="D10" s="169"/>
-      <c r="E10" s="170"/>
+      <c r="B10" s="166"/>
+      <c r="C10" s="166"/>
+      <c r="D10" s="166"/>
+      <c r="E10" s="167"/>
       <c r="F10" s="119"/>
     </row>
     <row r="11" spans="1:6" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -11030,13 +11042,13 @@
         <v>401</v>
       </c>
       <c r="C12" s="153" t="s">
-        <v>1373</v>
+        <v>1371</v>
       </c>
       <c r="D12" s="84" t="s">
         <v>402</v>
       </c>
       <c r="E12" s="152" t="s">
-        <v>1374</v>
+        <v>1372</v>
       </c>
       <c r="F12" s="86"/>
     </row>
@@ -11048,13 +11060,13 @@
         <v>403</v>
       </c>
       <c r="C13" s="154" t="s">
-        <v>1375</v>
+        <v>1373</v>
       </c>
       <c r="D13" s="88" t="s">
         <v>404</v>
       </c>
       <c r="E13" s="155" t="s">
-        <v>1376</v>
+        <v>1374</v>
       </c>
       <c r="F13" s="86"/>
     </row>
@@ -11522,7 +11534,7 @@
         <v>485</v>
       </c>
       <c r="C45" s="59" t="s">
-        <v>1392</v>
+        <v>1390</v>
       </c>
       <c r="D45" s="116"/>
       <c r="E45" s="120" t="s">
@@ -11535,14 +11547,14 @@
         <v>484</v>
       </c>
       <c r="B46" s="116" t="s">
-        <v>1395</v>
+        <v>1393</v>
       </c>
       <c r="C46" s="59" t="s">
-        <v>1393</v>
+        <v>1391</v>
       </c>
       <c r="D46" s="116"/>
       <c r="E46" s="120" t="s">
-        <v>1394</v>
+        <v>1392</v>
       </c>
       <c r="F46" s="119"/>
     </row>
@@ -11770,7 +11782,7 @@
         <v>522</v>
       </c>
       <c r="E61" s="120" t="s">
-        <v>1385</v>
+        <v>1383</v>
       </c>
       <c r="F61" s="119"/>
     </row>
@@ -11779,14 +11791,14 @@
         <v>519</v>
       </c>
       <c r="B62" s="116" t="s">
+        <v>1380</v>
+      </c>
+      <c r="C62" s="117" t="s">
         <v>1382</v>
-      </c>
-      <c r="C62" s="117" t="s">
-        <v>1384</v>
       </c>
       <c r="D62" s="116"/>
       <c r="E62" s="120" t="s">
-        <v>1383</v>
+        <v>1381</v>
       </c>
       <c r="F62" s="119"/>
     </row>
@@ -13335,13 +13347,13 @@
       <c r="F164" s="119"/>
     </row>
     <row r="165" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A165" s="162" t="s">
+      <c r="A165" s="168" t="s">
         <v>765</v>
       </c>
-      <c r="B165" s="163"/>
-      <c r="C165" s="163"/>
-      <c r="D165" s="163"/>
-      <c r="E165" s="164"/>
+      <c r="B165" s="169"/>
+      <c r="C165" s="169"/>
+      <c r="D165" s="169"/>
+      <c r="E165" s="170"/>
       <c r="F165" s="129" t="s">
         <v>766</v>
       </c>
@@ -13768,13 +13780,13 @@
         <v>815</v>
       </c>
       <c r="C193" s="59" t="s">
-        <v>1377</v>
+        <v>1375</v>
       </c>
       <c r="D193" s="116" t="s">
         <v>816</v>
       </c>
       <c r="E193" s="120" t="s">
-        <v>1381</v>
+        <v>1379</v>
       </c>
       <c r="F193" s="119"/>
     </row>
@@ -13783,14 +13795,14 @@
         <v>484</v>
       </c>
       <c r="B194" s="116" t="s">
-        <v>1378</v>
+        <v>1376</v>
       </c>
       <c r="C194" s="59" t="s">
-        <v>1379</v>
+        <v>1377</v>
       </c>
       <c r="D194" s="116"/>
       <c r="E194" s="120" t="s">
-        <v>1380</v>
+        <v>1378</v>
       </c>
       <c r="F194" s="119"/>
     </row>
@@ -13890,11 +13902,11 @@
         <v>827</v>
       </c>
       <c r="C201" s="117" t="s">
-        <v>1388</v>
+        <v>1386</v>
       </c>
       <c r="D201" s="116"/>
       <c r="E201" s="120" t="s">
-        <v>1391</v>
+        <v>1389</v>
       </c>
       <c r="F201" s="119"/>
     </row>
@@ -13903,7 +13915,7 @@
         <v>734</v>
       </c>
       <c r="B202" s="116" t="s">
-        <v>1390</v>
+        <v>1388</v>
       </c>
       <c r="C202" s="117" t="s">
         <v>43</v>
@@ -13919,14 +13931,14 @@
         <v>32</v>
       </c>
       <c r="B203" s="116" t="s">
-        <v>1389</v>
+        <v>1387</v>
       </c>
       <c r="C203" s="134" t="s">
-        <v>1386</v>
+        <v>1384</v>
       </c>
       <c r="D203" s="116"/>
       <c r="E203" s="120" t="s">
-        <v>1387</v>
+        <v>1385</v>
       </c>
       <c r="F203" s="119"/>
     </row>
@@ -14298,13 +14310,13 @@
         <v>866</v>
       </c>
       <c r="C228" s="59" t="s">
-        <v>1423</v>
+        <v>1421</v>
       </c>
       <c r="D228" s="116" t="s">
         <v>867</v>
       </c>
       <c r="E228" s="120" t="s">
-        <v>1424</v>
+        <v>1422</v>
       </c>
       <c r="F228" s="119"/>
     </row>
@@ -15244,18 +15256,6 @@
     </row>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="A225:E225"/>
-    <mergeCell ref="A186:E186"/>
-    <mergeCell ref="A190:E190"/>
-    <mergeCell ref="A197:E197"/>
-    <mergeCell ref="A208:E208"/>
-    <mergeCell ref="A214:E214"/>
-    <mergeCell ref="A58:E58"/>
-    <mergeCell ref="A2:E2"/>
-    <mergeCell ref="A10:E10"/>
-    <mergeCell ref="A14:E14"/>
-    <mergeCell ref="A24:E24"/>
-    <mergeCell ref="A43:E43"/>
     <mergeCell ref="A174:E174"/>
     <mergeCell ref="A157:E157"/>
     <mergeCell ref="A63:E63"/>
@@ -15266,6 +15266,18 @@
     <mergeCell ref="A146:E146"/>
     <mergeCell ref="A92:E92"/>
     <mergeCell ref="A165:E165"/>
+    <mergeCell ref="A58:E58"/>
+    <mergeCell ref="A2:E2"/>
+    <mergeCell ref="A10:E10"/>
+    <mergeCell ref="A14:E14"/>
+    <mergeCell ref="A24:E24"/>
+    <mergeCell ref="A43:E43"/>
+    <mergeCell ref="A225:E225"/>
+    <mergeCell ref="A186:E186"/>
+    <mergeCell ref="A190:E190"/>
+    <mergeCell ref="A197:E197"/>
+    <mergeCell ref="A208:E208"/>
+    <mergeCell ref="A214:E214"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -15536,13 +15548,13 @@
         <v>942</v>
       </c>
       <c r="C17" s="151" t="s">
-        <v>1367</v>
+        <v>1365</v>
       </c>
       <c r="D17" s="92" t="s">
         <v>934</v>
       </c>
       <c r="E17" s="152" t="s">
-        <v>1368</v>
+        <v>1366</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="80" x14ac:dyDescent="0.2">
@@ -15905,13 +15917,13 @@
         <v>1009</v>
       </c>
       <c r="C44" s="62" t="s">
-        <v>1423</v>
+        <v>1421</v>
       </c>
       <c r="D44" s="116" t="s">
         <v>1010</v>
       </c>
       <c r="E44" s="46" t="s">
-        <v>1424</v>
+        <v>1422</v>
       </c>
     </row>
     <row r="45" spans="1:6" ht="48" x14ac:dyDescent="0.2">
@@ -16791,7 +16803,7 @@
         <v>1159</v>
       </c>
       <c r="C43" s="62" t="s">
-        <v>1410</v>
+        <v>1408</v>
       </c>
       <c r="D43" s="5" t="s">
         <v>1160</v>
@@ -16883,13 +16895,13 @@
         <v>1171</v>
       </c>
       <c r="C49" s="62" t="s">
-        <v>1423</v>
+        <v>1421</v>
       </c>
       <c r="D49" s="116" t="s">
         <v>1010</v>
       </c>
       <c r="E49" s="63" t="s">
-        <v>1424</v>
+        <v>1422</v>
       </c>
     </row>
     <row r="50" spans="1:6" s="30" customFormat="1" ht="48" x14ac:dyDescent="0.2">
@@ -17252,47 +17264,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Readyforteam_x003f_ xmlns="565e1b1d-057e-4d85-b896-01a5881d8a45">false</Readyforteam_x003f_>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <SharedWithUsers xmlns="bf601f31-63a1-4825-9216-91d773c5ef9c">
-      <UserInfo>
-        <DisplayName>Erika Osti</DisplayName>
-        <AccountId>534</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Penny Johnson</DisplayName>
-        <AccountId>489</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Ben Childs</DisplayName>
-        <AccountId>643</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Thomas Leeds</DisplayName>
-        <AccountId>459</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Kasmyn Chen</DisplayName>
-        <AccountId>532</AccountId>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="565e1b1d-057e-4d85-b896-01a5881d8a45">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="2799d30d-6731-4efe-ac9b-c4895a8828d9" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010096D84A54A9CD274097F17166F184737D" ma:contentTypeVersion="21" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="2fd95a4cfdf4f2f51219070f5dff16a8">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="565e1b1d-057e-4d85-b896-01a5881d8a45" xmlns:ns3="bf601f31-63a1-4825-9216-91d773c5ef9c" xmlns:ns4="2799d30d-6731-4efe-ac9b-c4895a8828d9" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f7499f6f4dc8ad2a533df04863f63fa7" ns1:_="" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -17569,6 +17540,47 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Readyforteam_x003f_ xmlns="565e1b1d-057e-4d85-b896-01a5881d8a45">false</Readyforteam_x003f_>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <SharedWithUsers xmlns="bf601f31-63a1-4825-9216-91d773c5ef9c">
+      <UserInfo>
+        <DisplayName>Erika Osti</DisplayName>
+        <AccountId>534</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Penny Johnson</DisplayName>
+        <AccountId>489</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Ben Childs</DisplayName>
+        <AccountId>643</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Thomas Leeds</DisplayName>
+        <AccountId>459</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Kasmyn Chen</DisplayName>
+        <AccountId>532</AccountId>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="565e1b1d-057e-4d85-b896-01a5881d8a45">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="2799d30d-6731-4efe-ac9b-c4895a8828d9" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8D7CE8C7-18DC-484F-8376-ED09F13D44C8}">
   <ds:schemaRefs>
@@ -17578,19 +17590,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{017ACE96-8143-486E-8436-7787F6B96F4A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="565e1b1d-057e-4d85-b896-01a5881d8a45"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="bf601f31-63a1-4825-9216-91d773c5ef9c"/>
-    <ds:schemaRef ds:uri="2799d30d-6731-4efe-ac9b-c4895a8828d9"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EAFDB110-4046-4E72-A1EF-1908ABEC3151}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -17609,4 +17608,17 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{017ACE96-8143-486E-8436-7787F6B96F4A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="565e1b1d-057e-4d85-b896-01a5881d8a45"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="bf601f31-63a1-4825-9216-91d773c5ef9c"/>
+    <ds:schemaRef ds:uri="2799d30d-6731-4efe-ac9b-c4895a8828d9"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Fixing the bilingual journey on v11bi implant question.
</commit_message>
<xml_diff>
--- a/app/data/MCCD-localisation.xlsx
+++ b/app/data/MCCD-localisation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/JALAT/GIT/medical-certificate-of-cause-of-death/app/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20B743BA-F15E-6346-A52E-E8C7756BC73F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F79C97E6-962A-D44F-AF01-A47279EECD42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="14220" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -69,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2135" uniqueCount="1429">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2139" uniqueCount="1432">
   <si>
     <r>
       <rPr>
@@ -4200,12 +4200,6 @@
     <t>implantsPagePara</t>
   </si>
   <si>
-    <t>In some cases, it may be difficult to know with certainty all of the implantable medical devices that the deceased had fitted. Enter details of any implants using the records and information that you have available.</t>
-  </si>
-  <si>
-    <t>Mewn rhai achosion, gall fod yn anodd gwybod yn bendant am yr holl ddyfeisiau meddygol mewnblanadwy yr oedd yr ymadawedig wedi’u gosod. Rhowch fanylion unrhyw fewnblaniadau gan ddefnyddio'r cofnodion a'r wybodaeth sydd ar gael i chi.</t>
-  </si>
-  <si>
     <t>implantsYesDetails</t>
   </si>
   <si>
@@ -5665,7 +5659,22 @@
     <t>Bydd swyddfa'r arholwr meddygol yn cysylltu â chi os bydd yr arholwr meddygol, yn dilyn adolygiad a chraffu ar achos y farwolaeth, yn gofyn i chi ddiwygio'r MCCD hwn.</t>
   </si>
   <si>
-    <t>020</t>
+    <t>In some cases, it may be difficult to know with certainty all the implantable medical devices the deceased had fitted. Enter details of any implants using the records and information that you have available.</t>
+  </si>
+  <si>
+    <t>Mewn rhai achosion, gall fod yn anodd gwybod yn sicr yr holl ddyfeisiau meddygol mewnblannu yr oedd yr ymadawedig wedi'u ffitio. Rhowch fanylion unrhyw fewnblaniadau gan ddefnyddio'r cofnodion a'r wybodaeth sydd gennych ar gael.</t>
+  </si>
+  <si>
+    <t>implantsPageParaBilingual</t>
+  </si>
+  <si>
+    <t>You must enter details in English and Welsh, or in English only.</t>
+  </si>
+  <si>
+    <t>Rhaid i chi roi manylion yn Gymraeg a Saesneg, neu yn Saesneg yn unig.</t>
+  </si>
+  <si>
+    <t>021</t>
   </si>
 </sst>
 </file>
@@ -6618,6 +6627,15 @@
     <xf numFmtId="0" fontId="13" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -6634,15 +6652,6 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -7686,16 +7695,16 @@
         <v>243</v>
       </c>
       <c r="B2" s="5" t="s">
+        <v>1230</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>1231</v>
+      </c>
+      <c r="D2" s="5" t="s">
         <v>1232</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="F2" s="68" t="s">
         <v>1233</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>1234</v>
-      </c>
-      <c r="F2" s="68" t="s">
-        <v>1235</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="32" x14ac:dyDescent="0.2">
@@ -7703,13 +7712,13 @@
         <v>254</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>1236</v>
+        <v>1234</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>910</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>1237</v>
+        <v>1235</v>
       </c>
       <c r="E3" s="37" t="s">
         <v>911</v>
@@ -7720,13 +7729,13 @@
         <v>32</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>1238</v>
+        <v>1236</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>863</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>1239</v>
+        <v>1237</v>
       </c>
       <c r="E4" s="37" t="s">
         <v>865</v>
@@ -7734,36 +7743,36 @@
     </row>
     <row r="5" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
-        <v>1240</v>
+        <v>1238</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>1241</v>
+        <v>1239</v>
       </c>
       <c r="C5" s="6" t="s">
         <v>152</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>1242</v>
+        <v>1240</v>
       </c>
       <c r="F5" s="68" t="s">
-        <v>1235</v>
+        <v>1233</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
-        <v>1240</v>
+        <v>1238</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>1243</v>
+        <v>1241</v>
       </c>
       <c r="C6" s="6" t="s">
         <v>140</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>1242</v>
+        <v>1240</v>
       </c>
       <c r="F6" s="68" t="s">
-        <v>1235</v>
+        <v>1233</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="32" x14ac:dyDescent="0.2">
@@ -7771,13 +7780,13 @@
         <v>254</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>1244</v>
+        <v>1242</v>
       </c>
       <c r="C7" s="6" t="s">
         <v>913</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>1237</v>
+        <v>1235</v>
       </c>
       <c r="E7" s="37" t="s">
         <v>914</v>
@@ -7788,7 +7797,7 @@
         <v>32</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>1245</v>
+        <v>1243</v>
       </c>
       <c r="C8" s="6" t="s">
         <v>916</v>
@@ -7800,10 +7809,10 @@
     </row>
     <row r="9" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
-        <v>1240</v>
+        <v>1238</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>1246</v>
+        <v>1244</v>
       </c>
       <c r="C9" s="6" t="s">
         <v>922</v>
@@ -7815,22 +7824,22 @@
     </row>
     <row r="10" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="C10" s="27" t="s">
+        <v>1245</v>
+      </c>
+      <c r="D10" s="18" t="s">
+        <v>1246</v>
+      </c>
+      <c r="E10" s="37" t="s">
         <v>1247</v>
-      </c>
-      <c r="D10" s="18" t="s">
-        <v>1248</v>
-      </c>
-      <c r="E10" s="37" t="s">
-        <v>1249</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="C11" s="74" t="s">
-        <v>1250</v>
+        <v>1248</v>
       </c>
       <c r="D11" s="18"/>
       <c r="E11" s="37" t="s">
-        <v>1251</v>
+        <v>1249</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
@@ -7907,33 +7916,33 @@
         <v>243</v>
       </c>
       <c r="B2" s="92" t="s">
+        <v>1250</v>
+      </c>
+      <c r="C2" s="93" t="s">
+        <v>1251</v>
+      </c>
+      <c r="D2" s="92" t="s">
         <v>1252</v>
       </c>
-      <c r="C2" s="93" t="s">
+      <c r="E2" s="85" t="s">
         <v>1253</v>
-      </c>
-      <c r="D2" s="92" t="s">
-        <v>1254</v>
-      </c>
-      <c r="E2" s="85" t="s">
-        <v>1255</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="80" x14ac:dyDescent="0.2">
       <c r="A3" s="94" t="s">
+        <v>1254</v>
+      </c>
+      <c r="B3" s="95" t="s">
+        <v>1255</v>
+      </c>
+      <c r="C3" s="96" t="s">
         <v>1256</v>
       </c>
-      <c r="B3" s="95" t="s">
+      <c r="D3" s="95" t="s">
         <v>1257</v>
       </c>
-      <c r="C3" s="96" t="s">
+      <c r="E3" s="89" t="s">
         <v>1258</v>
-      </c>
-      <c r="D3" s="95" t="s">
-        <v>1259</v>
-      </c>
-      <c r="E3" s="89" t="s">
-        <v>1260</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="16" x14ac:dyDescent="0.2">
@@ -7941,16 +7950,16 @@
         <v>758</v>
       </c>
       <c r="B4" s="95" t="s">
-        <v>1261</v>
+        <v>1259</v>
       </c>
       <c r="C4" s="96" t="s">
-        <v>1262</v>
+        <v>1260</v>
       </c>
       <c r="D4" s="95" t="s">
         <v>404</v>
       </c>
       <c r="E4" s="89" t="s">
-        <v>1263</v>
+        <v>1261</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="60.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -7958,13 +7967,13 @@
         <v>410</v>
       </c>
       <c r="B5" s="105" t="s">
-        <v>1264</v>
+        <v>1262</v>
       </c>
       <c r="C5" s="106" t="s">
         <v>404</v>
       </c>
       <c r="D5" s="107" t="s">
-        <v>1265</v>
+        <v>1263</v>
       </c>
       <c r="E5" s="89" t="s">
         <v>404</v>
@@ -7975,13 +7984,13 @@
         <v>413</v>
       </c>
       <c r="B6" s="105" t="s">
-        <v>1266</v>
+        <v>1264</v>
       </c>
       <c r="C6" s="106" t="s">
         <v>404</v>
       </c>
       <c r="D6" s="107" t="s">
-        <v>1267</v>
+        <v>1265</v>
       </c>
       <c r="E6" s="89" t="s">
         <v>404</v>
@@ -8009,33 +8018,33 @@
         <v>243</v>
       </c>
       <c r="B8" s="95" t="s">
+        <v>1266</v>
+      </c>
+      <c r="C8" s="96" t="s">
+        <v>1267</v>
+      </c>
+      <c r="D8" s="95" t="s">
         <v>1268</v>
       </c>
-      <c r="C8" s="96" t="s">
+      <c r="E8" s="89" t="s">
         <v>1269</v>
-      </c>
-      <c r="D8" s="95" t="s">
-        <v>1270</v>
-      </c>
-      <c r="E8" s="89" t="s">
-        <v>1271</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="64" x14ac:dyDescent="0.2">
       <c r="A9" s="94" t="s">
-        <v>1256</v>
+        <v>1254</v>
       </c>
       <c r="B9" s="95" t="s">
+        <v>1270</v>
+      </c>
+      <c r="C9" s="96" t="s">
+        <v>1271</v>
+      </c>
+      <c r="D9" s="95" t="s">
         <v>1272</v>
       </c>
-      <c r="C9" s="96" t="s">
+      <c r="E9" s="89" t="s">
         <v>1273</v>
-      </c>
-      <c r="D9" s="95" t="s">
-        <v>1274</v>
-      </c>
-      <c r="E9" s="89" t="s">
-        <v>1275</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="16" x14ac:dyDescent="0.2">
@@ -8043,10 +8052,10 @@
         <v>758</v>
       </c>
       <c r="B10" s="95" t="s">
-        <v>1276</v>
+        <v>1274</v>
       </c>
       <c r="C10" s="96" t="s">
-        <v>1277</v>
+        <v>1275</v>
       </c>
       <c r="D10" s="95" t="s">
         <v>404</v>
@@ -8060,13 +8069,13 @@
         <v>410</v>
       </c>
       <c r="B11" s="105" t="s">
-        <v>1278</v>
+        <v>1276</v>
       </c>
       <c r="C11" s="106" t="s">
         <v>404</v>
       </c>
       <c r="D11" s="107" t="s">
-        <v>1265</v>
+        <v>1263</v>
       </c>
       <c r="E11" s="89" t="s">
         <v>404</v>
@@ -8077,13 +8086,13 @@
         <v>413</v>
       </c>
       <c r="B12" s="105" t="s">
-        <v>1279</v>
+        <v>1277</v>
       </c>
       <c r="C12" s="106" t="s">
         <v>404</v>
       </c>
       <c r="D12" s="107" t="s">
-        <v>1267</v>
+        <v>1265</v>
       </c>
       <c r="E12" s="89" t="s">
         <v>404</v>
@@ -8111,13 +8120,13 @@
         <v>243</v>
       </c>
       <c r="B14" s="95" t="s">
+        <v>1278</v>
+      </c>
+      <c r="C14" s="96" t="s">
+        <v>1279</v>
+      </c>
+      <c r="D14" s="95" t="s">
         <v>1280</v>
-      </c>
-      <c r="C14" s="96" t="s">
-        <v>1281</v>
-      </c>
-      <c r="D14" s="95" t="s">
-        <v>1282</v>
       </c>
       <c r="E14" s="89" t="s">
         <v>404</v>
@@ -8125,19 +8134,19 @@
     </row>
     <row r="15" spans="1:6" ht="96" x14ac:dyDescent="0.2">
       <c r="A15" s="94" t="s">
-        <v>1256</v>
+        <v>1254</v>
       </c>
       <c r="B15" s="95" t="s">
+        <v>1281</v>
+      </c>
+      <c r="C15" s="96" t="s">
+        <v>1282</v>
+      </c>
+      <c r="D15" s="95" t="s">
         <v>1283</v>
       </c>
-      <c r="C15" s="96" t="s">
+      <c r="E15" s="89" t="s">
         <v>1284</v>
-      </c>
-      <c r="D15" s="95" t="s">
-        <v>1285</v>
-      </c>
-      <c r="E15" s="89" t="s">
-        <v>1286</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="48" x14ac:dyDescent="0.2">
@@ -8145,13 +8154,13 @@
         <v>410</v>
       </c>
       <c r="B16" s="105" t="s">
-        <v>1287</v>
+        <v>1285</v>
       </c>
       <c r="C16" s="106" t="s">
         <v>404</v>
       </c>
       <c r="D16" s="107" t="s">
-        <v>1265</v>
+        <v>1263</v>
       </c>
       <c r="E16" s="89" t="s">
         <v>404</v>
@@ -8162,13 +8171,13 @@
         <v>413</v>
       </c>
       <c r="B17" s="105" t="s">
-        <v>1288</v>
+        <v>1286</v>
       </c>
       <c r="C17" s="106" t="s">
         <v>404</v>
       </c>
       <c r="D17" s="107" t="s">
-        <v>1267</v>
+        <v>1265</v>
       </c>
       <c r="E17" s="89" t="s">
         <v>404</v>
@@ -8179,16 +8188,16 @@
         <v>14</v>
       </c>
       <c r="B18" s="95" t="s">
-        <v>1289</v>
+        <v>1287</v>
       </c>
       <c r="C18" s="96" t="s">
-        <v>1290</v>
+        <v>1288</v>
       </c>
       <c r="D18" s="95" t="s">
         <v>404</v>
       </c>
       <c r="E18" s="89" t="s">
-        <v>1291</v>
+        <v>1289</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -8213,13 +8222,13 @@
         <v>243</v>
       </c>
       <c r="B20" s="95" t="s">
-        <v>1292</v>
+        <v>1290</v>
       </c>
       <c r="C20" s="96" t="s">
-        <v>1293</v>
+        <v>1291</v>
       </c>
       <c r="D20" s="95" t="s">
-        <v>1254</v>
+        <v>1252</v>
       </c>
       <c r="E20" s="89" t="s">
         <v>404</v>
@@ -8227,16 +8236,16 @@
     </row>
     <row r="21" spans="1:5" ht="48" x14ac:dyDescent="0.2">
       <c r="A21" s="94" t="s">
-        <v>1256</v>
+        <v>1254</v>
       </c>
       <c r="B21" s="95" t="s">
+        <v>1292</v>
+      </c>
+      <c r="C21" s="96" t="s">
+        <v>1293</v>
+      </c>
+      <c r="D21" s="95" t="s">
         <v>1294</v>
-      </c>
-      <c r="C21" s="96" t="s">
-        <v>1295</v>
-      </c>
-      <c r="D21" s="95" t="s">
-        <v>1296</v>
       </c>
       <c r="E21" s="89" t="s">
         <v>404</v>
@@ -8247,10 +8256,10 @@
         <v>758</v>
       </c>
       <c r="B22" s="95" t="s">
-        <v>1297</v>
+        <v>1295</v>
       </c>
       <c r="C22" s="96" t="s">
-        <v>1298</v>
+        <v>1296</v>
       </c>
       <c r="D22" s="95" t="s">
         <v>404</v>
@@ -8264,13 +8273,13 @@
         <v>410</v>
       </c>
       <c r="B23" s="105" t="s">
-        <v>1299</v>
+        <v>1297</v>
       </c>
       <c r="C23" s="106" t="s">
         <v>404</v>
       </c>
       <c r="D23" s="107" t="s">
-        <v>1265</v>
+        <v>1263</v>
       </c>
       <c r="E23" s="89" t="s">
         <v>404</v>
@@ -8281,13 +8290,13 @@
         <v>413</v>
       </c>
       <c r="B24" s="105" t="s">
-        <v>1300</v>
+        <v>1298</v>
       </c>
       <c r="C24" s="106" t="s">
         <v>404</v>
       </c>
       <c r="D24" s="107" t="s">
-        <v>1267</v>
+        <v>1265</v>
       </c>
       <c r="E24" s="89" t="s">
         <v>404</v>
@@ -8340,7 +8349,7 @@
     </row>
     <row r="2" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="193" t="s">
-        <v>1301</v>
+        <v>1299</v>
       </c>
       <c r="B2" s="194"/>
       <c r="C2" s="194"/>
@@ -8353,16 +8362,16 @@
         <v>243</v>
       </c>
       <c r="B3" s="5" t="s">
+        <v>1300</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>1301</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>1232</v>
+      </c>
+      <c r="E3" s="37" t="s">
         <v>1302</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>1303</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>1234</v>
-      </c>
-      <c r="E3" s="37" t="s">
-        <v>1304</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="32" x14ac:dyDescent="0.2">
@@ -8370,13 +8379,13 @@
         <v>261</v>
       </c>
       <c r="B4" s="5" t="s">
+        <v>1303</v>
+      </c>
+      <c r="C4" s="59" t="s">
+        <v>1304</v>
+      </c>
+      <c r="E4" s="37" t="s">
         <v>1305</v>
-      </c>
-      <c r="C4" s="59" t="s">
-        <v>1306</v>
-      </c>
-      <c r="E4" s="37" t="s">
-        <v>1307</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="16" x14ac:dyDescent="0.2">
@@ -8384,13 +8393,13 @@
         <v>254</v>
       </c>
       <c r="B5" s="5" t="s">
+        <v>1306</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>1307</v>
+      </c>
+      <c r="E5" s="37" t="s">
         <v>1308</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>1309</v>
-      </c>
-      <c r="E5" s="37" t="s">
-        <v>1310</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="80" x14ac:dyDescent="0.2">
@@ -8398,13 +8407,13 @@
         <v>261</v>
       </c>
       <c r="B6" s="5" t="s">
+        <v>1309</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>1310</v>
+      </c>
+      <c r="E6" s="37" t="s">
         <v>1311</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>1312</v>
-      </c>
-      <c r="E6" s="37" t="s">
-        <v>1313</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="32" x14ac:dyDescent="0.2">
@@ -8412,112 +8421,112 @@
         <v>254</v>
       </c>
       <c r="B7" s="5" t="s">
+        <v>1312</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>1313</v>
+      </c>
+      <c r="E7" s="37" t="s">
         <v>1314</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>1315</v>
-      </c>
-      <c r="E7" s="37" t="s">
-        <v>1316</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
+        <v>1315</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>1316</v>
+      </c>
+      <c r="C8" s="6" t="s">
         <v>1317</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="E8" s="37" t="s">
         <v>1318</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>1319</v>
-      </c>
-      <c r="E8" s="37" t="s">
-        <v>1320</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
+        <v>1319</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>1320</v>
+      </c>
+      <c r="C9" s="6" t="s">
         <v>1321</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="E9" s="37" t="s">
         <v>1322</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>1323</v>
-      </c>
-      <c r="E9" s="37" t="s">
-        <v>1324</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
-        <v>1321</v>
+        <v>1319</v>
       </c>
       <c r="B10" s="5" t="s">
+        <v>1323</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>1324</v>
+      </c>
+      <c r="E10" s="37" t="s">
         <v>1325</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>1326</v>
-      </c>
-      <c r="E10" s="37" t="s">
-        <v>1327</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
-        <v>1321</v>
+        <v>1319</v>
       </c>
       <c r="B11" s="5" t="s">
+        <v>1326</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>1327</v>
+      </c>
+      <c r="E11" s="37" t="s">
         <v>1328</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>1329</v>
-      </c>
-      <c r="E11" s="37" t="s">
-        <v>1330</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="5" t="s">
-        <v>1321</v>
+        <v>1319</v>
       </c>
       <c r="B12" s="5" t="s">
+        <v>1329</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>1330</v>
+      </c>
+      <c r="E12" s="37" t="s">
         <v>1331</v>
-      </c>
-      <c r="C12" s="6" t="s">
-        <v>1332</v>
-      </c>
-      <c r="E12" s="37" t="s">
-        <v>1333</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="s">
-        <v>1321</v>
+        <v>1319</v>
       </c>
       <c r="B13" s="5" t="s">
+        <v>1332</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>1333</v>
+      </c>
+      <c r="E13" s="37" t="s">
         <v>1334</v>
-      </c>
-      <c r="C13" s="6" t="s">
-        <v>1335</v>
-      </c>
-      <c r="E13" s="37" t="s">
-        <v>1336</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A14" s="5" t="s">
-        <v>1317</v>
+        <v>1315</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>1337</v>
+        <v>1335</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>1338</v>
+        <v>1336</v>
       </c>
       <c r="D14" s="1"/>
       <c r="E14" s="37" t="s">
-        <v>1339</v>
+        <v>1337</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="32" x14ac:dyDescent="0.2">
@@ -8525,14 +8534,14 @@
         <v>952</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>1340</v>
+        <v>1338</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>1341</v>
+        <v>1339</v>
       </c>
       <c r="D15" s="1"/>
       <c r="E15" s="37" t="s">
-        <v>1342</v>
+        <v>1340</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="16" x14ac:dyDescent="0.2">
@@ -8540,34 +8549,34 @@
         <v>14</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>1343</v>
+        <v>1341</v>
       </c>
       <c r="C16" s="74" t="s">
-        <v>1344</v>
+        <v>1342</v>
       </c>
       <c r="D16" s="18"/>
       <c r="E16" s="37" t="s">
-        <v>1345</v>
+        <v>1343</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A17" s="5" t="s">
+        <v>1344</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>1345</v>
+      </c>
+      <c r="C17" s="75" t="s">
         <v>1346</v>
-      </c>
-      <c r="B17" s="7" t="s">
-        <v>1347</v>
-      </c>
-      <c r="C17" s="75" t="s">
-        <v>1348</v>
       </c>
       <c r="D17" s="18"/>
       <c r="E17" s="37" t="s">
-        <v>1349</v>
+        <v>1347</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="193" t="s">
-        <v>1350</v>
+        <v>1348</v>
       </c>
       <c r="B18" s="194"/>
       <c r="C18" s="194"/>
@@ -8580,16 +8589,16 @@
         <v>243</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>1353</v>
+        <v>1351</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>1351</v>
+        <v>1349</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>1234</v>
+        <v>1232</v>
       </c>
       <c r="E19" s="37" t="s">
-        <v>1352</v>
+        <v>1350</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="96" x14ac:dyDescent="0.2">
@@ -8597,13 +8606,13 @@
         <v>261</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>1354</v>
+        <v>1352</v>
       </c>
       <c r="C20" s="59" t="s">
+        <v>1422</v>
+      </c>
+      <c r="E20" s="37" t="s">
         <v>1424</v>
-      </c>
-      <c r="E20" s="37" t="s">
-        <v>1426</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="16" x14ac:dyDescent="0.2">
@@ -8611,13 +8620,13 @@
         <v>254</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>1355</v>
+        <v>1353</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>1309</v>
+        <v>1307</v>
       </c>
       <c r="E21" s="37" t="s">
-        <v>1310</v>
+        <v>1308</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="80" x14ac:dyDescent="0.2">
@@ -8625,13 +8634,13 @@
         <v>261</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>1356</v>
+        <v>1354</v>
       </c>
       <c r="C22" s="6" t="s">
+        <v>1423</v>
+      </c>
+      <c r="E22" s="37" t="s">
         <v>1425</v>
-      </c>
-      <c r="E22" s="37" t="s">
-        <v>1427</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
@@ -8655,7 +8664,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E4" sqref="E4"/>
+      <selection pane="bottomLeft" activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -8695,13 +8704,13 @@
         <v>7</v>
       </c>
       <c r="C2" s="100" t="s">
-        <v>1428</v>
+        <v>1431</v>
       </c>
       <c r="D2" s="98" t="s">
         <v>8</v>
       </c>
       <c r="E2" s="99" t="s">
-        <v>1428</v>
+        <v>1431</v>
       </c>
       <c r="F2" s="98"/>
     </row>
@@ -8719,7 +8728,7 @@
         <v>12</v>
       </c>
       <c r="E3" s="37" t="s">
-        <v>1423</v>
+        <v>1421</v>
       </c>
       <c r="F3" s="5" t="s">
         <v>13</v>
@@ -9774,18 +9783,18 @@
     </row>
     <row r="67" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="B67" s="1" t="s">
-        <v>1367</v>
+        <v>1365</v>
       </c>
       <c r="C67" s="2" t="s">
+        <v>1366</v>
+      </c>
+      <c r="E67" s="40" t="s">
         <v>1368</v>
-      </c>
-      <c r="E67" s="40" t="s">
-        <v>1370</v>
       </c>
     </row>
     <row r="68" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="B68" s="1" t="s">
-        <v>1369</v>
+        <v>1367</v>
       </c>
       <c r="C68" s="2" t="s">
         <v>76</v>
@@ -10086,14 +10095,14 @@
         <v>243</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>1394</v>
+        <v>1392</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>1395</v>
+        <v>1393</v>
       </c>
       <c r="D2" s="5"/>
       <c r="E2" s="43" t="s">
-        <v>1403</v>
+        <v>1401</v>
       </c>
       <c r="F2" s="1"/>
     </row>
@@ -10102,19 +10111,19 @@
         <v>484</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>1396</v>
+        <v>1394</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>1397</v>
+        <v>1395</v>
       </c>
       <c r="D3" s="5"/>
       <c r="E3" s="43" t="s">
-        <v>1404</v>
+        <v>1402</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="159" t="s">
-        <v>1398</v>
+        <v>1396</v>
       </c>
       <c r="B4" s="160"/>
       <c r="C4" s="160"/>
@@ -10126,14 +10135,14 @@
         <v>243</v>
       </c>
       <c r="B5" s="5" t="s">
+        <v>1397</v>
+      </c>
+      <c r="C5" s="6" t="s">
         <v>1399</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>1401</v>
       </c>
       <c r="D5" s="5"/>
       <c r="E5" s="43" t="s">
-        <v>1405</v>
+        <v>1403</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="96" x14ac:dyDescent="0.2">
@@ -10141,14 +10150,14 @@
         <v>484</v>
       </c>
       <c r="B6" s="5" t="s">
+        <v>1398</v>
+      </c>
+      <c r="C6" s="6" t="s">
         <v>1400</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>1402</v>
       </c>
       <c r="D6" s="5"/>
       <c r="E6" s="43" t="s">
-        <v>1406</v>
+        <v>1404</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
@@ -10369,7 +10378,7 @@
         <v>243</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>1409</v>
+        <v>1407</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>276</v>
@@ -10393,7 +10402,7 @@
         <v>246</v>
       </c>
       <c r="E4" s="43" t="s">
-        <v>1410</v>
+        <v>1408</v>
       </c>
       <c r="F4" s="68" t="s">
         <v>280</v>
@@ -10407,13 +10416,13 @@
         <v>281</v>
       </c>
       <c r="C5" s="52" t="s">
-        <v>1415</v>
+        <v>1413</v>
       </c>
       <c r="D5" s="66" t="s">
         <v>282</v>
       </c>
       <c r="E5" s="156" t="s">
-        <v>1420</v>
+        <v>1418</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>283</v>
@@ -10427,13 +10436,13 @@
         <v>284</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>1416</v>
+        <v>1414</v>
       </c>
       <c r="D6" s="67" t="s">
         <v>285</v>
       </c>
       <c r="E6" s="157" t="s">
-        <v>1417</v>
+        <v>1415</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="160" x14ac:dyDescent="0.2">
@@ -10444,13 +10453,13 @@
         <v>286</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>1418</v>
+        <v>1416</v>
       </c>
       <c r="D7" s="67" t="s">
         <v>287</v>
       </c>
       <c r="E7" s="157" t="s">
-        <v>1419</v>
+        <v>1417</v>
       </c>
       <c r="F7" s="68" t="s">
         <v>288</v>
@@ -10652,7 +10661,7 @@
         <v>336</v>
       </c>
       <c r="C19" s="64" t="s">
-        <v>1407</v>
+        <v>1405</v>
       </c>
       <c r="D19" s="7" t="s">
         <v>337</v>
@@ -10786,17 +10795,17 @@
     </row>
     <row r="27" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A27" s="5" t="s">
-        <v>1413</v>
+        <v>1411</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>1414</v>
+        <v>1412</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>1411</v>
+        <v>1409</v>
       </c>
       <c r="D27" s="5"/>
       <c r="E27" s="37" t="s">
-        <v>1412</v>
+        <v>1410</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
@@ -10873,13 +10882,13 @@
       </c>
     </row>
     <row r="2" spans="1:6" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="162" t="s">
+      <c r="A2" s="165" t="s">
         <v>367</v>
       </c>
-      <c r="B2" s="163"/>
-      <c r="C2" s="163"/>
-      <c r="D2" s="163"/>
-      <c r="E2" s="164"/>
+      <c r="B2" s="166"/>
+      <c r="C2" s="166"/>
+      <c r="D2" s="166"/>
+      <c r="E2" s="167"/>
       <c r="F2" s="33"/>
     </row>
     <row r="3" spans="1:6" ht="48" x14ac:dyDescent="0.2">
@@ -11007,13 +11016,13 @@
       <c r="F9" s="119"/>
     </row>
     <row r="10" spans="1:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="165" t="s">
+      <c r="A10" s="168" t="s">
         <v>396</v>
       </c>
-      <c r="B10" s="166"/>
-      <c r="C10" s="166"/>
-      <c r="D10" s="166"/>
-      <c r="E10" s="167"/>
+      <c r="B10" s="169"/>
+      <c r="C10" s="169"/>
+      <c r="D10" s="169"/>
+      <c r="E10" s="170"/>
       <c r="F10" s="119"/>
     </row>
     <row r="11" spans="1:6" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -11042,13 +11051,13 @@
         <v>401</v>
       </c>
       <c r="C12" s="153" t="s">
-        <v>1371</v>
+        <v>1369</v>
       </c>
       <c r="D12" s="84" t="s">
         <v>402</v>
       </c>
       <c r="E12" s="152" t="s">
-        <v>1372</v>
+        <v>1370</v>
       </c>
       <c r="F12" s="86"/>
     </row>
@@ -11060,13 +11069,13 @@
         <v>403</v>
       </c>
       <c r="C13" s="154" t="s">
-        <v>1373</v>
+        <v>1371</v>
       </c>
       <c r="D13" s="88" t="s">
         <v>404</v>
       </c>
       <c r="E13" s="155" t="s">
-        <v>1374</v>
+        <v>1372</v>
       </c>
       <c r="F13" s="86"/>
     </row>
@@ -11534,7 +11543,7 @@
         <v>485</v>
       </c>
       <c r="C45" s="59" t="s">
-        <v>1390</v>
+        <v>1388</v>
       </c>
       <c r="D45" s="116"/>
       <c r="E45" s="120" t="s">
@@ -11547,14 +11556,14 @@
         <v>484</v>
       </c>
       <c r="B46" s="116" t="s">
-        <v>1393</v>
+        <v>1391</v>
       </c>
       <c r="C46" s="59" t="s">
-        <v>1391</v>
+        <v>1389</v>
       </c>
       <c r="D46" s="116"/>
       <c r="E46" s="120" t="s">
-        <v>1392</v>
+        <v>1390</v>
       </c>
       <c r="F46" s="119"/>
     </row>
@@ -11782,7 +11791,7 @@
         <v>522</v>
       </c>
       <c r="E61" s="120" t="s">
-        <v>1383</v>
+        <v>1381</v>
       </c>
       <c r="F61" s="119"/>
     </row>
@@ -11791,14 +11800,14 @@
         <v>519</v>
       </c>
       <c r="B62" s="116" t="s">
+        <v>1378</v>
+      </c>
+      <c r="C62" s="117" t="s">
         <v>1380</v>
-      </c>
-      <c r="C62" s="117" t="s">
-        <v>1382</v>
       </c>
       <c r="D62" s="116"/>
       <c r="E62" s="120" t="s">
-        <v>1381</v>
+        <v>1379</v>
       </c>
       <c r="F62" s="119"/>
     </row>
@@ -12984,7 +12993,7 @@
         <v>710</v>
       </c>
       <c r="C141" s="113" t="s">
-        <v>1358</v>
+        <v>1356</v>
       </c>
       <c r="D141" s="122" t="s">
         <v>711</v>
@@ -13074,7 +13083,7 @@
         <v>725</v>
       </c>
       <c r="C147" s="59" t="s">
-        <v>1357</v>
+        <v>1355</v>
       </c>
       <c r="D147" s="116" t="s">
         <v>726</v>
@@ -13105,14 +13114,14 @@
         <v>37</v>
       </c>
       <c r="B149" s="116" t="s">
+        <v>1357</v>
+      </c>
+      <c r="C149" s="59" t="s">
         <v>1359</v>
-      </c>
-      <c r="C149" s="59" t="s">
-        <v>1361</v>
       </c>
       <c r="D149" s="116"/>
       <c r="E149" s="120" t="s">
-        <v>1363</v>
+        <v>1361</v>
       </c>
       <c r="F149" s="119"/>
     </row>
@@ -13121,14 +13130,14 @@
         <v>37</v>
       </c>
       <c r="B150" s="116" t="s">
+        <v>1358</v>
+      </c>
+      <c r="C150" s="59" t="s">
         <v>1360</v>
-      </c>
-      <c r="C150" s="59" t="s">
-        <v>1362</v>
       </c>
       <c r="D150" s="116"/>
       <c r="E150" s="120" t="s">
-        <v>1364</v>
+        <v>1362</v>
       </c>
       <c r="F150" s="119"/>
     </row>
@@ -13347,13 +13356,13 @@
       <c r="F164" s="119"/>
     </row>
     <row r="165" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A165" s="168" t="s">
+      <c r="A165" s="162" t="s">
         <v>765</v>
       </c>
-      <c r="B165" s="169"/>
-      <c r="C165" s="169"/>
-      <c r="D165" s="169"/>
-      <c r="E165" s="170"/>
+      <c r="B165" s="163"/>
+      <c r="C165" s="163"/>
+      <c r="D165" s="163"/>
+      <c r="E165" s="164"/>
       <c r="F165" s="129" t="s">
         <v>766</v>
       </c>
@@ -13780,13 +13789,13 @@
         <v>815</v>
       </c>
       <c r="C193" s="59" t="s">
-        <v>1375</v>
+        <v>1373</v>
       </c>
       <c r="D193" s="116" t="s">
         <v>816</v>
       </c>
       <c r="E193" s="120" t="s">
-        <v>1379</v>
+        <v>1377</v>
       </c>
       <c r="F193" s="119"/>
     </row>
@@ -13795,14 +13804,14 @@
         <v>484</v>
       </c>
       <c r="B194" s="116" t="s">
-        <v>1376</v>
+        <v>1374</v>
       </c>
       <c r="C194" s="59" t="s">
-        <v>1377</v>
+        <v>1375</v>
       </c>
       <c r="D194" s="116"/>
       <c r="E194" s="120" t="s">
-        <v>1378</v>
+        <v>1376</v>
       </c>
       <c r="F194" s="119"/>
     </row>
@@ -13902,11 +13911,11 @@
         <v>827</v>
       </c>
       <c r="C201" s="117" t="s">
-        <v>1386</v>
+        <v>1384</v>
       </c>
       <c r="D201" s="116"/>
       <c r="E201" s="120" t="s">
-        <v>1389</v>
+        <v>1387</v>
       </c>
       <c r="F201" s="119"/>
     </row>
@@ -13915,7 +13924,7 @@
         <v>734</v>
       </c>
       <c r="B202" s="116" t="s">
-        <v>1388</v>
+        <v>1386</v>
       </c>
       <c r="C202" s="117" t="s">
         <v>43</v>
@@ -13931,14 +13940,14 @@
         <v>32</v>
       </c>
       <c r="B203" s="116" t="s">
-        <v>1387</v>
+        <v>1385</v>
       </c>
       <c r="C203" s="134" t="s">
-        <v>1384</v>
+        <v>1382</v>
       </c>
       <c r="D203" s="116"/>
       <c r="E203" s="120" t="s">
-        <v>1385</v>
+        <v>1383</v>
       </c>
       <c r="F203" s="119"/>
     </row>
@@ -14310,13 +14319,13 @@
         <v>866</v>
       </c>
       <c r="C228" s="59" t="s">
-        <v>1421</v>
+        <v>1419</v>
       </c>
       <c r="D228" s="116" t="s">
         <v>867</v>
       </c>
       <c r="E228" s="120" t="s">
-        <v>1422</v>
+        <v>1420</v>
       </c>
       <c r="F228" s="119"/>
     </row>
@@ -15256,6 +15265,18 @@
     </row>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="A225:E225"/>
+    <mergeCell ref="A186:E186"/>
+    <mergeCell ref="A190:E190"/>
+    <mergeCell ref="A197:E197"/>
+    <mergeCell ref="A208:E208"/>
+    <mergeCell ref="A214:E214"/>
+    <mergeCell ref="A58:E58"/>
+    <mergeCell ref="A2:E2"/>
+    <mergeCell ref="A10:E10"/>
+    <mergeCell ref="A14:E14"/>
+    <mergeCell ref="A24:E24"/>
+    <mergeCell ref="A43:E43"/>
     <mergeCell ref="A174:E174"/>
     <mergeCell ref="A157:E157"/>
     <mergeCell ref="A63:E63"/>
@@ -15266,18 +15287,6 @@
     <mergeCell ref="A146:E146"/>
     <mergeCell ref="A92:E92"/>
     <mergeCell ref="A165:E165"/>
-    <mergeCell ref="A58:E58"/>
-    <mergeCell ref="A2:E2"/>
-    <mergeCell ref="A10:E10"/>
-    <mergeCell ref="A14:E14"/>
-    <mergeCell ref="A24:E24"/>
-    <mergeCell ref="A43:E43"/>
-    <mergeCell ref="A225:E225"/>
-    <mergeCell ref="A186:E186"/>
-    <mergeCell ref="A190:E190"/>
-    <mergeCell ref="A197:E197"/>
-    <mergeCell ref="A208:E208"/>
-    <mergeCell ref="A214:E214"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -15285,11 +15294,11 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E7FE5E2-8B99-45DF-8804-30523FDA4B3A}">
-  <dimension ref="A1:F54"/>
+  <dimension ref="A1:F55"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A39" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D44" sqref="D44"/>
+      <pane ySplit="1" topLeftCell="A31" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -15548,13 +15557,13 @@
         <v>942</v>
       </c>
       <c r="C17" s="151" t="s">
-        <v>1365</v>
+        <v>1363</v>
       </c>
       <c r="D17" s="92" t="s">
         <v>934</v>
       </c>
       <c r="E17" s="152" t="s">
-        <v>1366</v>
+        <v>1364</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="80" x14ac:dyDescent="0.2">
@@ -15746,7 +15755,7 @@
         <v>981</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="96" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:6" ht="80" x14ac:dyDescent="0.2">
       <c r="A32" s="19" t="s">
         <v>261</v>
       </c>
@@ -15754,227 +15763,224 @@
         <v>982</v>
       </c>
       <c r="C32" s="21" t="s">
+        <v>1426</v>
+      </c>
+      <c r="E32" s="46" t="s">
+        <v>1427</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+      <c r="A33" s="19" t="s">
+        <v>261</v>
+      </c>
+      <c r="B33" s="19" t="s">
+        <v>1428</v>
+      </c>
+      <c r="C33" s="21" t="s">
+        <v>1429</v>
+      </c>
+      <c r="E33" s="46" t="s">
+        <v>1430</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+      <c r="A34" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="B34" s="19" t="s">
         <v>983</v>
       </c>
-      <c r="E32" s="46" t="s">
+      <c r="C34" s="21" t="s">
         <v>984</v>
       </c>
-    </row>
-    <row r="33" spans="1:6" ht="48" x14ac:dyDescent="0.2">
-      <c r="A33" s="19" t="s">
-        <v>37</v>
-      </c>
-      <c r="B33" s="19" t="s">
+      <c r="D34" s="26" t="s">
         <v>985</v>
       </c>
-      <c r="C33" s="21" t="s">
+      <c r="E34" s="46" t="s">
         <v>986</v>
       </c>
-      <c r="D33" s="26" t="s">
-        <v>987</v>
-      </c>
-      <c r="E33" s="46" t="s">
-        <v>988</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" ht="96" x14ac:dyDescent="0.2">
-      <c r="A34" s="18" t="s">
-        <v>410</v>
-      </c>
-      <c r="B34" s="28" t="s">
-        <v>989</v>
-      </c>
-      <c r="C34" s="27"/>
-      <c r="D34" s="18" t="s">
-        <v>990</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" ht="80" x14ac:dyDescent="0.2">
+    </row>
+    <row r="35" spans="1:6" ht="96" x14ac:dyDescent="0.2">
       <c r="A35" s="18" t="s">
         <v>410</v>
       </c>
       <c r="B35" s="28" t="s">
-        <v>991</v>
+        <v>987</v>
       </c>
       <c r="C35" s="27"/>
       <c r="D35" s="18" t="s">
-        <v>992</v>
+        <v>988</v>
       </c>
     </row>
     <row r="36" spans="1:6" ht="80" x14ac:dyDescent="0.2">
       <c r="A36" s="18" t="s">
-        <v>413</v>
+        <v>410</v>
       </c>
       <c r="B36" s="28" t="s">
-        <v>993</v>
+        <v>989</v>
       </c>
       <c r="C36" s="27"/>
       <c r="D36" s="18" t="s">
+        <v>990</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" ht="80" x14ac:dyDescent="0.2">
+      <c r="A37" s="18" t="s">
+        <v>413</v>
+      </c>
+      <c r="B37" s="28" t="s">
+        <v>991</v>
+      </c>
+      <c r="C37" s="27"/>
+      <c r="D37" s="18" t="s">
+        <v>992</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A38" s="171" t="s">
+        <v>993</v>
+      </c>
+      <c r="B38" s="172"/>
+      <c r="C38" s="172"/>
+      <c r="D38" s="172"/>
+      <c r="E38" s="173"/>
+    </row>
+    <row r="39" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+      <c r="A39" s="19" t="s">
+        <v>243</v>
+      </c>
+      <c r="B39" s="19" t="s">
         <v>994</v>
       </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A37" s="171" t="s">
+      <c r="C39" s="21" t="s">
         <v>995</v>
       </c>
-      <c r="B37" s="172"/>
-      <c r="C37" s="172"/>
-      <c r="D37" s="172"/>
-      <c r="E37" s="173"/>
-    </row>
-    <row r="38" spans="1:6" ht="48" x14ac:dyDescent="0.2">
-      <c r="A38" s="19" t="s">
-        <v>243</v>
-      </c>
-      <c r="B38" s="19" t="s">
+      <c r="D39" s="5" t="s">
         <v>996</v>
       </c>
-      <c r="C38" s="21" t="s">
+      <c r="E39" s="46" t="s">
         <v>997</v>
       </c>
-      <c r="D38" s="5" t="s">
+    </row>
+    <row r="40" spans="1:6" ht="64" x14ac:dyDescent="0.2">
+      <c r="A40" s="18" t="s">
+        <v>410</v>
+      </c>
+      <c r="B40" s="28" t="s">
         <v>998</v>
-      </c>
-      <c r="E38" s="46" t="s">
-        <v>999</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" ht="64" x14ac:dyDescent="0.2">
-      <c r="A39" s="18" t="s">
-        <v>410</v>
-      </c>
-      <c r="B39" s="28" t="s">
-        <v>1000</v>
-      </c>
-      <c r="C39" s="27"/>
-      <c r="D39" s="18" t="s">
-        <v>1001</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" ht="80" x14ac:dyDescent="0.2">
-      <c r="A40" s="18" t="s">
-        <v>413</v>
-      </c>
-      <c r="B40" s="28" t="s">
-        <v>1002</v>
       </c>
       <c r="C40" s="27"/>
       <c r="D40" s="18" t="s">
-        <v>994</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A41" s="177" t="s">
+        <v>999</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" ht="80" x14ac:dyDescent="0.2">
+      <c r="A41" s="18" t="s">
+        <v>413</v>
+      </c>
+      <c r="B41" s="28" t="s">
+        <v>1000</v>
+      </c>
+      <c r="C41" s="27"/>
+      <c r="D41" s="18" t="s">
+        <v>992</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A42" s="177" t="s">
+        <v>1001</v>
+      </c>
+      <c r="B42" s="178"/>
+      <c r="C42" s="178"/>
+      <c r="D42" s="178"/>
+      <c r="E42" s="179"/>
+    </row>
+    <row r="43" spans="1:6" ht="96" x14ac:dyDescent="0.2">
+      <c r="A43" s="116" t="s">
+        <v>243</v>
+      </c>
+      <c r="B43" s="116" t="s">
+        <v>1002</v>
+      </c>
+      <c r="C43" s="21" t="s">
+        <v>858</v>
+      </c>
+      <c r="D43" s="116" t="s">
         <v>1003</v>
       </c>
-      <c r="B41" s="178"/>
-      <c r="C41" s="178"/>
-      <c r="D41" s="178"/>
-      <c r="E41" s="179"/>
-    </row>
-    <row r="42" spans="1:6" ht="96" x14ac:dyDescent="0.2">
-      <c r="A42" s="116" t="s">
-        <v>243</v>
-      </c>
-      <c r="B42" s="116" t="s">
+      <c r="E43" s="46" t="s">
+        <v>860</v>
+      </c>
+      <c r="F43" s="72" t="s">
         <v>1004</v>
       </c>
-      <c r="C42" s="21" t="s">
-        <v>858</v>
-      </c>
-      <c r="D42" s="116" t="s">
+    </row>
+    <row r="44" spans="1:6" ht="80" x14ac:dyDescent="0.2">
+      <c r="A44" s="116" t="s">
+        <v>368</v>
+      </c>
+      <c r="B44" s="116" t="s">
         <v>1005</v>
       </c>
-      <c r="E42" s="46" t="s">
-        <v>860</v>
-      </c>
-      <c r="F42" s="72" t="s">
+      <c r="C44" s="21" t="s">
+        <v>916</v>
+      </c>
+      <c r="D44" s="116" t="s">
         <v>1006</v>
       </c>
-    </row>
-    <row r="43" spans="1:6" ht="80" x14ac:dyDescent="0.2">
-      <c r="A43" s="116" t="s">
-        <v>368</v>
-      </c>
-      <c r="B43" s="116" t="s">
-        <v>1007</v>
-      </c>
-      <c r="C43" s="21" t="s">
-        <v>916</v>
-      </c>
-      <c r="D43" s="116" t="s">
-        <v>1008</v>
-      </c>
-      <c r="E43" s="46" t="s">
+      <c r="E44" s="46" t="s">
         <v>917</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" ht="48" x14ac:dyDescent="0.2">
-      <c r="A44" s="116" t="s">
-        <v>261</v>
-      </c>
-      <c r="B44" s="116" t="s">
-        <v>1009</v>
-      </c>
-      <c r="C44" s="62" t="s">
-        <v>1421</v>
-      </c>
-      <c r="D44" s="116" t="s">
-        <v>1010</v>
-      </c>
-      <c r="E44" s="46" t="s">
-        <v>1422</v>
       </c>
     </row>
     <row r="45" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A45" s="116" t="s">
-        <v>382</v>
+        <v>261</v>
       </c>
       <c r="B45" s="116" t="s">
-        <v>1011</v>
-      </c>
-      <c r="C45" s="21" t="s">
-        <v>1012</v>
-      </c>
-      <c r="D45" s="121" t="s">
-        <v>1013</v>
+        <v>1007</v>
+      </c>
+      <c r="C45" s="62" t="s">
+        <v>1419</v>
+      </c>
+      <c r="D45" s="116" t="s">
+        <v>1008</v>
       </c>
       <c r="E45" s="46" t="s">
-        <v>1012</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" ht="64" x14ac:dyDescent="0.2">
+        <v>1420</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A46" s="116" t="s">
         <v>382</v>
       </c>
       <c r="B46" s="116" t="s">
-        <v>1014</v>
+        <v>1009</v>
       </c>
       <c r="C46" s="21" t="s">
-        <v>1015</v>
+        <v>1010</v>
       </c>
       <c r="D46" s="121" t="s">
-        <v>1016</v>
+        <v>1011</v>
       </c>
       <c r="E46" s="46" t="s">
-        <v>1017</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+        <v>1010</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" ht="64" x14ac:dyDescent="0.2">
       <c r="A47" s="116" t="s">
         <v>382</v>
       </c>
       <c r="B47" s="116" t="s">
-        <v>1018</v>
+        <v>1012</v>
       </c>
       <c r="C47" s="21" t="s">
-        <v>1019</v>
+        <v>1013</v>
       </c>
       <c r="D47" s="121" t="s">
-        <v>1020</v>
+        <v>1014</v>
       </c>
       <c r="E47" s="46" t="s">
-        <v>1021</v>
+        <v>1015</v>
       </c>
     </row>
     <row r="48" spans="1:6" ht="48" x14ac:dyDescent="0.2">
@@ -15982,95 +15988,95 @@
         <v>382</v>
       </c>
       <c r="B48" s="116" t="s">
+        <v>1016</v>
+      </c>
+      <c r="C48" s="21" t="s">
+        <v>1017</v>
+      </c>
+      <c r="D48" s="121" t="s">
+        <v>1018</v>
+      </c>
+      <c r="E48" s="46" t="s">
+        <v>1019</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+      <c r="A49" s="116" t="s">
+        <v>382</v>
+      </c>
+      <c r="B49" s="116" t="s">
+        <v>1020</v>
+      </c>
+      <c r="C49" s="21" t="s">
+        <v>1021</v>
+      </c>
+      <c r="D49" s="121" t="s">
         <v>1022</v>
       </c>
-      <c r="C48" s="21" t="s">
+      <c r="E49" s="46" t="s">
         <v>1023</v>
       </c>
-      <c r="D48" s="121" t="s">
+    </row>
+    <row r="50" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A50" s="91" t="s">
+        <v>382</v>
+      </c>
+      <c r="B50" s="92" t="s">
         <v>1024</v>
       </c>
-      <c r="E48" s="46" t="s">
+      <c r="C50" s="93" t="s">
         <v>1025</v>
       </c>
-    </row>
-    <row r="49" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A49" s="91" t="s">
-        <v>382</v>
-      </c>
-      <c r="B49" s="92" t="s">
+      <c r="D50" s="101" t="s">
+        <v>404</v>
+      </c>
+      <c r="E50" s="85" t="s">
         <v>1026</v>
       </c>
-      <c r="C49" s="93" t="s">
+    </row>
+    <row r="51" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A51" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="B51" s="19" t="s">
         <v>1027</v>
       </c>
-      <c r="D49" s="101" t="s">
-        <v>404</v>
-      </c>
-      <c r="E49" s="85" t="s">
-        <v>1028</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A50" s="19" t="s">
-        <v>32</v>
-      </c>
-      <c r="B50" s="19" t="s">
-        <v>1029</v>
-      </c>
-      <c r="C50" s="21" t="s">
+      <c r="C51" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="E50" s="46" t="s">
+      <c r="E51" s="46" t="s">
         <v>36</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" ht="48" x14ac:dyDescent="0.2">
-      <c r="A51" s="19" t="s">
-        <v>1030</v>
-      </c>
-      <c r="B51" s="19" t="s">
-        <v>1031</v>
-      </c>
-      <c r="C51" s="21" t="s">
-        <v>1032</v>
-      </c>
-      <c r="D51" s="19" t="s">
-        <v>1033</v>
-      </c>
-      <c r="F51" s="71" t="s">
-        <v>904</v>
       </c>
     </row>
     <row r="52" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A52" s="19" t="s">
+        <v>1028</v>
+      </c>
+      <c r="B52" s="19" t="s">
+        <v>1029</v>
+      </c>
+      <c r="C52" s="21" t="s">
         <v>1030</v>
       </c>
-      <c r="B52" s="19" t="s">
-        <v>1034</v>
-      </c>
-      <c r="C52" s="21" t="s">
-        <v>1035</v>
-      </c>
       <c r="D52" s="19" t="s">
-        <v>1033</v>
+        <v>1031</v>
       </c>
       <c r="F52" s="71" t="s">
         <v>904</v>
       </c>
     </row>
     <row r="53" spans="1:6" ht="48" x14ac:dyDescent="0.2">
-      <c r="A53" s="116" t="s">
-        <v>382</v>
-      </c>
-      <c r="B53" s="116" t="s">
-        <v>1036</v>
+      <c r="A53" s="19" t="s">
+        <v>1028</v>
+      </c>
+      <c r="B53" s="19" t="s">
+        <v>1032</v>
       </c>
       <c r="C53" s="21" t="s">
-        <v>1037</v>
-      </c>
-      <c r="D53" s="121" t="s">
-        <v>1038</v>
+        <v>1033</v>
+      </c>
+      <c r="D53" s="19" t="s">
+        <v>1031</v>
       </c>
       <c r="F53" s="71" t="s">
         <v>904</v>
@@ -16081,24 +16087,41 @@
         <v>382</v>
       </c>
       <c r="B54" s="116" t="s">
+        <v>1034</v>
+      </c>
+      <c r="C54" s="21" t="s">
+        <v>1035</v>
+      </c>
+      <c r="D54" s="121" t="s">
+        <v>1036</v>
+      </c>
+      <c r="F54" s="71" t="s">
+        <v>904</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+      <c r="A55" s="116" t="s">
+        <v>382</v>
+      </c>
+      <c r="B55" s="116" t="s">
+        <v>1037</v>
+      </c>
+      <c r="C55" s="21" t="s">
+        <v>1038</v>
+      </c>
+      <c r="D55" s="121" t="s">
         <v>1039</v>
       </c>
-      <c r="C54" s="21" t="s">
-        <v>1040</v>
-      </c>
-      <c r="D54" s="121" t="s">
-        <v>1041</v>
-      </c>
-      <c r="F54" s="71" t="s">
+      <c r="F55" s="71" t="s">
         <v>904</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="8">
     <mergeCell ref="A28:E28"/>
-    <mergeCell ref="A37:E37"/>
+    <mergeCell ref="A38:E38"/>
     <mergeCell ref="A12:E12"/>
-    <mergeCell ref="A41:E41"/>
+    <mergeCell ref="A42:E42"/>
     <mergeCell ref="A2:E2"/>
     <mergeCell ref="A24:E24"/>
     <mergeCell ref="A26:E26"/>
@@ -16153,16 +16176,16 @@
         <v>243</v>
       </c>
       <c r="B2" s="136" t="s">
-        <v>1042</v>
+        <v>1040</v>
       </c>
       <c r="C2" s="137" t="s">
-        <v>1043</v>
+        <v>1041</v>
       </c>
       <c r="D2" s="136" t="s">
         <v>246</v>
       </c>
       <c r="E2" s="138" t="s">
-        <v>1044</v>
+        <v>1042</v>
       </c>
       <c r="F2" s="135"/>
     </row>
@@ -16171,34 +16194,34 @@
         <v>952</v>
       </c>
       <c r="B3" s="136" t="s">
+        <v>1043</v>
+      </c>
+      <c r="C3" s="137" t="s">
+        <v>1044</v>
+      </c>
+      <c r="D3" s="136" t="s">
         <v>1045</v>
       </c>
-      <c r="C3" s="137" t="s">
+      <c r="E3" s="138" t="s">
         <v>1046</v>
-      </c>
-      <c r="D3" s="136" t="s">
-        <v>1047</v>
-      </c>
-      <c r="E3" s="138" t="s">
-        <v>1048</v>
       </c>
       <c r="F3" s="135"/>
     </row>
     <row r="4" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A4" s="136" t="s">
+        <v>1047</v>
+      </c>
+      <c r="B4" s="136" t="s">
+        <v>1048</v>
+      </c>
+      <c r="C4" s="137" t="s">
         <v>1049</v>
       </c>
-      <c r="B4" s="136" t="s">
+      <c r="D4" s="136" t="s">
         <v>1050</v>
       </c>
-      <c r="C4" s="137" t="s">
+      <c r="E4" s="138" t="s">
         <v>1051</v>
-      </c>
-      <c r="D4" s="136" t="s">
-        <v>1052</v>
-      </c>
-      <c r="E4" s="138" t="s">
-        <v>1053</v>
       </c>
       <c r="F4" s="135"/>
     </row>
@@ -16207,11 +16230,11 @@
         <v>410</v>
       </c>
       <c r="B5" s="139" t="s">
-        <v>1054</v>
+        <v>1052</v>
       </c>
       <c r="C5" s="27"/>
       <c r="D5" s="136" t="s">
-        <v>1055</v>
+        <v>1053</v>
       </c>
       <c r="E5" s="138"/>
       <c r="F5" s="135"/>
@@ -16221,84 +16244,84 @@
         <v>413</v>
       </c>
       <c r="B6" s="139" t="s">
-        <v>1056</v>
+        <v>1054</v>
       </c>
       <c r="C6" s="27"/>
       <c r="D6" s="136" t="s">
-        <v>1057</v>
+        <v>1055</v>
       </c>
       <c r="E6" s="138"/>
       <c r="F6" s="135"/>
     </row>
     <row r="7" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A7" s="136" t="s">
-        <v>1049</v>
+        <v>1047</v>
       </c>
       <c r="B7" s="136" t="s">
+        <v>1056</v>
+      </c>
+      <c r="C7" s="137" t="s">
+        <v>1057</v>
+      </c>
+      <c r="D7" s="136" t="s">
         <v>1058</v>
       </c>
-      <c r="C7" s="137" t="s">
+      <c r="E7" s="138" t="s">
         <v>1059</v>
-      </c>
-      <c r="D7" s="136" t="s">
-        <v>1060</v>
-      </c>
-      <c r="E7" s="138" t="s">
-        <v>1061</v>
       </c>
       <c r="F7" s="135"/>
     </row>
     <row r="8" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A8" s="136" t="s">
-        <v>1049</v>
+        <v>1047</v>
       </c>
       <c r="B8" s="136" t="s">
+        <v>1060</v>
+      </c>
+      <c r="C8" s="137" t="s">
+        <v>1061</v>
+      </c>
+      <c r="D8" s="136" t="s">
         <v>1062</v>
       </c>
-      <c r="C8" s="137" t="s">
+      <c r="E8" s="138" t="s">
         <v>1063</v>
-      </c>
-      <c r="D8" s="136" t="s">
-        <v>1064</v>
-      </c>
-      <c r="E8" s="138" t="s">
-        <v>1065</v>
       </c>
       <c r="F8" s="135"/>
     </row>
     <row r="9" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A9" s="136" t="s">
-        <v>1049</v>
+        <v>1047</v>
       </c>
       <c r="B9" s="136" t="s">
+        <v>1064</v>
+      </c>
+      <c r="C9" s="137" t="s">
+        <v>1065</v>
+      </c>
+      <c r="D9" s="136" t="s">
         <v>1066</v>
       </c>
-      <c r="C9" s="137" t="s">
+      <c r="E9" s="138" t="s">
         <v>1067</v>
-      </c>
-      <c r="D9" s="136" t="s">
-        <v>1068</v>
-      </c>
-      <c r="E9" s="138" t="s">
-        <v>1069</v>
       </c>
       <c r="F9" s="135"/>
     </row>
     <row r="10" spans="1:6" ht="64" x14ac:dyDescent="0.2">
       <c r="A10" s="136" t="s">
-        <v>1049</v>
+        <v>1047</v>
       </c>
       <c r="B10" s="136" t="s">
+        <v>1068</v>
+      </c>
+      <c r="C10" s="137" t="s">
+        <v>1069</v>
+      </c>
+      <c r="D10" s="136" t="s">
         <v>1070</v>
       </c>
-      <c r="C10" s="137" t="s">
+      <c r="E10" s="138" t="s">
         <v>1071</v>
-      </c>
-      <c r="D10" s="136" t="s">
-        <v>1072</v>
-      </c>
-      <c r="E10" s="138" t="s">
-        <v>1073</v>
       </c>
       <c r="F10" s="135"/>
     </row>
@@ -16307,32 +16330,32 @@
         <v>254</v>
       </c>
       <c r="B11" s="136" t="s">
+        <v>1072</v>
+      </c>
+      <c r="C11" s="137" t="s">
+        <v>1073</v>
+      </c>
+      <c r="D11" s="136" t="s">
         <v>1074</v>
-      </c>
-      <c r="C11" s="137" t="s">
-        <v>1075</v>
-      </c>
-      <c r="D11" s="136" t="s">
-        <v>1076</v>
       </c>
       <c r="E11" s="138"/>
       <c r="F11" s="135"/>
     </row>
     <row r="12" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A12" s="136" t="s">
-        <v>1049</v>
+        <v>1047</v>
       </c>
       <c r="B12" s="136" t="s">
+        <v>1075</v>
+      </c>
+      <c r="C12" s="137" t="s">
+        <v>1076</v>
+      </c>
+      <c r="D12" s="136" t="s">
         <v>1077</v>
       </c>
-      <c r="C12" s="137" t="s">
+      <c r="E12" s="138" t="s">
         <v>1078</v>
-      </c>
-      <c r="D12" s="136" t="s">
-        <v>1079</v>
-      </c>
-      <c r="E12" s="138" t="s">
-        <v>1080</v>
       </c>
       <c r="F12" s="135"/>
     </row>
@@ -16341,11 +16364,11 @@
         <v>410</v>
       </c>
       <c r="B13" s="28" t="s">
-        <v>1081</v>
+        <v>1079</v>
       </c>
       <c r="C13" s="138"/>
       <c r="D13" s="136" t="s">
-        <v>1082</v>
+        <v>1080</v>
       </c>
       <c r="E13" s="138"/>
       <c r="F13" s="135"/>
@@ -16355,83 +16378,83 @@
         <v>413</v>
       </c>
       <c r="B14" s="28" t="s">
-        <v>1083</v>
+        <v>1081</v>
       </c>
       <c r="C14" s="138"/>
       <c r="D14" s="136" t="s">
-        <v>1057</v>
+        <v>1055</v>
       </c>
       <c r="E14" s="138"/>
       <c r="F14" s="135"/>
     </row>
     <row r="15" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A15" s="136" t="s">
-        <v>1049</v>
+        <v>1047</v>
       </c>
       <c r="B15" s="136" t="s">
+        <v>1082</v>
+      </c>
+      <c r="C15" s="137" t="s">
+        <v>1083</v>
+      </c>
+      <c r="D15" s="136" t="s">
         <v>1084</v>
       </c>
-      <c r="C15" s="137" t="s">
+      <c r="E15" s="138" t="s">
         <v>1085</v>
-      </c>
-      <c r="D15" s="136" t="s">
-        <v>1086</v>
-      </c>
-      <c r="E15" s="138" t="s">
-        <v>1087</v>
       </c>
       <c r="F15" s="135"/>
     </row>
     <row r="16" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A16" s="136" t="s">
-        <v>1049</v>
+        <v>1047</v>
       </c>
       <c r="B16" s="136" t="s">
+        <v>1086</v>
+      </c>
+      <c r="C16" s="137" t="s">
+        <v>1087</v>
+      </c>
+      <c r="D16" s="136" t="s">
         <v>1088</v>
       </c>
-      <c r="C16" s="137" t="s">
+      <c r="E16" s="138" t="s">
         <v>1089</v>
-      </c>
-      <c r="D16" s="136" t="s">
-        <v>1090</v>
-      </c>
-      <c r="E16" s="138" t="s">
-        <v>1091</v>
       </c>
       <c r="F16" s="135"/>
     </row>
     <row r="17" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A17" s="136" t="s">
-        <v>1049</v>
+        <v>1047</v>
       </c>
       <c r="B17" s="136" t="s">
+        <v>1090</v>
+      </c>
+      <c r="C17" s="137" t="s">
+        <v>1091</v>
+      </c>
+      <c r="D17" s="136" t="s">
         <v>1092</v>
       </c>
-      <c r="C17" s="137" t="s">
+      <c r="E17" s="138" t="s">
         <v>1093</v>
-      </c>
-      <c r="D17" s="136" t="s">
-        <v>1094</v>
-      </c>
-      <c r="E17" s="138" t="s">
-        <v>1095</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="144" x14ac:dyDescent="0.2">
       <c r="A18" s="136" t="s">
-        <v>1049</v>
+        <v>1047</v>
       </c>
       <c r="B18" s="136" t="s">
+        <v>1094</v>
+      </c>
+      <c r="C18" s="137" t="s">
+        <v>1095</v>
+      </c>
+      <c r="D18" s="29" t="s">
         <v>1096</v>
       </c>
-      <c r="C18" s="137" t="s">
+      <c r="E18" s="138" t="s">
         <v>1097</v>
-      </c>
-      <c r="D18" s="29" t="s">
-        <v>1098</v>
-      </c>
-      <c r="E18" s="138" t="s">
-        <v>1099</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="80" x14ac:dyDescent="0.2">
@@ -16439,11 +16462,11 @@
         <v>410</v>
       </c>
       <c r="B19" s="28" t="s">
-        <v>1100</v>
+        <v>1098</v>
       </c>
       <c r="C19" s="27"/>
       <c r="D19" s="18" t="s">
-        <v>1101</v>
+        <v>1099</v>
       </c>
       <c r="E19" s="138"/>
     </row>
@@ -16452,11 +16475,11 @@
         <v>413</v>
       </c>
       <c r="B20" s="28" t="s">
-        <v>1102</v>
+        <v>1100</v>
       </c>
       <c r="C20" s="27"/>
       <c r="D20" s="18" t="s">
-        <v>1057</v>
+        <v>1055</v>
       </c>
       <c r="E20" s="138"/>
     </row>
@@ -16465,29 +16488,29 @@
         <v>413</v>
       </c>
       <c r="B21" s="28" t="s">
-        <v>1103</v>
+        <v>1101</v>
       </c>
       <c r="C21" s="27"/>
       <c r="D21" s="18" t="s">
-        <v>1104</v>
+        <v>1102</v>
       </c>
       <c r="E21" s="138"/>
     </row>
     <row r="22" spans="1:5" ht="112" x14ac:dyDescent="0.2">
       <c r="A22" s="136" t="s">
+        <v>1103</v>
+      </c>
+      <c r="B22" s="136" t="s">
+        <v>1104</v>
+      </c>
+      <c r="C22" s="137" t="s">
         <v>1105</v>
       </c>
-      <c r="B22" s="136" t="s">
+      <c r="D22" s="136" t="s">
         <v>1106</v>
       </c>
-      <c r="C22" s="137" t="s">
+      <c r="E22" s="138" t="s">
         <v>1107</v>
-      </c>
-      <c r="D22" s="136" t="s">
-        <v>1108</v>
-      </c>
-      <c r="E22" s="138" t="s">
-        <v>1109</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="48" x14ac:dyDescent="0.2">
@@ -16495,11 +16518,11 @@
         <v>410</v>
       </c>
       <c r="B23" s="28" t="s">
-        <v>1110</v>
+        <v>1108</v>
       </c>
       <c r="C23" s="27"/>
       <c r="D23" s="136" t="s">
-        <v>1111</v>
+        <v>1109</v>
       </c>
       <c r="E23" s="138"/>
     </row>
@@ -16508,11 +16531,11 @@
         <v>413</v>
       </c>
       <c r="B24" s="28" t="s">
-        <v>1112</v>
+        <v>1110</v>
       </c>
       <c r="C24" s="27"/>
       <c r="D24" s="136" t="s">
-        <v>1113</v>
+        <v>1111</v>
       </c>
       <c r="E24" s="138"/>
     </row>
@@ -16521,11 +16544,11 @@
         <v>413</v>
       </c>
       <c r="B25" s="28" t="s">
-        <v>1114</v>
+        <v>1112</v>
       </c>
       <c r="C25" s="27"/>
       <c r="D25" s="29" t="s">
-        <v>1115</v>
+        <v>1113</v>
       </c>
       <c r="E25" s="138"/>
     </row>
@@ -16534,38 +16557,38 @@
         <v>254</v>
       </c>
       <c r="B26" s="136" t="s">
+        <v>1114</v>
+      </c>
+      <c r="C26" s="137" t="s">
+        <v>1115</v>
+      </c>
+      <c r="D26" s="136" t="s">
+        <v>1074</v>
+      </c>
+      <c r="E26" s="138" t="s">
         <v>1116</v>
-      </c>
-      <c r="C26" s="137" t="s">
-        <v>1117</v>
-      </c>
-      <c r="D26" s="136" t="s">
-        <v>1076</v>
-      </c>
-      <c r="E26" s="138" t="s">
-        <v>1118</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A27" s="136" t="s">
-        <v>1049</v>
+        <v>1047</v>
       </c>
       <c r="B27" s="136" t="s">
+        <v>1117</v>
+      </c>
+      <c r="C27" s="137" t="s">
+        <v>1118</v>
+      </c>
+      <c r="D27" s="136" t="s">
         <v>1119</v>
       </c>
-      <c r="C27" s="137" t="s">
+      <c r="E27" s="138" t="s">
         <v>1120</v>
-      </c>
-      <c r="D27" s="136" t="s">
-        <v>1121</v>
-      </c>
-      <c r="E27" s="138" t="s">
-        <v>1122</v>
       </c>
     </row>
     <row r="28" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A28" s="186" t="s">
-        <v>1123</v>
+        <v>1121</v>
       </c>
       <c r="B28" s="187"/>
       <c r="C28" s="187"/>
@@ -16577,33 +16600,33 @@
         <v>243</v>
       </c>
       <c r="B29" s="141" t="s">
+        <v>1122</v>
+      </c>
+      <c r="C29" s="142" t="s">
+        <v>1123</v>
+      </c>
+      <c r="D29" s="5" t="s">
         <v>1124</v>
       </c>
-      <c r="C29" s="142" t="s">
+      <c r="E29" s="143" t="s">
         <v>1125</v>
-      </c>
-      <c r="D29" s="5" t="s">
-        <v>1126</v>
-      </c>
-      <c r="E29" s="143" t="s">
-        <v>1127</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="64" x14ac:dyDescent="0.2">
       <c r="A30" s="144" t="s">
+        <v>1126</v>
+      </c>
+      <c r="B30" s="144" t="s">
+        <v>1127</v>
+      </c>
+      <c r="C30" s="145" t="s">
         <v>1128</v>
       </c>
-      <c r="B30" s="144" t="s">
+      <c r="D30" s="144" t="s">
         <v>1129</v>
       </c>
-      <c r="C30" s="145" t="s">
+      <c r="E30" s="146" t="s">
         <v>1130</v>
-      </c>
-      <c r="D30" s="144" t="s">
-        <v>1131</v>
-      </c>
-      <c r="E30" s="146" t="s">
-        <v>1132</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="48" x14ac:dyDescent="0.2">
@@ -16611,11 +16634,11 @@
         <v>410</v>
       </c>
       <c r="B31" s="28" t="s">
-        <v>1133</v>
+        <v>1131</v>
       </c>
       <c r="C31" s="27"/>
       <c r="D31" s="18" t="s">
-        <v>1001</v>
+        <v>999</v>
       </c>
       <c r="E31" s="146"/>
     </row>
@@ -16624,17 +16647,17 @@
         <v>413</v>
       </c>
       <c r="B32" s="28" t="s">
-        <v>1134</v>
+        <v>1132</v>
       </c>
       <c r="C32" s="27"/>
       <c r="D32" s="18" t="s">
-        <v>994</v>
+        <v>992</v>
       </c>
       <c r="E32" s="146"/>
     </row>
     <row r="33" spans="1:6" s="13" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A33" s="189" t="s">
-        <v>1135</v>
+        <v>1133</v>
       </c>
       <c r="B33" s="190"/>
       <c r="C33" s="191"/>
@@ -16646,121 +16669,121 @@
         <v>243</v>
       </c>
       <c r="B34" s="147" t="s">
+        <v>1134</v>
+      </c>
+      <c r="C34" s="145" t="s">
+        <v>1135</v>
+      </c>
+      <c r="D34" s="50" t="s">
         <v>1136</v>
       </c>
-      <c r="C34" s="145" t="s">
+      <c r="E34" s="146" t="s">
         <v>1137</v>
-      </c>
-      <c r="D34" s="50" t="s">
-        <v>1138</v>
-      </c>
-      <c r="E34" s="146" t="s">
-        <v>1139</v>
       </c>
       <c r="F34" s="135"/>
     </row>
     <row r="35" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A35" s="144" t="s">
-        <v>1049</v>
+        <v>1047</v>
       </c>
       <c r="B35" s="148" t="s">
+        <v>1138</v>
+      </c>
+      <c r="C35" s="145" t="s">
+        <v>1139</v>
+      </c>
+      <c r="D35" s="149" t="s">
         <v>1140</v>
       </c>
-      <c r="C35" s="145" t="s">
+      <c r="E35" s="146" t="s">
         <v>1141</v>
-      </c>
-      <c r="D35" s="149" t="s">
-        <v>1142</v>
-      </c>
-      <c r="E35" s="146" t="s">
-        <v>1143</v>
       </c>
       <c r="F35" s="135"/>
     </row>
     <row r="36" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A36" s="144" t="s">
-        <v>1049</v>
+        <v>1047</v>
       </c>
       <c r="B36" s="148" t="s">
+        <v>1142</v>
+      </c>
+      <c r="C36" s="145" t="s">
+        <v>1143</v>
+      </c>
+      <c r="D36" s="149" t="s">
+        <v>1140</v>
+      </c>
+      <c r="E36" s="146" t="s">
         <v>1144</v>
-      </c>
-      <c r="C36" s="145" t="s">
-        <v>1145</v>
-      </c>
-      <c r="D36" s="149" t="s">
-        <v>1142</v>
-      </c>
-      <c r="E36" s="146" t="s">
-        <v>1146</v>
       </c>
       <c r="F36" s="135"/>
     </row>
     <row r="37" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A37" s="144" t="s">
-        <v>1049</v>
+        <v>1047</v>
       </c>
       <c r="B37" s="148" t="s">
+        <v>1145</v>
+      </c>
+      <c r="C37" s="49" t="s">
+        <v>1146</v>
+      </c>
+      <c r="D37" s="149" t="s">
+        <v>1140</v>
+      </c>
+      <c r="E37" s="146" t="s">
         <v>1147</v>
-      </c>
-      <c r="C37" s="49" t="s">
-        <v>1148</v>
-      </c>
-      <c r="D37" s="149" t="s">
-        <v>1142</v>
-      </c>
-      <c r="E37" s="146" t="s">
-        <v>1149</v>
       </c>
       <c r="F37" s="135"/>
     </row>
     <row r="38" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A38" s="144" t="s">
-        <v>1049</v>
+        <v>1047</v>
       </c>
       <c r="B38" s="148" t="s">
+        <v>1148</v>
+      </c>
+      <c r="C38" s="49" t="s">
+        <v>1149</v>
+      </c>
+      <c r="D38" s="149" t="s">
+        <v>1140</v>
+      </c>
+      <c r="E38" s="146" t="s">
         <v>1150</v>
-      </c>
-      <c r="C38" s="49" t="s">
-        <v>1151</v>
-      </c>
-      <c r="D38" s="149" t="s">
-        <v>1142</v>
-      </c>
-      <c r="E38" s="146" t="s">
-        <v>1152</v>
       </c>
       <c r="F38" s="135"/>
     </row>
     <row r="39" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A39" s="144" t="s">
-        <v>1049</v>
+        <v>1047</v>
       </c>
       <c r="B39" s="148" t="s">
+        <v>1151</v>
+      </c>
+      <c r="C39" s="49" t="s">
+        <v>1152</v>
+      </c>
+      <c r="D39" s="149" t="s">
+        <v>1140</v>
+      </c>
+      <c r="E39" s="146" t="s">
         <v>1153</v>
-      </c>
-      <c r="C39" s="49" t="s">
-        <v>1154</v>
-      </c>
-      <c r="D39" s="149" t="s">
-        <v>1142</v>
-      </c>
-      <c r="E39" s="146" t="s">
-        <v>1155</v>
       </c>
       <c r="F39" s="135"/>
     </row>
     <row r="40" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A40" s="144" t="s">
-        <v>1049</v>
+        <v>1047</v>
       </c>
       <c r="B40" s="148" t="s">
-        <v>1156</v>
+        <v>1154</v>
       </c>
       <c r="C40" s="49" t="s">
         <v>93</v>
       </c>
       <c r="D40" s="149" t="s">
-        <v>1142</v>
+        <v>1140</v>
       </c>
       <c r="E40" s="146" t="s">
         <v>95</v>
@@ -16772,11 +16795,11 @@
         <v>410</v>
       </c>
       <c r="B41" s="28" t="s">
-        <v>1157</v>
+        <v>1155</v>
       </c>
       <c r="C41" s="51"/>
       <c r="D41" s="18" t="s">
-        <v>1001</v>
+        <v>999</v>
       </c>
       <c r="E41" s="146"/>
       <c r="F41" s="135"/>
@@ -16786,11 +16809,11 @@
         <v>413</v>
       </c>
       <c r="B42" s="28" t="s">
-        <v>1158</v>
+        <v>1156</v>
       </c>
       <c r="C42" s="27"/>
       <c r="D42" s="18" t="s">
-        <v>994</v>
+        <v>992</v>
       </c>
       <c r="E42" s="146"/>
       <c r="F42" s="135"/>
@@ -16800,16 +16823,16 @@
         <v>243</v>
       </c>
       <c r="B43" s="136" t="s">
+        <v>1157</v>
+      </c>
+      <c r="C43" s="62" t="s">
+        <v>1406</v>
+      </c>
+      <c r="D43" s="5" t="s">
+        <v>1158</v>
+      </c>
+      <c r="E43" s="146" t="s">
         <v>1159</v>
-      </c>
-      <c r="C43" s="62" t="s">
-        <v>1408</v>
-      </c>
-      <c r="D43" s="5" t="s">
-        <v>1160</v>
-      </c>
-      <c r="E43" s="146" t="s">
-        <v>1161</v>
       </c>
       <c r="F43" s="135"/>
     </row>
@@ -16818,11 +16841,11 @@
         <v>410</v>
       </c>
       <c r="B44" s="28" t="s">
-        <v>1162</v>
+        <v>1160</v>
       </c>
       <c r="C44" s="27"/>
       <c r="D44" s="18" t="s">
-        <v>1001</v>
+        <v>999</v>
       </c>
       <c r="E44" s="146"/>
       <c r="F44" s="135"/>
@@ -16832,18 +16855,18 @@
         <v>413</v>
       </c>
       <c r="B45" s="28" t="s">
-        <v>1163</v>
+        <v>1161</v>
       </c>
       <c r="C45" s="27"/>
       <c r="D45" s="18" t="s">
-        <v>994</v>
+        <v>992</v>
       </c>
       <c r="E45" s="146"/>
       <c r="F45" s="135"/>
     </row>
     <row r="46" spans="1:6" s="13" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="186" t="s">
-        <v>1164</v>
+        <v>1162</v>
       </c>
       <c r="B46" s="187"/>
       <c r="C46" s="187"/>
@@ -16855,33 +16878,33 @@
         <v>243</v>
       </c>
       <c r="B47" s="144" t="s">
-        <v>1165</v>
+        <v>1163</v>
       </c>
       <c r="C47" s="62" t="s">
         <v>858</v>
       </c>
       <c r="D47" s="116" t="s">
-        <v>1166</v>
+        <v>1164</v>
       </c>
       <c r="E47" s="63" t="s">
         <v>860</v>
       </c>
       <c r="F47" s="38" t="s">
-        <v>1167</v>
+        <v>1165</v>
       </c>
     </row>
     <row r="48" spans="1:6" s="30" customFormat="1" ht="64" x14ac:dyDescent="0.2">
       <c r="A48" s="144" t="s">
-        <v>1168</v>
+        <v>1166</v>
       </c>
       <c r="B48" s="144" t="s">
-        <v>1169</v>
+        <v>1167</v>
       </c>
       <c r="C48" s="62" t="s">
         <v>922</v>
       </c>
       <c r="D48" s="116" t="s">
-        <v>1170</v>
+        <v>1168</v>
       </c>
       <c r="E48" s="63" t="s">
         <v>923</v>
@@ -16889,19 +16912,19 @@
     </row>
     <row r="49" spans="1:6" s="30" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A49" s="144" t="s">
-        <v>1128</v>
+        <v>1126</v>
       </c>
       <c r="B49" s="144" t="s">
-        <v>1171</v>
+        <v>1169</v>
       </c>
       <c r="C49" s="62" t="s">
-        <v>1421</v>
+        <v>1419</v>
       </c>
       <c r="D49" s="116" t="s">
-        <v>1010</v>
+        <v>1008</v>
       </c>
       <c r="E49" s="63" t="s">
-        <v>1422</v>
+        <v>1420</v>
       </c>
     </row>
     <row r="50" spans="1:6" s="30" customFormat="1" ht="48" x14ac:dyDescent="0.2">
@@ -16909,19 +16932,19 @@
         <v>382</v>
       </c>
       <c r="B50" s="136" t="s">
+        <v>1170</v>
+      </c>
+      <c r="C50" s="145" t="s">
+        <v>1171</v>
+      </c>
+      <c r="D50" s="121" t="s">
         <v>1172</v>
       </c>
-      <c r="C50" s="145" t="s">
+      <c r="E50" s="63" t="s">
+        <v>1051</v>
+      </c>
+      <c r="F50" s="73" t="s">
         <v>1173</v>
-      </c>
-      <c r="D50" s="121" t="s">
-        <v>1174</v>
-      </c>
-      <c r="E50" s="63" t="s">
-        <v>1053</v>
-      </c>
-      <c r="F50" s="73" t="s">
-        <v>1175</v>
       </c>
     </row>
     <row r="51" spans="1:6" s="30" customFormat="1" ht="48" x14ac:dyDescent="0.2">
@@ -16929,16 +16952,16 @@
         <v>382</v>
       </c>
       <c r="B51" s="136" t="s">
+        <v>1174</v>
+      </c>
+      <c r="C51" s="145" t="s">
+        <v>1175</v>
+      </c>
+      <c r="D51" s="121" t="s">
         <v>1176</v>
       </c>
-      <c r="C51" s="145" t="s">
+      <c r="E51" s="63" t="s">
         <v>1177</v>
-      </c>
-      <c r="D51" s="121" t="s">
-        <v>1178</v>
-      </c>
-      <c r="E51" s="63" t="s">
-        <v>1179</v>
       </c>
     </row>
     <row r="52" spans="1:6" s="30" customFormat="1" ht="64" x14ac:dyDescent="0.2">
@@ -16946,16 +16969,16 @@
         <v>382</v>
       </c>
       <c r="B52" s="136" t="s">
+        <v>1178</v>
+      </c>
+      <c r="C52" s="145" t="s">
+        <v>1179</v>
+      </c>
+      <c r="D52" s="121" t="s">
         <v>1180</v>
       </c>
-      <c r="C52" s="145" t="s">
+      <c r="E52" s="63" t="s">
         <v>1181</v>
-      </c>
-      <c r="D52" s="121" t="s">
-        <v>1182</v>
-      </c>
-      <c r="E52" s="63" t="s">
-        <v>1183</v>
       </c>
     </row>
     <row r="53" spans="1:6" s="30" customFormat="1" ht="64" x14ac:dyDescent="0.2">
@@ -16963,16 +16986,16 @@
         <v>382</v>
       </c>
       <c r="B53" s="136" t="s">
+        <v>1182</v>
+      </c>
+      <c r="C53" s="145" t="s">
+        <v>1183</v>
+      </c>
+      <c r="D53" s="121" t="s">
         <v>1184</v>
       </c>
-      <c r="C53" s="145" t="s">
+      <c r="E53" s="63" t="s">
         <v>1185</v>
-      </c>
-      <c r="D53" s="121" t="s">
-        <v>1186</v>
-      </c>
-      <c r="E53" s="63" t="s">
-        <v>1187</v>
       </c>
     </row>
     <row r="54" spans="1:6" s="30" customFormat="1" ht="48" x14ac:dyDescent="0.2">
@@ -16980,16 +17003,16 @@
         <v>382</v>
       </c>
       <c r="B54" s="136" t="s">
+        <v>1186</v>
+      </c>
+      <c r="C54" s="145" t="s">
+        <v>1187</v>
+      </c>
+      <c r="D54" s="121" t="s">
         <v>1188</v>
       </c>
-      <c r="C54" s="145" t="s">
+      <c r="E54" s="63" t="s">
         <v>1189</v>
-      </c>
-      <c r="D54" s="121" t="s">
-        <v>1190</v>
-      </c>
-      <c r="E54" s="63" t="s">
-        <v>1191</v>
       </c>
     </row>
     <row r="55" spans="1:6" s="30" customFormat="1" ht="32" x14ac:dyDescent="0.2">
@@ -16997,19 +17020,19 @@
         <v>382</v>
       </c>
       <c r="B55" s="136" t="s">
+        <v>1190</v>
+      </c>
+      <c r="C55" s="145" t="s">
+        <v>1191</v>
+      </c>
+      <c r="D55" s="121" t="s">
         <v>1192</v>
       </c>
-      <c r="C55" s="145" t="s">
+      <c r="E55" s="63" t="s">
+        <v>1078</v>
+      </c>
+      <c r="F55" s="73" t="s">
         <v>1193</v>
-      </c>
-      <c r="D55" s="121" t="s">
-        <v>1194</v>
-      </c>
-      <c r="E55" s="63" t="s">
-        <v>1080</v>
-      </c>
-      <c r="F55" s="73" t="s">
-        <v>1195</v>
       </c>
     </row>
     <row r="56" spans="1:6" s="30" customFormat="1" ht="48" x14ac:dyDescent="0.2">
@@ -17017,19 +17040,19 @@
         <v>382</v>
       </c>
       <c r="B56" s="136" t="s">
+        <v>1194</v>
+      </c>
+      <c r="C56" s="145" t="s">
+        <v>1195</v>
+      </c>
+      <c r="D56" s="121" t="s">
         <v>1196</v>
       </c>
-      <c r="C56" s="145" t="s">
+      <c r="E56" s="63" t="s">
         <v>1197</v>
       </c>
-      <c r="D56" s="121" t="s">
+      <c r="F56" s="73" t="s">
         <v>1198</v>
-      </c>
-      <c r="E56" s="63" t="s">
-        <v>1199</v>
-      </c>
-      <c r="F56" s="73" t="s">
-        <v>1200</v>
       </c>
     </row>
     <row r="57" spans="1:6" s="30" customFormat="1" ht="48" x14ac:dyDescent="0.2">
@@ -17037,19 +17060,19 @@
         <v>382</v>
       </c>
       <c r="B57" s="136" t="s">
+        <v>1199</v>
+      </c>
+      <c r="C57" s="145" t="s">
+        <v>1200</v>
+      </c>
+      <c r="D57" s="121" t="s">
         <v>1201</v>
       </c>
-      <c r="C57" s="145" t="s">
+      <c r="E57" s="63" t="s">
         <v>1202</v>
       </c>
-      <c r="D57" s="121" t="s">
+      <c r="F57" s="73" t="s">
         <v>1203</v>
-      </c>
-      <c r="E57" s="63" t="s">
-        <v>1204</v>
-      </c>
-      <c r="F57" s="73" t="s">
-        <v>1205</v>
       </c>
     </row>
     <row r="58" spans="1:6" s="30" customFormat="1" ht="32" x14ac:dyDescent="0.2">
@@ -17057,19 +17080,19 @@
         <v>382</v>
       </c>
       <c r="B58" s="136" t="s">
+        <v>1204</v>
+      </c>
+      <c r="C58" s="145" t="s">
+        <v>1205</v>
+      </c>
+      <c r="D58" s="121" t="s">
         <v>1206</v>
       </c>
-      <c r="C58" s="145" t="s">
+      <c r="E58" s="63" t="s">
         <v>1207</v>
       </c>
-      <c r="D58" s="121" t="s">
+      <c r="F58" s="73" t="s">
         <v>1208</v>
-      </c>
-      <c r="E58" s="63" t="s">
-        <v>1209</v>
-      </c>
-      <c r="F58" s="73" t="s">
-        <v>1210</v>
       </c>
     </row>
     <row r="59" spans="1:6" s="30" customFormat="1" ht="48" x14ac:dyDescent="0.2">
@@ -17077,16 +17100,16 @@
         <v>382</v>
       </c>
       <c r="B59" s="136" t="s">
+        <v>1209</v>
+      </c>
+      <c r="C59" s="145" t="s">
+        <v>1210</v>
+      </c>
+      <c r="D59" s="121" t="s">
         <v>1211</v>
       </c>
-      <c r="C59" s="145" t="s">
+      <c r="E59" s="63" t="s">
         <v>1212</v>
-      </c>
-      <c r="D59" s="121" t="s">
-        <v>1213</v>
-      </c>
-      <c r="E59" s="63" t="s">
-        <v>1214</v>
       </c>
     </row>
     <row r="60" spans="1:6" s="30" customFormat="1" ht="48" x14ac:dyDescent="0.2">
@@ -17094,16 +17117,16 @@
         <v>382</v>
       </c>
       <c r="B60" s="136" t="s">
+        <v>1213</v>
+      </c>
+      <c r="C60" s="145" t="s">
+        <v>1214</v>
+      </c>
+      <c r="D60" s="121" t="s">
         <v>1215</v>
       </c>
-      <c r="C60" s="145" t="s">
+      <c r="E60" s="63" t="s">
         <v>1216</v>
-      </c>
-      <c r="D60" s="121" t="s">
-        <v>1217</v>
-      </c>
-      <c r="E60" s="63" t="s">
-        <v>1218</v>
       </c>
     </row>
     <row r="61" spans="1:6" s="30" customFormat="1" ht="48" x14ac:dyDescent="0.2">
@@ -17111,16 +17134,16 @@
         <v>382</v>
       </c>
       <c r="B61" s="18" t="s">
+        <v>1217</v>
+      </c>
+      <c r="C61" s="145" t="s">
+        <v>1218</v>
+      </c>
+      <c r="D61" s="121" t="s">
         <v>1219</v>
       </c>
-      <c r="C61" s="145" t="s">
+      <c r="E61" s="63" t="s">
         <v>1220</v>
-      </c>
-      <c r="D61" s="121" t="s">
-        <v>1221</v>
-      </c>
-      <c r="E61" s="63" t="s">
-        <v>1222</v>
       </c>
     </row>
     <row r="62" spans="1:6" s="30" customFormat="1" ht="48" x14ac:dyDescent="0.2">
@@ -17128,16 +17151,16 @@
         <v>382</v>
       </c>
       <c r="B62" s="136" t="s">
+        <v>1221</v>
+      </c>
+      <c r="C62" s="145" t="s">
+        <v>1222</v>
+      </c>
+      <c r="D62" s="121" t="s">
         <v>1223</v>
       </c>
-      <c r="C62" s="145" t="s">
+      <c r="E62" s="79" t="s">
         <v>1224</v>
-      </c>
-      <c r="D62" s="121" t="s">
-        <v>1225</v>
-      </c>
-      <c r="E62" s="79" t="s">
-        <v>1226</v>
       </c>
     </row>
     <row r="63" spans="1:6" ht="16" x14ac:dyDescent="0.2">
@@ -17145,14 +17168,14 @@
         <v>732</v>
       </c>
       <c r="B63" s="144" t="s">
-        <v>1227</v>
+        <v>1225</v>
       </c>
       <c r="C63" s="145" t="s">
-        <v>1228</v>
+        <v>1226</v>
       </c>
       <c r="D63" s="148"/>
       <c r="E63" s="78" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="F63" s="135"/>
     </row>
@@ -17161,14 +17184,14 @@
         <v>732</v>
       </c>
       <c r="B64" s="144" t="s">
-        <v>1230</v>
+        <v>1228</v>
       </c>
       <c r="C64" s="145" t="s">
-        <v>1154</v>
+        <v>1152</v>
       </c>
       <c r="D64" s="148"/>
       <c r="E64" s="78" t="s">
-        <v>1155</v>
+        <v>1153</v>
       </c>
       <c r="F64" s="135"/>
     </row>
@@ -17177,14 +17200,14 @@
         <v>732</v>
       </c>
       <c r="B65" s="136" t="s">
-        <v>1231</v>
+        <v>1229</v>
       </c>
       <c r="C65" s="145" t="s">
-        <v>1141</v>
+        <v>1139</v>
       </c>
       <c r="D65" s="148"/>
       <c r="E65" s="78" t="s">
-        <v>1143</v>
+        <v>1141</v>
       </c>
       <c r="F65" s="135"/>
     </row>
@@ -17264,6 +17287,47 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Readyforteam_x003f_ xmlns="565e1b1d-057e-4d85-b896-01a5881d8a45">false</Readyforteam_x003f_>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <SharedWithUsers xmlns="bf601f31-63a1-4825-9216-91d773c5ef9c">
+      <UserInfo>
+        <DisplayName>Erika Osti</DisplayName>
+        <AccountId>534</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Penny Johnson</DisplayName>
+        <AccountId>489</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Ben Childs</DisplayName>
+        <AccountId>643</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Thomas Leeds</DisplayName>
+        <AccountId>459</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Kasmyn Chen</DisplayName>
+        <AccountId>532</AccountId>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="565e1b1d-057e-4d85-b896-01a5881d8a45">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="2799d30d-6731-4efe-ac9b-c4895a8828d9" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010096D84A54A9CD274097F17166F184737D" ma:contentTypeVersion="21" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="2fd95a4cfdf4f2f51219070f5dff16a8">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="565e1b1d-057e-4d85-b896-01a5881d8a45" xmlns:ns3="bf601f31-63a1-4825-9216-91d773c5ef9c" xmlns:ns4="2799d30d-6731-4efe-ac9b-c4895a8828d9" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f7499f6f4dc8ad2a533df04863f63fa7" ns1:_="" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -17540,47 +17604,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Readyforteam_x003f_ xmlns="565e1b1d-057e-4d85-b896-01a5881d8a45">false</Readyforteam_x003f_>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <SharedWithUsers xmlns="bf601f31-63a1-4825-9216-91d773c5ef9c">
-      <UserInfo>
-        <DisplayName>Erika Osti</DisplayName>
-        <AccountId>534</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Penny Johnson</DisplayName>
-        <AccountId>489</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Ben Childs</DisplayName>
-        <AccountId>643</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Thomas Leeds</DisplayName>
-        <AccountId>459</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Kasmyn Chen</DisplayName>
-        <AccountId>532</AccountId>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="565e1b1d-057e-4d85-b896-01a5881d8a45">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="2799d30d-6731-4efe-ac9b-c4895a8828d9" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8D7CE8C7-18DC-484F-8376-ED09F13D44C8}">
   <ds:schemaRefs>
@@ -17590,6 +17613,19 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{017ACE96-8143-486E-8436-7787F6B96F4A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="565e1b1d-057e-4d85-b896-01a5881d8a45"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="bf601f31-63a1-4825-9216-91d773c5ef9c"/>
+    <ds:schemaRef ds:uri="2799d30d-6731-4efe-ac9b-c4895a8828d9"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EAFDB110-4046-4E72-A1EF-1908ABEC3151}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -17608,17 +17644,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{017ACE96-8143-486E-8436-7787F6B96F4A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="565e1b1d-057e-4d85-b896-01a5881d8a45"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="bf601f31-63a1-4825-9216-91d773c5ef9c"/>
-    <ds:schemaRef ds:uri="2799d30d-6731-4efe-ac9b-c4895a8828d9"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
[MCCDB-862] Content amend - Ethnic group of the deceased
</commit_message>
<xml_diff>
--- a/app/data/MCCD-localisation.xlsx
+++ b/app/data/MCCD-localisation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/JALAT/GIT/medical-certificate-of-cause-of-death/app/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F79C97E6-962A-D44F-AF01-A47279EECD42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D96718BD-0164-9B41-9958-BEA6AF86793A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="14220" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -69,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2139" uniqueCount="1432">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2139" uniqueCount="1436">
   <si>
     <r>
       <rPr>
@@ -5674,7 +5674,19 @@
     <t>Rhaid i chi roi manylion yn Gymraeg a Saesneg, neu yn Saesneg yn unig.</t>
   </si>
   <si>
-    <t>021</t>
+    <t>Not known</t>
+  </si>
+  <si>
+    <t>Ddim yn hysbys</t>
+  </si>
+  <si>
+    <t>Select the ethnicity of the deceased person as it is recorded on the patient record. If there is no match with the list, or no ethnicity is recorded on the patient record, select 'not known'.</t>
+  </si>
+  <si>
+    <t>Dewiswch ethnigrwydd yr ymadawedig gan ei fod wedi'i gofnodi ar y cofnod cleifion. Os nad oes unrhyw gyd-fynd â'r rhestr, neu os nad oes unrhyw ethnigrwydd yn cael ei gofnodi ar y cofnod claf, dewiswch 'ddim yn hysbys'.</t>
+  </si>
+  <si>
+    <t>022</t>
   </si>
 </sst>
 </file>
@@ -6627,6 +6639,24 @@
     <xf numFmtId="0" fontId="13" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -6634,24 +6664,6 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -8664,7 +8676,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G3" sqref="G3"/>
+      <selection pane="bottomLeft" activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -8704,13 +8716,13 @@
         <v>7</v>
       </c>
       <c r="C2" s="100" t="s">
-        <v>1431</v>
+        <v>1435</v>
       </c>
       <c r="D2" s="98" t="s">
         <v>8</v>
       </c>
       <c r="E2" s="99" t="s">
-        <v>1431</v>
+        <v>1435</v>
       </c>
       <c r="F2" s="98"/>
     </row>
@@ -10846,8 +10858,8 @@
   <dimension ref="A1:F345"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A223" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F228" sqref="F228"/>
+      <pane ySplit="1" topLeftCell="A83" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D84" sqref="D84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -10882,13 +10894,13 @@
       </c>
     </row>
     <row r="2" spans="1:6" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="165" t="s">
+      <c r="A2" s="162" t="s">
         <v>367</v>
       </c>
-      <c r="B2" s="166"/>
-      <c r="C2" s="166"/>
-      <c r="D2" s="166"/>
-      <c r="E2" s="167"/>
+      <c r="B2" s="163"/>
+      <c r="C2" s="163"/>
+      <c r="D2" s="163"/>
+      <c r="E2" s="164"/>
       <c r="F2" s="33"/>
     </row>
     <row r="3" spans="1:6" ht="48" x14ac:dyDescent="0.2">
@@ -11016,13 +11028,13 @@
       <c r="F9" s="119"/>
     </row>
     <row r="10" spans="1:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="168" t="s">
+      <c r="A10" s="165" t="s">
         <v>396</v>
       </c>
-      <c r="B10" s="169"/>
-      <c r="C10" s="169"/>
-      <c r="D10" s="169"/>
-      <c r="E10" s="170"/>
+      <c r="B10" s="166"/>
+      <c r="C10" s="166"/>
+      <c r="D10" s="166"/>
+      <c r="E10" s="167"/>
       <c r="F10" s="119"/>
     </row>
     <row r="11" spans="1:6" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -12141,11 +12153,11 @@
         <v>572</v>
       </c>
       <c r="C84" s="117" t="s">
-        <v>573</v>
+        <v>1433</v>
       </c>
       <c r="D84" s="116"/>
       <c r="E84" s="120" t="s">
-        <v>574</v>
+        <v>1434</v>
       </c>
       <c r="F84" s="119" t="s">
         <v>575</v>
@@ -12255,11 +12267,11 @@
         <v>593</v>
       </c>
       <c r="C91" s="117" t="s">
-        <v>93</v>
+        <v>1431</v>
       </c>
       <c r="D91" s="116"/>
       <c r="E91" s="120" t="s">
-        <v>95</v>
+        <v>1432</v>
       </c>
       <c r="F91" s="119"/>
     </row>
@@ -13356,13 +13368,13 @@
       <c r="F164" s="119"/>
     </row>
     <row r="165" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A165" s="162" t="s">
+      <c r="A165" s="168" t="s">
         <v>765</v>
       </c>
-      <c r="B165" s="163"/>
-      <c r="C165" s="163"/>
-      <c r="D165" s="163"/>
-      <c r="E165" s="164"/>
+      <c r="B165" s="169"/>
+      <c r="C165" s="169"/>
+      <c r="D165" s="169"/>
+      <c r="E165" s="170"/>
       <c r="F165" s="129" t="s">
         <v>766</v>
       </c>
@@ -15265,18 +15277,6 @@
     </row>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="A225:E225"/>
-    <mergeCell ref="A186:E186"/>
-    <mergeCell ref="A190:E190"/>
-    <mergeCell ref="A197:E197"/>
-    <mergeCell ref="A208:E208"/>
-    <mergeCell ref="A214:E214"/>
-    <mergeCell ref="A58:E58"/>
-    <mergeCell ref="A2:E2"/>
-    <mergeCell ref="A10:E10"/>
-    <mergeCell ref="A14:E14"/>
-    <mergeCell ref="A24:E24"/>
-    <mergeCell ref="A43:E43"/>
     <mergeCell ref="A174:E174"/>
     <mergeCell ref="A157:E157"/>
     <mergeCell ref="A63:E63"/>
@@ -15287,6 +15287,18 @@
     <mergeCell ref="A146:E146"/>
     <mergeCell ref="A92:E92"/>
     <mergeCell ref="A165:E165"/>
+    <mergeCell ref="A58:E58"/>
+    <mergeCell ref="A2:E2"/>
+    <mergeCell ref="A10:E10"/>
+    <mergeCell ref="A14:E14"/>
+    <mergeCell ref="A24:E24"/>
+    <mergeCell ref="A43:E43"/>
+    <mergeCell ref="A225:E225"/>
+    <mergeCell ref="A186:E186"/>
+    <mergeCell ref="A190:E190"/>
+    <mergeCell ref="A197:E197"/>
+    <mergeCell ref="A208:E208"/>
+    <mergeCell ref="A214:E214"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -17287,47 +17299,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Readyforteam_x003f_ xmlns="565e1b1d-057e-4d85-b896-01a5881d8a45">false</Readyforteam_x003f_>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <SharedWithUsers xmlns="bf601f31-63a1-4825-9216-91d773c5ef9c">
-      <UserInfo>
-        <DisplayName>Erika Osti</DisplayName>
-        <AccountId>534</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Penny Johnson</DisplayName>
-        <AccountId>489</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Ben Childs</DisplayName>
-        <AccountId>643</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Thomas Leeds</DisplayName>
-        <AccountId>459</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Kasmyn Chen</DisplayName>
-        <AccountId>532</AccountId>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="565e1b1d-057e-4d85-b896-01a5881d8a45">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="2799d30d-6731-4efe-ac9b-c4895a8828d9" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010096D84A54A9CD274097F17166F184737D" ma:contentTypeVersion="21" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="2fd95a4cfdf4f2f51219070f5dff16a8">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="565e1b1d-057e-4d85-b896-01a5881d8a45" xmlns:ns3="bf601f31-63a1-4825-9216-91d773c5ef9c" xmlns:ns4="2799d30d-6731-4efe-ac9b-c4895a8828d9" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f7499f6f4dc8ad2a533df04863f63fa7" ns1:_="" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -17604,6 +17575,47 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Readyforteam_x003f_ xmlns="565e1b1d-057e-4d85-b896-01a5881d8a45">false</Readyforteam_x003f_>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <SharedWithUsers xmlns="bf601f31-63a1-4825-9216-91d773c5ef9c">
+      <UserInfo>
+        <DisplayName>Erika Osti</DisplayName>
+        <AccountId>534</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Penny Johnson</DisplayName>
+        <AccountId>489</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Ben Childs</DisplayName>
+        <AccountId>643</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Thomas Leeds</DisplayName>
+        <AccountId>459</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Kasmyn Chen</DisplayName>
+        <AccountId>532</AccountId>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="565e1b1d-057e-4d85-b896-01a5881d8a45">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="2799d30d-6731-4efe-ac9b-c4895a8828d9" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8D7CE8C7-18DC-484F-8376-ED09F13D44C8}">
   <ds:schemaRefs>
@@ -17613,19 +17625,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{017ACE96-8143-486E-8436-7787F6B96F4A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="565e1b1d-057e-4d85-b896-01a5881d8a45"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="bf601f31-63a1-4825-9216-91d773c5ef9c"/>
-    <ds:schemaRef ds:uri="2799d30d-6731-4efe-ac9b-c4895a8828d9"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EAFDB110-4046-4E72-A1EF-1908ABEC3151}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -17644,4 +17643,17 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{017ACE96-8143-486E-8436-7787F6B96F4A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="565e1b1d-057e-4d85-b896-01a5881d8a45"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="bf601f31-63a1-4825-9216-91d773c5ef9c"/>
+    <ds:schemaRef ds:uri="2799d30d-6731-4efe-ac9b-c4895a8828d9"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
[MCCDB-877] Content amend - The Cause of death page (over 28 days) - Fix for v11bi.
</commit_message>
<xml_diff>
--- a/app/data/MCCD-localisation.xlsx
+++ b/app/data/MCCD-localisation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/JALAT/GIT/medical-certificate-of-cause-of-death/app/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D96718BD-0164-9B41-9958-BEA6AF86793A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A7232F7-6A3F-1947-A2BB-E3D94CF2FDEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="14220" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="14220" firstSheet="3" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Using this document" sheetId="8" r:id="rId1"/>
@@ -69,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2139" uniqueCount="1436">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2148" uniqueCount="1444">
   <si>
     <r>
       <rPr>
@@ -4525,9 +4525,6 @@
     <t>codO281aMainDisease</t>
   </si>
   <si>
-    <t>1(a) disease or condition directly leading to death</t>
-  </si>
-  <si>
     <t>Mandatory field - Captures disease or condition directly leading to death</t>
   </si>
   <si>
@@ -4546,9 +4543,6 @@
     <t>codO281bDiseaseLeadingTo1a</t>
   </si>
   <si>
-    <t>1(b) other disease or condition leading to 1(a) (optional)</t>
-  </si>
-  <si>
     <t>Optional field - Captures disease or condition leading to 1a</t>
   </si>
   <si>
@@ -4558,9 +4552,6 @@
     <t>codO281cDiseaseLeadingTo1b</t>
   </si>
   <si>
-    <t>1(c) other disease or condition leading to 1(b) (optional)</t>
-  </si>
-  <si>
     <t>Optional field - Captures disease or condition leading to 1b</t>
   </si>
   <si>
@@ -4568,9 +4559,6 @@
   </si>
   <si>
     <t>codO281dDiseaseLeadingTo1c</t>
-  </si>
-  <si>
-    <t>1(d) other disease or condition leading to 1(c) (optional)</t>
   </si>
   <si>
     <t>Optional field - Captures disease or condition leading to 1c</t>
@@ -4697,13 +4685,7 @@
     <t>codO282OtherConditions</t>
   </si>
   <si>
-    <t>2 Other significant conditions contributing to their death (optional)</t>
-  </si>
-  <si>
     <t>Optional field - Captures other conditions that contributed to death.</t>
-  </si>
-  <si>
-    <t>2 Cyflyrau arwyddocaol eraill sy'n cyfrannu at eu marwolaeth (dewisol)</t>
   </si>
   <si>
     <t>Employment question</t>
@@ -5686,7 +5668,49 @@
     <t>Dewiswch ethnigrwydd yr ymadawedig gan ei fod wedi'i gofnodi ar y cofnod cleifion. Os nad oes unrhyw gyd-fynd â'r rhestr, neu os nad oes unrhyw ethnigrwydd yn cael ei gofnodi ar y cofnod claf, dewiswch 'ddim yn hysbys'.</t>
   </si>
   <si>
-    <t>022</t>
+    <t>1(b) Other disease or condition leading to 1(a) (optional)</t>
+  </si>
+  <si>
+    <t>1(c) Other disease or condition leading to 1(b) (optional)</t>
+  </si>
+  <si>
+    <t>1(d) Other disease or condition leading to 1(c) (optional)</t>
+  </si>
+  <si>
+    <t>1(a) Disease or condition directly leading to death</t>
+  </si>
+  <si>
+    <t>codO28SectionTitleTwoDescription</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>codO28SectionTitleOneDescription</t>
+  </si>
+  <si>
+    <t>Other significant condition contributing to the death but &lt;strong&gt;not&lt;/strong&gt; relating to the disease or condition causing it.</t>
+  </si>
+  <si>
+    <t>Cyflwr arwyddocaol arall sy'n cyfrannu at y farwolaeth ond &lt;strong&gt;nid yw'n&lt;/strong&gt; ymwneud â'r clefyd na'r cyflwr sy'n ei achosi.</t>
+  </si>
+  <si>
+    <t>The disease or condition thought to be the underlying cause of death should appear in the lowest completed line of part 1.</t>
+  </si>
+  <si>
+    <t>Dylai'r clefyd neu'r cyflwr y credir ei fod yn achos sylfaenol marwolaeth ymddangos yn y llinell isaf a gwblhawyd o ran 1.</t>
+  </si>
+  <si>
+    <t>Achos y farwolaeth (1)</t>
+  </si>
+  <si>
+    <t>024</t>
+  </si>
+  <si>
+    <t>2 Other significant condition (optional)</t>
+  </si>
+  <si>
+    <t>2 Cyflwr arwyddocaol arall (dewisol)</t>
   </si>
 </sst>
 </file>
@@ -7707,16 +7731,16 @@
         <v>243</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>1230</v>
+        <v>1224</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>1231</v>
+        <v>1225</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>1232</v>
+        <v>1226</v>
       </c>
       <c r="F2" s="68" t="s">
-        <v>1233</v>
+        <v>1227</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="32" x14ac:dyDescent="0.2">
@@ -7724,13 +7748,13 @@
         <v>254</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>1234</v>
+        <v>1228</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>910</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>1235</v>
+        <v>1229</v>
       </c>
       <c r="E3" s="37" t="s">
         <v>911</v>
@@ -7741,13 +7765,13 @@
         <v>32</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>1236</v>
+        <v>1230</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>863</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>1237</v>
+        <v>1231</v>
       </c>
       <c r="E4" s="37" t="s">
         <v>865</v>
@@ -7755,36 +7779,36 @@
     </row>
     <row r="5" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
-        <v>1238</v>
+        <v>1232</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>1239</v>
+        <v>1233</v>
       </c>
       <c r="C5" s="6" t="s">
         <v>152</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>1240</v>
+        <v>1234</v>
       </c>
       <c r="F5" s="68" t="s">
-        <v>1233</v>
+        <v>1227</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
-        <v>1238</v>
+        <v>1232</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>1241</v>
+        <v>1235</v>
       </c>
       <c r="C6" s="6" t="s">
         <v>140</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>1240</v>
+        <v>1234</v>
       </c>
       <c r="F6" s="68" t="s">
-        <v>1233</v>
+        <v>1227</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="32" x14ac:dyDescent="0.2">
@@ -7792,13 +7816,13 @@
         <v>254</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>1242</v>
+        <v>1236</v>
       </c>
       <c r="C7" s="6" t="s">
         <v>913</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>1235</v>
+        <v>1229</v>
       </c>
       <c r="E7" s="37" t="s">
         <v>914</v>
@@ -7809,7 +7833,7 @@
         <v>32</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>1243</v>
+        <v>1237</v>
       </c>
       <c r="C8" s="6" t="s">
         <v>916</v>
@@ -7821,10 +7845,10 @@
     </row>
     <row r="9" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
+        <v>1232</v>
+      </c>
+      <c r="B9" s="5" t="s">
         <v>1238</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>1244</v>
       </c>
       <c r="C9" s="6" t="s">
         <v>922</v>
@@ -7836,22 +7860,22 @@
     </row>
     <row r="10" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="C10" s="27" t="s">
-        <v>1245</v>
+        <v>1239</v>
       </c>
       <c r="D10" s="18" t="s">
-        <v>1246</v>
+        <v>1240</v>
       </c>
       <c r="E10" s="37" t="s">
-        <v>1247</v>
+        <v>1241</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="C11" s="74" t="s">
-        <v>1248</v>
+        <v>1242</v>
       </c>
       <c r="D11" s="18"/>
       <c r="E11" s="37" t="s">
-        <v>1249</v>
+        <v>1243</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
@@ -7888,7 +7912,7 @@
   <dimension ref="A1:F24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -7928,33 +7952,33 @@
         <v>243</v>
       </c>
       <c r="B2" s="92" t="s">
-        <v>1250</v>
+        <v>1244</v>
       </c>
       <c r="C2" s="93" t="s">
-        <v>1251</v>
+        <v>1245</v>
       </c>
       <c r="D2" s="92" t="s">
-        <v>1252</v>
+        <v>1246</v>
       </c>
       <c r="E2" s="85" t="s">
-        <v>1253</v>
+        <v>1247</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="80" x14ac:dyDescent="0.2">
       <c r="A3" s="94" t="s">
-        <v>1254</v>
+        <v>1248</v>
       </c>
       <c r="B3" s="95" t="s">
-        <v>1255</v>
+        <v>1249</v>
       </c>
       <c r="C3" s="96" t="s">
-        <v>1256</v>
+        <v>1250</v>
       </c>
       <c r="D3" s="95" t="s">
-        <v>1257</v>
+        <v>1251</v>
       </c>
       <c r="E3" s="89" t="s">
-        <v>1258</v>
+        <v>1252</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="16" x14ac:dyDescent="0.2">
@@ -7962,16 +7986,16 @@
         <v>758</v>
       </c>
       <c r="B4" s="95" t="s">
-        <v>1259</v>
+        <v>1253</v>
       </c>
       <c r="C4" s="96" t="s">
-        <v>1260</v>
+        <v>1254</v>
       </c>
       <c r="D4" s="95" t="s">
         <v>404</v>
       </c>
       <c r="E4" s="89" t="s">
-        <v>1261</v>
+        <v>1255</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="60.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -7979,13 +8003,13 @@
         <v>410</v>
       </c>
       <c r="B5" s="105" t="s">
-        <v>1262</v>
+        <v>1256</v>
       </c>
       <c r="C5" s="106" t="s">
         <v>404</v>
       </c>
       <c r="D5" s="107" t="s">
-        <v>1263</v>
+        <v>1257</v>
       </c>
       <c r="E5" s="89" t="s">
         <v>404</v>
@@ -7996,13 +8020,13 @@
         <v>413</v>
       </c>
       <c r="B6" s="105" t="s">
-        <v>1264</v>
+        <v>1258</v>
       </c>
       <c r="C6" s="106" t="s">
         <v>404</v>
       </c>
       <c r="D6" s="107" t="s">
-        <v>1265</v>
+        <v>1259</v>
       </c>
       <c r="E6" s="89" t="s">
         <v>404</v>
@@ -8030,33 +8054,33 @@
         <v>243</v>
       </c>
       <c r="B8" s="95" t="s">
-        <v>1266</v>
+        <v>1260</v>
       </c>
       <c r="C8" s="96" t="s">
-        <v>1267</v>
+        <v>1261</v>
       </c>
       <c r="D8" s="95" t="s">
-        <v>1268</v>
+        <v>1262</v>
       </c>
       <c r="E8" s="89" t="s">
-        <v>1269</v>
+        <v>1263</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="64" x14ac:dyDescent="0.2">
       <c r="A9" s="94" t="s">
-        <v>1254</v>
+        <v>1248</v>
       </c>
       <c r="B9" s="95" t="s">
-        <v>1270</v>
+        <v>1264</v>
       </c>
       <c r="C9" s="96" t="s">
-        <v>1271</v>
+        <v>1265</v>
       </c>
       <c r="D9" s="95" t="s">
-        <v>1272</v>
+        <v>1266</v>
       </c>
       <c r="E9" s="89" t="s">
-        <v>1273</v>
+        <v>1267</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="16" x14ac:dyDescent="0.2">
@@ -8064,10 +8088,10 @@
         <v>758</v>
       </c>
       <c r="B10" s="95" t="s">
-        <v>1274</v>
+        <v>1268</v>
       </c>
       <c r="C10" s="96" t="s">
-        <v>1275</v>
+        <v>1269</v>
       </c>
       <c r="D10" s="95" t="s">
         <v>404</v>
@@ -8081,13 +8105,13 @@
         <v>410</v>
       </c>
       <c r="B11" s="105" t="s">
-        <v>1276</v>
+        <v>1270</v>
       </c>
       <c r="C11" s="106" t="s">
         <v>404</v>
       </c>
       <c r="D11" s="107" t="s">
-        <v>1263</v>
+        <v>1257</v>
       </c>
       <c r="E11" s="89" t="s">
         <v>404</v>
@@ -8098,13 +8122,13 @@
         <v>413</v>
       </c>
       <c r="B12" s="105" t="s">
-        <v>1277</v>
+        <v>1271</v>
       </c>
       <c r="C12" s="106" t="s">
         <v>404</v>
       </c>
       <c r="D12" s="107" t="s">
-        <v>1265</v>
+        <v>1259</v>
       </c>
       <c r="E12" s="89" t="s">
         <v>404</v>
@@ -8132,13 +8156,13 @@
         <v>243</v>
       </c>
       <c r="B14" s="95" t="s">
-        <v>1278</v>
+        <v>1272</v>
       </c>
       <c r="C14" s="96" t="s">
-        <v>1279</v>
+        <v>1273</v>
       </c>
       <c r="D14" s="95" t="s">
-        <v>1280</v>
+        <v>1274</v>
       </c>
       <c r="E14" s="89" t="s">
         <v>404</v>
@@ -8146,19 +8170,19 @@
     </row>
     <row r="15" spans="1:6" ht="96" x14ac:dyDescent="0.2">
       <c r="A15" s="94" t="s">
-        <v>1254</v>
+        <v>1248</v>
       </c>
       <c r="B15" s="95" t="s">
-        <v>1281</v>
+        <v>1275</v>
       </c>
       <c r="C15" s="96" t="s">
-        <v>1282</v>
+        <v>1276</v>
       </c>
       <c r="D15" s="95" t="s">
-        <v>1283</v>
+        <v>1277</v>
       </c>
       <c r="E15" s="89" t="s">
-        <v>1284</v>
+        <v>1278</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="48" x14ac:dyDescent="0.2">
@@ -8166,13 +8190,13 @@
         <v>410</v>
       </c>
       <c r="B16" s="105" t="s">
-        <v>1285</v>
+        <v>1279</v>
       </c>
       <c r="C16" s="106" t="s">
         <v>404</v>
       </c>
       <c r="D16" s="107" t="s">
-        <v>1263</v>
+        <v>1257</v>
       </c>
       <c r="E16" s="89" t="s">
         <v>404</v>
@@ -8183,13 +8207,13 @@
         <v>413</v>
       </c>
       <c r="B17" s="105" t="s">
-        <v>1286</v>
+        <v>1280</v>
       </c>
       <c r="C17" s="106" t="s">
         <v>404</v>
       </c>
       <c r="D17" s="107" t="s">
-        <v>1265</v>
+        <v>1259</v>
       </c>
       <c r="E17" s="89" t="s">
         <v>404</v>
@@ -8200,16 +8224,16 @@
         <v>14</v>
       </c>
       <c r="B18" s="95" t="s">
-        <v>1287</v>
+        <v>1281</v>
       </c>
       <c r="C18" s="96" t="s">
-        <v>1288</v>
+        <v>1282</v>
       </c>
       <c r="D18" s="95" t="s">
         <v>404</v>
       </c>
       <c r="E18" s="89" t="s">
-        <v>1289</v>
+        <v>1283</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -8234,13 +8258,13 @@
         <v>243</v>
       </c>
       <c r="B20" s="95" t="s">
-        <v>1290</v>
+        <v>1284</v>
       </c>
       <c r="C20" s="96" t="s">
-        <v>1291</v>
+        <v>1285</v>
       </c>
       <c r="D20" s="95" t="s">
-        <v>1252</v>
+        <v>1246</v>
       </c>
       <c r="E20" s="89" t="s">
         <v>404</v>
@@ -8248,16 +8272,16 @@
     </row>
     <row r="21" spans="1:5" ht="48" x14ac:dyDescent="0.2">
       <c r="A21" s="94" t="s">
-        <v>1254</v>
+        <v>1248</v>
       </c>
       <c r="B21" s="95" t="s">
-        <v>1292</v>
+        <v>1286</v>
       </c>
       <c r="C21" s="96" t="s">
-        <v>1293</v>
+        <v>1287</v>
       </c>
       <c r="D21" s="95" t="s">
-        <v>1294</v>
+        <v>1288</v>
       </c>
       <c r="E21" s="89" t="s">
         <v>404</v>
@@ -8268,10 +8292,10 @@
         <v>758</v>
       </c>
       <c r="B22" s="95" t="s">
-        <v>1295</v>
+        <v>1289</v>
       </c>
       <c r="C22" s="96" t="s">
-        <v>1296</v>
+        <v>1290</v>
       </c>
       <c r="D22" s="95" t="s">
         <v>404</v>
@@ -8285,13 +8309,13 @@
         <v>410</v>
       </c>
       <c r="B23" s="105" t="s">
-        <v>1297</v>
+        <v>1291</v>
       </c>
       <c r="C23" s="106" t="s">
         <v>404</v>
       </c>
       <c r="D23" s="107" t="s">
-        <v>1263</v>
+        <v>1257</v>
       </c>
       <c r="E23" s="89" t="s">
         <v>404</v>
@@ -8302,13 +8326,13 @@
         <v>413</v>
       </c>
       <c r="B24" s="105" t="s">
-        <v>1298</v>
+        <v>1292</v>
       </c>
       <c r="C24" s="106" t="s">
         <v>404</v>
       </c>
       <c r="D24" s="107" t="s">
-        <v>1265</v>
+        <v>1259</v>
       </c>
       <c r="E24" s="89" t="s">
         <v>404</v>
@@ -8361,7 +8385,7 @@
     </row>
     <row r="2" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="193" t="s">
-        <v>1299</v>
+        <v>1293</v>
       </c>
       <c r="B2" s="194"/>
       <c r="C2" s="194"/>
@@ -8374,16 +8398,16 @@
         <v>243</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>1300</v>
+        <v>1294</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>1301</v>
+        <v>1295</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>1232</v>
+        <v>1226</v>
       </c>
       <c r="E3" s="37" t="s">
-        <v>1302</v>
+        <v>1296</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="32" x14ac:dyDescent="0.2">
@@ -8391,13 +8415,13 @@
         <v>261</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>1303</v>
+        <v>1297</v>
       </c>
       <c r="C4" s="59" t="s">
-        <v>1304</v>
+        <v>1298</v>
       </c>
       <c r="E4" s="37" t="s">
-        <v>1305</v>
+        <v>1299</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="16" x14ac:dyDescent="0.2">
@@ -8405,13 +8429,13 @@
         <v>254</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>1306</v>
+        <v>1300</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>1307</v>
+        <v>1301</v>
       </c>
       <c r="E5" s="37" t="s">
-        <v>1308</v>
+        <v>1302</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="80" x14ac:dyDescent="0.2">
@@ -8419,13 +8443,13 @@
         <v>261</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>1309</v>
+        <v>1303</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>1310</v>
+        <v>1304</v>
       </c>
       <c r="E6" s="37" t="s">
-        <v>1311</v>
+        <v>1305</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="32" x14ac:dyDescent="0.2">
@@ -8433,112 +8457,112 @@
         <v>254</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>1312</v>
+        <v>1306</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>1313</v>
+        <v>1307</v>
       </c>
       <c r="E7" s="37" t="s">
-        <v>1314</v>
+        <v>1308</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
-        <v>1315</v>
+        <v>1309</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>1316</v>
+        <v>1310</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>1317</v>
+        <v>1311</v>
       </c>
       <c r="E8" s="37" t="s">
-        <v>1318</v>
+        <v>1312</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
-        <v>1319</v>
+        <v>1313</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>1320</v>
+        <v>1314</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>1321</v>
+        <v>1315</v>
       </c>
       <c r="E9" s="37" t="s">
-        <v>1322</v>
+        <v>1316</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
+        <v>1313</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>1317</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>1318</v>
+      </c>
+      <c r="E10" s="37" t="s">
         <v>1319</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>1323</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>1324</v>
-      </c>
-      <c r="E10" s="37" t="s">
-        <v>1325</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
-        <v>1319</v>
+        <v>1313</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>1326</v>
+        <v>1320</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>1327</v>
+        <v>1321</v>
       </c>
       <c r="E11" s="37" t="s">
-        <v>1328</v>
+        <v>1322</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="5" t="s">
-        <v>1319</v>
+        <v>1313</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>1329</v>
+        <v>1323</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>1330</v>
+        <v>1324</v>
       </c>
       <c r="E12" s="37" t="s">
-        <v>1331</v>
+        <v>1325</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="s">
-        <v>1319</v>
+        <v>1313</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>1332</v>
+        <v>1326</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>1333</v>
+        <v>1327</v>
       </c>
       <c r="E13" s="37" t="s">
-        <v>1334</v>
+        <v>1328</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A14" s="5" t="s">
-        <v>1315</v>
+        <v>1309</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>1335</v>
+        <v>1329</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>1336</v>
+        <v>1330</v>
       </c>
       <c r="D14" s="1"/>
       <c r="E14" s="37" t="s">
-        <v>1337</v>
+        <v>1331</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="32" x14ac:dyDescent="0.2">
@@ -8546,14 +8570,14 @@
         <v>952</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>1338</v>
+        <v>1332</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>1339</v>
+        <v>1333</v>
       </c>
       <c r="D15" s="1"/>
       <c r="E15" s="37" t="s">
-        <v>1340</v>
+        <v>1334</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="16" x14ac:dyDescent="0.2">
@@ -8561,34 +8585,34 @@
         <v>14</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>1341</v>
+        <v>1335</v>
       </c>
       <c r="C16" s="74" t="s">
-        <v>1342</v>
+        <v>1336</v>
       </c>
       <c r="D16" s="18"/>
       <c r="E16" s="37" t="s">
-        <v>1343</v>
+        <v>1337</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A17" s="5" t="s">
-        <v>1344</v>
+        <v>1338</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>1345</v>
+        <v>1339</v>
       </c>
       <c r="C17" s="75" t="s">
-        <v>1346</v>
+        <v>1340</v>
       </c>
       <c r="D17" s="18"/>
       <c r="E17" s="37" t="s">
-        <v>1347</v>
+        <v>1341</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="193" t="s">
-        <v>1348</v>
+        <v>1342</v>
       </c>
       <c r="B18" s="194"/>
       <c r="C18" s="194"/>
@@ -8601,16 +8625,16 @@
         <v>243</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>1351</v>
+        <v>1345</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>1349</v>
+        <v>1343</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>1232</v>
+        <v>1226</v>
       </c>
       <c r="E19" s="37" t="s">
-        <v>1350</v>
+        <v>1344</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="96" x14ac:dyDescent="0.2">
@@ -8618,13 +8642,13 @@
         <v>261</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>1352</v>
+        <v>1346</v>
       </c>
       <c r="C20" s="59" t="s">
-        <v>1422</v>
+        <v>1416</v>
       </c>
       <c r="E20" s="37" t="s">
-        <v>1424</v>
+        <v>1418</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="16" x14ac:dyDescent="0.2">
@@ -8632,13 +8656,13 @@
         <v>254</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>1353</v>
+        <v>1347</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>1307</v>
+        <v>1301</v>
       </c>
       <c r="E21" s="37" t="s">
-        <v>1308</v>
+        <v>1302</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="80" x14ac:dyDescent="0.2">
@@ -8646,13 +8670,13 @@
         <v>261</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>1354</v>
+        <v>1348</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>1423</v>
+        <v>1417</v>
       </c>
       <c r="E22" s="37" t="s">
-        <v>1425</v>
+        <v>1419</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
@@ -8674,7 +8698,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F68"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="F3" sqref="F3"/>
     </sheetView>
@@ -8716,13 +8740,13 @@
         <v>7</v>
       </c>
       <c r="C2" s="100" t="s">
-        <v>1435</v>
+        <v>1441</v>
       </c>
       <c r="D2" s="98" t="s">
         <v>8</v>
       </c>
       <c r="E2" s="99" t="s">
-        <v>1435</v>
+        <v>1441</v>
       </c>
       <c r="F2" s="98"/>
     </row>
@@ -8740,7 +8764,7 @@
         <v>12</v>
       </c>
       <c r="E3" s="37" t="s">
-        <v>1421</v>
+        <v>1415</v>
       </c>
       <c r="F3" s="5" t="s">
         <v>13</v>
@@ -9795,18 +9819,18 @@
     </row>
     <row r="67" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="B67" s="1" t="s">
-        <v>1365</v>
+        <v>1359</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>1366</v>
+        <v>1360</v>
       </c>
       <c r="E67" s="40" t="s">
-        <v>1368</v>
+        <v>1362</v>
       </c>
     </row>
     <row r="68" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="B68" s="1" t="s">
-        <v>1367</v>
+        <v>1361</v>
       </c>
       <c r="C68" s="2" t="s">
         <v>76</v>
@@ -9825,7 +9849,7 @@
   <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
@@ -10107,14 +10131,14 @@
         <v>243</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>1392</v>
+        <v>1386</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>1393</v>
+        <v>1387</v>
       </c>
       <c r="D2" s="5"/>
       <c r="E2" s="43" t="s">
-        <v>1401</v>
+        <v>1395</v>
       </c>
       <c r="F2" s="1"/>
     </row>
@@ -10123,19 +10147,19 @@
         <v>484</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>1394</v>
+        <v>1388</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>1395</v>
+        <v>1389</v>
       </c>
       <c r="D3" s="5"/>
       <c r="E3" s="43" t="s">
-        <v>1402</v>
+        <v>1396</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="159" t="s">
-        <v>1396</v>
+        <v>1390</v>
       </c>
       <c r="B4" s="160"/>
       <c r="C4" s="160"/>
@@ -10147,14 +10171,14 @@
         <v>243</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>1397</v>
+        <v>1391</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>1399</v>
+        <v>1393</v>
       </c>
       <c r="D5" s="5"/>
       <c r="E5" s="43" t="s">
-        <v>1403</v>
+        <v>1397</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="96" x14ac:dyDescent="0.2">
@@ -10162,14 +10186,14 @@
         <v>484</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>1398</v>
+        <v>1392</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>1400</v>
+        <v>1394</v>
       </c>
       <c r="D6" s="5"/>
       <c r="E6" s="43" t="s">
-        <v>1404</v>
+        <v>1398</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
@@ -10333,7 +10357,7 @@
   <dimension ref="A1:F31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
@@ -10390,7 +10414,7 @@
         <v>243</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>1407</v>
+        <v>1401</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>276</v>
@@ -10414,7 +10438,7 @@
         <v>246</v>
       </c>
       <c r="E4" s="43" t="s">
-        <v>1408</v>
+        <v>1402</v>
       </c>
       <c r="F4" s="68" t="s">
         <v>280</v>
@@ -10428,13 +10452,13 @@
         <v>281</v>
       </c>
       <c r="C5" s="52" t="s">
-        <v>1413</v>
+        <v>1407</v>
       </c>
       <c r="D5" s="66" t="s">
         <v>282</v>
       </c>
       <c r="E5" s="156" t="s">
-        <v>1418</v>
+        <v>1412</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>283</v>
@@ -10448,13 +10472,13 @@
         <v>284</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>1414</v>
+        <v>1408</v>
       </c>
       <c r="D6" s="67" t="s">
         <v>285</v>
       </c>
       <c r="E6" s="157" t="s">
-        <v>1415</v>
+        <v>1409</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="160" x14ac:dyDescent="0.2">
@@ -10465,13 +10489,13 @@
         <v>286</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>1416</v>
+        <v>1410</v>
       </c>
       <c r="D7" s="67" t="s">
         <v>287</v>
       </c>
       <c r="E7" s="157" t="s">
-        <v>1417</v>
+        <v>1411</v>
       </c>
       <c r="F7" s="68" t="s">
         <v>288</v>
@@ -10673,7 +10697,7 @@
         <v>336</v>
       </c>
       <c r="C19" s="64" t="s">
-        <v>1405</v>
+        <v>1399</v>
       </c>
       <c r="D19" s="7" t="s">
         <v>337</v>
@@ -10807,17 +10831,17 @@
     </row>
     <row r="27" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A27" s="5" t="s">
-        <v>1411</v>
+        <v>1405</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>1412</v>
+        <v>1406</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>1409</v>
+        <v>1403</v>
       </c>
       <c r="D27" s="5"/>
       <c r="E27" s="37" t="s">
-        <v>1410</v>
+        <v>1404</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
@@ -11063,13 +11087,13 @@
         <v>401</v>
       </c>
       <c r="C12" s="153" t="s">
-        <v>1369</v>
+        <v>1363</v>
       </c>
       <c r="D12" s="84" t="s">
         <v>402</v>
       </c>
       <c r="E12" s="152" t="s">
-        <v>1370</v>
+        <v>1364</v>
       </c>
       <c r="F12" s="86"/>
     </row>
@@ -11081,13 +11105,13 @@
         <v>403</v>
       </c>
       <c r="C13" s="154" t="s">
-        <v>1371</v>
+        <v>1365</v>
       </c>
       <c r="D13" s="88" t="s">
         <v>404</v>
       </c>
       <c r="E13" s="155" t="s">
-        <v>1372</v>
+        <v>1366</v>
       </c>
       <c r="F13" s="86"/>
     </row>
@@ -11555,7 +11579,7 @@
         <v>485</v>
       </c>
       <c r="C45" s="59" t="s">
-        <v>1388</v>
+        <v>1382</v>
       </c>
       <c r="D45" s="116"/>
       <c r="E45" s="120" t="s">
@@ -11568,14 +11592,14 @@
         <v>484</v>
       </c>
       <c r="B46" s="116" t="s">
-        <v>1391</v>
+        <v>1385</v>
       </c>
       <c r="C46" s="59" t="s">
-        <v>1389</v>
+        <v>1383</v>
       </c>
       <c r="D46" s="116"/>
       <c r="E46" s="120" t="s">
-        <v>1390</v>
+        <v>1384</v>
       </c>
       <c r="F46" s="119"/>
     </row>
@@ -11803,7 +11827,7 @@
         <v>522</v>
       </c>
       <c r="E61" s="120" t="s">
-        <v>1381</v>
+        <v>1375</v>
       </c>
       <c r="F61" s="119"/>
     </row>
@@ -11812,14 +11836,14 @@
         <v>519</v>
       </c>
       <c r="B62" s="116" t="s">
-        <v>1378</v>
+        <v>1372</v>
       </c>
       <c r="C62" s="117" t="s">
-        <v>1380</v>
+        <v>1374</v>
       </c>
       <c r="D62" s="116"/>
       <c r="E62" s="120" t="s">
-        <v>1379</v>
+        <v>1373</v>
       </c>
       <c r="F62" s="119"/>
     </row>
@@ -12153,11 +12177,11 @@
         <v>572</v>
       </c>
       <c r="C84" s="117" t="s">
-        <v>1433</v>
+        <v>1427</v>
       </c>
       <c r="D84" s="116"/>
       <c r="E84" s="120" t="s">
-        <v>1434</v>
+        <v>1428</v>
       </c>
       <c r="F84" s="119" t="s">
         <v>575</v>
@@ -12267,11 +12291,11 @@
         <v>593</v>
       </c>
       <c r="C91" s="117" t="s">
-        <v>1431</v>
+        <v>1425</v>
       </c>
       <c r="D91" s="116"/>
       <c r="E91" s="120" t="s">
-        <v>1432</v>
+        <v>1426</v>
       </c>
       <c r="F91" s="119"/>
     </row>
@@ -13005,7 +13029,7 @@
         <v>710</v>
       </c>
       <c r="C141" s="113" t="s">
-        <v>1356</v>
+        <v>1350</v>
       </c>
       <c r="D141" s="122" t="s">
         <v>711</v>
@@ -13095,7 +13119,7 @@
         <v>725</v>
       </c>
       <c r="C147" s="59" t="s">
-        <v>1355</v>
+        <v>1349</v>
       </c>
       <c r="D147" s="116" t="s">
         <v>726</v>
@@ -13126,14 +13150,14 @@
         <v>37</v>
       </c>
       <c r="B149" s="116" t="s">
-        <v>1357</v>
+        <v>1351</v>
       </c>
       <c r="C149" s="59" t="s">
-        <v>1359</v>
+        <v>1353</v>
       </c>
       <c r="D149" s="116"/>
       <c r="E149" s="120" t="s">
-        <v>1361</v>
+        <v>1355</v>
       </c>
       <c r="F149" s="119"/>
     </row>
@@ -13142,14 +13166,14 @@
         <v>37</v>
       </c>
       <c r="B150" s="116" t="s">
-        <v>1358</v>
+        <v>1352</v>
       </c>
       <c r="C150" s="59" t="s">
-        <v>1360</v>
+        <v>1354</v>
       </c>
       <c r="D150" s="116"/>
       <c r="E150" s="120" t="s">
-        <v>1362</v>
+        <v>1356</v>
       </c>
       <c r="F150" s="119"/>
     </row>
@@ -13801,13 +13825,13 @@
         <v>815</v>
       </c>
       <c r="C193" s="59" t="s">
-        <v>1373</v>
+        <v>1367</v>
       </c>
       <c r="D193" s="116" t="s">
         <v>816</v>
       </c>
       <c r="E193" s="120" t="s">
-        <v>1377</v>
+        <v>1371</v>
       </c>
       <c r="F193" s="119"/>
     </row>
@@ -13816,14 +13840,14 @@
         <v>484</v>
       </c>
       <c r="B194" s="116" t="s">
-        <v>1374</v>
+        <v>1368</v>
       </c>
       <c r="C194" s="59" t="s">
-        <v>1375</v>
+        <v>1369</v>
       </c>
       <c r="D194" s="116"/>
       <c r="E194" s="120" t="s">
-        <v>1376</v>
+        <v>1370</v>
       </c>
       <c r="F194" s="119"/>
     </row>
@@ -13923,11 +13947,11 @@
         <v>827</v>
       </c>
       <c r="C201" s="117" t="s">
-        <v>1384</v>
+        <v>1378</v>
       </c>
       <c r="D201" s="116"/>
       <c r="E201" s="120" t="s">
-        <v>1387</v>
+        <v>1381</v>
       </c>
       <c r="F201" s="119"/>
     </row>
@@ -13936,7 +13960,7 @@
         <v>734</v>
       </c>
       <c r="B202" s="116" t="s">
-        <v>1386</v>
+        <v>1380</v>
       </c>
       <c r="C202" s="117" t="s">
         <v>43</v>
@@ -13952,14 +13976,14 @@
         <v>32</v>
       </c>
       <c r="B203" s="116" t="s">
-        <v>1385</v>
+        <v>1379</v>
       </c>
       <c r="C203" s="134" t="s">
-        <v>1382</v>
+        <v>1376</v>
       </c>
       <c r="D203" s="116"/>
       <c r="E203" s="120" t="s">
-        <v>1383</v>
+        <v>1377</v>
       </c>
       <c r="F203" s="119"/>
     </row>
@@ -14331,13 +14355,13 @@
         <v>866</v>
       </c>
       <c r="C228" s="59" t="s">
-        <v>1419</v>
+        <v>1413</v>
       </c>
       <c r="D228" s="116" t="s">
         <v>867</v>
       </c>
       <c r="E228" s="120" t="s">
-        <v>1420</v>
+        <v>1414</v>
       </c>
       <c r="F228" s="119"/>
     </row>
@@ -15569,13 +15593,13 @@
         <v>942</v>
       </c>
       <c r="C17" s="151" t="s">
-        <v>1363</v>
+        <v>1357</v>
       </c>
       <c r="D17" s="92" t="s">
         <v>934</v>
       </c>
       <c r="E17" s="152" t="s">
-        <v>1364</v>
+        <v>1358</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="80" x14ac:dyDescent="0.2">
@@ -15775,10 +15799,10 @@
         <v>982</v>
       </c>
       <c r="C32" s="21" t="s">
-        <v>1426</v>
+        <v>1420</v>
       </c>
       <c r="E32" s="46" t="s">
-        <v>1427</v>
+        <v>1421</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="32" x14ac:dyDescent="0.2">
@@ -15786,13 +15810,13 @@
         <v>261</v>
       </c>
       <c r="B33" s="19" t="s">
-        <v>1428</v>
+        <v>1422</v>
       </c>
       <c r="C33" s="21" t="s">
-        <v>1429</v>
+        <v>1423</v>
       </c>
       <c r="E33" s="46" t="s">
-        <v>1430</v>
+        <v>1424</v>
       </c>
     </row>
     <row r="34" spans="1:6" ht="48" x14ac:dyDescent="0.2">
@@ -15952,13 +15976,13 @@
         <v>1007</v>
       </c>
       <c r="C45" s="62" t="s">
-        <v>1419</v>
+        <v>1413</v>
       </c>
       <c r="D45" s="116" t="s">
         <v>1008</v>
       </c>
       <c r="E45" s="46" t="s">
-        <v>1420</v>
+        <v>1414</v>
       </c>
     </row>
     <row r="46" spans="1:6" ht="48" x14ac:dyDescent="0.2">
@@ -16145,11 +16169,11 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6CA2FE89-1BCA-4888-9BB6-D7A7737E07E4}">
-  <dimension ref="A1:F73"/>
+  <dimension ref="A1:F75"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A45" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F49" sqref="F49"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -16350,71 +16374,71 @@
       <c r="D11" s="136" t="s">
         <v>1074</v>
       </c>
-      <c r="E11" s="138"/>
+      <c r="E11" s="138" t="s">
+        <v>1440</v>
+      </c>
       <c r="F11" s="135"/>
     </row>
-    <row r="12" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A12" s="136" t="s">
+        <v>1434</v>
+      </c>
+      <c r="B12" s="136" t="s">
+        <v>1435</v>
+      </c>
+      <c r="C12" s="137" t="s">
+        <v>1438</v>
+      </c>
+      <c r="D12" s="136"/>
+      <c r="E12" s="138" t="s">
+        <v>1439</v>
+      </c>
+      <c r="F12" s="135"/>
+    </row>
+    <row r="13" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+      <c r="A13" s="136" t="s">
         <v>1047</v>
       </c>
-      <c r="B12" s="136" t="s">
+      <c r="B13" s="136" t="s">
         <v>1075</v>
       </c>
-      <c r="C12" s="137" t="s">
+      <c r="C13" s="137" t="s">
+        <v>1432</v>
+      </c>
+      <c r="D13" s="136" t="s">
         <v>1076</v>
       </c>
-      <c r="D12" s="136" t="s">
+      <c r="E13" s="138" t="s">
         <v>1077</v>
       </c>
-      <c r="E12" s="138" t="s">
-        <v>1078</v>
-      </c>
-      <c r="F12" s="135"/>
-    </row>
-    <row r="13" spans="1:6" ht="48" x14ac:dyDescent="0.2">
-      <c r="A13" s="136" t="s">
-        <v>410</v>
-      </c>
-      <c r="B13" s="28" t="s">
-        <v>1079</v>
-      </c>
-      <c r="C13" s="138"/>
-      <c r="D13" s="136" t="s">
-        <v>1080</v>
-      </c>
-      <c r="E13" s="138"/>
       <c r="F13" s="135"/>
     </row>
     <row r="14" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A14" s="136" t="s">
-        <v>413</v>
+        <v>410</v>
       </c>
       <c r="B14" s="28" t="s">
-        <v>1081</v>
+        <v>1078</v>
       </c>
       <c r="C14" s="138"/>
       <c r="D14" s="136" t="s">
-        <v>1055</v>
+        <v>1079</v>
       </c>
       <c r="E14" s="138"/>
       <c r="F14" s="135"/>
     </row>
-    <row r="15" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A15" s="136" t="s">
-        <v>1047</v>
-      </c>
-      <c r="B15" s="136" t="s">
-        <v>1082</v>
-      </c>
-      <c r="C15" s="137" t="s">
-        <v>1083</v>
-      </c>
+        <v>413</v>
+      </c>
+      <c r="B15" s="28" t="s">
+        <v>1080</v>
+      </c>
+      <c r="C15" s="138"/>
       <c r="D15" s="136" t="s">
-        <v>1084</v>
-      </c>
-      <c r="E15" s="138" t="s">
-        <v>1085</v>
-      </c>
+        <v>1055</v>
+      </c>
+      <c r="E15" s="138"/>
       <c r="F15" s="135"/>
     </row>
     <row r="16" spans="1:6" ht="32" x14ac:dyDescent="0.2">
@@ -16422,311 +16446,308 @@
         <v>1047</v>
       </c>
       <c r="B16" s="136" t="s">
-        <v>1086</v>
+        <v>1081</v>
       </c>
       <c r="C16" s="137" t="s">
-        <v>1087</v>
+        <v>1429</v>
       </c>
       <c r="D16" s="136" t="s">
-        <v>1088</v>
+        <v>1082</v>
       </c>
       <c r="E16" s="138" t="s">
-        <v>1089</v>
+        <v>1083</v>
       </c>
       <c r="F16" s="135"/>
     </row>
-    <row r="17" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A17" s="136" t="s">
         <v>1047</v>
       </c>
       <c r="B17" s="136" t="s">
-        <v>1090</v>
+        <v>1084</v>
       </c>
       <c r="C17" s="137" t="s">
-        <v>1091</v>
+        <v>1430</v>
       </c>
       <c r="D17" s="136" t="s">
-        <v>1092</v>
+        <v>1085</v>
       </c>
       <c r="E17" s="138" t="s">
-        <v>1093</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" ht="144" x14ac:dyDescent="0.2">
+        <v>1086</v>
+      </c>
+      <c r="F17" s="135"/>
+    </row>
+    <row r="18" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A18" s="136" t="s">
         <v>1047</v>
       </c>
       <c r="B18" s="136" t="s">
+        <v>1087</v>
+      </c>
+      <c r="C18" s="137" t="s">
+        <v>1431</v>
+      </c>
+      <c r="D18" s="136" t="s">
+        <v>1088</v>
+      </c>
+      <c r="E18" s="138" t="s">
+        <v>1089</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="144" x14ac:dyDescent="0.2">
+      <c r="A19" s="136" t="s">
+        <v>1047</v>
+      </c>
+      <c r="B19" s="136" t="s">
+        <v>1090</v>
+      </c>
+      <c r="C19" s="137" t="s">
+        <v>1091</v>
+      </c>
+      <c r="D19" s="29" t="s">
+        <v>1092</v>
+      </c>
+      <c r="E19" s="138" t="s">
+        <v>1093</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="80" x14ac:dyDescent="0.2">
+      <c r="A20" s="136" t="s">
+        <v>410</v>
+      </c>
+      <c r="B20" s="28" t="s">
         <v>1094</v>
-      </c>
-      <c r="C18" s="137" t="s">
-        <v>1095</v>
-      </c>
-      <c r="D18" s="29" t="s">
-        <v>1096</v>
-      </c>
-      <c r="E18" s="138" t="s">
-        <v>1097</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" ht="80" x14ac:dyDescent="0.2">
-      <c r="A19" s="136" t="s">
-        <v>410</v>
-      </c>
-      <c r="B19" s="28" t="s">
-        <v>1098</v>
-      </c>
-      <c r="C19" s="27"/>
-      <c r="D19" s="18" t="s">
-        <v>1099</v>
-      </c>
-      <c r="E19" s="138"/>
-    </row>
-    <row r="20" spans="1:5" ht="48" x14ac:dyDescent="0.2">
-      <c r="A20" s="136" t="s">
-        <v>413</v>
-      </c>
-      <c r="B20" s="28" t="s">
-        <v>1100</v>
       </c>
       <c r="C20" s="27"/>
       <c r="D20" s="18" t="s">
-        <v>1055</v>
+        <v>1095</v>
       </c>
       <c r="E20" s="138"/>
     </row>
-    <row r="21" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A21" s="136" t="s">
         <v>413</v>
       </c>
       <c r="B21" s="28" t="s">
-        <v>1101</v>
+        <v>1096</v>
       </c>
       <c r="C21" s="27"/>
       <c r="D21" s="18" t="s">
+        <v>1055</v>
+      </c>
+      <c r="E21" s="138"/>
+    </row>
+    <row r="22" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+      <c r="A22" s="136" t="s">
+        <v>413</v>
+      </c>
+      <c r="B22" s="28" t="s">
+        <v>1097</v>
+      </c>
+      <c r="C22" s="27"/>
+      <c r="D22" s="18" t="s">
+        <v>1098</v>
+      </c>
+      <c r="E22" s="138"/>
+    </row>
+    <row r="23" spans="1:6" ht="112" x14ac:dyDescent="0.2">
+      <c r="A23" s="136" t="s">
+        <v>1099</v>
+      </c>
+      <c r="B23" s="136" t="s">
+        <v>1100</v>
+      </c>
+      <c r="C23" s="137" t="s">
+        <v>1101</v>
+      </c>
+      <c r="D23" s="136" t="s">
         <v>1102</v>
       </c>
-      <c r="E21" s="138"/>
-    </row>
-    <row r="22" spans="1:5" ht="112" x14ac:dyDescent="0.2">
-      <c r="A22" s="136" t="s">
+      <c r="E23" s="138" t="s">
         <v>1103</v>
       </c>
-      <c r="B22" s="136" t="s">
+    </row>
+    <row r="24" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+      <c r="A24" s="136" t="s">
+        <v>410</v>
+      </c>
+      <c r="B24" s="28" t="s">
         <v>1104</v>
-      </c>
-      <c r="C22" s="137" t="s">
-        <v>1105</v>
-      </c>
-      <c r="D22" s="136" t="s">
-        <v>1106</v>
-      </c>
-      <c r="E22" s="138" t="s">
-        <v>1107</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" ht="48" x14ac:dyDescent="0.2">
-      <c r="A23" s="136" t="s">
-        <v>410</v>
-      </c>
-      <c r="B23" s="28" t="s">
-        <v>1108</v>
-      </c>
-      <c r="C23" s="27"/>
-      <c r="D23" s="136" t="s">
-        <v>1109</v>
-      </c>
-      <c r="E23" s="138"/>
-    </row>
-    <row r="24" spans="1:5" ht="32" x14ac:dyDescent="0.2">
-      <c r="A24" s="136" t="s">
-        <v>413</v>
-      </c>
-      <c r="B24" s="28" t="s">
-        <v>1110</v>
       </c>
       <c r="C24" s="27"/>
       <c r="D24" s="136" t="s">
-        <v>1111</v>
+        <v>1105</v>
       </c>
       <c r="E24" s="138"/>
     </row>
-    <row r="25" spans="1:5" ht="64" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A25" s="136" t="s">
         <v>413</v>
       </c>
       <c r="B25" s="28" t="s">
+        <v>1106</v>
+      </c>
+      <c r="C25" s="27"/>
+      <c r="D25" s="136" t="s">
+        <v>1107</v>
+      </c>
+      <c r="E25" s="138"/>
+    </row>
+    <row r="26" spans="1:6" ht="64" x14ac:dyDescent="0.2">
+      <c r="A26" s="136" t="s">
+        <v>413</v>
+      </c>
+      <c r="B26" s="28" t="s">
+        <v>1108</v>
+      </c>
+      <c r="C26" s="27"/>
+      <c r="D26" s="29" t="s">
+        <v>1109</v>
+      </c>
+      <c r="E26" s="138"/>
+    </row>
+    <row r="27" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A27" s="136" t="s">
+        <v>254</v>
+      </c>
+      <c r="B27" s="136" t="s">
+        <v>1110</v>
+      </c>
+      <c r="C27" s="137" t="s">
+        <v>1111</v>
+      </c>
+      <c r="D27" s="136" t="s">
+        <v>1074</v>
+      </c>
+      <c r="E27" s="138" t="s">
         <v>1112</v>
       </c>
-      <c r="C25" s="27"/>
-      <c r="D25" s="29" t="s">
+    </row>
+    <row r="28" spans="1:6" ht="64" x14ac:dyDescent="0.2">
+      <c r="A28" s="136" t="s">
+        <v>1434</v>
+      </c>
+      <c r="B28" s="136" t="s">
+        <v>1433</v>
+      </c>
+      <c r="C28" s="137" t="s">
+        <v>1436</v>
+      </c>
+      <c r="D28" s="136"/>
+      <c r="E28" s="138" t="s">
+        <v>1437</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+      <c r="A29" s="136" t="s">
+        <v>1047</v>
+      </c>
+      <c r="B29" s="136" t="s">
         <v>1113</v>
       </c>
-      <c r="E25" s="138"/>
-    </row>
-    <row r="26" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A26" s="136" t="s">
-        <v>254</v>
-      </c>
-      <c r="B26" s="136" t="s">
+      <c r="C29" s="137" t="s">
+        <v>1442</v>
+      </c>
+      <c r="D29" s="136" t="s">
         <v>1114</v>
       </c>
-      <c r="C26" s="137" t="s">
+      <c r="E29" s="138" t="s">
+        <v>1443</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" s="13" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="186" t="s">
         <v>1115</v>
       </c>
-      <c r="D26" s="136" t="s">
-        <v>1074</v>
-      </c>
-      <c r="E26" s="138" t="s">
+      <c r="B30" s="187"/>
+      <c r="C30" s="187"/>
+      <c r="D30" s="187"/>
+      <c r="E30" s="188"/>
+    </row>
+    <row r="31" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+      <c r="A31" s="140" t="s">
+        <v>243</v>
+      </c>
+      <c r="B31" s="141" t="s">
         <v>1116</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" ht="32" x14ac:dyDescent="0.2">
-      <c r="A27" s="136" t="s">
-        <v>1047</v>
-      </c>
-      <c r="B27" s="136" t="s">
+      <c r="C31" s="142" t="s">
         <v>1117</v>
       </c>
-      <c r="C27" s="137" t="s">
+      <c r="D31" s="5" t="s">
         <v>1118</v>
       </c>
-      <c r="D27" s="136" t="s">
+      <c r="E31" s="143" t="s">
         <v>1119</v>
       </c>
-      <c r="E27" s="138" t="s">
+    </row>
+    <row r="32" spans="1:6" ht="64" x14ac:dyDescent="0.2">
+      <c r="A32" s="144" t="s">
         <v>1120</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="186" t="s">
+      <c r="B32" s="144" t="s">
         <v>1121</v>
       </c>
-      <c r="B28" s="187"/>
-      <c r="C28" s="187"/>
-      <c r="D28" s="187"/>
-      <c r="E28" s="188"/>
-    </row>
-    <row r="29" spans="1:5" ht="48" x14ac:dyDescent="0.2">
-      <c r="A29" s="140" t="s">
-        <v>243</v>
-      </c>
-      <c r="B29" s="141" t="s">
+      <c r="C32" s="145" t="s">
         <v>1122</v>
       </c>
-      <c r="C29" s="142" t="s">
+      <c r="D32" s="144" t="s">
         <v>1123</v>
       </c>
-      <c r="D29" s="5" t="s">
+      <c r="E32" s="146" t="s">
         <v>1124</v>
       </c>
-      <c r="E29" s="143" t="s">
+    </row>
+    <row r="33" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+      <c r="A33" s="18" t="s">
+        <v>410</v>
+      </c>
+      <c r="B33" s="28" t="s">
         <v>1125</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" ht="64" x14ac:dyDescent="0.2">
-      <c r="A30" s="144" t="s">
+      <c r="C33" s="27"/>
+      <c r="D33" s="18" t="s">
+        <v>999</v>
+      </c>
+      <c r="E33" s="146"/>
+    </row>
+    <row r="34" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+      <c r="A34" s="18" t="s">
+        <v>413</v>
+      </c>
+      <c r="B34" s="28" t="s">
         <v>1126</v>
       </c>
-      <c r="B30" s="144" t="s">
+      <c r="C34" s="27"/>
+      <c r="D34" s="18" t="s">
+        <v>992</v>
+      </c>
+      <c r="E34" s="146"/>
+    </row>
+    <row r="35" spans="1:6" s="13" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="189" t="s">
         <v>1127</v>
       </c>
-      <c r="C30" s="145" t="s">
-        <v>1128</v>
-      </c>
-      <c r="D30" s="144" t="s">
-        <v>1129</v>
-      </c>
-      <c r="E30" s="146" t="s">
-        <v>1130</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" ht="48" x14ac:dyDescent="0.2">
-      <c r="A31" s="18" t="s">
-        <v>410</v>
-      </c>
-      <c r="B31" s="28" t="s">
-        <v>1131</v>
-      </c>
-      <c r="C31" s="27"/>
-      <c r="D31" s="18" t="s">
-        <v>999</v>
-      </c>
-      <c r="E31" s="146"/>
-    </row>
-    <row r="32" spans="1:5" ht="48" x14ac:dyDescent="0.2">
-      <c r="A32" s="18" t="s">
-        <v>413</v>
-      </c>
-      <c r="B32" s="28" t="s">
-        <v>1132</v>
-      </c>
-      <c r="C32" s="27"/>
-      <c r="D32" s="18" t="s">
-        <v>992</v>
-      </c>
-      <c r="E32" s="146"/>
-    </row>
-    <row r="33" spans="1:6" s="13" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="189" t="s">
-        <v>1133</v>
-      </c>
-      <c r="B33" s="190"/>
-      <c r="C33" s="191"/>
-      <c r="D33" s="190"/>
-      <c r="E33" s="192"/>
-    </row>
-    <row r="34" spans="1:6" ht="32" x14ac:dyDescent="0.2">
-      <c r="A34" s="144" t="s">
-        <v>243</v>
-      </c>
-      <c r="B34" s="147" t="s">
-        <v>1134</v>
-      </c>
-      <c r="C34" s="145" t="s">
-        <v>1135</v>
-      </c>
-      <c r="D34" s="50" t="s">
-        <v>1136</v>
-      </c>
-      <c r="E34" s="146" t="s">
-        <v>1137</v>
-      </c>
-      <c r="F34" s="135"/>
-    </row>
-    <row r="35" spans="1:6" ht="32" x14ac:dyDescent="0.2">
-      <c r="A35" s="144" t="s">
-        <v>1047</v>
-      </c>
-      <c r="B35" s="148" t="s">
-        <v>1138</v>
-      </c>
-      <c r="C35" s="145" t="s">
-        <v>1139</v>
-      </c>
-      <c r="D35" s="149" t="s">
-        <v>1140</v>
-      </c>
-      <c r="E35" s="146" t="s">
-        <v>1141</v>
-      </c>
-      <c r="F35" s="135"/>
+      <c r="B35" s="190"/>
+      <c r="C35" s="191"/>
+      <c r="D35" s="190"/>
+      <c r="E35" s="192"/>
     </row>
     <row r="36" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A36" s="144" t="s">
-        <v>1047</v>
-      </c>
-      <c r="B36" s="148" t="s">
-        <v>1142</v>
+        <v>243</v>
+      </c>
+      <c r="B36" s="147" t="s">
+        <v>1128</v>
       </c>
       <c r="C36" s="145" t="s">
-        <v>1143</v>
-      </c>
-      <c r="D36" s="149" t="s">
-        <v>1140</v>
+        <v>1129</v>
+      </c>
+      <c r="D36" s="50" t="s">
+        <v>1130</v>
       </c>
       <c r="E36" s="146" t="s">
-        <v>1144</v>
+        <v>1131</v>
       </c>
       <c r="F36" s="135"/>
     </row>
@@ -16735,16 +16756,16 @@
         <v>1047</v>
       </c>
       <c r="B37" s="148" t="s">
-        <v>1145</v>
-      </c>
-      <c r="C37" s="49" t="s">
-        <v>1146</v>
+        <v>1132</v>
+      </c>
+      <c r="C37" s="145" t="s">
+        <v>1133</v>
       </c>
       <c r="D37" s="149" t="s">
-        <v>1140</v>
+        <v>1134</v>
       </c>
       <c r="E37" s="146" t="s">
-        <v>1147</v>
+        <v>1135</v>
       </c>
       <c r="F37" s="135"/>
     </row>
@@ -16753,16 +16774,16 @@
         <v>1047</v>
       </c>
       <c r="B38" s="148" t="s">
-        <v>1148</v>
-      </c>
-      <c r="C38" s="49" t="s">
-        <v>1149</v>
+        <v>1136</v>
+      </c>
+      <c r="C38" s="145" t="s">
+        <v>1137</v>
       </c>
       <c r="D38" s="149" t="s">
-        <v>1140</v>
+        <v>1134</v>
       </c>
       <c r="E38" s="146" t="s">
-        <v>1150</v>
+        <v>1138</v>
       </c>
       <c r="F38" s="135"/>
     </row>
@@ -16771,16 +16792,16 @@
         <v>1047</v>
       </c>
       <c r="B39" s="148" t="s">
-        <v>1151</v>
+        <v>1139</v>
       </c>
       <c r="C39" s="49" t="s">
-        <v>1152</v>
+        <v>1140</v>
       </c>
       <c r="D39" s="149" t="s">
-        <v>1140</v>
+        <v>1134</v>
       </c>
       <c r="E39" s="146" t="s">
-        <v>1153</v>
+        <v>1141</v>
       </c>
       <c r="F39" s="135"/>
     </row>
@@ -16789,262 +16810,261 @@
         <v>1047</v>
       </c>
       <c r="B40" s="148" t="s">
-        <v>1154</v>
+        <v>1142</v>
       </c>
       <c r="C40" s="49" t="s">
+        <v>1143</v>
+      </c>
+      <c r="D40" s="149" t="s">
+        <v>1134</v>
+      </c>
+      <c r="E40" s="146" t="s">
+        <v>1144</v>
+      </c>
+      <c r="F40" s="135"/>
+    </row>
+    <row r="41" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+      <c r="A41" s="144" t="s">
+        <v>1047</v>
+      </c>
+      <c r="B41" s="148" t="s">
+        <v>1145</v>
+      </c>
+      <c r="C41" s="49" t="s">
+        <v>1146</v>
+      </c>
+      <c r="D41" s="149" t="s">
+        <v>1134</v>
+      </c>
+      <c r="E41" s="146" t="s">
+        <v>1147</v>
+      </c>
+      <c r="F41" s="135"/>
+    </row>
+    <row r="42" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+      <c r="A42" s="144" t="s">
+        <v>1047</v>
+      </c>
+      <c r="B42" s="148" t="s">
+        <v>1148</v>
+      </c>
+      <c r="C42" s="49" t="s">
         <v>93</v>
       </c>
-      <c r="D40" s="149" t="s">
-        <v>1140</v>
-      </c>
-      <c r="E40" s="146" t="s">
+      <c r="D42" s="149" t="s">
+        <v>1134</v>
+      </c>
+      <c r="E42" s="146" t="s">
         <v>95</v>
       </c>
-      <c r="F40" s="135"/>
-    </row>
-    <row r="41" spans="1:6" ht="48" x14ac:dyDescent="0.2">
-      <c r="A41" s="18" t="s">
+      <c r="F42" s="135"/>
+    </row>
+    <row r="43" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+      <c r="A43" s="18" t="s">
         <v>410</v>
       </c>
-      <c r="B41" s="28" t="s">
-        <v>1155</v>
-      </c>
-      <c r="C41" s="51"/>
-      <c r="D41" s="18" t="s">
+      <c r="B43" s="28" t="s">
+        <v>1149</v>
+      </c>
+      <c r="C43" s="51"/>
+      <c r="D43" s="18" t="s">
         <v>999</v>
       </c>
-      <c r="E41" s="146"/>
-      <c r="F41" s="135"/>
-    </row>
-    <row r="42" spans="1:6" ht="48" x14ac:dyDescent="0.2">
-      <c r="A42" s="18" t="s">
-        <v>413</v>
-      </c>
-      <c r="B42" s="28" t="s">
-        <v>1156</v>
-      </c>
-      <c r="C42" s="27"/>
-      <c r="D42" s="18" t="s">
-        <v>992</v>
-      </c>
-      <c r="E42" s="146"/>
-      <c r="F42" s="135"/>
-    </row>
-    <row r="43" spans="1:6" ht="48" x14ac:dyDescent="0.2">
-      <c r="A43" s="144" t="s">
-        <v>243</v>
-      </c>
-      <c r="B43" s="136" t="s">
-        <v>1157</v>
-      </c>
-      <c r="C43" s="62" t="s">
-        <v>1406</v>
-      </c>
-      <c r="D43" s="5" t="s">
-        <v>1158</v>
-      </c>
-      <c r="E43" s="146" t="s">
-        <v>1159</v>
-      </c>
+      <c r="E43" s="146"/>
       <c r="F43" s="135"/>
     </row>
     <row r="44" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A44" s="18" t="s">
-        <v>410</v>
+        <v>413</v>
       </c>
       <c r="B44" s="28" t="s">
-        <v>1160</v>
+        <v>1150</v>
       </c>
       <c r="C44" s="27"/>
       <c r="D44" s="18" t="s">
-        <v>999</v>
+        <v>992</v>
       </c>
       <c r="E44" s="146"/>
       <c r="F44" s="135"/>
     </row>
     <row r="45" spans="1:6" ht="48" x14ac:dyDescent="0.2">
-      <c r="A45" s="18" t="s">
+      <c r="A45" s="144" t="s">
+        <v>243</v>
+      </c>
+      <c r="B45" s="136" t="s">
+        <v>1151</v>
+      </c>
+      <c r="C45" s="62" t="s">
+        <v>1400</v>
+      </c>
+      <c r="D45" s="5" t="s">
+        <v>1152</v>
+      </c>
+      <c r="E45" s="146" t="s">
+        <v>1153</v>
+      </c>
+      <c r="F45" s="135"/>
+    </row>
+    <row r="46" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+      <c r="A46" s="18" t="s">
+        <v>410</v>
+      </c>
+      <c r="B46" s="28" t="s">
+        <v>1154</v>
+      </c>
+      <c r="C46" s="27"/>
+      <c r="D46" s="18" t="s">
+        <v>999</v>
+      </c>
+      <c r="E46" s="146"/>
+      <c r="F46" s="135"/>
+    </row>
+    <row r="47" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+      <c r="A47" s="18" t="s">
         <v>413</v>
       </c>
-      <c r="B45" s="28" t="s">
+      <c r="B47" s="28" t="s">
+        <v>1155</v>
+      </c>
+      <c r="C47" s="27"/>
+      <c r="D47" s="18" t="s">
+        <v>992</v>
+      </c>
+      <c r="E47" s="146"/>
+      <c r="F47" s="135"/>
+    </row>
+    <row r="48" spans="1:6" s="13" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A48" s="186" t="s">
+        <v>1156</v>
+      </c>
+      <c r="B48" s="187"/>
+      <c r="C48" s="187"/>
+      <c r="D48" s="187"/>
+      <c r="E48" s="188"/>
+    </row>
+    <row r="49" spans="1:6" s="30" customFormat="1" ht="64" x14ac:dyDescent="0.2">
+      <c r="A49" s="144" t="s">
+        <v>243</v>
+      </c>
+      <c r="B49" s="144" t="s">
+        <v>1157</v>
+      </c>
+      <c r="C49" s="62" t="s">
+        <v>858</v>
+      </c>
+      <c r="D49" s="116" t="s">
+        <v>1158</v>
+      </c>
+      <c r="E49" s="63" t="s">
+        <v>860</v>
+      </c>
+      <c r="F49" s="38" t="s">
+        <v>1159</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" s="30" customFormat="1" ht="64" x14ac:dyDescent="0.2">
+      <c r="A50" s="144" t="s">
+        <v>1160</v>
+      </c>
+      <c r="B50" s="144" t="s">
         <v>1161</v>
       </c>
-      <c r="C45" s="27"/>
-      <c r="D45" s="18" t="s">
-        <v>992</v>
-      </c>
-      <c r="E45" s="146"/>
-      <c r="F45" s="135"/>
-    </row>
-    <row r="46" spans="1:6" s="13" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="186" t="s">
+      <c r="C50" s="62" t="s">
+        <v>922</v>
+      </c>
+      <c r="D50" s="116" t="s">
         <v>1162</v>
       </c>
-      <c r="B46" s="187"/>
-      <c r="C46" s="187"/>
-      <c r="D46" s="187"/>
-      <c r="E46" s="188"/>
-    </row>
-    <row r="47" spans="1:6" s="30" customFormat="1" ht="64" x14ac:dyDescent="0.2">
-      <c r="A47" s="144" t="s">
-        <v>243</v>
-      </c>
-      <c r="B47" s="144" t="s">
+      <c r="E50" s="63" t="s">
+        <v>923</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" s="30" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+      <c r="A51" s="144" t="s">
+        <v>1120</v>
+      </c>
+      <c r="B51" s="144" t="s">
         <v>1163</v>
       </c>
-      <c r="C47" s="62" t="s">
-        <v>858</v>
-      </c>
-      <c r="D47" s="116" t="s">
-        <v>1164</v>
-      </c>
-      <c r="E47" s="63" t="s">
-        <v>860</v>
-      </c>
-      <c r="F47" s="38" t="s">
-        <v>1165</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" s="30" customFormat="1" ht="64" x14ac:dyDescent="0.2">
-      <c r="A48" s="144" t="s">
-        <v>1166</v>
-      </c>
-      <c r="B48" s="144" t="s">
-        <v>1167</v>
-      </c>
-      <c r="C48" s="62" t="s">
-        <v>922</v>
-      </c>
-      <c r="D48" s="116" t="s">
-        <v>1168</v>
-      </c>
-      <c r="E48" s="63" t="s">
-        <v>923</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" s="30" customFormat="1" ht="32" x14ac:dyDescent="0.2">
-      <c r="A49" s="144" t="s">
-        <v>1126</v>
-      </c>
-      <c r="B49" s="144" t="s">
-        <v>1169</v>
-      </c>
-      <c r="C49" s="62" t="s">
-        <v>1419</v>
-      </c>
-      <c r="D49" s="116" t="s">
+      <c r="C51" s="62" t="s">
+        <v>1413</v>
+      </c>
+      <c r="D51" s="116" t="s">
         <v>1008</v>
       </c>
-      <c r="E49" s="63" t="s">
-        <v>1420</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" s="30" customFormat="1" ht="48" x14ac:dyDescent="0.2">
-      <c r="A50" s="5" t="s">
-        <v>382</v>
-      </c>
-      <c r="B50" s="136" t="s">
-        <v>1170</v>
-      </c>
-      <c r="C50" s="145" t="s">
-        <v>1171</v>
-      </c>
-      <c r="D50" s="121" t="s">
-        <v>1172</v>
-      </c>
-      <c r="E50" s="63" t="s">
-        <v>1051</v>
-      </c>
-      <c r="F50" s="73" t="s">
-        <v>1173</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" s="30" customFormat="1" ht="48" x14ac:dyDescent="0.2">
-      <c r="A51" s="5" t="s">
-        <v>382</v>
-      </c>
-      <c r="B51" s="136" t="s">
-        <v>1174</v>
-      </c>
-      <c r="C51" s="145" t="s">
-        <v>1175</v>
-      </c>
-      <c r="D51" s="121" t="s">
-        <v>1176</v>
-      </c>
       <c r="E51" s="63" t="s">
-        <v>1177</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" s="30" customFormat="1" ht="64" x14ac:dyDescent="0.2">
+        <v>1414</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" s="30" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A52" s="5" t="s">
         <v>382</v>
       </c>
       <c r="B52" s="136" t="s">
-        <v>1178</v>
+        <v>1164</v>
       </c>
       <c r="C52" s="145" t="s">
-        <v>1179</v>
+        <v>1165</v>
       </c>
       <c r="D52" s="121" t="s">
-        <v>1180</v>
+        <v>1166</v>
       </c>
       <c r="E52" s="63" t="s">
-        <v>1181</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" s="30" customFormat="1" ht="64" x14ac:dyDescent="0.2">
+        <v>1051</v>
+      </c>
+      <c r="F52" s="73" t="s">
+        <v>1167</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" s="30" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A53" s="5" t="s">
         <v>382</v>
       </c>
       <c r="B53" s="136" t="s">
-        <v>1182</v>
+        <v>1168</v>
       </c>
       <c r="C53" s="145" t="s">
-        <v>1183</v>
+        <v>1169</v>
       </c>
       <c r="D53" s="121" t="s">
-        <v>1184</v>
+        <v>1170</v>
       </c>
       <c r="E53" s="63" t="s">
-        <v>1185</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" s="30" customFormat="1" ht="48" x14ac:dyDescent="0.2">
+        <v>1171</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" s="30" customFormat="1" ht="64" x14ac:dyDescent="0.2">
       <c r="A54" s="5" t="s">
         <v>382</v>
       </c>
       <c r="B54" s="136" t="s">
-        <v>1186</v>
+        <v>1172</v>
       </c>
       <c r="C54" s="145" t="s">
-        <v>1187</v>
+        <v>1173</v>
       </c>
       <c r="D54" s="121" t="s">
-        <v>1188</v>
+        <v>1174</v>
       </c>
       <c r="E54" s="63" t="s">
-        <v>1189</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" s="30" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+        <v>1175</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" s="30" customFormat="1" ht="64" x14ac:dyDescent="0.2">
       <c r="A55" s="5" t="s">
         <v>382</v>
       </c>
       <c r="B55" s="136" t="s">
-        <v>1190</v>
+        <v>1176</v>
       </c>
       <c r="C55" s="145" t="s">
-        <v>1191</v>
+        <v>1177</v>
       </c>
       <c r="D55" s="121" t="s">
-        <v>1192</v>
+        <v>1178</v>
       </c>
       <c r="E55" s="63" t="s">
-        <v>1078</v>
-      </c>
-      <c r="F55" s="73" t="s">
-        <v>1193</v>
+        <v>1179</v>
       </c>
     </row>
     <row r="56" spans="1:6" s="30" customFormat="1" ht="48" x14ac:dyDescent="0.2">
@@ -17052,59 +17072,56 @@
         <v>382</v>
       </c>
       <c r="B56" s="136" t="s">
-        <v>1194</v>
+        <v>1180</v>
       </c>
       <c r="C56" s="145" t="s">
-        <v>1195</v>
+        <v>1181</v>
       </c>
       <c r="D56" s="121" t="s">
-        <v>1196</v>
+        <v>1182</v>
       </c>
       <c r="E56" s="63" t="s">
-        <v>1197</v>
-      </c>
-      <c r="F56" s="73" t="s">
-        <v>1198</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6" s="30" customFormat="1" ht="48" x14ac:dyDescent="0.2">
+        <v>1183</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" s="30" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A57" s="5" t="s">
         <v>382</v>
       </c>
       <c r="B57" s="136" t="s">
-        <v>1199</v>
+        <v>1184</v>
       </c>
       <c r="C57" s="145" t="s">
-        <v>1200</v>
+        <v>1185</v>
       </c>
       <c r="D57" s="121" t="s">
-        <v>1201</v>
+        <v>1186</v>
       </c>
       <c r="E57" s="63" t="s">
-        <v>1202</v>
+        <v>1077</v>
       </c>
       <c r="F57" s="73" t="s">
-        <v>1203</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6" s="30" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+        <v>1187</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" s="30" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A58" s="5" t="s">
         <v>382</v>
       </c>
       <c r="B58" s="136" t="s">
-        <v>1204</v>
+        <v>1188</v>
       </c>
       <c r="C58" s="145" t="s">
-        <v>1205</v>
+        <v>1189</v>
       </c>
       <c r="D58" s="121" t="s">
-        <v>1206</v>
+        <v>1190</v>
       </c>
       <c r="E58" s="63" t="s">
-        <v>1207</v>
+        <v>1191</v>
       </c>
       <c r="F58" s="73" t="s">
-        <v>1208</v>
+        <v>1192</v>
       </c>
     </row>
     <row r="59" spans="1:6" s="30" customFormat="1" ht="48" x14ac:dyDescent="0.2">
@@ -17112,50 +17129,56 @@
         <v>382</v>
       </c>
       <c r="B59" s="136" t="s">
-        <v>1209</v>
+        <v>1193</v>
       </c>
       <c r="C59" s="145" t="s">
-        <v>1210</v>
+        <v>1194</v>
       </c>
       <c r="D59" s="121" t="s">
-        <v>1211</v>
+        <v>1195</v>
       </c>
       <c r="E59" s="63" t="s">
-        <v>1212</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6" s="30" customFormat="1" ht="48" x14ac:dyDescent="0.2">
+        <v>1196</v>
+      </c>
+      <c r="F59" s="73" t="s">
+        <v>1197</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" s="30" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A60" s="5" t="s">
         <v>382</v>
       </c>
       <c r="B60" s="136" t="s">
-        <v>1213</v>
+        <v>1198</v>
       </c>
       <c r="C60" s="145" t="s">
-        <v>1214</v>
+        <v>1199</v>
       </c>
       <c r="D60" s="121" t="s">
-        <v>1215</v>
+        <v>1200</v>
       </c>
       <c r="E60" s="63" t="s">
-        <v>1216</v>
+        <v>1201</v>
+      </c>
+      <c r="F60" s="73" t="s">
+        <v>1202</v>
       </c>
     </row>
     <row r="61" spans="1:6" s="30" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A61" s="5" t="s">
         <v>382</v>
       </c>
-      <c r="B61" s="18" t="s">
-        <v>1217</v>
+      <c r="B61" s="136" t="s">
+        <v>1203</v>
       </c>
       <c r="C61" s="145" t="s">
-        <v>1218</v>
+        <v>1204</v>
       </c>
       <c r="D61" s="121" t="s">
-        <v>1219</v>
+        <v>1205</v>
       </c>
       <c r="E61" s="63" t="s">
-        <v>1220</v>
+        <v>1206</v>
       </c>
     </row>
     <row r="62" spans="1:6" s="30" customFormat="1" ht="48" x14ac:dyDescent="0.2">
@@ -17163,85 +17186,103 @@
         <v>382</v>
       </c>
       <c r="B62" s="136" t="s">
-        <v>1221</v>
+        <v>1207</v>
       </c>
       <c r="C62" s="145" t="s">
-        <v>1222</v>
+        <v>1208</v>
       </c>
       <c r="D62" s="121" t="s">
-        <v>1223</v>
-      </c>
-      <c r="E62" s="79" t="s">
-        <v>1224</v>
-      </c>
-    </row>
-    <row r="63" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A63" s="144" t="s">
-        <v>732</v>
-      </c>
-      <c r="B63" s="144" t="s">
-        <v>1225</v>
+        <v>1209</v>
+      </c>
+      <c r="E62" s="63" t="s">
+        <v>1210</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" s="30" customFormat="1" ht="48" x14ac:dyDescent="0.2">
+      <c r="A63" s="5" t="s">
+        <v>382</v>
+      </c>
+      <c r="B63" s="18" t="s">
+        <v>1211</v>
       </c>
       <c r="C63" s="145" t="s">
-        <v>1226</v>
-      </c>
-      <c r="D63" s="148"/>
-      <c r="E63" s="78" t="s">
-        <v>1227</v>
-      </c>
-      <c r="F63" s="135"/>
-    </row>
-    <row r="64" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A64" s="144" t="s">
-        <v>732</v>
-      </c>
-      <c r="B64" s="144" t="s">
-        <v>1228</v>
+        <v>1212</v>
+      </c>
+      <c r="D63" s="121" t="s">
+        <v>1213</v>
+      </c>
+      <c r="E63" s="63" t="s">
+        <v>1214</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" s="30" customFormat="1" ht="48" x14ac:dyDescent="0.2">
+      <c r="A64" s="5" t="s">
+        <v>382</v>
+      </c>
+      <c r="B64" s="136" t="s">
+        <v>1215</v>
       </c>
       <c r="C64" s="145" t="s">
-        <v>1152</v>
-      </c>
-      <c r="D64" s="148"/>
-      <c r="E64" s="78" t="s">
-        <v>1153</v>
-      </c>
-      <c r="F64" s="135"/>
+        <v>1216</v>
+      </c>
+      <c r="D64" s="121" t="s">
+        <v>1217</v>
+      </c>
+      <c r="E64" s="79" t="s">
+        <v>1218</v>
+      </c>
     </row>
     <row r="65" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A65" s="144" t="s">
         <v>732</v>
       </c>
-      <c r="B65" s="136" t="s">
-        <v>1229</v>
+      <c r="B65" s="144" t="s">
+        <v>1219</v>
       </c>
       <c r="C65" s="145" t="s">
-        <v>1139</v>
+        <v>1220</v>
       </c>
       <c r="D65" s="148"/>
       <c r="E65" s="78" t="s">
-        <v>1141</v>
+        <v>1221</v>
       </c>
       <c r="F65" s="135"/>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A66" s="144"/>
-      <c r="B66" s="144"/>
-      <c r="C66" s="145"/>
+    <row r="66" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A66" s="144" t="s">
+        <v>732</v>
+      </c>
+      <c r="B66" s="144" t="s">
+        <v>1222</v>
+      </c>
+      <c r="C66" s="145" t="s">
+        <v>1146</v>
+      </c>
       <c r="D66" s="148"/>
-      <c r="E66" s="146"/>
+      <c r="E66" s="78" t="s">
+        <v>1147</v>
+      </c>
       <c r="F66" s="135"/>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A67" s="144"/>
-      <c r="B67" s="136"/>
-      <c r="C67" s="145"/>
+    <row r="67" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A67" s="144" t="s">
+        <v>732</v>
+      </c>
+      <c r="B67" s="136" t="s">
+        <v>1223</v>
+      </c>
+      <c r="C67" s="145" t="s">
+        <v>1133</v>
+      </c>
       <c r="D67" s="148"/>
-      <c r="E67" s="146"/>
+      <c r="E67" s="78" t="s">
+        <v>1135</v>
+      </c>
       <c r="F67" s="135"/>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A68" s="144"/>
-      <c r="B68" s="136"/>
+      <c r="B68" s="144"/>
       <c r="C68" s="145"/>
       <c r="D68" s="148"/>
       <c r="E68" s="146"/>
@@ -17251,39 +17292,55 @@
       <c r="A69" s="144"/>
       <c r="B69" s="136"/>
       <c r="C69" s="145"/>
-      <c r="D69" s="144"/>
-      <c r="E69" s="150"/>
+      <c r="D69" s="148"/>
+      <c r="E69" s="146"/>
       <c r="F69" s="135"/>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A70" s="144"/>
+      <c r="B70" s="136"/>
+      <c r="C70" s="145"/>
+      <c r="D70" s="148"/>
+      <c r="E70" s="146"/>
+      <c r="F70" s="135"/>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A71" s="144"/>
       <c r="B71" s="136"/>
       <c r="C71" s="145"/>
       <c r="D71" s="144"/>
-      <c r="E71" s="146"/>
+      <c r="E71" s="150"/>
       <c r="F71" s="135"/>
-    </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A72" s="144"/>
-      <c r="B72" s="136"/>
-      <c r="C72" s="145"/>
-      <c r="D72" s="144"/>
-      <c r="E72" s="146"/>
-      <c r="F72" s="135"/>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A73" s="144"/>
-      <c r="B73" s="144"/>
+      <c r="B73" s="136"/>
       <c r="C73" s="145"/>
       <c r="D73" s="144"/>
       <c r="E73" s="146"/>
       <c r="F73" s="135"/>
     </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A74" s="144"/>
+      <c r="B74" s="136"/>
+      <c r="C74" s="145"/>
+      <c r="D74" s="144"/>
+      <c r="E74" s="146"/>
+      <c r="F74" s="135"/>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A75" s="144"/>
+      <c r="B75" s="144"/>
+      <c r="C75" s="145"/>
+      <c r="D75" s="144"/>
+      <c r="E75" s="146"/>
+      <c r="F75" s="135"/>
+    </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="A28:E28"/>
-    <mergeCell ref="A33:E33"/>
-    <mergeCell ref="A46:E46"/>
+    <mergeCell ref="A30:E30"/>
+    <mergeCell ref="A35:E35"/>
+    <mergeCell ref="A48:E48"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
[MCCDB-870] Content amend: Change all Declaration H1s
</commit_message>
<xml_diff>
--- a/app/data/MCCD-localisation.xlsx
+++ b/app/data/MCCD-localisation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/JALAT/GIT/medical-certificate-of-cause-of-death/app/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A7232F7-6A3F-1947-A2BB-E3D94CF2FDEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52A9D321-8B77-1B4B-A04E-7B325D16E8EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="14220" firstSheet="3" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="520" windowWidth="25600" windowHeight="14220" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Using this document" sheetId="8" r:id="rId1"/>
@@ -69,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2148" uniqueCount="1444">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2148" uniqueCount="1438">
   <si>
     <r>
       <rPr>
@@ -5099,15 +5099,9 @@
     <t>apDeclarationPageTitle</t>
   </si>
   <si>
-    <t>Attending practitioner declaration</t>
-  </si>
-  <si>
     <t>Page title - describes the action of signing off the declaration in order to send the certificate for scrutiny.</t>
   </si>
   <si>
-    <t>Datganiad Ymarferydd sy'n Mynychu</t>
-  </si>
-  <si>
     <t>Checkbox</t>
   </si>
   <si>
@@ -5126,12 +5120,6 @@
     <t>apDeclarationSubmitForScrutiny</t>
   </si>
   <si>
-    <t>Submit for scrutiny</t>
-  </si>
-  <si>
-    <t>Cyflwyno ar gyfer craffu</t>
-  </si>
-  <si>
     <t>apDeclarationValidationSummaryNoTick</t>
   </si>
   <si>
@@ -5147,15 +5135,9 @@
     <t>meScrutinyDeclarationPageTitle</t>
   </si>
   <si>
-    <t>Medical examiner declaration</t>
-  </si>
-  <si>
     <t>Page title - describes the action of signing off the declaration post scrutiny.</t>
   </si>
   <si>
-    <t>Datganiad yr Archwiliwr Meddygol</t>
-  </si>
-  <si>
     <t>meScrutinyDeclarationContent</t>
   </si>
   <si>
@@ -5171,9 +5153,6 @@
     <t>meScrutinyReadyForRegistrar</t>
   </si>
   <si>
-    <t>Submit scrutiny</t>
-  </si>
-  <si>
     <t>meScrutinyDeclarationValidationSummaryNoTick</t>
   </si>
   <si>
@@ -5183,9 +5162,6 @@
     <t>meCertDeclarationPageTitle</t>
   </si>
   <si>
-    <t>Medical examiner declaration (ME Cert)</t>
-  </si>
-  <si>
     <t>Page title - describes the action of signing off the declaration for ME Cert.</t>
   </si>
   <si>
@@ -5210,18 +5186,9 @@
     <t>meCertDeclarationCTA</t>
   </si>
   <si>
-    <t>Complete MCCD</t>
-  </si>
-  <si>
-    <t>MCCD cyflawn</t>
-  </si>
-  <si>
     <t>meoDeclarationPageTitle</t>
   </si>
   <si>
-    <t>Medical examiner officer declaration</t>
-  </si>
-  <si>
     <t>meoDeclarationContent</t>
   </si>
   <si>
@@ -5232,9 +5199,6 @@
   </si>
   <si>
     <t>meoDeclarationSubmitForScrutiny</t>
-  </si>
-  <si>
-    <t>Submit for ME scrutiny</t>
   </si>
   <si>
     <t>meoDeclarationValidationSummaryNoTick</t>
@@ -5704,13 +5668,31 @@
     <t>Achos y farwolaeth (1)</t>
   </si>
   <si>
-    <t>024</t>
-  </si>
-  <si>
     <t>2 Other significant condition (optional)</t>
   </si>
   <si>
     <t>2 Cyflwr arwyddocaol arall (dewisol)</t>
+  </si>
+  <si>
+    <t>Declaration</t>
+  </si>
+  <si>
+    <t>Submit</t>
+  </si>
+  <si>
+    <t> Datganiad</t>
+  </si>
+  <si>
+    <t>Cyflwyno</t>
+  </si>
+  <si>
+    <t>Datganiad</t>
+  </si>
+  <si>
+    <t> Cyflwyno</t>
+  </si>
+  <si>
+    <t>025</t>
   </si>
 </sst>
 </file>
@@ -6186,7 +6168,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="195">
+  <cellXfs count="196">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -6663,6 +6645,15 @@
     <xf numFmtId="0" fontId="13" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -6681,15 +6672,6 @@
     <xf numFmtId="0" fontId="13" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
@@ -6761,6 +6743,9 @@
     </xf>
     <xf numFmtId="0" fontId="13" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -7912,8 +7897,8 @@
   <dimension ref="A1:F24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -7954,31 +7939,31 @@
       <c r="B2" s="92" t="s">
         <v>1244</v>
       </c>
-      <c r="C2" s="93" t="s">
+      <c r="C2" s="151" t="s">
+        <v>1431</v>
+      </c>
+      <c r="D2" s="92" t="s">
         <v>1245</v>
       </c>
-      <c r="D2" s="92" t="s">
-        <v>1246</v>
-      </c>
-      <c r="E2" s="85" t="s">
-        <v>1247</v>
+      <c r="E2" s="152" t="s">
+        <v>1435</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="80" x14ac:dyDescent="0.2">
       <c r="A3" s="94" t="s">
+        <v>1246</v>
+      </c>
+      <c r="B3" s="95" t="s">
+        <v>1247</v>
+      </c>
+      <c r="C3" s="96" t="s">
         <v>1248</v>
       </c>
-      <c r="B3" s="95" t="s">
+      <c r="D3" s="95" t="s">
         <v>1249</v>
       </c>
-      <c r="C3" s="96" t="s">
+      <c r="E3" s="89" t="s">
         <v>1250</v>
-      </c>
-      <c r="D3" s="95" t="s">
-        <v>1251</v>
-      </c>
-      <c r="E3" s="89" t="s">
-        <v>1252</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="16" x14ac:dyDescent="0.2">
@@ -7986,16 +7971,16 @@
         <v>758</v>
       </c>
       <c r="B4" s="95" t="s">
-        <v>1253</v>
-      </c>
-      <c r="C4" s="96" t="s">
-        <v>1254</v>
+        <v>1251</v>
+      </c>
+      <c r="C4" s="195" t="s">
+        <v>1432</v>
       </c>
       <c r="D4" s="95" t="s">
         <v>404</v>
       </c>
-      <c r="E4" s="89" t="s">
-        <v>1255</v>
+      <c r="E4" s="155" t="s">
+        <v>1434</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="60.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -8003,13 +7988,13 @@
         <v>410</v>
       </c>
       <c r="B5" s="105" t="s">
-        <v>1256</v>
+        <v>1252</v>
       </c>
       <c r="C5" s="106" t="s">
         <v>404</v>
       </c>
       <c r="D5" s="107" t="s">
-        <v>1257</v>
+        <v>1253</v>
       </c>
       <c r="E5" s="89" t="s">
         <v>404</v>
@@ -8020,13 +8005,13 @@
         <v>413</v>
       </c>
       <c r="B6" s="105" t="s">
-        <v>1258</v>
+        <v>1254</v>
       </c>
       <c r="C6" s="106" t="s">
         <v>404</v>
       </c>
       <c r="D6" s="107" t="s">
-        <v>1259</v>
+        <v>1255</v>
       </c>
       <c r="E6" s="89" t="s">
         <v>404</v>
@@ -8054,33 +8039,33 @@
         <v>243</v>
       </c>
       <c r="B8" s="95" t="s">
-        <v>1260</v>
-      </c>
-      <c r="C8" s="96" t="s">
-        <v>1261</v>
+        <v>1256</v>
+      </c>
+      <c r="C8" s="195" t="s">
+        <v>1431</v>
       </c>
       <c r="D8" s="95" t="s">
-        <v>1262</v>
-      </c>
-      <c r="E8" s="89" t="s">
-        <v>1263</v>
+        <v>1257</v>
+      </c>
+      <c r="E8" s="155" t="s">
+        <v>1435</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="64" x14ac:dyDescent="0.2">
       <c r="A9" s="94" t="s">
-        <v>1248</v>
+        <v>1246</v>
       </c>
       <c r="B9" s="95" t="s">
-        <v>1264</v>
+        <v>1258</v>
       </c>
       <c r="C9" s="96" t="s">
-        <v>1265</v>
+        <v>1259</v>
       </c>
       <c r="D9" s="95" t="s">
-        <v>1266</v>
+        <v>1260</v>
       </c>
       <c r="E9" s="89" t="s">
-        <v>1267</v>
+        <v>1261</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="16" x14ac:dyDescent="0.2">
@@ -8088,16 +8073,16 @@
         <v>758</v>
       </c>
       <c r="B10" s="95" t="s">
-        <v>1268</v>
-      </c>
-      <c r="C10" s="96" t="s">
-        <v>1269</v>
+        <v>1262</v>
+      </c>
+      <c r="C10" s="195" t="s">
+        <v>1432</v>
       </c>
       <c r="D10" s="95" t="s">
         <v>404</v>
       </c>
-      <c r="E10" s="89" t="s">
-        <v>404</v>
+      <c r="E10" s="155" t="s">
+        <v>1434</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -8105,13 +8090,13 @@
         <v>410</v>
       </c>
       <c r="B11" s="105" t="s">
-        <v>1270</v>
+        <v>1263</v>
       </c>
       <c r="C11" s="106" t="s">
         <v>404</v>
       </c>
       <c r="D11" s="107" t="s">
-        <v>1257</v>
+        <v>1253</v>
       </c>
       <c r="E11" s="89" t="s">
         <v>404</v>
@@ -8122,13 +8107,13 @@
         <v>413</v>
       </c>
       <c r="B12" s="105" t="s">
-        <v>1271</v>
+        <v>1264</v>
       </c>
       <c r="C12" s="106" t="s">
         <v>404</v>
       </c>
       <c r="D12" s="107" t="s">
-        <v>1259</v>
+        <v>1255</v>
       </c>
       <c r="E12" s="89" t="s">
         <v>404</v>
@@ -8156,33 +8141,33 @@
         <v>243</v>
       </c>
       <c r="B14" s="95" t="s">
-        <v>1272</v>
-      </c>
-      <c r="C14" s="96" t="s">
-        <v>1273</v>
+        <v>1265</v>
+      </c>
+      <c r="C14" s="195" t="s">
+        <v>1431</v>
       </c>
       <c r="D14" s="95" t="s">
-        <v>1274</v>
-      </c>
-      <c r="E14" s="89" t="s">
-        <v>404</v>
+        <v>1266</v>
+      </c>
+      <c r="E14" s="155" t="s">
+        <v>1433</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="96" x14ac:dyDescent="0.2">
       <c r="A15" s="94" t="s">
-        <v>1248</v>
+        <v>1246</v>
       </c>
       <c r="B15" s="95" t="s">
-        <v>1275</v>
+        <v>1267</v>
       </c>
       <c r="C15" s="96" t="s">
-        <v>1276</v>
+        <v>1268</v>
       </c>
       <c r="D15" s="95" t="s">
-        <v>1277</v>
+        <v>1269</v>
       </c>
       <c r="E15" s="89" t="s">
-        <v>1278</v>
+        <v>1270</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="48" x14ac:dyDescent="0.2">
@@ -8190,13 +8175,13 @@
         <v>410</v>
       </c>
       <c r="B16" s="105" t="s">
-        <v>1279</v>
+        <v>1271</v>
       </c>
       <c r="C16" s="106" t="s">
         <v>404</v>
       </c>
       <c r="D16" s="107" t="s">
-        <v>1257</v>
+        <v>1253</v>
       </c>
       <c r="E16" s="89" t="s">
         <v>404</v>
@@ -8207,13 +8192,13 @@
         <v>413</v>
       </c>
       <c r="B17" s="105" t="s">
-        <v>1280</v>
+        <v>1272</v>
       </c>
       <c r="C17" s="106" t="s">
         <v>404</v>
       </c>
       <c r="D17" s="107" t="s">
-        <v>1259</v>
+        <v>1255</v>
       </c>
       <c r="E17" s="89" t="s">
         <v>404</v>
@@ -8224,16 +8209,16 @@
         <v>14</v>
       </c>
       <c r="B18" s="95" t="s">
-        <v>1281</v>
-      </c>
-      <c r="C18" s="96" t="s">
-        <v>1282</v>
+        <v>1273</v>
+      </c>
+      <c r="C18" s="195" t="s">
+        <v>1432</v>
       </c>
       <c r="D18" s="95" t="s">
         <v>404</v>
       </c>
-      <c r="E18" s="89" t="s">
-        <v>1283</v>
+      <c r="E18" s="155" t="s">
+        <v>1434</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -8258,30 +8243,30 @@
         <v>243</v>
       </c>
       <c r="B20" s="95" t="s">
-        <v>1284</v>
-      </c>
-      <c r="C20" s="96" t="s">
-        <v>1285</v>
+        <v>1274</v>
+      </c>
+      <c r="C20" s="195" t="s">
+        <v>1431</v>
       </c>
       <c r="D20" s="95" t="s">
-        <v>1246</v>
-      </c>
-      <c r="E20" s="89" t="s">
-        <v>404</v>
+        <v>1245</v>
+      </c>
+      <c r="E20" s="155" t="s">
+        <v>1433</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="48" x14ac:dyDescent="0.2">
       <c r="A21" s="94" t="s">
-        <v>1248</v>
+        <v>1246</v>
       </c>
       <c r="B21" s="95" t="s">
-        <v>1286</v>
+        <v>1275</v>
       </c>
       <c r="C21" s="96" t="s">
-        <v>1287</v>
+        <v>1276</v>
       </c>
       <c r="D21" s="95" t="s">
-        <v>1288</v>
+        <v>1277</v>
       </c>
       <c r="E21" s="89" t="s">
         <v>404</v>
@@ -8292,16 +8277,16 @@
         <v>758</v>
       </c>
       <c r="B22" s="95" t="s">
-        <v>1289</v>
-      </c>
-      <c r="C22" s="96" t="s">
-        <v>1290</v>
+        <v>1278</v>
+      </c>
+      <c r="C22" s="195" t="s">
+        <v>1432</v>
       </c>
       <c r="D22" s="95" t="s">
         <v>404</v>
       </c>
-      <c r="E22" s="89" t="s">
-        <v>404</v>
+      <c r="E22" s="155" t="s">
+        <v>1436</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="48" x14ac:dyDescent="0.2">
@@ -8309,13 +8294,13 @@
         <v>410</v>
       </c>
       <c r="B23" s="105" t="s">
-        <v>1291</v>
+        <v>1279</v>
       </c>
       <c r="C23" s="106" t="s">
         <v>404</v>
       </c>
       <c r="D23" s="107" t="s">
-        <v>1257</v>
+        <v>1253</v>
       </c>
       <c r="E23" s="89" t="s">
         <v>404</v>
@@ -8326,13 +8311,13 @@
         <v>413</v>
       </c>
       <c r="B24" s="105" t="s">
-        <v>1292</v>
+        <v>1280</v>
       </c>
       <c r="C24" s="106" t="s">
         <v>404</v>
       </c>
       <c r="D24" s="107" t="s">
-        <v>1259</v>
+        <v>1255</v>
       </c>
       <c r="E24" s="89" t="s">
         <v>404</v>
@@ -8385,7 +8370,7 @@
     </row>
     <row r="2" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="193" t="s">
-        <v>1293</v>
+        <v>1281</v>
       </c>
       <c r="B2" s="194"/>
       <c r="C2" s="194"/>
@@ -8398,16 +8383,16 @@
         <v>243</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>1294</v>
+        <v>1282</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>1295</v>
+        <v>1283</v>
       </c>
       <c r="D3" s="5" t="s">
         <v>1226</v>
       </c>
       <c r="E3" s="37" t="s">
-        <v>1296</v>
+        <v>1284</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="32" x14ac:dyDescent="0.2">
@@ -8415,13 +8400,13 @@
         <v>261</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>1297</v>
+        <v>1285</v>
       </c>
       <c r="C4" s="59" t="s">
-        <v>1298</v>
+        <v>1286</v>
       </c>
       <c r="E4" s="37" t="s">
-        <v>1299</v>
+        <v>1287</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="16" x14ac:dyDescent="0.2">
@@ -8429,13 +8414,13 @@
         <v>254</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>1300</v>
+        <v>1288</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>1301</v>
+        <v>1289</v>
       </c>
       <c r="E5" s="37" t="s">
-        <v>1302</v>
+        <v>1290</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="80" x14ac:dyDescent="0.2">
@@ -8443,13 +8428,13 @@
         <v>261</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>1303</v>
+        <v>1291</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>1304</v>
+        <v>1292</v>
       </c>
       <c r="E6" s="37" t="s">
-        <v>1305</v>
+        <v>1293</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="32" x14ac:dyDescent="0.2">
@@ -8457,112 +8442,112 @@
         <v>254</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>1306</v>
+        <v>1294</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>1307</v>
+        <v>1295</v>
       </c>
       <c r="E7" s="37" t="s">
-        <v>1308</v>
+        <v>1296</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
-        <v>1309</v>
+        <v>1297</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>1310</v>
+        <v>1298</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>1311</v>
+        <v>1299</v>
       </c>
       <c r="E8" s="37" t="s">
-        <v>1312</v>
+        <v>1300</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
-        <v>1313</v>
+        <v>1301</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>1314</v>
+        <v>1302</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>1315</v>
+        <v>1303</v>
       </c>
       <c r="E9" s="37" t="s">
-        <v>1316</v>
+        <v>1304</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
-        <v>1313</v>
+        <v>1301</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>1317</v>
+        <v>1305</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>1318</v>
+        <v>1306</v>
       </c>
       <c r="E10" s="37" t="s">
-        <v>1319</v>
+        <v>1307</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
-        <v>1313</v>
+        <v>1301</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>1320</v>
+        <v>1308</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>1321</v>
+        <v>1309</v>
       </c>
       <c r="E11" s="37" t="s">
-        <v>1322</v>
+        <v>1310</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="5" t="s">
+        <v>1301</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>1311</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>1312</v>
+      </c>
+      <c r="E12" s="37" t="s">
         <v>1313</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>1323</v>
-      </c>
-      <c r="C12" s="6" t="s">
-        <v>1324</v>
-      </c>
-      <c r="E12" s="37" t="s">
-        <v>1325</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="s">
-        <v>1313</v>
+        <v>1301</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>1326</v>
+        <v>1314</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>1327</v>
+        <v>1315</v>
       </c>
       <c r="E13" s="37" t="s">
-        <v>1328</v>
+        <v>1316</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A14" s="5" t="s">
-        <v>1309</v>
+        <v>1297</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>1329</v>
+        <v>1317</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>1330</v>
+        <v>1318</v>
       </c>
       <c r="D14" s="1"/>
       <c r="E14" s="37" t="s">
-        <v>1331</v>
+        <v>1319</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="32" x14ac:dyDescent="0.2">
@@ -8570,14 +8555,14 @@
         <v>952</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>1332</v>
+        <v>1320</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>1333</v>
+        <v>1321</v>
       </c>
       <c r="D15" s="1"/>
       <c r="E15" s="37" t="s">
-        <v>1334</v>
+        <v>1322</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="16" x14ac:dyDescent="0.2">
@@ -8585,34 +8570,34 @@
         <v>14</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>1335</v>
+        <v>1323</v>
       </c>
       <c r="C16" s="74" t="s">
-        <v>1336</v>
+        <v>1324</v>
       </c>
       <c r="D16" s="18"/>
       <c r="E16" s="37" t="s">
-        <v>1337</v>
+        <v>1325</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A17" s="5" t="s">
-        <v>1338</v>
+        <v>1326</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>1339</v>
+        <v>1327</v>
       </c>
       <c r="C17" s="75" t="s">
-        <v>1340</v>
+        <v>1328</v>
       </c>
       <c r="D17" s="18"/>
       <c r="E17" s="37" t="s">
-        <v>1341</v>
+        <v>1329</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="193" t="s">
-        <v>1342</v>
+        <v>1330</v>
       </c>
       <c r="B18" s="194"/>
       <c r="C18" s="194"/>
@@ -8625,16 +8610,16 @@
         <v>243</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>1345</v>
+        <v>1333</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>1343</v>
+        <v>1331</v>
       </c>
       <c r="D19" s="5" t="s">
         <v>1226</v>
       </c>
       <c r="E19" s="37" t="s">
-        <v>1344</v>
+        <v>1332</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="96" x14ac:dyDescent="0.2">
@@ -8642,13 +8627,13 @@
         <v>261</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>1346</v>
+        <v>1334</v>
       </c>
       <c r="C20" s="59" t="s">
-        <v>1416</v>
+        <v>1404</v>
       </c>
       <c r="E20" s="37" t="s">
-        <v>1418</v>
+        <v>1406</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="16" x14ac:dyDescent="0.2">
@@ -8656,13 +8641,13 @@
         <v>254</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>1347</v>
+        <v>1335</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>1301</v>
+        <v>1289</v>
       </c>
       <c r="E21" s="37" t="s">
-        <v>1302</v>
+        <v>1290</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="80" x14ac:dyDescent="0.2">
@@ -8670,13 +8655,13 @@
         <v>261</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>1348</v>
+        <v>1336</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>1417</v>
+        <v>1405</v>
       </c>
       <c r="E22" s="37" t="s">
-        <v>1419</v>
+        <v>1407</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
@@ -8698,9 +8683,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F68"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F3" sqref="F3"/>
+      <selection pane="bottomLeft" activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -8740,13 +8725,13 @@
         <v>7</v>
       </c>
       <c r="C2" s="100" t="s">
-        <v>1441</v>
+        <v>1437</v>
       </c>
       <c r="D2" s="98" t="s">
         <v>8</v>
       </c>
       <c r="E2" s="99" t="s">
-        <v>1441</v>
+        <v>1437</v>
       </c>
       <c r="F2" s="98"/>
     </row>
@@ -8764,7 +8749,7 @@
         <v>12</v>
       </c>
       <c r="E3" s="37" t="s">
-        <v>1415</v>
+        <v>1403</v>
       </c>
       <c r="F3" s="5" t="s">
         <v>13</v>
@@ -9819,18 +9804,18 @@
     </row>
     <row r="67" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="B67" s="1" t="s">
-        <v>1359</v>
+        <v>1347</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>1360</v>
+        <v>1348</v>
       </c>
       <c r="E67" s="40" t="s">
-        <v>1362</v>
+        <v>1350</v>
       </c>
     </row>
     <row r="68" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="B68" s="1" t="s">
-        <v>1361</v>
+        <v>1349</v>
       </c>
       <c r="C68" s="2" t="s">
         <v>76</v>
@@ -10131,14 +10116,14 @@
         <v>243</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>1386</v>
+        <v>1374</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>1387</v>
+        <v>1375</v>
       </c>
       <c r="D2" s="5"/>
       <c r="E2" s="43" t="s">
-        <v>1395</v>
+        <v>1383</v>
       </c>
       <c r="F2" s="1"/>
     </row>
@@ -10147,19 +10132,19 @@
         <v>484</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>1388</v>
+        <v>1376</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>1389</v>
+        <v>1377</v>
       </c>
       <c r="D3" s="5"/>
       <c r="E3" s="43" t="s">
-        <v>1396</v>
+        <v>1384</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="159" t="s">
-        <v>1390</v>
+        <v>1378</v>
       </c>
       <c r="B4" s="160"/>
       <c r="C4" s="160"/>
@@ -10171,14 +10156,14 @@
         <v>243</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>1391</v>
+        <v>1379</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>1393</v>
+        <v>1381</v>
       </c>
       <c r="D5" s="5"/>
       <c r="E5" s="43" t="s">
-        <v>1397</v>
+        <v>1385</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="96" x14ac:dyDescent="0.2">
@@ -10186,14 +10171,14 @@
         <v>484</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>1392</v>
+        <v>1380</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>1394</v>
+        <v>1382</v>
       </c>
       <c r="D6" s="5"/>
       <c r="E6" s="43" t="s">
-        <v>1398</v>
+        <v>1386</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
@@ -10414,7 +10399,7 @@
         <v>243</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>1401</v>
+        <v>1389</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>276</v>
@@ -10438,7 +10423,7 @@
         <v>246</v>
       </c>
       <c r="E4" s="43" t="s">
-        <v>1402</v>
+        <v>1390</v>
       </c>
       <c r="F4" s="68" t="s">
         <v>280</v>
@@ -10452,13 +10437,13 @@
         <v>281</v>
       </c>
       <c r="C5" s="52" t="s">
-        <v>1407</v>
+        <v>1395</v>
       </c>
       <c r="D5" s="66" t="s">
         <v>282</v>
       </c>
       <c r="E5" s="156" t="s">
-        <v>1412</v>
+        <v>1400</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>283</v>
@@ -10472,13 +10457,13 @@
         <v>284</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>1408</v>
+        <v>1396</v>
       </c>
       <c r="D6" s="67" t="s">
         <v>285</v>
       </c>
       <c r="E6" s="157" t="s">
-        <v>1409</v>
+        <v>1397</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="160" x14ac:dyDescent="0.2">
@@ -10489,13 +10474,13 @@
         <v>286</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>1410</v>
+        <v>1398</v>
       </c>
       <c r="D7" s="67" t="s">
         <v>287</v>
       </c>
       <c r="E7" s="157" t="s">
-        <v>1411</v>
+        <v>1399</v>
       </c>
       <c r="F7" s="68" t="s">
         <v>288</v>
@@ -10697,7 +10682,7 @@
         <v>336</v>
       </c>
       <c r="C19" s="64" t="s">
-        <v>1399</v>
+        <v>1387</v>
       </c>
       <c r="D19" s="7" t="s">
         <v>337</v>
@@ -10831,17 +10816,17 @@
     </row>
     <row r="27" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A27" s="5" t="s">
-        <v>1405</v>
+        <v>1393</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>1406</v>
+        <v>1394</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>1403</v>
+        <v>1391</v>
       </c>
       <c r="D27" s="5"/>
       <c r="E27" s="37" t="s">
-        <v>1404</v>
+        <v>1392</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
@@ -10918,13 +10903,13 @@
       </c>
     </row>
     <row r="2" spans="1:6" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="162" t="s">
+      <c r="A2" s="165" t="s">
         <v>367</v>
       </c>
-      <c r="B2" s="163"/>
-      <c r="C2" s="163"/>
-      <c r="D2" s="163"/>
-      <c r="E2" s="164"/>
+      <c r="B2" s="166"/>
+      <c r="C2" s="166"/>
+      <c r="D2" s="166"/>
+      <c r="E2" s="167"/>
       <c r="F2" s="33"/>
     </row>
     <row r="3" spans="1:6" ht="48" x14ac:dyDescent="0.2">
@@ -11052,13 +11037,13 @@
       <c r="F9" s="119"/>
     </row>
     <row r="10" spans="1:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="165" t="s">
+      <c r="A10" s="168" t="s">
         <v>396</v>
       </c>
-      <c r="B10" s="166"/>
-      <c r="C10" s="166"/>
-      <c r="D10" s="166"/>
-      <c r="E10" s="167"/>
+      <c r="B10" s="169"/>
+      <c r="C10" s="169"/>
+      <c r="D10" s="169"/>
+      <c r="E10" s="170"/>
       <c r="F10" s="119"/>
     </row>
     <row r="11" spans="1:6" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -11087,13 +11072,13 @@
         <v>401</v>
       </c>
       <c r="C12" s="153" t="s">
-        <v>1363</v>
+        <v>1351</v>
       </c>
       <c r="D12" s="84" t="s">
         <v>402</v>
       </c>
       <c r="E12" s="152" t="s">
-        <v>1364</v>
+        <v>1352</v>
       </c>
       <c r="F12" s="86"/>
     </row>
@@ -11105,13 +11090,13 @@
         <v>403</v>
       </c>
       <c r="C13" s="154" t="s">
-        <v>1365</v>
+        <v>1353</v>
       </c>
       <c r="D13" s="88" t="s">
         <v>404</v>
       </c>
       <c r="E13" s="155" t="s">
-        <v>1366</v>
+        <v>1354</v>
       </c>
       <c r="F13" s="86"/>
     </row>
@@ -11579,7 +11564,7 @@
         <v>485</v>
       </c>
       <c r="C45" s="59" t="s">
-        <v>1382</v>
+        <v>1370</v>
       </c>
       <c r="D45" s="116"/>
       <c r="E45" s="120" t="s">
@@ -11592,14 +11577,14 @@
         <v>484</v>
       </c>
       <c r="B46" s="116" t="s">
-        <v>1385</v>
+        <v>1373</v>
       </c>
       <c r="C46" s="59" t="s">
-        <v>1383</v>
+        <v>1371</v>
       </c>
       <c r="D46" s="116"/>
       <c r="E46" s="120" t="s">
-        <v>1384</v>
+        <v>1372</v>
       </c>
       <c r="F46" s="119"/>
     </row>
@@ -11827,7 +11812,7 @@
         <v>522</v>
       </c>
       <c r="E61" s="120" t="s">
-        <v>1375</v>
+        <v>1363</v>
       </c>
       <c r="F61" s="119"/>
     </row>
@@ -11836,14 +11821,14 @@
         <v>519</v>
       </c>
       <c r="B62" s="116" t="s">
-        <v>1372</v>
+        <v>1360</v>
       </c>
       <c r="C62" s="117" t="s">
-        <v>1374</v>
+        <v>1362</v>
       </c>
       <c r="D62" s="116"/>
       <c r="E62" s="120" t="s">
-        <v>1373</v>
+        <v>1361</v>
       </c>
       <c r="F62" s="119"/>
     </row>
@@ -12177,11 +12162,11 @@
         <v>572</v>
       </c>
       <c r="C84" s="117" t="s">
-        <v>1427</v>
+        <v>1415</v>
       </c>
       <c r="D84" s="116"/>
       <c r="E84" s="120" t="s">
-        <v>1428</v>
+        <v>1416</v>
       </c>
       <c r="F84" s="119" t="s">
         <v>575</v>
@@ -12291,11 +12276,11 @@
         <v>593</v>
       </c>
       <c r="C91" s="117" t="s">
-        <v>1425</v>
+        <v>1413</v>
       </c>
       <c r="D91" s="116"/>
       <c r="E91" s="120" t="s">
-        <v>1426</v>
+        <v>1414</v>
       </c>
       <c r="F91" s="119"/>
     </row>
@@ -13029,7 +13014,7 @@
         <v>710</v>
       </c>
       <c r="C141" s="113" t="s">
-        <v>1350</v>
+        <v>1338</v>
       </c>
       <c r="D141" s="122" t="s">
         <v>711</v>
@@ -13119,7 +13104,7 @@
         <v>725</v>
       </c>
       <c r="C147" s="59" t="s">
-        <v>1349</v>
+        <v>1337</v>
       </c>
       <c r="D147" s="116" t="s">
         <v>726</v>
@@ -13150,14 +13135,14 @@
         <v>37</v>
       </c>
       <c r="B149" s="116" t="s">
-        <v>1351</v>
+        <v>1339</v>
       </c>
       <c r="C149" s="59" t="s">
-        <v>1353</v>
+        <v>1341</v>
       </c>
       <c r="D149" s="116"/>
       <c r="E149" s="120" t="s">
-        <v>1355</v>
+        <v>1343</v>
       </c>
       <c r="F149" s="119"/>
     </row>
@@ -13166,14 +13151,14 @@
         <v>37</v>
       </c>
       <c r="B150" s="116" t="s">
-        <v>1352</v>
+        <v>1340</v>
       </c>
       <c r="C150" s="59" t="s">
-        <v>1354</v>
+        <v>1342</v>
       </c>
       <c r="D150" s="116"/>
       <c r="E150" s="120" t="s">
-        <v>1356</v>
+        <v>1344</v>
       </c>
       <c r="F150" s="119"/>
     </row>
@@ -13392,13 +13377,13 @@
       <c r="F164" s="119"/>
     </row>
     <row r="165" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A165" s="168" t="s">
+      <c r="A165" s="162" t="s">
         <v>765</v>
       </c>
-      <c r="B165" s="169"/>
-      <c r="C165" s="169"/>
-      <c r="D165" s="169"/>
-      <c r="E165" s="170"/>
+      <c r="B165" s="163"/>
+      <c r="C165" s="163"/>
+      <c r="D165" s="163"/>
+      <c r="E165" s="164"/>
       <c r="F165" s="129" t="s">
         <v>766</v>
       </c>
@@ -13825,13 +13810,13 @@
         <v>815</v>
       </c>
       <c r="C193" s="59" t="s">
-        <v>1367</v>
+        <v>1355</v>
       </c>
       <c r="D193" s="116" t="s">
         <v>816</v>
       </c>
       <c r="E193" s="120" t="s">
-        <v>1371</v>
+        <v>1359</v>
       </c>
       <c r="F193" s="119"/>
     </row>
@@ -13840,14 +13825,14 @@
         <v>484</v>
       </c>
       <c r="B194" s="116" t="s">
-        <v>1368</v>
+        <v>1356</v>
       </c>
       <c r="C194" s="59" t="s">
-        <v>1369</v>
+        <v>1357</v>
       </c>
       <c r="D194" s="116"/>
       <c r="E194" s="120" t="s">
-        <v>1370</v>
+        <v>1358</v>
       </c>
       <c r="F194" s="119"/>
     </row>
@@ -13947,11 +13932,11 @@
         <v>827</v>
       </c>
       <c r="C201" s="117" t="s">
-        <v>1378</v>
+        <v>1366</v>
       </c>
       <c r="D201" s="116"/>
       <c r="E201" s="120" t="s">
-        <v>1381</v>
+        <v>1369</v>
       </c>
       <c r="F201" s="119"/>
     </row>
@@ -13960,7 +13945,7 @@
         <v>734</v>
       </c>
       <c r="B202" s="116" t="s">
-        <v>1380</v>
+        <v>1368</v>
       </c>
       <c r="C202" s="117" t="s">
         <v>43</v>
@@ -13976,14 +13961,14 @@
         <v>32</v>
       </c>
       <c r="B203" s="116" t="s">
-        <v>1379</v>
+        <v>1367</v>
       </c>
       <c r="C203" s="134" t="s">
-        <v>1376</v>
+        <v>1364</v>
       </c>
       <c r="D203" s="116"/>
       <c r="E203" s="120" t="s">
-        <v>1377</v>
+        <v>1365</v>
       </c>
       <c r="F203" s="119"/>
     </row>
@@ -14355,13 +14340,13 @@
         <v>866</v>
       </c>
       <c r="C228" s="59" t="s">
-        <v>1413</v>
+        <v>1401</v>
       </c>
       <c r="D228" s="116" t="s">
         <v>867</v>
       </c>
       <c r="E228" s="120" t="s">
-        <v>1414</v>
+        <v>1402</v>
       </c>
       <c r="F228" s="119"/>
     </row>
@@ -15301,6 +15286,18 @@
     </row>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="A225:E225"/>
+    <mergeCell ref="A186:E186"/>
+    <mergeCell ref="A190:E190"/>
+    <mergeCell ref="A197:E197"/>
+    <mergeCell ref="A208:E208"/>
+    <mergeCell ref="A214:E214"/>
+    <mergeCell ref="A58:E58"/>
+    <mergeCell ref="A2:E2"/>
+    <mergeCell ref="A10:E10"/>
+    <mergeCell ref="A14:E14"/>
+    <mergeCell ref="A24:E24"/>
+    <mergeCell ref="A43:E43"/>
     <mergeCell ref="A174:E174"/>
     <mergeCell ref="A157:E157"/>
     <mergeCell ref="A63:E63"/>
@@ -15311,18 +15308,6 @@
     <mergeCell ref="A146:E146"/>
     <mergeCell ref="A92:E92"/>
     <mergeCell ref="A165:E165"/>
-    <mergeCell ref="A58:E58"/>
-    <mergeCell ref="A2:E2"/>
-    <mergeCell ref="A10:E10"/>
-    <mergeCell ref="A14:E14"/>
-    <mergeCell ref="A24:E24"/>
-    <mergeCell ref="A43:E43"/>
-    <mergeCell ref="A225:E225"/>
-    <mergeCell ref="A186:E186"/>
-    <mergeCell ref="A190:E190"/>
-    <mergeCell ref="A197:E197"/>
-    <mergeCell ref="A208:E208"/>
-    <mergeCell ref="A214:E214"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -15593,13 +15578,13 @@
         <v>942</v>
       </c>
       <c r="C17" s="151" t="s">
-        <v>1357</v>
+        <v>1345</v>
       </c>
       <c r="D17" s="92" t="s">
         <v>934</v>
       </c>
       <c r="E17" s="152" t="s">
-        <v>1358</v>
+        <v>1346</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="80" x14ac:dyDescent="0.2">
@@ -15799,10 +15784,10 @@
         <v>982</v>
       </c>
       <c r="C32" s="21" t="s">
-        <v>1420</v>
+        <v>1408</v>
       </c>
       <c r="E32" s="46" t="s">
-        <v>1421</v>
+        <v>1409</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="32" x14ac:dyDescent="0.2">
@@ -15810,13 +15795,13 @@
         <v>261</v>
       </c>
       <c r="B33" s="19" t="s">
-        <v>1422</v>
+        <v>1410</v>
       </c>
       <c r="C33" s="21" t="s">
-        <v>1423</v>
+        <v>1411</v>
       </c>
       <c r="E33" s="46" t="s">
-        <v>1424</v>
+        <v>1412</v>
       </c>
     </row>
     <row r="34" spans="1:6" ht="48" x14ac:dyDescent="0.2">
@@ -15976,13 +15961,13 @@
         <v>1007</v>
       </c>
       <c r="C45" s="62" t="s">
-        <v>1413</v>
+        <v>1401</v>
       </c>
       <c r="D45" s="116" t="s">
         <v>1008</v>
       </c>
       <c r="E45" s="46" t="s">
-        <v>1414</v>
+        <v>1402</v>
       </c>
     </row>
     <row r="46" spans="1:6" ht="48" x14ac:dyDescent="0.2">
@@ -16171,7 +16156,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6CA2FE89-1BCA-4888-9BB6-D7A7737E07E4}">
   <dimension ref="A1:F75"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D28" sqref="D28"/>
     </sheetView>
@@ -16375,23 +16360,23 @@
         <v>1074</v>
       </c>
       <c r="E11" s="138" t="s">
-        <v>1440</v>
+        <v>1428</v>
       </c>
       <c r="F11" s="135"/>
     </row>
     <row r="12" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A12" s="136" t="s">
-        <v>1434</v>
+        <v>1422</v>
       </c>
       <c r="B12" s="136" t="s">
-        <v>1435</v>
+        <v>1423</v>
       </c>
       <c r="C12" s="137" t="s">
-        <v>1438</v>
+        <v>1426</v>
       </c>
       <c r="D12" s="136"/>
       <c r="E12" s="138" t="s">
-        <v>1439</v>
+        <v>1427</v>
       </c>
       <c r="F12" s="135"/>
     </row>
@@ -16403,7 +16388,7 @@
         <v>1075</v>
       </c>
       <c r="C13" s="137" t="s">
-        <v>1432</v>
+        <v>1420</v>
       </c>
       <c r="D13" s="136" t="s">
         <v>1076</v>
@@ -16449,7 +16434,7 @@
         <v>1081</v>
       </c>
       <c r="C16" s="137" t="s">
-        <v>1429</v>
+        <v>1417</v>
       </c>
       <c r="D16" s="136" t="s">
         <v>1082</v>
@@ -16467,7 +16452,7 @@
         <v>1084</v>
       </c>
       <c r="C17" s="137" t="s">
-        <v>1430</v>
+        <v>1418</v>
       </c>
       <c r="D17" s="136" t="s">
         <v>1085</v>
@@ -16485,7 +16470,7 @@
         <v>1087</v>
       </c>
       <c r="C18" s="137" t="s">
-        <v>1431</v>
+        <v>1419</v>
       </c>
       <c r="D18" s="136" t="s">
         <v>1088</v>
@@ -16625,17 +16610,17 @@
     </row>
     <row r="28" spans="1:6" ht="64" x14ac:dyDescent="0.2">
       <c r="A28" s="136" t="s">
-        <v>1434</v>
+        <v>1422</v>
       </c>
       <c r="B28" s="136" t="s">
-        <v>1433</v>
+        <v>1421</v>
       </c>
       <c r="C28" s="137" t="s">
-        <v>1436</v>
+        <v>1424</v>
       </c>
       <c r="D28" s="136"/>
       <c r="E28" s="138" t="s">
-        <v>1437</v>
+        <v>1425</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="32" x14ac:dyDescent="0.2">
@@ -16646,13 +16631,13 @@
         <v>1113</v>
       </c>
       <c r="C29" s="137" t="s">
-        <v>1442</v>
+        <v>1429</v>
       </c>
       <c r="D29" s="136" t="s">
         <v>1114</v>
       </c>
       <c r="E29" s="138" t="s">
-        <v>1443</v>
+        <v>1430</v>
       </c>
     </row>
     <row r="30" spans="1:6" s="13" customFormat="1" x14ac:dyDescent="0.2">
@@ -16895,7 +16880,7 @@
         <v>1151</v>
       </c>
       <c r="C45" s="62" t="s">
-        <v>1400</v>
+        <v>1388</v>
       </c>
       <c r="D45" s="5" t="s">
         <v>1152</v>
@@ -16987,13 +16972,13 @@
         <v>1163</v>
       </c>
       <c r="C51" s="62" t="s">
-        <v>1413</v>
+        <v>1401</v>
       </c>
       <c r="D51" s="116" t="s">
         <v>1008</v>
       </c>
       <c r="E51" s="63" t="s">
-        <v>1414</v>
+        <v>1402</v>
       </c>
     </row>
     <row r="52" spans="1:6" s="30" customFormat="1" ht="48" x14ac:dyDescent="0.2">
@@ -17356,6 +17341,47 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Readyforteam_x003f_ xmlns="565e1b1d-057e-4d85-b896-01a5881d8a45">false</Readyforteam_x003f_>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <SharedWithUsers xmlns="bf601f31-63a1-4825-9216-91d773c5ef9c">
+      <UserInfo>
+        <DisplayName>Erika Osti</DisplayName>
+        <AccountId>534</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Penny Johnson</DisplayName>
+        <AccountId>489</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Ben Childs</DisplayName>
+        <AccountId>643</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Thomas Leeds</DisplayName>
+        <AccountId>459</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Kasmyn Chen</DisplayName>
+        <AccountId>532</AccountId>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="565e1b1d-057e-4d85-b896-01a5881d8a45">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="2799d30d-6731-4efe-ac9b-c4895a8828d9" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010096D84A54A9CD274097F17166F184737D" ma:contentTypeVersion="21" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="2fd95a4cfdf4f2f51219070f5dff16a8">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="565e1b1d-057e-4d85-b896-01a5881d8a45" xmlns:ns3="bf601f31-63a1-4825-9216-91d773c5ef9c" xmlns:ns4="2799d30d-6731-4efe-ac9b-c4895a8828d9" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f7499f6f4dc8ad2a533df04863f63fa7" ns1:_="" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -17632,47 +17658,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Readyforteam_x003f_ xmlns="565e1b1d-057e-4d85-b896-01a5881d8a45">false</Readyforteam_x003f_>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <SharedWithUsers xmlns="bf601f31-63a1-4825-9216-91d773c5ef9c">
-      <UserInfo>
-        <DisplayName>Erika Osti</DisplayName>
-        <AccountId>534</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Penny Johnson</DisplayName>
-        <AccountId>489</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Ben Childs</DisplayName>
-        <AccountId>643</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Thomas Leeds</DisplayName>
-        <AccountId>459</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Kasmyn Chen</DisplayName>
-        <AccountId>532</AccountId>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="565e1b1d-057e-4d85-b896-01a5881d8a45">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="2799d30d-6731-4efe-ac9b-c4895a8828d9" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8D7CE8C7-18DC-484F-8376-ED09F13D44C8}">
   <ds:schemaRefs>
@@ -17682,6 +17667,19 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{017ACE96-8143-486E-8436-7787F6B96F4A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="565e1b1d-057e-4d85-b896-01a5881d8a45"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="bf601f31-63a1-4825-9216-91d773c5ef9c"/>
+    <ds:schemaRef ds:uri="2799d30d-6731-4efe-ac9b-c4895a8828d9"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EAFDB110-4046-4E72-A1EF-1908ABEC3151}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -17700,17 +17698,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{017ACE96-8143-486E-8436-7787F6B96F4A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="565e1b1d-057e-4d85-b896-01a5881d8a45"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="bf601f31-63a1-4825-9216-91d773c5ef9c"/>
-    <ds:schemaRef ds:uri="2799d30d-6731-4efe-ac9b-c4895a8828d9"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
[MCCDB-896] Content amend - the 'Give feedback' page
</commit_message>
<xml_diff>
--- a/app/data/MCCD-localisation.xlsx
+++ b/app/data/MCCD-localisation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/JALAT/GIT/medical-certificate-of-cause-of-death/app/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95FF176C-F8DC-4941-B908-49560ABB8BBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{155B98D3-B1BB-B84F-8622-8FBC099890A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="14100" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -5254,12 +5254,6 @@
     <t>confirmationPageGiveFeedbackQuestionOne</t>
   </si>
   <si>
-    <t>Overall, how did you feel about using our service today?</t>
-  </si>
-  <si>
-    <t>Yn gyffredinol, sut oeddech chi'n teimlo am ddefnyddio ein gwasanaeth heddiw?</t>
-  </si>
-  <si>
     <t>Radio</t>
   </si>
   <si>
@@ -5309,12 +5303,6 @@
   </si>
   <si>
     <t>confirmationPageGiveFeedbackQuestionTwo</t>
-  </si>
-  <si>
-    <t>How can we improve this service?</t>
-  </si>
-  <si>
-    <t>Sut gallwn ni wella'r gwasanaeth hwn?</t>
   </si>
   <si>
     <t>confirmationPageGiveFeedbackQuestionTwoHint</t>
@@ -5689,7 +5677,19 @@
     <t>Dewiswch ethnigrwydd yr ymadawedig gan ei fod wedi'i gofnodi ar y cofnod cleifion. Os nad oes unrhyw gyd-fynd â'r rhestr, neu os nad oes unrhyw ethnigrwydd yn cael ei gofnodi ar y cofnod claf, dewiswch 'heb ei nodi'.</t>
   </si>
   <si>
-    <t>026</t>
+    <t>How could we improve this service?</t>
+  </si>
+  <si>
+    <t>Sut allwn ni wella'r gwasanaeth hwn?</t>
+  </si>
+  <si>
+    <t>Overall, how did you feel about using our service?</t>
+  </si>
+  <si>
+    <t>Ar y cyfan, sut oeddech chi'n teimlo am ddefnyddio ein gwasanaeth?</t>
+  </si>
+  <si>
+    <t>028</t>
   </si>
 </sst>
 </file>
@@ -6645,6 +6645,24 @@
     <xf numFmtId="0" fontId="13" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -6652,24 +6670,6 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -7894,7 +7894,7 @@
   <dimension ref="A1:F24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
@@ -7937,13 +7937,13 @@
         <v>1241</v>
       </c>
       <c r="C2" s="151" t="s">
-        <v>1428</v>
+        <v>1424</v>
       </c>
       <c r="D2" s="92" t="s">
         <v>1242</v>
       </c>
       <c r="E2" s="152" t="s">
-        <v>1432</v>
+        <v>1428</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="80" x14ac:dyDescent="0.2">
@@ -7971,13 +7971,13 @@
         <v>1248</v>
       </c>
       <c r="C4" s="158" t="s">
-        <v>1429</v>
+        <v>1425</v>
       </c>
       <c r="D4" s="95" t="s">
         <v>404</v>
       </c>
       <c r="E4" s="155" t="s">
-        <v>1431</v>
+        <v>1427</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="60.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -8039,13 +8039,13 @@
         <v>1253</v>
       </c>
       <c r="C8" s="158" t="s">
-        <v>1428</v>
+        <v>1424</v>
       </c>
       <c r="D8" s="95" t="s">
         <v>1254</v>
       </c>
       <c r="E8" s="155" t="s">
-        <v>1432</v>
+        <v>1428</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="64" x14ac:dyDescent="0.2">
@@ -8073,13 +8073,13 @@
         <v>1259</v>
       </c>
       <c r="C10" s="158" t="s">
-        <v>1429</v>
+        <v>1425</v>
       </c>
       <c r="D10" s="95" t="s">
         <v>404</v>
       </c>
       <c r="E10" s="155" t="s">
-        <v>1431</v>
+        <v>1427</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -8141,13 +8141,13 @@
         <v>1262</v>
       </c>
       <c r="C14" s="158" t="s">
-        <v>1428</v>
+        <v>1424</v>
       </c>
       <c r="D14" s="95" t="s">
         <v>1263</v>
       </c>
       <c r="E14" s="155" t="s">
-        <v>1430</v>
+        <v>1426</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="96" x14ac:dyDescent="0.2">
@@ -8209,13 +8209,13 @@
         <v>1270</v>
       </c>
       <c r="C18" s="158" t="s">
-        <v>1429</v>
+        <v>1425</v>
       </c>
       <c r="D18" s="95" t="s">
         <v>404</v>
       </c>
       <c r="E18" s="155" t="s">
-        <v>1431</v>
+        <v>1427</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -8243,13 +8243,13 @@
         <v>1271</v>
       </c>
       <c r="C20" s="158" t="s">
-        <v>1428</v>
+        <v>1424</v>
       </c>
       <c r="D20" s="95" t="s">
         <v>1242</v>
       </c>
       <c r="E20" s="155" t="s">
-        <v>1430</v>
+        <v>1426</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="48" x14ac:dyDescent="0.2">
@@ -8277,13 +8277,13 @@
         <v>1275</v>
       </c>
       <c r="C22" s="158" t="s">
-        <v>1429</v>
+        <v>1425</v>
       </c>
       <c r="D22" s="95" t="s">
         <v>404</v>
       </c>
       <c r="E22" s="155" t="s">
-        <v>1433</v>
+        <v>1429</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="48" x14ac:dyDescent="0.2">
@@ -8330,8 +8330,8 @@
   <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D22" sqref="D22"/>
+      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -8448,7 +8448,7 @@
         <v>1293</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
         <v>1294</v>
       </c>
@@ -8456,80 +8456,80 @@
         <v>1295</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>1296</v>
+        <v>1434</v>
       </c>
       <c r="E8" s="37" t="s">
-        <v>1297</v>
+        <v>1435</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
+        <v>1296</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>1297</v>
+      </c>
+      <c r="C9" s="6" t="s">
         <v>1298</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="E9" s="37" t="s">
         <v>1299</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>1300</v>
-      </c>
-      <c r="E9" s="37" t="s">
-        <v>1301</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
-        <v>1298</v>
+        <v>1296</v>
       </c>
       <c r="B10" s="5" t="s">
+        <v>1300</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>1301</v>
+      </c>
+      <c r="E10" s="37" t="s">
         <v>1302</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>1303</v>
-      </c>
-      <c r="E10" s="37" t="s">
-        <v>1304</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
-        <v>1298</v>
+        <v>1296</v>
       </c>
       <c r="B11" s="5" t="s">
+        <v>1303</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>1304</v>
+      </c>
+      <c r="E11" s="37" t="s">
         <v>1305</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>1306</v>
-      </c>
-      <c r="E11" s="37" t="s">
-        <v>1307</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="5" t="s">
-        <v>1298</v>
+        <v>1296</v>
       </c>
       <c r="B12" s="5" t="s">
+        <v>1306</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>1307</v>
+      </c>
+      <c r="E12" s="37" t="s">
         <v>1308</v>
-      </c>
-      <c r="C12" s="6" t="s">
-        <v>1309</v>
-      </c>
-      <c r="E12" s="37" t="s">
-        <v>1310</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="s">
-        <v>1298</v>
+        <v>1296</v>
       </c>
       <c r="B13" s="5" t="s">
+        <v>1309</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>1310</v>
+      </c>
+      <c r="E13" s="37" t="s">
         <v>1311</v>
-      </c>
-      <c r="C13" s="6" t="s">
-        <v>1312</v>
-      </c>
-      <c r="E13" s="37" t="s">
-        <v>1313</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="32" x14ac:dyDescent="0.2">
@@ -8537,14 +8537,14 @@
         <v>1294</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>1314</v>
+        <v>1312</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>1315</v>
+        <v>1432</v>
       </c>
       <c r="D14" s="1"/>
       <c r="E14" s="37" t="s">
-        <v>1316</v>
+        <v>1433</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="32" x14ac:dyDescent="0.2">
@@ -8552,14 +8552,14 @@
         <v>949</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>1317</v>
+        <v>1313</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>1318</v>
+        <v>1314</v>
       </c>
       <c r="D15" s="1"/>
       <c r="E15" s="37" t="s">
-        <v>1319</v>
+        <v>1315</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="16" x14ac:dyDescent="0.2">
@@ -8567,34 +8567,34 @@
         <v>14</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>1320</v>
+        <v>1316</v>
       </c>
       <c r="C16" s="74" t="s">
-        <v>1321</v>
+        <v>1317</v>
       </c>
       <c r="D16" s="18"/>
       <c r="E16" s="37" t="s">
-        <v>1322</v>
+        <v>1318</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A17" s="5" t="s">
-        <v>1323</v>
+        <v>1319</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>1324</v>
+        <v>1320</v>
       </c>
       <c r="C17" s="75" t="s">
-        <v>1325</v>
+        <v>1321</v>
       </c>
       <c r="D17" s="18"/>
       <c r="E17" s="37" t="s">
-        <v>1326</v>
+        <v>1322</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="194" t="s">
-        <v>1327</v>
+        <v>1323</v>
       </c>
       <c r="B18" s="195"/>
       <c r="C18" s="195"/>
@@ -8607,16 +8607,16 @@
         <v>243</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>1330</v>
+        <v>1326</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>1328</v>
+        <v>1324</v>
       </c>
       <c r="D19" s="5" t="s">
         <v>1223</v>
       </c>
       <c r="E19" s="37" t="s">
-        <v>1329</v>
+        <v>1325</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="96" x14ac:dyDescent="0.2">
@@ -8624,13 +8624,13 @@
         <v>261</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>1331</v>
+        <v>1327</v>
       </c>
       <c r="C20" s="59" t="s">
-        <v>1401</v>
+        <v>1397</v>
       </c>
       <c r="E20" s="37" t="s">
-        <v>1403</v>
+        <v>1399</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="16" x14ac:dyDescent="0.2">
@@ -8638,7 +8638,7 @@
         <v>254</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>1332</v>
+        <v>1328</v>
       </c>
       <c r="C21" s="6" t="s">
         <v>1286</v>
@@ -8652,13 +8652,13 @@
         <v>261</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>1333</v>
+        <v>1329</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>1402</v>
+        <v>1398</v>
       </c>
       <c r="E22" s="37" t="s">
-        <v>1404</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
@@ -8682,7 +8682,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E3" sqref="E3"/>
+      <selection pane="bottomLeft" activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -8746,7 +8746,7 @@
         <v>12</v>
       </c>
       <c r="E3" s="37" t="s">
-        <v>1400</v>
+        <v>1396</v>
       </c>
       <c r="F3" s="5" t="s">
         <v>13</v>
@@ -9801,18 +9801,18 @@
     </row>
     <row r="67" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="B67" s="1" t="s">
-        <v>1344</v>
+        <v>1340</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>1345</v>
+        <v>1341</v>
       </c>
       <c r="E67" s="40" t="s">
-        <v>1347</v>
+        <v>1343</v>
       </c>
     </row>
     <row r="68" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="B68" s="1" t="s">
-        <v>1346</v>
+        <v>1342</v>
       </c>
       <c r="C68" s="2" t="s">
         <v>76</v>
@@ -10113,14 +10113,14 @@
         <v>243</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>1371</v>
+        <v>1367</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>1372</v>
+        <v>1368</v>
       </c>
       <c r="D2" s="5"/>
       <c r="E2" s="43" t="s">
-        <v>1380</v>
+        <v>1376</v>
       </c>
       <c r="F2" s="1"/>
     </row>
@@ -10129,19 +10129,19 @@
         <v>484</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>1373</v>
+        <v>1369</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>1374</v>
+        <v>1370</v>
       </c>
       <c r="D3" s="5"/>
       <c r="E3" s="43" t="s">
-        <v>1381</v>
+        <v>1377</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="160" t="s">
-        <v>1375</v>
+        <v>1371</v>
       </c>
       <c r="B4" s="161"/>
       <c r="C4" s="161"/>
@@ -10153,14 +10153,14 @@
         <v>243</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>1376</v>
+        <v>1372</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>1378</v>
+        <v>1374</v>
       </c>
       <c r="D5" s="5"/>
       <c r="E5" s="43" t="s">
-        <v>1382</v>
+        <v>1378</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="96" x14ac:dyDescent="0.2">
@@ -10168,14 +10168,14 @@
         <v>484</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>1377</v>
+        <v>1373</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>1379</v>
+        <v>1375</v>
       </c>
       <c r="D6" s="5"/>
       <c r="E6" s="43" t="s">
-        <v>1383</v>
+        <v>1379</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
@@ -10396,7 +10396,7 @@
         <v>243</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>1386</v>
+        <v>1382</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>276</v>
@@ -10420,7 +10420,7 @@
         <v>246</v>
       </c>
       <c r="E4" s="43" t="s">
-        <v>1387</v>
+        <v>1383</v>
       </c>
       <c r="F4" s="68" t="s">
         <v>280</v>
@@ -10434,13 +10434,13 @@
         <v>281</v>
       </c>
       <c r="C5" s="52" t="s">
-        <v>1392</v>
+        <v>1388</v>
       </c>
       <c r="D5" s="66" t="s">
         <v>282</v>
       </c>
       <c r="E5" s="156" t="s">
-        <v>1397</v>
+        <v>1393</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>283</v>
@@ -10454,13 +10454,13 @@
         <v>284</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>1393</v>
+        <v>1389</v>
       </c>
       <c r="D6" s="67" t="s">
         <v>285</v>
       </c>
       <c r="E6" s="157" t="s">
-        <v>1394</v>
+        <v>1390</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="160" x14ac:dyDescent="0.2">
@@ -10471,13 +10471,13 @@
         <v>286</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>1395</v>
+        <v>1391</v>
       </c>
       <c r="D7" s="67" t="s">
         <v>287</v>
       </c>
       <c r="E7" s="157" t="s">
-        <v>1396</v>
+        <v>1392</v>
       </c>
       <c r="F7" s="68" t="s">
         <v>288</v>
@@ -10679,7 +10679,7 @@
         <v>336</v>
       </c>
       <c r="C19" s="64" t="s">
-        <v>1384</v>
+        <v>1380</v>
       </c>
       <c r="D19" s="7" t="s">
         <v>337</v>
@@ -10813,17 +10813,17 @@
     </row>
     <row r="27" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A27" s="5" t="s">
-        <v>1390</v>
+        <v>1386</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>1391</v>
+        <v>1387</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>1388</v>
+        <v>1384</v>
       </c>
       <c r="D27" s="5"/>
       <c r="E27" s="37" t="s">
-        <v>1389</v>
+        <v>1385</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
@@ -10900,13 +10900,13 @@
       </c>
     </row>
     <row r="2" spans="1:6" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="166" t="s">
+      <c r="A2" s="163" t="s">
         <v>367</v>
       </c>
-      <c r="B2" s="167"/>
-      <c r="C2" s="167"/>
-      <c r="D2" s="167"/>
-      <c r="E2" s="168"/>
+      <c r="B2" s="164"/>
+      <c r="C2" s="164"/>
+      <c r="D2" s="164"/>
+      <c r="E2" s="165"/>
       <c r="F2" s="33"/>
     </row>
     <row r="3" spans="1:6" ht="48" x14ac:dyDescent="0.2">
@@ -11034,13 +11034,13 @@
       <c r="F9" s="119"/>
     </row>
     <row r="10" spans="1:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="169" t="s">
+      <c r="A10" s="166" t="s">
         <v>396</v>
       </c>
-      <c r="B10" s="170"/>
-      <c r="C10" s="170"/>
-      <c r="D10" s="170"/>
-      <c r="E10" s="171"/>
+      <c r="B10" s="167"/>
+      <c r="C10" s="167"/>
+      <c r="D10" s="167"/>
+      <c r="E10" s="168"/>
       <c r="F10" s="119"/>
     </row>
     <row r="11" spans="1:6" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -11069,13 +11069,13 @@
         <v>401</v>
       </c>
       <c r="C12" s="153" t="s">
-        <v>1348</v>
+        <v>1344</v>
       </c>
       <c r="D12" s="84" t="s">
         <v>402</v>
       </c>
       <c r="E12" s="152" t="s">
-        <v>1349</v>
+        <v>1345</v>
       </c>
       <c r="F12" s="86"/>
     </row>
@@ -11087,13 +11087,13 @@
         <v>403</v>
       </c>
       <c r="C13" s="154" t="s">
-        <v>1350</v>
+        <v>1346</v>
       </c>
       <c r="D13" s="88" t="s">
         <v>404</v>
       </c>
       <c r="E13" s="155" t="s">
-        <v>1351</v>
+        <v>1347</v>
       </c>
       <c r="F13" s="86"/>
     </row>
@@ -11561,7 +11561,7 @@
         <v>485</v>
       </c>
       <c r="C45" s="59" t="s">
-        <v>1367</v>
+        <v>1363</v>
       </c>
       <c r="D45" s="116"/>
       <c r="E45" s="120" t="s">
@@ -11574,14 +11574,14 @@
         <v>484</v>
       </c>
       <c r="B46" s="116" t="s">
-        <v>1370</v>
+        <v>1366</v>
       </c>
       <c r="C46" s="59" t="s">
-        <v>1368</v>
+        <v>1364</v>
       </c>
       <c r="D46" s="116"/>
       <c r="E46" s="120" t="s">
-        <v>1369</v>
+        <v>1365</v>
       </c>
       <c r="F46" s="119"/>
     </row>
@@ -11809,7 +11809,7 @@
         <v>522</v>
       </c>
       <c r="E61" s="120" t="s">
-        <v>1360</v>
+        <v>1356</v>
       </c>
       <c r="F61" s="119"/>
     </row>
@@ -11818,14 +11818,14 @@
         <v>519</v>
       </c>
       <c r="B62" s="116" t="s">
-        <v>1357</v>
+        <v>1353</v>
       </c>
       <c r="C62" s="117" t="s">
-        <v>1359</v>
+        <v>1355</v>
       </c>
       <c r="D62" s="116"/>
       <c r="E62" s="120" t="s">
-        <v>1358</v>
+        <v>1354</v>
       </c>
       <c r="F62" s="119"/>
     </row>
@@ -12159,11 +12159,11 @@
         <v>572</v>
       </c>
       <c r="C84" s="117" t="s">
-        <v>1412</v>
+        <v>1408</v>
       </c>
       <c r="D84" s="116"/>
       <c r="E84" s="120" t="s">
-        <v>1413</v>
+        <v>1409</v>
       </c>
       <c r="F84" s="119" t="s">
         <v>573</v>
@@ -12273,11 +12273,11 @@
         <v>591</v>
       </c>
       <c r="C91" s="117" t="s">
-        <v>1410</v>
+        <v>1406</v>
       </c>
       <c r="D91" s="116"/>
       <c r="E91" s="120" t="s">
-        <v>1411</v>
+        <v>1407</v>
       </c>
       <c r="F91" s="119"/>
     </row>
@@ -12317,11 +12317,11 @@
         <v>597</v>
       </c>
       <c r="C94" s="117" t="s">
-        <v>1434</v>
+        <v>1430</v>
       </c>
       <c r="D94" s="116"/>
       <c r="E94" s="120" t="s">
-        <v>1435</v>
+        <v>1431</v>
       </c>
       <c r="F94" s="119" t="s">
         <v>573</v>
@@ -13011,7 +13011,7 @@
         <v>707</v>
       </c>
       <c r="C141" s="113" t="s">
-        <v>1335</v>
+        <v>1331</v>
       </c>
       <c r="D141" s="122" t="s">
         <v>708</v>
@@ -13101,7 +13101,7 @@
         <v>722</v>
       </c>
       <c r="C147" s="59" t="s">
-        <v>1334</v>
+        <v>1330</v>
       </c>
       <c r="D147" s="116" t="s">
         <v>723</v>
@@ -13132,14 +13132,14 @@
         <v>37</v>
       </c>
       <c r="B149" s="116" t="s">
-        <v>1336</v>
+        <v>1332</v>
       </c>
       <c r="C149" s="59" t="s">
-        <v>1338</v>
+        <v>1334</v>
       </c>
       <c r="D149" s="116"/>
       <c r="E149" s="120" t="s">
-        <v>1340</v>
+        <v>1336</v>
       </c>
       <c r="F149" s="119"/>
     </row>
@@ -13148,14 +13148,14 @@
         <v>37</v>
       </c>
       <c r="B150" s="116" t="s">
-        <v>1337</v>
+        <v>1333</v>
       </c>
       <c r="C150" s="59" t="s">
-        <v>1339</v>
+        <v>1335</v>
       </c>
       <c r="D150" s="116"/>
       <c r="E150" s="120" t="s">
-        <v>1341</v>
+        <v>1337</v>
       </c>
       <c r="F150" s="119"/>
     </row>
@@ -13374,13 +13374,13 @@
       <c r="F164" s="119"/>
     </row>
     <row r="165" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A165" s="163" t="s">
+      <c r="A165" s="169" t="s">
         <v>762</v>
       </c>
-      <c r="B165" s="164"/>
-      <c r="C165" s="164"/>
-      <c r="D165" s="164"/>
-      <c r="E165" s="165"/>
+      <c r="B165" s="170"/>
+      <c r="C165" s="170"/>
+      <c r="D165" s="170"/>
+      <c r="E165" s="171"/>
       <c r="F165" s="129" t="s">
         <v>763</v>
       </c>
@@ -13807,13 +13807,13 @@
         <v>812</v>
       </c>
       <c r="C193" s="59" t="s">
-        <v>1352</v>
+        <v>1348</v>
       </c>
       <c r="D193" s="116" t="s">
         <v>813</v>
       </c>
       <c r="E193" s="120" t="s">
-        <v>1356</v>
+        <v>1352</v>
       </c>
       <c r="F193" s="119"/>
     </row>
@@ -13822,14 +13822,14 @@
         <v>484</v>
       </c>
       <c r="B194" s="116" t="s">
-        <v>1353</v>
+        <v>1349</v>
       </c>
       <c r="C194" s="59" t="s">
-        <v>1354</v>
+        <v>1350</v>
       </c>
       <c r="D194" s="116"/>
       <c r="E194" s="120" t="s">
-        <v>1355</v>
+        <v>1351</v>
       </c>
       <c r="F194" s="119"/>
     </row>
@@ -13929,11 +13929,11 @@
         <v>824</v>
       </c>
       <c r="C201" s="117" t="s">
-        <v>1363</v>
+        <v>1359</v>
       </c>
       <c r="D201" s="116"/>
       <c r="E201" s="120" t="s">
-        <v>1366</v>
+        <v>1362</v>
       </c>
       <c r="F201" s="119"/>
     </row>
@@ -13942,7 +13942,7 @@
         <v>731</v>
       </c>
       <c r="B202" s="116" t="s">
-        <v>1365</v>
+        <v>1361</v>
       </c>
       <c r="C202" s="117" t="s">
         <v>43</v>
@@ -13958,14 +13958,14 @@
         <v>32</v>
       </c>
       <c r="B203" s="116" t="s">
-        <v>1364</v>
+        <v>1360</v>
       </c>
       <c r="C203" s="134" t="s">
-        <v>1361</v>
+        <v>1357</v>
       </c>
       <c r="D203" s="116"/>
       <c r="E203" s="120" t="s">
-        <v>1362</v>
+        <v>1358</v>
       </c>
       <c r="F203" s="119"/>
     </row>
@@ -14337,13 +14337,13 @@
         <v>863</v>
       </c>
       <c r="C228" s="59" t="s">
-        <v>1398</v>
+        <v>1394</v>
       </c>
       <c r="D228" s="116" t="s">
         <v>864</v>
       </c>
       <c r="E228" s="120" t="s">
-        <v>1399</v>
+        <v>1395</v>
       </c>
       <c r="F228" s="119"/>
     </row>
@@ -15283,18 +15283,6 @@
     </row>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="A225:E225"/>
-    <mergeCell ref="A186:E186"/>
-    <mergeCell ref="A190:E190"/>
-    <mergeCell ref="A197:E197"/>
-    <mergeCell ref="A208:E208"/>
-    <mergeCell ref="A214:E214"/>
-    <mergeCell ref="A58:E58"/>
-    <mergeCell ref="A2:E2"/>
-    <mergeCell ref="A10:E10"/>
-    <mergeCell ref="A14:E14"/>
-    <mergeCell ref="A24:E24"/>
-    <mergeCell ref="A43:E43"/>
     <mergeCell ref="A174:E174"/>
     <mergeCell ref="A157:E157"/>
     <mergeCell ref="A63:E63"/>
@@ -15305,6 +15293,18 @@
     <mergeCell ref="A146:E146"/>
     <mergeCell ref="A92:E92"/>
     <mergeCell ref="A165:E165"/>
+    <mergeCell ref="A58:E58"/>
+    <mergeCell ref="A2:E2"/>
+    <mergeCell ref="A10:E10"/>
+    <mergeCell ref="A14:E14"/>
+    <mergeCell ref="A24:E24"/>
+    <mergeCell ref="A43:E43"/>
+    <mergeCell ref="A225:E225"/>
+    <mergeCell ref="A186:E186"/>
+    <mergeCell ref="A190:E190"/>
+    <mergeCell ref="A197:E197"/>
+    <mergeCell ref="A208:E208"/>
+    <mergeCell ref="A214:E214"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -15575,13 +15575,13 @@
         <v>939</v>
       </c>
       <c r="C17" s="151" t="s">
-        <v>1342</v>
+        <v>1338</v>
       </c>
       <c r="D17" s="92" t="s">
         <v>931</v>
       </c>
       <c r="E17" s="152" t="s">
-        <v>1343</v>
+        <v>1339</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="80" x14ac:dyDescent="0.2">
@@ -15781,10 +15781,10 @@
         <v>979</v>
       </c>
       <c r="C32" s="21" t="s">
-        <v>1405</v>
+        <v>1401</v>
       </c>
       <c r="E32" s="46" t="s">
-        <v>1406</v>
+        <v>1402</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="32" x14ac:dyDescent="0.2">
@@ -15792,13 +15792,13 @@
         <v>261</v>
       </c>
       <c r="B33" s="19" t="s">
-        <v>1407</v>
+        <v>1403</v>
       </c>
       <c r="C33" s="21" t="s">
-        <v>1408</v>
+        <v>1404</v>
       </c>
       <c r="E33" s="46" t="s">
-        <v>1409</v>
+        <v>1405</v>
       </c>
     </row>
     <row r="34" spans="1:6" ht="48" x14ac:dyDescent="0.2">
@@ -15958,13 +15958,13 @@
         <v>1004</v>
       </c>
       <c r="C45" s="62" t="s">
-        <v>1398</v>
+        <v>1394</v>
       </c>
       <c r="D45" s="116" t="s">
         <v>1005</v>
       </c>
       <c r="E45" s="46" t="s">
-        <v>1399</v>
+        <v>1395</v>
       </c>
     </row>
     <row r="46" spans="1:6" ht="48" x14ac:dyDescent="0.2">
@@ -16357,23 +16357,23 @@
         <v>1071</v>
       </c>
       <c r="E11" s="138" t="s">
-        <v>1425</v>
+        <v>1421</v>
       </c>
       <c r="F11" s="135"/>
     </row>
     <row r="12" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A12" s="136" t="s">
+        <v>1415</v>
+      </c>
+      <c r="B12" s="136" t="s">
+        <v>1416</v>
+      </c>
+      <c r="C12" s="137" t="s">
         <v>1419</v>
-      </c>
-      <c r="B12" s="136" t="s">
-        <v>1420</v>
-      </c>
-      <c r="C12" s="137" t="s">
-        <v>1423</v>
       </c>
       <c r="D12" s="136"/>
       <c r="E12" s="138" t="s">
-        <v>1424</v>
+        <v>1420</v>
       </c>
       <c r="F12" s="135"/>
     </row>
@@ -16385,7 +16385,7 @@
         <v>1072</v>
       </c>
       <c r="C13" s="137" t="s">
-        <v>1417</v>
+        <v>1413</v>
       </c>
       <c r="D13" s="136" t="s">
         <v>1073</v>
@@ -16431,7 +16431,7 @@
         <v>1078</v>
       </c>
       <c r="C16" s="137" t="s">
-        <v>1414</v>
+        <v>1410</v>
       </c>
       <c r="D16" s="136" t="s">
         <v>1079</v>
@@ -16449,7 +16449,7 @@
         <v>1081</v>
       </c>
       <c r="C17" s="137" t="s">
-        <v>1415</v>
+        <v>1411</v>
       </c>
       <c r="D17" s="136" t="s">
         <v>1082</v>
@@ -16467,7 +16467,7 @@
         <v>1084</v>
       </c>
       <c r="C18" s="137" t="s">
-        <v>1416</v>
+        <v>1412</v>
       </c>
       <c r="D18" s="136" t="s">
         <v>1085</v>
@@ -16607,17 +16607,17 @@
     </row>
     <row r="28" spans="1:6" ht="64" x14ac:dyDescent="0.2">
       <c r="A28" s="136" t="s">
-        <v>1419</v>
+        <v>1415</v>
       </c>
       <c r="B28" s="136" t="s">
-        <v>1418</v>
+        <v>1414</v>
       </c>
       <c r="C28" s="137" t="s">
-        <v>1421</v>
+        <v>1417</v>
       </c>
       <c r="D28" s="136"/>
       <c r="E28" s="138" t="s">
-        <v>1422</v>
+        <v>1418</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="32" x14ac:dyDescent="0.2">
@@ -16628,13 +16628,13 @@
         <v>1110</v>
       </c>
       <c r="C29" s="137" t="s">
-        <v>1426</v>
+        <v>1422</v>
       </c>
       <c r="D29" s="136" t="s">
         <v>1111</v>
       </c>
       <c r="E29" s="138" t="s">
-        <v>1427</v>
+        <v>1423</v>
       </c>
     </row>
     <row r="30" spans="1:6" s="13" customFormat="1" x14ac:dyDescent="0.2">
@@ -16877,7 +16877,7 @@
         <v>1148</v>
       </c>
       <c r="C45" s="62" t="s">
-        <v>1385</v>
+        <v>1381</v>
       </c>
       <c r="D45" s="5" t="s">
         <v>1149</v>
@@ -16969,13 +16969,13 @@
         <v>1160</v>
       </c>
       <c r="C51" s="62" t="s">
-        <v>1398</v>
+        <v>1394</v>
       </c>
       <c r="D51" s="116" t="s">
         <v>1005</v>
       </c>
       <c r="E51" s="63" t="s">
-        <v>1399</v>
+        <v>1395</v>
       </c>
     </row>
     <row r="52" spans="1:6" s="30" customFormat="1" ht="48" x14ac:dyDescent="0.2">
@@ -17606,15 +17606,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <Readyforteam_x003f_ xmlns="565e1b1d-057e-4d85-b896-01a5881d8a45">false</Readyforteam_x003f_>
@@ -17655,6 +17646,15 @@
 </p:properties>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EAFDB110-4046-4E72-A1EF-1908ABEC3151}">
   <ds:schemaRefs>
@@ -17677,14 +17677,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8D7CE8C7-18DC-484F-8376-ED09F13D44C8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{017ACE96-8143-486E-8436-7787F6B96F4A}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -17695,4 +17687,12 @@
     <ds:schemaRef ds:uri="2799d30d-6731-4efe-ac9b-c4895a8828d9"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8D7CE8C7-18DC-484F-8376-ED09F13D44C8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Adding an alternative version of the ethnicity question(s).
</commit_message>
<xml_diff>
--- a/app/data/MCCD-localisation.xlsx
+++ b/app/data/MCCD-localisation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/JALAT/GIT/medical-certificate-of-cause-of-death/app/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{155B98D3-B1BB-B84F-8622-8FBC099890A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63986951-DC2E-5843-9F26-6D07FE7486F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="14100" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -69,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2148" uniqueCount="1437">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2170" uniqueCount="1442">
   <si>
     <r>
       <rPr>
@@ -5689,7 +5689,22 @@
     <t>Ar y cyfan, sut oeddech chi'n teimlo am ddefnyddio ein gwasanaeth?</t>
   </si>
   <si>
-    <t>028</t>
+    <t>dpdEthnicityNotStatedWhite</t>
+  </si>
+  <si>
+    <t>dpdEthnicityNotStatedMixed</t>
+  </si>
+  <si>
+    <t>dpdEthnicityNotStatedAsian</t>
+  </si>
+  <si>
+    <t>dpdEthnicityNotStatedBlack</t>
+  </si>
+  <si>
+    <t>dpdEthnicityNotStatedOther</t>
+  </si>
+  <si>
+    <t>029</t>
   </si>
 </sst>
 </file>
@@ -6165,7 +6180,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="196">
+  <cellXfs count="200">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -6645,6 +6660,15 @@
     <xf numFmtId="0" fontId="13" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -6663,15 +6687,6 @@
     <xf numFmtId="0" fontId="13" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
@@ -6743,6 +6758,18 @@
     </xf>
     <xf numFmtId="0" fontId="13" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -8682,7 +8709,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F2" sqref="F2"/>
+      <selection pane="bottomLeft" activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -8722,13 +8749,13 @@
         <v>7</v>
       </c>
       <c r="C2" s="100" t="s">
-        <v>1436</v>
+        <v>1441</v>
       </c>
       <c r="D2" s="98" t="s">
         <v>8</v>
       </c>
       <c r="E2" s="99" t="s">
-        <v>1436</v>
+        <v>1441</v>
       </c>
       <c r="F2" s="98"/>
     </row>
@@ -10861,11 +10888,11 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B63483B8-55BE-4CA0-9111-55E5C0AEF6CB}">
-  <dimension ref="A1:F345"/>
+  <dimension ref="A1:F350"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A90" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D94" sqref="D94"/>
+      <pane ySplit="1" topLeftCell="A55" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C100" sqref="C100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -10900,13 +10927,13 @@
       </c>
     </row>
     <row r="2" spans="1:6" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="163" t="s">
+      <c r="A2" s="166" t="s">
         <v>367</v>
       </c>
-      <c r="B2" s="164"/>
-      <c r="C2" s="164"/>
-      <c r="D2" s="164"/>
-      <c r="E2" s="165"/>
+      <c r="B2" s="167"/>
+      <c r="C2" s="167"/>
+      <c r="D2" s="167"/>
+      <c r="E2" s="168"/>
       <c r="F2" s="33"/>
     </row>
     <row r="3" spans="1:6" ht="48" x14ac:dyDescent="0.2">
@@ -11034,13 +11061,13 @@
       <c r="F9" s="119"/>
     </row>
     <row r="10" spans="1:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="166" t="s">
+      <c r="A10" s="169" t="s">
         <v>396</v>
       </c>
-      <c r="B10" s="167"/>
-      <c r="C10" s="167"/>
-      <c r="D10" s="167"/>
-      <c r="E10" s="168"/>
+      <c r="B10" s="170"/>
+      <c r="C10" s="170"/>
+      <c r="D10" s="170"/>
+      <c r="E10" s="171"/>
       <c r="F10" s="119"/>
     </row>
     <row r="11" spans="1:6" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -12347,119 +12374,123 @@
         <v>600</v>
       </c>
     </row>
-    <row r="96" spans="1:6" ht="48" x14ac:dyDescent="0.2">
-      <c r="A96" s="116" t="s">
+    <row r="96" spans="1:6" ht="62.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A96" s="91" t="s">
         <v>84</v>
       </c>
-      <c r="B96" s="116" t="s">
-        <v>601</v>
-      </c>
-      <c r="C96" s="117" t="s">
-        <v>602</v>
-      </c>
-      <c r="D96" s="116" t="s">
-        <v>603</v>
-      </c>
-      <c r="E96" s="120" t="s">
-        <v>604</v>
-      </c>
-      <c r="F96" s="119"/>
-    </row>
-    <row r="97" spans="1:6" ht="32" x14ac:dyDescent="0.2">
-      <c r="A97" s="116" t="s">
+      <c r="B96" s="196" t="s">
+        <v>1436</v>
+      </c>
+      <c r="C96" s="93" t="s">
+        <v>599</v>
+      </c>
+      <c r="D96" s="92" t="s">
+        <v>404</v>
+      </c>
+      <c r="E96" s="152" t="s">
+        <v>1218</v>
+      </c>
+      <c r="F96" s="86"/>
+    </row>
+    <row r="97" spans="1:6" ht="62.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A97" s="91" t="s">
         <v>84</v>
       </c>
-      <c r="B97" s="116" t="s">
-        <v>605</v>
-      </c>
-      <c r="C97" s="117" t="s">
-        <v>606</v>
-      </c>
-      <c r="D97" s="116" t="s">
-        <v>607</v>
-      </c>
-      <c r="E97" s="120" t="s">
-        <v>608</v>
-      </c>
-      <c r="F97" s="119"/>
-    </row>
-    <row r="98" spans="1:6" ht="48" x14ac:dyDescent="0.2">
-      <c r="A98" s="116" t="s">
+      <c r="B97" s="196" t="s">
+        <v>1437</v>
+      </c>
+      <c r="C97" s="93" t="s">
+        <v>599</v>
+      </c>
+      <c r="D97" s="92" t="s">
+        <v>404</v>
+      </c>
+      <c r="E97" s="152" t="s">
+        <v>1218</v>
+      </c>
+      <c r="F97" s="86"/>
+    </row>
+    <row r="98" spans="1:6" ht="62.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A98" s="20" t="s">
         <v>84</v>
       </c>
-      <c r="B98" s="116" t="s">
-        <v>609</v>
-      </c>
-      <c r="C98" s="61" t="s">
-        <v>610</v>
-      </c>
-      <c r="D98" s="116" t="s">
-        <v>611</v>
-      </c>
-      <c r="E98" s="120" t="s">
-        <v>612</v>
-      </c>
-      <c r="F98" s="119"/>
-    </row>
-    <row r="99" spans="1:6" ht="48" x14ac:dyDescent="0.2">
-      <c r="A99" s="116" t="s">
+      <c r="B98" s="197" t="s">
+        <v>1438</v>
+      </c>
+      <c r="C98" s="198" t="s">
+        <v>599</v>
+      </c>
+      <c r="D98" s="197"/>
+      <c r="E98" s="199" t="s">
+        <v>1218</v>
+      </c>
+      <c r="F98" s="86"/>
+    </row>
+    <row r="99" spans="1:6" ht="62.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A99" s="20" t="s">
         <v>84</v>
       </c>
-      <c r="B99" s="116" t="s">
-        <v>613</v>
-      </c>
-      <c r="C99" s="117" t="s">
-        <v>614</v>
-      </c>
-      <c r="D99" s="116" t="s">
-        <v>615</v>
-      </c>
-      <c r="E99" s="120" t="s">
-        <v>616</v>
-      </c>
-      <c r="F99" s="119"/>
-    </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A100" s="116"/>
-      <c r="B100" s="116"/>
-      <c r="C100" s="117"/>
-      <c r="D100" s="116"/>
-      <c r="E100" s="120"/>
-      <c r="F100" s="119"/>
+      <c r="B99" s="197" t="s">
+        <v>1439</v>
+      </c>
+      <c r="C99" s="198" t="s">
+        <v>599</v>
+      </c>
+      <c r="D99" s="197"/>
+      <c r="E99" s="199" t="s">
+        <v>1218</v>
+      </c>
+      <c r="F99" s="86"/>
+    </row>
+    <row r="100" spans="1:6" ht="62.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A100" s="20" t="s">
+        <v>84</v>
+      </c>
+      <c r="B100" s="197" t="s">
+        <v>1440</v>
+      </c>
+      <c r="C100" s="198" t="s">
+        <v>599</v>
+      </c>
+      <c r="D100" s="197"/>
+      <c r="E100" s="199" t="s">
+        <v>1218</v>
+      </c>
+      <c r="F100" s="86"/>
     </row>
     <row r="101" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A101" s="116" t="s">
         <v>84</v>
       </c>
       <c r="B101" s="116" t="s">
-        <v>617</v>
+        <v>601</v>
       </c>
       <c r="C101" s="117" t="s">
-        <v>618</v>
+        <v>602</v>
       </c>
       <c r="D101" s="116" t="s">
-        <v>619</v>
+        <v>603</v>
       </c>
       <c r="E101" s="120" t="s">
-        <v>620</v>
+        <v>604</v>
       </c>
       <c r="F101" s="119"/>
     </row>
-    <row r="102" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A102" s="116" t="s">
         <v>84</v>
       </c>
       <c r="B102" s="116" t="s">
-        <v>621</v>
+        <v>605</v>
       </c>
       <c r="C102" s="117" t="s">
-        <v>622</v>
+        <v>606</v>
       </c>
       <c r="D102" s="116" t="s">
-        <v>623</v>
+        <v>607</v>
       </c>
       <c r="E102" s="120" t="s">
-        <v>624</v>
+        <v>608</v>
       </c>
       <c r="F102" s="119"/>
     </row>
@@ -12468,16 +12499,16 @@
         <v>84</v>
       </c>
       <c r="B103" s="116" t="s">
-        <v>625</v>
-      </c>
-      <c r="C103" s="117" t="s">
-        <v>626</v>
+        <v>609</v>
+      </c>
+      <c r="C103" s="61" t="s">
+        <v>610</v>
       </c>
       <c r="D103" s="116" t="s">
-        <v>627</v>
+        <v>611</v>
       </c>
       <c r="E103" s="120" t="s">
-        <v>628</v>
+        <v>612</v>
       </c>
       <c r="F103" s="119"/>
     </row>
@@ -12486,16 +12517,16 @@
         <v>84</v>
       </c>
       <c r="B104" s="116" t="s">
-        <v>629</v>
+        <v>613</v>
       </c>
       <c r="C104" s="117" t="s">
-        <v>630</v>
+        <v>614</v>
       </c>
       <c r="D104" s="116" t="s">
-        <v>631</v>
+        <v>615</v>
       </c>
       <c r="E104" s="120" t="s">
-        <v>632</v>
+        <v>616</v>
       </c>
       <c r="F104" s="119"/>
     </row>
@@ -12507,111 +12538,119 @@
       <c r="E105" s="120"/>
       <c r="F105" s="119"/>
     </row>
-    <row r="106" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A106" s="116" t="s">
         <v>84</v>
       </c>
       <c r="B106" s="116" t="s">
-        <v>633</v>
+        <v>617</v>
       </c>
       <c r="C106" s="117" t="s">
-        <v>634</v>
+        <v>618</v>
       </c>
       <c r="D106" s="116" t="s">
-        <v>635</v>
+        <v>619</v>
       </c>
       <c r="E106" s="120" t="s">
-        <v>636</v>
+        <v>620</v>
       </c>
       <c r="F106" s="119"/>
     </row>
-    <row r="107" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A107" s="116" t="s">
         <v>84</v>
       </c>
       <c r="B107" s="116" t="s">
-        <v>637</v>
+        <v>621</v>
       </c>
       <c r="C107" s="117" t="s">
-        <v>638</v>
+        <v>622</v>
       </c>
       <c r="D107" s="116" t="s">
-        <v>639</v>
+        <v>623</v>
       </c>
       <c r="E107" s="120" t="s">
-        <v>640</v>
+        <v>624</v>
       </c>
       <c r="F107" s="119"/>
     </row>
-    <row r="108" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A108" s="116" t="s">
         <v>84</v>
       </c>
       <c r="B108" s="116" t="s">
-        <v>641</v>
+        <v>625</v>
       </c>
       <c r="C108" s="117" t="s">
-        <v>642</v>
+        <v>626</v>
       </c>
       <c r="D108" s="116" t="s">
-        <v>643</v>
+        <v>627</v>
       </c>
       <c r="E108" s="120" t="s">
-        <v>644</v>
+        <v>628</v>
       </c>
       <c r="F108" s="119"/>
     </row>
-    <row r="109" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A109" s="116" t="s">
         <v>84</v>
       </c>
       <c r="B109" s="116" t="s">
-        <v>645</v>
+        <v>629</v>
       </c>
       <c r="C109" s="117" t="s">
-        <v>646</v>
+        <v>630</v>
       </c>
       <c r="D109" s="116" t="s">
-        <v>647</v>
+        <v>631</v>
       </c>
       <c r="E109" s="120" t="s">
-        <v>648</v>
+        <v>632</v>
       </c>
       <c r="F109" s="119"/>
     </row>
-    <row r="110" spans="1:6" ht="48" x14ac:dyDescent="0.2">
-      <c r="A110" s="116" t="s">
+    <row r="110" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A110" s="116"/>
+      <c r="B110" s="116"/>
+      <c r="C110" s="117"/>
+      <c r="D110" s="116"/>
+      <c r="E110" s="120"/>
+      <c r="F110" s="119"/>
+    </row>
+    <row r="111" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+      <c r="A111" s="116" t="s">
         <v>84</v>
       </c>
-      <c r="B110" s="116" t="s">
-        <v>649</v>
-      </c>
-      <c r="C110" s="117" t="s">
-        <v>650</v>
-      </c>
-      <c r="D110" s="116" t="s">
-        <v>651</v>
-      </c>
-      <c r="E110" s="120" t="s">
-        <v>652</v>
-      </c>
-      <c r="F110" s="119"/>
+      <c r="B111" s="116" t="s">
+        <v>633</v>
+      </c>
+      <c r="C111" s="117" t="s">
+        <v>634</v>
+      </c>
+      <c r="D111" s="116" t="s">
+        <v>635</v>
+      </c>
+      <c r="E111" s="120" t="s">
+        <v>636</v>
+      </c>
+      <c r="F111" s="119"/>
     </row>
     <row r="112" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A112" s="116" t="s">
         <v>84</v>
       </c>
       <c r="B112" s="116" t="s">
-        <v>653</v>
+        <v>637</v>
       </c>
       <c r="C112" s="117" t="s">
-        <v>654</v>
+        <v>638</v>
       </c>
       <c r="D112" s="116" t="s">
-        <v>655</v>
+        <v>639</v>
       </c>
       <c r="E112" s="120" t="s">
-        <v>656</v>
+        <v>640</v>
       </c>
       <c r="F112" s="119"/>
     </row>
@@ -12620,860 +12659,852 @@
         <v>84</v>
       </c>
       <c r="B113" s="116" t="s">
-        <v>657</v>
+        <v>641</v>
       </c>
       <c r="C113" s="117" t="s">
-        <v>658</v>
+        <v>642</v>
       </c>
       <c r="D113" s="116" t="s">
-        <v>659</v>
+        <v>643</v>
       </c>
       <c r="E113" s="120" t="s">
-        <v>660</v>
+        <v>644</v>
       </c>
       <c r="F113" s="119"/>
     </row>
-    <row r="114" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A114" s="116" t="s">
         <v>84</v>
       </c>
       <c r="B114" s="116" t="s">
-        <v>661</v>
+        <v>645</v>
       </c>
       <c r="C114" s="117" t="s">
-        <v>662</v>
+        <v>646</v>
       </c>
       <c r="D114" s="116" t="s">
-        <v>663</v>
+        <v>647</v>
       </c>
       <c r="E114" s="120" t="s">
-        <v>664</v>
+        <v>648</v>
       </c>
       <c r="F114" s="119"/>
     </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A115" s="116"/>
-      <c r="B115" s="116"/>
-      <c r="C115" s="117"/>
-      <c r="D115" s="116"/>
-      <c r="E115" s="120"/>
+    <row r="115" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+      <c r="A115" s="116" t="s">
+        <v>84</v>
+      </c>
+      <c r="B115" s="116" t="s">
+        <v>649</v>
+      </c>
+      <c r="C115" s="117" t="s">
+        <v>650</v>
+      </c>
+      <c r="D115" s="116" t="s">
+        <v>651</v>
+      </c>
+      <c r="E115" s="120" t="s">
+        <v>652</v>
+      </c>
       <c r="F115" s="119"/>
     </row>
-    <row r="116" spans="1:6" ht="32" x14ac:dyDescent="0.2">
-      <c r="A116" s="116" t="s">
-        <v>84</v>
-      </c>
-      <c r="B116" s="116" t="s">
-        <v>665</v>
-      </c>
-      <c r="C116" s="117" t="s">
-        <v>666</v>
-      </c>
-      <c r="D116" s="116" t="s">
-        <v>667</v>
-      </c>
-      <c r="E116" s="120" t="s">
-        <v>668</v>
-      </c>
-      <c r="F116" s="119"/>
-    </row>
-    <row r="117" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A117" s="116" t="s">
         <v>84</v>
       </c>
       <c r="B117" s="116" t="s">
-        <v>669</v>
+        <v>653</v>
       </c>
       <c r="C117" s="117" t="s">
-        <v>670</v>
+        <v>654</v>
       </c>
       <c r="D117" s="116" t="s">
-        <v>671</v>
+        <v>655</v>
       </c>
       <c r="E117" s="120" t="s">
-        <v>672</v>
+        <v>656</v>
       </c>
       <c r="F117" s="119"/>
     </row>
-    <row r="118" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A118" s="116"/>
-      <c r="B118" s="116"/>
-      <c r="C118" s="117"/>
-      <c r="D118" s="116"/>
-      <c r="E118" s="120"/>
+    <row r="118" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+      <c r="A118" s="116" t="s">
+        <v>84</v>
+      </c>
+      <c r="B118" s="116" t="s">
+        <v>657</v>
+      </c>
+      <c r="C118" s="117" t="s">
+        <v>658</v>
+      </c>
+      <c r="D118" s="116" t="s">
+        <v>659</v>
+      </c>
+      <c r="E118" s="120" t="s">
+        <v>660</v>
+      </c>
       <c r="F118" s="119"/>
     </row>
-    <row r="119" spans="1:6" ht="80" x14ac:dyDescent="0.2">
-      <c r="A119" s="120"/>
-      <c r="B119" s="120"/>
-      <c r="C119" s="120"/>
+    <row r="119" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+      <c r="A119" s="116" t="s">
+        <v>84</v>
+      </c>
+      <c r="B119" s="116" t="s">
+        <v>661</v>
+      </c>
+      <c r="C119" s="117" t="s">
+        <v>662</v>
+      </c>
       <c r="D119" s="116" t="s">
-        <v>673</v>
-      </c>
-      <c r="E119" s="120"/>
-      <c r="F119" s="119" t="s">
-        <v>674</v>
-      </c>
-    </row>
-    <row r="120" spans="1:6" ht="80" x14ac:dyDescent="0.2">
-      <c r="A120" s="120"/>
-      <c r="B120" s="120"/>
-      <c r="C120" s="120"/>
-      <c r="D120" s="116" t="s">
-        <v>675</v>
-      </c>
+        <v>663</v>
+      </c>
+      <c r="E119" s="120" t="s">
+        <v>664</v>
+      </c>
+      <c r="F119" s="119"/>
+    </row>
+    <row r="120" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A120" s="116"/>
+      <c r="B120" s="116"/>
+      <c r="C120" s="117"/>
+      <c r="D120" s="116"/>
       <c r="E120" s="120"/>
       <c r="F120" s="119"/>
     </row>
-    <row r="121" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A121" s="116" t="s">
+        <v>84</v>
+      </c>
+      <c r="B121" s="116" t="s">
+        <v>665</v>
+      </c>
+      <c r="C121" s="117" t="s">
+        <v>666</v>
+      </c>
+      <c r="D121" s="116" t="s">
+        <v>667</v>
+      </c>
+      <c r="E121" s="120" t="s">
+        <v>668</v>
+      </c>
+      <c r="F121" s="119"/>
+    </row>
+    <row r="122" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+      <c r="A122" s="116" t="s">
+        <v>84</v>
+      </c>
+      <c r="B122" s="116" t="s">
+        <v>669</v>
+      </c>
+      <c r="C122" s="117" t="s">
+        <v>670</v>
+      </c>
+      <c r="D122" s="116" t="s">
+        <v>671</v>
+      </c>
+      <c r="E122" s="120" t="s">
+        <v>672</v>
+      </c>
+      <c r="F122" s="119"/>
+    </row>
+    <row r="123" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A123" s="116"/>
+      <c r="B123" s="116"/>
+      <c r="C123" s="117"/>
+      <c r="D123" s="116"/>
+      <c r="E123" s="120"/>
+      <c r="F123" s="119"/>
+    </row>
+    <row r="124" spans="1:6" ht="80" x14ac:dyDescent="0.2">
+      <c r="A124" s="120"/>
+      <c r="B124" s="120"/>
+      <c r="C124" s="120"/>
+      <c r="D124" s="116" t="s">
+        <v>673</v>
+      </c>
+      <c r="E124" s="120"/>
+      <c r="F124" s="119" t="s">
+        <v>674</v>
+      </c>
+    </row>
+    <row r="125" spans="1:6" ht="80" x14ac:dyDescent="0.2">
+      <c r="A125" s="120"/>
+      <c r="B125" s="120"/>
+      <c r="C125" s="120"/>
+      <c r="D125" s="116" t="s">
+        <v>675</v>
+      </c>
+      <c r="E125" s="120"/>
+      <c r="F125" s="119"/>
+    </row>
+    <row r="126" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+      <c r="A126" s="116" t="s">
         <v>410</v>
       </c>
-      <c r="B121" s="116" t="s">
+      <c r="B126" s="116" t="s">
         <v>676</v>
       </c>
-      <c r="C121" s="120"/>
-      <c r="D121" s="20" t="s">
+      <c r="C126" s="120"/>
+      <c r="D126" s="20" t="s">
         <v>412</v>
       </c>
-      <c r="E121" s="120"/>
-      <c r="F121" s="119"/>
-    </row>
-    <row r="122" spans="1:6" ht="64" x14ac:dyDescent="0.2">
-      <c r="A122" s="116" t="s">
-        <v>413</v>
-      </c>
-      <c r="B122" s="116" t="s">
-        <v>677</v>
-      </c>
-      <c r="C122" s="120"/>
-      <c r="D122" s="20" t="s">
-        <v>415</v>
-      </c>
-      <c r="E122" s="120"/>
-      <c r="F122" s="119"/>
-    </row>
-    <row r="123" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A123" s="160" t="s">
-        <v>678</v>
-      </c>
-      <c r="B123" s="161"/>
-      <c r="C123" s="161"/>
-      <c r="D123" s="161"/>
-      <c r="E123" s="162"/>
-      <c r="F123" s="119"/>
-    </row>
-    <row r="124" spans="1:6" ht="32" x14ac:dyDescent="0.2">
-      <c r="A124" s="116" t="s">
-        <v>243</v>
-      </c>
-      <c r="B124" s="116" t="s">
-        <v>679</v>
-      </c>
-      <c r="C124" s="117" t="s">
-        <v>680</v>
-      </c>
-      <c r="D124" s="116" t="s">
-        <v>681</v>
-      </c>
-      <c r="E124" s="120" t="s">
-        <v>682</v>
-      </c>
-      <c r="F124" s="119"/>
-    </row>
-    <row r="125" spans="1:6" ht="80" x14ac:dyDescent="0.2">
-      <c r="A125" s="116" t="s">
-        <v>484</v>
-      </c>
-      <c r="B125" s="116" t="s">
-        <v>683</v>
-      </c>
-      <c r="C125" s="117" t="s">
-        <v>684</v>
-      </c>
-      <c r="D125" s="116" t="s">
-        <v>685</v>
-      </c>
-      <c r="E125" s="120" t="s">
-        <v>686</v>
-      </c>
-      <c r="F125" s="119"/>
-    </row>
-    <row r="126" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A126" s="116"/>
-      <c r="B126" s="116"/>
-      <c r="C126" s="117"/>
-      <c r="D126" s="116"/>
       <c r="E126" s="120"/>
       <c r="F126" s="119"/>
     </row>
-    <row r="127" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:6" ht="64" x14ac:dyDescent="0.2">
       <c r="A127" s="116" t="s">
-        <v>416</v>
+        <v>413</v>
       </c>
       <c r="B127" s="116" t="s">
-        <v>687</v>
-      </c>
-      <c r="C127" s="59" t="s">
-        <v>156</v>
-      </c>
-      <c r="D127" s="116"/>
-      <c r="E127" s="120" t="s">
-        <v>158</v>
-      </c>
+        <v>677</v>
+      </c>
+      <c r="C127" s="120"/>
+      <c r="D127" s="20" t="s">
+        <v>415</v>
+      </c>
+      <c r="E127" s="120"/>
       <c r="F127" s="119"/>
     </row>
-    <row r="128" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A128" s="116" t="s">
-        <v>416</v>
-      </c>
-      <c r="B128" s="116" t="s">
-        <v>688</v>
-      </c>
-      <c r="C128" s="59" t="s">
-        <v>160</v>
-      </c>
-      <c r="D128" s="116"/>
-      <c r="E128" s="120" t="s">
-        <v>162</v>
-      </c>
+    <row r="128" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A128" s="160" t="s">
+        <v>678</v>
+      </c>
+      <c r="B128" s="161"/>
+      <c r="C128" s="161"/>
+      <c r="D128" s="161"/>
+      <c r="E128" s="162"/>
       <c r="F128" s="119"/>
     </row>
-    <row r="129" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A129" s="116" t="s">
-        <v>416</v>
+        <v>243</v>
       </c>
       <c r="B129" s="116" t="s">
-        <v>689</v>
-      </c>
-      <c r="C129" s="59" t="s">
-        <v>164</v>
-      </c>
-      <c r="D129" s="116"/>
+        <v>679</v>
+      </c>
+      <c r="C129" s="117" t="s">
+        <v>680</v>
+      </c>
+      <c r="D129" s="116" t="s">
+        <v>681</v>
+      </c>
       <c r="E129" s="120" t="s">
-        <v>166</v>
+        <v>682</v>
       </c>
       <c r="F129" s="119"/>
     </row>
-    <row r="130" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A130" s="116"/>
-      <c r="B130" s="116"/>
-      <c r="C130" s="117"/>
-      <c r="D130" s="116"/>
-      <c r="E130" s="120"/>
+    <row r="130" spans="1:6" ht="80" x14ac:dyDescent="0.2">
+      <c r="A130" s="116" t="s">
+        <v>484</v>
+      </c>
+      <c r="B130" s="116" t="s">
+        <v>683</v>
+      </c>
+      <c r="C130" s="117" t="s">
+        <v>684</v>
+      </c>
+      <c r="D130" s="116" t="s">
+        <v>685</v>
+      </c>
+      <c r="E130" s="120" t="s">
+        <v>686</v>
+      </c>
       <c r="F130" s="119"/>
     </row>
-    <row r="131" spans="1:6" ht="64" x14ac:dyDescent="0.2">
-      <c r="A131" s="116" t="s">
-        <v>410</v>
-      </c>
-      <c r="B131" s="116" t="s">
-        <v>690</v>
-      </c>
-      <c r="C131" s="120"/>
-      <c r="D131" s="20" t="s">
-        <v>691</v>
-      </c>
+    <row r="131" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A131" s="116"/>
+      <c r="B131" s="116"/>
+      <c r="C131" s="117"/>
+      <c r="D131" s="116"/>
       <c r="E131" s="120"/>
       <c r="F131" s="119"/>
     </row>
-    <row r="132" spans="1:6" ht="80" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A132" s="116" t="s">
-        <v>413</v>
+        <v>416</v>
       </c>
       <c r="B132" s="116" t="s">
-        <v>692</v>
-      </c>
-      <c r="C132" s="120"/>
-      <c r="D132" s="20" t="s">
-        <v>693</v>
-      </c>
-      <c r="E132" s="120"/>
+        <v>687</v>
+      </c>
+      <c r="C132" s="59" t="s">
+        <v>156</v>
+      </c>
+      <c r="D132" s="116"/>
+      <c r="E132" s="120" t="s">
+        <v>158</v>
+      </c>
       <c r="F132" s="119"/>
     </row>
-    <row r="133" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A133" s="116" t="s">
-        <v>410</v>
+        <v>416</v>
       </c>
       <c r="B133" s="116" t="s">
-        <v>694</v>
-      </c>
-      <c r="C133" s="120"/>
-      <c r="D133" s="20" t="s">
-        <v>502</v>
-      </c>
-      <c r="E133" s="120"/>
+        <v>688</v>
+      </c>
+      <c r="C133" s="59" t="s">
+        <v>160</v>
+      </c>
+      <c r="D133" s="116"/>
+      <c r="E133" s="120" t="s">
+        <v>162</v>
+      </c>
       <c r="F133" s="119"/>
     </row>
-    <row r="134" spans="1:6" ht="64" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A134" s="116" t="s">
-        <v>413</v>
+        <v>416</v>
       </c>
       <c r="B134" s="116" t="s">
-        <v>695</v>
-      </c>
-      <c r="C134" s="120"/>
-      <c r="D134" s="20" t="s">
-        <v>504</v>
-      </c>
-      <c r="E134" s="120"/>
+        <v>689</v>
+      </c>
+      <c r="C134" s="59" t="s">
+        <v>164</v>
+      </c>
+      <c r="D134" s="116"/>
+      <c r="E134" s="120" t="s">
+        <v>166</v>
+      </c>
       <c r="F134" s="119"/>
     </row>
-    <row r="135" spans="1:6" ht="48" x14ac:dyDescent="0.2">
-      <c r="A135" s="116" t="s">
-        <v>410</v>
-      </c>
-      <c r="B135" s="116" t="s">
-        <v>696</v>
-      </c>
-      <c r="C135" s="120"/>
-      <c r="D135" s="20" t="s">
-        <v>697</v>
-      </c>
+    <row r="135" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A135" s="116"/>
+      <c r="B135" s="116"/>
+      <c r="C135" s="117"/>
+      <c r="D135" s="116"/>
       <c r="E135" s="120"/>
       <c r="F135" s="119"/>
     </row>
     <row r="136" spans="1:6" ht="64" x14ac:dyDescent="0.2">
       <c r="A136" s="116" t="s">
-        <v>413</v>
+        <v>410</v>
       </c>
       <c r="B136" s="116" t="s">
-        <v>698</v>
+        <v>690</v>
       </c>
       <c r="C136" s="120"/>
       <c r="D136" s="20" t="s">
-        <v>699</v>
+        <v>691</v>
       </c>
       <c r="E136" s="120"/>
       <c r="F136" s="119"/>
     </row>
-    <row r="137" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A137" s="160" t="s">
-        <v>700</v>
-      </c>
-      <c r="B137" s="161"/>
-      <c r="C137" s="161"/>
-      <c r="D137" s="161"/>
-      <c r="E137" s="162"/>
+    <row r="137" spans="1:6" ht="80" x14ac:dyDescent="0.2">
+      <c r="A137" s="116" t="s">
+        <v>413</v>
+      </c>
+      <c r="B137" s="116" t="s">
+        <v>692</v>
+      </c>
+      <c r="C137" s="120"/>
+      <c r="D137" s="20" t="s">
+        <v>693</v>
+      </c>
+      <c r="E137" s="120"/>
       <c r="F137" s="119"/>
     </row>
-    <row r="138" spans="1:6" ht="64" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A138" s="116" t="s">
-        <v>243</v>
+        <v>410</v>
       </c>
       <c r="B138" s="116" t="s">
-        <v>701</v>
-      </c>
-      <c r="C138" s="117" t="s">
-        <v>702</v>
-      </c>
-      <c r="D138" s="116" t="s">
-        <v>703</v>
-      </c>
-      <c r="E138" s="120" t="s">
-        <v>704</v>
-      </c>
+        <v>694</v>
+      </c>
+      <c r="C138" s="120"/>
+      <c r="D138" s="20" t="s">
+        <v>502</v>
+      </c>
+      <c r="E138" s="120"/>
       <c r="F138" s="119"/>
     </row>
-    <row r="139" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:6" ht="64" x14ac:dyDescent="0.2">
       <c r="A139" s="116" t="s">
-        <v>410</v>
+        <v>413</v>
       </c>
       <c r="B139" s="116" t="s">
-        <v>705</v>
+        <v>695</v>
       </c>
       <c r="C139" s="120"/>
       <c r="D139" s="20" t="s">
-        <v>412</v>
+        <v>504</v>
       </c>
       <c r="E139" s="120"/>
       <c r="F139" s="119"/>
     </row>
-    <row r="140" spans="1:6" ht="64" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A140" s="116" t="s">
-        <v>413</v>
+        <v>410</v>
       </c>
       <c r="B140" s="116" t="s">
-        <v>706</v>
+        <v>696</v>
       </c>
       <c r="C140" s="120"/>
       <c r="D140" s="20" t="s">
-        <v>415</v>
+        <v>697</v>
       </c>
       <c r="E140" s="120"/>
       <c r="F140" s="119"/>
     </row>
-    <row r="141" spans="1:6" ht="48" x14ac:dyDescent="0.2">
-      <c r="A141" s="122" t="s">
-        <v>37</v>
-      </c>
-      <c r="B141" s="122" t="s">
-        <v>707</v>
-      </c>
-      <c r="C141" s="113" t="s">
-        <v>1331</v>
-      </c>
-      <c r="D141" s="122" t="s">
-        <v>708</v>
-      </c>
-      <c r="E141" s="122" t="s">
-        <v>709</v>
-      </c>
-      <c r="F141" s="123" t="s">
-        <v>710</v>
-      </c>
-    </row>
-    <row r="142" spans="1:6" ht="48" x14ac:dyDescent="0.2">
-      <c r="A142" s="122" t="s">
-        <v>410</v>
-      </c>
-      <c r="B142" s="122" t="s">
-        <v>711</v>
-      </c>
-      <c r="C142" s="122"/>
-      <c r="D142" s="113" t="s">
-        <v>712</v>
-      </c>
-      <c r="E142" s="122"/>
-      <c r="F142" s="123" t="s">
-        <v>713</v>
-      </c>
+    <row r="141" spans="1:6" ht="64" x14ac:dyDescent="0.2">
+      <c r="A141" s="116" t="s">
+        <v>413</v>
+      </c>
+      <c r="B141" s="116" t="s">
+        <v>698</v>
+      </c>
+      <c r="C141" s="120"/>
+      <c r="D141" s="20" t="s">
+        <v>699</v>
+      </c>
+      <c r="E141" s="120"/>
+      <c r="F141" s="119"/>
+    </row>
+    <row r="142" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A142" s="160" t="s">
+        <v>700</v>
+      </c>
+      <c r="B142" s="161"/>
+      <c r="C142" s="161"/>
+      <c r="D142" s="161"/>
+      <c r="E142" s="162"/>
+      <c r="F142" s="119"/>
     </row>
     <row r="143" spans="1:6" ht="64" x14ac:dyDescent="0.2">
-      <c r="A143" s="122" t="s">
-        <v>413</v>
-      </c>
-      <c r="B143" s="122" t="s">
-        <v>714</v>
-      </c>
-      <c r="C143" s="122"/>
-      <c r="D143" s="113" t="s">
-        <v>715</v>
-      </c>
-      <c r="E143" s="122"/>
-      <c r="F143" s="123"/>
+      <c r="A143" s="116" t="s">
+        <v>243</v>
+      </c>
+      <c r="B143" s="116" t="s">
+        <v>701</v>
+      </c>
+      <c r="C143" s="117" t="s">
+        <v>702</v>
+      </c>
+      <c r="D143" s="116" t="s">
+        <v>703</v>
+      </c>
+      <c r="E143" s="120" t="s">
+        <v>704</v>
+      </c>
+      <c r="F143" s="119"/>
     </row>
     <row r="144" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A144" s="116" t="s">
         <v>410</v>
       </c>
       <c r="B144" s="116" t="s">
-        <v>716</v>
+        <v>705</v>
       </c>
       <c r="C144" s="120"/>
       <c r="D144" s="20" t="s">
-        <v>717</v>
+        <v>412</v>
       </c>
       <c r="E144" s="120"/>
-      <c r="F144" s="119" t="s">
-        <v>718</v>
-      </c>
+      <c r="F144" s="119"/>
     </row>
     <row r="145" spans="1:6" ht="64" x14ac:dyDescent="0.2">
       <c r="A145" s="116" t="s">
         <v>413</v>
       </c>
       <c r="B145" s="116" t="s">
-        <v>719</v>
+        <v>706</v>
       </c>
       <c r="C145" s="120"/>
       <c r="D145" s="20" t="s">
-        <v>720</v>
+        <v>415</v>
       </c>
       <c r="E145" s="120"/>
       <c r="F145" s="119"/>
     </row>
-    <row r="146" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A146" s="160" t="s">
+    <row r="146" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+      <c r="A146" s="122" t="s">
+        <v>37</v>
+      </c>
+      <c r="B146" s="122" t="s">
+        <v>707</v>
+      </c>
+      <c r="C146" s="113" t="s">
+        <v>1331</v>
+      </c>
+      <c r="D146" s="122" t="s">
+        <v>708</v>
+      </c>
+      <c r="E146" s="122" t="s">
+        <v>709</v>
+      </c>
+      <c r="F146" s="123" t="s">
+        <v>710</v>
+      </c>
+    </row>
+    <row r="147" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+      <c r="A147" s="122" t="s">
+        <v>410</v>
+      </c>
+      <c r="B147" s="122" t="s">
+        <v>711</v>
+      </c>
+      <c r="C147" s="122"/>
+      <c r="D147" s="113" t="s">
+        <v>712</v>
+      </c>
+      <c r="E147" s="122"/>
+      <c r="F147" s="123" t="s">
+        <v>713</v>
+      </c>
+    </row>
+    <row r="148" spans="1:6" ht="64" x14ac:dyDescent="0.2">
+      <c r="A148" s="122" t="s">
+        <v>413</v>
+      </c>
+      <c r="B148" s="122" t="s">
+        <v>714</v>
+      </c>
+      <c r="C148" s="122"/>
+      <c r="D148" s="113" t="s">
+        <v>715</v>
+      </c>
+      <c r="E148" s="122"/>
+      <c r="F148" s="123"/>
+    </row>
+    <row r="149" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+      <c r="A149" s="116" t="s">
+        <v>410</v>
+      </c>
+      <c r="B149" s="116" t="s">
+        <v>716</v>
+      </c>
+      <c r="C149" s="120"/>
+      <c r="D149" s="20" t="s">
+        <v>717</v>
+      </c>
+      <c r="E149" s="120"/>
+      <c r="F149" s="119" t="s">
+        <v>718</v>
+      </c>
+    </row>
+    <row r="150" spans="1:6" ht="64" x14ac:dyDescent="0.2">
+      <c r="A150" s="116" t="s">
+        <v>413</v>
+      </c>
+      <c r="B150" s="116" t="s">
+        <v>719</v>
+      </c>
+      <c r="C150" s="120"/>
+      <c r="D150" s="20" t="s">
+        <v>720</v>
+      </c>
+      <c r="E150" s="120"/>
+      <c r="F150" s="119"/>
+    </row>
+    <row r="151" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A151" s="160" t="s">
         <v>721</v>
       </c>
-      <c r="B146" s="161"/>
-      <c r="C146" s="161"/>
-      <c r="D146" s="161"/>
-      <c r="E146" s="162"/>
-      <c r="F146" s="119"/>
-    </row>
-    <row r="147" spans="1:6" ht="32" x14ac:dyDescent="0.2">
-      <c r="A147" s="116" t="s">
+      <c r="B151" s="161"/>
+      <c r="C151" s="161"/>
+      <c r="D151" s="161"/>
+      <c r="E151" s="162"/>
+      <c r="F151" s="119"/>
+    </row>
+    <row r="152" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+      <c r="A152" s="116" t="s">
         <v>243</v>
       </c>
-      <c r="B147" s="116" t="s">
+      <c r="B152" s="116" t="s">
         <v>722</v>
       </c>
-      <c r="C147" s="59" t="s">
+      <c r="C152" s="59" t="s">
         <v>1330</v>
       </c>
-      <c r="D147" s="116" t="s">
+      <c r="D152" s="116" t="s">
         <v>723</v>
       </c>
-      <c r="E147" s="120" t="s">
+      <c r="E152" s="120" t="s">
         <v>724</v>
-      </c>
-      <c r="F147" s="119"/>
-    </row>
-    <row r="148" spans="1:6" ht="48" x14ac:dyDescent="0.2">
-      <c r="A148" s="116" t="s">
-        <v>725</v>
-      </c>
-      <c r="B148" s="116" t="s">
-        <v>726</v>
-      </c>
-      <c r="C148" s="59" t="s">
-        <v>727</v>
-      </c>
-      <c r="D148" s="116"/>
-      <c r="E148" s="120" t="s">
-        <v>728</v>
-      </c>
-      <c r="F148" s="119"/>
-    </row>
-    <row r="149" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A149" s="116" t="s">
-        <v>37</v>
-      </c>
-      <c r="B149" s="116" t="s">
-        <v>1332</v>
-      </c>
-      <c r="C149" s="59" t="s">
-        <v>1334</v>
-      </c>
-      <c r="D149" s="116"/>
-      <c r="E149" s="120" t="s">
-        <v>1336</v>
-      </c>
-      <c r="F149" s="119"/>
-    </row>
-    <row r="150" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A150" s="116" t="s">
-        <v>37</v>
-      </c>
-      <c r="B150" s="116" t="s">
-        <v>1333</v>
-      </c>
-      <c r="C150" s="59" t="s">
-        <v>1335</v>
-      </c>
-      <c r="D150" s="116"/>
-      <c r="E150" s="120" t="s">
-        <v>1337</v>
-      </c>
-      <c r="F150" s="119"/>
-    </row>
-    <row r="151" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A151" s="116" t="s">
-        <v>729</v>
-      </c>
-      <c r="B151" s="116" t="s">
-        <v>730</v>
-      </c>
-      <c r="C151" s="117" t="s">
-        <v>76</v>
-      </c>
-      <c r="D151" s="116"/>
-      <c r="E151" s="120" t="s">
-        <v>78</v>
-      </c>
-      <c r="F151" s="119"/>
-    </row>
-    <row r="152" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A152" s="116" t="s">
-        <v>731</v>
-      </c>
-      <c r="B152" s="116" t="s">
-        <v>732</v>
-      </c>
-      <c r="C152" s="117" t="s">
-        <v>43</v>
-      </c>
-      <c r="D152" s="116"/>
-      <c r="E152" s="120" t="s">
-        <v>45</v>
       </c>
       <c r="F152" s="119"/>
     </row>
     <row r="153" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A153" s="116" t="s">
-        <v>410</v>
+        <v>725</v>
       </c>
       <c r="B153" s="116" t="s">
-        <v>733</v>
-      </c>
-      <c r="C153" s="120"/>
-      <c r="D153" s="20" t="s">
-        <v>734</v>
-      </c>
-      <c r="E153" s="120"/>
+        <v>726</v>
+      </c>
+      <c r="C153" s="59" t="s">
+        <v>727</v>
+      </c>
+      <c r="D153" s="116"/>
+      <c r="E153" s="120" t="s">
+        <v>728</v>
+      </c>
       <c r="F153" s="119"/>
     </row>
-    <row r="154" spans="1:6" ht="64" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A154" s="116" t="s">
-        <v>413</v>
+        <v>37</v>
       </c>
       <c r="B154" s="116" t="s">
-        <v>735</v>
-      </c>
-      <c r="C154" s="120"/>
-      <c r="D154" s="20" t="s">
-        <v>736</v>
-      </c>
-      <c r="E154" s="120"/>
+        <v>1332</v>
+      </c>
+      <c r="C154" s="59" t="s">
+        <v>1334</v>
+      </c>
+      <c r="D154" s="116"/>
+      <c r="E154" s="120" t="s">
+        <v>1336</v>
+      </c>
       <c r="F154" s="119"/>
     </row>
-    <row r="155" spans="1:6" ht="64" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A155" s="116" t="s">
-        <v>410</v>
+        <v>37</v>
       </c>
       <c r="B155" s="116" t="s">
-        <v>737</v>
-      </c>
-      <c r="C155" s="120"/>
-      <c r="D155" s="20" t="s">
-        <v>738</v>
-      </c>
-      <c r="E155" s="120"/>
-      <c r="F155" s="119" t="s">
-        <v>739</v>
-      </c>
-    </row>
-    <row r="156" spans="1:6" ht="64" x14ac:dyDescent="0.2">
+        <v>1333</v>
+      </c>
+      <c r="C155" s="59" t="s">
+        <v>1335</v>
+      </c>
+      <c r="D155" s="116"/>
+      <c r="E155" s="120" t="s">
+        <v>1337</v>
+      </c>
+      <c r="F155" s="119"/>
+    </row>
+    <row r="156" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A156" s="116" t="s">
-        <v>413</v>
+        <v>729</v>
       </c>
       <c r="B156" s="116" t="s">
-        <v>740</v>
-      </c>
-      <c r="C156" s="120"/>
-      <c r="D156" s="20" t="s">
-        <v>741</v>
-      </c>
-      <c r="E156" s="120"/>
+        <v>730</v>
+      </c>
+      <c r="C156" s="117" t="s">
+        <v>76</v>
+      </c>
+      <c r="D156" s="116"/>
+      <c r="E156" s="120" t="s">
+        <v>78</v>
+      </c>
       <c r="F156" s="119"/>
     </row>
-    <row r="157" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A157" s="160" t="s">
-        <v>742</v>
-      </c>
-      <c r="B157" s="161"/>
-      <c r="C157" s="161"/>
-      <c r="D157" s="161"/>
-      <c r="E157" s="162"/>
+    <row r="157" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A157" s="116" t="s">
+        <v>731</v>
+      </c>
+      <c r="B157" s="116" t="s">
+        <v>732</v>
+      </c>
+      <c r="C157" s="117" t="s">
+        <v>43</v>
+      </c>
+      <c r="D157" s="116"/>
+      <c r="E157" s="120" t="s">
+        <v>45</v>
+      </c>
       <c r="F157" s="119"/>
     </row>
     <row r="158" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A158" s="116" t="s">
-        <v>243</v>
+        <v>410</v>
       </c>
       <c r="B158" s="116" t="s">
-        <v>743</v>
-      </c>
-      <c r="C158" s="124" t="s">
-        <v>744</v>
-      </c>
-      <c r="D158" s="116" t="s">
-        <v>745</v>
-      </c>
-      <c r="E158" s="120" t="s">
-        <v>746</v>
-      </c>
+        <v>733</v>
+      </c>
+      <c r="C158" s="120"/>
+      <c r="D158" s="20" t="s">
+        <v>734</v>
+      </c>
+      <c r="E158" s="120"/>
       <c r="F158" s="119"/>
     </row>
     <row r="159" spans="1:6" ht="64" x14ac:dyDescent="0.2">
       <c r="A159" s="116" t="s">
-        <v>261</v>
+        <v>413</v>
       </c>
       <c r="B159" s="116" t="s">
-        <v>747</v>
-      </c>
-      <c r="C159" s="117" t="s">
-        <v>748</v>
-      </c>
-      <c r="D159" s="125" t="s">
-        <v>749</v>
-      </c>
-      <c r="E159" s="120" t="s">
-        <v>750</v>
-      </c>
+        <v>735</v>
+      </c>
+      <c r="C159" s="120"/>
+      <c r="D159" s="20" t="s">
+        <v>736</v>
+      </c>
+      <c r="E159" s="120"/>
       <c r="F159" s="119"/>
     </row>
-    <row r="160" spans="1:6" ht="32" x14ac:dyDescent="0.2">
-      <c r="A160" s="126" t="s">
-        <v>32</v>
+    <row r="160" spans="1:6" ht="64" x14ac:dyDescent="0.2">
+      <c r="A160" s="116" t="s">
+        <v>410</v>
       </c>
       <c r="B160" s="116" t="s">
-        <v>751</v>
-      </c>
-      <c r="C160" s="117" t="s">
-        <v>752</v>
-      </c>
-      <c r="D160" s="125" t="s">
-        <v>753</v>
-      </c>
-      <c r="E160" s="120" t="s">
-        <v>754</v>
-      </c>
-      <c r="F160" s="119"/>
-    </row>
-    <row r="161" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A161" s="126" t="s">
-        <v>755</v>
+        <v>737</v>
+      </c>
+      <c r="C160" s="120"/>
+      <c r="D160" s="20" t="s">
+        <v>738</v>
+      </c>
+      <c r="E160" s="120"/>
+      <c r="F160" s="119" t="s">
+        <v>739</v>
+      </c>
+    </row>
+    <row r="161" spans="1:6" ht="64" x14ac:dyDescent="0.2">
+      <c r="A161" s="116" t="s">
+        <v>413</v>
       </c>
       <c r="B161" s="116" t="s">
-        <v>756</v>
-      </c>
-      <c r="C161" s="127" t="s">
-        <v>47</v>
-      </c>
-      <c r="D161" s="125"/>
-      <c r="E161" s="120" t="s">
-        <v>49</v>
-      </c>
+        <v>740</v>
+      </c>
+      <c r="C161" s="120"/>
+      <c r="D161" s="20" t="s">
+        <v>741</v>
+      </c>
+      <c r="E161" s="120"/>
       <c r="F161" s="119"/>
     </row>
-    <row r="162" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A162" s="116" t="s">
-        <v>729</v>
-      </c>
-      <c r="B162" s="116" t="s">
-        <v>757</v>
-      </c>
-      <c r="C162" s="117" t="s">
-        <v>76</v>
-      </c>
-      <c r="D162" s="116"/>
-      <c r="E162" s="120" t="s">
-        <v>78</v>
-      </c>
+    <row r="162" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A162" s="160" t="s">
+        <v>742</v>
+      </c>
+      <c r="B162" s="161"/>
+      <c r="C162" s="161"/>
+      <c r="D162" s="161"/>
+      <c r="E162" s="162"/>
       <c r="F162" s="119"/>
     </row>
     <row r="163" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A163" s="116" t="s">
-        <v>410</v>
+        <v>243</v>
       </c>
       <c r="B163" s="116" t="s">
-        <v>758</v>
-      </c>
-      <c r="C163" s="128"/>
-      <c r="D163" s="20" t="s">
-        <v>759</v>
-      </c>
-      <c r="E163" s="120"/>
+        <v>743</v>
+      </c>
+      <c r="C163" s="124" t="s">
+        <v>744</v>
+      </c>
+      <c r="D163" s="116" t="s">
+        <v>745</v>
+      </c>
+      <c r="E163" s="120" t="s">
+        <v>746</v>
+      </c>
       <c r="F163" s="119"/>
     </row>
     <row r="164" spans="1:6" ht="64" x14ac:dyDescent="0.2">
       <c r="A164" s="116" t="s">
+        <v>261</v>
+      </c>
+      <c r="B164" s="116" t="s">
+        <v>747</v>
+      </c>
+      <c r="C164" s="117" t="s">
+        <v>748</v>
+      </c>
+      <c r="D164" s="125" t="s">
+        <v>749</v>
+      </c>
+      <c r="E164" s="120" t="s">
+        <v>750</v>
+      </c>
+      <c r="F164" s="119"/>
+    </row>
+    <row r="165" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+      <c r="A165" s="126" t="s">
+        <v>32</v>
+      </c>
+      <c r="B165" s="116" t="s">
+        <v>751</v>
+      </c>
+      <c r="C165" s="117" t="s">
+        <v>752</v>
+      </c>
+      <c r="D165" s="125" t="s">
+        <v>753</v>
+      </c>
+      <c r="E165" s="120" t="s">
+        <v>754</v>
+      </c>
+      <c r="F165" s="119"/>
+    </row>
+    <row r="166" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A166" s="126" t="s">
+        <v>755</v>
+      </c>
+      <c r="B166" s="116" t="s">
+        <v>756</v>
+      </c>
+      <c r="C166" s="127" t="s">
+        <v>47</v>
+      </c>
+      <c r="D166" s="125"/>
+      <c r="E166" s="120" t="s">
+        <v>49</v>
+      </c>
+      <c r="F166" s="119"/>
+    </row>
+    <row r="167" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A167" s="116" t="s">
+        <v>729</v>
+      </c>
+      <c r="B167" s="116" t="s">
+        <v>757</v>
+      </c>
+      <c r="C167" s="117" t="s">
+        <v>76</v>
+      </c>
+      <c r="D167" s="116"/>
+      <c r="E167" s="120" t="s">
+        <v>78</v>
+      </c>
+      <c r="F167" s="119"/>
+    </row>
+    <row r="168" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+      <c r="A168" s="116" t="s">
+        <v>410</v>
+      </c>
+      <c r="B168" s="116" t="s">
+        <v>758</v>
+      </c>
+      <c r="C168" s="128"/>
+      <c r="D168" s="20" t="s">
+        <v>759</v>
+      </c>
+      <c r="E168" s="120"/>
+      <c r="F168" s="119"/>
+    </row>
+    <row r="169" spans="1:6" ht="64" x14ac:dyDescent="0.2">
+      <c r="A169" s="116" t="s">
         <v>413</v>
       </c>
-      <c r="B164" s="116" t="s">
+      <c r="B169" s="116" t="s">
         <v>760</v>
       </c>
-      <c r="C164" s="120"/>
-      <c r="D164" s="20" t="s">
+      <c r="C169" s="120"/>
+      <c r="D169" s="20" t="s">
         <v>761</v>
       </c>
-      <c r="E164" s="120"/>
-      <c r="F164" s="119"/>
-    </row>
-    <row r="165" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A165" s="169" t="s">
+      <c r="E169" s="120"/>
+      <c r="F169" s="119"/>
+    </row>
+    <row r="170" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A170" s="163" t="s">
         <v>762</v>
       </c>
-      <c r="B165" s="170"/>
-      <c r="C165" s="170"/>
-      <c r="D165" s="170"/>
-      <c r="E165" s="171"/>
-      <c r="F165" s="129" t="s">
+      <c r="B170" s="164"/>
+      <c r="C170" s="164"/>
+      <c r="D170" s="164"/>
+      <c r="E170" s="165"/>
+      <c r="F170" s="129" t="s">
         <v>763</v>
-      </c>
-    </row>
-    <row r="166" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A166" s="116" t="s">
-        <v>243</v>
-      </c>
-      <c r="B166" s="116" t="s">
-        <v>764</v>
-      </c>
-      <c r="C166" s="130" t="s">
-        <v>765</v>
-      </c>
-      <c r="D166" s="114"/>
-      <c r="E166" s="131"/>
-      <c r="F166" s="129" t="s">
-        <v>766</v>
-      </c>
-    </row>
-    <row r="167" spans="1:6" ht="48" x14ac:dyDescent="0.2">
-      <c r="A167" s="116" t="s">
-        <v>261</v>
-      </c>
-      <c r="B167" s="116" t="s">
-        <v>767</v>
-      </c>
-      <c r="C167" s="117" t="s">
-        <v>748</v>
-      </c>
-      <c r="D167" s="114"/>
-      <c r="E167" s="131"/>
-      <c r="F167" s="129" t="s">
-        <v>766</v>
-      </c>
-    </row>
-    <row r="168" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A168" s="126" t="s">
-        <v>768</v>
-      </c>
-      <c r="B168" s="116" t="s">
-        <v>769</v>
-      </c>
-      <c r="C168" s="115" t="s">
-        <v>770</v>
-      </c>
-      <c r="D168" s="114"/>
-      <c r="E168" s="131"/>
-      <c r="F168" s="129" t="s">
-        <v>766</v>
-      </c>
-    </row>
-    <row r="169" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A169" s="126" t="s">
-        <v>32</v>
-      </c>
-      <c r="B169" s="116" t="s">
-        <v>771</v>
-      </c>
-      <c r="C169" s="130" t="s">
-        <v>772</v>
-      </c>
-      <c r="D169" s="114"/>
-      <c r="E169" s="131"/>
-      <c r="F169" s="129" t="s">
-        <v>766</v>
-      </c>
-    </row>
-    <row r="170" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A170" s="126" t="s">
-        <v>32</v>
-      </c>
-      <c r="B170" s="60" t="s">
-        <v>773</v>
-      </c>
-      <c r="C170" s="130" t="s">
-        <v>76</v>
-      </c>
-      <c r="D170" s="114"/>
-      <c r="E170" s="131"/>
-      <c r="F170" s="129" t="s">
-        <v>766</v>
       </c>
     </row>
     <row r="171" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A171" s="116" t="s">
-        <v>731</v>
+        <v>243</v>
       </c>
       <c r="B171" s="116" t="s">
-        <v>756</v>
+        <v>764</v>
       </c>
       <c r="C171" s="130" t="s">
-        <v>47</v>
+        <v>765</v>
       </c>
       <c r="D171" s="114"/>
       <c r="E171" s="131"/>
@@ -13481,12 +13512,16 @@
         <v>766</v>
       </c>
     </row>
-    <row r="172" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A172" s="116" t="s">
-        <v>410</v>
-      </c>
-      <c r="B172" s="132"/>
-      <c r="C172" s="133"/>
+        <v>261</v>
+      </c>
+      <c r="B172" s="116" t="s">
+        <v>767</v>
+      </c>
+      <c r="C172" s="117" t="s">
+        <v>748</v>
+      </c>
       <c r="D172" s="114"/>
       <c r="E172" s="131"/>
       <c r="F172" s="129" t="s">
@@ -13494,982 +13529,968 @@
       </c>
     </row>
     <row r="173" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A173" s="116" t="s">
-        <v>413</v>
-      </c>
-      <c r="B173" s="132"/>
-      <c r="C173" s="133"/>
+      <c r="A173" s="126" t="s">
+        <v>768</v>
+      </c>
+      <c r="B173" s="116" t="s">
+        <v>769</v>
+      </c>
+      <c r="C173" s="115" t="s">
+        <v>770</v>
+      </c>
       <c r="D173" s="114"/>
       <c r="E173" s="131"/>
       <c r="F173" s="129" t="s">
         <v>766</v>
       </c>
     </row>
-    <row r="174" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A174" s="160" t="s">
+    <row r="174" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A174" s="126" t="s">
+        <v>32</v>
+      </c>
+      <c r="B174" s="116" t="s">
+        <v>771</v>
+      </c>
+      <c r="C174" s="130" t="s">
+        <v>772</v>
+      </c>
+      <c r="D174" s="114"/>
+      <c r="E174" s="131"/>
+      <c r="F174" s="129" t="s">
+        <v>766</v>
+      </c>
+    </row>
+    <row r="175" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A175" s="126" t="s">
+        <v>32</v>
+      </c>
+      <c r="B175" s="60" t="s">
+        <v>773</v>
+      </c>
+      <c r="C175" s="130" t="s">
+        <v>76</v>
+      </c>
+      <c r="D175" s="114"/>
+      <c r="E175" s="131"/>
+      <c r="F175" s="129" t="s">
+        <v>766</v>
+      </c>
+    </row>
+    <row r="176" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A176" s="116" t="s">
+        <v>731</v>
+      </c>
+      <c r="B176" s="116" t="s">
+        <v>756</v>
+      </c>
+      <c r="C176" s="130" t="s">
+        <v>47</v>
+      </c>
+      <c r="D176" s="114"/>
+      <c r="E176" s="131"/>
+      <c r="F176" s="129" t="s">
+        <v>766</v>
+      </c>
+    </row>
+    <row r="177" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A177" s="116" t="s">
+        <v>410</v>
+      </c>
+      <c r="B177" s="132"/>
+      <c r="C177" s="133"/>
+      <c r="D177" s="114"/>
+      <c r="E177" s="131"/>
+      <c r="F177" s="129" t="s">
+        <v>766</v>
+      </c>
+    </row>
+    <row r="178" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A178" s="116" t="s">
+        <v>413</v>
+      </c>
+      <c r="B178" s="132"/>
+      <c r="C178" s="133"/>
+      <c r="D178" s="114"/>
+      <c r="E178" s="131"/>
+      <c r="F178" s="129" t="s">
+        <v>766</v>
+      </c>
+    </row>
+    <row r="179" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A179" s="160" t="s">
         <v>774</v>
       </c>
-      <c r="B174" s="161"/>
-      <c r="C174" s="161"/>
-      <c r="D174" s="161"/>
-      <c r="E174" s="162"/>
-      <c r="F174" s="119"/>
-    </row>
-    <row r="175" spans="1:6" ht="32" x14ac:dyDescent="0.2">
-      <c r="A175" s="91" t="s">
+      <c r="B179" s="161"/>
+      <c r="C179" s="161"/>
+      <c r="D179" s="161"/>
+      <c r="E179" s="162"/>
+      <c r="F179" s="119"/>
+    </row>
+    <row r="180" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+      <c r="A180" s="91" t="s">
         <v>243</v>
       </c>
-      <c r="B175" s="92" t="s">
+      <c r="B180" s="92" t="s">
         <v>775</v>
       </c>
-      <c r="C175" s="93" t="s">
+      <c r="C180" s="93" t="s">
         <v>776</v>
       </c>
-      <c r="D175" s="92" t="s">
+      <c r="D180" s="92" t="s">
         <v>777</v>
       </c>
-      <c r="E175" s="85" t="s">
+      <c r="E180" s="85" t="s">
         <v>778</v>
       </c>
-      <c r="F175" s="119"/>
-    </row>
-    <row r="176" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A176" s="94" t="s">
+      <c r="F180" s="119"/>
+    </row>
+    <row r="181" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A181" s="94" t="s">
         <v>416</v>
       </c>
-      <c r="B176" s="95" t="s">
+      <c r="B181" s="95" t="s">
         <v>779</v>
       </c>
-      <c r="C176" s="96" t="s">
+      <c r="C181" s="96" t="s">
         <v>56</v>
-      </c>
-      <c r="D176" s="95" t="s">
-        <v>404</v>
-      </c>
-      <c r="E176" s="89" t="s">
-        <v>58</v>
-      </c>
-      <c r="F176" s="119"/>
-    </row>
-    <row r="177" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A177" s="94" t="s">
-        <v>416</v>
-      </c>
-      <c r="B177" s="95" t="s">
-        <v>780</v>
-      </c>
-      <c r="C177" s="96" t="s">
-        <v>60</v>
-      </c>
-      <c r="D177" s="95" t="s">
-        <v>404</v>
-      </c>
-      <c r="E177" s="89" t="s">
-        <v>62</v>
-      </c>
-      <c r="F177" s="119"/>
-    </row>
-    <row r="178" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A178" s="94" t="s">
-        <v>416</v>
-      </c>
-      <c r="B178" s="95" t="s">
-        <v>781</v>
-      </c>
-      <c r="C178" s="96" t="s">
-        <v>64</v>
-      </c>
-      <c r="D178" s="95" t="s">
-        <v>404</v>
-      </c>
-      <c r="E178" s="89" t="s">
-        <v>66</v>
-      </c>
-      <c r="F178" s="119"/>
-    </row>
-    <row r="179" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A179" s="94" t="s">
-        <v>416</v>
-      </c>
-      <c r="B179" s="95" t="s">
-        <v>782</v>
-      </c>
-      <c r="C179" s="96" t="s">
-        <v>68</v>
-      </c>
-      <c r="D179" s="95" t="s">
-        <v>404</v>
-      </c>
-      <c r="E179" s="89" t="s">
-        <v>70</v>
-      </c>
-      <c r="F179" s="119"/>
-    </row>
-    <row r="180" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A180" s="94" t="s">
-        <v>416</v>
-      </c>
-      <c r="B180" s="95" t="s">
-        <v>783</v>
-      </c>
-      <c r="C180" s="96" t="s">
-        <v>39</v>
-      </c>
-      <c r="D180" s="95" t="s">
-        <v>404</v>
-      </c>
-      <c r="E180" s="89" t="s">
-        <v>41</v>
-      </c>
-      <c r="F180" s="119"/>
-    </row>
-    <row r="181" spans="1:6" ht="32" x14ac:dyDescent="0.2">
-      <c r="A181" s="94" t="s">
-        <v>32</v>
-      </c>
-      <c r="B181" s="95" t="s">
-        <v>784</v>
-      </c>
-      <c r="C181" s="97" t="s">
-        <v>785</v>
       </c>
       <c r="D181" s="95" t="s">
         <v>404</v>
       </c>
       <c r="E181" s="89" t="s">
+        <v>58</v>
+      </c>
+      <c r="F181" s="119"/>
+    </row>
+    <row r="182" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A182" s="94" t="s">
+        <v>416</v>
+      </c>
+      <c r="B182" s="95" t="s">
+        <v>780</v>
+      </c>
+      <c r="C182" s="96" t="s">
+        <v>60</v>
+      </c>
+      <c r="D182" s="95" t="s">
+        <v>404</v>
+      </c>
+      <c r="E182" s="89" t="s">
+        <v>62</v>
+      </c>
+      <c r="F182" s="119"/>
+    </row>
+    <row r="183" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A183" s="94" t="s">
+        <v>416</v>
+      </c>
+      <c r="B183" s="95" t="s">
+        <v>781</v>
+      </c>
+      <c r="C183" s="96" t="s">
+        <v>64</v>
+      </c>
+      <c r="D183" s="95" t="s">
+        <v>404</v>
+      </c>
+      <c r="E183" s="89" t="s">
+        <v>66</v>
+      </c>
+      <c r="F183" s="119"/>
+    </row>
+    <row r="184" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A184" s="94" t="s">
+        <v>416</v>
+      </c>
+      <c r="B184" s="95" t="s">
+        <v>782</v>
+      </c>
+      <c r="C184" s="96" t="s">
+        <v>68</v>
+      </c>
+      <c r="D184" s="95" t="s">
+        <v>404</v>
+      </c>
+      <c r="E184" s="89" t="s">
+        <v>70</v>
+      </c>
+      <c r="F184" s="119"/>
+    </row>
+    <row r="185" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A185" s="94" t="s">
+        <v>416</v>
+      </c>
+      <c r="B185" s="95" t="s">
+        <v>783</v>
+      </c>
+      <c r="C185" s="96" t="s">
+        <v>39</v>
+      </c>
+      <c r="D185" s="95" t="s">
+        <v>404</v>
+      </c>
+      <c r="E185" s="89" t="s">
+        <v>41</v>
+      </c>
+      <c r="F185" s="119"/>
+    </row>
+    <row r="186" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+      <c r="A186" s="94" t="s">
+        <v>32</v>
+      </c>
+      <c r="B186" s="95" t="s">
+        <v>784</v>
+      </c>
+      <c r="C186" s="97" t="s">
+        <v>785</v>
+      </c>
+      <c r="D186" s="95" t="s">
+        <v>404</v>
+      </c>
+      <c r="E186" s="89" t="s">
         <v>786</v>
       </c>
-      <c r="F181" s="119"/>
-    </row>
-    <row r="182" spans="1:6" ht="64" x14ac:dyDescent="0.2">
-      <c r="A182" s="116" t="s">
+      <c r="F186" s="119"/>
+    </row>
+    <row r="187" spans="1:6" ht="64" x14ac:dyDescent="0.2">
+      <c r="A187" s="116" t="s">
         <v>410</v>
       </c>
-      <c r="B182" s="116" t="s">
+      <c r="B187" s="116" t="s">
         <v>787</v>
       </c>
-      <c r="C182" s="120"/>
-      <c r="D182" s="20" t="s">
+      <c r="C187" s="120"/>
+      <c r="D187" s="20" t="s">
         <v>788</v>
       </c>
-      <c r="E182" s="120"/>
-      <c r="F182" s="119"/>
-    </row>
-    <row r="183" spans="1:6" ht="64" x14ac:dyDescent="0.2">
-      <c r="A183" s="116" t="s">
+      <c r="E187" s="120"/>
+      <c r="F187" s="119"/>
+    </row>
+    <row r="188" spans="1:6" ht="64" x14ac:dyDescent="0.2">
+      <c r="A188" s="116" t="s">
         <v>413</v>
       </c>
-      <c r="B183" s="116" t="s">
+      <c r="B188" s="116" t="s">
         <v>789</v>
-      </c>
-      <c r="C183" s="120"/>
-      <c r="D183" s="20" t="s">
-        <v>790</v>
-      </c>
-      <c r="E183" s="120"/>
-      <c r="F183" s="119"/>
-    </row>
-    <row r="184" spans="1:6" ht="48" x14ac:dyDescent="0.2">
-      <c r="A184" s="116" t="s">
-        <v>410</v>
-      </c>
-      <c r="B184" s="116" t="s">
-        <v>791</v>
-      </c>
-      <c r="C184" s="120"/>
-      <c r="D184" s="20" t="s">
-        <v>792</v>
-      </c>
-      <c r="E184" s="120"/>
-      <c r="F184" s="119"/>
-    </row>
-    <row r="185" spans="1:6" ht="64" x14ac:dyDescent="0.2">
-      <c r="A185" s="116" t="s">
-        <v>413</v>
-      </c>
-      <c r="B185" s="116" t="s">
-        <v>793</v>
-      </c>
-      <c r="C185" s="120"/>
-      <c r="D185" s="20" t="s">
-        <v>794</v>
-      </c>
-      <c r="E185" s="120"/>
-      <c r="F185" s="119"/>
-    </row>
-    <row r="186" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A186" s="160" t="s">
-        <v>795</v>
-      </c>
-      <c r="B186" s="161"/>
-      <c r="C186" s="161"/>
-      <c r="D186" s="161"/>
-      <c r="E186" s="162"/>
-      <c r="F186" s="119"/>
-    </row>
-    <row r="187" spans="1:6" ht="32" x14ac:dyDescent="0.2">
-      <c r="A187" s="116" t="s">
-        <v>243</v>
-      </c>
-      <c r="B187" s="116" t="s">
-        <v>796</v>
-      </c>
-      <c r="C187" s="117" t="s">
-        <v>797</v>
-      </c>
-      <c r="D187" s="116" t="s">
-        <v>777</v>
-      </c>
-      <c r="E187" s="120" t="s">
-        <v>798</v>
-      </c>
-      <c r="F187" s="119"/>
-    </row>
-    <row r="188" spans="1:6" ht="48" x14ac:dyDescent="0.2">
-      <c r="A188" s="116" t="s">
-        <v>410</v>
-      </c>
-      <c r="B188" s="116" t="s">
-        <v>799</v>
       </c>
       <c r="C188" s="120"/>
       <c r="D188" s="20" t="s">
-        <v>800</v>
+        <v>790</v>
       </c>
       <c r="E188" s="120"/>
       <c r="F188" s="119"/>
     </row>
-    <row r="189" spans="1:6" ht="64" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A189" s="116" t="s">
-        <v>413</v>
+        <v>410</v>
       </c>
       <c r="B189" s="116" t="s">
-        <v>801</v>
+        <v>791</v>
       </c>
       <c r="C189" s="120"/>
       <c r="D189" s="20" t="s">
-        <v>802</v>
+        <v>792</v>
       </c>
       <c r="E189" s="120"/>
       <c r="F189" s="119"/>
     </row>
-    <row r="190" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A190" s="160" t="s">
-        <v>803</v>
-      </c>
-      <c r="B190" s="161"/>
-      <c r="C190" s="161"/>
-      <c r="D190" s="161"/>
-      <c r="E190" s="162"/>
+    <row r="190" spans="1:6" ht="64" x14ac:dyDescent="0.2">
+      <c r="A190" s="116" t="s">
+        <v>413</v>
+      </c>
+      <c r="B190" s="116" t="s">
+        <v>793</v>
+      </c>
+      <c r="C190" s="120"/>
+      <c r="D190" s="20" t="s">
+        <v>794</v>
+      </c>
+      <c r="E190" s="120"/>
       <c r="F190" s="119"/>
     </row>
-    <row r="191" spans="1:6" ht="64" x14ac:dyDescent="0.2">
-      <c r="A191" s="116" t="s">
-        <v>243</v>
-      </c>
-      <c r="B191" s="116" t="s">
-        <v>804</v>
-      </c>
-      <c r="C191" s="117" t="s">
-        <v>805</v>
-      </c>
-      <c r="D191" s="116" t="s">
-        <v>806</v>
-      </c>
-      <c r="E191" s="120" t="s">
-        <v>807</v>
-      </c>
+    <row r="191" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A191" s="160" t="s">
+        <v>795</v>
+      </c>
+      <c r="B191" s="161"/>
+      <c r="C191" s="161"/>
+      <c r="D191" s="161"/>
+      <c r="E191" s="162"/>
       <c r="F191" s="119"/>
     </row>
     <row r="192" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A192" s="116" t="s">
-        <v>548</v>
+        <v>243</v>
       </c>
       <c r="B192" s="116" t="s">
-        <v>808</v>
+        <v>796</v>
       </c>
       <c r="C192" s="117" t="s">
-        <v>809</v>
+        <v>797</v>
       </c>
       <c r="D192" s="116" t="s">
-        <v>810</v>
+        <v>777</v>
       </c>
       <c r="E192" s="120" t="s">
-        <v>811</v>
+        <v>798</v>
       </c>
       <c r="F192" s="119"/>
     </row>
     <row r="193" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A193" s="116" t="s">
+        <v>410</v>
+      </c>
+      <c r="B193" s="116" t="s">
+        <v>799</v>
+      </c>
+      <c r="C193" s="120"/>
+      <c r="D193" s="20" t="s">
+        <v>800</v>
+      </c>
+      <c r="E193" s="120"/>
+      <c r="F193" s="119"/>
+    </row>
+    <row r="194" spans="1:6" ht="64" x14ac:dyDescent="0.2">
+      <c r="A194" s="116" t="s">
+        <v>413</v>
+      </c>
+      <c r="B194" s="116" t="s">
+        <v>801</v>
+      </c>
+      <c r="C194" s="120"/>
+      <c r="D194" s="20" t="s">
+        <v>802</v>
+      </c>
+      <c r="E194" s="120"/>
+      <c r="F194" s="119"/>
+    </row>
+    <row r="195" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A195" s="160" t="s">
+        <v>803</v>
+      </c>
+      <c r="B195" s="161"/>
+      <c r="C195" s="161"/>
+      <c r="D195" s="161"/>
+      <c r="E195" s="162"/>
+      <c r="F195" s="119"/>
+    </row>
+    <row r="196" spans="1:6" ht="64" x14ac:dyDescent="0.2">
+      <c r="A196" s="116" t="s">
+        <v>243</v>
+      </c>
+      <c r="B196" s="116" t="s">
+        <v>804</v>
+      </c>
+      <c r="C196" s="117" t="s">
+        <v>805</v>
+      </c>
+      <c r="D196" s="116" t="s">
+        <v>806</v>
+      </c>
+      <c r="E196" s="120" t="s">
+        <v>807</v>
+      </c>
+      <c r="F196" s="119"/>
+    </row>
+    <row r="197" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+      <c r="A197" s="116" t="s">
+        <v>548</v>
+      </c>
+      <c r="B197" s="116" t="s">
+        <v>808</v>
+      </c>
+      <c r="C197" s="117" t="s">
+        <v>809</v>
+      </c>
+      <c r="D197" s="116" t="s">
+        <v>810</v>
+      </c>
+      <c r="E197" s="120" t="s">
+        <v>811</v>
+      </c>
+      <c r="F197" s="119"/>
+    </row>
+    <row r="198" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+      <c r="A198" s="116" t="s">
         <v>484</v>
       </c>
-      <c r="B193" s="116" t="s">
+      <c r="B198" s="116" t="s">
         <v>812</v>
       </c>
-      <c r="C193" s="59" t="s">
+      <c r="C198" s="59" t="s">
         <v>1348</v>
       </c>
-      <c r="D193" s="116" t="s">
+      <c r="D198" s="116" t="s">
         <v>813</v>
       </c>
-      <c r="E193" s="120" t="s">
+      <c r="E198" s="120" t="s">
         <v>1352</v>
       </c>
-      <c r="F193" s="119"/>
-    </row>
-    <row r="194" spans="1:6" ht="32" x14ac:dyDescent="0.2">
-      <c r="A194" s="116" t="s">
+      <c r="F198" s="119"/>
+    </row>
+    <row r="199" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+      <c r="A199" s="116" t="s">
         <v>484</v>
       </c>
-      <c r="B194" s="116" t="s">
+      <c r="B199" s="116" t="s">
         <v>1349</v>
       </c>
-      <c r="C194" s="59" t="s">
+      <c r="C199" s="59" t="s">
         <v>1350</v>
-      </c>
-      <c r="D194" s="116"/>
-      <c r="E194" s="120" t="s">
-        <v>1351</v>
-      </c>
-      <c r="F194" s="119"/>
-    </row>
-    <row r="195" spans="1:6" ht="64" x14ac:dyDescent="0.2">
-      <c r="A195" s="116" t="s">
-        <v>410</v>
-      </c>
-      <c r="B195" s="116" t="s">
-        <v>814</v>
-      </c>
-      <c r="C195" s="120"/>
-      <c r="D195" s="20" t="s">
-        <v>815</v>
-      </c>
-      <c r="E195" s="120"/>
-      <c r="F195" s="119"/>
-    </row>
-    <row r="196" spans="1:6" ht="80" x14ac:dyDescent="0.2">
-      <c r="A196" s="116" t="s">
-        <v>413</v>
-      </c>
-      <c r="B196" s="116" t="s">
-        <v>816</v>
-      </c>
-      <c r="C196" s="120"/>
-      <c r="D196" s="20" t="s">
-        <v>817</v>
-      </c>
-      <c r="E196" s="120"/>
-      <c r="F196" s="119"/>
-    </row>
-    <row r="197" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A197" s="160" t="s">
-        <v>818</v>
-      </c>
-      <c r="B197" s="161"/>
-      <c r="C197" s="161"/>
-      <c r="D197" s="161"/>
-      <c r="E197" s="162"/>
-      <c r="F197" s="119"/>
-    </row>
-    <row r="198" spans="1:6" ht="32" x14ac:dyDescent="0.2">
-      <c r="A198" s="116" t="s">
-        <v>243</v>
-      </c>
-      <c r="B198" s="116" t="s">
-        <v>819</v>
-      </c>
-      <c r="C198" s="117" t="s">
-        <v>820</v>
-      </c>
-      <c r="D198" s="116" t="s">
-        <v>821</v>
-      </c>
-      <c r="E198" s="120" t="s">
-        <v>822</v>
-      </c>
-      <c r="F198" s="119"/>
-    </row>
-    <row r="199" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A199" s="116" t="s">
-        <v>416</v>
-      </c>
-      <c r="B199" s="116" t="s">
-        <v>823</v>
-      </c>
-      <c r="C199" s="117" t="s">
-        <v>39</v>
       </c>
       <c r="D199" s="116"/>
       <c r="E199" s="120" t="s">
-        <v>41</v>
+        <v>1351</v>
       </c>
       <c r="F199" s="119"/>
     </row>
-    <row r="200" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:6" ht="64" x14ac:dyDescent="0.2">
       <c r="A200" s="116" t="s">
-        <v>729</v>
+        <v>410</v>
       </c>
       <c r="B200" s="116" t="s">
-        <v>824</v>
-      </c>
-      <c r="C200" s="117" t="s">
-        <v>76</v>
-      </c>
-      <c r="D200" s="116"/>
-      <c r="E200" s="120" t="s">
-        <v>78</v>
-      </c>
+        <v>814</v>
+      </c>
+      <c r="C200" s="120"/>
+      <c r="D200" s="20" t="s">
+        <v>815</v>
+      </c>
+      <c r="E200" s="120"/>
       <c r="F200" s="119"/>
     </row>
-    <row r="201" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:6" ht="80" x14ac:dyDescent="0.2">
       <c r="A201" s="116" t="s">
-        <v>729</v>
+        <v>413</v>
       </c>
       <c r="B201" s="116" t="s">
-        <v>824</v>
-      </c>
-      <c r="C201" s="117" t="s">
-        <v>1359</v>
-      </c>
-      <c r="D201" s="116"/>
-      <c r="E201" s="120" t="s">
-        <v>1362</v>
-      </c>
+        <v>816</v>
+      </c>
+      <c r="C201" s="120"/>
+      <c r="D201" s="20" t="s">
+        <v>817</v>
+      </c>
+      <c r="E201" s="120"/>
       <c r="F201" s="119"/>
     </row>
-    <row r="202" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A202" s="116" t="s">
-        <v>731</v>
-      </c>
-      <c r="B202" s="116" t="s">
-        <v>1361</v>
-      </c>
-      <c r="C202" s="117" t="s">
-        <v>43</v>
-      </c>
-      <c r="D202" s="116"/>
-      <c r="E202" s="120" t="s">
-        <v>45</v>
-      </c>
+    <row r="202" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A202" s="160" t="s">
+        <v>818</v>
+      </c>
+      <c r="B202" s="161"/>
+      <c r="C202" s="161"/>
+      <c r="D202" s="161"/>
+      <c r="E202" s="162"/>
       <c r="F202" s="119"/>
     </row>
     <row r="203" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A203" s="116" t="s">
+        <v>243</v>
+      </c>
+      <c r="B203" s="116" t="s">
+        <v>819</v>
+      </c>
+      <c r="C203" s="117" t="s">
+        <v>820</v>
+      </c>
+      <c r="D203" s="116" t="s">
+        <v>821</v>
+      </c>
+      <c r="E203" s="120" t="s">
+        <v>822</v>
+      </c>
+      <c r="F203" s="119"/>
+    </row>
+    <row r="204" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A204" s="116" t="s">
+        <v>416</v>
+      </c>
+      <c r="B204" s="116" t="s">
+        <v>823</v>
+      </c>
+      <c r="C204" s="117" t="s">
+        <v>39</v>
+      </c>
+      <c r="D204" s="116"/>
+      <c r="E204" s="120" t="s">
+        <v>41</v>
+      </c>
+      <c r="F204" s="119"/>
+    </row>
+    <row r="205" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A205" s="116" t="s">
+        <v>729</v>
+      </c>
+      <c r="B205" s="116" t="s">
+        <v>824</v>
+      </c>
+      <c r="C205" s="117" t="s">
+        <v>76</v>
+      </c>
+      <c r="D205" s="116"/>
+      <c r="E205" s="120" t="s">
+        <v>78</v>
+      </c>
+      <c r="F205" s="119"/>
+    </row>
+    <row r="206" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A206" s="116" t="s">
+        <v>729</v>
+      </c>
+      <c r="B206" s="116" t="s">
+        <v>824</v>
+      </c>
+      <c r="C206" s="117" t="s">
+        <v>1359</v>
+      </c>
+      <c r="D206" s="116"/>
+      <c r="E206" s="120" t="s">
+        <v>1362</v>
+      </c>
+      <c r="F206" s="119"/>
+    </row>
+    <row r="207" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A207" s="116" t="s">
+        <v>731</v>
+      </c>
+      <c r="B207" s="116" t="s">
+        <v>1361</v>
+      </c>
+      <c r="C207" s="117" t="s">
+        <v>43</v>
+      </c>
+      <c r="D207" s="116"/>
+      <c r="E207" s="120" t="s">
+        <v>45</v>
+      </c>
+      <c r="F207" s="119"/>
+    </row>
+    <row r="208" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+      <c r="A208" s="116" t="s">
         <v>32</v>
       </c>
-      <c r="B203" s="116" t="s">
+      <c r="B208" s="116" t="s">
         <v>1360</v>
       </c>
-      <c r="C203" s="134" t="s">
+      <c r="C208" s="134" t="s">
         <v>1357</v>
       </c>
-      <c r="D203" s="116"/>
-      <c r="E203" s="120" t="s">
+      <c r="D208" s="116"/>
+      <c r="E208" s="120" t="s">
         <v>1358</v>
       </c>
-      <c r="F203" s="119"/>
-    </row>
-    <row r="204" spans="1:6" ht="48" x14ac:dyDescent="0.2">
-      <c r="A204" s="116" t="s">
-        <v>410</v>
-      </c>
-      <c r="B204" s="116" t="s">
-        <v>825</v>
-      </c>
-      <c r="C204" s="120"/>
-      <c r="D204" s="20" t="s">
-        <v>734</v>
-      </c>
-      <c r="E204" s="120"/>
-      <c r="F204" s="119"/>
-    </row>
-    <row r="205" spans="1:6" ht="64" x14ac:dyDescent="0.2">
-      <c r="A205" s="116" t="s">
-        <v>413</v>
-      </c>
-      <c r="B205" s="116" t="s">
-        <v>826</v>
-      </c>
-      <c r="C205" s="120"/>
-      <c r="D205" s="20" t="s">
-        <v>736</v>
-      </c>
-      <c r="E205" s="120"/>
-      <c r="F205" s="119"/>
-    </row>
-    <row r="206" spans="1:6" ht="48" x14ac:dyDescent="0.2">
-      <c r="A206" s="116" t="s">
-        <v>410</v>
-      </c>
-      <c r="B206" s="116" t="s">
-        <v>827</v>
-      </c>
-      <c r="C206" s="120"/>
-      <c r="D206" s="20" t="s">
-        <v>738</v>
-      </c>
-      <c r="E206" s="120"/>
-      <c r="F206" s="119"/>
-    </row>
-    <row r="207" spans="1:6" ht="64" x14ac:dyDescent="0.2">
-      <c r="A207" s="116" t="s">
-        <v>413</v>
-      </c>
-      <c r="B207" s="116" t="s">
-        <v>828</v>
-      </c>
-      <c r="C207" s="120"/>
-      <c r="D207" s="20" t="s">
-        <v>741</v>
-      </c>
-      <c r="E207" s="120"/>
-      <c r="F207" s="119"/>
-    </row>
-    <row r="208" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A208" s="160" t="s">
-        <v>829</v>
-      </c>
-      <c r="B208" s="161"/>
-      <c r="C208" s="161"/>
-      <c r="D208" s="161"/>
-      <c r="E208" s="162"/>
       <c r="F208" s="119"/>
     </row>
     <row r="209" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A209" s="116" t="s">
-        <v>243</v>
+        <v>410</v>
       </c>
       <c r="B209" s="116" t="s">
-        <v>830</v>
-      </c>
-      <c r="C209" s="117" t="s">
-        <v>831</v>
-      </c>
-      <c r="D209" s="116" t="s">
-        <v>832</v>
-      </c>
-      <c r="E209" s="120" t="s">
-        <v>54</v>
-      </c>
+        <v>825</v>
+      </c>
+      <c r="C209" s="120"/>
+      <c r="D209" s="20" t="s">
+        <v>734</v>
+      </c>
+      <c r="E209" s="120"/>
       <c r="F209" s="119"/>
     </row>
     <row r="210" spans="1:6" ht="64" x14ac:dyDescent="0.2">
       <c r="A210" s="116" t="s">
-        <v>261</v>
+        <v>413</v>
       </c>
       <c r="B210" s="116" t="s">
-        <v>833</v>
-      </c>
-      <c r="C210" s="117" t="s">
-        <v>748</v>
-      </c>
-      <c r="D210" s="125" t="s">
-        <v>834</v>
-      </c>
-      <c r="E210" s="120" t="s">
-        <v>750</v>
-      </c>
+        <v>826</v>
+      </c>
+      <c r="C210" s="120"/>
+      <c r="D210" s="20" t="s">
+        <v>736</v>
+      </c>
+      <c r="E210" s="120"/>
       <c r="F210" s="119"/>
     </row>
     <row r="211" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A211" s="116" t="s">
-        <v>32</v>
+        <v>410</v>
       </c>
       <c r="B211" s="116" t="s">
-        <v>835</v>
-      </c>
-      <c r="C211" s="117" t="s">
-        <v>752</v>
-      </c>
-      <c r="D211" s="125" t="s">
-        <v>836</v>
-      </c>
-      <c r="E211" s="120" t="s">
-        <v>754</v>
-      </c>
+        <v>827</v>
+      </c>
+      <c r="C211" s="120"/>
+      <c r="D211" s="20" t="s">
+        <v>738</v>
+      </c>
+      <c r="E211" s="120"/>
       <c r="F211" s="119"/>
     </row>
-    <row r="212" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+    <row r="212" spans="1:6" ht="64" x14ac:dyDescent="0.2">
       <c r="A212" s="116" t="s">
-        <v>410</v>
+        <v>413</v>
       </c>
       <c r="B212" s="116" t="s">
-        <v>837</v>
-      </c>
-      <c r="C212" s="128"/>
+        <v>828</v>
+      </c>
+      <c r="C212" s="120"/>
       <c r="D212" s="20" t="s">
-        <v>759</v>
+        <v>741</v>
       </c>
       <c r="E212" s="120"/>
       <c r="F212" s="119"/>
     </row>
-    <row r="213" spans="1:6" ht="64" x14ac:dyDescent="0.2">
-      <c r="A213" s="116" t="s">
+    <row r="213" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A213" s="160" t="s">
+        <v>829</v>
+      </c>
+      <c r="B213" s="161"/>
+      <c r="C213" s="161"/>
+      <c r="D213" s="161"/>
+      <c r="E213" s="162"/>
+      <c r="F213" s="119"/>
+    </row>
+    <row r="214" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+      <c r="A214" s="116" t="s">
+        <v>243</v>
+      </c>
+      <c r="B214" s="116" t="s">
+        <v>830</v>
+      </c>
+      <c r="C214" s="117" t="s">
+        <v>831</v>
+      </c>
+      <c r="D214" s="116" t="s">
+        <v>832</v>
+      </c>
+      <c r="E214" s="120" t="s">
+        <v>54</v>
+      </c>
+      <c r="F214" s="119"/>
+    </row>
+    <row r="215" spans="1:6" ht="64" x14ac:dyDescent="0.2">
+      <c r="A215" s="116" t="s">
+        <v>261</v>
+      </c>
+      <c r="B215" s="116" t="s">
+        <v>833</v>
+      </c>
+      <c r="C215" s="117" t="s">
+        <v>748</v>
+      </c>
+      <c r="D215" s="125" t="s">
+        <v>834</v>
+      </c>
+      <c r="E215" s="120" t="s">
+        <v>750</v>
+      </c>
+      <c r="F215" s="119"/>
+    </row>
+    <row r="216" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+      <c r="A216" s="116" t="s">
+        <v>32</v>
+      </c>
+      <c r="B216" s="116" t="s">
+        <v>835</v>
+      </c>
+      <c r="C216" s="117" t="s">
+        <v>752</v>
+      </c>
+      <c r="D216" s="125" t="s">
+        <v>836</v>
+      </c>
+      <c r="E216" s="120" t="s">
+        <v>754</v>
+      </c>
+      <c r="F216" s="119"/>
+    </row>
+    <row r="217" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+      <c r="A217" s="116" t="s">
+        <v>410</v>
+      </c>
+      <c r="B217" s="116" t="s">
+        <v>837</v>
+      </c>
+      <c r="C217" s="128"/>
+      <c r="D217" s="20" t="s">
+        <v>759</v>
+      </c>
+      <c r="E217" s="120"/>
+      <c r="F217" s="119"/>
+    </row>
+    <row r="218" spans="1:6" ht="64" x14ac:dyDescent="0.2">
+      <c r="A218" s="116" t="s">
         <v>413</v>
       </c>
-      <c r="B213" s="116" t="s">
+      <c r="B218" s="116" t="s">
         <v>838</v>
       </c>
-      <c r="C213" s="120"/>
-      <c r="D213" s="20" t="s">
+      <c r="C218" s="120"/>
+      <c r="D218" s="20" t="s">
         <v>761</v>
       </c>
-      <c r="E213" s="120"/>
-      <c r="F213" s="119"/>
-    </row>
-    <row r="214" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A214" s="160" t="s">
+      <c r="E218" s="120"/>
+      <c r="F218" s="119"/>
+    </row>
+    <row r="219" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A219" s="160" t="s">
         <v>839</v>
       </c>
-      <c r="B214" s="161"/>
-      <c r="C214" s="161"/>
-      <c r="D214" s="161"/>
-      <c r="E214" s="162"/>
-      <c r="F214" s="119"/>
-    </row>
-    <row r="215" spans="1:6" ht="32" x14ac:dyDescent="0.2">
-      <c r="A215" s="116" t="s">
+      <c r="B219" s="161"/>
+      <c r="C219" s="161"/>
+      <c r="D219" s="161"/>
+      <c r="E219" s="162"/>
+      <c r="F219" s="119"/>
+    </row>
+    <row r="220" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+      <c r="A220" s="116" t="s">
         <v>243</v>
       </c>
-      <c r="B215" s="116" t="s">
+      <c r="B220" s="116" t="s">
         <v>840</v>
       </c>
-      <c r="C215" s="117" t="s">
+      <c r="C220" s="117" t="s">
         <v>841</v>
       </c>
-      <c r="D215" s="116" t="s">
+      <c r="D220" s="116" t="s">
         <v>842</v>
       </c>
-      <c r="E215" s="120" t="s">
+      <c r="E220" s="120" t="s">
         <v>843</v>
       </c>
-      <c r="F215" s="119"/>
-    </row>
-    <row r="216" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A216" s="116" t="s">
+      <c r="F220" s="119"/>
+    </row>
+    <row r="221" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A221" s="116" t="s">
         <v>416</v>
       </c>
-      <c r="B216" s="116" t="s">
+      <c r="B221" s="116" t="s">
         <v>844</v>
       </c>
-      <c r="C216" s="117" t="s">
+      <c r="C221" s="117" t="s">
         <v>56</v>
       </c>
-      <c r="D216" s="116"/>
-      <c r="E216" s="120" t="s">
+      <c r="D221" s="116"/>
+      <c r="E221" s="120" t="s">
         <v>58</v>
       </c>
-      <c r="F216" s="119"/>
-    </row>
-    <row r="217" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A217" s="116" t="s">
+      <c r="F221" s="119"/>
+    </row>
+    <row r="222" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A222" s="116" t="s">
         <v>416</v>
       </c>
-      <c r="B217" s="116" t="s">
+      <c r="B222" s="116" t="s">
         <v>845</v>
       </c>
-      <c r="C217" s="117" t="s">
+      <c r="C222" s="117" t="s">
         <v>60</v>
       </c>
-      <c r="D217" s="116"/>
-      <c r="E217" s="120" t="s">
+      <c r="D222" s="116"/>
+      <c r="E222" s="120" t="s">
         <v>62</v>
       </c>
-      <c r="F217" s="119"/>
-    </row>
-    <row r="218" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A218" s="116" t="s">
+      <c r="F222" s="119"/>
+    </row>
+    <row r="223" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A223" s="116" t="s">
         <v>416</v>
       </c>
-      <c r="B218" s="116" t="s">
+      <c r="B223" s="116" t="s">
         <v>846</v>
       </c>
-      <c r="C218" s="117" t="s">
+      <c r="C223" s="117" t="s">
         <v>64</v>
       </c>
-      <c r="D218" s="116"/>
-      <c r="E218" s="120" t="s">
+      <c r="D223" s="116"/>
+      <c r="E223" s="120" t="s">
         <v>66</v>
       </c>
-      <c r="F218" s="119"/>
-    </row>
-    <row r="219" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A219" s="116" t="s">
+      <c r="F223" s="119"/>
+    </row>
+    <row r="224" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A224" s="116" t="s">
         <v>416</v>
       </c>
-      <c r="B219" s="116" t="s">
+      <c r="B224" s="116" t="s">
         <v>847</v>
       </c>
-      <c r="C219" s="117" t="s">
+      <c r="C224" s="117" t="s">
         <v>68</v>
       </c>
-      <c r="D219" s="116"/>
-      <c r="E219" s="120" t="s">
+      <c r="D224" s="116"/>
+      <c r="E224" s="120" t="s">
         <v>70</v>
       </c>
-      <c r="F219" s="119"/>
-    </row>
-    <row r="220" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A220" s="116" t="s">
+      <c r="F224" s="119"/>
+    </row>
+    <row r="225" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A225" s="116" t="s">
         <v>416</v>
       </c>
-      <c r="B220" s="116" t="s">
+      <c r="B225" s="116" t="s">
         <v>848</v>
       </c>
-      <c r="C220" s="117" t="s">
+      <c r="C225" s="117" t="s">
         <v>39</v>
       </c>
-      <c r="D220" s="116"/>
-      <c r="E220" s="120" t="s">
+      <c r="D225" s="116"/>
+      <c r="E225" s="120" t="s">
         <v>41</v>
       </c>
-      <c r="F220" s="119"/>
-    </row>
-    <row r="221" spans="1:6" ht="64" x14ac:dyDescent="0.2">
-      <c r="A221" s="116" t="s">
+      <c r="F225" s="119"/>
+    </row>
+    <row r="226" spans="1:6" ht="64" x14ac:dyDescent="0.2">
+      <c r="A226" s="116" t="s">
         <v>410</v>
       </c>
-      <c r="B221" s="116" t="s">
+      <c r="B226" s="116" t="s">
         <v>849</v>
       </c>
-      <c r="C221" s="120"/>
-      <c r="D221" s="20" t="s">
+      <c r="C226" s="120"/>
+      <c r="D226" s="20" t="s">
         <v>788</v>
       </c>
-      <c r="E221" s="120"/>
-      <c r="F221" s="119"/>
-    </row>
-    <row r="222" spans="1:6" ht="64" x14ac:dyDescent="0.2">
-      <c r="A222" s="116" t="s">
+      <c r="E226" s="120"/>
+      <c r="F226" s="119"/>
+    </row>
+    <row r="227" spans="1:6" ht="64" x14ac:dyDescent="0.2">
+      <c r="A227" s="116" t="s">
         <v>413</v>
       </c>
-      <c r="B222" s="116" t="s">
+      <c r="B227" s="116" t="s">
         <v>850</v>
       </c>
-      <c r="C222" s="120"/>
-      <c r="D222" s="20" t="s">
+      <c r="C227" s="120"/>
+      <c r="D227" s="20" t="s">
         <v>790</v>
       </c>
-      <c r="E222" s="120"/>
-      <c r="F222" s="119"/>
-    </row>
-    <row r="223" spans="1:6" ht="48" x14ac:dyDescent="0.2">
-      <c r="A223" s="116" t="s">
-        <v>410</v>
-      </c>
-      <c r="B223" s="116" t="s">
-        <v>851</v>
-      </c>
-      <c r="C223" s="120"/>
-      <c r="D223" s="20" t="s">
-        <v>792</v>
-      </c>
-      <c r="E223" s="120"/>
-      <c r="F223" s="119"/>
-    </row>
-    <row r="224" spans="1:6" ht="64" x14ac:dyDescent="0.2">
-      <c r="A224" s="116" t="s">
-        <v>413</v>
-      </c>
-      <c r="B224" s="116" t="s">
-        <v>852</v>
-      </c>
-      <c r="C224" s="120"/>
-      <c r="D224" s="20" t="s">
-        <v>794</v>
-      </c>
-      <c r="E224" s="120"/>
-      <c r="F224" s="119"/>
-    </row>
-    <row r="225" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A225" s="160" t="s">
-        <v>853</v>
-      </c>
-      <c r="B225" s="161"/>
-      <c r="C225" s="161"/>
-      <c r="D225" s="161"/>
-      <c r="E225" s="162"/>
-      <c r="F225" s="119"/>
-    </row>
-    <row r="226" spans="1:6" ht="48" x14ac:dyDescent="0.2">
-      <c r="A226" s="116" t="s">
-        <v>243</v>
-      </c>
-      <c r="B226" s="116" t="s">
-        <v>854</v>
-      </c>
-      <c r="C226" s="117" t="s">
-        <v>855</v>
-      </c>
-      <c r="D226" s="116" t="s">
-        <v>856</v>
-      </c>
-      <c r="E226" s="120" t="s">
-        <v>857</v>
-      </c>
-      <c r="F226" s="38" t="s">
-        <v>858</v>
-      </c>
-    </row>
-    <row r="227" spans="1:6" ht="48" x14ac:dyDescent="0.2">
-      <c r="A227" s="116" t="s">
-        <v>368</v>
-      </c>
-      <c r="B227" s="116" t="s">
-        <v>859</v>
-      </c>
-      <c r="C227" s="117" t="s">
-        <v>860</v>
-      </c>
-      <c r="D227" s="116" t="s">
-        <v>861</v>
-      </c>
-      <c r="E227" s="120" t="s">
-        <v>862</v>
-      </c>
+      <c r="E227" s="120"/>
       <c r="F227" s="119"/>
     </row>
     <row r="228" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A228" s="116" t="s">
+        <v>410</v>
+      </c>
+      <c r="B228" s="116" t="s">
+        <v>851</v>
+      </c>
+      <c r="C228" s="120"/>
+      <c r="D228" s="20" t="s">
+        <v>792</v>
+      </c>
+      <c r="E228" s="120"/>
+      <c r="F228" s="119"/>
+    </row>
+    <row r="229" spans="1:6" ht="64" x14ac:dyDescent="0.2">
+      <c r="A229" s="116" t="s">
+        <v>413</v>
+      </c>
+      <c r="B229" s="116" t="s">
+        <v>852</v>
+      </c>
+      <c r="C229" s="120"/>
+      <c r="D229" s="20" t="s">
+        <v>794</v>
+      </c>
+      <c r="E229" s="120"/>
+      <c r="F229" s="119"/>
+    </row>
+    <row r="230" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A230" s="160" t="s">
+        <v>853</v>
+      </c>
+      <c r="B230" s="161"/>
+      <c r="C230" s="161"/>
+      <c r="D230" s="161"/>
+      <c r="E230" s="162"/>
+      <c r="F230" s="119"/>
+    </row>
+    <row r="231" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+      <c r="A231" s="116" t="s">
+        <v>243</v>
+      </c>
+      <c r="B231" s="116" t="s">
+        <v>854</v>
+      </c>
+      <c r="C231" s="117" t="s">
+        <v>855</v>
+      </c>
+      <c r="D231" s="116" t="s">
+        <v>856</v>
+      </c>
+      <c r="E231" s="120" t="s">
+        <v>857</v>
+      </c>
+      <c r="F231" s="38" t="s">
+        <v>858</v>
+      </c>
+    </row>
+    <row r="232" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+      <c r="A232" s="116" t="s">
+        <v>368</v>
+      </c>
+      <c r="B232" s="116" t="s">
+        <v>859</v>
+      </c>
+      <c r="C232" s="117" t="s">
+        <v>860</v>
+      </c>
+      <c r="D232" s="116" t="s">
+        <v>861</v>
+      </c>
+      <c r="E232" s="120" t="s">
+        <v>862</v>
+      </c>
+      <c r="F232" s="119"/>
+    </row>
+    <row r="233" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+      <c r="A233" s="116" t="s">
         <v>261</v>
       </c>
-      <c r="B228" s="116" t="s">
+      <c r="B233" s="116" t="s">
         <v>863</v>
       </c>
-      <c r="C228" s="59" t="s">
+      <c r="C233" s="59" t="s">
         <v>1394</v>
       </c>
-      <c r="D228" s="116" t="s">
+      <c r="D233" s="116" t="s">
         <v>864</v>
       </c>
-      <c r="E228" s="120" t="s">
+      <c r="E233" s="120" t="s">
         <v>1395</v>
-      </c>
-      <c r="F228" s="119"/>
-    </row>
-    <row r="229" spans="1:6" ht="32" x14ac:dyDescent="0.2">
-      <c r="A229" s="116" t="s">
-        <v>382</v>
-      </c>
-      <c r="B229" s="116" t="s">
-        <v>865</v>
-      </c>
-      <c r="C229" s="117" t="s">
-        <v>866</v>
-      </c>
-      <c r="D229" s="121" t="s">
-        <v>867</v>
-      </c>
-      <c r="E229" s="120" t="s">
-        <v>868</v>
-      </c>
-      <c r="F229" s="119"/>
-    </row>
-    <row r="230" spans="1:6" ht="32" x14ac:dyDescent="0.2">
-      <c r="A230" s="116" t="s">
-        <v>382</v>
-      </c>
-      <c r="B230" s="116" t="s">
-        <v>869</v>
-      </c>
-      <c r="C230" s="117" t="s">
-        <v>384</v>
-      </c>
-      <c r="D230" s="121" t="s">
-        <v>870</v>
-      </c>
-      <c r="E230" s="120" t="s">
-        <v>386</v>
-      </c>
-      <c r="F230" s="119"/>
-    </row>
-    <row r="231" spans="1:6" ht="32" x14ac:dyDescent="0.2">
-      <c r="A231" s="116" t="s">
-        <v>382</v>
-      </c>
-      <c r="B231" s="116" t="s">
-        <v>871</v>
-      </c>
-      <c r="C231" s="117" t="s">
-        <v>872</v>
-      </c>
-      <c r="D231" s="121" t="s">
-        <v>873</v>
-      </c>
-      <c r="E231" s="120" t="s">
-        <v>874</v>
-      </c>
-      <c r="F231" s="119"/>
-    </row>
-    <row r="232" spans="1:6" ht="64" x14ac:dyDescent="0.2">
-      <c r="A232" s="116" t="s">
-        <v>382</v>
-      </c>
-      <c r="B232" s="116" t="s">
-        <v>875</v>
-      </c>
-      <c r="C232" s="117" t="s">
-        <v>876</v>
-      </c>
-      <c r="D232" s="121" t="s">
-        <v>877</v>
-      </c>
-      <c r="E232" s="120" t="s">
-        <v>878</v>
-      </c>
-      <c r="F232" s="119"/>
-    </row>
-    <row r="233" spans="1:6" ht="32" x14ac:dyDescent="0.2">
-      <c r="A233" s="116" t="s">
-        <v>382</v>
-      </c>
-      <c r="B233" s="116" t="s">
-        <v>879</v>
-      </c>
-      <c r="C233" s="117" t="s">
-        <v>880</v>
-      </c>
-      <c r="D233" s="121" t="s">
-        <v>881</v>
-      </c>
-      <c r="E233" s="120" t="s">
-        <v>882</v>
       </c>
       <c r="F233" s="119"/>
     </row>
     <row r="234" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A234" s="116" t="s">
-        <v>490</v>
+        <v>382</v>
       </c>
       <c r="B234" s="116" t="s">
-        <v>883</v>
+        <v>865</v>
       </c>
       <c r="C234" s="117" t="s">
-        <v>884</v>
+        <v>866</v>
       </c>
       <c r="D234" s="121" t="s">
-        <v>881</v>
+        <v>867</v>
       </c>
       <c r="E234" s="120" t="s">
-        <v>885</v>
+        <v>868</v>
       </c>
       <c r="F234" s="119"/>
     </row>
-    <row r="235" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+    <row r="235" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A235" s="116" t="s">
         <v>382</v>
       </c>
       <c r="B235" s="116" t="s">
-        <v>886</v>
+        <v>869</v>
       </c>
       <c r="C235" s="117" t="s">
-        <v>887</v>
+        <v>384</v>
       </c>
       <c r="D235" s="121" t="s">
-        <v>888</v>
+        <v>870</v>
       </c>
       <c r="E235" s="120" t="s">
-        <v>889</v>
+        <v>386</v>
       </c>
       <c r="F235" s="119"/>
     </row>
@@ -14478,180 +14499,235 @@
         <v>382</v>
       </c>
       <c r="B236" s="116" t="s">
-        <v>890</v>
+        <v>871</v>
       </c>
       <c r="C236" s="117" t="s">
-        <v>317</v>
+        <v>872</v>
       </c>
       <c r="D236" s="121" t="s">
-        <v>891</v>
+        <v>873</v>
       </c>
       <c r="E236" s="120" t="s">
-        <v>319</v>
+        <v>874</v>
       </c>
       <c r="F236" s="119"/>
     </row>
-    <row r="237" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+    <row r="237" spans="1:6" ht="64" x14ac:dyDescent="0.2">
       <c r="A237" s="116" t="s">
         <v>382</v>
       </c>
       <c r="B237" s="116" t="s">
-        <v>892</v>
+        <v>875</v>
       </c>
       <c r="C237" s="117" t="s">
-        <v>893</v>
+        <v>876</v>
       </c>
       <c r="D237" s="121" t="s">
-        <v>894</v>
+        <v>877</v>
       </c>
       <c r="E237" s="120" t="s">
-        <v>895</v>
+        <v>878</v>
       </c>
       <c r="F237" s="119"/>
     </row>
-    <row r="238" spans="1:6" ht="96" x14ac:dyDescent="0.2">
+    <row r="238" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A238" s="116" t="s">
         <v>382</v>
       </c>
       <c r="B238" s="116" t="s">
+        <v>879</v>
+      </c>
+      <c r="C238" s="117" t="s">
+        <v>880</v>
+      </c>
+      <c r="D238" s="121" t="s">
+        <v>881</v>
+      </c>
+      <c r="E238" s="120" t="s">
+        <v>882</v>
+      </c>
+      <c r="F238" s="119"/>
+    </row>
+    <row r="239" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+      <c r="A239" s="116" t="s">
+        <v>490</v>
+      </c>
+      <c r="B239" s="116" t="s">
+        <v>883</v>
+      </c>
+      <c r="C239" s="117" t="s">
+        <v>884</v>
+      </c>
+      <c r="D239" s="121" t="s">
+        <v>881</v>
+      </c>
+      <c r="E239" s="120" t="s">
+        <v>885</v>
+      </c>
+      <c r="F239" s="119"/>
+    </row>
+    <row r="240" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+      <c r="A240" s="116" t="s">
+        <v>382</v>
+      </c>
+      <c r="B240" s="116" t="s">
+        <v>886</v>
+      </c>
+      <c r="C240" s="117" t="s">
+        <v>887</v>
+      </c>
+      <c r="D240" s="121" t="s">
+        <v>888</v>
+      </c>
+      <c r="E240" s="120" t="s">
+        <v>889</v>
+      </c>
+      <c r="F240" s="119"/>
+    </row>
+    <row r="241" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+      <c r="A241" s="116" t="s">
+        <v>382</v>
+      </c>
+      <c r="B241" s="116" t="s">
+        <v>890</v>
+      </c>
+      <c r="C241" s="117" t="s">
+        <v>317</v>
+      </c>
+      <c r="D241" s="121" t="s">
+        <v>891</v>
+      </c>
+      <c r="E241" s="120" t="s">
+        <v>319</v>
+      </c>
+      <c r="F241" s="119"/>
+    </row>
+    <row r="242" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+      <c r="A242" s="116" t="s">
+        <v>382</v>
+      </c>
+      <c r="B242" s="116" t="s">
+        <v>892</v>
+      </c>
+      <c r="C242" s="117" t="s">
+        <v>893</v>
+      </c>
+      <c r="D242" s="121" t="s">
+        <v>894</v>
+      </c>
+      <c r="E242" s="120" t="s">
+        <v>895</v>
+      </c>
+      <c r="F242" s="119"/>
+    </row>
+    <row r="243" spans="1:6" ht="96" x14ac:dyDescent="0.2">
+      <c r="A243" s="116" t="s">
+        <v>382</v>
+      </c>
+      <c r="B243" s="116" t="s">
         <v>896</v>
       </c>
-      <c r="C238" s="117" t="s">
+      <c r="C243" s="117" t="s">
         <v>897</v>
       </c>
-      <c r="D238" s="121" t="s">
+      <c r="D243" s="121" t="s">
         <v>898</v>
       </c>
-      <c r="E238" s="120" t="s">
+      <c r="E243" s="120" t="s">
         <v>899</v>
       </c>
-      <c r="F238" s="119"/>
-    </row>
-    <row r="239" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A239" s="5"/>
-      <c r="B239" s="5"/>
-      <c r="C239" s="6" t="s">
-        <v>900</v>
-      </c>
-      <c r="D239" s="5"/>
-      <c r="E239" s="37"/>
-      <c r="F239" s="68" t="s">
-        <v>901</v>
-      </c>
-    </row>
-    <row r="240" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A240" s="5"/>
-      <c r="B240" s="5"/>
-      <c r="C240" s="6"/>
-      <c r="D240" s="5"/>
-      <c r="E240" s="37"/>
-    </row>
-    <row r="241" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A241" s="5"/>
-      <c r="B241" s="5"/>
-      <c r="C241" s="6"/>
-      <c r="D241" s="5"/>
-      <c r="E241" s="37"/>
-    </row>
-    <row r="242" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A242" s="5"/>
-      <c r="B242" s="5"/>
-      <c r="C242" s="6"/>
-      <c r="D242" s="5"/>
-      <c r="E242" s="37"/>
-    </row>
-    <row r="243" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A243" s="5"/>
-      <c r="B243" s="5"/>
-      <c r="C243" s="6"/>
-      <c r="D243" s="5"/>
-      <c r="E243" s="37"/>
-    </row>
-    <row r="244" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F243" s="119"/>
+    </row>
+    <row r="244" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A244" s="5"/>
       <c r="B244" s="5"/>
-      <c r="C244" s="6"/>
+      <c r="C244" s="6" t="s">
+        <v>900</v>
+      </c>
       <c r="D244" s="5"/>
       <c r="E244" s="37"/>
-    </row>
-    <row r="245" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F244" s="68" t="s">
+        <v>901</v>
+      </c>
+    </row>
+    <row r="245" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A245" s="5"/>
       <c r="B245" s="5"/>
       <c r="C245" s="6"/>
       <c r="D245" s="5"/>
       <c r="E245" s="37"/>
     </row>
-    <row r="246" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="246" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A246" s="5"/>
       <c r="B246" s="5"/>
       <c r="C246" s="6"/>
       <c r="D246" s="5"/>
       <c r="E246" s="37"/>
     </row>
-    <row r="247" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="247" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A247" s="5"/>
       <c r="B247" s="5"/>
       <c r="C247" s="6"/>
       <c r="D247" s="5"/>
       <c r="E247" s="37"/>
     </row>
-    <row r="248" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="248" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A248" s="5"/>
       <c r="B248" s="5"/>
       <c r="C248" s="6"/>
       <c r="D248" s="5"/>
       <c r="E248" s="37"/>
     </row>
-    <row r="249" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="249" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A249" s="5"/>
       <c r="B249" s="5"/>
       <c r="C249" s="6"/>
       <c r="D249" s="5"/>
       <c r="E249" s="37"/>
     </row>
-    <row r="250" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="250" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A250" s="5"/>
       <c r="B250" s="5"/>
       <c r="C250" s="6"/>
       <c r="D250" s="5"/>
       <c r="E250" s="37"/>
     </row>
-    <row r="251" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="251" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A251" s="5"/>
       <c r="B251" s="5"/>
       <c r="C251" s="6"/>
       <c r="D251" s="5"/>
       <c r="E251" s="37"/>
     </row>
-    <row r="252" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="252" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A252" s="5"/>
       <c r="B252" s="5"/>
       <c r="C252" s="6"/>
       <c r="D252" s="5"/>
       <c r="E252" s="37"/>
     </row>
-    <row r="253" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="253" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A253" s="5"/>
       <c r="B253" s="5"/>
       <c r="C253" s="6"/>
       <c r="D253" s="5"/>
       <c r="E253" s="37"/>
     </row>
-    <row r="254" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="254" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A254" s="5"/>
       <c r="B254" s="5"/>
       <c r="C254" s="6"/>
       <c r="D254" s="5"/>
       <c r="E254" s="37"/>
     </row>
-    <row r="255" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="255" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A255" s="5"/>
       <c r="B255" s="5"/>
       <c r="C255" s="6"/>
       <c r="D255" s="5"/>
       <c r="E255" s="37"/>
     </row>
-    <row r="256" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="256" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A256" s="5"/>
       <c r="B256" s="5"/>
       <c r="C256" s="6"/>
@@ -15281,30 +15357,65 @@
       <c r="D345" s="5"/>
       <c r="E345" s="37"/>
     </row>
+    <row r="346" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A346" s="5"/>
+      <c r="B346" s="5"/>
+      <c r="C346" s="6"/>
+      <c r="D346" s="5"/>
+      <c r="E346" s="37"/>
+    </row>
+    <row r="347" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A347" s="5"/>
+      <c r="B347" s="5"/>
+      <c r="C347" s="6"/>
+      <c r="D347" s="5"/>
+      <c r="E347" s="37"/>
+    </row>
+    <row r="348" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A348" s="5"/>
+      <c r="B348" s="5"/>
+      <c r="C348" s="6"/>
+      <c r="D348" s="5"/>
+      <c r="E348" s="37"/>
+    </row>
+    <row r="349" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A349" s="5"/>
+      <c r="B349" s="5"/>
+      <c r="C349" s="6"/>
+      <c r="D349" s="5"/>
+      <c r="E349" s="37"/>
+    </row>
+    <row r="350" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A350" s="5"/>
+      <c r="B350" s="5"/>
+      <c r="C350" s="6"/>
+      <c r="D350" s="5"/>
+      <c r="E350" s="37"/>
+    </row>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="A174:E174"/>
-    <mergeCell ref="A157:E157"/>
-    <mergeCell ref="A63:E63"/>
-    <mergeCell ref="A67:E67"/>
-    <mergeCell ref="A82:E82"/>
-    <mergeCell ref="A123:E123"/>
-    <mergeCell ref="A137:E137"/>
-    <mergeCell ref="A146:E146"/>
-    <mergeCell ref="A92:E92"/>
-    <mergeCell ref="A165:E165"/>
+    <mergeCell ref="A230:E230"/>
+    <mergeCell ref="A191:E191"/>
+    <mergeCell ref="A195:E195"/>
+    <mergeCell ref="A202:E202"/>
+    <mergeCell ref="A213:E213"/>
+    <mergeCell ref="A219:E219"/>
     <mergeCell ref="A58:E58"/>
     <mergeCell ref="A2:E2"/>
     <mergeCell ref="A10:E10"/>
     <mergeCell ref="A14:E14"/>
     <mergeCell ref="A24:E24"/>
     <mergeCell ref="A43:E43"/>
-    <mergeCell ref="A225:E225"/>
-    <mergeCell ref="A186:E186"/>
-    <mergeCell ref="A190:E190"/>
-    <mergeCell ref="A197:E197"/>
-    <mergeCell ref="A208:E208"/>
-    <mergeCell ref="A214:E214"/>
+    <mergeCell ref="A179:E179"/>
+    <mergeCell ref="A162:E162"/>
+    <mergeCell ref="A63:E63"/>
+    <mergeCell ref="A67:E67"/>
+    <mergeCell ref="A82:E82"/>
+    <mergeCell ref="A128:E128"/>
+    <mergeCell ref="A142:E142"/>
+    <mergeCell ref="A151:E151"/>
+    <mergeCell ref="A92:E92"/>
+    <mergeCell ref="A170:E170"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -17606,6 +17717,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <Readyforteam_x003f_ xmlns="565e1b1d-057e-4d85-b896-01a5881d8a45">false</Readyforteam_x003f_>
@@ -17646,15 +17766,6 @@
 </p:properties>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EAFDB110-4046-4E72-A1EF-1908ABEC3151}">
   <ds:schemaRefs>
@@ -17677,6 +17788,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8D7CE8C7-18DC-484F-8376-ED09F13D44C8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{017ACE96-8143-486E-8436-7787F6B96F4A}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -17687,12 +17806,4 @@
     <ds:schemaRef ds:uri="2799d30d-6731-4efe-ac9b-c4895a8828d9"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8D7CE8C7-18DC-484F-8376-ED09F13D44C8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
[MCCDB-946] Content amend - Cause of death
</commit_message>
<xml_diff>
--- a/app/data/MCCD-localisation.xlsx
+++ b/app/data/MCCD-localisation.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10414"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10512"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/JALAT/GIT/medical-certificate-of-cause-of-death/app/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63986951-DC2E-5843-9F26-6D07FE7486F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1E793BE-5F50-264E-A780-33F35D2187B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="14100" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -5632,12 +5632,6 @@
     <t>codO28SectionTitleOneDescription</t>
   </si>
   <si>
-    <t>Other significant condition contributing to the death but &lt;strong&gt;not&lt;/strong&gt; relating to the disease or condition causing it.</t>
-  </si>
-  <si>
-    <t>Cyflwr arwyddocaol arall sy'n cyfrannu at y farwolaeth ond &lt;strong&gt;nid yw'n&lt;/strong&gt; ymwneud â'r clefyd na'r cyflwr sy'n ei achosi.</t>
-  </si>
-  <si>
     <t>The disease or condition thought to be the underlying cause of death should appear in the lowest completed line of part 1.</t>
   </si>
   <si>
@@ -5647,12 +5641,6 @@
     <t>Achos y farwolaeth (1)</t>
   </si>
   <si>
-    <t>2 Other significant condition (optional)</t>
-  </si>
-  <si>
-    <t>2 Cyflwr arwyddocaol arall (dewisol)</t>
-  </si>
-  <si>
     <t>Declaration</t>
   </si>
   <si>
@@ -5704,7 +5692,19 @@
     <t>dpdEthnicityNotStatedOther</t>
   </si>
   <si>
-    <t>029</t>
+    <t>Other significant conditions contributing to the death but &lt;strong&gt;not&lt;/strong&gt; relating to the disease or condition causing it.</t>
+  </si>
+  <si>
+    <t>2 Other significant conditions (optional)</t>
+  </si>
+  <si>
+    <t>Cyflyrau arwyddocaol eraill sy'n cyfrannu at y farwolaeth ond &lt;strong&gt;nid yw'n&lt;/strong&gt; ymwneud â'r clefyd neu'r cyflwr sy'n ei achosi.</t>
+  </si>
+  <si>
+    <t>2 Amgylchiadau arwyddocaol eraill (dewisol)</t>
+  </si>
+  <si>
+    <t>030</t>
   </si>
 </sst>
 </file>
@@ -6648,6 +6648,18 @@
     <xf numFmtId="0" fontId="9" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -6660,6 +6672,24 @@
     <xf numFmtId="0" fontId="13" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -6669,24 +6699,6 @@
     <xf numFmtId="0" fontId="6" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
@@ -6758,18 +6770,6 @@
     </xf>
     <xf numFmtId="0" fontId="13" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -7154,538 +7154,538 @@
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A1" s="159" t="s">
+      <c r="A1" s="163" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="159"/>
-      <c r="C1" s="159"/>
-      <c r="D1" s="159"/>
-      <c r="E1" s="159"/>
-      <c r="F1" s="159"/>
-      <c r="G1" s="159"/>
-      <c r="H1" s="159"/>
-      <c r="I1" s="159"/>
-      <c r="J1" s="159"/>
-      <c r="K1" s="159"/>
-      <c r="L1" s="159"/>
+      <c r="B1" s="163"/>
+      <c r="C1" s="163"/>
+      <c r="D1" s="163"/>
+      <c r="E1" s="163"/>
+      <c r="F1" s="163"/>
+      <c r="G1" s="163"/>
+      <c r="H1" s="163"/>
+      <c r="I1" s="163"/>
+      <c r="J1" s="163"/>
+      <c r="K1" s="163"/>
+      <c r="L1" s="163"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A2" s="159"/>
-      <c r="B2" s="159"/>
-      <c r="C2" s="159"/>
-      <c r="D2" s="159"/>
-      <c r="E2" s="159"/>
-      <c r="F2" s="159"/>
-      <c r="G2" s="159"/>
-      <c r="H2" s="159"/>
-      <c r="I2" s="159"/>
-      <c r="J2" s="159"/>
-      <c r="K2" s="159"/>
-      <c r="L2" s="159"/>
+      <c r="A2" s="163"/>
+      <c r="B2" s="163"/>
+      <c r="C2" s="163"/>
+      <c r="D2" s="163"/>
+      <c r="E2" s="163"/>
+      <c r="F2" s="163"/>
+      <c r="G2" s="163"/>
+      <c r="H2" s="163"/>
+      <c r="I2" s="163"/>
+      <c r="J2" s="163"/>
+      <c r="K2" s="163"/>
+      <c r="L2" s="163"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A3" s="159"/>
-      <c r="B3" s="159"/>
-      <c r="C3" s="159"/>
-      <c r="D3" s="159"/>
-      <c r="E3" s="159"/>
-      <c r="F3" s="159"/>
-      <c r="G3" s="159"/>
-      <c r="H3" s="159"/>
-      <c r="I3" s="159"/>
-      <c r="J3" s="159"/>
-      <c r="K3" s="159"/>
-      <c r="L3" s="159"/>
+      <c r="A3" s="163"/>
+      <c r="B3" s="163"/>
+      <c r="C3" s="163"/>
+      <c r="D3" s="163"/>
+      <c r="E3" s="163"/>
+      <c r="F3" s="163"/>
+      <c r="G3" s="163"/>
+      <c r="H3" s="163"/>
+      <c r="I3" s="163"/>
+      <c r="J3" s="163"/>
+      <c r="K3" s="163"/>
+      <c r="L3" s="163"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A4" s="159"/>
-      <c r="B4" s="159"/>
-      <c r="C4" s="159"/>
-      <c r="D4" s="159"/>
-      <c r="E4" s="159"/>
-      <c r="F4" s="159"/>
-      <c r="G4" s="159"/>
-      <c r="H4" s="159"/>
-      <c r="I4" s="159"/>
-      <c r="J4" s="159"/>
-      <c r="K4" s="159"/>
-      <c r="L4" s="159"/>
+      <c r="A4" s="163"/>
+      <c r="B4" s="163"/>
+      <c r="C4" s="163"/>
+      <c r="D4" s="163"/>
+      <c r="E4" s="163"/>
+      <c r="F4" s="163"/>
+      <c r="G4" s="163"/>
+      <c r="H4" s="163"/>
+      <c r="I4" s="163"/>
+      <c r="J4" s="163"/>
+      <c r="K4" s="163"/>
+      <c r="L4" s="163"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A5" s="159"/>
-      <c r="B5" s="159"/>
-      <c r="C5" s="159"/>
-      <c r="D5" s="159"/>
-      <c r="E5" s="159"/>
-      <c r="F5" s="159"/>
-      <c r="G5" s="159"/>
-      <c r="H5" s="159"/>
-      <c r="I5" s="159"/>
-      <c r="J5" s="159"/>
-      <c r="K5" s="159"/>
-      <c r="L5" s="159"/>
+      <c r="A5" s="163"/>
+      <c r="B5" s="163"/>
+      <c r="C5" s="163"/>
+      <c r="D5" s="163"/>
+      <c r="E5" s="163"/>
+      <c r="F5" s="163"/>
+      <c r="G5" s="163"/>
+      <c r="H5" s="163"/>
+      <c r="I5" s="163"/>
+      <c r="J5" s="163"/>
+      <c r="K5" s="163"/>
+      <c r="L5" s="163"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A6" s="159"/>
-      <c r="B6" s="159"/>
-      <c r="C6" s="159"/>
-      <c r="D6" s="159"/>
-      <c r="E6" s="159"/>
-      <c r="F6" s="159"/>
-      <c r="G6" s="159"/>
-      <c r="H6" s="159"/>
-      <c r="I6" s="159"/>
-      <c r="J6" s="159"/>
-      <c r="K6" s="159"/>
-      <c r="L6" s="159"/>
+      <c r="A6" s="163"/>
+      <c r="B6" s="163"/>
+      <c r="C6" s="163"/>
+      <c r="D6" s="163"/>
+      <c r="E6" s="163"/>
+      <c r="F6" s="163"/>
+      <c r="G6" s="163"/>
+      <c r="H6" s="163"/>
+      <c r="I6" s="163"/>
+      <c r="J6" s="163"/>
+      <c r="K6" s="163"/>
+      <c r="L6" s="163"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A7" s="159"/>
-      <c r="B7" s="159"/>
-      <c r="C7" s="159"/>
-      <c r="D7" s="159"/>
-      <c r="E7" s="159"/>
-      <c r="F7" s="159"/>
-      <c r="G7" s="159"/>
-      <c r="H7" s="159"/>
-      <c r="I7" s="159"/>
-      <c r="J7" s="159"/>
-      <c r="K7" s="159"/>
-      <c r="L7" s="159"/>
+      <c r="A7" s="163"/>
+      <c r="B7" s="163"/>
+      <c r="C7" s="163"/>
+      <c r="D7" s="163"/>
+      <c r="E7" s="163"/>
+      <c r="F7" s="163"/>
+      <c r="G7" s="163"/>
+      <c r="H7" s="163"/>
+      <c r="I7" s="163"/>
+      <c r="J7" s="163"/>
+      <c r="K7" s="163"/>
+      <c r="L7" s="163"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A8" s="159"/>
-      <c r="B8" s="159"/>
-      <c r="C8" s="159"/>
-      <c r="D8" s="159"/>
-      <c r="E8" s="159"/>
-      <c r="F8" s="159"/>
-      <c r="G8" s="159"/>
-      <c r="H8" s="159"/>
-      <c r="I8" s="159"/>
-      <c r="J8" s="159"/>
-      <c r="K8" s="159"/>
-      <c r="L8" s="159"/>
+      <c r="A8" s="163"/>
+      <c r="B8" s="163"/>
+      <c r="C8" s="163"/>
+      <c r="D8" s="163"/>
+      <c r="E8" s="163"/>
+      <c r="F8" s="163"/>
+      <c r="G8" s="163"/>
+      <c r="H8" s="163"/>
+      <c r="I8" s="163"/>
+      <c r="J8" s="163"/>
+      <c r="K8" s="163"/>
+      <c r="L8" s="163"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A9" s="159"/>
-      <c r="B9" s="159"/>
-      <c r="C9" s="159"/>
-      <c r="D9" s="159"/>
-      <c r="E9" s="159"/>
-      <c r="F9" s="159"/>
-      <c r="G9" s="159"/>
-      <c r="H9" s="159"/>
-      <c r="I9" s="159"/>
-      <c r="J9" s="159"/>
-      <c r="K9" s="159"/>
-      <c r="L9" s="159"/>
+      <c r="A9" s="163"/>
+      <c r="B9" s="163"/>
+      <c r="C9" s="163"/>
+      <c r="D9" s="163"/>
+      <c r="E9" s="163"/>
+      <c r="F9" s="163"/>
+      <c r="G9" s="163"/>
+      <c r="H9" s="163"/>
+      <c r="I9" s="163"/>
+      <c r="J9" s="163"/>
+      <c r="K9" s="163"/>
+      <c r="L9" s="163"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A10" s="159"/>
-      <c r="B10" s="159"/>
-      <c r="C10" s="159"/>
-      <c r="D10" s="159"/>
-      <c r="E10" s="159"/>
-      <c r="F10" s="159"/>
-      <c r="G10" s="159"/>
-      <c r="H10" s="159"/>
-      <c r="I10" s="159"/>
-      <c r="J10" s="159"/>
-      <c r="K10" s="159"/>
-      <c r="L10" s="159"/>
+      <c r="A10" s="163"/>
+      <c r="B10" s="163"/>
+      <c r="C10" s="163"/>
+      <c r="D10" s="163"/>
+      <c r="E10" s="163"/>
+      <c r="F10" s="163"/>
+      <c r="G10" s="163"/>
+      <c r="H10" s="163"/>
+      <c r="I10" s="163"/>
+      <c r="J10" s="163"/>
+      <c r="K10" s="163"/>
+      <c r="L10" s="163"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A11" s="159"/>
-      <c r="B11" s="159"/>
-      <c r="C11" s="159"/>
-      <c r="D11" s="159"/>
-      <c r="E11" s="159"/>
-      <c r="F11" s="159"/>
-      <c r="G11" s="159"/>
-      <c r="H11" s="159"/>
-      <c r="I11" s="159"/>
-      <c r="J11" s="159"/>
-      <c r="K11" s="159"/>
-      <c r="L11" s="159"/>
+      <c r="A11" s="163"/>
+      <c r="B11" s="163"/>
+      <c r="C11" s="163"/>
+      <c r="D11" s="163"/>
+      <c r="E11" s="163"/>
+      <c r="F11" s="163"/>
+      <c r="G11" s="163"/>
+      <c r="H11" s="163"/>
+      <c r="I11" s="163"/>
+      <c r="J11" s="163"/>
+      <c r="K11" s="163"/>
+      <c r="L11" s="163"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A12" s="159"/>
-      <c r="B12" s="159"/>
-      <c r="C12" s="159"/>
-      <c r="D12" s="159"/>
-      <c r="E12" s="159"/>
-      <c r="F12" s="159"/>
-      <c r="G12" s="159"/>
-      <c r="H12" s="159"/>
-      <c r="I12" s="159"/>
-      <c r="J12" s="159"/>
-      <c r="K12" s="159"/>
-      <c r="L12" s="159"/>
+      <c r="A12" s="163"/>
+      <c r="B12" s="163"/>
+      <c r="C12" s="163"/>
+      <c r="D12" s="163"/>
+      <c r="E12" s="163"/>
+      <c r="F12" s="163"/>
+      <c r="G12" s="163"/>
+      <c r="H12" s="163"/>
+      <c r="I12" s="163"/>
+      <c r="J12" s="163"/>
+      <c r="K12" s="163"/>
+      <c r="L12" s="163"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A13" s="159"/>
-      <c r="B13" s="159"/>
-      <c r="C13" s="159"/>
-      <c r="D13" s="159"/>
-      <c r="E13" s="159"/>
-      <c r="F13" s="159"/>
-      <c r="G13" s="159"/>
-      <c r="H13" s="159"/>
-      <c r="I13" s="159"/>
-      <c r="J13" s="159"/>
-      <c r="K13" s="159"/>
-      <c r="L13" s="159"/>
+      <c r="A13" s="163"/>
+      <c r="B13" s="163"/>
+      <c r="C13" s="163"/>
+      <c r="D13" s="163"/>
+      <c r="E13" s="163"/>
+      <c r="F13" s="163"/>
+      <c r="G13" s="163"/>
+      <c r="H13" s="163"/>
+      <c r="I13" s="163"/>
+      <c r="J13" s="163"/>
+      <c r="K13" s="163"/>
+      <c r="L13" s="163"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A14" s="159"/>
-      <c r="B14" s="159"/>
-      <c r="C14" s="159"/>
-      <c r="D14" s="159"/>
-      <c r="E14" s="159"/>
-      <c r="F14" s="159"/>
-      <c r="G14" s="159"/>
-      <c r="H14" s="159"/>
-      <c r="I14" s="159"/>
-      <c r="J14" s="159"/>
-      <c r="K14" s="159"/>
-      <c r="L14" s="159"/>
+      <c r="A14" s="163"/>
+      <c r="B14" s="163"/>
+      <c r="C14" s="163"/>
+      <c r="D14" s="163"/>
+      <c r="E14" s="163"/>
+      <c r="F14" s="163"/>
+      <c r="G14" s="163"/>
+      <c r="H14" s="163"/>
+      <c r="I14" s="163"/>
+      <c r="J14" s="163"/>
+      <c r="K14" s="163"/>
+      <c r="L14" s="163"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A15" s="159"/>
-      <c r="B15" s="159"/>
-      <c r="C15" s="159"/>
-      <c r="D15" s="159"/>
-      <c r="E15" s="159"/>
-      <c r="F15" s="159"/>
-      <c r="G15" s="159"/>
-      <c r="H15" s="159"/>
-      <c r="I15" s="159"/>
-      <c r="J15" s="159"/>
-      <c r="K15" s="159"/>
-      <c r="L15" s="159"/>
+      <c r="A15" s="163"/>
+      <c r="B15" s="163"/>
+      <c r="C15" s="163"/>
+      <c r="D15" s="163"/>
+      <c r="E15" s="163"/>
+      <c r="F15" s="163"/>
+      <c r="G15" s="163"/>
+      <c r="H15" s="163"/>
+      <c r="I15" s="163"/>
+      <c r="J15" s="163"/>
+      <c r="K15" s="163"/>
+      <c r="L15" s="163"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A16" s="159"/>
-      <c r="B16" s="159"/>
-      <c r="C16" s="159"/>
-      <c r="D16" s="159"/>
-      <c r="E16" s="159"/>
-      <c r="F16" s="159"/>
-      <c r="G16" s="159"/>
-      <c r="H16" s="159"/>
-      <c r="I16" s="159"/>
-      <c r="J16" s="159"/>
-      <c r="K16" s="159"/>
-      <c r="L16" s="159"/>
+      <c r="A16" s="163"/>
+      <c r="B16" s="163"/>
+      <c r="C16" s="163"/>
+      <c r="D16" s="163"/>
+      <c r="E16" s="163"/>
+      <c r="F16" s="163"/>
+      <c r="G16" s="163"/>
+      <c r="H16" s="163"/>
+      <c r="I16" s="163"/>
+      <c r="J16" s="163"/>
+      <c r="K16" s="163"/>
+      <c r="L16" s="163"/>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A17" s="159"/>
-      <c r="B17" s="159"/>
-      <c r="C17" s="159"/>
-      <c r="D17" s="159"/>
-      <c r="E17" s="159"/>
-      <c r="F17" s="159"/>
-      <c r="G17" s="159"/>
-      <c r="H17" s="159"/>
-      <c r="I17" s="159"/>
-      <c r="J17" s="159"/>
-      <c r="K17" s="159"/>
-      <c r="L17" s="159"/>
+      <c r="A17" s="163"/>
+      <c r="B17" s="163"/>
+      <c r="C17" s="163"/>
+      <c r="D17" s="163"/>
+      <c r="E17" s="163"/>
+      <c r="F17" s="163"/>
+      <c r="G17" s="163"/>
+      <c r="H17" s="163"/>
+      <c r="I17" s="163"/>
+      <c r="J17" s="163"/>
+      <c r="K17" s="163"/>
+      <c r="L17" s="163"/>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A18" s="159"/>
-      <c r="B18" s="159"/>
-      <c r="C18" s="159"/>
-      <c r="D18" s="159"/>
-      <c r="E18" s="159"/>
-      <c r="F18" s="159"/>
-      <c r="G18" s="159"/>
-      <c r="H18" s="159"/>
-      <c r="I18" s="159"/>
-      <c r="J18" s="159"/>
-      <c r="K18" s="159"/>
-      <c r="L18" s="159"/>
+      <c r="A18" s="163"/>
+      <c r="B18" s="163"/>
+      <c r="C18" s="163"/>
+      <c r="D18" s="163"/>
+      <c r="E18" s="163"/>
+      <c r="F18" s="163"/>
+      <c r="G18" s="163"/>
+      <c r="H18" s="163"/>
+      <c r="I18" s="163"/>
+      <c r="J18" s="163"/>
+      <c r="K18" s="163"/>
+      <c r="L18" s="163"/>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A19" s="159"/>
-      <c r="B19" s="159"/>
-      <c r="C19" s="159"/>
-      <c r="D19" s="159"/>
-      <c r="E19" s="159"/>
-      <c r="F19" s="159"/>
-      <c r="G19" s="159"/>
-      <c r="H19" s="159"/>
-      <c r="I19" s="159"/>
-      <c r="J19" s="159"/>
-      <c r="K19" s="159"/>
-      <c r="L19" s="159"/>
+      <c r="A19" s="163"/>
+      <c r="B19" s="163"/>
+      <c r="C19" s="163"/>
+      <c r="D19" s="163"/>
+      <c r="E19" s="163"/>
+      <c r="F19" s="163"/>
+      <c r="G19" s="163"/>
+      <c r="H19" s="163"/>
+      <c r="I19" s="163"/>
+      <c r="J19" s="163"/>
+      <c r="K19" s="163"/>
+      <c r="L19" s="163"/>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A20" s="159"/>
-      <c r="B20" s="159"/>
-      <c r="C20" s="159"/>
-      <c r="D20" s="159"/>
-      <c r="E20" s="159"/>
-      <c r="F20" s="159"/>
-      <c r="G20" s="159"/>
-      <c r="H20" s="159"/>
-      <c r="I20" s="159"/>
-      <c r="J20" s="159"/>
-      <c r="K20" s="159"/>
-      <c r="L20" s="159"/>
+      <c r="A20" s="163"/>
+      <c r="B20" s="163"/>
+      <c r="C20" s="163"/>
+      <c r="D20" s="163"/>
+      <c r="E20" s="163"/>
+      <c r="F20" s="163"/>
+      <c r="G20" s="163"/>
+      <c r="H20" s="163"/>
+      <c r="I20" s="163"/>
+      <c r="J20" s="163"/>
+      <c r="K20" s="163"/>
+      <c r="L20" s="163"/>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A21" s="159"/>
-      <c r="B21" s="159"/>
-      <c r="C21" s="159"/>
-      <c r="D21" s="159"/>
-      <c r="E21" s="159"/>
-      <c r="F21" s="159"/>
-      <c r="G21" s="159"/>
-      <c r="H21" s="159"/>
-      <c r="I21" s="159"/>
-      <c r="J21" s="159"/>
-      <c r="K21" s="159"/>
-      <c r="L21" s="159"/>
+      <c r="A21" s="163"/>
+      <c r="B21" s="163"/>
+      <c r="C21" s="163"/>
+      <c r="D21" s="163"/>
+      <c r="E21" s="163"/>
+      <c r="F21" s="163"/>
+      <c r="G21" s="163"/>
+      <c r="H21" s="163"/>
+      <c r="I21" s="163"/>
+      <c r="J21" s="163"/>
+      <c r="K21" s="163"/>
+      <c r="L21" s="163"/>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A22" s="159"/>
-      <c r="B22" s="159"/>
-      <c r="C22" s="159"/>
-      <c r="D22" s="159"/>
-      <c r="E22" s="159"/>
-      <c r="F22" s="159"/>
-      <c r="G22" s="159"/>
-      <c r="H22" s="159"/>
-      <c r="I22" s="159"/>
-      <c r="J22" s="159"/>
-      <c r="K22" s="159"/>
-      <c r="L22" s="159"/>
+      <c r="A22" s="163"/>
+      <c r="B22" s="163"/>
+      <c r="C22" s="163"/>
+      <c r="D22" s="163"/>
+      <c r="E22" s="163"/>
+      <c r="F22" s="163"/>
+      <c r="G22" s="163"/>
+      <c r="H22" s="163"/>
+      <c r="I22" s="163"/>
+      <c r="J22" s="163"/>
+      <c r="K22" s="163"/>
+      <c r="L22" s="163"/>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A23" s="159"/>
-      <c r="B23" s="159"/>
-      <c r="C23" s="159"/>
-      <c r="D23" s="159"/>
-      <c r="E23" s="159"/>
-      <c r="F23" s="159"/>
-      <c r="G23" s="159"/>
-      <c r="H23" s="159"/>
-      <c r="I23" s="159"/>
-      <c r="J23" s="159"/>
-      <c r="K23" s="159"/>
-      <c r="L23" s="159"/>
+      <c r="A23" s="163"/>
+      <c r="B23" s="163"/>
+      <c r="C23" s="163"/>
+      <c r="D23" s="163"/>
+      <c r="E23" s="163"/>
+      <c r="F23" s="163"/>
+      <c r="G23" s="163"/>
+      <c r="H23" s="163"/>
+      <c r="I23" s="163"/>
+      <c r="J23" s="163"/>
+      <c r="K23" s="163"/>
+      <c r="L23" s="163"/>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A24" s="159"/>
-      <c r="B24" s="159"/>
-      <c r="C24" s="159"/>
-      <c r="D24" s="159"/>
-      <c r="E24" s="159"/>
-      <c r="F24" s="159"/>
-      <c r="G24" s="159"/>
-      <c r="H24" s="159"/>
-      <c r="I24" s="159"/>
-      <c r="J24" s="159"/>
-      <c r="K24" s="159"/>
-      <c r="L24" s="159"/>
+      <c r="A24" s="163"/>
+      <c r="B24" s="163"/>
+      <c r="C24" s="163"/>
+      <c r="D24" s="163"/>
+      <c r="E24" s="163"/>
+      <c r="F24" s="163"/>
+      <c r="G24" s="163"/>
+      <c r="H24" s="163"/>
+      <c r="I24" s="163"/>
+      <c r="J24" s="163"/>
+      <c r="K24" s="163"/>
+      <c r="L24" s="163"/>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A25" s="159"/>
-      <c r="B25" s="159"/>
-      <c r="C25" s="159"/>
-      <c r="D25" s="159"/>
-      <c r="E25" s="159"/>
-      <c r="F25" s="159"/>
-      <c r="G25" s="159"/>
-      <c r="H25" s="159"/>
-      <c r="I25" s="159"/>
-      <c r="J25" s="159"/>
-      <c r="K25" s="159"/>
-      <c r="L25" s="159"/>
+      <c r="A25" s="163"/>
+      <c r="B25" s="163"/>
+      <c r="C25" s="163"/>
+      <c r="D25" s="163"/>
+      <c r="E25" s="163"/>
+      <c r="F25" s="163"/>
+      <c r="G25" s="163"/>
+      <c r="H25" s="163"/>
+      <c r="I25" s="163"/>
+      <c r="J25" s="163"/>
+      <c r="K25" s="163"/>
+      <c r="L25" s="163"/>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A26" s="159"/>
-      <c r="B26" s="159"/>
-      <c r="C26" s="159"/>
-      <c r="D26" s="159"/>
-      <c r="E26" s="159"/>
-      <c r="F26" s="159"/>
-      <c r="G26" s="159"/>
-      <c r="H26" s="159"/>
-      <c r="I26" s="159"/>
-      <c r="J26" s="159"/>
-      <c r="K26" s="159"/>
-      <c r="L26" s="159"/>
+      <c r="A26" s="163"/>
+      <c r="B26" s="163"/>
+      <c r="C26" s="163"/>
+      <c r="D26" s="163"/>
+      <c r="E26" s="163"/>
+      <c r="F26" s="163"/>
+      <c r="G26" s="163"/>
+      <c r="H26" s="163"/>
+      <c r="I26" s="163"/>
+      <c r="J26" s="163"/>
+      <c r="K26" s="163"/>
+      <c r="L26" s="163"/>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A27" s="159"/>
-      <c r="B27" s="159"/>
-      <c r="C27" s="159"/>
-      <c r="D27" s="159"/>
-      <c r="E27" s="159"/>
-      <c r="F27" s="159"/>
-      <c r="G27" s="159"/>
-      <c r="H27" s="159"/>
-      <c r="I27" s="159"/>
-      <c r="J27" s="159"/>
-      <c r="K27" s="159"/>
-      <c r="L27" s="159"/>
+      <c r="A27" s="163"/>
+      <c r="B27" s="163"/>
+      <c r="C27" s="163"/>
+      <c r="D27" s="163"/>
+      <c r="E27" s="163"/>
+      <c r="F27" s="163"/>
+      <c r="G27" s="163"/>
+      <c r="H27" s="163"/>
+      <c r="I27" s="163"/>
+      <c r="J27" s="163"/>
+      <c r="K27" s="163"/>
+      <c r="L27" s="163"/>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A28" s="159"/>
-      <c r="B28" s="159"/>
-      <c r="C28" s="159"/>
-      <c r="D28" s="159"/>
-      <c r="E28" s="159"/>
-      <c r="F28" s="159"/>
-      <c r="G28" s="159"/>
-      <c r="H28" s="159"/>
-      <c r="I28" s="159"/>
-      <c r="J28" s="159"/>
-      <c r="K28" s="159"/>
-      <c r="L28" s="159"/>
+      <c r="A28" s="163"/>
+      <c r="B28" s="163"/>
+      <c r="C28" s="163"/>
+      <c r="D28" s="163"/>
+      <c r="E28" s="163"/>
+      <c r="F28" s="163"/>
+      <c r="G28" s="163"/>
+      <c r="H28" s="163"/>
+      <c r="I28" s="163"/>
+      <c r="J28" s="163"/>
+      <c r="K28" s="163"/>
+      <c r="L28" s="163"/>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A29" s="159"/>
-      <c r="B29" s="159"/>
-      <c r="C29" s="159"/>
-      <c r="D29" s="159"/>
-      <c r="E29" s="159"/>
-      <c r="F29" s="159"/>
-      <c r="G29" s="159"/>
-      <c r="H29" s="159"/>
-      <c r="I29" s="159"/>
-      <c r="J29" s="159"/>
-      <c r="K29" s="159"/>
-      <c r="L29" s="159"/>
+      <c r="A29" s="163"/>
+      <c r="B29" s="163"/>
+      <c r="C29" s="163"/>
+      <c r="D29" s="163"/>
+      <c r="E29" s="163"/>
+      <c r="F29" s="163"/>
+      <c r="G29" s="163"/>
+      <c r="H29" s="163"/>
+      <c r="I29" s="163"/>
+      <c r="J29" s="163"/>
+      <c r="K29" s="163"/>
+      <c r="L29" s="163"/>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A30" s="159"/>
-      <c r="B30" s="159"/>
-      <c r="C30" s="159"/>
-      <c r="D30" s="159"/>
-      <c r="E30" s="159"/>
-      <c r="F30" s="159"/>
-      <c r="G30" s="159"/>
-      <c r="H30" s="159"/>
-      <c r="I30" s="159"/>
-      <c r="J30" s="159"/>
-      <c r="K30" s="159"/>
-      <c r="L30" s="159"/>
+      <c r="A30" s="163"/>
+      <c r="B30" s="163"/>
+      <c r="C30" s="163"/>
+      <c r="D30" s="163"/>
+      <c r="E30" s="163"/>
+      <c r="F30" s="163"/>
+      <c r="G30" s="163"/>
+      <c r="H30" s="163"/>
+      <c r="I30" s="163"/>
+      <c r="J30" s="163"/>
+      <c r="K30" s="163"/>
+      <c r="L30" s="163"/>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A31" s="159"/>
-      <c r="B31" s="159"/>
-      <c r="C31" s="159"/>
-      <c r="D31" s="159"/>
-      <c r="E31" s="159"/>
-      <c r="F31" s="159"/>
-      <c r="G31" s="159"/>
-      <c r="H31" s="159"/>
-      <c r="I31" s="159"/>
-      <c r="J31" s="159"/>
-      <c r="K31" s="159"/>
-      <c r="L31" s="159"/>
+      <c r="A31" s="163"/>
+      <c r="B31" s="163"/>
+      <c r="C31" s="163"/>
+      <c r="D31" s="163"/>
+      <c r="E31" s="163"/>
+      <c r="F31" s="163"/>
+      <c r="G31" s="163"/>
+      <c r="H31" s="163"/>
+      <c r="I31" s="163"/>
+      <c r="J31" s="163"/>
+      <c r="K31" s="163"/>
+      <c r="L31" s="163"/>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A32" s="159"/>
-      <c r="B32" s="159"/>
-      <c r="C32" s="159"/>
-      <c r="D32" s="159"/>
-      <c r="E32" s="159"/>
-      <c r="F32" s="159"/>
-      <c r="G32" s="159"/>
-      <c r="H32" s="159"/>
-      <c r="I32" s="159"/>
-      <c r="J32" s="159"/>
-      <c r="K32" s="159"/>
-      <c r="L32" s="159"/>
+      <c r="A32" s="163"/>
+      <c r="B32" s="163"/>
+      <c r="C32" s="163"/>
+      <c r="D32" s="163"/>
+      <c r="E32" s="163"/>
+      <c r="F32" s="163"/>
+      <c r="G32" s="163"/>
+      <c r="H32" s="163"/>
+      <c r="I32" s="163"/>
+      <c r="J32" s="163"/>
+      <c r="K32" s="163"/>
+      <c r="L32" s="163"/>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A33" s="159"/>
-      <c r="B33" s="159"/>
-      <c r="C33" s="159"/>
-      <c r="D33" s="159"/>
-      <c r="E33" s="159"/>
-      <c r="F33" s="159"/>
-      <c r="G33" s="159"/>
-      <c r="H33" s="159"/>
-      <c r="I33" s="159"/>
-      <c r="J33" s="159"/>
-      <c r="K33" s="159"/>
-      <c r="L33" s="159"/>
+      <c r="A33" s="163"/>
+      <c r="B33" s="163"/>
+      <c r="C33" s="163"/>
+      <c r="D33" s="163"/>
+      <c r="E33" s="163"/>
+      <c r="F33" s="163"/>
+      <c r="G33" s="163"/>
+      <c r="H33" s="163"/>
+      <c r="I33" s="163"/>
+      <c r="J33" s="163"/>
+      <c r="K33" s="163"/>
+      <c r="L33" s="163"/>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A34" s="159"/>
-      <c r="B34" s="159"/>
-      <c r="C34" s="159"/>
-      <c r="D34" s="159"/>
-      <c r="E34" s="159"/>
-      <c r="F34" s="159"/>
-      <c r="G34" s="159"/>
-      <c r="H34" s="159"/>
-      <c r="I34" s="159"/>
-      <c r="J34" s="159"/>
-      <c r="K34" s="159"/>
-      <c r="L34" s="159"/>
+      <c r="A34" s="163"/>
+      <c r="B34" s="163"/>
+      <c r="C34" s="163"/>
+      <c r="D34" s="163"/>
+      <c r="E34" s="163"/>
+      <c r="F34" s="163"/>
+      <c r="G34" s="163"/>
+      <c r="H34" s="163"/>
+      <c r="I34" s="163"/>
+      <c r="J34" s="163"/>
+      <c r="K34" s="163"/>
+      <c r="L34" s="163"/>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A35" s="159"/>
-      <c r="B35" s="159"/>
-      <c r="C35" s="159"/>
-      <c r="D35" s="159"/>
-      <c r="E35" s="159"/>
-      <c r="F35" s="159"/>
-      <c r="G35" s="159"/>
-      <c r="H35" s="159"/>
-      <c r="I35" s="159"/>
-      <c r="J35" s="159"/>
-      <c r="K35" s="159"/>
-      <c r="L35" s="159"/>
+      <c r="A35" s="163"/>
+      <c r="B35" s="163"/>
+      <c r="C35" s="163"/>
+      <c r="D35" s="163"/>
+      <c r="E35" s="163"/>
+      <c r="F35" s="163"/>
+      <c r="G35" s="163"/>
+      <c r="H35" s="163"/>
+      <c r="I35" s="163"/>
+      <c r="J35" s="163"/>
+      <c r="K35" s="163"/>
+      <c r="L35" s="163"/>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A36" s="159"/>
-      <c r="B36" s="159"/>
-      <c r="C36" s="159"/>
-      <c r="D36" s="159"/>
-      <c r="E36" s="159"/>
-      <c r="F36" s="159"/>
-      <c r="G36" s="159"/>
-      <c r="H36" s="159"/>
-      <c r="I36" s="159"/>
-      <c r="J36" s="159"/>
-      <c r="K36" s="159"/>
-      <c r="L36" s="159"/>
+      <c r="A36" s="163"/>
+      <c r="B36" s="163"/>
+      <c r="C36" s="163"/>
+      <c r="D36" s="163"/>
+      <c r="E36" s="163"/>
+      <c r="F36" s="163"/>
+      <c r="G36" s="163"/>
+      <c r="H36" s="163"/>
+      <c r="I36" s="163"/>
+      <c r="J36" s="163"/>
+      <c r="K36" s="163"/>
+      <c r="L36" s="163"/>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A37" s="159"/>
-      <c r="B37" s="159"/>
-      <c r="C37" s="159"/>
-      <c r="D37" s="159"/>
-      <c r="E37" s="159"/>
-      <c r="F37" s="159"/>
-      <c r="G37" s="159"/>
-      <c r="H37" s="159"/>
-      <c r="I37" s="159"/>
-      <c r="J37" s="159"/>
-      <c r="K37" s="159"/>
-      <c r="L37" s="159"/>
+      <c r="A37" s="163"/>
+      <c r="B37" s="163"/>
+      <c r="C37" s="163"/>
+      <c r="D37" s="163"/>
+      <c r="E37" s="163"/>
+      <c r="F37" s="163"/>
+      <c r="G37" s="163"/>
+      <c r="H37" s="163"/>
+      <c r="I37" s="163"/>
+      <c r="J37" s="163"/>
+      <c r="K37" s="163"/>
+      <c r="L37" s="163"/>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A38" s="159"/>
-      <c r="B38" s="159"/>
-      <c r="C38" s="159"/>
-      <c r="D38" s="159"/>
-      <c r="E38" s="159"/>
-      <c r="F38" s="159"/>
-      <c r="G38" s="159"/>
-      <c r="H38" s="159"/>
-      <c r="I38" s="159"/>
-      <c r="J38" s="159"/>
-      <c r="K38" s="159"/>
-      <c r="L38" s="159"/>
+      <c r="A38" s="163"/>
+      <c r="B38" s="163"/>
+      <c r="C38" s="163"/>
+      <c r="D38" s="163"/>
+      <c r="E38" s="163"/>
+      <c r="F38" s="163"/>
+      <c r="G38" s="163"/>
+      <c r="H38" s="163"/>
+      <c r="I38" s="163"/>
+      <c r="J38" s="163"/>
+      <c r="K38" s="163"/>
+      <c r="L38" s="163"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -7964,13 +7964,13 @@
         <v>1241</v>
       </c>
       <c r="C2" s="151" t="s">
-        <v>1424</v>
+        <v>1420</v>
       </c>
       <c r="D2" s="92" t="s">
         <v>1242</v>
       </c>
       <c r="E2" s="152" t="s">
-        <v>1428</v>
+        <v>1424</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="80" x14ac:dyDescent="0.2">
@@ -7998,13 +7998,13 @@
         <v>1248</v>
       </c>
       <c r="C4" s="158" t="s">
-        <v>1425</v>
+        <v>1421</v>
       </c>
       <c r="D4" s="95" t="s">
         <v>404</v>
       </c>
       <c r="E4" s="155" t="s">
-        <v>1427</v>
+        <v>1423</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="60.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -8066,13 +8066,13 @@
         <v>1253</v>
       </c>
       <c r="C8" s="158" t="s">
-        <v>1424</v>
+        <v>1420</v>
       </c>
       <c r="D8" s="95" t="s">
         <v>1254</v>
       </c>
       <c r="E8" s="155" t="s">
-        <v>1428</v>
+        <v>1424</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="64" x14ac:dyDescent="0.2">
@@ -8100,13 +8100,13 @@
         <v>1259</v>
       </c>
       <c r="C10" s="158" t="s">
-        <v>1425</v>
+        <v>1421</v>
       </c>
       <c r="D10" s="95" t="s">
         <v>404</v>
       </c>
       <c r="E10" s="155" t="s">
-        <v>1427</v>
+        <v>1423</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -8168,13 +8168,13 @@
         <v>1262</v>
       </c>
       <c r="C14" s="158" t="s">
-        <v>1424</v>
+        <v>1420</v>
       </c>
       <c r="D14" s="95" t="s">
         <v>1263</v>
       </c>
       <c r="E14" s="155" t="s">
-        <v>1426</v>
+        <v>1422</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="96" x14ac:dyDescent="0.2">
@@ -8236,13 +8236,13 @@
         <v>1270</v>
       </c>
       <c r="C18" s="158" t="s">
-        <v>1425</v>
+        <v>1421</v>
       </c>
       <c r="D18" s="95" t="s">
         <v>404</v>
       </c>
       <c r="E18" s="155" t="s">
-        <v>1427</v>
+        <v>1423</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -8270,13 +8270,13 @@
         <v>1271</v>
       </c>
       <c r="C20" s="158" t="s">
-        <v>1424</v>
+        <v>1420</v>
       </c>
       <c r="D20" s="95" t="s">
         <v>1242</v>
       </c>
       <c r="E20" s="155" t="s">
-        <v>1426</v>
+        <v>1422</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="48" x14ac:dyDescent="0.2">
@@ -8304,13 +8304,13 @@
         <v>1275</v>
       </c>
       <c r="C22" s="158" t="s">
-        <v>1425</v>
+        <v>1421</v>
       </c>
       <c r="D22" s="95" t="s">
         <v>404</v>
       </c>
       <c r="E22" s="155" t="s">
-        <v>1429</v>
+        <v>1425</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="48" x14ac:dyDescent="0.2">
@@ -8393,14 +8393,14 @@
       </c>
     </row>
     <row r="2" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="194" t="s">
+      <c r="A2" s="198" t="s">
         <v>1278</v>
       </c>
-      <c r="B2" s="195"/>
-      <c r="C2" s="195"/>
-      <c r="D2" s="195"/>
-      <c r="E2" s="195"/>
-      <c r="F2" s="195"/>
+      <c r="B2" s="199"/>
+      <c r="C2" s="199"/>
+      <c r="D2" s="199"/>
+      <c r="E2" s="199"/>
+      <c r="F2" s="199"/>
     </row>
     <row r="3" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
@@ -8483,10 +8483,10 @@
         <v>1295</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>1434</v>
+        <v>1430</v>
       </c>
       <c r="E8" s="37" t="s">
-        <v>1435</v>
+        <v>1431</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="16" x14ac:dyDescent="0.2">
@@ -8567,11 +8567,11 @@
         <v>1312</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>1432</v>
+        <v>1428</v>
       </c>
       <c r="D14" s="1"/>
       <c r="E14" s="37" t="s">
-        <v>1433</v>
+        <v>1429</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="32" x14ac:dyDescent="0.2">
@@ -8620,14 +8620,14 @@
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A18" s="194" t="s">
+      <c r="A18" s="198" t="s">
         <v>1323</v>
       </c>
-      <c r="B18" s="195"/>
-      <c r="C18" s="195"/>
-      <c r="D18" s="195"/>
-      <c r="E18" s="195"/>
-      <c r="F18" s="195"/>
+      <c r="B18" s="199"/>
+      <c r="C18" s="199"/>
+      <c r="D18" s="199"/>
+      <c r="E18" s="199"/>
+      <c r="F18" s="199"/>
     </row>
     <row r="19" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A19" s="5" t="s">
@@ -8709,7 +8709,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C4" sqref="C4"/>
+      <selection pane="bottomLeft" activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -10167,13 +10167,13 @@
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" s="160" t="s">
+      <c r="A4" s="164" t="s">
         <v>1371</v>
       </c>
-      <c r="B4" s="161"/>
-      <c r="C4" s="161"/>
-      <c r="D4" s="161"/>
-      <c r="E4" s="162"/>
+      <c r="B4" s="165"/>
+      <c r="C4" s="165"/>
+      <c r="D4" s="165"/>
+      <c r="E4" s="166"/>
     </row>
     <row r="5" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
@@ -10927,13 +10927,13 @@
       </c>
     </row>
     <row r="2" spans="1:6" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="166" t="s">
+      <c r="A2" s="167" t="s">
         <v>367</v>
       </c>
-      <c r="B2" s="167"/>
-      <c r="C2" s="167"/>
-      <c r="D2" s="167"/>
-      <c r="E2" s="168"/>
+      <c r="B2" s="168"/>
+      <c r="C2" s="168"/>
+      <c r="D2" s="168"/>
+      <c r="E2" s="169"/>
       <c r="F2" s="33"/>
     </row>
     <row r="3" spans="1:6" ht="48" x14ac:dyDescent="0.2">
@@ -11061,13 +11061,13 @@
       <c r="F9" s="119"/>
     </row>
     <row r="10" spans="1:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="169" t="s">
+      <c r="A10" s="170" t="s">
         <v>396</v>
       </c>
-      <c r="B10" s="170"/>
-      <c r="C10" s="170"/>
-      <c r="D10" s="170"/>
-      <c r="E10" s="171"/>
+      <c r="B10" s="171"/>
+      <c r="C10" s="171"/>
+      <c r="D10" s="171"/>
+      <c r="E10" s="172"/>
       <c r="F10" s="119"/>
     </row>
     <row r="11" spans="1:6" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -11125,13 +11125,13 @@
       <c r="F13" s="86"/>
     </row>
     <row r="14" spans="1:6" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="160" t="s">
+      <c r="A14" s="164" t="s">
         <v>405</v>
       </c>
-      <c r="B14" s="161"/>
-      <c r="C14" s="161"/>
-      <c r="D14" s="161"/>
-      <c r="E14" s="162"/>
+      <c r="B14" s="165"/>
+      <c r="C14" s="165"/>
+      <c r="D14" s="165"/>
+      <c r="E14" s="166"/>
       <c r="F14" s="119"/>
     </row>
     <row r="15" spans="1:6" ht="48" x14ac:dyDescent="0.2">
@@ -11275,13 +11275,13 @@
       <c r="F23" s="119"/>
     </row>
     <row r="24" spans="1:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="160" t="s">
+      <c r="A24" s="164" t="s">
         <v>435</v>
       </c>
-      <c r="B24" s="161"/>
-      <c r="C24" s="161"/>
-      <c r="D24" s="161"/>
-      <c r="E24" s="162"/>
+      <c r="B24" s="165"/>
+      <c r="C24" s="165"/>
+      <c r="D24" s="165"/>
+      <c r="E24" s="166"/>
       <c r="F24" s="119"/>
     </row>
     <row r="25" spans="1:6" ht="32" x14ac:dyDescent="0.2">
@@ -11553,13 +11553,13 @@
       <c r="F42" s="119"/>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A43" s="160" t="s">
+      <c r="A43" s="164" t="s">
         <v>479</v>
       </c>
-      <c r="B43" s="161"/>
-      <c r="C43" s="161"/>
-      <c r="D43" s="161"/>
-      <c r="E43" s="162"/>
+      <c r="B43" s="165"/>
+      <c r="C43" s="165"/>
+      <c r="D43" s="165"/>
+      <c r="E43" s="166"/>
       <c r="F43" s="119"/>
     </row>
     <row r="44" spans="1:6" ht="32" x14ac:dyDescent="0.2">
@@ -11777,13 +11777,13 @@
       <c r="F57" s="119"/>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A58" s="160" t="s">
+      <c r="A58" s="164" t="s">
         <v>509</v>
       </c>
-      <c r="B58" s="161"/>
-      <c r="C58" s="161"/>
-      <c r="D58" s="161"/>
-      <c r="E58" s="162"/>
+      <c r="B58" s="165"/>
+      <c r="C58" s="165"/>
+      <c r="D58" s="165"/>
+      <c r="E58" s="166"/>
       <c r="F58" s="119"/>
     </row>
     <row r="59" spans="1:6" ht="64" x14ac:dyDescent="0.2">
@@ -11857,13 +11857,13 @@
       <c r="F62" s="119"/>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A63" s="160" t="s">
+      <c r="A63" s="164" t="s">
         <v>523</v>
       </c>
-      <c r="B63" s="161"/>
-      <c r="C63" s="161"/>
-      <c r="D63" s="161"/>
-      <c r="E63" s="162"/>
+      <c r="B63" s="165"/>
+      <c r="C63" s="165"/>
+      <c r="D63" s="165"/>
+      <c r="E63" s="166"/>
       <c r="F63" s="119"/>
     </row>
     <row r="64" spans="1:6" ht="48" x14ac:dyDescent="0.2">
@@ -11913,13 +11913,13 @@
       <c r="F66" s="119"/>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A67" s="160" t="s">
+      <c r="A67" s="164" t="s">
         <v>528</v>
       </c>
-      <c r="B67" s="161"/>
-      <c r="C67" s="161"/>
-      <c r="D67" s="161"/>
-      <c r="E67" s="162"/>
+      <c r="B67" s="165"/>
+      <c r="C67" s="165"/>
+      <c r="D67" s="165"/>
+      <c r="E67" s="166"/>
       <c r="F67" s="119"/>
     </row>
     <row r="68" spans="1:6" ht="32" x14ac:dyDescent="0.2">
@@ -12151,13 +12151,13 @@
       <c r="F81" s="119"/>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A82" s="160" t="s">
+      <c r="A82" s="164" t="s">
         <v>567</v>
       </c>
-      <c r="B82" s="161"/>
-      <c r="C82" s="161"/>
-      <c r="D82" s="161"/>
-      <c r="E82" s="162"/>
+      <c r="B82" s="165"/>
+      <c r="C82" s="165"/>
+      <c r="D82" s="165"/>
+      <c r="E82" s="166"/>
       <c r="F82" s="119"/>
     </row>
     <row r="83" spans="1:6" ht="62.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -12309,13 +12309,13 @@
       <c r="F91" s="119"/>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A92" s="160" t="s">
+      <c r="A92" s="164" t="s">
         <v>592</v>
       </c>
-      <c r="B92" s="161"/>
-      <c r="C92" s="161"/>
-      <c r="D92" s="161"/>
-      <c r="E92" s="162"/>
+      <c r="B92" s="165"/>
+      <c r="C92" s="165"/>
+      <c r="D92" s="165"/>
+      <c r="E92" s="166"/>
       <c r="F92" s="119"/>
     </row>
     <row r="93" spans="1:6" ht="48" x14ac:dyDescent="0.2">
@@ -12344,11 +12344,11 @@
         <v>597</v>
       </c>
       <c r="C94" s="117" t="s">
-        <v>1430</v>
+        <v>1426</v>
       </c>
       <c r="D94" s="116"/>
       <c r="E94" s="120" t="s">
-        <v>1431</v>
+        <v>1427</v>
       </c>
       <c r="F94" s="119" t="s">
         <v>573</v>
@@ -12378,8 +12378,8 @@
       <c r="A96" s="91" t="s">
         <v>84</v>
       </c>
-      <c r="B96" s="196" t="s">
-        <v>1436</v>
+      <c r="B96" s="159" t="s">
+        <v>1432</v>
       </c>
       <c r="C96" s="93" t="s">
         <v>599</v>
@@ -12396,8 +12396,8 @@
       <c r="A97" s="91" t="s">
         <v>84</v>
       </c>
-      <c r="B97" s="196" t="s">
-        <v>1437</v>
+      <c r="B97" s="159" t="s">
+        <v>1433</v>
       </c>
       <c r="C97" s="93" t="s">
         <v>599</v>
@@ -12414,14 +12414,14 @@
       <c r="A98" s="20" t="s">
         <v>84</v>
       </c>
-      <c r="B98" s="197" t="s">
-        <v>1438</v>
-      </c>
-      <c r="C98" s="198" t="s">
+      <c r="B98" s="160" t="s">
+        <v>1434</v>
+      </c>
+      <c r="C98" s="161" t="s">
         <v>599</v>
       </c>
-      <c r="D98" s="197"/>
-      <c r="E98" s="199" t="s">
+      <c r="D98" s="160"/>
+      <c r="E98" s="162" t="s">
         <v>1218</v>
       </c>
       <c r="F98" s="86"/>
@@ -12430,14 +12430,14 @@
       <c r="A99" s="20" t="s">
         <v>84</v>
       </c>
-      <c r="B99" s="197" t="s">
-        <v>1439</v>
-      </c>
-      <c r="C99" s="198" t="s">
+      <c r="B99" s="160" t="s">
+        <v>1435</v>
+      </c>
+      <c r="C99" s="161" t="s">
         <v>599</v>
       </c>
-      <c r="D99" s="197"/>
-      <c r="E99" s="199" t="s">
+      <c r="D99" s="160"/>
+      <c r="E99" s="162" t="s">
         <v>1218</v>
       </c>
       <c r="F99" s="86"/>
@@ -12446,14 +12446,14 @@
       <c r="A100" s="20" t="s">
         <v>84</v>
       </c>
-      <c r="B100" s="197" t="s">
-        <v>1440</v>
-      </c>
-      <c r="C100" s="198" t="s">
+      <c r="B100" s="160" t="s">
+        <v>1436</v>
+      </c>
+      <c r="C100" s="161" t="s">
         <v>599</v>
       </c>
-      <c r="D100" s="197"/>
-      <c r="E100" s="199" t="s">
+      <c r="D100" s="160"/>
+      <c r="E100" s="162" t="s">
         <v>1218</v>
       </c>
       <c r="F100" s="86"/>
@@ -12865,13 +12865,13 @@
       <c r="F127" s="119"/>
     </row>
     <row r="128" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A128" s="160" t="s">
+      <c r="A128" s="164" t="s">
         <v>678</v>
       </c>
-      <c r="B128" s="161"/>
-      <c r="C128" s="161"/>
-      <c r="D128" s="161"/>
-      <c r="E128" s="162"/>
+      <c r="B128" s="165"/>
+      <c r="C128" s="165"/>
+      <c r="D128" s="165"/>
+      <c r="E128" s="166"/>
       <c r="F128" s="119"/>
     </row>
     <row r="129" spans="1:6" ht="32" x14ac:dyDescent="0.2">
@@ -13059,13 +13059,13 @@
       <c r="F141" s="119"/>
     </row>
     <row r="142" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A142" s="160" t="s">
+      <c r="A142" s="164" t="s">
         <v>700</v>
       </c>
-      <c r="B142" s="161"/>
-      <c r="C142" s="161"/>
-      <c r="D142" s="161"/>
-      <c r="E142" s="162"/>
+      <c r="B142" s="165"/>
+      <c r="C142" s="165"/>
+      <c r="D142" s="165"/>
+      <c r="E142" s="166"/>
       <c r="F142" s="119"/>
     </row>
     <row r="143" spans="1:6" ht="64" x14ac:dyDescent="0.2">
@@ -13195,13 +13195,13 @@
       <c r="F150" s="119"/>
     </row>
     <row r="151" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A151" s="160" t="s">
+      <c r="A151" s="164" t="s">
         <v>721</v>
       </c>
-      <c r="B151" s="161"/>
-      <c r="C151" s="161"/>
-      <c r="D151" s="161"/>
-      <c r="E151" s="162"/>
+      <c r="B151" s="165"/>
+      <c r="C151" s="165"/>
+      <c r="D151" s="165"/>
+      <c r="E151" s="166"/>
       <c r="F151" s="119"/>
     </row>
     <row r="152" spans="1:6" ht="32" x14ac:dyDescent="0.2">
@@ -13361,13 +13361,13 @@
       <c r="F161" s="119"/>
     </row>
     <row r="162" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A162" s="160" t="s">
+      <c r="A162" s="164" t="s">
         <v>742</v>
       </c>
-      <c r="B162" s="161"/>
-      <c r="C162" s="161"/>
-      <c r="D162" s="161"/>
-      <c r="E162" s="162"/>
+      <c r="B162" s="165"/>
+      <c r="C162" s="165"/>
+      <c r="D162" s="165"/>
+      <c r="E162" s="166"/>
       <c r="F162" s="119"/>
     </row>
     <row r="163" spans="1:6" ht="48" x14ac:dyDescent="0.2">
@@ -13485,13 +13485,13 @@
       <c r="F169" s="119"/>
     </row>
     <row r="170" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A170" s="163" t="s">
+      <c r="A170" s="173" t="s">
         <v>762</v>
       </c>
-      <c r="B170" s="164"/>
-      <c r="C170" s="164"/>
-      <c r="D170" s="164"/>
-      <c r="E170" s="165"/>
+      <c r="B170" s="174"/>
+      <c r="C170" s="174"/>
+      <c r="D170" s="174"/>
+      <c r="E170" s="175"/>
       <c r="F170" s="129" t="s">
         <v>763</v>
       </c>
@@ -13617,13 +13617,13 @@
       </c>
     </row>
     <row r="179" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A179" s="160" t="s">
+      <c r="A179" s="164" t="s">
         <v>774</v>
       </c>
-      <c r="B179" s="161"/>
-      <c r="C179" s="161"/>
-      <c r="D179" s="161"/>
-      <c r="E179" s="162"/>
+      <c r="B179" s="165"/>
+      <c r="C179" s="165"/>
+      <c r="D179" s="165"/>
+      <c r="E179" s="166"/>
       <c r="F179" s="119"/>
     </row>
     <row r="180" spans="1:6" ht="32" x14ac:dyDescent="0.2">
@@ -13809,13 +13809,13 @@
       <c r="F190" s="119"/>
     </row>
     <row r="191" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A191" s="160" t="s">
+      <c r="A191" s="164" t="s">
         <v>795</v>
       </c>
-      <c r="B191" s="161"/>
-      <c r="C191" s="161"/>
-      <c r="D191" s="161"/>
-      <c r="E191" s="162"/>
+      <c r="B191" s="165"/>
+      <c r="C191" s="165"/>
+      <c r="D191" s="165"/>
+      <c r="E191" s="166"/>
       <c r="F191" s="119"/>
     </row>
     <row r="192" spans="1:6" ht="32" x14ac:dyDescent="0.2">
@@ -13865,13 +13865,13 @@
       <c r="F194" s="119"/>
     </row>
     <row r="195" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A195" s="160" t="s">
+      <c r="A195" s="164" t="s">
         <v>803</v>
       </c>
-      <c r="B195" s="161"/>
-      <c r="C195" s="161"/>
-      <c r="D195" s="161"/>
-      <c r="E195" s="162"/>
+      <c r="B195" s="165"/>
+      <c r="C195" s="165"/>
+      <c r="D195" s="165"/>
+      <c r="E195" s="166"/>
       <c r="F195" s="119"/>
     </row>
     <row r="196" spans="1:6" ht="64" x14ac:dyDescent="0.2">
@@ -13973,13 +13973,13 @@
       <c r="F201" s="119"/>
     </row>
     <row r="202" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A202" s="160" t="s">
+      <c r="A202" s="164" t="s">
         <v>818</v>
       </c>
-      <c r="B202" s="161"/>
-      <c r="C202" s="161"/>
-      <c r="D202" s="161"/>
-      <c r="E202" s="162"/>
+      <c r="B202" s="165"/>
+      <c r="C202" s="165"/>
+      <c r="D202" s="165"/>
+      <c r="E202" s="166"/>
       <c r="F202" s="119"/>
     </row>
     <row r="203" spans="1:6" ht="32" x14ac:dyDescent="0.2">
@@ -14137,13 +14137,13 @@
       <c r="F212" s="119"/>
     </row>
     <row r="213" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A213" s="160" t="s">
+      <c r="A213" s="164" t="s">
         <v>829</v>
       </c>
-      <c r="B213" s="161"/>
-      <c r="C213" s="161"/>
-      <c r="D213" s="161"/>
-      <c r="E213" s="162"/>
+      <c r="B213" s="165"/>
+      <c r="C213" s="165"/>
+      <c r="D213" s="165"/>
+      <c r="E213" s="166"/>
       <c r="F213" s="119"/>
     </row>
     <row r="214" spans="1:6" ht="48" x14ac:dyDescent="0.2">
@@ -14229,13 +14229,13 @@
       <c r="F218" s="119"/>
     </row>
     <row r="219" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A219" s="160" t="s">
+      <c r="A219" s="164" t="s">
         <v>839</v>
       </c>
-      <c r="B219" s="161"/>
-      <c r="C219" s="161"/>
-      <c r="D219" s="161"/>
-      <c r="E219" s="162"/>
+      <c r="B219" s="165"/>
+      <c r="C219" s="165"/>
+      <c r="D219" s="165"/>
+      <c r="E219" s="166"/>
       <c r="F219" s="119"/>
     </row>
     <row r="220" spans="1:6" ht="32" x14ac:dyDescent="0.2">
@@ -14393,13 +14393,13 @@
       <c r="F229" s="119"/>
     </row>
     <row r="230" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A230" s="160" t="s">
+      <c r="A230" s="164" t="s">
         <v>853</v>
       </c>
-      <c r="B230" s="161"/>
-      <c r="C230" s="161"/>
-      <c r="D230" s="161"/>
-      <c r="E230" s="162"/>
+      <c r="B230" s="165"/>
+      <c r="C230" s="165"/>
+      <c r="D230" s="165"/>
+      <c r="E230" s="166"/>
       <c r="F230" s="119"/>
     </row>
     <row r="231" spans="1:6" ht="48" x14ac:dyDescent="0.2">
@@ -15394,18 +15394,6 @@
     </row>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="A230:E230"/>
-    <mergeCell ref="A191:E191"/>
-    <mergeCell ref="A195:E195"/>
-    <mergeCell ref="A202:E202"/>
-    <mergeCell ref="A213:E213"/>
-    <mergeCell ref="A219:E219"/>
-    <mergeCell ref="A58:E58"/>
-    <mergeCell ref="A2:E2"/>
-    <mergeCell ref="A10:E10"/>
-    <mergeCell ref="A14:E14"/>
-    <mergeCell ref="A24:E24"/>
-    <mergeCell ref="A43:E43"/>
     <mergeCell ref="A179:E179"/>
     <mergeCell ref="A162:E162"/>
     <mergeCell ref="A63:E63"/>
@@ -15416,6 +15404,18 @@
     <mergeCell ref="A151:E151"/>
     <mergeCell ref="A92:E92"/>
     <mergeCell ref="A170:E170"/>
+    <mergeCell ref="A58:E58"/>
+    <mergeCell ref="A2:E2"/>
+    <mergeCell ref="A10:E10"/>
+    <mergeCell ref="A14:E14"/>
+    <mergeCell ref="A24:E24"/>
+    <mergeCell ref="A43:E43"/>
+    <mergeCell ref="A230:E230"/>
+    <mergeCell ref="A191:E191"/>
+    <mergeCell ref="A195:E195"/>
+    <mergeCell ref="A202:E202"/>
+    <mergeCell ref="A213:E213"/>
+    <mergeCell ref="A219:E219"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -15462,13 +15462,13 @@
       </c>
     </row>
     <row r="2" spans="1:6" s="24" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="175" t="s">
+      <c r="A2" s="179" t="s">
         <v>902</v>
       </c>
-      <c r="B2" s="176"/>
-      <c r="C2" s="176"/>
-      <c r="D2" s="176"/>
-      <c r="E2" s="177"/>
+      <c r="B2" s="180"/>
+      <c r="C2" s="180"/>
+      <c r="D2" s="180"/>
+      <c r="E2" s="181"/>
     </row>
     <row r="3" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="19" t="s">
@@ -15602,13 +15602,13 @@
       </c>
     </row>
     <row r="12" spans="1:6" s="24" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="175" t="s">
+      <c r="A12" s="179" t="s">
         <v>924</v>
       </c>
-      <c r="B12" s="176"/>
-      <c r="C12" s="176"/>
-      <c r="D12" s="176"/>
-      <c r="E12" s="177"/>
+      <c r="B12" s="180"/>
+      <c r="C12" s="180"/>
+      <c r="D12" s="180"/>
+      <c r="E12" s="181"/>
     </row>
     <row r="13" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A13" s="19" t="s">
@@ -15720,13 +15720,13 @@
       </c>
     </row>
     <row r="20" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="184" t="s">
+      <c r="A20" s="188" t="s">
         <v>944</v>
       </c>
-      <c r="B20" s="185"/>
-      <c r="C20" s="185"/>
-      <c r="D20" s="185"/>
-      <c r="E20" s="186"/>
+      <c r="B20" s="189"/>
+      <c r="C20" s="189"/>
+      <c r="D20" s="189"/>
+      <c r="E20" s="190"/>
     </row>
     <row r="21" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A21" s="5" t="s">
@@ -15774,13 +15774,13 @@
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A24" s="181" t="s">
+      <c r="A24" s="185" t="s">
         <v>957</v>
       </c>
-      <c r="B24" s="182"/>
-      <c r="C24" s="182"/>
-      <c r="D24" s="182"/>
-      <c r="E24" s="183"/>
+      <c r="B24" s="186"/>
+      <c r="C24" s="186"/>
+      <c r="D24" s="186"/>
+      <c r="E24" s="187"/>
     </row>
     <row r="25" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A25" s="18" t="s">
@@ -15798,13 +15798,13 @@
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A26" s="172" t="s">
+      <c r="A26" s="176" t="s">
         <v>961</v>
       </c>
-      <c r="B26" s="173"/>
-      <c r="C26" s="173"/>
-      <c r="D26" s="173"/>
-      <c r="E26" s="174"/>
+      <c r="B26" s="177"/>
+      <c r="C26" s="177"/>
+      <c r="D26" s="177"/>
+      <c r="E26" s="178"/>
     </row>
     <row r="27" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A27" s="18" t="s">
@@ -15822,13 +15822,13 @@
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A28" s="172" t="s">
+      <c r="A28" s="176" t="s">
         <v>965</v>
       </c>
-      <c r="B28" s="173"/>
-      <c r="C28" s="173"/>
-      <c r="D28" s="173"/>
-      <c r="E28" s="174"/>
+      <c r="B28" s="177"/>
+      <c r="C28" s="177"/>
+      <c r="D28" s="177"/>
+      <c r="E28" s="178"/>
     </row>
     <row r="29" spans="1:6" ht="112" x14ac:dyDescent="0.2">
       <c r="A29" s="91" t="s">
@@ -15966,13 +15966,13 @@
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A38" s="172" t="s">
+      <c r="A38" s="176" t="s">
         <v>990</v>
       </c>
-      <c r="B38" s="173"/>
-      <c r="C38" s="173"/>
-      <c r="D38" s="173"/>
-      <c r="E38" s="174"/>
+      <c r="B38" s="177"/>
+      <c r="C38" s="177"/>
+      <c r="D38" s="177"/>
+      <c r="E38" s="178"/>
     </row>
     <row r="39" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A39" s="19" t="s">
@@ -16016,13 +16016,13 @@
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A42" s="178" t="s">
+      <c r="A42" s="182" t="s">
         <v>998</v>
       </c>
-      <c r="B42" s="179"/>
-      <c r="C42" s="179"/>
-      <c r="D42" s="179"/>
-      <c r="E42" s="180"/>
+      <c r="B42" s="183"/>
+      <c r="C42" s="183"/>
+      <c r="D42" s="183"/>
+      <c r="E42" s="184"/>
     </row>
     <row r="43" spans="1:6" ht="96" x14ac:dyDescent="0.2">
       <c r="A43" s="116" t="s">
@@ -16265,8 +16265,8 @@
   <dimension ref="A1:F75"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D28" sqref="D28"/>
+      <pane ySplit="1" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -16468,7 +16468,7 @@
         <v>1071</v>
       </c>
       <c r="E11" s="138" t="s">
-        <v>1421</v>
+        <v>1419</v>
       </c>
       <c r="F11" s="135"/>
     </row>
@@ -16480,11 +16480,11 @@
         <v>1416</v>
       </c>
       <c r="C12" s="137" t="s">
-        <v>1419</v>
+        <v>1417</v>
       </c>
       <c r="D12" s="136"/>
       <c r="E12" s="138" t="s">
-        <v>1420</v>
+        <v>1418</v>
       </c>
       <c r="F12" s="135"/>
     </row>
@@ -16724,11 +16724,11 @@
         <v>1414</v>
       </c>
       <c r="C28" s="137" t="s">
-        <v>1417</v>
+        <v>1437</v>
       </c>
       <c r="D28" s="136"/>
       <c r="E28" s="138" t="s">
-        <v>1418</v>
+        <v>1439</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="32" x14ac:dyDescent="0.2">
@@ -16739,23 +16739,23 @@
         <v>1110</v>
       </c>
       <c r="C29" s="137" t="s">
-        <v>1422</v>
+        <v>1438</v>
       </c>
       <c r="D29" s="136" t="s">
         <v>1111</v>
       </c>
       <c r="E29" s="138" t="s">
-        <v>1423</v>
+        <v>1440</v>
       </c>
     </row>
     <row r="30" spans="1:6" s="13" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="187" t="s">
+      <c r="A30" s="191" t="s">
         <v>1112</v>
       </c>
-      <c r="B30" s="188"/>
-      <c r="C30" s="188"/>
-      <c r="D30" s="188"/>
-      <c r="E30" s="189"/>
+      <c r="B30" s="192"/>
+      <c r="C30" s="192"/>
+      <c r="D30" s="192"/>
+      <c r="E30" s="193"/>
     </row>
     <row r="31" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A31" s="140" t="s">
@@ -16818,13 +16818,13 @@
       <c r="E34" s="146"/>
     </row>
     <row r="35" spans="1:6" s="13" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="190" t="s">
+      <c r="A35" s="194" t="s">
         <v>1124</v>
       </c>
-      <c r="B35" s="191"/>
-      <c r="C35" s="192"/>
-      <c r="D35" s="191"/>
-      <c r="E35" s="193"/>
+      <c r="B35" s="195"/>
+      <c r="C35" s="196"/>
+      <c r="D35" s="195"/>
+      <c r="E35" s="197"/>
     </row>
     <row r="36" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A36" s="144" t="s">
@@ -17027,13 +17027,13 @@
       <c r="F47" s="135"/>
     </row>
     <row r="48" spans="1:6" s="13" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="187" t="s">
+      <c r="A48" s="191" t="s">
         <v>1153</v>
       </c>
-      <c r="B48" s="188"/>
-      <c r="C48" s="188"/>
-      <c r="D48" s="188"/>
-      <c r="E48" s="189"/>
+      <c r="B48" s="192"/>
+      <c r="C48" s="192"/>
+      <c r="D48" s="192"/>
+      <c r="E48" s="193"/>
     </row>
     <row r="49" spans="1:6" s="30" customFormat="1" ht="64" x14ac:dyDescent="0.2">
       <c r="A49" s="144" t="s">
@@ -17717,15 +17717,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <Readyforteam_x003f_ xmlns="565e1b1d-057e-4d85-b896-01a5881d8a45">false</Readyforteam_x003f_>
@@ -17766,6 +17757,15 @@
 </p:properties>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EAFDB110-4046-4E72-A1EF-1908ABEC3151}">
   <ds:schemaRefs>
@@ -17788,14 +17788,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8D7CE8C7-18DC-484F-8376-ED09F13D44C8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{017ACE96-8143-486E-8436-7787F6B96F4A}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -17806,4 +17798,12 @@
     <ds:schemaRef ds:uri="2799d30d-6731-4efe-ac9b-c4895a8828d9"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8D7CE8C7-18DC-484F-8376-ED09F13D44C8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
[MCCDB-947] Content amend - ME declaration after scrutiny
</commit_message>
<xml_diff>
--- a/app/data/MCCD-localisation.xlsx
+++ b/app/data/MCCD-localisation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/JALAT/GIT/medical-certificate-of-cause-of-death/app/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1E793BE-5F50-264E-A780-33F35D2187B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2703322A-8078-6642-B0AA-2AA9BB39B5CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="14100" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="14100" firstSheet="3" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Using this document" sheetId="8" r:id="rId1"/>
@@ -5159,13 +5159,7 @@
     <t>meCertDeclarationContent</t>
   </si>
   <si>
-    <t>I am a duly appointed medical examiner and I confirm that following my review the cause of death is as stated in this certificate to the best of my knowledge and belief.</t>
-  </si>
-  <si>
     <t>ME Cert - Declaration content.</t>
-  </si>
-  <si>
-    <t>Rwyf yn archwiliwr meddygol a benodwyd yn briodol ac rwy’n cadarnhau yn dilyn fy adolygiad bod achos y farwolaeth fel y’i nodir yn y dystysgrif hon hyd eithaf fy ngwybodaeth a’m cred.</t>
   </si>
   <si>
     <t>meCertDeclarationValidationSummaryNoTick</t>
@@ -5704,7 +5698,13 @@
     <t>2 Amgylchiadau arwyddocaol eraill (dewisol)</t>
   </si>
   <si>
-    <t>030</t>
+    <t>031</t>
+  </si>
+  <si>
+    <t>I am a duly appointed medical examiner and following scrutiny I confirm that the cause of death is as stated in this certificate to the best of my knowledge and belief.</t>
+  </si>
+  <si>
+    <t>Rwy'n arholwr meddygol a benodwyd yn briodol ac ar ôl craffu rwy'n cadarnhau bod achos y farwolaeth fel y nodir yn y dystysgrif hon hyd eithaf fy ngwybodaeth a'm cred.</t>
   </si>
 </sst>
 </file>
@@ -6672,6 +6672,15 @@
     <xf numFmtId="0" fontId="13" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -6688,15 +6697,6 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -7920,9 +7920,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E52C375-4A34-4943-A40B-CD02CAD0761B}">
   <dimension ref="A1:F24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F21" sqref="F21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -7964,13 +7964,13 @@
         <v>1241</v>
       </c>
       <c r="C2" s="151" t="s">
-        <v>1420</v>
+        <v>1418</v>
       </c>
       <c r="D2" s="92" t="s">
         <v>1242</v>
       </c>
       <c r="E2" s="152" t="s">
-        <v>1424</v>
+        <v>1422</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="80" x14ac:dyDescent="0.2">
@@ -7998,13 +7998,13 @@
         <v>1248</v>
       </c>
       <c r="C4" s="158" t="s">
-        <v>1421</v>
+        <v>1419</v>
       </c>
       <c r="D4" s="95" t="s">
         <v>404</v>
       </c>
       <c r="E4" s="155" t="s">
-        <v>1423</v>
+        <v>1421</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="60.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -8066,13 +8066,13 @@
         <v>1253</v>
       </c>
       <c r="C8" s="158" t="s">
-        <v>1420</v>
+        <v>1418</v>
       </c>
       <c r="D8" s="95" t="s">
         <v>1254</v>
       </c>
       <c r="E8" s="155" t="s">
-        <v>1424</v>
+        <v>1422</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="64" x14ac:dyDescent="0.2">
@@ -8100,13 +8100,13 @@
         <v>1259</v>
       </c>
       <c r="C10" s="158" t="s">
-        <v>1421</v>
+        <v>1419</v>
       </c>
       <c r="D10" s="95" t="s">
         <v>404</v>
       </c>
       <c r="E10" s="155" t="s">
-        <v>1423</v>
+        <v>1421</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -8168,30 +8168,30 @@
         <v>1262</v>
       </c>
       <c r="C14" s="158" t="s">
-        <v>1420</v>
+        <v>1418</v>
       </c>
       <c r="D14" s="95" t="s">
         <v>1263</v>
       </c>
       <c r="E14" s="155" t="s">
-        <v>1422</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="96" x14ac:dyDescent="0.2">
+        <v>1420</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="80" x14ac:dyDescent="0.2">
       <c r="A15" s="94" t="s">
         <v>1243</v>
       </c>
       <c r="B15" s="95" t="s">
         <v>1264</v>
       </c>
-      <c r="C15" s="96" t="s">
+      <c r="C15" s="158" t="s">
+        <v>1440</v>
+      </c>
+      <c r="D15" s="95" t="s">
         <v>1265</v>
       </c>
-      <c r="D15" s="95" t="s">
-        <v>1266</v>
-      </c>
-      <c r="E15" s="89" t="s">
-        <v>1267</v>
+      <c r="E15" s="155" t="s">
+        <v>1441</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="48" x14ac:dyDescent="0.2">
@@ -8199,7 +8199,7 @@
         <v>410</v>
       </c>
       <c r="B16" s="105" t="s">
-        <v>1268</v>
+        <v>1266</v>
       </c>
       <c r="C16" s="106" t="s">
         <v>404</v>
@@ -8216,7 +8216,7 @@
         <v>413</v>
       </c>
       <c r="B17" s="105" t="s">
-        <v>1269</v>
+        <v>1267</v>
       </c>
       <c r="C17" s="106" t="s">
         <v>404</v>
@@ -8233,16 +8233,16 @@
         <v>14</v>
       </c>
       <c r="B18" s="95" t="s">
-        <v>1270</v>
+        <v>1268</v>
       </c>
       <c r="C18" s="158" t="s">
-        <v>1421</v>
+        <v>1419</v>
       </c>
       <c r="D18" s="95" t="s">
         <v>404</v>
       </c>
       <c r="E18" s="155" t="s">
-        <v>1423</v>
+        <v>1421</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -8267,16 +8267,16 @@
         <v>243</v>
       </c>
       <c r="B20" s="95" t="s">
-        <v>1271</v>
+        <v>1269</v>
       </c>
       <c r="C20" s="158" t="s">
-        <v>1420</v>
+        <v>1418</v>
       </c>
       <c r="D20" s="95" t="s">
         <v>1242</v>
       </c>
       <c r="E20" s="155" t="s">
-        <v>1422</v>
+        <v>1420</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="48" x14ac:dyDescent="0.2">
@@ -8284,13 +8284,13 @@
         <v>1243</v>
       </c>
       <c r="B21" s="95" t="s">
+        <v>1270</v>
+      </c>
+      <c r="C21" s="96" t="s">
+        <v>1271</v>
+      </c>
+      <c r="D21" s="95" t="s">
         <v>1272</v>
-      </c>
-      <c r="C21" s="96" t="s">
-        <v>1273</v>
-      </c>
-      <c r="D21" s="95" t="s">
-        <v>1274</v>
       </c>
       <c r="E21" s="89" t="s">
         <v>404</v>
@@ -8301,16 +8301,16 @@
         <v>755</v>
       </c>
       <c r="B22" s="95" t="s">
-        <v>1275</v>
+        <v>1273</v>
       </c>
       <c r="C22" s="158" t="s">
-        <v>1421</v>
+        <v>1419</v>
       </c>
       <c r="D22" s="95" t="s">
         <v>404</v>
       </c>
       <c r="E22" s="155" t="s">
-        <v>1425</v>
+        <v>1423</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="48" x14ac:dyDescent="0.2">
@@ -8318,7 +8318,7 @@
         <v>410</v>
       </c>
       <c r="B23" s="105" t="s">
-        <v>1276</v>
+        <v>1274</v>
       </c>
       <c r="C23" s="106" t="s">
         <v>404</v>
@@ -8335,7 +8335,7 @@
         <v>413</v>
       </c>
       <c r="B24" s="105" t="s">
-        <v>1277</v>
+        <v>1275</v>
       </c>
       <c r="C24" s="106" t="s">
         <v>404</v>
@@ -8394,7 +8394,7 @@
     </row>
     <row r="2" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="198" t="s">
-        <v>1278</v>
+        <v>1276</v>
       </c>
       <c r="B2" s="199"/>
       <c r="C2" s="199"/>
@@ -8407,16 +8407,16 @@
         <v>243</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>1279</v>
+        <v>1277</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>1280</v>
+        <v>1278</v>
       </c>
       <c r="D3" s="5" t="s">
         <v>1223</v>
       </c>
       <c r="E3" s="37" t="s">
-        <v>1281</v>
+        <v>1279</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="32" x14ac:dyDescent="0.2">
@@ -8424,13 +8424,13 @@
         <v>261</v>
       </c>
       <c r="B4" s="5" t="s">
+        <v>1280</v>
+      </c>
+      <c r="C4" s="59" t="s">
+        <v>1281</v>
+      </c>
+      <c r="E4" s="37" t="s">
         <v>1282</v>
-      </c>
-      <c r="C4" s="59" t="s">
-        <v>1283</v>
-      </c>
-      <c r="E4" s="37" t="s">
-        <v>1284</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="16" x14ac:dyDescent="0.2">
@@ -8438,13 +8438,13 @@
         <v>254</v>
       </c>
       <c r="B5" s="5" t="s">
+        <v>1283</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>1284</v>
+      </c>
+      <c r="E5" s="37" t="s">
         <v>1285</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>1286</v>
-      </c>
-      <c r="E5" s="37" t="s">
-        <v>1287</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="80" x14ac:dyDescent="0.2">
@@ -8452,13 +8452,13 @@
         <v>261</v>
       </c>
       <c r="B6" s="5" t="s">
+        <v>1286</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>1287</v>
+      </c>
+      <c r="E6" s="37" t="s">
         <v>1288</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>1289</v>
-      </c>
-      <c r="E6" s="37" t="s">
-        <v>1290</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="32" x14ac:dyDescent="0.2">
@@ -8466,112 +8466,112 @@
         <v>254</v>
       </c>
       <c r="B7" s="5" t="s">
+        <v>1289</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>1290</v>
+      </c>
+      <c r="E7" s="37" t="s">
         <v>1291</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>1292</v>
-      </c>
-      <c r="E7" s="37" t="s">
-        <v>1293</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
-        <v>1294</v>
+        <v>1292</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>1295</v>
+        <v>1293</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>1430</v>
+        <v>1428</v>
       </c>
       <c r="E8" s="37" t="s">
-        <v>1431</v>
+        <v>1429</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
+        <v>1294</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>1295</v>
+      </c>
+      <c r="C9" s="6" t="s">
         <v>1296</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="E9" s="37" t="s">
         <v>1297</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>1298</v>
-      </c>
-      <c r="E9" s="37" t="s">
-        <v>1299</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
-        <v>1296</v>
+        <v>1294</v>
       </c>
       <c r="B10" s="5" t="s">
+        <v>1298</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>1299</v>
+      </c>
+      <c r="E10" s="37" t="s">
         <v>1300</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>1301</v>
-      </c>
-      <c r="E10" s="37" t="s">
-        <v>1302</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
-        <v>1296</v>
+        <v>1294</v>
       </c>
       <c r="B11" s="5" t="s">
+        <v>1301</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>1302</v>
+      </c>
+      <c r="E11" s="37" t="s">
         <v>1303</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>1304</v>
-      </c>
-      <c r="E11" s="37" t="s">
-        <v>1305</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="5" t="s">
-        <v>1296</v>
+        <v>1294</v>
       </c>
       <c r="B12" s="5" t="s">
+        <v>1304</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>1305</v>
+      </c>
+      <c r="E12" s="37" t="s">
         <v>1306</v>
-      </c>
-      <c r="C12" s="6" t="s">
-        <v>1307</v>
-      </c>
-      <c r="E12" s="37" t="s">
-        <v>1308</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="s">
-        <v>1296</v>
+        <v>1294</v>
       </c>
       <c r="B13" s="5" t="s">
+        <v>1307</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>1308</v>
+      </c>
+      <c r="E13" s="37" t="s">
         <v>1309</v>
-      </c>
-      <c r="C13" s="6" t="s">
-        <v>1310</v>
-      </c>
-      <c r="E13" s="37" t="s">
-        <v>1311</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A14" s="5" t="s">
-        <v>1294</v>
+        <v>1292</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>1312</v>
+        <v>1310</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>1428</v>
+        <v>1426</v>
       </c>
       <c r="D14" s="1"/>
       <c r="E14" s="37" t="s">
-        <v>1429</v>
+        <v>1427</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="32" x14ac:dyDescent="0.2">
@@ -8579,14 +8579,14 @@
         <v>949</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>1313</v>
+        <v>1311</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>1314</v>
+        <v>1312</v>
       </c>
       <c r="D15" s="1"/>
       <c r="E15" s="37" t="s">
-        <v>1315</v>
+        <v>1313</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="16" x14ac:dyDescent="0.2">
@@ -8594,34 +8594,34 @@
         <v>14</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>1316</v>
+        <v>1314</v>
       </c>
       <c r="C16" s="74" t="s">
-        <v>1317</v>
+        <v>1315</v>
       </c>
       <c r="D16" s="18"/>
       <c r="E16" s="37" t="s">
-        <v>1318</v>
+        <v>1316</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A17" s="5" t="s">
+        <v>1317</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>1318</v>
+      </c>
+      <c r="C17" s="75" t="s">
         <v>1319</v>
-      </c>
-      <c r="B17" s="7" t="s">
-        <v>1320</v>
-      </c>
-      <c r="C17" s="75" t="s">
-        <v>1321</v>
       </c>
       <c r="D17" s="18"/>
       <c r="E17" s="37" t="s">
-        <v>1322</v>
+        <v>1320</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="198" t="s">
-        <v>1323</v>
+        <v>1321</v>
       </c>
       <c r="B18" s="199"/>
       <c r="C18" s="199"/>
@@ -8634,16 +8634,16 @@
         <v>243</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>1326</v>
+        <v>1324</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>1324</v>
+        <v>1322</v>
       </c>
       <c r="D19" s="5" t="s">
         <v>1223</v>
       </c>
       <c r="E19" s="37" t="s">
-        <v>1325</v>
+        <v>1323</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="96" x14ac:dyDescent="0.2">
@@ -8651,13 +8651,13 @@
         <v>261</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="C20" s="59" t="s">
+        <v>1395</v>
+      </c>
+      <c r="E20" s="37" t="s">
         <v>1397</v>
-      </c>
-      <c r="E20" s="37" t="s">
-        <v>1399</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="16" x14ac:dyDescent="0.2">
@@ -8665,13 +8665,13 @@
         <v>254</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>1328</v>
+        <v>1326</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>1286</v>
+        <v>1284</v>
       </c>
       <c r="E21" s="37" t="s">
-        <v>1287</v>
+        <v>1285</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="80" x14ac:dyDescent="0.2">
@@ -8679,13 +8679,13 @@
         <v>261</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>1329</v>
+        <v>1327</v>
       </c>
       <c r="C22" s="6" t="s">
+        <v>1396</v>
+      </c>
+      <c r="E22" s="37" t="s">
         <v>1398</v>
-      </c>
-      <c r="E22" s="37" t="s">
-        <v>1400</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
@@ -8707,7 +8707,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F68"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="F3" sqref="F3"/>
     </sheetView>
@@ -8749,13 +8749,13 @@
         <v>7</v>
       </c>
       <c r="C2" s="100" t="s">
-        <v>1441</v>
+        <v>1439</v>
       </c>
       <c r="D2" s="98" t="s">
         <v>8</v>
       </c>
       <c r="E2" s="99" t="s">
-        <v>1441</v>
+        <v>1439</v>
       </c>
       <c r="F2" s="98"/>
     </row>
@@ -8773,7 +8773,7 @@
         <v>12</v>
       </c>
       <c r="E3" s="37" t="s">
-        <v>1396</v>
+        <v>1394</v>
       </c>
       <c r="F3" s="5" t="s">
         <v>13</v>
@@ -9828,18 +9828,18 @@
     </row>
     <row r="67" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="B67" s="1" t="s">
-        <v>1340</v>
+        <v>1338</v>
       </c>
       <c r="C67" s="2" t="s">
+        <v>1339</v>
+      </c>
+      <c r="E67" s="40" t="s">
         <v>1341</v>
-      </c>
-      <c r="E67" s="40" t="s">
-        <v>1343</v>
       </c>
     </row>
     <row r="68" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="B68" s="1" t="s">
-        <v>1342</v>
+        <v>1340</v>
       </c>
       <c r="C68" s="2" t="s">
         <v>76</v>
@@ -10140,14 +10140,14 @@
         <v>243</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>1367</v>
+        <v>1365</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>1368</v>
+        <v>1366</v>
       </c>
       <c r="D2" s="5"/>
       <c r="E2" s="43" t="s">
-        <v>1376</v>
+        <v>1374</v>
       </c>
       <c r="F2" s="1"/>
     </row>
@@ -10156,19 +10156,19 @@
         <v>484</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>1369</v>
+        <v>1367</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>1370</v>
+        <v>1368</v>
       </c>
       <c r="D3" s="5"/>
       <c r="E3" s="43" t="s">
-        <v>1377</v>
+        <v>1375</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="164" t="s">
-        <v>1371</v>
+        <v>1369</v>
       </c>
       <c r="B4" s="165"/>
       <c r="C4" s="165"/>
@@ -10180,14 +10180,14 @@
         <v>243</v>
       </c>
       <c r="B5" s="5" t="s">
+        <v>1370</v>
+      </c>
+      <c r="C5" s="6" t="s">
         <v>1372</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>1374</v>
       </c>
       <c r="D5" s="5"/>
       <c r="E5" s="43" t="s">
-        <v>1378</v>
+        <v>1376</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="96" x14ac:dyDescent="0.2">
@@ -10195,14 +10195,14 @@
         <v>484</v>
       </c>
       <c r="B6" s="5" t="s">
+        <v>1371</v>
+      </c>
+      <c r="C6" s="6" t="s">
         <v>1373</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>1375</v>
       </c>
       <c r="D6" s="5"/>
       <c r="E6" s="43" t="s">
-        <v>1379</v>
+        <v>1377</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
@@ -10423,7 +10423,7 @@
         <v>243</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>1382</v>
+        <v>1380</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>276</v>
@@ -10447,7 +10447,7 @@
         <v>246</v>
       </c>
       <c r="E4" s="43" t="s">
-        <v>1383</v>
+        <v>1381</v>
       </c>
       <c r="F4" s="68" t="s">
         <v>280</v>
@@ -10461,13 +10461,13 @@
         <v>281</v>
       </c>
       <c r="C5" s="52" t="s">
-        <v>1388</v>
+        <v>1386</v>
       </c>
       <c r="D5" s="66" t="s">
         <v>282</v>
       </c>
       <c r="E5" s="156" t="s">
-        <v>1393</v>
+        <v>1391</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>283</v>
@@ -10481,13 +10481,13 @@
         <v>284</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>1389</v>
+        <v>1387</v>
       </c>
       <c r="D6" s="67" t="s">
         <v>285</v>
       </c>
       <c r="E6" s="157" t="s">
-        <v>1390</v>
+        <v>1388</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="160" x14ac:dyDescent="0.2">
@@ -10498,13 +10498,13 @@
         <v>286</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>1391</v>
+        <v>1389</v>
       </c>
       <c r="D7" s="67" t="s">
         <v>287</v>
       </c>
       <c r="E7" s="157" t="s">
-        <v>1392</v>
+        <v>1390</v>
       </c>
       <c r="F7" s="68" t="s">
         <v>288</v>
@@ -10706,7 +10706,7 @@
         <v>336</v>
       </c>
       <c r="C19" s="64" t="s">
-        <v>1380</v>
+        <v>1378</v>
       </c>
       <c r="D19" s="7" t="s">
         <v>337</v>
@@ -10840,17 +10840,17 @@
     </row>
     <row r="27" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A27" s="5" t="s">
-        <v>1386</v>
+        <v>1384</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>1387</v>
+        <v>1385</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>1384</v>
+        <v>1382</v>
       </c>
       <c r="D27" s="5"/>
       <c r="E27" s="37" t="s">
-        <v>1385</v>
+        <v>1383</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
@@ -10927,13 +10927,13 @@
       </c>
     </row>
     <row r="2" spans="1:6" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="167" t="s">
+      <c r="A2" s="170" t="s">
         <v>367</v>
       </c>
-      <c r="B2" s="168"/>
-      <c r="C2" s="168"/>
-      <c r="D2" s="168"/>
-      <c r="E2" s="169"/>
+      <c r="B2" s="171"/>
+      <c r="C2" s="171"/>
+      <c r="D2" s="171"/>
+      <c r="E2" s="172"/>
       <c r="F2" s="33"/>
     </row>
     <row r="3" spans="1:6" ht="48" x14ac:dyDescent="0.2">
@@ -11061,13 +11061,13 @@
       <c r="F9" s="119"/>
     </row>
     <row r="10" spans="1:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="170" t="s">
+      <c r="A10" s="173" t="s">
         <v>396</v>
       </c>
-      <c r="B10" s="171"/>
-      <c r="C10" s="171"/>
-      <c r="D10" s="171"/>
-      <c r="E10" s="172"/>
+      <c r="B10" s="174"/>
+      <c r="C10" s="174"/>
+      <c r="D10" s="174"/>
+      <c r="E10" s="175"/>
       <c r="F10" s="119"/>
     </row>
     <row r="11" spans="1:6" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -11096,13 +11096,13 @@
         <v>401</v>
       </c>
       <c r="C12" s="153" t="s">
-        <v>1344</v>
+        <v>1342</v>
       </c>
       <c r="D12" s="84" t="s">
         <v>402</v>
       </c>
       <c r="E12" s="152" t="s">
-        <v>1345</v>
+        <v>1343</v>
       </c>
       <c r="F12" s="86"/>
     </row>
@@ -11114,13 +11114,13 @@
         <v>403</v>
       </c>
       <c r="C13" s="154" t="s">
-        <v>1346</v>
+        <v>1344</v>
       </c>
       <c r="D13" s="88" t="s">
         <v>404</v>
       </c>
       <c r="E13" s="155" t="s">
-        <v>1347</v>
+        <v>1345</v>
       </c>
       <c r="F13" s="86"/>
     </row>
@@ -11588,7 +11588,7 @@
         <v>485</v>
       </c>
       <c r="C45" s="59" t="s">
-        <v>1363</v>
+        <v>1361</v>
       </c>
       <c r="D45" s="116"/>
       <c r="E45" s="120" t="s">
@@ -11601,14 +11601,14 @@
         <v>484</v>
       </c>
       <c r="B46" s="116" t="s">
-        <v>1366</v>
+        <v>1364</v>
       </c>
       <c r="C46" s="59" t="s">
-        <v>1364</v>
+        <v>1362</v>
       </c>
       <c r="D46" s="116"/>
       <c r="E46" s="120" t="s">
-        <v>1365</v>
+        <v>1363</v>
       </c>
       <c r="F46" s="119"/>
     </row>
@@ -11836,7 +11836,7 @@
         <v>522</v>
       </c>
       <c r="E61" s="120" t="s">
-        <v>1356</v>
+        <v>1354</v>
       </c>
       <c r="F61" s="119"/>
     </row>
@@ -11845,14 +11845,14 @@
         <v>519</v>
       </c>
       <c r="B62" s="116" t="s">
+        <v>1351</v>
+      </c>
+      <c r="C62" s="117" t="s">
         <v>1353</v>
-      </c>
-      <c r="C62" s="117" t="s">
-        <v>1355</v>
       </c>
       <c r="D62" s="116"/>
       <c r="E62" s="120" t="s">
-        <v>1354</v>
+        <v>1352</v>
       </c>
       <c r="F62" s="119"/>
     </row>
@@ -12186,11 +12186,11 @@
         <v>572</v>
       </c>
       <c r="C84" s="117" t="s">
-        <v>1408</v>
+        <v>1406</v>
       </c>
       <c r="D84" s="116"/>
       <c r="E84" s="120" t="s">
-        <v>1409</v>
+        <v>1407</v>
       </c>
       <c r="F84" s="119" t="s">
         <v>573</v>
@@ -12300,11 +12300,11 @@
         <v>591</v>
       </c>
       <c r="C91" s="117" t="s">
-        <v>1406</v>
+        <v>1404</v>
       </c>
       <c r="D91" s="116"/>
       <c r="E91" s="120" t="s">
-        <v>1407</v>
+        <v>1405</v>
       </c>
       <c r="F91" s="119"/>
     </row>
@@ -12344,11 +12344,11 @@
         <v>597</v>
       </c>
       <c r="C94" s="117" t="s">
-        <v>1426</v>
+        <v>1424</v>
       </c>
       <c r="D94" s="116"/>
       <c r="E94" s="120" t="s">
-        <v>1427</v>
+        <v>1425</v>
       </c>
       <c r="F94" s="119" t="s">
         <v>573</v>
@@ -12379,7 +12379,7 @@
         <v>84</v>
       </c>
       <c r="B96" s="159" t="s">
-        <v>1432</v>
+        <v>1430</v>
       </c>
       <c r="C96" s="93" t="s">
         <v>599</v>
@@ -12397,7 +12397,7 @@
         <v>84</v>
       </c>
       <c r="B97" s="159" t="s">
-        <v>1433</v>
+        <v>1431</v>
       </c>
       <c r="C97" s="93" t="s">
         <v>599</v>
@@ -12415,7 +12415,7 @@
         <v>84</v>
       </c>
       <c r="B98" s="160" t="s">
-        <v>1434</v>
+        <v>1432</v>
       </c>
       <c r="C98" s="161" t="s">
         <v>599</v>
@@ -12431,7 +12431,7 @@
         <v>84</v>
       </c>
       <c r="B99" s="160" t="s">
-        <v>1435</v>
+        <v>1433</v>
       </c>
       <c r="C99" s="161" t="s">
         <v>599</v>
@@ -12447,7 +12447,7 @@
         <v>84</v>
       </c>
       <c r="B100" s="160" t="s">
-        <v>1436</v>
+        <v>1434</v>
       </c>
       <c r="C100" s="161" t="s">
         <v>599</v>
@@ -13122,7 +13122,7 @@
         <v>707</v>
       </c>
       <c r="C146" s="113" t="s">
-        <v>1331</v>
+        <v>1329</v>
       </c>
       <c r="D146" s="122" t="s">
         <v>708</v>
@@ -13212,7 +13212,7 @@
         <v>722</v>
       </c>
       <c r="C152" s="59" t="s">
-        <v>1330</v>
+        <v>1328</v>
       </c>
       <c r="D152" s="116" t="s">
         <v>723</v>
@@ -13243,14 +13243,14 @@
         <v>37</v>
       </c>
       <c r="B154" s="116" t="s">
+        <v>1330</v>
+      </c>
+      <c r="C154" s="59" t="s">
         <v>1332</v>
-      </c>
-      <c r="C154" s="59" t="s">
-        <v>1334</v>
       </c>
       <c r="D154" s="116"/>
       <c r="E154" s="120" t="s">
-        <v>1336</v>
+        <v>1334</v>
       </c>
       <c r="F154" s="119"/>
     </row>
@@ -13259,14 +13259,14 @@
         <v>37</v>
       </c>
       <c r="B155" s="116" t="s">
+        <v>1331</v>
+      </c>
+      <c r="C155" s="59" t="s">
         <v>1333</v>
-      </c>
-      <c r="C155" s="59" t="s">
-        <v>1335</v>
       </c>
       <c r="D155" s="116"/>
       <c r="E155" s="120" t="s">
-        <v>1337</v>
+        <v>1335</v>
       </c>
       <c r="F155" s="119"/>
     </row>
@@ -13485,13 +13485,13 @@
       <c r="F169" s="119"/>
     </row>
     <row r="170" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A170" s="173" t="s">
+      <c r="A170" s="167" t="s">
         <v>762</v>
       </c>
-      <c r="B170" s="174"/>
-      <c r="C170" s="174"/>
-      <c r="D170" s="174"/>
-      <c r="E170" s="175"/>
+      <c r="B170" s="168"/>
+      <c r="C170" s="168"/>
+      <c r="D170" s="168"/>
+      <c r="E170" s="169"/>
       <c r="F170" s="129" t="s">
         <v>763</v>
       </c>
@@ -13918,13 +13918,13 @@
         <v>812</v>
       </c>
       <c r="C198" s="59" t="s">
-        <v>1348</v>
+        <v>1346</v>
       </c>
       <c r="D198" s="116" t="s">
         <v>813</v>
       </c>
       <c r="E198" s="120" t="s">
-        <v>1352</v>
+        <v>1350</v>
       </c>
       <c r="F198" s="119"/>
     </row>
@@ -13933,14 +13933,14 @@
         <v>484</v>
       </c>
       <c r="B199" s="116" t="s">
-        <v>1349</v>
+        <v>1347</v>
       </c>
       <c r="C199" s="59" t="s">
-        <v>1350</v>
+        <v>1348</v>
       </c>
       <c r="D199" s="116"/>
       <c r="E199" s="120" t="s">
-        <v>1351</v>
+        <v>1349</v>
       </c>
       <c r="F199" s="119"/>
     </row>
@@ -14040,11 +14040,11 @@
         <v>824</v>
       </c>
       <c r="C206" s="117" t="s">
-        <v>1359</v>
+        <v>1357</v>
       </c>
       <c r="D206" s="116"/>
       <c r="E206" s="120" t="s">
-        <v>1362</v>
+        <v>1360</v>
       </c>
       <c r="F206" s="119"/>
     </row>
@@ -14053,7 +14053,7 @@
         <v>731</v>
       </c>
       <c r="B207" s="116" t="s">
-        <v>1361</v>
+        <v>1359</v>
       </c>
       <c r="C207" s="117" t="s">
         <v>43</v>
@@ -14069,14 +14069,14 @@
         <v>32</v>
       </c>
       <c r="B208" s="116" t="s">
-        <v>1360</v>
+        <v>1358</v>
       </c>
       <c r="C208" s="134" t="s">
-        <v>1357</v>
+        <v>1355</v>
       </c>
       <c r="D208" s="116"/>
       <c r="E208" s="120" t="s">
-        <v>1358</v>
+        <v>1356</v>
       </c>
       <c r="F208" s="119"/>
     </row>
@@ -14448,13 +14448,13 @@
         <v>863</v>
       </c>
       <c r="C233" s="59" t="s">
-        <v>1394</v>
+        <v>1392</v>
       </c>
       <c r="D233" s="116" t="s">
         <v>864</v>
       </c>
       <c r="E233" s="120" t="s">
-        <v>1395</v>
+        <v>1393</v>
       </c>
       <c r="F233" s="119"/>
     </row>
@@ -15394,6 +15394,18 @@
     </row>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="A230:E230"/>
+    <mergeCell ref="A191:E191"/>
+    <mergeCell ref="A195:E195"/>
+    <mergeCell ref="A202:E202"/>
+    <mergeCell ref="A213:E213"/>
+    <mergeCell ref="A219:E219"/>
+    <mergeCell ref="A58:E58"/>
+    <mergeCell ref="A2:E2"/>
+    <mergeCell ref="A10:E10"/>
+    <mergeCell ref="A14:E14"/>
+    <mergeCell ref="A24:E24"/>
+    <mergeCell ref="A43:E43"/>
     <mergeCell ref="A179:E179"/>
     <mergeCell ref="A162:E162"/>
     <mergeCell ref="A63:E63"/>
@@ -15404,18 +15416,6 @@
     <mergeCell ref="A151:E151"/>
     <mergeCell ref="A92:E92"/>
     <mergeCell ref="A170:E170"/>
-    <mergeCell ref="A58:E58"/>
-    <mergeCell ref="A2:E2"/>
-    <mergeCell ref="A10:E10"/>
-    <mergeCell ref="A14:E14"/>
-    <mergeCell ref="A24:E24"/>
-    <mergeCell ref="A43:E43"/>
-    <mergeCell ref="A230:E230"/>
-    <mergeCell ref="A191:E191"/>
-    <mergeCell ref="A195:E195"/>
-    <mergeCell ref="A202:E202"/>
-    <mergeCell ref="A213:E213"/>
-    <mergeCell ref="A219:E219"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -15686,13 +15686,13 @@
         <v>939</v>
       </c>
       <c r="C17" s="151" t="s">
-        <v>1338</v>
+        <v>1336</v>
       </c>
       <c r="D17" s="92" t="s">
         <v>931</v>
       </c>
       <c r="E17" s="152" t="s">
-        <v>1339</v>
+        <v>1337</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="80" x14ac:dyDescent="0.2">
@@ -15892,10 +15892,10 @@
         <v>979</v>
       </c>
       <c r="C32" s="21" t="s">
-        <v>1401</v>
+        <v>1399</v>
       </c>
       <c r="E32" s="46" t="s">
-        <v>1402</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="32" x14ac:dyDescent="0.2">
@@ -15903,13 +15903,13 @@
         <v>261</v>
       </c>
       <c r="B33" s="19" t="s">
+        <v>1401</v>
+      </c>
+      <c r="C33" s="21" t="s">
+        <v>1402</v>
+      </c>
+      <c r="E33" s="46" t="s">
         <v>1403</v>
-      </c>
-      <c r="C33" s="21" t="s">
-        <v>1404</v>
-      </c>
-      <c r="E33" s="46" t="s">
-        <v>1405</v>
       </c>
     </row>
     <row r="34" spans="1:6" ht="48" x14ac:dyDescent="0.2">
@@ -16069,13 +16069,13 @@
         <v>1004</v>
       </c>
       <c r="C45" s="62" t="s">
-        <v>1394</v>
+        <v>1392</v>
       </c>
       <c r="D45" s="116" t="s">
         <v>1005</v>
       </c>
       <c r="E45" s="46" t="s">
-        <v>1395</v>
+        <v>1393</v>
       </c>
     </row>
     <row r="46" spans="1:6" ht="48" x14ac:dyDescent="0.2">
@@ -16265,7 +16265,7 @@
   <dimension ref="A1:F75"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
@@ -16468,23 +16468,23 @@
         <v>1071</v>
       </c>
       <c r="E11" s="138" t="s">
-        <v>1419</v>
+        <v>1417</v>
       </c>
       <c r="F11" s="135"/>
     </row>
     <row r="12" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A12" s="136" t="s">
+        <v>1413</v>
+      </c>
+      <c r="B12" s="136" t="s">
+        <v>1414</v>
+      </c>
+      <c r="C12" s="137" t="s">
         <v>1415</v>
-      </c>
-      <c r="B12" s="136" t="s">
-        <v>1416</v>
-      </c>
-      <c r="C12" s="137" t="s">
-        <v>1417</v>
       </c>
       <c r="D12" s="136"/>
       <c r="E12" s="138" t="s">
-        <v>1418</v>
+        <v>1416</v>
       </c>
       <c r="F12" s="135"/>
     </row>
@@ -16496,7 +16496,7 @@
         <v>1072</v>
       </c>
       <c r="C13" s="137" t="s">
-        <v>1413</v>
+        <v>1411</v>
       </c>
       <c r="D13" s="136" t="s">
         <v>1073</v>
@@ -16542,7 +16542,7 @@
         <v>1078</v>
       </c>
       <c r="C16" s="137" t="s">
-        <v>1410</v>
+        <v>1408</v>
       </c>
       <c r="D16" s="136" t="s">
         <v>1079</v>
@@ -16560,7 +16560,7 @@
         <v>1081</v>
       </c>
       <c r="C17" s="137" t="s">
-        <v>1411</v>
+        <v>1409</v>
       </c>
       <c r="D17" s="136" t="s">
         <v>1082</v>
@@ -16578,7 +16578,7 @@
         <v>1084</v>
       </c>
       <c r="C18" s="137" t="s">
-        <v>1412</v>
+        <v>1410</v>
       </c>
       <c r="D18" s="136" t="s">
         <v>1085</v>
@@ -16718,17 +16718,17 @@
     </row>
     <row r="28" spans="1:6" ht="64" x14ac:dyDescent="0.2">
       <c r="A28" s="136" t="s">
-        <v>1415</v>
+        <v>1413</v>
       </c>
       <c r="B28" s="136" t="s">
-        <v>1414</v>
+        <v>1412</v>
       </c>
       <c r="C28" s="137" t="s">
-        <v>1437</v>
+        <v>1435</v>
       </c>
       <c r="D28" s="136"/>
       <c r="E28" s="138" t="s">
-        <v>1439</v>
+        <v>1437</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="32" x14ac:dyDescent="0.2">
@@ -16739,13 +16739,13 @@
         <v>1110</v>
       </c>
       <c r="C29" s="137" t="s">
-        <v>1438</v>
+        <v>1436</v>
       </c>
       <c r="D29" s="136" t="s">
         <v>1111</v>
       </c>
       <c r="E29" s="138" t="s">
-        <v>1440</v>
+        <v>1438</v>
       </c>
     </row>
     <row r="30" spans="1:6" s="13" customFormat="1" x14ac:dyDescent="0.2">
@@ -16988,7 +16988,7 @@
         <v>1148</v>
       </c>
       <c r="C45" s="62" t="s">
-        <v>1381</v>
+        <v>1379</v>
       </c>
       <c r="D45" s="5" t="s">
         <v>1149</v>
@@ -17080,13 +17080,13 @@
         <v>1160</v>
       </c>
       <c r="C51" s="62" t="s">
-        <v>1394</v>
+        <v>1392</v>
       </c>
       <c r="D51" s="116" t="s">
         <v>1005</v>
       </c>
       <c r="E51" s="63" t="s">
-        <v>1395</v>
+        <v>1393</v>
       </c>
     </row>
     <row r="52" spans="1:6" s="30" customFormat="1" ht="48" x14ac:dyDescent="0.2">
@@ -17717,6 +17717,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <Readyforteam_x003f_ xmlns="565e1b1d-057e-4d85-b896-01a5881d8a45">false</Readyforteam_x003f_>
@@ -17757,15 +17766,6 @@
 </p:properties>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EAFDB110-4046-4E72-A1EF-1908ABEC3151}">
   <ds:schemaRefs>
@@ -17788,6 +17788,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8D7CE8C7-18DC-484F-8376-ED09F13D44C8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{017ACE96-8143-486E-8436-7787F6B96F4A}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -17798,12 +17806,4 @@
     <ds:schemaRef ds:uri="2799d30d-6731-4efe-ac9b-c4895a8828d9"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8D7CE8C7-18DC-484F-8376-ED09F13D44C8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
[MCCDB-684] Content amend - The AP dashboard
</commit_message>
<xml_diff>
--- a/app/data/MCCD-localisation.xlsx
+++ b/app/data/MCCD-localisation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/JALAT/GIT/medical-certificate-of-cause-of-death/app/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2703322A-8078-6642-B0AA-2AA9BB39B5CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DBE28D6-832A-254A-9785-52113F0520ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="14100" firstSheet="3" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="14100" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Using this document" sheetId="8" r:id="rId1"/>
@@ -5539,9 +5539,6 @@
     <t>dashboardInactivityMessage</t>
   </si>
   <si>
-    <t>&lt;p class="govuk-body"&gt;This dashboard allows you to create a new Medical certificate of cause of death (MCCD) and manage current MCCDs.&lt;/p&gt;&lt;p class="govuk-body"&gt;This dashboard will list MCCDs that:&lt;/p&gt;&lt;ul class="govuk-list govuk-list--bullet"&gt;&lt;li&gt;you have submitted to a medical examiner for approval&lt;/li&gt;&lt;li&gt;have been approved by a medical examiner and need forwarding to the registrar’s office&lt;/li&gt;&lt;li&gt;have been rejected by a medical examiner and need amending&lt;/li&gt;&lt;/ul&gt;&lt;p class="govuk-body"&gt;Completed MCCDs will be removed after three months.&lt;/p&gt;</t>
-  </si>
-  <si>
     <t>&lt;p class="govuk-body"&gt;This dashboard gives you access to the Medical certificates of cause of death (MCCDs) assigned to you for review and approval.&lt;/p&gt;&lt;p class="govuk-body"&gt;An MCCD can only be approved when scrutiny of the proposed cause of death is complete.&lt;/p&gt;</t>
   </si>
   <si>
@@ -5554,9 +5551,6 @@
     <t>&lt;p class="govuk-body"&gt;Mae'r dangosfwrdd hwn yn rhoi mynediad i chi at y Tystysgrifau Meddygol o achos marwolaeth (MCCDs) sy'n cael eu cwblhau yn eich ymddiriedolaeth ar hyn o bryd. Gallwch weld cynnydd MCCDs a lawrlwytho MCCDs sydd wedi'u llofnodi i'w hanfon at y cofrestrydd.&lt;/p&gt;</t>
   </si>
   <si>
-    <t>&lt;p class="govuk-body"&gt;Mae'r dangosfwrdd hwn yn eich galluogi i greu Tystysgrif Feddygol achos marwolaeth (MCCD) newydd a rheoli MCCDs presennol.&lt;/p&gt;&lt;p class="govuk-body"&gt;Bydd y dangosfwrdd hwn yn rhestru MCCDs sydd:&lt;/p&gt;&lt;ul class="govuk-list govuk-list--bullet"&gt;&lt;li&gt;rydych wedi cyflwyno i archwiliwr meddygol i'w gymeradwyo&lt;/li&gt;&lt;li&gt;mae archwiliwr meddygol wedi gwrthod a rhaid i chi nawr ddiwygio&lt;/li&gt;&lt;li&gt;bod archwiliwr meddygol wedi cymeradwyo a bydd yn cael ei anfon ymlaen i swyddfa’r cofrestrydd gan swyddog archwiliwr meddygol&lt;/li&gt;&lt;/ul&gt;&lt;p class="govuk-body"&gt;Bydd MCCDs wedi'u cwblhau yn cael eu dileu ar ôl tri mis.&lt;/p&gt;</t>
-  </si>
-  <si>
     <t>Check that all the details are correct before continuing.</t>
   </si>
   <si>
@@ -5698,13 +5692,19 @@
     <t>2 Amgylchiadau arwyddocaol eraill (dewisol)</t>
   </si>
   <si>
-    <t>031</t>
-  </si>
-  <si>
     <t>I am a duly appointed medical examiner and following scrutiny I confirm that the cause of death is as stated in this certificate to the best of my knowledge and belief.</t>
   </si>
   <si>
     <t>Rwy'n arholwr meddygol a benodwyd yn briodol ac ar ôl craffu rwy'n cadarnhau bod achos y farwolaeth fel y nodir yn y dystysgrif hon hyd eithaf fy ngwybodaeth a'm cred.</t>
+  </si>
+  <si>
+    <t>&lt;p class="govuk-body"&gt;This dashboard allows you to create a new Medical certificate of cause of death (MCCD) and manage current MCCDs.&lt;/p&gt;&lt;p class="govuk-body"&gt;This dashboard will list MCCDs that:&lt;/p&gt;&lt;ul class="govuk-list govuk-list--bullet"&gt;&lt;li&gt;you have submitted to a medical examiner for approval&lt;/li&gt;&lt;li&gt;have been approved by a medical examiner&lt;/li&gt;&lt;li&gt;have been rejected by a medical examiner and need amending&lt;/li&gt;&lt;/ul&gt;&lt;p class="govuk-body"&gt;Completed MCCDs will be removed after three months.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p class="govuk-body"&gt;Mae'r dangosfwrdd hwn yn eich galluogi i greu Tystysgrif Feddygol achos marwolaeth (MCCD) newydd a rheoli MCCDs presennol.&lt;/p&gt;&lt;p dosbarth = "govuk-body"&gt;Bydd y dangosfwrdd hwn yn rhestru MCCDs bod:&lt;/p&gt;&lt;ul dosbarth = "govuk-list--bullet"&gt;&lt;li&gt;rydych wedi cyflwyno i arholwr meddygol i'w gymeradwyo&lt;/li&gt;&lt;li&gt;gan arholwr meddygol wedi cael eu gwrthod gan arholwr meddygol&lt;/li&gt;&lt;li&gt;ac mae angen ei ddiwygio&lt;/li&gt;&lt;/ul&gt;&lt;p dosbarth = "govuk-body"&gt;Bydd MCCDs wedi'u cwblhau yn cael eu dileu ar ôl tri mis.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>032</t>
   </si>
 </sst>
 </file>
@@ -6672,6 +6672,24 @@
     <xf numFmtId="0" fontId="13" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -6679,24 +6697,6 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -7920,7 +7920,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E52C375-4A34-4943-A40B-CD02CAD0761B}">
   <dimension ref="A1:F24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D15" sqref="D15"/>
     </sheetView>
@@ -7964,13 +7964,13 @@
         <v>1241</v>
       </c>
       <c r="C2" s="151" t="s">
-        <v>1418</v>
+        <v>1416</v>
       </c>
       <c r="D2" s="92" t="s">
         <v>1242</v>
       </c>
       <c r="E2" s="152" t="s">
-        <v>1422</v>
+        <v>1420</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="80" x14ac:dyDescent="0.2">
@@ -7998,13 +7998,13 @@
         <v>1248</v>
       </c>
       <c r="C4" s="158" t="s">
-        <v>1419</v>
+        <v>1417</v>
       </c>
       <c r="D4" s="95" t="s">
         <v>404</v>
       </c>
       <c r="E4" s="155" t="s">
-        <v>1421</v>
+        <v>1419</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="60.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -8066,13 +8066,13 @@
         <v>1253</v>
       </c>
       <c r="C8" s="158" t="s">
-        <v>1418</v>
+        <v>1416</v>
       </c>
       <c r="D8" s="95" t="s">
         <v>1254</v>
       </c>
       <c r="E8" s="155" t="s">
-        <v>1422</v>
+        <v>1420</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="64" x14ac:dyDescent="0.2">
@@ -8100,13 +8100,13 @@
         <v>1259</v>
       </c>
       <c r="C10" s="158" t="s">
-        <v>1419</v>
+        <v>1417</v>
       </c>
       <c r="D10" s="95" t="s">
         <v>404</v>
       </c>
       <c r="E10" s="155" t="s">
-        <v>1421</v>
+        <v>1419</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -8168,13 +8168,13 @@
         <v>1262</v>
       </c>
       <c r="C14" s="158" t="s">
-        <v>1418</v>
+        <v>1416</v>
       </c>
       <c r="D14" s="95" t="s">
         <v>1263</v>
       </c>
       <c r="E14" s="155" t="s">
-        <v>1420</v>
+        <v>1418</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="80" x14ac:dyDescent="0.2">
@@ -8185,13 +8185,13 @@
         <v>1264</v>
       </c>
       <c r="C15" s="158" t="s">
-        <v>1440</v>
+        <v>1437</v>
       </c>
       <c r="D15" s="95" t="s">
         <v>1265</v>
       </c>
       <c r="E15" s="155" t="s">
-        <v>1441</v>
+        <v>1438</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="48" x14ac:dyDescent="0.2">
@@ -8236,13 +8236,13 @@
         <v>1268</v>
       </c>
       <c r="C18" s="158" t="s">
-        <v>1419</v>
+        <v>1417</v>
       </c>
       <c r="D18" s="95" t="s">
         <v>404</v>
       </c>
       <c r="E18" s="155" t="s">
-        <v>1421</v>
+        <v>1419</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -8270,13 +8270,13 @@
         <v>1269</v>
       </c>
       <c r="C20" s="158" t="s">
-        <v>1418</v>
+        <v>1416</v>
       </c>
       <c r="D20" s="95" t="s">
         <v>1242</v>
       </c>
       <c r="E20" s="155" t="s">
-        <v>1420</v>
+        <v>1418</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="48" x14ac:dyDescent="0.2">
@@ -8304,13 +8304,13 @@
         <v>1273</v>
       </c>
       <c r="C22" s="158" t="s">
-        <v>1419</v>
+        <v>1417</v>
       </c>
       <c r="D22" s="95" t="s">
         <v>404</v>
       </c>
       <c r="E22" s="155" t="s">
-        <v>1423</v>
+        <v>1421</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="48" x14ac:dyDescent="0.2">
@@ -8483,10 +8483,10 @@
         <v>1293</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>1428</v>
+        <v>1426</v>
       </c>
       <c r="E8" s="37" t="s">
-        <v>1429</v>
+        <v>1427</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="16" x14ac:dyDescent="0.2">
@@ -8567,11 +8567,11 @@
         <v>1310</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>1426</v>
+        <v>1424</v>
       </c>
       <c r="D14" s="1"/>
       <c r="E14" s="37" t="s">
-        <v>1427</v>
+        <v>1425</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="32" x14ac:dyDescent="0.2">
@@ -8654,10 +8654,10 @@
         <v>1325</v>
       </c>
       <c r="C20" s="59" t="s">
+        <v>1393</v>
+      </c>
+      <c r="E20" s="37" t="s">
         <v>1395</v>
-      </c>
-      <c r="E20" s="37" t="s">
-        <v>1397</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="16" x14ac:dyDescent="0.2">
@@ -8682,10 +8682,10 @@
         <v>1327</v>
       </c>
       <c r="C22" s="6" t="s">
+        <v>1394</v>
+      </c>
+      <c r="E22" s="37" t="s">
         <v>1396</v>
-      </c>
-      <c r="E22" s="37" t="s">
-        <v>1398</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
@@ -8707,7 +8707,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F68"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="F3" sqref="F3"/>
     </sheetView>
@@ -8749,13 +8749,13 @@
         <v>7</v>
       </c>
       <c r="C2" s="100" t="s">
-        <v>1439</v>
+        <v>1441</v>
       </c>
       <c r="D2" s="98" t="s">
         <v>8</v>
       </c>
       <c r="E2" s="99" t="s">
-        <v>1439</v>
+        <v>1441</v>
       </c>
       <c r="F2" s="98"/>
     </row>
@@ -8773,7 +8773,7 @@
         <v>12</v>
       </c>
       <c r="E3" s="37" t="s">
-        <v>1394</v>
+        <v>1392</v>
       </c>
       <c r="F3" s="5" t="s">
         <v>13</v>
@@ -10366,7 +10366,7 @@
   <dimension ref="A1:F31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
@@ -10453,7 +10453,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="365" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" ht="288" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
         <v>248</v>
       </c>
@@ -10461,13 +10461,13 @@
         <v>281</v>
       </c>
       <c r="C5" s="52" t="s">
-        <v>1386</v>
+        <v>1439</v>
       </c>
       <c r="D5" s="66" t="s">
         <v>282</v>
       </c>
       <c r="E5" s="156" t="s">
-        <v>1391</v>
+        <v>1440</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>283</v>
@@ -10481,13 +10481,13 @@
         <v>284</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>1387</v>
+        <v>1386</v>
       </c>
       <c r="D6" s="67" t="s">
         <v>285</v>
       </c>
       <c r="E6" s="157" t="s">
-        <v>1388</v>
+        <v>1387</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="160" x14ac:dyDescent="0.2">
@@ -10498,13 +10498,13 @@
         <v>286</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>1389</v>
+        <v>1388</v>
       </c>
       <c r="D7" s="67" t="s">
         <v>287</v>
       </c>
       <c r="E7" s="157" t="s">
-        <v>1390</v>
+        <v>1389</v>
       </c>
       <c r="F7" s="68" t="s">
         <v>288</v>
@@ -10927,13 +10927,13 @@
       </c>
     </row>
     <row r="2" spans="1:6" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="170" t="s">
+      <c r="A2" s="167" t="s">
         <v>367</v>
       </c>
-      <c r="B2" s="171"/>
-      <c r="C2" s="171"/>
-      <c r="D2" s="171"/>
-      <c r="E2" s="172"/>
+      <c r="B2" s="168"/>
+      <c r="C2" s="168"/>
+      <c r="D2" s="168"/>
+      <c r="E2" s="169"/>
       <c r="F2" s="33"/>
     </row>
     <row r="3" spans="1:6" ht="48" x14ac:dyDescent="0.2">
@@ -11061,13 +11061,13 @@
       <c r="F9" s="119"/>
     </row>
     <row r="10" spans="1:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="173" t="s">
+      <c r="A10" s="170" t="s">
         <v>396</v>
       </c>
-      <c r="B10" s="174"/>
-      <c r="C10" s="174"/>
-      <c r="D10" s="174"/>
-      <c r="E10" s="175"/>
+      <c r="B10" s="171"/>
+      <c r="C10" s="171"/>
+      <c r="D10" s="171"/>
+      <c r="E10" s="172"/>
       <c r="F10" s="119"/>
     </row>
     <row r="11" spans="1:6" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -12186,11 +12186,11 @@
         <v>572</v>
       </c>
       <c r="C84" s="117" t="s">
-        <v>1406</v>
+        <v>1404</v>
       </c>
       <c r="D84" s="116"/>
       <c r="E84" s="120" t="s">
-        <v>1407</v>
+        <v>1405</v>
       </c>
       <c r="F84" s="119" t="s">
         <v>573</v>
@@ -12300,11 +12300,11 @@
         <v>591</v>
       </c>
       <c r="C91" s="117" t="s">
-        <v>1404</v>
+        <v>1402</v>
       </c>
       <c r="D91" s="116"/>
       <c r="E91" s="120" t="s">
-        <v>1405</v>
+        <v>1403</v>
       </c>
       <c r="F91" s="119"/>
     </row>
@@ -12344,11 +12344,11 @@
         <v>597</v>
       </c>
       <c r="C94" s="117" t="s">
-        <v>1424</v>
+        <v>1422</v>
       </c>
       <c r="D94" s="116"/>
       <c r="E94" s="120" t="s">
-        <v>1425</v>
+        <v>1423</v>
       </c>
       <c r="F94" s="119" t="s">
         <v>573</v>
@@ -12379,7 +12379,7 @@
         <v>84</v>
       </c>
       <c r="B96" s="159" t="s">
-        <v>1430</v>
+        <v>1428</v>
       </c>
       <c r="C96" s="93" t="s">
         <v>599</v>
@@ -12397,7 +12397,7 @@
         <v>84</v>
       </c>
       <c r="B97" s="159" t="s">
-        <v>1431</v>
+        <v>1429</v>
       </c>
       <c r="C97" s="93" t="s">
         <v>599</v>
@@ -12415,7 +12415,7 @@
         <v>84</v>
       </c>
       <c r="B98" s="160" t="s">
-        <v>1432</v>
+        <v>1430</v>
       </c>
       <c r="C98" s="161" t="s">
         <v>599</v>
@@ -12431,7 +12431,7 @@
         <v>84</v>
       </c>
       <c r="B99" s="160" t="s">
-        <v>1433</v>
+        <v>1431</v>
       </c>
       <c r="C99" s="161" t="s">
         <v>599</v>
@@ -12447,7 +12447,7 @@
         <v>84</v>
       </c>
       <c r="B100" s="160" t="s">
-        <v>1434</v>
+        <v>1432</v>
       </c>
       <c r="C100" s="161" t="s">
         <v>599</v>
@@ -13485,13 +13485,13 @@
       <c r="F169" s="119"/>
     </row>
     <row r="170" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A170" s="167" t="s">
+      <c r="A170" s="173" t="s">
         <v>762</v>
       </c>
-      <c r="B170" s="168"/>
-      <c r="C170" s="168"/>
-      <c r="D170" s="168"/>
-      <c r="E170" s="169"/>
+      <c r="B170" s="174"/>
+      <c r="C170" s="174"/>
+      <c r="D170" s="174"/>
+      <c r="E170" s="175"/>
       <c r="F170" s="129" t="s">
         <v>763</v>
       </c>
@@ -14448,13 +14448,13 @@
         <v>863</v>
       </c>
       <c r="C233" s="59" t="s">
-        <v>1392</v>
+        <v>1390</v>
       </c>
       <c r="D233" s="116" t="s">
         <v>864</v>
       </c>
       <c r="E233" s="120" t="s">
-        <v>1393</v>
+        <v>1391</v>
       </c>
       <c r="F233" s="119"/>
     </row>
@@ -15394,18 +15394,6 @@
     </row>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="A230:E230"/>
-    <mergeCell ref="A191:E191"/>
-    <mergeCell ref="A195:E195"/>
-    <mergeCell ref="A202:E202"/>
-    <mergeCell ref="A213:E213"/>
-    <mergeCell ref="A219:E219"/>
-    <mergeCell ref="A58:E58"/>
-    <mergeCell ref="A2:E2"/>
-    <mergeCell ref="A10:E10"/>
-    <mergeCell ref="A14:E14"/>
-    <mergeCell ref="A24:E24"/>
-    <mergeCell ref="A43:E43"/>
     <mergeCell ref="A179:E179"/>
     <mergeCell ref="A162:E162"/>
     <mergeCell ref="A63:E63"/>
@@ -15416,6 +15404,18 @@
     <mergeCell ref="A151:E151"/>
     <mergeCell ref="A92:E92"/>
     <mergeCell ref="A170:E170"/>
+    <mergeCell ref="A58:E58"/>
+    <mergeCell ref="A2:E2"/>
+    <mergeCell ref="A10:E10"/>
+    <mergeCell ref="A14:E14"/>
+    <mergeCell ref="A24:E24"/>
+    <mergeCell ref="A43:E43"/>
+    <mergeCell ref="A230:E230"/>
+    <mergeCell ref="A191:E191"/>
+    <mergeCell ref="A195:E195"/>
+    <mergeCell ref="A202:E202"/>
+    <mergeCell ref="A213:E213"/>
+    <mergeCell ref="A219:E219"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -15892,10 +15892,10 @@
         <v>979</v>
       </c>
       <c r="C32" s="21" t="s">
-        <v>1399</v>
+        <v>1397</v>
       </c>
       <c r="E32" s="46" t="s">
-        <v>1400</v>
+        <v>1398</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="32" x14ac:dyDescent="0.2">
@@ -15903,13 +15903,13 @@
         <v>261</v>
       </c>
       <c r="B33" s="19" t="s">
+        <v>1399</v>
+      </c>
+      <c r="C33" s="21" t="s">
+        <v>1400</v>
+      </c>
+      <c r="E33" s="46" t="s">
         <v>1401</v>
-      </c>
-      <c r="C33" s="21" t="s">
-        <v>1402</v>
-      </c>
-      <c r="E33" s="46" t="s">
-        <v>1403</v>
       </c>
     </row>
     <row r="34" spans="1:6" ht="48" x14ac:dyDescent="0.2">
@@ -16069,13 +16069,13 @@
         <v>1004</v>
       </c>
       <c r="C45" s="62" t="s">
-        <v>1392</v>
+        <v>1390</v>
       </c>
       <c r="D45" s="116" t="s">
         <v>1005</v>
       </c>
       <c r="E45" s="46" t="s">
-        <v>1393</v>
+        <v>1391</v>
       </c>
     </row>
     <row r="46" spans="1:6" ht="48" x14ac:dyDescent="0.2">
@@ -16468,23 +16468,23 @@
         <v>1071</v>
       </c>
       <c r="E11" s="138" t="s">
-        <v>1417</v>
+        <v>1415</v>
       </c>
       <c r="F11" s="135"/>
     </row>
     <row r="12" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A12" s="136" t="s">
+        <v>1411</v>
+      </c>
+      <c r="B12" s="136" t="s">
+        <v>1412</v>
+      </c>
+      <c r="C12" s="137" t="s">
         <v>1413</v>
-      </c>
-      <c r="B12" s="136" t="s">
-        <v>1414</v>
-      </c>
-      <c r="C12" s="137" t="s">
-        <v>1415</v>
       </c>
       <c r="D12" s="136"/>
       <c r="E12" s="138" t="s">
-        <v>1416</v>
+        <v>1414</v>
       </c>
       <c r="F12" s="135"/>
     </row>
@@ -16496,7 +16496,7 @@
         <v>1072</v>
       </c>
       <c r="C13" s="137" t="s">
-        <v>1411</v>
+        <v>1409</v>
       </c>
       <c r="D13" s="136" t="s">
         <v>1073</v>
@@ -16542,7 +16542,7 @@
         <v>1078</v>
       </c>
       <c r="C16" s="137" t="s">
-        <v>1408</v>
+        <v>1406</v>
       </c>
       <c r="D16" s="136" t="s">
         <v>1079</v>
@@ -16560,7 +16560,7 @@
         <v>1081</v>
       </c>
       <c r="C17" s="137" t="s">
-        <v>1409</v>
+        <v>1407</v>
       </c>
       <c r="D17" s="136" t="s">
         <v>1082</v>
@@ -16578,7 +16578,7 @@
         <v>1084</v>
       </c>
       <c r="C18" s="137" t="s">
-        <v>1410</v>
+        <v>1408</v>
       </c>
       <c r="D18" s="136" t="s">
         <v>1085</v>
@@ -16718,17 +16718,17 @@
     </row>
     <row r="28" spans="1:6" ht="64" x14ac:dyDescent="0.2">
       <c r="A28" s="136" t="s">
-        <v>1413</v>
+        <v>1411</v>
       </c>
       <c r="B28" s="136" t="s">
-        <v>1412</v>
+        <v>1410</v>
       </c>
       <c r="C28" s="137" t="s">
-        <v>1435</v>
+        <v>1433</v>
       </c>
       <c r="D28" s="136"/>
       <c r="E28" s="138" t="s">
-        <v>1437</v>
+        <v>1435</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="32" x14ac:dyDescent="0.2">
@@ -16739,13 +16739,13 @@
         <v>1110</v>
       </c>
       <c r="C29" s="137" t="s">
-        <v>1436</v>
+        <v>1434</v>
       </c>
       <c r="D29" s="136" t="s">
         <v>1111</v>
       </c>
       <c r="E29" s="138" t="s">
-        <v>1438</v>
+        <v>1436</v>
       </c>
     </row>
     <row r="30" spans="1:6" s="13" customFormat="1" x14ac:dyDescent="0.2">
@@ -17080,13 +17080,13 @@
         <v>1160</v>
       </c>
       <c r="C51" s="62" t="s">
-        <v>1392</v>
+        <v>1390</v>
       </c>
       <c r="D51" s="116" t="s">
         <v>1005</v>
       </c>
       <c r="E51" s="63" t="s">
-        <v>1393</v>
+        <v>1391</v>
       </c>
     </row>
     <row r="52" spans="1:6" s="30" customFormat="1" ht="48" x14ac:dyDescent="0.2">
@@ -17717,15 +17717,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <Readyforteam_x003f_ xmlns="565e1b1d-057e-4d85-b896-01a5881d8a45">false</Readyforteam_x003f_>
@@ -17766,6 +17757,15 @@
 </p:properties>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EAFDB110-4046-4E72-A1EF-1908ABEC3151}">
   <ds:schemaRefs>
@@ -17788,14 +17788,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8D7CE8C7-18DC-484F-8376-ED09F13D44C8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{017ACE96-8143-486E-8436-7787F6B96F4A}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -17806,4 +17798,12 @@
     <ds:schemaRef ds:uri="2799d30d-6731-4efe-ac9b-c4895a8828d9"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8D7CE8C7-18DC-484F-8376-ED09F13D44C8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
[MCCDB-907] Content amend - ME (cert) Confirmation page
</commit_message>
<xml_diff>
--- a/app/data/MCCD-localisation.xlsx
+++ b/app/data/MCCD-localisation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/JALAT/GIT/medical-certificate-of-cause-of-death/app/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DBE28D6-832A-254A-9785-52113F0520ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B4DE858-58D5-C044-9719-AECBC76F5CEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="14100" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="14100" firstSheet="4" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Using this document" sheetId="8" r:id="rId1"/>
@@ -5207,9 +5207,6 @@
     <t>confirmationPageContent</t>
   </si>
   <si>
-    <t>The medical certificate of cause of death has now been created.</t>
-  </si>
-  <si>
     <t>Mae tystysgrif feddygol achos marwolaeth bellach wedi'i chreu.</t>
   </si>
   <si>
@@ -5223,12 +5220,6 @@
   </si>
   <si>
     <t>confirmationPageWhatHappensNextContent</t>
-  </si>
-  <si>
-    <t>The medical certificate of cause of death will now be sent to the registrar. You can still view the certificate in your dashboard under completed certificates.</t>
-  </si>
-  <si>
-    <t>Bydd y dystysgrif feddygol o achos marwolaeth yn cael ei hanfon at y cofrestrydd yn awr. Gallwch barhau i weld y dystysgrif yn eich dangosfwrdd o dan dystysgrifau wedi'u cwblhau.</t>
   </si>
   <si>
     <t>confirmationPageSubheadingTwo</t>
@@ -5704,7 +5695,16 @@
     <t>&lt;p class="govuk-body"&gt;Mae'r dangosfwrdd hwn yn eich galluogi i greu Tystysgrif Feddygol achos marwolaeth (MCCD) newydd a rheoli MCCDs presennol.&lt;/p&gt;&lt;p dosbarth = "govuk-body"&gt;Bydd y dangosfwrdd hwn yn rhestru MCCDs bod:&lt;/p&gt;&lt;ul dosbarth = "govuk-list--bullet"&gt;&lt;li&gt;rydych wedi cyflwyno i arholwr meddygol i'w gymeradwyo&lt;/li&gt;&lt;li&gt;gan arholwr meddygol wedi cael eu gwrthod gan arholwr meddygol&lt;/li&gt;&lt;li&gt;ac mae angen ei ddiwygio&lt;/li&gt;&lt;/ul&gt;&lt;p dosbarth = "govuk-body"&gt;Bydd MCCDs wedi'u cwblhau yn cael eu dileu ar ôl tri mis.&lt;/p&gt;</t>
   </si>
   <si>
-    <t>032</t>
+    <t>The Medical certificate of cause of death (MCCD)  has been created and sent to the medical examiner office. This certificate will be available to view from your dashboard for 3 months.</t>
+  </si>
+  <si>
+    <t>Mae'r dystysgrif feddygol o achos marwolaeth (MCCD) wedi'i chreu a'i hanfon i'r swyddfa arholwr meddygol. Bydd y dystysgrif hon ar gael i'w gweld o'ch dangosfwrdd am 3 mis.</t>
+  </si>
+  <si>
+    <t>The Medical certificate of cause of death has now been created.</t>
+  </si>
+  <si>
+    <t>034</t>
   </si>
 </sst>
 </file>
@@ -7921,7 +7921,7 @@
   <dimension ref="A1:F24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
@@ -7964,13 +7964,13 @@
         <v>1241</v>
       </c>
       <c r="C2" s="151" t="s">
-        <v>1416</v>
+        <v>1413</v>
       </c>
       <c r="D2" s="92" t="s">
         <v>1242</v>
       </c>
       <c r="E2" s="152" t="s">
-        <v>1420</v>
+        <v>1417</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="80" x14ac:dyDescent="0.2">
@@ -7998,13 +7998,13 @@
         <v>1248</v>
       </c>
       <c r="C4" s="158" t="s">
-        <v>1417</v>
+        <v>1414</v>
       </c>
       <c r="D4" s="95" t="s">
         <v>404</v>
       </c>
       <c r="E4" s="155" t="s">
-        <v>1419</v>
+        <v>1416</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="60.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -8066,13 +8066,13 @@
         <v>1253</v>
       </c>
       <c r="C8" s="158" t="s">
-        <v>1416</v>
+        <v>1413</v>
       </c>
       <c r="D8" s="95" t="s">
         <v>1254</v>
       </c>
       <c r="E8" s="155" t="s">
-        <v>1420</v>
+        <v>1417</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="64" x14ac:dyDescent="0.2">
@@ -8100,13 +8100,13 @@
         <v>1259</v>
       </c>
       <c r="C10" s="158" t="s">
-        <v>1417</v>
+        <v>1414</v>
       </c>
       <c r="D10" s="95" t="s">
         <v>404</v>
       </c>
       <c r="E10" s="155" t="s">
-        <v>1419</v>
+        <v>1416</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -8168,13 +8168,13 @@
         <v>1262</v>
       </c>
       <c r="C14" s="158" t="s">
-        <v>1416</v>
+        <v>1413</v>
       </c>
       <c r="D14" s="95" t="s">
         <v>1263</v>
       </c>
       <c r="E14" s="155" t="s">
-        <v>1418</v>
+        <v>1415</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="80" x14ac:dyDescent="0.2">
@@ -8185,13 +8185,13 @@
         <v>1264</v>
       </c>
       <c r="C15" s="158" t="s">
-        <v>1437</v>
+        <v>1434</v>
       </c>
       <c r="D15" s="95" t="s">
         <v>1265</v>
       </c>
       <c r="E15" s="155" t="s">
-        <v>1438</v>
+        <v>1435</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="48" x14ac:dyDescent="0.2">
@@ -8236,13 +8236,13 @@
         <v>1268</v>
       </c>
       <c r="C18" s="158" t="s">
-        <v>1417</v>
+        <v>1414</v>
       </c>
       <c r="D18" s="95" t="s">
         <v>404</v>
       </c>
       <c r="E18" s="155" t="s">
-        <v>1419</v>
+        <v>1416</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -8270,13 +8270,13 @@
         <v>1269</v>
       </c>
       <c r="C20" s="158" t="s">
-        <v>1416</v>
+        <v>1413</v>
       </c>
       <c r="D20" s="95" t="s">
         <v>1242</v>
       </c>
       <c r="E20" s="155" t="s">
-        <v>1418</v>
+        <v>1415</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="48" x14ac:dyDescent="0.2">
@@ -8304,13 +8304,13 @@
         <v>1273</v>
       </c>
       <c r="C22" s="158" t="s">
-        <v>1417</v>
+        <v>1414</v>
       </c>
       <c r="D22" s="95" t="s">
         <v>404</v>
       </c>
       <c r="E22" s="155" t="s">
-        <v>1421</v>
+        <v>1418</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="48" x14ac:dyDescent="0.2">
@@ -8356,9 +8356,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{124C2F8F-96ED-4E65-B816-FFFEB93DC889}">
   <dimension ref="A1:F23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F8" sqref="F8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -8427,10 +8427,10 @@
         <v>1280</v>
       </c>
       <c r="C4" s="59" t="s">
+        <v>1440</v>
+      </c>
+      <c r="E4" s="37" t="s">
         <v>1281</v>
-      </c>
-      <c r="E4" s="37" t="s">
-        <v>1282</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="16" x14ac:dyDescent="0.2">
@@ -8438,13 +8438,13 @@
         <v>254</v>
       </c>
       <c r="B5" s="5" t="s">
+        <v>1282</v>
+      </c>
+      <c r="C5" s="6" t="s">
         <v>1283</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="E5" s="37" t="s">
         <v>1284</v>
-      </c>
-      <c r="E5" s="37" t="s">
-        <v>1285</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="80" x14ac:dyDescent="0.2">
@@ -8452,13 +8452,13 @@
         <v>261</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>1286</v>
+        <v>1285</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>1287</v>
+        <v>1438</v>
       </c>
       <c r="E6" s="37" t="s">
-        <v>1288</v>
+        <v>1439</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="32" x14ac:dyDescent="0.2">
@@ -8466,112 +8466,112 @@
         <v>254</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>1289</v>
+        <v>1286</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>1290</v>
+        <v>1287</v>
       </c>
       <c r="E7" s="37" t="s">
-        <v>1291</v>
+        <v>1288</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
-        <v>1292</v>
+        <v>1289</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>1293</v>
+        <v>1290</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>1426</v>
+        <v>1423</v>
       </c>
       <c r="E8" s="37" t="s">
-        <v>1427</v>
+        <v>1424</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
+        <v>1291</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>1292</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>1293</v>
+      </c>
+      <c r="E9" s="37" t="s">
         <v>1294</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>1295</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>1296</v>
-      </c>
-      <c r="E9" s="37" t="s">
-        <v>1297</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
-        <v>1294</v>
+        <v>1291</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>1298</v>
+        <v>1295</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>1299</v>
+        <v>1296</v>
       </c>
       <c r="E10" s="37" t="s">
-        <v>1300</v>
+        <v>1297</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
-        <v>1294</v>
+        <v>1291</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>1301</v>
+        <v>1298</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>1302</v>
+        <v>1299</v>
       </c>
       <c r="E11" s="37" t="s">
-        <v>1303</v>
+        <v>1300</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="5" t="s">
-        <v>1294</v>
+        <v>1291</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>1304</v>
+        <v>1301</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>1305</v>
+        <v>1302</v>
       </c>
       <c r="E12" s="37" t="s">
-        <v>1306</v>
+        <v>1303</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="s">
-        <v>1294</v>
+        <v>1291</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>1307</v>
+        <v>1304</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>1308</v>
+        <v>1305</v>
       </c>
       <c r="E13" s="37" t="s">
-        <v>1309</v>
+        <v>1306</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A14" s="5" t="s">
-        <v>1292</v>
+        <v>1289</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>1310</v>
+        <v>1307</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>1424</v>
+        <v>1421</v>
       </c>
       <c r="D14" s="1"/>
       <c r="E14" s="37" t="s">
-        <v>1425</v>
+        <v>1422</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="32" x14ac:dyDescent="0.2">
@@ -8579,14 +8579,14 @@
         <v>949</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>1311</v>
+        <v>1308</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>1312</v>
+        <v>1309</v>
       </c>
       <c r="D15" s="1"/>
       <c r="E15" s="37" t="s">
-        <v>1313</v>
+        <v>1310</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="16" x14ac:dyDescent="0.2">
@@ -8594,34 +8594,34 @@
         <v>14</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>1314</v>
+        <v>1311</v>
       </c>
       <c r="C16" s="74" t="s">
-        <v>1315</v>
+        <v>1312</v>
       </c>
       <c r="D16" s="18"/>
       <c r="E16" s="37" t="s">
-        <v>1316</v>
+        <v>1313</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A17" s="5" t="s">
-        <v>1317</v>
+        <v>1314</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>1318</v>
+        <v>1315</v>
       </c>
       <c r="C17" s="75" t="s">
-        <v>1319</v>
+        <v>1316</v>
       </c>
       <c r="D17" s="18"/>
       <c r="E17" s="37" t="s">
-        <v>1320</v>
+        <v>1317</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="198" t="s">
-        <v>1321</v>
+        <v>1318</v>
       </c>
       <c r="B18" s="199"/>
       <c r="C18" s="199"/>
@@ -8634,16 +8634,16 @@
         <v>243</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>1324</v>
+        <v>1321</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>1322</v>
+        <v>1319</v>
       </c>
       <c r="D19" s="5" t="s">
         <v>1223</v>
       </c>
       <c r="E19" s="37" t="s">
-        <v>1323</v>
+        <v>1320</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="96" x14ac:dyDescent="0.2">
@@ -8651,13 +8651,13 @@
         <v>261</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>1325</v>
+        <v>1322</v>
       </c>
       <c r="C20" s="59" t="s">
-        <v>1393</v>
+        <v>1390</v>
       </c>
       <c r="E20" s="37" t="s">
-        <v>1395</v>
+        <v>1392</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="16" x14ac:dyDescent="0.2">
@@ -8665,13 +8665,13 @@
         <v>254</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>1326</v>
+        <v>1323</v>
       </c>
       <c r="C21" s="6" t="s">
+        <v>1283</v>
+      </c>
+      <c r="E21" s="37" t="s">
         <v>1284</v>
-      </c>
-      <c r="E21" s="37" t="s">
-        <v>1285</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="80" x14ac:dyDescent="0.2">
@@ -8679,13 +8679,13 @@
         <v>261</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>1327</v>
+        <v>1324</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>1394</v>
+        <v>1391</v>
       </c>
       <c r="E22" s="37" t="s">
-        <v>1396</v>
+        <v>1393</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
@@ -8707,7 +8707,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F68"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="F3" sqref="F3"/>
     </sheetView>
@@ -8773,7 +8773,7 @@
         <v>12</v>
       </c>
       <c r="E3" s="37" t="s">
-        <v>1392</v>
+        <v>1389</v>
       </c>
       <c r="F3" s="5" t="s">
         <v>13</v>
@@ -9828,18 +9828,18 @@
     </row>
     <row r="67" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="B67" s="1" t="s">
+        <v>1335</v>
+      </c>
+      <c r="C67" s="2" t="s">
+        <v>1336</v>
+      </c>
+      <c r="E67" s="40" t="s">
         <v>1338</v>
-      </c>
-      <c r="C67" s="2" t="s">
-        <v>1339</v>
-      </c>
-      <c r="E67" s="40" t="s">
-        <v>1341</v>
       </c>
     </row>
     <row r="68" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="B68" s="1" t="s">
-        <v>1340</v>
+        <v>1337</v>
       </c>
       <c r="C68" s="2" t="s">
         <v>76</v>
@@ -10140,14 +10140,14 @@
         <v>243</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>1365</v>
+        <v>1362</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>1366</v>
+        <v>1363</v>
       </c>
       <c r="D2" s="5"/>
       <c r="E2" s="43" t="s">
-        <v>1374</v>
+        <v>1371</v>
       </c>
       <c r="F2" s="1"/>
     </row>
@@ -10156,19 +10156,19 @@
         <v>484</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>1367</v>
+        <v>1364</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>1368</v>
+        <v>1365</v>
       </c>
       <c r="D3" s="5"/>
       <c r="E3" s="43" t="s">
-        <v>1375</v>
+        <v>1372</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="164" t="s">
-        <v>1369</v>
+        <v>1366</v>
       </c>
       <c r="B4" s="165"/>
       <c r="C4" s="165"/>
@@ -10180,14 +10180,14 @@
         <v>243</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>1370</v>
+        <v>1367</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>1372</v>
+        <v>1369</v>
       </c>
       <c r="D5" s="5"/>
       <c r="E5" s="43" t="s">
-        <v>1376</v>
+        <v>1373</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="96" x14ac:dyDescent="0.2">
@@ -10195,14 +10195,14 @@
         <v>484</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>1371</v>
+        <v>1368</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>1373</v>
+        <v>1370</v>
       </c>
       <c r="D6" s="5"/>
       <c r="E6" s="43" t="s">
-        <v>1377</v>
+        <v>1374</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
@@ -10423,7 +10423,7 @@
         <v>243</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>1380</v>
+        <v>1377</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>276</v>
@@ -10447,7 +10447,7 @@
         <v>246</v>
       </c>
       <c r="E4" s="43" t="s">
-        <v>1381</v>
+        <v>1378</v>
       </c>
       <c r="F4" s="68" t="s">
         <v>280</v>
@@ -10461,13 +10461,13 @@
         <v>281</v>
       </c>
       <c r="C5" s="52" t="s">
-        <v>1439</v>
+        <v>1436</v>
       </c>
       <c r="D5" s="66" t="s">
         <v>282</v>
       </c>
       <c r="E5" s="156" t="s">
-        <v>1440</v>
+        <v>1437</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>283</v>
@@ -10481,13 +10481,13 @@
         <v>284</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>1386</v>
+        <v>1383</v>
       </c>
       <c r="D6" s="67" t="s">
         <v>285</v>
       </c>
       <c r="E6" s="157" t="s">
-        <v>1387</v>
+        <v>1384</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="160" x14ac:dyDescent="0.2">
@@ -10498,13 +10498,13 @@
         <v>286</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>1388</v>
+        <v>1385</v>
       </c>
       <c r="D7" s="67" t="s">
         <v>287</v>
       </c>
       <c r="E7" s="157" t="s">
-        <v>1389</v>
+        <v>1386</v>
       </c>
       <c r="F7" s="68" t="s">
         <v>288</v>
@@ -10706,7 +10706,7 @@
         <v>336</v>
       </c>
       <c r="C19" s="64" t="s">
-        <v>1378</v>
+        <v>1375</v>
       </c>
       <c r="D19" s="7" t="s">
         <v>337</v>
@@ -10840,17 +10840,17 @@
     </row>
     <row r="27" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A27" s="5" t="s">
-        <v>1384</v>
+        <v>1381</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>1385</v>
+        <v>1382</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>1382</v>
+        <v>1379</v>
       </c>
       <c r="D27" s="5"/>
       <c r="E27" s="37" t="s">
-        <v>1383</v>
+        <v>1380</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
@@ -11096,13 +11096,13 @@
         <v>401</v>
       </c>
       <c r="C12" s="153" t="s">
-        <v>1342</v>
+        <v>1339</v>
       </c>
       <c r="D12" s="84" t="s">
         <v>402</v>
       </c>
       <c r="E12" s="152" t="s">
-        <v>1343</v>
+        <v>1340</v>
       </c>
       <c r="F12" s="86"/>
     </row>
@@ -11114,13 +11114,13 @@
         <v>403</v>
       </c>
       <c r="C13" s="154" t="s">
-        <v>1344</v>
+        <v>1341</v>
       </c>
       <c r="D13" s="88" t="s">
         <v>404</v>
       </c>
       <c r="E13" s="155" t="s">
-        <v>1345</v>
+        <v>1342</v>
       </c>
       <c r="F13" s="86"/>
     </row>
@@ -11588,7 +11588,7 @@
         <v>485</v>
       </c>
       <c r="C45" s="59" t="s">
-        <v>1361</v>
+        <v>1358</v>
       </c>
       <c r="D45" s="116"/>
       <c r="E45" s="120" t="s">
@@ -11601,14 +11601,14 @@
         <v>484</v>
       </c>
       <c r="B46" s="116" t="s">
-        <v>1364</v>
+        <v>1361</v>
       </c>
       <c r="C46" s="59" t="s">
-        <v>1362</v>
+        <v>1359</v>
       </c>
       <c r="D46" s="116"/>
       <c r="E46" s="120" t="s">
-        <v>1363</v>
+        <v>1360</v>
       </c>
       <c r="F46" s="119"/>
     </row>
@@ -11836,7 +11836,7 @@
         <v>522</v>
       </c>
       <c r="E61" s="120" t="s">
-        <v>1354</v>
+        <v>1351</v>
       </c>
       <c r="F61" s="119"/>
     </row>
@@ -11845,14 +11845,14 @@
         <v>519</v>
       </c>
       <c r="B62" s="116" t="s">
-        <v>1351</v>
+        <v>1348</v>
       </c>
       <c r="C62" s="117" t="s">
-        <v>1353</v>
+        <v>1350</v>
       </c>
       <c r="D62" s="116"/>
       <c r="E62" s="120" t="s">
-        <v>1352</v>
+        <v>1349</v>
       </c>
       <c r="F62" s="119"/>
     </row>
@@ -12186,11 +12186,11 @@
         <v>572</v>
       </c>
       <c r="C84" s="117" t="s">
-        <v>1404</v>
+        <v>1401</v>
       </c>
       <c r="D84" s="116"/>
       <c r="E84" s="120" t="s">
-        <v>1405</v>
+        <v>1402</v>
       </c>
       <c r="F84" s="119" t="s">
         <v>573</v>
@@ -12300,11 +12300,11 @@
         <v>591</v>
       </c>
       <c r="C91" s="117" t="s">
-        <v>1402</v>
+        <v>1399</v>
       </c>
       <c r="D91" s="116"/>
       <c r="E91" s="120" t="s">
-        <v>1403</v>
+        <v>1400</v>
       </c>
       <c r="F91" s="119"/>
     </row>
@@ -12344,11 +12344,11 @@
         <v>597</v>
       </c>
       <c r="C94" s="117" t="s">
-        <v>1422</v>
+        <v>1419</v>
       </c>
       <c r="D94" s="116"/>
       <c r="E94" s="120" t="s">
-        <v>1423</v>
+        <v>1420</v>
       </c>
       <c r="F94" s="119" t="s">
         <v>573</v>
@@ -12379,7 +12379,7 @@
         <v>84</v>
       </c>
       <c r="B96" s="159" t="s">
-        <v>1428</v>
+        <v>1425</v>
       </c>
       <c r="C96" s="93" t="s">
         <v>599</v>
@@ -12397,7 +12397,7 @@
         <v>84</v>
       </c>
       <c r="B97" s="159" t="s">
-        <v>1429</v>
+        <v>1426</v>
       </c>
       <c r="C97" s="93" t="s">
         <v>599</v>
@@ -12415,7 +12415,7 @@
         <v>84</v>
       </c>
       <c r="B98" s="160" t="s">
-        <v>1430</v>
+        <v>1427</v>
       </c>
       <c r="C98" s="161" t="s">
         <v>599</v>
@@ -12431,7 +12431,7 @@
         <v>84</v>
       </c>
       <c r="B99" s="160" t="s">
-        <v>1431</v>
+        <v>1428</v>
       </c>
       <c r="C99" s="161" t="s">
         <v>599</v>
@@ -12447,7 +12447,7 @@
         <v>84</v>
       </c>
       <c r="B100" s="160" t="s">
-        <v>1432</v>
+        <v>1429</v>
       </c>
       <c r="C100" s="161" t="s">
         <v>599</v>
@@ -13122,7 +13122,7 @@
         <v>707</v>
       </c>
       <c r="C146" s="113" t="s">
-        <v>1329</v>
+        <v>1326</v>
       </c>
       <c r="D146" s="122" t="s">
         <v>708</v>
@@ -13212,7 +13212,7 @@
         <v>722</v>
       </c>
       <c r="C152" s="59" t="s">
-        <v>1328</v>
+        <v>1325</v>
       </c>
       <c r="D152" s="116" t="s">
         <v>723</v>
@@ -13243,14 +13243,14 @@
         <v>37</v>
       </c>
       <c r="B154" s="116" t="s">
-        <v>1330</v>
+        <v>1327</v>
       </c>
       <c r="C154" s="59" t="s">
-        <v>1332</v>
+        <v>1329</v>
       </c>
       <c r="D154" s="116"/>
       <c r="E154" s="120" t="s">
-        <v>1334</v>
+        <v>1331</v>
       </c>
       <c r="F154" s="119"/>
     </row>
@@ -13259,14 +13259,14 @@
         <v>37</v>
       </c>
       <c r="B155" s="116" t="s">
-        <v>1331</v>
+        <v>1328</v>
       </c>
       <c r="C155" s="59" t="s">
-        <v>1333</v>
+        <v>1330</v>
       </c>
       <c r="D155" s="116"/>
       <c r="E155" s="120" t="s">
-        <v>1335</v>
+        <v>1332</v>
       </c>
       <c r="F155" s="119"/>
     </row>
@@ -13918,13 +13918,13 @@
         <v>812</v>
       </c>
       <c r="C198" s="59" t="s">
-        <v>1346</v>
+        <v>1343</v>
       </c>
       <c r="D198" s="116" t="s">
         <v>813</v>
       </c>
       <c r="E198" s="120" t="s">
-        <v>1350</v>
+        <v>1347</v>
       </c>
       <c r="F198" s="119"/>
     </row>
@@ -13933,14 +13933,14 @@
         <v>484</v>
       </c>
       <c r="B199" s="116" t="s">
-        <v>1347</v>
+        <v>1344</v>
       </c>
       <c r="C199" s="59" t="s">
-        <v>1348</v>
+        <v>1345</v>
       </c>
       <c r="D199" s="116"/>
       <c r="E199" s="120" t="s">
-        <v>1349</v>
+        <v>1346</v>
       </c>
       <c r="F199" s="119"/>
     </row>
@@ -14040,11 +14040,11 @@
         <v>824</v>
       </c>
       <c r="C206" s="117" t="s">
-        <v>1357</v>
+        <v>1354</v>
       </c>
       <c r="D206" s="116"/>
       <c r="E206" s="120" t="s">
-        <v>1360</v>
+        <v>1357</v>
       </c>
       <c r="F206" s="119"/>
     </row>
@@ -14053,7 +14053,7 @@
         <v>731</v>
       </c>
       <c r="B207" s="116" t="s">
-        <v>1359</v>
+        <v>1356</v>
       </c>
       <c r="C207" s="117" t="s">
         <v>43</v>
@@ -14069,14 +14069,14 @@
         <v>32</v>
       </c>
       <c r="B208" s="116" t="s">
-        <v>1358</v>
+        <v>1355</v>
       </c>
       <c r="C208" s="134" t="s">
-        <v>1355</v>
+        <v>1352</v>
       </c>
       <c r="D208" s="116"/>
       <c r="E208" s="120" t="s">
-        <v>1356</v>
+        <v>1353</v>
       </c>
       <c r="F208" s="119"/>
     </row>
@@ -14448,13 +14448,13 @@
         <v>863</v>
       </c>
       <c r="C233" s="59" t="s">
-        <v>1390</v>
+        <v>1387</v>
       </c>
       <c r="D233" s="116" t="s">
         <v>864</v>
       </c>
       <c r="E233" s="120" t="s">
-        <v>1391</v>
+        <v>1388</v>
       </c>
       <c r="F233" s="119"/>
     </row>
@@ -15686,13 +15686,13 @@
         <v>939</v>
       </c>
       <c r="C17" s="151" t="s">
-        <v>1336</v>
+        <v>1333</v>
       </c>
       <c r="D17" s="92" t="s">
         <v>931</v>
       </c>
       <c r="E17" s="152" t="s">
-        <v>1337</v>
+        <v>1334</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="80" x14ac:dyDescent="0.2">
@@ -15892,10 +15892,10 @@
         <v>979</v>
       </c>
       <c r="C32" s="21" t="s">
-        <v>1397</v>
+        <v>1394</v>
       </c>
       <c r="E32" s="46" t="s">
-        <v>1398</v>
+        <v>1395</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="32" x14ac:dyDescent="0.2">
@@ -15903,13 +15903,13 @@
         <v>261</v>
       </c>
       <c r="B33" s="19" t="s">
-        <v>1399</v>
+        <v>1396</v>
       </c>
       <c r="C33" s="21" t="s">
-        <v>1400</v>
+        <v>1397</v>
       </c>
       <c r="E33" s="46" t="s">
-        <v>1401</v>
+        <v>1398</v>
       </c>
     </row>
     <row r="34" spans="1:6" ht="48" x14ac:dyDescent="0.2">
@@ -16069,13 +16069,13 @@
         <v>1004</v>
       </c>
       <c r="C45" s="62" t="s">
-        <v>1390</v>
+        <v>1387</v>
       </c>
       <c r="D45" s="116" t="s">
         <v>1005</v>
       </c>
       <c r="E45" s="46" t="s">
-        <v>1391</v>
+        <v>1388</v>
       </c>
     </row>
     <row r="46" spans="1:6" ht="48" x14ac:dyDescent="0.2">
@@ -16468,23 +16468,23 @@
         <v>1071</v>
       </c>
       <c r="E11" s="138" t="s">
-        <v>1415</v>
+        <v>1412</v>
       </c>
       <c r="F11" s="135"/>
     </row>
     <row r="12" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A12" s="136" t="s">
-        <v>1411</v>
+        <v>1408</v>
       </c>
       <c r="B12" s="136" t="s">
-        <v>1412</v>
+        <v>1409</v>
       </c>
       <c r="C12" s="137" t="s">
-        <v>1413</v>
+        <v>1410</v>
       </c>
       <c r="D12" s="136"/>
       <c r="E12" s="138" t="s">
-        <v>1414</v>
+        <v>1411</v>
       </c>
       <c r="F12" s="135"/>
     </row>
@@ -16496,7 +16496,7 @@
         <v>1072</v>
       </c>
       <c r="C13" s="137" t="s">
-        <v>1409</v>
+        <v>1406</v>
       </c>
       <c r="D13" s="136" t="s">
         <v>1073</v>
@@ -16542,7 +16542,7 @@
         <v>1078</v>
       </c>
       <c r="C16" s="137" t="s">
-        <v>1406</v>
+        <v>1403</v>
       </c>
       <c r="D16" s="136" t="s">
         <v>1079</v>
@@ -16560,7 +16560,7 @@
         <v>1081</v>
       </c>
       <c r="C17" s="137" t="s">
-        <v>1407</v>
+        <v>1404</v>
       </c>
       <c r="D17" s="136" t="s">
         <v>1082</v>
@@ -16578,7 +16578,7 @@
         <v>1084</v>
       </c>
       <c r="C18" s="137" t="s">
-        <v>1408</v>
+        <v>1405</v>
       </c>
       <c r="D18" s="136" t="s">
         <v>1085</v>
@@ -16718,17 +16718,17 @@
     </row>
     <row r="28" spans="1:6" ht="64" x14ac:dyDescent="0.2">
       <c r="A28" s="136" t="s">
-        <v>1411</v>
+        <v>1408</v>
       </c>
       <c r="B28" s="136" t="s">
-        <v>1410</v>
+        <v>1407</v>
       </c>
       <c r="C28" s="137" t="s">
-        <v>1433</v>
+        <v>1430</v>
       </c>
       <c r="D28" s="136"/>
       <c r="E28" s="138" t="s">
-        <v>1435</v>
+        <v>1432</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="32" x14ac:dyDescent="0.2">
@@ -16739,13 +16739,13 @@
         <v>1110</v>
       </c>
       <c r="C29" s="137" t="s">
-        <v>1434</v>
+        <v>1431</v>
       </c>
       <c r="D29" s="136" t="s">
         <v>1111</v>
       </c>
       <c r="E29" s="138" t="s">
-        <v>1436</v>
+        <v>1433</v>
       </c>
     </row>
     <row r="30" spans="1:6" s="13" customFormat="1" x14ac:dyDescent="0.2">
@@ -16988,7 +16988,7 @@
         <v>1148</v>
       </c>
       <c r="C45" s="62" t="s">
-        <v>1379</v>
+        <v>1376</v>
       </c>
       <c r="D45" s="5" t="s">
         <v>1149</v>
@@ -17080,13 +17080,13 @@
         <v>1160</v>
       </c>
       <c r="C51" s="62" t="s">
-        <v>1390</v>
+        <v>1387</v>
       </c>
       <c r="D51" s="116" t="s">
         <v>1005</v>
       </c>
       <c r="E51" s="63" t="s">
-        <v>1391</v>
+        <v>1388</v>
       </c>
     </row>
     <row r="52" spans="1:6" s="30" customFormat="1" ht="48" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Adding the "or" to the hospital name and postcode page in V11bi. Adding Or to the global translations.
</commit_message>
<xml_diff>
--- a/app/data/MCCD-localisation.xlsx
+++ b/app/data/MCCD-localisation.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10512"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10609"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/JALAT/GIT/medical-certificate-of-cause-of-death/app/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B4DE858-58D5-C044-9719-AECBC76F5CEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E16C9C00-C5B6-0F44-BBFF-6BCBFB6F0647}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="14100" firstSheet="4" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="14100" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Using this document" sheetId="8" r:id="rId1"/>
@@ -69,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2170" uniqueCount="1442">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2173" uniqueCount="1444">
   <si>
     <r>
       <rPr>
@@ -5704,7 +5704,13 @@
     <t>The Medical certificate of cause of death has now been created.</t>
   </si>
   <si>
-    <t>034</t>
+    <t>globalOr</t>
+  </si>
+  <si>
+    <t>Or</t>
+  </si>
+  <si>
+    <t>035</t>
   </si>
 </sst>
 </file>
@@ -6180,7 +6186,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="200">
+  <cellXfs count="203">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -6672,6 +6678,15 @@
     <xf numFmtId="0" fontId="13" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -6690,15 +6705,6 @@
     <xf numFmtId="0" fontId="13" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
@@ -6770,6 +6776,15 @@
     </xf>
     <xf numFmtId="0" fontId="13" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -8356,7 +8371,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{124C2F8F-96ED-4E65-B816-FFFEB93DC889}">
   <dimension ref="A1:F23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D6" sqref="D6"/>
     </sheetView>
@@ -8705,11 +8720,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F68"/>
+  <dimension ref="A1:F69"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F3" sqref="F3"/>
+      <selection pane="bottomLeft" activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -8749,13 +8764,13 @@
         <v>7</v>
       </c>
       <c r="C2" s="100" t="s">
-        <v>1441</v>
+        <v>1443</v>
       </c>
       <c r="D2" s="98" t="s">
         <v>8</v>
       </c>
       <c r="E2" s="99" t="s">
-        <v>1441</v>
+        <v>1443</v>
       </c>
       <c r="F2" s="98"/>
     </row>
@@ -9623,228 +9638,242 @@
     </row>
     <row r="52" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A52" s="86"/>
-      <c r="B52" s="86" t="s">
-        <v>203</v>
-      </c>
-      <c r="C52" s="102" t="s">
-        <v>81</v>
+      <c r="B52" s="200" t="s">
+        <v>1441</v>
+      </c>
+      <c r="C52" s="201" t="s">
+        <v>1442</v>
       </c>
       <c r="D52" s="86"/>
-      <c r="E52" s="103" t="s">
-        <v>204</v>
+      <c r="E52" s="202" t="s">
+        <v>493</v>
       </c>
       <c r="F52" s="86"/>
     </row>
     <row r="53" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A53" s="86"/>
       <c r="B53" s="86" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="C53" s="102" t="s">
-        <v>206</v>
+        <v>81</v>
       </c>
       <c r="D53" s="86"/>
       <c r="E53" s="103" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="F53" s="86"/>
     </row>
     <row r="54" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A54" s="86"/>
       <c r="B54" s="86" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="C54" s="102" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="D54" s="86"/>
       <c r="E54" s="103" t="s">
-        <v>162</v>
+        <v>207</v>
       </c>
       <c r="F54" s="86"/>
     </row>
     <row r="55" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A55" s="86"/>
       <c r="B55" s="86" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C55" s="102" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="D55" s="86"/>
       <c r="E55" s="103" t="s">
-        <v>158</v>
+        <v>162</v>
       </c>
       <c r="F55" s="86"/>
     </row>
     <row r="56" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A56" s="86"/>
       <c r="B56" s="86" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C56" s="102" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="D56" s="86"/>
       <c r="E56" s="103" t="s">
-        <v>214</v>
+        <v>158</v>
       </c>
       <c r="F56" s="86"/>
     </row>
     <row r="57" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A57" s="86"/>
       <c r="B57" s="86" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="C57" s="102" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="D57" s="86"/>
       <c r="E57" s="103" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="F57" s="86"/>
     </row>
     <row r="58" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A58" s="86"/>
       <c r="B58" s="86" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="C58" s="102" t="s">
-        <v>93</v>
+        <v>216</v>
       </c>
       <c r="D58" s="86"/>
       <c r="E58" s="103" t="s">
-        <v>95</v>
+        <v>217</v>
       </c>
       <c r="F58" s="86"/>
     </row>
     <row r="59" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A59" s="86"/>
       <c r="B59" s="86" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C59" s="102" t="s">
-        <v>220</v>
+        <v>93</v>
       </c>
       <c r="D59" s="86"/>
       <c r="E59" s="103" t="s">
-        <v>221</v>
+        <v>95</v>
       </c>
       <c r="F59" s="86"/>
     </row>
     <row r="60" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A60" s="86"/>
       <c r="B60" s="86" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="C60" s="102" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="D60" s="86"/>
       <c r="E60" s="103" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="F60" s="86"/>
     </row>
-    <row r="61" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A61" s="86"/>
       <c r="B61" s="86" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="C61" s="102" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="D61" s="86"/>
       <c r="E61" s="103" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="F61" s="86"/>
     </row>
-    <row r="62" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A62" s="86"/>
       <c r="B62" s="86" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="C62" s="102" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="D62" s="86"/>
       <c r="E62" s="103" t="s">
-        <v>230</v>
-      </c>
+        <v>227</v>
+      </c>
+      <c r="F62" s="86"/>
     </row>
     <row r="63" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A63" s="86"/>
       <c r="B63" s="86" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="C63" s="102" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="D63" s="86"/>
       <c r="E63" s="103" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
     </row>
     <row r="64" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A64" s="86"/>
       <c r="B64" s="86" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="C64" s="102" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="D64" s="86"/>
       <c r="E64" s="103" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
     </row>
     <row r="65" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A65" s="86"/>
       <c r="B65" s="86" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="C65" s="102" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="D65" s="86"/>
       <c r="E65" s="103" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
     </row>
     <row r="66" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A66" s="86"/>
       <c r="B66" s="86" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="C66" s="102" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="D66" s="86"/>
       <c r="E66" s="103" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A67" s="86"/>
+      <c r="B67" s="86" t="s">
+        <v>240</v>
+      </c>
+      <c r="C67" s="102" t="s">
+        <v>241</v>
+      </c>
+      <c r="D67" s="86"/>
+      <c r="E67" s="103" t="s">
         <v>242</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="B67" s="1" t="s">
-        <v>1335</v>
-      </c>
-      <c r="C67" s="2" t="s">
-        <v>1336</v>
-      </c>
-      <c r="E67" s="40" t="s">
-        <v>1338</v>
       </c>
     </row>
     <row r="68" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="B68" s="1" t="s">
+        <v>1335</v>
+      </c>
+      <c r="C68" s="2" t="s">
+        <v>1336</v>
+      </c>
+      <c r="E68" s="40" t="s">
+        <v>1338</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="B69" s="1" t="s">
         <v>1337</v>
       </c>
-      <c r="C68" s="2" t="s">
+      <c r="C69" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="E68" s="40" t="s">
+      <c r="E69" s="40" t="s">
         <v>78</v>
       </c>
     </row>
@@ -10927,13 +10956,13 @@
       </c>
     </row>
     <row r="2" spans="1:6" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="167" t="s">
+      <c r="A2" s="170" t="s">
         <v>367</v>
       </c>
-      <c r="B2" s="168"/>
-      <c r="C2" s="168"/>
-      <c r="D2" s="168"/>
-      <c r="E2" s="169"/>
+      <c r="B2" s="171"/>
+      <c r="C2" s="171"/>
+      <c r="D2" s="171"/>
+      <c r="E2" s="172"/>
       <c r="F2" s="33"/>
     </row>
     <row r="3" spans="1:6" ht="48" x14ac:dyDescent="0.2">
@@ -11061,13 +11090,13 @@
       <c r="F9" s="119"/>
     </row>
     <row r="10" spans="1:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="170" t="s">
+      <c r="A10" s="173" t="s">
         <v>396</v>
       </c>
-      <c r="B10" s="171"/>
-      <c r="C10" s="171"/>
-      <c r="D10" s="171"/>
-      <c r="E10" s="172"/>
+      <c r="B10" s="174"/>
+      <c r="C10" s="174"/>
+      <c r="D10" s="174"/>
+      <c r="E10" s="175"/>
       <c r="F10" s="119"/>
     </row>
     <row r="11" spans="1:6" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -13485,13 +13514,13 @@
       <c r="F169" s="119"/>
     </row>
     <row r="170" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A170" s="173" t="s">
+      <c r="A170" s="167" t="s">
         <v>762</v>
       </c>
-      <c r="B170" s="174"/>
-      <c r="C170" s="174"/>
-      <c r="D170" s="174"/>
-      <c r="E170" s="175"/>
+      <c r="B170" s="168"/>
+      <c r="C170" s="168"/>
+      <c r="D170" s="168"/>
+      <c r="E170" s="169"/>
       <c r="F170" s="129" t="s">
         <v>763</v>
       </c>
@@ -15394,6 +15423,18 @@
     </row>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="A230:E230"/>
+    <mergeCell ref="A191:E191"/>
+    <mergeCell ref="A195:E195"/>
+    <mergeCell ref="A202:E202"/>
+    <mergeCell ref="A213:E213"/>
+    <mergeCell ref="A219:E219"/>
+    <mergeCell ref="A58:E58"/>
+    <mergeCell ref="A2:E2"/>
+    <mergeCell ref="A10:E10"/>
+    <mergeCell ref="A14:E14"/>
+    <mergeCell ref="A24:E24"/>
+    <mergeCell ref="A43:E43"/>
     <mergeCell ref="A179:E179"/>
     <mergeCell ref="A162:E162"/>
     <mergeCell ref="A63:E63"/>
@@ -15404,18 +15445,6 @@
     <mergeCell ref="A151:E151"/>
     <mergeCell ref="A92:E92"/>
     <mergeCell ref="A170:E170"/>
-    <mergeCell ref="A58:E58"/>
-    <mergeCell ref="A2:E2"/>
-    <mergeCell ref="A10:E10"/>
-    <mergeCell ref="A14:E14"/>
-    <mergeCell ref="A24:E24"/>
-    <mergeCell ref="A43:E43"/>
-    <mergeCell ref="A230:E230"/>
-    <mergeCell ref="A191:E191"/>
-    <mergeCell ref="A195:E195"/>
-    <mergeCell ref="A202:E202"/>
-    <mergeCell ref="A213:E213"/>
-    <mergeCell ref="A219:E219"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -17440,6 +17469,56 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Readyforteam_x003f_ xmlns="565e1b1d-057e-4d85-b896-01a5881d8a45">false</Readyforteam_x003f_>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <SharedWithUsers xmlns="bf601f31-63a1-4825-9216-91d773c5ef9c">
+      <UserInfo>
+        <DisplayName>Erika Osti</DisplayName>
+        <AccountId>534</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Penny Johnson</DisplayName>
+        <AccountId>489</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Ben Childs</DisplayName>
+        <AccountId>643</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Thomas Leeds</DisplayName>
+        <AccountId>459</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Kasmyn Chen</DisplayName>
+        <AccountId>532</AccountId>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="565e1b1d-057e-4d85-b896-01a5881d8a45">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="2799d30d-6731-4efe-ac9b-c4895a8828d9" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010096D84A54A9CD274097F17166F184737D" ma:contentTypeVersion="21" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="2fd95a4cfdf4f2f51219070f5dff16a8">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="565e1b1d-057e-4d85-b896-01a5881d8a45" xmlns:ns3="bf601f31-63a1-4825-9216-91d773c5ef9c" xmlns:ns4="2799d30d-6731-4efe-ac9b-c4895a8828d9" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f7499f6f4dc8ad2a533df04863f63fa7" ns1:_="" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -17716,57 +17795,28 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Readyforteam_x003f_ xmlns="565e1b1d-057e-4d85-b896-01a5881d8a45">false</Readyforteam_x003f_>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <SharedWithUsers xmlns="bf601f31-63a1-4825-9216-91d773c5ef9c">
-      <UserInfo>
-        <DisplayName>Erika Osti</DisplayName>
-        <AccountId>534</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Penny Johnson</DisplayName>
-        <AccountId>489</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Ben Childs</DisplayName>
-        <AccountId>643</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Thomas Leeds</DisplayName>
-        <AccountId>459</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Kasmyn Chen</DisplayName>
-        <AccountId>532</AccountId>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="565e1b1d-057e-4d85-b896-01a5881d8a45">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="2799d30d-6731-4efe-ac9b-c4895a8828d9" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8D7CE8C7-18DC-484F-8376-ED09F13D44C8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{017ACE96-8143-486E-8436-7787F6B96F4A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="565e1b1d-057e-4d85-b896-01a5881d8a45"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="bf601f31-63a1-4825-9216-91d773c5ef9c"/>
+    <ds:schemaRef ds:uri="2799d30d-6731-4efe-ac9b-c4895a8828d9"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EAFDB110-4046-4E72-A1EF-1908ABEC3151}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -17785,25 +17835,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{017ACE96-8143-486E-8436-7787F6B96F4A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="565e1b1d-057e-4d85-b896-01a5881d8a45"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="bf601f31-63a1-4825-9216-91d773c5ef9c"/>
-    <ds:schemaRef ds:uri="2799d30d-6731-4efe-ac9b-c4895a8828d9"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8D7CE8C7-18DC-484F-8376-ED09F13D44C8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Updating the text for the MEO certificate review declaration.
</commit_message>
<xml_diff>
--- a/app/data/MCCD-localisation.xlsx
+++ b/app/data/MCCD-localisation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/JALAT/GIT/medical-certificate-of-cause-of-death/app/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EF71863-61AA-1D4E-B63B-789D103F5510}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B26DE70D-B64E-3A48-B34C-456AD2414A6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="14100" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -69,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2177" uniqueCount="1447">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2177" uniqueCount="1450">
   <si>
     <r>
       <rPr>
@@ -5168,9 +5168,6 @@
     <t>meoDeclarationContent</t>
   </si>
   <si>
-    <t>I confirm that I have reviewed this certificate to the best of my knowledge and belief, and that it is ready for medical examiner scrutiny.</t>
-  </si>
-  <si>
     <t>MEO Declaration content.</t>
   </si>
   <si>
@@ -5707,9 +5704,6 @@
     <t>Dychwelyd at dashboard</t>
   </si>
   <si>
-    <t>036</t>
-  </si>
-  <si>
     <t>globalBackToDashboard</t>
   </si>
   <si>
@@ -5720,6 +5714,21 @@
   </si>
   <si>
     <t>Don't use this…it's a mistake, just adding for legacy in v10-1</t>
+  </si>
+  <si>
+    <t>I confirm that I have reviewed this certificate and that it is ready for scrutiny and approval by a medical examiner.</t>
+  </si>
+  <si>
+    <t>Review of certificate</t>
+  </si>
+  <si>
+    <t>Adolygiad o'r dystysgrif</t>
+  </si>
+  <si>
+    <t> Rwy'n cadarnhau fy mod wedi adolygu'r dystysgrif hon a'i bod yn barod i'w archwilio a'i chymeradwyo gan arholwr meddygol.</t>
+  </si>
+  <si>
+    <t>037</t>
   </si>
 </sst>
 </file>
@@ -6684,6 +6693,9 @@
     <xf numFmtId="0" fontId="9" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -6696,6 +6708,24 @@
     <xf numFmtId="0" fontId="13" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -6705,24 +6735,6 @@
     <xf numFmtId="0" fontId="6" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
@@ -6794,9 +6806,6 @@
     </xf>
     <xf numFmtId="0" fontId="13" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -7181,538 +7190,538 @@
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A1" s="166" t="s">
+      <c r="A1" s="167" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="166"/>
-      <c r="C1" s="166"/>
-      <c r="D1" s="166"/>
-      <c r="E1" s="166"/>
-      <c r="F1" s="166"/>
-      <c r="G1" s="166"/>
-      <c r="H1" s="166"/>
-      <c r="I1" s="166"/>
-      <c r="J1" s="166"/>
-      <c r="K1" s="166"/>
-      <c r="L1" s="166"/>
+      <c r="B1" s="167"/>
+      <c r="C1" s="167"/>
+      <c r="D1" s="167"/>
+      <c r="E1" s="167"/>
+      <c r="F1" s="167"/>
+      <c r="G1" s="167"/>
+      <c r="H1" s="167"/>
+      <c r="I1" s="167"/>
+      <c r="J1" s="167"/>
+      <c r="K1" s="167"/>
+      <c r="L1" s="167"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A2" s="166"/>
-      <c r="B2" s="166"/>
-      <c r="C2" s="166"/>
-      <c r="D2" s="166"/>
-      <c r="E2" s="166"/>
-      <c r="F2" s="166"/>
-      <c r="G2" s="166"/>
-      <c r="H2" s="166"/>
-      <c r="I2" s="166"/>
-      <c r="J2" s="166"/>
-      <c r="K2" s="166"/>
-      <c r="L2" s="166"/>
+      <c r="A2" s="167"/>
+      <c r="B2" s="167"/>
+      <c r="C2" s="167"/>
+      <c r="D2" s="167"/>
+      <c r="E2" s="167"/>
+      <c r="F2" s="167"/>
+      <c r="G2" s="167"/>
+      <c r="H2" s="167"/>
+      <c r="I2" s="167"/>
+      <c r="J2" s="167"/>
+      <c r="K2" s="167"/>
+      <c r="L2" s="167"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A3" s="166"/>
-      <c r="B3" s="166"/>
-      <c r="C3" s="166"/>
-      <c r="D3" s="166"/>
-      <c r="E3" s="166"/>
-      <c r="F3" s="166"/>
-      <c r="G3" s="166"/>
-      <c r="H3" s="166"/>
-      <c r="I3" s="166"/>
-      <c r="J3" s="166"/>
-      <c r="K3" s="166"/>
-      <c r="L3" s="166"/>
+      <c r="A3" s="167"/>
+      <c r="B3" s="167"/>
+      <c r="C3" s="167"/>
+      <c r="D3" s="167"/>
+      <c r="E3" s="167"/>
+      <c r="F3" s="167"/>
+      <c r="G3" s="167"/>
+      <c r="H3" s="167"/>
+      <c r="I3" s="167"/>
+      <c r="J3" s="167"/>
+      <c r="K3" s="167"/>
+      <c r="L3" s="167"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A4" s="166"/>
-      <c r="B4" s="166"/>
-      <c r="C4" s="166"/>
-      <c r="D4" s="166"/>
-      <c r="E4" s="166"/>
-      <c r="F4" s="166"/>
-      <c r="G4" s="166"/>
-      <c r="H4" s="166"/>
-      <c r="I4" s="166"/>
-      <c r="J4" s="166"/>
-      <c r="K4" s="166"/>
-      <c r="L4" s="166"/>
+      <c r="A4" s="167"/>
+      <c r="B4" s="167"/>
+      <c r="C4" s="167"/>
+      <c r="D4" s="167"/>
+      <c r="E4" s="167"/>
+      <c r="F4" s="167"/>
+      <c r="G4" s="167"/>
+      <c r="H4" s="167"/>
+      <c r="I4" s="167"/>
+      <c r="J4" s="167"/>
+      <c r="K4" s="167"/>
+      <c r="L4" s="167"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A5" s="166"/>
-      <c r="B5" s="166"/>
-      <c r="C5" s="166"/>
-      <c r="D5" s="166"/>
-      <c r="E5" s="166"/>
-      <c r="F5" s="166"/>
-      <c r="G5" s="166"/>
-      <c r="H5" s="166"/>
-      <c r="I5" s="166"/>
-      <c r="J5" s="166"/>
-      <c r="K5" s="166"/>
-      <c r="L5" s="166"/>
+      <c r="A5" s="167"/>
+      <c r="B5" s="167"/>
+      <c r="C5" s="167"/>
+      <c r="D5" s="167"/>
+      <c r="E5" s="167"/>
+      <c r="F5" s="167"/>
+      <c r="G5" s="167"/>
+      <c r="H5" s="167"/>
+      <c r="I5" s="167"/>
+      <c r="J5" s="167"/>
+      <c r="K5" s="167"/>
+      <c r="L5" s="167"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A6" s="166"/>
-      <c r="B6" s="166"/>
-      <c r="C6" s="166"/>
-      <c r="D6" s="166"/>
-      <c r="E6" s="166"/>
-      <c r="F6" s="166"/>
-      <c r="G6" s="166"/>
-      <c r="H6" s="166"/>
-      <c r="I6" s="166"/>
-      <c r="J6" s="166"/>
-      <c r="K6" s="166"/>
-      <c r="L6" s="166"/>
+      <c r="A6" s="167"/>
+      <c r="B6" s="167"/>
+      <c r="C6" s="167"/>
+      <c r="D6" s="167"/>
+      <c r="E6" s="167"/>
+      <c r="F6" s="167"/>
+      <c r="G6" s="167"/>
+      <c r="H6" s="167"/>
+      <c r="I6" s="167"/>
+      <c r="J6" s="167"/>
+      <c r="K6" s="167"/>
+      <c r="L6" s="167"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A7" s="166"/>
-      <c r="B7" s="166"/>
-      <c r="C7" s="166"/>
-      <c r="D7" s="166"/>
-      <c r="E7" s="166"/>
-      <c r="F7" s="166"/>
-      <c r="G7" s="166"/>
-      <c r="H7" s="166"/>
-      <c r="I7" s="166"/>
-      <c r="J7" s="166"/>
-      <c r="K7" s="166"/>
-      <c r="L7" s="166"/>
+      <c r="A7" s="167"/>
+      <c r="B7" s="167"/>
+      <c r="C7" s="167"/>
+      <c r="D7" s="167"/>
+      <c r="E7" s="167"/>
+      <c r="F7" s="167"/>
+      <c r="G7" s="167"/>
+      <c r="H7" s="167"/>
+      <c r="I7" s="167"/>
+      <c r="J7" s="167"/>
+      <c r="K7" s="167"/>
+      <c r="L7" s="167"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A8" s="166"/>
-      <c r="B8" s="166"/>
-      <c r="C8" s="166"/>
-      <c r="D8" s="166"/>
-      <c r="E8" s="166"/>
-      <c r="F8" s="166"/>
-      <c r="G8" s="166"/>
-      <c r="H8" s="166"/>
-      <c r="I8" s="166"/>
-      <c r="J8" s="166"/>
-      <c r="K8" s="166"/>
-      <c r="L8" s="166"/>
+      <c r="A8" s="167"/>
+      <c r="B8" s="167"/>
+      <c r="C8" s="167"/>
+      <c r="D8" s="167"/>
+      <c r="E8" s="167"/>
+      <c r="F8" s="167"/>
+      <c r="G8" s="167"/>
+      <c r="H8" s="167"/>
+      <c r="I8" s="167"/>
+      <c r="J8" s="167"/>
+      <c r="K8" s="167"/>
+      <c r="L8" s="167"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A9" s="166"/>
-      <c r="B9" s="166"/>
-      <c r="C9" s="166"/>
-      <c r="D9" s="166"/>
-      <c r="E9" s="166"/>
-      <c r="F9" s="166"/>
-      <c r="G9" s="166"/>
-      <c r="H9" s="166"/>
-      <c r="I9" s="166"/>
-      <c r="J9" s="166"/>
-      <c r="K9" s="166"/>
-      <c r="L9" s="166"/>
+      <c r="A9" s="167"/>
+      <c r="B9" s="167"/>
+      <c r="C9" s="167"/>
+      <c r="D9" s="167"/>
+      <c r="E9" s="167"/>
+      <c r="F9" s="167"/>
+      <c r="G9" s="167"/>
+      <c r="H9" s="167"/>
+      <c r="I9" s="167"/>
+      <c r="J9" s="167"/>
+      <c r="K9" s="167"/>
+      <c r="L9" s="167"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A10" s="166"/>
-      <c r="B10" s="166"/>
-      <c r="C10" s="166"/>
-      <c r="D10" s="166"/>
-      <c r="E10" s="166"/>
-      <c r="F10" s="166"/>
-      <c r="G10" s="166"/>
-      <c r="H10" s="166"/>
-      <c r="I10" s="166"/>
-      <c r="J10" s="166"/>
-      <c r="K10" s="166"/>
-      <c r="L10" s="166"/>
+      <c r="A10" s="167"/>
+      <c r="B10" s="167"/>
+      <c r="C10" s="167"/>
+      <c r="D10" s="167"/>
+      <c r="E10" s="167"/>
+      <c r="F10" s="167"/>
+      <c r="G10" s="167"/>
+      <c r="H10" s="167"/>
+      <c r="I10" s="167"/>
+      <c r="J10" s="167"/>
+      <c r="K10" s="167"/>
+      <c r="L10" s="167"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A11" s="166"/>
-      <c r="B11" s="166"/>
-      <c r="C11" s="166"/>
-      <c r="D11" s="166"/>
-      <c r="E11" s="166"/>
-      <c r="F11" s="166"/>
-      <c r="G11" s="166"/>
-      <c r="H11" s="166"/>
-      <c r="I11" s="166"/>
-      <c r="J11" s="166"/>
-      <c r="K11" s="166"/>
-      <c r="L11" s="166"/>
+      <c r="A11" s="167"/>
+      <c r="B11" s="167"/>
+      <c r="C11" s="167"/>
+      <c r="D11" s="167"/>
+      <c r="E11" s="167"/>
+      <c r="F11" s="167"/>
+      <c r="G11" s="167"/>
+      <c r="H11" s="167"/>
+      <c r="I11" s="167"/>
+      <c r="J11" s="167"/>
+      <c r="K11" s="167"/>
+      <c r="L11" s="167"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A12" s="166"/>
-      <c r="B12" s="166"/>
-      <c r="C12" s="166"/>
-      <c r="D12" s="166"/>
-      <c r="E12" s="166"/>
-      <c r="F12" s="166"/>
-      <c r="G12" s="166"/>
-      <c r="H12" s="166"/>
-      <c r="I12" s="166"/>
-      <c r="J12" s="166"/>
-      <c r="K12" s="166"/>
-      <c r="L12" s="166"/>
+      <c r="A12" s="167"/>
+      <c r="B12" s="167"/>
+      <c r="C12" s="167"/>
+      <c r="D12" s="167"/>
+      <c r="E12" s="167"/>
+      <c r="F12" s="167"/>
+      <c r="G12" s="167"/>
+      <c r="H12" s="167"/>
+      <c r="I12" s="167"/>
+      <c r="J12" s="167"/>
+      <c r="K12" s="167"/>
+      <c r="L12" s="167"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A13" s="166"/>
-      <c r="B13" s="166"/>
-      <c r="C13" s="166"/>
-      <c r="D13" s="166"/>
-      <c r="E13" s="166"/>
-      <c r="F13" s="166"/>
-      <c r="G13" s="166"/>
-      <c r="H13" s="166"/>
-      <c r="I13" s="166"/>
-      <c r="J13" s="166"/>
-      <c r="K13" s="166"/>
-      <c r="L13" s="166"/>
+      <c r="A13" s="167"/>
+      <c r="B13" s="167"/>
+      <c r="C13" s="167"/>
+      <c r="D13" s="167"/>
+      <c r="E13" s="167"/>
+      <c r="F13" s="167"/>
+      <c r="G13" s="167"/>
+      <c r="H13" s="167"/>
+      <c r="I13" s="167"/>
+      <c r="J13" s="167"/>
+      <c r="K13" s="167"/>
+      <c r="L13" s="167"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A14" s="166"/>
-      <c r="B14" s="166"/>
-      <c r="C14" s="166"/>
-      <c r="D14" s="166"/>
-      <c r="E14" s="166"/>
-      <c r="F14" s="166"/>
-      <c r="G14" s="166"/>
-      <c r="H14" s="166"/>
-      <c r="I14" s="166"/>
-      <c r="J14" s="166"/>
-      <c r="K14" s="166"/>
-      <c r="L14" s="166"/>
+      <c r="A14" s="167"/>
+      <c r="B14" s="167"/>
+      <c r="C14" s="167"/>
+      <c r="D14" s="167"/>
+      <c r="E14" s="167"/>
+      <c r="F14" s="167"/>
+      <c r="G14" s="167"/>
+      <c r="H14" s="167"/>
+      <c r="I14" s="167"/>
+      <c r="J14" s="167"/>
+      <c r="K14" s="167"/>
+      <c r="L14" s="167"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A15" s="166"/>
-      <c r="B15" s="166"/>
-      <c r="C15" s="166"/>
-      <c r="D15" s="166"/>
-      <c r="E15" s="166"/>
-      <c r="F15" s="166"/>
-      <c r="G15" s="166"/>
-      <c r="H15" s="166"/>
-      <c r="I15" s="166"/>
-      <c r="J15" s="166"/>
-      <c r="K15" s="166"/>
-      <c r="L15" s="166"/>
+      <c r="A15" s="167"/>
+      <c r="B15" s="167"/>
+      <c r="C15" s="167"/>
+      <c r="D15" s="167"/>
+      <c r="E15" s="167"/>
+      <c r="F15" s="167"/>
+      <c r="G15" s="167"/>
+      <c r="H15" s="167"/>
+      <c r="I15" s="167"/>
+      <c r="J15" s="167"/>
+      <c r="K15" s="167"/>
+      <c r="L15" s="167"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A16" s="166"/>
-      <c r="B16" s="166"/>
-      <c r="C16" s="166"/>
-      <c r="D16" s="166"/>
-      <c r="E16" s="166"/>
-      <c r="F16" s="166"/>
-      <c r="G16" s="166"/>
-      <c r="H16" s="166"/>
-      <c r="I16" s="166"/>
-      <c r="J16" s="166"/>
-      <c r="K16" s="166"/>
-      <c r="L16" s="166"/>
+      <c r="A16" s="167"/>
+      <c r="B16" s="167"/>
+      <c r="C16" s="167"/>
+      <c r="D16" s="167"/>
+      <c r="E16" s="167"/>
+      <c r="F16" s="167"/>
+      <c r="G16" s="167"/>
+      <c r="H16" s="167"/>
+      <c r="I16" s="167"/>
+      <c r="J16" s="167"/>
+      <c r="K16" s="167"/>
+      <c r="L16" s="167"/>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A17" s="166"/>
-      <c r="B17" s="166"/>
-      <c r="C17" s="166"/>
-      <c r="D17" s="166"/>
-      <c r="E17" s="166"/>
-      <c r="F17" s="166"/>
-      <c r="G17" s="166"/>
-      <c r="H17" s="166"/>
-      <c r="I17" s="166"/>
-      <c r="J17" s="166"/>
-      <c r="K17" s="166"/>
-      <c r="L17" s="166"/>
+      <c r="A17" s="167"/>
+      <c r="B17" s="167"/>
+      <c r="C17" s="167"/>
+      <c r="D17" s="167"/>
+      <c r="E17" s="167"/>
+      <c r="F17" s="167"/>
+      <c r="G17" s="167"/>
+      <c r="H17" s="167"/>
+      <c r="I17" s="167"/>
+      <c r="J17" s="167"/>
+      <c r="K17" s="167"/>
+      <c r="L17" s="167"/>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A18" s="166"/>
-      <c r="B18" s="166"/>
-      <c r="C18" s="166"/>
-      <c r="D18" s="166"/>
-      <c r="E18" s="166"/>
-      <c r="F18" s="166"/>
-      <c r="G18" s="166"/>
-      <c r="H18" s="166"/>
-      <c r="I18" s="166"/>
-      <c r="J18" s="166"/>
-      <c r="K18" s="166"/>
-      <c r="L18" s="166"/>
+      <c r="A18" s="167"/>
+      <c r="B18" s="167"/>
+      <c r="C18" s="167"/>
+      <c r="D18" s="167"/>
+      <c r="E18" s="167"/>
+      <c r="F18" s="167"/>
+      <c r="G18" s="167"/>
+      <c r="H18" s="167"/>
+      <c r="I18" s="167"/>
+      <c r="J18" s="167"/>
+      <c r="K18" s="167"/>
+      <c r="L18" s="167"/>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A19" s="166"/>
-      <c r="B19" s="166"/>
-      <c r="C19" s="166"/>
-      <c r="D19" s="166"/>
-      <c r="E19" s="166"/>
-      <c r="F19" s="166"/>
-      <c r="G19" s="166"/>
-      <c r="H19" s="166"/>
-      <c r="I19" s="166"/>
-      <c r="J19" s="166"/>
-      <c r="K19" s="166"/>
-      <c r="L19" s="166"/>
+      <c r="A19" s="167"/>
+      <c r="B19" s="167"/>
+      <c r="C19" s="167"/>
+      <c r="D19" s="167"/>
+      <c r="E19" s="167"/>
+      <c r="F19" s="167"/>
+      <c r="G19" s="167"/>
+      <c r="H19" s="167"/>
+      <c r="I19" s="167"/>
+      <c r="J19" s="167"/>
+      <c r="K19" s="167"/>
+      <c r="L19" s="167"/>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A20" s="166"/>
-      <c r="B20" s="166"/>
-      <c r="C20" s="166"/>
-      <c r="D20" s="166"/>
-      <c r="E20" s="166"/>
-      <c r="F20" s="166"/>
-      <c r="G20" s="166"/>
-      <c r="H20" s="166"/>
-      <c r="I20" s="166"/>
-      <c r="J20" s="166"/>
-      <c r="K20" s="166"/>
-      <c r="L20" s="166"/>
+      <c r="A20" s="167"/>
+      <c r="B20" s="167"/>
+      <c r="C20" s="167"/>
+      <c r="D20" s="167"/>
+      <c r="E20" s="167"/>
+      <c r="F20" s="167"/>
+      <c r="G20" s="167"/>
+      <c r="H20" s="167"/>
+      <c r="I20" s="167"/>
+      <c r="J20" s="167"/>
+      <c r="K20" s="167"/>
+      <c r="L20" s="167"/>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A21" s="166"/>
-      <c r="B21" s="166"/>
-      <c r="C21" s="166"/>
-      <c r="D21" s="166"/>
-      <c r="E21" s="166"/>
-      <c r="F21" s="166"/>
-      <c r="G21" s="166"/>
-      <c r="H21" s="166"/>
-      <c r="I21" s="166"/>
-      <c r="J21" s="166"/>
-      <c r="K21" s="166"/>
-      <c r="L21" s="166"/>
+      <c r="A21" s="167"/>
+      <c r="B21" s="167"/>
+      <c r="C21" s="167"/>
+      <c r="D21" s="167"/>
+      <c r="E21" s="167"/>
+      <c r="F21" s="167"/>
+      <c r="G21" s="167"/>
+      <c r="H21" s="167"/>
+      <c r="I21" s="167"/>
+      <c r="J21" s="167"/>
+      <c r="K21" s="167"/>
+      <c r="L21" s="167"/>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A22" s="166"/>
-      <c r="B22" s="166"/>
-      <c r="C22" s="166"/>
-      <c r="D22" s="166"/>
-      <c r="E22" s="166"/>
-      <c r="F22" s="166"/>
-      <c r="G22" s="166"/>
-      <c r="H22" s="166"/>
-      <c r="I22" s="166"/>
-      <c r="J22" s="166"/>
-      <c r="K22" s="166"/>
-      <c r="L22" s="166"/>
+      <c r="A22" s="167"/>
+      <c r="B22" s="167"/>
+      <c r="C22" s="167"/>
+      <c r="D22" s="167"/>
+      <c r="E22" s="167"/>
+      <c r="F22" s="167"/>
+      <c r="G22" s="167"/>
+      <c r="H22" s="167"/>
+      <c r="I22" s="167"/>
+      <c r="J22" s="167"/>
+      <c r="K22" s="167"/>
+      <c r="L22" s="167"/>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A23" s="166"/>
-      <c r="B23" s="166"/>
-      <c r="C23" s="166"/>
-      <c r="D23" s="166"/>
-      <c r="E23" s="166"/>
-      <c r="F23" s="166"/>
-      <c r="G23" s="166"/>
-      <c r="H23" s="166"/>
-      <c r="I23" s="166"/>
-      <c r="J23" s="166"/>
-      <c r="K23" s="166"/>
-      <c r="L23" s="166"/>
+      <c r="A23" s="167"/>
+      <c r="B23" s="167"/>
+      <c r="C23" s="167"/>
+      <c r="D23" s="167"/>
+      <c r="E23" s="167"/>
+      <c r="F23" s="167"/>
+      <c r="G23" s="167"/>
+      <c r="H23" s="167"/>
+      <c r="I23" s="167"/>
+      <c r="J23" s="167"/>
+      <c r="K23" s="167"/>
+      <c r="L23" s="167"/>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A24" s="166"/>
-      <c r="B24" s="166"/>
-      <c r="C24" s="166"/>
-      <c r="D24" s="166"/>
-      <c r="E24" s="166"/>
-      <c r="F24" s="166"/>
-      <c r="G24" s="166"/>
-      <c r="H24" s="166"/>
-      <c r="I24" s="166"/>
-      <c r="J24" s="166"/>
-      <c r="K24" s="166"/>
-      <c r="L24" s="166"/>
+      <c r="A24" s="167"/>
+      <c r="B24" s="167"/>
+      <c r="C24" s="167"/>
+      <c r="D24" s="167"/>
+      <c r="E24" s="167"/>
+      <c r="F24" s="167"/>
+      <c r="G24" s="167"/>
+      <c r="H24" s="167"/>
+      <c r="I24" s="167"/>
+      <c r="J24" s="167"/>
+      <c r="K24" s="167"/>
+      <c r="L24" s="167"/>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A25" s="166"/>
-      <c r="B25" s="166"/>
-      <c r="C25" s="166"/>
-      <c r="D25" s="166"/>
-      <c r="E25" s="166"/>
-      <c r="F25" s="166"/>
-      <c r="G25" s="166"/>
-      <c r="H25" s="166"/>
-      <c r="I25" s="166"/>
-      <c r="J25" s="166"/>
-      <c r="K25" s="166"/>
-      <c r="L25" s="166"/>
+      <c r="A25" s="167"/>
+      <c r="B25" s="167"/>
+      <c r="C25" s="167"/>
+      <c r="D25" s="167"/>
+      <c r="E25" s="167"/>
+      <c r="F25" s="167"/>
+      <c r="G25" s="167"/>
+      <c r="H25" s="167"/>
+      <c r="I25" s="167"/>
+      <c r="J25" s="167"/>
+      <c r="K25" s="167"/>
+      <c r="L25" s="167"/>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A26" s="166"/>
-      <c r="B26" s="166"/>
-      <c r="C26" s="166"/>
-      <c r="D26" s="166"/>
-      <c r="E26" s="166"/>
-      <c r="F26" s="166"/>
-      <c r="G26" s="166"/>
-      <c r="H26" s="166"/>
-      <c r="I26" s="166"/>
-      <c r="J26" s="166"/>
-      <c r="K26" s="166"/>
-      <c r="L26" s="166"/>
+      <c r="A26" s="167"/>
+      <c r="B26" s="167"/>
+      <c r="C26" s="167"/>
+      <c r="D26" s="167"/>
+      <c r="E26" s="167"/>
+      <c r="F26" s="167"/>
+      <c r="G26" s="167"/>
+      <c r="H26" s="167"/>
+      <c r="I26" s="167"/>
+      <c r="J26" s="167"/>
+      <c r="K26" s="167"/>
+      <c r="L26" s="167"/>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A27" s="166"/>
-      <c r="B27" s="166"/>
-      <c r="C27" s="166"/>
-      <c r="D27" s="166"/>
-      <c r="E27" s="166"/>
-      <c r="F27" s="166"/>
-      <c r="G27" s="166"/>
-      <c r="H27" s="166"/>
-      <c r="I27" s="166"/>
-      <c r="J27" s="166"/>
-      <c r="K27" s="166"/>
-      <c r="L27" s="166"/>
+      <c r="A27" s="167"/>
+      <c r="B27" s="167"/>
+      <c r="C27" s="167"/>
+      <c r="D27" s="167"/>
+      <c r="E27" s="167"/>
+      <c r="F27" s="167"/>
+      <c r="G27" s="167"/>
+      <c r="H27" s="167"/>
+      <c r="I27" s="167"/>
+      <c r="J27" s="167"/>
+      <c r="K27" s="167"/>
+      <c r="L27" s="167"/>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A28" s="166"/>
-      <c r="B28" s="166"/>
-      <c r="C28" s="166"/>
-      <c r="D28" s="166"/>
-      <c r="E28" s="166"/>
-      <c r="F28" s="166"/>
-      <c r="G28" s="166"/>
-      <c r="H28" s="166"/>
-      <c r="I28" s="166"/>
-      <c r="J28" s="166"/>
-      <c r="K28" s="166"/>
-      <c r="L28" s="166"/>
+      <c r="A28" s="167"/>
+      <c r="B28" s="167"/>
+      <c r="C28" s="167"/>
+      <c r="D28" s="167"/>
+      <c r="E28" s="167"/>
+      <c r="F28" s="167"/>
+      <c r="G28" s="167"/>
+      <c r="H28" s="167"/>
+      <c r="I28" s="167"/>
+      <c r="J28" s="167"/>
+      <c r="K28" s="167"/>
+      <c r="L28" s="167"/>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A29" s="166"/>
-      <c r="B29" s="166"/>
-      <c r="C29" s="166"/>
-      <c r="D29" s="166"/>
-      <c r="E29" s="166"/>
-      <c r="F29" s="166"/>
-      <c r="G29" s="166"/>
-      <c r="H29" s="166"/>
-      <c r="I29" s="166"/>
-      <c r="J29" s="166"/>
-      <c r="K29" s="166"/>
-      <c r="L29" s="166"/>
+      <c r="A29" s="167"/>
+      <c r="B29" s="167"/>
+      <c r="C29" s="167"/>
+      <c r="D29" s="167"/>
+      <c r="E29" s="167"/>
+      <c r="F29" s="167"/>
+      <c r="G29" s="167"/>
+      <c r="H29" s="167"/>
+      <c r="I29" s="167"/>
+      <c r="J29" s="167"/>
+      <c r="K29" s="167"/>
+      <c r="L29" s="167"/>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A30" s="166"/>
-      <c r="B30" s="166"/>
-      <c r="C30" s="166"/>
-      <c r="D30" s="166"/>
-      <c r="E30" s="166"/>
-      <c r="F30" s="166"/>
-      <c r="G30" s="166"/>
-      <c r="H30" s="166"/>
-      <c r="I30" s="166"/>
-      <c r="J30" s="166"/>
-      <c r="K30" s="166"/>
-      <c r="L30" s="166"/>
+      <c r="A30" s="167"/>
+      <c r="B30" s="167"/>
+      <c r="C30" s="167"/>
+      <c r="D30" s="167"/>
+      <c r="E30" s="167"/>
+      <c r="F30" s="167"/>
+      <c r="G30" s="167"/>
+      <c r="H30" s="167"/>
+      <c r="I30" s="167"/>
+      <c r="J30" s="167"/>
+      <c r="K30" s="167"/>
+      <c r="L30" s="167"/>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A31" s="166"/>
-      <c r="B31" s="166"/>
-      <c r="C31" s="166"/>
-      <c r="D31" s="166"/>
-      <c r="E31" s="166"/>
-      <c r="F31" s="166"/>
-      <c r="G31" s="166"/>
-      <c r="H31" s="166"/>
-      <c r="I31" s="166"/>
-      <c r="J31" s="166"/>
-      <c r="K31" s="166"/>
-      <c r="L31" s="166"/>
+      <c r="A31" s="167"/>
+      <c r="B31" s="167"/>
+      <c r="C31" s="167"/>
+      <c r="D31" s="167"/>
+      <c r="E31" s="167"/>
+      <c r="F31" s="167"/>
+      <c r="G31" s="167"/>
+      <c r="H31" s="167"/>
+      <c r="I31" s="167"/>
+      <c r="J31" s="167"/>
+      <c r="K31" s="167"/>
+      <c r="L31" s="167"/>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A32" s="166"/>
-      <c r="B32" s="166"/>
-      <c r="C32" s="166"/>
-      <c r="D32" s="166"/>
-      <c r="E32" s="166"/>
-      <c r="F32" s="166"/>
-      <c r="G32" s="166"/>
-      <c r="H32" s="166"/>
-      <c r="I32" s="166"/>
-      <c r="J32" s="166"/>
-      <c r="K32" s="166"/>
-      <c r="L32" s="166"/>
+      <c r="A32" s="167"/>
+      <c r="B32" s="167"/>
+      <c r="C32" s="167"/>
+      <c r="D32" s="167"/>
+      <c r="E32" s="167"/>
+      <c r="F32" s="167"/>
+      <c r="G32" s="167"/>
+      <c r="H32" s="167"/>
+      <c r="I32" s="167"/>
+      <c r="J32" s="167"/>
+      <c r="K32" s="167"/>
+      <c r="L32" s="167"/>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A33" s="166"/>
-      <c r="B33" s="166"/>
-      <c r="C33" s="166"/>
-      <c r="D33" s="166"/>
-      <c r="E33" s="166"/>
-      <c r="F33" s="166"/>
-      <c r="G33" s="166"/>
-      <c r="H33" s="166"/>
-      <c r="I33" s="166"/>
-      <c r="J33" s="166"/>
-      <c r="K33" s="166"/>
-      <c r="L33" s="166"/>
+      <c r="A33" s="167"/>
+      <c r="B33" s="167"/>
+      <c r="C33" s="167"/>
+      <c r="D33" s="167"/>
+      <c r="E33" s="167"/>
+      <c r="F33" s="167"/>
+      <c r="G33" s="167"/>
+      <c r="H33" s="167"/>
+      <c r="I33" s="167"/>
+      <c r="J33" s="167"/>
+      <c r="K33" s="167"/>
+      <c r="L33" s="167"/>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A34" s="166"/>
-      <c r="B34" s="166"/>
-      <c r="C34" s="166"/>
-      <c r="D34" s="166"/>
-      <c r="E34" s="166"/>
-      <c r="F34" s="166"/>
-      <c r="G34" s="166"/>
-      <c r="H34" s="166"/>
-      <c r="I34" s="166"/>
-      <c r="J34" s="166"/>
-      <c r="K34" s="166"/>
-      <c r="L34" s="166"/>
+      <c r="A34" s="167"/>
+      <c r="B34" s="167"/>
+      <c r="C34" s="167"/>
+      <c r="D34" s="167"/>
+      <c r="E34" s="167"/>
+      <c r="F34" s="167"/>
+      <c r="G34" s="167"/>
+      <c r="H34" s="167"/>
+      <c r="I34" s="167"/>
+      <c r="J34" s="167"/>
+      <c r="K34" s="167"/>
+      <c r="L34" s="167"/>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A35" s="166"/>
-      <c r="B35" s="166"/>
-      <c r="C35" s="166"/>
-      <c r="D35" s="166"/>
-      <c r="E35" s="166"/>
-      <c r="F35" s="166"/>
-      <c r="G35" s="166"/>
-      <c r="H35" s="166"/>
-      <c r="I35" s="166"/>
-      <c r="J35" s="166"/>
-      <c r="K35" s="166"/>
-      <c r="L35" s="166"/>
+      <c r="A35" s="167"/>
+      <c r="B35" s="167"/>
+      <c r="C35" s="167"/>
+      <c r="D35" s="167"/>
+      <c r="E35" s="167"/>
+      <c r="F35" s="167"/>
+      <c r="G35" s="167"/>
+      <c r="H35" s="167"/>
+      <c r="I35" s="167"/>
+      <c r="J35" s="167"/>
+      <c r="K35" s="167"/>
+      <c r="L35" s="167"/>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A36" s="166"/>
-      <c r="B36" s="166"/>
-      <c r="C36" s="166"/>
-      <c r="D36" s="166"/>
-      <c r="E36" s="166"/>
-      <c r="F36" s="166"/>
-      <c r="G36" s="166"/>
-      <c r="H36" s="166"/>
-      <c r="I36" s="166"/>
-      <c r="J36" s="166"/>
-      <c r="K36" s="166"/>
-      <c r="L36" s="166"/>
+      <c r="A36" s="167"/>
+      <c r="B36" s="167"/>
+      <c r="C36" s="167"/>
+      <c r="D36" s="167"/>
+      <c r="E36" s="167"/>
+      <c r="F36" s="167"/>
+      <c r="G36" s="167"/>
+      <c r="H36" s="167"/>
+      <c r="I36" s="167"/>
+      <c r="J36" s="167"/>
+      <c r="K36" s="167"/>
+      <c r="L36" s="167"/>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A37" s="166"/>
-      <c r="B37" s="166"/>
-      <c r="C37" s="166"/>
-      <c r="D37" s="166"/>
-      <c r="E37" s="166"/>
-      <c r="F37" s="166"/>
-      <c r="G37" s="166"/>
-      <c r="H37" s="166"/>
-      <c r="I37" s="166"/>
-      <c r="J37" s="166"/>
-      <c r="K37" s="166"/>
-      <c r="L37" s="166"/>
+      <c r="A37" s="167"/>
+      <c r="B37" s="167"/>
+      <c r="C37" s="167"/>
+      <c r="D37" s="167"/>
+      <c r="E37" s="167"/>
+      <c r="F37" s="167"/>
+      <c r="G37" s="167"/>
+      <c r="H37" s="167"/>
+      <c r="I37" s="167"/>
+      <c r="J37" s="167"/>
+      <c r="K37" s="167"/>
+      <c r="L37" s="167"/>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A38" s="166"/>
-      <c r="B38" s="166"/>
-      <c r="C38" s="166"/>
-      <c r="D38" s="166"/>
-      <c r="E38" s="166"/>
-      <c r="F38" s="166"/>
-      <c r="G38" s="166"/>
-      <c r="H38" s="166"/>
-      <c r="I38" s="166"/>
-      <c r="J38" s="166"/>
-      <c r="K38" s="166"/>
-      <c r="L38" s="166"/>
+      <c r="A38" s="167"/>
+      <c r="B38" s="167"/>
+      <c r="C38" s="167"/>
+      <c r="D38" s="167"/>
+      <c r="E38" s="167"/>
+      <c r="F38" s="167"/>
+      <c r="G38" s="167"/>
+      <c r="H38" s="167"/>
+      <c r="I38" s="167"/>
+      <c r="J38" s="167"/>
+      <c r="K38" s="167"/>
+      <c r="L38" s="167"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -7948,8 +7957,8 @@
   <dimension ref="A1:F24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D15" sqref="D15"/>
+      <pane ySplit="1" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -7991,13 +8000,13 @@
         <v>1238</v>
       </c>
       <c r="C2" s="151" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="D2" s="92" t="s">
         <v>1239</v>
       </c>
       <c r="E2" s="152" t="s">
-        <v>1414</v>
+        <v>1413</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="80" x14ac:dyDescent="0.2">
@@ -8025,13 +8034,13 @@
         <v>1245</v>
       </c>
       <c r="C4" s="158" t="s">
-        <v>1411</v>
+        <v>1410</v>
       </c>
       <c r="D4" s="95" t="s">
         <v>401</v>
       </c>
       <c r="E4" s="155" t="s">
-        <v>1413</v>
+        <v>1412</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="60.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -8093,13 +8102,13 @@
         <v>1250</v>
       </c>
       <c r="C8" s="158" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="D8" s="95" t="s">
         <v>1251</v>
       </c>
       <c r="E8" s="155" t="s">
-        <v>1414</v>
+        <v>1413</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="64" x14ac:dyDescent="0.2">
@@ -8127,13 +8136,13 @@
         <v>1256</v>
       </c>
       <c r="C10" s="158" t="s">
-        <v>1411</v>
+        <v>1410</v>
       </c>
       <c r="D10" s="95" t="s">
         <v>401</v>
       </c>
       <c r="E10" s="155" t="s">
-        <v>1413</v>
+        <v>1412</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -8195,13 +8204,13 @@
         <v>1259</v>
       </c>
       <c r="C14" s="158" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="D14" s="95" t="s">
         <v>1260</v>
       </c>
       <c r="E14" s="155" t="s">
-        <v>1412</v>
+        <v>1411</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="80" x14ac:dyDescent="0.2">
@@ -8212,13 +8221,13 @@
         <v>1261</v>
       </c>
       <c r="C15" s="158" t="s">
-        <v>1431</v>
+        <v>1430</v>
       </c>
       <c r="D15" s="95" t="s">
         <v>1262</v>
       </c>
       <c r="E15" s="155" t="s">
-        <v>1432</v>
+        <v>1431</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="48" x14ac:dyDescent="0.2">
@@ -8263,13 +8272,13 @@
         <v>1265</v>
       </c>
       <c r="C18" s="158" t="s">
-        <v>1411</v>
+        <v>1410</v>
       </c>
       <c r="D18" s="95" t="s">
         <v>401</v>
       </c>
       <c r="E18" s="155" t="s">
-        <v>1413</v>
+        <v>1412</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -8297,30 +8306,30 @@
         <v>1266</v>
       </c>
       <c r="C20" s="158" t="s">
-        <v>1410</v>
+        <v>1446</v>
       </c>
       <c r="D20" s="95" t="s">
         <v>1239</v>
       </c>
       <c r="E20" s="155" t="s">
-        <v>1412</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" ht="48" x14ac:dyDescent="0.2">
+        <v>1447</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="64" x14ac:dyDescent="0.2">
       <c r="A21" s="94" t="s">
         <v>1240</v>
       </c>
       <c r="B21" s="95" t="s">
         <v>1267</v>
       </c>
-      <c r="C21" s="96" t="s">
+      <c r="C21" s="158" t="s">
+        <v>1445</v>
+      </c>
+      <c r="D21" s="95" t="s">
         <v>1268</v>
       </c>
-      <c r="D21" s="95" t="s">
-        <v>1269</v>
-      </c>
-      <c r="E21" s="89" t="s">
-        <v>401</v>
+      <c r="E21" s="155" t="s">
+        <v>1448</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -8328,16 +8337,16 @@
         <v>752</v>
       </c>
       <c r="B22" s="95" t="s">
-        <v>1270</v>
+        <v>1269</v>
       </c>
       <c r="C22" s="158" t="s">
-        <v>1411</v>
+        <v>1410</v>
       </c>
       <c r="D22" s="95" t="s">
         <v>401</v>
       </c>
       <c r="E22" s="155" t="s">
-        <v>1415</v>
+        <v>1414</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="48" x14ac:dyDescent="0.2">
@@ -8345,7 +8354,7 @@
         <v>407</v>
       </c>
       <c r="B23" s="105" t="s">
-        <v>1271</v>
+        <v>1270</v>
       </c>
       <c r="C23" s="106" t="s">
         <v>401</v>
@@ -8362,7 +8371,7 @@
         <v>410</v>
       </c>
       <c r="B24" s="105" t="s">
-        <v>1272</v>
+        <v>1271</v>
       </c>
       <c r="C24" s="106" t="s">
         <v>401</v>
@@ -8420,30 +8429,30 @@
       </c>
     </row>
     <row r="2" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="201" t="s">
-        <v>1273</v>
-      </c>
-      <c r="B2" s="202"/>
-      <c r="C2" s="202"/>
-      <c r="D2" s="202"/>
-      <c r="E2" s="202"/>
-      <c r="F2" s="202"/>
+      <c r="A2" s="202" t="s">
+        <v>1272</v>
+      </c>
+      <c r="B2" s="203"/>
+      <c r="C2" s="203"/>
+      <c r="D2" s="203"/>
+      <c r="E2" s="203"/>
+      <c r="F2" s="203"/>
     </row>
     <row r="3" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
         <v>240</v>
       </c>
       <c r="B3" s="5" t="s">
+        <v>1273</v>
+      </c>
+      <c r="C3" s="6" t="s">
         <v>1274</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>1275</v>
       </c>
       <c r="D3" s="5" t="s">
         <v>1220</v>
       </c>
       <c r="E3" s="37" t="s">
-        <v>1276</v>
+        <v>1275</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="32" x14ac:dyDescent="0.2">
@@ -8451,13 +8460,13 @@
         <v>258</v>
       </c>
       <c r="B4" s="5" t="s">
+        <v>1276</v>
+      </c>
+      <c r="C4" s="59" t="s">
+        <v>1436</v>
+      </c>
+      <c r="E4" s="37" t="s">
         <v>1277</v>
-      </c>
-      <c r="C4" s="59" t="s">
-        <v>1437</v>
-      </c>
-      <c r="E4" s="37" t="s">
-        <v>1278</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="16" x14ac:dyDescent="0.2">
@@ -8465,13 +8474,13 @@
         <v>251</v>
       </c>
       <c r="B5" s="5" t="s">
+        <v>1278</v>
+      </c>
+      <c r="C5" s="6" t="s">
         <v>1279</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="E5" s="37" t="s">
         <v>1280</v>
-      </c>
-      <c r="E5" s="37" t="s">
-        <v>1281</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="80" x14ac:dyDescent="0.2">
@@ -8479,13 +8488,13 @@
         <v>258</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>1282</v>
+        <v>1281</v>
       </c>
       <c r="C6" s="6" t="s">
+        <v>1434</v>
+      </c>
+      <c r="E6" s="37" t="s">
         <v>1435</v>
-      </c>
-      <c r="E6" s="37" t="s">
-        <v>1436</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="32" x14ac:dyDescent="0.2">
@@ -8493,112 +8502,112 @@
         <v>251</v>
       </c>
       <c r="B7" s="5" t="s">
+        <v>1282</v>
+      </c>
+      <c r="C7" s="6" t="s">
         <v>1283</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="E7" s="37" t="s">
         <v>1284</v>
-      </c>
-      <c r="E7" s="37" t="s">
-        <v>1285</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
+        <v>1285</v>
+      </c>
+      <c r="B8" s="5" t="s">
         <v>1286</v>
       </c>
-      <c r="B8" s="5" t="s">
-        <v>1287</v>
-      </c>
       <c r="C8" s="6" t="s">
+        <v>1419</v>
+      </c>
+      <c r="E8" s="37" t="s">
         <v>1420</v>
-      </c>
-      <c r="E8" s="37" t="s">
-        <v>1421</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
+        <v>1287</v>
+      </c>
+      <c r="B9" s="5" t="s">
         <v>1288</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="C9" s="6" t="s">
         <v>1289</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="E9" s="37" t="s">
         <v>1290</v>
-      </c>
-      <c r="E9" s="37" t="s">
-        <v>1291</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
-        <v>1288</v>
+        <v>1287</v>
       </c>
       <c r="B10" s="5" t="s">
+        <v>1291</v>
+      </c>
+      <c r="C10" s="6" t="s">
         <v>1292</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="E10" s="37" t="s">
         <v>1293</v>
-      </c>
-      <c r="E10" s="37" t="s">
-        <v>1294</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
-        <v>1288</v>
+        <v>1287</v>
       </c>
       <c r="B11" s="5" t="s">
+        <v>1294</v>
+      </c>
+      <c r="C11" s="6" t="s">
         <v>1295</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="E11" s="37" t="s">
         <v>1296</v>
-      </c>
-      <c r="E11" s="37" t="s">
-        <v>1297</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="5" t="s">
-        <v>1288</v>
+        <v>1287</v>
       </c>
       <c r="B12" s="5" t="s">
+        <v>1297</v>
+      </c>
+      <c r="C12" s="6" t="s">
         <v>1298</v>
       </c>
-      <c r="C12" s="6" t="s">
+      <c r="E12" s="37" t="s">
         <v>1299</v>
-      </c>
-      <c r="E12" s="37" t="s">
-        <v>1300</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="s">
-        <v>1288</v>
+        <v>1287</v>
       </c>
       <c r="B13" s="5" t="s">
+        <v>1300</v>
+      </c>
+      <c r="C13" s="6" t="s">
         <v>1301</v>
       </c>
-      <c r="C13" s="6" t="s">
+      <c r="E13" s="37" t="s">
         <v>1302</v>
-      </c>
-      <c r="E13" s="37" t="s">
-        <v>1303</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A14" s="5" t="s">
-        <v>1286</v>
+        <v>1285</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>1304</v>
+        <v>1303</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>1418</v>
+        <v>1417</v>
       </c>
       <c r="D14" s="1"/>
       <c r="E14" s="37" t="s">
-        <v>1419</v>
+        <v>1418</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="32" x14ac:dyDescent="0.2">
@@ -8606,14 +8615,14 @@
         <v>946</v>
       </c>
       <c r="B15" s="5" t="s">
+        <v>1304</v>
+      </c>
+      <c r="C15" s="6" t="s">
         <v>1305</v>
-      </c>
-      <c r="C15" s="6" t="s">
-        <v>1306</v>
       </c>
       <c r="D15" s="1"/>
       <c r="E15" s="37" t="s">
-        <v>1307</v>
+        <v>1306</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="16" x14ac:dyDescent="0.2">
@@ -8621,56 +8630,56 @@
         <v>14</v>
       </c>
       <c r="B16" s="5" t="s">
+        <v>1307</v>
+      </c>
+      <c r="C16" s="74" t="s">
         <v>1308</v>
-      </c>
-      <c r="C16" s="74" t="s">
-        <v>1309</v>
       </c>
       <c r="D16" s="18"/>
       <c r="E16" s="37" t="s">
-        <v>1310</v>
+        <v>1309</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A17" s="5" t="s">
+        <v>1310</v>
+      </c>
+      <c r="B17" s="7" t="s">
         <v>1311</v>
       </c>
-      <c r="B17" s="7" t="s">
+      <c r="C17" s="75" t="s">
         <v>1312</v>
-      </c>
-      <c r="C17" s="75" t="s">
-        <v>1313</v>
       </c>
       <c r="D17" s="18"/>
       <c r="E17" s="37" t="s">
+        <v>1313</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A18" s="202" t="s">
         <v>1314</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A18" s="201" t="s">
-        <v>1315</v>
-      </c>
-      <c r="B18" s="202"/>
-      <c r="C18" s="202"/>
-      <c r="D18" s="202"/>
-      <c r="E18" s="202"/>
-      <c r="F18" s="202"/>
+      <c r="B18" s="203"/>
+      <c r="C18" s="203"/>
+      <c r="D18" s="203"/>
+      <c r="E18" s="203"/>
+      <c r="F18" s="203"/>
     </row>
     <row r="19" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A19" s="5" t="s">
         <v>240</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>1318</v>
+        <v>1317</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>1316</v>
+        <v>1315</v>
       </c>
       <c r="D19" s="5" t="s">
         <v>1220</v>
       </c>
       <c r="E19" s="37" t="s">
-        <v>1317</v>
+        <v>1316</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="96" x14ac:dyDescent="0.2">
@@ -8678,13 +8687,13 @@
         <v>258</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>1319</v>
+        <v>1318</v>
       </c>
       <c r="C20" s="59" t="s">
-        <v>1387</v>
+        <v>1386</v>
       </c>
       <c r="E20" s="37" t="s">
-        <v>1389</v>
+        <v>1388</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="16" x14ac:dyDescent="0.2">
@@ -8692,13 +8701,13 @@
         <v>251</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>1320</v>
+        <v>1319</v>
       </c>
       <c r="C21" s="6" t="s">
+        <v>1279</v>
+      </c>
+      <c r="E21" s="37" t="s">
         <v>1280</v>
-      </c>
-      <c r="E21" s="37" t="s">
-        <v>1281</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="80" x14ac:dyDescent="0.2">
@@ -8706,13 +8715,13 @@
         <v>258</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>1321</v>
+        <v>1320</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>1388</v>
+        <v>1387</v>
       </c>
       <c r="E22" s="37" t="s">
-        <v>1390</v>
+        <v>1389</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
@@ -8736,7 +8745,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G4" sqref="G4"/>
+      <selection pane="bottomLeft" activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -8776,13 +8785,13 @@
         <v>7</v>
       </c>
       <c r="C2" s="100" t="s">
-        <v>1442</v>
+        <v>1449</v>
       </c>
       <c r="D2" s="98" t="s">
         <v>8</v>
       </c>
       <c r="E2" s="99" t="s">
-        <v>1442</v>
+        <v>1449</v>
       </c>
       <c r="F2" s="98"/>
     </row>
@@ -8800,7 +8809,7 @@
         <v>12</v>
       </c>
       <c r="E3" s="37" t="s">
-        <v>1386</v>
+        <v>1385</v>
       </c>
       <c r="F3" s="5" t="s">
         <v>13</v>
@@ -9651,10 +9660,10 @@
     <row r="52" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A52" s="86"/>
       <c r="B52" s="163" t="s">
+        <v>1437</v>
+      </c>
+      <c r="C52" s="164" t="s">
         <v>1438</v>
-      </c>
-      <c r="C52" s="164" t="s">
-        <v>1439</v>
       </c>
       <c r="D52" s="86"/>
       <c r="E52" s="165" t="s">
@@ -9857,46 +9866,46 @@
     <row r="67" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A67" s="86"/>
       <c r="B67" s="163" t="s">
-        <v>1443</v>
+        <v>1441</v>
       </c>
       <c r="C67" s="164" t="s">
-        <v>1444</v>
+        <v>1442</v>
       </c>
       <c r="D67" s="86"/>
       <c r="E67" s="165" t="s">
-        <v>1445</v>
-      </c>
-      <c r="F67" s="203" t="s">
-        <v>1446</v>
+        <v>1443</v>
+      </c>
+      <c r="F67" s="166" t="s">
+        <v>1444</v>
       </c>
     </row>
     <row r="68" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A68" s="86"/>
       <c r="B68" s="163" t="s">
-        <v>1440</v>
+        <v>1439</v>
       </c>
       <c r="C68" s="164" t="s">
-        <v>1313</v>
+        <v>1312</v>
       </c>
       <c r="D68" s="86"/>
       <c r="E68" s="165" t="s">
-        <v>1441</v>
+        <v>1440</v>
       </c>
     </row>
     <row r="69" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="B69" s="1" t="s">
+        <v>1331</v>
+      </c>
+      <c r="C69" s="2" t="s">
         <v>1332</v>
       </c>
-      <c r="C69" s="2" t="s">
-        <v>1333</v>
-      </c>
       <c r="E69" s="40" t="s">
-        <v>1335</v>
+        <v>1334</v>
       </c>
     </row>
     <row r="70" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="B70" s="1" t="s">
-        <v>1334</v>
+        <v>1333</v>
       </c>
       <c r="C70" s="2" t="s">
         <v>76</v>
@@ -10197,14 +10206,14 @@
         <v>240</v>
       </c>
       <c r="B2" s="5" t="s">
+        <v>1358</v>
+      </c>
+      <c r="C2" s="6" t="s">
         <v>1359</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>1360</v>
       </c>
       <c r="D2" s="5"/>
       <c r="E2" s="43" t="s">
-        <v>1368</v>
+        <v>1367</v>
       </c>
       <c r="F2" s="1"/>
     </row>
@@ -10213,38 +10222,38 @@
         <v>481</v>
       </c>
       <c r="B3" s="5" t="s">
+        <v>1360</v>
+      </c>
+      <c r="C3" s="6" t="s">
         <v>1361</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>1362</v>
       </c>
       <c r="D3" s="5"/>
       <c r="E3" s="43" t="s">
-        <v>1369</v>
+        <v>1368</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" s="167" t="s">
-        <v>1363</v>
-      </c>
-      <c r="B4" s="168"/>
-      <c r="C4" s="168"/>
-      <c r="D4" s="168"/>
-      <c r="E4" s="169"/>
+      <c r="A4" s="168" t="s">
+        <v>1362</v>
+      </c>
+      <c r="B4" s="169"/>
+      <c r="C4" s="169"/>
+      <c r="D4" s="169"/>
+      <c r="E4" s="170"/>
     </row>
     <row r="5" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
         <v>240</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>1364</v>
+        <v>1363</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>1366</v>
+        <v>1365</v>
       </c>
       <c r="D5" s="5"/>
       <c r="E5" s="43" t="s">
-        <v>1370</v>
+        <v>1369</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="96" x14ac:dyDescent="0.2">
@@ -10252,14 +10261,14 @@
         <v>481</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>1365</v>
+        <v>1364</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>1367</v>
+        <v>1366</v>
       </c>
       <c r="D6" s="5"/>
       <c r="E6" s="43" t="s">
-        <v>1371</v>
+        <v>1370</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
@@ -10480,7 +10489,7 @@
         <v>240</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>1374</v>
+        <v>1373</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>273</v>
@@ -10504,7 +10513,7 @@
         <v>243</v>
       </c>
       <c r="E4" s="43" t="s">
-        <v>1375</v>
+        <v>1374</v>
       </c>
       <c r="F4" s="68" t="s">
         <v>277</v>
@@ -10518,13 +10527,13 @@
         <v>278</v>
       </c>
       <c r="C5" s="52" t="s">
-        <v>1433</v>
+        <v>1432</v>
       </c>
       <c r="D5" s="66" t="s">
         <v>279</v>
       </c>
       <c r="E5" s="156" t="s">
-        <v>1434</v>
+        <v>1433</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>280</v>
@@ -10538,13 +10547,13 @@
         <v>281</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>1380</v>
+        <v>1379</v>
       </c>
       <c r="D6" s="67" t="s">
         <v>282</v>
       </c>
       <c r="E6" s="157" t="s">
-        <v>1381</v>
+        <v>1380</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="160" x14ac:dyDescent="0.2">
@@ -10555,13 +10564,13 @@
         <v>283</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>1382</v>
+        <v>1381</v>
       </c>
       <c r="D7" s="67" t="s">
         <v>284</v>
       </c>
       <c r="E7" s="157" t="s">
-        <v>1383</v>
+        <v>1382</v>
       </c>
       <c r="F7" s="68" t="s">
         <v>285</v>
@@ -10763,7 +10772,7 @@
         <v>333</v>
       </c>
       <c r="C19" s="64" t="s">
-        <v>1372</v>
+        <v>1371</v>
       </c>
       <c r="D19" s="7" t="s">
         <v>334</v>
@@ -10897,17 +10906,17 @@
     </row>
     <row r="27" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A27" s="5" t="s">
+        <v>1377</v>
+      </c>
+      <c r="B27" s="5" t="s">
         <v>1378</v>
       </c>
-      <c r="B27" s="5" t="s">
-        <v>1379</v>
-      </c>
       <c r="C27" s="6" t="s">
-        <v>1376</v>
+        <v>1375</v>
       </c>
       <c r="D27" s="5"/>
       <c r="E27" s="37" t="s">
-        <v>1377</v>
+        <v>1376</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
@@ -10984,13 +10993,13 @@
       </c>
     </row>
     <row r="2" spans="1:6" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="173" t="s">
+      <c r="A2" s="171" t="s">
         <v>364</v>
       </c>
-      <c r="B2" s="174"/>
-      <c r="C2" s="174"/>
-      <c r="D2" s="174"/>
-      <c r="E2" s="175"/>
+      <c r="B2" s="172"/>
+      <c r="C2" s="172"/>
+      <c r="D2" s="172"/>
+      <c r="E2" s="173"/>
       <c r="F2" s="33"/>
     </row>
     <row r="3" spans="1:6" ht="48" x14ac:dyDescent="0.2">
@@ -11118,13 +11127,13 @@
       <c r="F9" s="119"/>
     </row>
     <row r="10" spans="1:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="176" t="s">
+      <c r="A10" s="174" t="s">
         <v>393</v>
       </c>
-      <c r="B10" s="177"/>
-      <c r="C10" s="177"/>
-      <c r="D10" s="177"/>
-      <c r="E10" s="178"/>
+      <c r="B10" s="175"/>
+      <c r="C10" s="175"/>
+      <c r="D10" s="175"/>
+      <c r="E10" s="176"/>
       <c r="F10" s="119"/>
     </row>
     <row r="11" spans="1:6" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -11153,13 +11162,13 @@
         <v>398</v>
       </c>
       <c r="C12" s="153" t="s">
-        <v>1336</v>
+        <v>1335</v>
       </c>
       <c r="D12" s="84" t="s">
         <v>399</v>
       </c>
       <c r="E12" s="152" t="s">
-        <v>1337</v>
+        <v>1336</v>
       </c>
       <c r="F12" s="86"/>
     </row>
@@ -11171,24 +11180,24 @@
         <v>400</v>
       </c>
       <c r="C13" s="154" t="s">
-        <v>1338</v>
+        <v>1337</v>
       </c>
       <c r="D13" s="88" t="s">
         <v>401</v>
       </c>
       <c r="E13" s="155" t="s">
-        <v>1339</v>
+        <v>1338</v>
       </c>
       <c r="F13" s="86"/>
     </row>
     <row r="14" spans="1:6" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="167" t="s">
+      <c r="A14" s="168" t="s">
         <v>402</v>
       </c>
-      <c r="B14" s="168"/>
-      <c r="C14" s="168"/>
-      <c r="D14" s="168"/>
-      <c r="E14" s="169"/>
+      <c r="B14" s="169"/>
+      <c r="C14" s="169"/>
+      <c r="D14" s="169"/>
+      <c r="E14" s="170"/>
       <c r="F14" s="119"/>
     </row>
     <row r="15" spans="1:6" ht="48" x14ac:dyDescent="0.2">
@@ -11332,13 +11341,13 @@
       <c r="F23" s="119"/>
     </row>
     <row r="24" spans="1:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="167" t="s">
+      <c r="A24" s="168" t="s">
         <v>432</v>
       </c>
-      <c r="B24" s="168"/>
-      <c r="C24" s="168"/>
-      <c r="D24" s="168"/>
-      <c r="E24" s="169"/>
+      <c r="B24" s="169"/>
+      <c r="C24" s="169"/>
+      <c r="D24" s="169"/>
+      <c r="E24" s="170"/>
       <c r="F24" s="119"/>
     </row>
     <row r="25" spans="1:6" ht="32" x14ac:dyDescent="0.2">
@@ -11610,13 +11619,13 @@
       <c r="F42" s="119"/>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A43" s="167" t="s">
+      <c r="A43" s="168" t="s">
         <v>476</v>
       </c>
-      <c r="B43" s="168"/>
-      <c r="C43" s="168"/>
-      <c r="D43" s="168"/>
-      <c r="E43" s="169"/>
+      <c r="B43" s="169"/>
+      <c r="C43" s="169"/>
+      <c r="D43" s="169"/>
+      <c r="E43" s="170"/>
       <c r="F43" s="119"/>
     </row>
     <row r="44" spans="1:6" ht="32" x14ac:dyDescent="0.2">
@@ -11645,7 +11654,7 @@
         <v>482</v>
       </c>
       <c r="C45" s="59" t="s">
-        <v>1355</v>
+        <v>1354</v>
       </c>
       <c r="D45" s="116"/>
       <c r="E45" s="120" t="s">
@@ -11658,14 +11667,14 @@
         <v>481</v>
       </c>
       <c r="B46" s="116" t="s">
-        <v>1358</v>
+        <v>1357</v>
       </c>
       <c r="C46" s="59" t="s">
-        <v>1356</v>
+        <v>1355</v>
       </c>
       <c r="D46" s="116"/>
       <c r="E46" s="120" t="s">
-        <v>1357</v>
+        <v>1356</v>
       </c>
       <c r="F46" s="119"/>
     </row>
@@ -11834,13 +11843,13 @@
       <c r="F57" s="119"/>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A58" s="167" t="s">
+      <c r="A58" s="168" t="s">
         <v>506</v>
       </c>
-      <c r="B58" s="168"/>
-      <c r="C58" s="168"/>
-      <c r="D58" s="168"/>
-      <c r="E58" s="169"/>
+      <c r="B58" s="169"/>
+      <c r="C58" s="169"/>
+      <c r="D58" s="169"/>
+      <c r="E58" s="170"/>
       <c r="F58" s="119"/>
     </row>
     <row r="59" spans="1:6" ht="64" x14ac:dyDescent="0.2">
@@ -11893,7 +11902,7 @@
         <v>519</v>
       </c>
       <c r="E61" s="120" t="s">
-        <v>1348</v>
+        <v>1347</v>
       </c>
       <c r="F61" s="119"/>
     </row>
@@ -11902,25 +11911,25 @@
         <v>516</v>
       </c>
       <c r="B62" s="116" t="s">
-        <v>1345</v>
+        <v>1344</v>
       </c>
       <c r="C62" s="117" t="s">
-        <v>1347</v>
+        <v>1346</v>
       </c>
       <c r="D62" s="116"/>
       <c r="E62" s="120" t="s">
-        <v>1346</v>
+        <v>1345</v>
       </c>
       <c r="F62" s="119"/>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A63" s="167" t="s">
+      <c r="A63" s="168" t="s">
         <v>520</v>
       </c>
-      <c r="B63" s="168"/>
-      <c r="C63" s="168"/>
-      <c r="D63" s="168"/>
-      <c r="E63" s="169"/>
+      <c r="B63" s="169"/>
+      <c r="C63" s="169"/>
+      <c r="D63" s="169"/>
+      <c r="E63" s="170"/>
       <c r="F63" s="119"/>
     </row>
     <row r="64" spans="1:6" ht="48" x14ac:dyDescent="0.2">
@@ -11970,13 +11979,13 @@
       <c r="F66" s="119"/>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A67" s="167" t="s">
+      <c r="A67" s="168" t="s">
         <v>525</v>
       </c>
-      <c r="B67" s="168"/>
-      <c r="C67" s="168"/>
-      <c r="D67" s="168"/>
-      <c r="E67" s="169"/>
+      <c r="B67" s="169"/>
+      <c r="C67" s="169"/>
+      <c r="D67" s="169"/>
+      <c r="E67" s="170"/>
       <c r="F67" s="119"/>
     </row>
     <row r="68" spans="1:6" ht="32" x14ac:dyDescent="0.2">
@@ -12208,13 +12217,13 @@
       <c r="F81" s="119"/>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A82" s="167" t="s">
+      <c r="A82" s="168" t="s">
         <v>564</v>
       </c>
-      <c r="B82" s="168"/>
-      <c r="C82" s="168"/>
-      <c r="D82" s="168"/>
-      <c r="E82" s="169"/>
+      <c r="B82" s="169"/>
+      <c r="C82" s="169"/>
+      <c r="D82" s="169"/>
+      <c r="E82" s="170"/>
       <c r="F82" s="119"/>
     </row>
     <row r="83" spans="1:6" ht="62.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -12243,11 +12252,11 @@
         <v>569</v>
       </c>
       <c r="C84" s="117" t="s">
-        <v>1398</v>
+        <v>1397</v>
       </c>
       <c r="D84" s="116"/>
       <c r="E84" s="120" t="s">
-        <v>1399</v>
+        <v>1398</v>
       </c>
       <c r="F84" s="119" t="s">
         <v>570</v>
@@ -12357,22 +12366,22 @@
         <v>588</v>
       </c>
       <c r="C91" s="117" t="s">
-        <v>1396</v>
+        <v>1395</v>
       </c>
       <c r="D91" s="116"/>
       <c r="E91" s="120" t="s">
-        <v>1397</v>
+        <v>1396</v>
       </c>
       <c r="F91" s="119"/>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A92" s="167" t="s">
+      <c r="A92" s="168" t="s">
         <v>589</v>
       </c>
-      <c r="B92" s="168"/>
-      <c r="C92" s="168"/>
-      <c r="D92" s="168"/>
-      <c r="E92" s="169"/>
+      <c r="B92" s="169"/>
+      <c r="C92" s="169"/>
+      <c r="D92" s="169"/>
+      <c r="E92" s="170"/>
       <c r="F92" s="119"/>
     </row>
     <row r="93" spans="1:6" ht="48" x14ac:dyDescent="0.2">
@@ -12401,11 +12410,11 @@
         <v>594</v>
       </c>
       <c r="C94" s="117" t="s">
-        <v>1416</v>
+        <v>1415</v>
       </c>
       <c r="D94" s="116"/>
       <c r="E94" s="120" t="s">
-        <v>1417</v>
+        <v>1416</v>
       </c>
       <c r="F94" s="119" t="s">
         <v>570</v>
@@ -12436,7 +12445,7 @@
         <v>84</v>
       </c>
       <c r="B96" s="159" t="s">
-        <v>1422</v>
+        <v>1421</v>
       </c>
       <c r="C96" s="93" t="s">
         <v>596</v>
@@ -12454,7 +12463,7 @@
         <v>84</v>
       </c>
       <c r="B97" s="159" t="s">
-        <v>1423</v>
+        <v>1422</v>
       </c>
       <c r="C97" s="93" t="s">
         <v>596</v>
@@ -12472,7 +12481,7 @@
         <v>84</v>
       </c>
       <c r="B98" s="160" t="s">
-        <v>1424</v>
+        <v>1423</v>
       </c>
       <c r="C98" s="161" t="s">
         <v>596</v>
@@ -12488,7 +12497,7 @@
         <v>84</v>
       </c>
       <c r="B99" s="160" t="s">
-        <v>1425</v>
+        <v>1424</v>
       </c>
       <c r="C99" s="161" t="s">
         <v>596</v>
@@ -12504,7 +12513,7 @@
         <v>84</v>
       </c>
       <c r="B100" s="160" t="s">
-        <v>1426</v>
+        <v>1425</v>
       </c>
       <c r="C100" s="161" t="s">
         <v>596</v>
@@ -12922,13 +12931,13 @@
       <c r="F127" s="119"/>
     </row>
     <row r="128" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A128" s="167" t="s">
+      <c r="A128" s="168" t="s">
         <v>675</v>
       </c>
-      <c r="B128" s="168"/>
-      <c r="C128" s="168"/>
-      <c r="D128" s="168"/>
-      <c r="E128" s="169"/>
+      <c r="B128" s="169"/>
+      <c r="C128" s="169"/>
+      <c r="D128" s="169"/>
+      <c r="E128" s="170"/>
       <c r="F128" s="119"/>
     </row>
     <row r="129" spans="1:6" ht="32" x14ac:dyDescent="0.2">
@@ -13116,13 +13125,13 @@
       <c r="F141" s="119"/>
     </row>
     <row r="142" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A142" s="167" t="s">
+      <c r="A142" s="168" t="s">
         <v>697</v>
       </c>
-      <c r="B142" s="168"/>
-      <c r="C142" s="168"/>
-      <c r="D142" s="168"/>
-      <c r="E142" s="169"/>
+      <c r="B142" s="169"/>
+      <c r="C142" s="169"/>
+      <c r="D142" s="169"/>
+      <c r="E142" s="170"/>
       <c r="F142" s="119"/>
     </row>
     <row r="143" spans="1:6" ht="64" x14ac:dyDescent="0.2">
@@ -13179,7 +13188,7 @@
         <v>704</v>
       </c>
       <c r="C146" s="113" t="s">
-        <v>1323</v>
+        <v>1322</v>
       </c>
       <c r="D146" s="122" t="s">
         <v>705</v>
@@ -13252,13 +13261,13 @@
       <c r="F150" s="119"/>
     </row>
     <row r="151" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A151" s="167" t="s">
+      <c r="A151" s="168" t="s">
         <v>718</v>
       </c>
-      <c r="B151" s="168"/>
-      <c r="C151" s="168"/>
-      <c r="D151" s="168"/>
-      <c r="E151" s="169"/>
+      <c r="B151" s="169"/>
+      <c r="C151" s="169"/>
+      <c r="D151" s="169"/>
+      <c r="E151" s="170"/>
       <c r="F151" s="119"/>
     </row>
     <row r="152" spans="1:6" ht="32" x14ac:dyDescent="0.2">
@@ -13269,7 +13278,7 @@
         <v>719</v>
       </c>
       <c r="C152" s="59" t="s">
-        <v>1322</v>
+        <v>1321</v>
       </c>
       <c r="D152" s="116" t="s">
         <v>720</v>
@@ -13300,14 +13309,14 @@
         <v>37</v>
       </c>
       <c r="B154" s="116" t="s">
-        <v>1324</v>
+        <v>1323</v>
       </c>
       <c r="C154" s="59" t="s">
-        <v>1326</v>
+        <v>1325</v>
       </c>
       <c r="D154" s="116"/>
       <c r="E154" s="120" t="s">
-        <v>1328</v>
+        <v>1327</v>
       </c>
       <c r="F154" s="119"/>
     </row>
@@ -13316,14 +13325,14 @@
         <v>37</v>
       </c>
       <c r="B155" s="116" t="s">
-        <v>1325</v>
+        <v>1324</v>
       </c>
       <c r="C155" s="59" t="s">
-        <v>1327</v>
+        <v>1326</v>
       </c>
       <c r="D155" s="116"/>
       <c r="E155" s="120" t="s">
-        <v>1329</v>
+        <v>1328</v>
       </c>
       <c r="F155" s="119"/>
     </row>
@@ -13418,13 +13427,13 @@
       <c r="F161" s="119"/>
     </row>
     <row r="162" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A162" s="167" t="s">
+      <c r="A162" s="168" t="s">
         <v>739</v>
       </c>
-      <c r="B162" s="168"/>
-      <c r="C162" s="168"/>
-      <c r="D162" s="168"/>
-      <c r="E162" s="169"/>
+      <c r="B162" s="169"/>
+      <c r="C162" s="169"/>
+      <c r="D162" s="169"/>
+      <c r="E162" s="170"/>
       <c r="F162" s="119"/>
     </row>
     <row r="163" spans="1:6" ht="48" x14ac:dyDescent="0.2">
@@ -13542,13 +13551,13 @@
       <c r="F169" s="119"/>
     </row>
     <row r="170" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A170" s="170" t="s">
+      <c r="A170" s="177" t="s">
         <v>759</v>
       </c>
-      <c r="B170" s="171"/>
-      <c r="C170" s="171"/>
-      <c r="D170" s="171"/>
-      <c r="E170" s="172"/>
+      <c r="B170" s="178"/>
+      <c r="C170" s="178"/>
+      <c r="D170" s="178"/>
+      <c r="E170" s="179"/>
       <c r="F170" s="129" t="s">
         <v>760</v>
       </c>
@@ -13674,13 +13683,13 @@
       </c>
     </row>
     <row r="179" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A179" s="167" t="s">
+      <c r="A179" s="168" t="s">
         <v>771</v>
       </c>
-      <c r="B179" s="168"/>
-      <c r="C179" s="168"/>
-      <c r="D179" s="168"/>
-      <c r="E179" s="169"/>
+      <c r="B179" s="169"/>
+      <c r="C179" s="169"/>
+      <c r="D179" s="169"/>
+      <c r="E179" s="170"/>
       <c r="F179" s="119"/>
     </row>
     <row r="180" spans="1:6" ht="32" x14ac:dyDescent="0.2">
@@ -13866,13 +13875,13 @@
       <c r="F190" s="119"/>
     </row>
     <row r="191" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A191" s="167" t="s">
+      <c r="A191" s="168" t="s">
         <v>792</v>
       </c>
-      <c r="B191" s="168"/>
-      <c r="C191" s="168"/>
-      <c r="D191" s="168"/>
-      <c r="E191" s="169"/>
+      <c r="B191" s="169"/>
+      <c r="C191" s="169"/>
+      <c r="D191" s="169"/>
+      <c r="E191" s="170"/>
       <c r="F191" s="119"/>
     </row>
     <row r="192" spans="1:6" ht="32" x14ac:dyDescent="0.2">
@@ -13922,13 +13931,13 @@
       <c r="F194" s="119"/>
     </row>
     <row r="195" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A195" s="167" t="s">
+      <c r="A195" s="168" t="s">
         <v>800</v>
       </c>
-      <c r="B195" s="168"/>
-      <c r="C195" s="168"/>
-      <c r="D195" s="168"/>
-      <c r="E195" s="169"/>
+      <c r="B195" s="169"/>
+      <c r="C195" s="169"/>
+      <c r="D195" s="169"/>
+      <c r="E195" s="170"/>
       <c r="F195" s="119"/>
     </row>
     <row r="196" spans="1:6" ht="64" x14ac:dyDescent="0.2">
@@ -13975,13 +13984,13 @@
         <v>809</v>
       </c>
       <c r="C198" s="59" t="s">
-        <v>1340</v>
+        <v>1339</v>
       </c>
       <c r="D198" s="116" t="s">
         <v>810</v>
       </c>
       <c r="E198" s="120" t="s">
-        <v>1344</v>
+        <v>1343</v>
       </c>
       <c r="F198" s="119"/>
     </row>
@@ -13990,14 +13999,14 @@
         <v>481</v>
       </c>
       <c r="B199" s="116" t="s">
+        <v>1340</v>
+      </c>
+      <c r="C199" s="59" t="s">
         <v>1341</v>
-      </c>
-      <c r="C199" s="59" t="s">
-        <v>1342</v>
       </c>
       <c r="D199" s="116"/>
       <c r="E199" s="120" t="s">
-        <v>1343</v>
+        <v>1342</v>
       </c>
       <c r="F199" s="119"/>
     </row>
@@ -14030,13 +14039,13 @@
       <c r="F201" s="119"/>
     </row>
     <row r="202" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A202" s="167" t="s">
+      <c r="A202" s="168" t="s">
         <v>815</v>
       </c>
-      <c r="B202" s="168"/>
-      <c r="C202" s="168"/>
-      <c r="D202" s="168"/>
-      <c r="E202" s="169"/>
+      <c r="B202" s="169"/>
+      <c r="C202" s="169"/>
+      <c r="D202" s="169"/>
+      <c r="E202" s="170"/>
       <c r="F202" s="119"/>
     </row>
     <row r="203" spans="1:6" ht="32" x14ac:dyDescent="0.2">
@@ -14097,11 +14106,11 @@
         <v>821</v>
       </c>
       <c r="C206" s="117" t="s">
-        <v>1351</v>
+        <v>1350</v>
       </c>
       <c r="D206" s="116"/>
       <c r="E206" s="120" t="s">
-        <v>1354</v>
+        <v>1353</v>
       </c>
       <c r="F206" s="119"/>
     </row>
@@ -14110,7 +14119,7 @@
         <v>728</v>
       </c>
       <c r="B207" s="116" t="s">
-        <v>1353</v>
+        <v>1352</v>
       </c>
       <c r="C207" s="117" t="s">
         <v>43</v>
@@ -14126,14 +14135,14 @@
         <v>32</v>
       </c>
       <c r="B208" s="116" t="s">
-        <v>1352</v>
+        <v>1351</v>
       </c>
       <c r="C208" s="134" t="s">
-        <v>1349</v>
+        <v>1348</v>
       </c>
       <c r="D208" s="116"/>
       <c r="E208" s="120" t="s">
-        <v>1350</v>
+        <v>1349</v>
       </c>
       <c r="F208" s="119"/>
     </row>
@@ -14194,13 +14203,13 @@
       <c r="F212" s="119"/>
     </row>
     <row r="213" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A213" s="167" t="s">
+      <c r="A213" s="168" t="s">
         <v>826</v>
       </c>
-      <c r="B213" s="168"/>
-      <c r="C213" s="168"/>
-      <c r="D213" s="168"/>
-      <c r="E213" s="169"/>
+      <c r="B213" s="169"/>
+      <c r="C213" s="169"/>
+      <c r="D213" s="169"/>
+      <c r="E213" s="170"/>
       <c r="F213" s="119"/>
     </row>
     <row r="214" spans="1:6" ht="48" x14ac:dyDescent="0.2">
@@ -14286,13 +14295,13 @@
       <c r="F218" s="119"/>
     </row>
     <row r="219" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A219" s="167" t="s">
+      <c r="A219" s="168" t="s">
         <v>836</v>
       </c>
-      <c r="B219" s="168"/>
-      <c r="C219" s="168"/>
-      <c r="D219" s="168"/>
-      <c r="E219" s="169"/>
+      <c r="B219" s="169"/>
+      <c r="C219" s="169"/>
+      <c r="D219" s="169"/>
+      <c r="E219" s="170"/>
       <c r="F219" s="119"/>
     </row>
     <row r="220" spans="1:6" ht="32" x14ac:dyDescent="0.2">
@@ -14450,13 +14459,13 @@
       <c r="F229" s="119"/>
     </row>
     <row r="230" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A230" s="167" t="s">
+      <c r="A230" s="168" t="s">
         <v>850</v>
       </c>
-      <c r="B230" s="168"/>
-      <c r="C230" s="168"/>
-      <c r="D230" s="168"/>
-      <c r="E230" s="169"/>
+      <c r="B230" s="169"/>
+      <c r="C230" s="169"/>
+      <c r="D230" s="169"/>
+      <c r="E230" s="170"/>
       <c r="F230" s="119"/>
     </row>
     <row r="231" spans="1:6" ht="48" x14ac:dyDescent="0.2">
@@ -14505,13 +14514,13 @@
         <v>860</v>
       </c>
       <c r="C233" s="59" t="s">
-        <v>1384</v>
+        <v>1383</v>
       </c>
       <c r="D233" s="116" t="s">
         <v>861</v>
       </c>
       <c r="E233" s="120" t="s">
-        <v>1385</v>
+        <v>1384</v>
       </c>
       <c r="F233" s="119"/>
     </row>
@@ -15451,18 +15460,6 @@
     </row>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="A230:E230"/>
-    <mergeCell ref="A191:E191"/>
-    <mergeCell ref="A195:E195"/>
-    <mergeCell ref="A202:E202"/>
-    <mergeCell ref="A213:E213"/>
-    <mergeCell ref="A219:E219"/>
-    <mergeCell ref="A58:E58"/>
-    <mergeCell ref="A2:E2"/>
-    <mergeCell ref="A10:E10"/>
-    <mergeCell ref="A14:E14"/>
-    <mergeCell ref="A24:E24"/>
-    <mergeCell ref="A43:E43"/>
     <mergeCell ref="A179:E179"/>
     <mergeCell ref="A162:E162"/>
     <mergeCell ref="A63:E63"/>
@@ -15473,6 +15470,18 @@
     <mergeCell ref="A151:E151"/>
     <mergeCell ref="A92:E92"/>
     <mergeCell ref="A170:E170"/>
+    <mergeCell ref="A58:E58"/>
+    <mergeCell ref="A2:E2"/>
+    <mergeCell ref="A10:E10"/>
+    <mergeCell ref="A14:E14"/>
+    <mergeCell ref="A24:E24"/>
+    <mergeCell ref="A43:E43"/>
+    <mergeCell ref="A230:E230"/>
+    <mergeCell ref="A191:E191"/>
+    <mergeCell ref="A195:E195"/>
+    <mergeCell ref="A202:E202"/>
+    <mergeCell ref="A213:E213"/>
+    <mergeCell ref="A219:E219"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -15519,13 +15528,13 @@
       </c>
     </row>
     <row r="2" spans="1:6" s="24" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="182" t="s">
+      <c r="A2" s="183" t="s">
         <v>899</v>
       </c>
-      <c r="B2" s="183"/>
-      <c r="C2" s="183"/>
-      <c r="D2" s="183"/>
-      <c r="E2" s="184"/>
+      <c r="B2" s="184"/>
+      <c r="C2" s="184"/>
+      <c r="D2" s="184"/>
+      <c r="E2" s="185"/>
     </row>
     <row r="3" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="19" t="s">
@@ -15659,13 +15668,13 @@
       </c>
     </row>
     <row r="12" spans="1:6" s="24" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="182" t="s">
+      <c r="A12" s="183" t="s">
         <v>921</v>
       </c>
-      <c r="B12" s="183"/>
-      <c r="C12" s="183"/>
-      <c r="D12" s="183"/>
-      <c r="E12" s="184"/>
+      <c r="B12" s="184"/>
+      <c r="C12" s="184"/>
+      <c r="D12" s="184"/>
+      <c r="E12" s="185"/>
     </row>
     <row r="13" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A13" s="19" t="s">
@@ -15743,13 +15752,13 @@
         <v>936</v>
       </c>
       <c r="C17" s="151" t="s">
-        <v>1330</v>
+        <v>1329</v>
       </c>
       <c r="D17" s="92" t="s">
         <v>928</v>
       </c>
       <c r="E17" s="152" t="s">
-        <v>1331</v>
+        <v>1330</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="80" x14ac:dyDescent="0.2">
@@ -15777,13 +15786,13 @@
       </c>
     </row>
     <row r="20" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="191" t="s">
+      <c r="A20" s="192" t="s">
         <v>941</v>
       </c>
-      <c r="B20" s="192"/>
-      <c r="C20" s="192"/>
-      <c r="D20" s="192"/>
-      <c r="E20" s="193"/>
+      <c r="B20" s="193"/>
+      <c r="C20" s="193"/>
+      <c r="D20" s="193"/>
+      <c r="E20" s="194"/>
     </row>
     <row r="21" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A21" s="5" t="s">
@@ -15831,13 +15840,13 @@
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A24" s="188" t="s">
+      <c r="A24" s="189" t="s">
         <v>954</v>
       </c>
-      <c r="B24" s="189"/>
-      <c r="C24" s="189"/>
-      <c r="D24" s="189"/>
-      <c r="E24" s="190"/>
+      <c r="B24" s="190"/>
+      <c r="C24" s="190"/>
+      <c r="D24" s="190"/>
+      <c r="E24" s="191"/>
     </row>
     <row r="25" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A25" s="18" t="s">
@@ -15855,13 +15864,13 @@
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A26" s="179" t="s">
+      <c r="A26" s="180" t="s">
         <v>958</v>
       </c>
-      <c r="B26" s="180"/>
-      <c r="C26" s="180"/>
-      <c r="D26" s="180"/>
-      <c r="E26" s="181"/>
+      <c r="B26" s="181"/>
+      <c r="C26" s="181"/>
+      <c r="D26" s="181"/>
+      <c r="E26" s="182"/>
     </row>
     <row r="27" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A27" s="18" t="s">
@@ -15879,13 +15888,13 @@
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A28" s="179" t="s">
+      <c r="A28" s="180" t="s">
         <v>962</v>
       </c>
-      <c r="B28" s="180"/>
-      <c r="C28" s="180"/>
-      <c r="D28" s="180"/>
-      <c r="E28" s="181"/>
+      <c r="B28" s="181"/>
+      <c r="C28" s="181"/>
+      <c r="D28" s="181"/>
+      <c r="E28" s="182"/>
     </row>
     <row r="29" spans="1:6" ht="112" x14ac:dyDescent="0.2">
       <c r="A29" s="91" t="s">
@@ -15949,10 +15958,10 @@
         <v>976</v>
       </c>
       <c r="C32" s="21" t="s">
+        <v>1390</v>
+      </c>
+      <c r="E32" s="46" t="s">
         <v>1391</v>
-      </c>
-      <c r="E32" s="46" t="s">
-        <v>1392</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="32" x14ac:dyDescent="0.2">
@@ -15960,13 +15969,13 @@
         <v>258</v>
       </c>
       <c r="B33" s="19" t="s">
+        <v>1392</v>
+      </c>
+      <c r="C33" s="21" t="s">
         <v>1393</v>
       </c>
-      <c r="C33" s="21" t="s">
+      <c r="E33" s="46" t="s">
         <v>1394</v>
-      </c>
-      <c r="E33" s="46" t="s">
-        <v>1395</v>
       </c>
     </row>
     <row r="34" spans="1:6" ht="48" x14ac:dyDescent="0.2">
@@ -16023,13 +16032,13 @@
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A38" s="179" t="s">
+      <c r="A38" s="180" t="s">
         <v>987</v>
       </c>
-      <c r="B38" s="180"/>
-      <c r="C38" s="180"/>
-      <c r="D38" s="180"/>
-      <c r="E38" s="181"/>
+      <c r="B38" s="181"/>
+      <c r="C38" s="181"/>
+      <c r="D38" s="181"/>
+      <c r="E38" s="182"/>
     </row>
     <row r="39" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A39" s="19" t="s">
@@ -16073,13 +16082,13 @@
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A42" s="185" t="s">
+      <c r="A42" s="186" t="s">
         <v>995</v>
       </c>
-      <c r="B42" s="186"/>
-      <c r="C42" s="186"/>
-      <c r="D42" s="186"/>
-      <c r="E42" s="187"/>
+      <c r="B42" s="187"/>
+      <c r="C42" s="187"/>
+      <c r="D42" s="187"/>
+      <c r="E42" s="188"/>
     </row>
     <row r="43" spans="1:6" ht="96" x14ac:dyDescent="0.2">
       <c r="A43" s="116" t="s">
@@ -16126,13 +16135,13 @@
         <v>1001</v>
       </c>
       <c r="C45" s="62" t="s">
-        <v>1384</v>
+        <v>1383</v>
       </c>
       <c r="D45" s="116" t="s">
         <v>1002</v>
       </c>
       <c r="E45" s="46" t="s">
-        <v>1385</v>
+        <v>1384</v>
       </c>
     </row>
     <row r="46" spans="1:6" ht="48" x14ac:dyDescent="0.2">
@@ -16525,23 +16534,23 @@
         <v>1068</v>
       </c>
       <c r="E11" s="138" t="s">
-        <v>1409</v>
+        <v>1408</v>
       </c>
       <c r="F11" s="135"/>
     </row>
     <row r="12" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A12" s="136" t="s">
+        <v>1404</v>
+      </c>
+      <c r="B12" s="136" t="s">
         <v>1405</v>
       </c>
-      <c r="B12" s="136" t="s">
+      <c r="C12" s="137" t="s">
         <v>1406</v>
-      </c>
-      <c r="C12" s="137" t="s">
-        <v>1407</v>
       </c>
       <c r="D12" s="136"/>
       <c r="E12" s="138" t="s">
-        <v>1408</v>
+        <v>1407</v>
       </c>
       <c r="F12" s="135"/>
     </row>
@@ -16553,7 +16562,7 @@
         <v>1069</v>
       </c>
       <c r="C13" s="137" t="s">
-        <v>1403</v>
+        <v>1402</v>
       </c>
       <c r="D13" s="136" t="s">
         <v>1070</v>
@@ -16599,7 +16608,7 @@
         <v>1075</v>
       </c>
       <c r="C16" s="137" t="s">
-        <v>1400</v>
+        <v>1399</v>
       </c>
       <c r="D16" s="136" t="s">
         <v>1076</v>
@@ -16617,7 +16626,7 @@
         <v>1078</v>
       </c>
       <c r="C17" s="137" t="s">
-        <v>1401</v>
+        <v>1400</v>
       </c>
       <c r="D17" s="136" t="s">
         <v>1079</v>
@@ -16635,7 +16644,7 @@
         <v>1081</v>
       </c>
       <c r="C18" s="137" t="s">
-        <v>1402</v>
+        <v>1401</v>
       </c>
       <c r="D18" s="136" t="s">
         <v>1082</v>
@@ -16775,17 +16784,17 @@
     </row>
     <row r="28" spans="1:6" ht="64" x14ac:dyDescent="0.2">
       <c r="A28" s="136" t="s">
-        <v>1405</v>
+        <v>1404</v>
       </c>
       <c r="B28" s="136" t="s">
-        <v>1404</v>
+        <v>1403</v>
       </c>
       <c r="C28" s="137" t="s">
-        <v>1427</v>
+        <v>1426</v>
       </c>
       <c r="D28" s="136"/>
       <c r="E28" s="138" t="s">
-        <v>1429</v>
+        <v>1428</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="32" x14ac:dyDescent="0.2">
@@ -16796,23 +16805,23 @@
         <v>1107</v>
       </c>
       <c r="C29" s="137" t="s">
-        <v>1428</v>
+        <v>1427</v>
       </c>
       <c r="D29" s="136" t="s">
         <v>1108</v>
       </c>
       <c r="E29" s="138" t="s">
-        <v>1430</v>
+        <v>1429</v>
       </c>
     </row>
     <row r="30" spans="1:6" s="13" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="194" t="s">
+      <c r="A30" s="195" t="s">
         <v>1109</v>
       </c>
-      <c r="B30" s="195"/>
-      <c r="C30" s="195"/>
-      <c r="D30" s="195"/>
-      <c r="E30" s="196"/>
+      <c r="B30" s="196"/>
+      <c r="C30" s="196"/>
+      <c r="D30" s="196"/>
+      <c r="E30" s="197"/>
     </row>
     <row r="31" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A31" s="140" t="s">
@@ -16875,13 +16884,13 @@
       <c r="E34" s="146"/>
     </row>
     <row r="35" spans="1:6" s="13" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="197" t="s">
+      <c r="A35" s="198" t="s">
         <v>1121</v>
       </c>
-      <c r="B35" s="198"/>
-      <c r="C35" s="199"/>
-      <c r="D35" s="198"/>
-      <c r="E35" s="200"/>
+      <c r="B35" s="199"/>
+      <c r="C35" s="200"/>
+      <c r="D35" s="199"/>
+      <c r="E35" s="201"/>
     </row>
     <row r="36" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A36" s="144" t="s">
@@ -17045,7 +17054,7 @@
         <v>1145</v>
       </c>
       <c r="C45" s="62" t="s">
-        <v>1373</v>
+        <v>1372</v>
       </c>
       <c r="D45" s="5" t="s">
         <v>1146</v>
@@ -17084,13 +17093,13 @@
       <c r="F47" s="135"/>
     </row>
     <row r="48" spans="1:6" s="13" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="194" t="s">
+      <c r="A48" s="195" t="s">
         <v>1150</v>
       </c>
-      <c r="B48" s="195"/>
-      <c r="C48" s="195"/>
-      <c r="D48" s="195"/>
-      <c r="E48" s="196"/>
+      <c r="B48" s="196"/>
+      <c r="C48" s="196"/>
+      <c r="D48" s="196"/>
+      <c r="E48" s="197"/>
     </row>
     <row r="49" spans="1:6" s="30" customFormat="1" ht="64" x14ac:dyDescent="0.2">
       <c r="A49" s="144" t="s">
@@ -17137,13 +17146,13 @@
         <v>1157</v>
       </c>
       <c r="C51" s="62" t="s">
-        <v>1384</v>
+        <v>1383</v>
       </c>
       <c r="D51" s="116" t="s">
         <v>1002</v>
       </c>
       <c r="E51" s="63" t="s">
-        <v>1385</v>
+        <v>1384</v>
       </c>
     </row>
     <row r="52" spans="1:6" s="30" customFormat="1" ht="48" x14ac:dyDescent="0.2">
@@ -17497,47 +17506,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Readyforteam_x003f_ xmlns="565e1b1d-057e-4d85-b896-01a5881d8a45">false</Readyforteam_x003f_>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <SharedWithUsers xmlns="bf601f31-63a1-4825-9216-91d773c5ef9c">
-      <UserInfo>
-        <DisplayName>Erika Osti</DisplayName>
-        <AccountId>534</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Penny Johnson</DisplayName>
-        <AccountId>489</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Ben Childs</DisplayName>
-        <AccountId>643</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Thomas Leeds</DisplayName>
-        <AccountId>459</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Kasmyn Chen</DisplayName>
-        <AccountId>532</AccountId>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="565e1b1d-057e-4d85-b896-01a5881d8a45">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="2799d30d-6731-4efe-ac9b-c4895a8828d9" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010096D84A54A9CD274097F17166F184737D" ma:contentTypeVersion="21" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="2fd95a4cfdf4f2f51219070f5dff16a8">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="565e1b1d-057e-4d85-b896-01a5881d8a45" xmlns:ns3="bf601f31-63a1-4825-9216-91d773c5ef9c" xmlns:ns4="2799d30d-6731-4efe-ac9b-c4895a8828d9" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f7499f6f4dc8ad2a533df04863f63fa7" ns1:_="" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -17814,6 +17782,47 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Readyforteam_x003f_ xmlns="565e1b1d-057e-4d85-b896-01a5881d8a45">false</Readyforteam_x003f_>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <SharedWithUsers xmlns="bf601f31-63a1-4825-9216-91d773c5ef9c">
+      <UserInfo>
+        <DisplayName>Erika Osti</DisplayName>
+        <AccountId>534</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Penny Johnson</DisplayName>
+        <AccountId>489</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Ben Childs</DisplayName>
+        <AccountId>643</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Thomas Leeds</DisplayName>
+        <AccountId>459</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Kasmyn Chen</DisplayName>
+        <AccountId>532</AccountId>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="565e1b1d-057e-4d85-b896-01a5881d8a45">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="2799d30d-6731-4efe-ac9b-c4895a8828d9" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -17824,19 +17833,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{017ACE96-8143-486E-8436-7787F6B96F4A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="565e1b1d-057e-4d85-b896-01a5881d8a45"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="bf601f31-63a1-4825-9216-91d773c5ef9c"/>
-    <ds:schemaRef ds:uri="2799d30d-6731-4efe-ac9b-c4895a8828d9"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EAFDB110-4046-4E72-A1EF-1908ABEC3151}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -17857,6 +17853,19 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{017ACE96-8143-486E-8436-7787F6B96F4A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="565e1b1d-057e-4d85-b896-01a5881d8a45"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="bf601f31-63a1-4825-9216-91d773c5ef9c"/>
+    <ds:schemaRef ds:uri="2799d30d-6731-4efe-ac9b-c4895a8828d9"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8D7CE8C7-18DC-484F-8376-ED09F13D44C8}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
Updating text on button to "Submit for ME scrutiny".
</commit_message>
<xml_diff>
--- a/app/data/MCCD-localisation.xlsx
+++ b/app/data/MCCD-localisation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/JALAT/GIT/medical-certificate-of-cause-of-death/app/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B26DE70D-B64E-3A48-B34C-456AD2414A6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA7BC339-EE90-B74A-BD19-D60291ACF62E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="14100" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -69,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2177" uniqueCount="1450">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2177" uniqueCount="1451">
   <si>
     <r>
       <rPr>
@@ -5623,9 +5623,6 @@
     <t>Datganiad</t>
   </si>
   <si>
-    <t> Cyflwyno</t>
-  </si>
-  <si>
     <t>Select the ethnicity of the deceased person as it is recorded on the patient record. If there is no match with the list, or no ethnicity is recorded on the patient record, select 'not stated'.</t>
   </si>
   <si>
@@ -5728,7 +5725,13 @@
     <t> Rwy'n cadarnhau fy mod wedi adolygu'r dystysgrif hon a'i bod yn barod i'w archwilio a'i chymeradwyo gan arholwr meddygol.</t>
   </si>
   <si>
-    <t>037</t>
+    <t>Submit for ME scrutiny</t>
+  </si>
+  <si>
+    <t>Cyflwyno ar gyfer craffu ME</t>
+  </si>
+  <si>
+    <t>038</t>
   </si>
 </sst>
 </file>
@@ -6708,6 +6711,15 @@
     <xf numFmtId="0" fontId="13" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -6724,15 +6736,6 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -7958,7 +7961,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C25" sqref="C25"/>
+      <selection pane="bottomLeft" activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -8221,13 +8224,13 @@
         <v>1261</v>
       </c>
       <c r="C15" s="158" t="s">
-        <v>1430</v>
+        <v>1429</v>
       </c>
       <c r="D15" s="95" t="s">
         <v>1262</v>
       </c>
       <c r="E15" s="155" t="s">
-        <v>1431</v>
+        <v>1430</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="48" x14ac:dyDescent="0.2">
@@ -8306,13 +8309,13 @@
         <v>1266</v>
       </c>
       <c r="C20" s="158" t="s">
-        <v>1446</v>
+        <v>1445</v>
       </c>
       <c r="D20" s="95" t="s">
         <v>1239</v>
       </c>
       <c r="E20" s="155" t="s">
-        <v>1447</v>
+        <v>1446</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="64" x14ac:dyDescent="0.2">
@@ -8323,13 +8326,13 @@
         <v>1267</v>
       </c>
       <c r="C21" s="158" t="s">
-        <v>1445</v>
+        <v>1444</v>
       </c>
       <c r="D21" s="95" t="s">
         <v>1268</v>
       </c>
       <c r="E21" s="155" t="s">
-        <v>1448</v>
+        <v>1447</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -8340,13 +8343,13 @@
         <v>1269</v>
       </c>
       <c r="C22" s="158" t="s">
-        <v>1410</v>
+        <v>1448</v>
       </c>
       <c r="D22" s="95" t="s">
         <v>401</v>
       </c>
       <c r="E22" s="155" t="s">
-        <v>1414</v>
+        <v>1449</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="48" x14ac:dyDescent="0.2">
@@ -8463,7 +8466,7 @@
         <v>1276</v>
       </c>
       <c r="C4" s="59" t="s">
-        <v>1436</v>
+        <v>1435</v>
       </c>
       <c r="E4" s="37" t="s">
         <v>1277</v>
@@ -8491,10 +8494,10 @@
         <v>1281</v>
       </c>
       <c r="C6" s="6" t="s">
+        <v>1433</v>
+      </c>
+      <c r="E6" s="37" t="s">
         <v>1434</v>
-      </c>
-      <c r="E6" s="37" t="s">
-        <v>1435</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="32" x14ac:dyDescent="0.2">
@@ -8519,10 +8522,10 @@
         <v>1286</v>
       </c>
       <c r="C8" s="6" t="s">
+        <v>1418</v>
+      </c>
+      <c r="E8" s="37" t="s">
         <v>1419</v>
-      </c>
-      <c r="E8" s="37" t="s">
-        <v>1420</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="16" x14ac:dyDescent="0.2">
@@ -8603,11 +8606,11 @@
         <v>1303</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>1417</v>
+        <v>1416</v>
       </c>
       <c r="D14" s="1"/>
       <c r="E14" s="37" t="s">
-        <v>1418</v>
+        <v>1417</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="32" x14ac:dyDescent="0.2">
@@ -8745,7 +8748,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G3" sqref="G3"/>
+      <selection pane="bottomLeft" activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -8785,13 +8788,13 @@
         <v>7</v>
       </c>
       <c r="C2" s="100" t="s">
-        <v>1449</v>
+        <v>1450</v>
       </c>
       <c r="D2" s="98" t="s">
         <v>8</v>
       </c>
       <c r="E2" s="99" t="s">
-        <v>1449</v>
+        <v>1450</v>
       </c>
       <c r="F2" s="98"/>
     </row>
@@ -9660,10 +9663,10 @@
     <row r="52" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A52" s="86"/>
       <c r="B52" s="163" t="s">
+        <v>1436</v>
+      </c>
+      <c r="C52" s="164" t="s">
         <v>1437</v>
-      </c>
-      <c r="C52" s="164" t="s">
-        <v>1438</v>
       </c>
       <c r="D52" s="86"/>
       <c r="E52" s="165" t="s">
@@ -9866,30 +9869,30 @@
     <row r="67" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A67" s="86"/>
       <c r="B67" s="163" t="s">
+        <v>1440</v>
+      </c>
+      <c r="C67" s="164" t="s">
         <v>1441</v>
-      </c>
-      <c r="C67" s="164" t="s">
-        <v>1442</v>
       </c>
       <c r="D67" s="86"/>
       <c r="E67" s="165" t="s">
+        <v>1442</v>
+      </c>
+      <c r="F67" s="166" t="s">
         <v>1443</v>
-      </c>
-      <c r="F67" s="166" t="s">
-        <v>1444</v>
       </c>
     </row>
     <row r="68" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A68" s="86"/>
       <c r="B68" s="163" t="s">
-        <v>1439</v>
+        <v>1438</v>
       </c>
       <c r="C68" s="164" t="s">
         <v>1312</v>
       </c>
       <c r="D68" s="86"/>
       <c r="E68" s="165" t="s">
-        <v>1440</v>
+        <v>1439</v>
       </c>
     </row>
     <row r="69" spans="1:6" ht="16" x14ac:dyDescent="0.2">
@@ -10527,13 +10530,13 @@
         <v>278</v>
       </c>
       <c r="C5" s="52" t="s">
-        <v>1432</v>
+        <v>1431</v>
       </c>
       <c r="D5" s="66" t="s">
         <v>279</v>
       </c>
       <c r="E5" s="156" t="s">
-        <v>1433</v>
+        <v>1432</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>280</v>
@@ -10993,13 +10996,13 @@
       </c>
     </row>
     <row r="2" spans="1:6" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="171" t="s">
+      <c r="A2" s="174" t="s">
         <v>364</v>
       </c>
-      <c r="B2" s="172"/>
-      <c r="C2" s="172"/>
-      <c r="D2" s="172"/>
-      <c r="E2" s="173"/>
+      <c r="B2" s="175"/>
+      <c r="C2" s="175"/>
+      <c r="D2" s="175"/>
+      <c r="E2" s="176"/>
       <c r="F2" s="33"/>
     </row>
     <row r="3" spans="1:6" ht="48" x14ac:dyDescent="0.2">
@@ -11127,13 +11130,13 @@
       <c r="F9" s="119"/>
     </row>
     <row r="10" spans="1:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="174" t="s">
+      <c r="A10" s="177" t="s">
         <v>393</v>
       </c>
-      <c r="B10" s="175"/>
-      <c r="C10" s="175"/>
-      <c r="D10" s="175"/>
-      <c r="E10" s="176"/>
+      <c r="B10" s="178"/>
+      <c r="C10" s="178"/>
+      <c r="D10" s="178"/>
+      <c r="E10" s="179"/>
       <c r="F10" s="119"/>
     </row>
     <row r="11" spans="1:6" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -12410,11 +12413,11 @@
         <v>594</v>
       </c>
       <c r="C94" s="117" t="s">
-        <v>1415</v>
+        <v>1414</v>
       </c>
       <c r="D94" s="116"/>
       <c r="E94" s="120" t="s">
-        <v>1416</v>
+        <v>1415</v>
       </c>
       <c r="F94" s="119" t="s">
         <v>570</v>
@@ -12445,7 +12448,7 @@
         <v>84</v>
       </c>
       <c r="B96" s="159" t="s">
-        <v>1421</v>
+        <v>1420</v>
       </c>
       <c r="C96" s="93" t="s">
         <v>596</v>
@@ -12463,7 +12466,7 @@
         <v>84</v>
       </c>
       <c r="B97" s="159" t="s">
-        <v>1422</v>
+        <v>1421</v>
       </c>
       <c r="C97" s="93" t="s">
         <v>596</v>
@@ -12481,7 +12484,7 @@
         <v>84</v>
       </c>
       <c r="B98" s="160" t="s">
-        <v>1423</v>
+        <v>1422</v>
       </c>
       <c r="C98" s="161" t="s">
         <v>596</v>
@@ -12497,7 +12500,7 @@
         <v>84</v>
       </c>
       <c r="B99" s="160" t="s">
-        <v>1424</v>
+        <v>1423</v>
       </c>
       <c r="C99" s="161" t="s">
         <v>596</v>
@@ -12513,7 +12516,7 @@
         <v>84</v>
       </c>
       <c r="B100" s="160" t="s">
-        <v>1425</v>
+        <v>1424</v>
       </c>
       <c r="C100" s="161" t="s">
         <v>596</v>
@@ -13551,13 +13554,13 @@
       <c r="F169" s="119"/>
     </row>
     <row r="170" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A170" s="177" t="s">
+      <c r="A170" s="171" t="s">
         <v>759</v>
       </c>
-      <c r="B170" s="178"/>
-      <c r="C170" s="178"/>
-      <c r="D170" s="178"/>
-      <c r="E170" s="179"/>
+      <c r="B170" s="172"/>
+      <c r="C170" s="172"/>
+      <c r="D170" s="172"/>
+      <c r="E170" s="173"/>
       <c r="F170" s="129" t="s">
         <v>760</v>
       </c>
@@ -15460,6 +15463,18 @@
     </row>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="A230:E230"/>
+    <mergeCell ref="A191:E191"/>
+    <mergeCell ref="A195:E195"/>
+    <mergeCell ref="A202:E202"/>
+    <mergeCell ref="A213:E213"/>
+    <mergeCell ref="A219:E219"/>
+    <mergeCell ref="A58:E58"/>
+    <mergeCell ref="A2:E2"/>
+    <mergeCell ref="A10:E10"/>
+    <mergeCell ref="A14:E14"/>
+    <mergeCell ref="A24:E24"/>
+    <mergeCell ref="A43:E43"/>
     <mergeCell ref="A179:E179"/>
     <mergeCell ref="A162:E162"/>
     <mergeCell ref="A63:E63"/>
@@ -15470,18 +15485,6 @@
     <mergeCell ref="A151:E151"/>
     <mergeCell ref="A92:E92"/>
     <mergeCell ref="A170:E170"/>
-    <mergeCell ref="A58:E58"/>
-    <mergeCell ref="A2:E2"/>
-    <mergeCell ref="A10:E10"/>
-    <mergeCell ref="A14:E14"/>
-    <mergeCell ref="A24:E24"/>
-    <mergeCell ref="A43:E43"/>
-    <mergeCell ref="A230:E230"/>
-    <mergeCell ref="A191:E191"/>
-    <mergeCell ref="A195:E195"/>
-    <mergeCell ref="A202:E202"/>
-    <mergeCell ref="A213:E213"/>
-    <mergeCell ref="A219:E219"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -16790,11 +16793,11 @@
         <v>1403</v>
       </c>
       <c r="C28" s="137" t="s">
-        <v>1426</v>
+        <v>1425</v>
       </c>
       <c r="D28" s="136"/>
       <c r="E28" s="138" t="s">
-        <v>1428</v>
+        <v>1427</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="32" x14ac:dyDescent="0.2">
@@ -16805,13 +16808,13 @@
         <v>1107</v>
       </c>
       <c r="C29" s="137" t="s">
-        <v>1427</v>
+        <v>1426</v>
       </c>
       <c r="D29" s="136" t="s">
         <v>1108</v>
       </c>
       <c r="E29" s="138" t="s">
-        <v>1429</v>
+        <v>1428</v>
       </c>
     </row>
     <row r="30" spans="1:6" s="13" customFormat="1" x14ac:dyDescent="0.2">
@@ -17506,6 +17509,56 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Readyforteam_x003f_ xmlns="565e1b1d-057e-4d85-b896-01a5881d8a45">false</Readyforteam_x003f_>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <SharedWithUsers xmlns="bf601f31-63a1-4825-9216-91d773c5ef9c">
+      <UserInfo>
+        <DisplayName>Erika Osti</DisplayName>
+        <AccountId>534</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Penny Johnson</DisplayName>
+        <AccountId>489</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Ben Childs</DisplayName>
+        <AccountId>643</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Thomas Leeds</DisplayName>
+        <AccountId>459</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Kasmyn Chen</DisplayName>
+        <AccountId>532</AccountId>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="565e1b1d-057e-4d85-b896-01a5881d8a45">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="2799d30d-6731-4efe-ac9b-c4895a8828d9" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010096D84A54A9CD274097F17166F184737D" ma:contentTypeVersion="21" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="2fd95a4cfdf4f2f51219070f5dff16a8">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="565e1b1d-057e-4d85-b896-01a5881d8a45" xmlns:ns3="bf601f31-63a1-4825-9216-91d773c5ef9c" xmlns:ns4="2799d30d-6731-4efe-ac9b-c4895a8828d9" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f7499f6f4dc8ad2a533df04863f63fa7" ns1:_="" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -17782,57 +17835,28 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Readyforteam_x003f_ xmlns="565e1b1d-057e-4d85-b896-01a5881d8a45">false</Readyforteam_x003f_>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <SharedWithUsers xmlns="bf601f31-63a1-4825-9216-91d773c5ef9c">
-      <UserInfo>
-        <DisplayName>Erika Osti</DisplayName>
-        <AccountId>534</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Penny Johnson</DisplayName>
-        <AccountId>489</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Ben Childs</DisplayName>
-        <AccountId>643</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Thomas Leeds</DisplayName>
-        <AccountId>459</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Kasmyn Chen</DisplayName>
-        <AccountId>532</AccountId>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="565e1b1d-057e-4d85-b896-01a5881d8a45">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="2799d30d-6731-4efe-ac9b-c4895a8828d9" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8D7CE8C7-18DC-484F-8376-ED09F13D44C8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{017ACE96-8143-486E-8436-7787F6B96F4A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="565e1b1d-057e-4d85-b896-01a5881d8a45"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="bf601f31-63a1-4825-9216-91d773c5ef9c"/>
+    <ds:schemaRef ds:uri="2799d30d-6731-4efe-ac9b-c4895a8828d9"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EAFDB110-4046-4E72-A1EF-1908ABEC3151}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -17851,25 +17875,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{017ACE96-8143-486E-8436-7787F6B96F4A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="565e1b1d-057e-4d85-b896-01a5881d8a45"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="bf601f31-63a1-4825-9216-91d773c5ef9c"/>
-    <ds:schemaRef ds:uri="2799d30d-6731-4efe-ac9b-c4895a8828d9"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8D7CE8C7-18DC-484F-8376-ED09F13D44C8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
More dashboard translation into Welsh.
</commit_message>
<xml_diff>
--- a/app/data/MCCD-localisation.xlsx
+++ b/app/data/MCCD-localisation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/JALAT/GIT/medical-certificate-of-cause-of-death/app/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA7BC339-EE90-B74A-BD19-D60291ACF62E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B895360-9F9D-F94E-B066-21DA02A687E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="14100" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -5521,9 +5521,6 @@
     <t>&lt;p class="govuk-body"&gt;This dashboard gives you access to the Medical certificates of cause of death (MCCDs) assigned to you for review and approval.&lt;/p&gt;&lt;p class="govuk-body"&gt;An MCCD can only be approved when scrutiny of the proposed cause of death is complete.&lt;/p&gt;</t>
   </si>
   <si>
-    <t>&lt;p&gt;Mae'r dangosfwrdd hwn yn rhoi mynediad i chi at y Tystysgrifau Meddygol o achos marwolaeth (MCCDs) a neilltuwyd i chi i'w hadolygu a'u cymeradwyo.&lt;/p&gt;&lt;p&gt;Dim ond pan fydd y gwaith o graffu ar yr achos marwolaeth arfaethedig wedi'i gwblhau y gellir cymeradwyo MCCD.&lt;/p&gt;</t>
-  </si>
-  <si>
     <t>&lt;p class="govuk-body"&gt;This dashboard gives you access to the Medical certificates of cause of death (MCCDs) currently being completed in your trust. You can view the progress of MCCDs and download signed-off MCCDs to send to the registrar.&lt;/p&gt;</t>
   </si>
   <si>
@@ -5677,9 +5674,6 @@
     <t>&lt;p class="govuk-body"&gt;This dashboard allows you to create a new Medical certificate of cause of death (MCCD) and manage current MCCDs.&lt;/p&gt;&lt;p class="govuk-body"&gt;This dashboard will list MCCDs that:&lt;/p&gt;&lt;ul class="govuk-list govuk-list--bullet"&gt;&lt;li&gt;you have submitted to a medical examiner for approval&lt;/li&gt;&lt;li&gt;have been approved by a medical examiner&lt;/li&gt;&lt;li&gt;have been rejected by a medical examiner and need amending&lt;/li&gt;&lt;/ul&gt;&lt;p class="govuk-body"&gt;Completed MCCDs will be removed after three months.&lt;/p&gt;</t>
   </si>
   <si>
-    <t>&lt;p class="govuk-body"&gt;Mae'r dangosfwrdd hwn yn eich galluogi i greu Tystysgrif Feddygol achos marwolaeth (MCCD) newydd a rheoli MCCDs presennol.&lt;/p&gt;&lt;p dosbarth = "govuk-body"&gt;Bydd y dangosfwrdd hwn yn rhestru MCCDs bod:&lt;/p&gt;&lt;ul dosbarth = "govuk-list--bullet"&gt;&lt;li&gt;rydych wedi cyflwyno i arholwr meddygol i'w gymeradwyo&lt;/li&gt;&lt;li&gt;gan arholwr meddygol wedi cael eu gwrthod gan arholwr meddygol&lt;/li&gt;&lt;li&gt;ac mae angen ei ddiwygio&lt;/li&gt;&lt;/ul&gt;&lt;p dosbarth = "govuk-body"&gt;Bydd MCCDs wedi'u cwblhau yn cael eu dileu ar ôl tri mis.&lt;/p&gt;</t>
-  </si>
-  <si>
     <t>The Medical certificate of cause of death (MCCD)  has been created and sent to the medical examiner office. This certificate will be available to view from your dashboard for 3 months.</t>
   </si>
   <si>
@@ -5731,7 +5725,13 @@
     <t>Cyflwyno ar gyfer craffu ME</t>
   </si>
   <si>
-    <t>038</t>
+    <t>&lt;p class="govuk-body"&gt;Mae'r dangosfwrdd hwn yn eich galluogi i greu Tystysgrif Feddygol achos marwolaeth (MCCD) newydd a rheoli MCCDs presennol.&lt;/p&gt;&lt;p class="govuk-body"&gt;Bydd y dangosfwrdd hwn yn rhestru MCCDs bod:&lt;/p&gt;&lt;ul class="govuk-list govuk-list--bullet"&gt;&lt;li&gt;rydych wedi cyflwyno i arholwr meddygol i'w gymeradwyo&lt;/li&gt;&lt;li&gt;gan arholwr meddygol wedi cael eu gwrthod gan arholwr meddygol&lt;/li&gt;&lt;li&gt;ac mae angen ei ddiwygio&lt;/li&gt;&lt;/ul&gt;&lt;p dosbarth="govuk-body"&gt;Bydd MCCDs wedi'u cwblhau yn cael eu dileu ar ôl tri mis.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p class="govuk-body"&gt;Mae'r dangosfwrdd hwn yn rhoi mynediad i chi at y Tystysgrifau Meddygol o achos marwolaeth (MCCDs) a neilltuwyd i chi i'w hadolygu a'u cymeradwyo.&lt;/p&gt;&lt;p class="govuk-body"&gt;Dim ond pan fydd y gwaith o graffu ar yr achos marwolaeth arfaethedig wedi'i gwblhau y gellir cymeradwyo MCCD.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>039</t>
   </si>
 </sst>
 </file>
@@ -6711,6 +6711,24 @@
     <xf numFmtId="0" fontId="13" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -6718,24 +6736,6 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -8003,13 +8003,13 @@
         <v>1238</v>
       </c>
       <c r="C2" s="151" t="s">
-        <v>1409</v>
+        <v>1408</v>
       </c>
       <c r="D2" s="92" t="s">
         <v>1239</v>
       </c>
       <c r="E2" s="152" t="s">
-        <v>1413</v>
+        <v>1412</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="80" x14ac:dyDescent="0.2">
@@ -8037,13 +8037,13 @@
         <v>1245</v>
       </c>
       <c r="C4" s="158" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="D4" s="95" t="s">
         <v>401</v>
       </c>
       <c r="E4" s="155" t="s">
-        <v>1412</v>
+        <v>1411</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="60.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -8105,13 +8105,13 @@
         <v>1250</v>
       </c>
       <c r="C8" s="158" t="s">
-        <v>1409</v>
+        <v>1408</v>
       </c>
       <c r="D8" s="95" t="s">
         <v>1251</v>
       </c>
       <c r="E8" s="155" t="s">
-        <v>1413</v>
+        <v>1412</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="64" x14ac:dyDescent="0.2">
@@ -8139,13 +8139,13 @@
         <v>1256</v>
       </c>
       <c r="C10" s="158" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="D10" s="95" t="s">
         <v>401</v>
       </c>
       <c r="E10" s="155" t="s">
-        <v>1412</v>
+        <v>1411</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -8207,13 +8207,13 @@
         <v>1259</v>
       </c>
       <c r="C14" s="158" t="s">
-        <v>1409</v>
+        <v>1408</v>
       </c>
       <c r="D14" s="95" t="s">
         <v>1260</v>
       </c>
       <c r="E14" s="155" t="s">
-        <v>1411</v>
+        <v>1410</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="80" x14ac:dyDescent="0.2">
@@ -8224,13 +8224,13 @@
         <v>1261</v>
       </c>
       <c r="C15" s="158" t="s">
-        <v>1429</v>
+        <v>1428</v>
       </c>
       <c r="D15" s="95" t="s">
         <v>1262</v>
       </c>
       <c r="E15" s="155" t="s">
-        <v>1430</v>
+        <v>1429</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="48" x14ac:dyDescent="0.2">
@@ -8275,13 +8275,13 @@
         <v>1265</v>
       </c>
       <c r="C18" s="158" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="D18" s="95" t="s">
         <v>401</v>
       </c>
       <c r="E18" s="155" t="s">
-        <v>1412</v>
+        <v>1411</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -8309,13 +8309,13 @@
         <v>1266</v>
       </c>
       <c r="C20" s="158" t="s">
-        <v>1445</v>
+        <v>1443</v>
       </c>
       <c r="D20" s="95" t="s">
         <v>1239</v>
       </c>
       <c r="E20" s="155" t="s">
-        <v>1446</v>
+        <v>1444</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="64" x14ac:dyDescent="0.2">
@@ -8326,13 +8326,13 @@
         <v>1267</v>
       </c>
       <c r="C21" s="158" t="s">
-        <v>1444</v>
+        <v>1442</v>
       </c>
       <c r="D21" s="95" t="s">
         <v>1268</v>
       </c>
       <c r="E21" s="155" t="s">
-        <v>1447</v>
+        <v>1445</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -8343,13 +8343,13 @@
         <v>1269</v>
       </c>
       <c r="C22" s="158" t="s">
-        <v>1448</v>
+        <v>1446</v>
       </c>
       <c r="D22" s="95" t="s">
         <v>401</v>
       </c>
       <c r="E22" s="155" t="s">
-        <v>1449</v>
+        <v>1447</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="48" x14ac:dyDescent="0.2">
@@ -8466,7 +8466,7 @@
         <v>1276</v>
       </c>
       <c r="C4" s="59" t="s">
-        <v>1435</v>
+        <v>1433</v>
       </c>
       <c r="E4" s="37" t="s">
         <v>1277</v>
@@ -8494,10 +8494,10 @@
         <v>1281</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>1433</v>
+        <v>1431</v>
       </c>
       <c r="E6" s="37" t="s">
-        <v>1434</v>
+        <v>1432</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="32" x14ac:dyDescent="0.2">
@@ -8522,10 +8522,10 @@
         <v>1286</v>
       </c>
       <c r="C8" s="6" t="s">
+        <v>1417</v>
+      </c>
+      <c r="E8" s="37" t="s">
         <v>1418</v>
-      </c>
-      <c r="E8" s="37" t="s">
-        <v>1419</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="16" x14ac:dyDescent="0.2">
@@ -8606,11 +8606,11 @@
         <v>1303</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>1416</v>
+        <v>1415</v>
       </c>
       <c r="D14" s="1"/>
       <c r="E14" s="37" t="s">
-        <v>1417</v>
+        <v>1416</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="32" x14ac:dyDescent="0.2">
@@ -8693,10 +8693,10 @@
         <v>1318</v>
       </c>
       <c r="C20" s="59" t="s">
-        <v>1386</v>
+        <v>1385</v>
       </c>
       <c r="E20" s="37" t="s">
-        <v>1388</v>
+        <v>1387</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="16" x14ac:dyDescent="0.2">
@@ -8721,10 +8721,10 @@
         <v>1320</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>1387</v>
+        <v>1386</v>
       </c>
       <c r="E22" s="37" t="s">
-        <v>1389</v>
+        <v>1388</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
@@ -8748,7 +8748,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F3" sqref="F3"/>
+      <selection pane="bottomLeft" activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -8812,7 +8812,7 @@
         <v>12</v>
       </c>
       <c r="E3" s="37" t="s">
-        <v>1385</v>
+        <v>1384</v>
       </c>
       <c r="F3" s="5" t="s">
         <v>13</v>
@@ -9663,10 +9663,10 @@
     <row r="52" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A52" s="86"/>
       <c r="B52" s="163" t="s">
-        <v>1436</v>
+        <v>1434</v>
       </c>
       <c r="C52" s="164" t="s">
-        <v>1437</v>
+        <v>1435</v>
       </c>
       <c r="D52" s="86"/>
       <c r="E52" s="165" t="s">
@@ -9869,30 +9869,30 @@
     <row r="67" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A67" s="86"/>
       <c r="B67" s="163" t="s">
-        <v>1440</v>
+        <v>1438</v>
       </c>
       <c r="C67" s="164" t="s">
-        <v>1441</v>
+        <v>1439</v>
       </c>
       <c r="D67" s="86"/>
       <c r="E67" s="165" t="s">
-        <v>1442</v>
+        <v>1440</v>
       </c>
       <c r="F67" s="166" t="s">
-        <v>1443</v>
+        <v>1441</v>
       </c>
     </row>
     <row r="68" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A68" s="86"/>
       <c r="B68" s="163" t="s">
-        <v>1438</v>
+        <v>1436</v>
       </c>
       <c r="C68" s="164" t="s">
         <v>1312</v>
       </c>
       <c r="D68" s="86"/>
       <c r="E68" s="165" t="s">
-        <v>1439</v>
+        <v>1437</v>
       </c>
     </row>
     <row r="69" spans="1:6" ht="16" x14ac:dyDescent="0.2">
@@ -10436,7 +10436,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F5" sqref="F5"/>
+      <selection pane="bottomLeft" activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -10530,19 +10530,19 @@
         <v>278</v>
       </c>
       <c r="C5" s="52" t="s">
-        <v>1431</v>
+        <v>1430</v>
       </c>
       <c r="D5" s="66" t="s">
         <v>279</v>
       </c>
       <c r="E5" s="156" t="s">
-        <v>1432</v>
+        <v>1448</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="160" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" ht="176" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
         <v>258</v>
       </c>
@@ -10556,7 +10556,7 @@
         <v>282</v>
       </c>
       <c r="E6" s="157" t="s">
-        <v>1380</v>
+        <v>1449</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="160" x14ac:dyDescent="0.2">
@@ -10567,13 +10567,13 @@
         <v>283</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>1381</v>
+        <v>1380</v>
       </c>
       <c r="D7" s="67" t="s">
         <v>284</v>
       </c>
       <c r="E7" s="157" t="s">
-        <v>1382</v>
+        <v>1381</v>
       </c>
       <c r="F7" s="68" t="s">
         <v>285</v>
@@ -10996,13 +10996,13 @@
       </c>
     </row>
     <row r="2" spans="1:6" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="174" t="s">
+      <c r="A2" s="171" t="s">
         <v>364</v>
       </c>
-      <c r="B2" s="175"/>
-      <c r="C2" s="175"/>
-      <c r="D2" s="175"/>
-      <c r="E2" s="176"/>
+      <c r="B2" s="172"/>
+      <c r="C2" s="172"/>
+      <c r="D2" s="172"/>
+      <c r="E2" s="173"/>
       <c r="F2" s="33"/>
     </row>
     <row r="3" spans="1:6" ht="48" x14ac:dyDescent="0.2">
@@ -11130,13 +11130,13 @@
       <c r="F9" s="119"/>
     </row>
     <row r="10" spans="1:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="177" t="s">
+      <c r="A10" s="174" t="s">
         <v>393</v>
       </c>
-      <c r="B10" s="178"/>
-      <c r="C10" s="178"/>
-      <c r="D10" s="178"/>
-      <c r="E10" s="179"/>
+      <c r="B10" s="175"/>
+      <c r="C10" s="175"/>
+      <c r="D10" s="175"/>
+      <c r="E10" s="176"/>
       <c r="F10" s="119"/>
     </row>
     <row r="11" spans="1:6" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -12255,11 +12255,11 @@
         <v>569</v>
       </c>
       <c r="C84" s="117" t="s">
-        <v>1397</v>
+        <v>1396</v>
       </c>
       <c r="D84" s="116"/>
       <c r="E84" s="120" t="s">
-        <v>1398</v>
+        <v>1397</v>
       </c>
       <c r="F84" s="119" t="s">
         <v>570</v>
@@ -12369,11 +12369,11 @@
         <v>588</v>
       </c>
       <c r="C91" s="117" t="s">
-        <v>1395</v>
+        <v>1394</v>
       </c>
       <c r="D91" s="116"/>
       <c r="E91" s="120" t="s">
-        <v>1396</v>
+        <v>1395</v>
       </c>
       <c r="F91" s="119"/>
     </row>
@@ -12413,11 +12413,11 @@
         <v>594</v>
       </c>
       <c r="C94" s="117" t="s">
-        <v>1414</v>
+        <v>1413</v>
       </c>
       <c r="D94" s="116"/>
       <c r="E94" s="120" t="s">
-        <v>1415</v>
+        <v>1414</v>
       </c>
       <c r="F94" s="119" t="s">
         <v>570</v>
@@ -12448,7 +12448,7 @@
         <v>84</v>
       </c>
       <c r="B96" s="159" t="s">
-        <v>1420</v>
+        <v>1419</v>
       </c>
       <c r="C96" s="93" t="s">
         <v>596</v>
@@ -12466,7 +12466,7 @@
         <v>84</v>
       </c>
       <c r="B97" s="159" t="s">
-        <v>1421</v>
+        <v>1420</v>
       </c>
       <c r="C97" s="93" t="s">
         <v>596</v>
@@ -12484,7 +12484,7 @@
         <v>84</v>
       </c>
       <c r="B98" s="160" t="s">
-        <v>1422</v>
+        <v>1421</v>
       </c>
       <c r="C98" s="161" t="s">
         <v>596</v>
@@ -12500,7 +12500,7 @@
         <v>84</v>
       </c>
       <c r="B99" s="160" t="s">
-        <v>1423</v>
+        <v>1422</v>
       </c>
       <c r="C99" s="161" t="s">
         <v>596</v>
@@ -12516,7 +12516,7 @@
         <v>84</v>
       </c>
       <c r="B100" s="160" t="s">
-        <v>1424</v>
+        <v>1423</v>
       </c>
       <c r="C100" s="161" t="s">
         <v>596</v>
@@ -13554,13 +13554,13 @@
       <c r="F169" s="119"/>
     </row>
     <row r="170" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A170" s="171" t="s">
+      <c r="A170" s="177" t="s">
         <v>759</v>
       </c>
-      <c r="B170" s="172"/>
-      <c r="C170" s="172"/>
-      <c r="D170" s="172"/>
-      <c r="E170" s="173"/>
+      <c r="B170" s="178"/>
+      <c r="C170" s="178"/>
+      <c r="D170" s="178"/>
+      <c r="E170" s="179"/>
       <c r="F170" s="129" t="s">
         <v>760</v>
       </c>
@@ -14517,13 +14517,13 @@
         <v>860</v>
       </c>
       <c r="C233" s="59" t="s">
-        <v>1383</v>
+        <v>1382</v>
       </c>
       <c r="D233" s="116" t="s">
         <v>861</v>
       </c>
       <c r="E233" s="120" t="s">
-        <v>1384</v>
+        <v>1383</v>
       </c>
       <c r="F233" s="119"/>
     </row>
@@ -15463,18 +15463,6 @@
     </row>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="A230:E230"/>
-    <mergeCell ref="A191:E191"/>
-    <mergeCell ref="A195:E195"/>
-    <mergeCell ref="A202:E202"/>
-    <mergeCell ref="A213:E213"/>
-    <mergeCell ref="A219:E219"/>
-    <mergeCell ref="A58:E58"/>
-    <mergeCell ref="A2:E2"/>
-    <mergeCell ref="A10:E10"/>
-    <mergeCell ref="A14:E14"/>
-    <mergeCell ref="A24:E24"/>
-    <mergeCell ref="A43:E43"/>
     <mergeCell ref="A179:E179"/>
     <mergeCell ref="A162:E162"/>
     <mergeCell ref="A63:E63"/>
@@ -15485,6 +15473,18 @@
     <mergeCell ref="A151:E151"/>
     <mergeCell ref="A92:E92"/>
     <mergeCell ref="A170:E170"/>
+    <mergeCell ref="A58:E58"/>
+    <mergeCell ref="A2:E2"/>
+    <mergeCell ref="A10:E10"/>
+    <mergeCell ref="A14:E14"/>
+    <mergeCell ref="A24:E24"/>
+    <mergeCell ref="A43:E43"/>
+    <mergeCell ref="A230:E230"/>
+    <mergeCell ref="A191:E191"/>
+    <mergeCell ref="A195:E195"/>
+    <mergeCell ref="A202:E202"/>
+    <mergeCell ref="A213:E213"/>
+    <mergeCell ref="A219:E219"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -15961,10 +15961,10 @@
         <v>976</v>
       </c>
       <c r="C32" s="21" t="s">
+        <v>1389</v>
+      </c>
+      <c r="E32" s="46" t="s">
         <v>1390</v>
-      </c>
-      <c r="E32" s="46" t="s">
-        <v>1391</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="32" x14ac:dyDescent="0.2">
@@ -15972,13 +15972,13 @@
         <v>258</v>
       </c>
       <c r="B33" s="19" t="s">
+        <v>1391</v>
+      </c>
+      <c r="C33" s="21" t="s">
         <v>1392</v>
       </c>
-      <c r="C33" s="21" t="s">
+      <c r="E33" s="46" t="s">
         <v>1393</v>
-      </c>
-      <c r="E33" s="46" t="s">
-        <v>1394</v>
       </c>
     </row>
     <row r="34" spans="1:6" ht="48" x14ac:dyDescent="0.2">
@@ -16138,13 +16138,13 @@
         <v>1001</v>
       </c>
       <c r="C45" s="62" t="s">
-        <v>1383</v>
+        <v>1382</v>
       </c>
       <c r="D45" s="116" t="s">
         <v>1002</v>
       </c>
       <c r="E45" s="46" t="s">
-        <v>1384</v>
+        <v>1383</v>
       </c>
     </row>
     <row r="46" spans="1:6" ht="48" x14ac:dyDescent="0.2">
@@ -16537,23 +16537,23 @@
         <v>1068</v>
       </c>
       <c r="E11" s="138" t="s">
-        <v>1408</v>
+        <v>1407</v>
       </c>
       <c r="F11" s="135"/>
     </row>
     <row r="12" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A12" s="136" t="s">
+        <v>1403</v>
+      </c>
+      <c r="B12" s="136" t="s">
         <v>1404</v>
       </c>
-      <c r="B12" s="136" t="s">
+      <c r="C12" s="137" t="s">
         <v>1405</v>
-      </c>
-      <c r="C12" s="137" t="s">
-        <v>1406</v>
       </c>
       <c r="D12" s="136"/>
       <c r="E12" s="138" t="s">
-        <v>1407</v>
+        <v>1406</v>
       </c>
       <c r="F12" s="135"/>
     </row>
@@ -16565,7 +16565,7 @@
         <v>1069</v>
       </c>
       <c r="C13" s="137" t="s">
-        <v>1402</v>
+        <v>1401</v>
       </c>
       <c r="D13" s="136" t="s">
         <v>1070</v>
@@ -16611,7 +16611,7 @@
         <v>1075</v>
       </c>
       <c r="C16" s="137" t="s">
-        <v>1399</v>
+        <v>1398</v>
       </c>
       <c r="D16" s="136" t="s">
         <v>1076</v>
@@ -16629,7 +16629,7 @@
         <v>1078</v>
       </c>
       <c r="C17" s="137" t="s">
-        <v>1400</v>
+        <v>1399</v>
       </c>
       <c r="D17" s="136" t="s">
         <v>1079</v>
@@ -16647,7 +16647,7 @@
         <v>1081</v>
       </c>
       <c r="C18" s="137" t="s">
-        <v>1401</v>
+        <v>1400</v>
       </c>
       <c r="D18" s="136" t="s">
         <v>1082</v>
@@ -16787,17 +16787,17 @@
     </row>
     <row r="28" spans="1:6" ht="64" x14ac:dyDescent="0.2">
       <c r="A28" s="136" t="s">
-        <v>1404</v>
+        <v>1403</v>
       </c>
       <c r="B28" s="136" t="s">
-        <v>1403</v>
+        <v>1402</v>
       </c>
       <c r="C28" s="137" t="s">
-        <v>1425</v>
+        <v>1424</v>
       </c>
       <c r="D28" s="136"/>
       <c r="E28" s="138" t="s">
-        <v>1427</v>
+        <v>1426</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="32" x14ac:dyDescent="0.2">
@@ -16808,13 +16808,13 @@
         <v>1107</v>
       </c>
       <c r="C29" s="137" t="s">
-        <v>1426</v>
+        <v>1425</v>
       </c>
       <c r="D29" s="136" t="s">
         <v>1108</v>
       </c>
       <c r="E29" s="138" t="s">
-        <v>1428</v>
+        <v>1427</v>
       </c>
     </row>
     <row r="30" spans="1:6" s="13" customFormat="1" x14ac:dyDescent="0.2">
@@ -17149,13 +17149,13 @@
         <v>1157</v>
       </c>
       <c r="C51" s="62" t="s">
-        <v>1383</v>
+        <v>1382</v>
       </c>
       <c r="D51" s="116" t="s">
         <v>1002</v>
       </c>
       <c r="E51" s="63" t="s">
-        <v>1384</v>
+        <v>1383</v>
       </c>
     </row>
     <row r="52" spans="1:6" s="30" customFormat="1" ht="48" x14ac:dyDescent="0.2">
@@ -17518,47 +17518,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Readyforteam_x003f_ xmlns="565e1b1d-057e-4d85-b896-01a5881d8a45">false</Readyforteam_x003f_>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <SharedWithUsers xmlns="bf601f31-63a1-4825-9216-91d773c5ef9c">
-      <UserInfo>
-        <DisplayName>Erika Osti</DisplayName>
-        <AccountId>534</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Penny Johnson</DisplayName>
-        <AccountId>489</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Ben Childs</DisplayName>
-        <AccountId>643</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Thomas Leeds</DisplayName>
-        <AccountId>459</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Kasmyn Chen</DisplayName>
-        <AccountId>532</AccountId>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="565e1b1d-057e-4d85-b896-01a5881d8a45">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="2799d30d-6731-4efe-ac9b-c4895a8828d9" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010096D84A54A9CD274097F17166F184737D" ma:contentTypeVersion="21" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="2fd95a4cfdf4f2f51219070f5dff16a8">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="565e1b1d-057e-4d85-b896-01a5881d8a45" xmlns:ns3="bf601f31-63a1-4825-9216-91d773c5ef9c" xmlns:ns4="2799d30d-6731-4efe-ac9b-c4895a8828d9" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f7499f6f4dc8ad2a533df04863f63fa7" ns1:_="" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -17835,6 +17794,47 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Readyforteam_x003f_ xmlns="565e1b1d-057e-4d85-b896-01a5881d8a45">false</Readyforteam_x003f_>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <SharedWithUsers xmlns="bf601f31-63a1-4825-9216-91d773c5ef9c">
+      <UserInfo>
+        <DisplayName>Erika Osti</DisplayName>
+        <AccountId>534</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Penny Johnson</DisplayName>
+        <AccountId>489</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Ben Childs</DisplayName>
+        <AccountId>643</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Thomas Leeds</DisplayName>
+        <AccountId>459</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Kasmyn Chen</DisplayName>
+        <AccountId>532</AccountId>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="565e1b1d-057e-4d85-b896-01a5881d8a45">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="2799d30d-6731-4efe-ac9b-c4895a8828d9" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8D7CE8C7-18DC-484F-8376-ED09F13D44C8}">
   <ds:schemaRefs>
@@ -17844,19 +17844,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{017ACE96-8143-486E-8436-7787F6B96F4A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="565e1b1d-057e-4d85-b896-01a5881d8a45"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="bf601f31-63a1-4825-9216-91d773c5ef9c"/>
-    <ds:schemaRef ds:uri="2799d30d-6731-4efe-ac9b-c4895a8828d9"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EAFDB110-4046-4E72-A1EF-1908ABEC3151}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -17875,4 +17862,17 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{017ACE96-8143-486E-8436-7787F6B96F4A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="565e1b1d-057e-4d85-b896-01a5881d8a45"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="bf601f31-63a1-4825-9216-91d773c5ef9c"/>
+    <ds:schemaRef ds:uri="2799d30d-6731-4efe-ac9b-c4895a8828d9"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
[MCCDB-1160] Points 4 and 5.
</commit_message>
<xml_diff>
--- a/app/data/MCCD-localisation.xlsx
+++ b/app/data/MCCD-localisation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/JALAT/GIT/medical-certificate-of-cause-of-death/app/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1026DC30-6F07-C342-94FA-48D3C54C531C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D60A09CE-34D7-E64C-8DAA-EC93ABB7BEA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="14020" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="14020" firstSheet="3" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Using this document" sheetId="8" r:id="rId1"/>
@@ -4097,12 +4097,6 @@
     <t>boxBCheckboxText</t>
   </si>
   <si>
-    <t>I may be in a position later to give, on application by the Registrar General, additional information as to the cause of death for the purpose of more precise statistical classification.</t>
-  </si>
-  <si>
-    <t>Efallai y byddaf mewn sefyllfa yn ddiweddarach i roi, ar gais y Cofrestrydd Cyffredinol, wybodaeth ychwanegol am yr achos marwolaeth at ddiben dosbarthiad ystadegol mwy manwl gywir.</t>
-  </si>
-  <si>
     <t>Referring medical practitioner (ME cert)</t>
   </si>
   <si>
@@ -5569,9 +5563,6 @@
     <t>1(d) Other disease or condition leading to 1(c) (optional)</t>
   </si>
   <si>
-    <t>1(a) Disease or condition directly leading to death</t>
-  </si>
-  <si>
     <t>codO28SectionTitleTwoDescription</t>
   </si>
   <si>
@@ -5650,12 +5641,6 @@
     <t>2 Amgylchiadau arwyddocaol eraill (dewisol)</t>
   </si>
   <si>
-    <t>I am a duly appointed medical examiner and following scrutiny I confirm that the cause of death is as stated in this certificate to the best of my knowledge and belief.</t>
-  </si>
-  <si>
-    <t>Rwy'n arholwr meddygol a benodwyd yn briodol ac ar ôl craffu rwy'n cadarnhau bod achos y farwolaeth fel y nodir yn y dystysgrif hon hyd eithaf fy ngwybodaeth a'm cred.</t>
-  </si>
-  <si>
     <t>&lt;p class="govuk-body"&gt;This dashboard allows you to create a new Medical certificate of cause of death (MCCD) and manage current MCCDs.&lt;/p&gt;&lt;p class="govuk-body"&gt;This dashboard will list MCCDs that:&lt;/p&gt;&lt;ul class="govuk-list govuk-list--bullet"&gt;&lt;li&gt;you have submitted to a medical examiner for approval&lt;/li&gt;&lt;li&gt;have been approved by a medical examiner&lt;/li&gt;&lt;li&gt;have been rejected by a medical examiner and need amending&lt;/li&gt;&lt;/ul&gt;&lt;p class="govuk-body"&gt;Completed MCCDs will be removed after three months.&lt;/p&gt;</t>
   </si>
   <si>
@@ -5779,7 +5764,22 @@
     <t>Dyma'r dyddiad y dywedwyd wrthyf fel yr arholwr meddygol</t>
   </si>
   <si>
-    <t>045</t>
+    <t>I may be in a position to give, on application by the Registrar General, additional information as to the cause of death for the purpose of more precise statistical classification.</t>
+  </si>
+  <si>
+    <t>Efallai fy mod mewn sefyllfa i roi, ar gais gan y Cofrestrydd Cyffredinol, wybodaeth ychwanegol ynghylch achos y farwolaeth at ddibenion dosbarthu ystadegol mwy manwl gywir.</t>
+  </si>
+  <si>
+    <t>1(a) Disease or condition leading directly to death</t>
+  </si>
+  <si>
+    <t>047</t>
+  </si>
+  <si>
+    <t>I am a duly appointed medical examiner and following scrutiny I confirm to the best of my knowledge and belief that the cause of death is as stated on the certificate.</t>
+  </si>
+  <si>
+    <t>Rwy'n arholwr meddygol a benodwyd yn briodol ac ar ôl craffu rwy'n cadarnhau hyd eithaf fy ngwybodaeth a'm cred bod achos y farwolaeth fel y nodir ar y dystysgrif.</t>
   </si>
 </sst>
 </file>
@@ -6762,6 +6762,24 @@
     <xf numFmtId="0" fontId="13" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -6769,24 +6787,6 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -7830,16 +7830,16 @@
         <v>239</v>
       </c>
       <c r="B2" s="5" t="s">
+        <v>1213</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>1214</v>
+      </c>
+      <c r="D2" s="5" t="s">
         <v>1215</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="F2" s="68" t="s">
         <v>1216</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>1217</v>
-      </c>
-      <c r="F2" s="68" t="s">
-        <v>1218</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="32" x14ac:dyDescent="0.2">
@@ -7847,13 +7847,13 @@
         <v>250</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>1219</v>
+        <v>1217</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>901</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>1220</v>
+        <v>1218</v>
       </c>
       <c r="E3" s="37" t="s">
         <v>902</v>
@@ -7864,13 +7864,13 @@
         <v>32</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>1221</v>
+        <v>1219</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>854</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>1222</v>
+        <v>1220</v>
       </c>
       <c r="E4" s="37" t="s">
         <v>856</v>
@@ -7878,36 +7878,36 @@
     </row>
     <row r="5" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
-        <v>1223</v>
+        <v>1221</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>1224</v>
+        <v>1222</v>
       </c>
       <c r="C5" s="6" t="s">
         <v>152</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>1225</v>
+        <v>1223</v>
       </c>
       <c r="F5" s="68" t="s">
-        <v>1218</v>
+        <v>1216</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
-        <v>1223</v>
+        <v>1221</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>1226</v>
+        <v>1224</v>
       </c>
       <c r="C6" s="6" t="s">
         <v>140</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>1225</v>
+        <v>1223</v>
       </c>
       <c r="F6" s="68" t="s">
-        <v>1218</v>
+        <v>1216</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="32" x14ac:dyDescent="0.2">
@@ -7915,13 +7915,13 @@
         <v>250</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>1227</v>
+        <v>1225</v>
       </c>
       <c r="C7" s="6" t="s">
         <v>904</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>1220</v>
+        <v>1218</v>
       </c>
       <c r="E7" s="37" t="s">
         <v>905</v>
@@ -7932,7 +7932,7 @@
         <v>32</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>1228</v>
+        <v>1226</v>
       </c>
       <c r="C8" s="6" t="s">
         <v>907</v>
@@ -7944,10 +7944,10 @@
     </row>
     <row r="9" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
-        <v>1223</v>
+        <v>1221</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="C9" s="6" t="s">
         <v>913</v>
@@ -7959,22 +7959,22 @@
     </row>
     <row r="10" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="C10" s="27" t="s">
+        <v>1228</v>
+      </c>
+      <c r="D10" s="18" t="s">
+        <v>1229</v>
+      </c>
+      <c r="E10" s="37" t="s">
         <v>1230</v>
-      </c>
-      <c r="D10" s="18" t="s">
-        <v>1231</v>
-      </c>
-      <c r="E10" s="37" t="s">
-        <v>1232</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="C11" s="74" t="s">
-        <v>1233</v>
+        <v>1231</v>
       </c>
       <c r="D11" s="18"/>
       <c r="E11" s="37" t="s">
-        <v>1234</v>
+        <v>1232</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
@@ -8010,9 +8010,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E52C375-4A34-4943-A40B-CD02CAD0761B}">
   <dimension ref="A1:F24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E23" sqref="E23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -8051,33 +8051,33 @@
         <v>239</v>
       </c>
       <c r="B2" s="92" t="s">
-        <v>1235</v>
+        <v>1233</v>
       </c>
       <c r="C2" s="151" t="s">
-        <v>1403</v>
+        <v>1400</v>
       </c>
       <c r="D2" s="92" t="s">
-        <v>1236</v>
+        <v>1234</v>
       </c>
       <c r="E2" s="152" t="s">
-        <v>1407</v>
+        <v>1404</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="80" x14ac:dyDescent="0.2">
       <c r="A3" s="94" t="s">
+        <v>1235</v>
+      </c>
+      <c r="B3" s="95" t="s">
+        <v>1236</v>
+      </c>
+      <c r="C3" s="96" t="s">
         <v>1237</v>
       </c>
-      <c r="B3" s="95" t="s">
+      <c r="D3" s="95" t="s">
         <v>1238</v>
       </c>
-      <c r="C3" s="96" t="s">
+      <c r="E3" s="89" t="s">
         <v>1239</v>
-      </c>
-      <c r="D3" s="95" t="s">
-        <v>1240</v>
-      </c>
-      <c r="E3" s="89" t="s">
-        <v>1241</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="16" x14ac:dyDescent="0.2">
@@ -8085,16 +8085,16 @@
         <v>749</v>
       </c>
       <c r="B4" s="95" t="s">
-        <v>1242</v>
+        <v>1240</v>
       </c>
       <c r="C4" s="158" t="s">
-        <v>1404</v>
+        <v>1401</v>
       </c>
       <c r="D4" s="95" t="s">
         <v>400</v>
       </c>
       <c r="E4" s="155" t="s">
-        <v>1406</v>
+        <v>1403</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="60.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -8102,13 +8102,13 @@
         <v>406</v>
       </c>
       <c r="B5" s="105" t="s">
-        <v>1243</v>
+        <v>1241</v>
       </c>
       <c r="C5" s="106" t="s">
         <v>400</v>
       </c>
       <c r="D5" s="107" t="s">
-        <v>1244</v>
+        <v>1242</v>
       </c>
       <c r="E5" s="89" t="s">
         <v>400</v>
@@ -8119,13 +8119,13 @@
         <v>409</v>
       </c>
       <c r="B6" s="105" t="s">
-        <v>1245</v>
+        <v>1243</v>
       </c>
       <c r="C6" s="106" t="s">
         <v>400</v>
       </c>
       <c r="D6" s="107" t="s">
-        <v>1246</v>
+        <v>1244</v>
       </c>
       <c r="E6" s="89" t="s">
         <v>400</v>
@@ -8153,33 +8153,33 @@
         <v>239</v>
       </c>
       <c r="B8" s="95" t="s">
-        <v>1247</v>
+        <v>1245</v>
       </c>
       <c r="C8" s="158" t="s">
-        <v>1403</v>
+        <v>1400</v>
       </c>
       <c r="D8" s="95" t="s">
-        <v>1248</v>
+        <v>1246</v>
       </c>
       <c r="E8" s="155" t="s">
-        <v>1407</v>
+        <v>1404</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="64" x14ac:dyDescent="0.2">
       <c r="A9" s="94" t="s">
-        <v>1237</v>
+        <v>1235</v>
       </c>
       <c r="B9" s="95" t="s">
+        <v>1247</v>
+      </c>
+      <c r="C9" s="96" t="s">
+        <v>1248</v>
+      </c>
+      <c r="D9" s="95" t="s">
         <v>1249</v>
       </c>
-      <c r="C9" s="96" t="s">
+      <c r="E9" s="89" t="s">
         <v>1250</v>
-      </c>
-      <c r="D9" s="95" t="s">
-        <v>1251</v>
-      </c>
-      <c r="E9" s="89" t="s">
-        <v>1252</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="16" x14ac:dyDescent="0.2">
@@ -8187,16 +8187,16 @@
         <v>749</v>
       </c>
       <c r="B10" s="95" t="s">
-        <v>1253</v>
+        <v>1251</v>
       </c>
       <c r="C10" s="158" t="s">
-        <v>1404</v>
+        <v>1401</v>
       </c>
       <c r="D10" s="95" t="s">
         <v>400</v>
       </c>
       <c r="E10" s="155" t="s">
-        <v>1406</v>
+        <v>1403</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -8204,13 +8204,13 @@
         <v>406</v>
       </c>
       <c r="B11" s="105" t="s">
-        <v>1254</v>
+        <v>1252</v>
       </c>
       <c r="C11" s="106" t="s">
         <v>400</v>
       </c>
       <c r="D11" s="107" t="s">
-        <v>1244</v>
+        <v>1242</v>
       </c>
       <c r="E11" s="89" t="s">
         <v>400</v>
@@ -8221,13 +8221,13 @@
         <v>409</v>
       </c>
       <c r="B12" s="105" t="s">
-        <v>1255</v>
+        <v>1253</v>
       </c>
       <c r="C12" s="106" t="s">
         <v>400</v>
       </c>
       <c r="D12" s="107" t="s">
-        <v>1246</v>
+        <v>1244</v>
       </c>
       <c r="E12" s="89" t="s">
         <v>400</v>
@@ -8255,33 +8255,33 @@
         <v>239</v>
       </c>
       <c r="B14" s="95" t="s">
-        <v>1256</v>
+        <v>1254</v>
       </c>
       <c r="C14" s="158" t="s">
-        <v>1403</v>
+        <v>1400</v>
       </c>
       <c r="D14" s="95" t="s">
-        <v>1257</v>
+        <v>1255</v>
       </c>
       <c r="E14" s="155" t="s">
-        <v>1405</v>
+        <v>1402</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="80" x14ac:dyDescent="0.2">
       <c r="A15" s="94" t="s">
-        <v>1237</v>
+        <v>1235</v>
       </c>
       <c r="B15" s="95" t="s">
-        <v>1258</v>
+        <v>1256</v>
       </c>
       <c r="C15" s="158" t="s">
-        <v>1423</v>
+        <v>1465</v>
       </c>
       <c r="D15" s="95" t="s">
-        <v>1259</v>
+        <v>1257</v>
       </c>
       <c r="E15" s="155" t="s">
-        <v>1424</v>
+        <v>1466</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="48" x14ac:dyDescent="0.2">
@@ -8289,13 +8289,13 @@
         <v>406</v>
       </c>
       <c r="B16" s="105" t="s">
-        <v>1260</v>
+        <v>1258</v>
       </c>
       <c r="C16" s="106" t="s">
         <v>400</v>
       </c>
       <c r="D16" s="107" t="s">
-        <v>1244</v>
+        <v>1242</v>
       </c>
       <c r="E16" s="89" t="s">
         <v>400</v>
@@ -8306,13 +8306,13 @@
         <v>409</v>
       </c>
       <c r="B17" s="105" t="s">
-        <v>1261</v>
+        <v>1259</v>
       </c>
       <c r="C17" s="106" t="s">
         <v>400</v>
       </c>
       <c r="D17" s="107" t="s">
-        <v>1246</v>
+        <v>1244</v>
       </c>
       <c r="E17" s="89" t="s">
         <v>400</v>
@@ -8323,16 +8323,16 @@
         <v>14</v>
       </c>
       <c r="B18" s="95" t="s">
-        <v>1262</v>
+        <v>1260</v>
       </c>
       <c r="C18" s="158" t="s">
-        <v>1404</v>
+        <v>1401</v>
       </c>
       <c r="D18" s="95" t="s">
         <v>400</v>
       </c>
       <c r="E18" s="155" t="s">
-        <v>1406</v>
+        <v>1403</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -8357,33 +8357,33 @@
         <v>239</v>
       </c>
       <c r="B20" s="95" t="s">
-        <v>1263</v>
+        <v>1261</v>
       </c>
       <c r="C20" s="158" t="s">
-        <v>1438</v>
+        <v>1433</v>
       </c>
       <c r="D20" s="95" t="s">
-        <v>1236</v>
+        <v>1234</v>
       </c>
       <c r="E20" s="155" t="s">
-        <v>1439</v>
+        <v>1434</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="64" x14ac:dyDescent="0.2">
       <c r="A21" s="94" t="s">
-        <v>1237</v>
+        <v>1235</v>
       </c>
       <c r="B21" s="95" t="s">
-        <v>1264</v>
+        <v>1262</v>
       </c>
       <c r="C21" s="158" t="s">
-        <v>1437</v>
+        <v>1432</v>
       </c>
       <c r="D21" s="95" t="s">
-        <v>1265</v>
+        <v>1263</v>
       </c>
       <c r="E21" s="155" t="s">
-        <v>1440</v>
+        <v>1435</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -8391,16 +8391,16 @@
         <v>749</v>
       </c>
       <c r="B22" s="95" t="s">
-        <v>1266</v>
+        <v>1264</v>
       </c>
       <c r="C22" s="158" t="s">
-        <v>1441</v>
+        <v>1436</v>
       </c>
       <c r="D22" s="95" t="s">
         <v>400</v>
       </c>
       <c r="E22" s="155" t="s">
-        <v>1442</v>
+        <v>1437</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="48" x14ac:dyDescent="0.2">
@@ -8408,13 +8408,13 @@
         <v>406</v>
       </c>
       <c r="B23" s="105" t="s">
-        <v>1267</v>
+        <v>1265</v>
       </c>
       <c r="C23" s="106" t="s">
         <v>400</v>
       </c>
       <c r="D23" s="107" t="s">
-        <v>1244</v>
+        <v>1242</v>
       </c>
       <c r="E23" s="89" t="s">
         <v>400</v>
@@ -8425,13 +8425,13 @@
         <v>409</v>
       </c>
       <c r="B24" s="105" t="s">
-        <v>1268</v>
+        <v>1266</v>
       </c>
       <c r="C24" s="106" t="s">
         <v>400</v>
       </c>
       <c r="D24" s="107" t="s">
-        <v>1246</v>
+        <v>1244</v>
       </c>
       <c r="E24" s="89" t="s">
         <v>400</v>
@@ -8484,7 +8484,7 @@
     </row>
     <row r="2" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="203" t="s">
-        <v>1269</v>
+        <v>1267</v>
       </c>
       <c r="B2" s="204"/>
       <c r="C2" s="204"/>
@@ -8497,16 +8497,16 @@
         <v>239</v>
       </c>
       <c r="B3" s="5" t="s">
+        <v>1268</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>1269</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>1215</v>
+      </c>
+      <c r="E3" s="37" t="s">
         <v>1270</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>1271</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>1217</v>
-      </c>
-      <c r="E3" s="37" t="s">
-        <v>1272</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="32" x14ac:dyDescent="0.2">
@@ -8514,13 +8514,13 @@
         <v>257</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>1273</v>
+        <v>1271</v>
       </c>
       <c r="C4" s="59" t="s">
-        <v>1428</v>
+        <v>1423</v>
       </c>
       <c r="E4" s="37" t="s">
-        <v>1274</v>
+        <v>1272</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="16" x14ac:dyDescent="0.2">
@@ -8528,13 +8528,13 @@
         <v>250</v>
       </c>
       <c r="B5" s="5" t="s">
+        <v>1273</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>1274</v>
+      </c>
+      <c r="E5" s="37" t="s">
         <v>1275</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>1276</v>
-      </c>
-      <c r="E5" s="37" t="s">
-        <v>1277</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="80" x14ac:dyDescent="0.2">
@@ -8542,13 +8542,13 @@
         <v>257</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>1278</v>
+        <v>1276</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>1426</v>
+        <v>1421</v>
       </c>
       <c r="E6" s="37" t="s">
-        <v>1427</v>
+        <v>1422</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="32" x14ac:dyDescent="0.2">
@@ -8556,112 +8556,112 @@
         <v>250</v>
       </c>
       <c r="B7" s="5" t="s">
+        <v>1277</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>1278</v>
+      </c>
+      <c r="E7" s="37" t="s">
         <v>1279</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>1280</v>
-      </c>
-      <c r="E7" s="37" t="s">
-        <v>1281</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
-        <v>1282</v>
+        <v>1280</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>1283</v>
+        <v>1281</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>1412</v>
+        <v>1409</v>
       </c>
       <c r="E8" s="37" t="s">
-        <v>1413</v>
+        <v>1410</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
+        <v>1282</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>1283</v>
+      </c>
+      <c r="C9" s="6" t="s">
         <v>1284</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="E9" s="37" t="s">
         <v>1285</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>1286</v>
-      </c>
-      <c r="E9" s="37" t="s">
-        <v>1287</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
-        <v>1284</v>
+        <v>1282</v>
       </c>
       <c r="B10" s="5" t="s">
+        <v>1286</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>1287</v>
+      </c>
+      <c r="E10" s="37" t="s">
         <v>1288</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>1289</v>
-      </c>
-      <c r="E10" s="37" t="s">
-        <v>1290</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
-        <v>1284</v>
+        <v>1282</v>
       </c>
       <c r="B11" s="5" t="s">
+        <v>1289</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>1290</v>
+      </c>
+      <c r="E11" s="37" t="s">
         <v>1291</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>1292</v>
-      </c>
-      <c r="E11" s="37" t="s">
-        <v>1293</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="5" t="s">
-        <v>1284</v>
+        <v>1282</v>
       </c>
       <c r="B12" s="5" t="s">
+        <v>1292</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>1293</v>
+      </c>
+      <c r="E12" s="37" t="s">
         <v>1294</v>
-      </c>
-      <c r="C12" s="6" t="s">
-        <v>1295</v>
-      </c>
-      <c r="E12" s="37" t="s">
-        <v>1296</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="s">
-        <v>1284</v>
+        <v>1282</v>
       </c>
       <c r="B13" s="5" t="s">
+        <v>1295</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>1296</v>
+      </c>
+      <c r="E13" s="37" t="s">
         <v>1297</v>
-      </c>
-      <c r="C13" s="6" t="s">
-        <v>1298</v>
-      </c>
-      <c r="E13" s="37" t="s">
-        <v>1299</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A14" s="5" t="s">
-        <v>1282</v>
+        <v>1280</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>1300</v>
+        <v>1298</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>1410</v>
+        <v>1407</v>
       </c>
       <c r="D14" s="1"/>
       <c r="E14" s="37" t="s">
-        <v>1411</v>
+        <v>1408</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="32" x14ac:dyDescent="0.2">
@@ -8669,14 +8669,14 @@
         <v>943</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>1301</v>
+        <v>1299</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>1302</v>
+        <v>1300</v>
       </c>
       <c r="D15" s="1"/>
       <c r="E15" s="37" t="s">
-        <v>1303</v>
+        <v>1301</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="16" x14ac:dyDescent="0.2">
@@ -8684,34 +8684,34 @@
         <v>14</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>1304</v>
+        <v>1302</v>
       </c>
       <c r="C16" s="74" t="s">
-        <v>1305</v>
+        <v>1303</v>
       </c>
       <c r="D16" s="18"/>
       <c r="E16" s="37" t="s">
-        <v>1306</v>
+        <v>1304</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A17" s="5" t="s">
+        <v>1305</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>1306</v>
+      </c>
+      <c r="C17" s="75" t="s">
         <v>1307</v>
-      </c>
-      <c r="B17" s="7" t="s">
-        <v>1308</v>
-      </c>
-      <c r="C17" s="75" t="s">
-        <v>1309</v>
       </c>
       <c r="D17" s="18"/>
       <c r="E17" s="37" t="s">
-        <v>1310</v>
+        <v>1308</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="203" t="s">
-        <v>1311</v>
+        <v>1309</v>
       </c>
       <c r="B18" s="204"/>
       <c r="C18" s="204"/>
@@ -8724,16 +8724,16 @@
         <v>239</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>1314</v>
+        <v>1312</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>1312</v>
+        <v>1310</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>1217</v>
+        <v>1215</v>
       </c>
       <c r="E19" s="37" t="s">
-        <v>1313</v>
+        <v>1311</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="96" x14ac:dyDescent="0.2">
@@ -8741,13 +8741,13 @@
         <v>257</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>1315</v>
+        <v>1313</v>
       </c>
       <c r="C20" s="59" t="s">
+        <v>1378</v>
+      </c>
+      <c r="E20" s="37" t="s">
         <v>1380</v>
-      </c>
-      <c r="E20" s="37" t="s">
-        <v>1382</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="16" x14ac:dyDescent="0.2">
@@ -8755,13 +8755,13 @@
         <v>250</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>1316</v>
+        <v>1314</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>1276</v>
+        <v>1274</v>
       </c>
       <c r="E21" s="37" t="s">
-        <v>1277</v>
+        <v>1275</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="80" x14ac:dyDescent="0.2">
@@ -8769,13 +8769,13 @@
         <v>257</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>1317</v>
+        <v>1315</v>
       </c>
       <c r="C22" s="6" t="s">
+        <v>1379</v>
+      </c>
+      <c r="E22" s="37" t="s">
         <v>1381</v>
-      </c>
-      <c r="E22" s="37" t="s">
-        <v>1383</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
@@ -8797,9 +8797,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F71"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F3" sqref="F3"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -8839,13 +8839,13 @@
         <v>7</v>
       </c>
       <c r="C2" s="100" t="s">
-        <v>1466</v>
+        <v>1464</v>
       </c>
       <c r="D2" s="98" t="s">
         <v>8</v>
       </c>
       <c r="E2" s="99" t="s">
-        <v>1466</v>
+        <v>1464</v>
       </c>
       <c r="F2" s="98"/>
     </row>
@@ -8863,7 +8863,7 @@
         <v>12</v>
       </c>
       <c r="E3" s="37" t="s">
-        <v>1379</v>
+        <v>1377</v>
       </c>
       <c r="F3" s="5" t="s">
         <v>13</v>
@@ -9714,10 +9714,10 @@
     <row r="52" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A52" s="86"/>
       <c r="B52" s="163" t="s">
-        <v>1429</v>
+        <v>1424</v>
       </c>
       <c r="C52" s="164" t="s">
-        <v>1430</v>
+        <v>1425</v>
       </c>
       <c r="D52" s="86"/>
       <c r="E52" s="165" t="s">
@@ -9833,7 +9833,7 @@
       </c>
       <c r="D60" s="86"/>
       <c r="E60" s="165" t="s">
-        <v>1445</v>
+        <v>1440</v>
       </c>
       <c r="F60" s="86"/>
     </row>
@@ -9920,46 +9920,46 @@
     <row r="67" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A67" s="86"/>
       <c r="B67" s="163" t="s">
-        <v>1433</v>
+        <v>1428</v>
       </c>
       <c r="C67" s="164" t="s">
-        <v>1434</v>
+        <v>1429</v>
       </c>
       <c r="D67" s="86"/>
       <c r="E67" s="165" t="s">
-        <v>1435</v>
+        <v>1430</v>
       </c>
       <c r="F67" s="166" t="s">
-        <v>1436</v>
+        <v>1431</v>
       </c>
     </row>
     <row r="68" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A68" s="86"/>
       <c r="B68" s="163" t="s">
-        <v>1431</v>
+        <v>1426</v>
       </c>
       <c r="C68" s="164" t="s">
-        <v>1309</v>
+        <v>1307</v>
       </c>
       <c r="D68" s="86"/>
       <c r="E68" s="165" t="s">
-        <v>1432</v>
+        <v>1427</v>
       </c>
     </row>
     <row r="69" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="B69" s="1" t="s">
-        <v>1328</v>
+        <v>1326</v>
       </c>
       <c r="C69" s="2" t="s">
+        <v>1327</v>
+      </c>
+      <c r="E69" s="40" t="s">
         <v>1329</v>
-      </c>
-      <c r="E69" s="40" t="s">
-        <v>1331</v>
       </c>
     </row>
     <row r="70" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="B70" s="1" t="s">
-        <v>1330</v>
+        <v>1328</v>
       </c>
       <c r="C70" s="2" t="s">
         <v>76</v>
@@ -9970,13 +9970,13 @@
     </row>
     <row r="71" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="B71" s="1" t="s">
-        <v>1446</v>
+        <v>1441</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>1447</v>
+        <v>1442</v>
       </c>
       <c r="E71" s="40" t="s">
-        <v>1448</v>
+        <v>1443</v>
       </c>
     </row>
   </sheetData>
@@ -10271,14 +10271,14 @@
         <v>239</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>1353</v>
+        <v>1351</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>1354</v>
+        <v>1352</v>
       </c>
       <c r="D2" s="5"/>
       <c r="E2" s="43" t="s">
-        <v>1362</v>
+        <v>1360</v>
       </c>
       <c r="F2" s="1"/>
     </row>
@@ -10287,19 +10287,19 @@
         <v>480</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>1355</v>
+        <v>1353</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>1356</v>
+        <v>1354</v>
       </c>
       <c r="D3" s="5"/>
       <c r="E3" s="43" t="s">
-        <v>1363</v>
+        <v>1361</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="169" t="s">
-        <v>1357</v>
+        <v>1355</v>
       </c>
       <c r="B4" s="170"/>
       <c r="C4" s="170"/>
@@ -10311,14 +10311,14 @@
         <v>239</v>
       </c>
       <c r="B5" s="5" t="s">
+        <v>1356</v>
+      </c>
+      <c r="C5" s="6" t="s">
         <v>1358</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>1360</v>
       </c>
       <c r="D5" s="5"/>
       <c r="E5" s="43" t="s">
-        <v>1364</v>
+        <v>1362</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="96" x14ac:dyDescent="0.2">
@@ -10326,14 +10326,14 @@
         <v>480</v>
       </c>
       <c r="B6" s="5" t="s">
+        <v>1357</v>
+      </c>
+      <c r="C6" s="6" t="s">
         <v>1359</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>1361</v>
       </c>
       <c r="D6" s="5"/>
       <c r="E6" s="43" t="s">
-        <v>1365</v>
+        <v>1363</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
@@ -10554,7 +10554,7 @@
         <v>239</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>1368</v>
+        <v>1366</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>272</v>
@@ -10578,7 +10578,7 @@
         <v>242</v>
       </c>
       <c r="E4" s="43" t="s">
-        <v>1369</v>
+        <v>1367</v>
       </c>
       <c r="F4" s="68" t="s">
         <v>276</v>
@@ -10592,13 +10592,13 @@
         <v>277</v>
       </c>
       <c r="C5" s="52" t="s">
-        <v>1425</v>
+        <v>1420</v>
       </c>
       <c r="D5" s="66" t="s">
         <v>278</v>
       </c>
       <c r="E5" s="156" t="s">
-        <v>1443</v>
+        <v>1438</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>279</v>
@@ -10612,13 +10612,13 @@
         <v>280</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>1374</v>
+        <v>1372</v>
       </c>
       <c r="D6" s="67" t="s">
         <v>281</v>
       </c>
       <c r="E6" s="157" t="s">
-        <v>1444</v>
+        <v>1439</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="160" x14ac:dyDescent="0.2">
@@ -10629,13 +10629,13 @@
         <v>282</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>1375</v>
+        <v>1373</v>
       </c>
       <c r="D7" s="67" t="s">
         <v>283</v>
       </c>
       <c r="E7" s="157" t="s">
-        <v>1376</v>
+        <v>1374</v>
       </c>
       <c r="F7" s="68" t="s">
         <v>284</v>
@@ -10837,7 +10837,7 @@
         <v>332</v>
       </c>
       <c r="C19" s="64" t="s">
-        <v>1366</v>
+        <v>1364</v>
       </c>
       <c r="D19" s="7" t="s">
         <v>333</v>
@@ -10971,17 +10971,17 @@
     </row>
     <row r="27" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A27" s="5" t="s">
-        <v>1372</v>
+        <v>1370</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>1373</v>
+        <v>1371</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>1370</v>
+        <v>1368</v>
       </c>
       <c r="D27" s="5"/>
       <c r="E27" s="37" t="s">
-        <v>1371</v>
+        <v>1369</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
@@ -11058,13 +11058,13 @@
       </c>
     </row>
     <row r="2" spans="1:6" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="175" t="s">
+      <c r="A2" s="172" t="s">
         <v>363</v>
       </c>
-      <c r="B2" s="176"/>
-      <c r="C2" s="176"/>
-      <c r="D2" s="176"/>
-      <c r="E2" s="177"/>
+      <c r="B2" s="173"/>
+      <c r="C2" s="173"/>
+      <c r="D2" s="173"/>
+      <c r="E2" s="174"/>
       <c r="F2" s="33"/>
     </row>
     <row r="3" spans="1:6" ht="48" x14ac:dyDescent="0.2">
@@ -11192,13 +11192,13 @@
       <c r="F9" s="119"/>
     </row>
     <row r="10" spans="1:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="178" t="s">
+      <c r="A10" s="175" t="s">
         <v>392</v>
       </c>
-      <c r="B10" s="179"/>
-      <c r="C10" s="179"/>
-      <c r="D10" s="179"/>
-      <c r="E10" s="180"/>
+      <c r="B10" s="176"/>
+      <c r="C10" s="176"/>
+      <c r="D10" s="176"/>
+      <c r="E10" s="177"/>
       <c r="F10" s="119"/>
     </row>
     <row r="11" spans="1:6" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -11227,13 +11227,13 @@
         <v>397</v>
       </c>
       <c r="C12" s="153" t="s">
-        <v>1332</v>
+        <v>1330</v>
       </c>
       <c r="D12" s="84" t="s">
         <v>398</v>
       </c>
       <c r="E12" s="152" t="s">
-        <v>1333</v>
+        <v>1331</v>
       </c>
       <c r="F12" s="86"/>
     </row>
@@ -11245,13 +11245,13 @@
         <v>399</v>
       </c>
       <c r="C13" s="154" t="s">
-        <v>1334</v>
+        <v>1332</v>
       </c>
       <c r="D13" s="88" t="s">
         <v>400</v>
       </c>
       <c r="E13" s="155" t="s">
-        <v>1335</v>
+        <v>1333</v>
       </c>
       <c r="F13" s="86"/>
     </row>
@@ -11716,14 +11716,14 @@
         <v>480</v>
       </c>
       <c r="B45" s="116" t="s">
-        <v>1352</v>
+        <v>1350</v>
       </c>
       <c r="C45" s="59" t="s">
-        <v>1451</v>
+        <v>1446</v>
       </c>
       <c r="D45" s="116"/>
       <c r="E45" s="120" t="s">
-        <v>1452</v>
+        <v>1447</v>
       </c>
       <c r="F45" s="119"/>
     </row>
@@ -11732,10 +11732,10 @@
         <v>480</v>
       </c>
       <c r="B46" s="116" t="s">
-        <v>1450</v>
+        <v>1445</v>
       </c>
       <c r="C46" s="59" t="s">
-        <v>1351</v>
+        <v>1349</v>
       </c>
       <c r="D46" s="116"/>
       <c r="E46" s="120" t="s">
@@ -11751,11 +11751,11 @@
         <v>481</v>
       </c>
       <c r="C47" s="59" t="s">
-        <v>1449</v>
+        <v>1444</v>
       </c>
       <c r="D47" s="116"/>
       <c r="E47" s="120" t="s">
-        <v>1455</v>
+        <v>1450</v>
       </c>
       <c r="F47" s="119"/>
     </row>
@@ -11959,13 +11959,13 @@
         <v>511</v>
       </c>
       <c r="C61" s="117" t="s">
-        <v>1453</v>
+        <v>1448</v>
       </c>
       <c r="D61" s="116" t="s">
         <v>512</v>
       </c>
       <c r="E61" s="120" t="s">
-        <v>1454</v>
+        <v>1449</v>
       </c>
       <c r="F61" s="119"/>
     </row>
@@ -11983,7 +11983,7 @@
         <v>516</v>
       </c>
       <c r="E62" s="120" t="s">
-        <v>1344</v>
+        <v>1342</v>
       </c>
       <c r="F62" s="119"/>
     </row>
@@ -11992,14 +11992,14 @@
         <v>513</v>
       </c>
       <c r="B63" s="116" t="s">
+        <v>1339</v>
+      </c>
+      <c r="C63" s="117" t="s">
         <v>1341</v>
-      </c>
-      <c r="C63" s="117" t="s">
-        <v>1343</v>
       </c>
       <c r="D63" s="116"/>
       <c r="E63" s="120" t="s">
-        <v>1342</v>
+        <v>1340</v>
       </c>
       <c r="F63" s="119"/>
     </row>
@@ -12092,14 +12092,14 @@
         <v>480</v>
       </c>
       <c r="B70" s="125" t="s">
-        <v>1456</v>
+        <v>1451</v>
       </c>
       <c r="C70" s="167" t="s">
-        <v>1457</v>
+        <v>1452</v>
       </c>
       <c r="D70" s="125"/>
       <c r="E70" s="131" t="s">
-        <v>1458</v>
+        <v>1453</v>
       </c>
       <c r="F70" s="119"/>
     </row>
@@ -12349,11 +12349,11 @@
         <v>566</v>
       </c>
       <c r="C86" s="117" t="s">
-        <v>1391</v>
+        <v>1389</v>
       </c>
       <c r="D86" s="116"/>
       <c r="E86" s="120" t="s">
-        <v>1392</v>
+        <v>1390</v>
       </c>
       <c r="F86" s="119" t="s">
         <v>567</v>
@@ -12463,11 +12463,11 @@
         <v>585</v>
       </c>
       <c r="C93" s="117" t="s">
-        <v>1389</v>
+        <v>1387</v>
       </c>
       <c r="D93" s="116"/>
       <c r="E93" s="120" t="s">
-        <v>1390</v>
+        <v>1388</v>
       </c>
       <c r="F93" s="119"/>
     </row>
@@ -12507,11 +12507,11 @@
         <v>591</v>
       </c>
       <c r="C96" s="117" t="s">
-        <v>1408</v>
+        <v>1405</v>
       </c>
       <c r="D96" s="116"/>
       <c r="E96" s="120" t="s">
-        <v>1409</v>
+        <v>1406</v>
       </c>
       <c r="F96" s="119" t="s">
         <v>567</v>
@@ -12531,7 +12531,7 @@
         <v>400</v>
       </c>
       <c r="E97" s="152" t="s">
-        <v>1212</v>
+        <v>1210</v>
       </c>
       <c r="F97" s="86" t="s">
         <v>594</v>
@@ -12542,7 +12542,7 @@
         <v>84</v>
       </c>
       <c r="B98" s="159" t="s">
-        <v>1414</v>
+        <v>1411</v>
       </c>
       <c r="C98" s="93" t="s">
         <v>593</v>
@@ -12551,7 +12551,7 @@
         <v>400</v>
       </c>
       <c r="E98" s="152" t="s">
-        <v>1212</v>
+        <v>1210</v>
       </c>
       <c r="F98" s="86"/>
     </row>
@@ -12560,7 +12560,7 @@
         <v>84</v>
       </c>
       <c r="B99" s="159" t="s">
-        <v>1415</v>
+        <v>1412</v>
       </c>
       <c r="C99" s="93" t="s">
         <v>593</v>
@@ -12569,7 +12569,7 @@
         <v>400</v>
       </c>
       <c r="E99" s="152" t="s">
-        <v>1212</v>
+        <v>1210</v>
       </c>
       <c r="F99" s="86"/>
     </row>
@@ -12578,14 +12578,14 @@
         <v>84</v>
       </c>
       <c r="B100" s="160" t="s">
-        <v>1416</v>
+        <v>1413</v>
       </c>
       <c r="C100" s="161" t="s">
         <v>593</v>
       </c>
       <c r="D100" s="160"/>
       <c r="E100" s="162" t="s">
-        <v>1212</v>
+        <v>1210</v>
       </c>
       <c r="F100" s="86"/>
     </row>
@@ -12594,14 +12594,14 @@
         <v>84</v>
       </c>
       <c r="B101" s="160" t="s">
-        <v>1417</v>
+        <v>1414</v>
       </c>
       <c r="C101" s="161" t="s">
         <v>593</v>
       </c>
       <c r="D101" s="160"/>
       <c r="E101" s="162" t="s">
-        <v>1212</v>
+        <v>1210</v>
       </c>
       <c r="F101" s="86"/>
     </row>
@@ -12610,14 +12610,14 @@
         <v>84</v>
       </c>
       <c r="B102" s="160" t="s">
-        <v>1418</v>
+        <v>1415</v>
       </c>
       <c r="C102" s="161" t="s">
         <v>593</v>
       </c>
       <c r="D102" s="160"/>
       <c r="E102" s="162" t="s">
-        <v>1212</v>
+        <v>1210</v>
       </c>
       <c r="F102" s="86"/>
     </row>
@@ -13057,33 +13057,33 @@
     </row>
     <row r="132" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A132" s="116" t="s">
-        <v>1459</v>
+        <v>1454</v>
       </c>
       <c r="B132" s="116" t="s">
-        <v>1461</v>
+        <v>1456</v>
       </c>
       <c r="C132" s="117" t="s">
-        <v>1460</v>
+        <v>1455</v>
       </c>
       <c r="D132" s="116"/>
       <c r="E132" s="120" t="s">
-        <v>1464</v>
+        <v>1459</v>
       </c>
       <c r="F132" s="119"/>
     </row>
     <row r="133" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A133" s="116" t="s">
-        <v>1459</v>
+        <v>1454</v>
       </c>
       <c r="B133" s="116" t="s">
-        <v>1463</v>
+        <v>1458</v>
       </c>
       <c r="C133" s="117" t="s">
-        <v>1462</v>
+        <v>1457</v>
       </c>
       <c r="D133" s="116"/>
       <c r="E133" s="120" t="s">
-        <v>1465</v>
+        <v>1460</v>
       </c>
       <c r="F133" s="119"/>
     </row>
@@ -13317,7 +13317,7 @@
         <v>701</v>
       </c>
       <c r="C150" s="113" t="s">
-        <v>1319</v>
+        <v>1317</v>
       </c>
       <c r="D150" s="122" t="s">
         <v>702</v>
@@ -13407,7 +13407,7 @@
         <v>716</v>
       </c>
       <c r="C156" s="59" t="s">
-        <v>1318</v>
+        <v>1316</v>
       </c>
       <c r="D156" s="116" t="s">
         <v>717</v>
@@ -13438,14 +13438,14 @@
         <v>37</v>
       </c>
       <c r="B158" s="116" t="s">
+        <v>1318</v>
+      </c>
+      <c r="C158" s="59" t="s">
         <v>1320</v>
-      </c>
-      <c r="C158" s="59" t="s">
-        <v>1322</v>
       </c>
       <c r="D158" s="116"/>
       <c r="E158" s="120" t="s">
-        <v>1324</v>
+        <v>1322</v>
       </c>
       <c r="F158" s="119"/>
     </row>
@@ -13454,14 +13454,14 @@
         <v>37</v>
       </c>
       <c r="B159" s="116" t="s">
+        <v>1319</v>
+      </c>
+      <c r="C159" s="59" t="s">
         <v>1321</v>
-      </c>
-      <c r="C159" s="59" t="s">
-        <v>1323</v>
       </c>
       <c r="D159" s="116"/>
       <c r="E159" s="120" t="s">
-        <v>1325</v>
+        <v>1323</v>
       </c>
       <c r="F159" s="119"/>
     </row>
@@ -13680,13 +13680,13 @@
       <c r="F173" s="119"/>
     </row>
     <row r="174" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A174" s="172" t="s">
+      <c r="A174" s="178" t="s">
         <v>756</v>
       </c>
-      <c r="B174" s="173"/>
-      <c r="C174" s="173"/>
-      <c r="D174" s="173"/>
-      <c r="E174" s="174"/>
+      <c r="B174" s="179"/>
+      <c r="C174" s="179"/>
+      <c r="D174" s="179"/>
+      <c r="E174" s="180"/>
       <c r="F174" s="129" t="s">
         <v>757</v>
       </c>
@@ -14113,13 +14113,13 @@
         <v>806</v>
       </c>
       <c r="C202" s="59" t="s">
-        <v>1336</v>
+        <v>1334</v>
       </c>
       <c r="D202" s="116" t="s">
         <v>807</v>
       </c>
       <c r="E202" s="120" t="s">
-        <v>1340</v>
+        <v>1338</v>
       </c>
       <c r="F202" s="119"/>
     </row>
@@ -14128,14 +14128,14 @@
         <v>480</v>
       </c>
       <c r="B203" s="116" t="s">
-        <v>1337</v>
+        <v>1335</v>
       </c>
       <c r="C203" s="59" t="s">
-        <v>1338</v>
+        <v>1336</v>
       </c>
       <c r="D203" s="116"/>
       <c r="E203" s="120" t="s">
-        <v>1339</v>
+        <v>1337</v>
       </c>
       <c r="F203" s="119"/>
     </row>
@@ -14235,11 +14235,11 @@
         <v>818</v>
       </c>
       <c r="C210" s="117" t="s">
-        <v>1347</v>
+        <v>1345</v>
       </c>
       <c r="D210" s="116"/>
       <c r="E210" s="120" t="s">
-        <v>1350</v>
+        <v>1348</v>
       </c>
       <c r="F210" s="119"/>
     </row>
@@ -14248,7 +14248,7 @@
         <v>725</v>
       </c>
       <c r="B211" s="116" t="s">
-        <v>1349</v>
+        <v>1347</v>
       </c>
       <c r="C211" s="117" t="s">
         <v>43</v>
@@ -14264,14 +14264,14 @@
         <v>32</v>
       </c>
       <c r="B212" s="116" t="s">
-        <v>1348</v>
+        <v>1346</v>
       </c>
       <c r="C212" s="134" t="s">
-        <v>1345</v>
+        <v>1343</v>
       </c>
       <c r="D212" s="116"/>
       <c r="E212" s="120" t="s">
-        <v>1346</v>
+        <v>1344</v>
       </c>
       <c r="F212" s="119"/>
     </row>
@@ -14643,13 +14643,13 @@
         <v>857</v>
       </c>
       <c r="C237" s="59" t="s">
-        <v>1377</v>
+        <v>1375</v>
       </c>
       <c r="D237" s="116" t="s">
         <v>858</v>
       </c>
       <c r="E237" s="120" t="s">
-        <v>1378</v>
+        <v>1376</v>
       </c>
       <c r="F237" s="119"/>
     </row>
@@ -15589,18 +15589,6 @@
     </row>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="A234:E234"/>
-    <mergeCell ref="A195:E195"/>
-    <mergeCell ref="A199:E199"/>
-    <mergeCell ref="A206:E206"/>
-    <mergeCell ref="A217:E217"/>
-    <mergeCell ref="A223:E223"/>
-    <mergeCell ref="A59:E59"/>
-    <mergeCell ref="A2:E2"/>
-    <mergeCell ref="A10:E10"/>
-    <mergeCell ref="A14:E14"/>
-    <mergeCell ref="A24:E24"/>
-    <mergeCell ref="A43:E43"/>
     <mergeCell ref="A183:E183"/>
     <mergeCell ref="A166:E166"/>
     <mergeCell ref="A64:E64"/>
@@ -15611,6 +15599,18 @@
     <mergeCell ref="A155:E155"/>
     <mergeCell ref="A94:E94"/>
     <mergeCell ref="A174:E174"/>
+    <mergeCell ref="A59:E59"/>
+    <mergeCell ref="A2:E2"/>
+    <mergeCell ref="A10:E10"/>
+    <mergeCell ref="A14:E14"/>
+    <mergeCell ref="A24:E24"/>
+    <mergeCell ref="A43:E43"/>
+    <mergeCell ref="A234:E234"/>
+    <mergeCell ref="A195:E195"/>
+    <mergeCell ref="A199:E199"/>
+    <mergeCell ref="A206:E206"/>
+    <mergeCell ref="A217:E217"/>
+    <mergeCell ref="A223:E223"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -15621,8 +15621,8 @@
   <dimension ref="A1:F55"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A31" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D33" sqref="D33"/>
+      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -15881,13 +15881,13 @@
         <v>933</v>
       </c>
       <c r="C17" s="151" t="s">
-        <v>1326</v>
+        <v>1324</v>
       </c>
       <c r="D17" s="92" t="s">
         <v>925</v>
       </c>
       <c r="E17" s="152" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="80" x14ac:dyDescent="0.2">
@@ -15961,16 +15961,16 @@
         <v>948</v>
       </c>
       <c r="C23" s="82" t="s">
-        <v>949</v>
+        <v>1461</v>
       </c>
       <c r="D23" s="80"/>
       <c r="E23" s="81" t="s">
-        <v>950</v>
+        <v>1462</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" s="190" t="s">
-        <v>951</v>
+        <v>949</v>
       </c>
       <c r="B24" s="191"/>
       <c r="C24" s="191"/>
@@ -15982,19 +15982,19 @@
         <v>239</v>
       </c>
       <c r="B25" s="28" t="s">
-        <v>952</v>
+        <v>950</v>
       </c>
       <c r="C25" s="27" t="s">
-        <v>953</v>
+        <v>951</v>
       </c>
       <c r="D25" s="18"/>
       <c r="E25" s="46" t="s">
-        <v>954</v>
+        <v>952</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" s="181" t="s">
-        <v>955</v>
+        <v>953</v>
       </c>
       <c r="B26" s="182"/>
       <c r="C26" s="182"/>
@@ -16006,19 +16006,19 @@
         <v>239</v>
       </c>
       <c r="B27" s="28" t="s">
-        <v>956</v>
+        <v>954</v>
       </c>
       <c r="C27" s="27" t="s">
-        <v>957</v>
+        <v>955</v>
       </c>
       <c r="D27" s="18"/>
       <c r="E27" s="46" t="s">
-        <v>958</v>
+        <v>956</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" s="181" t="s">
-        <v>959</v>
+        <v>957</v>
       </c>
       <c r="B28" s="182"/>
       <c r="C28" s="182"/>
@@ -16030,19 +16030,19 @@
         <v>239</v>
       </c>
       <c r="B29" s="92" t="s">
+        <v>958</v>
+      </c>
+      <c r="C29" s="93" t="s">
+        <v>959</v>
+      </c>
+      <c r="D29" s="92" t="s">
         <v>960</v>
       </c>
-      <c r="C29" s="93" t="s">
+      <c r="E29" s="85" t="s">
         <v>961</v>
       </c>
-      <c r="D29" s="92" t="s">
+      <c r="F29" s="71" t="s">
         <v>962</v>
-      </c>
-      <c r="E29" s="85" t="s">
-        <v>963</v>
-      </c>
-      <c r="F29" s="71" t="s">
-        <v>964</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="48" x14ac:dyDescent="0.2">
@@ -16050,33 +16050,33 @@
         <v>943</v>
       </c>
       <c r="B30" s="95" t="s">
+        <v>963</v>
+      </c>
+      <c r="C30" s="96" t="s">
+        <v>964</v>
+      </c>
+      <c r="D30" s="95" t="s">
         <v>965</v>
       </c>
-      <c r="C30" s="96" t="s">
+      <c r="E30" s="89" t="s">
         <v>966</v>
-      </c>
-      <c r="D30" s="95" t="s">
-        <v>967</v>
-      </c>
-      <c r="E30" s="89" t="s">
-        <v>968</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="335" x14ac:dyDescent="0.2">
       <c r="A31" s="94" t="s">
+        <v>967</v>
+      </c>
+      <c r="B31" s="95" t="s">
+        <v>968</v>
+      </c>
+      <c r="C31" s="96" t="s">
         <v>969</v>
-      </c>
-      <c r="B31" s="95" t="s">
-        <v>970</v>
-      </c>
-      <c r="C31" s="96" t="s">
-        <v>971</v>
       </c>
       <c r="D31" s="95" t="s">
         <v>400</v>
       </c>
       <c r="E31" s="89" t="s">
-        <v>972</v>
+        <v>970</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="80" x14ac:dyDescent="0.2">
@@ -16084,13 +16084,13 @@
         <v>257</v>
       </c>
       <c r="B32" s="19" t="s">
-        <v>973</v>
+        <v>971</v>
       </c>
       <c r="C32" s="21" t="s">
-        <v>1384</v>
+        <v>1382</v>
       </c>
       <c r="E32" s="46" t="s">
-        <v>1385</v>
+        <v>1383</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="32" x14ac:dyDescent="0.2">
@@ -16098,13 +16098,13 @@
         <v>257</v>
       </c>
       <c r="B33" s="19" t="s">
+        <v>1384</v>
+      </c>
+      <c r="C33" s="21" t="s">
+        <v>1385</v>
+      </c>
+      <c r="E33" s="46" t="s">
         <v>1386</v>
-      </c>
-      <c r="C33" s="21" t="s">
-        <v>1387</v>
-      </c>
-      <c r="E33" s="46" t="s">
-        <v>1388</v>
       </c>
     </row>
     <row r="34" spans="1:6" ht="48" x14ac:dyDescent="0.2">
@@ -16112,16 +16112,16 @@
         <v>37</v>
       </c>
       <c r="B34" s="19" t="s">
+        <v>972</v>
+      </c>
+      <c r="C34" s="21" t="s">
+        <v>973</v>
+      </c>
+      <c r="D34" s="26" t="s">
         <v>974</v>
       </c>
-      <c r="C34" s="21" t="s">
+      <c r="E34" s="46" t="s">
         <v>975</v>
-      </c>
-      <c r="D34" s="26" t="s">
-        <v>976</v>
-      </c>
-      <c r="E34" s="46" t="s">
-        <v>977</v>
       </c>
     </row>
     <row r="35" spans="1:6" ht="96" x14ac:dyDescent="0.2">
@@ -16129,11 +16129,11 @@
         <v>406</v>
       </c>
       <c r="B35" s="28" t="s">
-        <v>978</v>
+        <v>976</v>
       </c>
       <c r="C35" s="27"/>
       <c r="D35" s="18" t="s">
-        <v>979</v>
+        <v>977</v>
       </c>
     </row>
     <row r="36" spans="1:6" ht="80" x14ac:dyDescent="0.2">
@@ -16141,11 +16141,11 @@
         <v>406</v>
       </c>
       <c r="B36" s="28" t="s">
-        <v>980</v>
+        <v>978</v>
       </c>
       <c r="C36" s="27"/>
       <c r="D36" s="18" t="s">
-        <v>981</v>
+        <v>979</v>
       </c>
     </row>
     <row r="37" spans="1:6" ht="80" x14ac:dyDescent="0.2">
@@ -16153,16 +16153,16 @@
         <v>409</v>
       </c>
       <c r="B37" s="28" t="s">
-        <v>982</v>
+        <v>980</v>
       </c>
       <c r="C37" s="27"/>
       <c r="D37" s="18" t="s">
-        <v>983</v>
+        <v>981</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" s="181" t="s">
-        <v>984</v>
+        <v>982</v>
       </c>
       <c r="B38" s="182"/>
       <c r="C38" s="182"/>
@@ -16174,16 +16174,16 @@
         <v>239</v>
       </c>
       <c r="B39" s="19" t="s">
+        <v>983</v>
+      </c>
+      <c r="C39" s="21" t="s">
+        <v>984</v>
+      </c>
+      <c r="D39" s="5" t="s">
         <v>985</v>
       </c>
-      <c r="C39" s="21" t="s">
+      <c r="E39" s="46" t="s">
         <v>986</v>
-      </c>
-      <c r="D39" s="5" t="s">
-        <v>987</v>
-      </c>
-      <c r="E39" s="46" t="s">
-        <v>988</v>
       </c>
     </row>
     <row r="40" spans="1:6" ht="64" x14ac:dyDescent="0.2">
@@ -16191,11 +16191,11 @@
         <v>406</v>
       </c>
       <c r="B40" s="28" t="s">
-        <v>989</v>
+        <v>987</v>
       </c>
       <c r="C40" s="27"/>
       <c r="D40" s="18" t="s">
-        <v>990</v>
+        <v>988</v>
       </c>
     </row>
     <row r="41" spans="1:6" ht="80" x14ac:dyDescent="0.2">
@@ -16203,16 +16203,16 @@
         <v>409</v>
       </c>
       <c r="B41" s="28" t="s">
-        <v>991</v>
+        <v>989</v>
       </c>
       <c r="C41" s="27"/>
       <c r="D41" s="18" t="s">
-        <v>983</v>
+        <v>981</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" s="187" t="s">
-        <v>992</v>
+        <v>990</v>
       </c>
       <c r="B42" s="188"/>
       <c r="C42" s="188"/>
@@ -16224,19 +16224,19 @@
         <v>239</v>
       </c>
       <c r="B43" s="116" t="s">
-        <v>993</v>
+        <v>991</v>
       </c>
       <c r="C43" s="21" t="s">
         <v>849</v>
       </c>
       <c r="D43" s="116" t="s">
-        <v>994</v>
+        <v>992</v>
       </c>
       <c r="E43" s="46" t="s">
         <v>851</v>
       </c>
       <c r="F43" s="72" t="s">
-        <v>995</v>
+        <v>993</v>
       </c>
     </row>
     <row r="44" spans="1:6" ht="80" x14ac:dyDescent="0.2">
@@ -16244,13 +16244,13 @@
         <v>364</v>
       </c>
       <c r="B44" s="116" t="s">
-        <v>996</v>
+        <v>994</v>
       </c>
       <c r="C44" s="21" t="s">
         <v>907</v>
       </c>
       <c r="D44" s="116" t="s">
-        <v>997</v>
+        <v>995</v>
       </c>
       <c r="E44" s="46" t="s">
         <v>908</v>
@@ -16261,16 +16261,16 @@
         <v>257</v>
       </c>
       <c r="B45" s="116" t="s">
-        <v>998</v>
+        <v>996</v>
       </c>
       <c r="C45" s="62" t="s">
-        <v>1377</v>
+        <v>1375</v>
       </c>
       <c r="D45" s="116" t="s">
-        <v>999</v>
+        <v>997</v>
       </c>
       <c r="E45" s="46" t="s">
-        <v>1378</v>
+        <v>1376</v>
       </c>
     </row>
     <row r="46" spans="1:6" ht="48" x14ac:dyDescent="0.2">
@@ -16278,16 +16278,16 @@
         <v>378</v>
       </c>
       <c r="B46" s="116" t="s">
+        <v>998</v>
+      </c>
+      <c r="C46" s="21" t="s">
+        <v>999</v>
+      </c>
+      <c r="D46" s="121" t="s">
         <v>1000</v>
       </c>
-      <c r="C46" s="21" t="s">
-        <v>1001</v>
-      </c>
-      <c r="D46" s="121" t="s">
-        <v>1002</v>
-      </c>
       <c r="E46" s="46" t="s">
-        <v>1001</v>
+        <v>999</v>
       </c>
     </row>
     <row r="47" spans="1:6" ht="64" x14ac:dyDescent="0.2">
@@ -16295,16 +16295,16 @@
         <v>378</v>
       </c>
       <c r="B47" s="116" t="s">
+        <v>1001</v>
+      </c>
+      <c r="C47" s="21" t="s">
+        <v>1002</v>
+      </c>
+      <c r="D47" s="121" t="s">
         <v>1003</v>
       </c>
-      <c r="C47" s="21" t="s">
+      <c r="E47" s="46" t="s">
         <v>1004</v>
-      </c>
-      <c r="D47" s="121" t="s">
-        <v>1005</v>
-      </c>
-      <c r="E47" s="46" t="s">
-        <v>1006</v>
       </c>
     </row>
     <row r="48" spans="1:6" ht="48" x14ac:dyDescent="0.2">
@@ -16312,16 +16312,16 @@
         <v>378</v>
       </c>
       <c r="B48" s="116" t="s">
+        <v>1005</v>
+      </c>
+      <c r="C48" s="21" t="s">
+        <v>1006</v>
+      </c>
+      <c r="D48" s="121" t="s">
         <v>1007</v>
       </c>
-      <c r="C48" s="21" t="s">
+      <c r="E48" s="46" t="s">
         <v>1008</v>
-      </c>
-      <c r="D48" s="121" t="s">
-        <v>1009</v>
-      </c>
-      <c r="E48" s="46" t="s">
-        <v>1010</v>
       </c>
     </row>
     <row r="49" spans="1:6" ht="48" x14ac:dyDescent="0.2">
@@ -16329,16 +16329,16 @@
         <v>378</v>
       </c>
       <c r="B49" s="116" t="s">
+        <v>1009</v>
+      </c>
+      <c r="C49" s="21" t="s">
+        <v>1010</v>
+      </c>
+      <c r="D49" s="121" t="s">
         <v>1011</v>
       </c>
-      <c r="C49" s="21" t="s">
+      <c r="E49" s="46" t="s">
         <v>1012</v>
-      </c>
-      <c r="D49" s="121" t="s">
-        <v>1013</v>
-      </c>
-      <c r="E49" s="46" t="s">
-        <v>1014</v>
       </c>
     </row>
     <row r="50" spans="1:6" ht="16" x14ac:dyDescent="0.2">
@@ -16346,16 +16346,16 @@
         <v>378</v>
       </c>
       <c r="B50" s="92" t="s">
-        <v>1015</v>
+        <v>1013</v>
       </c>
       <c r="C50" s="93" t="s">
-        <v>1016</v>
+        <v>1014</v>
       </c>
       <c r="D50" s="101" t="s">
         <v>400</v>
       </c>
       <c r="E50" s="85" t="s">
-        <v>1017</v>
+        <v>1015</v>
       </c>
     </row>
     <row r="51" spans="1:6" ht="16" x14ac:dyDescent="0.2">
@@ -16363,7 +16363,7 @@
         <v>32</v>
       </c>
       <c r="B51" s="19" t="s">
-        <v>1018</v>
+        <v>1016</v>
       </c>
       <c r="C51" s="21" t="s">
         <v>34</v>
@@ -16374,16 +16374,16 @@
     </row>
     <row r="52" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A52" s="19" t="s">
+        <v>1017</v>
+      </c>
+      <c r="B52" s="19" t="s">
+        <v>1018</v>
+      </c>
+      <c r="C52" s="21" t="s">
         <v>1019</v>
       </c>
-      <c r="B52" s="19" t="s">
+      <c r="D52" s="19" t="s">
         <v>1020</v>
-      </c>
-      <c r="C52" s="21" t="s">
-        <v>1021</v>
-      </c>
-      <c r="D52" s="19" t="s">
-        <v>1022</v>
       </c>
       <c r="F52" s="71" t="s">
         <v>895</v>
@@ -16391,16 +16391,16 @@
     </row>
     <row r="53" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A53" s="19" t="s">
-        <v>1019</v>
+        <v>1017</v>
       </c>
       <c r="B53" s="19" t="s">
-        <v>1023</v>
+        <v>1021</v>
       </c>
       <c r="C53" s="21" t="s">
-        <v>1024</v>
+        <v>1022</v>
       </c>
       <c r="D53" s="19" t="s">
-        <v>1022</v>
+        <v>1020</v>
       </c>
       <c r="F53" s="71" t="s">
         <v>895</v>
@@ -16411,13 +16411,13 @@
         <v>378</v>
       </c>
       <c r="B54" s="116" t="s">
+        <v>1023</v>
+      </c>
+      <c r="C54" s="21" t="s">
+        <v>1024</v>
+      </c>
+      <c r="D54" s="121" t="s">
         <v>1025</v>
-      </c>
-      <c r="C54" s="21" t="s">
-        <v>1026</v>
-      </c>
-      <c r="D54" s="121" t="s">
-        <v>1027</v>
       </c>
       <c r="F54" s="71" t="s">
         <v>895</v>
@@ -16428,13 +16428,13 @@
         <v>378</v>
       </c>
       <c r="B55" s="116" t="s">
+        <v>1026</v>
+      </c>
+      <c r="C55" s="21" t="s">
+        <v>1027</v>
+      </c>
+      <c r="D55" s="121" t="s">
         <v>1028</v>
-      </c>
-      <c r="C55" s="21" t="s">
-        <v>1029</v>
-      </c>
-      <c r="D55" s="121" t="s">
-        <v>1030</v>
       </c>
       <c r="F55" s="71" t="s">
         <v>895</v>
@@ -16460,8 +16460,8 @@
   <dimension ref="A1:F75"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E29" sqref="E29"/>
+      <pane ySplit="1" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -16500,16 +16500,16 @@
         <v>239</v>
       </c>
       <c r="B2" s="136" t="s">
-        <v>1031</v>
+        <v>1029</v>
       </c>
       <c r="C2" s="137" t="s">
-        <v>1032</v>
+        <v>1030</v>
       </c>
       <c r="D2" s="136" t="s">
         <v>242</v>
       </c>
       <c r="E2" s="138" t="s">
-        <v>1033</v>
+        <v>1031</v>
       </c>
       <c r="F2" s="135"/>
     </row>
@@ -16518,34 +16518,34 @@
         <v>943</v>
       </c>
       <c r="B3" s="136" t="s">
+        <v>1032</v>
+      </c>
+      <c r="C3" s="137" t="s">
+        <v>1033</v>
+      </c>
+      <c r="D3" s="136" t="s">
         <v>1034</v>
       </c>
-      <c r="C3" s="137" t="s">
+      <c r="E3" s="138" t="s">
         <v>1035</v>
-      </c>
-      <c r="D3" s="136" t="s">
-        <v>1036</v>
-      </c>
-      <c r="E3" s="138" t="s">
-        <v>1037</v>
       </c>
       <c r="F3" s="135"/>
     </row>
     <row r="4" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A4" s="136" t="s">
+        <v>1036</v>
+      </c>
+      <c r="B4" s="136" t="s">
+        <v>1037</v>
+      </c>
+      <c r="C4" s="137" t="s">
         <v>1038</v>
       </c>
-      <c r="B4" s="136" t="s">
+      <c r="D4" s="136" t="s">
         <v>1039</v>
       </c>
-      <c r="C4" s="137" t="s">
+      <c r="E4" s="138" t="s">
         <v>1040</v>
-      </c>
-      <c r="D4" s="136" t="s">
-        <v>1041</v>
-      </c>
-      <c r="E4" s="138" t="s">
-        <v>1042</v>
       </c>
       <c r="F4" s="135"/>
     </row>
@@ -16554,11 +16554,11 @@
         <v>406</v>
       </c>
       <c r="B5" s="139" t="s">
-        <v>1043</v>
+        <v>1041</v>
       </c>
       <c r="C5" s="27"/>
       <c r="D5" s="136" t="s">
-        <v>1044</v>
+        <v>1042</v>
       </c>
       <c r="E5" s="138"/>
       <c r="F5" s="135"/>
@@ -16568,84 +16568,84 @@
         <v>409</v>
       </c>
       <c r="B6" s="139" t="s">
-        <v>1045</v>
+        <v>1043</v>
       </c>
       <c r="C6" s="27"/>
       <c r="D6" s="136" t="s">
-        <v>1046</v>
+        <v>1044</v>
       </c>
       <c r="E6" s="138"/>
       <c r="F6" s="135"/>
     </row>
     <row r="7" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A7" s="136" t="s">
-        <v>1038</v>
+        <v>1036</v>
       </c>
       <c r="B7" s="136" t="s">
+        <v>1045</v>
+      </c>
+      <c r="C7" s="137" t="s">
+        <v>1046</v>
+      </c>
+      <c r="D7" s="136" t="s">
         <v>1047</v>
       </c>
-      <c r="C7" s="137" t="s">
+      <c r="E7" s="138" t="s">
         <v>1048</v>
-      </c>
-      <c r="D7" s="136" t="s">
-        <v>1049</v>
-      </c>
-      <c r="E7" s="138" t="s">
-        <v>1050</v>
       </c>
       <c r="F7" s="135"/>
     </row>
     <row r="8" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A8" s="136" t="s">
-        <v>1038</v>
+        <v>1036</v>
       </c>
       <c r="B8" s="136" t="s">
+        <v>1049</v>
+      </c>
+      <c r="C8" s="137" t="s">
+        <v>1050</v>
+      </c>
+      <c r="D8" s="136" t="s">
         <v>1051</v>
       </c>
-      <c r="C8" s="137" t="s">
+      <c r="E8" s="138" t="s">
         <v>1052</v>
-      </c>
-      <c r="D8" s="136" t="s">
-        <v>1053</v>
-      </c>
-      <c r="E8" s="138" t="s">
-        <v>1054</v>
       </c>
       <c r="F8" s="135"/>
     </row>
     <row r="9" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A9" s="136" t="s">
-        <v>1038</v>
+        <v>1036</v>
       </c>
       <c r="B9" s="136" t="s">
+        <v>1053</v>
+      </c>
+      <c r="C9" s="137" t="s">
+        <v>1054</v>
+      </c>
+      <c r="D9" s="136" t="s">
         <v>1055</v>
       </c>
-      <c r="C9" s="137" t="s">
+      <c r="E9" s="138" t="s">
         <v>1056</v>
-      </c>
-      <c r="D9" s="136" t="s">
-        <v>1057</v>
-      </c>
-      <c r="E9" s="138" t="s">
-        <v>1058</v>
       </c>
       <c r="F9" s="135"/>
     </row>
     <row r="10" spans="1:6" ht="64" x14ac:dyDescent="0.2">
       <c r="A10" s="136" t="s">
-        <v>1038</v>
+        <v>1036</v>
       </c>
       <c r="B10" s="136" t="s">
+        <v>1057</v>
+      </c>
+      <c r="C10" s="137" t="s">
+        <v>1058</v>
+      </c>
+      <c r="D10" s="136" t="s">
         <v>1059</v>
       </c>
-      <c r="C10" s="137" t="s">
+      <c r="E10" s="138" t="s">
         <v>1060</v>
-      </c>
-      <c r="D10" s="136" t="s">
-        <v>1061</v>
-      </c>
-      <c r="E10" s="138" t="s">
-        <v>1062</v>
       </c>
       <c r="F10" s="135"/>
     </row>
@@ -16654,50 +16654,50 @@
         <v>250</v>
       </c>
       <c r="B11" s="136" t="s">
+        <v>1061</v>
+      </c>
+      <c r="C11" s="137" t="s">
+        <v>1062</v>
+      </c>
+      <c r="D11" s="136" t="s">
         <v>1063</v>
       </c>
-      <c r="C11" s="137" t="s">
-        <v>1064</v>
-      </c>
-      <c r="D11" s="136" t="s">
-        <v>1065</v>
-      </c>
       <c r="E11" s="138" t="s">
-        <v>1402</v>
+        <v>1399</v>
       </c>
       <c r="F11" s="135"/>
     </row>
     <row r="12" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A12" s="136" t="s">
-        <v>1398</v>
+        <v>1395</v>
       </c>
       <c r="B12" s="136" t="s">
-        <v>1399</v>
+        <v>1396</v>
       </c>
       <c r="C12" s="137" t="s">
-        <v>1400</v>
+        <v>1397</v>
       </c>
       <c r="D12" s="136"/>
       <c r="E12" s="138" t="s">
-        <v>1401</v>
+        <v>1398</v>
       </c>
       <c r="F12" s="135"/>
     </row>
     <row r="13" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A13" s="136" t="s">
-        <v>1038</v>
+        <v>1036</v>
       </c>
       <c r="B13" s="136" t="s">
+        <v>1064</v>
+      </c>
+      <c r="C13" s="137" t="s">
+        <v>1463</v>
+      </c>
+      <c r="D13" s="136" t="s">
+        <v>1065</v>
+      </c>
+      <c r="E13" s="138" t="s">
         <v>1066</v>
-      </c>
-      <c r="C13" s="137" t="s">
-        <v>1396</v>
-      </c>
-      <c r="D13" s="136" t="s">
-        <v>1067</v>
-      </c>
-      <c r="E13" s="138" t="s">
-        <v>1068</v>
       </c>
       <c r="F13" s="135"/>
     </row>
@@ -16706,11 +16706,11 @@
         <v>406</v>
       </c>
       <c r="B14" s="28" t="s">
-        <v>1069</v>
+        <v>1067</v>
       </c>
       <c r="C14" s="138"/>
       <c r="D14" s="136" t="s">
-        <v>1070</v>
+        <v>1068</v>
       </c>
       <c r="E14" s="138"/>
       <c r="F14" s="135"/>
@@ -16720,83 +16720,83 @@
         <v>409</v>
       </c>
       <c r="B15" s="28" t="s">
-        <v>1071</v>
+        <v>1069</v>
       </c>
       <c r="C15" s="138"/>
       <c r="D15" s="136" t="s">
-        <v>1046</v>
+        <v>1044</v>
       </c>
       <c r="E15" s="138"/>
       <c r="F15" s="135"/>
     </row>
     <row r="16" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A16" s="136" t="s">
-        <v>1038</v>
+        <v>1036</v>
       </c>
       <c r="B16" s="136" t="s">
+        <v>1070</v>
+      </c>
+      <c r="C16" s="137" t="s">
+        <v>1391</v>
+      </c>
+      <c r="D16" s="136" t="s">
+        <v>1071</v>
+      </c>
+      <c r="E16" s="138" t="s">
         <v>1072</v>
-      </c>
-      <c r="C16" s="137" t="s">
-        <v>1393</v>
-      </c>
-      <c r="D16" s="136" t="s">
-        <v>1073</v>
-      </c>
-      <c r="E16" s="138" t="s">
-        <v>1074</v>
       </c>
       <c r="F16" s="135"/>
     </row>
     <row r="17" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A17" s="136" t="s">
-        <v>1038</v>
+        <v>1036</v>
       </c>
       <c r="B17" s="136" t="s">
+        <v>1073</v>
+      </c>
+      <c r="C17" s="137" t="s">
+        <v>1392</v>
+      </c>
+      <c r="D17" s="136" t="s">
+        <v>1074</v>
+      </c>
+      <c r="E17" s="138" t="s">
         <v>1075</v>
-      </c>
-      <c r="C17" s="137" t="s">
-        <v>1394</v>
-      </c>
-      <c r="D17" s="136" t="s">
-        <v>1076</v>
-      </c>
-      <c r="E17" s="138" t="s">
-        <v>1077</v>
       </c>
       <c r="F17" s="135"/>
     </row>
     <row r="18" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A18" s="136" t="s">
-        <v>1038</v>
+        <v>1036</v>
       </c>
       <c r="B18" s="136" t="s">
+        <v>1076</v>
+      </c>
+      <c r="C18" s="137" t="s">
+        <v>1393</v>
+      </c>
+      <c r="D18" s="136" t="s">
+        <v>1077</v>
+      </c>
+      <c r="E18" s="138" t="s">
         <v>1078</v>
-      </c>
-      <c r="C18" s="137" t="s">
-        <v>1395</v>
-      </c>
-      <c r="D18" s="136" t="s">
-        <v>1079</v>
-      </c>
-      <c r="E18" s="138" t="s">
-        <v>1080</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="144" x14ac:dyDescent="0.2">
       <c r="A19" s="136" t="s">
-        <v>1038</v>
+        <v>1036</v>
       </c>
       <c r="B19" s="136" t="s">
+        <v>1079</v>
+      </c>
+      <c r="C19" s="137" t="s">
+        <v>1080</v>
+      </c>
+      <c r="D19" s="29" t="s">
         <v>1081</v>
       </c>
-      <c r="C19" s="137" t="s">
+      <c r="E19" s="138" t="s">
         <v>1082</v>
-      </c>
-      <c r="D19" s="29" t="s">
-        <v>1083</v>
-      </c>
-      <c r="E19" s="138" t="s">
-        <v>1084</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="80" x14ac:dyDescent="0.2">
@@ -16804,11 +16804,11 @@
         <v>406</v>
       </c>
       <c r="B20" s="28" t="s">
-        <v>1085</v>
+        <v>1083</v>
       </c>
       <c r="C20" s="27"/>
       <c r="D20" s="18" t="s">
-        <v>1086</v>
+        <v>1084</v>
       </c>
       <c r="E20" s="138"/>
     </row>
@@ -16817,11 +16817,11 @@
         <v>409</v>
       </c>
       <c r="B21" s="28" t="s">
-        <v>1087</v>
+        <v>1085</v>
       </c>
       <c r="C21" s="27"/>
       <c r="D21" s="18" t="s">
-        <v>1046</v>
+        <v>1044</v>
       </c>
       <c r="E21" s="138"/>
     </row>
@@ -16830,29 +16830,29 @@
         <v>409</v>
       </c>
       <c r="B22" s="28" t="s">
-        <v>1088</v>
+        <v>1086</v>
       </c>
       <c r="C22" s="27"/>
       <c r="D22" s="18" t="s">
-        <v>1089</v>
+        <v>1087</v>
       </c>
       <c r="E22" s="138"/>
     </row>
     <row r="23" spans="1:6" ht="112" x14ac:dyDescent="0.2">
       <c r="A23" s="136" t="s">
+        <v>1088</v>
+      </c>
+      <c r="B23" s="136" t="s">
+        <v>1089</v>
+      </c>
+      <c r="C23" s="137" t="s">
         <v>1090</v>
       </c>
-      <c r="B23" s="136" t="s">
+      <c r="D23" s="136" t="s">
         <v>1091</v>
       </c>
-      <c r="C23" s="137" t="s">
+      <c r="E23" s="138" t="s">
         <v>1092</v>
-      </c>
-      <c r="D23" s="136" t="s">
-        <v>1093</v>
-      </c>
-      <c r="E23" s="138" t="s">
-        <v>1094</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="48" x14ac:dyDescent="0.2">
@@ -16860,11 +16860,11 @@
         <v>406</v>
       </c>
       <c r="B24" s="28" t="s">
-        <v>1095</v>
+        <v>1093</v>
       </c>
       <c r="C24" s="27"/>
       <c r="D24" s="136" t="s">
-        <v>1096</v>
+        <v>1094</v>
       </c>
       <c r="E24" s="138"/>
     </row>
@@ -16873,11 +16873,11 @@
         <v>409</v>
       </c>
       <c r="B25" s="28" t="s">
-        <v>1097</v>
+        <v>1095</v>
       </c>
       <c r="C25" s="27"/>
       <c r="D25" s="136" t="s">
-        <v>1098</v>
+        <v>1096</v>
       </c>
       <c r="E25" s="138"/>
     </row>
@@ -16886,11 +16886,11 @@
         <v>409</v>
       </c>
       <c r="B26" s="28" t="s">
-        <v>1099</v>
+        <v>1097</v>
       </c>
       <c r="C26" s="27"/>
       <c r="D26" s="29" t="s">
-        <v>1100</v>
+        <v>1098</v>
       </c>
       <c r="E26" s="138"/>
     </row>
@@ -16899,53 +16899,53 @@
         <v>250</v>
       </c>
       <c r="B27" s="136" t="s">
+        <v>1099</v>
+      </c>
+      <c r="C27" s="137" t="s">
+        <v>1100</v>
+      </c>
+      <c r="D27" s="136" t="s">
+        <v>1063</v>
+      </c>
+      <c r="E27" s="138" t="s">
         <v>1101</v>
-      </c>
-      <c r="C27" s="137" t="s">
-        <v>1102</v>
-      </c>
-      <c r="D27" s="136" t="s">
-        <v>1065</v>
-      </c>
-      <c r="E27" s="138" t="s">
-        <v>1103</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="64" x14ac:dyDescent="0.2">
       <c r="A28" s="136" t="s">
-        <v>1398</v>
+        <v>1395</v>
       </c>
       <c r="B28" s="136" t="s">
-        <v>1397</v>
+        <v>1394</v>
       </c>
       <c r="C28" s="137" t="s">
-        <v>1419</v>
+        <v>1416</v>
       </c>
       <c r="D28" s="136"/>
       <c r="E28" s="138" t="s">
-        <v>1421</v>
+        <v>1418</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A29" s="136" t="s">
-        <v>1038</v>
+        <v>1036</v>
       </c>
       <c r="B29" s="136" t="s">
-        <v>1104</v>
+        <v>1102</v>
       </c>
       <c r="C29" s="137" t="s">
-        <v>1420</v>
+        <v>1417</v>
       </c>
       <c r="D29" s="136" t="s">
-        <v>1105</v>
+        <v>1103</v>
       </c>
       <c r="E29" s="138" t="s">
-        <v>1422</v>
+        <v>1419</v>
       </c>
     </row>
     <row r="30" spans="1:6" s="13" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A30" s="196" t="s">
-        <v>1106</v>
+        <v>1104</v>
       </c>
       <c r="B30" s="197"/>
       <c r="C30" s="197"/>
@@ -16957,33 +16957,33 @@
         <v>239</v>
       </c>
       <c r="B31" s="141" t="s">
+        <v>1105</v>
+      </c>
+      <c r="C31" s="142" t="s">
+        <v>1106</v>
+      </c>
+      <c r="D31" s="5" t="s">
         <v>1107</v>
       </c>
-      <c r="C31" s="142" t="s">
+      <c r="E31" s="143" t="s">
         <v>1108</v>
-      </c>
-      <c r="D31" s="5" t="s">
-        <v>1109</v>
-      </c>
-      <c r="E31" s="143" t="s">
-        <v>1110</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="64" x14ac:dyDescent="0.2">
       <c r="A32" s="144" t="s">
+        <v>1109</v>
+      </c>
+      <c r="B32" s="144" t="s">
+        <v>1110</v>
+      </c>
+      <c r="C32" s="145" t="s">
         <v>1111</v>
       </c>
-      <c r="B32" s="144" t="s">
+      <c r="D32" s="144" t="s">
         <v>1112</v>
       </c>
-      <c r="C32" s="145" t="s">
+      <c r="E32" s="146" t="s">
         <v>1113</v>
-      </c>
-      <c r="D32" s="144" t="s">
-        <v>1114</v>
-      </c>
-      <c r="E32" s="146" t="s">
-        <v>1115</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="48" x14ac:dyDescent="0.2">
@@ -16991,11 +16991,11 @@
         <v>406</v>
       </c>
       <c r="B33" s="28" t="s">
-        <v>1116</v>
+        <v>1114</v>
       </c>
       <c r="C33" s="27"/>
       <c r="D33" s="18" t="s">
-        <v>990</v>
+        <v>988</v>
       </c>
       <c r="E33" s="146"/>
     </row>
@@ -17004,17 +17004,17 @@
         <v>409</v>
       </c>
       <c r="B34" s="28" t="s">
-        <v>1117</v>
+        <v>1115</v>
       </c>
       <c r="C34" s="27"/>
       <c r="D34" s="18" t="s">
-        <v>983</v>
+        <v>981</v>
       </c>
       <c r="E34" s="146"/>
     </row>
     <row r="35" spans="1:6" s="13" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A35" s="199" t="s">
-        <v>1118</v>
+        <v>1116</v>
       </c>
       <c r="B35" s="200"/>
       <c r="C35" s="201"/>
@@ -17026,121 +17026,121 @@
         <v>239</v>
       </c>
       <c r="B36" s="147" t="s">
+        <v>1117</v>
+      </c>
+      <c r="C36" s="145" t="s">
+        <v>1118</v>
+      </c>
+      <c r="D36" s="50" t="s">
         <v>1119</v>
       </c>
-      <c r="C36" s="145" t="s">
+      <c r="E36" s="146" t="s">
         <v>1120</v>
-      </c>
-      <c r="D36" s="50" t="s">
-        <v>1121</v>
-      </c>
-      <c r="E36" s="146" t="s">
-        <v>1122</v>
       </c>
       <c r="F36" s="135"/>
     </row>
     <row r="37" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A37" s="144" t="s">
-        <v>1038</v>
+        <v>1036</v>
       </c>
       <c r="B37" s="148" t="s">
+        <v>1121</v>
+      </c>
+      <c r="C37" s="145" t="s">
+        <v>1122</v>
+      </c>
+      <c r="D37" s="149" t="s">
         <v>1123</v>
       </c>
-      <c r="C37" s="145" t="s">
+      <c r="E37" s="146" t="s">
         <v>1124</v>
-      </c>
-      <c r="D37" s="149" t="s">
-        <v>1125</v>
-      </c>
-      <c r="E37" s="146" t="s">
-        <v>1126</v>
       </c>
       <c r="F37" s="135"/>
     </row>
     <row r="38" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A38" s="144" t="s">
-        <v>1038</v>
+        <v>1036</v>
       </c>
       <c r="B38" s="148" t="s">
+        <v>1125</v>
+      </c>
+      <c r="C38" s="145" t="s">
+        <v>1126</v>
+      </c>
+      <c r="D38" s="149" t="s">
+        <v>1123</v>
+      </c>
+      <c r="E38" s="146" t="s">
         <v>1127</v>
-      </c>
-      <c r="C38" s="145" t="s">
-        <v>1128</v>
-      </c>
-      <c r="D38" s="149" t="s">
-        <v>1125</v>
-      </c>
-      <c r="E38" s="146" t="s">
-        <v>1129</v>
       </c>
       <c r="F38" s="135"/>
     </row>
     <row r="39" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A39" s="144" t="s">
-        <v>1038</v>
+        <v>1036</v>
       </c>
       <c r="B39" s="148" t="s">
+        <v>1128</v>
+      </c>
+      <c r="C39" s="49" t="s">
+        <v>1129</v>
+      </c>
+      <c r="D39" s="149" t="s">
+        <v>1123</v>
+      </c>
+      <c r="E39" s="146" t="s">
         <v>1130</v>
-      </c>
-      <c r="C39" s="49" t="s">
-        <v>1131</v>
-      </c>
-      <c r="D39" s="149" t="s">
-        <v>1125</v>
-      </c>
-      <c r="E39" s="146" t="s">
-        <v>1132</v>
       </c>
       <c r="F39" s="135"/>
     </row>
     <row r="40" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A40" s="144" t="s">
-        <v>1038</v>
+        <v>1036</v>
       </c>
       <c r="B40" s="148" t="s">
+        <v>1131</v>
+      </c>
+      <c r="C40" s="49" t="s">
+        <v>1132</v>
+      </c>
+      <c r="D40" s="149" t="s">
+        <v>1123</v>
+      </c>
+      <c r="E40" s="146" t="s">
         <v>1133</v>
-      </c>
-      <c r="C40" s="49" t="s">
-        <v>1134</v>
-      </c>
-      <c r="D40" s="149" t="s">
-        <v>1125</v>
-      </c>
-      <c r="E40" s="146" t="s">
-        <v>1135</v>
       </c>
       <c r="F40" s="135"/>
     </row>
     <row r="41" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A41" s="144" t="s">
-        <v>1038</v>
+        <v>1036</v>
       </c>
       <c r="B41" s="148" t="s">
+        <v>1134</v>
+      </c>
+      <c r="C41" s="49" t="s">
+        <v>1135</v>
+      </c>
+      <c r="D41" s="149" t="s">
+        <v>1123</v>
+      </c>
+      <c r="E41" s="146" t="s">
         <v>1136</v>
-      </c>
-      <c r="C41" s="49" t="s">
-        <v>1137</v>
-      </c>
-      <c r="D41" s="149" t="s">
-        <v>1125</v>
-      </c>
-      <c r="E41" s="146" t="s">
-        <v>1138</v>
       </c>
       <c r="F41" s="135"/>
     </row>
     <row r="42" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A42" s="144" t="s">
-        <v>1038</v>
+        <v>1036</v>
       </c>
       <c r="B42" s="148" t="s">
-        <v>1139</v>
+        <v>1137</v>
       </c>
       <c r="C42" s="49" t="s">
         <v>93</v>
       </c>
       <c r="D42" s="149" t="s">
-        <v>1125</v>
+        <v>1123</v>
       </c>
       <c r="E42" s="146" t="s">
         <v>95</v>
@@ -17152,11 +17152,11 @@
         <v>406</v>
       </c>
       <c r="B43" s="28" t="s">
-        <v>1140</v>
+        <v>1138</v>
       </c>
       <c r="C43" s="51"/>
       <c r="D43" s="18" t="s">
-        <v>990</v>
+        <v>988</v>
       </c>
       <c r="E43" s="146"/>
       <c r="F43" s="135"/>
@@ -17166,11 +17166,11 @@
         <v>409</v>
       </c>
       <c r="B44" s="28" t="s">
-        <v>1141</v>
+        <v>1139</v>
       </c>
       <c r="C44" s="27"/>
       <c r="D44" s="18" t="s">
-        <v>983</v>
+        <v>981</v>
       </c>
       <c r="E44" s="146"/>
       <c r="F44" s="135"/>
@@ -17180,16 +17180,16 @@
         <v>239</v>
       </c>
       <c r="B45" s="136" t="s">
+        <v>1140</v>
+      </c>
+      <c r="C45" s="62" t="s">
+        <v>1365</v>
+      </c>
+      <c r="D45" s="5" t="s">
+        <v>1141</v>
+      </c>
+      <c r="E45" s="146" t="s">
         <v>1142</v>
-      </c>
-      <c r="C45" s="62" t="s">
-        <v>1367</v>
-      </c>
-      <c r="D45" s="5" t="s">
-        <v>1143</v>
-      </c>
-      <c r="E45" s="146" t="s">
-        <v>1144</v>
       </c>
       <c r="F45" s="135"/>
     </row>
@@ -17198,11 +17198,11 @@
         <v>406</v>
       </c>
       <c r="B46" s="28" t="s">
-        <v>1145</v>
+        <v>1143</v>
       </c>
       <c r="C46" s="27"/>
       <c r="D46" s="18" t="s">
-        <v>990</v>
+        <v>988</v>
       </c>
       <c r="E46" s="146"/>
       <c r="F46" s="135"/>
@@ -17212,18 +17212,18 @@
         <v>409</v>
       </c>
       <c r="B47" s="28" t="s">
-        <v>1146</v>
+        <v>1144</v>
       </c>
       <c r="C47" s="27"/>
       <c r="D47" s="18" t="s">
-        <v>983</v>
+        <v>981</v>
       </c>
       <c r="E47" s="146"/>
       <c r="F47" s="135"/>
     </row>
     <row r="48" spans="1:6" s="13" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="196" t="s">
-        <v>1147</v>
+        <v>1145</v>
       </c>
       <c r="B48" s="197"/>
       <c r="C48" s="197"/>
@@ -17235,33 +17235,33 @@
         <v>239</v>
       </c>
       <c r="B49" s="144" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="C49" s="62" t="s">
         <v>849</v>
       </c>
       <c r="D49" s="116" t="s">
-        <v>1149</v>
+        <v>1147</v>
       </c>
       <c r="E49" s="63" t="s">
         <v>851</v>
       </c>
       <c r="F49" s="38" t="s">
-        <v>1150</v>
+        <v>1148</v>
       </c>
     </row>
     <row r="50" spans="1:6" s="30" customFormat="1" ht="64" x14ac:dyDescent="0.2">
       <c r="A50" s="144" t="s">
-        <v>1151</v>
+        <v>1149</v>
       </c>
       <c r="B50" s="144" t="s">
-        <v>1152</v>
+        <v>1150</v>
       </c>
       <c r="C50" s="62" t="s">
         <v>913</v>
       </c>
       <c r="D50" s="116" t="s">
-        <v>1153</v>
+        <v>1151</v>
       </c>
       <c r="E50" s="63" t="s">
         <v>914</v>
@@ -17269,19 +17269,19 @@
     </row>
     <row r="51" spans="1:6" s="30" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A51" s="144" t="s">
-        <v>1111</v>
+        <v>1109</v>
       </c>
       <c r="B51" s="144" t="s">
-        <v>1154</v>
+        <v>1152</v>
       </c>
       <c r="C51" s="62" t="s">
-        <v>1377</v>
+        <v>1375</v>
       </c>
       <c r="D51" s="116" t="s">
-        <v>999</v>
+        <v>997</v>
       </c>
       <c r="E51" s="63" t="s">
-        <v>1378</v>
+        <v>1376</v>
       </c>
     </row>
     <row r="52" spans="1:6" s="30" customFormat="1" ht="48" x14ac:dyDescent="0.2">
@@ -17289,19 +17289,19 @@
         <v>378</v>
       </c>
       <c r="B52" s="136" t="s">
+        <v>1153</v>
+      </c>
+      <c r="C52" s="145" t="s">
+        <v>1154</v>
+      </c>
+      <c r="D52" s="121" t="s">
         <v>1155</v>
       </c>
-      <c r="C52" s="145" t="s">
+      <c r="E52" s="63" t="s">
+        <v>1040</v>
+      </c>
+      <c r="F52" s="73" t="s">
         <v>1156</v>
-      </c>
-      <c r="D52" s="121" t="s">
-        <v>1157</v>
-      </c>
-      <c r="E52" s="63" t="s">
-        <v>1042</v>
-      </c>
-      <c r="F52" s="73" t="s">
-        <v>1158</v>
       </c>
     </row>
     <row r="53" spans="1:6" s="30" customFormat="1" ht="48" x14ac:dyDescent="0.2">
@@ -17309,16 +17309,16 @@
         <v>378</v>
       </c>
       <c r="B53" s="136" t="s">
+        <v>1157</v>
+      </c>
+      <c r="C53" s="145" t="s">
+        <v>1158</v>
+      </c>
+      <c r="D53" s="121" t="s">
         <v>1159</v>
       </c>
-      <c r="C53" s="145" t="s">
+      <c r="E53" s="63" t="s">
         <v>1160</v>
-      </c>
-      <c r="D53" s="121" t="s">
-        <v>1161</v>
-      </c>
-      <c r="E53" s="63" t="s">
-        <v>1162</v>
       </c>
     </row>
     <row r="54" spans="1:6" s="30" customFormat="1" ht="64" x14ac:dyDescent="0.2">
@@ -17326,16 +17326,16 @@
         <v>378</v>
       </c>
       <c r="B54" s="136" t="s">
+        <v>1161</v>
+      </c>
+      <c r="C54" s="145" t="s">
+        <v>1162</v>
+      </c>
+      <c r="D54" s="121" t="s">
         <v>1163</v>
       </c>
-      <c r="C54" s="145" t="s">
+      <c r="E54" s="63" t="s">
         <v>1164</v>
-      </c>
-      <c r="D54" s="121" t="s">
-        <v>1165</v>
-      </c>
-      <c r="E54" s="63" t="s">
-        <v>1166</v>
       </c>
     </row>
     <row r="55" spans="1:6" s="30" customFormat="1" ht="64" x14ac:dyDescent="0.2">
@@ -17343,16 +17343,16 @@
         <v>378</v>
       </c>
       <c r="B55" s="136" t="s">
+        <v>1165</v>
+      </c>
+      <c r="C55" s="145" t="s">
+        <v>1166</v>
+      </c>
+      <c r="D55" s="121" t="s">
         <v>1167</v>
       </c>
-      <c r="C55" s="145" t="s">
+      <c r="E55" s="63" t="s">
         <v>1168</v>
-      </c>
-      <c r="D55" s="121" t="s">
-        <v>1169</v>
-      </c>
-      <c r="E55" s="63" t="s">
-        <v>1170</v>
       </c>
     </row>
     <row r="56" spans="1:6" s="30" customFormat="1" ht="48" x14ac:dyDescent="0.2">
@@ -17360,16 +17360,16 @@
         <v>378</v>
       </c>
       <c r="B56" s="136" t="s">
+        <v>1169</v>
+      </c>
+      <c r="C56" s="145" t="s">
+        <v>1170</v>
+      </c>
+      <c r="D56" s="121" t="s">
         <v>1171</v>
       </c>
-      <c r="C56" s="145" t="s">
+      <c r="E56" s="63" t="s">
         <v>1172</v>
-      </c>
-      <c r="D56" s="121" t="s">
-        <v>1173</v>
-      </c>
-      <c r="E56" s="63" t="s">
-        <v>1174</v>
       </c>
     </row>
     <row r="57" spans="1:6" s="30" customFormat="1" ht="32" x14ac:dyDescent="0.2">
@@ -17377,19 +17377,19 @@
         <v>378</v>
       </c>
       <c r="B57" s="136" t="s">
+        <v>1173</v>
+      </c>
+      <c r="C57" s="145" t="s">
+        <v>1174</v>
+      </c>
+      <c r="D57" s="121" t="s">
         <v>1175</v>
       </c>
-      <c r="C57" s="145" t="s">
+      <c r="E57" s="63" t="s">
+        <v>1066</v>
+      </c>
+      <c r="F57" s="73" t="s">
         <v>1176</v>
-      </c>
-      <c r="D57" s="121" t="s">
-        <v>1177</v>
-      </c>
-      <c r="E57" s="63" t="s">
-        <v>1068</v>
-      </c>
-      <c r="F57" s="73" t="s">
-        <v>1178</v>
       </c>
     </row>
     <row r="58" spans="1:6" s="30" customFormat="1" ht="48" x14ac:dyDescent="0.2">
@@ -17397,19 +17397,19 @@
         <v>378</v>
       </c>
       <c r="B58" s="136" t="s">
+        <v>1177</v>
+      </c>
+      <c r="C58" s="145" t="s">
+        <v>1178</v>
+      </c>
+      <c r="D58" s="121" t="s">
         <v>1179</v>
       </c>
-      <c r="C58" s="145" t="s">
+      <c r="E58" s="63" t="s">
         <v>1180</v>
       </c>
-      <c r="D58" s="121" t="s">
+      <c r="F58" s="73" t="s">
         <v>1181</v>
-      </c>
-      <c r="E58" s="63" t="s">
-        <v>1182</v>
-      </c>
-      <c r="F58" s="73" t="s">
-        <v>1183</v>
       </c>
     </row>
     <row r="59" spans="1:6" s="30" customFormat="1" ht="48" x14ac:dyDescent="0.2">
@@ -17417,19 +17417,19 @@
         <v>378</v>
       </c>
       <c r="B59" s="136" t="s">
+        <v>1182</v>
+      </c>
+      <c r="C59" s="145" t="s">
+        <v>1183</v>
+      </c>
+      <c r="D59" s="121" t="s">
         <v>1184</v>
       </c>
-      <c r="C59" s="145" t="s">
+      <c r="E59" s="63" t="s">
         <v>1185</v>
       </c>
-      <c r="D59" s="121" t="s">
+      <c r="F59" s="73" t="s">
         <v>1186</v>
-      </c>
-      <c r="E59" s="63" t="s">
-        <v>1187</v>
-      </c>
-      <c r="F59" s="73" t="s">
-        <v>1188</v>
       </c>
     </row>
     <row r="60" spans="1:6" s="30" customFormat="1" ht="32" x14ac:dyDescent="0.2">
@@ -17437,19 +17437,19 @@
         <v>378</v>
       </c>
       <c r="B60" s="136" t="s">
+        <v>1187</v>
+      </c>
+      <c r="C60" s="145" t="s">
+        <v>1188</v>
+      </c>
+      <c r="D60" s="121" t="s">
         <v>1189</v>
       </c>
-      <c r="C60" s="145" t="s">
+      <c r="E60" s="63" t="s">
         <v>1190</v>
       </c>
-      <c r="D60" s="121" t="s">
+      <c r="F60" s="73" t="s">
         <v>1191</v>
-      </c>
-      <c r="E60" s="63" t="s">
-        <v>1192</v>
-      </c>
-      <c r="F60" s="73" t="s">
-        <v>1193</v>
       </c>
     </row>
     <row r="61" spans="1:6" s="30" customFormat="1" ht="48" x14ac:dyDescent="0.2">
@@ -17457,16 +17457,16 @@
         <v>378</v>
       </c>
       <c r="B61" s="136" t="s">
+        <v>1192</v>
+      </c>
+      <c r="C61" s="145" t="s">
+        <v>1193</v>
+      </c>
+      <c r="D61" s="121" t="s">
         <v>1194</v>
       </c>
-      <c r="C61" s="145" t="s">
+      <c r="E61" s="63" t="s">
         <v>1195</v>
-      </c>
-      <c r="D61" s="121" t="s">
-        <v>1196</v>
-      </c>
-      <c r="E61" s="63" t="s">
-        <v>1197</v>
       </c>
     </row>
     <row r="62" spans="1:6" s="30" customFormat="1" ht="48" x14ac:dyDescent="0.2">
@@ -17474,16 +17474,16 @@
         <v>378</v>
       </c>
       <c r="B62" s="136" t="s">
+        <v>1196</v>
+      </c>
+      <c r="C62" s="145" t="s">
+        <v>1197</v>
+      </c>
+      <c r="D62" s="121" t="s">
         <v>1198</v>
       </c>
-      <c r="C62" s="145" t="s">
+      <c r="E62" s="63" t="s">
         <v>1199</v>
-      </c>
-      <c r="D62" s="121" t="s">
-        <v>1200</v>
-      </c>
-      <c r="E62" s="63" t="s">
-        <v>1201</v>
       </c>
     </row>
     <row r="63" spans="1:6" s="30" customFormat="1" ht="48" x14ac:dyDescent="0.2">
@@ -17491,16 +17491,16 @@
         <v>378</v>
       </c>
       <c r="B63" s="18" t="s">
+        <v>1200</v>
+      </c>
+      <c r="C63" s="145" t="s">
+        <v>1201</v>
+      </c>
+      <c r="D63" s="121" t="s">
         <v>1202</v>
       </c>
-      <c r="C63" s="145" t="s">
+      <c r="E63" s="63" t="s">
         <v>1203</v>
-      </c>
-      <c r="D63" s="121" t="s">
-        <v>1204</v>
-      </c>
-      <c r="E63" s="63" t="s">
-        <v>1205</v>
       </c>
     </row>
     <row r="64" spans="1:6" s="30" customFormat="1" ht="48" x14ac:dyDescent="0.2">
@@ -17508,16 +17508,16 @@
         <v>378</v>
       </c>
       <c r="B64" s="136" t="s">
+        <v>1204</v>
+      </c>
+      <c r="C64" s="145" t="s">
+        <v>1205</v>
+      </c>
+      <c r="D64" s="121" t="s">
         <v>1206</v>
       </c>
-      <c r="C64" s="145" t="s">
+      <c r="E64" s="79" t="s">
         <v>1207</v>
-      </c>
-      <c r="D64" s="121" t="s">
-        <v>1208</v>
-      </c>
-      <c r="E64" s="79" t="s">
-        <v>1209</v>
       </c>
     </row>
     <row r="65" spans="1:6" ht="16" x14ac:dyDescent="0.2">
@@ -17525,14 +17525,14 @@
         <v>723</v>
       </c>
       <c r="B65" s="144" t="s">
-        <v>1210</v>
+        <v>1208</v>
       </c>
       <c r="C65" s="145" t="s">
-        <v>1211</v>
+        <v>1209</v>
       </c>
       <c r="D65" s="148"/>
       <c r="E65" s="78" t="s">
-        <v>1212</v>
+        <v>1210</v>
       </c>
       <c r="F65" s="135"/>
     </row>
@@ -17541,14 +17541,14 @@
         <v>723</v>
       </c>
       <c r="B66" s="144" t="s">
-        <v>1213</v>
+        <v>1211</v>
       </c>
       <c r="C66" s="145" t="s">
-        <v>1137</v>
+        <v>1135</v>
       </c>
       <c r="D66" s="148"/>
       <c r="E66" s="78" t="s">
-        <v>1138</v>
+        <v>1136</v>
       </c>
       <c r="F66" s="135"/>
     </row>
@@ -17557,14 +17557,14 @@
         <v>723</v>
       </c>
       <c r="B67" s="136" t="s">
-        <v>1214</v>
+        <v>1212</v>
       </c>
       <c r="C67" s="145" t="s">
-        <v>1124</v>
+        <v>1122</v>
       </c>
       <c r="D67" s="148"/>
       <c r="E67" s="78" t="s">
-        <v>1126</v>
+        <v>1124</v>
       </c>
       <c r="F67" s="135"/>
     </row>
@@ -17635,15 +17635,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <Readyforteam_x003f_ xmlns="565e1b1d-057e-4d85-b896-01a5881d8a45">false</Readyforteam_x003f_>
@@ -17682,6 +17673,15 @@
     <TaxCatchAll xmlns="2799d30d-6731-4efe-ac9b-c4895a8828d9" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -17962,14 +17962,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8D7CE8C7-18DC-484F-8376-ED09F13D44C8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{017ACE96-8143-486E-8436-7787F6B96F4A}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -17978,6 +17970,14 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
     <ds:schemaRef ds:uri="bf601f31-63a1-4825-9216-91d773c5ef9c"/>
     <ds:schemaRef ds:uri="2799d30d-6731-4efe-ac9b-c4895a8828d9"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8D7CE8C7-18DC-484F-8376-ED09F13D44C8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Tidying up the MCCD summary logic (adding AP/ME cert functionality) and dealing with the AP/ME title.
</commit_message>
<xml_diff>
--- a/app/data/MCCD-localisation.xlsx
+++ b/app/data/MCCD-localisation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/JALAT/GIT/medical-certificate-of-cause-of-death/app/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82410B40-D77A-A04A-AAFD-7A3CF3A2A4CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2A23713-F8B2-164E-9341-874F0A2A6761}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="14020" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="14020" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Using this document" sheetId="8" r:id="rId1"/>
@@ -69,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2196" uniqueCount="1467">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2199" uniqueCount="1470">
   <si>
     <r>
       <rPr>
@@ -5779,7 +5779,16 @@
     <t>Dewiswch uned oedran</t>
   </si>
   <si>
-    <t>048</t>
+    <t>pmMCCDTasklistMedicalExaminersInformation</t>
+  </si>
+  <si>
+    <t>Medical examiner's information</t>
+  </si>
+  <si>
+    <t>Gwybodaeth yr arholwr meddygol</t>
+  </si>
+  <si>
+    <t>049</t>
   </si>
 </sst>
 </file>
@@ -6255,7 +6264,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="205">
+  <cellXfs count="208">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -6762,6 +6771,24 @@
     <xf numFmtId="0" fontId="13" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -6771,24 +6798,6 @@
     <xf numFmtId="0" fontId="6" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
@@ -6860,6 +6869,15 @@
     </xf>
     <xf numFmtId="0" fontId="13" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -7791,7 +7809,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F10" sqref="F10"/>
+      <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -8011,7 +8029,7 @@
   <dimension ref="A1:F24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
@@ -8447,7 +8465,7 @@
   <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
@@ -8839,13 +8857,13 @@
         <v>7</v>
       </c>
       <c r="C2" s="100" t="s">
-        <v>1466</v>
+        <v>1469</v>
       </c>
       <c r="D2" s="98" t="s">
         <v>8</v>
       </c>
       <c r="E2" s="99" t="s">
-        <v>1466</v>
+        <v>1469</v>
       </c>
       <c r="F2" s="98"/>
     </row>
@@ -10497,7 +10515,7 @@
   <dimension ref="A1:F31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
@@ -11058,13 +11076,13 @@
       </c>
     </row>
     <row r="2" spans="1:6" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="175" t="s">
+      <c r="A2" s="172" t="s">
         <v>363</v>
       </c>
-      <c r="B2" s="176"/>
-      <c r="C2" s="176"/>
-      <c r="D2" s="176"/>
-      <c r="E2" s="177"/>
+      <c r="B2" s="173"/>
+      <c r="C2" s="173"/>
+      <c r="D2" s="173"/>
+      <c r="E2" s="174"/>
       <c r="F2" s="33"/>
     </row>
     <row r="3" spans="1:6" ht="48" x14ac:dyDescent="0.2">
@@ -11192,13 +11210,13 @@
       <c r="F9" s="119"/>
     </row>
     <row r="10" spans="1:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="178" t="s">
+      <c r="A10" s="175" t="s">
         <v>392</v>
       </c>
-      <c r="B10" s="179"/>
-      <c r="C10" s="179"/>
-      <c r="D10" s="179"/>
-      <c r="E10" s="180"/>
+      <c r="B10" s="176"/>
+      <c r="C10" s="176"/>
+      <c r="D10" s="176"/>
+      <c r="E10" s="177"/>
       <c r="F10" s="119"/>
     </row>
     <row r="11" spans="1:6" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -13680,13 +13698,13 @@
       <c r="F173" s="119"/>
     </row>
     <row r="174" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A174" s="172" t="s">
+      <c r="A174" s="178" t="s">
         <v>754</v>
       </c>
-      <c r="B174" s="173"/>
-      <c r="C174" s="173"/>
-      <c r="D174" s="173"/>
-      <c r="E174" s="174"/>
+      <c r="B174" s="179"/>
+      <c r="C174" s="179"/>
+      <c r="D174" s="179"/>
+      <c r="E174" s="180"/>
       <c r="F174" s="129" t="s">
         <v>755</v>
       </c>
@@ -15589,18 +15607,6 @@
     </row>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="A234:E234"/>
-    <mergeCell ref="A195:E195"/>
-    <mergeCell ref="A199:E199"/>
-    <mergeCell ref="A206:E206"/>
-    <mergeCell ref="A217:E217"/>
-    <mergeCell ref="A223:E223"/>
-    <mergeCell ref="A59:E59"/>
-    <mergeCell ref="A2:E2"/>
-    <mergeCell ref="A10:E10"/>
-    <mergeCell ref="A14:E14"/>
-    <mergeCell ref="A24:E24"/>
-    <mergeCell ref="A43:E43"/>
     <mergeCell ref="A183:E183"/>
     <mergeCell ref="A166:E166"/>
     <mergeCell ref="A64:E64"/>
@@ -15611,6 +15617,18 @@
     <mergeCell ref="A155:E155"/>
     <mergeCell ref="A94:E94"/>
     <mergeCell ref="A174:E174"/>
+    <mergeCell ref="A59:E59"/>
+    <mergeCell ref="A2:E2"/>
+    <mergeCell ref="A10:E10"/>
+    <mergeCell ref="A14:E14"/>
+    <mergeCell ref="A24:E24"/>
+    <mergeCell ref="A43:E43"/>
+    <mergeCell ref="A234:E234"/>
+    <mergeCell ref="A195:E195"/>
+    <mergeCell ref="A199:E199"/>
+    <mergeCell ref="A206:E206"/>
+    <mergeCell ref="A217:E217"/>
+    <mergeCell ref="A223:E223"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -15618,11 +15636,11 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E7FE5E2-8B99-45DF-8804-30523FDA4B3A}">
-  <dimension ref="A1:F55"/>
+  <dimension ref="A1:F56"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F23" sqref="F23"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -15737,49 +15755,47 @@
       </c>
     </row>
     <row r="8" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A8" s="91" t="s">
+      <c r="B8" s="205" t="s">
+        <v>1466</v>
+      </c>
+      <c r="C8" s="206" t="s">
+        <v>1467</v>
+      </c>
+      <c r="D8" s="205"/>
+      <c r="E8" s="207" t="s">
+        <v>1468</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A9" s="91" t="s">
         <v>898</v>
       </c>
-      <c r="B8" s="92" t="s">
+      <c r="B9" s="159" t="s">
         <v>907</v>
       </c>
-      <c r="C8" s="93" t="s">
+      <c r="C9" s="93" t="s">
         <v>908</v>
       </c>
-      <c r="D8" s="92" t="s">
+      <c r="D9" s="92" t="s">
         <v>400</v>
       </c>
-      <c r="E8" s="85" t="s">
+      <c r="E9" s="85" t="s">
         <v>909</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A9" s="18" t="s">
+    <row r="10" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A10" s="18" t="s">
         <v>721</v>
       </c>
-      <c r="B9" s="28" t="s">
+      <c r="B10" s="28" t="s">
         <v>910</v>
       </c>
-      <c r="C9" s="27" t="s">
+      <c r="C10" s="27" t="s">
         <v>911</v>
       </c>
-      <c r="D9" s="18"/>
-      <c r="E9" s="46" t="s">
+      <c r="D10" s="18"/>
+      <c r="E10" s="46" t="s">
         <v>912</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A10" s="19" t="s">
-        <v>913</v>
-      </c>
-      <c r="B10" s="19" t="s">
-        <v>914</v>
-      </c>
-      <c r="C10" s="21" t="s">
-        <v>152</v>
-      </c>
-      <c r="E10" s="46" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="16" x14ac:dyDescent="0.2">
@@ -15787,56 +15803,53 @@
         <v>913</v>
       </c>
       <c r="B11" s="19" t="s">
+        <v>914</v>
+      </c>
+      <c r="C11" s="21" t="s">
+        <v>152</v>
+      </c>
+      <c r="E11" s="46" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A12" s="19" t="s">
+        <v>913</v>
+      </c>
+      <c r="B12" s="19" t="s">
         <v>915</v>
       </c>
-      <c r="C11" s="21" t="s">
+      <c r="C12" s="21" t="s">
         <v>140</v>
       </c>
-      <c r="E11" s="46" t="s">
+      <c r="E12" s="46" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="12" spans="1:6" s="24" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="184" t="s">
+    <row r="13" spans="1:6" s="24" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="184" t="s">
         <v>916</v>
       </c>
-      <c r="B12" s="185"/>
-      <c r="C12" s="185"/>
-      <c r="D12" s="185"/>
-      <c r="E12" s="186"/>
-    </row>
-    <row r="13" spans="1:6" ht="48" x14ac:dyDescent="0.2">
-      <c r="A13" s="19" t="s">
+      <c r="B13" s="185"/>
+      <c r="C13" s="185"/>
+      <c r="D13" s="185"/>
+      <c r="E13" s="186"/>
+    </row>
+    <row r="14" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+      <c r="A14" s="19" t="s">
         <v>239</v>
       </c>
-      <c r="B13" s="19" t="s">
+      <c r="B14" s="19" t="s">
         <v>917</v>
       </c>
-      <c r="C13" s="21" t="s">
+      <c r="C14" s="21" t="s">
         <v>918</v>
       </c>
-      <c r="D13" s="5" t="s">
+      <c r="D14" s="5" t="s">
         <v>919</v>
       </c>
-      <c r="E13" s="46" t="s">
+      <c r="E14" s="46" t="s">
         <v>920</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="32" x14ac:dyDescent="0.2">
-      <c r="A14" s="19" t="s">
-        <v>84</v>
-      </c>
-      <c r="B14" s="19" t="s">
-        <v>921</v>
-      </c>
-      <c r="C14" s="21" t="s">
-        <v>922</v>
-      </c>
-      <c r="D14" s="19" t="s">
-        <v>923</v>
-      </c>
-      <c r="E14" s="46" t="s">
-        <v>924</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="32" x14ac:dyDescent="0.2">
@@ -15844,484 +15857,484 @@
         <v>84</v>
       </c>
       <c r="B15" s="19" t="s">
-        <v>925</v>
+        <v>921</v>
       </c>
       <c r="C15" s="21" t="s">
-        <v>926</v>
+        <v>922</v>
       </c>
       <c r="D15" s="19" t="s">
         <v>923</v>
       </c>
       <c r="E15" s="46" t="s">
-        <v>927</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+        <v>924</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A16" s="19" t="s">
         <v>84</v>
       </c>
       <c r="B16" s="19" t="s">
-        <v>928</v>
+        <v>925</v>
       </c>
       <c r="C16" s="21" t="s">
-        <v>929</v>
+        <v>926</v>
       </c>
       <c r="D16" s="19" t="s">
         <v>923</v>
       </c>
       <c r="E16" s="46" t="s">
+        <v>927</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A17" s="19" t="s">
+        <v>84</v>
+      </c>
+      <c r="B17" s="19" t="s">
+        <v>928</v>
+      </c>
+      <c r="C17" s="21" t="s">
+        <v>929</v>
+      </c>
+      <c r="D17" s="19" t="s">
+        <v>923</v>
+      </c>
+      <c r="E17" s="46" t="s">
         <v>930</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="48" x14ac:dyDescent="0.2">
-      <c r="A17" s="91" t="s">
+    <row r="18" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+      <c r="A18" s="91" t="s">
         <v>84</v>
       </c>
-      <c r="B17" s="92" t="s">
+      <c r="B18" s="92" t="s">
         <v>931</v>
       </c>
-      <c r="C17" s="151" t="s">
+      <c r="C18" s="151" t="s">
         <v>1322</v>
       </c>
-      <c r="D17" s="92" t="s">
+      <c r="D18" s="92" t="s">
         <v>923</v>
       </c>
-      <c r="E17" s="152" t="s">
+      <c r="E18" s="152" t="s">
         <v>1323</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" ht="80" x14ac:dyDescent="0.2">
-      <c r="A18" s="18" t="s">
-        <v>406</v>
-      </c>
-      <c r="B18" s="28" t="s">
-        <v>932</v>
-      </c>
-      <c r="C18" s="27"/>
-      <c r="D18" s="18" t="s">
-        <v>933</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="80" x14ac:dyDescent="0.2">
       <c r="A19" s="18" t="s">
-        <v>409</v>
+        <v>406</v>
       </c>
       <c r="B19" s="28" t="s">
-        <v>934</v>
+        <v>932</v>
       </c>
       <c r="C19" s="27"/>
       <c r="D19" s="18" t="s">
+        <v>933</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="80" x14ac:dyDescent="0.2">
+      <c r="A20" s="18" t="s">
+        <v>409</v>
+      </c>
+      <c r="B20" s="28" t="s">
+        <v>934</v>
+      </c>
+      <c r="C20" s="27"/>
+      <c r="D20" s="18" t="s">
         <v>935</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="193" t="s">
+    <row r="21" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="193" t="s">
         <v>936</v>
       </c>
-      <c r="B20" s="194"/>
-      <c r="C20" s="194"/>
-      <c r="D20" s="194"/>
-      <c r="E20" s="195"/>
-    </row>
-    <row r="21" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A21" s="5" t="s">
+      <c r="B21" s="194"/>
+      <c r="C21" s="194"/>
+      <c r="D21" s="194"/>
+      <c r="E21" s="195"/>
+    </row>
+    <row r="22" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A22" s="5" t="s">
         <v>937</v>
       </c>
-      <c r="B21" s="91" t="s">
+      <c r="B22" s="91" t="s">
         <v>938</v>
       </c>
-      <c r="C21" s="6" t="s">
+      <c r="C22" s="6" t="s">
         <v>939</v>
-      </c>
-      <c r="D21" s="80"/>
-      <c r="E21" s="81" t="s">
-        <v>940</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A22" s="80" t="s">
-        <v>941</v>
-      </c>
-      <c r="B22" s="94" t="s">
-        <v>942</v>
-      </c>
-      <c r="C22" s="82" t="s">
-        <v>943</v>
       </c>
       <c r="D22" s="80"/>
       <c r="E22" s="81" t="s">
-        <v>944</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" ht="64" x14ac:dyDescent="0.2">
+        <v>940</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A23" s="80" t="s">
-        <v>945</v>
+        <v>941</v>
       </c>
       <c r="B23" s="94" t="s">
-        <v>946</v>
+        <v>942</v>
       </c>
       <c r="C23" s="82" t="s">
-        <v>1459</v>
+        <v>943</v>
       </c>
       <c r="D23" s="80"/>
       <c r="E23" s="81" t="s">
+        <v>944</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="64" x14ac:dyDescent="0.2">
+      <c r="A24" s="80" t="s">
+        <v>945</v>
+      </c>
+      <c r="B24" s="94" t="s">
+        <v>946</v>
+      </c>
+      <c r="C24" s="82" t="s">
+        <v>1459</v>
+      </c>
+      <c r="D24" s="80"/>
+      <c r="E24" s="81" t="s">
         <v>1460</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A24" s="190" t="s">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A25" s="190" t="s">
         <v>947</v>
       </c>
-      <c r="B24" s="191"/>
-      <c r="C24" s="191"/>
-      <c r="D24" s="191"/>
-      <c r="E24" s="192"/>
-    </row>
-    <row r="25" spans="1:6" ht="32" x14ac:dyDescent="0.2">
-      <c r="A25" s="18" t="s">
+      <c r="B25" s="191"/>
+      <c r="C25" s="191"/>
+      <c r="D25" s="191"/>
+      <c r="E25" s="192"/>
+    </row>
+    <row r="26" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+      <c r="A26" s="18" t="s">
         <v>239</v>
       </c>
-      <c r="B25" s="28" t="s">
+      <c r="B26" s="28" t="s">
         <v>948</v>
       </c>
-      <c r="C25" s="27" t="s">
+      <c r="C26" s="27" t="s">
         <v>949</v>
       </c>
-      <c r="D25" s="18"/>
-      <c r="E25" s="46" t="s">
+      <c r="D26" s="18"/>
+      <c r="E26" s="46" t="s">
         <v>950</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A26" s="181" t="s">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A27" s="181" t="s">
         <v>951</v>
       </c>
-      <c r="B26" s="182"/>
-      <c r="C26" s="182"/>
-      <c r="D26" s="182"/>
-      <c r="E26" s="183"/>
-    </row>
-    <row r="27" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A27" s="18" t="s">
+      <c r="B27" s="182"/>
+      <c r="C27" s="182"/>
+      <c r="D27" s="182"/>
+      <c r="E27" s="183"/>
+    </row>
+    <row r="28" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A28" s="18" t="s">
         <v>239</v>
       </c>
-      <c r="B27" s="28" t="s">
+      <c r="B28" s="28" t="s">
         <v>952</v>
       </c>
-      <c r="C27" s="27" t="s">
+      <c r="C28" s="27" t="s">
         <v>953</v>
       </c>
-      <c r="D27" s="18"/>
-      <c r="E27" s="46" t="s">
+      <c r="D28" s="18"/>
+      <c r="E28" s="46" t="s">
         <v>954</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A28" s="181" t="s">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A29" s="181" t="s">
         <v>955</v>
       </c>
-      <c r="B28" s="182"/>
-      <c r="C28" s="182"/>
-      <c r="D28" s="182"/>
-      <c r="E28" s="183"/>
-    </row>
-    <row r="29" spans="1:6" ht="112" x14ac:dyDescent="0.2">
-      <c r="A29" s="91" t="s">
+      <c r="B29" s="182"/>
+      <c r="C29" s="182"/>
+      <c r="D29" s="182"/>
+      <c r="E29" s="183"/>
+    </row>
+    <row r="30" spans="1:6" ht="112" x14ac:dyDescent="0.2">
+      <c r="A30" s="91" t="s">
         <v>239</v>
       </c>
-      <c r="B29" s="92" t="s">
+      <c r="B30" s="92" t="s">
         <v>956</v>
       </c>
-      <c r="C29" s="93" t="s">
+      <c r="C30" s="93" t="s">
         <v>957</v>
       </c>
-      <c r="D29" s="92" t="s">
+      <c r="D30" s="92" t="s">
         <v>958</v>
       </c>
-      <c r="E29" s="85" t="s">
+      <c r="E30" s="85" t="s">
         <v>959</v>
       </c>
-      <c r="F29" s="71" t="s">
+      <c r="F30" s="71" t="s">
         <v>960</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="48" x14ac:dyDescent="0.2">
-      <c r="A30" s="94" t="s">
+    <row r="31" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+      <c r="A31" s="94" t="s">
         <v>941</v>
       </c>
-      <c r="B30" s="95" t="s">
+      <c r="B31" s="95" t="s">
         <v>961</v>
       </c>
-      <c r="C30" s="96" t="s">
+      <c r="C31" s="96" t="s">
         <v>962</v>
       </c>
-      <c r="D30" s="95" t="s">
+      <c r="D31" s="95" t="s">
         <v>963</v>
       </c>
-      <c r="E30" s="89" t="s">
+      <c r="E31" s="89" t="s">
         <v>964</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="335" x14ac:dyDescent="0.2">
-      <c r="A31" s="94" t="s">
+    <row r="32" spans="1:6" ht="335" x14ac:dyDescent="0.2">
+      <c r="A32" s="94" t="s">
         <v>965</v>
       </c>
-      <c r="B31" s="95" t="s">
+      <c r="B32" s="95" t="s">
         <v>966</v>
       </c>
-      <c r="C31" s="96" t="s">
+      <c r="C32" s="96" t="s">
         <v>967</v>
       </c>
-      <c r="D31" s="95" t="s">
+      <c r="D32" s="95" t="s">
         <v>400</v>
       </c>
-      <c r="E31" s="89" t="s">
+      <c r="E32" s="89" t="s">
         <v>968</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="80" x14ac:dyDescent="0.2">
-      <c r="A32" s="19" t="s">
-        <v>257</v>
-      </c>
-      <c r="B32" s="19" t="s">
-        <v>969</v>
-      </c>
-      <c r="C32" s="21" t="s">
-        <v>1380</v>
-      </c>
-      <c r="E32" s="46" t="s">
-        <v>1381</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:6" ht="80" x14ac:dyDescent="0.2">
       <c r="A33" s="19" t="s">
         <v>257</v>
       </c>
       <c r="B33" s="19" t="s">
+        <v>969</v>
+      </c>
+      <c r="C33" s="21" t="s">
+        <v>1380</v>
+      </c>
+      <c r="E33" s="46" t="s">
+        <v>1381</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+      <c r="A34" s="19" t="s">
+        <v>257</v>
+      </c>
+      <c r="B34" s="19" t="s">
         <v>1382</v>
       </c>
-      <c r="C33" s="21" t="s">
+      <c r="C34" s="21" t="s">
         <v>1383</v>
       </c>
-      <c r="E33" s="46" t="s">
+      <c r="E34" s="46" t="s">
         <v>1384</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="48" x14ac:dyDescent="0.2">
-      <c r="A34" s="19" t="s">
+    <row r="35" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+      <c r="A35" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="B34" s="19" t="s">
+      <c r="B35" s="19" t="s">
         <v>970</v>
       </c>
-      <c r="C34" s="21" t="s">
+      <c r="C35" s="21" t="s">
         <v>971</v>
       </c>
-      <c r="D34" s="26" t="s">
+      <c r="D35" s="26" t="s">
         <v>972</v>
       </c>
-      <c r="E34" s="46" t="s">
+      <c r="E35" s="46" t="s">
         <v>973</v>
       </c>
     </row>
-    <row r="35" spans="1:6" ht="96" x14ac:dyDescent="0.2">
-      <c r="A35" s="18" t="s">
-        <v>406</v>
-      </c>
-      <c r="B35" s="28" t="s">
-        <v>974</v>
-      </c>
-      <c r="C35" s="27"/>
-      <c r="D35" s="18" t="s">
-        <v>975</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" ht="80" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:6" ht="96" x14ac:dyDescent="0.2">
       <c r="A36" s="18" t="s">
         <v>406</v>
       </c>
       <c r="B36" s="28" t="s">
-        <v>976</v>
+        <v>974</v>
       </c>
       <c r="C36" s="27"/>
       <c r="D36" s="18" t="s">
-        <v>977</v>
+        <v>975</v>
       </c>
     </row>
     <row r="37" spans="1:6" ht="80" x14ac:dyDescent="0.2">
       <c r="A37" s="18" t="s">
-        <v>409</v>
+        <v>406</v>
       </c>
       <c r="B37" s="28" t="s">
-        <v>978</v>
+        <v>976</v>
       </c>
       <c r="C37" s="27"/>
       <c r="D37" s="18" t="s">
+        <v>977</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" ht="80" x14ac:dyDescent="0.2">
+      <c r="A38" s="18" t="s">
+        <v>409</v>
+      </c>
+      <c r="B38" s="28" t="s">
+        <v>978</v>
+      </c>
+      <c r="C38" s="27"/>
+      <c r="D38" s="18" t="s">
         <v>979</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A38" s="181" t="s">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A39" s="181" t="s">
         <v>980</v>
       </c>
-      <c r="B38" s="182"/>
-      <c r="C38" s="182"/>
-      <c r="D38" s="182"/>
-      <c r="E38" s="183"/>
-    </row>
-    <row r="39" spans="1:6" ht="48" x14ac:dyDescent="0.2">
-      <c r="A39" s="19" t="s">
+      <c r="B39" s="182"/>
+      <c r="C39" s="182"/>
+      <c r="D39" s="182"/>
+      <c r="E39" s="183"/>
+    </row>
+    <row r="40" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+      <c r="A40" s="19" t="s">
         <v>239</v>
       </c>
-      <c r="B39" s="19" t="s">
+      <c r="B40" s="19" t="s">
         <v>981</v>
       </c>
-      <c r="C39" s="21" t="s">
+      <c r="C40" s="21" t="s">
         <v>982</v>
       </c>
-      <c r="D39" s="5" t="s">
+      <c r="D40" s="5" t="s">
         <v>983</v>
       </c>
-      <c r="E39" s="46" t="s">
+      <c r="E40" s="46" t="s">
         <v>984</v>
       </c>
     </row>
-    <row r="40" spans="1:6" ht="64" x14ac:dyDescent="0.2">
-      <c r="A40" s="18" t="s">
+    <row r="41" spans="1:6" ht="64" x14ac:dyDescent="0.2">
+      <c r="A41" s="18" t="s">
         <v>406</v>
       </c>
-      <c r="B40" s="28" t="s">
+      <c r="B41" s="28" t="s">
         <v>985</v>
-      </c>
-      <c r="C40" s="27"/>
-      <c r="D40" s="18" t="s">
-        <v>986</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" ht="80" x14ac:dyDescent="0.2">
-      <c r="A41" s="18" t="s">
-        <v>409</v>
-      </c>
-      <c r="B41" s="28" t="s">
-        <v>987</v>
       </c>
       <c r="C41" s="27"/>
       <c r="D41" s="18" t="s">
+        <v>986</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" ht="80" x14ac:dyDescent="0.2">
+      <c r="A42" s="18" t="s">
+        <v>409</v>
+      </c>
+      <c r="B42" s="28" t="s">
+        <v>987</v>
+      </c>
+      <c r="C42" s="27"/>
+      <c r="D42" s="18" t="s">
         <v>979</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A42" s="187" t="s">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A43" s="187" t="s">
         <v>988</v>
       </c>
-      <c r="B42" s="188"/>
-      <c r="C42" s="188"/>
-      <c r="D42" s="188"/>
-      <c r="E42" s="189"/>
-    </row>
-    <row r="43" spans="1:6" ht="96" x14ac:dyDescent="0.2">
-      <c r="A43" s="116" t="s">
+      <c r="B43" s="188"/>
+      <c r="C43" s="188"/>
+      <c r="D43" s="188"/>
+      <c r="E43" s="189"/>
+    </row>
+    <row r="44" spans="1:6" ht="96" x14ac:dyDescent="0.2">
+      <c r="A44" s="116" t="s">
         <v>239</v>
       </c>
-      <c r="B43" s="116" t="s">
+      <c r="B44" s="116" t="s">
         <v>989</v>
       </c>
-      <c r="C43" s="21" t="s">
+      <c r="C44" s="21" t="s">
         <v>847</v>
       </c>
-      <c r="D43" s="116" t="s">
+      <c r="D44" s="116" t="s">
         <v>990</v>
       </c>
-      <c r="E43" s="46" t="s">
+      <c r="E44" s="46" t="s">
         <v>849</v>
       </c>
-      <c r="F43" s="72" t="s">
+      <c r="F44" s="72" t="s">
         <v>991</v>
       </c>
     </row>
-    <row r="44" spans="1:6" ht="80" x14ac:dyDescent="0.2">
-      <c r="A44" s="116" t="s">
+    <row r="45" spans="1:6" ht="80" x14ac:dyDescent="0.2">
+      <c r="A45" s="116" t="s">
         <v>364</v>
       </c>
-      <c r="B44" s="116" t="s">
+      <c r="B45" s="116" t="s">
         <v>992</v>
       </c>
-      <c r="C44" s="21" t="s">
+      <c r="C45" s="21" t="s">
         <v>905</v>
       </c>
-      <c r="D44" s="116" t="s">
+      <c r="D45" s="116" t="s">
         <v>993</v>
       </c>
-      <c r="E44" s="46" t="s">
+      <c r="E45" s="46" t="s">
         <v>906</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" ht="48" x14ac:dyDescent="0.2">
-      <c r="A45" s="116" t="s">
-        <v>257</v>
-      </c>
-      <c r="B45" s="116" t="s">
-        <v>994</v>
-      </c>
-      <c r="C45" s="62" t="s">
-        <v>1373</v>
-      </c>
-      <c r="D45" s="116" t="s">
-        <v>995</v>
-      </c>
-      <c r="E45" s="46" t="s">
-        <v>1374</v>
       </c>
     </row>
     <row r="46" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A46" s="116" t="s">
-        <v>378</v>
+        <v>257</v>
       </c>
       <c r="B46" s="116" t="s">
-        <v>996</v>
-      </c>
-      <c r="C46" s="21" t="s">
-        <v>997</v>
-      </c>
-      <c r="D46" s="121" t="s">
-        <v>998</v>
+        <v>994</v>
+      </c>
+      <c r="C46" s="62" t="s">
+        <v>1373</v>
+      </c>
+      <c r="D46" s="116" t="s">
+        <v>995</v>
       </c>
       <c r="E46" s="46" t="s">
-        <v>997</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" ht="64" x14ac:dyDescent="0.2">
+        <v>1374</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A47" s="116" t="s">
         <v>378</v>
       </c>
       <c r="B47" s="116" t="s">
-        <v>999</v>
+        <v>996</v>
       </c>
       <c r="C47" s="21" t="s">
-        <v>1000</v>
+        <v>997</v>
       </c>
       <c r="D47" s="121" t="s">
-        <v>1001</v>
+        <v>998</v>
       </c>
       <c r="E47" s="46" t="s">
-        <v>1002</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+        <v>997</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" ht="64" x14ac:dyDescent="0.2">
       <c r="A48" s="116" t="s">
         <v>378</v>
       </c>
       <c r="B48" s="116" t="s">
-        <v>1003</v>
+        <v>999</v>
       </c>
       <c r="C48" s="21" t="s">
-        <v>1004</v>
+        <v>1000</v>
       </c>
       <c r="D48" s="121" t="s">
-        <v>1005</v>
+        <v>1001</v>
       </c>
       <c r="E48" s="46" t="s">
-        <v>1006</v>
+        <v>1002</v>
       </c>
     </row>
     <row r="49" spans="1:6" ht="48" x14ac:dyDescent="0.2">
@@ -16329,64 +16342,64 @@
         <v>378</v>
       </c>
       <c r="B49" s="116" t="s">
+        <v>1003</v>
+      </c>
+      <c r="C49" s="21" t="s">
+        <v>1004</v>
+      </c>
+      <c r="D49" s="121" t="s">
+        <v>1005</v>
+      </c>
+      <c r="E49" s="46" t="s">
+        <v>1006</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+      <c r="A50" s="116" t="s">
+        <v>378</v>
+      </c>
+      <c r="B50" s="116" t="s">
         <v>1007</v>
       </c>
-      <c r="C49" s="21" t="s">
+      <c r="C50" s="21" t="s">
         <v>1008</v>
       </c>
-      <c r="D49" s="121" t="s">
+      <c r="D50" s="121" t="s">
         <v>1009</v>
       </c>
-      <c r="E49" s="46" t="s">
+      <c r="E50" s="46" t="s">
         <v>1010</v>
       </c>
     </row>
-    <row r="50" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A50" s="91" t="s">
+    <row r="51" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A51" s="91" t="s">
         <v>378</v>
       </c>
-      <c r="B50" s="92" t="s">
+      <c r="B51" s="92" t="s">
         <v>1011</v>
       </c>
-      <c r="C50" s="93" t="s">
+      <c r="C51" s="93" t="s">
         <v>1012</v>
       </c>
-      <c r="D50" s="101" t="s">
+      <c r="D51" s="101" t="s">
         <v>400</v>
       </c>
-      <c r="E50" s="85" t="s">
+      <c r="E51" s="85" t="s">
         <v>1013</v>
       </c>
     </row>
-    <row r="51" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A51" s="19" t="s">
+    <row r="52" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A52" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="B51" s="19" t="s">
+      <c r="B52" s="19" t="s">
         <v>1014</v>
       </c>
-      <c r="C51" s="21" t="s">
+      <c r="C52" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="E51" s="46" t="s">
+      <c r="E52" s="46" t="s">
         <v>36</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" ht="48" x14ac:dyDescent="0.2">
-      <c r="A52" s="19" t="s">
-        <v>1015</v>
-      </c>
-      <c r="B52" s="19" t="s">
-        <v>1016</v>
-      </c>
-      <c r="C52" s="21" t="s">
-        <v>1017</v>
-      </c>
-      <c r="D52" s="19" t="s">
-        <v>1018</v>
-      </c>
-      <c r="F52" s="71" t="s">
-        <v>893</v>
       </c>
     </row>
     <row r="53" spans="1:6" ht="48" x14ac:dyDescent="0.2">
@@ -16394,10 +16407,10 @@
         <v>1015</v>
       </c>
       <c r="B53" s="19" t="s">
-        <v>1019</v>
+        <v>1016</v>
       </c>
       <c r="C53" s="21" t="s">
-        <v>1020</v>
+        <v>1017</v>
       </c>
       <c r="D53" s="19" t="s">
         <v>1018</v>
@@ -16407,17 +16420,17 @@
       </c>
     </row>
     <row r="54" spans="1:6" ht="48" x14ac:dyDescent="0.2">
-      <c r="A54" s="116" t="s">
-        <v>378</v>
-      </c>
-      <c r="B54" s="116" t="s">
-        <v>1021</v>
+      <c r="A54" s="19" t="s">
+        <v>1015</v>
+      </c>
+      <c r="B54" s="19" t="s">
+        <v>1019</v>
       </c>
       <c r="C54" s="21" t="s">
-        <v>1022</v>
-      </c>
-      <c r="D54" s="121" t="s">
-        <v>1023</v>
+        <v>1020</v>
+      </c>
+      <c r="D54" s="19" t="s">
+        <v>1018</v>
       </c>
       <c r="F54" s="71" t="s">
         <v>893</v>
@@ -16428,28 +16441,45 @@
         <v>378</v>
       </c>
       <c r="B55" s="116" t="s">
-        <v>1024</v>
+        <v>1021</v>
       </c>
       <c r="C55" s="21" t="s">
-        <v>1025</v>
+        <v>1022</v>
       </c>
       <c r="D55" s="121" t="s">
-        <v>1026</v>
+        <v>1023</v>
       </c>
       <c r="F55" s="71" t="s">
         <v>893</v>
       </c>
     </row>
+    <row r="56" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+      <c r="A56" s="116" t="s">
+        <v>378</v>
+      </c>
+      <c r="B56" s="116" t="s">
+        <v>1024</v>
+      </c>
+      <c r="C56" s="21" t="s">
+        <v>1025</v>
+      </c>
+      <c r="D56" s="121" t="s">
+        <v>1026</v>
+      </c>
+      <c r="F56" s="71" t="s">
+        <v>893</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="8">
-    <mergeCell ref="A28:E28"/>
-    <mergeCell ref="A38:E38"/>
-    <mergeCell ref="A12:E12"/>
-    <mergeCell ref="A42:E42"/>
+    <mergeCell ref="A29:E29"/>
+    <mergeCell ref="A39:E39"/>
+    <mergeCell ref="A13:E13"/>
+    <mergeCell ref="A43:E43"/>
     <mergeCell ref="A2:E2"/>
-    <mergeCell ref="A24:E24"/>
-    <mergeCell ref="A26:E26"/>
-    <mergeCell ref="A20:E20"/>
+    <mergeCell ref="A25:E25"/>
+    <mergeCell ref="A27:E27"/>
+    <mergeCell ref="A21:E21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -16460,7 +16490,7 @@
   <dimension ref="A1:F75"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
@@ -17635,6 +17665,56 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Readyforteam_x003f_ xmlns="565e1b1d-057e-4d85-b896-01a5881d8a45">false</Readyforteam_x003f_>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <SharedWithUsers xmlns="bf601f31-63a1-4825-9216-91d773c5ef9c">
+      <UserInfo>
+        <DisplayName>Erika Osti</DisplayName>
+        <AccountId>534</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Penny Johnson</DisplayName>
+        <AccountId>489</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Ben Childs</DisplayName>
+        <AccountId>643</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Thomas Leeds</DisplayName>
+        <AccountId>459</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Kasmyn Chen</DisplayName>
+        <AccountId>532</AccountId>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="565e1b1d-057e-4d85-b896-01a5881d8a45">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="2799d30d-6731-4efe-ac9b-c4895a8828d9" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010096D84A54A9CD274097F17166F184737D" ma:contentTypeVersion="21" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="2fd95a4cfdf4f2f51219070f5dff16a8">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="565e1b1d-057e-4d85-b896-01a5881d8a45" xmlns:ns3="bf601f31-63a1-4825-9216-91d773c5ef9c" xmlns:ns4="2799d30d-6731-4efe-ac9b-c4895a8828d9" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f7499f6f4dc8ad2a533df04863f63fa7" ns1:_="" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -17911,57 +17991,28 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{017ACE96-8143-486E-8436-7787F6B96F4A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="565e1b1d-057e-4d85-b896-01a5881d8a45"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="bf601f31-63a1-4825-9216-91d773c5ef9c"/>
+    <ds:schemaRef ds:uri="2799d30d-6731-4efe-ac9b-c4895a8828d9"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Readyforteam_x003f_ xmlns="565e1b1d-057e-4d85-b896-01a5881d8a45">false</Readyforteam_x003f_>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <SharedWithUsers xmlns="bf601f31-63a1-4825-9216-91d773c5ef9c">
-      <UserInfo>
-        <DisplayName>Erika Osti</DisplayName>
-        <AccountId>534</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Penny Johnson</DisplayName>
-        <AccountId>489</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Ben Childs</DisplayName>
-        <AccountId>643</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Thomas Leeds</DisplayName>
-        <AccountId>459</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Kasmyn Chen</DisplayName>
-        <AccountId>532</AccountId>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="565e1b1d-057e-4d85-b896-01a5881d8a45">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="2799d30d-6731-4efe-ac9b-c4895a8828d9" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8D7CE8C7-18DC-484F-8376-ED09F13D44C8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EAFDB110-4046-4E72-A1EF-1908ABEC3151}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -17980,25 +18031,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8D7CE8C7-18DC-484F-8376-ED09F13D44C8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{017ACE96-8143-486E-8436-7787F6B96F4A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="565e1b1d-057e-4d85-b896-01a5881d8a45"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="bf601f31-63a1-4825-9216-91d773c5ef9c"/>
-    <ds:schemaRef ds:uri="2799d30d-6731-4efe-ac9b-c4895a8828d9"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Making the declaration wording changes in V11bi and fixing a typo in V10-1.
</commit_message>
<xml_diff>
--- a/app/data/MCCD-localisation.xlsx
+++ b/app/data/MCCD-localisation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/JALAT/GIT/medical-certificate-of-cause-of-death/app/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA006F86-786F-4147-85DE-366AAF404C0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DA6ED16-19CD-0544-BFDD-0826DCBCEDA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="14020" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="14020" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Using this document" sheetId="8" r:id="rId1"/>
@@ -69,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2235" uniqueCount="1497">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2233" uniqueCount="1495">
   <si>
     <r>
       <rPr>
@@ -5099,15 +5099,6 @@
     <t>meScrutinyDeclarationContent</t>
   </si>
   <si>
-    <t>I am a duly appointed medical examiner and following scrutiny I confirm that the cause of death is as stated on the certificate.</t>
-  </si>
-  <si>
-    <t>ME Scrutiny - Declaration content.</t>
-  </si>
-  <si>
-    <t>Rwyf yn archwiliwr meddygol a benodwyd yn briodol ac yn dilyn craffu rwy’n cadarnhau bod achos y farwolaeth fel y’i nodir ar y dystysgrif.</t>
-  </si>
-  <si>
     <t>meScrutinyReadyForRegistrar</t>
   </si>
   <si>
@@ -5124,9 +5115,6 @@
   </si>
   <si>
     <t>meCertDeclarationContent</t>
-  </si>
-  <si>
-    <t>ME Cert - Declaration content.</t>
   </si>
   <si>
     <t>meCertDeclarationValidationSummaryNoTick</t>
@@ -5764,12 +5752,6 @@
     <t>1(a) Disease or condition leading directly to death</t>
   </si>
   <si>
-    <t>I am a duly appointed medical examiner and following scrutiny I confirm to the best of my knowledge and belief that the cause of death is as stated on the certificate.</t>
-  </si>
-  <si>
-    <t>Rwy'n arholwr meddygol a benodwyd yn briodol ac ar ôl craffu rwy'n cadarnhau hyd eithaf fy ngwybodaeth a'm cred bod achos y farwolaeth fel y nodir ar y dystysgrif.</t>
-  </si>
-  <si>
     <t>Select age unit</t>
   </si>
   <si>
@@ -5869,7 +5851,19 @@
     <t>Ni allem ddod o hyd i gyfeiriad sy'n cyd-fynd &lt;strong&gt;[query]&lt;/strong&gt;. Chwiliwch eto neu rhowch y cyfeiriad â llaw.</t>
   </si>
   <si>
-    <t>051</t>
+    <t>I am a duly appointed medical examiner and following scrutiny I confirm that the cause of death is as stated in this certificate to the best of my knowledge and belief.</t>
+  </si>
+  <si>
+    <t>Rwy'n arholwr meddygol a benodwyd yn briodol ac ar ôl craffu rwy'n cadarnhau bod achos y farwolaeth fel y nodir yn y dystysgrif hon hyd eithaf fy ngwybodaeth a'm cred.</t>
+  </si>
+  <si>
+    <t>I am a duly appointed medical examiner and following my review I confirm that the cause of death is as stated in this certificate to the best of my knowledge and belief.</t>
+  </si>
+  <si>
+    <t>Rwy'n arholwr meddygol a benodwyd yn briodol ac yn dilyn fy adolygiad rwy'n cadarnhau bod achos y farwolaeth fel y nodir yn y dystysgrif hon hyd eithaf fy ngwybodaeth a'm cred.</t>
+  </si>
+  <si>
+    <t>052</t>
   </si>
 </sst>
 </file>
@@ -6345,7 +6339,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="216">
+  <cellXfs count="217">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -6885,6 +6879,15 @@
     <xf numFmtId="0" fontId="13" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -6903,15 +6906,6 @@
     <xf numFmtId="0" fontId="13" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
@@ -6983,6 +6977,9 @@
     </xf>
     <xf numFmtId="0" fontId="13" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -8134,8 +8131,8 @@
   <dimension ref="A1:F24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C15" sqref="C15"/>
+      <pane ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -8177,13 +8174,13 @@
         <v>1230</v>
       </c>
       <c r="C2" s="151" t="s">
-        <v>1397</v>
+        <v>1393</v>
       </c>
       <c r="D2" s="92" t="s">
         <v>1231</v>
       </c>
       <c r="E2" s="152" t="s">
-        <v>1401</v>
+        <v>1397</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="80" x14ac:dyDescent="0.2">
@@ -8211,13 +8208,13 @@
         <v>1237</v>
       </c>
       <c r="C4" s="158" t="s">
-        <v>1398</v>
+        <v>1394</v>
       </c>
       <c r="D4" s="95" t="s">
         <v>400</v>
       </c>
       <c r="E4" s="155" t="s">
-        <v>1400</v>
+        <v>1396</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="60.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -8279,30 +8276,28 @@
         <v>1242</v>
       </c>
       <c r="C8" s="158" t="s">
-        <v>1397</v>
+        <v>1393</v>
       </c>
       <c r="D8" s="95" t="s">
         <v>1243</v>
       </c>
       <c r="E8" s="155" t="s">
-        <v>1401</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="64" x14ac:dyDescent="0.2">
+        <v>1397</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="80" x14ac:dyDescent="0.2">
       <c r="A9" s="94" t="s">
         <v>1232</v>
       </c>
       <c r="B9" s="95" t="s">
         <v>1244</v>
       </c>
-      <c r="C9" s="96" t="s">
-        <v>1245</v>
-      </c>
-      <c r="D9" s="95" t="s">
-        <v>1246</v>
-      </c>
-      <c r="E9" s="89" t="s">
-        <v>1247</v>
+      <c r="C9" s="158" t="s">
+        <v>1490</v>
+      </c>
+      <c r="D9" s="216"/>
+      <c r="E9" s="155" t="s">
+        <v>1491</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="16" x14ac:dyDescent="0.2">
@@ -8310,16 +8305,16 @@
         <v>747</v>
       </c>
       <c r="B10" s="95" t="s">
-        <v>1248</v>
+        <v>1245</v>
       </c>
       <c r="C10" s="158" t="s">
-        <v>1398</v>
+        <v>1394</v>
       </c>
       <c r="D10" s="95" t="s">
         <v>400</v>
       </c>
       <c r="E10" s="155" t="s">
-        <v>1400</v>
+        <v>1396</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -8327,7 +8322,7 @@
         <v>406</v>
       </c>
       <c r="B11" s="105" t="s">
-        <v>1249</v>
+        <v>1246</v>
       </c>
       <c r="C11" s="106" t="s">
         <v>400</v>
@@ -8344,7 +8339,7 @@
         <v>409</v>
       </c>
       <c r="B12" s="105" t="s">
-        <v>1250</v>
+        <v>1247</v>
       </c>
       <c r="C12" s="106" t="s">
         <v>400</v>
@@ -8378,33 +8373,31 @@
         <v>239</v>
       </c>
       <c r="B14" s="95" t="s">
-        <v>1251</v>
+        <v>1248</v>
       </c>
       <c r="C14" s="158" t="s">
-        <v>1397</v>
+        <v>1393</v>
       </c>
       <c r="D14" s="95" t="s">
-        <v>1252</v>
+        <v>1249</v>
       </c>
       <c r="E14" s="155" t="s">
-        <v>1399</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="80" x14ac:dyDescent="0.2">
+        <v>1395</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="96" x14ac:dyDescent="0.2">
       <c r="A15" s="94" t="s">
         <v>1232</v>
       </c>
       <c r="B15" s="95" t="s">
-        <v>1253</v>
+        <v>1250</v>
       </c>
       <c r="C15" s="158" t="s">
-        <v>1461</v>
-      </c>
-      <c r="D15" s="95" t="s">
-        <v>1254</v>
-      </c>
+        <v>1492</v>
+      </c>
+      <c r="D15" s="216"/>
       <c r="E15" s="155" t="s">
-        <v>1462</v>
+        <v>1493</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="48" x14ac:dyDescent="0.2">
@@ -8412,7 +8405,7 @@
         <v>406</v>
       </c>
       <c r="B16" s="105" t="s">
-        <v>1255</v>
+        <v>1251</v>
       </c>
       <c r="C16" s="106" t="s">
         <v>400</v>
@@ -8429,7 +8422,7 @@
         <v>409</v>
       </c>
       <c r="B17" s="105" t="s">
-        <v>1256</v>
+        <v>1252</v>
       </c>
       <c r="C17" s="106" t="s">
         <v>400</v>
@@ -8446,16 +8439,16 @@
         <v>14</v>
       </c>
       <c r="B18" s="95" t="s">
-        <v>1257</v>
+        <v>1253</v>
       </c>
       <c r="C18" s="158" t="s">
-        <v>1398</v>
+        <v>1394</v>
       </c>
       <c r="D18" s="95" t="s">
         <v>400</v>
       </c>
       <c r="E18" s="155" t="s">
-        <v>1400</v>
+        <v>1396</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -8480,16 +8473,16 @@
         <v>239</v>
       </c>
       <c r="B20" s="95" t="s">
-        <v>1258</v>
+        <v>1254</v>
       </c>
       <c r="C20" s="158" t="s">
-        <v>1430</v>
+        <v>1426</v>
       </c>
       <c r="D20" s="95" t="s">
         <v>1231</v>
       </c>
       <c r="E20" s="155" t="s">
-        <v>1431</v>
+        <v>1427</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="64" x14ac:dyDescent="0.2">
@@ -8497,16 +8490,16 @@
         <v>1232</v>
       </c>
       <c r="B21" s="95" t="s">
-        <v>1259</v>
+        <v>1255</v>
       </c>
       <c r="C21" s="158" t="s">
-        <v>1429</v>
+        <v>1425</v>
       </c>
       <c r="D21" s="95" t="s">
-        <v>1260</v>
+        <v>1256</v>
       </c>
       <c r="E21" s="155" t="s">
-        <v>1432</v>
+        <v>1428</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -8514,16 +8507,16 @@
         <v>747</v>
       </c>
       <c r="B22" s="95" t="s">
-        <v>1261</v>
+        <v>1257</v>
       </c>
       <c r="C22" s="158" t="s">
-        <v>1433</v>
+        <v>1429</v>
       </c>
       <c r="D22" s="95" t="s">
         <v>400</v>
       </c>
       <c r="E22" s="155" t="s">
-        <v>1434</v>
+        <v>1430</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="48" x14ac:dyDescent="0.2">
@@ -8531,7 +8524,7 @@
         <v>406</v>
       </c>
       <c r="B23" s="105" t="s">
-        <v>1262</v>
+        <v>1258</v>
       </c>
       <c r="C23" s="106" t="s">
         <v>400</v>
@@ -8548,7 +8541,7 @@
         <v>409</v>
       </c>
       <c r="B24" s="105" t="s">
-        <v>1263</v>
+        <v>1259</v>
       </c>
       <c r="C24" s="106" t="s">
         <v>400</v>
@@ -8607,7 +8600,7 @@
     </row>
     <row r="2" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="214" t="s">
-        <v>1264</v>
+        <v>1260</v>
       </c>
       <c r="B2" s="215"/>
       <c r="C2" s="215"/>
@@ -8620,16 +8613,16 @@
         <v>239</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>1265</v>
+        <v>1261</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>1266</v>
+        <v>1262</v>
       </c>
       <c r="D3" s="5" t="s">
         <v>1212</v>
       </c>
       <c r="E3" s="37" t="s">
-        <v>1267</v>
+        <v>1263</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="32" x14ac:dyDescent="0.2">
@@ -8637,13 +8630,13 @@
         <v>257</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>1268</v>
+        <v>1264</v>
       </c>
       <c r="C4" s="59" t="s">
-        <v>1420</v>
+        <v>1416</v>
       </c>
       <c r="E4" s="37" t="s">
-        <v>1269</v>
+        <v>1265</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="16" x14ac:dyDescent="0.2">
@@ -8651,13 +8644,13 @@
         <v>250</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>1270</v>
+        <v>1266</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>1271</v>
+        <v>1267</v>
       </c>
       <c r="E5" s="37" t="s">
-        <v>1272</v>
+        <v>1268</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="80" x14ac:dyDescent="0.2">
@@ -8665,13 +8658,13 @@
         <v>257</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>1273</v>
+        <v>1269</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>1418</v>
+        <v>1414</v>
       </c>
       <c r="E6" s="37" t="s">
-        <v>1419</v>
+        <v>1415</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="32" x14ac:dyDescent="0.2">
@@ -8679,112 +8672,112 @@
         <v>250</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>1274</v>
+        <v>1270</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>1275</v>
+        <v>1271</v>
       </c>
       <c r="E7" s="37" t="s">
-        <v>1276</v>
+        <v>1272</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
-        <v>1277</v>
+        <v>1273</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>1278</v>
+        <v>1274</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>1406</v>
+        <v>1402</v>
       </c>
       <c r="E8" s="37" t="s">
-        <v>1407</v>
+        <v>1403</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
-        <v>1279</v>
+        <v>1275</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>1280</v>
+        <v>1276</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>1281</v>
+        <v>1277</v>
       </c>
       <c r="E9" s="37" t="s">
-        <v>1282</v>
+        <v>1278</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
+        <v>1275</v>
+      </c>
+      <c r="B10" s="5" t="s">
         <v>1279</v>
       </c>
-      <c r="B10" s="5" t="s">
-        <v>1283</v>
-      </c>
       <c r="C10" s="6" t="s">
-        <v>1284</v>
+        <v>1280</v>
       </c>
       <c r="E10" s="37" t="s">
-        <v>1285</v>
+        <v>1281</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
-        <v>1279</v>
+        <v>1275</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>1286</v>
+        <v>1282</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>1287</v>
+        <v>1283</v>
       </c>
       <c r="E11" s="37" t="s">
-        <v>1288</v>
+        <v>1284</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="5" t="s">
-        <v>1279</v>
+        <v>1275</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>1289</v>
+        <v>1285</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>1290</v>
+        <v>1286</v>
       </c>
       <c r="E12" s="37" t="s">
-        <v>1291</v>
+        <v>1287</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="s">
-        <v>1279</v>
+        <v>1275</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>1292</v>
+        <v>1288</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>1293</v>
+        <v>1289</v>
       </c>
       <c r="E13" s="37" t="s">
-        <v>1294</v>
+        <v>1290</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A14" s="5" t="s">
-        <v>1277</v>
+        <v>1273</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>1295</v>
+        <v>1291</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>1404</v>
+        <v>1400</v>
       </c>
       <c r="D14" s="1"/>
       <c r="E14" s="37" t="s">
-        <v>1405</v>
+        <v>1401</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="32" x14ac:dyDescent="0.2">
@@ -8792,14 +8785,14 @@
         <v>940</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>1296</v>
+        <v>1292</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>1297</v>
+        <v>1293</v>
       </c>
       <c r="D15" s="1"/>
       <c r="E15" s="37" t="s">
-        <v>1298</v>
+        <v>1294</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="16" x14ac:dyDescent="0.2">
@@ -8807,34 +8800,34 @@
         <v>14</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>1299</v>
+        <v>1295</v>
       </c>
       <c r="C16" s="74" t="s">
-        <v>1300</v>
+        <v>1296</v>
       </c>
       <c r="D16" s="18"/>
       <c r="E16" s="37" t="s">
-        <v>1301</v>
+        <v>1297</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A17" s="5" t="s">
-        <v>1302</v>
+        <v>1298</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>1303</v>
+        <v>1299</v>
       </c>
       <c r="C17" s="75" t="s">
-        <v>1304</v>
+        <v>1300</v>
       </c>
       <c r="D17" s="18"/>
       <c r="E17" s="37" t="s">
-        <v>1305</v>
+        <v>1301</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="214" t="s">
-        <v>1306</v>
+        <v>1302</v>
       </c>
       <c r="B18" s="215"/>
       <c r="C18" s="215"/>
@@ -8847,16 +8840,16 @@
         <v>239</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>1309</v>
+        <v>1305</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>1307</v>
+        <v>1303</v>
       </c>
       <c r="D19" s="5" t="s">
         <v>1212</v>
       </c>
       <c r="E19" s="37" t="s">
-        <v>1308</v>
+        <v>1304</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="96" x14ac:dyDescent="0.2">
@@ -8864,13 +8857,13 @@
         <v>257</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>1310</v>
+        <v>1306</v>
       </c>
       <c r="C20" s="59" t="s">
-        <v>1375</v>
+        <v>1371</v>
       </c>
       <c r="E20" s="37" t="s">
-        <v>1377</v>
+        <v>1373</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="16" x14ac:dyDescent="0.2">
@@ -8878,13 +8871,13 @@
         <v>250</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>1311</v>
+        <v>1307</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>1271</v>
+        <v>1267</v>
       </c>
       <c r="E21" s="37" t="s">
-        <v>1272</v>
+        <v>1268</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="80" x14ac:dyDescent="0.2">
@@ -8892,13 +8885,13 @@
         <v>257</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>1312</v>
+        <v>1308</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>1376</v>
+        <v>1372</v>
       </c>
       <c r="E22" s="37" t="s">
-        <v>1378</v>
+        <v>1374</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
@@ -8922,7 +8915,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D3" sqref="D3"/>
+      <selection pane="bottomLeft" activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -8962,13 +8955,13 @@
         <v>7</v>
       </c>
       <c r="C2" s="100" t="s">
-        <v>1496</v>
+        <v>1494</v>
       </c>
       <c r="D2" s="98" t="s">
         <v>8</v>
       </c>
       <c r="E2" s="99" t="s">
-        <v>1496</v>
+        <v>1494</v>
       </c>
       <c r="F2" s="98"/>
     </row>
@@ -8986,7 +8979,7 @@
         <v>12</v>
       </c>
       <c r="E3" s="37" t="s">
-        <v>1374</v>
+        <v>1370</v>
       </c>
       <c r="F3" s="5" t="s">
         <v>13</v>
@@ -9051,7 +9044,7 @@
     <row r="7" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="5"/>
       <c r="B7" s="5" t="s">
-        <v>1471</v>
+        <v>1465</v>
       </c>
       <c r="C7" s="6" t="s">
         <v>349</v>
@@ -9851,10 +9844,10 @@
     <row r="53" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A53" s="86"/>
       <c r="B53" s="163" t="s">
-        <v>1421</v>
+        <v>1417</v>
       </c>
       <c r="C53" s="164" t="s">
-        <v>1422</v>
+        <v>1418</v>
       </c>
       <c r="D53" s="86"/>
       <c r="E53" s="165" t="s">
@@ -9970,7 +9963,7 @@
       </c>
       <c r="D61" s="86"/>
       <c r="E61" s="165" t="s">
-        <v>1437</v>
+        <v>1433</v>
       </c>
       <c r="F61" s="86"/>
     </row>
@@ -10057,46 +10050,46 @@
     <row r="68" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A68" s="86"/>
       <c r="B68" s="163" t="s">
-        <v>1425</v>
+        <v>1421</v>
       </c>
       <c r="C68" s="164" t="s">
-        <v>1426</v>
+        <v>1422</v>
       </c>
       <c r="D68" s="86"/>
       <c r="E68" s="165" t="s">
-        <v>1427</v>
+        <v>1423</v>
       </c>
       <c r="F68" s="166" t="s">
-        <v>1428</v>
+        <v>1424</v>
       </c>
     </row>
     <row r="69" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A69" s="86"/>
       <c r="B69" s="163" t="s">
-        <v>1423</v>
+        <v>1419</v>
       </c>
       <c r="C69" s="164" t="s">
-        <v>1304</v>
+        <v>1300</v>
       </c>
       <c r="D69" s="86"/>
       <c r="E69" s="165" t="s">
-        <v>1424</v>
+        <v>1420</v>
       </c>
     </row>
     <row r="70" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="B70" s="1" t="s">
-        <v>1323</v>
+        <v>1319</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>1324</v>
+        <v>1320</v>
       </c>
       <c r="E70" s="40" t="s">
-        <v>1326</v>
+        <v>1322</v>
       </c>
     </row>
     <row r="71" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="B71" s="1" t="s">
-        <v>1325</v>
+        <v>1321</v>
       </c>
       <c r="C71" s="2" t="s">
         <v>76</v>
@@ -10107,13 +10100,13 @@
     </row>
     <row r="72" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="B72" s="1" t="s">
-        <v>1438</v>
+        <v>1434</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>1439</v>
+        <v>1435</v>
       </c>
       <c r="E72" s="40" t="s">
-        <v>1440</v>
+        <v>1436</v>
       </c>
     </row>
   </sheetData>
@@ -10408,14 +10401,14 @@
         <v>239</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>1348</v>
+        <v>1344</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>1349</v>
+        <v>1345</v>
       </c>
       <c r="D2" s="5"/>
       <c r="E2" s="43" t="s">
-        <v>1357</v>
+        <v>1353</v>
       </c>
       <c r="F2" s="1"/>
     </row>
@@ -10424,19 +10417,19 @@
         <v>480</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>1350</v>
+        <v>1346</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>1351</v>
+        <v>1347</v>
       </c>
       <c r="D3" s="5"/>
       <c r="E3" s="43" t="s">
-        <v>1358</v>
+        <v>1354</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="180" t="s">
-        <v>1352</v>
+        <v>1348</v>
       </c>
       <c r="B4" s="181"/>
       <c r="C4" s="181"/>
@@ -10448,14 +10441,14 @@
         <v>239</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>1353</v>
+        <v>1349</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>1355</v>
+        <v>1351</v>
       </c>
       <c r="D5" s="5"/>
       <c r="E5" s="43" t="s">
-        <v>1359</v>
+        <v>1355</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="96" x14ac:dyDescent="0.2">
@@ -10463,14 +10456,14 @@
         <v>480</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>1354</v>
+        <v>1350</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>1356</v>
+        <v>1352</v>
       </c>
       <c r="D6" s="5"/>
       <c r="E6" s="43" t="s">
-        <v>1360</v>
+        <v>1356</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
@@ -10691,7 +10684,7 @@
         <v>239</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>1363</v>
+        <v>1359</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>272</v>
@@ -10715,7 +10708,7 @@
         <v>242</v>
       </c>
       <c r="E4" s="43" t="s">
-        <v>1364</v>
+        <v>1360</v>
       </c>
       <c r="F4" s="68" t="s">
         <v>276</v>
@@ -10729,13 +10722,13 @@
         <v>277</v>
       </c>
       <c r="C5" s="52" t="s">
-        <v>1417</v>
+        <v>1413</v>
       </c>
       <c r="D5" s="66" t="s">
         <v>278</v>
       </c>
       <c r="E5" s="156" t="s">
-        <v>1435</v>
+        <v>1431</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>279</v>
@@ -10749,13 +10742,13 @@
         <v>280</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>1369</v>
+        <v>1365</v>
       </c>
       <c r="D6" s="67" t="s">
         <v>281</v>
       </c>
       <c r="E6" s="157" t="s">
-        <v>1436</v>
+        <v>1432</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="160" x14ac:dyDescent="0.2">
@@ -10766,13 +10759,13 @@
         <v>282</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>1370</v>
+        <v>1366</v>
       </c>
       <c r="D7" s="67" t="s">
         <v>283</v>
       </c>
       <c r="E7" s="157" t="s">
-        <v>1371</v>
+        <v>1367</v>
       </c>
       <c r="F7" s="68" t="s">
         <v>284</v>
@@ -10974,7 +10967,7 @@
         <v>332</v>
       </c>
       <c r="C19" s="64" t="s">
-        <v>1361</v>
+        <v>1357</v>
       </c>
       <c r="D19" s="7" t="s">
         <v>333</v>
@@ -11108,17 +11101,17 @@
     </row>
     <row r="27" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A27" s="5" t="s">
-        <v>1367</v>
+        <v>1363</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>1368</v>
+        <v>1364</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>1365</v>
+        <v>1361</v>
       </c>
       <c r="D27" s="5"/>
       <c r="E27" s="37" t="s">
-        <v>1366</v>
+        <v>1362</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
@@ -11195,13 +11188,13 @@
       </c>
     </row>
     <row r="2" spans="1:6" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="183" t="s">
+      <c r="A2" s="186" t="s">
         <v>363</v>
       </c>
-      <c r="B2" s="184"/>
-      <c r="C2" s="184"/>
-      <c r="D2" s="184"/>
-      <c r="E2" s="185"/>
+      <c r="B2" s="187"/>
+      <c r="C2" s="187"/>
+      <c r="D2" s="187"/>
+      <c r="E2" s="188"/>
       <c r="F2" s="33"/>
     </row>
     <row r="3" spans="1:6" ht="48" x14ac:dyDescent="0.2">
@@ -11329,13 +11322,13 @@
       <c r="F9" s="119"/>
     </row>
     <row r="10" spans="1:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="186" t="s">
+      <c r="A10" s="189" t="s">
         <v>392</v>
       </c>
-      <c r="B10" s="187"/>
-      <c r="C10" s="187"/>
-      <c r="D10" s="187"/>
-      <c r="E10" s="188"/>
+      <c r="B10" s="190"/>
+      <c r="C10" s="190"/>
+      <c r="D10" s="190"/>
+      <c r="E10" s="191"/>
       <c r="F10" s="119"/>
     </row>
     <row r="11" spans="1:6" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -11364,13 +11357,13 @@
         <v>397</v>
       </c>
       <c r="C12" s="153" t="s">
-        <v>1327</v>
+        <v>1323</v>
       </c>
       <c r="D12" s="84" t="s">
         <v>398</v>
       </c>
       <c r="E12" s="152" t="s">
-        <v>1328</v>
+        <v>1324</v>
       </c>
       <c r="F12" s="86"/>
     </row>
@@ -11382,13 +11375,13 @@
         <v>399</v>
       </c>
       <c r="C13" s="154" t="s">
-        <v>1329</v>
+        <v>1325</v>
       </c>
       <c r="D13" s="88" t="s">
         <v>400</v>
       </c>
       <c r="E13" s="155" t="s">
-        <v>1330</v>
+        <v>1326</v>
       </c>
       <c r="F13" s="86"/>
     </row>
@@ -11544,7 +11537,7 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" s="180" t="s">
-        <v>1468</v>
+        <v>1462</v>
       </c>
       <c r="B24" s="181"/>
       <c r="C24" s="181"/>
@@ -11557,10 +11550,10 @@
         <v>239</v>
       </c>
       <c r="B25" s="132" t="s">
-        <v>1469</v>
+        <v>1463</v>
       </c>
       <c r="C25" s="133" t="s">
-        <v>1470</v>
+        <v>1464</v>
       </c>
       <c r="D25" s="114"/>
       <c r="E25" s="131"/>
@@ -11571,14 +11564,14 @@
         <v>373</v>
       </c>
       <c r="B26" s="132" t="s">
-        <v>1472</v>
+        <v>1466</v>
       </c>
       <c r="C26" s="133" t="s">
-        <v>1480</v>
+        <v>1474</v>
       </c>
       <c r="D26" s="114"/>
       <c r="E26" s="131" t="s">
-        <v>1481</v>
+        <v>1475</v>
       </c>
       <c r="F26" s="119"/>
     </row>
@@ -11587,30 +11580,30 @@
         <v>373</v>
       </c>
       <c r="B27" s="132" t="s">
-        <v>1474</v>
+        <v>1468</v>
       </c>
       <c r="C27" s="133" t="s">
-        <v>1473</v>
+        <v>1467</v>
       </c>
       <c r="D27" s="114"/>
       <c r="E27" s="131" t="s">
-        <v>1475</v>
+        <v>1469</v>
       </c>
       <c r="F27" s="119"/>
     </row>
     <row r="28" spans="1:6" s="178" customFormat="1" ht="96" x14ac:dyDescent="0.2">
       <c r="A28" s="172" t="s">
-        <v>1479</v>
+        <v>1473</v>
       </c>
       <c r="B28" s="173" t="s">
-        <v>1476</v>
+        <v>1470</v>
       </c>
       <c r="C28" s="174" t="s">
-        <v>1477</v>
+        <v>1471</v>
       </c>
       <c r="D28" s="175"/>
       <c r="E28" s="176" t="s">
-        <v>1478</v>
+        <v>1472</v>
       </c>
       <c r="F28" s="177"/>
     </row>
@@ -11925,14 +11918,14 @@
         <v>480</v>
       </c>
       <c r="B50" s="116" t="s">
-        <v>1347</v>
+        <v>1343</v>
       </c>
       <c r="C50" s="59" t="s">
-        <v>1443</v>
+        <v>1439</v>
       </c>
       <c r="D50" s="116"/>
       <c r="E50" s="120" t="s">
-        <v>1444</v>
+        <v>1440</v>
       </c>
       <c r="F50" s="119"/>
     </row>
@@ -11941,10 +11934,10 @@
         <v>480</v>
       </c>
       <c r="B51" s="116" t="s">
-        <v>1442</v>
+        <v>1438</v>
       </c>
       <c r="C51" s="59" t="s">
-        <v>1346</v>
+        <v>1342</v>
       </c>
       <c r="D51" s="116"/>
       <c r="E51" s="120" t="s">
@@ -11960,11 +11953,11 @@
         <v>481</v>
       </c>
       <c r="C52" s="59" t="s">
-        <v>1441</v>
+        <v>1437</v>
       </c>
       <c r="D52" s="116"/>
       <c r="E52" s="120" t="s">
-        <v>1447</v>
+        <v>1443</v>
       </c>
       <c r="F52" s="119"/>
     </row>
@@ -12168,13 +12161,13 @@
         <v>511</v>
       </c>
       <c r="C66" s="117" t="s">
-        <v>1445</v>
+        <v>1441</v>
       </c>
       <c r="D66" s="116" t="s">
         <v>512</v>
       </c>
       <c r="E66" s="120" t="s">
-        <v>1446</v>
+        <v>1442</v>
       </c>
       <c r="F66" s="119"/>
     </row>
@@ -12192,7 +12185,7 @@
         <v>516</v>
       </c>
       <c r="E67" s="120" t="s">
-        <v>1339</v>
+        <v>1335</v>
       </c>
       <c r="F67" s="119"/>
     </row>
@@ -12201,14 +12194,14 @@
         <v>513</v>
       </c>
       <c r="B68" s="116" t="s">
-        <v>1336</v>
+        <v>1332</v>
       </c>
       <c r="C68" s="117" t="s">
-        <v>1338</v>
+        <v>1334</v>
       </c>
       <c r="D68" s="116"/>
       <c r="E68" s="120" t="s">
-        <v>1337</v>
+        <v>1333</v>
       </c>
       <c r="F68" s="119"/>
     </row>
@@ -12301,14 +12294,14 @@
         <v>480</v>
       </c>
       <c r="B75" s="125" t="s">
-        <v>1448</v>
+        <v>1444</v>
       </c>
       <c r="C75" s="167" t="s">
-        <v>1449</v>
+        <v>1445</v>
       </c>
       <c r="D75" s="125"/>
       <c r="E75" s="131" t="s">
-        <v>1450</v>
+        <v>1446</v>
       </c>
       <c r="F75" s="119"/>
     </row>
@@ -12428,13 +12421,13 @@
         <v>546</v>
       </c>
       <c r="C82" s="158" t="s">
-        <v>1463</v>
+        <v>1457</v>
       </c>
       <c r="D82" s="95" t="s">
         <v>400</v>
       </c>
       <c r="E82" s="155" t="s">
-        <v>1464</v>
+        <v>1458</v>
       </c>
       <c r="F82" s="119"/>
     </row>
@@ -12560,11 +12553,11 @@
         <v>564</v>
       </c>
       <c r="C91" s="117" t="s">
-        <v>1386</v>
+        <v>1382</v>
       </c>
       <c r="D91" s="116"/>
       <c r="E91" s="120" t="s">
-        <v>1387</v>
+        <v>1383</v>
       </c>
       <c r="F91" s="119"/>
     </row>
@@ -12672,11 +12665,11 @@
         <v>583</v>
       </c>
       <c r="C98" s="117" t="s">
-        <v>1384</v>
+        <v>1380</v>
       </c>
       <c r="D98" s="116"/>
       <c r="E98" s="120" t="s">
-        <v>1385</v>
+        <v>1381</v>
       </c>
       <c r="F98" s="119"/>
     </row>
@@ -12718,11 +12711,11 @@
         <v>589</v>
       </c>
       <c r="C101" s="117" t="s">
-        <v>1402</v>
+        <v>1398</v>
       </c>
       <c r="D101" s="116"/>
       <c r="E101" s="120" t="s">
-        <v>1403</v>
+        <v>1399</v>
       </c>
       <c r="F101" s="86" t="s">
         <v>592</v>
@@ -12751,7 +12744,7 @@
         <v>84</v>
       </c>
       <c r="B103" s="159" t="s">
-        <v>1408</v>
+        <v>1404</v>
       </c>
       <c r="C103" s="93" t="s">
         <v>591</v>
@@ -12769,7 +12762,7 @@
         <v>84</v>
       </c>
       <c r="B104" s="159" t="s">
-        <v>1409</v>
+        <v>1405</v>
       </c>
       <c r="C104" s="93" t="s">
         <v>591</v>
@@ -12787,7 +12780,7 @@
         <v>84</v>
       </c>
       <c r="B105" s="160" t="s">
-        <v>1410</v>
+        <v>1406</v>
       </c>
       <c r="C105" s="161" t="s">
         <v>591</v>
@@ -12803,7 +12796,7 @@
         <v>84</v>
       </c>
       <c r="B106" s="160" t="s">
-        <v>1411</v>
+        <v>1407</v>
       </c>
       <c r="C106" s="161" t="s">
         <v>591</v>
@@ -12819,7 +12812,7 @@
         <v>84</v>
       </c>
       <c r="B107" s="160" t="s">
-        <v>1412</v>
+        <v>1408</v>
       </c>
       <c r="C107" s="161" t="s">
         <v>591</v>
@@ -13268,33 +13261,33 @@
     </row>
     <row r="137" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A137" s="116" t="s">
-        <v>1451</v>
+        <v>1447</v>
       </c>
       <c r="B137" s="116" t="s">
-        <v>1453</v>
+        <v>1449</v>
       </c>
       <c r="C137" s="117" t="s">
-        <v>1452</v>
+        <v>1448</v>
       </c>
       <c r="D137" s="116"/>
       <c r="E137" s="120" t="s">
-        <v>1456</v>
+        <v>1452</v>
       </c>
       <c r="F137" s="119"/>
     </row>
     <row r="138" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A138" s="116" t="s">
+        <v>1447</v>
+      </c>
+      <c r="B138" s="116" t="s">
         <v>1451</v>
       </c>
-      <c r="B138" s="116" t="s">
-        <v>1455</v>
-      </c>
       <c r="C138" s="117" t="s">
-        <v>1454</v>
+        <v>1450</v>
       </c>
       <c r="D138" s="116"/>
       <c r="E138" s="120" t="s">
-        <v>1457</v>
+        <v>1453</v>
       </c>
       <c r="F138" s="119"/>
     </row>
@@ -13530,7 +13523,7 @@
         <v>699</v>
       </c>
       <c r="C155" s="113" t="s">
-        <v>1314</v>
+        <v>1310</v>
       </c>
       <c r="D155" s="122" t="s">
         <v>700</v>
@@ -13618,7 +13611,7 @@
         <v>714</v>
       </c>
       <c r="C161" s="59" t="s">
-        <v>1313</v>
+        <v>1309</v>
       </c>
       <c r="D161" s="116" t="s">
         <v>715</v>
@@ -13649,14 +13642,14 @@
         <v>37</v>
       </c>
       <c r="B163" s="116" t="s">
-        <v>1315</v>
+        <v>1311</v>
       </c>
       <c r="C163" s="59" t="s">
-        <v>1317</v>
+        <v>1313</v>
       </c>
       <c r="D163" s="116"/>
       <c r="E163" s="120" t="s">
-        <v>1319</v>
+        <v>1315</v>
       </c>
       <c r="F163" s="119"/>
     </row>
@@ -13665,14 +13658,14 @@
         <v>37</v>
       </c>
       <c r="B164" s="116" t="s">
-        <v>1316</v>
+        <v>1312</v>
       </c>
       <c r="C164" s="59" t="s">
-        <v>1318</v>
+        <v>1314</v>
       </c>
       <c r="D164" s="116"/>
       <c r="E164" s="120" t="s">
-        <v>1320</v>
+        <v>1316</v>
       </c>
       <c r="F164" s="119"/>
     </row>
@@ -13893,13 +13886,13 @@
       </c>
     </row>
     <row r="179" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A179" s="189" t="s">
+      <c r="A179" s="183" t="s">
         <v>754</v>
       </c>
-      <c r="B179" s="190"/>
-      <c r="C179" s="190"/>
-      <c r="D179" s="190"/>
-      <c r="E179" s="191"/>
+      <c r="B179" s="184"/>
+      <c r="C179" s="184"/>
+      <c r="D179" s="184"/>
+      <c r="E179" s="185"/>
       <c r="F179" s="129" t="s">
         <v>758</v>
       </c>
@@ -13916,7 +13909,7 @@
       </c>
       <c r="D180" s="114"/>
       <c r="E180" s="131" t="s">
-        <v>1489</v>
+        <v>1483</v>
       </c>
       <c r="F180" s="129" t="s">
         <v>758</v>
@@ -13934,7 +13927,7 @@
       </c>
       <c r="D181" s="114"/>
       <c r="E181" s="131" t="s">
-        <v>1490</v>
+        <v>1484</v>
       </c>
       <c r="F181" s="129" t="s">
         <v>758</v>
@@ -13966,7 +13959,7 @@
       </c>
       <c r="D183" s="114"/>
       <c r="E183" s="131" t="s">
-        <v>1491</v>
+        <v>1485</v>
       </c>
       <c r="F183" s="129" t="s">
         <v>758</v>
@@ -13984,7 +13977,7 @@
       </c>
       <c r="D184" s="114"/>
       <c r="E184" s="131" t="s">
-        <v>1492</v>
+        <v>1486</v>
       </c>
       <c r="F184" s="129" t="s">
         <v>758</v>
@@ -14032,7 +14025,7 @@
     </row>
     <row r="188" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A188" s="180" t="s">
-        <v>1482</v>
+        <v>1476</v>
       </c>
       <c r="B188" s="181"/>
       <c r="C188" s="181"/>
@@ -14045,29 +14038,29 @@
         <v>239</v>
       </c>
       <c r="B189" s="132" t="s">
-        <v>1483</v>
+        <v>1477</v>
       </c>
       <c r="C189" s="133" t="s">
-        <v>1482</v>
+        <v>1476</v>
       </c>
       <c r="D189" s="114"/>
       <c r="E189" s="131" t="s">
-        <v>1486</v>
+        <v>1480</v>
       </c>
       <c r="F189" s="119"/>
     </row>
     <row r="190" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A190" s="1" t="s">
-        <v>1488</v>
+        <v>1482</v>
       </c>
       <c r="B190" s="1" t="s">
-        <v>1484</v>
+        <v>1478</v>
       </c>
       <c r="C190" s="2" t="s">
-        <v>1485</v>
+        <v>1479</v>
       </c>
       <c r="E190" s="40" t="s">
-        <v>1487</v>
+        <v>1481</v>
       </c>
     </row>
     <row r="191" spans="1:6" ht="48" x14ac:dyDescent="0.2">
@@ -14075,13 +14068,13 @@
         <v>257</v>
       </c>
       <c r="B191" s="1" t="s">
-        <v>1493</v>
+        <v>1487</v>
       </c>
       <c r="C191" s="2" t="s">
-        <v>1494</v>
+        <v>1488</v>
       </c>
       <c r="E191" s="40" t="s">
-        <v>1495</v>
+        <v>1489</v>
       </c>
     </row>
     <row r="192" spans="1:6" x14ac:dyDescent="0.2">
@@ -14386,13 +14379,13 @@
         <v>803</v>
       </c>
       <c r="C211" s="59" t="s">
-        <v>1331</v>
+        <v>1327</v>
       </c>
       <c r="D211" s="116" t="s">
         <v>804</v>
       </c>
       <c r="E211" s="120" t="s">
-        <v>1335</v>
+        <v>1331</v>
       </c>
       <c r="F211" s="119"/>
     </row>
@@ -14401,14 +14394,14 @@
         <v>480</v>
       </c>
       <c r="B212" s="116" t="s">
-        <v>1332</v>
+        <v>1328</v>
       </c>
       <c r="C212" s="59" t="s">
-        <v>1333</v>
+        <v>1329</v>
       </c>
       <c r="D212" s="116"/>
       <c r="E212" s="120" t="s">
-        <v>1334</v>
+        <v>1330</v>
       </c>
       <c r="F212" s="119"/>
     </row>
@@ -14508,11 +14501,11 @@
         <v>815</v>
       </c>
       <c r="C219" s="117" t="s">
-        <v>1342</v>
+        <v>1338</v>
       </c>
       <c r="D219" s="116"/>
       <c r="E219" s="120" t="s">
-        <v>1345</v>
+        <v>1341</v>
       </c>
       <c r="F219" s="119"/>
     </row>
@@ -14521,7 +14514,7 @@
         <v>723</v>
       </c>
       <c r="B220" s="116" t="s">
-        <v>1344</v>
+        <v>1340</v>
       </c>
       <c r="C220" s="117" t="s">
         <v>43</v>
@@ -14537,14 +14530,14 @@
         <v>32</v>
       </c>
       <c r="B221" s="116" t="s">
-        <v>1343</v>
+        <v>1339</v>
       </c>
       <c r="C221" s="134" t="s">
-        <v>1340</v>
+        <v>1336</v>
       </c>
       <c r="D221" s="116"/>
       <c r="E221" s="120" t="s">
-        <v>1341</v>
+        <v>1337</v>
       </c>
       <c r="F221" s="119"/>
     </row>
@@ -14916,13 +14909,13 @@
         <v>854</v>
       </c>
       <c r="C246" s="59" t="s">
-        <v>1372</v>
+        <v>1368</v>
       </c>
       <c r="D246" s="116" t="s">
         <v>855</v>
       </c>
       <c r="E246" s="120" t="s">
-        <v>1373</v>
+        <v>1369</v>
       </c>
       <c r="F246" s="119"/>
     </row>
@@ -15861,6 +15854,19 @@
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="A243:E243"/>
+    <mergeCell ref="A204:E204"/>
+    <mergeCell ref="A208:E208"/>
+    <mergeCell ref="A215:E215"/>
+    <mergeCell ref="A226:E226"/>
+    <mergeCell ref="A232:E232"/>
+    <mergeCell ref="A64:E64"/>
+    <mergeCell ref="A2:E2"/>
+    <mergeCell ref="A10:E10"/>
+    <mergeCell ref="A14:E14"/>
+    <mergeCell ref="A29:E29"/>
+    <mergeCell ref="A48:E48"/>
+    <mergeCell ref="A24:E24"/>
     <mergeCell ref="A192:E192"/>
     <mergeCell ref="A171:E171"/>
     <mergeCell ref="A69:E69"/>
@@ -15872,19 +15878,6 @@
     <mergeCell ref="A99:E99"/>
     <mergeCell ref="A179:E179"/>
     <mergeCell ref="A188:E188"/>
-    <mergeCell ref="A64:E64"/>
-    <mergeCell ref="A2:E2"/>
-    <mergeCell ref="A10:E10"/>
-    <mergeCell ref="A14:E14"/>
-    <mergeCell ref="A29:E29"/>
-    <mergeCell ref="A48:E48"/>
-    <mergeCell ref="A24:E24"/>
-    <mergeCell ref="A243:E243"/>
-    <mergeCell ref="A204:E204"/>
-    <mergeCell ref="A208:E208"/>
-    <mergeCell ref="A215:E215"/>
-    <mergeCell ref="A226:E226"/>
-    <mergeCell ref="A232:E232"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -16012,14 +16005,14 @@
     </row>
     <row r="8" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="B8" s="168" t="s">
-        <v>1465</v>
+        <v>1459</v>
       </c>
       <c r="C8" s="169" t="s">
-        <v>1466</v>
+        <v>1460</v>
       </c>
       <c r="D8" s="168"/>
       <c r="E8" s="170" t="s">
-        <v>1467</v>
+        <v>1461</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="16" x14ac:dyDescent="0.2">
@@ -16167,13 +16160,13 @@
         <v>930</v>
       </c>
       <c r="C18" s="151" t="s">
-        <v>1321</v>
+        <v>1317</v>
       </c>
       <c r="D18" s="92" t="s">
         <v>922</v>
       </c>
       <c r="E18" s="152" t="s">
-        <v>1322</v>
+        <v>1318</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="80" x14ac:dyDescent="0.2">
@@ -16247,11 +16240,11 @@
         <v>945</v>
       </c>
       <c r="C24" s="82" t="s">
-        <v>1458</v>
+        <v>1454</v>
       </c>
       <c r="D24" s="80"/>
       <c r="E24" s="81" t="s">
-        <v>1459</v>
+        <v>1455</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
@@ -16373,10 +16366,10 @@
         <v>968</v>
       </c>
       <c r="C33" s="21" t="s">
-        <v>1379</v>
+        <v>1375</v>
       </c>
       <c r="E33" s="46" t="s">
-        <v>1380</v>
+        <v>1376</v>
       </c>
     </row>
     <row r="34" spans="1:6" ht="32" x14ac:dyDescent="0.2">
@@ -16384,13 +16377,13 @@
         <v>257</v>
       </c>
       <c r="B34" s="19" t="s">
-        <v>1381</v>
+        <v>1377</v>
       </c>
       <c r="C34" s="21" t="s">
-        <v>1382</v>
+        <v>1378</v>
       </c>
       <c r="E34" s="46" t="s">
-        <v>1383</v>
+        <v>1379</v>
       </c>
     </row>
     <row r="35" spans="1:6" ht="48" x14ac:dyDescent="0.2">
@@ -16550,13 +16543,13 @@
         <v>993</v>
       </c>
       <c r="C46" s="62" t="s">
-        <v>1372</v>
+        <v>1368</v>
       </c>
       <c r="D46" s="116" t="s">
         <v>994</v>
       </c>
       <c r="E46" s="46" t="s">
-        <v>1373</v>
+        <v>1369</v>
       </c>
     </row>
     <row r="47" spans="1:6" ht="48" x14ac:dyDescent="0.2">
@@ -16949,23 +16942,23 @@
         <v>1060</v>
       </c>
       <c r="E11" s="138" t="s">
-        <v>1396</v>
+        <v>1392</v>
       </c>
       <c r="F11" s="135"/>
     </row>
     <row r="12" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A12" s="136" t="s">
-        <v>1392</v>
+        <v>1388</v>
       </c>
       <c r="B12" s="136" t="s">
-        <v>1393</v>
+        <v>1389</v>
       </c>
       <c r="C12" s="137" t="s">
-        <v>1394</v>
+        <v>1390</v>
       </c>
       <c r="D12" s="136"/>
       <c r="E12" s="138" t="s">
-        <v>1395</v>
+        <v>1391</v>
       </c>
       <c r="F12" s="135"/>
     </row>
@@ -16977,7 +16970,7 @@
         <v>1061</v>
       </c>
       <c r="C13" s="137" t="s">
-        <v>1460</v>
+        <v>1456</v>
       </c>
       <c r="D13" s="136" t="s">
         <v>1062</v>
@@ -17023,7 +17016,7 @@
         <v>1067</v>
       </c>
       <c r="C16" s="137" t="s">
-        <v>1388</v>
+        <v>1384</v>
       </c>
       <c r="D16" s="136" t="s">
         <v>1068</v>
@@ -17041,7 +17034,7 @@
         <v>1070</v>
       </c>
       <c r="C17" s="137" t="s">
-        <v>1389</v>
+        <v>1385</v>
       </c>
       <c r="D17" s="136" t="s">
         <v>1071</v>
@@ -17059,7 +17052,7 @@
         <v>1073</v>
       </c>
       <c r="C18" s="137" t="s">
-        <v>1390</v>
+        <v>1386</v>
       </c>
       <c r="D18" s="136" t="s">
         <v>1074</v>
@@ -17199,17 +17192,17 @@
     </row>
     <row r="28" spans="1:6" ht="64" x14ac:dyDescent="0.2">
       <c r="A28" s="136" t="s">
-        <v>1392</v>
+        <v>1388</v>
       </c>
       <c r="B28" s="136" t="s">
-        <v>1391</v>
+        <v>1387</v>
       </c>
       <c r="C28" s="137" t="s">
-        <v>1413</v>
+        <v>1409</v>
       </c>
       <c r="D28" s="136"/>
       <c r="E28" s="138" t="s">
-        <v>1415</v>
+        <v>1411</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="32" x14ac:dyDescent="0.2">
@@ -17220,13 +17213,13 @@
         <v>1099</v>
       </c>
       <c r="C29" s="137" t="s">
-        <v>1414</v>
+        <v>1410</v>
       </c>
       <c r="D29" s="136" t="s">
         <v>1100</v>
       </c>
       <c r="E29" s="138" t="s">
-        <v>1416</v>
+        <v>1412</v>
       </c>
     </row>
     <row r="30" spans="1:6" s="13" customFormat="1" x14ac:dyDescent="0.2">
@@ -17469,7 +17462,7 @@
         <v>1137</v>
       </c>
       <c r="C45" s="62" t="s">
-        <v>1362</v>
+        <v>1358</v>
       </c>
       <c r="D45" s="5" t="s">
         <v>1138</v>
@@ -17561,13 +17554,13 @@
         <v>1149</v>
       </c>
       <c r="C51" s="62" t="s">
-        <v>1372</v>
+        <v>1368</v>
       </c>
       <c r="D51" s="116" t="s">
         <v>994</v>
       </c>
       <c r="E51" s="63" t="s">
-        <v>1373</v>
+        <v>1369</v>
       </c>
     </row>
     <row r="52" spans="1:6" s="30" customFormat="1" ht="48" x14ac:dyDescent="0.2">
@@ -18198,6 +18191,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <Readyforteam_x003f_ xmlns="565e1b1d-057e-4d85-b896-01a5881d8a45">false</Readyforteam_x003f_>
@@ -18238,15 +18240,6 @@
 </p:properties>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EAFDB110-4046-4E72-A1EF-1908ABEC3151}">
   <ds:schemaRefs>
@@ -18269,6 +18262,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8D7CE8C7-18DC-484F-8376-ED09F13D44C8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{017ACE96-8143-486E-8436-7787F6B96F4A}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -18279,12 +18280,4 @@
     <ds:schemaRef ds:uri="2799d30d-6731-4efe-ac9b-c4895a8828d9"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8D7CE8C7-18DC-484F-8376-ED09F13D44C8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Adding Welsh translations to GMC number.
</commit_message>
<xml_diff>
--- a/app/data/MCCD-localisation.xlsx
+++ b/app/data/MCCD-localisation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/JALAT/GIT/medical-certificate-of-cause-of-death/app/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0EA5F2D-91E3-924E-B24E-393C9DDFC3A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B91DA744-8E87-BF46-8DD6-C1D362CDBD34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="14020" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -69,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2237" uniqueCount="1498">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2258" uniqueCount="1516">
   <si>
     <r>
       <rPr>
@@ -5863,9 +5863,6 @@
     <t>Rwy'n arholwr meddygol a benodwyd yn briodol ac yn dilyn fy adolygiad rwy'n cadarnhau bod achos y farwolaeth fel y nodir yn y dystysgrif hon hyd eithaf fy ngwybodaeth a'm cred.</t>
   </si>
   <si>
-    <t>053</t>
-  </si>
-  <si>
     <t>dpdConfirmDetailsPrimaryQualification</t>
   </si>
   <si>
@@ -5873,6 +5870,63 @@
   </si>
   <si>
     <t>Cymhwyster cynradd</t>
+  </si>
+  <si>
+    <t>GMC number page</t>
+  </si>
+  <si>
+    <t>gmcPageTitle</t>
+  </si>
+  <si>
+    <t>gmcConfirmPageTitle</t>
+  </si>
+  <si>
+    <t>Confirm your GMC number</t>
+  </si>
+  <si>
+    <t>cta</t>
+  </si>
+  <si>
+    <t>gmcConfirmCTA</t>
+  </si>
+  <si>
+    <t>Use this number</t>
+  </si>
+  <si>
+    <t>link text</t>
+  </si>
+  <si>
+    <t>gmcConfirmLinkText</t>
+  </si>
+  <si>
+    <t>Change GMC number</t>
+  </si>
+  <si>
+    <t>Cadarnhau eich rhif GMC</t>
+  </si>
+  <si>
+    <t>Defnyddiwch y rhif hwn</t>
+  </si>
+  <si>
+    <t>Newid rhif GMC</t>
+  </si>
+  <si>
+    <t>What is your GMC number?</t>
+  </si>
+  <si>
+    <t>gmcHintText</t>
+  </si>
+  <si>
+    <t>Must be 7 digits long</t>
+  </si>
+  <si>
+    <t>Beth yw eich rhif GMC?</t>
+  </si>
+  <si>
+    <t>Rhaid iddo fod yn 7 digid o hyd</t>
+  </si>
+  <si>
+    <t>054</t>
   </si>
 </sst>
 </file>
@@ -6891,6 +6945,15 @@
     <xf numFmtId="0" fontId="13" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -6907,15 +6970,6 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -8924,7 +8978,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D3" sqref="D3"/>
+      <selection pane="bottomLeft" activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -8964,13 +9018,13 @@
         <v>7</v>
       </c>
       <c r="C2" s="100" t="s">
-        <v>1494</v>
+        <v>1515</v>
       </c>
       <c r="D2" s="98" t="s">
         <v>8</v>
       </c>
       <c r="E2" s="99" t="s">
-        <v>1494</v>
+        <v>1515</v>
       </c>
       <c r="F2" s="98"/>
     </row>
@@ -10373,7 +10427,7 @@
   <dimension ref="A1:F27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -10476,46 +10530,88 @@
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7" s="5"/>
-      <c r="B7" s="5"/>
-      <c r="C7" s="6"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="43"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8" s="5"/>
-      <c r="B8" s="5"/>
-      <c r="C8" s="6"/>
+      <c r="A7" s="181" t="s">
+        <v>1497</v>
+      </c>
+      <c r="B7" s="182"/>
+      <c r="C7" s="182"/>
+      <c r="D7" s="182"/>
+      <c r="E7" s="183"/>
+    </row>
+    <row r="8" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A8" s="5" t="s">
+        <v>239</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>1499</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>1500</v>
+      </c>
       <c r="D8" s="5"/>
-      <c r="E8" s="43"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9" s="5"/>
-      <c r="B9" s="5"/>
-      <c r="C9" s="6"/>
+      <c r="E8" s="43" t="s">
+        <v>1507</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A9" s="5" t="s">
+        <v>1501</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>1502</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>1503</v>
+      </c>
       <c r="D9" s="5"/>
-      <c r="E9" s="43"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10" s="5"/>
-      <c r="B10" s="5"/>
-      <c r="C10" s="6"/>
+      <c r="E9" s="43" t="s">
+        <v>1508</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A10" s="5" t="s">
+        <v>1504</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>1505</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>1506</v>
+      </c>
       <c r="D10" s="5"/>
-      <c r="E10" s="43"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11" s="5"/>
-      <c r="B11" s="5"/>
-      <c r="C11" s="6"/>
+      <c r="E10" s="43" t="s">
+        <v>1509</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A11" s="5" t="s">
+        <v>239</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>1498</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>1510</v>
+      </c>
       <c r="D11" s="5"/>
-      <c r="E11" s="43"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A12" s="5"/>
-      <c r="B12" s="5"/>
-      <c r="C12" s="6"/>
+      <c r="E11" s="43" t="s">
+        <v>1513</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A12" s="5" t="s">
+        <v>480</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>1511</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>1512</v>
+      </c>
       <c r="D12" s="5"/>
-      <c r="E12" s="43"/>
+      <c r="E12" s="43" t="s">
+        <v>1514</v>
+      </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="5"/>
@@ -10623,8 +10719,9 @@
       <c r="E27" s="43"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="A4:E4"/>
+    <mergeCell ref="A7:E7"/>
   </mergeCells>
   <phoneticPr fontId="27" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -11197,13 +11294,13 @@
       </c>
     </row>
     <row r="2" spans="1:6" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="184" t="s">
+      <c r="A2" s="187" t="s">
         <v>363</v>
       </c>
-      <c r="B2" s="185"/>
-      <c r="C2" s="185"/>
-      <c r="D2" s="185"/>
-      <c r="E2" s="186"/>
+      <c r="B2" s="188"/>
+      <c r="C2" s="188"/>
+      <c r="D2" s="188"/>
+      <c r="E2" s="189"/>
       <c r="F2" s="33"/>
     </row>
     <row r="3" spans="1:6" ht="48" x14ac:dyDescent="0.2">
@@ -11301,14 +11398,14 @@
         <v>378</v>
       </c>
       <c r="B8" s="119" t="s">
+        <v>1494</v>
+      </c>
+      <c r="C8" s="117" t="s">
         <v>1495</v>
-      </c>
-      <c r="C8" s="117" t="s">
-        <v>1496</v>
       </c>
       <c r="D8" s="121"/>
       <c r="E8" s="120" t="s">
-        <v>1497</v>
+        <v>1496</v>
       </c>
       <c r="F8" s="119"/>
     </row>
@@ -11347,13 +11444,13 @@
       <c r="F10" s="119"/>
     </row>
     <row r="11" spans="1:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="187" t="s">
+      <c r="A11" s="190" t="s">
         <v>392</v>
       </c>
-      <c r="B11" s="188"/>
-      <c r="C11" s="188"/>
-      <c r="D11" s="188"/>
-      <c r="E11" s="189"/>
+      <c r="B11" s="191"/>
+      <c r="C11" s="191"/>
+      <c r="D11" s="191"/>
+      <c r="E11" s="192"/>
       <c r="F11" s="119"/>
     </row>
     <row r="12" spans="1:6" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -13911,13 +14008,13 @@
       </c>
     </row>
     <row r="180" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A180" s="190" t="s">
+      <c r="A180" s="184" t="s">
         <v>754</v>
       </c>
-      <c r="B180" s="191"/>
-      <c r="C180" s="191"/>
-      <c r="D180" s="191"/>
-      <c r="E180" s="192"/>
+      <c r="B180" s="185"/>
+      <c r="C180" s="185"/>
+      <c r="D180" s="185"/>
+      <c r="E180" s="186"/>
       <c r="F180" s="129" t="s">
         <v>758</v>
       </c>
@@ -15879,6 +15976,19 @@
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="A244:E244"/>
+    <mergeCell ref="A205:E205"/>
+    <mergeCell ref="A209:E209"/>
+    <mergeCell ref="A216:E216"/>
+    <mergeCell ref="A227:E227"/>
+    <mergeCell ref="A233:E233"/>
+    <mergeCell ref="A65:E65"/>
+    <mergeCell ref="A2:E2"/>
+    <mergeCell ref="A11:E11"/>
+    <mergeCell ref="A15:E15"/>
+    <mergeCell ref="A30:E30"/>
+    <mergeCell ref="A49:E49"/>
+    <mergeCell ref="A25:E25"/>
     <mergeCell ref="A193:E193"/>
     <mergeCell ref="A172:E172"/>
     <mergeCell ref="A70:E70"/>
@@ -15890,19 +16000,6 @@
     <mergeCell ref="A100:E100"/>
     <mergeCell ref="A180:E180"/>
     <mergeCell ref="A189:E189"/>
-    <mergeCell ref="A65:E65"/>
-    <mergeCell ref="A2:E2"/>
-    <mergeCell ref="A11:E11"/>
-    <mergeCell ref="A15:E15"/>
-    <mergeCell ref="A30:E30"/>
-    <mergeCell ref="A49:E49"/>
-    <mergeCell ref="A25:E25"/>
-    <mergeCell ref="A244:E244"/>
-    <mergeCell ref="A205:E205"/>
-    <mergeCell ref="A209:E209"/>
-    <mergeCell ref="A216:E216"/>
-    <mergeCell ref="A227:E227"/>
-    <mergeCell ref="A233:E233"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -18216,6 +18313,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <Readyforteam_x003f_ xmlns="565e1b1d-057e-4d85-b896-01a5881d8a45">false</Readyforteam_x003f_>
@@ -18256,15 +18362,6 @@
 </p:properties>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EAFDB110-4046-4E72-A1EF-1908ABEC3151}">
   <ds:schemaRefs>
@@ -18287,6 +18384,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8D7CE8C7-18DC-484F-8376-ED09F13D44C8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{017ACE96-8143-486E-8436-7787F6B96F4A}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -18297,12 +18402,4 @@
     <ds:schemaRef ds:uri="2799d30d-6731-4efe-ac9b-c4895a8828d9"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8D7CE8C7-18DC-484F-8376-ED09F13D44C8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Making the timeout value editable from settings.
</commit_message>
<xml_diff>
--- a/app/data/MCCD-localisation.xlsx
+++ b/app/data/MCCD-localisation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/JALAT/GIT/medical-certificate-of-cause-of-death/app/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B91DA744-8E87-BF46-8DD6-C1D362CDBD34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69884473-3B97-214C-9465-BB7CD2C4DAD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="14020" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -5464,12 +5464,6 @@
     <t>Dangosfwrdd swyddfa</t>
   </si>
   <si>
-    <t>You will be logged out of the system after 15 minutes of inactivity.</t>
-  </si>
-  <si>
-    <t>Byddwch yn cael eich allgofnodi o'r system ar ôl 15 munud o anweithgarwch.</t>
-  </si>
-  <si>
     <t>Inset text</t>
   </si>
   <si>
@@ -5926,7 +5920,13 @@
     <t>Rhaid iddo fod yn 7 digid o hyd</t>
   </si>
   <si>
-    <t>054</t>
+    <t>You will be logged out of the system after 999 minutes of inactivity.</t>
+  </si>
+  <si>
+    <t>Byddwch yn cael eich allgofnodi o'r system ar ôl 999 munud o anweithgarwch.</t>
+  </si>
+  <si>
+    <t>055</t>
   </si>
 </sst>
 </file>
@@ -6945,6 +6945,24 @@
     <xf numFmtId="0" fontId="13" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -6952,24 +6970,6 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -8237,13 +8237,13 @@
         <v>1230</v>
       </c>
       <c r="C2" s="151" t="s">
-        <v>1393</v>
+        <v>1391</v>
       </c>
       <c r="D2" s="92" t="s">
         <v>1231</v>
       </c>
       <c r="E2" s="152" t="s">
-        <v>1397</v>
+        <v>1395</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="80" x14ac:dyDescent="0.2">
@@ -8271,13 +8271,13 @@
         <v>1237</v>
       </c>
       <c r="C4" s="158" t="s">
-        <v>1394</v>
+        <v>1392</v>
       </c>
       <c r="D4" s="95" t="s">
         <v>400</v>
       </c>
       <c r="E4" s="155" t="s">
-        <v>1396</v>
+        <v>1394</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="60.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -8339,13 +8339,13 @@
         <v>1242</v>
       </c>
       <c r="C8" s="158" t="s">
-        <v>1393</v>
+        <v>1391</v>
       </c>
       <c r="D8" s="95" t="s">
         <v>1243</v>
       </c>
       <c r="E8" s="155" t="s">
-        <v>1397</v>
+        <v>1395</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="80" x14ac:dyDescent="0.2">
@@ -8356,11 +8356,11 @@
         <v>1244</v>
       </c>
       <c r="C9" s="158" t="s">
-        <v>1490</v>
+        <v>1488</v>
       </c>
       <c r="D9" s="179"/>
       <c r="E9" s="155" t="s">
-        <v>1491</v>
+        <v>1489</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="16" x14ac:dyDescent="0.2">
@@ -8371,13 +8371,13 @@
         <v>1245</v>
       </c>
       <c r="C10" s="158" t="s">
-        <v>1394</v>
+        <v>1392</v>
       </c>
       <c r="D10" s="95" t="s">
         <v>400</v>
       </c>
       <c r="E10" s="155" t="s">
-        <v>1396</v>
+        <v>1394</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -8439,13 +8439,13 @@
         <v>1248</v>
       </c>
       <c r="C14" s="158" t="s">
-        <v>1393</v>
+        <v>1391</v>
       </c>
       <c r="D14" s="95" t="s">
         <v>1249</v>
       </c>
       <c r="E14" s="155" t="s">
-        <v>1395</v>
+        <v>1393</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="96" x14ac:dyDescent="0.2">
@@ -8456,11 +8456,11 @@
         <v>1250</v>
       </c>
       <c r="C15" s="158" t="s">
-        <v>1492</v>
+        <v>1490</v>
       </c>
       <c r="D15" s="179"/>
       <c r="E15" s="155" t="s">
-        <v>1493</v>
+        <v>1491</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="48" x14ac:dyDescent="0.2">
@@ -8505,13 +8505,13 @@
         <v>1253</v>
       </c>
       <c r="C18" s="158" t="s">
-        <v>1394</v>
+        <v>1392</v>
       </c>
       <c r="D18" s="95" t="s">
         <v>400</v>
       </c>
       <c r="E18" s="155" t="s">
-        <v>1396</v>
+        <v>1394</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -8539,13 +8539,13 @@
         <v>1254</v>
       </c>
       <c r="C20" s="158" t="s">
-        <v>1426</v>
+        <v>1424</v>
       </c>
       <c r="D20" s="95" t="s">
         <v>1231</v>
       </c>
       <c r="E20" s="155" t="s">
-        <v>1427</v>
+        <v>1425</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="64" x14ac:dyDescent="0.2">
@@ -8556,13 +8556,13 @@
         <v>1255</v>
       </c>
       <c r="C21" s="158" t="s">
-        <v>1425</v>
+        <v>1423</v>
       </c>
       <c r="D21" s="95" t="s">
         <v>1256</v>
       </c>
       <c r="E21" s="155" t="s">
-        <v>1428</v>
+        <v>1426</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -8573,13 +8573,13 @@
         <v>1257</v>
       </c>
       <c r="C22" s="158" t="s">
-        <v>1429</v>
+        <v>1427</v>
       </c>
       <c r="D22" s="95" t="s">
         <v>400</v>
       </c>
       <c r="E22" s="155" t="s">
-        <v>1430</v>
+        <v>1428</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="48" x14ac:dyDescent="0.2">
@@ -8696,7 +8696,7 @@
         <v>1264</v>
       </c>
       <c r="C4" s="59" t="s">
-        <v>1416</v>
+        <v>1414</v>
       </c>
       <c r="E4" s="37" t="s">
         <v>1265</v>
@@ -8724,10 +8724,10 @@
         <v>1269</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>1414</v>
+        <v>1412</v>
       </c>
       <c r="E6" s="37" t="s">
-        <v>1415</v>
+        <v>1413</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="32" x14ac:dyDescent="0.2">
@@ -8752,10 +8752,10 @@
         <v>1274</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>1402</v>
+        <v>1400</v>
       </c>
       <c r="E8" s="37" t="s">
-        <v>1403</v>
+        <v>1401</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="16" x14ac:dyDescent="0.2">
@@ -8836,11 +8836,11 @@
         <v>1291</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>1400</v>
+        <v>1398</v>
       </c>
       <c r="D14" s="1"/>
       <c r="E14" s="37" t="s">
-        <v>1401</v>
+        <v>1399</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="32" x14ac:dyDescent="0.2">
@@ -8923,10 +8923,10 @@
         <v>1306</v>
       </c>
       <c r="C20" s="59" t="s">
+        <v>1369</v>
+      </c>
+      <c r="E20" s="37" t="s">
         <v>1371</v>
-      </c>
-      <c r="E20" s="37" t="s">
-        <v>1373</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="16" x14ac:dyDescent="0.2">
@@ -8951,10 +8951,10 @@
         <v>1308</v>
       </c>
       <c r="C22" s="6" t="s">
+        <v>1370</v>
+      </c>
+      <c r="E22" s="37" t="s">
         <v>1372</v>
-      </c>
-      <c r="E22" s="37" t="s">
-        <v>1374</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
@@ -9042,7 +9042,7 @@
         <v>12</v>
       </c>
       <c r="E3" s="37" t="s">
-        <v>1370</v>
+        <v>1368</v>
       </c>
       <c r="F3" s="5" t="s">
         <v>13</v>
@@ -9107,7 +9107,7 @@
     <row r="7" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="5"/>
       <c r="B7" s="5" t="s">
-        <v>1465</v>
+        <v>1463</v>
       </c>
       <c r="C7" s="6" t="s">
         <v>349</v>
@@ -9907,10 +9907,10 @@
     <row r="53" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A53" s="86"/>
       <c r="B53" s="163" t="s">
-        <v>1417</v>
+        <v>1415</v>
       </c>
       <c r="C53" s="164" t="s">
-        <v>1418</v>
+        <v>1416</v>
       </c>
       <c r="D53" s="86"/>
       <c r="E53" s="165" t="s">
@@ -10026,7 +10026,7 @@
       </c>
       <c r="D61" s="86"/>
       <c r="E61" s="165" t="s">
-        <v>1433</v>
+        <v>1431</v>
       </c>
       <c r="F61" s="86"/>
     </row>
@@ -10113,30 +10113,30 @@
     <row r="68" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A68" s="86"/>
       <c r="B68" s="163" t="s">
-        <v>1421</v>
+        <v>1419</v>
       </c>
       <c r="C68" s="164" t="s">
-        <v>1422</v>
+        <v>1420</v>
       </c>
       <c r="D68" s="86"/>
       <c r="E68" s="165" t="s">
-        <v>1423</v>
+        <v>1421</v>
       </c>
       <c r="F68" s="166" t="s">
-        <v>1424</v>
+        <v>1422</v>
       </c>
     </row>
     <row r="69" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A69" s="86"/>
       <c r="B69" s="163" t="s">
-        <v>1419</v>
+        <v>1417</v>
       </c>
       <c r="C69" s="164" t="s">
         <v>1300</v>
       </c>
       <c r="D69" s="86"/>
       <c r="E69" s="165" t="s">
-        <v>1420</v>
+        <v>1418</v>
       </c>
     </row>
     <row r="70" spans="1:6" ht="16" x14ac:dyDescent="0.2">
@@ -10163,13 +10163,13 @@
     </row>
     <row r="72" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="B72" s="1" t="s">
+        <v>1432</v>
+      </c>
+      <c r="C72" s="2" t="s">
+        <v>1433</v>
+      </c>
+      <c r="E72" s="40" t="s">
         <v>1434</v>
-      </c>
-      <c r="C72" s="2" t="s">
-        <v>1435</v>
-      </c>
-      <c r="E72" s="40" t="s">
-        <v>1436</v>
       </c>
     </row>
   </sheetData>
@@ -10531,7 +10531,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="181" t="s">
-        <v>1497</v>
+        <v>1495</v>
       </c>
       <c r="B7" s="182"/>
       <c r="C7" s="182"/>
@@ -10543,44 +10543,44 @@
         <v>239</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>1499</v>
+        <v>1497</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>1500</v>
+        <v>1498</v>
       </c>
       <c r="D8" s="5"/>
       <c r="E8" s="43" t="s">
-        <v>1507</v>
+        <v>1505</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
+        <v>1499</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>1500</v>
+      </c>
+      <c r="C9" s="6" t="s">
         <v>1501</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>1502</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>1503</v>
       </c>
       <c r="D9" s="5"/>
       <c r="E9" s="43" t="s">
-        <v>1508</v>
+        <v>1506</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
+        <v>1502</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>1503</v>
+      </c>
+      <c r="C10" s="6" t="s">
         <v>1504</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>1505</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>1506</v>
       </c>
       <c r="D10" s="5"/>
       <c r="E10" s="43" t="s">
-        <v>1509</v>
+        <v>1507</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="16" x14ac:dyDescent="0.2">
@@ -10588,14 +10588,14 @@
         <v>239</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>1498</v>
+        <v>1496</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>1510</v>
+        <v>1508</v>
       </c>
       <c r="D11" s="5"/>
       <c r="E11" s="43" t="s">
-        <v>1513</v>
+        <v>1511</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="16" x14ac:dyDescent="0.2">
@@ -10603,14 +10603,14 @@
         <v>480</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>1511</v>
+        <v>1509</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>1512</v>
+        <v>1510</v>
       </c>
       <c r="D12" s="5"/>
       <c r="E12" s="43" t="s">
-        <v>1514</v>
+        <v>1512</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
@@ -10733,8 +10733,8 @@
   <dimension ref="A1:F31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D7" sqref="D7"/>
+      <pane ySplit="1" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -10828,13 +10828,13 @@
         <v>277</v>
       </c>
       <c r="C5" s="52" t="s">
-        <v>1413</v>
+        <v>1411</v>
       </c>
       <c r="D5" s="66" t="s">
         <v>278</v>
       </c>
       <c r="E5" s="156" t="s">
-        <v>1431</v>
+        <v>1429</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>279</v>
@@ -10848,13 +10848,13 @@
         <v>280</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>1365</v>
+        <v>1363</v>
       </c>
       <c r="D6" s="67" t="s">
         <v>281</v>
       </c>
       <c r="E6" s="157" t="s">
-        <v>1432</v>
+        <v>1430</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="160" x14ac:dyDescent="0.2">
@@ -10865,13 +10865,13 @@
         <v>282</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>1366</v>
+        <v>1364</v>
       </c>
       <c r="D7" s="67" t="s">
         <v>283</v>
       </c>
       <c r="E7" s="157" t="s">
-        <v>1367</v>
+        <v>1365</v>
       </c>
       <c r="F7" s="68" t="s">
         <v>284</v>
@@ -11207,17 +11207,17 @@
     </row>
     <row r="27" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A27" s="5" t="s">
-        <v>1363</v>
+        <v>1361</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>1364</v>
+        <v>1362</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>1361</v>
+        <v>1513</v>
       </c>
       <c r="D27" s="5"/>
       <c r="E27" s="37" t="s">
-        <v>1362</v>
+        <v>1514</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
@@ -11294,13 +11294,13 @@
       </c>
     </row>
     <row r="2" spans="1:6" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="187" t="s">
+      <c r="A2" s="184" t="s">
         <v>363</v>
       </c>
-      <c r="B2" s="188"/>
-      <c r="C2" s="188"/>
-      <c r="D2" s="188"/>
-      <c r="E2" s="189"/>
+      <c r="B2" s="185"/>
+      <c r="C2" s="185"/>
+      <c r="D2" s="185"/>
+      <c r="E2" s="186"/>
       <c r="F2" s="33"/>
     </row>
     <row r="3" spans="1:6" ht="48" x14ac:dyDescent="0.2">
@@ -11398,14 +11398,14 @@
         <v>378</v>
       </c>
       <c r="B8" s="119" t="s">
-        <v>1494</v>
+        <v>1492</v>
       </c>
       <c r="C8" s="117" t="s">
-        <v>1495</v>
+        <v>1493</v>
       </c>
       <c r="D8" s="121"/>
       <c r="E8" s="120" t="s">
-        <v>1496</v>
+        <v>1494</v>
       </c>
       <c r="F8" s="119"/>
     </row>
@@ -11444,13 +11444,13 @@
       <c r="F10" s="119"/>
     </row>
     <row r="11" spans="1:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="190" t="s">
+      <c r="A11" s="187" t="s">
         <v>392</v>
       </c>
-      <c r="B11" s="191"/>
-      <c r="C11" s="191"/>
-      <c r="D11" s="191"/>
-      <c r="E11" s="192"/>
+      <c r="B11" s="188"/>
+      <c r="C11" s="188"/>
+      <c r="D11" s="188"/>
+      <c r="E11" s="189"/>
       <c r="F11" s="119"/>
     </row>
     <row r="12" spans="1:6" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -11659,7 +11659,7 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" s="181" t="s">
-        <v>1462</v>
+        <v>1460</v>
       </c>
       <c r="B25" s="182"/>
       <c r="C25" s="182"/>
@@ -11672,10 +11672,10 @@
         <v>239</v>
       </c>
       <c r="B26" s="132" t="s">
-        <v>1463</v>
+        <v>1461</v>
       </c>
       <c r="C26" s="133" t="s">
-        <v>1464</v>
+        <v>1462</v>
       </c>
       <c r="D26" s="114"/>
       <c r="E26" s="131"/>
@@ -11686,14 +11686,14 @@
         <v>373</v>
       </c>
       <c r="B27" s="132" t="s">
-        <v>1466</v>
+        <v>1464</v>
       </c>
       <c r="C27" s="133" t="s">
-        <v>1474</v>
+        <v>1472</v>
       </c>
       <c r="D27" s="114"/>
       <c r="E27" s="131" t="s">
-        <v>1475</v>
+        <v>1473</v>
       </c>
       <c r="F27" s="119"/>
     </row>
@@ -11702,30 +11702,30 @@
         <v>373</v>
       </c>
       <c r="B28" s="132" t="s">
-        <v>1468</v>
+        <v>1466</v>
       </c>
       <c r="C28" s="133" t="s">
-        <v>1467</v>
+        <v>1465</v>
       </c>
       <c r="D28" s="114"/>
       <c r="E28" s="131" t="s">
-        <v>1469</v>
+        <v>1467</v>
       </c>
       <c r="F28" s="119"/>
     </row>
     <row r="29" spans="1:6" s="178" customFormat="1" ht="96" x14ac:dyDescent="0.2">
       <c r="A29" s="172" t="s">
-        <v>1473</v>
+        <v>1471</v>
       </c>
       <c r="B29" s="173" t="s">
-        <v>1470</v>
+        <v>1468</v>
       </c>
       <c r="C29" s="174" t="s">
-        <v>1471</v>
+        <v>1469</v>
       </c>
       <c r="D29" s="175"/>
       <c r="E29" s="176" t="s">
-        <v>1472</v>
+        <v>1470</v>
       </c>
       <c r="F29" s="177"/>
     </row>
@@ -12043,11 +12043,11 @@
         <v>1343</v>
       </c>
       <c r="C51" s="59" t="s">
-        <v>1439</v>
+        <v>1437</v>
       </c>
       <c r="D51" s="116"/>
       <c r="E51" s="120" t="s">
-        <v>1440</v>
+        <v>1438</v>
       </c>
       <c r="F51" s="119"/>
     </row>
@@ -12056,7 +12056,7 @@
         <v>480</v>
       </c>
       <c r="B52" s="116" t="s">
-        <v>1438</v>
+        <v>1436</v>
       </c>
       <c r="C52" s="59" t="s">
         <v>1342</v>
@@ -12075,11 +12075,11 @@
         <v>481</v>
       </c>
       <c r="C53" s="59" t="s">
-        <v>1437</v>
+        <v>1435</v>
       </c>
       <c r="D53" s="116"/>
       <c r="E53" s="120" t="s">
-        <v>1443</v>
+        <v>1441</v>
       </c>
       <c r="F53" s="119"/>
     </row>
@@ -12283,13 +12283,13 @@
         <v>511</v>
       </c>
       <c r="C67" s="117" t="s">
-        <v>1441</v>
+        <v>1439</v>
       </c>
       <c r="D67" s="116" t="s">
         <v>512</v>
       </c>
       <c r="E67" s="120" t="s">
-        <v>1442</v>
+        <v>1440</v>
       </c>
       <c r="F67" s="119"/>
     </row>
@@ -12416,14 +12416,14 @@
         <v>480</v>
       </c>
       <c r="B76" s="125" t="s">
-        <v>1444</v>
+        <v>1442</v>
       </c>
       <c r="C76" s="167" t="s">
-        <v>1445</v>
+        <v>1443</v>
       </c>
       <c r="D76" s="125"/>
       <c r="E76" s="131" t="s">
-        <v>1446</v>
+        <v>1444</v>
       </c>
       <c r="F76" s="119"/>
     </row>
@@ -12543,13 +12543,13 @@
         <v>546</v>
       </c>
       <c r="C83" s="158" t="s">
-        <v>1457</v>
+        <v>1455</v>
       </c>
       <c r="D83" s="95" t="s">
         <v>400</v>
       </c>
       <c r="E83" s="155" t="s">
-        <v>1458</v>
+        <v>1456</v>
       </c>
       <c r="F83" s="119"/>
     </row>
@@ -12675,11 +12675,11 @@
         <v>564</v>
       </c>
       <c r="C92" s="117" t="s">
-        <v>1382</v>
+        <v>1380</v>
       </c>
       <c r="D92" s="116"/>
       <c r="E92" s="120" t="s">
-        <v>1383</v>
+        <v>1381</v>
       </c>
       <c r="F92" s="119"/>
     </row>
@@ -12787,11 +12787,11 @@
         <v>583</v>
       </c>
       <c r="C99" s="117" t="s">
-        <v>1380</v>
+        <v>1378</v>
       </c>
       <c r="D99" s="116"/>
       <c r="E99" s="120" t="s">
-        <v>1381</v>
+        <v>1379</v>
       </c>
       <c r="F99" s="119"/>
     </row>
@@ -12833,11 +12833,11 @@
         <v>589</v>
       </c>
       <c r="C102" s="117" t="s">
-        <v>1398</v>
+        <v>1396</v>
       </c>
       <c r="D102" s="116"/>
       <c r="E102" s="120" t="s">
-        <v>1399</v>
+        <v>1397</v>
       </c>
       <c r="F102" s="86" t="s">
         <v>592</v>
@@ -12866,7 +12866,7 @@
         <v>84</v>
       </c>
       <c r="B104" s="159" t="s">
-        <v>1404</v>
+        <v>1402</v>
       </c>
       <c r="C104" s="93" t="s">
         <v>591</v>
@@ -12884,7 +12884,7 @@
         <v>84</v>
       </c>
       <c r="B105" s="159" t="s">
-        <v>1405</v>
+        <v>1403</v>
       </c>
       <c r="C105" s="93" t="s">
         <v>591</v>
@@ -12902,7 +12902,7 @@
         <v>84</v>
       </c>
       <c r="B106" s="160" t="s">
-        <v>1406</v>
+        <v>1404</v>
       </c>
       <c r="C106" s="161" t="s">
         <v>591</v>
@@ -12918,7 +12918,7 @@
         <v>84</v>
       </c>
       <c r="B107" s="160" t="s">
-        <v>1407</v>
+        <v>1405</v>
       </c>
       <c r="C107" s="161" t="s">
         <v>591</v>
@@ -12934,7 +12934,7 @@
         <v>84</v>
       </c>
       <c r="B108" s="160" t="s">
-        <v>1408</v>
+        <v>1406</v>
       </c>
       <c r="C108" s="161" t="s">
         <v>591</v>
@@ -13383,33 +13383,33 @@
     </row>
     <row r="138" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A138" s="116" t="s">
+        <v>1445</v>
+      </c>
+      <c r="B138" s="116" t="s">
         <v>1447</v>
       </c>
-      <c r="B138" s="116" t="s">
-        <v>1449</v>
-      </c>
       <c r="C138" s="117" t="s">
-        <v>1448</v>
+        <v>1446</v>
       </c>
       <c r="D138" s="116"/>
       <c r="E138" s="120" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="F138" s="119"/>
     </row>
     <row r="139" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A139" s="116" t="s">
-        <v>1447</v>
+        <v>1445</v>
       </c>
       <c r="B139" s="116" t="s">
-        <v>1451</v>
+        <v>1449</v>
       </c>
       <c r="C139" s="117" t="s">
-        <v>1450</v>
+        <v>1448</v>
       </c>
       <c r="D139" s="116"/>
       <c r="E139" s="120" t="s">
-        <v>1453</v>
+        <v>1451</v>
       </c>
       <c r="F139" s="119"/>
     </row>
@@ -14008,13 +14008,13 @@
       </c>
     </row>
     <row r="180" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A180" s="184" t="s">
+      <c r="A180" s="190" t="s">
         <v>754</v>
       </c>
-      <c r="B180" s="185"/>
-      <c r="C180" s="185"/>
-      <c r="D180" s="185"/>
-      <c r="E180" s="186"/>
+      <c r="B180" s="191"/>
+      <c r="C180" s="191"/>
+      <c r="D180" s="191"/>
+      <c r="E180" s="192"/>
       <c r="F180" s="129" t="s">
         <v>758</v>
       </c>
@@ -14031,7 +14031,7 @@
       </c>
       <c r="D181" s="114"/>
       <c r="E181" s="131" t="s">
-        <v>1483</v>
+        <v>1481</v>
       </c>
       <c r="F181" s="129" t="s">
         <v>758</v>
@@ -14049,7 +14049,7 @@
       </c>
       <c r="D182" s="114"/>
       <c r="E182" s="131" t="s">
-        <v>1484</v>
+        <v>1482</v>
       </c>
       <c r="F182" s="129" t="s">
         <v>758</v>
@@ -14081,7 +14081,7 @@
       </c>
       <c r="D184" s="114"/>
       <c r="E184" s="131" t="s">
-        <v>1485</v>
+        <v>1483</v>
       </c>
       <c r="F184" s="129" t="s">
         <v>758</v>
@@ -14099,7 +14099,7 @@
       </c>
       <c r="D185" s="114"/>
       <c r="E185" s="131" t="s">
-        <v>1486</v>
+        <v>1484</v>
       </c>
       <c r="F185" s="129" t="s">
         <v>758</v>
@@ -14147,7 +14147,7 @@
     </row>
     <row r="189" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A189" s="181" t="s">
-        <v>1476</v>
+        <v>1474</v>
       </c>
       <c r="B189" s="182"/>
       <c r="C189" s="182"/>
@@ -14160,29 +14160,29 @@
         <v>239</v>
       </c>
       <c r="B190" s="132" t="s">
-        <v>1477</v>
+        <v>1475</v>
       </c>
       <c r="C190" s="133" t="s">
-        <v>1476</v>
+        <v>1474</v>
       </c>
       <c r="D190" s="114"/>
       <c r="E190" s="131" t="s">
-        <v>1480</v>
+        <v>1478</v>
       </c>
       <c r="F190" s="119"/>
     </row>
     <row r="191" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A191" s="1" t="s">
-        <v>1482</v>
+        <v>1480</v>
       </c>
       <c r="B191" s="1" t="s">
-        <v>1478</v>
+        <v>1476</v>
       </c>
       <c r="C191" s="2" t="s">
+        <v>1477</v>
+      </c>
+      <c r="E191" s="40" t="s">
         <v>1479</v>
-      </c>
-      <c r="E191" s="40" t="s">
-        <v>1481</v>
       </c>
     </row>
     <row r="192" spans="1:6" ht="48" x14ac:dyDescent="0.2">
@@ -14190,13 +14190,13 @@
         <v>257</v>
       </c>
       <c r="B192" s="1" t="s">
+        <v>1485</v>
+      </c>
+      <c r="C192" s="2" t="s">
+        <v>1486</v>
+      </c>
+      <c r="E192" s="40" t="s">
         <v>1487</v>
-      </c>
-      <c r="C192" s="2" t="s">
-        <v>1488</v>
-      </c>
-      <c r="E192" s="40" t="s">
-        <v>1489</v>
       </c>
     </row>
     <row r="193" spans="1:6" x14ac:dyDescent="0.2">
@@ -15031,13 +15031,13 @@
         <v>854</v>
       </c>
       <c r="C247" s="59" t="s">
-        <v>1368</v>
+        <v>1366</v>
       </c>
       <c r="D247" s="116" t="s">
         <v>855</v>
       </c>
       <c r="E247" s="120" t="s">
-        <v>1369</v>
+        <v>1367</v>
       </c>
       <c r="F247" s="119"/>
     </row>
@@ -15976,19 +15976,6 @@
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="A244:E244"/>
-    <mergeCell ref="A205:E205"/>
-    <mergeCell ref="A209:E209"/>
-    <mergeCell ref="A216:E216"/>
-    <mergeCell ref="A227:E227"/>
-    <mergeCell ref="A233:E233"/>
-    <mergeCell ref="A65:E65"/>
-    <mergeCell ref="A2:E2"/>
-    <mergeCell ref="A11:E11"/>
-    <mergeCell ref="A15:E15"/>
-    <mergeCell ref="A30:E30"/>
-    <mergeCell ref="A49:E49"/>
-    <mergeCell ref="A25:E25"/>
     <mergeCell ref="A193:E193"/>
     <mergeCell ref="A172:E172"/>
     <mergeCell ref="A70:E70"/>
@@ -16000,6 +15987,19 @@
     <mergeCell ref="A100:E100"/>
     <mergeCell ref="A180:E180"/>
     <mergeCell ref="A189:E189"/>
+    <mergeCell ref="A65:E65"/>
+    <mergeCell ref="A2:E2"/>
+    <mergeCell ref="A11:E11"/>
+    <mergeCell ref="A15:E15"/>
+    <mergeCell ref="A30:E30"/>
+    <mergeCell ref="A49:E49"/>
+    <mergeCell ref="A25:E25"/>
+    <mergeCell ref="A244:E244"/>
+    <mergeCell ref="A205:E205"/>
+    <mergeCell ref="A209:E209"/>
+    <mergeCell ref="A216:E216"/>
+    <mergeCell ref="A227:E227"/>
+    <mergeCell ref="A233:E233"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -16127,14 +16127,14 @@
     </row>
     <row r="8" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="B8" s="168" t="s">
-        <v>1459</v>
+        <v>1457</v>
       </c>
       <c r="C8" s="169" t="s">
-        <v>1460</v>
+        <v>1458</v>
       </c>
       <c r="D8" s="168"/>
       <c r="E8" s="170" t="s">
-        <v>1461</v>
+        <v>1459</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="16" x14ac:dyDescent="0.2">
@@ -16362,11 +16362,11 @@
         <v>945</v>
       </c>
       <c r="C24" s="82" t="s">
-        <v>1454</v>
+        <v>1452</v>
       </c>
       <c r="D24" s="80"/>
       <c r="E24" s="81" t="s">
-        <v>1455</v>
+        <v>1453</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
@@ -16488,10 +16488,10 @@
         <v>968</v>
       </c>
       <c r="C33" s="21" t="s">
-        <v>1375</v>
+        <v>1373</v>
       </c>
       <c r="E33" s="46" t="s">
-        <v>1376</v>
+        <v>1374</v>
       </c>
     </row>
     <row r="34" spans="1:6" ht="32" x14ac:dyDescent="0.2">
@@ -16499,13 +16499,13 @@
         <v>257</v>
       </c>
       <c r="B34" s="19" t="s">
+        <v>1375</v>
+      </c>
+      <c r="C34" s="21" t="s">
+        <v>1376</v>
+      </c>
+      <c r="E34" s="46" t="s">
         <v>1377</v>
-      </c>
-      <c r="C34" s="21" t="s">
-        <v>1378</v>
-      </c>
-      <c r="E34" s="46" t="s">
-        <v>1379</v>
       </c>
     </row>
     <row r="35" spans="1:6" ht="48" x14ac:dyDescent="0.2">
@@ -16665,13 +16665,13 @@
         <v>993</v>
       </c>
       <c r="C46" s="62" t="s">
-        <v>1368</v>
+        <v>1366</v>
       </c>
       <c r="D46" s="116" t="s">
         <v>994</v>
       </c>
       <c r="E46" s="46" t="s">
-        <v>1369</v>
+        <v>1367</v>
       </c>
     </row>
     <row r="47" spans="1:6" ht="48" x14ac:dyDescent="0.2">
@@ -17064,23 +17064,23 @@
         <v>1060</v>
       </c>
       <c r="E11" s="138" t="s">
-        <v>1392</v>
+        <v>1390</v>
       </c>
       <c r="F11" s="135"/>
     </row>
     <row r="12" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A12" s="136" t="s">
+        <v>1386</v>
+      </c>
+      <c r="B12" s="136" t="s">
+        <v>1387</v>
+      </c>
+      <c r="C12" s="137" t="s">
         <v>1388</v>
-      </c>
-      <c r="B12" s="136" t="s">
-        <v>1389</v>
-      </c>
-      <c r="C12" s="137" t="s">
-        <v>1390</v>
       </c>
       <c r="D12" s="136"/>
       <c r="E12" s="138" t="s">
-        <v>1391</v>
+        <v>1389</v>
       </c>
       <c r="F12" s="135"/>
     </row>
@@ -17092,7 +17092,7 @@
         <v>1061</v>
       </c>
       <c r="C13" s="137" t="s">
-        <v>1456</v>
+        <v>1454</v>
       </c>
       <c r="D13" s="136" t="s">
         <v>1062</v>
@@ -17138,7 +17138,7 @@
         <v>1067</v>
       </c>
       <c r="C16" s="137" t="s">
-        <v>1384</v>
+        <v>1382</v>
       </c>
       <c r="D16" s="136" t="s">
         <v>1068</v>
@@ -17156,7 +17156,7 @@
         <v>1070</v>
       </c>
       <c r="C17" s="137" t="s">
-        <v>1385</v>
+        <v>1383</v>
       </c>
       <c r="D17" s="136" t="s">
         <v>1071</v>
@@ -17174,7 +17174,7 @@
         <v>1073</v>
       </c>
       <c r="C18" s="137" t="s">
-        <v>1386</v>
+        <v>1384</v>
       </c>
       <c r="D18" s="136" t="s">
         <v>1074</v>
@@ -17314,17 +17314,17 @@
     </row>
     <row r="28" spans="1:6" ht="64" x14ac:dyDescent="0.2">
       <c r="A28" s="136" t="s">
-        <v>1388</v>
+        <v>1386</v>
       </c>
       <c r="B28" s="136" t="s">
-        <v>1387</v>
+        <v>1385</v>
       </c>
       <c r="C28" s="137" t="s">
-        <v>1409</v>
+        <v>1407</v>
       </c>
       <c r="D28" s="136"/>
       <c r="E28" s="138" t="s">
-        <v>1411</v>
+        <v>1409</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="32" x14ac:dyDescent="0.2">
@@ -17335,13 +17335,13 @@
         <v>1099</v>
       </c>
       <c r="C29" s="137" t="s">
-        <v>1410</v>
+        <v>1408</v>
       </c>
       <c r="D29" s="136" t="s">
         <v>1100</v>
       </c>
       <c r="E29" s="138" t="s">
-        <v>1412</v>
+        <v>1410</v>
       </c>
     </row>
     <row r="30" spans="1:6" s="13" customFormat="1" x14ac:dyDescent="0.2">
@@ -17676,13 +17676,13 @@
         <v>1149</v>
       </c>
       <c r="C51" s="62" t="s">
-        <v>1368</v>
+        <v>1366</v>
       </c>
       <c r="D51" s="116" t="s">
         <v>994</v>
       </c>
       <c r="E51" s="63" t="s">
-        <v>1369</v>
+        <v>1367</v>
       </c>
     </row>
     <row r="52" spans="1:6" s="30" customFormat="1" ht="48" x14ac:dyDescent="0.2">
@@ -18313,15 +18313,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <Readyforteam_x003f_ xmlns="565e1b1d-057e-4d85-b896-01a5881d8a45">false</Readyforteam_x003f_>
@@ -18362,6 +18353,15 @@
 </p:properties>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EAFDB110-4046-4E72-A1EF-1908ABEC3151}">
   <ds:schemaRefs>
@@ -18384,14 +18384,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8D7CE8C7-18DC-484F-8376-ED09F13D44C8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{017ACE96-8143-486E-8436-7787F6B96F4A}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -18402,4 +18394,12 @@
     <ds:schemaRef ds:uri="2799d30d-6731-4efe-ac9b-c4895a8828d9"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8D7CE8C7-18DC-484F-8376-ED09F13D44C8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Missing titles on Confirm address. Reworking the optional markers on Exact location and Location death hospital. Missing welsh.
</commit_message>
<xml_diff>
--- a/app/data/MCCD-localisation.xlsx
+++ b/app/data/MCCD-localisation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/JALAT/GIT/medical-certificate-of-cause-of-death/app/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69884473-3B97-214C-9465-BB7CD2C4DAD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34AB2EFE-427B-0C4F-B09A-7C92A8EF8A7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="14020" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="13940" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Using this document" sheetId="8" r:id="rId1"/>
@@ -69,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2258" uniqueCount="1516">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2267" uniqueCount="1528">
   <si>
     <r>
       <rPr>
@@ -5926,7 +5926,43 @@
     <t>Byddwch yn cael eich allgofnodi o'r system ar ôl 999 munud o anweithgarwch.</t>
   </si>
   <si>
-    <t>055</t>
+    <t>dpdConfirmHospitalAddressPageTitle</t>
+  </si>
+  <si>
+    <t>Confirm hospital address</t>
+  </si>
+  <si>
+    <t>Cadarnhau cyfeiriad ysbyty</t>
+  </si>
+  <si>
+    <t>Address line 2</t>
+  </si>
+  <si>
+    <t>Town or city</t>
+  </si>
+  <si>
+    <t>County</t>
+  </si>
+  <si>
+    <t>Llinell cyfeiriad 2</t>
+  </si>
+  <si>
+    <t>Tref neu ddinas</t>
+  </si>
+  <si>
+    <t>Sir</t>
+  </si>
+  <si>
+    <t>dpdEnterAddressInWelsh</t>
+  </si>
+  <si>
+    <t>Enter address &lt;strong&gt;in Welsh&lt;/strong&gt;</t>
+  </si>
+  <si>
+    <t>Rhowch gyfeiriad &lt;strong&gt;yn Gymraeg&lt;/strong&gt;</t>
+  </si>
+  <si>
+    <t>057</t>
   </si>
 </sst>
 </file>
@@ -6402,7 +6438,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="217">
+  <cellXfs count="219">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -7043,6 +7079,12 @@
     </xf>
     <xf numFmtId="0" fontId="13" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -8978,7 +9020,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F3" sqref="F3"/>
+      <selection pane="bottomLeft" activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -9018,13 +9060,13 @@
         <v>7</v>
       </c>
       <c r="C2" s="100" t="s">
-        <v>1515</v>
+        <v>1527</v>
       </c>
       <c r="D2" s="98" t="s">
         <v>8</v>
       </c>
       <c r="E2" s="99" t="s">
-        <v>1515</v>
+        <v>1527</v>
       </c>
       <c r="F2" s="98"/>
     </row>
@@ -10733,8 +10775,8 @@
   <dimension ref="A1:F31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F27" sqref="F27"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -11255,11 +11297,11 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B63483B8-55BE-4CA0-9111-55E5C0AEF6CB}">
-  <dimension ref="A1:F364"/>
+  <dimension ref="A1:F366"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D8" sqref="D8"/>
+      <pane ySplit="1" topLeftCell="A193" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B203" sqref="B203"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -14037,52 +14079,52 @@
         <v>758</v>
       </c>
     </row>
-    <row r="182" spans="1:6" ht="64" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A182" s="116" t="s">
-        <v>257</v>
+        <v>239</v>
       </c>
       <c r="B182" s="116" t="s">
-        <v>759</v>
-      </c>
-      <c r="C182" s="117" t="s">
-        <v>740</v>
+        <v>1515</v>
+      </c>
+      <c r="C182" s="130" t="s">
+        <v>1516</v>
       </c>
       <c r="D182" s="114"/>
       <c r="E182" s="131" t="s">
-        <v>1482</v>
+        <v>1517</v>
       </c>
       <c r="F182" s="129" t="s">
         <v>758</v>
       </c>
     </row>
-    <row r="183" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A183" s="126" t="s">
-        <v>760</v>
+    <row r="183" spans="1:6" ht="64" x14ac:dyDescent="0.2">
+      <c r="A183" s="116" t="s">
+        <v>257</v>
       </c>
       <c r="B183" s="116" t="s">
-        <v>761</v>
-      </c>
-      <c r="C183" s="115"/>
+        <v>759</v>
+      </c>
+      <c r="C183" s="117" t="s">
+        <v>740</v>
+      </c>
       <c r="D183" s="114"/>
-      <c r="E183" s="131"/>
+      <c r="E183" s="131" t="s">
+        <v>1482</v>
+      </c>
       <c r="F183" s="129" t="s">
         <v>758</v>
       </c>
     </row>
     <row r="184" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A184" s="126" t="s">
-        <v>32</v>
+        <v>760</v>
       </c>
       <c r="B184" s="116" t="s">
-        <v>762</v>
-      </c>
-      <c r="C184" s="130" t="s">
-        <v>763</v>
-      </c>
+        <v>761</v>
+      </c>
+      <c r="C184" s="115"/>
       <c r="D184" s="114"/>
-      <c r="E184" s="131" t="s">
-        <v>1483</v>
-      </c>
+      <c r="E184" s="131"/>
       <c r="F184" s="129" t="s">
         <v>758</v>
       </c>
@@ -14091,33 +14133,33 @@
       <c r="A185" s="126" t="s">
         <v>32</v>
       </c>
-      <c r="B185" s="60" t="s">
-        <v>764</v>
+      <c r="B185" s="116" t="s">
+        <v>762</v>
       </c>
       <c r="C185" s="130" t="s">
-        <v>76</v>
+        <v>763</v>
       </c>
       <c r="D185" s="114"/>
       <c r="E185" s="131" t="s">
-        <v>1484</v>
+        <v>1483</v>
       </c>
       <c r="F185" s="129" t="s">
         <v>758</v>
       </c>
     </row>
     <row r="186" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A186" s="116" t="s">
-        <v>723</v>
-      </c>
-      <c r="B186" s="116" t="s">
-        <v>748</v>
+      <c r="A186" s="126" t="s">
+        <v>32</v>
+      </c>
+      <c r="B186" s="60" t="s">
+        <v>764</v>
       </c>
       <c r="C186" s="130" t="s">
-        <v>47</v>
+        <v>76</v>
       </c>
       <c r="D186" s="114"/>
       <c r="E186" s="131" t="s">
-        <v>49</v>
+        <v>1484</v>
       </c>
       <c r="F186" s="129" t="s">
         <v>758</v>
@@ -14125,123 +14167,123 @@
     </row>
     <row r="187" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A187" s="116" t="s">
-        <v>406</v>
-      </c>
-      <c r="B187" s="132"/>
-      <c r="C187" s="133"/>
+        <v>723</v>
+      </c>
+      <c r="B187" s="116" t="s">
+        <v>748</v>
+      </c>
+      <c r="C187" s="130" t="s">
+        <v>47</v>
+      </c>
       <c r="D187" s="114"/>
-      <c r="E187" s="131"/>
+      <c r="E187" s="131" t="s">
+        <v>49</v>
+      </c>
       <c r="F187" s="129" t="s">
         <v>758</v>
       </c>
     </row>
     <row r="188" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A188" s="116" t="s">
-        <v>409</v>
+        <v>406</v>
       </c>
       <c r="B188" s="132"/>
       <c r="C188" s="133"/>
       <c r="D188" s="114"/>
       <c r="E188" s="131"/>
-      <c r="F188" s="119"/>
-    </row>
-    <row r="189" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A189" s="181" t="s">
+      <c r="F188" s="129" t="s">
+        <v>758</v>
+      </c>
+    </row>
+    <row r="189" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A189" s="116" t="s">
+        <v>409</v>
+      </c>
+      <c r="B189" s="132"/>
+      <c r="C189" s="133"/>
+      <c r="D189" s="114"/>
+      <c r="E189" s="131"/>
+      <c r="F189" s="119"/>
+    </row>
+    <row r="190" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A190" s="181" t="s">
         <v>1474</v>
       </c>
-      <c r="B189" s="182"/>
-      <c r="C189" s="182"/>
-      <c r="D189" s="182"/>
-      <c r="E189" s="183"/>
-      <c r="F189" s="119"/>
-    </row>
-    <row r="190" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A190" s="171" t="s">
+      <c r="B190" s="182"/>
+      <c r="C190" s="182"/>
+      <c r="D190" s="182"/>
+      <c r="E190" s="183"/>
+      <c r="F190" s="119"/>
+    </row>
+    <row r="191" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A191" s="171" t="s">
         <v>239</v>
       </c>
-      <c r="B190" s="132" t="s">
+      <c r="B191" s="132" t="s">
         <v>1475</v>
       </c>
-      <c r="C190" s="133" t="s">
+      <c r="C191" s="133" t="s">
         <v>1474</v>
       </c>
-      <c r="D190" s="114"/>
-      <c r="E190" s="131" t="s">
+      <c r="D191" s="114"/>
+      <c r="E191" s="131" t="s">
         <v>1478</v>
       </c>
-      <c r="F190" s="119"/>
-    </row>
-    <row r="191" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A191" s="1" t="s">
+      <c r="F191" s="119"/>
+    </row>
+    <row r="192" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A192" s="1" t="s">
         <v>1480</v>
       </c>
-      <c r="B191" s="1" t="s">
+      <c r="B192" s="1" t="s">
         <v>1476</v>
       </c>
-      <c r="C191" s="2" t="s">
+      <c r="C192" s="2" t="s">
         <v>1477</v>
       </c>
-      <c r="E191" s="40" t="s">
+      <c r="E192" s="40" t="s">
         <v>1479</v>
       </c>
     </row>
-    <row r="192" spans="1:6" ht="48" x14ac:dyDescent="0.2">
-      <c r="A192" s="1" t="s">
+    <row r="193" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+      <c r="A193" s="1" t="s">
         <v>257</v>
       </c>
-      <c r="B192" s="1" t="s">
+      <c r="B193" s="1" t="s">
         <v>1485</v>
       </c>
-      <c r="C192" s="2" t="s">
+      <c r="C193" s="2" t="s">
         <v>1486</v>
       </c>
-      <c r="E192" s="40" t="s">
+      <c r="E193" s="40" t="s">
         <v>1487</v>
       </c>
     </row>
-    <row r="193" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A193" s="181" t="s">
+    <row r="194" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A194" s="181" t="s">
         <v>765</v>
       </c>
-      <c r="B193" s="182"/>
-      <c r="C193" s="182"/>
-      <c r="D193" s="182"/>
-      <c r="E193" s="183"/>
-      <c r="F193" s="119"/>
-    </row>
-    <row r="194" spans="1:6" ht="32" x14ac:dyDescent="0.2">
-      <c r="A194" s="91" t="s">
+      <c r="B194" s="182"/>
+      <c r="C194" s="182"/>
+      <c r="D194" s="182"/>
+      <c r="E194" s="183"/>
+      <c r="F194" s="119"/>
+    </row>
+    <row r="195" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+      <c r="A195" s="91" t="s">
         <v>239</v>
       </c>
-      <c r="B194" s="92" t="s">
+      <c r="B195" s="92" t="s">
         <v>766</v>
       </c>
-      <c r="C194" s="93" t="s">
+      <c r="C195" s="93" t="s">
         <v>767</v>
       </c>
-      <c r="D194" s="92" t="s">
+      <c r="D195" s="92" t="s">
         <v>768</v>
       </c>
-      <c r="E194" s="85" t="s">
+      <c r="E195" s="85" t="s">
         <v>769</v>
-      </c>
-      <c r="F194" s="119"/>
-    </row>
-    <row r="195" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A195" s="94" t="s">
-        <v>412</v>
-      </c>
-      <c r="B195" s="95" t="s">
-        <v>770</v>
-      </c>
-      <c r="C195" s="96" t="s">
-        <v>56</v>
-      </c>
-      <c r="D195" s="95" t="s">
-        <v>400</v>
-      </c>
-      <c r="E195" s="89" t="s">
-        <v>58</v>
       </c>
       <c r="F195" s="119"/>
     </row>
@@ -14250,16 +14292,16 @@
         <v>412</v>
       </c>
       <c r="B196" s="95" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
       <c r="C196" s="96" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="D196" s="95" t="s">
         <v>400</v>
       </c>
       <c r="E196" s="89" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="F196" s="119"/>
     </row>
@@ -14268,16 +14310,16 @@
         <v>412</v>
       </c>
       <c r="B197" s="95" t="s">
-        <v>772</v>
-      </c>
-      <c r="C197" s="96" t="s">
-        <v>64</v>
+        <v>771</v>
+      </c>
+      <c r="C197" s="158" t="s">
+        <v>1518</v>
       </c>
       <c r="D197" s="95" t="s">
         <v>400</v>
       </c>
-      <c r="E197" s="89" t="s">
-        <v>66</v>
+      <c r="E197" s="155" t="s">
+        <v>1521</v>
       </c>
       <c r="F197" s="119"/>
     </row>
@@ -14286,16 +14328,16 @@
         <v>412</v>
       </c>
       <c r="B198" s="95" t="s">
-        <v>773</v>
-      </c>
-      <c r="C198" s="96" t="s">
-        <v>68</v>
+        <v>772</v>
+      </c>
+      <c r="C198" s="158" t="s">
+        <v>1519</v>
       </c>
       <c r="D198" s="95" t="s">
         <v>400</v>
       </c>
-      <c r="E198" s="89" t="s">
-        <v>70</v>
+      <c r="E198" s="155" t="s">
+        <v>1522</v>
       </c>
       <c r="F198" s="119"/>
     </row>
@@ -14304,75 +14346,81 @@
         <v>412</v>
       </c>
       <c r="B199" s="95" t="s">
-        <v>774</v>
-      </c>
-      <c r="C199" s="96" t="s">
-        <v>39</v>
+        <v>773</v>
+      </c>
+      <c r="C199" s="158" t="s">
+        <v>1520</v>
       </c>
       <c r="D199" s="95" t="s">
         <v>400</v>
       </c>
-      <c r="E199" s="89" t="s">
-        <v>41</v>
+      <c r="E199" s="155" t="s">
+        <v>1523</v>
       </c>
       <c r="F199" s="119"/>
     </row>
-    <row r="200" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A200" s="94" t="s">
-        <v>32</v>
+        <v>412</v>
       </c>
       <c r="B200" s="95" t="s">
-        <v>775</v>
-      </c>
-      <c r="C200" s="97" t="s">
-        <v>776</v>
+        <v>774</v>
+      </c>
+      <c r="C200" s="96" t="s">
+        <v>39</v>
       </c>
       <c r="D200" s="95" t="s">
         <v>400</v>
       </c>
       <c r="E200" s="89" t="s">
+        <v>41</v>
+      </c>
+      <c r="F200" s="119"/>
+    </row>
+    <row r="201" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+      <c r="A201" s="94" t="s">
+        <v>32</v>
+      </c>
+      <c r="B201" s="95" t="s">
+        <v>775</v>
+      </c>
+      <c r="C201" s="97" t="s">
+        <v>776</v>
+      </c>
+      <c r="D201" s="95" t="s">
+        <v>400</v>
+      </c>
+      <c r="E201" s="89" t="s">
         <v>777</v>
       </c>
-      <c r="F200" s="119"/>
-    </row>
-    <row r="201" spans="1:6" ht="64" x14ac:dyDescent="0.2">
-      <c r="A201" s="116" t="s">
-        <v>406</v>
-      </c>
-      <c r="B201" s="116" t="s">
-        <v>778</v>
-      </c>
-      <c r="C201" s="120"/>
-      <c r="D201" s="20" t="s">
-        <v>779</v>
-      </c>
-      <c r="E201" s="120"/>
       <c r="F201" s="119"/>
     </row>
-    <row r="202" spans="1:6" ht="64" x14ac:dyDescent="0.2">
-      <c r="A202" s="116" t="s">
-        <v>409</v>
-      </c>
-      <c r="B202" s="116" t="s">
-        <v>780</v>
-      </c>
-      <c r="C202" s="120"/>
-      <c r="D202" s="20" t="s">
-        <v>781</v>
-      </c>
-      <c r="E202" s="120"/>
+    <row r="202" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A202" s="217" t="s">
+        <v>1445</v>
+      </c>
+      <c r="B202" s="179" t="s">
+        <v>1524</v>
+      </c>
+      <c r="C202" s="218" t="s">
+        <v>1525</v>
+      </c>
+      <c r="D202" s="95"/>
+      <c r="E202" s="155" t="s">
+        <v>1526</v>
+      </c>
       <c r="F202" s="119"/>
     </row>
-    <row r="203" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+    <row r="203" spans="1:6" ht="64" x14ac:dyDescent="0.2">
       <c r="A203" s="116" t="s">
         <v>406</v>
       </c>
       <c r="B203" s="116" t="s">
-        <v>782</v>
+        <v>778</v>
       </c>
       <c r="C203" s="120"/>
       <c r="D203" s="20" t="s">
-        <v>783</v>
+        <v>779</v>
       </c>
       <c r="E203" s="120"/>
       <c r="F203" s="119"/>
@@ -14382,313 +14430,313 @@
         <v>409</v>
       </c>
       <c r="B204" s="116" t="s">
-        <v>784</v>
+        <v>780</v>
       </c>
       <c r="C204" s="120"/>
       <c r="D204" s="20" t="s">
-        <v>785</v>
+        <v>781</v>
       </c>
       <c r="E204" s="120"/>
       <c r="F204" s="119"/>
     </row>
-    <row r="205" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A205" s="181" t="s">
+    <row r="205" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+      <c r="A205" s="116" t="s">
+        <v>406</v>
+      </c>
+      <c r="B205" s="116" t="s">
+        <v>782</v>
+      </c>
+      <c r="C205" s="120"/>
+      <c r="D205" s="20" t="s">
+        <v>783</v>
+      </c>
+      <c r="E205" s="120"/>
+      <c r="F205" s="119"/>
+    </row>
+    <row r="206" spans="1:6" ht="64" x14ac:dyDescent="0.2">
+      <c r="A206" s="116" t="s">
+        <v>409</v>
+      </c>
+      <c r="B206" s="116" t="s">
+        <v>784</v>
+      </c>
+      <c r="C206" s="120"/>
+      <c r="D206" s="20" t="s">
+        <v>785</v>
+      </c>
+      <c r="E206" s="120"/>
+      <c r="F206" s="119"/>
+    </row>
+    <row r="207" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A207" s="181" t="s">
         <v>786</v>
       </c>
-      <c r="B205" s="182"/>
-      <c r="C205" s="182"/>
-      <c r="D205" s="182"/>
-      <c r="E205" s="183"/>
-      <c r="F205" s="119"/>
-    </row>
-    <row r="206" spans="1:6" ht="32" x14ac:dyDescent="0.2">
-      <c r="A206" s="116" t="s">
+      <c r="B207" s="182"/>
+      <c r="C207" s="182"/>
+      <c r="D207" s="182"/>
+      <c r="E207" s="183"/>
+      <c r="F207" s="119"/>
+    </row>
+    <row r="208" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+      <c r="A208" s="116" t="s">
         <v>239</v>
       </c>
-      <c r="B206" s="116" t="s">
+      <c r="B208" s="116" t="s">
         <v>787</v>
       </c>
-      <c r="C206" s="117" t="s">
+      <c r="C208" s="117" t="s">
         <v>788</v>
       </c>
-      <c r="D206" s="116" t="s">
+      <c r="D208" s="116" t="s">
         <v>768</v>
       </c>
-      <c r="E206" s="120" t="s">
+      <c r="E208" s="120" t="s">
         <v>789</v>
       </c>
-      <c r="F206" s="119"/>
-    </row>
-    <row r="207" spans="1:6" ht="48" x14ac:dyDescent="0.2">
-      <c r="A207" s="116" t="s">
+      <c r="F208" s="119"/>
+    </row>
+    <row r="209" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+      <c r="A209" s="116" t="s">
         <v>406</v>
       </c>
-      <c r="B207" s="116" t="s">
+      <c r="B209" s="116" t="s">
         <v>790</v>
       </c>
-      <c r="C207" s="120"/>
-      <c r="D207" s="20" t="s">
+      <c r="C209" s="120"/>
+      <c r="D209" s="20" t="s">
         <v>791</v>
       </c>
-      <c r="E207" s="120"/>
-      <c r="F207" s="119"/>
-    </row>
-    <row r="208" spans="1:6" ht="64" x14ac:dyDescent="0.2">
-      <c r="A208" s="116" t="s">
-        <v>409</v>
-      </c>
-      <c r="B208" s="116" t="s">
-        <v>792</v>
-      </c>
-      <c r="C208" s="120"/>
-      <c r="D208" s="20" t="s">
-        <v>793</v>
-      </c>
-      <c r="E208" s="120"/>
-      <c r="F208" s="119"/>
-    </row>
-    <row r="209" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A209" s="181" t="s">
-        <v>794</v>
-      </c>
-      <c r="B209" s="182"/>
-      <c r="C209" s="182"/>
-      <c r="D209" s="182"/>
-      <c r="E209" s="183"/>
+      <c r="E209" s="120"/>
       <c r="F209" s="119"/>
     </row>
     <row r="210" spans="1:6" ht="64" x14ac:dyDescent="0.2">
       <c r="A210" s="116" t="s">
+        <v>409</v>
+      </c>
+      <c r="B210" s="116" t="s">
+        <v>792</v>
+      </c>
+      <c r="C210" s="120"/>
+      <c r="D210" s="20" t="s">
+        <v>793</v>
+      </c>
+      <c r="E210" s="120"/>
+      <c r="F210" s="119"/>
+    </row>
+    <row r="211" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A211" s="181" t="s">
+        <v>794</v>
+      </c>
+      <c r="B211" s="182"/>
+      <c r="C211" s="182"/>
+      <c r="D211" s="182"/>
+      <c r="E211" s="183"/>
+      <c r="F211" s="119"/>
+    </row>
+    <row r="212" spans="1:6" ht="64" x14ac:dyDescent="0.2">
+      <c r="A212" s="116" t="s">
         <v>239</v>
       </c>
-      <c r="B210" s="116" t="s">
+      <c r="B212" s="116" t="s">
         <v>795</v>
       </c>
-      <c r="C210" s="117" t="s">
+      <c r="C212" s="117" t="s">
         <v>796</v>
       </c>
-      <c r="D210" s="116" t="s">
+      <c r="D212" s="116" t="s">
         <v>797</v>
       </c>
-      <c r="E210" s="120" t="s">
+      <c r="E212" s="120" t="s">
         <v>798</v>
-      </c>
-      <c r="F210" s="119"/>
-    </row>
-    <row r="211" spans="1:6" ht="32" x14ac:dyDescent="0.2">
-      <c r="A211" s="116" t="s">
-        <v>542</v>
-      </c>
-      <c r="B211" s="116" t="s">
-        <v>799</v>
-      </c>
-      <c r="C211" s="117" t="s">
-        <v>800</v>
-      </c>
-      <c r="D211" s="116" t="s">
-        <v>801</v>
-      </c>
-      <c r="E211" s="120" t="s">
-        <v>802</v>
-      </c>
-      <c r="F211" s="119"/>
-    </row>
-    <row r="212" spans="1:6" ht="48" x14ac:dyDescent="0.2">
-      <c r="A212" s="116" t="s">
-        <v>480</v>
-      </c>
-      <c r="B212" s="116" t="s">
-        <v>803</v>
-      </c>
-      <c r="C212" s="59" t="s">
-        <v>1327</v>
-      </c>
-      <c r="D212" s="116" t="s">
-        <v>804</v>
-      </c>
-      <c r="E212" s="120" t="s">
-        <v>1331</v>
       </c>
       <c r="F212" s="119"/>
     </row>
     <row r="213" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A213" s="116" t="s">
+        <v>542</v>
+      </c>
+      <c r="B213" s="116" t="s">
+        <v>799</v>
+      </c>
+      <c r="C213" s="117" t="s">
+        <v>800</v>
+      </c>
+      <c r="D213" s="116" t="s">
+        <v>801</v>
+      </c>
+      <c r="E213" s="120" t="s">
+        <v>802</v>
+      </c>
+      <c r="F213" s="119"/>
+    </row>
+    <row r="214" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+      <c r="A214" s="116" t="s">
         <v>480</v>
       </c>
-      <c r="B213" s="116" t="s">
+      <c r="B214" s="116" t="s">
+        <v>803</v>
+      </c>
+      <c r="C214" s="59" t="s">
+        <v>1327</v>
+      </c>
+      <c r="D214" s="116" t="s">
+        <v>804</v>
+      </c>
+      <c r="E214" s="120" t="s">
+        <v>1331</v>
+      </c>
+      <c r="F214" s="119"/>
+    </row>
+    <row r="215" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+      <c r="A215" s="116" t="s">
+        <v>480</v>
+      </c>
+      <c r="B215" s="116" t="s">
         <v>1328</v>
       </c>
-      <c r="C213" s="59" t="s">
+      <c r="C215" s="59" t="s">
         <v>1329</v>
       </c>
-      <c r="D213" s="116"/>
-      <c r="E213" s="120" t="s">
+      <c r="D215" s="116"/>
+      <c r="E215" s="120" t="s">
         <v>1330</v>
       </c>
-      <c r="F213" s="119"/>
-    </row>
-    <row r="214" spans="1:6" ht="64" x14ac:dyDescent="0.2">
-      <c r="A214" s="116" t="s">
+      <c r="F215" s="119"/>
+    </row>
+    <row r="216" spans="1:6" ht="64" x14ac:dyDescent="0.2">
+      <c r="A216" s="116" t="s">
         <v>406</v>
       </c>
-      <c r="B214" s="116" t="s">
+      <c r="B216" s="116" t="s">
         <v>805</v>
       </c>
-      <c r="C214" s="120"/>
-      <c r="D214" s="20" t="s">
+      <c r="C216" s="120"/>
+      <c r="D216" s="20" t="s">
         <v>806</v>
       </c>
-      <c r="E214" s="120"/>
-      <c r="F214" s="119"/>
-    </row>
-    <row r="215" spans="1:6" ht="80" x14ac:dyDescent="0.2">
-      <c r="A215" s="116" t="s">
+      <c r="E216" s="120"/>
+      <c r="F216" s="119"/>
+    </row>
+    <row r="217" spans="1:6" ht="80" x14ac:dyDescent="0.2">
+      <c r="A217" s="116" t="s">
         <v>409</v>
       </c>
-      <c r="B215" s="116" t="s">
+      <c r="B217" s="116" t="s">
         <v>807</v>
       </c>
-      <c r="C215" s="120"/>
-      <c r="D215" s="20" t="s">
+      <c r="C217" s="120"/>
+      <c r="D217" s="20" t="s">
         <v>808</v>
       </c>
-      <c r="E215" s="120"/>
-      <c r="F215" s="119"/>
-    </row>
-    <row r="216" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A216" s="181" t="s">
+      <c r="E217" s="120"/>
+      <c r="F217" s="119"/>
+    </row>
+    <row r="218" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A218" s="181" t="s">
         <v>809</v>
       </c>
-      <c r="B216" s="182"/>
-      <c r="C216" s="182"/>
-      <c r="D216" s="182"/>
-      <c r="E216" s="183"/>
-      <c r="F216" s="119"/>
-    </row>
-    <row r="217" spans="1:6" ht="32" x14ac:dyDescent="0.2">
-      <c r="A217" s="116" t="s">
+      <c r="B218" s="182"/>
+      <c r="C218" s="182"/>
+      <c r="D218" s="182"/>
+      <c r="E218" s="183"/>
+      <c r="F218" s="119"/>
+    </row>
+    <row r="219" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+      <c r="A219" s="116" t="s">
         <v>239</v>
       </c>
-      <c r="B217" s="116" t="s">
+      <c r="B219" s="116" t="s">
         <v>810</v>
       </c>
-      <c r="C217" s="117" t="s">
+      <c r="C219" s="117" t="s">
         <v>811</v>
       </c>
-      <c r="D217" s="116" t="s">
+      <c r="D219" s="116" t="s">
         <v>812</v>
       </c>
-      <c r="E217" s="120" t="s">
+      <c r="E219" s="120" t="s">
         <v>813</v>
-      </c>
-      <c r="F217" s="119"/>
-    </row>
-    <row r="218" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A218" s="116" t="s">
-        <v>412</v>
-      </c>
-      <c r="B218" s="116" t="s">
-        <v>814</v>
-      </c>
-      <c r="C218" s="117" t="s">
-        <v>39</v>
-      </c>
-      <c r="D218" s="116"/>
-      <c r="E218" s="120" t="s">
-        <v>41</v>
-      </c>
-      <c r="F218" s="119"/>
-    </row>
-    <row r="219" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A219" s="116" t="s">
-        <v>721</v>
-      </c>
-      <c r="B219" s="116" t="s">
-        <v>815</v>
-      </c>
-      <c r="C219" s="117" t="s">
-        <v>76</v>
-      </c>
-      <c r="D219" s="116"/>
-      <c r="E219" s="120" t="s">
-        <v>78</v>
       </c>
       <c r="F219" s="119"/>
     </row>
     <row r="220" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A220" s="116" t="s">
-        <v>721</v>
+        <v>412</v>
       </c>
       <c r="B220" s="116" t="s">
-        <v>815</v>
+        <v>814</v>
       </c>
       <c r="C220" s="117" t="s">
-        <v>1338</v>
+        <v>39</v>
       </c>
       <c r="D220" s="116"/>
       <c r="E220" s="120" t="s">
-        <v>1341</v>
+        <v>41</v>
       </c>
       <c r="F220" s="119"/>
     </row>
     <row r="221" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A221" s="116" t="s">
-        <v>723</v>
+        <v>721</v>
       </c>
       <c r="B221" s="116" t="s">
-        <v>1340</v>
+        <v>815</v>
       </c>
       <c r="C221" s="117" t="s">
-        <v>43</v>
+        <v>76</v>
       </c>
       <c r="D221" s="116"/>
       <c r="E221" s="120" t="s">
-        <v>45</v>
+        <v>78</v>
       </c>
       <c r="F221" s="119"/>
     </row>
-    <row r="222" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+    <row r="222" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A222" s="116" t="s">
-        <v>32</v>
+        <v>721</v>
       </c>
       <c r="B222" s="116" t="s">
-        <v>1339</v>
-      </c>
-      <c r="C222" s="134" t="s">
-        <v>1336</v>
+        <v>815</v>
+      </c>
+      <c r="C222" s="117" t="s">
+        <v>1338</v>
       </c>
       <c r="D222" s="116"/>
       <c r="E222" s="120" t="s">
+        <v>1341</v>
+      </c>
+      <c r="F222" s="119"/>
+    </row>
+    <row r="223" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A223" s="116" t="s">
+        <v>723</v>
+      </c>
+      <c r="B223" s="116" t="s">
+        <v>1340</v>
+      </c>
+      <c r="C223" s="117" t="s">
+        <v>43</v>
+      </c>
+      <c r="D223" s="116"/>
+      <c r="E223" s="120" t="s">
+        <v>45</v>
+      </c>
+      <c r="F223" s="119"/>
+    </row>
+    <row r="224" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+      <c r="A224" s="116" t="s">
+        <v>32</v>
+      </c>
+      <c r="B224" s="116" t="s">
+        <v>1339</v>
+      </c>
+      <c r="C224" s="134" t="s">
+        <v>1336</v>
+      </c>
+      <c r="D224" s="116"/>
+      <c r="E224" s="120" t="s">
         <v>1337</v>
       </c>
-      <c r="F222" s="119"/>
-    </row>
-    <row r="223" spans="1:6" ht="48" x14ac:dyDescent="0.2">
-      <c r="A223" s="116" t="s">
-        <v>406</v>
-      </c>
-      <c r="B223" s="116" t="s">
-        <v>816</v>
-      </c>
-      <c r="C223" s="120"/>
-      <c r="D223" s="20" t="s">
-        <v>726</v>
-      </c>
-      <c r="E223" s="120"/>
-      <c r="F223" s="119"/>
-    </row>
-    <row r="224" spans="1:6" ht="64" x14ac:dyDescent="0.2">
-      <c r="A224" s="116" t="s">
-        <v>409</v>
-      </c>
-      <c r="B224" s="116" t="s">
-        <v>817</v>
-      </c>
-      <c r="C224" s="120"/>
-      <c r="D224" s="20" t="s">
-        <v>728</v>
-      </c>
-      <c r="E224" s="120"/>
       <c r="F224" s="119"/>
     </row>
     <row r="225" spans="1:6" ht="48" x14ac:dyDescent="0.2">
@@ -14696,11 +14744,11 @@
         <v>406</v>
       </c>
       <c r="B225" s="116" t="s">
-        <v>818</v>
+        <v>816</v>
       </c>
       <c r="C225" s="120"/>
       <c r="D225" s="20" t="s">
-        <v>730</v>
+        <v>726</v>
       </c>
       <c r="E225" s="120"/>
       <c r="F225" s="119"/>
@@ -14710,164 +14758,160 @@
         <v>409</v>
       </c>
       <c r="B226" s="116" t="s">
-        <v>819</v>
+        <v>817</v>
       </c>
       <c r="C226" s="120"/>
       <c r="D226" s="20" t="s">
-        <v>733</v>
+        <v>728</v>
       </c>
       <c r="E226" s="120"/>
       <c r="F226" s="119"/>
     </row>
-    <row r="227" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A227" s="181" t="s">
+    <row r="227" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+      <c r="A227" s="116" t="s">
+        <v>406</v>
+      </c>
+      <c r="B227" s="116" t="s">
+        <v>818</v>
+      </c>
+      <c r="C227" s="120"/>
+      <c r="D227" s="20" t="s">
+        <v>730</v>
+      </c>
+      <c r="E227" s="120"/>
+      <c r="F227" s="119"/>
+    </row>
+    <row r="228" spans="1:6" ht="64" x14ac:dyDescent="0.2">
+      <c r="A228" s="116" t="s">
+        <v>409</v>
+      </c>
+      <c r="B228" s="116" t="s">
+        <v>819</v>
+      </c>
+      <c r="C228" s="120"/>
+      <c r="D228" s="20" t="s">
+        <v>733</v>
+      </c>
+      <c r="E228" s="120"/>
+      <c r="F228" s="119"/>
+    </row>
+    <row r="229" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A229" s="181" t="s">
         <v>820</v>
       </c>
-      <c r="B227" s="182"/>
-      <c r="C227" s="182"/>
-      <c r="D227" s="182"/>
-      <c r="E227" s="183"/>
-      <c r="F227" s="119"/>
-    </row>
-    <row r="228" spans="1:6" ht="48" x14ac:dyDescent="0.2">
-      <c r="A228" s="116" t="s">
-        <v>239</v>
-      </c>
-      <c r="B228" s="116" t="s">
-        <v>821</v>
-      </c>
-      <c r="C228" s="117" t="s">
-        <v>822</v>
-      </c>
-      <c r="D228" s="116" t="s">
-        <v>823</v>
-      </c>
-      <c r="E228" s="120" t="s">
-        <v>54</v>
-      </c>
-      <c r="F228" s="119"/>
-    </row>
-    <row r="229" spans="1:6" ht="64" x14ac:dyDescent="0.2">
-      <c r="A229" s="116" t="s">
-        <v>257</v>
-      </c>
-      <c r="B229" s="116" t="s">
-        <v>824</v>
-      </c>
-      <c r="C229" s="117" t="s">
-        <v>740</v>
-      </c>
-      <c r="D229" s="125" t="s">
-        <v>825</v>
-      </c>
-      <c r="E229" s="120" t="s">
-        <v>742</v>
-      </c>
+      <c r="B229" s="182"/>
+      <c r="C229" s="182"/>
+      <c r="D229" s="182"/>
+      <c r="E229" s="183"/>
       <c r="F229" s="119"/>
     </row>
     <row r="230" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A230" s="116" t="s">
+        <v>239</v>
+      </c>
+      <c r="B230" s="116" t="s">
+        <v>821</v>
+      </c>
+      <c r="C230" s="117" t="s">
+        <v>822</v>
+      </c>
+      <c r="D230" s="116" t="s">
+        <v>823</v>
+      </c>
+      <c r="E230" s="120" t="s">
+        <v>54</v>
+      </c>
+      <c r="F230" s="119"/>
+    </row>
+    <row r="231" spans="1:6" ht="64" x14ac:dyDescent="0.2">
+      <c r="A231" s="116" t="s">
+        <v>257</v>
+      </c>
+      <c r="B231" s="116" t="s">
+        <v>824</v>
+      </c>
+      <c r="C231" s="117" t="s">
+        <v>740</v>
+      </c>
+      <c r="D231" s="125" t="s">
+        <v>825</v>
+      </c>
+      <c r="E231" s="120" t="s">
+        <v>742</v>
+      </c>
+      <c r="F231" s="119"/>
+    </row>
+    <row r="232" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+      <c r="A232" s="116" t="s">
         <v>32</v>
       </c>
-      <c r="B230" s="116" t="s">
+      <c r="B232" s="116" t="s">
         <v>826</v>
       </c>
-      <c r="C230" s="117" t="s">
+      <c r="C232" s="117" t="s">
         <v>744</v>
       </c>
-      <c r="D230" s="125" t="s">
+      <c r="D232" s="125" t="s">
         <v>827</v>
       </c>
-      <c r="E230" s="120" t="s">
+      <c r="E232" s="120" t="s">
         <v>746</v>
       </c>
-      <c r="F230" s="119"/>
-    </row>
-    <row r="231" spans="1:6" ht="48" x14ac:dyDescent="0.2">
-      <c r="A231" s="116" t="s">
+      <c r="F232" s="119"/>
+    </row>
+    <row r="233" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+      <c r="A233" s="116" t="s">
         <v>406</v>
       </c>
-      <c r="B231" s="116" t="s">
+      <c r="B233" s="116" t="s">
         <v>828</v>
       </c>
-      <c r="C231" s="128"/>
-      <c r="D231" s="20" t="s">
+      <c r="C233" s="128"/>
+      <c r="D233" s="20" t="s">
         <v>751</v>
       </c>
-      <c r="E231" s="120"/>
-      <c r="F231" s="119"/>
-    </row>
-    <row r="232" spans="1:6" ht="64" x14ac:dyDescent="0.2">
-      <c r="A232" s="116" t="s">
+      <c r="E233" s="120"/>
+      <c r="F233" s="119"/>
+    </row>
+    <row r="234" spans="1:6" ht="64" x14ac:dyDescent="0.2">
+      <c r="A234" s="116" t="s">
         <v>409</v>
       </c>
-      <c r="B232" s="116" t="s">
+      <c r="B234" s="116" t="s">
         <v>829</v>
       </c>
-      <c r="C232" s="120"/>
-      <c r="D232" s="20" t="s">
+      <c r="C234" s="120"/>
+      <c r="D234" s="20" t="s">
         <v>753</v>
       </c>
-      <c r="E232" s="120"/>
-      <c r="F232" s="119"/>
-    </row>
-    <row r="233" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A233" s="181" t="s">
+      <c r="E234" s="120"/>
+      <c r="F234" s="119"/>
+    </row>
+    <row r="235" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A235" s="181" t="s">
         <v>830</v>
       </c>
-      <c r="B233" s="182"/>
-      <c r="C233" s="182"/>
-      <c r="D233" s="182"/>
-      <c r="E233" s="183"/>
-      <c r="F233" s="119"/>
-    </row>
-    <row r="234" spans="1:6" ht="32" x14ac:dyDescent="0.2">
-      <c r="A234" s="116" t="s">
+      <c r="B235" s="182"/>
+      <c r="C235" s="182"/>
+      <c r="D235" s="182"/>
+      <c r="E235" s="183"/>
+      <c r="F235" s="119"/>
+    </row>
+    <row r="236" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+      <c r="A236" s="116" t="s">
         <v>239</v>
       </c>
-      <c r="B234" s="116" t="s">
+      <c r="B236" s="116" t="s">
         <v>831</v>
       </c>
-      <c r="C234" s="117" t="s">
+      <c r="C236" s="117" t="s">
         <v>832</v>
       </c>
-      <c r="D234" s="116" t="s">
+      <c r="D236" s="116" t="s">
         <v>833</v>
       </c>
-      <c r="E234" s="120" t="s">
+      <c r="E236" s="120" t="s">
         <v>834</v>
-      </c>
-      <c r="F234" s="119"/>
-    </row>
-    <row r="235" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A235" s="116" t="s">
-        <v>412</v>
-      </c>
-      <c r="B235" s="116" t="s">
-        <v>835</v>
-      </c>
-      <c r="C235" s="117" t="s">
-        <v>56</v>
-      </c>
-      <c r="D235" s="116"/>
-      <c r="E235" s="120" t="s">
-        <v>58</v>
-      </c>
-      <c r="F235" s="119"/>
-    </row>
-    <row r="236" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A236" s="116" t="s">
-        <v>412</v>
-      </c>
-      <c r="B236" s="116" t="s">
-        <v>836</v>
-      </c>
-      <c r="C236" s="117" t="s">
-        <v>60</v>
-      </c>
-      <c r="D236" s="116"/>
-      <c r="E236" s="120" t="s">
-        <v>62</v>
       </c>
       <c r="F236" s="119"/>
     </row>
@@ -14876,14 +14920,14 @@
         <v>412</v>
       </c>
       <c r="B237" s="116" t="s">
-        <v>837</v>
+        <v>835</v>
       </c>
       <c r="C237" s="117" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="D237" s="116"/>
       <c r="E237" s="120" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="F237" s="119"/>
     </row>
@@ -14892,14 +14936,14 @@
         <v>412</v>
       </c>
       <c r="B238" s="116" t="s">
-        <v>838</v>
+        <v>836</v>
       </c>
       <c r="C238" s="117" t="s">
-        <v>68</v>
+        <v>1518</v>
       </c>
       <c r="D238" s="116"/>
       <c r="E238" s="120" t="s">
-        <v>70</v>
+        <v>1521</v>
       </c>
       <c r="F238" s="119"/>
     </row>
@@ -14908,55 +14952,59 @@
         <v>412</v>
       </c>
       <c r="B239" s="116" t="s">
-        <v>839</v>
+        <v>837</v>
       </c>
       <c r="C239" s="117" t="s">
-        <v>39</v>
+        <v>1519</v>
       </c>
       <c r="D239" s="116"/>
       <c r="E239" s="120" t="s">
+        <v>1522</v>
+      </c>
+      <c r="F239" s="119"/>
+    </row>
+    <row r="240" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A240" s="116" t="s">
+        <v>412</v>
+      </c>
+      <c r="B240" s="116" t="s">
+        <v>838</v>
+      </c>
+      <c r="C240" s="117" t="s">
+        <v>1520</v>
+      </c>
+      <c r="D240" s="116"/>
+      <c r="E240" s="120" t="s">
+        <v>1523</v>
+      </c>
+      <c r="F240" s="119"/>
+    </row>
+    <row r="241" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A241" s="116" t="s">
+        <v>412</v>
+      </c>
+      <c r="B241" s="116" t="s">
+        <v>839</v>
+      </c>
+      <c r="C241" s="117" t="s">
+        <v>39</v>
+      </c>
+      <c r="D241" s="116"/>
+      <c r="E241" s="120" t="s">
         <v>41</v>
       </c>
-      <c r="F239" s="119"/>
-    </row>
-    <row r="240" spans="1:6" ht="64" x14ac:dyDescent="0.2">
-      <c r="A240" s="116" t="s">
-        <v>406</v>
-      </c>
-      <c r="B240" s="116" t="s">
-        <v>840</v>
-      </c>
-      <c r="C240" s="120"/>
-      <c r="D240" s="20" t="s">
-        <v>779</v>
-      </c>
-      <c r="E240" s="120"/>
-      <c r="F240" s="119"/>
-    </row>
-    <row r="241" spans="1:6" ht="64" x14ac:dyDescent="0.2">
-      <c r="A241" s="116" t="s">
-        <v>409</v>
-      </c>
-      <c r="B241" s="116" t="s">
-        <v>841</v>
-      </c>
-      <c r="C241" s="120"/>
-      <c r="D241" s="20" t="s">
-        <v>781</v>
-      </c>
-      <c r="E241" s="120"/>
       <c r="F241" s="119"/>
     </row>
-    <row r="242" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+    <row r="242" spans="1:6" ht="64" x14ac:dyDescent="0.2">
       <c r="A242" s="116" t="s">
         <v>406</v>
       </c>
       <c r="B242" s="116" t="s">
-        <v>842</v>
+        <v>840</v>
       </c>
       <c r="C242" s="120"/>
       <c r="D242" s="20" t="s">
-        <v>783</v>
+        <v>779</v>
       </c>
       <c r="E242" s="120"/>
       <c r="F242" s="119"/>
@@ -14966,114 +15014,106 @@
         <v>409</v>
       </c>
       <c r="B243" s="116" t="s">
-        <v>843</v>
+        <v>841</v>
       </c>
       <c r="C243" s="120"/>
       <c r="D243" s="20" t="s">
-        <v>785</v>
+        <v>781</v>
       </c>
       <c r="E243" s="120"/>
       <c r="F243" s="119"/>
     </row>
     <row r="244" spans="1:6" ht="48" x14ac:dyDescent="0.2">
-      <c r="A244" s="181" t="s">
+      <c r="A244" s="116" t="s">
+        <v>406</v>
+      </c>
+      <c r="B244" s="116" t="s">
+        <v>842</v>
+      </c>
+      <c r="C244" s="120"/>
+      <c r="D244" s="20" t="s">
+        <v>783</v>
+      </c>
+      <c r="E244" s="120"/>
+      <c r="F244" s="119"/>
+    </row>
+    <row r="245" spans="1:6" ht="64" x14ac:dyDescent="0.2">
+      <c r="A245" s="116" t="s">
+        <v>409</v>
+      </c>
+      <c r="B245" s="116" t="s">
+        <v>843</v>
+      </c>
+      <c r="C245" s="120"/>
+      <c r="D245" s="20" t="s">
+        <v>785</v>
+      </c>
+      <c r="E245" s="120"/>
+      <c r="F245" s="119"/>
+    </row>
+    <row r="246" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+      <c r="A246" s="181" t="s">
         <v>844</v>
       </c>
-      <c r="B244" s="182"/>
-      <c r="C244" s="182"/>
-      <c r="D244" s="182"/>
-      <c r="E244" s="183"/>
-      <c r="F244" s="38" t="s">
+      <c r="B246" s="182"/>
+      <c r="C246" s="182"/>
+      <c r="D246" s="182"/>
+      <c r="E246" s="183"/>
+      <c r="F246" s="38" t="s">
         <v>849</v>
       </c>
-    </row>
-    <row r="245" spans="1:6" ht="48" x14ac:dyDescent="0.2">
-      <c r="A245" s="116" t="s">
-        <v>239</v>
-      </c>
-      <c r="B245" s="116" t="s">
-        <v>845</v>
-      </c>
-      <c r="C245" s="117" t="s">
-        <v>846</v>
-      </c>
-      <c r="D245" s="116" t="s">
-        <v>847</v>
-      </c>
-      <c r="E245" s="120" t="s">
-        <v>848</v>
-      </c>
-      <c r="F245" s="119"/>
-    </row>
-    <row r="246" spans="1:6" ht="48" x14ac:dyDescent="0.2">
-      <c r="A246" s="116" t="s">
-        <v>364</v>
-      </c>
-      <c r="B246" s="116" t="s">
-        <v>850</v>
-      </c>
-      <c r="C246" s="117" t="s">
-        <v>851</v>
-      </c>
-      <c r="D246" s="116" t="s">
-        <v>852</v>
-      </c>
-      <c r="E246" s="120" t="s">
-        <v>853</v>
-      </c>
-      <c r="F246" s="119"/>
     </row>
     <row r="247" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A247" s="116" t="s">
+        <v>239</v>
+      </c>
+      <c r="B247" s="116" t="s">
+        <v>845</v>
+      </c>
+      <c r="C247" s="117" t="s">
+        <v>846</v>
+      </c>
+      <c r="D247" s="116" t="s">
+        <v>847</v>
+      </c>
+      <c r="E247" s="120" t="s">
+        <v>848</v>
+      </c>
+      <c r="F247" s="119"/>
+    </row>
+    <row r="248" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+      <c r="A248" s="116" t="s">
+        <v>364</v>
+      </c>
+      <c r="B248" s="116" t="s">
+        <v>850</v>
+      </c>
+      <c r="C248" s="117" t="s">
+        <v>851</v>
+      </c>
+      <c r="D248" s="116" t="s">
+        <v>852</v>
+      </c>
+      <c r="E248" s="120" t="s">
+        <v>853</v>
+      </c>
+      <c r="F248" s="119"/>
+    </row>
+    <row r="249" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+      <c r="A249" s="116" t="s">
         <v>257</v>
       </c>
-      <c r="B247" s="116" t="s">
+      <c r="B249" s="116" t="s">
         <v>854</v>
       </c>
-      <c r="C247" s="59" t="s">
+      <c r="C249" s="59" t="s">
         <v>1366</v>
       </c>
-      <c r="D247" s="116" t="s">
+      <c r="D249" s="116" t="s">
         <v>855</v>
       </c>
-      <c r="E247" s="120" t="s">
+      <c r="E249" s="120" t="s">
         <v>1367</v>
-      </c>
-      <c r="F247" s="119"/>
-    </row>
-    <row r="248" spans="1:6" ht="32" x14ac:dyDescent="0.2">
-      <c r="A248" s="116" t="s">
-        <v>378</v>
-      </c>
-      <c r="B248" s="116" t="s">
-        <v>856</v>
-      </c>
-      <c r="C248" s="117" t="s">
-        <v>857</v>
-      </c>
-      <c r="D248" s="121" t="s">
-        <v>858</v>
-      </c>
-      <c r="E248" s="120" t="s">
-        <v>859</v>
-      </c>
-      <c r="F248" s="119"/>
-    </row>
-    <row r="249" spans="1:6" ht="32" x14ac:dyDescent="0.2">
-      <c r="A249" s="116" t="s">
-        <v>378</v>
-      </c>
-      <c r="B249" s="116" t="s">
-        <v>860</v>
-      </c>
-      <c r="C249" s="117" t="s">
-        <v>380</v>
-      </c>
-      <c r="D249" s="121" t="s">
-        <v>861</v>
-      </c>
-      <c r="E249" s="120" t="s">
-        <v>382</v>
       </c>
       <c r="F249" s="119"/>
     </row>
@@ -15082,34 +15122,34 @@
         <v>378</v>
       </c>
       <c r="B250" s="116" t="s">
-        <v>862</v>
+        <v>856</v>
       </c>
       <c r="C250" s="117" t="s">
-        <v>863</v>
+        <v>857</v>
       </c>
       <c r="D250" s="121" t="s">
-        <v>864</v>
+        <v>858</v>
       </c>
       <c r="E250" s="120" t="s">
-        <v>865</v>
+        <v>859</v>
       </c>
       <c r="F250" s="119"/>
     </row>
-    <row r="251" spans="1:6" ht="64" x14ac:dyDescent="0.2">
+    <row r="251" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A251" s="116" t="s">
         <v>378</v>
       </c>
       <c r="B251" s="116" t="s">
-        <v>866</v>
+        <v>860</v>
       </c>
       <c r="C251" s="117" t="s">
-        <v>867</v>
+        <v>380</v>
       </c>
       <c r="D251" s="121" t="s">
-        <v>868</v>
+        <v>861</v>
       </c>
       <c r="E251" s="120" t="s">
-        <v>869</v>
+        <v>382</v>
       </c>
       <c r="F251" s="119"/>
     </row>
@@ -15118,70 +15158,70 @@
         <v>378</v>
       </c>
       <c r="B252" s="116" t="s">
-        <v>870</v>
+        <v>862</v>
       </c>
       <c r="C252" s="117" t="s">
-        <v>871</v>
+        <v>863</v>
       </c>
       <c r="D252" s="121" t="s">
-        <v>872</v>
+        <v>864</v>
       </c>
       <c r="E252" s="120" t="s">
-        <v>873</v>
+        <v>865</v>
       </c>
       <c r="F252" s="119"/>
     </row>
-    <row r="253" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+    <row r="253" spans="1:6" ht="64" x14ac:dyDescent="0.2">
       <c r="A253" s="116" t="s">
-        <v>486</v>
+        <v>378</v>
       </c>
       <c r="B253" s="116" t="s">
-        <v>874</v>
+        <v>866</v>
       </c>
       <c r="C253" s="117" t="s">
-        <v>875</v>
+        <v>867</v>
       </c>
       <c r="D253" s="121" t="s">
-        <v>872</v>
+        <v>868</v>
       </c>
       <c r="E253" s="120" t="s">
-        <v>876</v>
+        <v>869</v>
       </c>
       <c r="F253" s="119"/>
     </row>
-    <row r="254" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+    <row r="254" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A254" s="116" t="s">
         <v>378</v>
       </c>
       <c r="B254" s="116" t="s">
-        <v>877</v>
+        <v>870</v>
       </c>
       <c r="C254" s="117" t="s">
-        <v>878</v>
+        <v>871</v>
       </c>
       <c r="D254" s="121" t="s">
-        <v>879</v>
+        <v>872</v>
       </c>
       <c r="E254" s="120" t="s">
-        <v>880</v>
+        <v>873</v>
       </c>
       <c r="F254" s="119"/>
     </row>
     <row r="255" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A255" s="116" t="s">
-        <v>378</v>
+        <v>486</v>
       </c>
       <c r="B255" s="116" t="s">
-        <v>881</v>
+        <v>874</v>
       </c>
       <c r="C255" s="117" t="s">
-        <v>313</v>
+        <v>875</v>
       </c>
       <c r="D255" s="121" t="s">
-        <v>882</v>
+        <v>872</v>
       </c>
       <c r="E255" s="120" t="s">
-        <v>315</v>
+        <v>876</v>
       </c>
       <c r="F255" s="119"/>
     </row>
@@ -15190,59 +15230,81 @@
         <v>378</v>
       </c>
       <c r="B256" s="116" t="s">
-        <v>883</v>
+        <v>877</v>
       </c>
       <c r="C256" s="117" t="s">
-        <v>884</v>
+        <v>878</v>
       </c>
       <c r="D256" s="121" t="s">
-        <v>885</v>
+        <v>879</v>
       </c>
       <c r="E256" s="120" t="s">
-        <v>886</v>
+        <v>880</v>
       </c>
       <c r="F256" s="119"/>
     </row>
-    <row r="257" spans="1:6" ht="96" x14ac:dyDescent="0.2">
+    <row r="257" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A257" s="116" t="s">
         <v>378</v>
       </c>
       <c r="B257" s="116" t="s">
+        <v>881</v>
+      </c>
+      <c r="C257" s="117" t="s">
+        <v>313</v>
+      </c>
+      <c r="D257" s="121" t="s">
+        <v>882</v>
+      </c>
+      <c r="E257" s="120" t="s">
+        <v>315</v>
+      </c>
+      <c r="F257" s="119"/>
+    </row>
+    <row r="258" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+      <c r="A258" s="116" t="s">
+        <v>378</v>
+      </c>
+      <c r="B258" s="116" t="s">
+        <v>883</v>
+      </c>
+      <c r="C258" s="117" t="s">
+        <v>884</v>
+      </c>
+      <c r="D258" s="121" t="s">
+        <v>885</v>
+      </c>
+      <c r="E258" s="120" t="s">
+        <v>886</v>
+      </c>
+      <c r="F258" s="119"/>
+    </row>
+    <row r="259" spans="1:6" ht="96" x14ac:dyDescent="0.2">
+      <c r="A259" s="116" t="s">
+        <v>378</v>
+      </c>
+      <c r="B259" s="116" t="s">
         <v>887</v>
       </c>
-      <c r="C257" s="117" t="s">
+      <c r="C259" s="117" t="s">
         <v>888</v>
       </c>
-      <c r="D257" s="121" t="s">
+      <c r="D259" s="121" t="s">
         <v>889</v>
       </c>
-      <c r="E257" s="120" t="s">
+      <c r="E259" s="120" t="s">
         <v>890</v>
       </c>
-      <c r="F257" s="68" t="s">
+      <c r="F259" s="68" t="s">
         <v>892</v>
       </c>
     </row>
-    <row r="258" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A258" s="5"/>
-      <c r="B258" s="5"/>
-      <c r="C258" s="6" t="s">
-        <v>891</v>
-      </c>
-      <c r="D258" s="5"/>
-      <c r="E258" s="37"/>
-    </row>
-    <row r="259" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A259" s="5"/>
-      <c r="B259" s="5"/>
-      <c r="C259" s="6"/>
-      <c r="D259" s="5"/>
-      <c r="E259" s="37"/>
-    </row>
-    <row r="260" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="260" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A260" s="5"/>
       <c r="B260" s="5"/>
-      <c r="C260" s="6"/>
+      <c r="C260" s="6" t="s">
+        <v>891</v>
+      </c>
       <c r="D260" s="5"/>
       <c r="E260" s="37"/>
     </row>
@@ -15974,9 +16036,23 @@
       <c r="D364" s="5"/>
       <c r="E364" s="37"/>
     </row>
+    <row r="365" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A365" s="5"/>
+      <c r="B365" s="5"/>
+      <c r="C365" s="6"/>
+      <c r="D365" s="5"/>
+      <c r="E365" s="37"/>
+    </row>
+    <row r="366" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A366" s="5"/>
+      <c r="B366" s="5"/>
+      <c r="C366" s="6"/>
+      <c r="D366" s="5"/>
+      <c r="E366" s="37"/>
+    </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="A193:E193"/>
+    <mergeCell ref="A194:E194"/>
     <mergeCell ref="A172:E172"/>
     <mergeCell ref="A70:E70"/>
     <mergeCell ref="A74:E74"/>
@@ -15986,7 +16062,7 @@
     <mergeCell ref="A161:E161"/>
     <mergeCell ref="A100:E100"/>
     <mergeCell ref="A180:E180"/>
-    <mergeCell ref="A189:E189"/>
+    <mergeCell ref="A190:E190"/>
     <mergeCell ref="A65:E65"/>
     <mergeCell ref="A2:E2"/>
     <mergeCell ref="A11:E11"/>
@@ -15994,12 +16070,12 @@
     <mergeCell ref="A30:E30"/>
     <mergeCell ref="A49:E49"/>
     <mergeCell ref="A25:E25"/>
-    <mergeCell ref="A244:E244"/>
-    <mergeCell ref="A205:E205"/>
-    <mergeCell ref="A209:E209"/>
-    <mergeCell ref="A216:E216"/>
-    <mergeCell ref="A227:E227"/>
-    <mergeCell ref="A233:E233"/>
+    <mergeCell ref="A246:E246"/>
+    <mergeCell ref="A207:E207"/>
+    <mergeCell ref="A211:E211"/>
+    <mergeCell ref="A218:E218"/>
+    <mergeCell ref="A229:E229"/>
+    <mergeCell ref="A235:E235"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Missing translation on Place of death.
</commit_message>
<xml_diff>
--- a/app/data/MCCD-localisation.xlsx
+++ b/app/data/MCCD-localisation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/JALAT/GIT/medical-certificate-of-cause-of-death/app/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34AB2EFE-427B-0C4F-B09A-7C92A8EF8A7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AE7AC70-6BA0-DD4C-A4A3-5FDC55E2C16C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="13940" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="13940" firstSheet="1" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Using this document" sheetId="8" r:id="rId1"/>
@@ -69,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2267" uniqueCount="1528">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2271" uniqueCount="1531">
   <si>
     <r>
       <rPr>
@@ -5963,6 +5963,15 @@
   </si>
   <si>
     <t>057</t>
+  </si>
+  <si>
+    <t>dpdApproximateLocationHintBilingual</t>
+  </si>
+  <si>
+    <t>Enter location in English and Welsh, or in English only.</t>
+  </si>
+  <si>
+    <t>Nodwch leoliad yn Gymraeg a Saesneg, neu yn Saesneg yn unig.</t>
   </si>
 </sst>
 </file>
@@ -6969,6 +6978,12 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -6981,6 +6996,15 @@
     <xf numFmtId="0" fontId="13" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -6999,15 +7023,6 @@
     <xf numFmtId="0" fontId="13" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
@@ -7079,12 +7094,6 @@
     </xf>
     <xf numFmtId="0" fontId="13" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -7469,538 +7478,538 @@
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A1" s="180" t="s">
+      <c r="A1" s="182" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="180"/>
-      <c r="C1" s="180"/>
-      <c r="D1" s="180"/>
-      <c r="E1" s="180"/>
-      <c r="F1" s="180"/>
-      <c r="G1" s="180"/>
-      <c r="H1" s="180"/>
-      <c r="I1" s="180"/>
-      <c r="J1" s="180"/>
-      <c r="K1" s="180"/>
-      <c r="L1" s="180"/>
+      <c r="B1" s="182"/>
+      <c r="C1" s="182"/>
+      <c r="D1" s="182"/>
+      <c r="E1" s="182"/>
+      <c r="F1" s="182"/>
+      <c r="G1" s="182"/>
+      <c r="H1" s="182"/>
+      <c r="I1" s="182"/>
+      <c r="J1" s="182"/>
+      <c r="K1" s="182"/>
+      <c r="L1" s="182"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A2" s="180"/>
-      <c r="B2" s="180"/>
-      <c r="C2" s="180"/>
-      <c r="D2" s="180"/>
-      <c r="E2" s="180"/>
-      <c r="F2" s="180"/>
-      <c r="G2" s="180"/>
-      <c r="H2" s="180"/>
-      <c r="I2" s="180"/>
-      <c r="J2" s="180"/>
-      <c r="K2" s="180"/>
-      <c r="L2" s="180"/>
+      <c r="A2" s="182"/>
+      <c r="B2" s="182"/>
+      <c r="C2" s="182"/>
+      <c r="D2" s="182"/>
+      <c r="E2" s="182"/>
+      <c r="F2" s="182"/>
+      <c r="G2" s="182"/>
+      <c r="H2" s="182"/>
+      <c r="I2" s="182"/>
+      <c r="J2" s="182"/>
+      <c r="K2" s="182"/>
+      <c r="L2" s="182"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A3" s="180"/>
-      <c r="B3" s="180"/>
-      <c r="C3" s="180"/>
-      <c r="D3" s="180"/>
-      <c r="E3" s="180"/>
-      <c r="F3" s="180"/>
-      <c r="G3" s="180"/>
-      <c r="H3" s="180"/>
-      <c r="I3" s="180"/>
-      <c r="J3" s="180"/>
-      <c r="K3" s="180"/>
-      <c r="L3" s="180"/>
+      <c r="A3" s="182"/>
+      <c r="B3" s="182"/>
+      <c r="C3" s="182"/>
+      <c r="D3" s="182"/>
+      <c r="E3" s="182"/>
+      <c r="F3" s="182"/>
+      <c r="G3" s="182"/>
+      <c r="H3" s="182"/>
+      <c r="I3" s="182"/>
+      <c r="J3" s="182"/>
+      <c r="K3" s="182"/>
+      <c r="L3" s="182"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A4" s="180"/>
-      <c r="B4" s="180"/>
-      <c r="C4" s="180"/>
-      <c r="D4" s="180"/>
-      <c r="E4" s="180"/>
-      <c r="F4" s="180"/>
-      <c r="G4" s="180"/>
-      <c r="H4" s="180"/>
-      <c r="I4" s="180"/>
-      <c r="J4" s="180"/>
-      <c r="K4" s="180"/>
-      <c r="L4" s="180"/>
+      <c r="A4" s="182"/>
+      <c r="B4" s="182"/>
+      <c r="C4" s="182"/>
+      <c r="D4" s="182"/>
+      <c r="E4" s="182"/>
+      <c r="F4" s="182"/>
+      <c r="G4" s="182"/>
+      <c r="H4" s="182"/>
+      <c r="I4" s="182"/>
+      <c r="J4" s="182"/>
+      <c r="K4" s="182"/>
+      <c r="L4" s="182"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A5" s="180"/>
-      <c r="B5" s="180"/>
-      <c r="C5" s="180"/>
-      <c r="D5" s="180"/>
-      <c r="E5" s="180"/>
-      <c r="F5" s="180"/>
-      <c r="G5" s="180"/>
-      <c r="H5" s="180"/>
-      <c r="I5" s="180"/>
-      <c r="J5" s="180"/>
-      <c r="K5" s="180"/>
-      <c r="L5" s="180"/>
+      <c r="A5" s="182"/>
+      <c r="B5" s="182"/>
+      <c r="C5" s="182"/>
+      <c r="D5" s="182"/>
+      <c r="E5" s="182"/>
+      <c r="F5" s="182"/>
+      <c r="G5" s="182"/>
+      <c r="H5" s="182"/>
+      <c r="I5" s="182"/>
+      <c r="J5" s="182"/>
+      <c r="K5" s="182"/>
+      <c r="L5" s="182"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A6" s="180"/>
-      <c r="B6" s="180"/>
-      <c r="C6" s="180"/>
-      <c r="D6" s="180"/>
-      <c r="E6" s="180"/>
-      <c r="F6" s="180"/>
-      <c r="G6" s="180"/>
-      <c r="H6" s="180"/>
-      <c r="I6" s="180"/>
-      <c r="J6" s="180"/>
-      <c r="K6" s="180"/>
-      <c r="L6" s="180"/>
+      <c r="A6" s="182"/>
+      <c r="B6" s="182"/>
+      <c r="C6" s="182"/>
+      <c r="D6" s="182"/>
+      <c r="E6" s="182"/>
+      <c r="F6" s="182"/>
+      <c r="G6" s="182"/>
+      <c r="H6" s="182"/>
+      <c r="I6" s="182"/>
+      <c r="J6" s="182"/>
+      <c r="K6" s="182"/>
+      <c r="L6" s="182"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A7" s="180"/>
-      <c r="B7" s="180"/>
-      <c r="C7" s="180"/>
-      <c r="D7" s="180"/>
-      <c r="E7" s="180"/>
-      <c r="F7" s="180"/>
-      <c r="G7" s="180"/>
-      <c r="H7" s="180"/>
-      <c r="I7" s="180"/>
-      <c r="J7" s="180"/>
-      <c r="K7" s="180"/>
-      <c r="L7" s="180"/>
+      <c r="A7" s="182"/>
+      <c r="B7" s="182"/>
+      <c r="C7" s="182"/>
+      <c r="D7" s="182"/>
+      <c r="E7" s="182"/>
+      <c r="F7" s="182"/>
+      <c r="G7" s="182"/>
+      <c r="H7" s="182"/>
+      <c r="I7" s="182"/>
+      <c r="J7" s="182"/>
+      <c r="K7" s="182"/>
+      <c r="L7" s="182"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A8" s="180"/>
-      <c r="B8" s="180"/>
-      <c r="C8" s="180"/>
-      <c r="D8" s="180"/>
-      <c r="E8" s="180"/>
-      <c r="F8" s="180"/>
-      <c r="G8" s="180"/>
-      <c r="H8" s="180"/>
-      <c r="I8" s="180"/>
-      <c r="J8" s="180"/>
-      <c r="K8" s="180"/>
-      <c r="L8" s="180"/>
+      <c r="A8" s="182"/>
+      <c r="B8" s="182"/>
+      <c r="C8" s="182"/>
+      <c r="D8" s="182"/>
+      <c r="E8" s="182"/>
+      <c r="F8" s="182"/>
+      <c r="G8" s="182"/>
+      <c r="H8" s="182"/>
+      <c r="I8" s="182"/>
+      <c r="J8" s="182"/>
+      <c r="K8" s="182"/>
+      <c r="L8" s="182"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A9" s="180"/>
-      <c r="B9" s="180"/>
-      <c r="C9" s="180"/>
-      <c r="D9" s="180"/>
-      <c r="E9" s="180"/>
-      <c r="F9" s="180"/>
-      <c r="G9" s="180"/>
-      <c r="H9" s="180"/>
-      <c r="I9" s="180"/>
-      <c r="J9" s="180"/>
-      <c r="K9" s="180"/>
-      <c r="L9" s="180"/>
+      <c r="A9" s="182"/>
+      <c r="B9" s="182"/>
+      <c r="C9" s="182"/>
+      <c r="D9" s="182"/>
+      <c r="E9" s="182"/>
+      <c r="F9" s="182"/>
+      <c r="G9" s="182"/>
+      <c r="H9" s="182"/>
+      <c r="I9" s="182"/>
+      <c r="J9" s="182"/>
+      <c r="K9" s="182"/>
+      <c r="L9" s="182"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A10" s="180"/>
-      <c r="B10" s="180"/>
-      <c r="C10" s="180"/>
-      <c r="D10" s="180"/>
-      <c r="E10" s="180"/>
-      <c r="F10" s="180"/>
-      <c r="G10" s="180"/>
-      <c r="H10" s="180"/>
-      <c r="I10" s="180"/>
-      <c r="J10" s="180"/>
-      <c r="K10" s="180"/>
-      <c r="L10" s="180"/>
+      <c r="A10" s="182"/>
+      <c r="B10" s="182"/>
+      <c r="C10" s="182"/>
+      <c r="D10" s="182"/>
+      <c r="E10" s="182"/>
+      <c r="F10" s="182"/>
+      <c r="G10" s="182"/>
+      <c r="H10" s="182"/>
+      <c r="I10" s="182"/>
+      <c r="J10" s="182"/>
+      <c r="K10" s="182"/>
+      <c r="L10" s="182"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A11" s="180"/>
-      <c r="B11" s="180"/>
-      <c r="C11" s="180"/>
-      <c r="D11" s="180"/>
-      <c r="E11" s="180"/>
-      <c r="F11" s="180"/>
-      <c r="G11" s="180"/>
-      <c r="H11" s="180"/>
-      <c r="I11" s="180"/>
-      <c r="J11" s="180"/>
-      <c r="K11" s="180"/>
-      <c r="L11" s="180"/>
+      <c r="A11" s="182"/>
+      <c r="B11" s="182"/>
+      <c r="C11" s="182"/>
+      <c r="D11" s="182"/>
+      <c r="E11" s="182"/>
+      <c r="F11" s="182"/>
+      <c r="G11" s="182"/>
+      <c r="H11" s="182"/>
+      <c r="I11" s="182"/>
+      <c r="J11" s="182"/>
+      <c r="K11" s="182"/>
+      <c r="L11" s="182"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A12" s="180"/>
-      <c r="B12" s="180"/>
-      <c r="C12" s="180"/>
-      <c r="D12" s="180"/>
-      <c r="E12" s="180"/>
-      <c r="F12" s="180"/>
-      <c r="G12" s="180"/>
-      <c r="H12" s="180"/>
-      <c r="I12" s="180"/>
-      <c r="J12" s="180"/>
-      <c r="K12" s="180"/>
-      <c r="L12" s="180"/>
+      <c r="A12" s="182"/>
+      <c r="B12" s="182"/>
+      <c r="C12" s="182"/>
+      <c r="D12" s="182"/>
+      <c r="E12" s="182"/>
+      <c r="F12" s="182"/>
+      <c r="G12" s="182"/>
+      <c r="H12" s="182"/>
+      <c r="I12" s="182"/>
+      <c r="J12" s="182"/>
+      <c r="K12" s="182"/>
+      <c r="L12" s="182"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A13" s="180"/>
-      <c r="B13" s="180"/>
-      <c r="C13" s="180"/>
-      <c r="D13" s="180"/>
-      <c r="E13" s="180"/>
-      <c r="F13" s="180"/>
-      <c r="G13" s="180"/>
-      <c r="H13" s="180"/>
-      <c r="I13" s="180"/>
-      <c r="J13" s="180"/>
-      <c r="K13" s="180"/>
-      <c r="L13" s="180"/>
+      <c r="A13" s="182"/>
+      <c r="B13" s="182"/>
+      <c r="C13" s="182"/>
+      <c r="D13" s="182"/>
+      <c r="E13" s="182"/>
+      <c r="F13" s="182"/>
+      <c r="G13" s="182"/>
+      <c r="H13" s="182"/>
+      <c r="I13" s="182"/>
+      <c r="J13" s="182"/>
+      <c r="K13" s="182"/>
+      <c r="L13" s="182"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A14" s="180"/>
-      <c r="B14" s="180"/>
-      <c r="C14" s="180"/>
-      <c r="D14" s="180"/>
-      <c r="E14" s="180"/>
-      <c r="F14" s="180"/>
-      <c r="G14" s="180"/>
-      <c r="H14" s="180"/>
-      <c r="I14" s="180"/>
-      <c r="J14" s="180"/>
-      <c r="K14" s="180"/>
-      <c r="L14" s="180"/>
+      <c r="A14" s="182"/>
+      <c r="B14" s="182"/>
+      <c r="C14" s="182"/>
+      <c r="D14" s="182"/>
+      <c r="E14" s="182"/>
+      <c r="F14" s="182"/>
+      <c r="G14" s="182"/>
+      <c r="H14" s="182"/>
+      <c r="I14" s="182"/>
+      <c r="J14" s="182"/>
+      <c r="K14" s="182"/>
+      <c r="L14" s="182"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A15" s="180"/>
-      <c r="B15" s="180"/>
-      <c r="C15" s="180"/>
-      <c r="D15" s="180"/>
-      <c r="E15" s="180"/>
-      <c r="F15" s="180"/>
-      <c r="G15" s="180"/>
-      <c r="H15" s="180"/>
-      <c r="I15" s="180"/>
-      <c r="J15" s="180"/>
-      <c r="K15" s="180"/>
-      <c r="L15" s="180"/>
+      <c r="A15" s="182"/>
+      <c r="B15" s="182"/>
+      <c r="C15" s="182"/>
+      <c r="D15" s="182"/>
+      <c r="E15" s="182"/>
+      <c r="F15" s="182"/>
+      <c r="G15" s="182"/>
+      <c r="H15" s="182"/>
+      <c r="I15" s="182"/>
+      <c r="J15" s="182"/>
+      <c r="K15" s="182"/>
+      <c r="L15" s="182"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A16" s="180"/>
-      <c r="B16" s="180"/>
-      <c r="C16" s="180"/>
-      <c r="D16" s="180"/>
-      <c r="E16" s="180"/>
-      <c r="F16" s="180"/>
-      <c r="G16" s="180"/>
-      <c r="H16" s="180"/>
-      <c r="I16" s="180"/>
-      <c r="J16" s="180"/>
-      <c r="K16" s="180"/>
-      <c r="L16" s="180"/>
+      <c r="A16" s="182"/>
+      <c r="B16" s="182"/>
+      <c r="C16" s="182"/>
+      <c r="D16" s="182"/>
+      <c r="E16" s="182"/>
+      <c r="F16" s="182"/>
+      <c r="G16" s="182"/>
+      <c r="H16" s="182"/>
+      <c r="I16" s="182"/>
+      <c r="J16" s="182"/>
+      <c r="K16" s="182"/>
+      <c r="L16" s="182"/>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A17" s="180"/>
-      <c r="B17" s="180"/>
-      <c r="C17" s="180"/>
-      <c r="D17" s="180"/>
-      <c r="E17" s="180"/>
-      <c r="F17" s="180"/>
-      <c r="G17" s="180"/>
-      <c r="H17" s="180"/>
-      <c r="I17" s="180"/>
-      <c r="J17" s="180"/>
-      <c r="K17" s="180"/>
-      <c r="L17" s="180"/>
+      <c r="A17" s="182"/>
+      <c r="B17" s="182"/>
+      <c r="C17" s="182"/>
+      <c r="D17" s="182"/>
+      <c r="E17" s="182"/>
+      <c r="F17" s="182"/>
+      <c r="G17" s="182"/>
+      <c r="H17" s="182"/>
+      <c r="I17" s="182"/>
+      <c r="J17" s="182"/>
+      <c r="K17" s="182"/>
+      <c r="L17" s="182"/>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A18" s="180"/>
-      <c r="B18" s="180"/>
-      <c r="C18" s="180"/>
-      <c r="D18" s="180"/>
-      <c r="E18" s="180"/>
-      <c r="F18" s="180"/>
-      <c r="G18" s="180"/>
-      <c r="H18" s="180"/>
-      <c r="I18" s="180"/>
-      <c r="J18" s="180"/>
-      <c r="K18" s="180"/>
-      <c r="L18" s="180"/>
+      <c r="A18" s="182"/>
+      <c r="B18" s="182"/>
+      <c r="C18" s="182"/>
+      <c r="D18" s="182"/>
+      <c r="E18" s="182"/>
+      <c r="F18" s="182"/>
+      <c r="G18" s="182"/>
+      <c r="H18" s="182"/>
+      <c r="I18" s="182"/>
+      <c r="J18" s="182"/>
+      <c r="K18" s="182"/>
+      <c r="L18" s="182"/>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A19" s="180"/>
-      <c r="B19" s="180"/>
-      <c r="C19" s="180"/>
-      <c r="D19" s="180"/>
-      <c r="E19" s="180"/>
-      <c r="F19" s="180"/>
-      <c r="G19" s="180"/>
-      <c r="H19" s="180"/>
-      <c r="I19" s="180"/>
-      <c r="J19" s="180"/>
-      <c r="K19" s="180"/>
-      <c r="L19" s="180"/>
+      <c r="A19" s="182"/>
+      <c r="B19" s="182"/>
+      <c r="C19" s="182"/>
+      <c r="D19" s="182"/>
+      <c r="E19" s="182"/>
+      <c r="F19" s="182"/>
+      <c r="G19" s="182"/>
+      <c r="H19" s="182"/>
+      <c r="I19" s="182"/>
+      <c r="J19" s="182"/>
+      <c r="K19" s="182"/>
+      <c r="L19" s="182"/>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A20" s="180"/>
-      <c r="B20" s="180"/>
-      <c r="C20" s="180"/>
-      <c r="D20" s="180"/>
-      <c r="E20" s="180"/>
-      <c r="F20" s="180"/>
-      <c r="G20" s="180"/>
-      <c r="H20" s="180"/>
-      <c r="I20" s="180"/>
-      <c r="J20" s="180"/>
-      <c r="K20" s="180"/>
-      <c r="L20" s="180"/>
+      <c r="A20" s="182"/>
+      <c r="B20" s="182"/>
+      <c r="C20" s="182"/>
+      <c r="D20" s="182"/>
+      <c r="E20" s="182"/>
+      <c r="F20" s="182"/>
+      <c r="G20" s="182"/>
+      <c r="H20" s="182"/>
+      <c r="I20" s="182"/>
+      <c r="J20" s="182"/>
+      <c r="K20" s="182"/>
+      <c r="L20" s="182"/>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A21" s="180"/>
-      <c r="B21" s="180"/>
-      <c r="C21" s="180"/>
-      <c r="D21" s="180"/>
-      <c r="E21" s="180"/>
-      <c r="F21" s="180"/>
-      <c r="G21" s="180"/>
-      <c r="H21" s="180"/>
-      <c r="I21" s="180"/>
-      <c r="J21" s="180"/>
-      <c r="K21" s="180"/>
-      <c r="L21" s="180"/>
+      <c r="A21" s="182"/>
+      <c r="B21" s="182"/>
+      <c r="C21" s="182"/>
+      <c r="D21" s="182"/>
+      <c r="E21" s="182"/>
+      <c r="F21" s="182"/>
+      <c r="G21" s="182"/>
+      <c r="H21" s="182"/>
+      <c r="I21" s="182"/>
+      <c r="J21" s="182"/>
+      <c r="K21" s="182"/>
+      <c r="L21" s="182"/>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A22" s="180"/>
-      <c r="B22" s="180"/>
-      <c r="C22" s="180"/>
-      <c r="D22" s="180"/>
-      <c r="E22" s="180"/>
-      <c r="F22" s="180"/>
-      <c r="G22" s="180"/>
-      <c r="H22" s="180"/>
-      <c r="I22" s="180"/>
-      <c r="J22" s="180"/>
-      <c r="K22" s="180"/>
-      <c r="L22" s="180"/>
+      <c r="A22" s="182"/>
+      <c r="B22" s="182"/>
+      <c r="C22" s="182"/>
+      <c r="D22" s="182"/>
+      <c r="E22" s="182"/>
+      <c r="F22" s="182"/>
+      <c r="G22" s="182"/>
+      <c r="H22" s="182"/>
+      <c r="I22" s="182"/>
+      <c r="J22" s="182"/>
+      <c r="K22" s="182"/>
+      <c r="L22" s="182"/>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A23" s="180"/>
-      <c r="B23" s="180"/>
-      <c r="C23" s="180"/>
-      <c r="D23" s="180"/>
-      <c r="E23" s="180"/>
-      <c r="F23" s="180"/>
-      <c r="G23" s="180"/>
-      <c r="H23" s="180"/>
-      <c r="I23" s="180"/>
-      <c r="J23" s="180"/>
-      <c r="K23" s="180"/>
-      <c r="L23" s="180"/>
+      <c r="A23" s="182"/>
+      <c r="B23" s="182"/>
+      <c r="C23" s="182"/>
+      <c r="D23" s="182"/>
+      <c r="E23" s="182"/>
+      <c r="F23" s="182"/>
+      <c r="G23" s="182"/>
+      <c r="H23" s="182"/>
+      <c r="I23" s="182"/>
+      <c r="J23" s="182"/>
+      <c r="K23" s="182"/>
+      <c r="L23" s="182"/>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A24" s="180"/>
-      <c r="B24" s="180"/>
-      <c r="C24" s="180"/>
-      <c r="D24" s="180"/>
-      <c r="E24" s="180"/>
-      <c r="F24" s="180"/>
-      <c r="G24" s="180"/>
-      <c r="H24" s="180"/>
-      <c r="I24" s="180"/>
-      <c r="J24" s="180"/>
-      <c r="K24" s="180"/>
-      <c r="L24" s="180"/>
+      <c r="A24" s="182"/>
+      <c r="B24" s="182"/>
+      <c r="C24" s="182"/>
+      <c r="D24" s="182"/>
+      <c r="E24" s="182"/>
+      <c r="F24" s="182"/>
+      <c r="G24" s="182"/>
+      <c r="H24" s="182"/>
+      <c r="I24" s="182"/>
+      <c r="J24" s="182"/>
+      <c r="K24" s="182"/>
+      <c r="L24" s="182"/>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A25" s="180"/>
-      <c r="B25" s="180"/>
-      <c r="C25" s="180"/>
-      <c r="D25" s="180"/>
-      <c r="E25" s="180"/>
-      <c r="F25" s="180"/>
-      <c r="G25" s="180"/>
-      <c r="H25" s="180"/>
-      <c r="I25" s="180"/>
-      <c r="J25" s="180"/>
-      <c r="K25" s="180"/>
-      <c r="L25" s="180"/>
+      <c r="A25" s="182"/>
+      <c r="B25" s="182"/>
+      <c r="C25" s="182"/>
+      <c r="D25" s="182"/>
+      <c r="E25" s="182"/>
+      <c r="F25" s="182"/>
+      <c r="G25" s="182"/>
+      <c r="H25" s="182"/>
+      <c r="I25" s="182"/>
+      <c r="J25" s="182"/>
+      <c r="K25" s="182"/>
+      <c r="L25" s="182"/>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A26" s="180"/>
-      <c r="B26" s="180"/>
-      <c r="C26" s="180"/>
-      <c r="D26" s="180"/>
-      <c r="E26" s="180"/>
-      <c r="F26" s="180"/>
-      <c r="G26" s="180"/>
-      <c r="H26" s="180"/>
-      <c r="I26" s="180"/>
-      <c r="J26" s="180"/>
-      <c r="K26" s="180"/>
-      <c r="L26" s="180"/>
+      <c r="A26" s="182"/>
+      <c r="B26" s="182"/>
+      <c r="C26" s="182"/>
+      <c r="D26" s="182"/>
+      <c r="E26" s="182"/>
+      <c r="F26" s="182"/>
+      <c r="G26" s="182"/>
+      <c r="H26" s="182"/>
+      <c r="I26" s="182"/>
+      <c r="J26" s="182"/>
+      <c r="K26" s="182"/>
+      <c r="L26" s="182"/>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A27" s="180"/>
-      <c r="B27" s="180"/>
-      <c r="C27" s="180"/>
-      <c r="D27" s="180"/>
-      <c r="E27" s="180"/>
-      <c r="F27" s="180"/>
-      <c r="G27" s="180"/>
-      <c r="H27" s="180"/>
-      <c r="I27" s="180"/>
-      <c r="J27" s="180"/>
-      <c r="K27" s="180"/>
-      <c r="L27" s="180"/>
+      <c r="A27" s="182"/>
+      <c r="B27" s="182"/>
+      <c r="C27" s="182"/>
+      <c r="D27" s="182"/>
+      <c r="E27" s="182"/>
+      <c r="F27" s="182"/>
+      <c r="G27" s="182"/>
+      <c r="H27" s="182"/>
+      <c r="I27" s="182"/>
+      <c r="J27" s="182"/>
+      <c r="K27" s="182"/>
+      <c r="L27" s="182"/>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A28" s="180"/>
-      <c r="B28" s="180"/>
-      <c r="C28" s="180"/>
-      <c r="D28" s="180"/>
-      <c r="E28" s="180"/>
-      <c r="F28" s="180"/>
-      <c r="G28" s="180"/>
-      <c r="H28" s="180"/>
-      <c r="I28" s="180"/>
-      <c r="J28" s="180"/>
-      <c r="K28" s="180"/>
-      <c r="L28" s="180"/>
+      <c r="A28" s="182"/>
+      <c r="B28" s="182"/>
+      <c r="C28" s="182"/>
+      <c r="D28" s="182"/>
+      <c r="E28" s="182"/>
+      <c r="F28" s="182"/>
+      <c r="G28" s="182"/>
+      <c r="H28" s="182"/>
+      <c r="I28" s="182"/>
+      <c r="J28" s="182"/>
+      <c r="K28" s="182"/>
+      <c r="L28" s="182"/>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A29" s="180"/>
-      <c r="B29" s="180"/>
-      <c r="C29" s="180"/>
-      <c r="D29" s="180"/>
-      <c r="E29" s="180"/>
-      <c r="F29" s="180"/>
-      <c r="G29" s="180"/>
-      <c r="H29" s="180"/>
-      <c r="I29" s="180"/>
-      <c r="J29" s="180"/>
-      <c r="K29" s="180"/>
-      <c r="L29" s="180"/>
+      <c r="A29" s="182"/>
+      <c r="B29" s="182"/>
+      <c r="C29" s="182"/>
+      <c r="D29" s="182"/>
+      <c r="E29" s="182"/>
+      <c r="F29" s="182"/>
+      <c r="G29" s="182"/>
+      <c r="H29" s="182"/>
+      <c r="I29" s="182"/>
+      <c r="J29" s="182"/>
+      <c r="K29" s="182"/>
+      <c r="L29" s="182"/>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A30" s="180"/>
-      <c r="B30" s="180"/>
-      <c r="C30" s="180"/>
-      <c r="D30" s="180"/>
-      <c r="E30" s="180"/>
-      <c r="F30" s="180"/>
-      <c r="G30" s="180"/>
-      <c r="H30" s="180"/>
-      <c r="I30" s="180"/>
-      <c r="J30" s="180"/>
-      <c r="K30" s="180"/>
-      <c r="L30" s="180"/>
+      <c r="A30" s="182"/>
+      <c r="B30" s="182"/>
+      <c r="C30" s="182"/>
+      <c r="D30" s="182"/>
+      <c r="E30" s="182"/>
+      <c r="F30" s="182"/>
+      <c r="G30" s="182"/>
+      <c r="H30" s="182"/>
+      <c r="I30" s="182"/>
+      <c r="J30" s="182"/>
+      <c r="K30" s="182"/>
+      <c r="L30" s="182"/>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A31" s="180"/>
-      <c r="B31" s="180"/>
-      <c r="C31" s="180"/>
-      <c r="D31" s="180"/>
-      <c r="E31" s="180"/>
-      <c r="F31" s="180"/>
-      <c r="G31" s="180"/>
-      <c r="H31" s="180"/>
-      <c r="I31" s="180"/>
-      <c r="J31" s="180"/>
-      <c r="K31" s="180"/>
-      <c r="L31" s="180"/>
+      <c r="A31" s="182"/>
+      <c r="B31" s="182"/>
+      <c r="C31" s="182"/>
+      <c r="D31" s="182"/>
+      <c r="E31" s="182"/>
+      <c r="F31" s="182"/>
+      <c r="G31" s="182"/>
+      <c r="H31" s="182"/>
+      <c r="I31" s="182"/>
+      <c r="J31" s="182"/>
+      <c r="K31" s="182"/>
+      <c r="L31" s="182"/>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A32" s="180"/>
-      <c r="B32" s="180"/>
-      <c r="C32" s="180"/>
-      <c r="D32" s="180"/>
-      <c r="E32" s="180"/>
-      <c r="F32" s="180"/>
-      <c r="G32" s="180"/>
-      <c r="H32" s="180"/>
-      <c r="I32" s="180"/>
-      <c r="J32" s="180"/>
-      <c r="K32" s="180"/>
-      <c r="L32" s="180"/>
+      <c r="A32" s="182"/>
+      <c r="B32" s="182"/>
+      <c r="C32" s="182"/>
+      <c r="D32" s="182"/>
+      <c r="E32" s="182"/>
+      <c r="F32" s="182"/>
+      <c r="G32" s="182"/>
+      <c r="H32" s="182"/>
+      <c r="I32" s="182"/>
+      <c r="J32" s="182"/>
+      <c r="K32" s="182"/>
+      <c r="L32" s="182"/>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A33" s="180"/>
-      <c r="B33" s="180"/>
-      <c r="C33" s="180"/>
-      <c r="D33" s="180"/>
-      <c r="E33" s="180"/>
-      <c r="F33" s="180"/>
-      <c r="G33" s="180"/>
-      <c r="H33" s="180"/>
-      <c r="I33" s="180"/>
-      <c r="J33" s="180"/>
-      <c r="K33" s="180"/>
-      <c r="L33" s="180"/>
+      <c r="A33" s="182"/>
+      <c r="B33" s="182"/>
+      <c r="C33" s="182"/>
+      <c r="D33" s="182"/>
+      <c r="E33" s="182"/>
+      <c r="F33" s="182"/>
+      <c r="G33" s="182"/>
+      <c r="H33" s="182"/>
+      <c r="I33" s="182"/>
+      <c r="J33" s="182"/>
+      <c r="K33" s="182"/>
+      <c r="L33" s="182"/>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A34" s="180"/>
-      <c r="B34" s="180"/>
-      <c r="C34" s="180"/>
-      <c r="D34" s="180"/>
-      <c r="E34" s="180"/>
-      <c r="F34" s="180"/>
-      <c r="G34" s="180"/>
-      <c r="H34" s="180"/>
-      <c r="I34" s="180"/>
-      <c r="J34" s="180"/>
-      <c r="K34" s="180"/>
-      <c r="L34" s="180"/>
+      <c r="A34" s="182"/>
+      <c r="B34" s="182"/>
+      <c r="C34" s="182"/>
+      <c r="D34" s="182"/>
+      <c r="E34" s="182"/>
+      <c r="F34" s="182"/>
+      <c r="G34" s="182"/>
+      <c r="H34" s="182"/>
+      <c r="I34" s="182"/>
+      <c r="J34" s="182"/>
+      <c r="K34" s="182"/>
+      <c r="L34" s="182"/>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A35" s="180"/>
-      <c r="B35" s="180"/>
-      <c r="C35" s="180"/>
-      <c r="D35" s="180"/>
-      <c r="E35" s="180"/>
-      <c r="F35" s="180"/>
-      <c r="G35" s="180"/>
-      <c r="H35" s="180"/>
-      <c r="I35" s="180"/>
-      <c r="J35" s="180"/>
-      <c r="K35" s="180"/>
-      <c r="L35" s="180"/>
+      <c r="A35" s="182"/>
+      <c r="B35" s="182"/>
+      <c r="C35" s="182"/>
+      <c r="D35" s="182"/>
+      <c r="E35" s="182"/>
+      <c r="F35" s="182"/>
+      <c r="G35" s="182"/>
+      <c r="H35" s="182"/>
+      <c r="I35" s="182"/>
+      <c r="J35" s="182"/>
+      <c r="K35" s="182"/>
+      <c r="L35" s="182"/>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A36" s="180"/>
-      <c r="B36" s="180"/>
-      <c r="C36" s="180"/>
-      <c r="D36" s="180"/>
-      <c r="E36" s="180"/>
-      <c r="F36" s="180"/>
-      <c r="G36" s="180"/>
-      <c r="H36" s="180"/>
-      <c r="I36" s="180"/>
-      <c r="J36" s="180"/>
-      <c r="K36" s="180"/>
-      <c r="L36" s="180"/>
+      <c r="A36" s="182"/>
+      <c r="B36" s="182"/>
+      <c r="C36" s="182"/>
+      <c r="D36" s="182"/>
+      <c r="E36" s="182"/>
+      <c r="F36" s="182"/>
+      <c r="G36" s="182"/>
+      <c r="H36" s="182"/>
+      <c r="I36" s="182"/>
+      <c r="J36" s="182"/>
+      <c r="K36" s="182"/>
+      <c r="L36" s="182"/>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A37" s="180"/>
-      <c r="B37" s="180"/>
-      <c r="C37" s="180"/>
-      <c r="D37" s="180"/>
-      <c r="E37" s="180"/>
-      <c r="F37" s="180"/>
-      <c r="G37" s="180"/>
-      <c r="H37" s="180"/>
-      <c r="I37" s="180"/>
-      <c r="J37" s="180"/>
-      <c r="K37" s="180"/>
-      <c r="L37" s="180"/>
+      <c r="A37" s="182"/>
+      <c r="B37" s="182"/>
+      <c r="C37" s="182"/>
+      <c r="D37" s="182"/>
+      <c r="E37" s="182"/>
+      <c r="F37" s="182"/>
+      <c r="G37" s="182"/>
+      <c r="H37" s="182"/>
+      <c r="I37" s="182"/>
+      <c r="J37" s="182"/>
+      <c r="K37" s="182"/>
+      <c r="L37" s="182"/>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A38" s="180"/>
-      <c r="B38" s="180"/>
-      <c r="C38" s="180"/>
-      <c r="D38" s="180"/>
-      <c r="E38" s="180"/>
-      <c r="F38" s="180"/>
-      <c r="G38" s="180"/>
-      <c r="H38" s="180"/>
-      <c r="I38" s="180"/>
-      <c r="J38" s="180"/>
-      <c r="K38" s="180"/>
-      <c r="L38" s="180"/>
+      <c r="A38" s="182"/>
+      <c r="B38" s="182"/>
+      <c r="C38" s="182"/>
+      <c r="D38" s="182"/>
+      <c r="E38" s="182"/>
+      <c r="F38" s="182"/>
+      <c r="G38" s="182"/>
+      <c r="H38" s="182"/>
+      <c r="I38" s="182"/>
+      <c r="J38" s="182"/>
+      <c r="K38" s="182"/>
+      <c r="L38" s="182"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -8704,14 +8713,14 @@
       </c>
     </row>
     <row r="2" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="215" t="s">
+      <c r="A2" s="217" t="s">
         <v>1260</v>
       </c>
-      <c r="B2" s="216"/>
-      <c r="C2" s="216"/>
-      <c r="D2" s="216"/>
-      <c r="E2" s="216"/>
-      <c r="F2" s="216"/>
+      <c r="B2" s="218"/>
+      <c r="C2" s="218"/>
+      <c r="D2" s="218"/>
+      <c r="E2" s="218"/>
+      <c r="F2" s="218"/>
     </row>
     <row r="3" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
@@ -8931,14 +8940,14 @@
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A18" s="215" t="s">
+      <c r="A18" s="217" t="s">
         <v>1302</v>
       </c>
-      <c r="B18" s="216"/>
-      <c r="C18" s="216"/>
-      <c r="D18" s="216"/>
-      <c r="E18" s="216"/>
-      <c r="F18" s="216"/>
+      <c r="B18" s="218"/>
+      <c r="C18" s="218"/>
+      <c r="D18" s="218"/>
+      <c r="E18" s="218"/>
+      <c r="F18" s="218"/>
     </row>
     <row r="19" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A19" s="5" t="s">
@@ -9018,8 +9027,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F72"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A33" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
@@ -10533,13 +10542,13 @@
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" s="181" t="s">
+      <c r="A4" s="183" t="s">
         <v>1348</v>
       </c>
-      <c r="B4" s="182"/>
-      <c r="C4" s="182"/>
-      <c r="D4" s="182"/>
-      <c r="E4" s="183"/>
+      <c r="B4" s="184"/>
+      <c r="C4" s="184"/>
+      <c r="D4" s="184"/>
+      <c r="E4" s="185"/>
     </row>
     <row r="5" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
@@ -10572,13 +10581,13 @@
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7" s="181" t="s">
+      <c r="A7" s="183" t="s">
         <v>1495</v>
       </c>
-      <c r="B7" s="182"/>
-      <c r="C7" s="182"/>
-      <c r="D7" s="182"/>
-      <c r="E7" s="183"/>
+      <c r="B7" s="184"/>
+      <c r="C7" s="184"/>
+      <c r="D7" s="184"/>
+      <c r="E7" s="185"/>
     </row>
     <row r="8" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
@@ -11297,11 +11306,11 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B63483B8-55BE-4CA0-9111-55E5C0AEF6CB}">
-  <dimension ref="A1:F366"/>
+  <dimension ref="A1:F367"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A193" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B203" sqref="B203"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A205" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B213" sqref="B213"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -11336,13 +11345,13 @@
       </c>
     </row>
     <row r="2" spans="1:6" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="184" t="s">
+      <c r="A2" s="189" t="s">
         <v>363</v>
       </c>
-      <c r="B2" s="185"/>
-      <c r="C2" s="185"/>
-      <c r="D2" s="185"/>
-      <c r="E2" s="186"/>
+      <c r="B2" s="190"/>
+      <c r="C2" s="190"/>
+      <c r="D2" s="190"/>
+      <c r="E2" s="191"/>
       <c r="F2" s="33"/>
     </row>
     <row r="3" spans="1:6" ht="48" x14ac:dyDescent="0.2">
@@ -11486,13 +11495,13 @@
       <c r="F10" s="119"/>
     </row>
     <row r="11" spans="1:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="187" t="s">
+      <c r="A11" s="192" t="s">
         <v>392</v>
       </c>
-      <c r="B11" s="188"/>
-      <c r="C11" s="188"/>
-      <c r="D11" s="188"/>
-      <c r="E11" s="189"/>
+      <c r="B11" s="193"/>
+      <c r="C11" s="193"/>
+      <c r="D11" s="193"/>
+      <c r="E11" s="194"/>
       <c r="F11" s="119"/>
     </row>
     <row r="12" spans="1:6" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -11550,13 +11559,13 @@
       <c r="F14" s="86"/>
     </row>
     <row r="15" spans="1:6" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="181" t="s">
+      <c r="A15" s="183" t="s">
         <v>401</v>
       </c>
-      <c r="B15" s="182"/>
-      <c r="C15" s="182"/>
-      <c r="D15" s="182"/>
-      <c r="E15" s="183"/>
+      <c r="B15" s="184"/>
+      <c r="C15" s="184"/>
+      <c r="D15" s="184"/>
+      <c r="E15" s="185"/>
       <c r="F15" s="119"/>
     </row>
     <row r="16" spans="1:6" ht="48" x14ac:dyDescent="0.2">
@@ -11700,13 +11709,13 @@
       <c r="F24" s="119"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A25" s="181" t="s">
+      <c r="A25" s="183" t="s">
         <v>1460</v>
       </c>
-      <c r="B25" s="182"/>
-      <c r="C25" s="182"/>
-      <c r="D25" s="182"/>
-      <c r="E25" s="183"/>
+      <c r="B25" s="184"/>
+      <c r="C25" s="184"/>
+      <c r="D25" s="184"/>
+      <c r="E25" s="185"/>
       <c r="F25" s="119"/>
     </row>
     <row r="26" spans="1:6" ht="32" x14ac:dyDescent="0.2">
@@ -11772,13 +11781,13 @@
       <c r="F29" s="177"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A30" s="181" t="s">
+      <c r="A30" s="183" t="s">
         <v>431</v>
       </c>
-      <c r="B30" s="182"/>
-      <c r="C30" s="182"/>
-      <c r="D30" s="182"/>
-      <c r="E30" s="183"/>
+      <c r="B30" s="184"/>
+      <c r="C30" s="184"/>
+      <c r="D30" s="184"/>
+      <c r="E30" s="185"/>
       <c r="F30" s="119"/>
     </row>
     <row r="31" spans="1:6" ht="32" x14ac:dyDescent="0.2">
@@ -12050,13 +12059,13 @@
       <c r="F48" s="119"/>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A49" s="181" t="s">
+      <c r="A49" s="183" t="s">
         <v>475</v>
       </c>
-      <c r="B49" s="182"/>
-      <c r="C49" s="182"/>
-      <c r="D49" s="182"/>
-      <c r="E49" s="183"/>
+      <c r="B49" s="184"/>
+      <c r="C49" s="184"/>
+      <c r="D49" s="184"/>
+      <c r="E49" s="185"/>
       <c r="F49" s="119"/>
     </row>
     <row r="50" spans="1:6" ht="32" x14ac:dyDescent="0.2">
@@ -12290,13 +12299,13 @@
       <c r="F64" s="119"/>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A65" s="181" t="s">
+      <c r="A65" s="183" t="s">
         <v>505</v>
       </c>
-      <c r="B65" s="182"/>
-      <c r="C65" s="182"/>
-      <c r="D65" s="182"/>
-      <c r="E65" s="183"/>
+      <c r="B65" s="184"/>
+      <c r="C65" s="184"/>
+      <c r="D65" s="184"/>
+      <c r="E65" s="185"/>
       <c r="F65" s="119"/>
     </row>
     <row r="66" spans="1:6" ht="64" x14ac:dyDescent="0.2">
@@ -12370,13 +12379,13 @@
       <c r="F69" s="119"/>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A70" s="181" t="s">
+      <c r="A70" s="183" t="s">
         <v>517</v>
       </c>
-      <c r="B70" s="182"/>
-      <c r="C70" s="182"/>
-      <c r="D70" s="182"/>
-      <c r="E70" s="183"/>
+      <c r="B70" s="184"/>
+      <c r="C70" s="184"/>
+      <c r="D70" s="184"/>
+      <c r="E70" s="185"/>
       <c r="F70" s="119"/>
     </row>
     <row r="71" spans="1:6" ht="48" x14ac:dyDescent="0.2">
@@ -12426,13 +12435,13 @@
       <c r="F73" s="119"/>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A74" s="181" t="s">
+      <c r="A74" s="183" t="s">
         <v>522</v>
       </c>
-      <c r="B74" s="182"/>
-      <c r="C74" s="182"/>
-      <c r="D74" s="182"/>
-      <c r="E74" s="183"/>
+      <c r="B74" s="184"/>
+      <c r="C74" s="184"/>
+      <c r="D74" s="184"/>
+      <c r="E74" s="185"/>
       <c r="F74" s="119"/>
     </row>
     <row r="75" spans="1:6" ht="32" x14ac:dyDescent="0.2">
@@ -12680,13 +12689,13 @@
       <c r="F89" s="119"/>
     </row>
     <row r="90" spans="1:6" ht="62.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A90" s="181" t="s">
+      <c r="A90" s="183" t="s">
         <v>559</v>
       </c>
-      <c r="B90" s="182"/>
-      <c r="C90" s="182"/>
-      <c r="D90" s="182"/>
-      <c r="E90" s="183"/>
+      <c r="B90" s="184"/>
+      <c r="C90" s="184"/>
+      <c r="D90" s="184"/>
+      <c r="E90" s="185"/>
       <c r="F90" s="119"/>
     </row>
     <row r="91" spans="1:6" ht="62.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -12838,13 +12847,13 @@
       <c r="F99" s="119"/>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A100" s="181" t="s">
+      <c r="A100" s="183" t="s">
         <v>584</v>
       </c>
-      <c r="B100" s="182"/>
-      <c r="C100" s="182"/>
-      <c r="D100" s="182"/>
-      <c r="E100" s="183"/>
+      <c r="B100" s="184"/>
+      <c r="C100" s="184"/>
+      <c r="D100" s="184"/>
+      <c r="E100" s="185"/>
       <c r="F100" s="119"/>
     </row>
     <row r="101" spans="1:6" ht="62.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -13396,13 +13405,13 @@
       <c r="F135" s="119"/>
     </row>
     <row r="136" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A136" s="181" t="s">
+      <c r="A136" s="183" t="s">
         <v>670</v>
       </c>
-      <c r="B136" s="182"/>
-      <c r="C136" s="182"/>
-      <c r="D136" s="182"/>
-      <c r="E136" s="183"/>
+      <c r="B136" s="184"/>
+      <c r="C136" s="184"/>
+      <c r="D136" s="184"/>
+      <c r="E136" s="185"/>
       <c r="F136" s="119"/>
     </row>
     <row r="137" spans="1:6" ht="32" x14ac:dyDescent="0.2">
@@ -13622,13 +13631,13 @@
       <c r="F151" s="119"/>
     </row>
     <row r="152" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A152" s="181" t="s">
+      <c r="A152" s="183" t="s">
         <v>692</v>
       </c>
-      <c r="B152" s="182"/>
-      <c r="C152" s="182"/>
-      <c r="D152" s="182"/>
-      <c r="E152" s="183"/>
+      <c r="B152" s="184"/>
+      <c r="C152" s="184"/>
+      <c r="D152" s="184"/>
+      <c r="E152" s="185"/>
       <c r="F152" s="119"/>
     </row>
     <row r="153" spans="1:6" ht="64" x14ac:dyDescent="0.2">
@@ -13758,13 +13767,13 @@
       <c r="F160" s="119"/>
     </row>
     <row r="161" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A161" s="181" t="s">
+      <c r="A161" s="183" t="s">
         <v>713</v>
       </c>
-      <c r="B161" s="182"/>
-      <c r="C161" s="182"/>
-      <c r="D161" s="182"/>
-      <c r="E161" s="183"/>
+      <c r="B161" s="184"/>
+      <c r="C161" s="184"/>
+      <c r="D161" s="184"/>
+      <c r="E161" s="185"/>
       <c r="F161" s="119"/>
     </row>
     <row r="162" spans="1:6" ht="32" x14ac:dyDescent="0.2">
@@ -13924,13 +13933,13 @@
       <c r="F171" s="119"/>
     </row>
     <row r="172" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A172" s="181" t="s">
+      <c r="A172" s="183" t="s">
         <v>734</v>
       </c>
-      <c r="B172" s="182"/>
-      <c r="C172" s="182"/>
-      <c r="D172" s="182"/>
-      <c r="E172" s="183"/>
+      <c r="B172" s="184"/>
+      <c r="C172" s="184"/>
+      <c r="D172" s="184"/>
+      <c r="E172" s="185"/>
       <c r="F172" s="119"/>
     </row>
     <row r="173" spans="1:6" ht="48" x14ac:dyDescent="0.2">
@@ -14050,13 +14059,13 @@
       </c>
     </row>
     <row r="180" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A180" s="190" t="s">
+      <c r="A180" s="186" t="s">
         <v>754</v>
       </c>
-      <c r="B180" s="191"/>
-      <c r="C180" s="191"/>
-      <c r="D180" s="191"/>
-      <c r="E180" s="192"/>
+      <c r="B180" s="187"/>
+      <c r="C180" s="187"/>
+      <c r="D180" s="187"/>
+      <c r="E180" s="188"/>
       <c r="F180" s="129" t="s">
         <v>758</v>
       </c>
@@ -14206,13 +14215,13 @@
       <c r="F189" s="119"/>
     </row>
     <row r="190" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A190" s="181" t="s">
+      <c r="A190" s="183" t="s">
         <v>1474</v>
       </c>
-      <c r="B190" s="182"/>
-      <c r="C190" s="182"/>
-      <c r="D190" s="182"/>
-      <c r="E190" s="183"/>
+      <c r="B190" s="184"/>
+      <c r="C190" s="184"/>
+      <c r="D190" s="184"/>
+      <c r="E190" s="185"/>
       <c r="F190" s="119"/>
     </row>
     <row r="191" spans="1:6" ht="16" x14ac:dyDescent="0.2">
@@ -14260,13 +14269,13 @@
       </c>
     </row>
     <row r="194" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A194" s="181" t="s">
+      <c r="A194" s="183" t="s">
         <v>765</v>
       </c>
-      <c r="B194" s="182"/>
-      <c r="C194" s="182"/>
-      <c r="D194" s="182"/>
-      <c r="E194" s="183"/>
+      <c r="B194" s="184"/>
+      <c r="C194" s="184"/>
+      <c r="D194" s="184"/>
+      <c r="E194" s="185"/>
       <c r="F194" s="119"/>
     </row>
     <row r="195" spans="1:6" ht="32" x14ac:dyDescent="0.2">
@@ -14396,13 +14405,13 @@
       <c r="F201" s="119"/>
     </row>
     <row r="202" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A202" s="217" t="s">
+      <c r="A202" s="180" t="s">
         <v>1445</v>
       </c>
       <c r="B202" s="179" t="s">
         <v>1524</v>
       </c>
-      <c r="C202" s="218" t="s">
+      <c r="C202" s="181" t="s">
         <v>1525</v>
       </c>
       <c r="D202" s="95"/>
@@ -14468,13 +14477,13 @@
       <c r="F206" s="119"/>
     </row>
     <row r="207" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A207" s="181" t="s">
+      <c r="A207" s="183" t="s">
         <v>786</v>
       </c>
-      <c r="B207" s="182"/>
-      <c r="C207" s="182"/>
-      <c r="D207" s="182"/>
-      <c r="E207" s="183"/>
+      <c r="B207" s="184"/>
+      <c r="C207" s="184"/>
+      <c r="D207" s="184"/>
+      <c r="E207" s="185"/>
       <c r="F207" s="119"/>
     </row>
     <row r="208" spans="1:6" ht="32" x14ac:dyDescent="0.2">
@@ -14524,13 +14533,13 @@
       <c r="F210" s="119"/>
     </row>
     <row r="211" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A211" s="181" t="s">
+      <c r="A211" s="183" t="s">
         <v>794</v>
       </c>
-      <c r="B211" s="182"/>
-      <c r="C211" s="182"/>
-      <c r="D211" s="182"/>
-      <c r="E211" s="183"/>
+      <c r="B211" s="184"/>
+      <c r="C211" s="184"/>
+      <c r="D211" s="184"/>
+      <c r="E211" s="185"/>
       <c r="F211" s="119"/>
     </row>
     <row r="212" spans="1:6" ht="64" x14ac:dyDescent="0.2">
@@ -14553,141 +14562,141 @@
     </row>
     <row r="213" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A213" s="116" t="s">
+        <v>480</v>
+      </c>
+      <c r="B213" s="116" t="s">
+        <v>1528</v>
+      </c>
+      <c r="C213" s="117" t="s">
+        <v>1529</v>
+      </c>
+      <c r="D213" s="116"/>
+      <c r="E213" s="120" t="s">
+        <v>1530</v>
+      </c>
+      <c r="F213" s="119"/>
+    </row>
+    <row r="214" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+      <c r="A214" s="116" t="s">
         <v>542</v>
       </c>
-      <c r="B213" s="116" t="s">
+      <c r="B214" s="116" t="s">
         <v>799</v>
       </c>
-      <c r="C213" s="117" t="s">
+      <c r="C214" s="117" t="s">
         <v>800</v>
       </c>
-      <c r="D213" s="116" t="s">
+      <c r="D214" s="116" t="s">
         <v>801</v>
       </c>
-      <c r="E213" s="120" t="s">
+      <c r="E214" s="120" t="s">
         <v>802</v>
       </c>
-      <c r="F213" s="119"/>
-    </row>
-    <row r="214" spans="1:6" ht="48" x14ac:dyDescent="0.2">
-      <c r="A214" s="116" t="s">
-        <v>480</v>
-      </c>
-      <c r="B214" s="116" t="s">
-        <v>803</v>
-      </c>
-      <c r="C214" s="59" t="s">
-        <v>1327</v>
-      </c>
-      <c r="D214" s="116" t="s">
-        <v>804</v>
-      </c>
-      <c r="E214" s="120" t="s">
-        <v>1331</v>
-      </c>
       <c r="F214" s="119"/>
     </row>
-    <row r="215" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+    <row r="215" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A215" s="116" t="s">
         <v>480</v>
       </c>
       <c r="B215" s="116" t="s">
+        <v>803</v>
+      </c>
+      <c r="C215" s="59" t="s">
+        <v>1327</v>
+      </c>
+      <c r="D215" s="116" t="s">
+        <v>804</v>
+      </c>
+      <c r="E215" s="120" t="s">
+        <v>1331</v>
+      </c>
+      <c r="F215" s="119"/>
+    </row>
+    <row r="216" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+      <c r="A216" s="116" t="s">
+        <v>480</v>
+      </c>
+      <c r="B216" s="116" t="s">
         <v>1328</v>
       </c>
-      <c r="C215" s="59" t="s">
+      <c r="C216" s="59" t="s">
         <v>1329</v>
       </c>
-      <c r="D215" s="116"/>
-      <c r="E215" s="120" t="s">
+      <c r="D216" s="116"/>
+      <c r="E216" s="120" t="s">
         <v>1330</v>
       </c>
-      <c r="F215" s="119"/>
-    </row>
-    <row r="216" spans="1:6" ht="64" x14ac:dyDescent="0.2">
-      <c r="A216" s="116" t="s">
+      <c r="F216" s="119"/>
+    </row>
+    <row r="217" spans="1:6" ht="64" x14ac:dyDescent="0.2">
+      <c r="A217" s="116" t="s">
         <v>406</v>
       </c>
-      <c r="B216" s="116" t="s">
+      <c r="B217" s="116" t="s">
         <v>805</v>
-      </c>
-      <c r="C216" s="120"/>
-      <c r="D216" s="20" t="s">
-        <v>806</v>
-      </c>
-      <c r="E216" s="120"/>
-      <c r="F216" s="119"/>
-    </row>
-    <row r="217" spans="1:6" ht="80" x14ac:dyDescent="0.2">
-      <c r="A217" s="116" t="s">
-        <v>409</v>
-      </c>
-      <c r="B217" s="116" t="s">
-        <v>807</v>
       </c>
       <c r="C217" s="120"/>
       <c r="D217" s="20" t="s">
-        <v>808</v>
+        <v>806</v>
       </c>
       <c r="E217" s="120"/>
       <c r="F217" s="119"/>
     </row>
-    <row r="218" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A218" s="181" t="s">
+    <row r="218" spans="1:6" ht="80" x14ac:dyDescent="0.2">
+      <c r="A218" s="116" t="s">
+        <v>409</v>
+      </c>
+      <c r="B218" s="116" t="s">
+        <v>807</v>
+      </c>
+      <c r="C218" s="120"/>
+      <c r="D218" s="20" t="s">
+        <v>808</v>
+      </c>
+      <c r="E218" s="120"/>
+      <c r="F218" s="119"/>
+    </row>
+    <row r="219" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A219" s="183" t="s">
         <v>809</v>
       </c>
-      <c r="B218" s="182"/>
-      <c r="C218" s="182"/>
-      <c r="D218" s="182"/>
-      <c r="E218" s="183"/>
-      <c r="F218" s="119"/>
-    </row>
-    <row r="219" spans="1:6" ht="32" x14ac:dyDescent="0.2">
-      <c r="A219" s="116" t="s">
+      <c r="B219" s="184"/>
+      <c r="C219" s="184"/>
+      <c r="D219" s="184"/>
+      <c r="E219" s="185"/>
+      <c r="F219" s="119"/>
+    </row>
+    <row r="220" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+      <c r="A220" s="116" t="s">
         <v>239</v>
       </c>
-      <c r="B219" s="116" t="s">
+      <c r="B220" s="116" t="s">
         <v>810</v>
       </c>
-      <c r="C219" s="117" t="s">
+      <c r="C220" s="117" t="s">
         <v>811</v>
       </c>
-      <c r="D219" s="116" t="s">
+      <c r="D220" s="116" t="s">
         <v>812</v>
       </c>
-      <c r="E219" s="120" t="s">
+      <c r="E220" s="120" t="s">
         <v>813</v>
-      </c>
-      <c r="F219" s="119"/>
-    </row>
-    <row r="220" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A220" s="116" t="s">
-        <v>412</v>
-      </c>
-      <c r="B220" s="116" t="s">
-        <v>814</v>
-      </c>
-      <c r="C220" s="117" t="s">
-        <v>39</v>
-      </c>
-      <c r="D220" s="116"/>
-      <c r="E220" s="120" t="s">
-        <v>41</v>
       </c>
       <c r="F220" s="119"/>
     </row>
     <row r="221" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A221" s="116" t="s">
-        <v>721</v>
+        <v>412</v>
       </c>
       <c r="B221" s="116" t="s">
-        <v>815</v>
+        <v>814</v>
       </c>
       <c r="C221" s="117" t="s">
-        <v>76</v>
+        <v>39</v>
       </c>
       <c r="D221" s="116"/>
       <c r="E221" s="120" t="s">
-        <v>78</v>
+        <v>41</v>
       </c>
       <c r="F221" s="119"/>
     </row>
@@ -14699,235 +14708,235 @@
         <v>815</v>
       </c>
       <c r="C222" s="117" t="s">
-        <v>1338</v>
+        <v>76</v>
       </c>
       <c r="D222" s="116"/>
       <c r="E222" s="120" t="s">
-        <v>1341</v>
+        <v>78</v>
       </c>
       <c r="F222" s="119"/>
     </row>
     <row r="223" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A223" s="116" t="s">
-        <v>723</v>
+        <v>721</v>
       </c>
       <c r="B223" s="116" t="s">
-        <v>1340</v>
+        <v>815</v>
       </c>
       <c r="C223" s="117" t="s">
-        <v>43</v>
+        <v>1338</v>
       </c>
       <c r="D223" s="116"/>
       <c r="E223" s="120" t="s">
-        <v>45</v>
+        <v>1341</v>
       </c>
       <c r="F223" s="119"/>
     </row>
-    <row r="224" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+    <row r="224" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A224" s="116" t="s">
-        <v>32</v>
+        <v>723</v>
       </c>
       <c r="B224" s="116" t="s">
-        <v>1339</v>
-      </c>
-      <c r="C224" s="134" t="s">
-        <v>1336</v>
+        <v>1340</v>
+      </c>
+      <c r="C224" s="117" t="s">
+        <v>43</v>
       </c>
       <c r="D224" s="116"/>
       <c r="E224" s="120" t="s">
+        <v>45</v>
+      </c>
+      <c r="F224" s="119"/>
+    </row>
+    <row r="225" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+      <c r="A225" s="116" t="s">
+        <v>32</v>
+      </c>
+      <c r="B225" s="116" t="s">
+        <v>1339</v>
+      </c>
+      <c r="C225" s="134" t="s">
+        <v>1336</v>
+      </c>
+      <c r="D225" s="116"/>
+      <c r="E225" s="120" t="s">
         <v>1337</v>
       </c>
-      <c r="F224" s="119"/>
-    </row>
-    <row r="225" spans="1:6" ht="48" x14ac:dyDescent="0.2">
-      <c r="A225" s="116" t="s">
+      <c r="F225" s="119"/>
+    </row>
+    <row r="226" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+      <c r="A226" s="116" t="s">
         <v>406</v>
       </c>
-      <c r="B225" s="116" t="s">
+      <c r="B226" s="116" t="s">
         <v>816</v>
-      </c>
-      <c r="C225" s="120"/>
-      <c r="D225" s="20" t="s">
-        <v>726</v>
-      </c>
-      <c r="E225" s="120"/>
-      <c r="F225" s="119"/>
-    </row>
-    <row r="226" spans="1:6" ht="64" x14ac:dyDescent="0.2">
-      <c r="A226" s="116" t="s">
-        <v>409</v>
-      </c>
-      <c r="B226" s="116" t="s">
-        <v>817</v>
       </c>
       <c r="C226" s="120"/>
       <c r="D226" s="20" t="s">
-        <v>728</v>
+        <v>726</v>
       </c>
       <c r="E226" s="120"/>
       <c r="F226" s="119"/>
     </row>
-    <row r="227" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+    <row r="227" spans="1:6" ht="64" x14ac:dyDescent="0.2">
       <c r="A227" s="116" t="s">
-        <v>406</v>
+        <v>409</v>
       </c>
       <c r="B227" s="116" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="C227" s="120"/>
       <c r="D227" s="20" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="E227" s="120"/>
       <c r="F227" s="119"/>
     </row>
-    <row r="228" spans="1:6" ht="64" x14ac:dyDescent="0.2">
+    <row r="228" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A228" s="116" t="s">
-        <v>409</v>
+        <v>406</v>
       </c>
       <c r="B228" s="116" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
       <c r="C228" s="120"/>
       <c r="D228" s="20" t="s">
-        <v>733</v>
+        <v>730</v>
       </c>
       <c r="E228" s="120"/>
       <c r="F228" s="119"/>
     </row>
-    <row r="229" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A229" s="181" t="s">
+    <row r="229" spans="1:6" ht="64" x14ac:dyDescent="0.2">
+      <c r="A229" s="116" t="s">
+        <v>409</v>
+      </c>
+      <c r="B229" s="116" t="s">
+        <v>819</v>
+      </c>
+      <c r="C229" s="120"/>
+      <c r="D229" s="20" t="s">
+        <v>733</v>
+      </c>
+      <c r="E229" s="120"/>
+      <c r="F229" s="119"/>
+    </row>
+    <row r="230" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A230" s="183" t="s">
         <v>820</v>
       </c>
-      <c r="B229" s="182"/>
-      <c r="C229" s="182"/>
-      <c r="D229" s="182"/>
-      <c r="E229" s="183"/>
-      <c r="F229" s="119"/>
-    </row>
-    <row r="230" spans="1:6" ht="48" x14ac:dyDescent="0.2">
-      <c r="A230" s="116" t="s">
+      <c r="B230" s="184"/>
+      <c r="C230" s="184"/>
+      <c r="D230" s="184"/>
+      <c r="E230" s="185"/>
+      <c r="F230" s="119"/>
+    </row>
+    <row r="231" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+      <c r="A231" s="116" t="s">
         <v>239</v>
       </c>
-      <c r="B230" s="116" t="s">
+      <c r="B231" s="116" t="s">
         <v>821</v>
       </c>
-      <c r="C230" s="117" t="s">
+      <c r="C231" s="117" t="s">
         <v>822</v>
       </c>
-      <c r="D230" s="116" t="s">
+      <c r="D231" s="116" t="s">
         <v>823</v>
       </c>
-      <c r="E230" s="120" t="s">
+      <c r="E231" s="120" t="s">
         <v>54</v>
       </c>
-      <c r="F230" s="119"/>
-    </row>
-    <row r="231" spans="1:6" ht="64" x14ac:dyDescent="0.2">
-      <c r="A231" s="116" t="s">
+      <c r="F231" s="119"/>
+    </row>
+    <row r="232" spans="1:6" ht="64" x14ac:dyDescent="0.2">
+      <c r="A232" s="116" t="s">
         <v>257</v>
       </c>
-      <c r="B231" s="116" t="s">
+      <c r="B232" s="116" t="s">
         <v>824</v>
       </c>
-      <c r="C231" s="117" t="s">
+      <c r="C232" s="117" t="s">
         <v>740</v>
       </c>
-      <c r="D231" s="125" t="s">
+      <c r="D232" s="125" t="s">
         <v>825</v>
       </c>
-      <c r="E231" s="120" t="s">
+      <c r="E232" s="120" t="s">
         <v>742</v>
-      </c>
-      <c r="F231" s="119"/>
-    </row>
-    <row r="232" spans="1:6" ht="48" x14ac:dyDescent="0.2">
-      <c r="A232" s="116" t="s">
-        <v>32</v>
-      </c>
-      <c r="B232" s="116" t="s">
-        <v>826</v>
-      </c>
-      <c r="C232" s="117" t="s">
-        <v>744</v>
-      </c>
-      <c r="D232" s="125" t="s">
-        <v>827</v>
-      </c>
-      <c r="E232" s="120" t="s">
-        <v>746</v>
       </c>
       <c r="F232" s="119"/>
     </row>
     <row r="233" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A233" s="116" t="s">
+        <v>32</v>
+      </c>
+      <c r="B233" s="116" t="s">
+        <v>826</v>
+      </c>
+      <c r="C233" s="117" t="s">
+        <v>744</v>
+      </c>
+      <c r="D233" s="125" t="s">
+        <v>827</v>
+      </c>
+      <c r="E233" s="120" t="s">
+        <v>746</v>
+      </c>
+      <c r="F233" s="119"/>
+    </row>
+    <row r="234" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+      <c r="A234" s="116" t="s">
         <v>406</v>
       </c>
-      <c r="B233" s="116" t="s">
+      <c r="B234" s="116" t="s">
         <v>828</v>
       </c>
-      <c r="C233" s="128"/>
-      <c r="D233" s="20" t="s">
+      <c r="C234" s="128"/>
+      <c r="D234" s="20" t="s">
         <v>751</v>
-      </c>
-      <c r="E233" s="120"/>
-      <c r="F233" s="119"/>
-    </row>
-    <row r="234" spans="1:6" ht="64" x14ac:dyDescent="0.2">
-      <c r="A234" s="116" t="s">
-        <v>409</v>
-      </c>
-      <c r="B234" s="116" t="s">
-        <v>829</v>
-      </c>
-      <c r="C234" s="120"/>
-      <c r="D234" s="20" t="s">
-        <v>753</v>
       </c>
       <c r="E234" s="120"/>
       <c r="F234" s="119"/>
     </row>
-    <row r="235" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A235" s="181" t="s">
+    <row r="235" spans="1:6" ht="64" x14ac:dyDescent="0.2">
+      <c r="A235" s="116" t="s">
+        <v>409</v>
+      </c>
+      <c r="B235" s="116" t="s">
+        <v>829</v>
+      </c>
+      <c r="C235" s="120"/>
+      <c r="D235" s="20" t="s">
+        <v>753</v>
+      </c>
+      <c r="E235" s="120"/>
+      <c r="F235" s="119"/>
+    </row>
+    <row r="236" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A236" s="183" t="s">
         <v>830</v>
       </c>
-      <c r="B235" s="182"/>
-      <c r="C235" s="182"/>
-      <c r="D235" s="182"/>
-      <c r="E235" s="183"/>
-      <c r="F235" s="119"/>
-    </row>
-    <row r="236" spans="1:6" ht="32" x14ac:dyDescent="0.2">
-      <c r="A236" s="116" t="s">
+      <c r="B236" s="184"/>
+      <c r="C236" s="184"/>
+      <c r="D236" s="184"/>
+      <c r="E236" s="185"/>
+      <c r="F236" s="119"/>
+    </row>
+    <row r="237" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+      <c r="A237" s="116" t="s">
         <v>239</v>
       </c>
-      <c r="B236" s="116" t="s">
+      <c r="B237" s="116" t="s">
         <v>831</v>
       </c>
-      <c r="C236" s="117" t="s">
+      <c r="C237" s="117" t="s">
         <v>832</v>
       </c>
-      <c r="D236" s="116" t="s">
+      <c r="D237" s="116" t="s">
         <v>833</v>
       </c>
-      <c r="E236" s="120" t="s">
+      <c r="E237" s="120" t="s">
         <v>834</v>
-      </c>
-      <c r="F236" s="119"/>
-    </row>
-    <row r="237" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A237" s="116" t="s">
-        <v>412</v>
-      </c>
-      <c r="B237" s="116" t="s">
-        <v>835</v>
-      </c>
-      <c r="C237" s="117" t="s">
-        <v>56</v>
-      </c>
-      <c r="D237" s="116"/>
-      <c r="E237" s="120" t="s">
-        <v>58</v>
       </c>
       <c r="F237" s="119"/>
     </row>
@@ -14936,14 +14945,14 @@
         <v>412</v>
       </c>
       <c r="B238" s="116" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
       <c r="C238" s="117" t="s">
-        <v>1518</v>
+        <v>56</v>
       </c>
       <c r="D238" s="116"/>
       <c r="E238" s="120" t="s">
-        <v>1521</v>
+        <v>58</v>
       </c>
       <c r="F238" s="119"/>
     </row>
@@ -14952,14 +14961,14 @@
         <v>412</v>
       </c>
       <c r="B239" s="116" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
       <c r="C239" s="117" t="s">
-        <v>1519</v>
+        <v>1518</v>
       </c>
       <c r="D239" s="116"/>
       <c r="E239" s="120" t="s">
-        <v>1522</v>
+        <v>1521</v>
       </c>
       <c r="F239" s="119"/>
     </row>
@@ -14968,14 +14977,14 @@
         <v>412</v>
       </c>
       <c r="B240" s="116" t="s">
-        <v>838</v>
+        <v>837</v>
       </c>
       <c r="C240" s="117" t="s">
-        <v>1520</v>
+        <v>1519</v>
       </c>
       <c r="D240" s="116"/>
       <c r="E240" s="120" t="s">
-        <v>1523</v>
+        <v>1522</v>
       </c>
       <c r="F240" s="119"/>
     </row>
@@ -14984,154 +14993,152 @@
         <v>412</v>
       </c>
       <c r="B241" s="116" t="s">
-        <v>839</v>
+        <v>838</v>
       </c>
       <c r="C241" s="117" t="s">
-        <v>39</v>
+        <v>1520</v>
       </c>
       <c r="D241" s="116"/>
       <c r="E241" s="120" t="s">
+        <v>1523</v>
+      </c>
+      <c r="F241" s="119"/>
+    </row>
+    <row r="242" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A242" s="116" t="s">
+        <v>412</v>
+      </c>
+      <c r="B242" s="116" t="s">
+        <v>839</v>
+      </c>
+      <c r="C242" s="117" t="s">
+        <v>39</v>
+      </c>
+      <c r="D242" s="116"/>
+      <c r="E242" s="120" t="s">
         <v>41</v>
       </c>
-      <c r="F241" s="119"/>
-    </row>
-    <row r="242" spans="1:6" ht="64" x14ac:dyDescent="0.2">
-      <c r="A242" s="116" t="s">
-        <v>406</v>
-      </c>
-      <c r="B242" s="116" t="s">
-        <v>840</v>
-      </c>
-      <c r="C242" s="120"/>
-      <c r="D242" s="20" t="s">
-        <v>779</v>
-      </c>
-      <c r="E242" s="120"/>
       <c r="F242" s="119"/>
     </row>
     <row r="243" spans="1:6" ht="64" x14ac:dyDescent="0.2">
       <c r="A243" s="116" t="s">
-        <v>409</v>
+        <v>406</v>
       </c>
       <c r="B243" s="116" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
       <c r="C243" s="120"/>
       <c r="D243" s="20" t="s">
-        <v>781</v>
+        <v>779</v>
       </c>
       <c r="E243" s="120"/>
       <c r="F243" s="119"/>
     </row>
-    <row r="244" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+    <row r="244" spans="1:6" ht="64" x14ac:dyDescent="0.2">
       <c r="A244" s="116" t="s">
-        <v>406</v>
+        <v>409</v>
       </c>
       <c r="B244" s="116" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
       <c r="C244" s="120"/>
       <c r="D244" s="20" t="s">
-        <v>783</v>
+        <v>781</v>
       </c>
       <c r="E244" s="120"/>
       <c r="F244" s="119"/>
     </row>
-    <row r="245" spans="1:6" ht="64" x14ac:dyDescent="0.2">
+    <row r="245" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A245" s="116" t="s">
-        <v>409</v>
+        <v>406</v>
       </c>
       <c r="B245" s="116" t="s">
-        <v>843</v>
+        <v>842</v>
       </c>
       <c r="C245" s="120"/>
       <c r="D245" s="20" t="s">
-        <v>785</v>
+        <v>783</v>
       </c>
       <c r="E245" s="120"/>
       <c r="F245" s="119"/>
     </row>
-    <row r="246" spans="1:6" ht="48" x14ac:dyDescent="0.2">
-      <c r="A246" s="181" t="s">
+    <row r="246" spans="1:6" ht="64" x14ac:dyDescent="0.2">
+      <c r="A246" s="116" t="s">
+        <v>409</v>
+      </c>
+      <c r="B246" s="116" t="s">
+        <v>843</v>
+      </c>
+      <c r="C246" s="120"/>
+      <c r="D246" s="20" t="s">
+        <v>785</v>
+      </c>
+      <c r="E246" s="120"/>
+      <c r="F246" s="119"/>
+    </row>
+    <row r="247" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+      <c r="A247" s="183" t="s">
         <v>844</v>
       </c>
-      <c r="B246" s="182"/>
-      <c r="C246" s="182"/>
-      <c r="D246" s="182"/>
-      <c r="E246" s="183"/>
-      <c r="F246" s="38" t="s">
+      <c r="B247" s="184"/>
+      <c r="C247" s="184"/>
+      <c r="D247" s="184"/>
+      <c r="E247" s="185"/>
+      <c r="F247" s="38" t="s">
         <v>849</v>
       </c>
-    </row>
-    <row r="247" spans="1:6" ht="48" x14ac:dyDescent="0.2">
-      <c r="A247" s="116" t="s">
-        <v>239</v>
-      </c>
-      <c r="B247" s="116" t="s">
-        <v>845</v>
-      </c>
-      <c r="C247" s="117" t="s">
-        <v>846</v>
-      </c>
-      <c r="D247" s="116" t="s">
-        <v>847</v>
-      </c>
-      <c r="E247" s="120" t="s">
-        <v>848</v>
-      </c>
-      <c r="F247" s="119"/>
     </row>
     <row r="248" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A248" s="116" t="s">
-        <v>364</v>
+        <v>239</v>
       </c>
       <c r="B248" s="116" t="s">
-        <v>850</v>
+        <v>845</v>
       </c>
       <c r="C248" s="117" t="s">
-        <v>851</v>
+        <v>846</v>
       </c>
       <c r="D248" s="116" t="s">
-        <v>852</v>
+        <v>847</v>
       </c>
       <c r="E248" s="120" t="s">
-        <v>853</v>
+        <v>848</v>
       </c>
       <c r="F248" s="119"/>
     </row>
     <row r="249" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A249" s="116" t="s">
+        <v>364</v>
+      </c>
+      <c r="B249" s="116" t="s">
+        <v>850</v>
+      </c>
+      <c r="C249" s="117" t="s">
+        <v>851</v>
+      </c>
+      <c r="D249" s="116" t="s">
+        <v>852</v>
+      </c>
+      <c r="E249" s="120" t="s">
+        <v>853</v>
+      </c>
+      <c r="F249" s="119"/>
+    </row>
+    <row r="250" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+      <c r="A250" s="116" t="s">
         <v>257</v>
       </c>
-      <c r="B249" s="116" t="s">
+      <c r="B250" s="116" t="s">
         <v>854</v>
       </c>
-      <c r="C249" s="59" t="s">
+      <c r="C250" s="59" t="s">
         <v>1366</v>
       </c>
-      <c r="D249" s="116" t="s">
+      <c r="D250" s="116" t="s">
         <v>855</v>
       </c>
-      <c r="E249" s="120" t="s">
+      <c r="E250" s="120" t="s">
         <v>1367</v>
-      </c>
-      <c r="F249" s="119"/>
-    </row>
-    <row r="250" spans="1:6" ht="32" x14ac:dyDescent="0.2">
-      <c r="A250" s="116" t="s">
-        <v>378</v>
-      </c>
-      <c r="B250" s="116" t="s">
-        <v>856</v>
-      </c>
-      <c r="C250" s="117" t="s">
-        <v>857</v>
-      </c>
-      <c r="D250" s="121" t="s">
-        <v>858</v>
-      </c>
-      <c r="E250" s="120" t="s">
-        <v>859</v>
       </c>
       <c r="F250" s="119"/>
     </row>
@@ -15140,16 +15147,16 @@
         <v>378</v>
       </c>
       <c r="B251" s="116" t="s">
-        <v>860</v>
+        <v>856</v>
       </c>
       <c r="C251" s="117" t="s">
-        <v>380</v>
+        <v>857</v>
       </c>
       <c r="D251" s="121" t="s">
-        <v>861</v>
+        <v>858</v>
       </c>
       <c r="E251" s="120" t="s">
-        <v>382</v>
+        <v>859</v>
       </c>
       <c r="F251" s="119"/>
     </row>
@@ -15158,160 +15165,171 @@
         <v>378</v>
       </c>
       <c r="B252" s="116" t="s">
-        <v>862</v>
+        <v>860</v>
       </c>
       <c r="C252" s="117" t="s">
-        <v>863</v>
+        <v>380</v>
       </c>
       <c r="D252" s="121" t="s">
-        <v>864</v>
+        <v>861</v>
       </c>
       <c r="E252" s="120" t="s">
-        <v>865</v>
+        <v>382</v>
       </c>
       <c r="F252" s="119"/>
     </row>
-    <row r="253" spans="1:6" ht="64" x14ac:dyDescent="0.2">
+    <row r="253" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A253" s="116" t="s">
         <v>378</v>
       </c>
       <c r="B253" s="116" t="s">
-        <v>866</v>
+        <v>862</v>
       </c>
       <c r="C253" s="117" t="s">
-        <v>867</v>
+        <v>863</v>
       </c>
       <c r="D253" s="121" t="s">
-        <v>868</v>
+        <v>864</v>
       </c>
       <c r="E253" s="120" t="s">
-        <v>869</v>
+        <v>865</v>
       </c>
       <c r="F253" s="119"/>
     </row>
-    <row r="254" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+    <row r="254" spans="1:6" ht="64" x14ac:dyDescent="0.2">
       <c r="A254" s="116" t="s">
         <v>378</v>
       </c>
       <c r="B254" s="116" t="s">
-        <v>870</v>
+        <v>866</v>
       </c>
       <c r="C254" s="117" t="s">
-        <v>871</v>
+        <v>867</v>
       </c>
       <c r="D254" s="121" t="s">
-        <v>872</v>
+        <v>868</v>
       </c>
       <c r="E254" s="120" t="s">
-        <v>873</v>
+        <v>869</v>
       </c>
       <c r="F254" s="119"/>
     </row>
     <row r="255" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A255" s="116" t="s">
-        <v>486</v>
+        <v>378</v>
       </c>
       <c r="B255" s="116" t="s">
-        <v>874</v>
+        <v>870</v>
       </c>
       <c r="C255" s="117" t="s">
-        <v>875</v>
+        <v>871</v>
       </c>
       <c r="D255" s="121" t="s">
         <v>872</v>
       </c>
       <c r="E255" s="120" t="s">
+        <v>873</v>
+      </c>
+      <c r="F255" s="119"/>
+    </row>
+    <row r="256" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+      <c r="A256" s="116" t="s">
+        <v>486</v>
+      </c>
+      <c r="B256" s="116" t="s">
+        <v>874</v>
+      </c>
+      <c r="C256" s="117" t="s">
+        <v>875</v>
+      </c>
+      <c r="D256" s="121" t="s">
+        <v>872</v>
+      </c>
+      <c r="E256" s="120" t="s">
         <v>876</v>
       </c>
-      <c r="F255" s="119"/>
-    </row>
-    <row r="256" spans="1:6" ht="48" x14ac:dyDescent="0.2">
-      <c r="A256" s="116" t="s">
-        <v>378</v>
-      </c>
-      <c r="B256" s="116" t="s">
-        <v>877</v>
-      </c>
-      <c r="C256" s="117" t="s">
-        <v>878</v>
-      </c>
-      <c r="D256" s="121" t="s">
-        <v>879</v>
-      </c>
-      <c r="E256" s="120" t="s">
-        <v>880</v>
-      </c>
       <c r="F256" s="119"/>
     </row>
-    <row r="257" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+    <row r="257" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A257" s="116" t="s">
         <v>378</v>
       </c>
       <c r="B257" s="116" t="s">
-        <v>881</v>
+        <v>877</v>
       </c>
       <c r="C257" s="117" t="s">
-        <v>313</v>
+        <v>878</v>
       </c>
       <c r="D257" s="121" t="s">
-        <v>882</v>
+        <v>879</v>
       </c>
       <c r="E257" s="120" t="s">
-        <v>315</v>
+        <v>880</v>
       </c>
       <c r="F257" s="119"/>
     </row>
-    <row r="258" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+    <row r="258" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A258" s="116" t="s">
         <v>378</v>
       </c>
       <c r="B258" s="116" t="s">
-        <v>883</v>
+        <v>881</v>
       </c>
       <c r="C258" s="117" t="s">
-        <v>884</v>
+        <v>313</v>
       </c>
       <c r="D258" s="121" t="s">
-        <v>885</v>
+        <v>882</v>
       </c>
       <c r="E258" s="120" t="s">
-        <v>886</v>
+        <v>315</v>
       </c>
       <c r="F258" s="119"/>
     </row>
-    <row r="259" spans="1:6" ht="96" x14ac:dyDescent="0.2">
+    <row r="259" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A259" s="116" t="s">
         <v>378</v>
       </c>
       <c r="B259" s="116" t="s">
+        <v>883</v>
+      </c>
+      <c r="C259" s="117" t="s">
+        <v>884</v>
+      </c>
+      <c r="D259" s="121" t="s">
+        <v>885</v>
+      </c>
+      <c r="E259" s="120" t="s">
+        <v>886</v>
+      </c>
+      <c r="F259" s="119"/>
+    </row>
+    <row r="260" spans="1:6" ht="96" x14ac:dyDescent="0.2">
+      <c r="A260" s="116" t="s">
+        <v>378</v>
+      </c>
+      <c r="B260" s="116" t="s">
         <v>887</v>
       </c>
-      <c r="C259" s="117" t="s">
+      <c r="C260" s="117" t="s">
         <v>888</v>
       </c>
-      <c r="D259" s="121" t="s">
+      <c r="D260" s="121" t="s">
         <v>889</v>
       </c>
-      <c r="E259" s="120" t="s">
+      <c r="E260" s="120" t="s">
         <v>890</v>
       </c>
-      <c r="F259" s="68" t="s">
+      <c r="F260" s="68" t="s">
         <v>892</v>
       </c>
     </row>
-    <row r="260" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A260" s="5"/>
-      <c r="B260" s="5"/>
-      <c r="C260" s="6" t="s">
-        <v>891</v>
-      </c>
-      <c r="D260" s="5"/>
-      <c r="E260" s="37"/>
-    </row>
-    <row r="261" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="261" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A261" s="5"/>
       <c r="B261" s="5"/>
-      <c r="C261" s="6"/>
+      <c r="C261" s="6" t="s">
+        <v>891</v>
+      </c>
       <c r="D261" s="5"/>
       <c r="E261" s="37"/>
     </row>
@@ -16050,8 +16068,28 @@
       <c r="D366" s="5"/>
       <c r="E366" s="37"/>
     </row>
+    <row r="367" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A367" s="5"/>
+      <c r="B367" s="5"/>
+      <c r="C367" s="6"/>
+      <c r="D367" s="5"/>
+      <c r="E367" s="37"/>
+    </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="A247:E247"/>
+    <mergeCell ref="A207:E207"/>
+    <mergeCell ref="A211:E211"/>
+    <mergeCell ref="A219:E219"/>
+    <mergeCell ref="A230:E230"/>
+    <mergeCell ref="A236:E236"/>
+    <mergeCell ref="A65:E65"/>
+    <mergeCell ref="A2:E2"/>
+    <mergeCell ref="A11:E11"/>
+    <mergeCell ref="A15:E15"/>
+    <mergeCell ref="A30:E30"/>
+    <mergeCell ref="A49:E49"/>
+    <mergeCell ref="A25:E25"/>
     <mergeCell ref="A194:E194"/>
     <mergeCell ref="A172:E172"/>
     <mergeCell ref="A70:E70"/>
@@ -16063,19 +16101,6 @@
     <mergeCell ref="A100:E100"/>
     <mergeCell ref="A180:E180"/>
     <mergeCell ref="A190:E190"/>
-    <mergeCell ref="A65:E65"/>
-    <mergeCell ref="A2:E2"/>
-    <mergeCell ref="A11:E11"/>
-    <mergeCell ref="A15:E15"/>
-    <mergeCell ref="A30:E30"/>
-    <mergeCell ref="A49:E49"/>
-    <mergeCell ref="A25:E25"/>
-    <mergeCell ref="A246:E246"/>
-    <mergeCell ref="A207:E207"/>
-    <mergeCell ref="A211:E211"/>
-    <mergeCell ref="A218:E218"/>
-    <mergeCell ref="A229:E229"/>
-    <mergeCell ref="A235:E235"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -16122,13 +16147,13 @@
       </c>
     </row>
     <row r="2" spans="1:6" s="24" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="196" t="s">
+      <c r="A2" s="198" t="s">
         <v>893</v>
       </c>
-      <c r="B2" s="197"/>
-      <c r="C2" s="197"/>
-      <c r="D2" s="197"/>
-      <c r="E2" s="198"/>
+      <c r="B2" s="199"/>
+      <c r="C2" s="199"/>
+      <c r="D2" s="199"/>
+      <c r="E2" s="200"/>
     </row>
     <row r="3" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="19" t="s">
@@ -16274,13 +16299,13 @@
       </c>
     </row>
     <row r="13" spans="1:6" s="24" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="196" t="s">
+      <c r="A13" s="198" t="s">
         <v>915</v>
       </c>
-      <c r="B13" s="197"/>
-      <c r="C13" s="197"/>
-      <c r="D13" s="197"/>
-      <c r="E13" s="198"/>
+      <c r="B13" s="199"/>
+      <c r="C13" s="199"/>
+      <c r="D13" s="199"/>
+      <c r="E13" s="200"/>
     </row>
     <row r="14" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A14" s="19" t="s">
@@ -16392,13 +16417,13 @@
       </c>
     </row>
     <row r="21" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="205" t="s">
+      <c r="A21" s="207" t="s">
         <v>935</v>
       </c>
-      <c r="B21" s="206"/>
-      <c r="C21" s="206"/>
-      <c r="D21" s="206"/>
-      <c r="E21" s="207"/>
+      <c r="B21" s="208"/>
+      <c r="C21" s="208"/>
+      <c r="D21" s="208"/>
+      <c r="E21" s="209"/>
     </row>
     <row r="22" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A22" s="5" t="s">
@@ -16446,13 +16471,13 @@
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A25" s="202" t="s">
+      <c r="A25" s="204" t="s">
         <v>946</v>
       </c>
-      <c r="B25" s="203"/>
-      <c r="C25" s="203"/>
-      <c r="D25" s="203"/>
-      <c r="E25" s="204"/>
+      <c r="B25" s="205"/>
+      <c r="C25" s="205"/>
+      <c r="D25" s="205"/>
+      <c r="E25" s="206"/>
     </row>
     <row r="26" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A26" s="18" t="s">
@@ -16470,13 +16495,13 @@
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A27" s="193" t="s">
+      <c r="A27" s="195" t="s">
         <v>950</v>
       </c>
-      <c r="B27" s="194"/>
-      <c r="C27" s="194"/>
-      <c r="D27" s="194"/>
-      <c r="E27" s="195"/>
+      <c r="B27" s="196"/>
+      <c r="C27" s="196"/>
+      <c r="D27" s="196"/>
+      <c r="E27" s="197"/>
     </row>
     <row r="28" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A28" s="18" t="s">
@@ -16494,13 +16519,13 @@
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A29" s="193" t="s">
+      <c r="A29" s="195" t="s">
         <v>954</v>
       </c>
-      <c r="B29" s="194"/>
-      <c r="C29" s="194"/>
-      <c r="D29" s="194"/>
-      <c r="E29" s="195"/>
+      <c r="B29" s="196"/>
+      <c r="C29" s="196"/>
+      <c r="D29" s="196"/>
+      <c r="E29" s="197"/>
     </row>
     <row r="30" spans="1:6" ht="112" x14ac:dyDescent="0.2">
       <c r="A30" s="91" t="s">
@@ -16638,13 +16663,13 @@
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A39" s="193" t="s">
+      <c r="A39" s="195" t="s">
         <v>979</v>
       </c>
-      <c r="B39" s="194"/>
-      <c r="C39" s="194"/>
-      <c r="D39" s="194"/>
-      <c r="E39" s="195"/>
+      <c r="B39" s="196"/>
+      <c r="C39" s="196"/>
+      <c r="D39" s="196"/>
+      <c r="E39" s="197"/>
     </row>
     <row r="40" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A40" s="19" t="s">
@@ -16688,13 +16713,13 @@
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A43" s="199" t="s">
+      <c r="A43" s="201" t="s">
         <v>987</v>
       </c>
-      <c r="B43" s="200"/>
-      <c r="C43" s="200"/>
-      <c r="D43" s="200"/>
-      <c r="E43" s="201"/>
+      <c r="B43" s="202"/>
+      <c r="C43" s="202"/>
+      <c r="D43" s="202"/>
+      <c r="E43" s="203"/>
     </row>
     <row r="44" spans="1:6" ht="96" x14ac:dyDescent="0.2">
       <c r="A44" s="116" t="s">
@@ -17421,13 +17446,13 @@
       </c>
     </row>
     <row r="30" spans="1:6" s="13" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="208" t="s">
+      <c r="A30" s="210" t="s">
         <v>1101</v>
       </c>
-      <c r="B30" s="209"/>
-      <c r="C30" s="209"/>
-      <c r="D30" s="209"/>
-      <c r="E30" s="210"/>
+      <c r="B30" s="211"/>
+      <c r="C30" s="211"/>
+      <c r="D30" s="211"/>
+      <c r="E30" s="212"/>
     </row>
     <row r="31" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A31" s="140" t="s">
@@ -17490,13 +17515,13 @@
       <c r="E34" s="146"/>
     </row>
     <row r="35" spans="1:6" s="13" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="211" t="s">
+      <c r="A35" s="213" t="s">
         <v>1113</v>
       </c>
-      <c r="B35" s="212"/>
-      <c r="C35" s="213"/>
-      <c r="D35" s="212"/>
-      <c r="E35" s="214"/>
+      <c r="B35" s="214"/>
+      <c r="C35" s="215"/>
+      <c r="D35" s="214"/>
+      <c r="E35" s="216"/>
     </row>
     <row r="36" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A36" s="144" t="s">
@@ -17699,13 +17724,13 @@
       <c r="F47" s="135"/>
     </row>
     <row r="48" spans="1:6" s="13" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="208" t="s">
+      <c r="A48" s="210" t="s">
         <v>1142</v>
       </c>
-      <c r="B48" s="209"/>
-      <c r="C48" s="209"/>
-      <c r="D48" s="209"/>
-      <c r="E48" s="210"/>
+      <c r="B48" s="211"/>
+      <c r="C48" s="211"/>
+      <c r="D48" s="211"/>
+      <c r="E48" s="212"/>
     </row>
     <row r="49" spans="1:6" s="30" customFormat="1" ht="64" x14ac:dyDescent="0.2">
       <c r="A49" s="144" t="s">
@@ -18389,6 +18414,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <Readyforteam_x003f_ xmlns="565e1b1d-057e-4d85-b896-01a5881d8a45">false</Readyforteam_x003f_>
@@ -18429,15 +18463,6 @@
 </p:properties>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EAFDB110-4046-4E72-A1EF-1908ABEC3151}">
   <ds:schemaRefs>
@@ -18460,6 +18485,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8D7CE8C7-18DC-484F-8376-ED09F13D44C8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{017ACE96-8143-486E-8436-7787F6B96F4A}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -18470,12 +18503,4 @@
     <ds:schemaRef ds:uri="2799d30d-6731-4efe-ac9b-c4895a8828d9"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8D7CE8C7-18DC-484F-8376-ED09F13D44C8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Tidying up translation on bottom of confirmation page in V11bi.
</commit_message>
<xml_diff>
--- a/app/data/MCCD-localisation.xlsx
+++ b/app/data/MCCD-localisation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/JALAT/GIT/medical-certificate-of-cause-of-death/app/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AE7AC70-6BA0-DD4C-A4A3-5FDC55E2C16C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{008EAA24-5044-F64B-868A-97D3DE1C8F15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="13940" firstSheet="1" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="13940" firstSheet="4" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Using this document" sheetId="8" r:id="rId1"/>
@@ -69,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2271" uniqueCount="1531">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2279" uniqueCount="1537">
   <si>
     <r>
       <rPr>
@@ -5177,13 +5177,6 @@
     <t>confirmationPageSubheadingTwo</t>
   </si>
   <si>
-    <t>Give feedback (optional)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rhoi adborth (dewisol)
-</t>
-  </si>
-  <si>
     <t>Paragraph
 /Bold</t>
   </si>
@@ -5972,6 +5965,31 @@
   </si>
   <si>
     <t>Nodwch leoliad yn Gymraeg a Saesneg, neu yn Saesneg yn unig.</t>
+  </si>
+  <si>
+    <t>Give feedback</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rhoi adborth
+</t>
+  </si>
+  <si>
+    <t>confirmationPageTimeToComplete</t>
+  </si>
+  <si>
+    <t>(takes about 5 minutes)</t>
+  </si>
+  <si>
+    <t>(Mae'n cymryd tua 5 munud)</t>
+  </si>
+  <si>
+    <t>confirmationPageTellUsWhatYouThink</t>
+  </si>
+  <si>
+    <t>Tell us what you think about the Complete an MCCD service</t>
+  </si>
+  <si>
+    <t>Dywedwch wrthym beth yw eich barn am y Complete an MCCD service</t>
   </si>
 </sst>
 </file>
@@ -6447,7 +6465,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="219">
+  <cellXfs count="224">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -6996,6 +7014,24 @@
     <xf numFmtId="0" fontId="13" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -7005,24 +7041,6 @@
     <xf numFmtId="0" fontId="6" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
@@ -7094,6 +7112,21 @@
     </xf>
     <xf numFmtId="0" fontId="13" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -8288,13 +8321,13 @@
         <v>1230</v>
       </c>
       <c r="C2" s="151" t="s">
-        <v>1391</v>
+        <v>1389</v>
       </c>
       <c r="D2" s="92" t="s">
         <v>1231</v>
       </c>
       <c r="E2" s="152" t="s">
-        <v>1395</v>
+        <v>1393</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="80" x14ac:dyDescent="0.2">
@@ -8322,13 +8355,13 @@
         <v>1237</v>
       </c>
       <c r="C4" s="158" t="s">
-        <v>1392</v>
+        <v>1390</v>
       </c>
       <c r="D4" s="95" t="s">
         <v>400</v>
       </c>
       <c r="E4" s="155" t="s">
-        <v>1394</v>
+        <v>1392</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="60.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -8390,13 +8423,13 @@
         <v>1242</v>
       </c>
       <c r="C8" s="158" t="s">
-        <v>1391</v>
+        <v>1389</v>
       </c>
       <c r="D8" s="95" t="s">
         <v>1243</v>
       </c>
       <c r="E8" s="155" t="s">
-        <v>1395</v>
+        <v>1393</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="80" x14ac:dyDescent="0.2">
@@ -8407,11 +8440,11 @@
         <v>1244</v>
       </c>
       <c r="C9" s="158" t="s">
-        <v>1488</v>
+        <v>1486</v>
       </c>
       <c r="D9" s="179"/>
       <c r="E9" s="155" t="s">
-        <v>1489</v>
+        <v>1487</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="16" x14ac:dyDescent="0.2">
@@ -8422,13 +8455,13 @@
         <v>1245</v>
       </c>
       <c r="C10" s="158" t="s">
-        <v>1392</v>
+        <v>1390</v>
       </c>
       <c r="D10" s="95" t="s">
         <v>400</v>
       </c>
       <c r="E10" s="155" t="s">
-        <v>1394</v>
+        <v>1392</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -8490,13 +8523,13 @@
         <v>1248</v>
       </c>
       <c r="C14" s="158" t="s">
-        <v>1391</v>
+        <v>1389</v>
       </c>
       <c r="D14" s="95" t="s">
         <v>1249</v>
       </c>
       <c r="E14" s="155" t="s">
-        <v>1393</v>
+        <v>1391</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="96" x14ac:dyDescent="0.2">
@@ -8507,11 +8540,11 @@
         <v>1250</v>
       </c>
       <c r="C15" s="158" t="s">
-        <v>1490</v>
+        <v>1488</v>
       </c>
       <c r="D15" s="179"/>
       <c r="E15" s="155" t="s">
-        <v>1491</v>
+        <v>1489</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="48" x14ac:dyDescent="0.2">
@@ -8556,13 +8589,13 @@
         <v>1253</v>
       </c>
       <c r="C18" s="158" t="s">
-        <v>1392</v>
+        <v>1390</v>
       </c>
       <c r="D18" s="95" t="s">
         <v>400</v>
       </c>
       <c r="E18" s="155" t="s">
-        <v>1394</v>
+        <v>1392</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -8590,13 +8623,13 @@
         <v>1254</v>
       </c>
       <c r="C20" s="158" t="s">
-        <v>1424</v>
+        <v>1422</v>
       </c>
       <c r="D20" s="95" t="s">
         <v>1231</v>
       </c>
       <c r="E20" s="155" t="s">
-        <v>1425</v>
+        <v>1423</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="64" x14ac:dyDescent="0.2">
@@ -8607,13 +8640,13 @@
         <v>1255</v>
       </c>
       <c r="C21" s="158" t="s">
-        <v>1423</v>
+        <v>1421</v>
       </c>
       <c r="D21" s="95" t="s">
         <v>1256</v>
       </c>
       <c r="E21" s="155" t="s">
-        <v>1426</v>
+        <v>1424</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -8624,13 +8657,13 @@
         <v>1257</v>
       </c>
       <c r="C22" s="158" t="s">
-        <v>1427</v>
+        <v>1425</v>
       </c>
       <c r="D22" s="95" t="s">
         <v>400</v>
       </c>
       <c r="E22" s="155" t="s">
-        <v>1428</v>
+        <v>1426</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="48" x14ac:dyDescent="0.2">
@@ -8674,11 +8707,11 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{124C2F8F-96ED-4E65-B816-FFFEB93DC889}">
-  <dimension ref="A1:F23"/>
+  <dimension ref="A1:F25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -8747,7 +8780,7 @@
         <v>1264</v>
       </c>
       <c r="C4" s="59" t="s">
-        <v>1414</v>
+        <v>1412</v>
       </c>
       <c r="E4" s="37" t="s">
         <v>1265</v>
@@ -8775,10 +8808,10 @@
         <v>1269</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>1412</v>
+        <v>1410</v>
       </c>
       <c r="E6" s="37" t="s">
-        <v>1413</v>
+        <v>1411</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="32" x14ac:dyDescent="0.2">
@@ -8789,109 +8822,109 @@
         <v>1270</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>1271</v>
+        <v>1529</v>
       </c>
       <c r="E7" s="37" t="s">
-        <v>1272</v>
+        <v>1530</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
-        <v>1273</v>
+        <v>1271</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>1274</v>
+        <v>1272</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>1400</v>
+        <v>1398</v>
       </c>
       <c r="E8" s="37" t="s">
-        <v>1401</v>
+        <v>1399</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
+        <v>1273</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>1274</v>
+      </c>
+      <c r="C9" s="6" t="s">
         <v>1275</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="E9" s="37" t="s">
         <v>1276</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>1277</v>
-      </c>
-      <c r="E9" s="37" t="s">
-        <v>1278</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
-        <v>1275</v>
+        <v>1273</v>
       </c>
       <c r="B10" s="5" t="s">
+        <v>1277</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>1278</v>
+      </c>
+      <c r="E10" s="37" t="s">
         <v>1279</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>1280</v>
-      </c>
-      <c r="E10" s="37" t="s">
-        <v>1281</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
-        <v>1275</v>
+        <v>1273</v>
       </c>
       <c r="B11" s="5" t="s">
+        <v>1280</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>1281</v>
+      </c>
+      <c r="E11" s="37" t="s">
         <v>1282</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>1283</v>
-      </c>
-      <c r="E11" s="37" t="s">
-        <v>1284</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="5" t="s">
-        <v>1275</v>
+        <v>1273</v>
       </c>
       <c r="B12" s="5" t="s">
+        <v>1283</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>1284</v>
+      </c>
+      <c r="E12" s="37" t="s">
         <v>1285</v>
-      </c>
-      <c r="C12" s="6" t="s">
-        <v>1286</v>
-      </c>
-      <c r="E12" s="37" t="s">
-        <v>1287</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="s">
-        <v>1275</v>
+        <v>1273</v>
       </c>
       <c r="B13" s="5" t="s">
+        <v>1286</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>1287</v>
+      </c>
+      <c r="E13" s="37" t="s">
         <v>1288</v>
-      </c>
-      <c r="C13" s="6" t="s">
-        <v>1289</v>
-      </c>
-      <c r="E13" s="37" t="s">
-        <v>1290</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A14" s="5" t="s">
-        <v>1273</v>
+        <v>1271</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>1291</v>
+        <v>1289</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>1398</v>
+        <v>1396</v>
       </c>
       <c r="D14" s="1"/>
       <c r="E14" s="37" t="s">
-        <v>1399</v>
+        <v>1397</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="32" x14ac:dyDescent="0.2">
@@ -8899,14 +8932,14 @@
         <v>940</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>1292</v>
+        <v>1290</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>1293</v>
+        <v>1291</v>
       </c>
       <c r="D15" s="1"/>
       <c r="E15" s="37" t="s">
-        <v>1294</v>
+        <v>1292</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="16" x14ac:dyDescent="0.2">
@@ -8914,110 +8947,140 @@
         <v>14</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>1295</v>
+        <v>1293</v>
       </c>
       <c r="C16" s="74" t="s">
-        <v>1296</v>
+        <v>1294</v>
       </c>
       <c r="D16" s="18"/>
       <c r="E16" s="37" t="s">
-        <v>1297</v>
+        <v>1295</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A17" s="5" t="s">
+        <v>1296</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>1297</v>
+      </c>
+      <c r="C17" s="75" t="s">
         <v>1298</v>
-      </c>
-      <c r="B17" s="7" t="s">
-        <v>1299</v>
-      </c>
-      <c r="C17" s="75" t="s">
-        <v>1300</v>
       </c>
       <c r="D17" s="18"/>
       <c r="E17" s="37" t="s">
+        <v>1299</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+      <c r="A18" s="219" t="s">
+        <v>486</v>
+      </c>
+      <c r="B18" s="220" t="s">
+        <v>1534</v>
+      </c>
+      <c r="C18" s="221" t="s">
+        <v>1535</v>
+      </c>
+      <c r="D18" s="222"/>
+      <c r="E18" s="223" t="s">
+        <v>1536</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A19" s="219" t="s">
+        <v>486</v>
+      </c>
+      <c r="B19" s="220" t="s">
+        <v>1531</v>
+      </c>
+      <c r="C19" s="221" t="s">
+        <v>1532</v>
+      </c>
+      <c r="D19" s="222"/>
+      <c r="E19" s="223" t="s">
+        <v>1533</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A20" s="217" t="s">
+        <v>1300</v>
+      </c>
+      <c r="B20" s="218"/>
+      <c r="C20" s="218"/>
+      <c r="D20" s="218"/>
+      <c r="E20" s="218"/>
+      <c r="F20" s="218"/>
+    </row>
+    <row r="21" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+      <c r="A21" s="5" t="s">
+        <v>239</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>1303</v>
+      </c>
+      <c r="C21" s="6" t="s">
         <v>1301</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A18" s="217" t="s">
+      <c r="D21" s="5" t="s">
+        <v>1212</v>
+      </c>
+      <c r="E21" s="37" t="s">
         <v>1302</v>
       </c>
-      <c r="B18" s="218"/>
-      <c r="C18" s="218"/>
-      <c r="D18" s="218"/>
-      <c r="E18" s="218"/>
-      <c r="F18" s="218"/>
-    </row>
-    <row r="19" spans="1:6" ht="48" x14ac:dyDescent="0.2">
-      <c r="A19" s="5" t="s">
-        <v>239</v>
-      </c>
-      <c r="B19" s="5" t="s">
-        <v>1305</v>
-      </c>
-      <c r="C19" s="6" t="s">
-        <v>1303</v>
-      </c>
-      <c r="D19" s="5" t="s">
-        <v>1212</v>
-      </c>
-      <c r="E19" s="37" t="s">
-        <v>1304</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" ht="96" x14ac:dyDescent="0.2">
-      <c r="A20" s="5" t="s">
-        <v>257</v>
-      </c>
-      <c r="B20" s="5" t="s">
-        <v>1306</v>
-      </c>
-      <c r="C20" s="59" t="s">
-        <v>1369</v>
-      </c>
-      <c r="E20" s="37" t="s">
-        <v>1371</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A21" s="5" t="s">
-        <v>250</v>
-      </c>
-      <c r="B21" s="5" t="s">
-        <v>1307</v>
-      </c>
-      <c r="C21" s="6" t="s">
-        <v>1267</v>
-      </c>
-      <c r="E21" s="37" t="s">
-        <v>1268</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" ht="80" x14ac:dyDescent="0.2">
+    </row>
+    <row r="22" spans="1:6" ht="96" x14ac:dyDescent="0.2">
       <c r="A22" s="5" t="s">
         <v>257</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>1308</v>
-      </c>
-      <c r="C22" s="6" t="s">
+        <v>1304</v>
+      </c>
+      <c r="C22" s="59" t="s">
+        <v>1367</v>
+      </c>
+      <c r="E22" s="37" t="s">
+        <v>1369</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A23" s="5" t="s">
+        <v>250</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>1305</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>1267</v>
+      </c>
+      <c r="E23" s="37" t="s">
+        <v>1268</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="80" x14ac:dyDescent="0.2">
+      <c r="A24" s="5" t="s">
+        <v>257</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>1306</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>1368</v>
+      </c>
+      <c r="E24" s="37" t="s">
         <v>1370</v>
       </c>
-      <c r="E22" s="37" t="s">
-        <v>1372</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A23" s="18"/>
-      <c r="B23" s="28"/>
-      <c r="C23" s="74"/>
-      <c r="D23" s="18"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A25" s="18"/>
+      <c r="B25" s="28"/>
+      <c r="C25" s="74"/>
+      <c r="D25" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A2:F2"/>
-    <mergeCell ref="A18:F18"/>
+    <mergeCell ref="A20:F20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -9069,13 +9132,13 @@
         <v>7</v>
       </c>
       <c r="C2" s="100" t="s">
-        <v>1527</v>
+        <v>1525</v>
       </c>
       <c r="D2" s="98" t="s">
         <v>8</v>
       </c>
       <c r="E2" s="99" t="s">
-        <v>1527</v>
+        <v>1525</v>
       </c>
       <c r="F2" s="98"/>
     </row>
@@ -9093,7 +9156,7 @@
         <v>12</v>
       </c>
       <c r="E3" s="37" t="s">
-        <v>1368</v>
+        <v>1366</v>
       </c>
       <c r="F3" s="5" t="s">
         <v>13</v>
@@ -9158,7 +9221,7 @@
     <row r="7" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="5"/>
       <c r="B7" s="5" t="s">
-        <v>1463</v>
+        <v>1461</v>
       </c>
       <c r="C7" s="6" t="s">
         <v>349</v>
@@ -9958,10 +10021,10 @@
     <row r="53" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A53" s="86"/>
       <c r="B53" s="163" t="s">
-        <v>1415</v>
+        <v>1413</v>
       </c>
       <c r="C53" s="164" t="s">
-        <v>1416</v>
+        <v>1414</v>
       </c>
       <c r="D53" s="86"/>
       <c r="E53" s="165" t="s">
@@ -10077,7 +10140,7 @@
       </c>
       <c r="D61" s="86"/>
       <c r="E61" s="165" t="s">
-        <v>1431</v>
+        <v>1429</v>
       </c>
       <c r="F61" s="86"/>
     </row>
@@ -10164,46 +10227,46 @@
     <row r="68" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A68" s="86"/>
       <c r="B68" s="163" t="s">
-        <v>1419</v>
+        <v>1417</v>
       </c>
       <c r="C68" s="164" t="s">
-        <v>1420</v>
+        <v>1418</v>
       </c>
       <c r="D68" s="86"/>
       <c r="E68" s="165" t="s">
-        <v>1421</v>
+        <v>1419</v>
       </c>
       <c r="F68" s="166" t="s">
-        <v>1422</v>
+        <v>1420</v>
       </c>
     </row>
     <row r="69" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A69" s="86"/>
       <c r="B69" s="163" t="s">
-        <v>1417</v>
+        <v>1415</v>
       </c>
       <c r="C69" s="164" t="s">
-        <v>1300</v>
+        <v>1298</v>
       </c>
       <c r="D69" s="86"/>
       <c r="E69" s="165" t="s">
-        <v>1418</v>
+        <v>1416</v>
       </c>
     </row>
     <row r="70" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="B70" s="1" t="s">
-        <v>1319</v>
+        <v>1317</v>
       </c>
       <c r="C70" s="2" t="s">
+        <v>1318</v>
+      </c>
+      <c r="E70" s="40" t="s">
         <v>1320</v>
-      </c>
-      <c r="E70" s="40" t="s">
-        <v>1322</v>
       </c>
     </row>
     <row r="71" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="B71" s="1" t="s">
-        <v>1321</v>
+        <v>1319</v>
       </c>
       <c r="C71" s="2" t="s">
         <v>76</v>
@@ -10214,13 +10277,13 @@
     </row>
     <row r="72" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="B72" s="1" t="s">
+        <v>1430</v>
+      </c>
+      <c r="C72" s="2" t="s">
+        <v>1431</v>
+      </c>
+      <c r="E72" s="40" t="s">
         <v>1432</v>
-      </c>
-      <c r="C72" s="2" t="s">
-        <v>1433</v>
-      </c>
-      <c r="E72" s="40" t="s">
-        <v>1434</v>
       </c>
     </row>
   </sheetData>
@@ -10515,14 +10578,14 @@
         <v>239</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>1344</v>
+        <v>1342</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>1345</v>
+        <v>1343</v>
       </c>
       <c r="D2" s="5"/>
       <c r="E2" s="43" t="s">
-        <v>1353</v>
+        <v>1351</v>
       </c>
       <c r="F2" s="1"/>
     </row>
@@ -10531,19 +10594,19 @@
         <v>480</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>1346</v>
+        <v>1344</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>1347</v>
+        <v>1345</v>
       </c>
       <c r="D3" s="5"/>
       <c r="E3" s="43" t="s">
-        <v>1354</v>
+        <v>1352</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="183" t="s">
-        <v>1348</v>
+        <v>1346</v>
       </c>
       <c r="B4" s="184"/>
       <c r="C4" s="184"/>
@@ -10555,14 +10618,14 @@
         <v>239</v>
       </c>
       <c r="B5" s="5" t="s">
+        <v>1347</v>
+      </c>
+      <c r="C5" s="6" t="s">
         <v>1349</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>1351</v>
       </c>
       <c r="D5" s="5"/>
       <c r="E5" s="43" t="s">
-        <v>1355</v>
+        <v>1353</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="96" x14ac:dyDescent="0.2">
@@ -10570,19 +10633,19 @@
         <v>480</v>
       </c>
       <c r="B6" s="5" t="s">
+        <v>1348</v>
+      </c>
+      <c r="C6" s="6" t="s">
         <v>1350</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>1352</v>
       </c>
       <c r="D6" s="5"/>
       <c r="E6" s="43" t="s">
-        <v>1356</v>
+        <v>1354</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="183" t="s">
-        <v>1495</v>
+        <v>1493</v>
       </c>
       <c r="B7" s="184"/>
       <c r="C7" s="184"/>
@@ -10594,44 +10657,44 @@
         <v>239</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>1497</v>
+        <v>1495</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>1498</v>
+        <v>1496</v>
       </c>
       <c r="D8" s="5"/>
       <c r="E8" s="43" t="s">
-        <v>1505</v>
+        <v>1503</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
+        <v>1497</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>1498</v>
+      </c>
+      <c r="C9" s="6" t="s">
         <v>1499</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>1500</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>1501</v>
       </c>
       <c r="D9" s="5"/>
       <c r="E9" s="43" t="s">
-        <v>1506</v>
+        <v>1504</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
+        <v>1500</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>1501</v>
+      </c>
+      <c r="C10" s="6" t="s">
         <v>1502</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>1503</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>1504</v>
       </c>
       <c r="D10" s="5"/>
       <c r="E10" s="43" t="s">
-        <v>1507</v>
+        <v>1505</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="16" x14ac:dyDescent="0.2">
@@ -10639,14 +10702,14 @@
         <v>239</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>1496</v>
+        <v>1494</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>1508</v>
+        <v>1506</v>
       </c>
       <c r="D11" s="5"/>
       <c r="E11" s="43" t="s">
-        <v>1511</v>
+        <v>1509</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="16" x14ac:dyDescent="0.2">
@@ -10654,14 +10717,14 @@
         <v>480</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>1509</v>
+        <v>1507</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>1510</v>
+        <v>1508</v>
       </c>
       <c r="D12" s="5"/>
       <c r="E12" s="43" t="s">
-        <v>1512</v>
+        <v>1510</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
@@ -10841,7 +10904,7 @@
         <v>239</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>1359</v>
+        <v>1357</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>272</v>
@@ -10865,7 +10928,7 @@
         <v>242</v>
       </c>
       <c r="E4" s="43" t="s">
-        <v>1360</v>
+        <v>1358</v>
       </c>
       <c r="F4" s="68" t="s">
         <v>276</v>
@@ -10879,13 +10942,13 @@
         <v>277</v>
       </c>
       <c r="C5" s="52" t="s">
-        <v>1411</v>
+        <v>1409</v>
       </c>
       <c r="D5" s="66" t="s">
         <v>278</v>
       </c>
       <c r="E5" s="156" t="s">
-        <v>1429</v>
+        <v>1427</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>279</v>
@@ -10899,13 +10962,13 @@
         <v>280</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>1363</v>
+        <v>1361</v>
       </c>
       <c r="D6" s="67" t="s">
         <v>281</v>
       </c>
       <c r="E6" s="157" t="s">
-        <v>1430</v>
+        <v>1428</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="160" x14ac:dyDescent="0.2">
@@ -10916,13 +10979,13 @@
         <v>282</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>1364</v>
+        <v>1362</v>
       </c>
       <c r="D7" s="67" t="s">
         <v>283</v>
       </c>
       <c r="E7" s="157" t="s">
-        <v>1365</v>
+        <v>1363</v>
       </c>
       <c r="F7" s="68" t="s">
         <v>284</v>
@@ -11124,7 +11187,7 @@
         <v>332</v>
       </c>
       <c r="C19" s="64" t="s">
-        <v>1357</v>
+        <v>1355</v>
       </c>
       <c r="D19" s="7" t="s">
         <v>333</v>
@@ -11258,17 +11321,17 @@
     </row>
     <row r="27" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A27" s="5" t="s">
-        <v>1361</v>
+        <v>1359</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>1362</v>
+        <v>1360</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>1513</v>
+        <v>1511</v>
       </c>
       <c r="D27" s="5"/>
       <c r="E27" s="37" t="s">
-        <v>1514</v>
+        <v>1512</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
@@ -11308,7 +11371,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B63483B8-55BE-4CA0-9111-55E5C0AEF6CB}">
   <dimension ref="A1:F367"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A205" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B213" sqref="B213"/>
     </sheetView>
@@ -11345,13 +11408,13 @@
       </c>
     </row>
     <row r="2" spans="1:6" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="189" t="s">
+      <c r="A2" s="186" t="s">
         <v>363</v>
       </c>
-      <c r="B2" s="190"/>
-      <c r="C2" s="190"/>
-      <c r="D2" s="190"/>
-      <c r="E2" s="191"/>
+      <c r="B2" s="187"/>
+      <c r="C2" s="187"/>
+      <c r="D2" s="187"/>
+      <c r="E2" s="188"/>
       <c r="F2" s="33"/>
     </row>
     <row r="3" spans="1:6" ht="48" x14ac:dyDescent="0.2">
@@ -11449,14 +11512,14 @@
         <v>378</v>
       </c>
       <c r="B8" s="119" t="s">
-        <v>1492</v>
+        <v>1490</v>
       </c>
       <c r="C8" s="117" t="s">
-        <v>1493</v>
+        <v>1491</v>
       </c>
       <c r="D8" s="121"/>
       <c r="E8" s="120" t="s">
-        <v>1494</v>
+        <v>1492</v>
       </c>
       <c r="F8" s="119"/>
     </row>
@@ -11495,13 +11558,13 @@
       <c r="F10" s="119"/>
     </row>
     <row r="11" spans="1:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="192" t="s">
+      <c r="A11" s="189" t="s">
         <v>392</v>
       </c>
-      <c r="B11" s="193"/>
-      <c r="C11" s="193"/>
-      <c r="D11" s="193"/>
-      <c r="E11" s="194"/>
+      <c r="B11" s="190"/>
+      <c r="C11" s="190"/>
+      <c r="D11" s="190"/>
+      <c r="E11" s="191"/>
       <c r="F11" s="119"/>
     </row>
     <row r="12" spans="1:6" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -11530,13 +11593,13 @@
         <v>397</v>
       </c>
       <c r="C13" s="153" t="s">
-        <v>1323</v>
+        <v>1321</v>
       </c>
       <c r="D13" s="84" t="s">
         <v>398</v>
       </c>
       <c r="E13" s="152" t="s">
-        <v>1324</v>
+        <v>1322</v>
       </c>
       <c r="F13" s="86"/>
     </row>
@@ -11548,13 +11611,13 @@
         <v>399</v>
       </c>
       <c r="C14" s="154" t="s">
-        <v>1325</v>
+        <v>1323</v>
       </c>
       <c r="D14" s="88" t="s">
         <v>400</v>
       </c>
       <c r="E14" s="155" t="s">
-        <v>1326</v>
+        <v>1324</v>
       </c>
       <c r="F14" s="86"/>
     </row>
@@ -11710,7 +11773,7 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" s="183" t="s">
-        <v>1460</v>
+        <v>1458</v>
       </c>
       <c r="B25" s="184"/>
       <c r="C25" s="184"/>
@@ -11723,10 +11786,10 @@
         <v>239</v>
       </c>
       <c r="B26" s="132" t="s">
-        <v>1461</v>
+        <v>1459</v>
       </c>
       <c r="C26" s="133" t="s">
-        <v>1462</v>
+        <v>1460</v>
       </c>
       <c r="D26" s="114"/>
       <c r="E26" s="131"/>
@@ -11737,14 +11800,14 @@
         <v>373</v>
       </c>
       <c r="B27" s="132" t="s">
-        <v>1464</v>
+        <v>1462</v>
       </c>
       <c r="C27" s="133" t="s">
-        <v>1472</v>
+        <v>1470</v>
       </c>
       <c r="D27" s="114"/>
       <c r="E27" s="131" t="s">
-        <v>1473</v>
+        <v>1471</v>
       </c>
       <c r="F27" s="119"/>
     </row>
@@ -11753,30 +11816,30 @@
         <v>373</v>
       </c>
       <c r="B28" s="132" t="s">
-        <v>1466</v>
+        <v>1464</v>
       </c>
       <c r="C28" s="133" t="s">
-        <v>1465</v>
+        <v>1463</v>
       </c>
       <c r="D28" s="114"/>
       <c r="E28" s="131" t="s">
-        <v>1467</v>
+        <v>1465</v>
       </c>
       <c r="F28" s="119"/>
     </row>
     <row r="29" spans="1:6" s="178" customFormat="1" ht="96" x14ac:dyDescent="0.2">
       <c r="A29" s="172" t="s">
-        <v>1471</v>
+        <v>1469</v>
       </c>
       <c r="B29" s="173" t="s">
-        <v>1468</v>
+        <v>1466</v>
       </c>
       <c r="C29" s="174" t="s">
-        <v>1469</v>
+        <v>1467</v>
       </c>
       <c r="D29" s="175"/>
       <c r="E29" s="176" t="s">
-        <v>1470</v>
+        <v>1468</v>
       </c>
       <c r="F29" s="177"/>
     </row>
@@ -12091,14 +12154,14 @@
         <v>480</v>
       </c>
       <c r="B51" s="116" t="s">
-        <v>1343</v>
+        <v>1341</v>
       </c>
       <c r="C51" s="59" t="s">
-        <v>1437</v>
+        <v>1435</v>
       </c>
       <c r="D51" s="116"/>
       <c r="E51" s="120" t="s">
-        <v>1438</v>
+        <v>1436</v>
       </c>
       <c r="F51" s="119"/>
     </row>
@@ -12107,10 +12170,10 @@
         <v>480</v>
       </c>
       <c r="B52" s="116" t="s">
-        <v>1436</v>
+        <v>1434</v>
       </c>
       <c r="C52" s="59" t="s">
-        <v>1342</v>
+        <v>1340</v>
       </c>
       <c r="D52" s="116"/>
       <c r="E52" s="120" t="s">
@@ -12126,11 +12189,11 @@
         <v>481</v>
       </c>
       <c r="C53" s="59" t="s">
-        <v>1435</v>
+        <v>1433</v>
       </c>
       <c r="D53" s="116"/>
       <c r="E53" s="120" t="s">
-        <v>1441</v>
+        <v>1439</v>
       </c>
       <c r="F53" s="119"/>
     </row>
@@ -12334,13 +12397,13 @@
         <v>511</v>
       </c>
       <c r="C67" s="117" t="s">
-        <v>1439</v>
+        <v>1437</v>
       </c>
       <c r="D67" s="116" t="s">
         <v>512</v>
       </c>
       <c r="E67" s="120" t="s">
-        <v>1440</v>
+        <v>1438</v>
       </c>
       <c r="F67" s="119"/>
     </row>
@@ -12358,7 +12421,7 @@
         <v>516</v>
       </c>
       <c r="E68" s="120" t="s">
-        <v>1335</v>
+        <v>1333</v>
       </c>
       <c r="F68" s="119"/>
     </row>
@@ -12367,14 +12430,14 @@
         <v>513</v>
       </c>
       <c r="B69" s="116" t="s">
+        <v>1330</v>
+      </c>
+      <c r="C69" s="117" t="s">
         <v>1332</v>
-      </c>
-      <c r="C69" s="117" t="s">
-        <v>1334</v>
       </c>
       <c r="D69" s="116"/>
       <c r="E69" s="120" t="s">
-        <v>1333</v>
+        <v>1331</v>
       </c>
       <c r="F69" s="119"/>
     </row>
@@ -12467,14 +12530,14 @@
         <v>480</v>
       </c>
       <c r="B76" s="125" t="s">
-        <v>1442</v>
+        <v>1440</v>
       </c>
       <c r="C76" s="167" t="s">
-        <v>1443</v>
+        <v>1441</v>
       </c>
       <c r="D76" s="125"/>
       <c r="E76" s="131" t="s">
-        <v>1444</v>
+        <v>1442</v>
       </c>
       <c r="F76" s="119"/>
     </row>
@@ -12594,13 +12657,13 @@
         <v>546</v>
       </c>
       <c r="C83" s="158" t="s">
-        <v>1455</v>
+        <v>1453</v>
       </c>
       <c r="D83" s="95" t="s">
         <v>400</v>
       </c>
       <c r="E83" s="155" t="s">
-        <v>1456</v>
+        <v>1454</v>
       </c>
       <c r="F83" s="119"/>
     </row>
@@ -12726,11 +12789,11 @@
         <v>564</v>
       </c>
       <c r="C92" s="117" t="s">
-        <v>1380</v>
+        <v>1378</v>
       </c>
       <c r="D92" s="116"/>
       <c r="E92" s="120" t="s">
-        <v>1381</v>
+        <v>1379</v>
       </c>
       <c r="F92" s="119"/>
     </row>
@@ -12838,11 +12901,11 @@
         <v>583</v>
       </c>
       <c r="C99" s="117" t="s">
-        <v>1378</v>
+        <v>1376</v>
       </c>
       <c r="D99" s="116"/>
       <c r="E99" s="120" t="s">
-        <v>1379</v>
+        <v>1377</v>
       </c>
       <c r="F99" s="119"/>
     </row>
@@ -12884,11 +12947,11 @@
         <v>589</v>
       </c>
       <c r="C102" s="117" t="s">
-        <v>1396</v>
+        <v>1394</v>
       </c>
       <c r="D102" s="116"/>
       <c r="E102" s="120" t="s">
-        <v>1397</v>
+        <v>1395</v>
       </c>
       <c r="F102" s="86" t="s">
         <v>592</v>
@@ -12917,7 +12980,7 @@
         <v>84</v>
       </c>
       <c r="B104" s="159" t="s">
-        <v>1402</v>
+        <v>1400</v>
       </c>
       <c r="C104" s="93" t="s">
         <v>591</v>
@@ -12935,7 +12998,7 @@
         <v>84</v>
       </c>
       <c r="B105" s="159" t="s">
-        <v>1403</v>
+        <v>1401</v>
       </c>
       <c r="C105" s="93" t="s">
         <v>591</v>
@@ -12953,7 +13016,7 @@
         <v>84</v>
       </c>
       <c r="B106" s="160" t="s">
-        <v>1404</v>
+        <v>1402</v>
       </c>
       <c r="C106" s="161" t="s">
         <v>591</v>
@@ -12969,7 +13032,7 @@
         <v>84</v>
       </c>
       <c r="B107" s="160" t="s">
-        <v>1405</v>
+        <v>1403</v>
       </c>
       <c r="C107" s="161" t="s">
         <v>591</v>
@@ -12985,7 +13048,7 @@
         <v>84</v>
       </c>
       <c r="B108" s="160" t="s">
-        <v>1406</v>
+        <v>1404</v>
       </c>
       <c r="C108" s="161" t="s">
         <v>591</v>
@@ -13434,33 +13497,33 @@
     </row>
     <row r="138" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A138" s="116" t="s">
+        <v>1443</v>
+      </c>
+      <c r="B138" s="116" t="s">
         <v>1445</v>
       </c>
-      <c r="B138" s="116" t="s">
-        <v>1447</v>
-      </c>
       <c r="C138" s="117" t="s">
-        <v>1446</v>
+        <v>1444</v>
       </c>
       <c r="D138" s="116"/>
       <c r="E138" s="120" t="s">
-        <v>1450</v>
+        <v>1448</v>
       </c>
       <c r="F138" s="119"/>
     </row>
     <row r="139" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A139" s="116" t="s">
-        <v>1445</v>
+        <v>1443</v>
       </c>
       <c r="B139" s="116" t="s">
-        <v>1449</v>
+        <v>1447</v>
       </c>
       <c r="C139" s="117" t="s">
-        <v>1448</v>
+        <v>1446</v>
       </c>
       <c r="D139" s="116"/>
       <c r="E139" s="120" t="s">
-        <v>1451</v>
+        <v>1449</v>
       </c>
       <c r="F139" s="119"/>
     </row>
@@ -13696,7 +13759,7 @@
         <v>699</v>
       </c>
       <c r="C156" s="113" t="s">
-        <v>1310</v>
+        <v>1308</v>
       </c>
       <c r="D156" s="122" t="s">
         <v>700</v>
@@ -13784,7 +13847,7 @@
         <v>714</v>
       </c>
       <c r="C162" s="59" t="s">
-        <v>1309</v>
+        <v>1307</v>
       </c>
       <c r="D162" s="116" t="s">
         <v>715</v>
@@ -13815,14 +13878,14 @@
         <v>37</v>
       </c>
       <c r="B164" s="116" t="s">
+        <v>1309</v>
+      </c>
+      <c r="C164" s="59" t="s">
         <v>1311</v>
-      </c>
-      <c r="C164" s="59" t="s">
-        <v>1313</v>
       </c>
       <c r="D164" s="116"/>
       <c r="E164" s="120" t="s">
-        <v>1315</v>
+        <v>1313</v>
       </c>
       <c r="F164" s="119"/>
     </row>
@@ -13831,14 +13894,14 @@
         <v>37</v>
       </c>
       <c r="B165" s="116" t="s">
+        <v>1310</v>
+      </c>
+      <c r="C165" s="59" t="s">
         <v>1312</v>
-      </c>
-      <c r="C165" s="59" t="s">
-        <v>1314</v>
       </c>
       <c r="D165" s="116"/>
       <c r="E165" s="120" t="s">
-        <v>1316</v>
+        <v>1314</v>
       </c>
       <c r="F165" s="119"/>
     </row>
@@ -14059,13 +14122,13 @@
       </c>
     </row>
     <row r="180" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A180" s="186" t="s">
+      <c r="A180" s="192" t="s">
         <v>754</v>
       </c>
-      <c r="B180" s="187"/>
-      <c r="C180" s="187"/>
-      <c r="D180" s="187"/>
-      <c r="E180" s="188"/>
+      <c r="B180" s="193"/>
+      <c r="C180" s="193"/>
+      <c r="D180" s="193"/>
+      <c r="E180" s="194"/>
       <c r="F180" s="129" t="s">
         <v>758</v>
       </c>
@@ -14082,7 +14145,7 @@
       </c>
       <c r="D181" s="114"/>
       <c r="E181" s="131" t="s">
-        <v>1481</v>
+        <v>1479</v>
       </c>
       <c r="F181" s="129" t="s">
         <v>758</v>
@@ -14093,14 +14156,14 @@
         <v>239</v>
       </c>
       <c r="B182" s="116" t="s">
-        <v>1515</v>
+        <v>1513</v>
       </c>
       <c r="C182" s="130" t="s">
-        <v>1516</v>
+        <v>1514</v>
       </c>
       <c r="D182" s="114"/>
       <c r="E182" s="131" t="s">
-        <v>1517</v>
+        <v>1515</v>
       </c>
       <c r="F182" s="129" t="s">
         <v>758</v>
@@ -14118,7 +14181,7 @@
       </c>
       <c r="D183" s="114"/>
       <c r="E183" s="131" t="s">
-        <v>1482</v>
+        <v>1480</v>
       </c>
       <c r="F183" s="129" t="s">
         <v>758</v>
@@ -14150,7 +14213,7 @@
       </c>
       <c r="D185" s="114"/>
       <c r="E185" s="131" t="s">
-        <v>1483</v>
+        <v>1481</v>
       </c>
       <c r="F185" s="129" t="s">
         <v>758</v>
@@ -14168,7 +14231,7 @@
       </c>
       <c r="D186" s="114"/>
       <c r="E186" s="131" t="s">
-        <v>1484</v>
+        <v>1482</v>
       </c>
       <c r="F186" s="129" t="s">
         <v>758</v>
@@ -14216,7 +14279,7 @@
     </row>
     <row r="190" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A190" s="183" t="s">
-        <v>1474</v>
+        <v>1472</v>
       </c>
       <c r="B190" s="184"/>
       <c r="C190" s="184"/>
@@ -14229,29 +14292,29 @@
         <v>239</v>
       </c>
       <c r="B191" s="132" t="s">
-        <v>1475</v>
+        <v>1473</v>
       </c>
       <c r="C191" s="133" t="s">
-        <v>1474</v>
+        <v>1472</v>
       </c>
       <c r="D191" s="114"/>
       <c r="E191" s="131" t="s">
-        <v>1478</v>
+        <v>1476</v>
       </c>
       <c r="F191" s="119"/>
     </row>
     <row r="192" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A192" s="1" t="s">
-        <v>1480</v>
+        <v>1478</v>
       </c>
       <c r="B192" s="1" t="s">
-        <v>1476</v>
+        <v>1474</v>
       </c>
       <c r="C192" s="2" t="s">
+        <v>1475</v>
+      </c>
+      <c r="E192" s="40" t="s">
         <v>1477</v>
-      </c>
-      <c r="E192" s="40" t="s">
-        <v>1479</v>
       </c>
     </row>
     <row r="193" spans="1:6" ht="48" x14ac:dyDescent="0.2">
@@ -14259,13 +14322,13 @@
         <v>257</v>
       </c>
       <c r="B193" s="1" t="s">
+        <v>1483</v>
+      </c>
+      <c r="C193" s="2" t="s">
+        <v>1484</v>
+      </c>
+      <c r="E193" s="40" t="s">
         <v>1485</v>
-      </c>
-      <c r="C193" s="2" t="s">
-        <v>1486</v>
-      </c>
-      <c r="E193" s="40" t="s">
-        <v>1487</v>
       </c>
     </row>
     <row r="194" spans="1:6" x14ac:dyDescent="0.2">
@@ -14322,13 +14385,13 @@
         <v>771</v>
       </c>
       <c r="C197" s="158" t="s">
-        <v>1518</v>
+        <v>1516</v>
       </c>
       <c r="D197" s="95" t="s">
         <v>400</v>
       </c>
       <c r="E197" s="155" t="s">
-        <v>1521</v>
+        <v>1519</v>
       </c>
       <c r="F197" s="119"/>
     </row>
@@ -14340,13 +14403,13 @@
         <v>772</v>
       </c>
       <c r="C198" s="158" t="s">
-        <v>1519</v>
+        <v>1517</v>
       </c>
       <c r="D198" s="95" t="s">
         <v>400</v>
       </c>
       <c r="E198" s="155" t="s">
-        <v>1522</v>
+        <v>1520</v>
       </c>
       <c r="F198" s="119"/>
     </row>
@@ -14358,13 +14421,13 @@
         <v>773</v>
       </c>
       <c r="C199" s="158" t="s">
-        <v>1520</v>
+        <v>1518</v>
       </c>
       <c r="D199" s="95" t="s">
         <v>400</v>
       </c>
       <c r="E199" s="155" t="s">
-        <v>1523</v>
+        <v>1521</v>
       </c>
       <c r="F199" s="119"/>
     </row>
@@ -14406,17 +14469,17 @@
     </row>
     <row r="202" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A202" s="180" t="s">
-        <v>1445</v>
+        <v>1443</v>
       </c>
       <c r="B202" s="179" t="s">
-        <v>1524</v>
+        <v>1522</v>
       </c>
       <c r="C202" s="181" t="s">
-        <v>1525</v>
+        <v>1523</v>
       </c>
       <c r="D202" s="95"/>
       <c r="E202" s="155" t="s">
-        <v>1526</v>
+        <v>1524</v>
       </c>
       <c r="F202" s="119"/>
     </row>
@@ -14565,14 +14628,14 @@
         <v>480</v>
       </c>
       <c r="B213" s="116" t="s">
-        <v>1528</v>
+        <v>1526</v>
       </c>
       <c r="C213" s="117" t="s">
-        <v>1529</v>
+        <v>1527</v>
       </c>
       <c r="D213" s="116"/>
       <c r="E213" s="120" t="s">
-        <v>1530</v>
+        <v>1528</v>
       </c>
       <c r="F213" s="119"/>
     </row>
@@ -14602,13 +14665,13 @@
         <v>803</v>
       </c>
       <c r="C215" s="59" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="D215" s="116" t="s">
         <v>804</v>
       </c>
       <c r="E215" s="120" t="s">
-        <v>1331</v>
+        <v>1329</v>
       </c>
       <c r="F215" s="119"/>
     </row>
@@ -14617,14 +14680,14 @@
         <v>480</v>
       </c>
       <c r="B216" s="116" t="s">
-        <v>1328</v>
+        <v>1326</v>
       </c>
       <c r="C216" s="59" t="s">
-        <v>1329</v>
+        <v>1327</v>
       </c>
       <c r="D216" s="116"/>
       <c r="E216" s="120" t="s">
-        <v>1330</v>
+        <v>1328</v>
       </c>
       <c r="F216" s="119"/>
     </row>
@@ -14724,11 +14787,11 @@
         <v>815</v>
       </c>
       <c r="C223" s="117" t="s">
-        <v>1338</v>
+        <v>1336</v>
       </c>
       <c r="D223" s="116"/>
       <c r="E223" s="120" t="s">
-        <v>1341</v>
+        <v>1339</v>
       </c>
       <c r="F223" s="119"/>
     </row>
@@ -14737,7 +14800,7 @@
         <v>723</v>
       </c>
       <c r="B224" s="116" t="s">
-        <v>1340</v>
+        <v>1338</v>
       </c>
       <c r="C224" s="117" t="s">
         <v>43</v>
@@ -14753,14 +14816,14 @@
         <v>32</v>
       </c>
       <c r="B225" s="116" t="s">
-        <v>1339</v>
+        <v>1337</v>
       </c>
       <c r="C225" s="134" t="s">
-        <v>1336</v>
+        <v>1334</v>
       </c>
       <c r="D225" s="116"/>
       <c r="E225" s="120" t="s">
-        <v>1337</v>
+        <v>1335</v>
       </c>
       <c r="F225" s="119"/>
     </row>
@@ -14964,11 +15027,11 @@
         <v>836</v>
       </c>
       <c r="C239" s="117" t="s">
-        <v>1518</v>
+        <v>1516</v>
       </c>
       <c r="D239" s="116"/>
       <c r="E239" s="120" t="s">
-        <v>1521</v>
+        <v>1519</v>
       </c>
       <c r="F239" s="119"/>
     </row>
@@ -14980,11 +15043,11 @@
         <v>837</v>
       </c>
       <c r="C240" s="117" t="s">
-        <v>1519</v>
+        <v>1517</v>
       </c>
       <c r="D240" s="116"/>
       <c r="E240" s="120" t="s">
-        <v>1522</v>
+        <v>1520</v>
       </c>
       <c r="F240" s="119"/>
     </row>
@@ -14996,11 +15059,11 @@
         <v>838</v>
       </c>
       <c r="C241" s="117" t="s">
-        <v>1520</v>
+        <v>1518</v>
       </c>
       <c r="D241" s="116"/>
       <c r="E241" s="120" t="s">
-        <v>1523</v>
+        <v>1521</v>
       </c>
       <c r="F241" s="119"/>
     </row>
@@ -15132,13 +15195,13 @@
         <v>854</v>
       </c>
       <c r="C250" s="59" t="s">
-        <v>1366</v>
+        <v>1364</v>
       </c>
       <c r="D250" s="116" t="s">
         <v>855</v>
       </c>
       <c r="E250" s="120" t="s">
-        <v>1367</v>
+        <v>1365</v>
       </c>
       <c r="F250" s="119"/>
     </row>
@@ -16077,19 +16140,6 @@
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="A247:E247"/>
-    <mergeCell ref="A207:E207"/>
-    <mergeCell ref="A211:E211"/>
-    <mergeCell ref="A219:E219"/>
-    <mergeCell ref="A230:E230"/>
-    <mergeCell ref="A236:E236"/>
-    <mergeCell ref="A65:E65"/>
-    <mergeCell ref="A2:E2"/>
-    <mergeCell ref="A11:E11"/>
-    <mergeCell ref="A15:E15"/>
-    <mergeCell ref="A30:E30"/>
-    <mergeCell ref="A49:E49"/>
-    <mergeCell ref="A25:E25"/>
     <mergeCell ref="A194:E194"/>
     <mergeCell ref="A172:E172"/>
     <mergeCell ref="A70:E70"/>
@@ -16101,6 +16151,19 @@
     <mergeCell ref="A100:E100"/>
     <mergeCell ref="A180:E180"/>
     <mergeCell ref="A190:E190"/>
+    <mergeCell ref="A65:E65"/>
+    <mergeCell ref="A2:E2"/>
+    <mergeCell ref="A11:E11"/>
+    <mergeCell ref="A15:E15"/>
+    <mergeCell ref="A30:E30"/>
+    <mergeCell ref="A49:E49"/>
+    <mergeCell ref="A25:E25"/>
+    <mergeCell ref="A247:E247"/>
+    <mergeCell ref="A207:E207"/>
+    <mergeCell ref="A211:E211"/>
+    <mergeCell ref="A219:E219"/>
+    <mergeCell ref="A230:E230"/>
+    <mergeCell ref="A236:E236"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -16228,14 +16291,14 @@
     </row>
     <row r="8" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="B8" s="168" t="s">
-        <v>1457</v>
+        <v>1455</v>
       </c>
       <c r="C8" s="169" t="s">
-        <v>1458</v>
+        <v>1456</v>
       </c>
       <c r="D8" s="168"/>
       <c r="E8" s="170" t="s">
-        <v>1459</v>
+        <v>1457</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="16" x14ac:dyDescent="0.2">
@@ -16383,13 +16446,13 @@
         <v>930</v>
       </c>
       <c r="C18" s="151" t="s">
-        <v>1317</v>
+        <v>1315</v>
       </c>
       <c r="D18" s="92" t="s">
         <v>922</v>
       </c>
       <c r="E18" s="152" t="s">
-        <v>1318</v>
+        <v>1316</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="80" x14ac:dyDescent="0.2">
@@ -16463,11 +16526,11 @@
         <v>945</v>
       </c>
       <c r="C24" s="82" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="D24" s="80"/>
       <c r="E24" s="81" t="s">
-        <v>1453</v>
+        <v>1451</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
@@ -16589,10 +16652,10 @@
         <v>968</v>
       </c>
       <c r="C33" s="21" t="s">
-        <v>1373</v>
+        <v>1371</v>
       </c>
       <c r="E33" s="46" t="s">
-        <v>1374</v>
+        <v>1372</v>
       </c>
     </row>
     <row r="34" spans="1:6" ht="32" x14ac:dyDescent="0.2">
@@ -16600,13 +16663,13 @@
         <v>257</v>
       </c>
       <c r="B34" s="19" t="s">
+        <v>1373</v>
+      </c>
+      <c r="C34" s="21" t="s">
+        <v>1374</v>
+      </c>
+      <c r="E34" s="46" t="s">
         <v>1375</v>
-      </c>
-      <c r="C34" s="21" t="s">
-        <v>1376</v>
-      </c>
-      <c r="E34" s="46" t="s">
-        <v>1377</v>
       </c>
     </row>
     <row r="35" spans="1:6" ht="48" x14ac:dyDescent="0.2">
@@ -16766,13 +16829,13 @@
         <v>993</v>
       </c>
       <c r="C46" s="62" t="s">
-        <v>1366</v>
+        <v>1364</v>
       </c>
       <c r="D46" s="116" t="s">
         <v>994</v>
       </c>
       <c r="E46" s="46" t="s">
-        <v>1367</v>
+        <v>1365</v>
       </c>
     </row>
     <row r="47" spans="1:6" ht="48" x14ac:dyDescent="0.2">
@@ -17165,23 +17228,23 @@
         <v>1060</v>
       </c>
       <c r="E11" s="138" t="s">
-        <v>1390</v>
+        <v>1388</v>
       </c>
       <c r="F11" s="135"/>
     </row>
     <row r="12" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A12" s="136" t="s">
+        <v>1384</v>
+      </c>
+      <c r="B12" s="136" t="s">
+        <v>1385</v>
+      </c>
+      <c r="C12" s="137" t="s">
         <v>1386</v>
-      </c>
-      <c r="B12" s="136" t="s">
-        <v>1387</v>
-      </c>
-      <c r="C12" s="137" t="s">
-        <v>1388</v>
       </c>
       <c r="D12" s="136"/>
       <c r="E12" s="138" t="s">
-        <v>1389</v>
+        <v>1387</v>
       </c>
       <c r="F12" s="135"/>
     </row>
@@ -17193,7 +17256,7 @@
         <v>1061</v>
       </c>
       <c r="C13" s="137" t="s">
-        <v>1454</v>
+        <v>1452</v>
       </c>
       <c r="D13" s="136" t="s">
         <v>1062</v>
@@ -17239,7 +17302,7 @@
         <v>1067</v>
       </c>
       <c r="C16" s="137" t="s">
-        <v>1382</v>
+        <v>1380</v>
       </c>
       <c r="D16" s="136" t="s">
         <v>1068</v>
@@ -17257,7 +17320,7 @@
         <v>1070</v>
       </c>
       <c r="C17" s="137" t="s">
-        <v>1383</v>
+        <v>1381</v>
       </c>
       <c r="D17" s="136" t="s">
         <v>1071</v>
@@ -17275,7 +17338,7 @@
         <v>1073</v>
       </c>
       <c r="C18" s="137" t="s">
-        <v>1384</v>
+        <v>1382</v>
       </c>
       <c r="D18" s="136" t="s">
         <v>1074</v>
@@ -17415,17 +17478,17 @@
     </row>
     <row r="28" spans="1:6" ht="64" x14ac:dyDescent="0.2">
       <c r="A28" s="136" t="s">
-        <v>1386</v>
+        <v>1384</v>
       </c>
       <c r="B28" s="136" t="s">
-        <v>1385</v>
+        <v>1383</v>
       </c>
       <c r="C28" s="137" t="s">
-        <v>1407</v>
+        <v>1405</v>
       </c>
       <c r="D28" s="136"/>
       <c r="E28" s="138" t="s">
-        <v>1409</v>
+        <v>1407</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="32" x14ac:dyDescent="0.2">
@@ -17436,13 +17499,13 @@
         <v>1099</v>
       </c>
       <c r="C29" s="137" t="s">
-        <v>1408</v>
+        <v>1406</v>
       </c>
       <c r="D29" s="136" t="s">
         <v>1100</v>
       </c>
       <c r="E29" s="138" t="s">
-        <v>1410</v>
+        <v>1408</v>
       </c>
     </row>
     <row r="30" spans="1:6" s="13" customFormat="1" x14ac:dyDescent="0.2">
@@ -17685,7 +17748,7 @@
         <v>1137</v>
       </c>
       <c r="C45" s="62" t="s">
-        <v>1358</v>
+        <v>1356</v>
       </c>
       <c r="D45" s="5" t="s">
         <v>1138</v>
@@ -17777,13 +17840,13 @@
         <v>1149</v>
       </c>
       <c r="C51" s="62" t="s">
-        <v>1366</v>
+        <v>1364</v>
       </c>
       <c r="D51" s="116" t="s">
         <v>994</v>
       </c>
       <c r="E51" s="63" t="s">
-        <v>1367</v>
+        <v>1365</v>
       </c>
     </row>
     <row r="52" spans="1:6" s="30" customFormat="1" ht="48" x14ac:dyDescent="0.2">
@@ -18414,15 +18477,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <Readyforteam_x003f_ xmlns="565e1b1d-057e-4d85-b896-01a5881d8a45">false</Readyforteam_x003f_>
@@ -18463,6 +18517,15 @@
 </p:properties>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EAFDB110-4046-4E72-A1EF-1908ABEC3151}">
   <ds:schemaRefs>
@@ -18485,14 +18548,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8D7CE8C7-18DC-484F-8376-ED09F13D44C8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{017ACE96-8143-486E-8436-7787F6B96F4A}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -18503,4 +18558,12 @@
     <ds:schemaRef ds:uri="2799d30d-6731-4efe-ac9b-c4895a8828d9"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8D7CE8C7-18DC-484F-8376-ED09F13D44C8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Adding welsh translations for the Confirmation page(s).
</commit_message>
<xml_diff>
--- a/app/data/MCCD-localisation.xlsx
+++ b/app/data/MCCD-localisation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/JALAT/GIT/medical-certificate-of-cause-of-death/app/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{008EAA24-5044-F64B-868A-97D3DE1C8F15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8498484-7167-6243-89C4-BECCFD5CB06C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="13940" firstSheet="4" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="13940" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Using this document" sheetId="8" r:id="rId1"/>
@@ -69,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2279" uniqueCount="1537">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2315" uniqueCount="1566">
   <si>
     <r>
       <rPr>
@@ -5144,9 +5144,6 @@
     <t>meoValidationMessageNoTick</t>
   </si>
   <si>
-    <t>Certificate created</t>
-  </si>
-  <si>
     <t>confirmationPageTitle</t>
   </si>
   <si>
@@ -5264,9 +5261,6 @@
   </si>
   <si>
     <t>Dychwelyd i'r dangosfwrdd</t>
-  </si>
-  <si>
-    <t>Certificate submitted for scrutiny</t>
   </si>
   <si>
     <t>Medical certificate of cause of death submitted for scrutiny</t>
@@ -5955,9 +5949,6 @@
     <t>Rhowch gyfeiriad &lt;strong&gt;yn Gymraeg&lt;/strong&gt;</t>
   </si>
   <si>
-    <t>057</t>
-  </si>
-  <si>
     <t>dpdApproximateLocationHintBilingual</t>
   </si>
   <si>
@@ -5990,6 +5981,102 @@
   </si>
   <si>
     <t>Dywedwch wrthym beth yw eich barn am y Complete an MCCD service</t>
+  </si>
+  <si>
+    <t>AP Certificate submitted for scrutiny</t>
+  </si>
+  <si>
+    <t>AP Certificate needs amendments</t>
+  </si>
+  <si>
+    <t>Certificate returned to the attending practitioner</t>
+  </si>
+  <si>
+    <t>Tystysgrif yn cael ei dychwelyd i'r ymarferydd sy'n mynychu</t>
+  </si>
+  <si>
+    <t>meCertificateNeedsAmendsPageTitle</t>
+  </si>
+  <si>
+    <t>meCertificateNeedsAmendsPageContent</t>
+  </si>
+  <si>
+    <t>&lt;p class="govuk-body-l"&gt;Rhaid i chi gysylltu â'r ymarferydd sy'n mynychu i'w hysbysu bod yn rhaid diwygio'r dystysgrif feddygol hon o achos marwolaeth (MCCD).&lt;/p&gt;&lt;h2 class="govuk-heading-m"&gt;Beth sy'n digwydd nesaf&lt;/h2&gt;&lt;p class = "govuk-body"&gt;Ar ôl i'r ymarferydd sy'n mynychu ddiwygio'r MCCD hwn bydd ar gael i'w weld ar ddangosfwrdd yr arholwr meddygol sydd wedi'i farcio 'I gael ei lofnodi gan arholwr meddygol'.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p class="govuk-body-l"&gt;You must contact the attending practitioner to inform them that this Medical certificate of cause of death (MCCD) must be amended.&lt;/p&gt;&lt;h2 class="govuk-heading-m"&gt;What happens next&lt;/h2&gt;&lt;p class="govuk-body"&gt;After the attending practitioner has amended this MCCD it will be available to view on the medical examiner dashboard marked ‘For sign off by medical examiner’.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>AP Certificate passed scrutiny</t>
+  </si>
+  <si>
+    <t>meCertificatePassedScrutinyPageTitle</t>
+  </si>
+  <si>
+    <t>&lt;p class="govuk-body-l"&gt;You have signed off this Medical certificate of cause of death (MCCD) following scrutiny of the cause of death.&lt;/p&gt;&lt;h2 class="govuk-heading-m"&gt;What happens next&lt;/h2&gt;&lt;p class="govuk-body"&gt;This MCCD will be sent to the local register office by your medical examiner office. There is nothing further for you to do.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p class="govuk-body-l"&gt;Rydych wedi llofnodi'r dystysgrif feddygol hon o achos marwolaeth (MCCD) yn dilyn craffu ar achos y farwolaeth.&lt;/p&gt;&lt;h2 class="govuk-heading-m"&gt;Beth sy'n digwydd nesaf&lt;/h2&gt;&lt;p class = "govuk-body"&gt;Bydd y MCCD hwn yn cael ei anfon i'r swyddfa gofrestru leol gan eich swyddfa arholwr meddygol. Nid oes unrhyw beth arall i'w wneud i chi.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>meCertificatePassedScrutinyPageContent</t>
+  </si>
+  <si>
+    <t>Medical certificate of cause of death approved</t>
+  </si>
+  <si>
+    <t>Tystysgrif feddygol achos marwolaeth wedi'i chymeradwyo</t>
+  </si>
+  <si>
+    <t>ME Certificate created</t>
+  </si>
+  <si>
+    <t>AP Certificate reviewed by MEO</t>
+  </si>
+  <si>
+    <t>meoCertificatePassedReviewPageTitle</t>
+  </si>
+  <si>
+    <t>meoCertificatePassedReviewPageContent</t>
+  </si>
+  <si>
+    <t>HTML</t>
+  </si>
+  <si>
+    <t>Certificate sent to medical examiners for sign-off</t>
+  </si>
+  <si>
+    <t>&lt;p class="govuk-body-l"&gt;Medical examiners in your organisation will now be able to access this certificate from their dashboard. They can review and sign off this certificate as part of the scrutiny process.&lt;/p&gt;&lt;h2 class="govuk-heading-m"&gt;What happens next&lt;/h2&gt;&lt;p class="govuk-body"&gt;When a medical examiner has signed off this certificate you must sign back into the MCCD digital service, download the signed-off certificate, and send it to the local register office.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>AP/ME Certificate sent to local register office</t>
+  </si>
+  <si>
+    <t>meoCertificateSentPageTitle</t>
+  </si>
+  <si>
+    <t>meoCertificateSentPageContent</t>
+  </si>
+  <si>
+    <t>Certificate downloaded and sent to the local register office</t>
+  </si>
+  <si>
+    <t>&lt;h2 class="govuk-heading-m"&gt;What happens next&lt;/h2&gt;&lt;p class="govuk-body"&gt;No further action is required.&lt;/p&gt;&lt;p class="govuk-body"&gt;This MCCD will be available to view from your dashboard for three months.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;h2 class="govuk-heading-m"&gt;Beth sy'n digwydd nesaf&lt;/h2&gt;&lt;p class = "govuk-body"&gt;Nid oes angen gweithredu pellach.&lt;/p&gt;&lt;p class="govuk-body"&gt;Bydd y MCCD hwn ar gael i'w weld o'ch dangosfwrdd am dri mis.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>Lawrlwythwyd y dystysgrif a'i hanfon i'r swyddfa gofrestru leol</t>
+  </si>
+  <si>
+    <t>Tystysgrif wedi'i hanfon at arholwyr meddygol ar gyfer llofnodi</t>
+  </si>
+  <si>
+    <t>&lt;p class="govuk-body-l"&gt;Bydd arholwyr meddygol yn eich sefydliad nawr yn gallu cael mynediad at y dystysgrif hon o'u dangosfwrdd. Gallant adolygu a llofnodi'r dystysgrif hon fel rhan o'r broses graffu.&lt;/p&gt;&lt;h2 class="govuk-heading-m"&gt;Beth sy'n digwydd nesaf&lt;/h2&gt;&lt;p class = "govuk-body"&gt;Pan fydd arholwr meddygol wedi llofnodi'r dystysgrif hon mae'n rhaid i chi lofnodi yn ôl i wasanaeth digidol MCC, lawrlwytho'r dystysgrif wedi'i llofnodi, a'i hanfon i'r swyddfa gofrestru leol.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>058</t>
   </si>
 </sst>
 </file>
@@ -6465,7 +6552,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="224">
+  <cellXfs count="222">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -7002,6 +7089,15 @@
     <xf numFmtId="0" fontId="9" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -7014,6 +7110,15 @@
     <xf numFmtId="0" fontId="13" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -7032,15 +7137,6 @@
     <xf numFmtId="0" fontId="13" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
@@ -7112,21 +7208,6 @@
     </xf>
     <xf numFmtId="0" fontId="13" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -7511,538 +7592,538 @@
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A1" s="182" t="s">
+      <c r="A1" s="185" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="182"/>
-      <c r="C1" s="182"/>
-      <c r="D1" s="182"/>
-      <c r="E1" s="182"/>
-      <c r="F1" s="182"/>
-      <c r="G1" s="182"/>
-      <c r="H1" s="182"/>
-      <c r="I1" s="182"/>
-      <c r="J1" s="182"/>
-      <c r="K1" s="182"/>
-      <c r="L1" s="182"/>
+      <c r="B1" s="185"/>
+      <c r="C1" s="185"/>
+      <c r="D1" s="185"/>
+      <c r="E1" s="185"/>
+      <c r="F1" s="185"/>
+      <c r="G1" s="185"/>
+      <c r="H1" s="185"/>
+      <c r="I1" s="185"/>
+      <c r="J1" s="185"/>
+      <c r="K1" s="185"/>
+      <c r="L1" s="185"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A2" s="182"/>
-      <c r="B2" s="182"/>
-      <c r="C2" s="182"/>
-      <c r="D2" s="182"/>
-      <c r="E2" s="182"/>
-      <c r="F2" s="182"/>
-      <c r="G2" s="182"/>
-      <c r="H2" s="182"/>
-      <c r="I2" s="182"/>
-      <c r="J2" s="182"/>
-      <c r="K2" s="182"/>
-      <c r="L2" s="182"/>
+      <c r="A2" s="185"/>
+      <c r="B2" s="185"/>
+      <c r="C2" s="185"/>
+      <c r="D2" s="185"/>
+      <c r="E2" s="185"/>
+      <c r="F2" s="185"/>
+      <c r="G2" s="185"/>
+      <c r="H2" s="185"/>
+      <c r="I2" s="185"/>
+      <c r="J2" s="185"/>
+      <c r="K2" s="185"/>
+      <c r="L2" s="185"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A3" s="182"/>
-      <c r="B3" s="182"/>
-      <c r="C3" s="182"/>
-      <c r="D3" s="182"/>
-      <c r="E3" s="182"/>
-      <c r="F3" s="182"/>
-      <c r="G3" s="182"/>
-      <c r="H3" s="182"/>
-      <c r="I3" s="182"/>
-      <c r="J3" s="182"/>
-      <c r="K3" s="182"/>
-      <c r="L3" s="182"/>
+      <c r="A3" s="185"/>
+      <c r="B3" s="185"/>
+      <c r="C3" s="185"/>
+      <c r="D3" s="185"/>
+      <c r="E3" s="185"/>
+      <c r="F3" s="185"/>
+      <c r="G3" s="185"/>
+      <c r="H3" s="185"/>
+      <c r="I3" s="185"/>
+      <c r="J3" s="185"/>
+      <c r="K3" s="185"/>
+      <c r="L3" s="185"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A4" s="182"/>
-      <c r="B4" s="182"/>
-      <c r="C4" s="182"/>
-      <c r="D4" s="182"/>
-      <c r="E4" s="182"/>
-      <c r="F4" s="182"/>
-      <c r="G4" s="182"/>
-      <c r="H4" s="182"/>
-      <c r="I4" s="182"/>
-      <c r="J4" s="182"/>
-      <c r="K4" s="182"/>
-      <c r="L4" s="182"/>
+      <c r="A4" s="185"/>
+      <c r="B4" s="185"/>
+      <c r="C4" s="185"/>
+      <c r="D4" s="185"/>
+      <c r="E4" s="185"/>
+      <c r="F4" s="185"/>
+      <c r="G4" s="185"/>
+      <c r="H4" s="185"/>
+      <c r="I4" s="185"/>
+      <c r="J4" s="185"/>
+      <c r="K4" s="185"/>
+      <c r="L4" s="185"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A5" s="182"/>
-      <c r="B5" s="182"/>
-      <c r="C5" s="182"/>
-      <c r="D5" s="182"/>
-      <c r="E5" s="182"/>
-      <c r="F5" s="182"/>
-      <c r="G5" s="182"/>
-      <c r="H5" s="182"/>
-      <c r="I5" s="182"/>
-      <c r="J5" s="182"/>
-      <c r="K5" s="182"/>
-      <c r="L5" s="182"/>
+      <c r="A5" s="185"/>
+      <c r="B5" s="185"/>
+      <c r="C5" s="185"/>
+      <c r="D5" s="185"/>
+      <c r="E5" s="185"/>
+      <c r="F5" s="185"/>
+      <c r="G5" s="185"/>
+      <c r="H5" s="185"/>
+      <c r="I5" s="185"/>
+      <c r="J5" s="185"/>
+      <c r="K5" s="185"/>
+      <c r="L5" s="185"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A6" s="182"/>
-      <c r="B6" s="182"/>
-      <c r="C6" s="182"/>
-      <c r="D6" s="182"/>
-      <c r="E6" s="182"/>
-      <c r="F6" s="182"/>
-      <c r="G6" s="182"/>
-      <c r="H6" s="182"/>
-      <c r="I6" s="182"/>
-      <c r="J6" s="182"/>
-      <c r="K6" s="182"/>
-      <c r="L6" s="182"/>
+      <c r="A6" s="185"/>
+      <c r="B6" s="185"/>
+      <c r="C6" s="185"/>
+      <c r="D6" s="185"/>
+      <c r="E6" s="185"/>
+      <c r="F6" s="185"/>
+      <c r="G6" s="185"/>
+      <c r="H6" s="185"/>
+      <c r="I6" s="185"/>
+      <c r="J6" s="185"/>
+      <c r="K6" s="185"/>
+      <c r="L6" s="185"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A7" s="182"/>
-      <c r="B7" s="182"/>
-      <c r="C7" s="182"/>
-      <c r="D7" s="182"/>
-      <c r="E7" s="182"/>
-      <c r="F7" s="182"/>
-      <c r="G7" s="182"/>
-      <c r="H7" s="182"/>
-      <c r="I7" s="182"/>
-      <c r="J7" s="182"/>
-      <c r="K7" s="182"/>
-      <c r="L7" s="182"/>
+      <c r="A7" s="185"/>
+      <c r="B7" s="185"/>
+      <c r="C7" s="185"/>
+      <c r="D7" s="185"/>
+      <c r="E7" s="185"/>
+      <c r="F7" s="185"/>
+      <c r="G7" s="185"/>
+      <c r="H7" s="185"/>
+      <c r="I7" s="185"/>
+      <c r="J7" s="185"/>
+      <c r="K7" s="185"/>
+      <c r="L7" s="185"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A8" s="182"/>
-      <c r="B8" s="182"/>
-      <c r="C8" s="182"/>
-      <c r="D8" s="182"/>
-      <c r="E8" s="182"/>
-      <c r="F8" s="182"/>
-      <c r="G8" s="182"/>
-      <c r="H8" s="182"/>
-      <c r="I8" s="182"/>
-      <c r="J8" s="182"/>
-      <c r="K8" s="182"/>
-      <c r="L8" s="182"/>
+      <c r="A8" s="185"/>
+      <c r="B8" s="185"/>
+      <c r="C8" s="185"/>
+      <c r="D8" s="185"/>
+      <c r="E8" s="185"/>
+      <c r="F8" s="185"/>
+      <c r="G8" s="185"/>
+      <c r="H8" s="185"/>
+      <c r="I8" s="185"/>
+      <c r="J8" s="185"/>
+      <c r="K8" s="185"/>
+      <c r="L8" s="185"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A9" s="182"/>
-      <c r="B9" s="182"/>
-      <c r="C9" s="182"/>
-      <c r="D9" s="182"/>
-      <c r="E9" s="182"/>
-      <c r="F9" s="182"/>
-      <c r="G9" s="182"/>
-      <c r="H9" s="182"/>
-      <c r="I9" s="182"/>
-      <c r="J9" s="182"/>
-      <c r="K9" s="182"/>
-      <c r="L9" s="182"/>
+      <c r="A9" s="185"/>
+      <c r="B9" s="185"/>
+      <c r="C9" s="185"/>
+      <c r="D9" s="185"/>
+      <c r="E9" s="185"/>
+      <c r="F9" s="185"/>
+      <c r="G9" s="185"/>
+      <c r="H9" s="185"/>
+      <c r="I9" s="185"/>
+      <c r="J9" s="185"/>
+      <c r="K9" s="185"/>
+      <c r="L9" s="185"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A10" s="182"/>
-      <c r="B10" s="182"/>
-      <c r="C10" s="182"/>
-      <c r="D10" s="182"/>
-      <c r="E10" s="182"/>
-      <c r="F10" s="182"/>
-      <c r="G10" s="182"/>
-      <c r="H10" s="182"/>
-      <c r="I10" s="182"/>
-      <c r="J10" s="182"/>
-      <c r="K10" s="182"/>
-      <c r="L10" s="182"/>
+      <c r="A10" s="185"/>
+      <c r="B10" s="185"/>
+      <c r="C10" s="185"/>
+      <c r="D10" s="185"/>
+      <c r="E10" s="185"/>
+      <c r="F10" s="185"/>
+      <c r="G10" s="185"/>
+      <c r="H10" s="185"/>
+      <c r="I10" s="185"/>
+      <c r="J10" s="185"/>
+      <c r="K10" s="185"/>
+      <c r="L10" s="185"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A11" s="182"/>
-      <c r="B11" s="182"/>
-      <c r="C11" s="182"/>
-      <c r="D11" s="182"/>
-      <c r="E11" s="182"/>
-      <c r="F11" s="182"/>
-      <c r="G11" s="182"/>
-      <c r="H11" s="182"/>
-      <c r="I11" s="182"/>
-      <c r="J11" s="182"/>
-      <c r="K11" s="182"/>
-      <c r="L11" s="182"/>
+      <c r="A11" s="185"/>
+      <c r="B11" s="185"/>
+      <c r="C11" s="185"/>
+      <c r="D11" s="185"/>
+      <c r="E11" s="185"/>
+      <c r="F11" s="185"/>
+      <c r="G11" s="185"/>
+      <c r="H11" s="185"/>
+      <c r="I11" s="185"/>
+      <c r="J11" s="185"/>
+      <c r="K11" s="185"/>
+      <c r="L11" s="185"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A12" s="182"/>
-      <c r="B12" s="182"/>
-      <c r="C12" s="182"/>
-      <c r="D12" s="182"/>
-      <c r="E12" s="182"/>
-      <c r="F12" s="182"/>
-      <c r="G12" s="182"/>
-      <c r="H12" s="182"/>
-      <c r="I12" s="182"/>
-      <c r="J12" s="182"/>
-      <c r="K12" s="182"/>
-      <c r="L12" s="182"/>
+      <c r="A12" s="185"/>
+      <c r="B12" s="185"/>
+      <c r="C12" s="185"/>
+      <c r="D12" s="185"/>
+      <c r="E12" s="185"/>
+      <c r="F12" s="185"/>
+      <c r="G12" s="185"/>
+      <c r="H12" s="185"/>
+      <c r="I12" s="185"/>
+      <c r="J12" s="185"/>
+      <c r="K12" s="185"/>
+      <c r="L12" s="185"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A13" s="182"/>
-      <c r="B13" s="182"/>
-      <c r="C13" s="182"/>
-      <c r="D13" s="182"/>
-      <c r="E13" s="182"/>
-      <c r="F13" s="182"/>
-      <c r="G13" s="182"/>
-      <c r="H13" s="182"/>
-      <c r="I13" s="182"/>
-      <c r="J13" s="182"/>
-      <c r="K13" s="182"/>
-      <c r="L13" s="182"/>
+      <c r="A13" s="185"/>
+      <c r="B13" s="185"/>
+      <c r="C13" s="185"/>
+      <c r="D13" s="185"/>
+      <c r="E13" s="185"/>
+      <c r="F13" s="185"/>
+      <c r="G13" s="185"/>
+      <c r="H13" s="185"/>
+      <c r="I13" s="185"/>
+      <c r="J13" s="185"/>
+      <c r="K13" s="185"/>
+      <c r="L13" s="185"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A14" s="182"/>
-      <c r="B14" s="182"/>
-      <c r="C14" s="182"/>
-      <c r="D14" s="182"/>
-      <c r="E14" s="182"/>
-      <c r="F14" s="182"/>
-      <c r="G14" s="182"/>
-      <c r="H14" s="182"/>
-      <c r="I14" s="182"/>
-      <c r="J14" s="182"/>
-      <c r="K14" s="182"/>
-      <c r="L14" s="182"/>
+      <c r="A14" s="185"/>
+      <c r="B14" s="185"/>
+      <c r="C14" s="185"/>
+      <c r="D14" s="185"/>
+      <c r="E14" s="185"/>
+      <c r="F14" s="185"/>
+      <c r="G14" s="185"/>
+      <c r="H14" s="185"/>
+      <c r="I14" s="185"/>
+      <c r="J14" s="185"/>
+      <c r="K14" s="185"/>
+      <c r="L14" s="185"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A15" s="182"/>
-      <c r="B15" s="182"/>
-      <c r="C15" s="182"/>
-      <c r="D15" s="182"/>
-      <c r="E15" s="182"/>
-      <c r="F15" s="182"/>
-      <c r="G15" s="182"/>
-      <c r="H15" s="182"/>
-      <c r="I15" s="182"/>
-      <c r="J15" s="182"/>
-      <c r="K15" s="182"/>
-      <c r="L15" s="182"/>
+      <c r="A15" s="185"/>
+      <c r="B15" s="185"/>
+      <c r="C15" s="185"/>
+      <c r="D15" s="185"/>
+      <c r="E15" s="185"/>
+      <c r="F15" s="185"/>
+      <c r="G15" s="185"/>
+      <c r="H15" s="185"/>
+      <c r="I15" s="185"/>
+      <c r="J15" s="185"/>
+      <c r="K15" s="185"/>
+      <c r="L15" s="185"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A16" s="182"/>
-      <c r="B16" s="182"/>
-      <c r="C16" s="182"/>
-      <c r="D16" s="182"/>
-      <c r="E16" s="182"/>
-      <c r="F16" s="182"/>
-      <c r="G16" s="182"/>
-      <c r="H16" s="182"/>
-      <c r="I16" s="182"/>
-      <c r="J16" s="182"/>
-      <c r="K16" s="182"/>
-      <c r="L16" s="182"/>
+      <c r="A16" s="185"/>
+      <c r="B16" s="185"/>
+      <c r="C16" s="185"/>
+      <c r="D16" s="185"/>
+      <c r="E16" s="185"/>
+      <c r="F16" s="185"/>
+      <c r="G16" s="185"/>
+      <c r="H16" s="185"/>
+      <c r="I16" s="185"/>
+      <c r="J16" s="185"/>
+      <c r="K16" s="185"/>
+      <c r="L16" s="185"/>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A17" s="182"/>
-      <c r="B17" s="182"/>
-      <c r="C17" s="182"/>
-      <c r="D17" s="182"/>
-      <c r="E17" s="182"/>
-      <c r="F17" s="182"/>
-      <c r="G17" s="182"/>
-      <c r="H17" s="182"/>
-      <c r="I17" s="182"/>
-      <c r="J17" s="182"/>
-      <c r="K17" s="182"/>
-      <c r="L17" s="182"/>
+      <c r="A17" s="185"/>
+      <c r="B17" s="185"/>
+      <c r="C17" s="185"/>
+      <c r="D17" s="185"/>
+      <c r="E17" s="185"/>
+      <c r="F17" s="185"/>
+      <c r="G17" s="185"/>
+      <c r="H17" s="185"/>
+      <c r="I17" s="185"/>
+      <c r="J17" s="185"/>
+      <c r="K17" s="185"/>
+      <c r="L17" s="185"/>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A18" s="182"/>
-      <c r="B18" s="182"/>
-      <c r="C18" s="182"/>
-      <c r="D18" s="182"/>
-      <c r="E18" s="182"/>
-      <c r="F18" s="182"/>
-      <c r="G18" s="182"/>
-      <c r="H18" s="182"/>
-      <c r="I18" s="182"/>
-      <c r="J18" s="182"/>
-      <c r="K18" s="182"/>
-      <c r="L18" s="182"/>
+      <c r="A18" s="185"/>
+      <c r="B18" s="185"/>
+      <c r="C18" s="185"/>
+      <c r="D18" s="185"/>
+      <c r="E18" s="185"/>
+      <c r="F18" s="185"/>
+      <c r="G18" s="185"/>
+      <c r="H18" s="185"/>
+      <c r="I18" s="185"/>
+      <c r="J18" s="185"/>
+      <c r="K18" s="185"/>
+      <c r="L18" s="185"/>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A19" s="182"/>
-      <c r="B19" s="182"/>
-      <c r="C19" s="182"/>
-      <c r="D19" s="182"/>
-      <c r="E19" s="182"/>
-      <c r="F19" s="182"/>
-      <c r="G19" s="182"/>
-      <c r="H19" s="182"/>
-      <c r="I19" s="182"/>
-      <c r="J19" s="182"/>
-      <c r="K19" s="182"/>
-      <c r="L19" s="182"/>
+      <c r="A19" s="185"/>
+      <c r="B19" s="185"/>
+      <c r="C19" s="185"/>
+      <c r="D19" s="185"/>
+      <c r="E19" s="185"/>
+      <c r="F19" s="185"/>
+      <c r="G19" s="185"/>
+      <c r="H19" s="185"/>
+      <c r="I19" s="185"/>
+      <c r="J19" s="185"/>
+      <c r="K19" s="185"/>
+      <c r="L19" s="185"/>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A20" s="182"/>
-      <c r="B20" s="182"/>
-      <c r="C20" s="182"/>
-      <c r="D20" s="182"/>
-      <c r="E20" s="182"/>
-      <c r="F20" s="182"/>
-      <c r="G20" s="182"/>
-      <c r="H20" s="182"/>
-      <c r="I20" s="182"/>
-      <c r="J20" s="182"/>
-      <c r="K20" s="182"/>
-      <c r="L20" s="182"/>
+      <c r="A20" s="185"/>
+      <c r="B20" s="185"/>
+      <c r="C20" s="185"/>
+      <c r="D20" s="185"/>
+      <c r="E20" s="185"/>
+      <c r="F20" s="185"/>
+      <c r="G20" s="185"/>
+      <c r="H20" s="185"/>
+      <c r="I20" s="185"/>
+      <c r="J20" s="185"/>
+      <c r="K20" s="185"/>
+      <c r="L20" s="185"/>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A21" s="182"/>
-      <c r="B21" s="182"/>
-      <c r="C21" s="182"/>
-      <c r="D21" s="182"/>
-      <c r="E21" s="182"/>
-      <c r="F21" s="182"/>
-      <c r="G21" s="182"/>
-      <c r="H21" s="182"/>
-      <c r="I21" s="182"/>
-      <c r="J21" s="182"/>
-      <c r="K21" s="182"/>
-      <c r="L21" s="182"/>
+      <c r="A21" s="185"/>
+      <c r="B21" s="185"/>
+      <c r="C21" s="185"/>
+      <c r="D21" s="185"/>
+      <c r="E21" s="185"/>
+      <c r="F21" s="185"/>
+      <c r="G21" s="185"/>
+      <c r="H21" s="185"/>
+      <c r="I21" s="185"/>
+      <c r="J21" s="185"/>
+      <c r="K21" s="185"/>
+      <c r="L21" s="185"/>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A22" s="182"/>
-      <c r="B22" s="182"/>
-      <c r="C22" s="182"/>
-      <c r="D22" s="182"/>
-      <c r="E22" s="182"/>
-      <c r="F22" s="182"/>
-      <c r="G22" s="182"/>
-      <c r="H22" s="182"/>
-      <c r="I22" s="182"/>
-      <c r="J22" s="182"/>
-      <c r="K22" s="182"/>
-      <c r="L22" s="182"/>
+      <c r="A22" s="185"/>
+      <c r="B22" s="185"/>
+      <c r="C22" s="185"/>
+      <c r="D22" s="185"/>
+      <c r="E22" s="185"/>
+      <c r="F22" s="185"/>
+      <c r="G22" s="185"/>
+      <c r="H22" s="185"/>
+      <c r="I22" s="185"/>
+      <c r="J22" s="185"/>
+      <c r="K22" s="185"/>
+      <c r="L22" s="185"/>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A23" s="182"/>
-      <c r="B23" s="182"/>
-      <c r="C23" s="182"/>
-      <c r="D23" s="182"/>
-      <c r="E23" s="182"/>
-      <c r="F23" s="182"/>
-      <c r="G23" s="182"/>
-      <c r="H23" s="182"/>
-      <c r="I23" s="182"/>
-      <c r="J23" s="182"/>
-      <c r="K23" s="182"/>
-      <c r="L23" s="182"/>
+      <c r="A23" s="185"/>
+      <c r="B23" s="185"/>
+      <c r="C23" s="185"/>
+      <c r="D23" s="185"/>
+      <c r="E23" s="185"/>
+      <c r="F23" s="185"/>
+      <c r="G23" s="185"/>
+      <c r="H23" s="185"/>
+      <c r="I23" s="185"/>
+      <c r="J23" s="185"/>
+      <c r="K23" s="185"/>
+      <c r="L23" s="185"/>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A24" s="182"/>
-      <c r="B24" s="182"/>
-      <c r="C24" s="182"/>
-      <c r="D24" s="182"/>
-      <c r="E24" s="182"/>
-      <c r="F24" s="182"/>
-      <c r="G24" s="182"/>
-      <c r="H24" s="182"/>
-      <c r="I24" s="182"/>
-      <c r="J24" s="182"/>
-      <c r="K24" s="182"/>
-      <c r="L24" s="182"/>
+      <c r="A24" s="185"/>
+      <c r="B24" s="185"/>
+      <c r="C24" s="185"/>
+      <c r="D24" s="185"/>
+      <c r="E24" s="185"/>
+      <c r="F24" s="185"/>
+      <c r="G24" s="185"/>
+      <c r="H24" s="185"/>
+      <c r="I24" s="185"/>
+      <c r="J24" s="185"/>
+      <c r="K24" s="185"/>
+      <c r="L24" s="185"/>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A25" s="182"/>
-      <c r="B25" s="182"/>
-      <c r="C25" s="182"/>
-      <c r="D25" s="182"/>
-      <c r="E25" s="182"/>
-      <c r="F25" s="182"/>
-      <c r="G25" s="182"/>
-      <c r="H25" s="182"/>
-      <c r="I25" s="182"/>
-      <c r="J25" s="182"/>
-      <c r="K25" s="182"/>
-      <c r="L25" s="182"/>
+      <c r="A25" s="185"/>
+      <c r="B25" s="185"/>
+      <c r="C25" s="185"/>
+      <c r="D25" s="185"/>
+      <c r="E25" s="185"/>
+      <c r="F25" s="185"/>
+      <c r="G25" s="185"/>
+      <c r="H25" s="185"/>
+      <c r="I25" s="185"/>
+      <c r="J25" s="185"/>
+      <c r="K25" s="185"/>
+      <c r="L25" s="185"/>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A26" s="182"/>
-      <c r="B26" s="182"/>
-      <c r="C26" s="182"/>
-      <c r="D26" s="182"/>
-      <c r="E26" s="182"/>
-      <c r="F26" s="182"/>
-      <c r="G26" s="182"/>
-      <c r="H26" s="182"/>
-      <c r="I26" s="182"/>
-      <c r="J26" s="182"/>
-      <c r="K26" s="182"/>
-      <c r="L26" s="182"/>
+      <c r="A26" s="185"/>
+      <c r="B26" s="185"/>
+      <c r="C26" s="185"/>
+      <c r="D26" s="185"/>
+      <c r="E26" s="185"/>
+      <c r="F26" s="185"/>
+      <c r="G26" s="185"/>
+      <c r="H26" s="185"/>
+      <c r="I26" s="185"/>
+      <c r="J26" s="185"/>
+      <c r="K26" s="185"/>
+      <c r="L26" s="185"/>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A27" s="182"/>
-      <c r="B27" s="182"/>
-      <c r="C27" s="182"/>
-      <c r="D27" s="182"/>
-      <c r="E27" s="182"/>
-      <c r="F27" s="182"/>
-      <c r="G27" s="182"/>
-      <c r="H27" s="182"/>
-      <c r="I27" s="182"/>
-      <c r="J27" s="182"/>
-      <c r="K27" s="182"/>
-      <c r="L27" s="182"/>
+      <c r="A27" s="185"/>
+      <c r="B27" s="185"/>
+      <c r="C27" s="185"/>
+      <c r="D27" s="185"/>
+      <c r="E27" s="185"/>
+      <c r="F27" s="185"/>
+      <c r="G27" s="185"/>
+      <c r="H27" s="185"/>
+      <c r="I27" s="185"/>
+      <c r="J27" s="185"/>
+      <c r="K27" s="185"/>
+      <c r="L27" s="185"/>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A28" s="182"/>
-      <c r="B28" s="182"/>
-      <c r="C28" s="182"/>
-      <c r="D28" s="182"/>
-      <c r="E28" s="182"/>
-      <c r="F28" s="182"/>
-      <c r="G28" s="182"/>
-      <c r="H28" s="182"/>
-      <c r="I28" s="182"/>
-      <c r="J28" s="182"/>
-      <c r="K28" s="182"/>
-      <c r="L28" s="182"/>
+      <c r="A28" s="185"/>
+      <c r="B28" s="185"/>
+      <c r="C28" s="185"/>
+      <c r="D28" s="185"/>
+      <c r="E28" s="185"/>
+      <c r="F28" s="185"/>
+      <c r="G28" s="185"/>
+      <c r="H28" s="185"/>
+      <c r="I28" s="185"/>
+      <c r="J28" s="185"/>
+      <c r="K28" s="185"/>
+      <c r="L28" s="185"/>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A29" s="182"/>
-      <c r="B29" s="182"/>
-      <c r="C29" s="182"/>
-      <c r="D29" s="182"/>
-      <c r="E29" s="182"/>
-      <c r="F29" s="182"/>
-      <c r="G29" s="182"/>
-      <c r="H29" s="182"/>
-      <c r="I29" s="182"/>
-      <c r="J29" s="182"/>
-      <c r="K29" s="182"/>
-      <c r="L29" s="182"/>
+      <c r="A29" s="185"/>
+      <c r="B29" s="185"/>
+      <c r="C29" s="185"/>
+      <c r="D29" s="185"/>
+      <c r="E29" s="185"/>
+      <c r="F29" s="185"/>
+      <c r="G29" s="185"/>
+      <c r="H29" s="185"/>
+      <c r="I29" s="185"/>
+      <c r="J29" s="185"/>
+      <c r="K29" s="185"/>
+      <c r="L29" s="185"/>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A30" s="182"/>
-      <c r="B30" s="182"/>
-      <c r="C30" s="182"/>
-      <c r="D30" s="182"/>
-      <c r="E30" s="182"/>
-      <c r="F30" s="182"/>
-      <c r="G30" s="182"/>
-      <c r="H30" s="182"/>
-      <c r="I30" s="182"/>
-      <c r="J30" s="182"/>
-      <c r="K30" s="182"/>
-      <c r="L30" s="182"/>
+      <c r="A30" s="185"/>
+      <c r="B30" s="185"/>
+      <c r="C30" s="185"/>
+      <c r="D30" s="185"/>
+      <c r="E30" s="185"/>
+      <c r="F30" s="185"/>
+      <c r="G30" s="185"/>
+      <c r="H30" s="185"/>
+      <c r="I30" s="185"/>
+      <c r="J30" s="185"/>
+      <c r="K30" s="185"/>
+      <c r="L30" s="185"/>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A31" s="182"/>
-      <c r="B31" s="182"/>
-      <c r="C31" s="182"/>
-      <c r="D31" s="182"/>
-      <c r="E31" s="182"/>
-      <c r="F31" s="182"/>
-      <c r="G31" s="182"/>
-      <c r="H31" s="182"/>
-      <c r="I31" s="182"/>
-      <c r="J31" s="182"/>
-      <c r="K31" s="182"/>
-      <c r="L31" s="182"/>
+      <c r="A31" s="185"/>
+      <c r="B31" s="185"/>
+      <c r="C31" s="185"/>
+      <c r="D31" s="185"/>
+      <c r="E31" s="185"/>
+      <c r="F31" s="185"/>
+      <c r="G31" s="185"/>
+      <c r="H31" s="185"/>
+      <c r="I31" s="185"/>
+      <c r="J31" s="185"/>
+      <c r="K31" s="185"/>
+      <c r="L31" s="185"/>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A32" s="182"/>
-      <c r="B32" s="182"/>
-      <c r="C32" s="182"/>
-      <c r="D32" s="182"/>
-      <c r="E32" s="182"/>
-      <c r="F32" s="182"/>
-      <c r="G32" s="182"/>
-      <c r="H32" s="182"/>
-      <c r="I32" s="182"/>
-      <c r="J32" s="182"/>
-      <c r="K32" s="182"/>
-      <c r="L32" s="182"/>
+      <c r="A32" s="185"/>
+      <c r="B32" s="185"/>
+      <c r="C32" s="185"/>
+      <c r="D32" s="185"/>
+      <c r="E32" s="185"/>
+      <c r="F32" s="185"/>
+      <c r="G32" s="185"/>
+      <c r="H32" s="185"/>
+      <c r="I32" s="185"/>
+      <c r="J32" s="185"/>
+      <c r="K32" s="185"/>
+      <c r="L32" s="185"/>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A33" s="182"/>
-      <c r="B33" s="182"/>
-      <c r="C33" s="182"/>
-      <c r="D33" s="182"/>
-      <c r="E33" s="182"/>
-      <c r="F33" s="182"/>
-      <c r="G33" s="182"/>
-      <c r="H33" s="182"/>
-      <c r="I33" s="182"/>
-      <c r="J33" s="182"/>
-      <c r="K33" s="182"/>
-      <c r="L33" s="182"/>
+      <c r="A33" s="185"/>
+      <c r="B33" s="185"/>
+      <c r="C33" s="185"/>
+      <c r="D33" s="185"/>
+      <c r="E33" s="185"/>
+      <c r="F33" s="185"/>
+      <c r="G33" s="185"/>
+      <c r="H33" s="185"/>
+      <c r="I33" s="185"/>
+      <c r="J33" s="185"/>
+      <c r="K33" s="185"/>
+      <c r="L33" s="185"/>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A34" s="182"/>
-      <c r="B34" s="182"/>
-      <c r="C34" s="182"/>
-      <c r="D34" s="182"/>
-      <c r="E34" s="182"/>
-      <c r="F34" s="182"/>
-      <c r="G34" s="182"/>
-      <c r="H34" s="182"/>
-      <c r="I34" s="182"/>
-      <c r="J34" s="182"/>
-      <c r="K34" s="182"/>
-      <c r="L34" s="182"/>
+      <c r="A34" s="185"/>
+      <c r="B34" s="185"/>
+      <c r="C34" s="185"/>
+      <c r="D34" s="185"/>
+      <c r="E34" s="185"/>
+      <c r="F34" s="185"/>
+      <c r="G34" s="185"/>
+      <c r="H34" s="185"/>
+      <c r="I34" s="185"/>
+      <c r="J34" s="185"/>
+      <c r="K34" s="185"/>
+      <c r="L34" s="185"/>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A35" s="182"/>
-      <c r="B35" s="182"/>
-      <c r="C35" s="182"/>
-      <c r="D35" s="182"/>
-      <c r="E35" s="182"/>
-      <c r="F35" s="182"/>
-      <c r="G35" s="182"/>
-      <c r="H35" s="182"/>
-      <c r="I35" s="182"/>
-      <c r="J35" s="182"/>
-      <c r="K35" s="182"/>
-      <c r="L35" s="182"/>
+      <c r="A35" s="185"/>
+      <c r="B35" s="185"/>
+      <c r="C35" s="185"/>
+      <c r="D35" s="185"/>
+      <c r="E35" s="185"/>
+      <c r="F35" s="185"/>
+      <c r="G35" s="185"/>
+      <c r="H35" s="185"/>
+      <c r="I35" s="185"/>
+      <c r="J35" s="185"/>
+      <c r="K35" s="185"/>
+      <c r="L35" s="185"/>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A36" s="182"/>
-      <c r="B36" s="182"/>
-      <c r="C36" s="182"/>
-      <c r="D36" s="182"/>
-      <c r="E36" s="182"/>
-      <c r="F36" s="182"/>
-      <c r="G36" s="182"/>
-      <c r="H36" s="182"/>
-      <c r="I36" s="182"/>
-      <c r="J36" s="182"/>
-      <c r="K36" s="182"/>
-      <c r="L36" s="182"/>
+      <c r="A36" s="185"/>
+      <c r="B36" s="185"/>
+      <c r="C36" s="185"/>
+      <c r="D36" s="185"/>
+      <c r="E36" s="185"/>
+      <c r="F36" s="185"/>
+      <c r="G36" s="185"/>
+      <c r="H36" s="185"/>
+      <c r="I36" s="185"/>
+      <c r="J36" s="185"/>
+      <c r="K36" s="185"/>
+      <c r="L36" s="185"/>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A37" s="182"/>
-      <c r="B37" s="182"/>
-      <c r="C37" s="182"/>
-      <c r="D37" s="182"/>
-      <c r="E37" s="182"/>
-      <c r="F37" s="182"/>
-      <c r="G37" s="182"/>
-      <c r="H37" s="182"/>
-      <c r="I37" s="182"/>
-      <c r="J37" s="182"/>
-      <c r="K37" s="182"/>
-      <c r="L37" s="182"/>
+      <c r="A37" s="185"/>
+      <c r="B37" s="185"/>
+      <c r="C37" s="185"/>
+      <c r="D37" s="185"/>
+      <c r="E37" s="185"/>
+      <c r="F37" s="185"/>
+      <c r="G37" s="185"/>
+      <c r="H37" s="185"/>
+      <c r="I37" s="185"/>
+      <c r="J37" s="185"/>
+      <c r="K37" s="185"/>
+      <c r="L37" s="185"/>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A38" s="182"/>
-      <c r="B38" s="182"/>
-      <c r="C38" s="182"/>
-      <c r="D38" s="182"/>
-      <c r="E38" s="182"/>
-      <c r="F38" s="182"/>
-      <c r="G38" s="182"/>
-      <c r="H38" s="182"/>
-      <c r="I38" s="182"/>
-      <c r="J38" s="182"/>
-      <c r="K38" s="182"/>
-      <c r="L38" s="182"/>
+      <c r="A38" s="185"/>
+      <c r="B38" s="185"/>
+      <c r="C38" s="185"/>
+      <c r="D38" s="185"/>
+      <c r="E38" s="185"/>
+      <c r="F38" s="185"/>
+      <c r="G38" s="185"/>
+      <c r="H38" s="185"/>
+      <c r="I38" s="185"/>
+      <c r="J38" s="185"/>
+      <c r="K38" s="185"/>
+      <c r="L38" s="185"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -8321,13 +8402,13 @@
         <v>1230</v>
       </c>
       <c r="C2" s="151" t="s">
-        <v>1389</v>
+        <v>1387</v>
       </c>
       <c r="D2" s="92" t="s">
         <v>1231</v>
       </c>
       <c r="E2" s="152" t="s">
-        <v>1393</v>
+        <v>1391</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="80" x14ac:dyDescent="0.2">
@@ -8355,13 +8436,13 @@
         <v>1237</v>
       </c>
       <c r="C4" s="158" t="s">
-        <v>1390</v>
+        <v>1388</v>
       </c>
       <c r="D4" s="95" t="s">
         <v>400</v>
       </c>
       <c r="E4" s="155" t="s">
-        <v>1392</v>
+        <v>1390</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="60.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -8423,13 +8504,13 @@
         <v>1242</v>
       </c>
       <c r="C8" s="158" t="s">
-        <v>1389</v>
+        <v>1387</v>
       </c>
       <c r="D8" s="95" t="s">
         <v>1243</v>
       </c>
       <c r="E8" s="155" t="s">
-        <v>1393</v>
+        <v>1391</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="80" x14ac:dyDescent="0.2">
@@ -8440,11 +8521,11 @@
         <v>1244</v>
       </c>
       <c r="C9" s="158" t="s">
-        <v>1486</v>
+        <v>1484</v>
       </c>
       <c r="D9" s="179"/>
       <c r="E9" s="155" t="s">
-        <v>1487</v>
+        <v>1485</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="16" x14ac:dyDescent="0.2">
@@ -8455,13 +8536,13 @@
         <v>1245</v>
       </c>
       <c r="C10" s="158" t="s">
-        <v>1390</v>
+        <v>1388</v>
       </c>
       <c r="D10" s="95" t="s">
         <v>400</v>
       </c>
       <c r="E10" s="155" t="s">
-        <v>1392</v>
+        <v>1390</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -8523,13 +8604,13 @@
         <v>1248</v>
       </c>
       <c r="C14" s="158" t="s">
-        <v>1389</v>
+        <v>1387</v>
       </c>
       <c r="D14" s="95" t="s">
         <v>1249</v>
       </c>
       <c r="E14" s="155" t="s">
-        <v>1391</v>
+        <v>1389</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="96" x14ac:dyDescent="0.2">
@@ -8540,11 +8621,11 @@
         <v>1250</v>
       </c>
       <c r="C15" s="158" t="s">
-        <v>1488</v>
+        <v>1486</v>
       </c>
       <c r="D15" s="179"/>
       <c r="E15" s="155" t="s">
-        <v>1489</v>
+        <v>1487</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="48" x14ac:dyDescent="0.2">
@@ -8589,13 +8670,13 @@
         <v>1253</v>
       </c>
       <c r="C18" s="158" t="s">
-        <v>1390</v>
+        <v>1388</v>
       </c>
       <c r="D18" s="95" t="s">
         <v>400</v>
       </c>
       <c r="E18" s="155" t="s">
-        <v>1392</v>
+        <v>1390</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -8623,13 +8704,13 @@
         <v>1254</v>
       </c>
       <c r="C20" s="158" t="s">
-        <v>1422</v>
+        <v>1420</v>
       </c>
       <c r="D20" s="95" t="s">
         <v>1231</v>
       </c>
       <c r="E20" s="155" t="s">
-        <v>1423</v>
+        <v>1421</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="64" x14ac:dyDescent="0.2">
@@ -8640,13 +8721,13 @@
         <v>1255</v>
       </c>
       <c r="C21" s="158" t="s">
-        <v>1421</v>
+        <v>1419</v>
       </c>
       <c r="D21" s="95" t="s">
         <v>1256</v>
       </c>
       <c r="E21" s="155" t="s">
-        <v>1424</v>
+        <v>1422</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -8657,13 +8738,13 @@
         <v>1257</v>
       </c>
       <c r="C22" s="158" t="s">
-        <v>1425</v>
+        <v>1423</v>
       </c>
       <c r="D22" s="95" t="s">
         <v>400</v>
       </c>
       <c r="E22" s="155" t="s">
-        <v>1426</v>
+        <v>1424</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="48" x14ac:dyDescent="0.2">
@@ -8707,11 +8788,11 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{124C2F8F-96ED-4E65-B816-FFFEB93DC889}">
-  <dimension ref="A1:F25"/>
+  <dimension ref="A1:F36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C19" sqref="C19"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -8746,30 +8827,30 @@
       </c>
     </row>
     <row r="2" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="217" t="s">
-        <v>1260</v>
-      </c>
-      <c r="B2" s="218"/>
-      <c r="C2" s="218"/>
-      <c r="D2" s="218"/>
-      <c r="E2" s="218"/>
-      <c r="F2" s="218"/>
+      <c r="A2" s="220" t="s">
+        <v>1549</v>
+      </c>
+      <c r="B2" s="221"/>
+      <c r="C2" s="221"/>
+      <c r="D2" s="221"/>
+      <c r="E2" s="221"/>
+      <c r="F2" s="221"/>
     </row>
     <row r="3" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
         <v>239</v>
       </c>
       <c r="B3" s="5" t="s">
+        <v>1260</v>
+      </c>
+      <c r="C3" s="6" t="s">
         <v>1261</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>1262</v>
       </c>
       <c r="D3" s="5" t="s">
         <v>1212</v>
       </c>
       <c r="E3" s="37" t="s">
-        <v>1263</v>
+        <v>1262</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="32" x14ac:dyDescent="0.2">
@@ -8777,13 +8858,13 @@
         <v>257</v>
       </c>
       <c r="B4" s="5" t="s">
+        <v>1263</v>
+      </c>
+      <c r="C4" s="59" t="s">
+        <v>1410</v>
+      </c>
+      <c r="E4" s="37" t="s">
         <v>1264</v>
-      </c>
-      <c r="C4" s="59" t="s">
-        <v>1412</v>
-      </c>
-      <c r="E4" s="37" t="s">
-        <v>1265</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="16" x14ac:dyDescent="0.2">
@@ -8791,13 +8872,13 @@
         <v>250</v>
       </c>
       <c r="B5" s="5" t="s">
+        <v>1265</v>
+      </c>
+      <c r="C5" s="6" t="s">
         <v>1266</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="E5" s="37" t="s">
         <v>1267</v>
-      </c>
-      <c r="E5" s="37" t="s">
-        <v>1268</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="80" x14ac:dyDescent="0.2">
@@ -8805,13 +8886,13 @@
         <v>257</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>1269</v>
+        <v>1268</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>1410</v>
+        <v>1408</v>
       </c>
       <c r="E6" s="37" t="s">
-        <v>1411</v>
+        <v>1409</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="32" x14ac:dyDescent="0.2">
@@ -8819,112 +8900,112 @@
         <v>250</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>1270</v>
+        <v>1269</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>1529</v>
+        <v>1526</v>
       </c>
       <c r="E7" s="37" t="s">
-        <v>1530</v>
+        <v>1527</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
+        <v>1270</v>
+      </c>
+      <c r="B8" s="5" t="s">
         <v>1271</v>
       </c>
-      <c r="B8" s="5" t="s">
-        <v>1272</v>
-      </c>
       <c r="C8" s="6" t="s">
-        <v>1398</v>
+        <v>1396</v>
       </c>
       <c r="E8" s="37" t="s">
-        <v>1399</v>
+        <v>1397</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
+        <v>1272</v>
+      </c>
+      <c r="B9" s="5" t="s">
         <v>1273</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="C9" s="6" t="s">
         <v>1274</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="E9" s="37" t="s">
         <v>1275</v>
-      </c>
-      <c r="E9" s="37" t="s">
-        <v>1276</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
-        <v>1273</v>
+        <v>1272</v>
       </c>
       <c r="B10" s="5" t="s">
+        <v>1276</v>
+      </c>
+      <c r="C10" s="6" t="s">
         <v>1277</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="E10" s="37" t="s">
         <v>1278</v>
-      </c>
-      <c r="E10" s="37" t="s">
-        <v>1279</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
-        <v>1273</v>
+        <v>1272</v>
       </c>
       <c r="B11" s="5" t="s">
+        <v>1279</v>
+      </c>
+      <c r="C11" s="6" t="s">
         <v>1280</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="E11" s="37" t="s">
         <v>1281</v>
-      </c>
-      <c r="E11" s="37" t="s">
-        <v>1282</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="5" t="s">
-        <v>1273</v>
+        <v>1272</v>
       </c>
       <c r="B12" s="5" t="s">
+        <v>1282</v>
+      </c>
+      <c r="C12" s="6" t="s">
         <v>1283</v>
       </c>
-      <c r="C12" s="6" t="s">
+      <c r="E12" s="37" t="s">
         <v>1284</v>
-      </c>
-      <c r="E12" s="37" t="s">
-        <v>1285</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="s">
-        <v>1273</v>
+        <v>1272</v>
       </c>
       <c r="B13" s="5" t="s">
+        <v>1285</v>
+      </c>
+      <c r="C13" s="6" t="s">
         <v>1286</v>
       </c>
-      <c r="C13" s="6" t="s">
+      <c r="E13" s="37" t="s">
         <v>1287</v>
-      </c>
-      <c r="E13" s="37" t="s">
-        <v>1288</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A14" s="5" t="s">
-        <v>1271</v>
+        <v>1270</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>1289</v>
+        <v>1288</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>1396</v>
+        <v>1394</v>
       </c>
       <c r="D14" s="1"/>
       <c r="E14" s="37" t="s">
-        <v>1397</v>
+        <v>1395</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="32" x14ac:dyDescent="0.2">
@@ -8932,14 +9013,14 @@
         <v>940</v>
       </c>
       <c r="B15" s="5" t="s">
+        <v>1289</v>
+      </c>
+      <c r="C15" s="6" t="s">
         <v>1290</v>
-      </c>
-      <c r="C15" s="6" t="s">
-        <v>1291</v>
       </c>
       <c r="D15" s="1"/>
       <c r="E15" s="37" t="s">
-        <v>1292</v>
+        <v>1291</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="16" x14ac:dyDescent="0.2">
@@ -8947,86 +9028,86 @@
         <v>14</v>
       </c>
       <c r="B16" s="5" t="s">
+        <v>1292</v>
+      </c>
+      <c r="C16" s="74" t="s">
         <v>1293</v>
-      </c>
-      <c r="C16" s="74" t="s">
-        <v>1294</v>
       </c>
       <c r="D16" s="18"/>
       <c r="E16" s="37" t="s">
-        <v>1295</v>
+        <v>1294</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A17" s="5" t="s">
+        <v>1295</v>
+      </c>
+      <c r="B17" s="7" t="s">
         <v>1296</v>
       </c>
-      <c r="B17" s="7" t="s">
+      <c r="C17" s="75" t="s">
         <v>1297</v>
-      </c>
-      <c r="C17" s="75" t="s">
-        <v>1298</v>
       </c>
       <c r="D17" s="18"/>
       <c r="E17" s="37" t="s">
-        <v>1299</v>
+        <v>1298</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="32" x14ac:dyDescent="0.2">
-      <c r="A18" s="219" t="s">
+      <c r="A18" s="182" t="s">
         <v>486</v>
       </c>
-      <c r="B18" s="220" t="s">
+      <c r="B18" s="1" t="s">
+        <v>1531</v>
+      </c>
+      <c r="C18" s="183" t="s">
+        <v>1532</v>
+      </c>
+      <c r="D18" s="184"/>
+      <c r="E18" s="40" t="s">
+        <v>1533</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A19" s="182" t="s">
+        <v>486</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>1528</v>
+      </c>
+      <c r="C19" s="183" t="s">
+        <v>1529</v>
+      </c>
+      <c r="D19" s="184"/>
+      <c r="E19" s="40" t="s">
+        <v>1530</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A20" s="220" t="s">
         <v>1534</v>
       </c>
-      <c r="C18" s="221" t="s">
-        <v>1535</v>
-      </c>
-      <c r="D18" s="222"/>
-      <c r="E18" s="223" t="s">
-        <v>1536</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A19" s="219" t="s">
-        <v>486</v>
-      </c>
-      <c r="B19" s="220" t="s">
-        <v>1531</v>
-      </c>
-      <c r="C19" s="221" t="s">
-        <v>1532</v>
-      </c>
-      <c r="D19" s="222"/>
-      <c r="E19" s="223" t="s">
-        <v>1533</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A20" s="217" t="s">
-        <v>1300</v>
-      </c>
-      <c r="B20" s="218"/>
-      <c r="C20" s="218"/>
-      <c r="D20" s="218"/>
-      <c r="E20" s="218"/>
-      <c r="F20" s="218"/>
+      <c r="B20" s="221"/>
+      <c r="C20" s="221"/>
+      <c r="D20" s="221"/>
+      <c r="E20" s="221"/>
+      <c r="F20" s="221"/>
     </row>
     <row r="21" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A21" s="5" t="s">
         <v>239</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>1303</v>
+        <v>1301</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>1301</v>
+        <v>1299</v>
       </c>
       <c r="D21" s="5" t="s">
         <v>1212</v>
       </c>
       <c r="E21" s="37" t="s">
-        <v>1302</v>
+        <v>1300</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="96" x14ac:dyDescent="0.2">
@@ -9034,13 +9115,13 @@
         <v>257</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>1304</v>
+        <v>1302</v>
       </c>
       <c r="C22" s="59" t="s">
+        <v>1365</v>
+      </c>
+      <c r="E22" s="37" t="s">
         <v>1367</v>
-      </c>
-      <c r="E22" s="37" t="s">
-        <v>1369</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="16" x14ac:dyDescent="0.2">
@@ -9048,13 +9129,13 @@
         <v>250</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>1305</v>
+        <v>1303</v>
       </c>
       <c r="C23" s="6" t="s">
+        <v>1266</v>
+      </c>
+      <c r="E23" s="37" t="s">
         <v>1267</v>
-      </c>
-      <c r="E23" s="37" t="s">
-        <v>1268</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="80" x14ac:dyDescent="0.2">
@@ -9062,25 +9143,175 @@
         <v>257</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>1306</v>
+        <v>1304</v>
       </c>
       <c r="C24" s="6" t="s">
+        <v>1366</v>
+      </c>
+      <c r="E24" s="37" t="s">
         <v>1368</v>
       </c>
-      <c r="E24" s="37" t="s">
-        <v>1370</v>
-      </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A25" s="18"/>
-      <c r="B25" s="28"/>
-      <c r="C25" s="74"/>
-      <c r="D25" s="18"/>
+      <c r="A25" s="220" t="s">
+        <v>1535</v>
+      </c>
+      <c r="B25" s="221"/>
+      <c r="C25" s="221"/>
+      <c r="D25" s="221"/>
+      <c r="E25" s="221"/>
+      <c r="F25" s="221"/>
+    </row>
+    <row r="26" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+      <c r="A26" s="5" t="s">
+        <v>239</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>1538</v>
+      </c>
+      <c r="C26" s="6" t="s">
+        <v>1536</v>
+      </c>
+      <c r="E26" s="37" t="s">
+        <v>1537</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="208" x14ac:dyDescent="0.2">
+      <c r="A27" s="5" t="s">
+        <v>1553</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>1539</v>
+      </c>
+      <c r="C27" s="6" t="s">
+        <v>1541</v>
+      </c>
+      <c r="E27" s="37" t="s">
+        <v>1540</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A28" s="220" t="s">
+        <v>1542</v>
+      </c>
+      <c r="B28" s="221"/>
+      <c r="C28" s="221"/>
+      <c r="D28" s="221"/>
+      <c r="E28" s="221"/>
+      <c r="F28" s="221"/>
+    </row>
+    <row r="29" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+      <c r="A29" s="5" t="s">
+        <v>239</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>1543</v>
+      </c>
+      <c r="C29" s="6" t="s">
+        <v>1547</v>
+      </c>
+      <c r="E29" s="37" t="s">
+        <v>1548</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="176" x14ac:dyDescent="0.2">
+      <c r="A30" s="5" t="s">
+        <v>1553</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>1546</v>
+      </c>
+      <c r="C30" s="6" t="s">
+        <v>1544</v>
+      </c>
+      <c r="E30" s="37" t="s">
+        <v>1545</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A31" s="220" t="s">
+        <v>1550</v>
+      </c>
+      <c r="B31" s="221"/>
+      <c r="C31" s="221"/>
+      <c r="D31" s="221"/>
+      <c r="E31" s="221"/>
+      <c r="F31" s="221"/>
+    </row>
+    <row r="32" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+      <c r="A32" s="5" t="s">
+        <v>239</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>1551</v>
+      </c>
+      <c r="C32" s="6" t="s">
+        <v>1554</v>
+      </c>
+      <c r="E32" s="37" t="s">
+        <v>1563</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="224" x14ac:dyDescent="0.2">
+      <c r="A33" s="5" t="s">
+        <v>1553</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>1552</v>
+      </c>
+      <c r="C33" s="6" t="s">
+        <v>1555</v>
+      </c>
+      <c r="E33" s="37" t="s">
+        <v>1564</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A34" s="220" t="s">
+        <v>1556</v>
+      </c>
+      <c r="B34" s="221"/>
+      <c r="C34" s="221"/>
+      <c r="D34" s="221"/>
+      <c r="E34" s="221"/>
+      <c r="F34" s="221"/>
+    </row>
+    <row r="35" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+      <c r="A35" s="5" t="s">
+        <v>239</v>
+      </c>
+      <c r="B35" s="5" t="s">
+        <v>1557</v>
+      </c>
+      <c r="C35" s="6" t="s">
+        <v>1559</v>
+      </c>
+      <c r="E35" s="37" t="s">
+        <v>1562</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" ht="112" x14ac:dyDescent="0.2">
+      <c r="A36" s="5" t="s">
+        <v>1553</v>
+      </c>
+      <c r="B36" s="5" t="s">
+        <v>1558</v>
+      </c>
+      <c r="C36" s="6" t="s">
+        <v>1560</v>
+      </c>
+      <c r="E36" s="37" t="s">
+        <v>1561</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="6">
+    <mergeCell ref="A34:F34"/>
     <mergeCell ref="A2:F2"/>
     <mergeCell ref="A20:F20"/>
+    <mergeCell ref="A25:F25"/>
+    <mergeCell ref="A28:F28"/>
+    <mergeCell ref="A31:F31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -9090,9 +9321,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F72"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A33" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -9132,13 +9363,13 @@
         <v>7</v>
       </c>
       <c r="C2" s="100" t="s">
-        <v>1525</v>
+        <v>1565</v>
       </c>
       <c r="D2" s="98" t="s">
         <v>8</v>
       </c>
       <c r="E2" s="99" t="s">
-        <v>1525</v>
+        <v>1565</v>
       </c>
       <c r="F2" s="98"/>
     </row>
@@ -9156,7 +9387,7 @@
         <v>12</v>
       </c>
       <c r="E3" s="37" t="s">
-        <v>1366</v>
+        <v>1364</v>
       </c>
       <c r="F3" s="5" t="s">
         <v>13</v>
@@ -9221,7 +9452,7 @@
     <row r="7" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="5"/>
       <c r="B7" s="5" t="s">
-        <v>1461</v>
+        <v>1459</v>
       </c>
       <c r="C7" s="6" t="s">
         <v>349</v>
@@ -10021,10 +10252,10 @@
     <row r="53" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A53" s="86"/>
       <c r="B53" s="163" t="s">
-        <v>1413</v>
+        <v>1411</v>
       </c>
       <c r="C53" s="164" t="s">
-        <v>1414</v>
+        <v>1412</v>
       </c>
       <c r="D53" s="86"/>
       <c r="E53" s="165" t="s">
@@ -10140,7 +10371,7 @@
       </c>
       <c r="D61" s="86"/>
       <c r="E61" s="165" t="s">
-        <v>1429</v>
+        <v>1427</v>
       </c>
       <c r="F61" s="86"/>
     </row>
@@ -10227,46 +10458,46 @@
     <row r="68" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A68" s="86"/>
       <c r="B68" s="163" t="s">
-        <v>1417</v>
+        <v>1415</v>
       </c>
       <c r="C68" s="164" t="s">
-        <v>1418</v>
+        <v>1416</v>
       </c>
       <c r="D68" s="86"/>
       <c r="E68" s="165" t="s">
-        <v>1419</v>
+        <v>1417</v>
       </c>
       <c r="F68" s="166" t="s">
-        <v>1420</v>
+        <v>1418</v>
       </c>
     </row>
     <row r="69" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A69" s="86"/>
       <c r="B69" s="163" t="s">
-        <v>1415</v>
+        <v>1413</v>
       </c>
       <c r="C69" s="164" t="s">
-        <v>1298</v>
+        <v>1297</v>
       </c>
       <c r="D69" s="86"/>
       <c r="E69" s="165" t="s">
-        <v>1416</v>
+        <v>1414</v>
       </c>
     </row>
     <row r="70" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="B70" s="1" t="s">
-        <v>1317</v>
+        <v>1315</v>
       </c>
       <c r="C70" s="2" t="s">
+        <v>1316</v>
+      </c>
+      <c r="E70" s="40" t="s">
         <v>1318</v>
-      </c>
-      <c r="E70" s="40" t="s">
-        <v>1320</v>
       </c>
     </row>
     <row r="71" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="B71" s="1" t="s">
-        <v>1319</v>
+        <v>1317</v>
       </c>
       <c r="C71" s="2" t="s">
         <v>76</v>
@@ -10277,13 +10508,13 @@
     </row>
     <row r="72" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="B72" s="1" t="s">
+        <v>1428</v>
+      </c>
+      <c r="C72" s="2" t="s">
+        <v>1429</v>
+      </c>
+      <c r="E72" s="40" t="s">
         <v>1430</v>
-      </c>
-      <c r="C72" s="2" t="s">
-        <v>1431</v>
-      </c>
-      <c r="E72" s="40" t="s">
-        <v>1432</v>
       </c>
     </row>
   </sheetData>
@@ -10578,14 +10809,14 @@
         <v>239</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>1342</v>
+        <v>1340</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>1343</v>
+        <v>1341</v>
       </c>
       <c r="D2" s="5"/>
       <c r="E2" s="43" t="s">
-        <v>1351</v>
+        <v>1349</v>
       </c>
       <c r="F2" s="1"/>
     </row>
@@ -10594,38 +10825,38 @@
         <v>480</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>1344</v>
+        <v>1342</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>1345</v>
+        <v>1343</v>
       </c>
       <c r="D3" s="5"/>
       <c r="E3" s="43" t="s">
-        <v>1352</v>
+        <v>1350</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" s="183" t="s">
-        <v>1346</v>
-      </c>
-      <c r="B4" s="184"/>
-      <c r="C4" s="184"/>
-      <c r="D4" s="184"/>
-      <c r="E4" s="185"/>
+      <c r="A4" s="186" t="s">
+        <v>1344</v>
+      </c>
+      <c r="B4" s="187"/>
+      <c r="C4" s="187"/>
+      <c r="D4" s="187"/>
+      <c r="E4" s="188"/>
     </row>
     <row r="5" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
         <v>239</v>
       </c>
       <c r="B5" s="5" t="s">
+        <v>1345</v>
+      </c>
+      <c r="C5" s="6" t="s">
         <v>1347</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>1349</v>
       </c>
       <c r="D5" s="5"/>
       <c r="E5" s="43" t="s">
-        <v>1353</v>
+        <v>1351</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="96" x14ac:dyDescent="0.2">
@@ -10633,68 +10864,68 @@
         <v>480</v>
       </c>
       <c r="B6" s="5" t="s">
+        <v>1346</v>
+      </c>
+      <c r="C6" s="6" t="s">
         <v>1348</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>1350</v>
       </c>
       <c r="D6" s="5"/>
       <c r="E6" s="43" t="s">
-        <v>1354</v>
+        <v>1352</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7" s="183" t="s">
-        <v>1493</v>
-      </c>
-      <c r="B7" s="184"/>
-      <c r="C7" s="184"/>
-      <c r="D7" s="184"/>
-      <c r="E7" s="185"/>
+      <c r="A7" s="186" t="s">
+        <v>1491</v>
+      </c>
+      <c r="B7" s="187"/>
+      <c r="C7" s="187"/>
+      <c r="D7" s="187"/>
+      <c r="E7" s="188"/>
     </row>
     <row r="8" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
         <v>239</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>1495</v>
+        <v>1493</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>1496</v>
+        <v>1494</v>
       </c>
       <c r="D8" s="5"/>
       <c r="E8" s="43" t="s">
-        <v>1503</v>
+        <v>1501</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
+        <v>1495</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>1496</v>
+      </c>
+      <c r="C9" s="6" t="s">
         <v>1497</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>1498</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>1499</v>
       </c>
       <c r="D9" s="5"/>
       <c r="E9" s="43" t="s">
-        <v>1504</v>
+        <v>1502</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
+        <v>1498</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>1499</v>
+      </c>
+      <c r="C10" s="6" t="s">
         <v>1500</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>1501</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>1502</v>
       </c>
       <c r="D10" s="5"/>
       <c r="E10" s="43" t="s">
-        <v>1505</v>
+        <v>1503</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="16" x14ac:dyDescent="0.2">
@@ -10702,14 +10933,14 @@
         <v>239</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>1494</v>
+        <v>1492</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>1506</v>
+        <v>1504</v>
       </c>
       <c r="D11" s="5"/>
       <c r="E11" s="43" t="s">
-        <v>1509</v>
+        <v>1507</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="16" x14ac:dyDescent="0.2">
@@ -10717,14 +10948,14 @@
         <v>480</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>1507</v>
+        <v>1505</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>1508</v>
+        <v>1506</v>
       </c>
       <c r="D12" s="5"/>
       <c r="E12" s="43" t="s">
-        <v>1510</v>
+        <v>1508</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
@@ -10904,7 +11135,7 @@
         <v>239</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>1357</v>
+        <v>1355</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>272</v>
@@ -10928,7 +11159,7 @@
         <v>242</v>
       </c>
       <c r="E4" s="43" t="s">
-        <v>1358</v>
+        <v>1356</v>
       </c>
       <c r="F4" s="68" t="s">
         <v>276</v>
@@ -10942,13 +11173,13 @@
         <v>277</v>
       </c>
       <c r="C5" s="52" t="s">
-        <v>1409</v>
+        <v>1407</v>
       </c>
       <c r="D5" s="66" t="s">
         <v>278</v>
       </c>
       <c r="E5" s="156" t="s">
-        <v>1427</v>
+        <v>1425</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>279</v>
@@ -10962,13 +11193,13 @@
         <v>280</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>1361</v>
+        <v>1359</v>
       </c>
       <c r="D6" s="67" t="s">
         <v>281</v>
       </c>
       <c r="E6" s="157" t="s">
-        <v>1428</v>
+        <v>1426</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="160" x14ac:dyDescent="0.2">
@@ -10979,13 +11210,13 @@
         <v>282</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>1362</v>
+        <v>1360</v>
       </c>
       <c r="D7" s="67" t="s">
         <v>283</v>
       </c>
       <c r="E7" s="157" t="s">
-        <v>1363</v>
+        <v>1361</v>
       </c>
       <c r="F7" s="68" t="s">
         <v>284</v>
@@ -11187,7 +11418,7 @@
         <v>332</v>
       </c>
       <c r="C19" s="64" t="s">
-        <v>1355</v>
+        <v>1353</v>
       </c>
       <c r="D19" s="7" t="s">
         <v>333</v>
@@ -11321,17 +11552,17 @@
     </row>
     <row r="27" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A27" s="5" t="s">
-        <v>1359</v>
+        <v>1357</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>1360</v>
+        <v>1358</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>1511</v>
+        <v>1509</v>
       </c>
       <c r="D27" s="5"/>
       <c r="E27" s="37" t="s">
-        <v>1512</v>
+        <v>1510</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
@@ -11408,13 +11639,13 @@
       </c>
     </row>
     <row r="2" spans="1:6" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="186" t="s">
+      <c r="A2" s="192" t="s">
         <v>363</v>
       </c>
-      <c r="B2" s="187"/>
-      <c r="C2" s="187"/>
-      <c r="D2" s="187"/>
-      <c r="E2" s="188"/>
+      <c r="B2" s="193"/>
+      <c r="C2" s="193"/>
+      <c r="D2" s="193"/>
+      <c r="E2" s="194"/>
       <c r="F2" s="33"/>
     </row>
     <row r="3" spans="1:6" ht="48" x14ac:dyDescent="0.2">
@@ -11512,14 +11743,14 @@
         <v>378</v>
       </c>
       <c r="B8" s="119" t="s">
-        <v>1490</v>
+        <v>1488</v>
       </c>
       <c r="C8" s="117" t="s">
-        <v>1491</v>
+        <v>1489</v>
       </c>
       <c r="D8" s="121"/>
       <c r="E8" s="120" t="s">
-        <v>1492</v>
+        <v>1490</v>
       </c>
       <c r="F8" s="119"/>
     </row>
@@ -11558,13 +11789,13 @@
       <c r="F10" s="119"/>
     </row>
     <row r="11" spans="1:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="189" t="s">
+      <c r="A11" s="195" t="s">
         <v>392</v>
       </c>
-      <c r="B11" s="190"/>
-      <c r="C11" s="190"/>
-      <c r="D11" s="190"/>
-      <c r="E11" s="191"/>
+      <c r="B11" s="196"/>
+      <c r="C11" s="196"/>
+      <c r="D11" s="196"/>
+      <c r="E11" s="197"/>
       <c r="F11" s="119"/>
     </row>
     <row r="12" spans="1:6" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -11593,13 +11824,13 @@
         <v>397</v>
       </c>
       <c r="C13" s="153" t="s">
-        <v>1321</v>
+        <v>1319</v>
       </c>
       <c r="D13" s="84" t="s">
         <v>398</v>
       </c>
       <c r="E13" s="152" t="s">
-        <v>1322</v>
+        <v>1320</v>
       </c>
       <c r="F13" s="86"/>
     </row>
@@ -11611,24 +11842,24 @@
         <v>399</v>
       </c>
       <c r="C14" s="154" t="s">
-        <v>1323</v>
+        <v>1321</v>
       </c>
       <c r="D14" s="88" t="s">
         <v>400</v>
       </c>
       <c r="E14" s="155" t="s">
-        <v>1324</v>
+        <v>1322</v>
       </c>
       <c r="F14" s="86"/>
     </row>
     <row r="15" spans="1:6" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="183" t="s">
+      <c r="A15" s="186" t="s">
         <v>401</v>
       </c>
-      <c r="B15" s="184"/>
-      <c r="C15" s="184"/>
-      <c r="D15" s="184"/>
-      <c r="E15" s="185"/>
+      <c r="B15" s="187"/>
+      <c r="C15" s="187"/>
+      <c r="D15" s="187"/>
+      <c r="E15" s="188"/>
       <c r="F15" s="119"/>
     </row>
     <row r="16" spans="1:6" ht="48" x14ac:dyDescent="0.2">
@@ -11772,13 +12003,13 @@
       <c r="F24" s="119"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A25" s="183" t="s">
-        <v>1458</v>
-      </c>
-      <c r="B25" s="184"/>
-      <c r="C25" s="184"/>
-      <c r="D25" s="184"/>
-      <c r="E25" s="185"/>
+      <c r="A25" s="186" t="s">
+        <v>1456</v>
+      </c>
+      <c r="B25" s="187"/>
+      <c r="C25" s="187"/>
+      <c r="D25" s="187"/>
+      <c r="E25" s="188"/>
       <c r="F25" s="119"/>
     </row>
     <row r="26" spans="1:6" ht="32" x14ac:dyDescent="0.2">
@@ -11786,10 +12017,10 @@
         <v>239</v>
       </c>
       <c r="B26" s="132" t="s">
-        <v>1459</v>
+        <v>1457</v>
       </c>
       <c r="C26" s="133" t="s">
-        <v>1460</v>
+        <v>1458</v>
       </c>
       <c r="D26" s="114"/>
       <c r="E26" s="131"/>
@@ -11800,14 +12031,14 @@
         <v>373</v>
       </c>
       <c r="B27" s="132" t="s">
-        <v>1462</v>
+        <v>1460</v>
       </c>
       <c r="C27" s="133" t="s">
-        <v>1470</v>
+        <v>1468</v>
       </c>
       <c r="D27" s="114"/>
       <c r="E27" s="131" t="s">
-        <v>1471</v>
+        <v>1469</v>
       </c>
       <c r="F27" s="119"/>
     </row>
@@ -11816,41 +12047,41 @@
         <v>373</v>
       </c>
       <c r="B28" s="132" t="s">
-        <v>1464</v>
+        <v>1462</v>
       </c>
       <c r="C28" s="133" t="s">
-        <v>1463</v>
+        <v>1461</v>
       </c>
       <c r="D28" s="114"/>
       <c r="E28" s="131" t="s">
-        <v>1465</v>
+        <v>1463</v>
       </c>
       <c r="F28" s="119"/>
     </row>
     <row r="29" spans="1:6" s="178" customFormat="1" ht="96" x14ac:dyDescent="0.2">
       <c r="A29" s="172" t="s">
-        <v>1469</v>
+        <v>1467</v>
       </c>
       <c r="B29" s="173" t="s">
-        <v>1466</v>
+        <v>1464</v>
       </c>
       <c r="C29" s="174" t="s">
-        <v>1467</v>
+        <v>1465</v>
       </c>
       <c r="D29" s="175"/>
       <c r="E29" s="176" t="s">
-        <v>1468</v>
+        <v>1466</v>
       </c>
       <c r="F29" s="177"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A30" s="183" t="s">
+      <c r="A30" s="186" t="s">
         <v>431</v>
       </c>
-      <c r="B30" s="184"/>
-      <c r="C30" s="184"/>
-      <c r="D30" s="184"/>
-      <c r="E30" s="185"/>
+      <c r="B30" s="187"/>
+      <c r="C30" s="187"/>
+      <c r="D30" s="187"/>
+      <c r="E30" s="188"/>
       <c r="F30" s="119"/>
     </row>
     <row r="31" spans="1:6" ht="32" x14ac:dyDescent="0.2">
@@ -12122,13 +12353,13 @@
       <c r="F48" s="119"/>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A49" s="183" t="s">
+      <c r="A49" s="186" t="s">
         <v>475</v>
       </c>
-      <c r="B49" s="184"/>
-      <c r="C49" s="184"/>
-      <c r="D49" s="184"/>
-      <c r="E49" s="185"/>
+      <c r="B49" s="187"/>
+      <c r="C49" s="187"/>
+      <c r="D49" s="187"/>
+      <c r="E49" s="188"/>
       <c r="F49" s="119"/>
     </row>
     <row r="50" spans="1:6" ht="32" x14ac:dyDescent="0.2">
@@ -12154,14 +12385,14 @@
         <v>480</v>
       </c>
       <c r="B51" s="116" t="s">
-        <v>1341</v>
+        <v>1339</v>
       </c>
       <c r="C51" s="59" t="s">
-        <v>1435</v>
+        <v>1433</v>
       </c>
       <c r="D51" s="116"/>
       <c r="E51" s="120" t="s">
-        <v>1436</v>
+        <v>1434</v>
       </c>
       <c r="F51" s="119"/>
     </row>
@@ -12170,10 +12401,10 @@
         <v>480</v>
       </c>
       <c r="B52" s="116" t="s">
-        <v>1434</v>
+        <v>1432</v>
       </c>
       <c r="C52" s="59" t="s">
-        <v>1340</v>
+        <v>1338</v>
       </c>
       <c r="D52" s="116"/>
       <c r="E52" s="120" t="s">
@@ -12189,11 +12420,11 @@
         <v>481</v>
       </c>
       <c r="C53" s="59" t="s">
-        <v>1433</v>
+        <v>1431</v>
       </c>
       <c r="D53" s="116"/>
       <c r="E53" s="120" t="s">
-        <v>1439</v>
+        <v>1437</v>
       </c>
       <c r="F53" s="119"/>
     </row>
@@ -12362,13 +12593,13 @@
       <c r="F64" s="119"/>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A65" s="183" t="s">
+      <c r="A65" s="186" t="s">
         <v>505</v>
       </c>
-      <c r="B65" s="184"/>
-      <c r="C65" s="184"/>
-      <c r="D65" s="184"/>
-      <c r="E65" s="185"/>
+      <c r="B65" s="187"/>
+      <c r="C65" s="187"/>
+      <c r="D65" s="187"/>
+      <c r="E65" s="188"/>
       <c r="F65" s="119"/>
     </row>
     <row r="66" spans="1:6" ht="64" x14ac:dyDescent="0.2">
@@ -12397,13 +12628,13 @@
         <v>511</v>
       </c>
       <c r="C67" s="117" t="s">
-        <v>1437</v>
+        <v>1435</v>
       </c>
       <c r="D67" s="116" t="s">
         <v>512</v>
       </c>
       <c r="E67" s="120" t="s">
-        <v>1438</v>
+        <v>1436</v>
       </c>
       <c r="F67" s="119"/>
     </row>
@@ -12421,7 +12652,7 @@
         <v>516</v>
       </c>
       <c r="E68" s="120" t="s">
-        <v>1333</v>
+        <v>1331</v>
       </c>
       <c r="F68" s="119"/>
     </row>
@@ -12430,25 +12661,25 @@
         <v>513</v>
       </c>
       <c r="B69" s="116" t="s">
+        <v>1328</v>
+      </c>
+      <c r="C69" s="117" t="s">
         <v>1330</v>
-      </c>
-      <c r="C69" s="117" t="s">
-        <v>1332</v>
       </c>
       <c r="D69" s="116"/>
       <c r="E69" s="120" t="s">
-        <v>1331</v>
+        <v>1329</v>
       </c>
       <c r="F69" s="119"/>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A70" s="183" t="s">
+      <c r="A70" s="186" t="s">
         <v>517</v>
       </c>
-      <c r="B70" s="184"/>
-      <c r="C70" s="184"/>
-      <c r="D70" s="184"/>
-      <c r="E70" s="185"/>
+      <c r="B70" s="187"/>
+      <c r="C70" s="187"/>
+      <c r="D70" s="187"/>
+      <c r="E70" s="188"/>
       <c r="F70" s="119"/>
     </row>
     <row r="71" spans="1:6" ht="48" x14ac:dyDescent="0.2">
@@ -12498,13 +12729,13 @@
       <c r="F73" s="119"/>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A74" s="183" t="s">
+      <c r="A74" s="186" t="s">
         <v>522</v>
       </c>
-      <c r="B74" s="184"/>
-      <c r="C74" s="184"/>
-      <c r="D74" s="184"/>
-      <c r="E74" s="185"/>
+      <c r="B74" s="187"/>
+      <c r="C74" s="187"/>
+      <c r="D74" s="187"/>
+      <c r="E74" s="188"/>
       <c r="F74" s="119"/>
     </row>
     <row r="75" spans="1:6" ht="32" x14ac:dyDescent="0.2">
@@ -12530,14 +12761,14 @@
         <v>480</v>
       </c>
       <c r="B76" s="125" t="s">
-        <v>1440</v>
+        <v>1438</v>
       </c>
       <c r="C76" s="167" t="s">
-        <v>1441</v>
+        <v>1439</v>
       </c>
       <c r="D76" s="125"/>
       <c r="E76" s="131" t="s">
-        <v>1442</v>
+        <v>1440</v>
       </c>
       <c r="F76" s="119"/>
     </row>
@@ -12657,13 +12888,13 @@
         <v>546</v>
       </c>
       <c r="C83" s="158" t="s">
-        <v>1453</v>
+        <v>1451</v>
       </c>
       <c r="D83" s="95" t="s">
         <v>400</v>
       </c>
       <c r="E83" s="155" t="s">
-        <v>1454</v>
+        <v>1452</v>
       </c>
       <c r="F83" s="119"/>
     </row>
@@ -12752,13 +12983,13 @@
       <c r="F89" s="119"/>
     </row>
     <row r="90" spans="1:6" ht="62.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A90" s="183" t="s">
+      <c r="A90" s="186" t="s">
         <v>559</v>
       </c>
-      <c r="B90" s="184"/>
-      <c r="C90" s="184"/>
-      <c r="D90" s="184"/>
-      <c r="E90" s="185"/>
+      <c r="B90" s="187"/>
+      <c r="C90" s="187"/>
+      <c r="D90" s="187"/>
+      <c r="E90" s="188"/>
       <c r="F90" s="119"/>
     </row>
     <row r="91" spans="1:6" ht="62.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -12789,11 +13020,11 @@
         <v>564</v>
       </c>
       <c r="C92" s="117" t="s">
-        <v>1378</v>
+        <v>1376</v>
       </c>
       <c r="D92" s="116"/>
       <c r="E92" s="120" t="s">
-        <v>1379</v>
+        <v>1377</v>
       </c>
       <c r="F92" s="119"/>
     </row>
@@ -12901,22 +13132,22 @@
         <v>583</v>
       </c>
       <c r="C99" s="117" t="s">
-        <v>1376</v>
+        <v>1374</v>
       </c>
       <c r="D99" s="116"/>
       <c r="E99" s="120" t="s">
-        <v>1377</v>
+        <v>1375</v>
       </c>
       <c r="F99" s="119"/>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A100" s="183" t="s">
+      <c r="A100" s="186" t="s">
         <v>584</v>
       </c>
-      <c r="B100" s="184"/>
-      <c r="C100" s="184"/>
-      <c r="D100" s="184"/>
-      <c r="E100" s="185"/>
+      <c r="B100" s="187"/>
+      <c r="C100" s="187"/>
+      <c r="D100" s="187"/>
+      <c r="E100" s="188"/>
       <c r="F100" s="119"/>
     </row>
     <row r="101" spans="1:6" ht="62.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -12947,11 +13178,11 @@
         <v>589</v>
       </c>
       <c r="C102" s="117" t="s">
-        <v>1394</v>
+        <v>1392</v>
       </c>
       <c r="D102" s="116"/>
       <c r="E102" s="120" t="s">
-        <v>1395</v>
+        <v>1393</v>
       </c>
       <c r="F102" s="86" t="s">
         <v>592</v>
@@ -12980,7 +13211,7 @@
         <v>84</v>
       </c>
       <c r="B104" s="159" t="s">
-        <v>1400</v>
+        <v>1398</v>
       </c>
       <c r="C104" s="93" t="s">
         <v>591</v>
@@ -12998,7 +13229,7 @@
         <v>84</v>
       </c>
       <c r="B105" s="159" t="s">
-        <v>1401</v>
+        <v>1399</v>
       </c>
       <c r="C105" s="93" t="s">
         <v>591</v>
@@ -13016,7 +13247,7 @@
         <v>84</v>
       </c>
       <c r="B106" s="160" t="s">
-        <v>1402</v>
+        <v>1400</v>
       </c>
       <c r="C106" s="161" t="s">
         <v>591</v>
@@ -13032,7 +13263,7 @@
         <v>84</v>
       </c>
       <c r="B107" s="160" t="s">
-        <v>1403</v>
+        <v>1401</v>
       </c>
       <c r="C107" s="161" t="s">
         <v>591</v>
@@ -13048,7 +13279,7 @@
         <v>84</v>
       </c>
       <c r="B108" s="160" t="s">
-        <v>1404</v>
+        <v>1402</v>
       </c>
       <c r="C108" s="161" t="s">
         <v>591</v>
@@ -13468,13 +13699,13 @@
       <c r="F135" s="119"/>
     </row>
     <row r="136" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A136" s="183" t="s">
+      <c r="A136" s="186" t="s">
         <v>670</v>
       </c>
-      <c r="B136" s="184"/>
-      <c r="C136" s="184"/>
-      <c r="D136" s="184"/>
-      <c r="E136" s="185"/>
+      <c r="B136" s="187"/>
+      <c r="C136" s="187"/>
+      <c r="D136" s="187"/>
+      <c r="E136" s="188"/>
       <c r="F136" s="119"/>
     </row>
     <row r="137" spans="1:6" ht="32" x14ac:dyDescent="0.2">
@@ -13497,33 +13728,33 @@
     </row>
     <row r="138" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A138" s="116" t="s">
+        <v>1441</v>
+      </c>
+      <c r="B138" s="116" t="s">
         <v>1443</v>
       </c>
-      <c r="B138" s="116" t="s">
-        <v>1445</v>
-      </c>
       <c r="C138" s="117" t="s">
-        <v>1444</v>
+        <v>1442</v>
       </c>
       <c r="D138" s="116"/>
       <c r="E138" s="120" t="s">
-        <v>1448</v>
+        <v>1446</v>
       </c>
       <c r="F138" s="119"/>
     </row>
     <row r="139" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A139" s="116" t="s">
-        <v>1443</v>
+        <v>1441</v>
       </c>
       <c r="B139" s="116" t="s">
-        <v>1447</v>
+        <v>1445</v>
       </c>
       <c r="C139" s="117" t="s">
-        <v>1446</v>
+        <v>1444</v>
       </c>
       <c r="D139" s="116"/>
       <c r="E139" s="120" t="s">
-        <v>1449</v>
+        <v>1447</v>
       </c>
       <c r="F139" s="119"/>
     </row>
@@ -13694,13 +13925,13 @@
       <c r="F151" s="119"/>
     </row>
     <row r="152" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A152" s="183" t="s">
+      <c r="A152" s="186" t="s">
         <v>692</v>
       </c>
-      <c r="B152" s="184"/>
-      <c r="C152" s="184"/>
-      <c r="D152" s="184"/>
-      <c r="E152" s="185"/>
+      <c r="B152" s="187"/>
+      <c r="C152" s="187"/>
+      <c r="D152" s="187"/>
+      <c r="E152" s="188"/>
       <c r="F152" s="119"/>
     </row>
     <row r="153" spans="1:6" ht="64" x14ac:dyDescent="0.2">
@@ -13759,7 +13990,7 @@
         <v>699</v>
       </c>
       <c r="C156" s="113" t="s">
-        <v>1308</v>
+        <v>1306</v>
       </c>
       <c r="D156" s="122" t="s">
         <v>700</v>
@@ -13830,13 +14061,13 @@
       <c r="F160" s="119"/>
     </row>
     <row r="161" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A161" s="183" t="s">
+      <c r="A161" s="186" t="s">
         <v>713</v>
       </c>
-      <c r="B161" s="184"/>
-      <c r="C161" s="184"/>
-      <c r="D161" s="184"/>
-      <c r="E161" s="185"/>
+      <c r="B161" s="187"/>
+      <c r="C161" s="187"/>
+      <c r="D161" s="187"/>
+      <c r="E161" s="188"/>
       <c r="F161" s="119"/>
     </row>
     <row r="162" spans="1:6" ht="32" x14ac:dyDescent="0.2">
@@ -13847,7 +14078,7 @@
         <v>714</v>
       </c>
       <c r="C162" s="59" t="s">
-        <v>1307</v>
+        <v>1305</v>
       </c>
       <c r="D162" s="116" t="s">
         <v>715</v>
@@ -13878,14 +14109,14 @@
         <v>37</v>
       </c>
       <c r="B164" s="116" t="s">
+        <v>1307</v>
+      </c>
+      <c r="C164" s="59" t="s">
         <v>1309</v>
-      </c>
-      <c r="C164" s="59" t="s">
-        <v>1311</v>
       </c>
       <c r="D164" s="116"/>
       <c r="E164" s="120" t="s">
-        <v>1313</v>
+        <v>1311</v>
       </c>
       <c r="F164" s="119"/>
     </row>
@@ -13894,14 +14125,14 @@
         <v>37</v>
       </c>
       <c r="B165" s="116" t="s">
+        <v>1308</v>
+      </c>
+      <c r="C165" s="59" t="s">
         <v>1310</v>
-      </c>
-      <c r="C165" s="59" t="s">
-        <v>1312</v>
       </c>
       <c r="D165" s="116"/>
       <c r="E165" s="120" t="s">
-        <v>1314</v>
+        <v>1312</v>
       </c>
       <c r="F165" s="119"/>
     </row>
@@ -13996,13 +14227,13 @@
       <c r="F171" s="119"/>
     </row>
     <row r="172" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A172" s="183" t="s">
+      <c r="A172" s="186" t="s">
         <v>734</v>
       </c>
-      <c r="B172" s="184"/>
-      <c r="C172" s="184"/>
-      <c r="D172" s="184"/>
-      <c r="E172" s="185"/>
+      <c r="B172" s="187"/>
+      <c r="C172" s="187"/>
+      <c r="D172" s="187"/>
+      <c r="E172" s="188"/>
       <c r="F172" s="119"/>
     </row>
     <row r="173" spans="1:6" ht="48" x14ac:dyDescent="0.2">
@@ -14122,13 +14353,13 @@
       </c>
     </row>
     <row r="180" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A180" s="192" t="s">
+      <c r="A180" s="189" t="s">
         <v>754</v>
       </c>
-      <c r="B180" s="193"/>
-      <c r="C180" s="193"/>
-      <c r="D180" s="193"/>
-      <c r="E180" s="194"/>
+      <c r="B180" s="190"/>
+      <c r="C180" s="190"/>
+      <c r="D180" s="190"/>
+      <c r="E180" s="191"/>
       <c r="F180" s="129" t="s">
         <v>758</v>
       </c>
@@ -14145,7 +14376,7 @@
       </c>
       <c r="D181" s="114"/>
       <c r="E181" s="131" t="s">
-        <v>1479</v>
+        <v>1477</v>
       </c>
       <c r="F181" s="129" t="s">
         <v>758</v>
@@ -14156,14 +14387,14 @@
         <v>239</v>
       </c>
       <c r="B182" s="116" t="s">
-        <v>1513</v>
+        <v>1511</v>
       </c>
       <c r="C182" s="130" t="s">
-        <v>1514</v>
+        <v>1512</v>
       </c>
       <c r="D182" s="114"/>
       <c r="E182" s="131" t="s">
-        <v>1515</v>
+        <v>1513</v>
       </c>
       <c r="F182" s="129" t="s">
         <v>758</v>
@@ -14181,7 +14412,7 @@
       </c>
       <c r="D183" s="114"/>
       <c r="E183" s="131" t="s">
-        <v>1480</v>
+        <v>1478</v>
       </c>
       <c r="F183" s="129" t="s">
         <v>758</v>
@@ -14213,7 +14444,7 @@
       </c>
       <c r="D185" s="114"/>
       <c r="E185" s="131" t="s">
-        <v>1481</v>
+        <v>1479</v>
       </c>
       <c r="F185" s="129" t="s">
         <v>758</v>
@@ -14231,7 +14462,7 @@
       </c>
       <c r="D186" s="114"/>
       <c r="E186" s="131" t="s">
-        <v>1482</v>
+        <v>1480</v>
       </c>
       <c r="F186" s="129" t="s">
         <v>758</v>
@@ -14278,13 +14509,13 @@
       <c r="F189" s="119"/>
     </row>
     <row r="190" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A190" s="183" t="s">
-        <v>1472</v>
-      </c>
-      <c r="B190" s="184"/>
-      <c r="C190" s="184"/>
-      <c r="D190" s="184"/>
-      <c r="E190" s="185"/>
+      <c r="A190" s="186" t="s">
+        <v>1470</v>
+      </c>
+      <c r="B190" s="187"/>
+      <c r="C190" s="187"/>
+      <c r="D190" s="187"/>
+      <c r="E190" s="188"/>
       <c r="F190" s="119"/>
     </row>
     <row r="191" spans="1:6" ht="16" x14ac:dyDescent="0.2">
@@ -14292,29 +14523,29 @@
         <v>239</v>
       </c>
       <c r="B191" s="132" t="s">
-        <v>1473</v>
+        <v>1471</v>
       </c>
       <c r="C191" s="133" t="s">
-        <v>1472</v>
+        <v>1470</v>
       </c>
       <c r="D191" s="114"/>
       <c r="E191" s="131" t="s">
-        <v>1476</v>
+        <v>1474</v>
       </c>
       <c r="F191" s="119"/>
     </row>
     <row r="192" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A192" s="1" t="s">
-        <v>1478</v>
+        <v>1476</v>
       </c>
       <c r="B192" s="1" t="s">
-        <v>1474</v>
+        <v>1472</v>
       </c>
       <c r="C192" s="2" t="s">
+        <v>1473</v>
+      </c>
+      <c r="E192" s="40" t="s">
         <v>1475</v>
-      </c>
-      <c r="E192" s="40" t="s">
-        <v>1477</v>
       </c>
     </row>
     <row r="193" spans="1:6" ht="48" x14ac:dyDescent="0.2">
@@ -14322,23 +14553,23 @@
         <v>257</v>
       </c>
       <c r="B193" s="1" t="s">
+        <v>1481</v>
+      </c>
+      <c r="C193" s="2" t="s">
+        <v>1482</v>
+      </c>
+      <c r="E193" s="40" t="s">
         <v>1483</v>
       </c>
-      <c r="C193" s="2" t="s">
-        <v>1484</v>
-      </c>
-      <c r="E193" s="40" t="s">
-        <v>1485</v>
-      </c>
     </row>
     <row r="194" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A194" s="183" t="s">
+      <c r="A194" s="186" t="s">
         <v>765</v>
       </c>
-      <c r="B194" s="184"/>
-      <c r="C194" s="184"/>
-      <c r="D194" s="184"/>
-      <c r="E194" s="185"/>
+      <c r="B194" s="187"/>
+      <c r="C194" s="187"/>
+      <c r="D194" s="187"/>
+      <c r="E194" s="188"/>
       <c r="F194" s="119"/>
     </row>
     <row r="195" spans="1:6" ht="32" x14ac:dyDescent="0.2">
@@ -14385,13 +14616,13 @@
         <v>771</v>
       </c>
       <c r="C197" s="158" t="s">
-        <v>1516</v>
+        <v>1514</v>
       </c>
       <c r="D197" s="95" t="s">
         <v>400</v>
       </c>
       <c r="E197" s="155" t="s">
-        <v>1519</v>
+        <v>1517</v>
       </c>
       <c r="F197" s="119"/>
     </row>
@@ -14403,13 +14634,13 @@
         <v>772</v>
       </c>
       <c r="C198" s="158" t="s">
-        <v>1517</v>
+        <v>1515</v>
       </c>
       <c r="D198" s="95" t="s">
         <v>400</v>
       </c>
       <c r="E198" s="155" t="s">
-        <v>1520</v>
+        <v>1518</v>
       </c>
       <c r="F198" s="119"/>
     </row>
@@ -14421,13 +14652,13 @@
         <v>773</v>
       </c>
       <c r="C199" s="158" t="s">
-        <v>1518</v>
+        <v>1516</v>
       </c>
       <c r="D199" s="95" t="s">
         <v>400</v>
       </c>
       <c r="E199" s="155" t="s">
-        <v>1521</v>
+        <v>1519</v>
       </c>
       <c r="F199" s="119"/>
     </row>
@@ -14469,17 +14700,17 @@
     </row>
     <row r="202" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A202" s="180" t="s">
-        <v>1443</v>
+        <v>1441</v>
       </c>
       <c r="B202" s="179" t="s">
-        <v>1522</v>
+        <v>1520</v>
       </c>
       <c r="C202" s="181" t="s">
-        <v>1523</v>
+        <v>1521</v>
       </c>
       <c r="D202" s="95"/>
       <c r="E202" s="155" t="s">
-        <v>1524</v>
+        <v>1522</v>
       </c>
       <c r="F202" s="119"/>
     </row>
@@ -14540,13 +14771,13 @@
       <c r="F206" s="119"/>
     </row>
     <row r="207" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A207" s="183" t="s">
+      <c r="A207" s="186" t="s">
         <v>786</v>
       </c>
-      <c r="B207" s="184"/>
-      <c r="C207" s="184"/>
-      <c r="D207" s="184"/>
-      <c r="E207" s="185"/>
+      <c r="B207" s="187"/>
+      <c r="C207" s="187"/>
+      <c r="D207" s="187"/>
+      <c r="E207" s="188"/>
       <c r="F207" s="119"/>
     </row>
     <row r="208" spans="1:6" ht="32" x14ac:dyDescent="0.2">
@@ -14596,13 +14827,13 @@
       <c r="F210" s="119"/>
     </row>
     <row r="211" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A211" s="183" t="s">
+      <c r="A211" s="186" t="s">
         <v>794</v>
       </c>
-      <c r="B211" s="184"/>
-      <c r="C211" s="184"/>
-      <c r="D211" s="184"/>
-      <c r="E211" s="185"/>
+      <c r="B211" s="187"/>
+      <c r="C211" s="187"/>
+      <c r="D211" s="187"/>
+      <c r="E211" s="188"/>
       <c r="F211" s="119"/>
     </row>
     <row r="212" spans="1:6" ht="64" x14ac:dyDescent="0.2">
@@ -14628,14 +14859,14 @@
         <v>480</v>
       </c>
       <c r="B213" s="116" t="s">
-        <v>1526</v>
+        <v>1523</v>
       </c>
       <c r="C213" s="117" t="s">
-        <v>1527</v>
+        <v>1524</v>
       </c>
       <c r="D213" s="116"/>
       <c r="E213" s="120" t="s">
-        <v>1528</v>
+        <v>1525</v>
       </c>
       <c r="F213" s="119"/>
     </row>
@@ -14665,13 +14896,13 @@
         <v>803</v>
       </c>
       <c r="C215" s="59" t="s">
-        <v>1325</v>
+        <v>1323</v>
       </c>
       <c r="D215" s="116" t="s">
         <v>804</v>
       </c>
       <c r="E215" s="120" t="s">
-        <v>1329</v>
+        <v>1327</v>
       </c>
       <c r="F215" s="119"/>
     </row>
@@ -14680,14 +14911,14 @@
         <v>480</v>
       </c>
       <c r="B216" s="116" t="s">
-        <v>1326</v>
+        <v>1324</v>
       </c>
       <c r="C216" s="59" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="D216" s="116"/>
       <c r="E216" s="120" t="s">
-        <v>1328</v>
+        <v>1326</v>
       </c>
       <c r="F216" s="119"/>
     </row>
@@ -14720,13 +14951,13 @@
       <c r="F218" s="119"/>
     </row>
     <row r="219" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A219" s="183" t="s">
+      <c r="A219" s="186" t="s">
         <v>809</v>
       </c>
-      <c r="B219" s="184"/>
-      <c r="C219" s="184"/>
-      <c r="D219" s="184"/>
-      <c r="E219" s="185"/>
+      <c r="B219" s="187"/>
+      <c r="C219" s="187"/>
+      <c r="D219" s="187"/>
+      <c r="E219" s="188"/>
       <c r="F219" s="119"/>
     </row>
     <row r="220" spans="1:6" ht="32" x14ac:dyDescent="0.2">
@@ -14787,11 +15018,11 @@
         <v>815</v>
       </c>
       <c r="C223" s="117" t="s">
-        <v>1336</v>
+        <v>1334</v>
       </c>
       <c r="D223" s="116"/>
       <c r="E223" s="120" t="s">
-        <v>1339</v>
+        <v>1337</v>
       </c>
       <c r="F223" s="119"/>
     </row>
@@ -14800,7 +15031,7 @@
         <v>723</v>
       </c>
       <c r="B224" s="116" t="s">
-        <v>1338</v>
+        <v>1336</v>
       </c>
       <c r="C224" s="117" t="s">
         <v>43</v>
@@ -14816,14 +15047,14 @@
         <v>32</v>
       </c>
       <c r="B225" s="116" t="s">
-        <v>1337</v>
+        <v>1335</v>
       </c>
       <c r="C225" s="134" t="s">
-        <v>1334</v>
+        <v>1332</v>
       </c>
       <c r="D225" s="116"/>
       <c r="E225" s="120" t="s">
-        <v>1335</v>
+        <v>1333</v>
       </c>
       <c r="F225" s="119"/>
     </row>
@@ -14884,13 +15115,13 @@
       <c r="F229" s="119"/>
     </row>
     <row r="230" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A230" s="183" t="s">
+      <c r="A230" s="186" t="s">
         <v>820</v>
       </c>
-      <c r="B230" s="184"/>
-      <c r="C230" s="184"/>
-      <c r="D230" s="184"/>
-      <c r="E230" s="185"/>
+      <c r="B230" s="187"/>
+      <c r="C230" s="187"/>
+      <c r="D230" s="187"/>
+      <c r="E230" s="188"/>
       <c r="F230" s="119"/>
     </row>
     <row r="231" spans="1:6" ht="48" x14ac:dyDescent="0.2">
@@ -14976,13 +15207,13 @@
       <c r="F235" s="119"/>
     </row>
     <row r="236" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A236" s="183" t="s">
+      <c r="A236" s="186" t="s">
         <v>830</v>
       </c>
-      <c r="B236" s="184"/>
-      <c r="C236" s="184"/>
-      <c r="D236" s="184"/>
-      <c r="E236" s="185"/>
+      <c r="B236" s="187"/>
+      <c r="C236" s="187"/>
+      <c r="D236" s="187"/>
+      <c r="E236" s="188"/>
       <c r="F236" s="119"/>
     </row>
     <row r="237" spans="1:6" ht="32" x14ac:dyDescent="0.2">
@@ -15027,11 +15258,11 @@
         <v>836</v>
       </c>
       <c r="C239" s="117" t="s">
-        <v>1516</v>
+        <v>1514</v>
       </c>
       <c r="D239" s="116"/>
       <c r="E239" s="120" t="s">
-        <v>1519</v>
+        <v>1517</v>
       </c>
       <c r="F239" s="119"/>
     </row>
@@ -15043,11 +15274,11 @@
         <v>837</v>
       </c>
       <c r="C240" s="117" t="s">
-        <v>1517</v>
+        <v>1515</v>
       </c>
       <c r="D240" s="116"/>
       <c r="E240" s="120" t="s">
-        <v>1520</v>
+        <v>1518</v>
       </c>
       <c r="F240" s="119"/>
     </row>
@@ -15059,11 +15290,11 @@
         <v>838</v>
       </c>
       <c r="C241" s="117" t="s">
-        <v>1518</v>
+        <v>1516</v>
       </c>
       <c r="D241" s="116"/>
       <c r="E241" s="120" t="s">
-        <v>1521</v>
+        <v>1519</v>
       </c>
       <c r="F241" s="119"/>
     </row>
@@ -15140,13 +15371,13 @@
       <c r="F246" s="119"/>
     </row>
     <row r="247" spans="1:6" ht="48" x14ac:dyDescent="0.2">
-      <c r="A247" s="183" t="s">
+      <c r="A247" s="186" t="s">
         <v>844</v>
       </c>
-      <c r="B247" s="184"/>
-      <c r="C247" s="184"/>
-      <c r="D247" s="184"/>
-      <c r="E247" s="185"/>
+      <c r="B247" s="187"/>
+      <c r="C247" s="187"/>
+      <c r="D247" s="187"/>
+      <c r="E247" s="188"/>
       <c r="F247" s="38" t="s">
         <v>849</v>
       </c>
@@ -15195,13 +15426,13 @@
         <v>854</v>
       </c>
       <c r="C250" s="59" t="s">
-        <v>1364</v>
+        <v>1362</v>
       </c>
       <c r="D250" s="116" t="s">
         <v>855</v>
       </c>
       <c r="E250" s="120" t="s">
-        <v>1365</v>
+        <v>1363</v>
       </c>
       <c r="F250" s="119"/>
     </row>
@@ -16140,6 +16371,19 @@
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="A247:E247"/>
+    <mergeCell ref="A207:E207"/>
+    <mergeCell ref="A211:E211"/>
+    <mergeCell ref="A219:E219"/>
+    <mergeCell ref="A230:E230"/>
+    <mergeCell ref="A236:E236"/>
+    <mergeCell ref="A65:E65"/>
+    <mergeCell ref="A2:E2"/>
+    <mergeCell ref="A11:E11"/>
+    <mergeCell ref="A15:E15"/>
+    <mergeCell ref="A30:E30"/>
+    <mergeCell ref="A49:E49"/>
+    <mergeCell ref="A25:E25"/>
     <mergeCell ref="A194:E194"/>
     <mergeCell ref="A172:E172"/>
     <mergeCell ref="A70:E70"/>
@@ -16151,19 +16395,6 @@
     <mergeCell ref="A100:E100"/>
     <mergeCell ref="A180:E180"/>
     <mergeCell ref="A190:E190"/>
-    <mergeCell ref="A65:E65"/>
-    <mergeCell ref="A2:E2"/>
-    <mergeCell ref="A11:E11"/>
-    <mergeCell ref="A15:E15"/>
-    <mergeCell ref="A30:E30"/>
-    <mergeCell ref="A49:E49"/>
-    <mergeCell ref="A25:E25"/>
-    <mergeCell ref="A247:E247"/>
-    <mergeCell ref="A207:E207"/>
-    <mergeCell ref="A211:E211"/>
-    <mergeCell ref="A219:E219"/>
-    <mergeCell ref="A230:E230"/>
-    <mergeCell ref="A236:E236"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -16210,13 +16441,13 @@
       </c>
     </row>
     <row r="2" spans="1:6" s="24" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="198" t="s">
+      <c r="A2" s="201" t="s">
         <v>893</v>
       </c>
-      <c r="B2" s="199"/>
-      <c r="C2" s="199"/>
-      <c r="D2" s="199"/>
-      <c r="E2" s="200"/>
+      <c r="B2" s="202"/>
+      <c r="C2" s="202"/>
+      <c r="D2" s="202"/>
+      <c r="E2" s="203"/>
     </row>
     <row r="3" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="19" t="s">
@@ -16291,14 +16522,14 @@
     </row>
     <row r="8" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="B8" s="168" t="s">
-        <v>1455</v>
+        <v>1453</v>
       </c>
       <c r="C8" s="169" t="s">
-        <v>1456</v>
+        <v>1454</v>
       </c>
       <c r="D8" s="168"/>
       <c r="E8" s="170" t="s">
-        <v>1457</v>
+        <v>1455</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="16" x14ac:dyDescent="0.2">
@@ -16362,13 +16593,13 @@
       </c>
     </row>
     <row r="13" spans="1:6" s="24" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="198" t="s">
+      <c r="A13" s="201" t="s">
         <v>915</v>
       </c>
-      <c r="B13" s="199"/>
-      <c r="C13" s="199"/>
-      <c r="D13" s="199"/>
-      <c r="E13" s="200"/>
+      <c r="B13" s="202"/>
+      <c r="C13" s="202"/>
+      <c r="D13" s="202"/>
+      <c r="E13" s="203"/>
     </row>
     <row r="14" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A14" s="19" t="s">
@@ -16446,13 +16677,13 @@
         <v>930</v>
       </c>
       <c r="C18" s="151" t="s">
-        <v>1315</v>
+        <v>1313</v>
       </c>
       <c r="D18" s="92" t="s">
         <v>922</v>
       </c>
       <c r="E18" s="152" t="s">
-        <v>1316</v>
+        <v>1314</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="80" x14ac:dyDescent="0.2">
@@ -16480,13 +16711,13 @@
       </c>
     </row>
     <row r="21" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="207" t="s">
+      <c r="A21" s="210" t="s">
         <v>935</v>
       </c>
-      <c r="B21" s="208"/>
-      <c r="C21" s="208"/>
-      <c r="D21" s="208"/>
-      <c r="E21" s="209"/>
+      <c r="B21" s="211"/>
+      <c r="C21" s="211"/>
+      <c r="D21" s="211"/>
+      <c r="E21" s="212"/>
     </row>
     <row r="22" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A22" s="5" t="s">
@@ -16526,21 +16757,21 @@
         <v>945</v>
       </c>
       <c r="C24" s="82" t="s">
-        <v>1450</v>
+        <v>1448</v>
       </c>
       <c r="D24" s="80"/>
       <c r="E24" s="81" t="s">
-        <v>1451</v>
+        <v>1449</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A25" s="204" t="s">
+      <c r="A25" s="207" t="s">
         <v>946</v>
       </c>
-      <c r="B25" s="205"/>
-      <c r="C25" s="205"/>
-      <c r="D25" s="205"/>
-      <c r="E25" s="206"/>
+      <c r="B25" s="208"/>
+      <c r="C25" s="208"/>
+      <c r="D25" s="208"/>
+      <c r="E25" s="209"/>
     </row>
     <row r="26" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A26" s="18" t="s">
@@ -16558,13 +16789,13 @@
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A27" s="195" t="s">
+      <c r="A27" s="198" t="s">
         <v>950</v>
       </c>
-      <c r="B27" s="196"/>
-      <c r="C27" s="196"/>
-      <c r="D27" s="196"/>
-      <c r="E27" s="197"/>
+      <c r="B27" s="199"/>
+      <c r="C27" s="199"/>
+      <c r="D27" s="199"/>
+      <c r="E27" s="200"/>
     </row>
     <row r="28" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A28" s="18" t="s">
@@ -16582,13 +16813,13 @@
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A29" s="195" t="s">
+      <c r="A29" s="198" t="s">
         <v>954</v>
       </c>
-      <c r="B29" s="196"/>
-      <c r="C29" s="196"/>
-      <c r="D29" s="196"/>
-      <c r="E29" s="197"/>
+      <c r="B29" s="199"/>
+      <c r="C29" s="199"/>
+      <c r="D29" s="199"/>
+      <c r="E29" s="200"/>
     </row>
     <row r="30" spans="1:6" ht="112" x14ac:dyDescent="0.2">
       <c r="A30" s="91" t="s">
@@ -16652,10 +16883,10 @@
         <v>968</v>
       </c>
       <c r="C33" s="21" t="s">
-        <v>1371</v>
+        <v>1369</v>
       </c>
       <c r="E33" s="46" t="s">
-        <v>1372</v>
+        <v>1370</v>
       </c>
     </row>
     <row r="34" spans="1:6" ht="32" x14ac:dyDescent="0.2">
@@ -16663,13 +16894,13 @@
         <v>257</v>
       </c>
       <c r="B34" s="19" t="s">
+        <v>1371</v>
+      </c>
+      <c r="C34" s="21" t="s">
+        <v>1372</v>
+      </c>
+      <c r="E34" s="46" t="s">
         <v>1373</v>
-      </c>
-      <c r="C34" s="21" t="s">
-        <v>1374</v>
-      </c>
-      <c r="E34" s="46" t="s">
-        <v>1375</v>
       </c>
     </row>
     <row r="35" spans="1:6" ht="48" x14ac:dyDescent="0.2">
@@ -16726,13 +16957,13 @@
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A39" s="195" t="s">
+      <c r="A39" s="198" t="s">
         <v>979</v>
       </c>
-      <c r="B39" s="196"/>
-      <c r="C39" s="196"/>
-      <c r="D39" s="196"/>
-      <c r="E39" s="197"/>
+      <c r="B39" s="199"/>
+      <c r="C39" s="199"/>
+      <c r="D39" s="199"/>
+      <c r="E39" s="200"/>
     </row>
     <row r="40" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A40" s="19" t="s">
@@ -16776,13 +17007,13 @@
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A43" s="201" t="s">
+      <c r="A43" s="204" t="s">
         <v>987</v>
       </c>
-      <c r="B43" s="202"/>
-      <c r="C43" s="202"/>
-      <c r="D43" s="202"/>
-      <c r="E43" s="203"/>
+      <c r="B43" s="205"/>
+      <c r="C43" s="205"/>
+      <c r="D43" s="205"/>
+      <c r="E43" s="206"/>
     </row>
     <row r="44" spans="1:6" ht="96" x14ac:dyDescent="0.2">
       <c r="A44" s="116" t="s">
@@ -16829,13 +17060,13 @@
         <v>993</v>
       </c>
       <c r="C46" s="62" t="s">
-        <v>1364</v>
+        <v>1362</v>
       </c>
       <c r="D46" s="116" t="s">
         <v>994</v>
       </c>
       <c r="E46" s="46" t="s">
-        <v>1365</v>
+        <v>1363</v>
       </c>
     </row>
     <row r="47" spans="1:6" ht="48" x14ac:dyDescent="0.2">
@@ -17228,23 +17459,23 @@
         <v>1060</v>
       </c>
       <c r="E11" s="138" t="s">
-        <v>1388</v>
+        <v>1386</v>
       </c>
       <c r="F11" s="135"/>
     </row>
     <row r="12" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A12" s="136" t="s">
+        <v>1382</v>
+      </c>
+      <c r="B12" s="136" t="s">
+        <v>1383</v>
+      </c>
+      <c r="C12" s="137" t="s">
         <v>1384</v>
-      </c>
-      <c r="B12" s="136" t="s">
-        <v>1385</v>
-      </c>
-      <c r="C12" s="137" t="s">
-        <v>1386</v>
       </c>
       <c r="D12" s="136"/>
       <c r="E12" s="138" t="s">
-        <v>1387</v>
+        <v>1385</v>
       </c>
       <c r="F12" s="135"/>
     </row>
@@ -17256,7 +17487,7 @@
         <v>1061</v>
       </c>
       <c r="C13" s="137" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="D13" s="136" t="s">
         <v>1062</v>
@@ -17302,7 +17533,7 @@
         <v>1067</v>
       </c>
       <c r="C16" s="137" t="s">
-        <v>1380</v>
+        <v>1378</v>
       </c>
       <c r="D16" s="136" t="s">
         <v>1068</v>
@@ -17320,7 +17551,7 @@
         <v>1070</v>
       </c>
       <c r="C17" s="137" t="s">
-        <v>1381</v>
+        <v>1379</v>
       </c>
       <c r="D17" s="136" t="s">
         <v>1071</v>
@@ -17338,7 +17569,7 @@
         <v>1073</v>
       </c>
       <c r="C18" s="137" t="s">
-        <v>1382</v>
+        <v>1380</v>
       </c>
       <c r="D18" s="136" t="s">
         <v>1074</v>
@@ -17478,17 +17709,17 @@
     </row>
     <row r="28" spans="1:6" ht="64" x14ac:dyDescent="0.2">
       <c r="A28" s="136" t="s">
-        <v>1384</v>
+        <v>1382</v>
       </c>
       <c r="B28" s="136" t="s">
-        <v>1383</v>
+        <v>1381</v>
       </c>
       <c r="C28" s="137" t="s">
-        <v>1405</v>
+        <v>1403</v>
       </c>
       <c r="D28" s="136"/>
       <c r="E28" s="138" t="s">
-        <v>1407</v>
+        <v>1405</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="32" x14ac:dyDescent="0.2">
@@ -17499,23 +17730,23 @@
         <v>1099</v>
       </c>
       <c r="C29" s="137" t="s">
-        <v>1406</v>
+        <v>1404</v>
       </c>
       <c r="D29" s="136" t="s">
         <v>1100</v>
       </c>
       <c r="E29" s="138" t="s">
-        <v>1408</v>
+        <v>1406</v>
       </c>
     </row>
     <row r="30" spans="1:6" s="13" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="210" t="s">
+      <c r="A30" s="213" t="s">
         <v>1101</v>
       </c>
-      <c r="B30" s="211"/>
-      <c r="C30" s="211"/>
-      <c r="D30" s="211"/>
-      <c r="E30" s="212"/>
+      <c r="B30" s="214"/>
+      <c r="C30" s="214"/>
+      <c r="D30" s="214"/>
+      <c r="E30" s="215"/>
     </row>
     <row r="31" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A31" s="140" t="s">
@@ -17578,13 +17809,13 @@
       <c r="E34" s="146"/>
     </row>
     <row r="35" spans="1:6" s="13" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="213" t="s">
+      <c r="A35" s="216" t="s">
         <v>1113</v>
       </c>
-      <c r="B35" s="214"/>
-      <c r="C35" s="215"/>
-      <c r="D35" s="214"/>
-      <c r="E35" s="216"/>
+      <c r="B35" s="217"/>
+      <c r="C35" s="218"/>
+      <c r="D35" s="217"/>
+      <c r="E35" s="219"/>
     </row>
     <row r="36" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A36" s="144" t="s">
@@ -17748,7 +17979,7 @@
         <v>1137</v>
       </c>
       <c r="C45" s="62" t="s">
-        <v>1356</v>
+        <v>1354</v>
       </c>
       <c r="D45" s="5" t="s">
         <v>1138</v>
@@ -17787,13 +18018,13 @@
       <c r="F47" s="135"/>
     </row>
     <row r="48" spans="1:6" s="13" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="210" t="s">
+      <c r="A48" s="213" t="s">
         <v>1142</v>
       </c>
-      <c r="B48" s="211"/>
-      <c r="C48" s="211"/>
-      <c r="D48" s="211"/>
-      <c r="E48" s="212"/>
+      <c r="B48" s="214"/>
+      <c r="C48" s="214"/>
+      <c r="D48" s="214"/>
+      <c r="E48" s="215"/>
     </row>
     <row r="49" spans="1:6" s="30" customFormat="1" ht="64" x14ac:dyDescent="0.2">
       <c r="A49" s="144" t="s">
@@ -17840,13 +18071,13 @@
         <v>1149</v>
       </c>
       <c r="C51" s="62" t="s">
-        <v>1364</v>
+        <v>1362</v>
       </c>
       <c r="D51" s="116" t="s">
         <v>994</v>
       </c>
       <c r="E51" s="63" t="s">
-        <v>1365</v>
+        <v>1363</v>
       </c>
     </row>
     <row r="52" spans="1:6" s="30" customFormat="1" ht="48" x14ac:dyDescent="0.2">
@@ -18477,6 +18708,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <Readyforteam_x003f_ xmlns="565e1b1d-057e-4d85-b896-01a5881d8a45">false</Readyforteam_x003f_>
@@ -18517,15 +18757,6 @@
 </p:properties>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EAFDB110-4046-4E72-A1EF-1908ABEC3151}">
   <ds:schemaRefs>
@@ -18548,6 +18779,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8D7CE8C7-18DC-484F-8376-ED09F13D44C8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{017ACE96-8143-486E-8436-7787F6B96F4A}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -18558,12 +18797,4 @@
     <ds:schemaRef ds:uri="2799d30d-6731-4efe-ac9b-c4895a8828d9"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8D7CE8C7-18DC-484F-8376-ED09F13D44C8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Adding Welsh to Feedback confirmation page. Fixing a bug-ette on the routing.
</commit_message>
<xml_diff>
--- a/app/data/MCCD-localisation.xlsx
+++ b/app/data/MCCD-localisation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/JALAT/GIT/medical-certificate-of-cause-of-death/app/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8498484-7167-6243-89C4-BECCFD5CB06C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2CB59DA-8CC7-0B47-A0F9-5F0AA20A4185}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="13940" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="13940" firstSheet="4" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Using this document" sheetId="8" r:id="rId1"/>
@@ -69,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2315" uniqueCount="1566">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2324" uniqueCount="1573">
   <si>
     <r>
       <rPr>
@@ -6077,6 +6077,27 @@
   </si>
   <si>
     <t>058</t>
+  </si>
+  <si>
+    <t>Feedback page confirmation</t>
+  </si>
+  <si>
+    <t>feedbackPageTitle</t>
+  </si>
+  <si>
+    <t>feedbackPageContent</t>
+  </si>
+  <si>
+    <t>Thank you for submitting your feedback</t>
+  </si>
+  <si>
+    <t>Diolch am gyflwyno eich adborth</t>
+  </si>
+  <si>
+    <t>&lt;h2 class="govuk-heading-m"&gt;What happens next&lt;/h2&gt;&lt;p class="govuk-body"&gt;Your feedback will be analysed to gain insight into how well our service is performing and identify opportunities for improvement.&lt;/p&gt;&lt;p class="govuk-body"&gt;In some instances, if appropriate, you will be contacted with a response.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;h2 class="govuk-heading-m"&gt;Beth sy'n digwydd nesaf&lt;/h2&gt;&lt;p class="govuk-body"&gt;Bydd eich adborth yn cael ei ddadansoddi i gael mewnwelediad i ba mor dda mae ein gwasanaeth yn perfformio a nodi cyfleoedd i wella.&lt;/p&gt;&lt;p class="govuk-body"&gt;Mewn rhai achosion, os yw'n briodol, byddwn yn cysylltu â chi gydag ymateb.&lt;/p&gt;</t>
   </si>
 </sst>
 </file>
@@ -8788,11 +8809,11 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{124C2F8F-96ED-4E65-B816-FFFEB93DC889}">
-  <dimension ref="A1:F36"/>
+  <dimension ref="A1:F39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D35" sqref="D35"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A33" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E39" sqref="E39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -9304,8 +9325,47 @@
         <v>1561</v>
       </c>
     </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A37" s="220" t="s">
+        <v>1566</v>
+      </c>
+      <c r="B37" s="221"/>
+      <c r="C37" s="221"/>
+      <c r="D37" s="221"/>
+      <c r="E37" s="221"/>
+      <c r="F37" s="221"/>
+    </row>
+    <row r="38" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A38" s="5" t="s">
+        <v>239</v>
+      </c>
+      <c r="B38" s="5" t="s">
+        <v>1567</v>
+      </c>
+      <c r="C38" s="6" t="s">
+        <v>1569</v>
+      </c>
+      <c r="E38" s="37" t="s">
+        <v>1570</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" ht="160" x14ac:dyDescent="0.2">
+      <c r="A39" s="5" t="s">
+        <v>1553</v>
+      </c>
+      <c r="B39" s="5" t="s">
+        <v>1568</v>
+      </c>
+      <c r="C39" s="6" t="s">
+        <v>1571</v>
+      </c>
+      <c r="E39" s="37" t="s">
+        <v>1572</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="7">
+    <mergeCell ref="A37:F37"/>
     <mergeCell ref="A34:F34"/>
     <mergeCell ref="A2:F2"/>
     <mergeCell ref="A20:F20"/>
@@ -9321,7 +9381,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F72"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D3" sqref="D3"/>
     </sheetView>
@@ -17256,7 +17316,7 @@
   <dimension ref="A1:F75"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Missing Welsh on Feedback title page.
</commit_message>
<xml_diff>
--- a/app/data/MCCD-localisation.xlsx
+++ b/app/data/MCCD-localisation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/JALAT/GIT/medical-certificate-of-cause-of-death/app/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2CB59DA-8CC7-0B47-A0F9-5F0AA20A4185}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B3D222E-139D-0F40-826F-90B4A358D575}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="13940" firstSheet="4" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -69,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2324" uniqueCount="1573">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2329" uniqueCount="1577">
   <si>
     <r>
       <rPr>
@@ -6085,9 +6085,6 @@
     <t>feedbackPageTitle</t>
   </si>
   <si>
-    <t>feedbackPageContent</t>
-  </si>
-  <si>
     <t>Thank you for submitting your feedback</t>
   </si>
   <si>
@@ -6098,6 +6095,21 @@
   </si>
   <si>
     <t>&lt;h2 class="govuk-heading-m"&gt;Beth sy'n digwydd nesaf&lt;/h2&gt;&lt;p class="govuk-body"&gt;Bydd eich adborth yn cael ei ddadansoddi i gael mewnwelediad i ba mor dda mae ein gwasanaeth yn perfformio a nodi cyfleoedd i wella.&lt;/p&gt;&lt;p class="govuk-body"&gt;Mewn rhai achosion, os yw'n briodol, byddwn yn cysylltu â chi gydag ymateb.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>Feedback page</t>
+  </si>
+  <si>
+    <t>feedbackConfirmationPageTitle</t>
+  </si>
+  <si>
+    <t>feedbackConfirmationPageContent</t>
+  </si>
+  <si>
+    <t>Give feedback on Complete a Medical certificate of cause of death</t>
+  </si>
+  <si>
+    <t>Rhoi adborth ar gwblhau tystysgrif feddygol achos marwolaeth</t>
   </si>
 </sst>
 </file>
@@ -7131,6 +7143,24 @@
     <xf numFmtId="0" fontId="13" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -7138,24 +7168,6 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -8809,11 +8821,11 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{124C2F8F-96ED-4E65-B816-FFFEB93DC889}">
-  <dimension ref="A1:F39"/>
+  <dimension ref="A1:F41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A33" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E39" sqref="E39"/>
+      <pane ySplit="1" topLeftCell="A36" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D40" sqref="D40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -9327,7 +9339,7 @@
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" s="220" t="s">
-        <v>1566</v>
+        <v>1572</v>
       </c>
       <c r="B37" s="221"/>
       <c r="C37" s="221"/>
@@ -9335,43 +9347,68 @@
       <c r="E37" s="221"/>
       <c r="F37" s="221"/>
     </row>
-    <row r="38" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A38" s="5" t="s">
-        <v>239</v>
+        <v>1553</v>
       </c>
       <c r="B38" s="5" t="s">
         <v>1567</v>
       </c>
       <c r="C38" s="6" t="s">
+        <v>1575</v>
+      </c>
+      <c r="E38" s="37" t="s">
+        <v>1576</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A39" s="220" t="s">
+        <v>1566</v>
+      </c>
+      <c r="B39" s="221"/>
+      <c r="C39" s="221"/>
+      <c r="D39" s="221"/>
+      <c r="E39" s="221"/>
+      <c r="F39" s="221"/>
+    </row>
+    <row r="40" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A40" s="5" t="s">
+        <v>239</v>
+      </c>
+      <c r="B40" s="5" t="s">
+        <v>1573</v>
+      </c>
+      <c r="C40" s="6" t="s">
+        <v>1568</v>
+      </c>
+      <c r="E40" s="37" t="s">
         <v>1569</v>
       </c>
-      <c r="E38" s="37" t="s">
+    </row>
+    <row r="41" spans="1:6" ht="160" x14ac:dyDescent="0.2">
+      <c r="A41" s="5" t="s">
+        <v>1553</v>
+      </c>
+      <c r="B41" s="5" t="s">
+        <v>1574</v>
+      </c>
+      <c r="C41" s="6" t="s">
         <v>1570</v>
       </c>
-    </row>
-    <row r="39" spans="1:6" ht="160" x14ac:dyDescent="0.2">
-      <c r="A39" s="5" t="s">
-        <v>1553</v>
-      </c>
-      <c r="B39" s="5" t="s">
-        <v>1568</v>
-      </c>
-      <c r="C39" s="6" t="s">
+      <c r="E41" s="37" t="s">
         <v>1571</v>
       </c>
-      <c r="E39" s="37" t="s">
-        <v>1572</v>
-      </c>
     </row>
   </sheetData>
-  <mergeCells count="7">
-    <mergeCell ref="A37:F37"/>
+  <mergeCells count="8">
+    <mergeCell ref="A39:F39"/>
     <mergeCell ref="A34:F34"/>
     <mergeCell ref="A2:F2"/>
     <mergeCell ref="A20:F20"/>
     <mergeCell ref="A25:F25"/>
     <mergeCell ref="A28:F28"/>
     <mergeCell ref="A31:F31"/>
+    <mergeCell ref="A37:F37"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -11699,13 +11736,13 @@
       </c>
     </row>
     <row r="2" spans="1:6" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="192" t="s">
+      <c r="A2" s="189" t="s">
         <v>363</v>
       </c>
-      <c r="B2" s="193"/>
-      <c r="C2" s="193"/>
-      <c r="D2" s="193"/>
-      <c r="E2" s="194"/>
+      <c r="B2" s="190"/>
+      <c r="C2" s="190"/>
+      <c r="D2" s="190"/>
+      <c r="E2" s="191"/>
       <c r="F2" s="33"/>
     </row>
     <row r="3" spans="1:6" ht="48" x14ac:dyDescent="0.2">
@@ -11849,13 +11886,13 @@
       <c r="F10" s="119"/>
     </row>
     <row r="11" spans="1:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="195" t="s">
+      <c r="A11" s="192" t="s">
         <v>392</v>
       </c>
-      <c r="B11" s="196"/>
-      <c r="C11" s="196"/>
-      <c r="D11" s="196"/>
-      <c r="E11" s="197"/>
+      <c r="B11" s="193"/>
+      <c r="C11" s="193"/>
+      <c r="D11" s="193"/>
+      <c r="E11" s="194"/>
       <c r="F11" s="119"/>
     </row>
     <row r="12" spans="1:6" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -14413,13 +14450,13 @@
       </c>
     </row>
     <row r="180" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A180" s="189" t="s">
+      <c r="A180" s="195" t="s">
         <v>754</v>
       </c>
-      <c r="B180" s="190"/>
-      <c r="C180" s="190"/>
-      <c r="D180" s="190"/>
-      <c r="E180" s="191"/>
+      <c r="B180" s="196"/>
+      <c r="C180" s="196"/>
+      <c r="D180" s="196"/>
+      <c r="E180" s="197"/>
       <c r="F180" s="129" t="s">
         <v>758</v>
       </c>
@@ -16431,19 +16468,6 @@
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="A247:E247"/>
-    <mergeCell ref="A207:E207"/>
-    <mergeCell ref="A211:E211"/>
-    <mergeCell ref="A219:E219"/>
-    <mergeCell ref="A230:E230"/>
-    <mergeCell ref="A236:E236"/>
-    <mergeCell ref="A65:E65"/>
-    <mergeCell ref="A2:E2"/>
-    <mergeCell ref="A11:E11"/>
-    <mergeCell ref="A15:E15"/>
-    <mergeCell ref="A30:E30"/>
-    <mergeCell ref="A49:E49"/>
-    <mergeCell ref="A25:E25"/>
     <mergeCell ref="A194:E194"/>
     <mergeCell ref="A172:E172"/>
     <mergeCell ref="A70:E70"/>
@@ -16455,6 +16479,19 @@
     <mergeCell ref="A100:E100"/>
     <mergeCell ref="A180:E180"/>
     <mergeCell ref="A190:E190"/>
+    <mergeCell ref="A65:E65"/>
+    <mergeCell ref="A2:E2"/>
+    <mergeCell ref="A11:E11"/>
+    <mergeCell ref="A15:E15"/>
+    <mergeCell ref="A30:E30"/>
+    <mergeCell ref="A49:E49"/>
+    <mergeCell ref="A25:E25"/>
+    <mergeCell ref="A247:E247"/>
+    <mergeCell ref="A207:E207"/>
+    <mergeCell ref="A211:E211"/>
+    <mergeCell ref="A219:E219"/>
+    <mergeCell ref="A230:E230"/>
+    <mergeCell ref="A236:E236"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -18768,15 +18805,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <Readyforteam_x003f_ xmlns="565e1b1d-057e-4d85-b896-01a5881d8a45">false</Readyforteam_x003f_>
@@ -18817,6 +18845,15 @@
 </p:properties>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EAFDB110-4046-4E72-A1EF-1908ABEC3151}">
   <ds:schemaRefs>
@@ -18839,14 +18876,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8D7CE8C7-18DC-484F-8376-ED09F13D44C8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{017ACE96-8143-486E-8436-7787F6B96F4A}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -18857,4 +18886,12 @@
     <ds:schemaRef ds:uri="2799d30d-6731-4efe-ac9b-c4895a8828d9"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8D7CE8C7-18DC-484F-8376-ED09F13D44C8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Inset text translations on MCCD summary screen.
</commit_message>
<xml_diff>
--- a/app/data/MCCD-localisation.xlsx
+++ b/app/data/MCCD-localisation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/JALAT/GIT/medical-certificate-of-cause-of-death/app/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B3D222E-139D-0F40-826F-90B4A358D575}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4C0F239-8442-3941-8B04-4FC318C07D0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="13940" firstSheet="4" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="13940" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Using this document" sheetId="8" r:id="rId1"/>
@@ -18,13 +18,14 @@
     <sheet name="Start page" sheetId="7" r:id="rId3"/>
     <sheet name="CIS2 pages" sheetId="9" r:id="rId4"/>
     <sheet name="Onboarding" sheetId="12" r:id="rId5"/>
-    <sheet name="Dashboard" sheetId="2" r:id="rId6"/>
-    <sheet name="Deceased persons details" sheetId="3" r:id="rId7"/>
-    <sheet name="Actions after death" sheetId="4" r:id="rId8"/>
-    <sheet name="Cause of death" sheetId="5" r:id="rId9"/>
-    <sheet name="MCCD Tasklist" sheetId="10" r:id="rId10"/>
-    <sheet name="Declaration and submission" sheetId="6" r:id="rId11"/>
-    <sheet name="Confirmation page" sheetId="11" r:id="rId12"/>
+    <sheet name="Summary" sheetId="13" r:id="rId6"/>
+    <sheet name="Dashboard" sheetId="2" r:id="rId7"/>
+    <sheet name="Deceased persons details" sheetId="3" r:id="rId8"/>
+    <sheet name="Actions after death" sheetId="4" r:id="rId9"/>
+    <sheet name="Cause of death" sheetId="5" r:id="rId10"/>
+    <sheet name="MCCD Tasklist" sheetId="10" r:id="rId11"/>
+    <sheet name="Declaration and submission" sheetId="6" r:id="rId12"/>
+    <sheet name="Confirmation page" sheetId="11" r:id="rId13"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -69,7 +70,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2329" uniqueCount="1577">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2366" uniqueCount="1603">
   <si>
     <r>
       <rPr>
@@ -6110,6 +6111,84 @@
   </si>
   <si>
     <t>Rhoi adborth ar gwblhau tystysgrif feddygol achos marwolaeth</t>
+  </si>
+  <si>
+    <t>globalCertificateType</t>
+  </si>
+  <si>
+    <t>Certificate type</t>
+  </si>
+  <si>
+    <t>Math o dystysgrif</t>
+  </si>
+  <si>
+    <t>globalReferenceNumber</t>
+  </si>
+  <si>
+    <t>Reference number</t>
+  </si>
+  <si>
+    <t>Rhif cyfeirnod</t>
+  </si>
+  <si>
+    <t>Summary screen</t>
+  </si>
+  <si>
+    <t>Inset</t>
+  </si>
+  <si>
+    <t>This MCCD must be amended. Contact your medical examiner officer to find out what amendments you must make.</t>
+  </si>
+  <si>
+    <t>summaryCertificateNeedsAmends</t>
+  </si>
+  <si>
+    <t>This MCCD has been reviewed and signed off by a medical examiner. The medical examiner office will forward this certificate to the local register office.&lt;br /&gt;&lt;br /&gt;There is nothing further for you to do.</t>
+  </si>
+  <si>
+    <t>This MCCD has been signed off by a medical examiner and sent to the local register office.&lt;br /&gt;&lt;br /&gt;There is nothing further for you to do.</t>
+  </si>
+  <si>
+    <t>summaryCertificateWaitingForSubmission</t>
+  </si>
+  <si>
+    <t>summaryCertificateSubmitted</t>
+  </si>
+  <si>
+    <t>Rhaid diwygio'r MCCD hwn. Cysylltwch â'ch swyddog arholwr meddygol i ddarganfod pa welliannau y mae'n rhaid i chi eu gwneud.</t>
+  </si>
+  <si>
+    <t>Mae'r MCCD hwn wedi cael ei adolygu a'i gymeradwyo gan arholwr meddygol. Bydd y swyddfa arholwr meddygol yn anfon y dystysgrif hon i'r swyddfa gofrestru leol.&lt;br / &gt;&lt;br / &gt;Nid oes unrhyw beth pellach i chi ei wneud.</t>
+  </si>
+  <si>
+    <t>Mae'r MCCD hwn wedi cael ei gymeradwyo gan arholwr meddygol a'i anfon i'r swyddfa gofrestru leol.&lt;br / &gt;&lt;br /&gt;Nid oes unrhyw beth pellach i chi ei wneud.</t>
+  </si>
+  <si>
+    <t>This MCCD has been sent to the local register office.&lt;br /&gt;&lt;br /&gt;There is nothing further for you to do.</t>
+  </si>
+  <si>
+    <t>summaryMECertificateSubmitted</t>
+  </si>
+  <si>
+    <t>Mae'r MCCD hwn wedi'i anfon i'r swyddfa gofrestru leol.&lt;br /&gt;&lt;br /&gt;Nid oes unrhyw beth pellach i chi ei wneud.</t>
+  </si>
+  <si>
+    <t>summaryCertificateAmendsNotSubmitted</t>
+  </si>
+  <si>
+    <t>You have amended this MCCD, but you still need to submit these changes.&lt;br /&gt;&lt;br /&gt;Review this certificate, read and select the declaration at the bottom, and submit your amendments.</t>
+  </si>
+  <si>
+    <t>summaryCertificateAmendsNotSubmittedByAP</t>
+  </si>
+  <si>
+    <t>The attending practitioner has amended this MCCD but still needs to sign the declaration and submit this certificate. This MCCD cannot be sent to a medical examiner for review until this has been done.</t>
+  </si>
+  <si>
+    <t>Rydych chi wedi diwygio'r MCCD hwn, ond mae angen i chi gyflwyno'r newidiadau hyn o hyd. &lt;br / &gt;&lt;br /&gt;Adolygu'r dystysgrif hon, darllen a dewis y datganiad ar y gwaelod, a chyflwyno eich gwelliannau.</t>
+  </si>
+  <si>
+    <t>Mae'r ymarferydd sy'n mynychu wedi diwygio'r MCCD hwn ond mae angen llofnodi'r datganiad a chyflwyno'r dystysgrif hon o hyd. Ni ellir anfon y MCCD hwn at arholwr meddygol i'w adolygu nes bod hyn wedi'i wneud.</t>
   </si>
 </sst>
 </file>
@@ -6585,7 +6664,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="222">
+  <cellXfs count="225">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -7143,6 +7222,15 @@
     <xf numFmtId="0" fontId="13" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -7161,15 +7249,6 @@
     <xf numFmtId="0" fontId="13" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
@@ -7242,6 +7321,13 @@
     <xf numFmtId="0" fontId="13" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="20% - Accent2" xfId="1" builtinId="34"/>
@@ -8167,6 +8253,1185 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6CA2FE89-1BCA-4888-9BB6-D7A7737E07E4}">
+  <dimension ref="A1:F75"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C13" sqref="C13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="33.6640625" style="16" customWidth="1"/>
+    <col min="2" max="2" width="59.33203125" style="16" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="33.6640625" style="17" customWidth="1"/>
+    <col min="4" max="4" width="39.5" style="16" customWidth="1"/>
+    <col min="5" max="5" width="33.6640625" style="48" customWidth="1"/>
+    <col min="6" max="6" width="24.83203125" style="12" customWidth="1"/>
+    <col min="7" max="16384" width="9.1640625" style="12"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A1" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="47" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="135" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A2" s="136" t="s">
+        <v>239</v>
+      </c>
+      <c r="B2" s="136" t="s">
+        <v>1026</v>
+      </c>
+      <c r="C2" s="137" t="s">
+        <v>1027</v>
+      </c>
+      <c r="D2" s="136" t="s">
+        <v>242</v>
+      </c>
+      <c r="E2" s="138" t="s">
+        <v>1028</v>
+      </c>
+      <c r="F2" s="135"/>
+    </row>
+    <row r="3" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+      <c r="A3" s="136" t="s">
+        <v>940</v>
+      </c>
+      <c r="B3" s="136" t="s">
+        <v>1029</v>
+      </c>
+      <c r="C3" s="137" t="s">
+        <v>1030</v>
+      </c>
+      <c r="D3" s="136" t="s">
+        <v>1031</v>
+      </c>
+      <c r="E3" s="138" t="s">
+        <v>1032</v>
+      </c>
+      <c r="F3" s="135"/>
+    </row>
+    <row r="4" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+      <c r="A4" s="136" t="s">
+        <v>1033</v>
+      </c>
+      <c r="B4" s="136" t="s">
+        <v>1034</v>
+      </c>
+      <c r="C4" s="137" t="s">
+        <v>1035</v>
+      </c>
+      <c r="D4" s="136" t="s">
+        <v>1036</v>
+      </c>
+      <c r="E4" s="138" t="s">
+        <v>1037</v>
+      </c>
+      <c r="F4" s="135"/>
+    </row>
+    <row r="5" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+      <c r="A5" s="136" t="s">
+        <v>406</v>
+      </c>
+      <c r="B5" s="139" t="s">
+        <v>1038</v>
+      </c>
+      <c r="C5" s="27"/>
+      <c r="D5" s="136" t="s">
+        <v>1039</v>
+      </c>
+      <c r="E5" s="138"/>
+      <c r="F5" s="135"/>
+    </row>
+    <row r="6" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+      <c r="A6" s="136" t="s">
+        <v>409</v>
+      </c>
+      <c r="B6" s="139" t="s">
+        <v>1040</v>
+      </c>
+      <c r="C6" s="27"/>
+      <c r="D6" s="136" t="s">
+        <v>1041</v>
+      </c>
+      <c r="E6" s="138"/>
+      <c r="F6" s="135"/>
+    </row>
+    <row r="7" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+      <c r="A7" s="136" t="s">
+        <v>1033</v>
+      </c>
+      <c r="B7" s="136" t="s">
+        <v>1042</v>
+      </c>
+      <c r="C7" s="137" t="s">
+        <v>1043</v>
+      </c>
+      <c r="D7" s="136" t="s">
+        <v>1044</v>
+      </c>
+      <c r="E7" s="138" t="s">
+        <v>1045</v>
+      </c>
+      <c r="F7" s="135"/>
+    </row>
+    <row r="8" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+      <c r="A8" s="136" t="s">
+        <v>1033</v>
+      </c>
+      <c r="B8" s="136" t="s">
+        <v>1046</v>
+      </c>
+      <c r="C8" s="137" t="s">
+        <v>1047</v>
+      </c>
+      <c r="D8" s="136" t="s">
+        <v>1048</v>
+      </c>
+      <c r="E8" s="138" t="s">
+        <v>1049</v>
+      </c>
+      <c r="F8" s="135"/>
+    </row>
+    <row r="9" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+      <c r="A9" s="136" t="s">
+        <v>1033</v>
+      </c>
+      <c r="B9" s="136" t="s">
+        <v>1050</v>
+      </c>
+      <c r="C9" s="137" t="s">
+        <v>1051</v>
+      </c>
+      <c r="D9" s="136" t="s">
+        <v>1052</v>
+      </c>
+      <c r="E9" s="138" t="s">
+        <v>1053</v>
+      </c>
+      <c r="F9" s="135"/>
+    </row>
+    <row r="10" spans="1:6" ht="64" x14ac:dyDescent="0.2">
+      <c r="A10" s="136" t="s">
+        <v>1033</v>
+      </c>
+      <c r="B10" s="136" t="s">
+        <v>1054</v>
+      </c>
+      <c r="C10" s="137" t="s">
+        <v>1055</v>
+      </c>
+      <c r="D10" s="136" t="s">
+        <v>1056</v>
+      </c>
+      <c r="E10" s="138" t="s">
+        <v>1057</v>
+      </c>
+      <c r="F10" s="135"/>
+    </row>
+    <row r="11" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A11" s="136" t="s">
+        <v>250</v>
+      </c>
+      <c r="B11" s="136" t="s">
+        <v>1058</v>
+      </c>
+      <c r="C11" s="137" t="s">
+        <v>1059</v>
+      </c>
+      <c r="D11" s="136" t="s">
+        <v>1060</v>
+      </c>
+      <c r="E11" s="138" t="s">
+        <v>1386</v>
+      </c>
+      <c r="F11" s="135"/>
+    </row>
+    <row r="12" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+      <c r="A12" s="136" t="s">
+        <v>1382</v>
+      </c>
+      <c r="B12" s="136" t="s">
+        <v>1383</v>
+      </c>
+      <c r="C12" s="137" t="s">
+        <v>1384</v>
+      </c>
+      <c r="D12" s="136"/>
+      <c r="E12" s="138" t="s">
+        <v>1385</v>
+      </c>
+      <c r="F12" s="135"/>
+    </row>
+    <row r="13" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+      <c r="A13" s="136" t="s">
+        <v>1033</v>
+      </c>
+      <c r="B13" s="136" t="s">
+        <v>1061</v>
+      </c>
+      <c r="C13" s="137" t="s">
+        <v>1450</v>
+      </c>
+      <c r="D13" s="136" t="s">
+        <v>1062</v>
+      </c>
+      <c r="E13" s="138" t="s">
+        <v>1063</v>
+      </c>
+      <c r="F13" s="135"/>
+    </row>
+    <row r="14" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+      <c r="A14" s="136" t="s">
+        <v>406</v>
+      </c>
+      <c r="B14" s="28" t="s">
+        <v>1064</v>
+      </c>
+      <c r="C14" s="138"/>
+      <c r="D14" s="136" t="s">
+        <v>1065</v>
+      </c>
+      <c r="E14" s="138"/>
+      <c r="F14" s="135"/>
+    </row>
+    <row r="15" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+      <c r="A15" s="136" t="s">
+        <v>409</v>
+      </c>
+      <c r="B15" s="28" t="s">
+        <v>1066</v>
+      </c>
+      <c r="C15" s="138"/>
+      <c r="D15" s="136" t="s">
+        <v>1041</v>
+      </c>
+      <c r="E15" s="138"/>
+      <c r="F15" s="135"/>
+    </row>
+    <row r="16" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+      <c r="A16" s="136" t="s">
+        <v>1033</v>
+      </c>
+      <c r="B16" s="136" t="s">
+        <v>1067</v>
+      </c>
+      <c r="C16" s="137" t="s">
+        <v>1378</v>
+      </c>
+      <c r="D16" s="136" t="s">
+        <v>1068</v>
+      </c>
+      <c r="E16" s="138" t="s">
+        <v>1069</v>
+      </c>
+      <c r="F16" s="135"/>
+    </row>
+    <row r="17" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+      <c r="A17" s="136" t="s">
+        <v>1033</v>
+      </c>
+      <c r="B17" s="136" t="s">
+        <v>1070</v>
+      </c>
+      <c r="C17" s="137" t="s">
+        <v>1379</v>
+      </c>
+      <c r="D17" s="136" t="s">
+        <v>1071</v>
+      </c>
+      <c r="E17" s="138" t="s">
+        <v>1072</v>
+      </c>
+      <c r="F17" s="135"/>
+    </row>
+    <row r="18" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+      <c r="A18" s="136" t="s">
+        <v>1033</v>
+      </c>
+      <c r="B18" s="136" t="s">
+        <v>1073</v>
+      </c>
+      <c r="C18" s="137" t="s">
+        <v>1380</v>
+      </c>
+      <c r="D18" s="136" t="s">
+        <v>1074</v>
+      </c>
+      <c r="E18" s="138" t="s">
+        <v>1075</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="144" x14ac:dyDescent="0.2">
+      <c r="A19" s="136" t="s">
+        <v>1033</v>
+      </c>
+      <c r="B19" s="136" t="s">
+        <v>1076</v>
+      </c>
+      <c r="C19" s="137" t="s">
+        <v>1077</v>
+      </c>
+      <c r="D19" s="29" t="s">
+        <v>1078</v>
+      </c>
+      <c r="E19" s="138" t="s">
+        <v>1079</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="80" x14ac:dyDescent="0.2">
+      <c r="A20" s="136" t="s">
+        <v>406</v>
+      </c>
+      <c r="B20" s="28" t="s">
+        <v>1080</v>
+      </c>
+      <c r="C20" s="27"/>
+      <c r="D20" s="18" t="s">
+        <v>1081</v>
+      </c>
+      <c r="E20" s="138"/>
+    </row>
+    <row r="21" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+      <c r="A21" s="136" t="s">
+        <v>409</v>
+      </c>
+      <c r="B21" s="28" t="s">
+        <v>1082</v>
+      </c>
+      <c r="C21" s="27"/>
+      <c r="D21" s="18" t="s">
+        <v>1041</v>
+      </c>
+      <c r="E21" s="138"/>
+    </row>
+    <row r="22" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+      <c r="A22" s="136" t="s">
+        <v>409</v>
+      </c>
+      <c r="B22" s="28" t="s">
+        <v>1083</v>
+      </c>
+      <c r="C22" s="27"/>
+      <c r="D22" s="18" t="s">
+        <v>1084</v>
+      </c>
+      <c r="E22" s="138"/>
+    </row>
+    <row r="23" spans="1:6" ht="112" x14ac:dyDescent="0.2">
+      <c r="A23" s="136" t="s">
+        <v>1085</v>
+      </c>
+      <c r="B23" s="136" t="s">
+        <v>1086</v>
+      </c>
+      <c r="C23" s="137" t="s">
+        <v>1087</v>
+      </c>
+      <c r="D23" s="136" t="s">
+        <v>1088</v>
+      </c>
+      <c r="E23" s="138" t="s">
+        <v>1089</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+      <c r="A24" s="136" t="s">
+        <v>406</v>
+      </c>
+      <c r="B24" s="28" t="s">
+        <v>1090</v>
+      </c>
+      <c r="C24" s="27"/>
+      <c r="D24" s="136" t="s">
+        <v>1091</v>
+      </c>
+      <c r="E24" s="138"/>
+    </row>
+    <row r="25" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+      <c r="A25" s="136" t="s">
+        <v>409</v>
+      </c>
+      <c r="B25" s="28" t="s">
+        <v>1092</v>
+      </c>
+      <c r="C25" s="27"/>
+      <c r="D25" s="136" t="s">
+        <v>1093</v>
+      </c>
+      <c r="E25" s="138"/>
+    </row>
+    <row r="26" spans="1:6" ht="64" x14ac:dyDescent="0.2">
+      <c r="A26" s="136" t="s">
+        <v>409</v>
+      </c>
+      <c r="B26" s="28" t="s">
+        <v>1094</v>
+      </c>
+      <c r="C26" s="27"/>
+      <c r="D26" s="29" t="s">
+        <v>1095</v>
+      </c>
+      <c r="E26" s="138"/>
+    </row>
+    <row r="27" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A27" s="136" t="s">
+        <v>250</v>
+      </c>
+      <c r="B27" s="136" t="s">
+        <v>1096</v>
+      </c>
+      <c r="C27" s="137" t="s">
+        <v>1097</v>
+      </c>
+      <c r="D27" s="136" t="s">
+        <v>1060</v>
+      </c>
+      <c r="E27" s="138" t="s">
+        <v>1098</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="64" x14ac:dyDescent="0.2">
+      <c r="A28" s="136" t="s">
+        <v>1382</v>
+      </c>
+      <c r="B28" s="136" t="s">
+        <v>1381</v>
+      </c>
+      <c r="C28" s="137" t="s">
+        <v>1403</v>
+      </c>
+      <c r="D28" s="136"/>
+      <c r="E28" s="138" t="s">
+        <v>1405</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+      <c r="A29" s="136" t="s">
+        <v>1033</v>
+      </c>
+      <c r="B29" s="136" t="s">
+        <v>1099</v>
+      </c>
+      <c r="C29" s="137" t="s">
+        <v>1404</v>
+      </c>
+      <c r="D29" s="136" t="s">
+        <v>1100</v>
+      </c>
+      <c r="E29" s="138" t="s">
+        <v>1406</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" s="13" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="213" t="s">
+        <v>1101</v>
+      </c>
+      <c r="B30" s="214"/>
+      <c r="C30" s="214"/>
+      <c r="D30" s="214"/>
+      <c r="E30" s="215"/>
+    </row>
+    <row r="31" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+      <c r="A31" s="140" t="s">
+        <v>239</v>
+      </c>
+      <c r="B31" s="141" t="s">
+        <v>1102</v>
+      </c>
+      <c r="C31" s="142" t="s">
+        <v>1103</v>
+      </c>
+      <c r="D31" s="5" t="s">
+        <v>1104</v>
+      </c>
+      <c r="E31" s="143" t="s">
+        <v>1105</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="64" x14ac:dyDescent="0.2">
+      <c r="A32" s="144" t="s">
+        <v>1106</v>
+      </c>
+      <c r="B32" s="144" t="s">
+        <v>1107</v>
+      </c>
+      <c r="C32" s="145" t="s">
+        <v>1108</v>
+      </c>
+      <c r="D32" s="144" t="s">
+        <v>1109</v>
+      </c>
+      <c r="E32" s="146" t="s">
+        <v>1110</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+      <c r="A33" s="18" t="s">
+        <v>406</v>
+      </c>
+      <c r="B33" s="28" t="s">
+        <v>1111</v>
+      </c>
+      <c r="C33" s="27"/>
+      <c r="D33" s="18" t="s">
+        <v>985</v>
+      </c>
+      <c r="E33" s="146"/>
+    </row>
+    <row r="34" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+      <c r="A34" s="18" t="s">
+        <v>409</v>
+      </c>
+      <c r="B34" s="28" t="s">
+        <v>1112</v>
+      </c>
+      <c r="C34" s="27"/>
+      <c r="D34" s="18" t="s">
+        <v>978</v>
+      </c>
+      <c r="E34" s="146"/>
+    </row>
+    <row r="35" spans="1:6" s="13" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="216" t="s">
+        <v>1113</v>
+      </c>
+      <c r="B35" s="217"/>
+      <c r="C35" s="218"/>
+      <c r="D35" s="217"/>
+      <c r="E35" s="219"/>
+    </row>
+    <row r="36" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+      <c r="A36" s="144" t="s">
+        <v>239</v>
+      </c>
+      <c r="B36" s="147" t="s">
+        <v>1114</v>
+      </c>
+      <c r="C36" s="145" t="s">
+        <v>1115</v>
+      </c>
+      <c r="D36" s="50" t="s">
+        <v>1116</v>
+      </c>
+      <c r="E36" s="146" t="s">
+        <v>1117</v>
+      </c>
+      <c r="F36" s="135"/>
+    </row>
+    <row r="37" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+      <c r="A37" s="144" t="s">
+        <v>1033</v>
+      </c>
+      <c r="B37" s="148" t="s">
+        <v>1118</v>
+      </c>
+      <c r="C37" s="145" t="s">
+        <v>1119</v>
+      </c>
+      <c r="D37" s="149" t="s">
+        <v>1120</v>
+      </c>
+      <c r="E37" s="146" t="s">
+        <v>1121</v>
+      </c>
+      <c r="F37" s="135"/>
+    </row>
+    <row r="38" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+      <c r="A38" s="144" t="s">
+        <v>1033</v>
+      </c>
+      <c r="B38" s="148" t="s">
+        <v>1122</v>
+      </c>
+      <c r="C38" s="145" t="s">
+        <v>1123</v>
+      </c>
+      <c r="D38" s="149" t="s">
+        <v>1120</v>
+      </c>
+      <c r="E38" s="146" t="s">
+        <v>1124</v>
+      </c>
+      <c r="F38" s="135"/>
+    </row>
+    <row r="39" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+      <c r="A39" s="144" t="s">
+        <v>1033</v>
+      </c>
+      <c r="B39" s="148" t="s">
+        <v>1125</v>
+      </c>
+      <c r="C39" s="49" t="s">
+        <v>1126</v>
+      </c>
+      <c r="D39" s="149" t="s">
+        <v>1120</v>
+      </c>
+      <c r="E39" s="146" t="s">
+        <v>1127</v>
+      </c>
+      <c r="F39" s="135"/>
+    </row>
+    <row r="40" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+      <c r="A40" s="144" t="s">
+        <v>1033</v>
+      </c>
+      <c r="B40" s="148" t="s">
+        <v>1128</v>
+      </c>
+      <c r="C40" s="49" t="s">
+        <v>1129</v>
+      </c>
+      <c r="D40" s="149" t="s">
+        <v>1120</v>
+      </c>
+      <c r="E40" s="146" t="s">
+        <v>1130</v>
+      </c>
+      <c r="F40" s="135"/>
+    </row>
+    <row r="41" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+      <c r="A41" s="144" t="s">
+        <v>1033</v>
+      </c>
+      <c r="B41" s="148" t="s">
+        <v>1131</v>
+      </c>
+      <c r="C41" s="49" t="s">
+        <v>1132</v>
+      </c>
+      <c r="D41" s="149" t="s">
+        <v>1120</v>
+      </c>
+      <c r="E41" s="146" t="s">
+        <v>1133</v>
+      </c>
+      <c r="F41" s="135"/>
+    </row>
+    <row r="42" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+      <c r="A42" s="144" t="s">
+        <v>1033</v>
+      </c>
+      <c r="B42" s="148" t="s">
+        <v>1134</v>
+      </c>
+      <c r="C42" s="49" t="s">
+        <v>93</v>
+      </c>
+      <c r="D42" s="149" t="s">
+        <v>1120</v>
+      </c>
+      <c r="E42" s="146" t="s">
+        <v>95</v>
+      </c>
+      <c r="F42" s="135"/>
+    </row>
+    <row r="43" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+      <c r="A43" s="18" t="s">
+        <v>406</v>
+      </c>
+      <c r="B43" s="28" t="s">
+        <v>1135</v>
+      </c>
+      <c r="C43" s="51"/>
+      <c r="D43" s="18" t="s">
+        <v>985</v>
+      </c>
+      <c r="E43" s="146"/>
+      <c r="F43" s="135"/>
+    </row>
+    <row r="44" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+      <c r="A44" s="18" t="s">
+        <v>409</v>
+      </c>
+      <c r="B44" s="28" t="s">
+        <v>1136</v>
+      </c>
+      <c r="C44" s="27"/>
+      <c r="D44" s="18" t="s">
+        <v>978</v>
+      </c>
+      <c r="E44" s="146"/>
+      <c r="F44" s="135"/>
+    </row>
+    <row r="45" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+      <c r="A45" s="144" t="s">
+        <v>239</v>
+      </c>
+      <c r="B45" s="136" t="s">
+        <v>1137</v>
+      </c>
+      <c r="C45" s="62" t="s">
+        <v>1354</v>
+      </c>
+      <c r="D45" s="5" t="s">
+        <v>1138</v>
+      </c>
+      <c r="E45" s="146" t="s">
+        <v>1139</v>
+      </c>
+      <c r="F45" s="135"/>
+    </row>
+    <row r="46" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+      <c r="A46" s="18" t="s">
+        <v>406</v>
+      </c>
+      <c r="B46" s="28" t="s">
+        <v>1140</v>
+      </c>
+      <c r="C46" s="27"/>
+      <c r="D46" s="18" t="s">
+        <v>985</v>
+      </c>
+      <c r="E46" s="146"/>
+      <c r="F46" s="135"/>
+    </row>
+    <row r="47" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+      <c r="A47" s="18" t="s">
+        <v>409</v>
+      </c>
+      <c r="B47" s="28" t="s">
+        <v>1141</v>
+      </c>
+      <c r="C47" s="27"/>
+      <c r="D47" s="18" t="s">
+        <v>978</v>
+      </c>
+      <c r="E47" s="146"/>
+      <c r="F47" s="135"/>
+    </row>
+    <row r="48" spans="1:6" s="13" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A48" s="213" t="s">
+        <v>1142</v>
+      </c>
+      <c r="B48" s="214"/>
+      <c r="C48" s="214"/>
+      <c r="D48" s="214"/>
+      <c r="E48" s="215"/>
+    </row>
+    <row r="49" spans="1:6" s="30" customFormat="1" ht="64" x14ac:dyDescent="0.2">
+      <c r="A49" s="144" t="s">
+        <v>239</v>
+      </c>
+      <c r="B49" s="144" t="s">
+        <v>1143</v>
+      </c>
+      <c r="C49" s="62" t="s">
+        <v>846</v>
+      </c>
+      <c r="D49" s="116" t="s">
+        <v>1144</v>
+      </c>
+      <c r="E49" s="63" t="s">
+        <v>848</v>
+      </c>
+      <c r="F49" s="38" t="s">
+        <v>1145</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" s="30" customFormat="1" ht="64" x14ac:dyDescent="0.2">
+      <c r="A50" s="144" t="s">
+        <v>1146</v>
+      </c>
+      <c r="B50" s="144" t="s">
+        <v>1147</v>
+      </c>
+      <c r="C50" s="62" t="s">
+        <v>910</v>
+      </c>
+      <c r="D50" s="116" t="s">
+        <v>1148</v>
+      </c>
+      <c r="E50" s="63" t="s">
+        <v>911</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" s="30" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+      <c r="A51" s="144" t="s">
+        <v>1106</v>
+      </c>
+      <c r="B51" s="144" t="s">
+        <v>1149</v>
+      </c>
+      <c r="C51" s="62" t="s">
+        <v>1362</v>
+      </c>
+      <c r="D51" s="116" t="s">
+        <v>994</v>
+      </c>
+      <c r="E51" s="63" t="s">
+        <v>1363</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" s="30" customFormat="1" ht="48" x14ac:dyDescent="0.2">
+      <c r="A52" s="5" t="s">
+        <v>378</v>
+      </c>
+      <c r="B52" s="136" t="s">
+        <v>1150</v>
+      </c>
+      <c r="C52" s="145" t="s">
+        <v>1151</v>
+      </c>
+      <c r="D52" s="121" t="s">
+        <v>1152</v>
+      </c>
+      <c r="E52" s="63" t="s">
+        <v>1037</v>
+      </c>
+      <c r="F52" s="73" t="s">
+        <v>1153</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" s="30" customFormat="1" ht="48" x14ac:dyDescent="0.2">
+      <c r="A53" s="5" t="s">
+        <v>378</v>
+      </c>
+      <c r="B53" s="136" t="s">
+        <v>1154</v>
+      </c>
+      <c r="C53" s="145" t="s">
+        <v>1155</v>
+      </c>
+      <c r="D53" s="121" t="s">
+        <v>1156</v>
+      </c>
+      <c r="E53" s="63" t="s">
+        <v>1157</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" s="30" customFormat="1" ht="64" x14ac:dyDescent="0.2">
+      <c r="A54" s="5" t="s">
+        <v>378</v>
+      </c>
+      <c r="B54" s="136" t="s">
+        <v>1158</v>
+      </c>
+      <c r="C54" s="145" t="s">
+        <v>1159</v>
+      </c>
+      <c r="D54" s="121" t="s">
+        <v>1160</v>
+      </c>
+      <c r="E54" s="63" t="s">
+        <v>1161</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" s="30" customFormat="1" ht="64" x14ac:dyDescent="0.2">
+      <c r="A55" s="5" t="s">
+        <v>378</v>
+      </c>
+      <c r="B55" s="136" t="s">
+        <v>1162</v>
+      </c>
+      <c r="C55" s="145" t="s">
+        <v>1163</v>
+      </c>
+      <c r="D55" s="121" t="s">
+        <v>1164</v>
+      </c>
+      <c r="E55" s="63" t="s">
+        <v>1165</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" s="30" customFormat="1" ht="48" x14ac:dyDescent="0.2">
+      <c r="A56" s="5" t="s">
+        <v>378</v>
+      </c>
+      <c r="B56" s="136" t="s">
+        <v>1166</v>
+      </c>
+      <c r="C56" s="145" t="s">
+        <v>1167</v>
+      </c>
+      <c r="D56" s="121" t="s">
+        <v>1168</v>
+      </c>
+      <c r="E56" s="63" t="s">
+        <v>1169</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" s="30" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+      <c r="A57" s="5" t="s">
+        <v>378</v>
+      </c>
+      <c r="B57" s="136" t="s">
+        <v>1170</v>
+      </c>
+      <c r="C57" s="145" t="s">
+        <v>1171</v>
+      </c>
+      <c r="D57" s="121" t="s">
+        <v>1172</v>
+      </c>
+      <c r="E57" s="63" t="s">
+        <v>1063</v>
+      </c>
+      <c r="F57" s="73" t="s">
+        <v>1173</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" s="30" customFormat="1" ht="48" x14ac:dyDescent="0.2">
+      <c r="A58" s="5" t="s">
+        <v>378</v>
+      </c>
+      <c r="B58" s="136" t="s">
+        <v>1174</v>
+      </c>
+      <c r="C58" s="145" t="s">
+        <v>1175</v>
+      </c>
+      <c r="D58" s="121" t="s">
+        <v>1176</v>
+      </c>
+      <c r="E58" s="63" t="s">
+        <v>1177</v>
+      </c>
+      <c r="F58" s="73" t="s">
+        <v>1178</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" s="30" customFormat="1" ht="48" x14ac:dyDescent="0.2">
+      <c r="A59" s="5" t="s">
+        <v>378</v>
+      </c>
+      <c r="B59" s="136" t="s">
+        <v>1179</v>
+      </c>
+      <c r="C59" s="145" t="s">
+        <v>1180</v>
+      </c>
+      <c r="D59" s="121" t="s">
+        <v>1181</v>
+      </c>
+      <c r="E59" s="63" t="s">
+        <v>1182</v>
+      </c>
+      <c r="F59" s="73" t="s">
+        <v>1183</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" s="30" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+      <c r="A60" s="5" t="s">
+        <v>378</v>
+      </c>
+      <c r="B60" s="136" t="s">
+        <v>1184</v>
+      </c>
+      <c r="C60" s="145" t="s">
+        <v>1185</v>
+      </c>
+      <c r="D60" s="121" t="s">
+        <v>1186</v>
+      </c>
+      <c r="E60" s="63" t="s">
+        <v>1187</v>
+      </c>
+      <c r="F60" s="73" t="s">
+        <v>1188</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" s="30" customFormat="1" ht="48" x14ac:dyDescent="0.2">
+      <c r="A61" s="5" t="s">
+        <v>378</v>
+      </c>
+      <c r="B61" s="136" t="s">
+        <v>1189</v>
+      </c>
+      <c r="C61" s="145" t="s">
+        <v>1190</v>
+      </c>
+      <c r="D61" s="121" t="s">
+        <v>1191</v>
+      </c>
+      <c r="E61" s="63" t="s">
+        <v>1192</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" s="30" customFormat="1" ht="48" x14ac:dyDescent="0.2">
+      <c r="A62" s="5" t="s">
+        <v>378</v>
+      </c>
+      <c r="B62" s="136" t="s">
+        <v>1193</v>
+      </c>
+      <c r="C62" s="145" t="s">
+        <v>1194</v>
+      </c>
+      <c r="D62" s="121" t="s">
+        <v>1195</v>
+      </c>
+      <c r="E62" s="63" t="s">
+        <v>1196</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" s="30" customFormat="1" ht="48" x14ac:dyDescent="0.2">
+      <c r="A63" s="5" t="s">
+        <v>378</v>
+      </c>
+      <c r="B63" s="18" t="s">
+        <v>1197</v>
+      </c>
+      <c r="C63" s="145" t="s">
+        <v>1198</v>
+      </c>
+      <c r="D63" s="121" t="s">
+        <v>1199</v>
+      </c>
+      <c r="E63" s="63" t="s">
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" s="30" customFormat="1" ht="48" x14ac:dyDescent="0.2">
+      <c r="A64" s="5" t="s">
+        <v>378</v>
+      </c>
+      <c r="B64" s="136" t="s">
+        <v>1201</v>
+      </c>
+      <c r="C64" s="145" t="s">
+        <v>1202</v>
+      </c>
+      <c r="D64" s="121" t="s">
+        <v>1203</v>
+      </c>
+      <c r="E64" s="79" t="s">
+        <v>1204</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A65" s="144" t="s">
+        <v>721</v>
+      </c>
+      <c r="B65" s="144" t="s">
+        <v>1205</v>
+      </c>
+      <c r="C65" s="145" t="s">
+        <v>1206</v>
+      </c>
+      <c r="D65" s="148"/>
+      <c r="E65" s="78" t="s">
+        <v>1207</v>
+      </c>
+      <c r="F65" s="135"/>
+    </row>
+    <row r="66" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A66" s="144" t="s">
+        <v>721</v>
+      </c>
+      <c r="B66" s="144" t="s">
+        <v>1208</v>
+      </c>
+      <c r="C66" s="145" t="s">
+        <v>1132</v>
+      </c>
+      <c r="D66" s="148"/>
+      <c r="E66" s="78" t="s">
+        <v>1133</v>
+      </c>
+      <c r="F66" s="135"/>
+    </row>
+    <row r="67" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A67" s="144" t="s">
+        <v>721</v>
+      </c>
+      <c r="B67" s="136" t="s">
+        <v>1209</v>
+      </c>
+      <c r="C67" s="145" t="s">
+        <v>1119</v>
+      </c>
+      <c r="D67" s="148"/>
+      <c r="E67" s="78" t="s">
+        <v>1121</v>
+      </c>
+      <c r="F67" s="135"/>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A68" s="144"/>
+      <c r="B68" s="144"/>
+      <c r="C68" s="145"/>
+      <c r="D68" s="148"/>
+      <c r="E68" s="146"/>
+      <c r="F68" s="135"/>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A69" s="144"/>
+      <c r="B69" s="136"/>
+      <c r="C69" s="145"/>
+      <c r="D69" s="148"/>
+      <c r="E69" s="146"/>
+      <c r="F69" s="135"/>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A70" s="144"/>
+      <c r="B70" s="136"/>
+      <c r="C70" s="145"/>
+      <c r="D70" s="148"/>
+      <c r="E70" s="146"/>
+      <c r="F70" s="135"/>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A71" s="144"/>
+      <c r="B71" s="136"/>
+      <c r="C71" s="145"/>
+      <c r="D71" s="144"/>
+      <c r="E71" s="150"/>
+      <c r="F71" s="135"/>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A73" s="144"/>
+      <c r="B73" s="136"/>
+      <c r="C73" s="145"/>
+      <c r="D73" s="144"/>
+      <c r="E73" s="146"/>
+      <c r="F73" s="135"/>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A74" s="144"/>
+      <c r="B74" s="136"/>
+      <c r="C74" s="145"/>
+      <c r="D74" s="144"/>
+      <c r="E74" s="146"/>
+      <c r="F74" s="135"/>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A75" s="144"/>
+      <c r="B75" s="144"/>
+      <c r="C75" s="145"/>
+      <c r="D75" s="144"/>
+      <c r="E75" s="146"/>
+      <c r="F75" s="135"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A30:E30"/>
+    <mergeCell ref="A35:E35"/>
+    <mergeCell ref="A48:E48"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{609E324E-AF17-46CE-B967-049626EE1948}">
   <dimension ref="A1:F17"/>
   <sheetViews>
@@ -8387,7 +9652,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E52C375-4A34-4943-A40B-CD02CAD0761B}">
   <dimension ref="A1:F24"/>
   <sheetViews>
@@ -8819,11 +10084,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{124C2F8F-96ED-4E65-B816-FFFEB93DC889}">
   <dimension ref="A1:F41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A36" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D40" sqref="D40"/>
     </sheetView>
@@ -9416,11 +10681,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F72"/>
+  <dimension ref="A1:F74"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D3" sqref="D3"/>
+      <pane ySplit="1" topLeftCell="A61" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B75" sqref="B75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -10612,6 +11877,28 @@
       </c>
       <c r="E72" s="40" t="s">
         <v>1430</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="B73" s="1" t="s">
+        <v>1577</v>
+      </c>
+      <c r="C73" s="2" t="s">
+        <v>1578</v>
+      </c>
+      <c r="E73" s="40" t="s">
+        <v>1579</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="B74" s="1" t="s">
+        <v>1580</v>
+      </c>
+      <c r="C74" s="2" t="s">
+        <v>1581</v>
+      </c>
+      <c r="E74" s="40" t="s">
+        <v>1582</v>
       </c>
     </row>
   </sheetData>
@@ -10869,7 +12156,7 @@
   <dimension ref="A1:F27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -11171,11 +12458,254 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A815E382-9B20-F542-848C-24BE43C046DB}">
+  <dimension ref="A1:F22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="16.5" customWidth="1"/>
+    <col min="2" max="2" width="37.33203125" customWidth="1"/>
+    <col min="3" max="3" width="33.5" style="224" customWidth="1"/>
+    <col min="4" max="4" width="20.1640625" customWidth="1"/>
+    <col min="5" max="5" width="60.6640625" customWidth="1"/>
+    <col min="6" max="6" width="21.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="222" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="39" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" s="186" t="s">
+        <v>1583</v>
+      </c>
+      <c r="B2" s="187"/>
+      <c r="C2" s="187"/>
+      <c r="D2" s="187"/>
+      <c r="E2" s="188"/>
+    </row>
+    <row r="3" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+      <c r="A3" s="5" t="s">
+        <v>1584</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>1586</v>
+      </c>
+      <c r="C3" s="223" t="s">
+        <v>1585</v>
+      </c>
+      <c r="D3" s="5"/>
+      <c r="E3" s="43" t="s">
+        <v>1591</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="96" x14ac:dyDescent="0.2">
+      <c r="A4" s="5" t="s">
+        <v>1584</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>1589</v>
+      </c>
+      <c r="C4" s="223" t="s">
+        <v>1587</v>
+      </c>
+      <c r="D4" s="5"/>
+      <c r="E4" s="43" t="s">
+        <v>1592</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="64" x14ac:dyDescent="0.2">
+      <c r="A5" s="5" t="s">
+        <v>1584</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>1590</v>
+      </c>
+      <c r="C5" s="223" t="s">
+        <v>1588</v>
+      </c>
+      <c r="D5" s="5"/>
+      <c r="E5" s="43" t="s">
+        <v>1593</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+      <c r="A6" s="5" t="s">
+        <v>1584</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>1595</v>
+      </c>
+      <c r="C6" s="223" t="s">
+        <v>1594</v>
+      </c>
+      <c r="D6" s="5"/>
+      <c r="E6" s="43" t="s">
+        <v>1596</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="80" x14ac:dyDescent="0.2">
+      <c r="A7" s="5" t="s">
+        <v>1584</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>1597</v>
+      </c>
+      <c r="C7" s="223" t="s">
+        <v>1598</v>
+      </c>
+      <c r="D7" s="5"/>
+      <c r="E7" s="43" t="s">
+        <v>1601</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="96" x14ac:dyDescent="0.2">
+      <c r="A8" s="5" t="s">
+        <v>1584</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>1599</v>
+      </c>
+      <c r="C8" s="223" t="s">
+        <v>1600</v>
+      </c>
+      <c r="D8" s="5"/>
+      <c r="E8" s="43" t="s">
+        <v>1602</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" s="5"/>
+      <c r="B9" s="5"/>
+      <c r="C9" s="223"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="43"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" s="5"/>
+      <c r="B10" s="5"/>
+      <c r="C10" s="223"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="43"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" s="5"/>
+      <c r="B11" s="5"/>
+      <c r="C11" s="223"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="43"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" s="5"/>
+      <c r="B12" s="5"/>
+      <c r="C12" s="223"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="43"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" s="5"/>
+      <c r="B13" s="5"/>
+      <c r="C13" s="223"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="43"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14" s="5"/>
+      <c r="B14" s="5"/>
+      <c r="C14" s="223"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="43"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15" s="5"/>
+      <c r="B15" s="5"/>
+      <c r="C15" s="223"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="43"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16" s="5"/>
+      <c r="B16" s="5"/>
+      <c r="C16" s="223"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="43"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17" s="5"/>
+      <c r="B17" s="5"/>
+      <c r="C17" s="223"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="43"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18" s="5"/>
+      <c r="B18" s="5"/>
+      <c r="C18" s="223"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="43"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19" s="5"/>
+      <c r="B19" s="5"/>
+      <c r="C19" s="223"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="43"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20" s="5"/>
+      <c r="B20" s="5"/>
+      <c r="C20" s="223"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="43"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21" s="5"/>
+      <c r="B21" s="5"/>
+      <c r="C21" s="223"/>
+      <c r="D21" s="5"/>
+      <c r="E21" s="43"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22" s="5"/>
+      <c r="B22" s="5"/>
+      <c r="C22" s="223"/>
+      <c r="D22" s="5"/>
+      <c r="E22" s="43"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A2:E2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{344327F7-D7B0-4B8B-A26A-307F32EA23BD}">
   <dimension ref="A1:F31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
@@ -11695,7 +13225,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B63483B8-55BE-4CA0-9111-55E5C0AEF6CB}">
   <dimension ref="A1:F367"/>
   <sheetViews>
@@ -11736,13 +13266,13 @@
       </c>
     </row>
     <row r="2" spans="1:6" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="189" t="s">
+      <c r="A2" s="192" t="s">
         <v>363</v>
       </c>
-      <c r="B2" s="190"/>
-      <c r="C2" s="190"/>
-      <c r="D2" s="190"/>
-      <c r="E2" s="191"/>
+      <c r="B2" s="193"/>
+      <c r="C2" s="193"/>
+      <c r="D2" s="193"/>
+      <c r="E2" s="194"/>
       <c r="F2" s="33"/>
     </row>
     <row r="3" spans="1:6" ht="48" x14ac:dyDescent="0.2">
@@ -11886,13 +13416,13 @@
       <c r="F10" s="119"/>
     </row>
     <row r="11" spans="1:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="192" t="s">
+      <c r="A11" s="195" t="s">
         <v>392</v>
       </c>
-      <c r="B11" s="193"/>
-      <c r="C11" s="193"/>
-      <c r="D11" s="193"/>
-      <c r="E11" s="194"/>
+      <c r="B11" s="196"/>
+      <c r="C11" s="196"/>
+      <c r="D11" s="196"/>
+      <c r="E11" s="197"/>
       <c r="F11" s="119"/>
     </row>
     <row r="12" spans="1:6" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -14450,13 +15980,13 @@
       </c>
     </row>
     <row r="180" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A180" s="195" t="s">
+      <c r="A180" s="189" t="s">
         <v>754</v>
       </c>
-      <c r="B180" s="196"/>
-      <c r="C180" s="196"/>
-      <c r="D180" s="196"/>
-      <c r="E180" s="197"/>
+      <c r="B180" s="190"/>
+      <c r="C180" s="190"/>
+      <c r="D180" s="190"/>
+      <c r="E180" s="191"/>
       <c r="F180" s="129" t="s">
         <v>758</v>
       </c>
@@ -16468,6 +17998,19 @@
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="A247:E247"/>
+    <mergeCell ref="A207:E207"/>
+    <mergeCell ref="A211:E211"/>
+    <mergeCell ref="A219:E219"/>
+    <mergeCell ref="A230:E230"/>
+    <mergeCell ref="A236:E236"/>
+    <mergeCell ref="A65:E65"/>
+    <mergeCell ref="A2:E2"/>
+    <mergeCell ref="A11:E11"/>
+    <mergeCell ref="A15:E15"/>
+    <mergeCell ref="A30:E30"/>
+    <mergeCell ref="A49:E49"/>
+    <mergeCell ref="A25:E25"/>
     <mergeCell ref="A194:E194"/>
     <mergeCell ref="A172:E172"/>
     <mergeCell ref="A70:E70"/>
@@ -16479,25 +18022,12 @@
     <mergeCell ref="A100:E100"/>
     <mergeCell ref="A180:E180"/>
     <mergeCell ref="A190:E190"/>
-    <mergeCell ref="A65:E65"/>
-    <mergeCell ref="A2:E2"/>
-    <mergeCell ref="A11:E11"/>
-    <mergeCell ref="A15:E15"/>
-    <mergeCell ref="A30:E30"/>
-    <mergeCell ref="A49:E49"/>
-    <mergeCell ref="A25:E25"/>
-    <mergeCell ref="A247:E247"/>
-    <mergeCell ref="A207:E207"/>
-    <mergeCell ref="A211:E211"/>
-    <mergeCell ref="A219:E219"/>
-    <mergeCell ref="A230:E230"/>
-    <mergeCell ref="A236:E236"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E7FE5E2-8B99-45DF-8804-30523FDA4B3A}">
   <dimension ref="A1:F56"/>
   <sheetViews>
@@ -17343,1185 +18873,6 @@
     <mergeCell ref="A25:E25"/>
     <mergeCell ref="A27:E27"/>
     <mergeCell ref="A21:E21"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6CA2FE89-1BCA-4888-9BB6-D7A7737E07E4}">
-  <dimension ref="A1:F75"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C13" sqref="C13"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="33.6640625" style="16" customWidth="1"/>
-    <col min="2" max="2" width="59.33203125" style="16" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="33.6640625" style="17" customWidth="1"/>
-    <col min="4" max="4" width="39.5" style="16" customWidth="1"/>
-    <col min="5" max="5" width="33.6640625" style="48" customWidth="1"/>
-    <col min="6" max="6" width="24.83203125" style="12" customWidth="1"/>
-    <col min="7" max="16384" width="9.1640625" style="12"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A1" s="14" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" s="15" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="E1" s="47" t="s">
-        <v>5</v>
-      </c>
-      <c r="F1" s="135" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A2" s="136" t="s">
-        <v>239</v>
-      </c>
-      <c r="B2" s="136" t="s">
-        <v>1026</v>
-      </c>
-      <c r="C2" s="137" t="s">
-        <v>1027</v>
-      </c>
-      <c r="D2" s="136" t="s">
-        <v>242</v>
-      </c>
-      <c r="E2" s="138" t="s">
-        <v>1028</v>
-      </c>
-      <c r="F2" s="135"/>
-    </row>
-    <row r="3" spans="1:6" ht="32" x14ac:dyDescent="0.2">
-      <c r="A3" s="136" t="s">
-        <v>940</v>
-      </c>
-      <c r="B3" s="136" t="s">
-        <v>1029</v>
-      </c>
-      <c r="C3" s="137" t="s">
-        <v>1030</v>
-      </c>
-      <c r="D3" s="136" t="s">
-        <v>1031</v>
-      </c>
-      <c r="E3" s="138" t="s">
-        <v>1032</v>
-      </c>
-      <c r="F3" s="135"/>
-    </row>
-    <row r="4" spans="1:6" ht="32" x14ac:dyDescent="0.2">
-      <c r="A4" s="136" t="s">
-        <v>1033</v>
-      </c>
-      <c r="B4" s="136" t="s">
-        <v>1034</v>
-      </c>
-      <c r="C4" s="137" t="s">
-        <v>1035</v>
-      </c>
-      <c r="D4" s="136" t="s">
-        <v>1036</v>
-      </c>
-      <c r="E4" s="138" t="s">
-        <v>1037</v>
-      </c>
-      <c r="F4" s="135"/>
-    </row>
-    <row r="5" spans="1:6" ht="48" x14ac:dyDescent="0.2">
-      <c r="A5" s="136" t="s">
-        <v>406</v>
-      </c>
-      <c r="B5" s="139" t="s">
-        <v>1038</v>
-      </c>
-      <c r="C5" s="27"/>
-      <c r="D5" s="136" t="s">
-        <v>1039</v>
-      </c>
-      <c r="E5" s="138"/>
-      <c r="F5" s="135"/>
-    </row>
-    <row r="6" spans="1:6" ht="48" x14ac:dyDescent="0.2">
-      <c r="A6" s="136" t="s">
-        <v>409</v>
-      </c>
-      <c r="B6" s="139" t="s">
-        <v>1040</v>
-      </c>
-      <c r="C6" s="27"/>
-      <c r="D6" s="136" t="s">
-        <v>1041</v>
-      </c>
-      <c r="E6" s="138"/>
-      <c r="F6" s="135"/>
-    </row>
-    <row r="7" spans="1:6" ht="48" x14ac:dyDescent="0.2">
-      <c r="A7" s="136" t="s">
-        <v>1033</v>
-      </c>
-      <c r="B7" s="136" t="s">
-        <v>1042</v>
-      </c>
-      <c r="C7" s="137" t="s">
-        <v>1043</v>
-      </c>
-      <c r="D7" s="136" t="s">
-        <v>1044</v>
-      </c>
-      <c r="E7" s="138" t="s">
-        <v>1045</v>
-      </c>
-      <c r="F7" s="135"/>
-    </row>
-    <row r="8" spans="1:6" ht="48" x14ac:dyDescent="0.2">
-      <c r="A8" s="136" t="s">
-        <v>1033</v>
-      </c>
-      <c r="B8" s="136" t="s">
-        <v>1046</v>
-      </c>
-      <c r="C8" s="137" t="s">
-        <v>1047</v>
-      </c>
-      <c r="D8" s="136" t="s">
-        <v>1048</v>
-      </c>
-      <c r="E8" s="138" t="s">
-        <v>1049</v>
-      </c>
-      <c r="F8" s="135"/>
-    </row>
-    <row r="9" spans="1:6" ht="48" x14ac:dyDescent="0.2">
-      <c r="A9" s="136" t="s">
-        <v>1033</v>
-      </c>
-      <c r="B9" s="136" t="s">
-        <v>1050</v>
-      </c>
-      <c r="C9" s="137" t="s">
-        <v>1051</v>
-      </c>
-      <c r="D9" s="136" t="s">
-        <v>1052</v>
-      </c>
-      <c r="E9" s="138" t="s">
-        <v>1053</v>
-      </c>
-      <c r="F9" s="135"/>
-    </row>
-    <row r="10" spans="1:6" ht="64" x14ac:dyDescent="0.2">
-      <c r="A10" s="136" t="s">
-        <v>1033</v>
-      </c>
-      <c r="B10" s="136" t="s">
-        <v>1054</v>
-      </c>
-      <c r="C10" s="137" t="s">
-        <v>1055</v>
-      </c>
-      <c r="D10" s="136" t="s">
-        <v>1056</v>
-      </c>
-      <c r="E10" s="138" t="s">
-        <v>1057</v>
-      </c>
-      <c r="F10" s="135"/>
-    </row>
-    <row r="11" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A11" s="136" t="s">
-        <v>250</v>
-      </c>
-      <c r="B11" s="136" t="s">
-        <v>1058</v>
-      </c>
-      <c r="C11" s="137" t="s">
-        <v>1059</v>
-      </c>
-      <c r="D11" s="136" t="s">
-        <v>1060</v>
-      </c>
-      <c r="E11" s="138" t="s">
-        <v>1386</v>
-      </c>
-      <c r="F11" s="135"/>
-    </row>
-    <row r="12" spans="1:6" ht="48" x14ac:dyDescent="0.2">
-      <c r="A12" s="136" t="s">
-        <v>1382</v>
-      </c>
-      <c r="B12" s="136" t="s">
-        <v>1383</v>
-      </c>
-      <c r="C12" s="137" t="s">
-        <v>1384</v>
-      </c>
-      <c r="D12" s="136"/>
-      <c r="E12" s="138" t="s">
-        <v>1385</v>
-      </c>
-      <c r="F12" s="135"/>
-    </row>
-    <row r="13" spans="1:6" ht="32" x14ac:dyDescent="0.2">
-      <c r="A13" s="136" t="s">
-        <v>1033</v>
-      </c>
-      <c r="B13" s="136" t="s">
-        <v>1061</v>
-      </c>
-      <c r="C13" s="137" t="s">
-        <v>1450</v>
-      </c>
-      <c r="D13" s="136" t="s">
-        <v>1062</v>
-      </c>
-      <c r="E13" s="138" t="s">
-        <v>1063</v>
-      </c>
-      <c r="F13" s="135"/>
-    </row>
-    <row r="14" spans="1:6" ht="48" x14ac:dyDescent="0.2">
-      <c r="A14" s="136" t="s">
-        <v>406</v>
-      </c>
-      <c r="B14" s="28" t="s">
-        <v>1064</v>
-      </c>
-      <c r="C14" s="138"/>
-      <c r="D14" s="136" t="s">
-        <v>1065</v>
-      </c>
-      <c r="E14" s="138"/>
-      <c r="F14" s="135"/>
-    </row>
-    <row r="15" spans="1:6" ht="48" x14ac:dyDescent="0.2">
-      <c r="A15" s="136" t="s">
-        <v>409</v>
-      </c>
-      <c r="B15" s="28" t="s">
-        <v>1066</v>
-      </c>
-      <c r="C15" s="138"/>
-      <c r="D15" s="136" t="s">
-        <v>1041</v>
-      </c>
-      <c r="E15" s="138"/>
-      <c r="F15" s="135"/>
-    </row>
-    <row r="16" spans="1:6" ht="32" x14ac:dyDescent="0.2">
-      <c r="A16" s="136" t="s">
-        <v>1033</v>
-      </c>
-      <c r="B16" s="136" t="s">
-        <v>1067</v>
-      </c>
-      <c r="C16" s="137" t="s">
-        <v>1378</v>
-      </c>
-      <c r="D16" s="136" t="s">
-        <v>1068</v>
-      </c>
-      <c r="E16" s="138" t="s">
-        <v>1069</v>
-      </c>
-      <c r="F16" s="135"/>
-    </row>
-    <row r="17" spans="1:6" ht="32" x14ac:dyDescent="0.2">
-      <c r="A17" s="136" t="s">
-        <v>1033</v>
-      </c>
-      <c r="B17" s="136" t="s">
-        <v>1070</v>
-      </c>
-      <c r="C17" s="137" t="s">
-        <v>1379</v>
-      </c>
-      <c r="D17" s="136" t="s">
-        <v>1071</v>
-      </c>
-      <c r="E17" s="138" t="s">
-        <v>1072</v>
-      </c>
-      <c r="F17" s="135"/>
-    </row>
-    <row r="18" spans="1:6" ht="32" x14ac:dyDescent="0.2">
-      <c r="A18" s="136" t="s">
-        <v>1033</v>
-      </c>
-      <c r="B18" s="136" t="s">
-        <v>1073</v>
-      </c>
-      <c r="C18" s="137" t="s">
-        <v>1380</v>
-      </c>
-      <c r="D18" s="136" t="s">
-        <v>1074</v>
-      </c>
-      <c r="E18" s="138" t="s">
-        <v>1075</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" ht="144" x14ac:dyDescent="0.2">
-      <c r="A19" s="136" t="s">
-        <v>1033</v>
-      </c>
-      <c r="B19" s="136" t="s">
-        <v>1076</v>
-      </c>
-      <c r="C19" s="137" t="s">
-        <v>1077</v>
-      </c>
-      <c r="D19" s="29" t="s">
-        <v>1078</v>
-      </c>
-      <c r="E19" s="138" t="s">
-        <v>1079</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" ht="80" x14ac:dyDescent="0.2">
-      <c r="A20" s="136" t="s">
-        <v>406</v>
-      </c>
-      <c r="B20" s="28" t="s">
-        <v>1080</v>
-      </c>
-      <c r="C20" s="27"/>
-      <c r="D20" s="18" t="s">
-        <v>1081</v>
-      </c>
-      <c r="E20" s="138"/>
-    </row>
-    <row r="21" spans="1:6" ht="48" x14ac:dyDescent="0.2">
-      <c r="A21" s="136" t="s">
-        <v>409</v>
-      </c>
-      <c r="B21" s="28" t="s">
-        <v>1082</v>
-      </c>
-      <c r="C21" s="27"/>
-      <c r="D21" s="18" t="s">
-        <v>1041</v>
-      </c>
-      <c r="E21" s="138"/>
-    </row>
-    <row r="22" spans="1:6" ht="32" x14ac:dyDescent="0.2">
-      <c r="A22" s="136" t="s">
-        <v>409</v>
-      </c>
-      <c r="B22" s="28" t="s">
-        <v>1083</v>
-      </c>
-      <c r="C22" s="27"/>
-      <c r="D22" s="18" t="s">
-        <v>1084</v>
-      </c>
-      <c r="E22" s="138"/>
-    </row>
-    <row r="23" spans="1:6" ht="112" x14ac:dyDescent="0.2">
-      <c r="A23" s="136" t="s">
-        <v>1085</v>
-      </c>
-      <c r="B23" s="136" t="s">
-        <v>1086</v>
-      </c>
-      <c r="C23" s="137" t="s">
-        <v>1087</v>
-      </c>
-      <c r="D23" s="136" t="s">
-        <v>1088</v>
-      </c>
-      <c r="E23" s="138" t="s">
-        <v>1089</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" ht="48" x14ac:dyDescent="0.2">
-      <c r="A24" s="136" t="s">
-        <v>406</v>
-      </c>
-      <c r="B24" s="28" t="s">
-        <v>1090</v>
-      </c>
-      <c r="C24" s="27"/>
-      <c r="D24" s="136" t="s">
-        <v>1091</v>
-      </c>
-      <c r="E24" s="138"/>
-    </row>
-    <row r="25" spans="1:6" ht="32" x14ac:dyDescent="0.2">
-      <c r="A25" s="136" t="s">
-        <v>409</v>
-      </c>
-      <c r="B25" s="28" t="s">
-        <v>1092</v>
-      </c>
-      <c r="C25" s="27"/>
-      <c r="D25" s="136" t="s">
-        <v>1093</v>
-      </c>
-      <c r="E25" s="138"/>
-    </row>
-    <row r="26" spans="1:6" ht="64" x14ac:dyDescent="0.2">
-      <c r="A26" s="136" t="s">
-        <v>409</v>
-      </c>
-      <c r="B26" s="28" t="s">
-        <v>1094</v>
-      </c>
-      <c r="C26" s="27"/>
-      <c r="D26" s="29" t="s">
-        <v>1095</v>
-      </c>
-      <c r="E26" s="138"/>
-    </row>
-    <row r="27" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A27" s="136" t="s">
-        <v>250</v>
-      </c>
-      <c r="B27" s="136" t="s">
-        <v>1096</v>
-      </c>
-      <c r="C27" s="137" t="s">
-        <v>1097</v>
-      </c>
-      <c r="D27" s="136" t="s">
-        <v>1060</v>
-      </c>
-      <c r="E27" s="138" t="s">
-        <v>1098</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" ht="64" x14ac:dyDescent="0.2">
-      <c r="A28" s="136" t="s">
-        <v>1382</v>
-      </c>
-      <c r="B28" s="136" t="s">
-        <v>1381</v>
-      </c>
-      <c r="C28" s="137" t="s">
-        <v>1403</v>
-      </c>
-      <c r="D28" s="136"/>
-      <c r="E28" s="138" t="s">
-        <v>1405</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" ht="32" x14ac:dyDescent="0.2">
-      <c r="A29" s="136" t="s">
-        <v>1033</v>
-      </c>
-      <c r="B29" s="136" t="s">
-        <v>1099</v>
-      </c>
-      <c r="C29" s="137" t="s">
-        <v>1404</v>
-      </c>
-      <c r="D29" s="136" t="s">
-        <v>1100</v>
-      </c>
-      <c r="E29" s="138" t="s">
-        <v>1406</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" s="13" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="213" t="s">
-        <v>1101</v>
-      </c>
-      <c r="B30" s="214"/>
-      <c r="C30" s="214"/>
-      <c r="D30" s="214"/>
-      <c r="E30" s="215"/>
-    </row>
-    <row r="31" spans="1:6" ht="48" x14ac:dyDescent="0.2">
-      <c r="A31" s="140" t="s">
-        <v>239</v>
-      </c>
-      <c r="B31" s="141" t="s">
-        <v>1102</v>
-      </c>
-      <c r="C31" s="142" t="s">
-        <v>1103</v>
-      </c>
-      <c r="D31" s="5" t="s">
-        <v>1104</v>
-      </c>
-      <c r="E31" s="143" t="s">
-        <v>1105</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" ht="64" x14ac:dyDescent="0.2">
-      <c r="A32" s="144" t="s">
-        <v>1106</v>
-      </c>
-      <c r="B32" s="144" t="s">
-        <v>1107</v>
-      </c>
-      <c r="C32" s="145" t="s">
-        <v>1108</v>
-      </c>
-      <c r="D32" s="144" t="s">
-        <v>1109</v>
-      </c>
-      <c r="E32" s="146" t="s">
-        <v>1110</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" ht="48" x14ac:dyDescent="0.2">
-      <c r="A33" s="18" t="s">
-        <v>406</v>
-      </c>
-      <c r="B33" s="28" t="s">
-        <v>1111</v>
-      </c>
-      <c r="C33" s="27"/>
-      <c r="D33" s="18" t="s">
-        <v>985</v>
-      </c>
-      <c r="E33" s="146"/>
-    </row>
-    <row r="34" spans="1:6" ht="48" x14ac:dyDescent="0.2">
-      <c r="A34" s="18" t="s">
-        <v>409</v>
-      </c>
-      <c r="B34" s="28" t="s">
-        <v>1112</v>
-      </c>
-      <c r="C34" s="27"/>
-      <c r="D34" s="18" t="s">
-        <v>978</v>
-      </c>
-      <c r="E34" s="146"/>
-    </row>
-    <row r="35" spans="1:6" s="13" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="216" t="s">
-        <v>1113</v>
-      </c>
-      <c r="B35" s="217"/>
-      <c r="C35" s="218"/>
-      <c r="D35" s="217"/>
-      <c r="E35" s="219"/>
-    </row>
-    <row r="36" spans="1:6" ht="32" x14ac:dyDescent="0.2">
-      <c r="A36" s="144" t="s">
-        <v>239</v>
-      </c>
-      <c r="B36" s="147" t="s">
-        <v>1114</v>
-      </c>
-      <c r="C36" s="145" t="s">
-        <v>1115</v>
-      </c>
-      <c r="D36" s="50" t="s">
-        <v>1116</v>
-      </c>
-      <c r="E36" s="146" t="s">
-        <v>1117</v>
-      </c>
-      <c r="F36" s="135"/>
-    </row>
-    <row r="37" spans="1:6" ht="32" x14ac:dyDescent="0.2">
-      <c r="A37" s="144" t="s">
-        <v>1033</v>
-      </c>
-      <c r="B37" s="148" t="s">
-        <v>1118</v>
-      </c>
-      <c r="C37" s="145" t="s">
-        <v>1119</v>
-      </c>
-      <c r="D37" s="149" t="s">
-        <v>1120</v>
-      </c>
-      <c r="E37" s="146" t="s">
-        <v>1121</v>
-      </c>
-      <c r="F37" s="135"/>
-    </row>
-    <row r="38" spans="1:6" ht="32" x14ac:dyDescent="0.2">
-      <c r="A38" s="144" t="s">
-        <v>1033</v>
-      </c>
-      <c r="B38" s="148" t="s">
-        <v>1122</v>
-      </c>
-      <c r="C38" s="145" t="s">
-        <v>1123</v>
-      </c>
-      <c r="D38" s="149" t="s">
-        <v>1120</v>
-      </c>
-      <c r="E38" s="146" t="s">
-        <v>1124</v>
-      </c>
-      <c r="F38" s="135"/>
-    </row>
-    <row r="39" spans="1:6" ht="32" x14ac:dyDescent="0.2">
-      <c r="A39" s="144" t="s">
-        <v>1033</v>
-      </c>
-      <c r="B39" s="148" t="s">
-        <v>1125</v>
-      </c>
-      <c r="C39" s="49" t="s">
-        <v>1126</v>
-      </c>
-      <c r="D39" s="149" t="s">
-        <v>1120</v>
-      </c>
-      <c r="E39" s="146" t="s">
-        <v>1127</v>
-      </c>
-      <c r="F39" s="135"/>
-    </row>
-    <row r="40" spans="1:6" ht="32" x14ac:dyDescent="0.2">
-      <c r="A40" s="144" t="s">
-        <v>1033</v>
-      </c>
-      <c r="B40" s="148" t="s">
-        <v>1128</v>
-      </c>
-      <c r="C40" s="49" t="s">
-        <v>1129</v>
-      </c>
-      <c r="D40" s="149" t="s">
-        <v>1120</v>
-      </c>
-      <c r="E40" s="146" t="s">
-        <v>1130</v>
-      </c>
-      <c r="F40" s="135"/>
-    </row>
-    <row r="41" spans="1:6" ht="32" x14ac:dyDescent="0.2">
-      <c r="A41" s="144" t="s">
-        <v>1033</v>
-      </c>
-      <c r="B41" s="148" t="s">
-        <v>1131</v>
-      </c>
-      <c r="C41" s="49" t="s">
-        <v>1132</v>
-      </c>
-      <c r="D41" s="149" t="s">
-        <v>1120</v>
-      </c>
-      <c r="E41" s="146" t="s">
-        <v>1133</v>
-      </c>
-      <c r="F41" s="135"/>
-    </row>
-    <row r="42" spans="1:6" ht="32" x14ac:dyDescent="0.2">
-      <c r="A42" s="144" t="s">
-        <v>1033</v>
-      </c>
-      <c r="B42" s="148" t="s">
-        <v>1134</v>
-      </c>
-      <c r="C42" s="49" t="s">
-        <v>93</v>
-      </c>
-      <c r="D42" s="149" t="s">
-        <v>1120</v>
-      </c>
-      <c r="E42" s="146" t="s">
-        <v>95</v>
-      </c>
-      <c r="F42" s="135"/>
-    </row>
-    <row r="43" spans="1:6" ht="48" x14ac:dyDescent="0.2">
-      <c r="A43" s="18" t="s">
-        <v>406</v>
-      </c>
-      <c r="B43" s="28" t="s">
-        <v>1135</v>
-      </c>
-      <c r="C43" s="51"/>
-      <c r="D43" s="18" t="s">
-        <v>985</v>
-      </c>
-      <c r="E43" s="146"/>
-      <c r="F43" s="135"/>
-    </row>
-    <row r="44" spans="1:6" ht="48" x14ac:dyDescent="0.2">
-      <c r="A44" s="18" t="s">
-        <v>409</v>
-      </c>
-      <c r="B44" s="28" t="s">
-        <v>1136</v>
-      </c>
-      <c r="C44" s="27"/>
-      <c r="D44" s="18" t="s">
-        <v>978</v>
-      </c>
-      <c r="E44" s="146"/>
-      <c r="F44" s="135"/>
-    </row>
-    <row r="45" spans="1:6" ht="48" x14ac:dyDescent="0.2">
-      <c r="A45" s="144" t="s">
-        <v>239</v>
-      </c>
-      <c r="B45" s="136" t="s">
-        <v>1137</v>
-      </c>
-      <c r="C45" s="62" t="s">
-        <v>1354</v>
-      </c>
-      <c r="D45" s="5" t="s">
-        <v>1138</v>
-      </c>
-      <c r="E45" s="146" t="s">
-        <v>1139</v>
-      </c>
-      <c r="F45" s="135"/>
-    </row>
-    <row r="46" spans="1:6" ht="48" x14ac:dyDescent="0.2">
-      <c r="A46" s="18" t="s">
-        <v>406</v>
-      </c>
-      <c r="B46" s="28" t="s">
-        <v>1140</v>
-      </c>
-      <c r="C46" s="27"/>
-      <c r="D46" s="18" t="s">
-        <v>985</v>
-      </c>
-      <c r="E46" s="146"/>
-      <c r="F46" s="135"/>
-    </row>
-    <row r="47" spans="1:6" ht="48" x14ac:dyDescent="0.2">
-      <c r="A47" s="18" t="s">
-        <v>409</v>
-      </c>
-      <c r="B47" s="28" t="s">
-        <v>1141</v>
-      </c>
-      <c r="C47" s="27"/>
-      <c r="D47" s="18" t="s">
-        <v>978</v>
-      </c>
-      <c r="E47" s="146"/>
-      <c r="F47" s="135"/>
-    </row>
-    <row r="48" spans="1:6" s="13" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="213" t="s">
-        <v>1142</v>
-      </c>
-      <c r="B48" s="214"/>
-      <c r="C48" s="214"/>
-      <c r="D48" s="214"/>
-      <c r="E48" s="215"/>
-    </row>
-    <row r="49" spans="1:6" s="30" customFormat="1" ht="64" x14ac:dyDescent="0.2">
-      <c r="A49" s="144" t="s">
-        <v>239</v>
-      </c>
-      <c r="B49" s="144" t="s">
-        <v>1143</v>
-      </c>
-      <c r="C49" s="62" t="s">
-        <v>846</v>
-      </c>
-      <c r="D49" s="116" t="s">
-        <v>1144</v>
-      </c>
-      <c r="E49" s="63" t="s">
-        <v>848</v>
-      </c>
-      <c r="F49" s="38" t="s">
-        <v>1145</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" s="30" customFormat="1" ht="64" x14ac:dyDescent="0.2">
-      <c r="A50" s="144" t="s">
-        <v>1146</v>
-      </c>
-      <c r="B50" s="144" t="s">
-        <v>1147</v>
-      </c>
-      <c r="C50" s="62" t="s">
-        <v>910</v>
-      </c>
-      <c r="D50" s="116" t="s">
-        <v>1148</v>
-      </c>
-      <c r="E50" s="63" t="s">
-        <v>911</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" s="30" customFormat="1" ht="32" x14ac:dyDescent="0.2">
-      <c r="A51" s="144" t="s">
-        <v>1106</v>
-      </c>
-      <c r="B51" s="144" t="s">
-        <v>1149</v>
-      </c>
-      <c r="C51" s="62" t="s">
-        <v>1362</v>
-      </c>
-      <c r="D51" s="116" t="s">
-        <v>994</v>
-      </c>
-      <c r="E51" s="63" t="s">
-        <v>1363</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" s="30" customFormat="1" ht="48" x14ac:dyDescent="0.2">
-      <c r="A52" s="5" t="s">
-        <v>378</v>
-      </c>
-      <c r="B52" s="136" t="s">
-        <v>1150</v>
-      </c>
-      <c r="C52" s="145" t="s">
-        <v>1151</v>
-      </c>
-      <c r="D52" s="121" t="s">
-        <v>1152</v>
-      </c>
-      <c r="E52" s="63" t="s">
-        <v>1037</v>
-      </c>
-      <c r="F52" s="73" t="s">
-        <v>1153</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" s="30" customFormat="1" ht="48" x14ac:dyDescent="0.2">
-      <c r="A53" s="5" t="s">
-        <v>378</v>
-      </c>
-      <c r="B53" s="136" t="s">
-        <v>1154</v>
-      </c>
-      <c r="C53" s="145" t="s">
-        <v>1155</v>
-      </c>
-      <c r="D53" s="121" t="s">
-        <v>1156</v>
-      </c>
-      <c r="E53" s="63" t="s">
-        <v>1157</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" s="30" customFormat="1" ht="64" x14ac:dyDescent="0.2">
-      <c r="A54" s="5" t="s">
-        <v>378</v>
-      </c>
-      <c r="B54" s="136" t="s">
-        <v>1158</v>
-      </c>
-      <c r="C54" s="145" t="s">
-        <v>1159</v>
-      </c>
-      <c r="D54" s="121" t="s">
-        <v>1160</v>
-      </c>
-      <c r="E54" s="63" t="s">
-        <v>1161</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" s="30" customFormat="1" ht="64" x14ac:dyDescent="0.2">
-      <c r="A55" s="5" t="s">
-        <v>378</v>
-      </c>
-      <c r="B55" s="136" t="s">
-        <v>1162</v>
-      </c>
-      <c r="C55" s="145" t="s">
-        <v>1163</v>
-      </c>
-      <c r="D55" s="121" t="s">
-        <v>1164</v>
-      </c>
-      <c r="E55" s="63" t="s">
-        <v>1165</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6" s="30" customFormat="1" ht="48" x14ac:dyDescent="0.2">
-      <c r="A56" s="5" t="s">
-        <v>378</v>
-      </c>
-      <c r="B56" s="136" t="s">
-        <v>1166</v>
-      </c>
-      <c r="C56" s="145" t="s">
-        <v>1167</v>
-      </c>
-      <c r="D56" s="121" t="s">
-        <v>1168</v>
-      </c>
-      <c r="E56" s="63" t="s">
-        <v>1169</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6" s="30" customFormat="1" ht="32" x14ac:dyDescent="0.2">
-      <c r="A57" s="5" t="s">
-        <v>378</v>
-      </c>
-      <c r="B57" s="136" t="s">
-        <v>1170</v>
-      </c>
-      <c r="C57" s="145" t="s">
-        <v>1171</v>
-      </c>
-      <c r="D57" s="121" t="s">
-        <v>1172</v>
-      </c>
-      <c r="E57" s="63" t="s">
-        <v>1063</v>
-      </c>
-      <c r="F57" s="73" t="s">
-        <v>1173</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6" s="30" customFormat="1" ht="48" x14ac:dyDescent="0.2">
-      <c r="A58" s="5" t="s">
-        <v>378</v>
-      </c>
-      <c r="B58" s="136" t="s">
-        <v>1174</v>
-      </c>
-      <c r="C58" s="145" t="s">
-        <v>1175</v>
-      </c>
-      <c r="D58" s="121" t="s">
-        <v>1176</v>
-      </c>
-      <c r="E58" s="63" t="s">
-        <v>1177</v>
-      </c>
-      <c r="F58" s="73" t="s">
-        <v>1178</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6" s="30" customFormat="1" ht="48" x14ac:dyDescent="0.2">
-      <c r="A59" s="5" t="s">
-        <v>378</v>
-      </c>
-      <c r="B59" s="136" t="s">
-        <v>1179</v>
-      </c>
-      <c r="C59" s="145" t="s">
-        <v>1180</v>
-      </c>
-      <c r="D59" s="121" t="s">
-        <v>1181</v>
-      </c>
-      <c r="E59" s="63" t="s">
-        <v>1182</v>
-      </c>
-      <c r="F59" s="73" t="s">
-        <v>1183</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6" s="30" customFormat="1" ht="32" x14ac:dyDescent="0.2">
-      <c r="A60" s="5" t="s">
-        <v>378</v>
-      </c>
-      <c r="B60" s="136" t="s">
-        <v>1184</v>
-      </c>
-      <c r="C60" s="145" t="s">
-        <v>1185</v>
-      </c>
-      <c r="D60" s="121" t="s">
-        <v>1186</v>
-      </c>
-      <c r="E60" s="63" t="s">
-        <v>1187</v>
-      </c>
-      <c r="F60" s="73" t="s">
-        <v>1188</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6" s="30" customFormat="1" ht="48" x14ac:dyDescent="0.2">
-      <c r="A61" s="5" t="s">
-        <v>378</v>
-      </c>
-      <c r="B61" s="136" t="s">
-        <v>1189</v>
-      </c>
-      <c r="C61" s="145" t="s">
-        <v>1190</v>
-      </c>
-      <c r="D61" s="121" t="s">
-        <v>1191</v>
-      </c>
-      <c r="E61" s="63" t="s">
-        <v>1192</v>
-      </c>
-    </row>
-    <row r="62" spans="1:6" s="30" customFormat="1" ht="48" x14ac:dyDescent="0.2">
-      <c r="A62" s="5" t="s">
-        <v>378</v>
-      </c>
-      <c r="B62" s="136" t="s">
-        <v>1193</v>
-      </c>
-      <c r="C62" s="145" t="s">
-        <v>1194</v>
-      </c>
-      <c r="D62" s="121" t="s">
-        <v>1195</v>
-      </c>
-      <c r="E62" s="63" t="s">
-        <v>1196</v>
-      </c>
-    </row>
-    <row r="63" spans="1:6" s="30" customFormat="1" ht="48" x14ac:dyDescent="0.2">
-      <c r="A63" s="5" t="s">
-        <v>378</v>
-      </c>
-      <c r="B63" s="18" t="s">
-        <v>1197</v>
-      </c>
-      <c r="C63" s="145" t="s">
-        <v>1198</v>
-      </c>
-      <c r="D63" s="121" t="s">
-        <v>1199</v>
-      </c>
-      <c r="E63" s="63" t="s">
-        <v>1200</v>
-      </c>
-    </row>
-    <row r="64" spans="1:6" s="30" customFormat="1" ht="48" x14ac:dyDescent="0.2">
-      <c r="A64" s="5" t="s">
-        <v>378</v>
-      </c>
-      <c r="B64" s="136" t="s">
-        <v>1201</v>
-      </c>
-      <c r="C64" s="145" t="s">
-        <v>1202</v>
-      </c>
-      <c r="D64" s="121" t="s">
-        <v>1203</v>
-      </c>
-      <c r="E64" s="79" t="s">
-        <v>1204</v>
-      </c>
-    </row>
-    <row r="65" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A65" s="144" t="s">
-        <v>721</v>
-      </c>
-      <c r="B65" s="144" t="s">
-        <v>1205</v>
-      </c>
-      <c r="C65" s="145" t="s">
-        <v>1206</v>
-      </c>
-      <c r="D65" s="148"/>
-      <c r="E65" s="78" t="s">
-        <v>1207</v>
-      </c>
-      <c r="F65" s="135"/>
-    </row>
-    <row r="66" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A66" s="144" t="s">
-        <v>721</v>
-      </c>
-      <c r="B66" s="144" t="s">
-        <v>1208</v>
-      </c>
-      <c